<commit_message>
fix: Report non-overlapping surface, subsurface, and total acreage counts in aggregates.
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O81"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,50 +461,35 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>gis_acres</t>
+          <t>parcel_count</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>clipped_acres</t>
+          <t>surface_acres</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>parcel_count</t>
+          <t>surface_parcel_count</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>surface_gis_acres</t>
+          <t>subsurface_acres</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>surface_clipped_acres</t>
+          <t>subsurface_parcel_count</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>surface_parcel_count</t>
+          <t>total_acres</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>subsurface_gis_acres</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>subsurface_clipped_acres</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>subsurface_parcel_count</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>reservation_acres</t>
         </is>
@@ -537,33 +522,24 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>11786.732</v>
+        <v>293</v>
       </c>
       <c r="G2" t="n">
-        <v>11786.67</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>11786.73</v>
+      </c>
+      <c r="J2" t="n">
         <v>293</v>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>11786.73</v>
       </c>
       <c r="L2" t="n">
-        <v>11786.732</v>
-      </c>
-      <c r="M2" t="n">
-        <v>11786.67</v>
-      </c>
-      <c r="N2" t="n">
-        <v>293</v>
-      </c>
-      <c r="O2" t="n">
         <v>114474.93</v>
       </c>
     </row>
@@ -594,33 +570,24 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>369.806</v>
+        <v>3</v>
       </c>
       <c r="G3" t="n">
-        <v>179.11</v>
+        <v>17.01</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>207.711</v>
+        <v>81.20999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>17.01</v>
+        <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>98.22</v>
       </c>
       <c r="L3" t="n">
-        <v>162.095</v>
-      </c>
-      <c r="M3" t="n">
-        <v>162.1</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2</v>
-      </c>
-      <c r="O3" t="n">
         <v>1534569.87</v>
       </c>
     </row>
@@ -651,33 +618,24 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>44.728</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>44.73</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>1</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>44.73</v>
       </c>
       <c r="L4" t="n">
-        <v>44.728</v>
-      </c>
-      <c r="M4" t="n">
-        <v>44.73</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" t="n">
         <v>2241.16</v>
       </c>
     </row>
@@ -710,33 +668,24 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>7155.03</v>
+        <v>181</v>
       </c>
       <c r="G5" t="n">
-        <v>7155.03</v>
+        <v>310.96</v>
       </c>
       <c r="H5" t="n">
-        <v>181</v>
+        <v>8</v>
       </c>
       <c r="I5" t="n">
-        <v>310.94</v>
+        <v>6844.08</v>
       </c>
       <c r="J5" t="n">
-        <v>310.94</v>
+        <v>173</v>
       </c>
       <c r="K5" t="n">
-        <v>8</v>
+        <v>7155.04</v>
       </c>
       <c r="L5" t="n">
-        <v>6844.09</v>
-      </c>
-      <c r="M5" t="n">
-        <v>6844.09</v>
-      </c>
-      <c r="N5" t="n">
-        <v>173</v>
-      </c>
-      <c r="O5" t="n">
         <v>664252.92</v>
       </c>
     </row>
@@ -767,33 +716,24 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>764.422</v>
+        <v>8</v>
       </c>
       <c r="G6" t="n">
-        <v>254.67</v>
+        <v>205.55</v>
       </c>
       <c r="H6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I6" t="n">
-        <v>710.715</v>
+        <v>49.11</v>
       </c>
       <c r="J6" t="n">
-        <v>205.56</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>6</v>
+        <v>254.66</v>
       </c>
       <c r="L6" t="n">
-        <v>53.70699999999999</v>
-      </c>
-      <c r="M6" t="n">
-        <v>49.11</v>
-      </c>
-      <c r="N6" t="n">
-        <v>2</v>
-      </c>
-      <c r="O6" t="n">
         <v>4571.99</v>
       </c>
     </row>
@@ -824,33 +764,24 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1265.184</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
+        <v>632.17</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>632.17</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
         <v>1264.34</v>
       </c>
-      <c r="H7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" t="n">
-        <v>632.592</v>
-      </c>
-      <c r="J7" t="n">
-        <v>632.17</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1</v>
-      </c>
       <c r="L7" t="n">
-        <v>632.592</v>
-      </c>
-      <c r="M7" t="n">
-        <v>632.17</v>
-      </c>
-      <c r="N7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" t="n">
         <v>32730.33</v>
       </c>
     </row>
@@ -883,33 +814,24 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>22243.3</v>
+        <v>555</v>
       </c>
       <c r="G8" t="n">
-        <v>22243.3</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>22203.23</v>
+      </c>
+      <c r="J8" t="n">
         <v>555</v>
       </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>22203.23</v>
       </c>
       <c r="L8" t="n">
-        <v>22243.3</v>
-      </c>
-      <c r="M8" t="n">
-        <v>22243.3</v>
-      </c>
-      <c r="N8" t="n">
-        <v>555</v>
-      </c>
-      <c r="O8" t="n">
         <v>4456452.1</v>
       </c>
     </row>
@@ -940,33 +862,24 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>51905.667</v>
+        <v>851</v>
       </c>
       <c r="G9" t="n">
-        <v>51905.6</v>
+        <v>20429.93</v>
       </c>
       <c r="H9" t="n">
-        <v>851</v>
+        <v>42</v>
       </c>
       <c r="I9" t="n">
-        <v>20429.924</v>
+        <v>31475.74</v>
       </c>
       <c r="J9" t="n">
-        <v>20429.94</v>
+        <v>809</v>
       </c>
       <c r="K9" t="n">
-        <v>42</v>
+        <v>51905.67</v>
       </c>
       <c r="L9" t="n">
-        <v>31475.743</v>
-      </c>
-      <c r="M9" t="n">
-        <v>31475.66</v>
-      </c>
-      <c r="N9" t="n">
-        <v>809</v>
-      </c>
-      <c r="O9" t="n">
         <v>2841283.82</v>
       </c>
     </row>
@@ -1000,33 +913,24 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>79240.25</v>
+        <v>1978</v>
       </c>
       <c r="G10" t="n">
-        <v>79238.73</v>
+        <v>8928.620000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>1978</v>
+        <v>235</v>
       </c>
       <c r="I10" t="n">
-        <v>8930.15</v>
+        <v>67019.86</v>
       </c>
       <c r="J10" t="n">
-        <v>8928.629999999999</v>
+        <v>1743</v>
       </c>
       <c r="K10" t="n">
-        <v>235</v>
+        <v>75948.48</v>
       </c>
       <c r="L10" t="n">
-        <v>70310.10000000001</v>
-      </c>
-      <c r="M10" t="n">
-        <v>70310.10000000001</v>
-      </c>
-      <c r="N10" t="n">
-        <v>1743</v>
-      </c>
-      <c r="O10" t="n">
         <v>5232808.01</v>
       </c>
     </row>
@@ -1059,33 +963,24 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>31672.1</v>
+        <v>764</v>
       </c>
       <c r="G11" t="n">
-        <v>31672.1</v>
+        <v>2182.96</v>
       </c>
       <c r="H11" t="n">
-        <v>764</v>
+        <v>41</v>
       </c>
       <c r="I11" t="n">
-        <v>2342.35</v>
+        <v>28842.21</v>
       </c>
       <c r="J11" t="n">
-        <v>2342.35</v>
+        <v>723</v>
       </c>
       <c r="K11" t="n">
-        <v>41</v>
+        <v>31025.17</v>
       </c>
       <c r="L11" t="n">
-        <v>29329.75</v>
-      </c>
-      <c r="M11" t="n">
-        <v>29329.75</v>
-      </c>
-      <c r="N11" t="n">
-        <v>723</v>
-      </c>
-      <c r="O11" t="n">
         <v>4773452.85</v>
       </c>
     </row>
@@ -1119,33 +1014,24 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>47909.95</v>
+        <v>1188</v>
       </c>
       <c r="G12" t="n">
-        <v>47909.95</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>47069.62</v>
+      </c>
+      <c r="J12" t="n">
         <v>1188</v>
       </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>47069.62</v>
       </c>
       <c r="L12" t="n">
-        <v>47909.95</v>
-      </c>
-      <c r="M12" t="n">
-        <v>47909.95</v>
-      </c>
-      <c r="N12" t="n">
-        <v>1188</v>
-      </c>
-      <c r="O12" t="n">
         <v>6995550.73</v>
       </c>
     </row>
@@ -1177,33 +1063,24 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>20405.29</v>
+        <v>525</v>
       </c>
       <c r="G13" t="n">
-        <v>20405.22</v>
+        <v>3761.53</v>
       </c>
       <c r="H13" t="n">
-        <v>525</v>
+        <v>106</v>
       </c>
       <c r="I13" t="n">
-        <v>3761.6</v>
+        <v>16524.48</v>
       </c>
       <c r="J13" t="n">
-        <v>3761.53</v>
+        <v>419</v>
       </c>
       <c r="K13" t="n">
-        <v>106</v>
+        <v>20286.01</v>
       </c>
       <c r="L13" t="n">
-        <v>16643.69</v>
-      </c>
-      <c r="M13" t="n">
-        <v>16643.69</v>
-      </c>
-      <c r="N13" t="n">
-        <v>419</v>
-      </c>
-      <c r="O13" t="n">
         <v>725652.6800000001</v>
       </c>
     </row>
@@ -1234,33 +1111,24 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>634.5450000000001</v>
+        <v>16</v>
       </c>
       <c r="G14" t="n">
-        <v>634.55</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>634.54</v>
+      </c>
+      <c r="J14" t="n">
         <v>16</v>
       </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>634.54</v>
       </c>
       <c r="L14" t="n">
-        <v>634.5450000000001</v>
-      </c>
-      <c r="M14" t="n">
-        <v>634.55</v>
-      </c>
-      <c r="N14" t="n">
-        <v>16</v>
-      </c>
-      <c r="O14" t="n">
         <v>52186.55</v>
       </c>
     </row>
@@ -1297,33 +1165,24 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>45421.529</v>
+        <v>206</v>
       </c>
       <c r="G15" t="n">
-        <v>40617.33</v>
+        <v>18229.58</v>
       </c>
       <c r="H15" t="n">
-        <v>206</v>
+        <v>88</v>
       </c>
       <c r="I15" t="n">
-        <v>20631.723</v>
+        <v>22387.66</v>
       </c>
       <c r="J15" t="n">
-        <v>18229.63</v>
+        <v>118</v>
       </c>
       <c r="K15" t="n">
-        <v>88</v>
+        <v>40617.24000000001</v>
       </c>
       <c r="L15" t="n">
-        <v>24789.806</v>
-      </c>
-      <c r="M15" t="n">
-        <v>22387.7</v>
-      </c>
-      <c r="N15" t="n">
-        <v>118</v>
-      </c>
-      <c r="O15" t="n">
         <v>344276.22</v>
       </c>
     </row>
@@ -1354,33 +1213,24 @@
         </is>
       </c>
       <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>84.06</v>
       </c>
-      <c r="G16" t="n">
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
         <v>84.06</v>
       </c>
-      <c r="H16" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
       <c r="L16" t="n">
-        <v>84.06</v>
-      </c>
-      <c r="M16" t="n">
-        <v>84.06</v>
-      </c>
-      <c r="N16" t="n">
-        <v>1</v>
-      </c>
-      <c r="O16" t="n">
         <v>1398198.68</v>
       </c>
     </row>
@@ -1413,33 +1263,24 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>16022.74</v>
+        <v>399</v>
       </c>
       <c r="G17" t="n">
-        <v>16022.74</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>15982.61</v>
+      </c>
+      <c r="J17" t="n">
         <v>399</v>
       </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>15982.61</v>
       </c>
       <c r="L17" t="n">
-        <v>16022.74</v>
-      </c>
-      <c r="M17" t="n">
-        <v>16022.74</v>
-      </c>
-      <c r="N17" t="n">
-        <v>399</v>
-      </c>
-      <c r="O17" t="n">
         <v>3063071.94</v>
       </c>
     </row>
@@ -1470,33 +1311,24 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1309.297</v>
+        <v>7</v>
       </c>
       <c r="G18" t="n">
-        <v>1186.43</v>
+        <v>941.63</v>
       </c>
       <c r="H18" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I18" t="n">
-        <v>1064.487</v>
+        <v>244.82</v>
       </c>
       <c r="J18" t="n">
-        <v>941.62</v>
+        <v>2</v>
       </c>
       <c r="K18" t="n">
-        <v>5</v>
+        <v>1186.45</v>
       </c>
       <c r="L18" t="n">
-        <v>244.81</v>
-      </c>
-      <c r="M18" t="n">
-        <v>244.81</v>
-      </c>
-      <c r="N18" t="n">
-        <v>2</v>
-      </c>
-      <c r="O18" t="n">
         <v>2458845.11</v>
       </c>
     </row>
@@ -1527,33 +1359,24 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>2006.328</v>
+        <v>58</v>
       </c>
       <c r="G19" t="n">
-        <v>2006.29</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2006.32</v>
+      </c>
+      <c r="J19" t="n">
         <v>58</v>
       </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>2006.32</v>
       </c>
       <c r="L19" t="n">
-        <v>2006.328</v>
-      </c>
-      <c r="M19" t="n">
-        <v>2006.29</v>
-      </c>
-      <c r="N19" t="n">
-        <v>58</v>
-      </c>
-      <c r="O19" t="n">
         <v>296231.76</v>
       </c>
     </row>
@@ -1584,33 +1407,24 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>111140.484</v>
+        <v>338</v>
       </c>
       <c r="G20" t="n">
-        <v>108896.68</v>
+        <v>29278.81</v>
       </c>
       <c r="H20" t="n">
-        <v>338</v>
+        <v>78</v>
       </c>
       <c r="I20" t="n">
-        <v>30159.664</v>
+        <v>65596.08</v>
       </c>
       <c r="J20" t="n">
-        <v>29278.76</v>
+        <v>260</v>
       </c>
       <c r="K20" t="n">
-        <v>78</v>
+        <v>94874.89</v>
       </c>
       <c r="L20" t="n">
-        <v>80980.82000000001</v>
-      </c>
-      <c r="M20" t="n">
-        <v>79617.92</v>
-      </c>
-      <c r="N20" t="n">
-        <v>260</v>
-      </c>
-      <c r="O20" t="n">
         <v>1318272.89</v>
       </c>
     </row>
@@ -1641,33 +1455,24 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>474.738</v>
+        <v>12</v>
       </c>
       <c r="G21" t="n">
+        <v>226.66</v>
+      </c>
+      <c r="H21" t="n">
+        <v>6</v>
+      </c>
+      <c r="I21" t="n">
+        <v>226.66</v>
+      </c>
+      <c r="J21" t="n">
+        <v>6</v>
+      </c>
+      <c r="K21" t="n">
         <v>453.32</v>
       </c>
-      <c r="H21" t="n">
-        <v>12</v>
-      </c>
-      <c r="I21" t="n">
-        <v>237.369</v>
-      </c>
-      <c r="J21" t="n">
-        <v>226.66</v>
-      </c>
-      <c r="K21" t="n">
-        <v>6</v>
-      </c>
       <c r="L21" t="n">
-        <v>237.369</v>
-      </c>
-      <c r="M21" t="n">
-        <v>226.66</v>
-      </c>
-      <c r="N21" t="n">
-        <v>6</v>
-      </c>
-      <c r="O21" t="n">
         <v>101276.52</v>
       </c>
     </row>
@@ -1698,33 +1503,24 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>44212.075</v>
+        <v>70</v>
       </c>
       <c r="G22" t="n">
-        <v>39372.1</v>
+        <v>19686.06</v>
       </c>
       <c r="H22" t="n">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="I22" t="n">
-        <v>22106.045</v>
+        <v>19686.06</v>
       </c>
       <c r="J22" t="n">
-        <v>19686.05</v>
+        <v>35</v>
       </c>
       <c r="K22" t="n">
-        <v>35</v>
+        <v>39372.12</v>
       </c>
       <c r="L22" t="n">
-        <v>22106.03</v>
-      </c>
-      <c r="M22" t="n">
-        <v>19686.05</v>
-      </c>
-      <c r="N22" t="n">
-        <v>35</v>
-      </c>
-      <c r="O22" t="n">
         <v>651951.87</v>
       </c>
     </row>
@@ -1758,33 +1554,24 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>105944.502</v>
+        <v>868</v>
       </c>
       <c r="G23" t="n">
-        <v>104944.19</v>
+        <v>2865.67</v>
       </c>
       <c r="H23" t="n">
-        <v>868</v>
+        <v>25</v>
       </c>
       <c r="I23" t="n">
-        <v>2866.188</v>
+        <v>102078.33</v>
       </c>
       <c r="J23" t="n">
-        <v>2865.66</v>
+        <v>843</v>
       </c>
       <c r="K23" t="n">
-        <v>25</v>
+        <v>104944</v>
       </c>
       <c r="L23" t="n">
-        <v>103078.314</v>
-      </c>
-      <c r="M23" t="n">
-        <v>102078.53</v>
-      </c>
-      <c r="N23" t="n">
-        <v>843</v>
-      </c>
-      <c r="O23" t="n">
         <v>1014109</v>
       </c>
     </row>
@@ -1816,33 +1603,24 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>243.739</v>
+        <v>5</v>
       </c>
       <c r="G24" t="n">
-        <v>243.73</v>
+        <v>27.22</v>
       </c>
       <c r="H24" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>27.221</v>
+        <v>216.52</v>
       </c>
       <c r="J24" t="n">
-        <v>27.22</v>
+        <v>4</v>
       </c>
       <c r="K24" t="n">
-        <v>1</v>
+        <v>243.74</v>
       </c>
       <c r="L24" t="n">
-        <v>216.518</v>
-      </c>
-      <c r="M24" t="n">
-        <v>216.51</v>
-      </c>
-      <c r="N24" t="n">
-        <v>4</v>
-      </c>
-      <c r="O24" t="n">
         <v>543920</v>
       </c>
     </row>
@@ -1873,33 +1651,24 @@
         </is>
       </c>
       <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
         <v>160.95</v>
       </c>
-      <c r="G25" t="n">
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
         <v>160.95</v>
       </c>
-      <c r="H25" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
       <c r="L25" t="n">
-        <v>160.95</v>
-      </c>
-      <c r="M25" t="n">
-        <v>160.95</v>
-      </c>
-      <c r="N25" t="n">
-        <v>1</v>
-      </c>
-      <c r="O25" t="n">
         <v>52435.46</v>
       </c>
     </row>
@@ -1931,33 +1700,24 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>8072.879</v>
+        <v>46</v>
       </c>
       <c r="G26" t="n">
-        <v>3891.69</v>
+        <v>1809.4</v>
       </c>
       <c r="H26" t="n">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="I26" t="n">
-        <v>3631.97</v>
+        <v>1725.02</v>
       </c>
       <c r="J26" t="n">
-        <v>1809.39</v>
+        <v>31</v>
       </c>
       <c r="K26" t="n">
-        <v>15</v>
+        <v>3534.42</v>
       </c>
       <c r="L26" t="n">
-        <v>4440.909</v>
-      </c>
-      <c r="M26" t="n">
-        <v>2082.3</v>
-      </c>
-      <c r="N26" t="n">
-        <v>31</v>
-      </c>
-      <c r="O26" t="n">
         <v>2110405.94</v>
       </c>
     </row>
@@ -1988,33 +1748,24 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>2214.385</v>
+        <v>11</v>
       </c>
       <c r="G27" t="n">
-        <v>1156.51</v>
+        <v>536.51</v>
       </c>
       <c r="H27" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I27" t="n">
-        <v>955.763</v>
+        <v>619.86</v>
       </c>
       <c r="J27" t="n">
-        <v>536.53</v>
+        <v>5</v>
       </c>
       <c r="K27" t="n">
-        <v>6</v>
+        <v>1156.37</v>
       </c>
       <c r="L27" t="n">
-        <v>1258.622</v>
-      </c>
-      <c r="M27" t="n">
-        <v>619.98</v>
-      </c>
-      <c r="N27" t="n">
-        <v>5</v>
-      </c>
-      <c r="O27" t="n">
         <v>52129.25</v>
       </c>
     </row>
@@ -2045,33 +1796,24 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>370.899</v>
+        <v>9</v>
       </c>
       <c r="G28" t="n">
-        <v>198.29</v>
+        <v>35.13</v>
       </c>
       <c r="H28" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I28" t="n">
-        <v>120.493</v>
+        <v>101.78</v>
       </c>
       <c r="J28" t="n">
-        <v>35.13</v>
+        <v>6</v>
       </c>
       <c r="K28" t="n">
-        <v>3</v>
+        <v>136.91</v>
       </c>
       <c r="L28" t="n">
-        <v>250.406</v>
-      </c>
-      <c r="M28" t="n">
-        <v>163.16</v>
-      </c>
-      <c r="N28" t="n">
-        <v>6</v>
-      </c>
-      <c r="O28" t="n">
         <v>48256.09</v>
       </c>
     </row>
@@ -2102,33 +1844,24 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>8155.178</v>
+        <v>30</v>
       </c>
       <c r="G29" t="n">
-        <v>3285.09</v>
+        <v>1640.9</v>
       </c>
       <c r="H29" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I29" t="n">
-        <v>3986.139</v>
+        <v>1644.18</v>
       </c>
       <c r="J29" t="n">
-        <v>1640.9</v>
+        <v>14</v>
       </c>
       <c r="K29" t="n">
-        <v>16</v>
+        <v>3285.08</v>
       </c>
       <c r="L29" t="n">
-        <v>4169.039</v>
-      </c>
-      <c r="M29" t="n">
-        <v>1644.19</v>
-      </c>
-      <c r="N29" t="n">
-        <v>14</v>
-      </c>
-      <c r="O29" t="n">
         <v>178570.82</v>
       </c>
     </row>
@@ -2159,33 +1892,24 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>2922.643</v>
+        <v>3</v>
       </c>
       <c r="G30" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>29.84</v>
+      </c>
+      <c r="J30" t="n">
+        <v>2</v>
+      </c>
+      <c r="K30" t="n">
         <v>45.64</v>
       </c>
-      <c r="H30" t="n">
-        <v>3</v>
-      </c>
-      <c r="I30" t="n">
-        <v>1135.455</v>
-      </c>
-      <c r="J30" t="n">
-        <v>15.8</v>
-      </c>
-      <c r="K30" t="n">
-        <v>1</v>
-      </c>
       <c r="L30" t="n">
-        <v>1787.188</v>
-      </c>
-      <c r="M30" t="n">
-        <v>29.84</v>
-      </c>
-      <c r="N30" t="n">
-        <v>2</v>
-      </c>
-      <c r="O30" t="n">
         <v>1769675.91</v>
       </c>
     </row>
@@ -2216,33 +1940,24 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>7742.12</v>
+        <v>196</v>
       </c>
       <c r="G31" t="n">
-        <v>7732.27</v>
+        <v>529.04</v>
       </c>
       <c r="H31" t="n">
-        <v>196</v>
+        <v>15</v>
       </c>
       <c r="I31" t="n">
-        <v>538.91</v>
+        <v>7203.18</v>
       </c>
       <c r="J31" t="n">
-        <v>529.0600000000001</v>
+        <v>181</v>
       </c>
       <c r="K31" t="n">
-        <v>15</v>
+        <v>7732.22</v>
       </c>
       <c r="L31" t="n">
-        <v>7203.21</v>
-      </c>
-      <c r="M31" t="n">
-        <v>7203.21</v>
-      </c>
-      <c r="N31" t="n">
-        <v>181</v>
-      </c>
-      <c r="O31" t="n">
         <v>242350.66</v>
       </c>
     </row>
@@ -2273,33 +1988,24 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1219.839</v>
+        <v>36</v>
       </c>
       <c r="G32" t="n">
-        <v>1219.82</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1219.84</v>
+      </c>
+      <c r="J32" t="n">
         <v>36</v>
       </c>
-      <c r="I32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" t="n">
-        <v>0</v>
-      </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>1219.84</v>
       </c>
       <c r="L32" t="n">
-        <v>1219.839</v>
-      </c>
-      <c r="M32" t="n">
-        <v>1219.82</v>
-      </c>
-      <c r="N32" t="n">
-        <v>36</v>
-      </c>
-      <c r="O32" t="n">
         <v>297507.55</v>
       </c>
     </row>
@@ -2330,33 +2036,24 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1583.269</v>
+        <v>43</v>
       </c>
       <c r="G33" t="n">
-        <v>1494.6</v>
+        <v>97.43000000000001</v>
       </c>
       <c r="H33" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="I33" t="n">
-        <v>97</v>
+        <v>1397.18</v>
       </c>
       <c r="J33" t="n">
-        <v>97.43000000000001</v>
+        <v>39</v>
       </c>
       <c r="K33" t="n">
-        <v>4</v>
+        <v>1494.61</v>
       </c>
       <c r="L33" t="n">
-        <v>1486.269</v>
-      </c>
-      <c r="M33" t="n">
-        <v>1397.17</v>
-      </c>
-      <c r="N33" t="n">
-        <v>39</v>
-      </c>
-      <c r="O33" t="n">
         <v>90758.94</v>
       </c>
     </row>
@@ -2387,33 +2084,24 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>531.588</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
         <v>39.41</v>
       </c>
-      <c r="H34" t="n">
+      <c r="J34" t="n">
         <v>1</v>
       </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>39.41</v>
       </c>
       <c r="L34" t="n">
-        <v>531.588</v>
-      </c>
-      <c r="M34" t="n">
-        <v>39.41</v>
-      </c>
-      <c r="N34" t="n">
-        <v>1</v>
-      </c>
-      <c r="O34" t="n">
         <v>5238.47</v>
       </c>
     </row>
@@ -2445,33 +2133,24 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>19597.77</v>
+        <v>495</v>
       </c>
       <c r="G35" t="n">
-        <v>19572.62</v>
+        <v>1518.34</v>
       </c>
       <c r="H35" t="n">
-        <v>495</v>
+        <v>42</v>
       </c>
       <c r="I35" t="n">
-        <v>1518.44</v>
+        <v>18054.33</v>
       </c>
       <c r="J35" t="n">
-        <v>1518.34</v>
+        <v>453</v>
       </c>
       <c r="K35" t="n">
-        <v>42</v>
+        <v>19572.67</v>
       </c>
       <c r="L35" t="n">
-        <v>18079.33</v>
-      </c>
-      <c r="M35" t="n">
-        <v>18054.28</v>
-      </c>
-      <c r="N35" t="n">
-        <v>453</v>
-      </c>
-      <c r="O35" t="n">
         <v>317981.64</v>
       </c>
     </row>
@@ -2503,33 +2182,24 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>1878.61</v>
+        <v>47</v>
       </c>
       <c r="G36" t="n">
-        <v>1792.5</v>
+        <v>79.93000000000001</v>
       </c>
       <c r="H36" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="I36" t="n">
-        <v>80.96000000000001</v>
+        <v>1712.58</v>
       </c>
       <c r="J36" t="n">
-        <v>79.92</v>
+        <v>45</v>
       </c>
       <c r="K36" t="n">
-        <v>2</v>
+        <v>1792.51</v>
       </c>
       <c r="L36" t="n">
-        <v>1797.65</v>
-      </c>
-      <c r="M36" t="n">
-        <v>1712.58</v>
-      </c>
-      <c r="N36" t="n">
-        <v>45</v>
-      </c>
-      <c r="O36" t="n">
         <v>70677.17</v>
       </c>
     </row>
@@ -2561,33 +2231,24 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>10894.33</v>
+        <v>273</v>
       </c>
       <c r="G37" t="n">
-        <v>10894.33</v>
+        <v>1982.04</v>
       </c>
       <c r="H37" t="n">
-        <v>273</v>
+        <v>50</v>
       </c>
       <c r="I37" t="n">
-        <v>1982.02</v>
+        <v>8912.360000000001</v>
       </c>
       <c r="J37" t="n">
-        <v>1982.02</v>
+        <v>223</v>
       </c>
       <c r="K37" t="n">
-        <v>50</v>
+        <v>10894.4</v>
       </c>
       <c r="L37" t="n">
-        <v>8912.309999999999</v>
-      </c>
-      <c r="M37" t="n">
-        <v>8912.309999999999</v>
-      </c>
-      <c r="N37" t="n">
-        <v>223</v>
-      </c>
-      <c r="O37" t="n">
         <v>161318.75</v>
       </c>
     </row>
@@ -2620,33 +2281,24 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>49653.27</v>
+        <v>1251</v>
       </c>
       <c r="G38" t="n">
-        <v>49651.05</v>
+        <v>5897.88</v>
       </c>
       <c r="H38" t="n">
-        <v>1251</v>
+        <v>158</v>
       </c>
       <c r="I38" t="n">
-        <v>5900.08</v>
+        <v>43425.65</v>
       </c>
       <c r="J38" t="n">
-        <v>5897.86</v>
+        <v>1093</v>
       </c>
       <c r="K38" t="n">
-        <v>158</v>
+        <v>49323.53</v>
       </c>
       <c r="L38" t="n">
-        <v>43753.19</v>
-      </c>
-      <c r="M38" t="n">
-        <v>43753.19</v>
-      </c>
-      <c r="N38" t="n">
-        <v>1093</v>
-      </c>
-      <c r="O38" t="n">
         <v>4114525.57</v>
       </c>
     </row>
@@ -2678,33 +2330,24 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>1215.73</v>
+        <v>31</v>
       </c>
       <c r="G39" t="n">
-        <v>1215.73</v>
+        <v>211.77</v>
       </c>
       <c r="H39" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="I39" t="n">
-        <v>211.76</v>
+        <v>1003.97</v>
       </c>
       <c r="J39" t="n">
-        <v>211.76</v>
+        <v>25</v>
       </c>
       <c r="K39" t="n">
-        <v>6</v>
+        <v>1215.74</v>
       </c>
       <c r="L39" t="n">
-        <v>1003.97</v>
-      </c>
-      <c r="M39" t="n">
-        <v>1003.97</v>
-      </c>
-      <c r="N39" t="n">
-        <v>25</v>
-      </c>
-      <c r="O39" t="n">
         <v>123815.99</v>
       </c>
     </row>
@@ -2737,33 +2380,24 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>26309.621</v>
+        <v>695</v>
       </c>
       <c r="G40" t="n">
-        <v>26296.82</v>
+        <v>11225.27</v>
       </c>
       <c r="H40" t="n">
-        <v>695</v>
+        <v>298</v>
       </c>
       <c r="I40" t="n">
-        <v>11237</v>
+        <v>15071.48</v>
       </c>
       <c r="J40" t="n">
-        <v>11225.33</v>
+        <v>397</v>
       </c>
       <c r="K40" t="n">
-        <v>298</v>
+        <v>26296.75</v>
       </c>
       <c r="L40" t="n">
-        <v>15072.621</v>
-      </c>
-      <c r="M40" t="n">
-        <v>15071.49</v>
-      </c>
-      <c r="N40" t="n">
-        <v>397</v>
-      </c>
-      <c r="O40" t="n">
         <v>536257.4300000001</v>
       </c>
     </row>
@@ -2794,33 +2428,24 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>295869.783</v>
+        <v>7559</v>
       </c>
       <c r="G41" t="n">
-        <v>294895.97</v>
+        <v>142232.55</v>
       </c>
       <c r="H41" t="n">
-        <v>7559</v>
+        <v>3640</v>
       </c>
       <c r="I41" t="n">
-        <v>142905.527</v>
+        <v>149223.03</v>
       </c>
       <c r="J41" t="n">
-        <v>142422.32</v>
+        <v>3919</v>
       </c>
       <c r="K41" t="n">
-        <v>3640</v>
+        <v>291455.58</v>
       </c>
       <c r="L41" t="n">
-        <v>152964.256</v>
-      </c>
-      <c r="M41" t="n">
-        <v>152473.65</v>
-      </c>
-      <c r="N41" t="n">
-        <v>3919</v>
-      </c>
-      <c r="O41" t="n">
         <v>823718.64</v>
       </c>
     </row>
@@ -2851,33 +2476,24 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>11.969</v>
+        <v>1</v>
       </c>
       <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
         <v>11.59</v>
       </c>
-      <c r="H42" t="n">
+      <c r="J42" t="n">
         <v>1</v>
       </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>11.59</v>
       </c>
       <c r="L42" t="n">
-        <v>11.969</v>
-      </c>
-      <c r="M42" t="n">
-        <v>11.59</v>
-      </c>
-      <c r="N42" t="n">
-        <v>1</v>
-      </c>
-      <c r="O42" t="n">
         <v>29207.77</v>
       </c>
     </row>
@@ -2908,33 +2524,24 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>3788.782</v>
+        <v>100</v>
       </c>
       <c r="G43" t="n">
-        <v>3788.53</v>
+        <v>958.14</v>
       </c>
       <c r="H43" t="n">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="I43" t="n">
-        <v>958.14</v>
+        <v>2791.18</v>
       </c>
       <c r="J43" t="n">
-        <v>958.15</v>
+        <v>74</v>
       </c>
       <c r="K43" t="n">
-        <v>26</v>
+        <v>3749.32</v>
       </c>
       <c r="L43" t="n">
-        <v>2830.642</v>
-      </c>
-      <c r="M43" t="n">
-        <v>2830.38</v>
-      </c>
-      <c r="N43" t="n">
-        <v>74</v>
-      </c>
-      <c r="O43" t="n">
         <v>65523.3</v>
       </c>
     </row>
@@ -2967,33 +2574,24 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>41074.707</v>
+        <v>547</v>
       </c>
       <c r="G44" t="n">
-        <v>40768.78</v>
+        <v>304.15</v>
       </c>
       <c r="H44" t="n">
-        <v>547</v>
+        <v>10</v>
       </c>
       <c r="I44" t="n">
-        <v>362.938</v>
+        <v>40464.51</v>
       </c>
       <c r="J44" t="n">
-        <v>304.16</v>
+        <v>537</v>
       </c>
       <c r="K44" t="n">
-        <v>10</v>
+        <v>40768.66</v>
       </c>
       <c r="L44" t="n">
-        <v>40711.769</v>
-      </c>
-      <c r="M44" t="n">
-        <v>40464.62</v>
-      </c>
-      <c r="N44" t="n">
-        <v>537</v>
-      </c>
-      <c r="O44" t="n">
         <v>15581907.1</v>
       </c>
     </row>
@@ -3024,33 +2622,24 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>7277.24</v>
+        <v>184</v>
       </c>
       <c r="G45" t="n">
-        <v>7041.14</v>
+        <v>72.62</v>
       </c>
       <c r="H45" t="n">
-        <v>184</v>
+        <v>5</v>
       </c>
       <c r="I45" t="n">
-        <v>196.51</v>
+        <v>6968.54</v>
       </c>
       <c r="J45" t="n">
-        <v>72.63</v>
+        <v>179</v>
       </c>
       <c r="K45" t="n">
-        <v>5</v>
+        <v>7041.16</v>
       </c>
       <c r="L45" t="n">
-        <v>7080.73</v>
-      </c>
-      <c r="M45" t="n">
-        <v>6968.51</v>
-      </c>
-      <c r="N45" t="n">
-        <v>179</v>
-      </c>
-      <c r="O45" t="n">
         <v>77846.99000000001</v>
       </c>
     </row>
@@ -3081,33 +2670,24 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>55838.806</v>
+        <v>1400</v>
       </c>
       <c r="G46" t="n">
-        <v>55840.23</v>
+        <v>24644.52</v>
       </c>
       <c r="H46" t="n">
-        <v>1400</v>
+        <v>618</v>
       </c>
       <c r="I46" t="n">
-        <v>24643</v>
+        <v>31195.81</v>
       </c>
       <c r="J46" t="n">
-        <v>24644.48</v>
+        <v>782</v>
       </c>
       <c r="K46" t="n">
-        <v>618</v>
+        <v>55840.33</v>
       </c>
       <c r="L46" t="n">
-        <v>31195.806</v>
-      </c>
-      <c r="M46" t="n">
-        <v>31195.75</v>
-      </c>
-      <c r="N46" t="n">
-        <v>782</v>
-      </c>
-      <c r="O46" t="n">
         <v>287930.15</v>
       </c>
     </row>
@@ -3145,33 +2725,24 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>16820.282</v>
+        <v>143</v>
       </c>
       <c r="G47" t="n">
-        <v>16326.26</v>
+        <v>4476.66</v>
       </c>
       <c r="H47" t="n">
-        <v>143</v>
+        <v>37</v>
       </c>
       <c r="I47" t="n">
-        <v>4668.765</v>
+        <v>11849.65</v>
       </c>
       <c r="J47" t="n">
-        <v>4476.64</v>
+        <v>106</v>
       </c>
       <c r="K47" t="n">
-        <v>37</v>
+        <v>16326.31</v>
       </c>
       <c r="L47" t="n">
-        <v>12151.517</v>
-      </c>
-      <c r="M47" t="n">
-        <v>11849.62</v>
-      </c>
-      <c r="N47" t="n">
-        <v>106</v>
-      </c>
-      <c r="O47" t="n">
         <v>771137.79</v>
       </c>
     </row>
@@ -3203,33 +2774,24 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>25341.24</v>
+        <v>643</v>
       </c>
       <c r="G48" t="n">
-        <v>25338.49</v>
+        <v>3626.53</v>
       </c>
       <c r="H48" t="n">
-        <v>643</v>
+        <v>97</v>
       </c>
       <c r="I48" t="n">
-        <v>3629.29</v>
+        <v>21551.98</v>
       </c>
       <c r="J48" t="n">
-        <v>3626.54</v>
+        <v>546</v>
       </c>
       <c r="K48" t="n">
-        <v>97</v>
+        <v>25178.51</v>
       </c>
       <c r="L48" t="n">
-        <v>21711.95</v>
-      </c>
-      <c r="M48" t="n">
-        <v>21711.95</v>
-      </c>
-      <c r="N48" t="n">
-        <v>546</v>
-      </c>
-      <c r="O48" t="n">
         <v>343426.64</v>
       </c>
     </row>
@@ -3260,33 +2822,24 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>23405.043</v>
+        <v>313</v>
       </c>
       <c r="G49" t="n">
+        <v>12032.57</v>
+      </c>
+      <c r="H49" t="n">
+        <v>27</v>
+      </c>
+      <c r="I49" t="n">
+        <v>10988.27</v>
+      </c>
+      <c r="J49" t="n">
+        <v>286</v>
+      </c>
+      <c r="K49" t="n">
         <v>23020.84</v>
       </c>
-      <c r="H49" t="n">
-        <v>313</v>
-      </c>
-      <c r="I49" t="n">
-        <v>12416.771</v>
-      </c>
-      <c r="J49" t="n">
-        <v>12032.55</v>
-      </c>
-      <c r="K49" t="n">
-        <v>27</v>
-      </c>
       <c r="L49" t="n">
-        <v>10988.272</v>
-      </c>
-      <c r="M49" t="n">
-        <v>10988.29</v>
-      </c>
-      <c r="N49" t="n">
-        <v>286</v>
-      </c>
-      <c r="O49" t="n">
         <v>2784063.94</v>
       </c>
     </row>
@@ -3317,33 +2870,24 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>948.04</v>
+        <v>24</v>
       </c>
       <c r="G50" t="n">
-        <v>948.04</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>948.05</v>
+      </c>
+      <c r="J50" t="n">
         <v>24</v>
       </c>
-      <c r="I50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" t="n">
-        <v>0</v>
-      </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>948.05</v>
       </c>
       <c r="L50" t="n">
-        <v>948.04</v>
-      </c>
-      <c r="M50" t="n">
-        <v>948.04</v>
-      </c>
-      <c r="N50" t="n">
-        <v>24</v>
-      </c>
-      <c r="O50" t="n">
         <v>106846.86</v>
       </c>
     </row>
@@ -3374,33 +2918,24 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>39.105</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
         <v>36.96</v>
       </c>
-      <c r="H51" t="n">
+      <c r="J51" t="n">
         <v>1</v>
       </c>
-      <c r="I51" t="n">
-        <v>0</v>
-      </c>
-      <c r="J51" t="n">
-        <v>0</v>
-      </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>36.96</v>
       </c>
       <c r="L51" t="n">
-        <v>39.105</v>
-      </c>
-      <c r="M51" t="n">
-        <v>36.96</v>
-      </c>
-      <c r="N51" t="n">
-        <v>1</v>
-      </c>
-      <c r="O51" t="n">
         <v>1823.16</v>
       </c>
     </row>
@@ -3431,33 +2966,24 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>92.36500000000001</v>
+        <v>2</v>
       </c>
       <c r="G52" t="n">
-        <v>92.36000000000001</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>92.36</v>
+      </c>
+      <c r="J52" t="n">
         <v>2</v>
       </c>
-      <c r="I52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J52" t="n">
-        <v>0</v>
-      </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>92.36</v>
       </c>
       <c r="L52" t="n">
-        <v>92.36500000000001</v>
-      </c>
-      <c r="M52" t="n">
-        <v>92.36000000000001</v>
-      </c>
-      <c r="N52" t="n">
-        <v>2</v>
-      </c>
-      <c r="O52" t="n">
         <v>207557.7</v>
       </c>
     </row>
@@ -3488,33 +3014,24 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>72.42399999999999</v>
+        <v>4</v>
       </c>
       <c r="G53" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="H53" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="J53" t="n">
+        <v>2</v>
+      </c>
+      <c r="K53" t="n">
         <v>71.8</v>
       </c>
-      <c r="H53" t="n">
-        <v>4</v>
-      </c>
-      <c r="I53" t="n">
-        <v>36.212</v>
-      </c>
-      <c r="J53" t="n">
-        <v>35.9</v>
-      </c>
-      <c r="K53" t="n">
-        <v>2</v>
-      </c>
       <c r="L53" t="n">
-        <v>36.212</v>
-      </c>
-      <c r="M53" t="n">
-        <v>35.9</v>
-      </c>
-      <c r="N53" t="n">
-        <v>2</v>
-      </c>
-      <c r="O53" t="n">
         <v>836376.45</v>
       </c>
     </row>
@@ -3545,33 +3062,24 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>10502.57</v>
+        <v>31</v>
       </c>
       <c r="G54" t="n">
-        <v>8645.950000000001</v>
+        <v>161.53</v>
       </c>
       <c r="H54" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="I54" t="n">
-        <v>161.53</v>
+        <v>8403.98</v>
       </c>
       <c r="J54" t="n">
-        <v>161.53</v>
+        <v>28</v>
       </c>
       <c r="K54" t="n">
-        <v>3</v>
+        <v>8565.51</v>
       </c>
       <c r="L54" t="n">
-        <v>10341.04</v>
-      </c>
-      <c r="M54" t="n">
-        <v>8484.42</v>
-      </c>
-      <c r="N54" t="n">
-        <v>28</v>
-      </c>
-      <c r="O54" t="n">
         <v>112474.13</v>
       </c>
     </row>
@@ -3602,33 +3110,24 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>5297.898</v>
+        <v>84</v>
       </c>
       <c r="G55" t="n">
-        <v>3311.72</v>
+        <v>232.14</v>
       </c>
       <c r="H55" t="n">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="I55" t="n">
-        <v>2216.634</v>
+        <v>3079.6</v>
       </c>
       <c r="J55" t="n">
-        <v>232.14</v>
+        <v>80</v>
       </c>
       <c r="K55" t="n">
-        <v>4</v>
+        <v>3311.74</v>
       </c>
       <c r="L55" t="n">
-        <v>3081.264</v>
-      </c>
-      <c r="M55" t="n">
-        <v>3079.58</v>
-      </c>
-      <c r="N55" t="n">
-        <v>80</v>
-      </c>
-      <c r="O55" t="n">
         <v>1340326.83</v>
       </c>
     </row>
@@ -3661,33 +3160,24 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>21730.23</v>
+        <v>555</v>
       </c>
       <c r="G56" t="n">
-        <v>21730.23</v>
+        <v>2709.98</v>
       </c>
       <c r="H56" t="n">
-        <v>555</v>
+        <v>79</v>
       </c>
       <c r="I56" t="n">
-        <v>2709.97</v>
+        <v>18940.78</v>
       </c>
       <c r="J56" t="n">
-        <v>2709.97</v>
+        <v>476</v>
       </c>
       <c r="K56" t="n">
-        <v>79</v>
+        <v>21650.76</v>
       </c>
       <c r="L56" t="n">
-        <v>19020.26</v>
-      </c>
-      <c r="M56" t="n">
-        <v>19020.26</v>
-      </c>
-      <c r="N56" t="n">
-        <v>476</v>
-      </c>
-      <c r="O56" t="n">
         <v>480109.99</v>
       </c>
     </row>
@@ -3718,33 +3208,24 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>595.65</v>
+        <v>2</v>
       </c>
       <c r="G57" t="n">
-        <v>592.1700000000001</v>
+        <v>0</v>
       </c>
       <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>592.17</v>
+      </c>
+      <c r="J57" t="n">
         <v>2</v>
       </c>
-      <c r="I57" t="n">
-        <v>0</v>
-      </c>
-      <c r="J57" t="n">
-        <v>0</v>
-      </c>
       <c r="K57" t="n">
-        <v>0</v>
+        <v>592.17</v>
       </c>
       <c r="L57" t="n">
-        <v>595.65</v>
-      </c>
-      <c r="M57" t="n">
-        <v>592.1700000000001</v>
-      </c>
-      <c r="N57" t="n">
-        <v>2</v>
-      </c>
-      <c r="O57" t="n">
         <v>53588.78</v>
       </c>
     </row>
@@ -3775,33 +3256,24 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>1245.904</v>
+        <v>2</v>
       </c>
       <c r="G58" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="H58" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="J58" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" t="n">
         <v>41.4</v>
       </c>
-      <c r="H58" t="n">
-        <v>2</v>
-      </c>
-      <c r="I58" t="n">
-        <v>622.952</v>
-      </c>
-      <c r="J58" t="n">
-        <v>20.7</v>
-      </c>
-      <c r="K58" t="n">
-        <v>1</v>
-      </c>
       <c r="L58" t="n">
-        <v>622.952</v>
-      </c>
-      <c r="M58" t="n">
-        <v>20.7</v>
-      </c>
-      <c r="N58" t="n">
-        <v>1</v>
-      </c>
-      <c r="O58" t="n">
         <v>1858136.26</v>
       </c>
     </row>
@@ -3832,33 +3304,24 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>640.048</v>
+        <v>16</v>
       </c>
       <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
         <v>640.05</v>
       </c>
-      <c r="H59" t="n">
+      <c r="J59" t="n">
         <v>16</v>
       </c>
-      <c r="I59" t="n">
-        <v>0</v>
-      </c>
-      <c r="J59" t="n">
-        <v>0</v>
-      </c>
       <c r="K59" t="n">
-        <v>0</v>
+        <v>640.05</v>
       </c>
       <c r="L59" t="n">
-        <v>640.048</v>
-      </c>
-      <c r="M59" t="n">
-        <v>640.05</v>
-      </c>
-      <c r="N59" t="n">
-        <v>16</v>
-      </c>
-      <c r="O59" t="n">
         <v>51826.81</v>
       </c>
     </row>
@@ -3889,33 +3352,24 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>2501.792</v>
+        <v>64</v>
       </c>
       <c r="G60" t="n">
-        <v>2501.81</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>2501.79</v>
+      </c>
+      <c r="J60" t="n">
         <v>64</v>
       </c>
-      <c r="I60" t="n">
-        <v>0</v>
-      </c>
-      <c r="J60" t="n">
-        <v>0</v>
-      </c>
       <c r="K60" t="n">
-        <v>0</v>
+        <v>2501.79</v>
       </c>
       <c r="L60" t="n">
-        <v>2501.792</v>
-      </c>
-      <c r="M60" t="n">
-        <v>2501.81</v>
-      </c>
-      <c r="N60" t="n">
-        <v>64</v>
-      </c>
-      <c r="O60" t="n">
         <v>79958.52</v>
       </c>
     </row>
@@ -3946,7 +3400,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>2337.334</v>
+        <v>6</v>
       </c>
       <c r="G61" t="n">
         <v>2337.21</v>
@@ -3955,24 +3409,15 @@
         <v>6</v>
       </c>
       <c r="I61" t="n">
-        <v>2337.334</v>
+        <v>0</v>
       </c>
       <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
         <v>2337.21</v>
       </c>
-      <c r="K61" t="n">
-        <v>6</v>
-      </c>
       <c r="L61" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" t="n">
         <v>117388.4</v>
       </c>
     </row>
@@ -4003,33 +3448,24 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>161.83</v>
+        <v>4</v>
       </c>
       <c r="G62" t="n">
-        <v>161.83</v>
+        <v>0</v>
       </c>
       <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>120.64</v>
+      </c>
+      <c r="J62" t="n">
         <v>4</v>
       </c>
-      <c r="I62" t="n">
-        <v>0</v>
-      </c>
-      <c r="J62" t="n">
-        <v>0</v>
-      </c>
       <c r="K62" t="n">
-        <v>0</v>
+        <v>120.64</v>
       </c>
       <c r="L62" t="n">
-        <v>161.83</v>
-      </c>
-      <c r="M62" t="n">
-        <v>161.83</v>
-      </c>
-      <c r="N62" t="n">
-        <v>4</v>
-      </c>
-      <c r="O62" t="n">
         <v>367982.08</v>
       </c>
     </row>
@@ -4060,33 +3496,24 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>80.95099999999999</v>
+        <v>1</v>
       </c>
       <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
         <v>20.3</v>
       </c>
-      <c r="H63" t="n">
+      <c r="J63" t="n">
         <v>1</v>
       </c>
-      <c r="I63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J63" t="n">
-        <v>0</v>
-      </c>
       <c r="K63" t="n">
-        <v>0</v>
+        <v>20.3</v>
       </c>
       <c r="L63" t="n">
-        <v>80.95099999999999</v>
-      </c>
-      <c r="M63" t="n">
-        <v>20.3</v>
-      </c>
-      <c r="N63" t="n">
-        <v>1</v>
-      </c>
-      <c r="O63" t="n">
         <v>3746.52</v>
       </c>
     </row>
@@ -4117,33 +3544,24 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>2390.45</v>
+        <v>18</v>
       </c>
       <c r="G64" t="n">
-        <v>2390.42</v>
+        <v>0</v>
       </c>
       <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>2390.3</v>
+      </c>
+      <c r="J64" t="n">
         <v>18</v>
       </c>
-      <c r="I64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J64" t="n">
-        <v>0</v>
-      </c>
       <c r="K64" t="n">
-        <v>0</v>
+        <v>2390.3</v>
       </c>
       <c r="L64" t="n">
-        <v>2390.45</v>
-      </c>
-      <c r="M64" t="n">
-        <v>2390.42</v>
-      </c>
-      <c r="N64" t="n">
-        <v>18</v>
-      </c>
-      <c r="O64" t="n">
         <v>681609.67</v>
       </c>
     </row>
@@ -4177,33 +3595,24 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>33739.79</v>
+        <v>373</v>
       </c>
       <c r="G65" t="n">
-        <v>32811.2</v>
+        <v>4883.92</v>
       </c>
       <c r="H65" t="n">
-        <v>373</v>
+        <v>56</v>
       </c>
       <c r="I65" t="n">
-        <v>5124.75</v>
+        <v>27927.29</v>
       </c>
       <c r="J65" t="n">
-        <v>4883.94</v>
+        <v>317</v>
       </c>
       <c r="K65" t="n">
-        <v>56</v>
+        <v>32811.21</v>
       </c>
       <c r="L65" t="n">
-        <v>28615.04</v>
-      </c>
-      <c r="M65" t="n">
-        <v>27927.26</v>
-      </c>
-      <c r="N65" t="n">
-        <v>317</v>
-      </c>
-      <c r="O65" t="n">
         <v>247878.71</v>
       </c>
     </row>
@@ -4234,33 +3643,24 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>195.859</v>
+        <v>1</v>
       </c>
       <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
         <v>18.84</v>
       </c>
-      <c r="H66" t="n">
+      <c r="J66" t="n">
         <v>1</v>
       </c>
-      <c r="I66" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" t="n">
-        <v>0</v>
-      </c>
       <c r="K66" t="n">
-        <v>0</v>
+        <v>18.84</v>
       </c>
       <c r="L66" t="n">
-        <v>195.859</v>
-      </c>
-      <c r="M66" t="n">
-        <v>18.84</v>
-      </c>
-      <c r="N66" t="n">
-        <v>1</v>
-      </c>
-      <c r="O66" t="n">
         <v>158625.43</v>
       </c>
     </row>
@@ -4291,33 +3691,24 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>330.452</v>
+        <v>6</v>
       </c>
       <c r="G67" t="n">
-        <v>329.83</v>
+        <v>277.57</v>
       </c>
       <c r="H67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I67" t="n">
-        <v>278.157</v>
+        <v>52.27</v>
       </c>
       <c r="J67" t="n">
-        <v>277.56</v>
+        <v>1</v>
       </c>
       <c r="K67" t="n">
-        <v>5</v>
+        <v>329.84</v>
       </c>
       <c r="L67" t="n">
-        <v>52.295</v>
-      </c>
-      <c r="M67" t="n">
-        <v>52.27</v>
-      </c>
-      <c r="N67" t="n">
-        <v>1</v>
-      </c>
-      <c r="O67" t="n">
         <v>1737.94</v>
       </c>
     </row>
@@ -4353,33 +3744,24 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>119540.142</v>
+        <v>739</v>
       </c>
       <c r="G68" t="n">
-        <v>116988.82</v>
+        <v>46823.4</v>
       </c>
       <c r="H68" t="n">
-        <v>739</v>
+        <v>217</v>
       </c>
       <c r="I68" t="n">
-        <v>46924.222</v>
+        <v>70165.38</v>
       </c>
       <c r="J68" t="n">
-        <v>46823.46</v>
+        <v>522</v>
       </c>
       <c r="K68" t="n">
-        <v>217</v>
+        <v>116988.78</v>
       </c>
       <c r="L68" t="n">
-        <v>72615.92</v>
-      </c>
-      <c r="M68" t="n">
-        <v>70165.36</v>
-      </c>
-      <c r="N68" t="n">
-        <v>522</v>
-      </c>
-      <c r="O68" t="n">
         <v>2347732.03</v>
       </c>
     </row>
@@ -4411,33 +3793,24 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>17243.46</v>
+        <v>33</v>
       </c>
       <c r="G69" t="n">
-        <v>14611.31</v>
+        <v>4903.52</v>
       </c>
       <c r="H69" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="I69" t="n">
-        <v>6219.609</v>
+        <v>9707.76</v>
       </c>
       <c r="J69" t="n">
-        <v>4903.53</v>
+        <v>21</v>
       </c>
       <c r="K69" t="n">
-        <v>12</v>
+        <v>14611.28</v>
       </c>
       <c r="L69" t="n">
-        <v>11023.851</v>
-      </c>
-      <c r="M69" t="n">
-        <v>9707.780000000001</v>
-      </c>
-      <c r="N69" t="n">
-        <v>21</v>
-      </c>
-      <c r="O69" t="n">
         <v>2781661.64</v>
       </c>
     </row>
@@ -4469,33 +3842,24 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>6001.37</v>
+        <v>152</v>
       </c>
       <c r="G70" t="n">
-        <v>5997.74</v>
+        <v>186.91</v>
       </c>
       <c r="H70" t="n">
-        <v>152</v>
+        <v>6</v>
       </c>
       <c r="I70" t="n">
-        <v>186.92</v>
+        <v>5810.78</v>
       </c>
       <c r="J70" t="n">
-        <v>186.92</v>
+        <v>146</v>
       </c>
       <c r="K70" t="n">
-        <v>6</v>
+        <v>5997.69</v>
       </c>
       <c r="L70" t="n">
-        <v>5814.45</v>
-      </c>
-      <c r="M70" t="n">
-        <v>5810.82</v>
-      </c>
-      <c r="N70" t="n">
-        <v>146</v>
-      </c>
-      <c r="O70" t="n">
         <v>91880.64999999999</v>
       </c>
     </row>
@@ -4531,33 +3895,24 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>512489.94</v>
+        <v>1463</v>
       </c>
       <c r="G71" t="n">
-        <v>511561.62</v>
+        <v>230995.4</v>
       </c>
       <c r="H71" t="n">
-        <v>1463</v>
+        <v>672</v>
       </c>
       <c r="I71" t="n">
-        <v>231152.38</v>
+        <v>280566.13</v>
       </c>
       <c r="J71" t="n">
-        <v>230995.48</v>
+        <v>791</v>
       </c>
       <c r="K71" t="n">
-        <v>672</v>
+        <v>511561.53</v>
       </c>
       <c r="L71" t="n">
-        <v>281337.56</v>
-      </c>
-      <c r="M71" t="n">
-        <v>280566.14</v>
-      </c>
-      <c r="N71" t="n">
-        <v>791</v>
-      </c>
-      <c r="O71" t="n">
         <v>4504964.31</v>
       </c>
     </row>
@@ -4588,33 +3943,24 @@
         </is>
       </c>
       <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
         <v>27.71</v>
       </c>
-      <c r="G72" t="n">
+      <c r="J72" t="n">
+        <v>1</v>
+      </c>
+      <c r="K72" t="n">
         <v>27.71</v>
       </c>
-      <c r="H72" t="n">
-        <v>1</v>
-      </c>
-      <c r="I72" t="n">
-        <v>0</v>
-      </c>
-      <c r="J72" t="n">
-        <v>0</v>
-      </c>
-      <c r="K72" t="n">
-        <v>0</v>
-      </c>
       <c r="L72" t="n">
-        <v>27.71</v>
-      </c>
-      <c r="M72" t="n">
-        <v>27.71</v>
-      </c>
-      <c r="N72" t="n">
-        <v>1</v>
-      </c>
-      <c r="O72" t="n">
         <v>293080.11</v>
       </c>
     </row>
@@ -4646,33 +3992,24 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>847.182</v>
+        <v>4</v>
       </c>
       <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="n">
         <v>834.13</v>
       </c>
-      <c r="H73" t="n">
+      <c r="J73" t="n">
         <v>4</v>
       </c>
-      <c r="I73" t="n">
-        <v>0</v>
-      </c>
-      <c r="J73" t="n">
-        <v>0</v>
-      </c>
       <c r="K73" t="n">
-        <v>0</v>
+        <v>834.13</v>
       </c>
       <c r="L73" t="n">
-        <v>847.182</v>
-      </c>
-      <c r="M73" t="n">
-        <v>834.13</v>
-      </c>
-      <c r="N73" t="n">
-        <v>4</v>
-      </c>
-      <c r="O73" t="n">
         <v>598651.62</v>
       </c>
     </row>
@@ -4703,33 +4040,24 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>444.212</v>
+        <v>5</v>
       </c>
       <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
         <v>441.49</v>
       </c>
-      <c r="H74" t="n">
+      <c r="J74" t="n">
         <v>5</v>
       </c>
-      <c r="I74" t="n">
-        <v>0</v>
-      </c>
-      <c r="J74" t="n">
-        <v>0</v>
-      </c>
       <c r="K74" t="n">
-        <v>0</v>
+        <v>441.49</v>
       </c>
       <c r="L74" t="n">
-        <v>444.212</v>
-      </c>
-      <c r="M74" t="n">
-        <v>441.49</v>
-      </c>
-      <c r="N74" t="n">
-        <v>5</v>
-      </c>
-      <c r="O74" t="n">
         <v>657110.6</v>
       </c>
     </row>
@@ -4760,33 +4088,24 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>44469.537</v>
+        <v>1141</v>
       </c>
       <c r="G75" t="n">
-        <v>44452.01</v>
+        <v>17197.01</v>
       </c>
       <c r="H75" t="n">
-        <v>1141</v>
+        <v>440</v>
       </c>
       <c r="I75" t="n">
-        <v>17205.066</v>
+        <v>27174.74</v>
       </c>
       <c r="J75" t="n">
-        <v>17197.05</v>
+        <v>701</v>
       </c>
       <c r="K75" t="n">
-        <v>440</v>
+        <v>44371.75</v>
       </c>
       <c r="L75" t="n">
-        <v>27264.471</v>
-      </c>
-      <c r="M75" t="n">
-        <v>27254.96</v>
-      </c>
-      <c r="N75" t="n">
-        <v>701</v>
-      </c>
-      <c r="O75" t="n">
         <v>747912.54</v>
       </c>
     </row>
@@ -4820,33 +4139,24 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>6198.783</v>
+        <v>89</v>
       </c>
       <c r="G76" t="n">
-        <v>5971.53</v>
+        <v>3665.45</v>
       </c>
       <c r="H76" t="n">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="I76" t="n">
-        <v>3871.371</v>
+        <v>2301.95</v>
       </c>
       <c r="J76" t="n">
-        <v>3667.7</v>
+        <v>39</v>
       </c>
       <c r="K76" t="n">
-        <v>50</v>
+        <v>5967.4</v>
       </c>
       <c r="L76" t="n">
-        <v>2327.412</v>
-      </c>
-      <c r="M76" t="n">
-        <v>2303.83</v>
-      </c>
-      <c r="N76" t="n">
-        <v>39</v>
-      </c>
-      <c r="O76" t="n">
         <v>2066861.74</v>
       </c>
     </row>
@@ -4877,33 +4187,24 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>1248.084</v>
+        <v>2</v>
       </c>
       <c r="G77" t="n">
+        <v>62.54</v>
+      </c>
+      <c r="H77" t="n">
+        <v>1</v>
+      </c>
+      <c r="I77" t="n">
+        <v>62.54</v>
+      </c>
+      <c r="J77" t="n">
+        <v>1</v>
+      </c>
+      <c r="K77" t="n">
         <v>125.08</v>
       </c>
-      <c r="H77" t="n">
-        <v>2</v>
-      </c>
-      <c r="I77" t="n">
-        <v>624.042</v>
-      </c>
-      <c r="J77" t="n">
-        <v>62.54</v>
-      </c>
-      <c r="K77" t="n">
-        <v>1</v>
-      </c>
       <c r="L77" t="n">
-        <v>624.042</v>
-      </c>
-      <c r="M77" t="n">
-        <v>62.54</v>
-      </c>
-      <c r="N77" t="n">
-        <v>1</v>
-      </c>
-      <c r="O77" t="n">
         <v>9807.360000000001</v>
       </c>
     </row>
@@ -4938,33 +4239,24 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>103715.528</v>
+        <v>304</v>
       </c>
       <c r="G78" t="n">
-        <v>91828.75</v>
+        <v>46922.33</v>
       </c>
       <c r="H78" t="n">
-        <v>304</v>
+        <v>152</v>
       </c>
       <c r="I78" t="n">
-        <v>52884.966</v>
+        <v>44906.36</v>
       </c>
       <c r="J78" t="n">
-        <v>46922.37</v>
+        <v>152</v>
       </c>
       <c r="K78" t="n">
-        <v>152</v>
+        <v>91828.69</v>
       </c>
       <c r="L78" t="n">
-        <v>50830.562</v>
-      </c>
-      <c r="M78" t="n">
-        <v>44906.38</v>
-      </c>
-      <c r="N78" t="n">
-        <v>152</v>
-      </c>
-      <c r="O78" t="n">
         <v>1376779.33</v>
       </c>
     </row>
@@ -4995,33 +4287,24 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>411.472</v>
+        <v>11</v>
       </c>
       <c r="G79" t="n">
-        <v>411.48</v>
+        <v>0</v>
       </c>
       <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
+        <v>411.47</v>
+      </c>
+      <c r="J79" t="n">
         <v>11</v>
       </c>
-      <c r="I79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" t="n">
-        <v>0</v>
-      </c>
       <c r="K79" t="n">
-        <v>0</v>
+        <v>411.47</v>
       </c>
       <c r="L79" t="n">
-        <v>411.472</v>
-      </c>
-      <c r="M79" t="n">
-        <v>411.48</v>
-      </c>
-      <c r="N79" t="n">
-        <v>11</v>
-      </c>
-      <c r="O79" t="n">
         <v>441528.7</v>
       </c>
     </row>
@@ -5052,33 +4335,24 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>2078.968</v>
+        <v>52</v>
       </c>
       <c r="G80" t="n">
-        <v>2079</v>
+        <v>0</v>
       </c>
       <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
+        <v>2078.97</v>
+      </c>
+      <c r="J80" t="n">
         <v>52</v>
       </c>
-      <c r="I80" t="n">
-        <v>0</v>
-      </c>
-      <c r="J80" t="n">
-        <v>0</v>
-      </c>
       <c r="K80" t="n">
-        <v>0</v>
+        <v>2078.97</v>
       </c>
       <c r="L80" t="n">
-        <v>2078.968</v>
-      </c>
-      <c r="M80" t="n">
-        <v>2079</v>
-      </c>
-      <c r="N80" t="n">
-        <v>52</v>
-      </c>
-      <c r="O80" t="n">
         <v>134256.19</v>
       </c>
     </row>
@@ -5110,33 +4384,24 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>8137.749</v>
+        <v>189</v>
       </c>
       <c r="G81" t="n">
-        <v>8132.809999999999</v>
+        <v>62.57</v>
       </c>
       <c r="H81" t="n">
-        <v>189</v>
+        <v>2</v>
       </c>
       <c r="I81" t="n">
-        <v>63</v>
+        <v>8070.27</v>
       </c>
       <c r="J81" t="n">
-        <v>62.57</v>
+        <v>187</v>
       </c>
       <c r="K81" t="n">
-        <v>2</v>
+        <v>8132.84</v>
       </c>
       <c r="L81" t="n">
-        <v>8074.749</v>
-      </c>
-      <c r="M81" t="n">
-        <v>8070.24</v>
-      </c>
-      <c r="N81" t="n">
-        <v>187</v>
-      </c>
-      <c r="O81" t="n">
         <v>462553.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: Report non-overlapping surface, subsurface, and total acreage counts in aggregates. (#17)
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O81"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,50 +461,35 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>gis_acres</t>
+          <t>parcel_count</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>clipped_acres</t>
+          <t>surface_acres</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>parcel_count</t>
+          <t>surface_parcel_count</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>surface_gis_acres</t>
+          <t>subsurface_acres</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>surface_clipped_acres</t>
+          <t>subsurface_parcel_count</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>surface_parcel_count</t>
+          <t>total_acres</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>subsurface_gis_acres</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>subsurface_clipped_acres</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>subsurface_parcel_count</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>reservation_acres</t>
         </is>
@@ -537,33 +522,24 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>11786.732</v>
+        <v>293</v>
       </c>
       <c r="G2" t="n">
-        <v>11786.67</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>11786.73</v>
+      </c>
+      <c r="J2" t="n">
         <v>293</v>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>11786.73</v>
       </c>
       <c r="L2" t="n">
-        <v>11786.732</v>
-      </c>
-      <c r="M2" t="n">
-        <v>11786.67</v>
-      </c>
-      <c r="N2" t="n">
-        <v>293</v>
-      </c>
-      <c r="O2" t="n">
         <v>114474.93</v>
       </c>
     </row>
@@ -594,33 +570,24 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>369.806</v>
+        <v>3</v>
       </c>
       <c r="G3" t="n">
-        <v>179.11</v>
+        <v>17.01</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>207.711</v>
+        <v>81.20999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>17.01</v>
+        <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>98.22</v>
       </c>
       <c r="L3" t="n">
-        <v>162.095</v>
-      </c>
-      <c r="M3" t="n">
-        <v>162.1</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2</v>
-      </c>
-      <c r="O3" t="n">
         <v>1534569.87</v>
       </c>
     </row>
@@ -651,33 +618,24 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>44.728</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>44.73</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>1</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>44.73</v>
       </c>
       <c r="L4" t="n">
-        <v>44.728</v>
-      </c>
-      <c r="M4" t="n">
-        <v>44.73</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" t="n">
         <v>2241.16</v>
       </c>
     </row>
@@ -710,33 +668,24 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>7155.03</v>
+        <v>181</v>
       </c>
       <c r="G5" t="n">
-        <v>7155.03</v>
+        <v>310.96</v>
       </c>
       <c r="H5" t="n">
-        <v>181</v>
+        <v>8</v>
       </c>
       <c r="I5" t="n">
-        <v>310.94</v>
+        <v>6844.08</v>
       </c>
       <c r="J5" t="n">
-        <v>310.94</v>
+        <v>173</v>
       </c>
       <c r="K5" t="n">
-        <v>8</v>
+        <v>7155.04</v>
       </c>
       <c r="L5" t="n">
-        <v>6844.09</v>
-      </c>
-      <c r="M5" t="n">
-        <v>6844.09</v>
-      </c>
-      <c r="N5" t="n">
-        <v>173</v>
-      </c>
-      <c r="O5" t="n">
         <v>664252.92</v>
       </c>
     </row>
@@ -767,33 +716,24 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>764.422</v>
+        <v>8</v>
       </c>
       <c r="G6" t="n">
-        <v>254.67</v>
+        <v>205.55</v>
       </c>
       <c r="H6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I6" t="n">
-        <v>710.715</v>
+        <v>49.11</v>
       </c>
       <c r="J6" t="n">
-        <v>205.56</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>6</v>
+        <v>254.66</v>
       </c>
       <c r="L6" t="n">
-        <v>53.70699999999999</v>
-      </c>
-      <c r="M6" t="n">
-        <v>49.11</v>
-      </c>
-      <c r="N6" t="n">
-        <v>2</v>
-      </c>
-      <c r="O6" t="n">
         <v>4571.99</v>
       </c>
     </row>
@@ -824,33 +764,24 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1265.184</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
+        <v>632.17</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>632.17</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
         <v>1264.34</v>
       </c>
-      <c r="H7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" t="n">
-        <v>632.592</v>
-      </c>
-      <c r="J7" t="n">
-        <v>632.17</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1</v>
-      </c>
       <c r="L7" t="n">
-        <v>632.592</v>
-      </c>
-      <c r="M7" t="n">
-        <v>632.17</v>
-      </c>
-      <c r="N7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" t="n">
         <v>32730.33</v>
       </c>
     </row>
@@ -883,33 +814,24 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>22243.3</v>
+        <v>555</v>
       </c>
       <c r="G8" t="n">
-        <v>22243.3</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>22203.23</v>
+      </c>
+      <c r="J8" t="n">
         <v>555</v>
       </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>22203.23</v>
       </c>
       <c r="L8" t="n">
-        <v>22243.3</v>
-      </c>
-      <c r="M8" t="n">
-        <v>22243.3</v>
-      </c>
-      <c r="N8" t="n">
-        <v>555</v>
-      </c>
-      <c r="O8" t="n">
         <v>4456452.1</v>
       </c>
     </row>
@@ -940,33 +862,24 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>51905.667</v>
+        <v>851</v>
       </c>
       <c r="G9" t="n">
-        <v>51905.6</v>
+        <v>20429.93</v>
       </c>
       <c r="H9" t="n">
-        <v>851</v>
+        <v>42</v>
       </c>
       <c r="I9" t="n">
-        <v>20429.924</v>
+        <v>31475.74</v>
       </c>
       <c r="J9" t="n">
-        <v>20429.94</v>
+        <v>809</v>
       </c>
       <c r="K9" t="n">
-        <v>42</v>
+        <v>51905.67</v>
       </c>
       <c r="L9" t="n">
-        <v>31475.743</v>
-      </c>
-      <c r="M9" t="n">
-        <v>31475.66</v>
-      </c>
-      <c r="N9" t="n">
-        <v>809</v>
-      </c>
-      <c r="O9" t="n">
         <v>2841283.82</v>
       </c>
     </row>
@@ -1000,33 +913,24 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>79240.25</v>
+        <v>1978</v>
       </c>
       <c r="G10" t="n">
-        <v>79238.73</v>
+        <v>8928.620000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>1978</v>
+        <v>235</v>
       </c>
       <c r="I10" t="n">
-        <v>8930.15</v>
+        <v>67019.86</v>
       </c>
       <c r="J10" t="n">
-        <v>8928.629999999999</v>
+        <v>1743</v>
       </c>
       <c r="K10" t="n">
-        <v>235</v>
+        <v>75948.48</v>
       </c>
       <c r="L10" t="n">
-        <v>70310.10000000001</v>
-      </c>
-      <c r="M10" t="n">
-        <v>70310.10000000001</v>
-      </c>
-      <c r="N10" t="n">
-        <v>1743</v>
-      </c>
-      <c r="O10" t="n">
         <v>5232808.01</v>
       </c>
     </row>
@@ -1059,33 +963,24 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>31672.1</v>
+        <v>764</v>
       </c>
       <c r="G11" t="n">
-        <v>31672.1</v>
+        <v>2182.96</v>
       </c>
       <c r="H11" t="n">
-        <v>764</v>
+        <v>41</v>
       </c>
       <c r="I11" t="n">
-        <v>2342.35</v>
+        <v>28842.21</v>
       </c>
       <c r="J11" t="n">
-        <v>2342.35</v>
+        <v>723</v>
       </c>
       <c r="K11" t="n">
-        <v>41</v>
+        <v>31025.17</v>
       </c>
       <c r="L11" t="n">
-        <v>29329.75</v>
-      </c>
-      <c r="M11" t="n">
-        <v>29329.75</v>
-      </c>
-      <c r="N11" t="n">
-        <v>723</v>
-      </c>
-      <c r="O11" t="n">
         <v>4773452.85</v>
       </c>
     </row>
@@ -1119,33 +1014,24 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>47909.95</v>
+        <v>1188</v>
       </c>
       <c r="G12" t="n">
-        <v>47909.95</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>47069.62</v>
+      </c>
+      <c r="J12" t="n">
         <v>1188</v>
       </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>47069.62</v>
       </c>
       <c r="L12" t="n">
-        <v>47909.95</v>
-      </c>
-      <c r="M12" t="n">
-        <v>47909.95</v>
-      </c>
-      <c r="N12" t="n">
-        <v>1188</v>
-      </c>
-      <c r="O12" t="n">
         <v>6995550.73</v>
       </c>
     </row>
@@ -1177,33 +1063,24 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>20405.29</v>
+        <v>525</v>
       </c>
       <c r="G13" t="n">
-        <v>20405.22</v>
+        <v>3761.53</v>
       </c>
       <c r="H13" t="n">
-        <v>525</v>
+        <v>106</v>
       </c>
       <c r="I13" t="n">
-        <v>3761.6</v>
+        <v>16524.48</v>
       </c>
       <c r="J13" t="n">
-        <v>3761.53</v>
+        <v>419</v>
       </c>
       <c r="K13" t="n">
-        <v>106</v>
+        <v>20286.01</v>
       </c>
       <c r="L13" t="n">
-        <v>16643.69</v>
-      </c>
-      <c r="M13" t="n">
-        <v>16643.69</v>
-      </c>
-      <c r="N13" t="n">
-        <v>419</v>
-      </c>
-      <c r="O13" t="n">
         <v>725652.6800000001</v>
       </c>
     </row>
@@ -1234,33 +1111,24 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>634.5450000000001</v>
+        <v>16</v>
       </c>
       <c r="G14" t="n">
-        <v>634.55</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>634.54</v>
+      </c>
+      <c r="J14" t="n">
         <v>16</v>
       </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>634.54</v>
       </c>
       <c r="L14" t="n">
-        <v>634.5450000000001</v>
-      </c>
-      <c r="M14" t="n">
-        <v>634.55</v>
-      </c>
-      <c r="N14" t="n">
-        <v>16</v>
-      </c>
-      <c r="O14" t="n">
         <v>52186.55</v>
       </c>
     </row>
@@ -1297,33 +1165,24 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>45421.529</v>
+        <v>206</v>
       </c>
       <c r="G15" t="n">
-        <v>40617.33</v>
+        <v>18229.58</v>
       </c>
       <c r="H15" t="n">
-        <v>206</v>
+        <v>88</v>
       </c>
       <c r="I15" t="n">
-        <v>20631.723</v>
+        <v>22387.66</v>
       </c>
       <c r="J15" t="n">
-        <v>18229.63</v>
+        <v>118</v>
       </c>
       <c r="K15" t="n">
-        <v>88</v>
+        <v>40617.24000000001</v>
       </c>
       <c r="L15" t="n">
-        <v>24789.806</v>
-      </c>
-      <c r="M15" t="n">
-        <v>22387.7</v>
-      </c>
-      <c r="N15" t="n">
-        <v>118</v>
-      </c>
-      <c r="O15" t="n">
         <v>344276.22</v>
       </c>
     </row>
@@ -1354,33 +1213,24 @@
         </is>
       </c>
       <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>84.06</v>
       </c>
-      <c r="G16" t="n">
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
         <v>84.06</v>
       </c>
-      <c r="H16" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
       <c r="L16" t="n">
-        <v>84.06</v>
-      </c>
-      <c r="M16" t="n">
-        <v>84.06</v>
-      </c>
-      <c r="N16" t="n">
-        <v>1</v>
-      </c>
-      <c r="O16" t="n">
         <v>1398198.68</v>
       </c>
     </row>
@@ -1413,33 +1263,24 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>16022.74</v>
+        <v>399</v>
       </c>
       <c r="G17" t="n">
-        <v>16022.74</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>15982.61</v>
+      </c>
+      <c r="J17" t="n">
         <v>399</v>
       </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>15982.61</v>
       </c>
       <c r="L17" t="n">
-        <v>16022.74</v>
-      </c>
-      <c r="M17" t="n">
-        <v>16022.74</v>
-      </c>
-      <c r="N17" t="n">
-        <v>399</v>
-      </c>
-      <c r="O17" t="n">
         <v>3063071.94</v>
       </c>
     </row>
@@ -1470,33 +1311,24 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1309.297</v>
+        <v>7</v>
       </c>
       <c r="G18" t="n">
-        <v>1186.43</v>
+        <v>941.63</v>
       </c>
       <c r="H18" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I18" t="n">
-        <v>1064.487</v>
+        <v>244.82</v>
       </c>
       <c r="J18" t="n">
-        <v>941.62</v>
+        <v>2</v>
       </c>
       <c r="K18" t="n">
-        <v>5</v>
+        <v>1186.45</v>
       </c>
       <c r="L18" t="n">
-        <v>244.81</v>
-      </c>
-      <c r="M18" t="n">
-        <v>244.81</v>
-      </c>
-      <c r="N18" t="n">
-        <v>2</v>
-      </c>
-      <c r="O18" t="n">
         <v>2458845.11</v>
       </c>
     </row>
@@ -1527,33 +1359,24 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>2006.328</v>
+        <v>58</v>
       </c>
       <c r="G19" t="n">
-        <v>2006.29</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2006.32</v>
+      </c>
+      <c r="J19" t="n">
         <v>58</v>
       </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>2006.32</v>
       </c>
       <c r="L19" t="n">
-        <v>2006.328</v>
-      </c>
-      <c r="M19" t="n">
-        <v>2006.29</v>
-      </c>
-      <c r="N19" t="n">
-        <v>58</v>
-      </c>
-      <c r="O19" t="n">
         <v>296231.76</v>
       </c>
     </row>
@@ -1584,33 +1407,24 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>111140.484</v>
+        <v>338</v>
       </c>
       <c r="G20" t="n">
-        <v>108896.68</v>
+        <v>29278.81</v>
       </c>
       <c r="H20" t="n">
-        <v>338</v>
+        <v>78</v>
       </c>
       <c r="I20" t="n">
-        <v>30159.664</v>
+        <v>65596.08</v>
       </c>
       <c r="J20" t="n">
-        <v>29278.76</v>
+        <v>260</v>
       </c>
       <c r="K20" t="n">
-        <v>78</v>
+        <v>94874.89</v>
       </c>
       <c r="L20" t="n">
-        <v>80980.82000000001</v>
-      </c>
-      <c r="M20" t="n">
-        <v>79617.92</v>
-      </c>
-      <c r="N20" t="n">
-        <v>260</v>
-      </c>
-      <c r="O20" t="n">
         <v>1318272.89</v>
       </c>
     </row>
@@ -1641,33 +1455,24 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>474.738</v>
+        <v>12</v>
       </c>
       <c r="G21" t="n">
+        <v>226.66</v>
+      </c>
+      <c r="H21" t="n">
+        <v>6</v>
+      </c>
+      <c r="I21" t="n">
+        <v>226.66</v>
+      </c>
+      <c r="J21" t="n">
+        <v>6</v>
+      </c>
+      <c r="K21" t="n">
         <v>453.32</v>
       </c>
-      <c r="H21" t="n">
-        <v>12</v>
-      </c>
-      <c r="I21" t="n">
-        <v>237.369</v>
-      </c>
-      <c r="J21" t="n">
-        <v>226.66</v>
-      </c>
-      <c r="K21" t="n">
-        <v>6</v>
-      </c>
       <c r="L21" t="n">
-        <v>237.369</v>
-      </c>
-      <c r="M21" t="n">
-        <v>226.66</v>
-      </c>
-      <c r="N21" t="n">
-        <v>6</v>
-      </c>
-      <c r="O21" t="n">
         <v>101276.52</v>
       </c>
     </row>
@@ -1698,33 +1503,24 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>44212.075</v>
+        <v>70</v>
       </c>
       <c r="G22" t="n">
-        <v>39372.1</v>
+        <v>19686.06</v>
       </c>
       <c r="H22" t="n">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="I22" t="n">
-        <v>22106.045</v>
+        <v>19686.06</v>
       </c>
       <c r="J22" t="n">
-        <v>19686.05</v>
+        <v>35</v>
       </c>
       <c r="K22" t="n">
-        <v>35</v>
+        <v>39372.12</v>
       </c>
       <c r="L22" t="n">
-        <v>22106.03</v>
-      </c>
-      <c r="M22" t="n">
-        <v>19686.05</v>
-      </c>
-      <c r="N22" t="n">
-        <v>35</v>
-      </c>
-      <c r="O22" t="n">
         <v>651951.87</v>
       </c>
     </row>
@@ -1758,33 +1554,24 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>105944.502</v>
+        <v>868</v>
       </c>
       <c r="G23" t="n">
-        <v>104944.19</v>
+        <v>2865.67</v>
       </c>
       <c r="H23" t="n">
-        <v>868</v>
+        <v>25</v>
       </c>
       <c r="I23" t="n">
-        <v>2866.188</v>
+        <v>102078.33</v>
       </c>
       <c r="J23" t="n">
-        <v>2865.66</v>
+        <v>843</v>
       </c>
       <c r="K23" t="n">
-        <v>25</v>
+        <v>104944</v>
       </c>
       <c r="L23" t="n">
-        <v>103078.314</v>
-      </c>
-      <c r="M23" t="n">
-        <v>102078.53</v>
-      </c>
-      <c r="N23" t="n">
-        <v>843</v>
-      </c>
-      <c r="O23" t="n">
         <v>1014109</v>
       </c>
     </row>
@@ -1816,33 +1603,24 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>243.739</v>
+        <v>5</v>
       </c>
       <c r="G24" t="n">
-        <v>243.73</v>
+        <v>27.22</v>
       </c>
       <c r="H24" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>27.221</v>
+        <v>216.52</v>
       </c>
       <c r="J24" t="n">
-        <v>27.22</v>
+        <v>4</v>
       </c>
       <c r="K24" t="n">
-        <v>1</v>
+        <v>243.74</v>
       </c>
       <c r="L24" t="n">
-        <v>216.518</v>
-      </c>
-      <c r="M24" t="n">
-        <v>216.51</v>
-      </c>
-      <c r="N24" t="n">
-        <v>4</v>
-      </c>
-      <c r="O24" t="n">
         <v>543920</v>
       </c>
     </row>
@@ -1873,33 +1651,24 @@
         </is>
       </c>
       <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
         <v>160.95</v>
       </c>
-      <c r="G25" t="n">
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
         <v>160.95</v>
       </c>
-      <c r="H25" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
       <c r="L25" t="n">
-        <v>160.95</v>
-      </c>
-      <c r="M25" t="n">
-        <v>160.95</v>
-      </c>
-      <c r="N25" t="n">
-        <v>1</v>
-      </c>
-      <c r="O25" t="n">
         <v>52435.46</v>
       </c>
     </row>
@@ -1931,33 +1700,24 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>8072.879</v>
+        <v>46</v>
       </c>
       <c r="G26" t="n">
-        <v>3891.69</v>
+        <v>1809.4</v>
       </c>
       <c r="H26" t="n">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="I26" t="n">
-        <v>3631.97</v>
+        <v>1725.02</v>
       </c>
       <c r="J26" t="n">
-        <v>1809.39</v>
+        <v>31</v>
       </c>
       <c r="K26" t="n">
-        <v>15</v>
+        <v>3534.42</v>
       </c>
       <c r="L26" t="n">
-        <v>4440.909</v>
-      </c>
-      <c r="M26" t="n">
-        <v>2082.3</v>
-      </c>
-      <c r="N26" t="n">
-        <v>31</v>
-      </c>
-      <c r="O26" t="n">
         <v>2110405.94</v>
       </c>
     </row>
@@ -1988,33 +1748,24 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>2214.385</v>
+        <v>11</v>
       </c>
       <c r="G27" t="n">
-        <v>1156.51</v>
+        <v>536.51</v>
       </c>
       <c r="H27" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I27" t="n">
-        <v>955.763</v>
+        <v>619.86</v>
       </c>
       <c r="J27" t="n">
-        <v>536.53</v>
+        <v>5</v>
       </c>
       <c r="K27" t="n">
-        <v>6</v>
+        <v>1156.37</v>
       </c>
       <c r="L27" t="n">
-        <v>1258.622</v>
-      </c>
-      <c r="M27" t="n">
-        <v>619.98</v>
-      </c>
-      <c r="N27" t="n">
-        <v>5</v>
-      </c>
-      <c r="O27" t="n">
         <v>52129.25</v>
       </c>
     </row>
@@ -2045,33 +1796,24 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>370.899</v>
+        <v>9</v>
       </c>
       <c r="G28" t="n">
-        <v>198.29</v>
+        <v>35.13</v>
       </c>
       <c r="H28" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I28" t="n">
-        <v>120.493</v>
+        <v>101.78</v>
       </c>
       <c r="J28" t="n">
-        <v>35.13</v>
+        <v>6</v>
       </c>
       <c r="K28" t="n">
-        <v>3</v>
+        <v>136.91</v>
       </c>
       <c r="L28" t="n">
-        <v>250.406</v>
-      </c>
-      <c r="M28" t="n">
-        <v>163.16</v>
-      </c>
-      <c r="N28" t="n">
-        <v>6</v>
-      </c>
-      <c r="O28" t="n">
         <v>48256.09</v>
       </c>
     </row>
@@ -2102,33 +1844,24 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>8155.178</v>
+        <v>30</v>
       </c>
       <c r="G29" t="n">
-        <v>3285.09</v>
+        <v>1640.9</v>
       </c>
       <c r="H29" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I29" t="n">
-        <v>3986.139</v>
+        <v>1644.18</v>
       </c>
       <c r="J29" t="n">
-        <v>1640.9</v>
+        <v>14</v>
       </c>
       <c r="K29" t="n">
-        <v>16</v>
+        <v>3285.08</v>
       </c>
       <c r="L29" t="n">
-        <v>4169.039</v>
-      </c>
-      <c r="M29" t="n">
-        <v>1644.19</v>
-      </c>
-      <c r="N29" t="n">
-        <v>14</v>
-      </c>
-      <c r="O29" t="n">
         <v>178570.82</v>
       </c>
     </row>
@@ -2159,33 +1892,24 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>2922.643</v>
+        <v>3</v>
       </c>
       <c r="G30" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>29.84</v>
+      </c>
+      <c r="J30" t="n">
+        <v>2</v>
+      </c>
+      <c r="K30" t="n">
         <v>45.64</v>
       </c>
-      <c r="H30" t="n">
-        <v>3</v>
-      </c>
-      <c r="I30" t="n">
-        <v>1135.455</v>
-      </c>
-      <c r="J30" t="n">
-        <v>15.8</v>
-      </c>
-      <c r="K30" t="n">
-        <v>1</v>
-      </c>
       <c r="L30" t="n">
-        <v>1787.188</v>
-      </c>
-      <c r="M30" t="n">
-        <v>29.84</v>
-      </c>
-      <c r="N30" t="n">
-        <v>2</v>
-      </c>
-      <c r="O30" t="n">
         <v>1769675.91</v>
       </c>
     </row>
@@ -2216,33 +1940,24 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>7742.12</v>
+        <v>196</v>
       </c>
       <c r="G31" t="n">
-        <v>7732.27</v>
+        <v>529.04</v>
       </c>
       <c r="H31" t="n">
-        <v>196</v>
+        <v>15</v>
       </c>
       <c r="I31" t="n">
-        <v>538.91</v>
+        <v>7203.18</v>
       </c>
       <c r="J31" t="n">
-        <v>529.0600000000001</v>
+        <v>181</v>
       </c>
       <c r="K31" t="n">
-        <v>15</v>
+        <v>7732.22</v>
       </c>
       <c r="L31" t="n">
-        <v>7203.21</v>
-      </c>
-      <c r="M31" t="n">
-        <v>7203.21</v>
-      </c>
-      <c r="N31" t="n">
-        <v>181</v>
-      </c>
-      <c r="O31" t="n">
         <v>242350.66</v>
       </c>
     </row>
@@ -2273,33 +1988,24 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1219.839</v>
+        <v>36</v>
       </c>
       <c r="G32" t="n">
-        <v>1219.82</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1219.84</v>
+      </c>
+      <c r="J32" t="n">
         <v>36</v>
       </c>
-      <c r="I32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" t="n">
-        <v>0</v>
-      </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>1219.84</v>
       </c>
       <c r="L32" t="n">
-        <v>1219.839</v>
-      </c>
-      <c r="M32" t="n">
-        <v>1219.82</v>
-      </c>
-      <c r="N32" t="n">
-        <v>36</v>
-      </c>
-      <c r="O32" t="n">
         <v>297507.55</v>
       </c>
     </row>
@@ -2330,33 +2036,24 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1583.269</v>
+        <v>43</v>
       </c>
       <c r="G33" t="n">
-        <v>1494.6</v>
+        <v>97.43000000000001</v>
       </c>
       <c r="H33" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="I33" t="n">
-        <v>97</v>
+        <v>1397.18</v>
       </c>
       <c r="J33" t="n">
-        <v>97.43000000000001</v>
+        <v>39</v>
       </c>
       <c r="K33" t="n">
-        <v>4</v>
+        <v>1494.61</v>
       </c>
       <c r="L33" t="n">
-        <v>1486.269</v>
-      </c>
-      <c r="M33" t="n">
-        <v>1397.17</v>
-      </c>
-      <c r="N33" t="n">
-        <v>39</v>
-      </c>
-      <c r="O33" t="n">
         <v>90758.94</v>
       </c>
     </row>
@@ -2387,33 +2084,24 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>531.588</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
         <v>39.41</v>
       </c>
-      <c r="H34" t="n">
+      <c r="J34" t="n">
         <v>1</v>
       </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>39.41</v>
       </c>
       <c r="L34" t="n">
-        <v>531.588</v>
-      </c>
-      <c r="M34" t="n">
-        <v>39.41</v>
-      </c>
-      <c r="N34" t="n">
-        <v>1</v>
-      </c>
-      <c r="O34" t="n">
         <v>5238.47</v>
       </c>
     </row>
@@ -2445,33 +2133,24 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>19597.77</v>
+        <v>495</v>
       </c>
       <c r="G35" t="n">
-        <v>19572.62</v>
+        <v>1518.34</v>
       </c>
       <c r="H35" t="n">
-        <v>495</v>
+        <v>42</v>
       </c>
       <c r="I35" t="n">
-        <v>1518.44</v>
+        <v>18054.33</v>
       </c>
       <c r="J35" t="n">
-        <v>1518.34</v>
+        <v>453</v>
       </c>
       <c r="K35" t="n">
-        <v>42</v>
+        <v>19572.67</v>
       </c>
       <c r="L35" t="n">
-        <v>18079.33</v>
-      </c>
-      <c r="M35" t="n">
-        <v>18054.28</v>
-      </c>
-      <c r="N35" t="n">
-        <v>453</v>
-      </c>
-      <c r="O35" t="n">
         <v>317981.64</v>
       </c>
     </row>
@@ -2503,33 +2182,24 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>1878.61</v>
+        <v>47</v>
       </c>
       <c r="G36" t="n">
-        <v>1792.5</v>
+        <v>79.93000000000001</v>
       </c>
       <c r="H36" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="I36" t="n">
-        <v>80.96000000000001</v>
+        <v>1712.58</v>
       </c>
       <c r="J36" t="n">
-        <v>79.92</v>
+        <v>45</v>
       </c>
       <c r="K36" t="n">
-        <v>2</v>
+        <v>1792.51</v>
       </c>
       <c r="L36" t="n">
-        <v>1797.65</v>
-      </c>
-      <c r="M36" t="n">
-        <v>1712.58</v>
-      </c>
-      <c r="N36" t="n">
-        <v>45</v>
-      </c>
-      <c r="O36" t="n">
         <v>70677.17</v>
       </c>
     </row>
@@ -2561,33 +2231,24 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>10894.33</v>
+        <v>273</v>
       </c>
       <c r="G37" t="n">
-        <v>10894.33</v>
+        <v>1982.04</v>
       </c>
       <c r="H37" t="n">
-        <v>273</v>
+        <v>50</v>
       </c>
       <c r="I37" t="n">
-        <v>1982.02</v>
+        <v>8912.360000000001</v>
       </c>
       <c r="J37" t="n">
-        <v>1982.02</v>
+        <v>223</v>
       </c>
       <c r="K37" t="n">
-        <v>50</v>
+        <v>10894.4</v>
       </c>
       <c r="L37" t="n">
-        <v>8912.309999999999</v>
-      </c>
-      <c r="M37" t="n">
-        <v>8912.309999999999</v>
-      </c>
-      <c r="N37" t="n">
-        <v>223</v>
-      </c>
-      <c r="O37" t="n">
         <v>161318.75</v>
       </c>
     </row>
@@ -2620,33 +2281,24 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>49653.27</v>
+        <v>1251</v>
       </c>
       <c r="G38" t="n">
-        <v>49651.05</v>
+        <v>5897.88</v>
       </c>
       <c r="H38" t="n">
-        <v>1251</v>
+        <v>158</v>
       </c>
       <c r="I38" t="n">
-        <v>5900.08</v>
+        <v>43425.65</v>
       </c>
       <c r="J38" t="n">
-        <v>5897.86</v>
+        <v>1093</v>
       </c>
       <c r="K38" t="n">
-        <v>158</v>
+        <v>49323.53</v>
       </c>
       <c r="L38" t="n">
-        <v>43753.19</v>
-      </c>
-      <c r="M38" t="n">
-        <v>43753.19</v>
-      </c>
-      <c r="N38" t="n">
-        <v>1093</v>
-      </c>
-      <c r="O38" t="n">
         <v>4114525.57</v>
       </c>
     </row>
@@ -2678,33 +2330,24 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>1215.73</v>
+        <v>31</v>
       </c>
       <c r="G39" t="n">
-        <v>1215.73</v>
+        <v>211.77</v>
       </c>
       <c r="H39" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="I39" t="n">
-        <v>211.76</v>
+        <v>1003.97</v>
       </c>
       <c r="J39" t="n">
-        <v>211.76</v>
+        <v>25</v>
       </c>
       <c r="K39" t="n">
-        <v>6</v>
+        <v>1215.74</v>
       </c>
       <c r="L39" t="n">
-        <v>1003.97</v>
-      </c>
-      <c r="M39" t="n">
-        <v>1003.97</v>
-      </c>
-      <c r="N39" t="n">
-        <v>25</v>
-      </c>
-      <c r="O39" t="n">
         <v>123815.99</v>
       </c>
     </row>
@@ -2737,33 +2380,24 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>26309.621</v>
+        <v>695</v>
       </c>
       <c r="G40" t="n">
-        <v>26296.82</v>
+        <v>11225.27</v>
       </c>
       <c r="H40" t="n">
-        <v>695</v>
+        <v>298</v>
       </c>
       <c r="I40" t="n">
-        <v>11237</v>
+        <v>15071.48</v>
       </c>
       <c r="J40" t="n">
-        <v>11225.33</v>
+        <v>397</v>
       </c>
       <c r="K40" t="n">
-        <v>298</v>
+        <v>26296.75</v>
       </c>
       <c r="L40" t="n">
-        <v>15072.621</v>
-      </c>
-      <c r="M40" t="n">
-        <v>15071.49</v>
-      </c>
-      <c r="N40" t="n">
-        <v>397</v>
-      </c>
-      <c r="O40" t="n">
         <v>536257.4300000001</v>
       </c>
     </row>
@@ -2794,33 +2428,24 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>295869.783</v>
+        <v>7559</v>
       </c>
       <c r="G41" t="n">
-        <v>294895.97</v>
+        <v>142232.55</v>
       </c>
       <c r="H41" t="n">
-        <v>7559</v>
+        <v>3640</v>
       </c>
       <c r="I41" t="n">
-        <v>142905.527</v>
+        <v>149223.03</v>
       </c>
       <c r="J41" t="n">
-        <v>142422.32</v>
+        <v>3919</v>
       </c>
       <c r="K41" t="n">
-        <v>3640</v>
+        <v>291455.58</v>
       </c>
       <c r="L41" t="n">
-        <v>152964.256</v>
-      </c>
-      <c r="M41" t="n">
-        <v>152473.65</v>
-      </c>
-      <c r="N41" t="n">
-        <v>3919</v>
-      </c>
-      <c r="O41" t="n">
         <v>823718.64</v>
       </c>
     </row>
@@ -2851,33 +2476,24 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>11.969</v>
+        <v>1</v>
       </c>
       <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
         <v>11.59</v>
       </c>
-      <c r="H42" t="n">
+      <c r="J42" t="n">
         <v>1</v>
       </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>11.59</v>
       </c>
       <c r="L42" t="n">
-        <v>11.969</v>
-      </c>
-      <c r="M42" t="n">
-        <v>11.59</v>
-      </c>
-      <c r="N42" t="n">
-        <v>1</v>
-      </c>
-      <c r="O42" t="n">
         <v>29207.77</v>
       </c>
     </row>
@@ -2908,33 +2524,24 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>3788.782</v>
+        <v>100</v>
       </c>
       <c r="G43" t="n">
-        <v>3788.53</v>
+        <v>958.14</v>
       </c>
       <c r="H43" t="n">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="I43" t="n">
-        <v>958.14</v>
+        <v>2791.18</v>
       </c>
       <c r="J43" t="n">
-        <v>958.15</v>
+        <v>74</v>
       </c>
       <c r="K43" t="n">
-        <v>26</v>
+        <v>3749.32</v>
       </c>
       <c r="L43" t="n">
-        <v>2830.642</v>
-      </c>
-      <c r="M43" t="n">
-        <v>2830.38</v>
-      </c>
-      <c r="N43" t="n">
-        <v>74</v>
-      </c>
-      <c r="O43" t="n">
         <v>65523.3</v>
       </c>
     </row>
@@ -2967,33 +2574,24 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>41074.707</v>
+        <v>547</v>
       </c>
       <c r="G44" t="n">
-        <v>40768.78</v>
+        <v>304.15</v>
       </c>
       <c r="H44" t="n">
-        <v>547</v>
+        <v>10</v>
       </c>
       <c r="I44" t="n">
-        <v>362.938</v>
+        <v>40464.51</v>
       </c>
       <c r="J44" t="n">
-        <v>304.16</v>
+        <v>537</v>
       </c>
       <c r="K44" t="n">
-        <v>10</v>
+        <v>40768.66</v>
       </c>
       <c r="L44" t="n">
-        <v>40711.769</v>
-      </c>
-      <c r="M44" t="n">
-        <v>40464.62</v>
-      </c>
-      <c r="N44" t="n">
-        <v>537</v>
-      </c>
-      <c r="O44" t="n">
         <v>15581907.1</v>
       </c>
     </row>
@@ -3024,33 +2622,24 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>7277.24</v>
+        <v>184</v>
       </c>
       <c r="G45" t="n">
-        <v>7041.14</v>
+        <v>72.62</v>
       </c>
       <c r="H45" t="n">
-        <v>184</v>
+        <v>5</v>
       </c>
       <c r="I45" t="n">
-        <v>196.51</v>
+        <v>6968.54</v>
       </c>
       <c r="J45" t="n">
-        <v>72.63</v>
+        <v>179</v>
       </c>
       <c r="K45" t="n">
-        <v>5</v>
+        <v>7041.16</v>
       </c>
       <c r="L45" t="n">
-        <v>7080.73</v>
-      </c>
-      <c r="M45" t="n">
-        <v>6968.51</v>
-      </c>
-      <c r="N45" t="n">
-        <v>179</v>
-      </c>
-      <c r="O45" t="n">
         <v>77846.99000000001</v>
       </c>
     </row>
@@ -3081,33 +2670,24 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>55838.806</v>
+        <v>1400</v>
       </c>
       <c r="G46" t="n">
-        <v>55840.23</v>
+        <v>24644.52</v>
       </c>
       <c r="H46" t="n">
-        <v>1400</v>
+        <v>618</v>
       </c>
       <c r="I46" t="n">
-        <v>24643</v>
+        <v>31195.81</v>
       </c>
       <c r="J46" t="n">
-        <v>24644.48</v>
+        <v>782</v>
       </c>
       <c r="K46" t="n">
-        <v>618</v>
+        <v>55840.33</v>
       </c>
       <c r="L46" t="n">
-        <v>31195.806</v>
-      </c>
-      <c r="M46" t="n">
-        <v>31195.75</v>
-      </c>
-      <c r="N46" t="n">
-        <v>782</v>
-      </c>
-      <c r="O46" t="n">
         <v>287930.15</v>
       </c>
     </row>
@@ -3145,33 +2725,24 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>16820.282</v>
+        <v>143</v>
       </c>
       <c r="G47" t="n">
-        <v>16326.26</v>
+        <v>4476.66</v>
       </c>
       <c r="H47" t="n">
-        <v>143</v>
+        <v>37</v>
       </c>
       <c r="I47" t="n">
-        <v>4668.765</v>
+        <v>11849.65</v>
       </c>
       <c r="J47" t="n">
-        <v>4476.64</v>
+        <v>106</v>
       </c>
       <c r="K47" t="n">
-        <v>37</v>
+        <v>16326.31</v>
       </c>
       <c r="L47" t="n">
-        <v>12151.517</v>
-      </c>
-      <c r="M47" t="n">
-        <v>11849.62</v>
-      </c>
-      <c r="N47" t="n">
-        <v>106</v>
-      </c>
-      <c r="O47" t="n">
         <v>771137.79</v>
       </c>
     </row>
@@ -3203,33 +2774,24 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>25341.24</v>
+        <v>643</v>
       </c>
       <c r="G48" t="n">
-        <v>25338.49</v>
+        <v>3626.53</v>
       </c>
       <c r="H48" t="n">
-        <v>643</v>
+        <v>97</v>
       </c>
       <c r="I48" t="n">
-        <v>3629.29</v>
+        <v>21551.98</v>
       </c>
       <c r="J48" t="n">
-        <v>3626.54</v>
+        <v>546</v>
       </c>
       <c r="K48" t="n">
-        <v>97</v>
+        <v>25178.51</v>
       </c>
       <c r="L48" t="n">
-        <v>21711.95</v>
-      </c>
-      <c r="M48" t="n">
-        <v>21711.95</v>
-      </c>
-      <c r="N48" t="n">
-        <v>546</v>
-      </c>
-      <c r="O48" t="n">
         <v>343426.64</v>
       </c>
     </row>
@@ -3260,33 +2822,24 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>23405.043</v>
+        <v>313</v>
       </c>
       <c r="G49" t="n">
+        <v>12032.57</v>
+      </c>
+      <c r="H49" t="n">
+        <v>27</v>
+      </c>
+      <c r="I49" t="n">
+        <v>10988.27</v>
+      </c>
+      <c r="J49" t="n">
+        <v>286</v>
+      </c>
+      <c r="K49" t="n">
         <v>23020.84</v>
       </c>
-      <c r="H49" t="n">
-        <v>313</v>
-      </c>
-      <c r="I49" t="n">
-        <v>12416.771</v>
-      </c>
-      <c r="J49" t="n">
-        <v>12032.55</v>
-      </c>
-      <c r="K49" t="n">
-        <v>27</v>
-      </c>
       <c r="L49" t="n">
-        <v>10988.272</v>
-      </c>
-      <c r="M49" t="n">
-        <v>10988.29</v>
-      </c>
-      <c r="N49" t="n">
-        <v>286</v>
-      </c>
-      <c r="O49" t="n">
         <v>2784063.94</v>
       </c>
     </row>
@@ -3317,33 +2870,24 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>948.04</v>
+        <v>24</v>
       </c>
       <c r="G50" t="n">
-        <v>948.04</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>948.05</v>
+      </c>
+      <c r="J50" t="n">
         <v>24</v>
       </c>
-      <c r="I50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" t="n">
-        <v>0</v>
-      </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>948.05</v>
       </c>
       <c r="L50" t="n">
-        <v>948.04</v>
-      </c>
-      <c r="M50" t="n">
-        <v>948.04</v>
-      </c>
-      <c r="N50" t="n">
-        <v>24</v>
-      </c>
-      <c r="O50" t="n">
         <v>106846.86</v>
       </c>
     </row>
@@ -3374,33 +2918,24 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>39.105</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
         <v>36.96</v>
       </c>
-      <c r="H51" t="n">
+      <c r="J51" t="n">
         <v>1</v>
       </c>
-      <c r="I51" t="n">
-        <v>0</v>
-      </c>
-      <c r="J51" t="n">
-        <v>0</v>
-      </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>36.96</v>
       </c>
       <c r="L51" t="n">
-        <v>39.105</v>
-      </c>
-      <c r="M51" t="n">
-        <v>36.96</v>
-      </c>
-      <c r="N51" t="n">
-        <v>1</v>
-      </c>
-      <c r="O51" t="n">
         <v>1823.16</v>
       </c>
     </row>
@@ -3431,33 +2966,24 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>92.36500000000001</v>
+        <v>2</v>
       </c>
       <c r="G52" t="n">
-        <v>92.36000000000001</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>92.36</v>
+      </c>
+      <c r="J52" t="n">
         <v>2</v>
       </c>
-      <c r="I52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J52" t="n">
-        <v>0</v>
-      </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>92.36</v>
       </c>
       <c r="L52" t="n">
-        <v>92.36500000000001</v>
-      </c>
-      <c r="M52" t="n">
-        <v>92.36000000000001</v>
-      </c>
-      <c r="N52" t="n">
-        <v>2</v>
-      </c>
-      <c r="O52" t="n">
         <v>207557.7</v>
       </c>
     </row>
@@ -3488,33 +3014,24 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>72.42399999999999</v>
+        <v>4</v>
       </c>
       <c r="G53" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="H53" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="J53" t="n">
+        <v>2</v>
+      </c>
+      <c r="K53" t="n">
         <v>71.8</v>
       </c>
-      <c r="H53" t="n">
-        <v>4</v>
-      </c>
-      <c r="I53" t="n">
-        <v>36.212</v>
-      </c>
-      <c r="J53" t="n">
-        <v>35.9</v>
-      </c>
-      <c r="K53" t="n">
-        <v>2</v>
-      </c>
       <c r="L53" t="n">
-        <v>36.212</v>
-      </c>
-      <c r="M53" t="n">
-        <v>35.9</v>
-      </c>
-      <c r="N53" t="n">
-        <v>2</v>
-      </c>
-      <c r="O53" t="n">
         <v>836376.45</v>
       </c>
     </row>
@@ -3545,33 +3062,24 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>10502.57</v>
+        <v>31</v>
       </c>
       <c r="G54" t="n">
-        <v>8645.950000000001</v>
+        <v>161.53</v>
       </c>
       <c r="H54" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="I54" t="n">
-        <v>161.53</v>
+        <v>8403.98</v>
       </c>
       <c r="J54" t="n">
-        <v>161.53</v>
+        <v>28</v>
       </c>
       <c r="K54" t="n">
-        <v>3</v>
+        <v>8565.51</v>
       </c>
       <c r="L54" t="n">
-        <v>10341.04</v>
-      </c>
-      <c r="M54" t="n">
-        <v>8484.42</v>
-      </c>
-      <c r="N54" t="n">
-        <v>28</v>
-      </c>
-      <c r="O54" t="n">
         <v>112474.13</v>
       </c>
     </row>
@@ -3602,33 +3110,24 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>5297.898</v>
+        <v>84</v>
       </c>
       <c r="G55" t="n">
-        <v>3311.72</v>
+        <v>232.14</v>
       </c>
       <c r="H55" t="n">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="I55" t="n">
-        <v>2216.634</v>
+        <v>3079.6</v>
       </c>
       <c r="J55" t="n">
-        <v>232.14</v>
+        <v>80</v>
       </c>
       <c r="K55" t="n">
-        <v>4</v>
+        <v>3311.74</v>
       </c>
       <c r="L55" t="n">
-        <v>3081.264</v>
-      </c>
-      <c r="M55" t="n">
-        <v>3079.58</v>
-      </c>
-      <c r="N55" t="n">
-        <v>80</v>
-      </c>
-      <c r="O55" t="n">
         <v>1340326.83</v>
       </c>
     </row>
@@ -3661,33 +3160,24 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>21730.23</v>
+        <v>555</v>
       </c>
       <c r="G56" t="n">
-        <v>21730.23</v>
+        <v>2709.98</v>
       </c>
       <c r="H56" t="n">
-        <v>555</v>
+        <v>79</v>
       </c>
       <c r="I56" t="n">
-        <v>2709.97</v>
+        <v>18940.78</v>
       </c>
       <c r="J56" t="n">
-        <v>2709.97</v>
+        <v>476</v>
       </c>
       <c r="K56" t="n">
-        <v>79</v>
+        <v>21650.76</v>
       </c>
       <c r="L56" t="n">
-        <v>19020.26</v>
-      </c>
-      <c r="M56" t="n">
-        <v>19020.26</v>
-      </c>
-      <c r="N56" t="n">
-        <v>476</v>
-      </c>
-      <c r="O56" t="n">
         <v>480109.99</v>
       </c>
     </row>
@@ -3718,33 +3208,24 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>595.65</v>
+        <v>2</v>
       </c>
       <c r="G57" t="n">
-        <v>592.1700000000001</v>
+        <v>0</v>
       </c>
       <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>592.17</v>
+      </c>
+      <c r="J57" t="n">
         <v>2</v>
       </c>
-      <c r="I57" t="n">
-        <v>0</v>
-      </c>
-      <c r="J57" t="n">
-        <v>0</v>
-      </c>
       <c r="K57" t="n">
-        <v>0</v>
+        <v>592.17</v>
       </c>
       <c r="L57" t="n">
-        <v>595.65</v>
-      </c>
-      <c r="M57" t="n">
-        <v>592.1700000000001</v>
-      </c>
-      <c r="N57" t="n">
-        <v>2</v>
-      </c>
-      <c r="O57" t="n">
         <v>53588.78</v>
       </c>
     </row>
@@ -3775,33 +3256,24 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>1245.904</v>
+        <v>2</v>
       </c>
       <c r="G58" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="H58" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="J58" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" t="n">
         <v>41.4</v>
       </c>
-      <c r="H58" t="n">
-        <v>2</v>
-      </c>
-      <c r="I58" t="n">
-        <v>622.952</v>
-      </c>
-      <c r="J58" t="n">
-        <v>20.7</v>
-      </c>
-      <c r="K58" t="n">
-        <v>1</v>
-      </c>
       <c r="L58" t="n">
-        <v>622.952</v>
-      </c>
-      <c r="M58" t="n">
-        <v>20.7</v>
-      </c>
-      <c r="N58" t="n">
-        <v>1</v>
-      </c>
-      <c r="O58" t="n">
         <v>1858136.26</v>
       </c>
     </row>
@@ -3832,33 +3304,24 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>640.048</v>
+        <v>16</v>
       </c>
       <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
         <v>640.05</v>
       </c>
-      <c r="H59" t="n">
+      <c r="J59" t="n">
         <v>16</v>
       </c>
-      <c r="I59" t="n">
-        <v>0</v>
-      </c>
-      <c r="J59" t="n">
-        <v>0</v>
-      </c>
       <c r="K59" t="n">
-        <v>0</v>
+        <v>640.05</v>
       </c>
       <c r="L59" t="n">
-        <v>640.048</v>
-      </c>
-      <c r="M59" t="n">
-        <v>640.05</v>
-      </c>
-      <c r="N59" t="n">
-        <v>16</v>
-      </c>
-      <c r="O59" t="n">
         <v>51826.81</v>
       </c>
     </row>
@@ -3889,33 +3352,24 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>2501.792</v>
+        <v>64</v>
       </c>
       <c r="G60" t="n">
-        <v>2501.81</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>2501.79</v>
+      </c>
+      <c r="J60" t="n">
         <v>64</v>
       </c>
-      <c r="I60" t="n">
-        <v>0</v>
-      </c>
-      <c r="J60" t="n">
-        <v>0</v>
-      </c>
       <c r="K60" t="n">
-        <v>0</v>
+        <v>2501.79</v>
       </c>
       <c r="L60" t="n">
-        <v>2501.792</v>
-      </c>
-      <c r="M60" t="n">
-        <v>2501.81</v>
-      </c>
-      <c r="N60" t="n">
-        <v>64</v>
-      </c>
-      <c r="O60" t="n">
         <v>79958.52</v>
       </c>
     </row>
@@ -3946,7 +3400,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>2337.334</v>
+        <v>6</v>
       </c>
       <c r="G61" t="n">
         <v>2337.21</v>
@@ -3955,24 +3409,15 @@
         <v>6</v>
       </c>
       <c r="I61" t="n">
-        <v>2337.334</v>
+        <v>0</v>
       </c>
       <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
         <v>2337.21</v>
       </c>
-      <c r="K61" t="n">
-        <v>6</v>
-      </c>
       <c r="L61" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" t="n">
         <v>117388.4</v>
       </c>
     </row>
@@ -4003,33 +3448,24 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>161.83</v>
+        <v>4</v>
       </c>
       <c r="G62" t="n">
-        <v>161.83</v>
+        <v>0</v>
       </c>
       <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>120.64</v>
+      </c>
+      <c r="J62" t="n">
         <v>4</v>
       </c>
-      <c r="I62" t="n">
-        <v>0</v>
-      </c>
-      <c r="J62" t="n">
-        <v>0</v>
-      </c>
       <c r="K62" t="n">
-        <v>0</v>
+        <v>120.64</v>
       </c>
       <c r="L62" t="n">
-        <v>161.83</v>
-      </c>
-      <c r="M62" t="n">
-        <v>161.83</v>
-      </c>
-      <c r="N62" t="n">
-        <v>4</v>
-      </c>
-      <c r="O62" t="n">
         <v>367982.08</v>
       </c>
     </row>
@@ -4060,33 +3496,24 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>80.95099999999999</v>
+        <v>1</v>
       </c>
       <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
         <v>20.3</v>
       </c>
-      <c r="H63" t="n">
+      <c r="J63" t="n">
         <v>1</v>
       </c>
-      <c r="I63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J63" t="n">
-        <v>0</v>
-      </c>
       <c r="K63" t="n">
-        <v>0</v>
+        <v>20.3</v>
       </c>
       <c r="L63" t="n">
-        <v>80.95099999999999</v>
-      </c>
-      <c r="M63" t="n">
-        <v>20.3</v>
-      </c>
-      <c r="N63" t="n">
-        <v>1</v>
-      </c>
-      <c r="O63" t="n">
         <v>3746.52</v>
       </c>
     </row>
@@ -4117,33 +3544,24 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>2390.45</v>
+        <v>18</v>
       </c>
       <c r="G64" t="n">
-        <v>2390.42</v>
+        <v>0</v>
       </c>
       <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>2390.3</v>
+      </c>
+      <c r="J64" t="n">
         <v>18</v>
       </c>
-      <c r="I64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J64" t="n">
-        <v>0</v>
-      </c>
       <c r="K64" t="n">
-        <v>0</v>
+        <v>2390.3</v>
       </c>
       <c r="L64" t="n">
-        <v>2390.45</v>
-      </c>
-      <c r="M64" t="n">
-        <v>2390.42</v>
-      </c>
-      <c r="N64" t="n">
-        <v>18</v>
-      </c>
-      <c r="O64" t="n">
         <v>681609.67</v>
       </c>
     </row>
@@ -4177,33 +3595,24 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>33739.79</v>
+        <v>373</v>
       </c>
       <c r="G65" t="n">
-        <v>32811.2</v>
+        <v>4883.92</v>
       </c>
       <c r="H65" t="n">
-        <v>373</v>
+        <v>56</v>
       </c>
       <c r="I65" t="n">
-        <v>5124.75</v>
+        <v>27927.29</v>
       </c>
       <c r="J65" t="n">
-        <v>4883.94</v>
+        <v>317</v>
       </c>
       <c r="K65" t="n">
-        <v>56</v>
+        <v>32811.21</v>
       </c>
       <c r="L65" t="n">
-        <v>28615.04</v>
-      </c>
-      <c r="M65" t="n">
-        <v>27927.26</v>
-      </c>
-      <c r="N65" t="n">
-        <v>317</v>
-      </c>
-      <c r="O65" t="n">
         <v>247878.71</v>
       </c>
     </row>
@@ -4234,33 +3643,24 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>195.859</v>
+        <v>1</v>
       </c>
       <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
         <v>18.84</v>
       </c>
-      <c r="H66" t="n">
+      <c r="J66" t="n">
         <v>1</v>
       </c>
-      <c r="I66" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" t="n">
-        <v>0</v>
-      </c>
       <c r="K66" t="n">
-        <v>0</v>
+        <v>18.84</v>
       </c>
       <c r="L66" t="n">
-        <v>195.859</v>
-      </c>
-      <c r="M66" t="n">
-        <v>18.84</v>
-      </c>
-      <c r="N66" t="n">
-        <v>1</v>
-      </c>
-      <c r="O66" t="n">
         <v>158625.43</v>
       </c>
     </row>
@@ -4291,33 +3691,24 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>330.452</v>
+        <v>6</v>
       </c>
       <c r="G67" t="n">
-        <v>329.83</v>
+        <v>277.57</v>
       </c>
       <c r="H67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I67" t="n">
-        <v>278.157</v>
+        <v>52.27</v>
       </c>
       <c r="J67" t="n">
-        <v>277.56</v>
+        <v>1</v>
       </c>
       <c r="K67" t="n">
-        <v>5</v>
+        <v>329.84</v>
       </c>
       <c r="L67" t="n">
-        <v>52.295</v>
-      </c>
-      <c r="M67" t="n">
-        <v>52.27</v>
-      </c>
-      <c r="N67" t="n">
-        <v>1</v>
-      </c>
-      <c r="O67" t="n">
         <v>1737.94</v>
       </c>
     </row>
@@ -4353,33 +3744,24 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>119540.142</v>
+        <v>739</v>
       </c>
       <c r="G68" t="n">
-        <v>116988.82</v>
+        <v>46823.4</v>
       </c>
       <c r="H68" t="n">
-        <v>739</v>
+        <v>217</v>
       </c>
       <c r="I68" t="n">
-        <v>46924.222</v>
+        <v>70165.38</v>
       </c>
       <c r="J68" t="n">
-        <v>46823.46</v>
+        <v>522</v>
       </c>
       <c r="K68" t="n">
-        <v>217</v>
+        <v>116988.78</v>
       </c>
       <c r="L68" t="n">
-        <v>72615.92</v>
-      </c>
-      <c r="M68" t="n">
-        <v>70165.36</v>
-      </c>
-      <c r="N68" t="n">
-        <v>522</v>
-      </c>
-      <c r="O68" t="n">
         <v>2347732.03</v>
       </c>
     </row>
@@ -4411,33 +3793,24 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>17243.46</v>
+        <v>33</v>
       </c>
       <c r="G69" t="n">
-        <v>14611.31</v>
+        <v>4903.52</v>
       </c>
       <c r="H69" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="I69" t="n">
-        <v>6219.609</v>
+        <v>9707.76</v>
       </c>
       <c r="J69" t="n">
-        <v>4903.53</v>
+        <v>21</v>
       </c>
       <c r="K69" t="n">
-        <v>12</v>
+        <v>14611.28</v>
       </c>
       <c r="L69" t="n">
-        <v>11023.851</v>
-      </c>
-      <c r="M69" t="n">
-        <v>9707.780000000001</v>
-      </c>
-      <c r="N69" t="n">
-        <v>21</v>
-      </c>
-      <c r="O69" t="n">
         <v>2781661.64</v>
       </c>
     </row>
@@ -4469,33 +3842,24 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>6001.37</v>
+        <v>152</v>
       </c>
       <c r="G70" t="n">
-        <v>5997.74</v>
+        <v>186.91</v>
       </c>
       <c r="H70" t="n">
-        <v>152</v>
+        <v>6</v>
       </c>
       <c r="I70" t="n">
-        <v>186.92</v>
+        <v>5810.78</v>
       </c>
       <c r="J70" t="n">
-        <v>186.92</v>
+        <v>146</v>
       </c>
       <c r="K70" t="n">
-        <v>6</v>
+        <v>5997.69</v>
       </c>
       <c r="L70" t="n">
-        <v>5814.45</v>
-      </c>
-      <c r="M70" t="n">
-        <v>5810.82</v>
-      </c>
-      <c r="N70" t="n">
-        <v>146</v>
-      </c>
-      <c r="O70" t="n">
         <v>91880.64999999999</v>
       </c>
     </row>
@@ -4531,33 +3895,24 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>512489.94</v>
+        <v>1463</v>
       </c>
       <c r="G71" t="n">
-        <v>511561.62</v>
+        <v>230995.4</v>
       </c>
       <c r="H71" t="n">
-        <v>1463</v>
+        <v>672</v>
       </c>
       <c r="I71" t="n">
-        <v>231152.38</v>
+        <v>280566.13</v>
       </c>
       <c r="J71" t="n">
-        <v>230995.48</v>
+        <v>791</v>
       </c>
       <c r="K71" t="n">
-        <v>672</v>
+        <v>511561.53</v>
       </c>
       <c r="L71" t="n">
-        <v>281337.56</v>
-      </c>
-      <c r="M71" t="n">
-        <v>280566.14</v>
-      </c>
-      <c r="N71" t="n">
-        <v>791</v>
-      </c>
-      <c r="O71" t="n">
         <v>4504964.31</v>
       </c>
     </row>
@@ -4588,33 +3943,24 @@
         </is>
       </c>
       <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
         <v>27.71</v>
       </c>
-      <c r="G72" t="n">
+      <c r="J72" t="n">
+        <v>1</v>
+      </c>
+      <c r="K72" t="n">
         <v>27.71</v>
       </c>
-      <c r="H72" t="n">
-        <v>1</v>
-      </c>
-      <c r="I72" t="n">
-        <v>0</v>
-      </c>
-      <c r="J72" t="n">
-        <v>0</v>
-      </c>
-      <c r="K72" t="n">
-        <v>0</v>
-      </c>
       <c r="L72" t="n">
-        <v>27.71</v>
-      </c>
-      <c r="M72" t="n">
-        <v>27.71</v>
-      </c>
-      <c r="N72" t="n">
-        <v>1</v>
-      </c>
-      <c r="O72" t="n">
         <v>293080.11</v>
       </c>
     </row>
@@ -4646,33 +3992,24 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>847.182</v>
+        <v>4</v>
       </c>
       <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="n">
         <v>834.13</v>
       </c>
-      <c r="H73" t="n">
+      <c r="J73" t="n">
         <v>4</v>
       </c>
-      <c r="I73" t="n">
-        <v>0</v>
-      </c>
-      <c r="J73" t="n">
-        <v>0</v>
-      </c>
       <c r="K73" t="n">
-        <v>0</v>
+        <v>834.13</v>
       </c>
       <c r="L73" t="n">
-        <v>847.182</v>
-      </c>
-      <c r="M73" t="n">
-        <v>834.13</v>
-      </c>
-      <c r="N73" t="n">
-        <v>4</v>
-      </c>
-      <c r="O73" t="n">
         <v>598651.62</v>
       </c>
     </row>
@@ -4703,33 +4040,24 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>444.212</v>
+        <v>5</v>
       </c>
       <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
         <v>441.49</v>
       </c>
-      <c r="H74" t="n">
+      <c r="J74" t="n">
         <v>5</v>
       </c>
-      <c r="I74" t="n">
-        <v>0</v>
-      </c>
-      <c r="J74" t="n">
-        <v>0</v>
-      </c>
       <c r="K74" t="n">
-        <v>0</v>
+        <v>441.49</v>
       </c>
       <c r="L74" t="n">
-        <v>444.212</v>
-      </c>
-      <c r="M74" t="n">
-        <v>441.49</v>
-      </c>
-      <c r="N74" t="n">
-        <v>5</v>
-      </c>
-      <c r="O74" t="n">
         <v>657110.6</v>
       </c>
     </row>
@@ -4760,33 +4088,24 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>44469.537</v>
+        <v>1141</v>
       </c>
       <c r="G75" t="n">
-        <v>44452.01</v>
+        <v>17197.01</v>
       </c>
       <c r="H75" t="n">
-        <v>1141</v>
+        <v>440</v>
       </c>
       <c r="I75" t="n">
-        <v>17205.066</v>
+        <v>27174.74</v>
       </c>
       <c r="J75" t="n">
-        <v>17197.05</v>
+        <v>701</v>
       </c>
       <c r="K75" t="n">
-        <v>440</v>
+        <v>44371.75</v>
       </c>
       <c r="L75" t="n">
-        <v>27264.471</v>
-      </c>
-      <c r="M75" t="n">
-        <v>27254.96</v>
-      </c>
-      <c r="N75" t="n">
-        <v>701</v>
-      </c>
-      <c r="O75" t="n">
         <v>747912.54</v>
       </c>
     </row>
@@ -4820,33 +4139,24 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>6198.783</v>
+        <v>89</v>
       </c>
       <c r="G76" t="n">
-        <v>5971.53</v>
+        <v>3665.45</v>
       </c>
       <c r="H76" t="n">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="I76" t="n">
-        <v>3871.371</v>
+        <v>2301.95</v>
       </c>
       <c r="J76" t="n">
-        <v>3667.7</v>
+        <v>39</v>
       </c>
       <c r="K76" t="n">
-        <v>50</v>
+        <v>5967.4</v>
       </c>
       <c r="L76" t="n">
-        <v>2327.412</v>
-      </c>
-      <c r="M76" t="n">
-        <v>2303.83</v>
-      </c>
-      <c r="N76" t="n">
-        <v>39</v>
-      </c>
-      <c r="O76" t="n">
         <v>2066861.74</v>
       </c>
     </row>
@@ -4877,33 +4187,24 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>1248.084</v>
+        <v>2</v>
       </c>
       <c r="G77" t="n">
+        <v>62.54</v>
+      </c>
+      <c r="H77" t="n">
+        <v>1</v>
+      </c>
+      <c r="I77" t="n">
+        <v>62.54</v>
+      </c>
+      <c r="J77" t="n">
+        <v>1</v>
+      </c>
+      <c r="K77" t="n">
         <v>125.08</v>
       </c>
-      <c r="H77" t="n">
-        <v>2</v>
-      </c>
-      <c r="I77" t="n">
-        <v>624.042</v>
-      </c>
-      <c r="J77" t="n">
-        <v>62.54</v>
-      </c>
-      <c r="K77" t="n">
-        <v>1</v>
-      </c>
       <c r="L77" t="n">
-        <v>624.042</v>
-      </c>
-      <c r="M77" t="n">
-        <v>62.54</v>
-      </c>
-      <c r="N77" t="n">
-        <v>1</v>
-      </c>
-      <c r="O77" t="n">
         <v>9807.360000000001</v>
       </c>
     </row>
@@ -4938,33 +4239,24 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>103715.528</v>
+        <v>304</v>
       </c>
       <c r="G78" t="n">
-        <v>91828.75</v>
+        <v>46922.33</v>
       </c>
       <c r="H78" t="n">
-        <v>304</v>
+        <v>152</v>
       </c>
       <c r="I78" t="n">
-        <v>52884.966</v>
+        <v>44906.36</v>
       </c>
       <c r="J78" t="n">
-        <v>46922.37</v>
+        <v>152</v>
       </c>
       <c r="K78" t="n">
-        <v>152</v>
+        <v>91828.69</v>
       </c>
       <c r="L78" t="n">
-        <v>50830.562</v>
-      </c>
-      <c r="M78" t="n">
-        <v>44906.38</v>
-      </c>
-      <c r="N78" t="n">
-        <v>152</v>
-      </c>
-      <c r="O78" t="n">
         <v>1376779.33</v>
       </c>
     </row>
@@ -4995,33 +4287,24 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>411.472</v>
+        <v>11</v>
       </c>
       <c r="G79" t="n">
-        <v>411.48</v>
+        <v>0</v>
       </c>
       <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
+        <v>411.47</v>
+      </c>
+      <c r="J79" t="n">
         <v>11</v>
       </c>
-      <c r="I79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" t="n">
-        <v>0</v>
-      </c>
       <c r="K79" t="n">
-        <v>0</v>
+        <v>411.47</v>
       </c>
       <c r="L79" t="n">
-        <v>411.472</v>
-      </c>
-      <c r="M79" t="n">
-        <v>411.48</v>
-      </c>
-      <c r="N79" t="n">
-        <v>11</v>
-      </c>
-      <c r="O79" t="n">
         <v>441528.7</v>
       </c>
     </row>
@@ -5052,33 +4335,24 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>2078.968</v>
+        <v>52</v>
       </c>
       <c r="G80" t="n">
-        <v>2079</v>
+        <v>0</v>
       </c>
       <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
+        <v>2078.97</v>
+      </c>
+      <c r="J80" t="n">
         <v>52</v>
       </c>
-      <c r="I80" t="n">
-        <v>0</v>
-      </c>
-      <c r="J80" t="n">
-        <v>0</v>
-      </c>
       <c r="K80" t="n">
-        <v>0</v>
+        <v>2078.97</v>
       </c>
       <c r="L80" t="n">
-        <v>2078.968</v>
-      </c>
-      <c r="M80" t="n">
-        <v>2079</v>
-      </c>
-      <c r="N80" t="n">
-        <v>52</v>
-      </c>
-      <c r="O80" t="n">
         <v>134256.19</v>
       </c>
     </row>
@@ -5110,33 +4384,24 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>8137.749</v>
+        <v>189</v>
       </c>
       <c r="G81" t="n">
-        <v>8132.809999999999</v>
+        <v>62.57</v>
       </c>
       <c r="H81" t="n">
-        <v>189</v>
+        <v>2</v>
       </c>
       <c r="I81" t="n">
-        <v>63</v>
+        <v>8070.27</v>
       </c>
       <c r="J81" t="n">
-        <v>62.57</v>
+        <v>187</v>
       </c>
       <c r="K81" t="n">
-        <v>2</v>
+        <v>8132.84</v>
       </c>
       <c r="L81" t="n">
-        <v>8074.749</v>
-      </c>
-      <c r="M81" t="n">
-        <v>8070.24</v>
-      </c>
-      <c r="N81" t="n">
-        <v>187</v>
-      </c>
-      <c r="O81" t="n">
         <v>462553.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: Stringify trust_name and rights_type aggregations.
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -513,12 +513,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -561,12 +561,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['Common Schools' 'Dept. of Transportation' 'None Listed']</t>
+          <t>Common Schools, Dept. of Transportation, None Listed</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['Surface' 'subsurface' 'Subsurface']</t>
+          <t>Surface, subsurface, Subsurface</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -609,12 +609,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['TRUST FUND: SCHOOL']</t>
+          <t>TRUST FUND: SCHOOL</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -657,14 +657,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['Public Building' 'Common Schools' 'State Educational Institutions'
- 'Oklahoma State University' 'University Preparatory'
- 'University of Oklahoma' 'Normal Schools']</t>
+          <t>Public Building, Common Schools, State Educational Institutions, Oklahoma State University, University Preparatory, University of Oklahoma, Normal Schools</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['subsurface' 'surface']</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -707,12 +705,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['Common School and Indemnity']</t>
+          <t>Common School and Indemnity</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -755,12 +753,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['School Lands']</t>
+          <t>School Lands</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -803,14 +801,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['Common Schools' 'Oklahoma State University' 'Normal Schools'
- 'University Preparatory' 'Connors State College' 'Langston University'
- 'State Educational Institutions']</t>
+          <t>Common Schools, Oklahoma State University, Normal Schools, University Preparatory, Connors State College, Langston University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['subsurface']</t>
+          <t>subsurface</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -853,12 +849,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['Rural Credit' 'School and Public Lands' 'Common School' 'Indemnity']</t>
+          <t>Rural Credit, School and Public Lands, Common School, Indemnity</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -901,15 +897,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['Oklahoma State University' 'University of Oklahoma' 'Common Schools'
- 'Greer 33' 'State Educational Institutions' 'Normal Schools'
- 'University Preparatory' 'Langston University' 'Wildlife Conservation'
- 'Redlands Community College' 'University Hospitals Authority &amp; Trust']</t>
+          <t>Oklahoma State University, University of Oklahoma, Common Schools, Greer 33, State Educational Institutions, Normal Schools, University Preparatory, Langston University, Wildlife Conservation, Redlands Community College, University Hospitals Authority &amp; Trust</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['surface' 'subsurface']</t>
+          <t>surface, subsurface</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -952,14 +945,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['Common Schools' 'State Educational Institutions'
- 'University Preparatory' 'Oklahoma State University' 'Other Agency'
- 'Wildlife Conservation' 'Normal Schools' 'Aeronautics Commission']</t>
+          <t>Common Schools, State Educational Institutions, University Preparatory, Oklahoma State University, Other Agency, Wildlife Conservation, Normal Schools, Aeronautics Commission</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['subsurface' 'surface']</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1002,15 +993,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['Common Schools' 'State Educational Institutions'
- 'University of Oklahoma' 'Langston University'
- 'Oklahoma State University' 'Normal Schools' 'University Preparatory'
- 'Other Agency' 'Wildlife Conservation']</t>
+          <t>Common Schools, State Educational Institutions, University of Oklahoma, Langston University, Oklahoma State University, Normal Schools, University Preparatory, Other Agency, Wildlife Conservation</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['subsurface']</t>
+          <t>subsurface</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -1053,13 +1041,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['Oklahoma State University' 'Common Schools' 'Normal Schools'
- 'Wildlife Conservation' 'Other Agency' 'State Educational Institutions']</t>
+          <t>Oklahoma State University, Common Schools, Normal Schools, Wildlife Conservation, Other Agency, State Educational Institutions</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['surface' 'subsurface']</t>
+          <t>surface, subsurface</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1102,12 +1089,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1150,18 +1137,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>['Dept. of Parks and Recreation' '100.00% Dept. of Parks and Recreation'
- 'Public School (Indemnity, Schools, Common Schools)'
- '100.00% Public School (Indemnity, Schools, Common Schools)'
- '100.00% Normal School' '100.00% University of Idaho'
- 'State Hospital South (Insane Asylum)' 'Normal School'
- 'Agricultural College' '100.00% Dept. of Fish and Game' 'General Fund'
- '100.00% General Fund']</t>
+          <t>Dept. of Parks and Recreation, 100.00% Dept. of Parks and Recreation, Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), 100.00% Normal School, 100.00% University of Idaho, State Hospital South (Insane Asylum), Normal School, Agricultural College, 100.00% Dept. of Fish and Game, General Fund, 100.00% General Fund</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1204,12 +1185,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>['Common School and Indemnity']</t>
+          <t>Common School and Indemnity</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1252,14 +1233,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>['Common Schools' 'Other Agency' 'Wildlife Conservation'
- 'State Educational Institutions' 'Normal Schools'
- 'University of Oklahoma']</t>
+          <t>Common Schools, Other Agency, Wildlife Conservation, State Educational Institutions, Normal Schools, University of Oklahoma</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>['subsurface']</t>
+          <t>subsurface</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1302,12 +1281,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>['Surface' 'subsurface']</t>
+          <t>Surface, subsurface</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1350,12 +1329,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['Rural Credit' 'Common School']</t>
+          <t>Rural Credit, Common School</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1398,12 +1377,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>['Common Schools' 'University of Montana']</t>
+          <t>Common Schools, University of Montana</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>['subsurface' 'Surface']</t>
+          <t>subsurface, Surface</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1446,12 +1425,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['TRUST FUND: SCHOOL']</t>
+          <t>TRUST FUND: SCHOOL</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1494,12 +1473,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>['Surface' 'subsurface']</t>
+          <t>Surface, subsurface</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1542,15 +1521,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>['BANK OFÔøΩNORTHÔøΩDAKOTA' 'SOVEREIGNÔøΩLANDS' 'COMMON SCHOOLS'
- 'NDÔøΩSTATEÔøΩUNIVERSITY' 'ND INDUSTRIAL SCHOOL' 'SCHOOL OF MINES'
- 'ELLENDALE' 'SCHOOL FOR THE BLIND' 'ND SCHOOL OF SCIENCE'
- 'UNIVERSITY OF ND' 'NDÔøΩSTATEÔøΩTREASURER' 'MAYVILLE' 'VALLEY CITY']</t>
+          <t>BANK OFÔøΩNORTHÔøΩDAKOTA, SOVEREIGNÔøΩLANDS, COMMON SCHOOLS, NDÔøΩSTATEÔøΩUNIVERSITY, ND INDUSTRIAL SCHOOL, SCHOOL OF MINES, ELLENDALE, SCHOOL FOR THE BLIND, ND SCHOOL OF SCIENCE, UNIVERSITY OF ND, NDÔøΩSTATEÔøΩTREASURER, MAYVILLE, VALLEY CITY</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1593,13 +1569,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>['Dept. of Transportation' '100.00% State Hospital South (Insane Asylum)'
- 'Public School (Indemnity, Schools, Common Schools)']</t>
+          <t>Dept. of Transportation, 100.00% State Hospital South (Insane Asylum), Public School (Indemnity, Schools, Common Schools)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1642,12 +1617,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1690,13 +1665,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>['None Listed' 'Common Schools'
- 'Public Land Trust Income - Navigable Rivers']</t>
+          <t>None Listed, Common Schools, Public Land Trust Income - Navigable Rivers</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>['Subsurface' 'subsurface' 'Surface']</t>
+          <t>Subsurface, subsurface, Surface</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1739,12 +1713,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>['PENITENTIARY LAND FUND' 'NAVIGABLE STREAMBEDS' 'School Lands']</t>
+          <t>PENITENTIARY LAND FUND, NAVIGABLE STREAMBEDS, School Lands</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1787,12 +1761,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>['TRUST FUND: UNIVERSITY' 'TRUST FUND: SWAMP' 'TRUST FUND: SCHOOL']</t>
+          <t>TRUST FUND: UNIVERSITY, TRUST FUND: SWAMP, TRUST FUND: SCHOOL</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1835,12 +1809,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>['PERM CMN SCHLS (INDMTY SELEC)' 'PERM COMMON SCHLS']</t>
+          <t>PERM CMN SCHLS (INDMTY SELEC), PERM COMMON SCHLS</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1883,12 +1857,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>['PERM COMMON SCHLS' 'AGRICULTURE &amp; MECHANICAL CLLGE']</t>
+          <t>PERM COMMON SCHLS, AGRICULTURE &amp; MECHANICAL CLLGE</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1931,12 +1905,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>['Oklahoma State University' 'Common Schools' 'Other Agency']</t>
+          <t>Oklahoma State University, Common Schools, Other Agency</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>['surface' 'subsurface']</t>
+          <t>surface, subsurface</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1979,12 +1953,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -2027,12 +2001,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>['Common Schools' 'Carrie Tingley Hospital']</t>
+          <t>Common Schools, Carrie Tingley Hospital</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -2075,12 +2049,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>['Charitable/Educational/Penal &amp; Reformatory Instit.']</t>
+          <t>Charitable/Educational/Penal &amp; Reformatory Instit.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -2123,13 +2097,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>['State Educational Institutions' 'Oklahoma State University'
- 'Common Schools' 'Public Building']</t>
+          <t>State Educational Institutions, Oklahoma State University, Common Schools, Public Building</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>['subsurface' 'surface']</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -2172,13 +2145,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>['Common Schools' 'State Educational Institutions' 'Public Building'
- 'Oklahoma State University']</t>
+          <t>Common Schools, State Educational Institutions, Public Building, Oklahoma State University</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>['subsurface' 'surface']</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -2221,13 +2193,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>['Common Schools' 'Oklahoma State University'
- 'State Educational Institutions']</t>
+          <t>Common Schools, Oklahoma State University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>['subsurface' 'surface']</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -2270,14 +2241,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>['Common Schools' 'Greer 33' 'Oklahoma State University'
- 'State Educational Institutions' 'University Preparatory'
- 'Public Building' 'Normal Schools']</t>
+          <t>Common Schools, Greer 33, Oklahoma State University, State Educational Institutions, University Preparatory, Public Building, Normal Schools</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>['subsurface' 'surface']</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -2320,13 +2289,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>['State Educational Institutions' 'Common Schools' 'Public Building'
- 'Oklahoma State University']</t>
+          <t>State Educational Institutions, Common Schools, Public Building, Oklahoma State University</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>['subsurface' 'surface']</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -2369,14 +2337,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>['Common Schools' 'Eastern New Mexico University'
- 'New Mexico State University'
- 'New Mexico Institute of Mining and Technology']</t>
+          <t>Common Schools, Eastern New Mexico University, New Mexico State University, New Mexico Institute of Mining and Technology</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2419,12 +2385,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>['TRUST FUND: SWAMP' 'TRUST FUND: SCHOOL' 'TRUST FUND: IND SCHOOL']</t>
+          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -2467,12 +2433,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>['Common School and Indemnity']</t>
+          <t>Common School and Indemnity</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -2515,12 +2481,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>['TRUST FUND: SCHOOL' 'TRUST FUND: IND SCHOOL']</t>
+          <t>TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -2563,14 +2529,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>['PERM COMMON SCHLS' 'PERM CMN SCHLS (INDMTY SELEC)' 'COUNTY BOND'
- 'New Mexico Institute of Mining and Technology' 'Common Schools'
- 'Public Schools']</t>
+          <t>PERM COMMON SCHLS, PERM CMN SCHLS (INDMTY SELEC), COUNTY BOND, New Mexico Institute of Mining and Technology, Common Schools, Public Schools</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -2613,12 +2577,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -2661,12 +2625,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2709,19 +2673,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>['Public School (Indemnity, Schools, Common Schools)'
- '100.00% Public School (Indemnity, Schools, Common Schools)'
- 'Dept. of Fish and Game' '100.00% Agricultural College'
- '100.00% Charitable Institute' '100.00% Normal School'
- '100.00% Forest Purposes (Dept. of Forestry)'
- '100.00% University of Idaho' '100.00% Dept. of Fish and Game'
- '100.00% Dept. of Health and Welfare' 'Dept. of Health and Welfare'
- '100.00% General Fund' '100.00% Dept. of Transportation']</t>
+          <t>Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), Dept. of Fish and Game, 100.00% Agricultural College, 100.00% Charitable Institute, 100.00% Normal School, 100.00% Forest Purposes (Dept. of Forestry), 100.00% University of Idaho, 100.00% Dept. of Fish and Game, 100.00% Dept. of Health and Welfare, Dept. of Health and Welfare, 100.00% General Fund, 100.00% Dept. of Transportation</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -2764,13 +2721,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>['Oklahoma State University' 'Common Schools' 'Public Building'
- 'State Educational Institutions' 'Other Agency']</t>
+          <t>Oklahoma State University, Common Schools, Public Building, State Educational Institutions, Other Agency</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>['surface' 'subsurface']</t>
+          <t>surface, subsurface</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -2813,12 +2769,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>['School and Public Lands' 'Indemnity' 'Rural Credit' 'Common School']</t>
+          <t>School and Public Lands, Indemnity, Rural Credit, Common School</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -2861,12 +2817,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>['Common Schools' 'Public Building']</t>
+          <t>Common Schools, Public Building</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>['subsurface']</t>
+          <t>subsurface</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -2909,12 +2865,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>['TRUST FUND: SCHOOL']</t>
+          <t>TRUST FUND: SCHOOL</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -2957,12 +2913,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>['Escheat' 'Common School and Indemnity']</t>
+          <t>Escheat, Common School and Indemnity</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -3005,12 +2961,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>['TRUST FUND: IND SCHOOL' 'TRUST FUND: SWAMP']</t>
+          <t>TRUST FUND: IND SCHOOL, TRUST FUND: SWAMP</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -3053,12 +3009,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>['subsurface' 'Surface']</t>
+          <t>subsurface, Surface</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -3101,12 +3057,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>['Rural Credit' 'School and Public Lands' 'Common School']</t>
+          <t>Rural Credit, School and Public Lands, Common School</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -3149,14 +3105,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>['Oklahoma State University' 'Common Schools'
- 'State Educational Institutions' 'University of Oklahoma'
- 'Normal Schools' 'Other Agency']</t>
+          <t>Oklahoma State University, Common Schools, State Educational Institutions, University of Oklahoma, Normal Schools, Other Agency</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>['surface' 'subsurface']</t>
+          <t>surface, subsurface</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -3199,12 +3153,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>['PERM CMN SCHLS (INDMTY SELEC)' '02-90-0021 FED PATENT']</t>
+          <t>PERM CMN SCHLS (INDMTY SELEC), 02-90-0021 FED PATENT</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -3247,12 +3201,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>['PERM COMMON SCHLS']</t>
+          <t>PERM COMMON SCHLS</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -3295,12 +3249,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -3343,12 +3297,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F60" t="n">
@@ -3391,12 +3345,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>['Common K-12']</t>
+          <t>Common K-12</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>['Surface']</t>
+          <t>Surface</t>
         </is>
       </c>
       <c r="F61" t="n">
@@ -3439,12 +3393,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>['Oklahoma State University']</t>
+          <t>Oklahoma State University</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>['subsurface']</t>
+          <t>subsurface</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -3487,12 +3441,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F63" t="n">
@@ -3535,12 +3489,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>['Common School']</t>
+          <t>Common School</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>['subsurface']</t>
+          <t>subsurface</t>
         </is>
       </c>
       <c r="F64" t="n">
@@ -3583,15 +3537,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>['BANK OFÔøΩNORTHÔøΩDAKOTA' 'COMMON SCHOOLS' 'STATE HOSPITAL'
- 'VALLEY/MAYVILLE' 'SCHOOL FOR THE DEAF' 'ND STATE UNIVERSITY'
- 'ND SCHOOL OF SCIENCE' 'VALLEY CITY' 'VETERANS HOME' 'ELLENDALE'
- 'MAYVILLE' 'ND INDUSTRIAL SCHOOL']</t>
+          <t>BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, STATE HOSPITAL, VALLEY/MAYVILLE, SCHOOL FOR THE DEAF, ND STATE UNIVERSITY, ND SCHOOL OF SCIENCE, VALLEY CITY, VETERANS HOME, ELLENDALE, MAYVILLE, ND INDUSTRIAL SCHOOL</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -3634,12 +3585,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>['Common School and Indemnity']</t>
+          <t>Common School and Indemnity</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F66" t="n">
@@ -3682,12 +3633,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>['Administrative Site']</t>
+          <t>Administrative Site</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F67" t="n">
@@ -3730,17 +3681,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>['Rural Credit' 'School and Public Lands' 'Indemnity'
- 'BANK OFÔøΩNORTHÔøΩDAKOTA' 'COMMON SCHOOLS' 'ND SCHOOL OF SCIENCE'
- 'CAPITOL BUILDING' 'VETERANS HOME' 'MAYVILLE' 'SCHOOL OF MINES'
- 'UNIVERSITY OF ND' 'ND INDUSTRIAL SCHOOL' 'ND STATE UNIVERSITY'
- 'NDÔøΩSTATEÔøΩUNIVERSITY' 'ELLENDALE' 'SCHOOL FOR THE DEAF'
- 'STATEÔøΩHOSPITAL' 'VALLEY/MAYVILLE']</t>
+          <t>Rural Credit, School and Public Lands, Indemnity, BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, ND SCHOOL OF SCIENCE, CAPITOL BUILDING, VETERANS HOME, MAYVILLE, SCHOOL OF MINES, UNIVERSITY OF ND, ND INDUSTRIAL SCHOOL, ND STATE UNIVERSITY, NDÔøΩSTATEÔøΩUNIVERSITY, ELLENDALE, SCHOOL FOR THE DEAF, STATEÔøΩHOSPITAL, VALLEY/MAYVILLE</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F68" t="n">
@@ -3783,13 +3729,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>['COUNTY BOND' 'UNIVERSITY' 'ST CHRTBL, PENAL &amp; REFORM INST'
- 'PERM COMMON SCHLS' 'SCHOOL OF MINES']</t>
+          <t>COUNTY BOND, UNIVERSITY, ST CHRTBL, PENAL &amp; REFORM INST, PERM COMMON SCHLS, SCHOOL OF MINES</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F69" t="n">
@@ -3832,13 +3777,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>['Public Building' 'Common Schools' 'Oklahoma State University'
- 'State Educational Institutions']</t>
+          <t>Public Building, Common Schools, Oklahoma State University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>['subsurface' 'surface']</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -3881,17 +3825,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>['Public Schools' 'Recreation Exchange' 'Multi-Beneficiary'
- 'College of Mines and Earth Sciences' 'UtahÔøΩStateÔøΩHospital'
- 'Reservoirs' 'UtahÔøΩSchools for the Deaf' 'University ofÔøΩUtah'
- 'UtahÔøΩStateÔøΩUniversity' 'Juvenile Justice Services'
- 'UtahÔøΩSchools for the Blind' 'Teaching Colleges at Public Universities'
- 'Public Buildings' 'Miners Hospital']</t>
+          <t>Public Schools, Recreation Exchange, Multi-Beneficiary, College of Mines and Earth Sciences, UtahÔøΩStateÔøΩHospital, Reservoirs, UtahÔøΩSchools for the Deaf, University ofÔøΩUtah, UtahÔøΩStateÔøΩUniversity, Juvenile Justice Services, UtahÔøΩSchools for the Blind, Teaching Colleges at Public Universities, Public Buildings, Miners Hospital</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F71" t="n">
@@ -3934,12 +3873,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F72" t="n">
@@ -3982,13 +3921,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>['Public Schools' 'UtahÔøΩSchools for the Blind'
- 'UtahÔøΩStateÔøΩUniversity']</t>
+          <t>Public Schools, UtahÔøΩSchools for the Blind, UtahÔøΩStateÔøΩUniversity</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F73" t="n">
@@ -4031,12 +3969,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F74" t="n">
@@ -4079,12 +4017,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>['TRUST FUND: SWAMP' 'TRUST FUND: SCHOOL' 'TRUST FUND: IND SCHOOL']</t>
+          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -4127,15 +4065,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>['Department of Environmental Quality' 'Farm Loan' 'Escheat'
- 'Board of Charities and Reform' 'Game and Fish Commission'
- 'Acquired Farm Loan' 'State Charitable, Educational, Penal &amp; Reform Inst'
- 'Common School']</t>
+          <t>Department of Environmental Quality, Farm Loan, Escheat, Board of Charities and Reform, Game and Fish Commission, Acquired Farm Loan, State Charitable, Educational, Penal &amp; Reform Inst, Common School</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F76" t="n">
@@ -4178,12 +4113,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>['School Lands']</t>
+          <t>School Lands</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>['Surface' 'Subsurface']</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F77" t="n">
@@ -4226,16 +4161,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>['Common School and Indemnity' 'State Forest Transfer' 'Escheat'
- 'Scientific School' 'Community Forest Trust' 'Normal School'
- 'Natural Resources Conservation Area'
- 'Charitable/Educational/Penal &amp; Reformatory Instit.'
- 'University - Transferred']</t>
+          <t>Common School and Indemnity, State Forest Transfer, Escheat, Scientific School, Community Forest Trust, Normal School, Natural Resources Conservation Area, Charitable/Educational/Penal &amp; Reformatory Instit., University - Transferred</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F78" t="n">
@@ -4278,12 +4209,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>['Rural Credit' 'Common School']</t>
+          <t>Rural Credit, Common School</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F79" t="n">
@@ -4326,12 +4257,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>['Common Schools']</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>['Subsurface']</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F80" t="n">
@@ -4374,13 +4305,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>['PERM CMN SCHLS (INDMTY SELEC)' 'Saline Lands, University of New Mexico'
- 'Common Schools' 'New Mexico School for the Visually Handicapped']</t>
+          <t>PERM CMN SCHLS (INDMTY SELEC), Saline Lands, University of New Mexico, Common Schools, New Mexico School for the Visually Handicapped</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>['Subsurface' 'Surface']</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F81" t="n">

</xml_diff>

<commit_message>
fix: Correct type mismtach and rebuild datasets.
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,7 +546,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1215734.4919286212 2919412.348803906 0, -1215739.2418993178 2919415.854489744 0, -1215752.301648532 2919425.0016529365 0, -1215801.1184896445 2919460.5409494657 0, -1215880.1351253951 2919458.194114684 0, -1215935.7465738817 2919456.662823337 0, -1216017.514904797 2919424.4208201505 0, -1216301.6985192918 2919383.909817556 0, -1216379.7725044978 2919372.857053071 0, -1216421.4827175136 2919404.798627857 0, -1216469.9646424958 2919466.6185278543 0, -1216487.0923211551 2919489.0687451703 0, -1216593.3096698693 2919789.9906576937 0, -1216651.6264636929 2919845.8770137485 0, -1216722.102225036 2919913.20975236 0, -1216831.1752236811 2920017.569721035 0, -1216842.6006949407 2920051.4157221178 0, -1216862.8363486752 2920111.6435212083 0, -1216862.7034745696 2920112.4260375807 0, -1216853.6560083632 2920085.5366167566 0, -1216843.1038769977 2920059.6028733077 0, -1216788.3014150327 2920007.3321183003 0, -1216697.798992958 2919912.0946244993 0, -1216633.1836969352 2919850.462773938 0, -1216599.6502633595 2919815.1742660655 0, -1216567.797031382 2919770.1383114094 0, -1216565.3659194517 2919760.2612490105 0, -1216511.7640747712 2919615.50416238 0, -1216496.3529543676 2919552.8790510045 0, -1216472.969075556 2919514.3247987595 0, -1216439.8650943723 2919472.5683507663 0, -1216418.8132326123 2919456.8300753315 0, -1216358.015127779 2919455.0348798954 0, -1216318.5462705519 2919461.0072452463 0, -1216263.0451418571 2919466.0366023434 0, -1216119.5758356226 2919487.7435471755 0, -1216003.1941593739 2919521.9833337013 0, -1215961.895446596 2919538.5249132873 0, -1215933.7719486097 2919539.620839089 0, -1215858.3285944469 2919530.32260102 0, -1215818.4702780903 2919531.876578283 0, -1215803.123633326 2919510.222797078 0, -1215726.7621123476 2919429.118585371 0, -1215704.0221886155 2919391.4580905 0, -1215619.2137624647 2919251.0013917703 0, -1215629.2988838274 2919241.1229922394 0, -1215629.3130592303 2919241.146159707 0, -1215734.4919286212 2919412.348803906 0)), ((-1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0)))</t>
+          <t>POLYGON Z ((-1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0))</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -561,22 +561,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Common Schools, Dept. of Transportation, None Listed</t>
+          <t>Dept. of Transportation, None Listed</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Surface, subsurface, Subsurface</t>
+          <t>subsurface, Subsurface</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>17.01</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>81.20999999999999</v>
@@ -585,7 +585,7 @@
         <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>98.22</v>
+        <v>81.20999999999999</v>
       </c>
       <c r="L3" t="n">
         <v>1534569.87</v>
@@ -657,7 +657,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Public Building, Common Schools, State Educational Institutions, Oklahoma State University, University Preparatory, University of Oklahoma, Normal Schools</t>
+          <t>Common Schools, Oklahoma State University, State Educational Institutions, Public Building, University Preparatory, University of Oklahoma, Normal Schools</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Common Schools, Oklahoma State University, Normal Schools, University Preparatory, Connors State College, Langston University, State Educational Institutions</t>
+          <t>Common Schools, Normal Schools, University Preparatory, Connors State College, Oklahoma State University, Langston University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Rural Credit, School and Public Lands, Common School, Indemnity</t>
+          <t>Common School, Rural Credit, School and Public Lands, Indemnity</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Oklahoma State University, University of Oklahoma, Common Schools, Greer 33, State Educational Institutions, Normal Schools, University Preparatory, Langston University, Wildlife Conservation, Redlands Community College, University Hospitals Authority &amp; Trust</t>
+          <t>Oklahoma State University, University of Oklahoma, Common Schools, State Educational Institutions, Greer 33, Normal Schools, University Preparatory, Langston University, Wildlife Conservation, Redlands Community College, University Hospitals Authority &amp; Trust</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -945,7 +945,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, University Preparatory, Oklahoma State University, Other Agency, Wildlife Conservation, Normal Schools, Aeronautics Commission</t>
+          <t>Oklahoma State University, Common Schools, Normal Schools, State Educational Institutions, University Preparatory, Other Agency, Wildlife Conservation, Aeronautics Commission</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -993,7 +993,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, University of Oklahoma, Langston University, Oklahoma State University, Normal Schools, University Preparatory, Other Agency, Wildlife Conservation</t>
+          <t>University of Oklahoma, State Educational Institutions, Common Schools, Normal Schools, University Preparatory, Oklahoma State University, Langston University, Other Agency, Wildlife Conservation</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dept. of Parks and Recreation, 100.00% Dept. of Parks and Recreation, Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), 100.00% Normal School, 100.00% University of Idaho, State Hospital South (Insane Asylum), Normal School, Agricultural College, 100.00% Dept. of Fish and Game, General Fund, 100.00% General Fund</t>
+          <t>Dept. of Parks and Recreation, 100.00% Dept. of Parks and Recreation, Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), 100.00% Normal School, 100.00% University of Idaho, State Hospital South (Insane Asylum), Normal School, Agricultural College, 100.00% Dept. of Fish and Game, 100.00% General Fund, General Fund</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Rural Credit, Common School</t>
+          <t>Common School, Rural Credit</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1362,7 +1362,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1406379.8180101914 2835502.9676008387 0, -1406473.9785516895 2835521.734531294 0, -1406778.7770429626 2835582.4882667917 0, -1406872.8312997553 2835601.148932945 0, -1406791.7645722493 2835992.9266004586 0, -1406710.698745883 2836384.702508994 0, -1406629.6366764735 2836776.4711096287 0, -1406548.5739271764 2837168.2345223785 0, -1406152.1431418383 2837088.956904065 0, -1406087.6405494164 2837076.280484532 0, -1405796.91670816 2837018.1569047323 0, -1405755.7083628573 2837009.698301688 0, -1405535.803621465 2836965.9663151815 0, -1405487.176097592 2836956.2471401114 0, -1405359.2691901615 2836930.461773824 0, -1405080.115136758 2836874.9046132243 0, -1404962.8255844747 2836851.2476163614 0, -1405025.8156075906 2836537.4335374683 0, -1405029.769174486 2836517.7370062955 0, -1405041.4965421397 2836459.306839623 0, -1405041.4965422011 2836459.306839316 0, -1405081.6600892353 2836258.4058300443 0, -1405108.2831449925 2836126.578187748 0, -1405120.0309416638 2836067.337313631 0, -1405133.2551556446 2836000.645850542 0, -1405186.659309687 2835735.386966785 0, -1405188.114813715 2835727.329112005 0, -1405192.8804176834 2835703.5856685042 0, -1405198.701406638 2835675.389715876 0, -1405261.8129454285 2835360.1547357994 0, -1405265.1738896933 2835344.2151984107 0, -1405277.2234497615 2835283.407895384 0, -1405277.2234497755 2835283.4078953867 0, -1405277.2234497757 2835283.4078953853 0, -1405581.9305416776 2835344.089946119 0, -1405676.1759969064 2835362.862839606 0, -1405980.8366573509 2835423.550296702 0, -1406075.138144352 2835442.2583379205 0, -1406202.3274685177 2835467.601562032 0, -1406379.8180101914 2835502.9676008387 0)), ((-1399306.9140826785 2840269.7509606453 0, -1399308.926485363 2840259.6770075844 0, -1399310.6939220119 2840250.9220541627 0, -1399335.4899758273 2840125.914068922 0, -1399347.1961440216 2840066.79943821 0, -1399356.4079068387 2840020.2810208434 0, -1399368.1809894112 2839960.4057747424 0, -1399384.6546780465 2839877.227700831 0, -1399462.396458146 2839484.6995438226 0, -1399540.139008013 2839092.1665506647 0, -1399542.905688448 2839092.835199241 0, -1399556.3294038298 2839095.3861888293 0, -1399556.329404045 2839095.3861888703 0, -1399561.6720821362 2839096.376602012 0, -1399582.007635379 2839100.423022579 0, -1399599.5649045492 2839103.916675662 0, -1399623.3376730068 2839108.6470440533 0, -1399644.5027693652 2839112.8586522965 0, -1399667.8546858106 2839117.505222619 0, -1399689.9714188937 2839121.9060038663 0, -1399712.3326666437 2839126.3553711157 0, -1399735.4324632378 2839130.9517879887 0, -1399753.6615634388 2839134.578885354 0, -1399780.8692110055 2839139.992492276 0, -1399798.1407629494 2839143.429084783 0, -1399826.33910559 2839149.039729029 0, -1399842.651850635 2839152.2853515954 0, -1399871.8019453995 2839158.085069711 0, -1399883.9572934853 2839160.5036009005 0, -1399916.771608468 2839167.0324040405 0, -1399928.497425498 2839169.3652046104 0, -1399934.4273121587 2839170.492037641 0, -1399937.3344581702 2839171.1505293464 0, -1399937.334458662 2839171.150529451 0, -1399937.3344694409 2839171.1505315923 0, -1399961.7740465652 2839175.991441545 0, -1399972.9727293379 2839178.2173738675 0, -1400007.6713144428 2839185.123969481 0, -1400014.3015124146 2839186.44347234 0, -1400053.0843019113 2839194.164184724 0, -1400059.1674090049 2839195.3749906607 0, -1400062.5253671096 2839196.043416641 0, -1400098.5195565978 2839203.2079879213 0, -1400103.2938011107 2839204.1582646235 0, -1400135.8492566794 2839210.638179495 0, -1400135.84925794 2839210.638179746 0, -1400143.9549004098 2839212.251141099 0, -1400147.7740981488 2839213.0111707496 0, -1400189.1188868866 2839221.238374427 0, -1400322.934807602 2839247.8660599813 0, -1400331.4578416802 2839249.561483696 0, -1400334.5232879098 2839250.1564733693 0, -1400337.289539137 2839250.8269082224 0, -1400438.6676987924 2839270.9013746134 0, -1400616.4727830754 2839306.2846389473 0, -1400666.7624768384 2839316.2673303704 0, -1400731.7096861927 2839329.18493668 0, -1400734.4720727175 2839329.8709867066 0, -1400774.2737872985 2839337.662505503 0, -1400819.7837660834 2839346.7515740218 0, -1401125.8721471464 2839407.6680866037 0, -1401128.8917457967 2839408.235767459 0, -1401123.9478869513 2839432.9798185662 0, -1401114.9923184975 2839478.068050874 0, -1401105.4885421125 2839525.9158027335 0, -1401103.154785328 2839537.809666259 0, -1401103.15478518 2839537.809667019 0, -1401067.6565216575 2839720.071360423 0, -1401063.830226231 2839739.28926802 0, -1401063.2021711767 2839742.434400068 0, -1401053.3518599859 2839788.545631688 0, -1401050.9229196983 2839800.7740466096 0, -1401050.9229196971 2839800.7740466157 0, -1401053.6475980359 2839801.596686764 0, -1400999.4443926136 2840062.6907491884 0, -1400998.724069705 2840066.308780294 0, -1400989.0886561542 2840114.569291522 0, -1400975.3905077311 2840183.1795261377 0, -1400973.5361308318 2840190.382025044 0, -1400973.536130806 2840190.382025154 0, -1400972.9550610757 2840193.3075143024 0, -1400954.6895441287 2840190.4323968505 0, -1400920.226759528 2840183.5676653488 0, -1400578.8062332084 2840115.124226884 0, -1400575.8805057171 2840114.2936359607 0, -1400575.7633936796 2840117.3285491103 0, -1400574.844702643 2840122.2522871094 0, -1400574.022585394 2840126.3318334757 0, -1400566.8949736727 2840162.4611979346 0, -1400542.6533913193 2840284.271411241 0, -1400539.2966141847 2840301.1361504267 0, -1400517.715227514 2840409.5622253655 0, -1400512.0344126902 2840438.1135863895 0, -1400502.104311991 2840485.9874962857 0, -1400497.9721403266 2840506.8058186676 0, -1400497.390664912 2840509.80477352 0, -1400452.1259811474 2840738.4564959686 0, -1400451.4587958015 2840741.808285925 0, -1400428.6235849268 2840856.2023643884 0, -1400420.8018900126 2840895.468983268 0, -1400420.069223923 2840899.301431375 0, -1400274.7199397993 2840870.543052567 0, -1400213.4646311947 2840858.3298914144 0, -1400023.1088309977 2840820.26744506 0, -1400022.4191629284 2840823.311960139 0, -1399739.523394895 2840764.6045222455 0, -1399736.5386692584 2840764.0057220142 0, -1399709.2365354546 2840758.5145079345 0, -1399626.1434866686 2840741.2589619365 0, -1399229.1764102448 2840662.2699850057 0, -1399306.9140804114 2840269.750971841 0, -1399306.9140826785 2840269.7509606453 0)), ((-1399229.1764102448 2840662.2699850057 0, -1399151.2946448606 2841054.7992079007 0, -1398754.3652302015 2840975.7562494082 0, -1398357.4368467703 2840896.7085765144 0, -1398434.9954991627 2840504.121791033 0, -1398832.0885730598 2840583.1832069866 0, -1399229.1764102448 2840662.2699850057 0)), ((-1410207.0886851817 2841171.569820003 0, -1410292.106862424 2841187.9271961376 0, -1410693.8600138929 2841265.8675316847 0, -1410641.7045664315 2841528.5669757756 0, -1410634.2942596902 2841565.9644431355 0, -1410616.0088154103 2841658.7990578404 0, -1410598.9623274822 2841744.276462479 0, -1410583.5237163594 2841822.194011335 0, -1410567.3071516913 2841904.0386808235 0, -1410550.4485024924 2841989.125877908 0, -1410546.7760295542 2842007.661339168 0, -1410538.1586854516 2842051.725978964 0, -1410475.0699257555 2842369.6151062693 0, -1410460.3759917119 2842444.344847481 0, -1410410.353163191 2842696.3028291394 0, -1410373.9500720813 2842880.5766738653 0, -1410314.8445090398 2842868.6933648163 0, -1410314.8445067066 2842868.6933643688 0, -1410074.8976017982 2842822.7379557453 0, -1409974.2514204897 2842803.210860995 0, -1409926.9607263294 2842794.120359546 0, -1409574.4517075391 2842726.364992527 0, -1409539.7596685698 2842719.476227892 0, -1409539.1167997618 2842719.3485740544 0, -1409539.1167996211 2842719.3485740265 0, -1409407.3427740564 2842693.406117487 0, -1409174.87310327 2842647.185105116 0, -1409135.3708942847 2842639.3610066515 0, -1408775.2871312238 2842568.0429873103 0, -1408775.2871312243 2842568.042987308 0, -1408775.2871312224 2842568.0429873075 0, -1408791.982561276 2842482.1825481723 0, -1408859.431612287 2842135.3088754904 0, -1408936.0102514483 2841742.172147534 0, -1409010.5622617726 2841352.679039439 0, -1409011.4184577104 2841348.2058882047 0, -1409086.8267116826 2840954.237889088 0, -1409107.1392109245 2840958.307386213 0, -1409374.2239804657 2841010.0749029545 0, -1409488.590801991 2841032.1093411823 0, -1409488.590810442 2841032.1093428046 0, -1409488.5908287365 2841032.1093463674 0, -1409735.5629954843 2841080.1273449566 0, -1409890.3520447423 2841110.0070721535 0, -1410027.3861210642 2841136.7169916257 0, -1410207.0886851817 2841171.569820003 0)), ((-1404413.0040087868 2845598.7170888362 0, -1404411.9634668445 2845599.4135239385 0, -1404403.6665685656 2845604.966773168 0, -1404367.6175215868 2845629.094281301 0, -1404365.3857084531 2845630.5880346466 0, -1404365.3856752666 2845630.588048675 0, -1404359.7842581766 2845634.337058641 0, -1404209.994285118 2845697.6924938657 0, -1403967.0449391939 2845739.4757514074 0, -1403962.6991410798 2845740.222877639 0, -1403925.888990231 2845756.5350805065 0, -1403811.697381762 2845808.3746001213 0, -1403763.0290770517 2845813.871618658 0, -1403678.995867877 2845799.875162555 0, -1403644.1093635445 2845787.7281875107 0, -1403561.9104531568 2845792.578875461 0, -1403546.0403714462 2845795.453029865 0, -1403471.1140033456 2845809.0260385834 0, -1403350.954397719 2845815.8751161206 0, -1403137.9662648952 2845786.6090687537 0, -1403161.1101112196 2845669.769369071 0, -1403161.3519901694 2845669.741687514 0, -1403161.3953671006 2845669.522701863 0, -1403166.1869040276 2845668.9743470913 0, -1403166.6076956226 2845666.871903373 0, -1403587.2478790737 2845618.1462674816 0, -1403645.7782884282 2845611.3678443404 0, -1403671.7299334654 2845608.36233764 0, -1403654.8238005526 2845469.124905376 0, -1403609.740873767 2845474.285456348 0, -1403190.3208668637 2845522.3126093117 0, -1403267.3277244826 2845133.712013439 0, -1403345.307317196 2844741.3896947694 0, -1403345.3073174688 2844741.3896933924 0, -1403351.278613076 2844742.575062426 0, -1403351.9856773617 2844739.030921994 0, -1403739.775040757 2844819.6959529603 0, -1403739.7750432093 2844819.695953447 0, -1403739.775176096 2844819.695979834 0, -1404142.2220031724 2844899.538941732 0, -1404538.6548402628 2844972.33059754 0, -1404934.1430632109 2845049.787531759 0, -1404468.8456640067 2845562.344196431 0, -1404413.0040087868 2845598.7170888362 0)), ((-1404384.173923037 2845913.506921877 0, -1404460.723088921 2845877.299411543 0, -1404498.694650209 2845842.6323788343 0, -1404543.1465726472 2845794.266376779 0, -1404553.1898897956 2845768.42480921 0, -1404560.4058094958 2845767.591449572 0, -1404562.263610549 2845762.872978879 0, -1404602.726522319 2845758.1884405124 0, -1404617.3759774447 2845736.0786963697 0, -1404641.038383801 2845700.366122346 0, -1404770.6570928784 2845608.785523316 0, -1404825.8077152742 2845544.414600234 0, -1404824.4991240369 2845551.0100588636 0, -1404835.93094067 2845538.743090079 0, -1404776.9849010152 2845832.7790643815 0, -1404698.3157223004 2846224.9341655592 0, -1404619.6501308896 2846617.0814418728 0, -1404613.1333087308 2846615.800988013 0, -1404611.440918708 2846624.325265719 0, -1404217.1673162603 2846545.7387325265 0, -1403822.8913253082 2846467.1743903724 0, -1403428.6090668149 2846388.631626333 0, -1403034.3220979962 2846310.11094714 0, -1403053.4782844791 2846213.634980691 0, -1403098.5972614503 2845986.403067261 0, -1403102.6692528867 2845986.22169955 0, -1403103.248347781 2845983.290500964 0, -1403194.7240722105 2845979.1141459174 0, -1403449.0559606147 2846028.010740485 0, -1403504.9632931324 2846028.6813831767 0, -1403799.7788403556 2846032.221859208 0, -1403917.369560205 2846021.144461339 0, -1404023.201279463 2846011.177178477 0, -1404120.1833968922 2845982.644777186 0, -1404347.9635557476 2845922.9921767535 0, -1404384.173923037 2845913.506921877 0)), ((-1397408.2962231054 2850092.3249010867 0, -1397368.4896856248 2850084.068534674 0, -1397446.3713279825 2849691.2643500497 0, -1397505.381414212 2849392.6996998107 0, -1397510.6108350344 2849365.822199518 0, -1397524.2513040218 2849298.457697818 0, -1397541.4491653107 2849211.7165610585 0, -1397541.458220491 2849211.6708892966 0, -1397542.5345600036 2849206.2421379318 0, -1397543.8495907197 2849199.6533351694 0, -1397552.4185829689 2849156.451312542 0, -1397575.9850958055 2849037.5695722825 0, -1397592.0332196734 2848956.627131109 0, -1397592.679842527 2848953.3228822346 0, -1397592.6798425396 2848953.3228821703 0, -1397602.13302944 2848905.6434157547 0, -1397665.8361152133 2848583.3899085936 0, -1397680.0171525239 2848512.827412834 0, -1397680.0171525334 2848512.8274127864 0, -1397929.700960232 2848562.7028559577 0, -1397929.7009632865 2848562.702856566 0, -1397948.4323890347 2848566.4242267665 0, -1397957.4309592475 2848568.2419514772 0, -1397957.4309620752 2848568.241952046 0, -1398077.2551434217 2848592.176531594 0, -1398141.5814011388 2848605.029787731 0, -1398239.0745437716 2848624.510235964 0, -1398247.1236719787 2848626.1050571734 0, -1398282.7133075856 2848633.219462183 0, -1398287.580911698 2848634.192208714 0, -1398327.5059190358 2848642.169873064 0, -1398332.0947335428 2848643.086969197 0, -1398372.692625795 2848651.1939333444 0, -1398377.8822906353 2848652.2453921833 0, -1398377.8822907384 2848652.2453922043 0, -1398377.8822960923 2848652.2453932827 0, -1398474.4887164899 2848671.5479072505 0, -1398871.7176727587 2848750.941513455 0, -1398936.6503813192 2848763.925655422 0, -1398962.2122963727 2848769.0345055317 0, -1399102.7436877913 2848797.11353484 0, -1399111.7925354156 2848798.9398238114 0, -1399113.3217560383 2848799.2471367856 0, -1399268.9442821615 2848830.357851166 0, -1399266.4973957373 2848842.226063975 0, -1399231.7310575226 2849019.0364407757 0, -1399231.7310429218 2849019.036515031 0, -1399221.9107939033 2849069.0883870637 0, -1399215.8337490482 2849099.6392980004 0, -1399215.8337490472 2849099.639298005 0, -1399215.833740717 2849099.639340032 0, -1399191.420180221 2849223.420864117 0, -1399191.322303488 2849223.9171182876 0, -1399113.7035125983 2849617.4718418084 0, -1399036.0835453114 2850011.0212396816 0, -1398958.4665678807 2850404.5660594977 0, -1398945.88544305 2850402.2433631923 0, -1398647.0857153283 2850341.77419907 0, -1398647.0857049285 2850341.774196965 0, -1398647.085704724 2850341.7741969237 0, -1398622.6991095608 2850336.8458357486 0, -1398618.7863314683 2850336.06729265 0, -1398618.7863266538 2850336.0672917007 0, -1398560.9794564047 2850324.409822854 0, -1398193.5005080379 2850250.547556947 0, -1398163.4883337207 2850244.272879605 0, -1397765.99050446 2850164.157983164 0, -1397408.2962231054 2850092.3249010867 0)), ((-1408499.7917902402 2851897.0108265877 0, -1408421.0447701633 2852289.2328041033 0, -1408208.4406804384 2852246.8743553446 0, -1408024.111393916 2852209.763787432 0, -1407803.8467946316 2852165.883525409 0, -1407627.1719187878 2852130.313602257 0, -1407230.2294260436 2852050.8889755737 0, -1407230.2294255465 2852050.888975477 0, -1407206.2683501462 2852046.303831964 0, -1406833.2804088348 2851971.486434671 0, -1406833.280408835 2851971.4864346697 0, -1406911.933817793 2851579.414764962 0, -1406921.6758014641 2851530.0046396935 0, -1406934.686355972 2851465.14776617 0, -1406956.335386052 2851357.2290452607 0, -1406990.586042128 2851187.337697579 0, -1406990.5860421804 2851187.3376973188 0, -1406990.5860422545 2851187.3376969495 0, -1407041.0215364834 2850935.08214724 0, -1407069.2414205894 2850795.256210503 0, -1407069.2414206765 2850795.2562100706 0, -1407069.2414206867 2850795.2562100184 0, -1407073.5684860025 2850772.8424741207 0, -1407147.89795659 2850403.1700436547 0, -1407147.8979565974 2850403.170043656 0, -1407147.897956598 2850403.1700436533 0, -1407506.3690000873 2850474.723267223 0, -1407544.9384991385 2850482.421997814 0, -1407941.9745221676 2850561.6962001207 0, -1408339.0062130108 2850640.9927756977 0, -1408736.0331859435 2850720.3115733187 0, -1408657.41158823 2851111.919579926 0, -1408657.2847018465 2851112.5515910415 0, -1408578.5377025602 2851504.7836576267 0, -1408499.7917902402 2851897.0108265877 0)), ((-1402322.4997742055 2855962.8549554977 0, -1401926.2423490663 2855884.0684591965 0, -1401529.9818892553 2855805.3075370626 0, -1401133.7178690603 2855726.5661011315 0, -1401213.211228292 2855335.412905123 0, -1401292.708138397 2854944.2551045995 0, -1401372.2039204885 2854553.0919847465 0, -1401451.7031004892 2854161.9246495627 0, -1401847.939906079 2854240.6579817794 0, -1402244.174336076 2854319.414166907 0, -1402640.4039476456 2854398.195590499 0, -1403036.6295266182 2854476.9962373967 0, -1402957.1582407928 2854868.1687561497 0, -1402877.6877139623 2855259.339419323 0, -1402798.2189316931 2855650.5022341553 0, -1402718.750697533 2856041.6632575803 0, -1402322.4997742055 2855962.8549554977 0)), ((-1411751.5853603992 2856418.185144432 0, -1411754.7571084467 2856429.033555226 0, -1411767.7582414288 2856473.501728358 0, -1411817.3561956498 2856643.1425894992 0, -1411842.2963358818 2856728.4480426703 0, -1411857.2971659566 2856779.7566173365 0, -1411866.2335776836 2856810.323187832 0, -1411899.5147161097 2856924.1581729716 0, -1411899.2923966853 2856930.5015921816 0, -1411897.9417615307 2856969.061157462 0, -1411894.9402896597 2857054.74085981 0, -1411894.5358408932 2857066.285733073 0, -1411894.0926921885 2857078.934847568 0, -1411893.5171049975 2857095.3595575998 0, -1411891.713688685 2857146.8214332475 0, -1411889.994330014 2857195.9125946364 0, -1411889.699684305 2857204.325522127 0, -1411880.874398725 2857470.4536910965 0, -1411878.0360349421 2857552.343632654 0, -1411875.6033314364 2857624.912060565 0, -1411877.2522324275 2857628.9538111114 0, -1411915.182499596 2857721.932867112 0, -1411933.3960081232 2857766.5799572086 0, -1411978.6628281383 2857877.543262183 0, -1411987.1789034253 2857898.418955808 0, -1411967.8125782465 2857894.7388543542 0, -1411940.9460620254 2857889.3657909026 0, -1411827.0057558136 2857866.5978943333 0, -1411816.2609931997 2857864.4504358424 0, -1411785.6653254726 2857858.335715912 0, -1411778.7458917818 2857856.7582134116 0, -1411778.7458915478 2857856.758213361 0, -1411594.861806844 2857819.9848252423 0, -1411383.7384575654 2857777.7640921324 0, -1411367.0593044949 2857774.617511555 0, -1410990.311091655 2857698.9297966924 0, -1410858.0004306268 2857672.622335774 0, -1410596.879148821 2857620.1174235255 0, -1410621.9852533883 2857491.62132465 0, -1410633.7672996472 2857431.7274165326 0, -1410674.0526222952 2857227.8057096056 0, -1410674.0526223222 2857227.805709468 0, -1410751.224144693 2856835.4917604737 0, -1410757.8768594344 2856800.8060144023 0, -1410820.825048066 2856480.8087421665 0, -1410828.3986047867 2856443.173116284 0, -1410828.3986047988 2856443.1731162234 0, -1410828.3986048105 2856443.173116164 0, -1410842.1263099334 2856372.5611441107 0, -1410905.5745906155 2856050.8465852523 0, -1411295.5805096321 2856130.8219032804 0, -1411432.25054098 2856158.360234526 0, -1411432.2505409804 2856158.360234527 0, -1411432.3744690558 2856158.659060573 0, -1411528.0464481325 2856236.440972607 0, -1411560.3916010382 2856262.7377897943 0, -1411667.3655141646 2856349.7080069594 0, -1411702.6279902614 2856378.379090404 0, -1411740.73912433 2856409.366361044 0, -1411751.5853603992 2856418.185144432 0)), ((-1405261.3863524538 2859814.963898068 0, -1405651.2703595373 2859892.5344997076 0, -1406048.3939748404 2859971.7027081377 0, -1406445.5149132037 2860050.8938099025 0, -1406842.6286486182 2860130.1098150183 0, -1406842.628648618 2860130.1098150196 0, -1406764.8265913033 2860522.0183203532 0, -1406688.7504382622 2860905.23269522 0, -1406687.0248609448 2860913.924854412 0, -1406687.0248609437 2860913.924854418 0, -1406415.590490284 2860859.6128464383 0, -1406290.115452382 2860834.5054980735 0, -1405897.4905057237 2860756.1532146623 0, -1405893.2084571854 2860755.084839173 0, -1405815.6258750965 2861146.7138585607 0, -1406212.4251978938 2861226.269456487 0, -1406609.224541734 2861305.8234384237 0, -1406531.4236872834 2861697.717321509 0, -1406531.4236872534 2861697.717321503 0, -1406531.4236872522 2861697.717321509 0, -1406134.7369737187 2861618.013712855 0, -1405738.045266009 2861538.3353076545 0, -1405341.3495085759 2861458.6764138103 0, -1404944.6466850971 2861379.042249062 0, -1405022.0205961196 2860987.6359433997 0, -1405099.3936611253 2860596.2250118344 0, -1405176.7677404573 2860204.8092027605 0, -1404780.8769870354 2860124.730539985 0, -1404858.3628771487 2859733.3601081683 0, -1404935.3719751574 2859342.672009466 0, -1405331.1001697828 2859423.1280607716 0, -1405254.1434443628 2859813.3853914333 0, -1405261.3863524538 2859814.963898068 0)), ((-1402682.2020684432 2864118.7237778557 0, -1402695.4529211784 2864121.2283095215 0, -1402695.4529211782 2864121.228309523 0, -1402616.8936437613 2864513.0297153555 0, -1402538.3358605783 2864904.823133617 0, -1402499.8153482743 2865096.9325434817 0, -1402459.7765047003 2865296.6141715446 0, -1402419.7474271564 2865496.252592065 0, -1402381.2202299368 2865688.4006322375 0, -1402381.2202299358 2865688.4006322417 0, -1401983.5451695155 2865608.8553613233 0, -1401712.7970666003 2865554.720197429 0, -1401585.8632989998 2865529.3320246567 0, -1401188.179284525 2865449.831439479 0, -1401188.1792117932 2865449.831424936 0, -1401097.3997936426 2865431.6841614405 0, -1401084.8622124526 2865429.1840025107 0, -1400799.226584094 2865372.3078978863 0, -1400790.4886198821 2865370.35311039 0, -1400868.6112097064 2864978.9369326024 0, -1400945.8802026587 2864590.1986702695 0, -1400946.7321918367 2864587.5186793273 0, -1401024.8546978398 2864196.092250667 0, -1401100.9681356936 2863813.8579939683 0, -1401102.9804730942 2863804.661391134 0, -1401161.397036985 2863816.255982978 0, -1401501.1095115985 2863883.7670430006 0, -1401558.569074346 2863895.1879364145 0, -1401899.2323785443 2863962.904431385 0, -1401955.7386749384 2863974.1206539576 0, -1402297.3480475233 2864042.044840975 0, -1402352.9085788366 2864053.0954119097 0, -1402682.2020684432 2864118.7237778557 0)), ((-1411465.037336772 2865648.779537992 0, -1411463.8557415532 2865655.0362547883 0, -1411467.7572204815 2865655.390586278 0, -1411528.471929807 2865656.642773342 0, -1411528.4719302277 2865656.6427733493 0, -1411528.471930238 2865656.6427733507 0, -1411528.4719302412 2865656.6427733507 0, -1411569.6250164183 2865661.9779159166 0, -1411578.782938681 2865663.366841497 0, -1411605.6501287578 2865674.490354063 0, -1411625.477942975 2865682.6947615296 0, -1411631.7469223023 2865685.3064114386 0, -1411632.7949084023 2865685.7423111056 0, -1411635.878725861 2865685.393298609 0, -1411647.15672865 2865684.1156663178 0, -1411652.734374543 2865683.483661498 0, -1411663.069627925 2865682.308265712 0, -1411676.9610435506 2865680.725924123 0, -1411731.4632386134 2865723.2860093727 0, -1411740.6671240507 2865730.519389325 0, -1411822.090020838 2865718.2191672903 0, -1411838.3978266304 2865715.9588456973 0, -1411841.073689812 2865717.1605165387 0, -1411983.169821221 2865779.4717531553 0, -1411983.1698278135 2865779.4717560387 0, -1411999.7797165555 2865786.7246760647 0, -1412158.2912243297 2865835.9466782827 0, -1412170.146075653 2865836.9489773572 0, -1412170.146076222 2865836.9489774047 0, -1412229.6105864234 2865841.7906655665 0, -1412229.6105864223 2865841.790665572 0, -1412229.6105864225 2865841.790665572 0, -1412229.6105863927 2865841.7906657173 0, -1412219.1846687484 2865892.884224412 0, -1412162.0192036116 2866176.968186281 0, -1412082.825008011 2866569.0058447286 0, -1412002.6728112134 2866961.1972452626 0, -1411922.5221962316 2867353.380643108 0, -1411922.5221962258 2867353.3806431065 0, -1411922.522196224 2867353.3806431163 0, -1411583.5471875449 2867284.2856640294 0, -1411524.470183467 2867272.0276043857 0, -1411445.3103906135 2867256.03696549 0, -1411360.55465754 2867238.708295354 0, -1411126.4154879246 2867190.697131833 0, -1411025.867544467 2867170.3460400575 0, -1410917.9101386506 2867148.296874894 0, -1410817.3561835214 2867127.759786799 0, -1410728.3555018317 2867109.3920901567 0, -1410728.3549554553 2867109.3919785875 0, -1410610.287801935 2867085.2829328044 0, -1410330.3074244468 2867028.109796696 0, -1410330.291306805 2867028.1065054135 0, -1410361.2985384562 2866873.7711350676 0, -1410409.33354803 2866634.6905706557 0, -1410420.9139694646 2866577.055654584 0, -1410440.2146718572 2866480.997461124 0, -1410440.2146719096 2866480.9974608603 0, -1410456.6149111663 2866398.174093309 0, -1410463.2236422338 2866365.1634405 0, -1410488.222008319 2866241.2386903674 0, -1410504.0888303516 2866161.32310462 0, -1410519.0021884008 2866088.0397656164 0, -1410519.002188406 2866088.0397655913 0, -1410566.296370515 2865852.6473873486 0, -1410597.9484032183 2865695.10541922 0, -1410644.2002541109 2865464.0360314716 0, -1410644.2099788839 2865464.0379698332 0, -1410644.2113585516 2865464.0310786646 0, -1410684.423421186 2865472.053394944 0, -1411044.5673082075 2865544.3390496573 0, -1411064.664278303 2865548.3758619865 0, -1411303.885356992 2865596.5309854182 0, -1411444.901632407 2865624.715773975 0, -1411454.7045603914 2865626.808822695 0, -1411468.8876433342 2865629.512212369 0, -1411468.8876433324 2865629.512212379 0, -1411465.037336772 2865648.779537992 0)), ((-1405352.3578766033 2869543.935077524 0, -1405359.1363504976 2869545.2042935197 0, -1405436.3132154464 2869560.2322490425 0, -1405502.746418892 2869573.2515146 0, -1405502.7464338238 2869573.2515175208 0, -1405720.6097105232 2869615.720096893 0, -1406118.040747909 2869693.2168943826 0, -1406295.4979188778 2869727.8309028526 0, -1406335.326025477 2869735.548965003 0, -1406368.3830205046 2869742.047260953 0, -1406368.3830230972 2869742.047261461 0, -1406515.4696160685 2869770.7362509747 0, -1406515.4696160683 2869770.736250976 0, -1406515.3518045028 2869771.324431194 0, -1406436.8880400027 2870163.058756294 0, -1406358.3075719213 2870555.3763669888 0, -1406349.6235684261 2870598.7326819636 0, -1406349.6235644566 2870598.7327020443 0, -1406348.2495920586 2870605.7389051924 0, -1406343.9503185805 2870627.2036582665 0, -1406334.9120333896 2870672.1828832966 0, -1406279.7301098744 2870947.689329546 0, -1406259.8342604002 2871047.0207821187 0, -1406256.6776818188 2871062.9237264954 0, -1406248.9494264596 2871101.3638142054 0, -1406201.1516861857 2871339.9969154075 0, -1405935.8783990357 2871288.0464658416 0, -1405919.2268095443 2871284.7765399343 0, -1405859.9066085038 2871273.1582050133 0, -1405856.2419319113 2871272.450294864 0, -1405856.241927392 2871272.4502939982 0, -1405803.751681128 2871262.170407299 0, -1405658.300430607 2871233.6943604634 0, -1405644.932170153 2871231.0641286485 0, -1405623.858496985 2871226.937981929 0, -1405605.0992181995 2871223.278679066 0, -1405605.0992040872 2871223.278676319 0, -1405406.3471053601 2871184.366241646 0, -1405435.624495818 2871038.2277601827 0, -1405437.0592010934 2871031.0664098286 0, -1405441.9988417523 2871006.4998400114 0, -1405484.3701475295 2870794.999082076 0, -1405484.9057895474 2870792.2393457848 0, -1405479.7815442246 2870791.226744264 0, -1405424.8324013767 2870780.4771098006 0, -1405420.8968640964 2870779.7077110303 0, -1405370.7645056879 2870769.9052323746 0, -1405367.6517246566 2870769.2986274436 0, -1405283.9653302229 2870752.933274581 0, -1405255.9106829148 2870747.465511902 0, -1405255.9106593088 2870747.46550731 0, -1405205.8767456764 2870737.7331411466 0, -1405087.490981406 2870714.534637766 0, -1405066.3558166963 2870710.5732503003 0, -1404937.6800193107 2870685.241462984 0, -1404912.420841931 2870680.2812086833 0, -1404873.690080004 2870672.728276086 0, -1404690.0778117212 2870636.8252614536 0, -1404690.077166699 2870636.8251353293 0, -1404690.0771666993 2870636.825135328 0, -1404708.0471434693 2870547.146432178 0, -1404710.958022651 2870532.710837276 0, -1404753.5632293806 2870320.0914300634 0, -1404767.9136741732 2870248.445385562 0, -1404768.6279536458 2870244.8196088024 0, -1404768.6279536616 2870244.819608721 0, -1404775.7641339956 2870209.20661129 0, -1404775.7641365211 2870209.206598999 0, -1404776.9359453998 2870203.4499911657 0, -1404809.6746020482 2870040.0693464084 0, -1404828.469240713 2869946.2757398025 0, -1404829.4227403163 2869941.5171959335 0, -1404831.863324543 2869929.2458460294 0, -1404847.1798434148 2869852.8091909704 0, -1404851.4089969185 2869831.7039236957 0, -1404851.4422845743 2869831.5378041933 0, -1404852.1575244702 2869828.0605850974 0, -1404853.231110614 2869822.7023808896 0, -1404856.9175901003 2869804.3054733314 0, -1404883.9239550708 2869669.5310635734 0, -1404889.6944281512 2869640.6415555426 0, -1404889.6944321946 2869640.6415352616 0, -1404925.732661221 2869460.793662609 0, -1405323.1722710785 2869538.245600288 0, -1405352.3578766033 2869543.935077524 0)), ((-1403270.9110435373 2873607.989720598 0, -1403195.57265247 2873987.095011088 0, -1402798.6169425067 2873907.8261163756 0, -1402874.1480264233 2873528.383814522 0, -1402952.0604383987 2873136.965264704 0, -1403348.7412445976 2873216.3452473097 0, -1403270.9110435373 2873607.989720598 0)), ((-1400722.020211627 2873987.416916897 0, -1400659.8349719865 2874300.9579526847 0, -1400582.1008802357 2874692.897713141 0, -1400504.368199048 2875084.8295678613 0, -1400504.3681990472 2875084.8295678655 0, -1400306.06796822 2875046.0779310446 0, -1400108.2805656404 2875006.994913384 0, -1399712.1886875827 2874929.1824742686 0, -1399316.0923516774 2874851.392322538 0, -1398919.9918312414 2874773.6246947986 0, -1398997.4825770769 2874381.3695183387 0, -1399074.9721307347 2873989.109292349 0, -1399152.464837142 2873596.8441945347 0, -1399229.9583728071 2873204.574122286 0, -1399626.3009079173 2873282.6651033484 0, -1400022.6398035127 2873360.7752654627 0, -1400418.9757098868 2873438.911310901 0, -1400341.2951306698 2873830.9661018522 0, -1400408.590619487 2873844.220564607 0, -1400737.569628418 2873909.015992905 0, -1400737.5696284168 2873909.0159929106 0, -1400737.5696284187 2873909.015992911 0, -1400722.020211627 2873987.416916897 0)), ((-1409103.6964492481 2875025.2421185113 0, -1409141.8900567754 2875032.891256656 0, -1409213.6801065572 2875047.2731291484 0, -1409213.6801090706 2875047.273129647 0, -1409229.77988655 2875050.449152512 0, -1409285.8021089113 2875061.721309533 0, -1409285.8021396676 2875061.7213157113 0, -1409535.654514666 2875111.773087116 0, -1409929.4117891053 2875190.679700427 0, -1409971.24784557 2875199.065926775 0, -1409971.2478463105 2875199.065926921 0, -1409978.7519803427 2875200.531137577 0, -1410108.979261336 2875226.637376353 0, -1410140.157719893 2875232.924347864 0, -1410323.172103583 2875269.6090371227 0, -1410323.1721035815 2875269.609037131 0, -1410323.1721035817 2875269.609037131 0, -1410280.0390395173 2875485.7118710545 0, -1410275.657886319 2875507.7470515314 0, -1410272.7716184133 2875522.122472482 0, -1410244.8465344294 2875662.031449576 0, -1410244.846486525 2875662.031689817 0, -1410238.80266182 2875692.360027673 0, -1410188.7019879804 2875943.3155002077 0, -1410185.8364133637 2875957.6702931076 0, -1410166.5198291473 2876054.448420859 0, -1410154.9493124203 2876112.3908099523 0, -1410129.6492050847 2876239.1153764776 0, -1410097.0531707695 2876404.0092286854 0, -1410096.267817752 2876406.490527884 0, -1410095.9545911942 2876406.9131187014 0, -1410092.6124654415 2876411.4155137967 0, -1410071.9405331241 2876439.594348282 0, -1410067.334844834 2876445.872557595 0, -1410044.8896179674 2876476.467052874 0, -1410017.2528691767 2876514.1379344515 0, -1410017.2528691764 2876514.1379344515 0, -1410017.2513635792 2876514.139986689 0, -1409975.5495828802 2876541.3013308863 0, -1409950.1803787204 2876557.8212493835 0, -1409908.6595203627 2876584.8949637697 0, -1409866.487935356 2876612.392758426 0, -1409766.4990217146 2876677.5969618005 0, -1409766.4997185215 2876677.6499651307 0, -1409766.2500051307 2876677.812799691 0, -1409766.6451122717 2876704.2036529 0, -1409767.1408562034 2876737.3104113834 0, -1409767.507660834 2876761.8052125834 0, -1409769.9336998635 2876795.1547505893 0, -1409764.5592822868 2876794.095048755 0, -1409627.5944055112 2876766.6532114935 0, -1409510.6739233304 2876743.2241767757 0, -1409446.8540509548 2876730.4106893907 0, -1409310.6548475022 2876703.0646280306 0, -1409263.1621494931 2876693.52887364 0, -1409260.287299188 2876692.9515570784 0, -1409230.218035185 2876686.8663708684 0, -1408832.1384908531 2876608.0227922006 0, -1408774.6639410295 2876596.8008374856 0, -1408728.6500602255 2876587.657983948 0, -1408514.9915482828 2876545.2276930353 0, -1408514.9915142735 2876545.2276862813 0, -1408455.7443594562 2876533.474764181 0, -1408452.775912659 2876532.908685063 0, -1408434.0567597842 2876529.2021547086 0, -1408446.2223965924 2876468.189760085 0, -1408486.3784147138 2876266.7236018917 0, -1408489.3887333323 2876251.6218461953 0, -1408512.5581591323</t>
+          <t>MULTIPOLYGON Z (((-1406379.8180101914 2835502.9676008387 0, -1406473.9785516895 2835521.734531294 0, -1406778.7770429626 2835582.4882667917 0, -1406872.8312997553 2835601.148932945 0, -1406791.7645722493 2835992.9266004586 0, -1406710.698745883 2836384.702508994 0, -1406629.6366764735 2836776.4711096287 0, -1406548.5739271764 2837168.2345223785 0, -1406152.1431418383 2837088.956904065 0, -1406087.6405494164 2837076.280484532 0, -1405796.91670816 2837018.1569047323 0, -1405755.7083628573 2837009.698301688 0, -1405535.803621465 2836965.9663151815 0, -1405487.176097592 2836956.2471401114 0, -1405359.2691901615 2836930.461773824 0, -1405080.115136758 2836874.9046132243 0, -1404962.8255844747 2836851.2476163614 0, -1405025.8156075906 2836537.4335374683 0, -1405029.769174486 2836517.7370062955 0, -1405041.4965421397 2836459.306839623 0, -1405041.4965422011 2836459.306839316 0, -1405081.6600892353 2836258.4058300443 0, -1405108.2831449925 2836126.578187748 0, -1405120.0309416638 2836067.337313631 0, -1405133.2551556446 2836000.645850542 0, -1405186.659309687 2835735.386966785 0, -1405188.114813715 2835727.329112005 0, -1405192.8804176834 2835703.5856685042 0, -1405198.701406638 2835675.389715876 0, -1405261.8129454285 2835360.1547357994 0, -1405265.1738896933 2835344.2151984107 0, -1405277.2234497615 2835283.407895384 0, -1405277.2234497755 2835283.4078953867 0, -1405277.2234497757 2835283.4078953853 0, -1405581.9305416776 2835344.089946119 0, -1405676.1759969064 2835362.862839606 0, -1405980.8366573509 2835423.550296702 0, -1406075.138144352 2835442.2583379205 0, -1406202.3274685177 2835467.601562032 0, -1406379.8180101914 2835502.9676008387 0)), ((-1399356.4079068387 2840020.2810208434 0, -1399368.1809894112 2839960.4057747424 0, -1399384.6546780465 2839877.227700831 0, -1399462.396458146 2839484.6995438226 0, -1399540.139008013 2839092.1665506647 0, -1399542.905688448 2839092.835199241 0, -1399556.3294038298 2839095.3861888293 0, -1399556.3294040805 2839095.3861888773 0, -1399561.6720821362 2839096.376602012 0, -1399582.007635379 2839100.423022579 0, -1399599.5649045492 2839103.916675662 0, -1399623.3376730068 2839108.6470440533 0, -1399644.5027693652 2839112.8586522965 0, -1399667.8546858106 2839117.505222619 0, -1399689.9714188937 2839121.9060038663 0, -1399712.3326666437 2839126.3553711157 0, -1399735.4324632378 2839130.9517879887 0, -1399753.6615634388 2839134.578885354 0, -1399780.8692110055 2839139.992492276 0, -1399798.1407629494 2839143.429084783 0, -1399826.33910559 2839149.039729029 0, -1399842.651850635 2839152.2853515954 0, -1399871.8019453995 2839158.085069711 0, -1399883.9572934853 2839160.5036009005 0, -1399916.771608468 2839167.0324040405 0, -1399928.497425498 2839169.3652046104 0, -1399934.4273121587 2839170.492037641 0, -1399937.3344581702 2839171.1505293464 0, -1399937.334458662 2839171.150529451 0, -1399937.3344698094 2839171.1505316654 0, -1399961.7740465652 2839175.991441545 0, -1399972.9727293379 2839178.2173738675 0, -1400007.6713144428 2839185.123969481 0, -1400014.3015124146 2839186.44347234 0, -1400053.0843019113 2839194.164184724 0, -1400059.1674090049 2839195.3749906607 0, -1400062.5253671096 2839196.043416641 0, -1400098.5195565978 2839203.2079879213 0, -1400103.2938011107 2839204.1582646235 0, -1400135.8492566794 2839210.638179495 0, -1400143.9549004098 2839212.251141099 0, -1400147.7740981488 2839213.0111707496 0, -1400189.1188868866 2839221.238374427 0, -1400322.934807602 2839247.8660599813 0, -1400331.4578416802 2839249.561483696 0, -1400334.5232879098 2839250.1564733693 0, -1400337.289539137 2839250.8269082224 0, -1400438.6676987924 2839270.9013746134 0, -1400616.4727830754 2839306.2846389473 0, -1400666.7624768384 2839316.2673303704 0, -1400731.7096861927 2839329.18493668 0, -1400734.4720727175 2839329.8709867066 0, -1400774.2737872985 2839337.662505503 0, -1400819.7837660834 2839346.7515740218 0, -1401125.8721471464 2839407.6680866037 0, -1401128.8917457967 2839408.235767459 0, -1401123.9478869513 2839432.9798185662 0, -1401114.9923184975 2839478.068050874 0, -1401105.4885421125 2839525.9158027335 0, -1401103.154785328 2839537.809666259 0, -1401103.15478518 2839537.809667019 0, -1401067.6565216575 2839720.071360423 0, -1401063.830226231 2839739.28926802 0, -1401063.2021711767 2839742.434400068 0, -1401053.3518599859 2839788.545631688 0, -1401050.9229196983 2839800.7740466096 0, -1401050.9229196971 2839800.7740466157 0, -1401053.6475980359 2839801.596686764 0, -1400999.4443926136 2840062.6907491884 0, -1400998.724069705 2840066.308780294 0, -1400989.0886561542 2840114.569291522 0, -1400975.3905077311 2840183.1795261377 0, -1400973.5361308325 2840190.3820250407 0, -1400973.536130806 2840190.382025154 0, -1400972.9550610757 2840193.3075143024 0, -1400954.6895441287 2840190.4323968505 0, -1400920.226759528 2840183.5676653488 0, -1400578.8062332084 2840115.124226884 0, -1400575.8805057171 2840114.2936359607 0, -1400575.7633936796 2840117.3285491103 0, -1400574.844702643 2840122.2522871094 0, -1400574.022585394 2840126.3318334757 0, -1400566.8949736727 2840162.4611979346 0, -1400542.6533913193 2840284.271411241 0, -1400539.2966141847 2840301.1361504267 0, -1400517.715227514 2840409.5622253655 0, -1400512.0344126902 2840438.1135863895 0, -1400502.104311991 2840485.9874962857 0, -1400497.9721403266 2840506.8058186676 0, -1400497.390664912 2840509.80477352 0, -1400452.1259811474 2840738.4564959686 0, -1400451.4587958015 2840741.808285925 0, -1400428.6235849268 2840856.2023643884 0, -1400420.8018900126 2840895.468983268 0, -1400420.069223923 2840899.301431375 0, -1400274.7199397993 2840870.543052567 0, -1400213.4646311947 2840858.3298914144 0, -1400023.1088309977 2840820.26744506 0, -1400022.4191629284 2840823.311960139 0, -1399739.523394895 2840764.6045222455 0, -1399736.5386692584 2840764.0057220142 0, -1399709.2365354546 2840758.5145079345 0, -1399626.1434866686 2840741.2589619365 0, -1399229.1764102448 2840662.2699850057 0, -1399306.9140804114 2840269.750971841 0, -1399306.9140826785 2840269.7509606453 0, -1399308.926485363 2840259.6770075844 0, -1399310.6939220119 2840250.9220541627 0, -1399335.4899758273 2840125.914068922 0, -1399347.1961440216 2840066.79943821 0, -1399356.4079068387 2840020.2810208434 0)), ((-1399229.1764102448 2840662.2699850057 0, -1399151.2946448606 2841054.7992079007 0, -1398754.3652302015 2840975.7562494082 0, -1398357.4368467703 2840896.7085765144 0, -1398434.9954991627 2840504.121791033 0, -1398832.0885730598 2840583.1832069866 0, -1399229.1764102448 2840662.2699850057 0)), ((-1410207.0886851817 2841171.569820003 0, -1410292.106862424 2841187.9271961376 0, -1410693.8600138929 2841265.8675316847 0, -1410641.7045664315 2841528.5669757756 0, -1410634.2942596902 2841565.9644431355 0, -1410616.0088154103 2841658.7990578404 0, -1410598.9623274822 2841744.276462479 0, -1410583.5237163594 2841822.194011335 0, -1410567.3071516913 2841904.0386808235 0, -1410550.4485024924 2841989.125877908 0, -1410546.7760295542 2842007.661339168 0, -1410538.1586854516 2842051.725978964 0, -1410475.0699257555 2842369.6151062693 0, -1410460.3759917119 2842444.344847481 0, -1410410.353163191 2842696.3028291394 0, -1410373.9500720813 2842880.5766738653 0, -1410314.8445090398 2842868.6933648163 0, -1410314.8445067066 2842868.6933643688 0, -1410074.8976017982 2842822.7379557453 0, -1409974.2514204897 2842803.210860995 0, -1409926.9607263294 2842794.120359546 0, -1409574.4517075391 2842726.364992527 0, -1409539.7596685698 2842719.476227892 0, -1409539.1167997618 2842719.3485740544 0, -1409539.1167996211 2842719.3485740265 0, -1409407.3427740564 2842693.406117487 0, -1409174.87310327 2842647.185105116 0, -1409135.3708942847 2842639.3610066515 0, -1408775.2871312238 2842568.0429873103 0, -1408775.2871312243 2842568.042987308 0, -1408775.2871312224 2842568.0429873075 0, -1408791.982561276 2842482.1825481723 0, -1408859.431612287 2842135.3088754904 0, -1408936.0102514483 2841742.172147534 0, -1409010.5622617726 2841352.679039439 0, -1409011.4184577104 2841348.2058882047 0, -1409086.8267116826 2840954.237889088 0, -1409107.1392109245 2840958.307386213 0, -1409374.2239804657 2841010.0749029545 0, -1409488.590801991 2841032.1093411823 0, -1409488.590810442 2841032.1093428046 0, -1409488.5908287365 2841032.1093463674 0, -1409735.5629954843 2841080.1273449566 0, -1409890.3520447423 2841110.0070721535 0, -1410027.3861210642 2841136.7169916257 0, -1410207.0886851817 2841171.569820003 0)), ((-1404413.0040087868 2845598.7170888362 0, -1404411.9634668445 2845599.4135239385 0, -1404403.6665685656 2845604.966773168 0, -1404367.6175215868 2845629.094281301 0, -1404365.3857084531 2845630.5880346466 0, -1404365.3856752666 2845630.588048675 0, -1404359.7842581766 2845634.337058641 0, -1404209.994285118 2845697.6924938657 0, -1403967.0449391939 2845739.4757514074 0, -1403962.6991410798 2845740.222877639 0, -1403925.888990231 2845756.5350805065 0, -1403811.697381762 2845808.3746001213 0, -1403763.0290770517 2845813.871618658 0, -1403678.995867877 2845799.875162555 0, -1403644.1093635445 2845787.7281875107 0, -1403561.9104531568 2845792.578875461 0, -1403546.0403714462 2845795.453029865 0, -1403471.1140033456 2845809.0260385834 0, -1403350.954397719 2845815.8751161206 0, -1403137.9662648952 2845786.6090687537 0, -1403161.1101112196 2845669.769369071 0, -1403161.3519901694 2845669.741687514 0, -1403161.3953671006 2845669.522701863 0, -1403166.1869040276 2845668.9743470913 0, -1403166.6076956226 2845666.871903373 0, -1403587.2478790737 2845618.1462674816 0, -1403645.7782884282 2845611.3678443404 0, -1403671.7299334654 2845608.36233764 0, -1403654.8238005526 2845469.124905376 0, -1403609.740873767 2845474.285456348 0, -1403190.3208668637 2845522.3126093117 0, -1403267.3277244826 2845133.712013439 0, -1403345.307317196 2844741.3896947694 0, -1403345.3073174688 2844741.3896933924 0, -1403351.278613076 2844742.575062426 0, -1403351.9856773617 2844739.030921994 0, -1403739.775040757 2844819.6959529603 0, -1403739.7750432093 2844819.695953447 0, -1403739.775176096 2844819.695979834 0, -1404142.2220031724 2844899.538941732 0, -1404538.6548402628 2844972.33059754 0, -1404934.1430632109 2845049.787531759 0, -1404468.8456640067 2845562.344196431 0, -1404413.0040087868 2845598.7170888362 0)), ((-1404384.173923037 2845913.506921877 0, -1404460.723088921 2845877.299411543 0, -1404498.694650209 2845842.6323788343 0, -1404543.1465726472 2845794.266376779 0, -1404553.1898897956 2845768.42480921 0, -1404560.4058094958 2845767.591449572 0, -1404562.263610549 2845762.872978879 0, -1404602.726522319 2845758.1884405124 0, -1404617.3759774447 2845736.0786963697 0, -1404641.038383801 2845700.366122346 0, -1404770.6570928784 2845608.785523316 0, -1404825.8077152742 2845544.414600234 0, -1404824.4991240369 2845551.0100588636 0, -1404835.93094067 2845538.743090079 0, -1404776.9849010152 2845832.7790643815 0, -1404698.3157223004 2846224.9341655592 0, -1404619.6501308896 2846617.0814418728 0, -1404613.1333087308 2846615.800988013 0, -1404611.440918708 2846624.325265719 0, -1404217.1673162603 2846545.7387325265 0, -1403822.8913253082 2846467.1743903724 0, -1403428.6090668149 2846388.631626333 0, -1403034.3220979962 2846310.11094714 0, -1403053.4782844791 2846213.634980691 0, -1403098.5972614503 2845986.403067261 0, -1403102.6692528867 2845986.22169955 0, -1403103.248347781 2845983.290500964 0, -1403194.7240722105 2845979.1141459174 0, -1403449.0559606147 2846028.010740485 0, -1403504.9632931324 2846028.6813831767 0, -1403799.7788403556 2846032.221859208 0, -1403917.369560205 2846021.144461339 0, -1404023.201279463 2846011.177178477 0, -1404120.1833968922 2845982.644777186 0, -1404347.9635557476 2845922.9921767535 0, -1404384.173923037 2845913.506921877 0)), ((-1397408.2962231054 2850092.3249010867 0, -1397368.4896856248 2850084.068534674 0, -1397446.3713279825 2849691.2643500497 0, -1397505.381414212 2849392.6996998107 0, -1397510.6108350344 2849365.822199518 0, -1397524.2513040218 2849298.457697818 0, -1397541.4491653107 2849211.7165610585 0, -1397541.458220491 2849211.6708892966 0, -1397542.5345600036 2849206.2421379318 0, -1397543.8495907197 2849199.6533351694 0, -1397552.4185829689 2849156.451312542 0, -1397575.9850958055 2849037.5695722825 0, -1397592.0332196734 2848956.627131109 0, -1397592.679842527 2848953.3228822346 0, -1397592.6798425396 2848953.3228821703 0, -1397602.13302944 2848905.6434157547 0, -1397665.8361152133 2848583.3899085936 0, -1397680.0171525239 2848512.827412834 0, -1397680.0171525334 2848512.8274127864 0, -1397929.700960232 2848562.7028559577 0, -1397929.7009632865 2848562.702856566 0, -1397948.4323890347 2848566.4242267665 0, -1397957.4309592475 2848568.2419514772 0, -1397957.4309620752 2848568.241952046 0, -1398077.2551434217 2848592.176531594 0, -1398141.5814011388 2848605.029787731 0, -1398239.0745437716 2848624.510235964 0, -1398247.1236719787 2848626.1050571734 0, -1398282.7133075856 2848633.219462183 0, -1398287.580911698 2848634.192208714 0, -1398327.5059190358 2848642.169873064 0, -1398332.0947335428 2848643.086969197 0, -1398372.692625795 2848651.1939333444 0, -1398377.8822906353 2848652.2453921833 0, -1398377.8822907384 2848652.2453922043 0, -1398377.8822960923 2848652.2453932827 0, -1398474.4887164899 2848671.5479072505 0, -1398871.7176727587 2848750.941513455 0, -1398936.6503813192 2848763.925655422 0, -1398962.2122963727 2848769.0345055317 0, -1399102.7436877913 2848797.11353484 0, -1399111.7925354156 2848798.9398238114 0, -1399113.3217560383 2848799.2471367856 0, -1399268.9442821615 2848830.357851166 0, -1399266.4973957373 2848842.226063975 0, -1399231.7310575226 2849019.0364407757 0, -1399231.7310429218 2849019.036515031 0, -1399221.9107939033 2849069.0883870637 0, -1399215.8337490482 2849099.6392980004 0, -1399215.8337490472 2849099.639298005 0, -1399215.833740717 2849099.639340032 0, -1399191.420180221 2849223.420864117 0, -1399191.322303488 2849223.9171182876 0, -1399113.7035125983 2849617.4718418084 0, -1399036.0835453114 2850011.0212396816 0, -1398958.4665678807 2850404.5660594977 0, -1398945.88544305 2850402.2433631923 0, -1398647.0857153283 2850341.77419907 0, -1398647.0857049285 2850341.774196965 0, -1398647.085704724 2850341.7741969237 0, -1398622.6991095608 2850336.8458357486 0, -1398618.7863314683 2850336.06729265 0, -1398618.7863266538 2850336.0672917007 0, -1398560.9794564047 2850324.409822854 0, -1398193.5005080379 2850250.547556947 0, -1398163.4883337207 2850244.272879605 0, -1397765.99050446 2850164.157983164 0, -1397408.2962231054 2850092.3249010867 0)), ((-1408499.7917902402 2851897.0108265877 0, -1408421.0447701633 2852289.2328041033 0, -1408208.4406804384 2852246.8743553446 0, -1408024.111393916 2852209.763787432 0, -1407803.8467946316 2852165.883525409 0, -1407627.1719187878 2852130.313602257 0, -1407230.2294260436 2852050.8889755737 0, -1407230.2294255465 2852050.888975477 0, -1407206.2683501462 2852046.303831964 0, -1406833.2804088348 2851971.486434671 0, -1406833.280408835 2851971.4864346697 0, -1406911.933817793 2851579.414764962 0, -1406921.6758014641 2851530.0046396935 0, -1406934.686355972 2851465.14776617 0, -1406956.335386052 2851357.2290452607 0, -1406990.586042128 2851187.337697579 0, -1406990.5860421804 2851187.3376973188 0, -1406990.5860422545 2851187.3376969495 0, -1407041.0215364834 2850935.08214724 0, -1407069.2414205894 2850795.256210503 0, -1407069.2414206765 2850795.2562100706 0, -1407069.2414206867 2850795.2562100184 0, -1407073.5684860025 2850772.8424741207 0, -1407147.89795659 2850403.1700436547 0, -1407147.8979565974 2850403.170043656 0, -1407147.897956598 2850403.1700436533 0, -1407506.3690000873 2850474.723267223 0, -1407544.9384991385 2850482.421997814 0, -1407941.9745221676 2850561.6962001207 0, -1408339.0062130108 2850640.9927756977 0, -1408736.0331859435 2850720.3115733187 0, -1408657.41158823 2851111.919579926 0, -1408657.2847018465 2851112.5515910415 0, -1408578.5377025602 2851504.7836576267 0, -1408499.7917902402 2851897.0108265877 0)), ((-1402322.4997742055 2855962.8549554977 0, -1401926.2423490663 2855884.0684591965 0, -1401529.9818892553 2855805.3075370626 0, -1401133.7178690603 2855726.5661011315 0, -1401213.211228292 2855335.412905123 0, -1401292.708138397 2854944.2551045995 0, -1401372.2039204885 2854553.0919847465 0, -1401451.7031004892 2854161.9246495627 0, -1401847.939906079 2854240.6579817794 0, -1402244.174336076 2854319.414166907 0, -1402640.4039476456 2854398.195590499 0, -1403036.6295266182 2854476.9962373967 0, -1402957.1582407928 2854868.1687561497 0, -1402877.6877139623 2855259.339419323 0, -1402798.2189316931 2855650.5022341553 0, -1402718.750697533 2856041.6632575803 0, -1402322.4997742055 2855962.8549554977 0)), ((-1411751.5853603992 2856418.185144432 0, -1411754.7571084467 2856429.033555226 0, -1411767.7582414288 2856473.501728358 0, -1411817.3561956498 2856643.1425894992 0, -1411842.2963358818 2856728.4480426703 0, -1411857.2971659566 2856779.7566173365 0, -1411866.2335776836 2856810.323187832 0, -1411899.5147161097 2856924.1581729716 0, -1411899.2923966853 2856930.5015921816 0, -1411897.9417615307 2856969.061157462 0, -1411894.9402896597 2857054.74085981 0, -1411894.5358408932 2857066.285733073 0, -1411894.0926921885 2857078.934847568 0, -1411893.5171049975 2857095.3595575998 0, -1411891.713688685 2857146.8214332475 0, -1411889.994330014 2857195.9125946364 0, -1411889.699684305 2857204.325522127 0, -1411880.874398725 2857470.4536910965 0, -1411878.0360349421 2857552.343632654 0, -1411875.6033314364 2857624.912060565 0, -1411877.2522324275 2857628.9538111114 0, -1411915.182499596 2857721.932867112 0, -1411933.3960081232 2857766.5799572086 0, -1411978.6628281383 2857877.543262183 0, -1411987.1789034253 2857898.418955808 0, -1411967.8125782465 2857894.7388543542 0, -1411940.9460620254 2857889.3657909026 0, -1411827.0057558136 2857866.5978943333 0, -1411816.2609931997 2857864.4504358424 0, -1411785.6653254726 2857858.335715912 0, -1411778.7458917818 2857856.7582134116 0, -1411778.7458915478 2857856.758213361 0, -1411594.861806844 2857819.9848252423 0, -1411383.7384575654 2857777.7640921324 0, -1411367.0593044949 2857774.617511555 0, -1410990.311091655 2857698.9297966924 0, -1410858.0004306268 2857672.622335774 0, -1410596.879148821 2857620.1174235255 0, -1410621.9852533883 2857491.62132465 0, -1410633.7672996472 2857431.7274165326 0, -1410674.0526222952 2857227.8057096056 0, -1410674.0526223222 2857227.805709468 0, -1410751.224144693 2856835.4917604737 0, -1410757.8768594344 2856800.8060144023 0, -1410820.825048066 2856480.8087421665 0, -1410828.3986047867 2856443.173116284 0, -1410828.3986047988 2856443.1731162234 0, -1410828.3986048105 2856443.173116164 0, -1410842.1263099334 2856372.5611441107 0, -1410905.5745906155 2856050.8465852523 0, -1411295.5805096321 2856130.8219032804 0, -1411432.25054098 2856158.360234526 0, -1411432.2505409804 2856158.360234527 0, -1411432.3744690558 2856158.659060573 0, -1411528.0464481325 2856236.440972607 0, -1411560.3916010382 2856262.7377897943 0, -1411667.3655141646 2856349.7080069594 0, -1411702.6279902614 2856378.379090404 0, -1411740.73912433 2856409.366361044 0, -1411751.5853603992 2856418.185144432 0)), ((-1405261.3863524538 2859814.963898068 0, -1405651.2703595373 2859892.5344997076 0, -1406048.3939748404 2859971.7027081377 0, -1406445.5149132037 2860050.8938099025 0, -1406842.6286486182 2860130.1098150183 0, -1406842.628648618 2860130.1098150196 0, -1406764.8265913033 2860522.0183203532 0, -1406688.7504382622 2860905.23269522 0, -1406687.0248609448 2860913.924854412 0, -1406687.0248609437 2860913.924854418 0, -1406415.590490284 2860859.6128464383 0, -1406290.115452382 2860834.5054980735 0, -1405897.4905057237 2860756.1532146623 0, -1405893.2084571854 2860755.084839173 0, -1405815.6258750965 2861146.7138585607 0, -1406212.4251978938 2861226.269456487 0, -1406609.224541734 2861305.8234384237 0, -1406531.4236872834 2861697.717321509 0, -1406531.4236872534 2861697.717321503 0, -1406531.4236872522 2861697.717321509 0, -1406134.7369737187 2861618.013712855 0, -1405738.045266009 2861538.3353076545 0, -1405341.3495085759 2861458.6764138103 0, -1404944.6466850971 2861379.042249062 0, -1405022.0205961196 2860987.6359433997 0, -1405099.3936611253 2860596.2250118344 0, -1405176.7677404573 2860204.8092027605 0, -1404780.8769870354 2860124.730539985 0, -1404858.3628771487 2859733.3601081683 0, -1404935.3719751574 2859342.672009466 0, -1405331.1001697828 2859423.1280607716 0, -1405254.1434443628 2859813.3853914333 0, -1405261.3863524538 2859814.963898068 0)), ((-1402682.2020684432 2864118.7237778557 0, -1402695.4529211784 2864121.2283095215 0, -1402695.4529211782 2864121.228309523 0, -1402616.8936437613 2864513.0297153555 0, -1402538.3358605783 2864904.823133617 0, -1402499.8153482743 2865096.9325434817 0, -1402459.7765047003 2865296.6141715446 0, -1402419.7474271564 2865496.252592065 0, -1402381.2202299368 2865688.4006322375 0, -1402381.2202299358 2865688.4006322417 0, -1401983.5451695155 2865608.8553613233 0, -1401712.7970666003 2865554.720197429 0, -1401585.8632989998 2865529.3320246567 0, -1401188.179284525 2865449.831439479 0, -1401188.1792117932 2865449.831424936 0, -1401097.3997936426 2865431.6841614405 0, -1401084.8622124526 2865429.1840025107 0, -1400799.226584094 2865372.3078978863 0, -1400790.4886198821 2865370.35311039 0, -1400868.6112097064 2864978.9369326024 0, -1400945.8802026587 2864590.1986702695 0, -1400946.7321918367 2864587.5186793273 0, -1401024.8546978398 2864196.092250667 0, -1401100.9681356936 2863813.8579939683 0, -1401102.9804730942 2863804.661391134 0, -1401161.397036985 2863816.255982978 0, -1401501.1095115985 2863883.7670430006 0, -1401558.569074346 2863895.1879364145 0, -1401899.2323785443 2863962.904431385 0, -1401955.7386749384 2863974.1206539576 0, -1402297.3480475233 2864042.044840975 0, -1402352.9085788366 2864053.0954119097 0, -1402682.2020684432 2864118.7237778557 0)), ((-1411465.037336772 2865648.779537992 0, -1411463.8557415532 2865655.0362547883 0, -1411467.7572204815 2865655.390586278 0, -1411528.471929807 2865656.642773342 0, -1411528.4719302277 2865656.6427733493 0, -1411528.471930238 2865656.6427733507 0, -1411528.4719302412 2865656.6427733507 0, -1411569.6250164183 2865661.9779159166 0, -1411578.782938681 2865663.366841497 0, -1411605.6501287578 2865674.490354063 0, -1411625.477942975 2865682.6947615296 0, -1411631.7469223023 2865685.3064114386 0, -1411632.7949084023 2865685.7423111056 0, -1411635.878725861 2865685.393298609 0, -1411647.15672865 2865684.1156663178 0, -1411652.734374543 2865683.483661498 0, -1411663.069627925 2865682.308265712 0, -1411676.9610435506 2865680.725924123 0, -1411731.4632386134 2865723.2860093727 0, -1411740.6671240507 2865730.519389325 0, -1411822.090020838 2865718.2191672903 0, -1411838.3978266304 2865715.9588456973 0, -1411841.073689812 2865717.1605165387 0, -1411983.169821221 2865779.4717531553 0, -1411983.1698278135 2865779.4717560387 0, -1411999.7797165555 2865786.7246760647 0, -1412158.2912243297 2865835.9466782827 0, -1412170.146075653 2865836.9489773572 0, -1412170.146076222 2865836.9489774047 0, -1412229.6105864234 2865841.7906655665 0, -1412229.6105864223 2865841.790665572 0, -1412229.6105864225 2865841.790665572 0, -1412229.6105863927 2865841.7906657173 0, -1412219.1846687484 2865892.884224412 0, -1412162.0192036116 2866176.968186281 0, -1412082.825008011 2866569.0058447286 0, -1412002.6728112134 2866961.1972452626 0, -1411922.5221962316 2867353.380643108 0, -1411922.5221962258 2867353.3806431065 0, -1411922.522196224 2867353.3806431163 0, -1411583.5471875449 2867284.2856640294 0, -1411524.470183467 2867272.0276043857 0, -1411445.3103906135 2867256.03696549 0, -1411360.55465754 2867238.708295354 0, -1411126.4154879246 2867190.697131833 0, -1411025.867544467 2867170.3460400575 0, -1410917.9101386506 2867148.296874894 0, -1410817.3561835214 2867127.759786799 0, -1410728.3555018317 2867109.3920901567 0, -1410728.3549554553 2867109.3919785875 0, -1410610.287801935 2867085.2829328044 0, -1410330.3074244468 2867028.109796696 0, -1410330.291306805 2867028.1065054135 0, -1410361.2985384562 2866873.7711350676 0, -1410409.33354803 2866634.6905706557 0, -1410420.9139694646 2866577.055654584 0, -1410440.2146718572 2866480.997461124 0, -1410440.2146719096 2866480.9974608603 0, -1410456.6149111663 2866398.174093309 0, -1410463.2236422338 2866365.1634405 0, -1410488.222008319 2866241.2386903674 0, -1410504.0888303516 2866161.32310462 0, -1410519.0021884008 2866088.0397656164 0, -1410519.002188406 2866088.0397655913 0, -1410566.296370515 2865852.6473873486 0, -1410597.9484032183 2865695.10541922 0, -1410644.2002541109 2865464.0360314716 0, -1410644.2099788839 2865464.0379698332 0, -1410644.2113585516 2865464.0310786646 0, -1410684.423421186 2865472.053394944 0, -1411044.5673082075 2865544.3390496573 0, -1411064.664278303 2865548.3758619865 0, -1411303.885356992 2865596.5309854182 0, -1411444.901632407 2865624.715773975 0, -1411454.7045603914 2865626.808822695 0, -1411468.8876433342 2865629.512212369 0, -1411468.8876433324 2865629.512212379 0, -1411465.037336772 2865648.779537992 0)), ((-1405352.3578766033 2869543.935077524 0, -1405359.1363504976 2869545.2042935197 0, -1405436.3132154464 2869560.2322490425 0, -1405502.746418892 2869573.2515146 0, -1405502.7464338238 2869573.2515175208 0, -1405720.6097105232 2869615.720096893 0, -1406118.040747909 2869693.2168943826 0, -1406295.4979188778 2869727.8309028526 0, -1406335.326025477 2869735.548965003 0, -1406368.3830205046 2869742.047260953 0, -1406368.3830230972 2869742.047261461 0, -1406515.4696160685 2869770.7362509747 0, -1406515.4696160683 2869770.736250976 0, -1406515.3518045028 2869771.324431194 0, -1406436.8880400027 2870163.058756294 0, -1406358.3075719213 2870555.3763669888 0, -1406349.6235684261 2870598.7326819636 0, -1406349.6235644566 2870598.7327020443 0, -1406348.2495920586 2870605.7389051924 0, -1406343.9503185805 2870627.2036582665 0, -1406334.9120333896 2870672.1828832966 0, -1406279.7301098744 2870947.689329546 0, -1406259.8342604002 2871047.0207821187 0, -1406256.6776818188 2871062.9237264954 0, -1406248.9494264596 2871101.3638142054 0, -1406201.1516861857 2871339.9969154075 0, -1405935.8783990357 2871288.0464658416 0, -1405919.2268095443 2871284.7765399343 0, -1405859.9066085038 2871273.1582050133 0, -1405856.2419319113 2871272.450294864 0, -1405856.241927392 2871272.4502939982 0, -1405803.751681128 2871262.170407299 0, -1405658.300430607 2871233.6943604634 0, -1405644.932170153 2871231.0641286485 0, -1405623.858496985 2871226.937981929 0, -1405605.0992181995 2871223.278679066 0, -1405605.0992040872 2871223.278676319 0, -1405406.3471053601 2871184.366241646 0, -1405435.624495818 2871038.2277601827 0, -1405437.0592010934 2871031.0664098286 0, -1405441.9988417523 2871006.4998400114 0, -1405484.3701475295 2870794.999082076 0, -1405484.9057895474 2870792.2393457848 0, -1405479.7815442246 2870791.226744264 0, -1405424.8324013767 2870780.4771098006 0, -1405420.8968640964 2870779.7077110303 0, -1405370.7645056879 2870769.9052323746 0, -1405367.6517246566 2870769.2986274436 0, -1405283.9653302229 2870752.933274581 0, -1405255.9106829148 2870747.465511902 0, -1405255.9106593088 2870747.46550731 0, -1405205.8767456764 2870737.7331411466 0, -1405087.490981406 2870714.534637766 0, -1405066.3558166963 2870710.5732503003 0, -1404937.6800193107 2870685.241462984 0, -1404912.420841931 2870680.2812086833 0, -1404873.690080004 2870672.728276086 0, -1404690.0778117212 2870636.8252614536 0, -1404690.077166699 2870636.8251353293 0, -1404690.0771666993 2870636.825135328 0, -1404708.0471434693 2870547.146432178 0, -1404710.958022651 2870532.710837276 0, -1404753.5632293806 2870320.0914300634 0, -1404767.9136741732 2870248.445385562 0, -1404768.6279536458 2870244.8196088024 0, -1404768.6279536616 2870244.819608721 0, -1404775.7641339956 2870209.20661129 0, -1404775.7641365211 2870209.206598999 0, -1404776.9359453998 2870203.4499911657 0, -1404809.6746020482 2870040.0693464084 0, -1404828.469240713 2869946.2757398025 0, -1404829.4227403163 2869941.5171959335 0, -1404831.863324543 2869929.2458460294 0, -1404847.1798434148 2869852.8091909704 0, -1404851.4089969185 2869831.7039236957 0, -1404851.4422845743 2869831.5378041933 0, -1404852.1575244702 2869828.0605850974 0, -1404853.231110614 2869822.7023808896 0, -1404856.9175901003 2869804.3054733314 0, -1404883.9239550708 2869669.5310635734 0, -1404889.6944281512 2869640.6415555426 0, -1404889.6944321946 2869640.6415352616 0, -1404925.732661221 2869460.793662609 0, -1405323.1722710785 2869538.245600288 0, -1405352.3578766033 2869543.935077524 0)), ((-1403270.9110435373 2873607.989720598 0, -1403195.57265247 2873987.095011088 0, -1402798.6169425067 2873907.8261163756 0, -1402874.1480264233 2873528.383814522 0, -1402952.0604383987 2873136.965264704 0, -1403348.7412445976 2873216.3452473097 0, -1403270.9110435373 2873607.989720598 0)), ((-1400722.020211627 2873987.416916897 0, -1400659.8349719865 2874300.9579526847 0, -1400582.1008802357 2874692.897713141 0, -1400504.368199048 2875084.8295678613 0, -1400504.3681990472 2875084.8295678655 0, -1400306.06796822 2875046.0779310446 0, -1400108.2805656404 2875006.994913384 0, -1399712.1886875827 2874929.1824742686 0, -1399316.0923516774 2874851.392322538 0, -1398919.9918312414 2874773.6246947986 0, -1398997.4825770769 2874381.3695183387 0, -1399074.9721307347 2873989.109292349 0, -1399152.464837142 2873596.8441945347 0, -1399229.9583728071 2873204.574122286 0, -1399626.3009079173 2873282.6651033484 0, -1400022.6398035127 2873360.7752654627 0, -1400418.9757098868 2873438.911310901 0, -1400341.2951306698 2873830.9661018522 0, -1400408.590619487 2873844.220564607 0, -1400737.569628418 2873909.015992905 0, -1400737.5696284168 2873909.0159929106 0, -1400737.5696284187 2873909.015992911 0, -1400722.020211627 2873987.416916897 0)), ((-1409103.6964492481 2875025.2421185113 0, -1409141.8900567754 2875032.891256656 0, -1409213.6801065572 2875047.2731291484 0, -1409213.6801090706 2875047.273129647 0, -1409229.77988655 2875050.449152512 0, -1409285.8021089113 2875061.721309533 0, -1409285.8021396676 2875061.7213157113 0, -1409535.654514666 2875111.773087116 0, -1409929.4117891053 2875190.679700427 0, -1409971.24784557 2875199.065926775 0, -1409971.2478463105 2875199.065926921 0, -1409978.7519803427 2875200.531137577 0, -1410108.979261336 2875226.637376353 0, -1410140.157719893 2875232.924347864 0, -1410323.172103583 2875269.6090371227 0, -1410323.1721035815 2875269.609037131 0, -1410323.1721035817 2875269.609037131 0, -1410280.0390395173 2875485.7118710545 0, -1410275.657886319 2875507.7470515314 0, -1410272.7716184133 2875522.122472482 0, -1410244.8465344294 2875662.031449576 0, -1410244.846486525 2875662.031689817 0, -1410238.80266182 2875692.360027673 0, -1410188.7019879804 2875943.3155002077 0, -1410185.8364133637 2875957.6702931076 0, -1410166.5198291473 2876054.448420859 0, -1410154.9493124203 2876112.3908099523 0, -1410129.6492050847 2876239.1153764776 0, -1410097.0531707695 2876404.0092286854 0, -1410096.267817752 2876406.490527884 0, -1410095.9545911942 2876406.9131187014 0, -1410092.6124654415 2876411.4155137967 0, -1410071.9405331241 2876439.594348282 0, -1410067.334844834 2876445.872557595 0, -1410044.8896179674 2876476.467052874 0, -1410017.2528691767 2876514.1379344515 0, -1410017.2528691764 2876514.1379344515 0, -1410017.2513635792 2876514.139986689 0, -1409975.5495828802 2876541.3013308863 0, -1409950.1803787204 2876557.8212493835 0, -1409908.6595203627 2876584.8949637697 0, -1409866.487935356 2876612.392758426 0, -1409766.4990217146 2876677.5969618005 0, -1409766.4997185215 2876677.6499651307 0, -1409766.2500051307 2876677.812799691 0, -1409766.6451122717 2876704.2036529 0, -1409767.1408562034 2876737.3104113834 0, -1409767.507660834 2876761.8052125834 0, -1409769.9336998635 2876795.1547505893 0, -1409764.5592822868 2876794.095048755 0, -1409627.5944055112 2876766.6532114935 0, -1409510.6739233304 2876743.2241767757 0, -1409446.8540509548 2876730.4106893907 0, -1409310.6548475022 2876703.0646280306 0, -1409263.1621494931 2876693.52887364 0, -1409260.287299188 2876692.9515570784 0, -1409230.218035185 2876686.8663708684 0, -1408832.1384908531 2876608.0227922006 0, -1408774.6639410295 2876596.8008374856 0, -1408728.6500602255 2876587.657983948 0, -1408514.9915482828 2876545.2276930353 0, -1408514.9915142735 2876545.2276862813 0, -1408455.7443594562 2876533.474764181 0, -1408452.775912659 2876532.908685063 0, -1408434.0567597842 2876529.2021547086 0, -1408446.2223965924 2876468.189760085 0, -1408486.3784147138 2876266.7236018917 0, -1408489.3887333323 2876251.6218461953 0, -1408512.5581591323 2876135.3886321625 0, -1408529.94382</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>BANK OFÔøΩNORTHÔøΩDAKOTA, SOVEREIGNÔøΩLANDS, COMMON SCHOOLS, NDÔøΩSTATEÔøΩUNIVERSITY, ND INDUSTRIAL SCHOOL, SCHOOL OF MINES, ELLENDALE, SCHOOL FOR THE BLIND, ND SCHOOL OF SCIENCE, UNIVERSITY OF ND, NDÔøΩSTATEÔøΩTREASURER, MAYVILLE, VALLEY CITY</t>
+          <t>SOVEREIGNÔøΩLANDS, COMMON SCHOOLS, BANK OFÔøΩNORTHÔøΩDAKOTA, NDÔøΩSTATEÔøΩUNIVERSITY, ND INDUSTRIAL SCHOOL, SCHOOL OF MINES, ELLENDALE, SCHOOL FOR THE BLIND, ND SCHOOL OF SCIENCE, UNIVERSITY OF ND, NDÔøΩSTATEÔøΩTREASURER, MAYVILLE, VALLEY CITY</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Dept. of Transportation, 100.00% State Hospital South (Insane Asylum), Public School (Indemnity, Schools, Common Schools)</t>
+          <t>Public School (Indemnity, Schools, Common Schools), Dept. of Transportation, 100.00% State Hospital South (Insane Asylum)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1650,7 +1650,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-778111.123129531 2849966.4205661775 0, -778152.0380063502 2849995.857612358 0, -778232.4635076745 2850022.7648026235 0, -778232.4635694196 2850022.7648232784 0, -778272.3694730203 2850005.137503722 0, -778286.1607537577 2849979.6017443314 0, -778296.920254595 2849936.9769389974 0, -778336.2231786009 2849907.0715158912 0, -778393.8367818684 2849849.3580969116 0, -778393.8430354721 2849849.360552195 0, -778393.8430511502 2849849.360536491 0, -778403.6653998105 2849853.216998893 0, -778428.6853912089 2849863.0403224714 0, -778428.6854091042 2849863.040385179 0, -778428.6991688223 2849863.0457875365 0, -778443.4649263347 2849914.8092266163 0, -778414.1937640968 2849949.001410578 0, -778371.7344926831 2850017.615826767 0, -778382.3051193785 2850074.338933517 0, -778398.5470595541 2850082.064149347 0, -778403.3046900313 2850084.3265774795 0, -778446.810059922 2850176.3057739446 0, -778447.2446485488 2850181.0248513315 0, -778455.2041889131 2850268.246773478 0, -778429.6688173915 2850307.581051144 0, -778392.1623876267 2850337.822753677 0, -778391.2678431092 2850381.5535695823 0, -778409.1754104488 2850423.8003512262 0, -778443.3267647222 2850418.882471604 0, -778472.0479189741 2850425.3049393725 0, -778472.0487260116 2850425.3051198344 0, -778472.1538681126 2850425.351573998 0, -778539.5934494556 2850455.1479067337 0, -778539.5934506133 2850455.1479104175 0, -778539.6047455587 2850455.1529007806 0, -778556.6351373835 2850509.3733091513 0, -778560.1761920195 2850560.9527782807 0, -778547.8672037215 2850595.660859155 0, -778537.9140969089 2850606.129185271 0, -778520.642783997 2850623.4954078286 0, -778493.3349725715 2850650.953595447 0, -778451.0096472857 2850697.8333630995 0, -778412.2927054393 2850735.7666474488 0, -778332.2267194751 2850801.4565049415 0, -778302.6506236638 2850831.477270452 0, -778261.3214377748 2850858.485909124 0, -778219.6404445403 2850879.0038987314 0, -778186.4701389986 2850893.9341213712 0, -778155.5423610273 2850942.964488242 0, -778155.3875860953 2850943.902271544 0, -778153.8866063681 2850952.996727043 0, -778144.8386589016 2851007.818732372 0, -778144.838656444 2851007.8187473714 0, -778143.8777997025 2851013.701355991 0, -778149.8737242838 2851080.1654093326 0, -778164.1845627591 2851163.640269842 0, -778188.4564350559 2851188.1242920617 0, -778205.9905316551 2851205.810038239 0, -778226.8356577648 2851241.215181279 0, -778255.9156079143 2851286.877953428 0, -778270.0726153597 2851365.3265308696 0, -778270.072638942 2851365.326661501 0, -778270.0726389335 2851365.3266615 0, -778270.0726389342 2851365.326661504 0, -778094.4605108831 2851346.208892302 0, -777690.6850503956 2851302.830592308 0, -777690.6850503958 2851302.8305923063 0, -777690.6850503882 2851302.8305923054 0, -777733.9628193304 2850906.4917634716 0, -777777.2388194209 2850510.150120197 0, -777820.9831457793 2850114.3101011575 0, -777864.7277990956 2849718.467504392 0, -777460.6128714907 2849673.6653484977 0, -777056.4934434132 2849628.885801183 0, -777056.4934434134 2849628.885801181 0, -777056.4934434058 2849628.8858011803 0, -777099.6764418286 2849232.3232875033 0, -777503.5643492694 2849277.22811051 0, -777690.8115454458 2849298.045287109 0, -777908.4311447623 2849322.23911069 0, -777951.249948151 2848933.928056874 0, -777951.249948158 2848933.92805688 0, -777951.2499481585 2848933.9280568752 0, -777951.4898512964 2848934.1258694273 0, -778018.9447448857 2848989.745918616 0, -778066.8683336076 2849016.709277986 0, -778107.8935463295 2849031.885046103 0, -778107.8935678903 2849031.885071271 0, -778107.8998301893 2849031.887387773 0, -778165.2545033393 2849098.842157993 0, -778111.3076032304 2849130.168651748 0, -778087.6126041275 2849186.3163977806 0, -778126.6375942499 2849232.727695082 0, -778223.3552550377 2849265.8186636334 0, -778254.8962661957 2849265.7881828006 0, -778317.3286196977 2849256.3805453232 0, -778320.3206548779 2849255.9305497576 0, -778382.8332636404 2849238.0703015476 0, -778423.6735988836 2849259.0496166716 0, -778428.9827689723 2849261.776760421 0, -778454.2196999231 2849278.691583925 0, -778488.0754617819 2849356.2284987266 0, -778488.6501968709 2849382.5362317674 0, -778489.152936014 2849406.1901539196 0, -778450.2355246089 2849445.274848413 0, -778352.5313618146 2849449.953824687 0, -778312.1611298464 2849447.1315117213 0, -778292.6974834282 2849465.247074199 0, -778251.9586401515 2849503.1628931905 0, -778240.67791667 2849566.0853533074 0, -778195.7662688775 2849622.488102977 0, -778177.5478470904 2849623.076913356 0, -778120.4627838772 2849639.9752028664 0, -778096.8846394607 2849645.720705325 0, -778000.5748267936 2849733.491153451 0, -778000.5748146558 2849733.491172231 0, -777995.0456996908 2849742.0505981613 0, -778024.6618800078 2849822.4492694708 0, -778065.4236408372 2849893.553183616 0, -778095.0547552725 2849940.7998997993 0, -778111.123129531 2849966.4205661775 0)), ((-779039.152479286 2865439.924130304 0, -779023.0279794952 2865448.293106738 0, -778993.7520421153 2865463.826756115 0, -778970.6611095731 2865476.0778305396 0, -778968.6561214548 2865477.1415926316 0, -778956.4113200627 2865482.241545986 0, -778946.6793083777 2865486.32109739 0, -778934.1801994797 2865491.5606448776 0, -778917.3725716695 2865498.641953889 0, -778939.3769872008 2865584.7747839727 0, -778976.8123785012 2865626.5557441814 0, -779070.4881821149 2865731.398700857 0, -779138.7121427488 2865757.6186342165 0, -779193.8966056061 2865744.298193133 0, -779227.2728923232 2865741.3936695904 0, -779262.9244508899 2865760.6726428876 0, -779323.3717550738 2865789.4067152063 0, -779310.5830200284 2865837.322463818 0, -779310.5830133609 2865837.322488929 0, -779309.2371529589 2865842.397671633 0, -779304.6237460255 2865848.684998582 0, -779292.6560994192 2865864.9949638876 0, -779287.2914060361 2865886.224715173 0, -779291.490815091 2865924.855617001 0, -779300.0528537801 2865939.7354915333 0, -779325.8083980508 2865984.182716592 0, -779329.5936830095 2865990.877125187 0, -779335.7647028733 2866001.3645638414 0, -779340.7360346571 2866009.9421461234 0, -779342.2131859002 2866012.3954330594 0, -779342.2131859086 2866012.3954330618 0, -779342.2131859087 2866012.395433061 0, -779342.2131880341 2866012.395433664 0, -779372.151402374 2866020.876621468 0, -779379.3495333014 2866022.90937798 0, -779387.2382461597 2866026.0080900206 0, -779414.3932899326 2866036.6744328826 0, -779419.9555692682 2866038.8594160196 0, -779469.6521037758 2866035.7577639148 0, -779505.5638708652 2866029.304145113 0, -779509.6160760403 2866028.57596547 0, -779586.2511909457 2866048.736966126 0, -779617.6114337902 2866070.9433910954 0, -779668.0572842329 2866133.4988183226 0, -779713.5557304206 2866181.3759299745 0, -779699.7635778274 2866250.2194864987 0, -779699.6693577461 2866250.696038443 0, -779673.6980300663 2866306.686730672 0, -779666.9540606847 2866309.5274188924 0, -779658.3149942142 2866313.166358084 0, -779631.6438362749 2866328.9537691833 0, -779599.8944918101 2866347.747102227 0, -779591.8881338246 2866352.7793916864 0, -779591.8881273797 2866352.7793957484 0, -779583.9506848671 2866357.808552827 0, -779568.3500247455 2866367.6919736937 0, -779554.0057215543 2866376.817223519 0, -779553.0384076122 2866378.842453414 0, -779551.4617086295 2866382.143530564 0, -779551.4617066641 2866382.1435346873 0, -779528.7638745711 2866429.7637730306 0, -779525.9447666332 2866449.6653061714 0, -779525.1477111776 2866455.5680601005 0, -779509.1860784377 2866573.1947606048 0, -779549.4492355619 2866622.156958724 0, -779585.8910487035 2866644.055816147 0, -779617.0343096714 2866656.3589980225 0, -779657.055098304 2866678.170773459 0, -779675.9214310695 2866702.196313196 0, -779686.9074296867 2866716.193585674 0, -779688.6923568146 2866718.467497366 0, -779731.2478500814 2866748.2971152854 0, -779735.0626553502 2866750.8928653626 0, -779745.1792336187 2866773.911404346 0, -779746.3262182855 2866776.5126066078 0, -779756.6804523873 2866780.2930155494 0, -779760.5911791024 2866781.6816453673 0, -779765.1353403393 2866783.4185599373 0, -779780.7410285155 2866801.9090242246 0, -779782.5802469932 2866804.0885802833 0, -779783.9213599105 2866811.0940339374 0, -779783.9907325234 2866811.4505314506 0, -779788.6696253056 2866835.16151928 0, -779793.970550902 2866838.8543598186 0, -779793.9705511765 2866838.8543600063 0, -779796.9830574616 2866840.9154834338 0, -779799.3910429042 2866842.5239838576 0, -779809.7036107051 2866849.3774993685 0, -779814.9315585205 2866854.655198107 0, -779817.2558039882 2866857.0005583656 0, -779849.9090321712 2866890.2079449045 0, -779851.6497902453 2866891.9764218726 0, -779851.9474376016 2866892.2784973974 0, -779851.948620692 2866892.2796980888 0, -779855.1715612088 2866893.450912427 0, -779855.1715615301 2866893.450912543 0, -779883.5784008092 2866903.5945362016 0, -779889.4830955303 2866906.0520811765 0, -779889.4830956871 2866906.052081239 0, -779899.4872820814 2866910.0145255593 0, -779902.7661595201 2866909.1573240245 0, -779903.06432163 2866909.0727239456 0, -779941.7597677703 2866901.0007285383 0, -779945.6779448233 2866900.181854022 0, -779990.7910749582 2866884.045822849 0, -780030.6135322689 2866836.682446488 0, -780033.2684257341 2866833.597392254 0, -780033.2684354124 2866833.59738504 0, -780035.5375477438 2866831.904521111 0, -780057.7257643872 2866815.6568061677 0, -780064.1461269036 2866818.502320128 0, -780090.9366377833 2866830.3917377423 0, -780133.89057774 2866842.597644402 0, -780150.4058261721 2866852.3191592274 0, -780150.411989451 2866852.3350040643 0, -780150.4600618072 2866852.3633030327 0, -780175.428586096 2866916.474325607 0, -780189.5268056914 2866982.7689993717 0, -780182.4600024628 2867001.0239812057 0, -780182.3555241922 2867001.0592753175 0, -780182.3460716568 2867001.083688821 0, -780171.1883500539 2867004.8316912395 0, -780171.188347239 2867004.8316921904 0, -780149.7691617253 2867012.024510049 0, -780113.6291492814 2867097.1966597107 0, -780112.5635850911 2867179.7537893984 0, -780119.5752173394 2867199.9731411543 0, -780119.5752190775 2867199.973146141 0, -780124.6908509599 2867214.502216883 0, -780127.9139902004 2867223.6557753137 0, -780127.913991517 2867223.6557789934 0, -780137.4979773352 2867250.2324645696 0, -780178.9906645096 2867279.6379998005 0, -780179.1848188583 2867279.775487024 0, -780196.6391077609 2867292.1453208667 0, -780196.6444624714 2867292.154038222 0, -780196.7084945008 2867292.1994353007 0, -780219.2578227344 2867328.912949185 0, -780235.8500057842 2867380.125415139 0, -780235.0224535076 2867424.9112286805 0, -780223.0311947786 2867462.8745537414 0, -780214.7739112539 2867483.972928059 0, -780212.2158848194 2867490.689476867 0, -780211.8137265675 2867491.3326835395 0, -780210.2229013377 2867493.8770287107 0, -780210.222900861 2867493.877029491 0, -780203.9572028025 2867504.257186381 0, -780187.6526605099 2867515.9848600714 0, -780172.9110753008 2867540.9148804476 0, -780108.4302354697 2867585.6731637605 0, -780108.3680211534 2867585.63938935 0, -780108.3545303716 2867585.648749364 0, -780086.1618562269 2867573.594301091 0, -780064.7922477692 2867543.212531911 0, -780015.172118825 2867545.1532341493 0, -779981.4447819251 2867558.5686488766 0, -779960.3008234018 2867566.992400341 0, -779954.7320235713 2867569.1731972136 0, -779952.0898931359 2867570.228046003 0, -779952.0898924158 2867570.228046878 0, -779933.4884271858 2867592.9712232375 0, -779931.8133636253 2867595.2339429366 0, -779920.4619358924 2867613.6809061766 0, -779914.5769850386 2867623.4378382144 0, -779906.2403500113 2867637.2861757823 0, -779909.7839589368 2867660.69840403 0, -779910.8196514907 2867667.540766627 0, -779910.819651789 2867667.540768598 0, -779913.2101330699 2867683.2267922917 0, -779921.0107550346 2867694.4813809455 0, -779921.0107599307 2867694.481387992 0, -779935.6925738538 2867715.5333454106 0, -779941.7260559902 2867722.2085948098 0, -779938.8574386678 2867732.09062936 0, -779942.7537764932 2867738.28435054 0, -779953.4220376707 2867755.2412652266 0, -779958.6876414513 2867760.5741329957 0, -779986.6780746016 2867788.9244766654 0, -779994.4211631832 2867833.4695059485 0, -779996.0619575984 2867843.330221665 0, -780011.4805325873 2867878.64794406 0, -780016.4294372235 2867889.9838030394 0, -780021.2511991784 2867901.2779533747 0, -780035.1559595682 2867933.8245187956 0, -780067.3044794233 2867958.099728915 0, -780092.3876133718 2867976.934358336 0, -780129.5150795655 2867976.8573418804 0, -780143.2501499564 2867976.7104670755 0, -780154.1347760144 2867970.2724514757 0, -780162.0250643261 2867966.2409890736 0, -780175.9838638561 2867959.2371197087 0, -780208.9271376494 2867942.498026442 0, -780211.8219856764 2867941.0769677185 0, -780230.718415916 2867961.4392033685 0, -780257.9387566276 2867990.4320396497 0, -780270.7877296533 2868008.664862903 0, -780271.4156469837 2868030.8659969084 0, -780271.5125259771 2868035.891481801 0, -780271.6917727466 2868042.667724333 0, -780271.1457061982 2868045.415702571 0, -780267.2596377166 2868048.030826591 0, -780253.6413667245 2868058.8683116804 0, -780257.2126298236 2868082.1137912082 0, -780258.9307758686 2868093.286304257 0, -780258.1532994827 2868103.3527499135 0, -780256.0195743253 2868131.016723943 0, -780267.8618371518 2868157.734759952 0, -780275.7022799109 2868175.388378105 0, -780283.7983055882 2868179.5489601586 0, -780292.6615983079 2868183.7742528054 0, -780354.078242831 2868213.054084066 0, -780369.8741598591 2868209.5798874223 0, -780390.6740443747 2868205.0054862285 0, -780430.7194506521 2868157.6157531324 0, -780465.6122176911 2868123.0502816536 0, -780499.7822652165 2868108.0142097017 0, -780530.2662878109 2868100.6320033004 0, -780561.2797663695 2868096.1173576936 0, -780585.229592231 2868116.792696185 0, -780591.0638451594 2868121.8172028866 0, -780624.0195790911 2868153.9296654146 0, -780643.824291495 2868181.95309038 0, -780674.2701028391 2868231.3114375924 0, -780667.647170231 2868287.642819418 0, -780616.1934146394 2868341.3145533646 0, -780507.0768621111 2868362.4499460557 0, -780457.2872171006 2868398.598726522 0, -780449.404758897 2868423.2172151553 0, -780437.8880136701 2868459.33193768 0, -780438.5095848306 2868483.186428469 0, -780439.0009394187 2868500.6547144447 0, -780439.8144682248 2868530.312555635 0, -780468.3067455092 2868558.260272274 0, -780500.407432749 2868589.6802325044 0, -780508.0750506903 2868590.5639736885 0, -780529.5642923648 2868593.031618096 0, -780607.6072858134 2868608.3802648797 0, -780638.321222069 2868629.9391305605 0, -780647.700380725 2868636.5278843227 0, -780651.56526434 2868643.8651430532 0, -780652.9061471489 2868646.433761697 0, -780655.1950769854 2868650.9467331795 0, -780660.1665794743 2868660.6458233334 0, -780679.864017195 2868676.355004451 0, -780714.946225137 2868699.9128579376 0, -780743.0561164145 2868725.705022825 0, -780758.935581237 2868737.913406749 0, -780771.7703215113 2868755.5970413806 0, -780782.0069733132 2868771.081739324 0, -780758.0237120664 2868806.7965130196 0, -780741.8468468265 2868788.8999802982 0, -780733.2992106574 2868779.4440627513 0, -780678.7923149357 2868764.3483426278 0, -780660.1429525369 2868758.9684430636 0, -780658.5017949716 2868756.0317070684 0, -780656.7962791208 2868752.9729189766 0, -780649.5004004847 2868739.8882335406 0, -780642.4107917225 2868741.3814160144 0, -780614.7483967241 2868747.16278265 0, -780620.0283193644 2868770.6165203536 0, -780621.9438328906 2868779.125455868 0, -780617.1331207319 2868794.1621076036 0, -780608.5842629903 2868820.8827284453 0, -780610.4017453694 2868829.684730192 0, -780620.786809104 2868879.735953714 0, -780623.0206860149 2868890.5036827917 0, -780623.7801947279 2868894.1227484457 0, -780624.8843686173 2868899.486581847 0, -780629.1621139545 2868906.5911678923 0, -780645.4627844561 2868933.6927095293 0, -780665.7848580597 2868946.047142861 0, -780673.2674873873 2868950.5959313135 0, -780711.3980113654 2868978.7783207335 0, -780729.7938893085 2868998.102228022 0, -780806.5890987276 2869042.5713849533 0, -780829.2104213691 2869055.652398372 0, -780846.7317857399 2869077.7908078814 0, -780849.6888465665 2869093.1635548575 0, -780851.2444533325 2869101.205827288 0, -780859.1080571082 2869106.840241632 0, -780880.0671380667 2869121.6901659234 0, -780904.5848287079 2869147.0680197002 0, -780921.8018630006 2869228.848461901 0, -780933.9451154479 2869278.0984647786 0, -780937.0773687472 2869290.7618271643 0, -780932.6817647588 2869314.222176287 0, -780592.4494464375 2869276.510103586 0, -780581.8633916792 2869275.322169444 0, -780567.0906029015 2869273.687439044 0, -780379.9151030026 2869252.798227524 0, -780381.1025343707 2869240.0205894937 0, -780383.0646016569 2869217.729473123 0, -780399.8209768042 2869054.593767323 0, -780199.4815631429 2869031.6136801844 0, -780203.080664142 2868998.261281361 0, -780204.655392828 2868983.713981458 0, -780220.9781707377 2868835.5410523666 0, -780218.0416167416 2868835.220864358 0, -780018.8788017232 2868813.224142559 0, -780040.9544328884 2868615.3333827914 0, -779839.1214824963 2868592.593344387 0, -779860.9283054336 2868395.968623219 0, -779860.828353818 2868395.9572289027 0, -779860.8258508032 2868395.9799712407 0, -779796.6513697552 2868388.657097032 0, -779840.3492388529 2867994.546192049 0, -779830.6159661649 2867993.376086266 0, -779721.0984120859 2867980.393429644 0, -779721.0738629557 2867980.3909338894 0, -779721.0739095071 2867980.3905237895 0, -779538.1912544267 2867958.699190479 0, -779567.3780728334 2867697.7170125665 0, -779583.1859263789 2867557.450209374 0, -779583.1859263411 2867557.45020937 0, -779583.3632852 2867554.6543739727 0, -779621.887920612 2867195.499852003 0, -779626.0347395401 2867161.275451751 0, -779423.8093009266 2867139.980027611 0, -779423.8585457572 2867139.514386206 0, -779423.78805035 2867139.5064977612 0, -779443.4744816157 2866953.0341884177 0, -779446.6159386438 2866923.454483797 0, -779465.5197998745 2866745.580134709 0, -779302.7630156983 2866727.718068347 0, -779302.7629729796 2866727.7180636683 0, -779264.7313398954 2866723.53681002 0, -779264.5992211195 2866723.5222846875 0, -779264.7791592191 2866720.7265381604 0, -779307.7513682813 2866327.328534183 0, -779304.9079350996 2866327.0745835477 0, -779300.9590657263 2866326.6702074828 0, -779153.7570984508 2866310.424541069 0, -779126.2156186483 2866307.361045627 0, -779125.8700102569 2866307.315473458 0, -779106.148184011 2866305.145636247 0, -779106.194800808 2866304.721086294 0, -779105.9362982546 2866304.6869999627 0, -779107.8416011414 2866287.525426021 0, -779118.403661055 2866192.183078766 0, -779121.943787134 2866160.692226106 0, -779122.7684254933 2866153.3506462113 0, -779125.2419485286 2866131.254306182 0, -779149.6119593101 2865909.3109809356 0, -779145.2762115606 2865908.8863971997 0, -779144.4407769815 2865908.8045861954 0, -779140.3282349799 2865908.3484188453 0, -779130.3583803957 2865907.2381662573 0, -779051.6946062817 2865898.477727759 0, -778947.9796811765 2865887.046657124 0, -778925.8803831866 2865884.459117109 0, -778745.9815095876 2865864.2462161575 0, -778748.0973385327 2865839.5907291775 0, -778788.7313347592 2865472.488801352 0, -778789.1232820231 2865468.892843553 0, -778782.8493347741 2865468.133675343 0, -778770.8662202087 2865466.777084145 0, -778587.2785353988 2865446.6961526177 0, -778630.5060057266 2865050.817523389 0, -778795.9364610518 2865069.071144758 0, -778829.1488904493 2865072.7371318964 0, -778832.1191208631 2865073.0992569556 0, -778875.3544676013 2864677.2069002697 0, -778821.0044294996 2864671.1840836187 0, -778673.6318773903 2864654.931451717 0, -778716.7582594071 2864259.0396635346 0, -778846.0666581673 2864273.1639524833 0, -778919.5771365796 2864281.3721959386 0, -778923.4298074759 2864281.7881243434 0, -779011.2024317926 2864291.481546741 0, -779021.4239533767 2864292.7003727993 0, -779040.0241077212 2864294.802851747 0, -779048.0950406332 2864304.9275779794 0, -779081.51011605 2864346.6919513326 0, -779103.2222831812 2864379.2385333944 0, -779110.4115474825 2864400.7378377835 0, -779145.2388073046 2864504.909856213 0, -779145.2373684415 2864504.9142325423 0, -779145.2398763419 2864504.9217334674 0, -779105.4091129539 2864626.054522275 0, -779107.6021636605 2864666.8165470483 0, -779114.191915418 2864703.5070613227 0, -779120.2681808715 2864737.406605333 0, -779152.3886458386 2864800.707789942 0, -779192.2797327498 2864828.211610813 0, -779215.7149021933 2864853.127852828 0, -779262.4077841557 2864910.8684776765 0, -779262.4055274363 2864910.876613737 0, -779262.4090644304 2864910.8809871553 0, -779254.9582020501 2864937.7329249955 0, -779267.8374664417 2864984.89326154 0, -779271.255752108 2865019.5770358304 0, -779271.2549658094 2865019.584497317 0, -779271.2558011949 2865019.592966862 0, -779268.6462162543 2865044.3403834435 0, -779243.0937434582 2865062.3057162617 0, -779231.5169619516 2865081.0065179598 0, -779228.8898344346 2865104.702292179 0, -779214.1056601275 2865115.198077089 0, -779205.6575091856 2865125.4143026145 0, -779202.9635111759 2865130.8248968916 0, -779202.909264674 2865130.8649468077 0, -779202.1647279778 2865131.4146344624 0, -779201.4792949216 2865131.9206862 0, -779201.3140513613 2865132.04268468 0, -779196.9972393411 2865134.977016463 0, -779181.7520377578 2865145.3398674186 0, -779181.7306119628 2865145.3444808493 0, -779176.4806674288 2865146.474905855 0, -779168.5528792638 2865148.175910826 0, -779157.1356959858 2865152.3430054043 0, -779146.6797055126 2865156.1514428747 0, -779139.7253875722 2865157.584441535 0, -779134.2441885404 2865158.71260292 0, -779134.0559668748 2865158.7513434244 0, -779125.9651313591 2865159.8935043905 0, -779079.2908318003 2865206.865736912 0, -779053.740847804 2865248.6332662883 0, -779060.3669293413 2865293.016810817 0, -779072.521815128 2865371.894083655 0, -779072.5202583339 2865371.897731961 0, -779072.5223159426 2865371.911083353 0, -779070.2483823916 2865377.2218135255 0, -779057.6609545639 2865406.748632715 0, -779042.7205976748 2865433.5028620926 0, -779039.152479286 2865439.924130304 0), (-779150.1806210199 2865909.373383448 0, -779150.1813775826 2865909.366741886 0, -779149.6119593101 2865909.3109809356 0, -779150.1806210199 2865909.373383448 0), (-779861.8286988554 2868386.8681159625 0, -779862.8004075689 2868378.804957592 0, -779861.8286988555 2868386.868115961 0, -779861.8286988554 2868386.8681159625 0), (-779174.191770332 2865911.9384812503 0, -779174.1917702062 2865911.9384812354 0, -779172.9852149499 2865911.798587795 0, -779174.191770332 2865911.9384812503 0)), ((-785071.1520494085 2884237.5328455777 0, -785074.0743182834 2884251.245471162 0, -785074.0743187336 2884251.245473275 0, -785072.8350446203 2884251.8137203488 0, -785059.5933640503 2884257.886078278 0, -785058.4655225205 2884258.4033064526 0, -785029.9331651429 2884271.4876718954 0, -784982.5444845094 2884293.218891352 0, -784982.5329867667 2884293.224081307 0, -784981.2149508686 2884293.828500253 0, -784981.2147696365 2884293.8286640937 0, -784981.1467549306 2884293.859853873 0, -784981.1130963754 2884293.9201835813 0, -784981.1126494949 2884293.9209845713 0, -784942.4933314892 2884328.8343114667 0, -784938.2966815983 2884346.38967372 0, -784936.6179760093 2884353.4133089255 0, -784936.4155603364 2884354.2629710403 0, -784935.9100860038 2884356.388015854 0, -784928.5993805551 2884386.991325736 0, -784993.285410236 2884560.2029558844 0, -785012.5606098194 2884631.6563191717 0, -785012.5606306553 2884631.6563964025 0, -785012.56075832 2884631.6565387323 0, -785100.1409543537 2884729.2930047493 0, -785100.1382688797 2884729.2942893715 0, -785100.1383894685 2884729.2944238125 0, -785100.0426378414 2884729.3402275466 0, -785100.0479940528 2884729.3461995577 0, -784865.9550747823 2884841.3273328207 0, -784870.340734311 2884898.9978950107 0, -785089.1225307342 2885040.6966766133 0, -785137.4241029804 2885071.9800291564 0, -785137.4241168518 2885071.9800381204 0, -785144.7563596909 2885076.7156066117 0, -785149.5507473459 2885089.185002046 0, -785149.5507482933 2885089.1850045086 0, -785181.1397999076 2885171.1300373194 0, -785181.053034548 2885171.1755495123 0, -785181.0546302543 2885171.1796889217 0, -785068.2787474302 2885230.336112334 0, -785090.9109817881 2885300.809213529 0, -785167.8188858558 2885335.1925203144 0, -785137.469540249 2885398.2045503845 0, -785134.704310118 2885449.9587178538 0, -785134.6223183037 2885449.9492915287 0, -785134.6191365693 2885450.009068597 0, -784753.0042645405 2885403.7581594787 0, -784796.9568533582 2885008.159964477 0, -784840.9078724972 2884612.558932737 0, -784887.075394753 2884217.026761061 0, -784911.6030819823 2884002.4308323604 0, -784911.6851222854 2884002.415955814 0, -784911.6851257501 2884002.415925501 0, -784944.0389234985 2883996.549170707 0, -784952.7095800161 2883994.9769096673 0, -784952.8177494847 2883994.957295599 0, -784952.8177494848 2883994.957295599 0, -784967.5701537884 2883992.282283246 0, -785000.7248227113 2884032.8557939967 0, -784985.4464197728 2884082.796609726 0, -784985.4170368295 2884082.8926543295 0, -784985.4169973311 2884082.892783439 0, -784985.4749725992 2884082.943058755 0, -784986.1639220841 2884083.540505809 0, -784987.2354451539 2884084.469715156 0, -784987.2354451566 2884084.4697151585 0, -785018.3869469 2884111.4838480535 0, -785018.3869469035 2884111.4838480563 0, -785020.9831284193 2884113.7352192122 0, -785050.1615275689 2884139.0394245973 0, -785065.6032716993 2884211.4965632465 0, -785071.1520494085 2884237.5328455777 0)), ((-677953.8032069259 2817491.995393068 0, -678069.7167141542 2817509.6469280994 0, -678217.8576353688 2817488.848912527 0, -678360.5968406689 2817380.5145609425 0, -678422.363924916 2817266.043436793 0, -678472.6245951293 2817096.2507114923 0, -678561.0224409284 2817067.0342389997 0, -678545.320390724 2817204.245976727 0, -678491.7559608689 2817388.0985640883 0, -678341.5493091701 2817544.846515532 0, -678153.6668712639 2817578.174609607 0, -677972.3188691082 2817569.1404563193 0, -677884.9331917596 2817555.833059413 0, -677953.8032069259 2817491.995393068 0)), ((-677231.108041418 2817868.8189695026 0, -677243.7302638481 2817848.087077101 0, -677302.6825308974 2817777.5864733313 0, -677371.2711007164 2817664.9247852275 0, -677400.605370943 2817672.2437291546 0, -677343.919459624 2817721.1919580186 0, -677257.1413748725 2817875.2061114036 0, -677199.6587318564 2818002.712525519 0, -677137.3316518572 2818079.93129337 0, -677140.9925296828 2817942.3201913605 0, -677201.7502498041 2817918.0844985824 0, -677231.108041418 2817868.8189695026 0)), ((-684318.6846920928 2819500.932570692 0, -684372.1220427881 2819423.543772798 0, -684378.6398463694 2819238.7881175373 0, -684378.9312386372 2819230.7932612128 0, -684379.3043926465 2819228.0124945026 0, -684392.8650749848 2818848.5049169254 0, -684393.3477382112 2818835.2632447104 0, -684633.7653833054 2818860.799628752 0, -684627.3292304148 2818944.117061264 0, -684620.1144404393 2819141.882059492 0, -684519.2542157422 2819443.795445804 0, -684466.7083714664 2819447.0300505226 0, -684318.6846920928 2819500.932570692 0)), ((-758564.3085984066 2818681.459485316 0, -758612.9349165041 2818669.7694761525 0, -758683.0315532052 2818659.023409713 0, -758684.2664664839 2818658.954652578 0, -758690.4925450943 2818658.607998822 0, -758705.2007471576 2818864.2361701773 0, -758703.6352082351 2818877.7171009136 0, -758702.3916274216 2818888.419208434 0, -758698.6599958367 2818888.360734387 0, -758673.240844335 2819122.967706949 0, -758671.1253143873 2819142.654787704 0, -758662.8618090664 2819219.5519139674 0, -758662.0386418796 2819227.72897034 0, -758660.8380965086 2819238.730063153 0, -758659.9974660431 2819245.63617677 0, -758654.9995410803 2819291.004841916 0, -758652.8177214448 2819311.114481737 0, -758649.6994803348 2819339.5311173634 0, -758648.8960344149 2819346.865086477 0, -758646.4922947071 2819369.0005113664 0, -758631.8576979493 2819379.1870485577 0, -758536.064134595 2819446.324745872 0, -758514.8718126633 2819461.2477754466 0, -758485.6581259697 2819504.5401307573 0, -758478.5390067782 2819503.793334076 0, -758387.1776951574 2819494.239560099 0, -758383.9344536605 2819501.2761283335 0, -758294.8821531541 2819698.4999611787 0, -758222.8901628957 2819794.6144463588 0, -758219.1547436661 2819795.8039818443 0, -758135.0313326333 2819821.8674609046 0, -758066.521909814 2819843.067383866 0, -757828.6292486495 2819916.503110772 0, -757799.3222543218 2819925.9983771066 0, -757755.6494078401 2819941.3006530274 0, -757752.8907657883 2819942.5764507395 0, -757704.5660675837 2819959.9000758203 0, -757701.6393355912 2819959.065462002 0, -757699.643904292 2819961.551829715 0, -757561.1458225977 2820074.960448736 0, -757555.8430975865 2820070.8414156293 0, -757550.9735694206 2820074.982238254 0, -757481.9404218218 2820018.2084677597 0, -757482.4561308704 2820013.8361315764 0, -757482.4561308703 2820013.8361315764 0, -757492.1058916934 2819932.0225614556 0, -757503.4412317734 2819842.025062935 0, -757501.9678061336 2819800.163542735 0, -757517.7576863117 2819733.44784273 0, -757623.4385056113 2819484.6797583695 0, -757637.5009377657 2819425.2618666664 0, -757661.7956097596 2819370.4721926623 0, -757696.0177974278 2819292.0024861433 0, -757721.922390823 2819205.035827121 0, -757736.6275908743 2819174.638084911 0, -757737.0165452119 2819173.334920214 0, -757741.4280077589 2819166.1500806683 0, -757741.428007759 2819166.1500806683 0, -757759.8850263678 2819136.089592614 0, -758197.1008297182 2818993.8735601115 0, -758327.2708448981 2818883.1271426165 0, -758362.0488636584 2818801.7491274294 0, -758377.9835691601 2818772.7022241666 0, -758394.1881798329 2818730.436357328 0, -758398.940881438 2818721.82847353 0, -758419.1923586403 2818716.3461524355 0, -758564.3085984066 2818681.459485316 0)), ((-685406.7749890666 2820150.9731799574 0, -685400.3319445832 2820348.786152655 0, -685393.7911048346 2820549.7388392347 0, -684839.8720346185 2820545.634140948 0, -684839.8720105918 2820545.621117336 0, -684840.3312223172 2820441.6714656926 0, -684871.2681394718 2820357.0635166476 0, -684910.5715663977 2820275.264069664 0, -684992.4791806015 2820152.7612019363 0, -685041.0750198234 2820020.280271287 0, -685041.077481309 2820020.273531119 0, -685064.4136583988 2819956.652698548 0, -685086.3190185177 2819896.9329020516 0, -685138.9726904748 2819842.5020072707 0, -685194.0354687502 2819799.1662575803 0, -685236.5853367789 2819768.847604989 0, -685236.550166813 2819768.8443257883 0, -685236.5450051151 2819768.843828265 0, -684916.6440199587 2819739.5957859433 0, -684916.6440229195 2819739.595781044 0, -684945.6328751008 2819692.7802545377 0, -684945.6625750877 2819692.73131614 0, -684967.7097781891 2819656.4264919492 0, -684997.8398916608 2819621.014111073 0, -685028.3835677358 2819585.1347657465 0, -685028.3999501476 2819585.1155179623 0, -685037.9384010277 2819582.1730363164 0, -685039.1387194602 2819581.802820588 0, -685103.4861764351 2819561.9635363007 0, -685137.0040355758 2819558.360435938 0, -685179.2472731313 2819551.5159108536 0, -685249.391375077 2819527.3632100928 0, -685306.5188882543 2819512.9642430195 0, -685362.1588061354 2819484.907158246 0, -685431.8660218114 2819453.3149557426 0, -685468.9920896178 2819440.5144576817 0, -685563.888679765 2819407.7955109654 0, -685636.2613541516 2819379.6873441306 0, -685640.6739805538 2819377.9735447094 0, -685702.3709854203 2819361.1076629325 0, -685728.2820672604 2819354.0240989714 0, -685728.9251393601 2819353.8482212727 0, -685806.5335374678 2819363.7610720047 0, -685853.7612179846 2819381.721241745 0, -685888.7005642356 2819397.951743835 0, -685922.4854385246 2819418.581234686 0, -685945.6799238139 2819433.9883979373 0, -685869.4123479467 2819821.0368117904 0, -685863.1288250255 2819823.518940691 0, -685864.1816556539 2819827.1815945944 0, -685540.204894181 2819957.386556406 0, -685415.1722053345 2820100.280244374 0, -685408.1481832038 2820108.339061455 0, -685406.7749890666 2820150.9731799574 0)), ((-684408.1490245973 2819867.199147018 0, -684403.7568967363 2819871.7894599894 0, -684366.1728107164 2819918.800327894 0, -684341.6640185011 2819940.294274738 0, -683920.27431122 2820381.750421679 0, -683913.815141469 2820393.1697519096 0, -683817.1119588523 2820564.133764186 0, -683798.7212036223 2820574.091676301 0, -683734.6547211821 2820608.784698552 0, -683729.2433599001 2820611.71585344 0, -683724.973466479 2820619.263663777 0, -683663.3630113038 2820646.328719441 0, -683606.6740045693 2820746.548567463 0, -683551.2397670313 2820767.638794945 0, -683489.7714684663 2820795.144686282 0, -683480.872286895 2820888.9620507676 0, -683290.4365471886 2821207.273167537 0, -683311.2688215015 2821326.1315004327 0, -683303.2284282156 2821410.9116964876 0, -683382.457</t>
+          <t>MULTIPOLYGON Z (((-779304.9079350996 2866327.0745835477 0, -779300.9590657263 2866326.6702074828 0, -779153.7570984508 2866310.424541069 0, -779126.2156186483 2866307.361045627 0, -779125.8700102569 2866307.315473458 0, -779106.148184011 2866305.145636247 0, -779106.194800808 2866304.721086294 0, -779105.9362982546 2866304.6869999627 0, -779107.8416011414 2866287.525426021 0, -779118.403661055 2866192.183078766 0, -779121.943787134 2866160.692226106 0, -779122.7684254933 2866153.3506462113 0, -779125.2419485286 2866131.254306182 0, -779149.6119593101 2865909.3109809356 0, -779150.1806210199 2865909.373383448 0, -779150.1813775826 2865909.366741886 0, -779145.2762115606 2865908.8863971997 0, -779144.4407769815 2865908.8045861954 0, -779140.3282349799 2865908.3484188453 0, -779130.3583803957 2865907.2381662573 0, -779051.6946062817 2865898.477727759 0, -778947.9796811765 2865887.046657124 0, -778925.8803831866 2865884.459117109 0, -778745.9815095876 2865864.2462161575 0, -778748.0973385327 2865839.5907291775 0, -778788.7313347592 2865472.488801352 0, -778789.1232820227 2865468.8928435566 0, -778782.8493347741 2865468.133675343 0, -778770.8662202087 2865466.777084145 0, -778587.2785353988 2865446.6961526177 0, -778630.5060057266 2865050.817523389 0, -778795.9364610518 2865069.071144758 0, -778829.1488904493 2865072.7371318964 0, -778832.1191208631 2865073.0992569556 0, -778875.3544676013 2864677.2069002697 0, -778821.0044294996 2864671.1840836187 0, -778673.6318773903 2864654.931451717 0, -778716.7582594071 2864259.0396635346 0, -778846.0666581673 2864273.1639524833 0, -778919.5771365796 2864281.3721959386 0, -778923.4298074759 2864281.7881243434 0, -779011.2024317926 2864291.481546741 0, -779021.4239533767 2864292.7003727993 0, -779040.0241077212 2864294.802851747 0, -779040.0241161513 2864294.802862341 0, -779048.0950406332 2864304.9275779794 0, -779081.5100963196 2864346.691926683 0, -779081.51011605 2864346.6919513326 0, -779081.5101339425 2864346.6919781645 0, -779103.2222831812 2864379.2385333944 0, -779110.4115474825 2864400.7378377835 0, -779145.2388073046 2864504.909856213 0, -779145.2373684414 2864504.9142325423 0, -779145.2398763419 2864504.9217334674 0, -779145.239876338 2864504.921733479 0, -779145.2398763392 2864504.9217334827 0, -779105.4091129539 2864626.054522275 0, -779107.6021636605 2864666.8165470483 0, -779114.1918241585 2864703.506553551 0, -779114.191915418 2864703.5070613227 0, -779114.1920173957 2864703.5076306025 0, -779120.2681808715 2864737.406605333 0, -779152.3886458386 2864800.707789942 0, -779192.2797327498 2864828.211610813 0, -779215.7149021933 2864853.127852828 0, -779262.4077841557 2864910.8684776765 0, -779262.4055274364 2864910.876613737 0, -779262.4090644304 2864910.8809871553 0, -779254.9582020501 2864937.7329249955 0, -779267.8374664417 2864984.89326154 0, -779271.255752108 2865019.5770358304 0, -779271.2549658094 2865019.584497317 0, -779271.2558011949 2865019.592966862 0, -779268.6462162543 2865044.3403834435 0, -779268.6462162522 2865044.340383445 0, -779268.6462162477 2865044.3403834878 0, -779243.0937434582 2865062.3057162617 0, -779231.5169619516 2865081.0065179598 0, -779228.8898344346 2865104.702292179 0, -779214.1056601275 2865115.198077089 0, -779205.6575091856 2865125.4143026145 0, -779202.9635111759 2865130.8248968916 0, -779202.9092646397 2865130.8649468333 0, -779201.9461432174 2865131.5760144787 0, -779201.3687132479 2865132.002328087 0, -779201.3140513613 2865132.04268468 0, -779196.9972393411 2865134.977016463 0, -779181.7520377578 2865145.3398674186 0, -779181.7448222385 2865145.341421074 0, -779181.7306119628 2865145.3444808493 0, -779176.4806674288 2865146.474905855 0, -779168.5528792638 2865148.175910826 0, -779157.1356959858 2865152.3430054043 0, -779146.6797055126 2865156.1514428747 0, -779139.7253875722 2865157.584441535 0, -779134.0559668748 2865158.7513434244 0, -779134.0559668734 2865158.7513434244 0, -779134.0559668269 2865158.751343434 0, -779125.9651313591 2865159.8935043905 0, -779079.2908318003 2865206.865736912 0, -779053.740847804 2865248.6332662883 0, -779060.3669293413 2865293.016810817 0, -779072.521815128 2865371.894083655 0, -779072.5202583339 2865371.897731961 0, -779072.5223159426 2865371.911083353 0, -779070.2483823916 2865377.2218135255 0, -779057.6609545639 2865406.748632715 0, -779042.7205976748 2865433.5028620926 0, -779039.152479286 2865439.924130304 0, -779023.0279794952 2865448.293106738 0, -778993.7520421153 2865463.826756115 0, -778970.6611095731 2865476.0778305396 0, -778968.6561214548 2865477.1415926316 0, -778956.4113200627 2865482.241545986 0, -778946.6793083777 2865486.32109739 0, -778946.6793082762 2865486.3210973786 0, -778934.1801994797 2865491.5606448776 0, -778917.3725716695 2865498.641953889 0, -778939.3769872008 2865584.7747839727 0, -778976.8123785012 2865626.5557441814 0, -779070.4881821149 2865731.398700857 0, -779138.7121427488 2865757.6186342165 0, -779193.8966056061 2865744.298193133 0, -779227.2728923232 2865741.3936695904 0, -779262.9244508899 2865760.6726428876 0, -779323.3717550738 2865789.4067152063 0, -779310.5830200284 2865837.322463818 0, -779310.5830133636 2865837.3224889184 0, -779309.2371529589 2865842.397671633 0, -779309.2371529434 2865842.397671654 0, -779309.2371529362 2865842.3976716814 0, -779304.6237460255 2865848.684998582 0, -779292.6560994192 2865864.9949638876 0, -779287.2914060361 2865886.2247151732 0, -779291.490815091 2865924.855617001 0, -779300.0528537801 2865939.7354915333 0, -779325.8083980508 2865984.182716592 0, -779329.5936830095 2865990.877125187 0, -779335.7647028733 2866001.3645638414 0, -779340.7360346571 2866009.9421461234 0, -779342.2131859002 2866012.3954330594 0, -779342.2131859086 2866012.3954330618 0, -779342.2131859087 2866012.395433061 0, -779342.2131880341 2866012.395433664 0, -779372.151402374 2866020.876621468 0, -779379.3495333014 2866022.90937798 0, -779387.2382461597 2866026.0080900206 0, -779414.3932899326 2866036.6744328826 0, -779419.9555692682 2866038.8594160196 0, -779469.6521037758 2866035.7577639148 0, -779505.5638708652 2866029.304145113 0, -779509.6160760403 2866028.57596547 0, -779586.2511909457 2866048.736966126 0, -779617.6114337902 2866070.9433910954 0, -779668.0572842329 2866133.4988183226 0, -779713.5557304206 2866181.3759299745 0, -779699.7635778274 2866250.2194864987 0, -779699.6693577461 2866250.696038443 0, -779673.6980300663 2866306.686730672 0, -779666.9540606847 2866309.5274188924 0, -779658.3149942142 2866313.166358084 0, -779631.6438362749 2866328.9537691833 0, -779599.8944918101 2866347.747102227 0, -779591.8881338246 2866352.7793916864 0, -779591.8881273797 2866352.7793957484 0, -779583.9506848671 2866357.808552827 0, -779568.3500247455 2866367.6919736937 0, -779554.0057215543 2866376.817223519 0, -779553.0384076122 2866378.842453414 0, -779551.4617086295 2866382.143530564 0, -779551.4617066641 2866382.1435346873 0, -779528.7638745711 2866429.7637730306 0, -779525.9447666332 2866449.6653061714 0, -779525.1477111776 2866455.5680601005 0, -779509.1860784377 2866573.1947606048 0, -779549.4492355619 2866622.156958724 0, -779585.8910487035 2866644.055816147 0, -779617.0343096714 2866656.3589980225 0, -779657.055098304 2866678.170773459 0, -779675.9214310695 2866702.196313196 0, -779686.9074296867 2866716.193585674 0, -779688.6923568146 2866718.467497366 0, -779731.2478500814 2866748.2971152854 0, -779735.0626553502 2866750.8928653626 0, -779745.1792336187 2866773.911404346 0, -779746.3262182855 2866776.5126066078 0, -779756.6804523873 2866780.2930155494 0, -779760.5911791024 2866781.6816453673 0, -779765.1353403393 2866783.4185599373 0, -779780.7410285155 2866801.9090242246 0, -779782.5802469932 2866804.0885802833 0, -779783.9213599105 2866811.0940339374 0, -779783.9907325234 2866811.4505314506 0, -779788.6696253056 2866835.16151928 0, -779793.970550902 2866838.8543598186 0, -779793.9705511765 2866838.8543600063 0, -779796.9830574616 2866840.9154834338 0, -779799.3910429042 2866842.5239838576 0, -779809.7036107051 2866849.3774993685 0, -779814.9315585205 2866854.655198107 0, -779817.2558039882 2866857.0005583656 0, -779849.9090321712 2866890.2079449045 0, -779851.6497902453 2866891.9764218726 0, -779851.9474376016 2866892.2784973974 0, -779851.948620692 2866892.2796980888 0, -779855.1715612088 2866893.450912427 0, -779855.1715615301 2866893.450912543 0, -779883.5784008092 2866903.5945362016 0, -779889.4830955303 2866906.0520811765 0, -779889.4830956871 2866906.052081239 0, -779899.4872820814 2866910.0145255593 0, -779902.7661595201 2866909.1573240245 0, -779903.06432163 2866909.0727239456 0, -779941.7597677703 2866901.0007285383 0, -779945.6779448233 2866900.181854022 0, -779990.7910749582 2866884.045822849 0, -780030.6135322689 2866836.682446488 0, -780033.2684257341 2866833.597392254 0, -780033.2684354124 2866833.59738504 0, -780035.5375477438 2866831.904521111 0, -780057.7257643872 2866815.6568061677 0, -780064.1461269036 2866818.502320128 0, -780090.9366377833 2866830.3917377423 0, -780133.89057774 2866842.597644402 0, -780150.4058261721 2866852.3191592274 0, -780150.411989451 2866852.3350040643 0, -780150.4600618072 2866852.3633030327 0, -780175.428586096 2866916.474325607 0, -780189.5268056914 2866982.7689993717 0, -780182.4600024628 2867001.0239812057 0, -780182.3555241922 2867001.0592753175 0, -780182.3460716568 2867001.083688821 0, -780171.1883500539 2867004.8316912395 0, -780171.188347239 2867004.8316921904 0, -780149.7691617253 2867012.024510049 0, -780113.6291492814 2867097.1966597107 0, -780112.5635850911 2867179.7537893984 0, -780119.5752173394 2867199.9731411543 0, -780119.5752190775 2867199.973146141 0, -780124.6908509599 2867214.502216883 0, -780127.9139902004 2867223.6557753137 0, -780127.913991517 2867223.6557789934 0, -780137.4979773352 2867250.2324645696 0, -780178.9906645096 2867279.6379998005 0, -780179.1848188583 2867279.775487024 0, -780196.6391077609 2867292.1453208667 0, -780196.6444624714 2867292.154038222 0, -780196.7084945008 2867292.1994353007 0, -780219.2578227344 2867328.912949185 0, -780235.8500057842 2867380.125415139 0, -780235.0224535076 2867424.9112286805 0, -780223.0311947786 2867462.8745537414 0, -780214.7739112539 2867483.972928059 0, -780212.2158848194 2867490.689476867 0, -780211.8137265675 2867491.3326835395 0, -780210.2229013377 2867493.8770287107 0, -780210.222900861 2867493.877029491 0, -780203.9572028025 2867504.257186381 0, -780187.6526605099 2867515.9848600714 0, -780172.9110753008 2867540.9148804476 0, -780108.4302354697 2867585.6731637605 0, -780108.3680211534 2867585.63938935 0, -780108.3545303716 2867585.648749364 0, -780086.1618562269 2867573.594301091 0, -780064.7922477692 2867543.212531911 0, -780015.172118825 2867545.1532341493 0, -779981.4447819251 2867558.5686488766 0, -779960.3008234018 2867566.992400341 0, -779954.7320235713 2867569.1731972136 0, -779952.0898931359 2867570.228046003 0, -779952.0898924158 2867570.228046878 0, -779933.4884271858 2867592.9712232375 0, -779931.8133636253 2867595.2339429366 0, -779920.4619358924 2867613.6809061766 0, -779914.5769850386 2867623.4378382144 0, -779906.2403500113 2867637.2861757823 0, -779909.7839589368 2867660.69840403 0, -779910.8196514907 2867667.540766627 0, -779910.819651789 2867667.540768598 0, -779913.2101330699 2867683.2267922917 0, -779921.0107550346 2867694.4813809455 0, -779921.0107599307 2867694.481387992 0, -779935.6925738538 2867715.5333454106 0, -779941.7260559902 2867722.2085948098 0, -779938.8574386678 2867732.09062936 0, -779942.7537764932 2867738.28435054 0, -779953.4220376707 2867755.2412652266 0, -779958.6876414513 2867760.5741329957 0, -779986.6780746016 2867788.9244766654 0, -779994.4211631832 2867833.4695059485 0, -779996.0619575984 2867843.330221665 0, -780011.4805325873 2867878.64794406 0, -780016.4294372235 2867889.9838030394 0, -780021.2511991784 2867901.2779533747 0, -780035.1559595682 2867933.8245187956 0, -780067.3044794233 2867958.099728915 0, -780092.3876133718 2867976.934358336 0, -780129.5150795655 2867976.8573418804 0, -780143.2501499564 2867976.7104670755 0, -780154.1347760144 2867970.2724514757 0, -780162.0250643261 2867966.2409890736 0, -780175.9838638561 2867959.2371197087 0, -780208.9271376494 2867942.498026442 0, -780211.8219856764 2867941.0769677185 0, -780230.718415916 2867961.4392033685 0, -780257.9387566276 2867990.4320396497 0, -780270.7877296533 2868008.664862903 0, -780271.4156469837 2868030.8659969084 0, -780271.5125259771 2868035.891481801 0, -780271.6917727466 2868042.667724333 0, -780271.1457061982 2868045.415702571 0, -780267.2596377166 2868048.030826591 0, -780253.6413667245 2868058.8683116804 0, -780257.2126298236 2868082.1137912082 0, -780258.9307758686 2868093.286304257 0, -780258.1532994827 2868103.3527499135 0, -780256.0195743253 2868131.016723943 0, -780267.8618371518 2868157.734759952 0, -780275.7022799109 2868175.388378105 0, -780283.7983055882 2868179.5489601586 0, -780292.6615983079 2868183.7742528054 0, -780354.078242831 2868213.054084066 0, -780369.8741598591 2868209.5798874223 0, -780390.6740443747 2868205.0054862285 0, -780430.7194506521 2868157.6157531324 0, -780465.6122176911 2868123.0502816536 0, -780499.7822652165 2868108.0142097017 0, -780530.2662878109 2868100.6320033004 0, -780561.2797663695 2868096.1173576936 0, -780585.229592231 2868116.792696185 0, -780591.0638451594 2868121.8172028866 0, -780624.0195790911 2868153.9296654146 0, -780643.824291495 2868181.95309038 0, -780674.2701028391 2868231.3114375924 0, -780667.647170231 2868287.642819418 0, -780616.1934146394 2868341.3145533646 0, -780507.0768621111 2868362.4499460557 0, -780457.2872171006 2868398.598726522 0, -780449.404758897 2868423.2172151553 0, -780437.8880136701 2868459.33193768 0, -780438.5095848306 2868483.186428469 0, -780439.0009394187 2868500.6547144447 0, -780439.8144682248 2868530.312555635 0, -780468.3067455092 2868558.260272274 0, -780500.407432749 2868589.6802325044 0, -780508.0750506903 2868590.5639736885 0, -780529.5642923648 2868593.031618096 0, -780607.6072858134 2868608.3802648797 0, -780638.321222069 2868629.9391305605 0, -780647.700380725 2868636.5278843227 0, -780651.56526434 2868643.8651430532 0, -780652.9061471489 2868646.433761697 0, -780655.1950769854 2868650.9467331795 0, -780660.1665794743 2868660.6458233334 0, -780679.864017195 2868676.355004451 0, -780714.946225137 2868699.9128579376 0, -780743.0561164145 2868725.705022825 0, -780758.935581237 2868737.913406749 0, -780771.7703215113 2868755.5970413806 0, -780782.0069733132 2868771.081739324 0, -780758.0237120664 2868806.7965130196 0, -780741.8468468265 2868788.8999802982 0, -780733.2992106574 2868779.4440627513 0, -780678.7923149357 2868764.3483426278 0, -780660.1429525369 2868758.9684430636 0, -780658.5017949716 2868756.0317070684 0, -780656.7962791208 2868752.9729189766 0, -780649.5004004847 2868739.8882335406 0, -780642.4107917225 2868741.3814160144 0, -780614.7483967241 2868747.16278265 0, -780620.0283193644 2868770.6165203536 0, -780621.9438328906 2868779.125455868 0, -780617.1331207319 2868794.1621076036 0, -780608.5842629903 2868820.8827284453 0, -780610.4017453694 2868829.684730192 0, -780620.786809104 2868879.735953714 0, -780623.0206860149 2868890.5036827917 0, -780623.7801947279 2868894.1227484457 0, -780624.8843686173 2868899.486581847 0, -780629.1621139545 2868906.5911678923 0, -780645.4627844561 2868933.6927095293 0, -780665.7848580597 2868946.047142861 0, -780673.2674873873 2868950.5959313135 0, -780711.3980113654 2868978.7783207335 0, -780729.7938893085 2868998.102228022 0, -780806.5890987276 2869042.5713849533 0, -780829.2104213691 2869055.652398372 0, -780846.7317857399 2869077.7908078814 0, -780849.6888465665 2869093.1635548575 0, -780851.2444533325 2869101.205827288 0, -780859.1080571082 2869106.840241632 0, -780880.0671380667 2869121.6901659234 0, -780904.5848287079 2869147.0680197002 0, -780921.8018630006 2869228.848461901 0, -780933.9451154479 2869278.0984647786 0, -780937.0773687472 2869290.7618271643 0, -780932.6817647588 2869314.222176287 0, -780592.4494464375 2869276.510103586 0, -780581.8633916792 2869275.322169444 0, -780567.0906029015 2869273.687439044 0, -780379.9151030026 2869252.798227524 0, -780381.1025343707 2869240.0205894937 0, -780383.0646016569 2869217.729473123 0, -780399.8209768042 2869054.593767323 0, -780199.4815631429 2869031.6136801844 0, -780203.080664142 2868998.261281361 0, -780204.655392828 2868983.713981458 0, -780220.9781707377 2868835.5410523666 0, -780218.0416167416 2868835.220864358 0, -780018.8788017232 2868813.224142559 0, -780040.9544328884 2868615.3333827914 0, -779839.1214824963 2868592.593344387 0, -779860.9283054336 2868395.968623219 0, -779860.828353818 2868395.9572289027 0, -779860.8258508032 2868395.9799712407 0, -779796.6513697552 2868388.657097032 0, -779840.3492388529 2867994.546192049 0, -779830.6159661649 2867993.376086266 0, -779721.0984120859 2867980.393429644 0, -779721.0738629557 2867980.3909338894 0, -779721.0739095071 2867980.3905237895 0, -779538.1912544267 2867958.699190479 0, -779567.3780728334 2867697.7170125665 0, -779583.1859263789 2867557.450209374 0, -779583.1859263411 2867557.45020937 0, -779583.3632852 2867554.6543739727 0, -779621.887920612 2867195.499852003 0, -779626.0347395401 2867161.275451751 0, -779423.8093009266 2867139.980027611 0, -779423.8585457572 2867139.514386206 0, -779423.78805035 2867139.5064977612 0, -779443.4744816157 2866953.0341884177 0, -779446.6159386438 2866923.454483797 0, -779465.5197998745 2866745.580134709 0, -779302.7630156983 2866727.718068347 0, -779302.7629729796 2866727.7180636683 0, -779264.7313398954 2866723.53681002 0, -779264.5992211195 2866723.5222846875 0, -779264.7791592191 2866720.7265381604 0, -779307.7513682813 2866327.328534183 0, -779304.9079350996 2866327.0745835477 0), (-779174.191770332 2865911.9384812503 0, -779174.1917702062 2865911.9384812354 0, -779172.9852149499 2865911.798587795 0, -779174.191770332 2865911.9384812503 0)), ((-785065.6032716993 2884211.4965632465 0, -785071.1520494085 2884237.5328455777 0, -785074.0743182834 2884251.245471162 0, -785074.0743187336 2884251.245473275 0, -785072.8350446203 2884251.8137203488 0, -785059.5933640503 2884257.886078278 0, -785058.4655225205 2884258.4033064526 0, -785029.9331651429 2884271.4876718954 0, -784982.5444845094 2884293.218891352 0, -784982.5329867667 2884293.224081307 0, -784981.2149508686 2884293.828500253 0, -784981.2147696365 2884293.8286640937 0, -784981.1467549306 2884293.859853873 0, -784981.1130963754 2884293.9201835813 0, -784981.1126494949 2884293.9209845713 0, -784942.4933314892 2884328.8343114667 0, -784938.2966815983 2884346.38967372 0, -784936.6179760093 2884353.4133089255 0, -784936.4155603364 2884354.2629710403 0, -784935.9100860038 2884356.388015854 0, -784928.5993805551 2884386.991325736 0, -784993.285410236 2884560.2029558844 0, -785012.5606098194 2884631.6563191717 0, -785012.5606306553 2884631.6563964025 0, -785012.56075832 2884631.6565387323 0, -785100.1409543537 2884729.2930047493 0, -785100.1382688797 2884729.2942893715 0, -785100.1383894685 2884729.2944238125 0, -785100.0426378414 2884729.3402275466 0, -785100.0479940528 2884729.3461995577 0, -784865.9550747823 2884841.3273328207 0, -784870.340734311 2884898.9978950107 0, -785089.1225307342 2885040.6966766133 0, -785137.4241029804 2885071.9800291564 0, -785137.4241168518 2885071.9800381204 0, -785144.7563596909 2885076.7156066117 0, -785149.5507473459 2885089.185002046 0, -785149.5507482933 2885089.1850045086 0, -785181.1397999076 2885171.1300373194 0, -785181.053034548 2885171.1755495123 0, -785181.0546302543 2885171.1796889217 0, -785068.2787474302 2885230.336112334 0, -785090.9109817881 2885300.809213529 0, -785167.8188858558 2885335.1925203144 0, -785137.469540249 2885398.2045503845 0, -785134.704310118 2885449.9587178538 0, -785134.6223183037 2885449.9492915287 0, -785134.6191365693 2885450.009068597 0, -784753.0042645405 2885403.7581594787 0, -784796.9568533582 2885008.159964477 0, -784840.9078724972 2884612.558932737 0, -784887.075394753 2884217.026761061 0, -784911.6030819823 2884002.4308323604 0, -784911.6851222854 2884002.415955814 0, -784911.6851257501 2884002.415925501 0, -784944.0389234985 2883996.549170707 0, -784952.7095800161 2883994.9769096673 0, -784952.8177494847 2883994.957295599 0, -784952.8177494848 2883994.957295599 0, -784967.5701537884 2883992.282283246 0, -785000.7248227113 2884032.8557939967 0, -784985.4464197728 2884082.796609726 0, -784985.4170368295 2884082.8926543295 0, -784985.4169973311 2884082.892783439 0, -784985.4749725992 2884082.943058755 0, -784986.1639220841 2884083.540505809 0, -784987.2354451539 2884084.469715156 0, -784987.2354451566 2884084.4697151585 0, -785018.3869469 2884111.4838480535 0, -785018.3869469035 2884111.4838480563 0, -785020.9831284193 2884113.7352192122 0, -785050.1615275689 2884139.0394245973 0, -785065.6032716993 2884211.4965632465 0)), ((-778018.9447448857 2848989.745918616 0, -778066.8683336076 2849016.709277986 0, -778107.8935463295 2849031.885046103 0, -778107.8935678903 2849031.885071271 0, -778107.8998301893 2849031.887387773 0, -778165.2545033393 2849098.842157993 0, -778111.3076032304 2849130.168651748 0, -778087.6126041275 2849186.3163977806 0, -778126.6375942499 2849232.727695082 0, -778223.3552550377 2849265.8186636334 0, -778254.8962661957 2849265.7881828006 0, -778317.3286196977 2849256.3805453232 0, -778320.3206548779 2849255.9305497576 0, -778382.8332636404 2849238.0703015476 0, -778423.6735988836 2849259.0496166716 0, -778428.9827689723 2849261.776760421 0, -778454.2196999231 2849278.691583925 0, -778488.0754617819 2849356.2284987266 0, -778488.6501968709 2849382.5362317674 0, -778489.152936014 2849406.1901539196 0, -778450.2355246089 2849445.274848413 0, -778352.5313618146 2849449.953824687 0, -778312.1611298464 2849447.1315117213 0, -778292.6974834282 2849465.247074199 0, -778251.9586401515 2849503.1628931905 0, -778240.67791667 2849566.0853533074 0, -778195.7662688775 2849622.488102977 0, -778177.5478470904 2849623.076913356 0, -778120.4627838772 2849639.9752028664 0, -778096.8846394607 2849645.720705325 0, -778000.5748267936 2849733.491153451 0, -778000.5748146558 2849733.491172231 0, -777995.0456996908 2849742.0505981613 0, -778024.6618800078 2849822.4492694708 0, -778065.4236408372 2849893.553183616 0, -778095.0547552725 2849940.7998997993 0, -778111.123129531 2849966.4205661775 0, -778152.0380063502 2849995.857612358 0, -778232.4635076745 2850022.7648026235 0, -778232.4635694196 2850022.7648232784 0, -778272.3694730203 2850005.137503722 0, -778286.1607537577 2849979.6017443314 0, -778296.920254595 2849936.9769389974 0, -778336.2231786009 2849907.0715158912 0, -778393.8367818684 2849849.3580969116 0, -778393.8430354721 2849849.360552195 0, -778393.8430511502 2849849.360536491 0, -778403.6653998105 2849853.216998893 0, -778428.6853912089 2849863.0403224714 0, -778428.6854091042 2849863.040385179 0, -778428.6991688223 2849863.0457875365 0, -778443.4649263347 2849914.8092266163 0, -778414.1937640968 2849949.001410578 0, -778371.7344926831 2850017.615826767 0, -778382.3051193785 2850074.338933517 0, -778398.5470595541 2850082.064149347 0, -778403.3046900313 2850084.3265774795 0, -778446.810059922 2850176.3057739446 0, -778447.2446485488 2850181.0248513315 0, -778455.2041889131 2850268.246773478 0, -778429.6688173915 2850307.581051144 0, -778392.1623876267 2850337.822753677 0, -778391.2678431092 2850381.5535695823 0, -778409.1754104488 2850423.8003512262 0, -778443.3267647222 2850418.882471604 0, -778472.0479189741 2850425.3049393725 0, -778472.0487260116 2850425.3051198344 0, -778472.1538681126 2850425.351573998 0, -778539.5934494556 2850455.1479067337 0, -778539.5934506133 2850455.1479104175 0, -778539.6047455587 2850455.1529007806 0, -778556.6351373835 2850509.3733091513 0, -778560.1761920195 2850560.9527782807 0, -778547.8672037215 2850595.660859155 0, -778537.9140969089 2850606.129185271 0, -778520.642783997 2850623.4954078286 0, -778493.3349725715 2850650.953595447 0, -778451.0096472857 2850697.8333630995 0, -778412.2927054393 2850735.7666474488 0, -778332.2267194751 2850801.4565049415 0, -778302.6506236638 2850831.477270452 0, -778261.3214377748 2850858.485909124 0, -778219.6404445403 2850879.0038987314 0, -778186.4701389986 2850893.9341213712 0, -778155.5423610273 2850942.964488242 0, -778155.3875860953 2850943.902271544 0, -778153.8866063681 2850952.996727043 0, -778144.8386589016 2851007.818732372 0, -778144.838656444 2851007.8187473714 0, -778143.8777997025 2851013.701355991 0, -778149.8737242838 2851080.1654093326 0, -778164.1845627591 2851163.640269842 0, -778188.4564350559 2851188.1242920617 0, -778205.9905316551 2851205.810038239 0, -778226.8356577648 2851241.215181279 0, -778255.9156079143 2851286.877953428 0, -778270.0726153597 2851365.3265308696 0, -778270.072638942 2851365.326661501 0, -778270.0726389335 2851365.3266615 0, -778270.0726389342 2851365.326661504 0, -778094.4605108831 2851346.208892302 0, -777690.6850503956 2851302.830592308 0, -777690.6850503958 2851302.8305923063 0, -777690.6850503882 2851302.8305923054 0, -777733.9628193304 2850906.4917634716 0, -777777.2388194209 2850510.150120197 0, -777820.9831457793 2850114.3101011575 0, -777864.7277990956 2849718.467504392 0, -777460.6128714907 2849673.6653484977 0, -777056.4934434132 2849628.885801183 0, -777056.4934434134 2849628.885801181 0, -777056.4934434058 2849628.8858011803 0, -777099.6764418286 2849232.3232875033 0, -777503.5643492694 2849277.22811051 0, -777690.8115454458 2849298.045287109 0, -777908.4311447623 2849322.23911069 0, -777951.249948151 2848933.928056874 0, -777951.249948158 2848933.92805688 0, -777951.2499481585 2848933.9280568752 0, -777951.4898512964 2848934.1258694273 0, -778018.9447448857 2848989.745918616 0)), ((-775704.8974972891 2861917.3864071863 0, -775748.9644106021 2861520.776052916 0, -776152.9127795845 2861565.5854092953 0, -776152.9127961973 2861565.5854111384 0, -776553.9168441865 2861610.0682845274 0, -776556.8636252692 2861610.390778591 0, -776512.039852616 2862006.354712643 0, -776467.216922884 2862402.3131001843 0, -776466.9929051308 2862404.3219294287 0, -776423.0514987482 2862798.356692091 0, -776019.7807803612 2862754.2477628333 0, -775616.5129932838 2862710.1317281877 0, -775616.7509383601 2862707.339991846 0, -775660.8313339656 2862313.9912819895 0, -775661.0604045603 2862311.1987747676 0, -775704.8974972891 2861917.3864071863 0)))</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1665,31 +1665,31 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>None Listed, Common Schools, Public Land Trust Income - Navigable Rivers</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Subsurface, subsurface, Surface</t>
+          <t>subsurface, Surface</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="G26" t="n">
-        <v>1809.4</v>
+        <v>1183.38</v>
       </c>
       <c r="H26" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I26" t="n">
-        <v>1725.02</v>
+        <v>1054.27</v>
       </c>
       <c r="J26" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="K26" t="n">
-        <v>3534.42</v>
+        <v>2237.65</v>
       </c>
       <c r="L26" t="n">
         <v>2110405.94</v>
@@ -1698,7 +1698,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1722347.3590887182 1241236.1226395366 0, -1722378.978481109 1241226.6656640186 0, -1722458.0590248206 1241214.3619041357 0, -1722511.0244963982 1241209.64816162 0, -1722554.9108853338 1241209.2290898764 0, -1722573.2574028883 1241209.0540111328 0, -1722619.8481824573 1241210.135066921 0, -1722651.3319137658 1241215.0706257604 0, -1722682.5981761983 1241220.9879581626 0, -1722708.2435573405 1241227.6669537546 0, -1722709.5477916386 1241228.0066600225 0, -1722745.0125975516 1241237.9475634922 0, -1722776.2787327354 1241243.8649960575 0, -1722784.8158541396 1241246.5779228427 0, -1722808.6150244088 1241254.1408575638 0, -1722845.5848813362 1241266.4767380522 0, -1722851.2141634866 1241269.2062787032 0, -1722904.4176961277 1241295.0027672967 0, -1722931.0321193866 1241308.1281024928 0, -1722956.3408534867 1241327.1445511675 0, -1722983.8075472587 1241345.6103498647 0, -1723012.7796750604 1241366.4711491766 0, -1723056.3874646388 1241403.976641978 0, -1723075.4393329283 1241423.663191418 0, -1723077.4803774995 1241425.9903314833 0, -1723099.0068817858 1241450.5344244046 0, -1723124.515092653 1241477.8367388353 0, -1723147.4297913224 1241507.6535189159 0, -1723165.4931102102 1241536.392342372 0, -1723193.8396936913 1241601.412638931 0, -1723209.8264970898 1241644.112965642 0, -1723218.0693761532 1241675.8206161677 0, -1723223.1834689046 1241707.8632057626 0, -1723227.110158572 1241740.6721114677 0, -1723227.3697827994 1241758.299072991 0, -1723227.490938815 1241766.511721777 0, -1723223.1203431368 1241795.4164874577 0, -1723216.591583556 1241824.8717889888 0, -1723194.2481291608 1241888.9307157993 0, -1723191.2465811328 1241898.1658365303 0, -1723181.4444746135 1241928.3238711308 0, -1723169.9463166813 1241961.8260648944 0, -1723156.9700882272 1242034.1478473837 0, -1723154.20692709 1242069.5589382623 0, -1723153.6513406222 1242076.6790162898 0, -1723152.7261972136 1242108.4100066365 0, -1723152.7500927413 1242108.7320616634 0, -1723150.208765948 1242110.7701281658 0, -1723106.6430053764 1242145.714618138 0, -1723094.3103107193 1242391.8233115352 0, -1723111.9207210592 1242612.7974887264 0, -1723223.9138330873 1242782.587060279 0, -1723029.603357652 1242879.8031119374 0, -1723029.602232531 1242879.8028472173 0, -1723029.585444656 1242879.8112464237 0, -1722884.2021506082 1242845.6052545607 0, -1722884.0032644228 1242845.6278090398 0, -1722757.3192187187 1242863.5770453282 0, -1722733.3568359872 1242879.1896421772 0, -1722733.3527278912 1242879.1889246006 0, -1722733.3389890755 1242879.197876182 0, -1722559.6401527082 1243013.8007383328 0, -1722381.6339916687 1242949.53811921 0, -1722232.672660665 1242832.3087205358 0, -1722211.1041122193 1242787.965799454 0, -1721996.7433034913 1242750.5225927236 0, -1722003.6491573025 1242716.5649391306 0, -1722003.4785811466 1242716.544707561 0, -1722073.9175046657 1242361.0715618066 0, -1722080.7294661691 1242326.694809999 0, -1722153.0310744173 1241961.8344069486 0, -1721764.424998388 1241891.068965686 0, -1721366.1294605085 1241818.5546973892 0, -1720979.3183402896 1241748.1524682967 0, -1720972.6732262475 1241746.9431201753 0, -1720586.7628300434 1241676.72268317 0, -1720406.9748293536 1241642.9505246803 0, -1720355.4043134027 1241635.7290223027 0, -1720331.8072004942 1241631.964132609 0, -1720266.5560556562 1241619.4766118755 0, -1720264.2451736396 1241616.33845115 0, -1720240.328073899 1241583.8592163166 0, -1720213.1145884478 1241545.876842757 0, -1720206.239817999 1241537.1404345052 0, -1720175.7812797052 1241498.4348461167 0, -1720117.2735897598 1241413.3225018526 0, -1720074.5715069098 1241353.3557109775 0, -1720068.2504339456 1241331.347701848 0, -1720067.8685424912 1241305.5083018334 0, -1720071.2679676383 1241276.3881464894 0, -1720083.61689073 1241248.2264821115 0, -1720108.2617918705 1241219.7063913245 0, -1720130.295560692 1241202.9680343617 0, -1720197.6765641028 1241186.2199534823 0, -1720273.1628833918 1241200.430675972 0, -1720343.965099368 1241213.7592215824 0, -1720387.9010476028 1241230.3286424568 0, -1720442.8701737248 1241248.7231904976 0, -1720502.2555709393 1241270.1592070626 0, -1720569.2850051324 1241298.4448821677 0, -1720631.3635780402 1241321.509484366 0, -1720656.1041292115 1241328.8255317586 0, -1720656.1919981353 1241328.8515153455 0, -1720673.4018369738 1241333.9406108344 0, -1720751.3217416313 1241363.6157461514 0, -1720779.1239249345 1241375.9743005778 0, -1720839.6970031105 1241396.6443093063 0, -1720867.6166970753 1241403.8781641305 0, -1720909.0201827416 1241409.987069465 0, -1720971.8690523116 1241424.9817720288 0, -1721025.7679832708 1241439.018070436 0, -1721040.422373618 1241441.1608262327 0, -1721080.0024789404 1241446.948017187 0, -1721118.0598608023 1241454.3739352655 0, -1721168.6308853503 1241460.4596318211 0, -1721213.380481255 1241465.2518001262 0, -1721286.802439242 1241478.4752963868 0, -1721324.2250700656 1241479.579163603 0, -1721403.93976753 1241473.5970794298 0, -1721440.4980931187 1241473.9168606205 0, -1721481.1606803727 1241474.2725525228 0, -1721556.1418710703 1241462.0877432576 0, -1721597.1462023102 1241451.62527158 0, -1721616.9167840271 1241448.386496333 0, -1721647.8530407362 1241443.3186712575 0, -1721689.3924369845 1241435.0353536338 0, -1721730.8318611628 1241422.6091250256 0, -1721812.840776079 1241401.6841761821 0, -1721854.4980541016 1241388.276426463 0, -1721863.7109090104 1241385.9255508024 0, -1721884.7117926555 1241380.5671934842 0, -1721916.3311244752 1241371.1099750742 0, -1721970.5019116465 1241356.3617224116 0, -1722005.9024231657 1241343.6242233745 0, -1722048.7475203713 1241329.449915905 0, -1722080.1492643817 1241320.9747471123 0, -1722098.284799741 1241312.6421258582 0, -1722119.33101951 1241304.9563377919 0, -1722143.406089291 1241292.7925285716 0, -1722175.4606723138 1241281.3717397756 0, -1722216.9003799972 1241268.9456731929 0, -1722262.5322767175 1241255.7107134452 0, -1722283.2675461078 1241249.6965605556 0, -1722295.9735278878 1241247.0056232987 0, -1722299.0169854849 1241246.361047292 0, -1722347.3590887182 1241236.1226395366 0), (-1723009.6320559324 1241731.4823028664 0, -1723015.5545509255 1241746.463191892 0, -1723014.774587201 1241744.489667424 0, -1723011.709418197 1241736.7367974606 0, -1723009.6320559324 1241731.4823028664 0), (-1722610.5526441797 1241224.6314802137 0, -1722708.167260696 1241245.7283784277 0, -1722705.0190924767 1241245.047048451 0, -1722702.9337487202 1241244.5958083365 0, -1722610.5526441797 1241224.6314802137 0), (-1722454.2543153085 1241304.430653828 0, -1722454.2543160145 1241304.4306540184 0, -1722454.98907467 1241304.055503984 0, -1722454.2543153085 1241304.430653828 0), (-1722414.2925843324 1241324.8341496456 0, -1722400.8516707958 1241359.638348673 0, -1722378.0255372766 1241418.7451582972 0, -1722414.2925843324 1241324.8341496456 0)), ((-1726744.1875113233 1247804.5482547088 0, -1726667.2191239798 1248203.6930200334 0, -1726272.475200279 1248126.9230959278 0, -1726349.5557299664 1247727.7893932688 0, -1726744.1875113233 1247804.5482547088 0)))</t>
+          <t>MULTIPOLYGON Z (((-1720266.5560556562 1241619.4766118755 0, -1720264.2451736396 1241616.33845115 0, -1720240.328073899 1241583.8592163166 0, -1720213.1145884478 1241545.876842757 0, -1720206.239817999 1241537.1404345052 0, -1720175.7812797052 1241498.4348461167 0, -1720117.2735897598 1241413.3225018526 0, -1720074.5715069098 1241353.3557109775 0, -1720068.2504339456 1241331.347701848 0, -1720067.8685424912 1241305.5083018334 0, -1720071.2679676383 1241276.3881464894 0, -1720083.61689073 1241248.2264821115 0, -1720108.2617918705 1241219.7063913245 0, -1720130.295560692 1241202.9680343617 0, -1720197.6765641028 1241186.2199534823 0, -1720273.1628833918 1241200.430675972 0, -1720343.965099368 1241213.7592215824 0, -1720387.9010476028 1241230.3286424568 0, -1720442.8701737248 1241248.7231904976 0, -1720502.2555709393 1241270.1592070626 0, -1720569.2850051324 1241298.4448821677 0, -1720631.3635780402 1241321.509484366 0, -1720656.1041292115 1241328.8255317586 0, -1720656.1919981353 1241328.8515153455 0, -1720673.4018369738 1241333.9406108344 0, -1720751.3217416313 1241363.6157461514 0, -1720779.1239249345 1241375.9743005778 0, -1720839.6970031105 1241396.6443093063 0, -1720867.6166970753 1241403.8781641305 0, -1720909.0201827416 1241409.987069465 0, -1720971.8690523116 1241424.9817720288 0, -1721025.7679832708 1241439.018070436 0, -1721040.422373618 1241441.1608262327 0, -1721080.0024789404 1241446.948017187 0, -1721118.0598608023 1241454.3739352655 0, -1721168.6308853503 1241460.4596318211 0, -1721213.380481255 1241465.2518001262 0, -1721286.802439242 1241478.4752963868 0, -1721324.2250700656 1241479.579163603 0, -1721403.93976753 1241473.5970794298 0, -1721440.4980931187 1241473.9168606205 0, -1721481.1606803727 1241474.2725525228 0, -1721556.1418710703 1241462.0877432576 0, -1721597.1462023102 1241451.62527158 0, -1721616.9167840271 1241448.386496333 0, -1721647.8530407362 1241443.3186712575 0, -1721689.3924369845 1241435.0353536338 0, -1721730.8318611628 1241422.6091250256 0, -1721812.840776079 1241401.6841761821 0, -1721854.4980541016 1241388.276426463 0, -1721863.7109090104 1241385.9255508024 0, -1721884.7117926555 1241380.5671934842 0, -1721916.3311244752 1241371.1099750742 0, -1721970.5019116465 1241356.3617224116 0, -1722005.9024231657 1241343.6242233745 0, -1722048.7475203713 1241329.449915905 0, -1722080.1492643817 1241320.9747471123 0, -1722098.284799741 1241312.6421258582 0, -1722119.33101951 1241304.9563377919 0, -1722143.406089291 1241292.7925285716 0, -1722175.4606723138 1241281.3717397756 0, -1722216.9003799972 1241268.9456731929 0, -1722262.5322767175 1241255.7107134452 0, -1722283.2675461078 1241249.6965605556 0, -1722295.9735278878 1241247.0056232987 0, -1722299.0169854849 1241246.361047292 0, -1722252.9485856215 1241478.6413275711 0, -1722272.6254606016 1241475.3149359988 0, -1722378.0255372766 1241418.7451582972 0, -1722414.2925843324 1241324.8341496456 0, -1722454.1728438796 1241304.4086799675 0, -1722454.2543160145 1241304.4306540184 0, -1722454.98907467 1241304.055503984 0, -1722610.5526441797 1241224.6314802137 0, -1722708.167260696 1241245.7283784277 0, -1722769.9371245964 1241296.428067863 0, -1722919.9237587042 1241484.540896977 0, -1722964.7576367015 1241617.9722237035 0, -1723002.2130112445 1241712.7152698801 0, -1723009.6320559324 1241731.4823028664 0, -1723015.5545509255 1241746.463191892 0, -1723191.6603304711 1241896.8928183888 0, -1723191.2465811328 1241898.1658365303 0, -1723181.4444746135 1241928.3238711308 0, -1723169.9463166813 1241961.8260648944 0, -1723156.9700882272 1242034.1478473837 0, -1723153.6513406222 1242076.6790162898 0, -1723152.7261972136 1242108.4100066365 0, -1723152.7500927413 1242108.7320616634 0, -1723150.208765948 1242110.7701281658 0, -1723106.6430053764 1242145.714618138 0, -1723094.3103107193 1242391.8233115352 0, -1723111.9207210592 1242612.7974887264 0, -1723223.9138330873 1242782.587060279 0, -1723029.603357652 1242879.8031119374 0, -1723029.602232531 1242879.8028472173 0, -1723029.585444656 1242879.8112464237 0, -1722884.2021506082 1242845.6052545607 0, -1722884.0032644228 1242845.6278090398 0, -1722757.3192187187 1242863.5770453282 0, -1722733.3568359872 1242879.1896421772 0, -1722733.3527278912 1242879.1889246006 0, -1722733.3389890755 1242879.197876182 0, -1722559.6401527082 1243013.8007383328 0, -1722381.6339916687 1242949.53811921 0, -1722232.672660665 1242832.3087205358 0, -1722211.1041122193 1242787.965799454 0, -1721996.7433034913 1242750.5225927236 0, -1722003.6491573025 1242716.5649391306 0, -1722003.4785811466 1242716.544707561 0, -1722073.9175046657 1242361.0715618066 0, -1722080.7294661691 1242326.694809999 0, -1722153.0310744173 1241961.8344069486 0, -1721764.424998388 1241891.068965686 0, -1721366.1294605085 1241818.5546973892 0, -1720979.3183402896 1241748.1524682967 0, -1720972.6732262475 1241746.9431201753 0, -1720586.7628300434 1241676.72268317 0, -1720406.9748293536 1241642.9505246803 0, -1720355.4043134027 1241635.7290223027 0, -1720331.8072004942 1241631.964132609 0, -1720266.5560556562 1241619.4766118755 0)), ((-1726349.5557299664 1247727.7893932688 0, -1726744.1875113233 1247804.5482547088 0, -1726667.2191239798 1248203.6930200334 0, -1726272.475200279 1248126.9230959278 0, -1726349.5557299664 1247727.7893932688 0)))</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1713,22 +1713,22 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PENITENTIARY LAND FUND, NAVIGABLE STREAMBEDS, School Lands</t>
+          <t>PENITENTIARY LAND FUND, School Lands</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G27" t="n">
-        <v>536.51</v>
+        <v>367.17</v>
       </c>
       <c r="H27" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I27" t="n">
         <v>619.86</v>
@@ -1737,7 +1737,7 @@
         <v>5</v>
       </c>
       <c r="K27" t="n">
-        <v>1156.37</v>
+        <v>987.03</v>
       </c>
       <c r="L27" t="n">
         <v>52129.25</v>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1905,12 +1905,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Oklahoma State University, Common Schools, Other Agency</t>
+          <t>Common Schools, Oklahoma State University, Other Agency</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>surface, subsurface</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -2097,12 +2097,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>State Educational Institutions, Oklahoma State University, Common Schools, Public Building</t>
+          <t>Oklahoma State University, Common Schools, State Educational Institutions, Public Building</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>subsurface, surface</t>
+          <t>surface, subsurface</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, Public Building, Oklahoma State University</t>
+          <t>Common Schools, Public Building, State Educational Institutions, Oklahoma State University</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Common Schools, Greer 33, Oklahoma State University, State Educational Institutions, University Preparatory, Public Building, Normal Schools</t>
+          <t>Common Schools, Greer 33, Oklahoma State University, State Educational Institutions, University Preparatory, Normal Schools, Public Building</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>State Educational Institutions, Common Schools, Public Building, Oklahoma State University</t>
+          <t>Common Schools, State Educational Institutions, Public Building, Oklahoma State University</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), Dept. of Fish and Game, 100.00% Agricultural College, 100.00% Charitable Institute, 100.00% Normal School, 100.00% Forest Purposes (Dept. of Forestry), 100.00% University of Idaho, 100.00% Dept. of Fish and Game, 100.00% Dept. of Health and Welfare, Dept. of Health and Welfare, 100.00% General Fund, 100.00% Dept. of Transportation</t>
+          <t>Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), Dept. of Fish and Game, 100.00% Agricultural College, 100.00% Dept. of Transportation, 100.00% Charitable Institute, 100.00% Normal School, 100.00% Forest Purposes (Dept. of Forestry), 100.00% University of Idaho, 100.00% Dept. of Fish and Game, 100.00% Dept. of Health and Welfare, Dept. of Health and Welfare, 100.00% General Fund</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, STATE HOSPITAL, VALLEY/MAYVILLE, SCHOOL FOR THE DEAF, ND STATE UNIVERSITY, ND SCHOOL OF SCIENCE, VALLEY CITY, VETERANS HOME, ELLENDALE, MAYVILLE, ND INDUSTRIAL SCHOOL</t>
+          <t>COMMON SCHOOLS, BANK OFÔøΩNORTHÔøΩDAKOTA, STATE HOSPITAL, VALLEY/MAYVILLE, SCHOOL FOR THE DEAF, ND STATE UNIVERSITY, ND SCHOOL OF SCIENCE, VALLEY CITY, VETERANS HOME, ELLENDALE, MAYVILLE, ND INDUSTRIAL SCHOOL</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3570,12 +3570,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1664100.0121284036 2965338.7654427923 0, -1663999.4695497244 2965379.7210711455 0, -1664020.5066267399 2965362.712489979 0, -1664113.950854609 2965324.4462060267 0, -1664114.2313182952 2965324.367111401 0, -1664111.1788303582 2965337.0181473573 0, -1664100.0121284036 2965338.7654427923 0)), ((-1663759.0497988292 2965522.6614214736 0, -1663622.6939214163 2965600.2512186817 0, -1663556.8513078566 2965632.399373433 0, -1663422.5190301985 2965672.6931485054 0, -1663333.18452634 2965691.5473255995 0, -1663254.4814397362 2965705.207975173 0, -1663180.884130269 2965726.798973366 0, -1663098.5475386158 2965746.8080340233 0, -1663025.1290540951 2965778.7546608355 0, -1662910.0294940504 2965820.8421138846 0, -1662861.863442064 2965838.7155494974 0, -1662726.9999577163 2965903.080960916 0, -1662665.0101153927 2965935.511776588 0, -1662575.2567217865 2966011.5176111967 0, -1662512.4478622496 2966052.1918395762 0, -1662408.1118847448 2966135.649747651 0, -1662363.65538063 2966200.7205385747 0, -1662304.0634256515 2966310.2496420993 0, -1662271.6141911214 2966362.8314835713 0, -1662241.0140750348 2966400.381565996 0, -1662199.6818378742 2966427.783666996 0, -1662176.794089121 2966435.7822622946 0, -1662181.8431938915 2966418.5055073504 0, -1662198.101661121 2966396.4603498555 0, -1662243.9333120761 2966357.3526089326 0, -1662268.1700962489 2966313.6442167456 0, -1662285.0021017974 2966277.407075364 0, -1662305.1251161357 2966236.0901758783 0, -1662325.7425396738 2966197.253899609 0, -1662352.9994726032 2966155.324634322 0, -1662363.3754003395 2966123.008460601 0, -1662366.880078718 2966115.1412538616 0, -1662385.3321085796 2966073.7339914837 0, -1662487.7458373671 2966030.730320794 0, -1662607.3782301024 2965908.913562891 0, -1662683.7728323797 2965860.1873174678 0, -1662738.5967986537 2965847.0115358024 0, -1662848.444701723 2965820.6111051645 0, -1662920.3638127327 2965803.32496469 0, -1663118.9152078175 2965703.4399412116 0, -1663194.674353364 2965678.2584710866 0, -1663214.8318499771 2965671.5586890937 0, -1663244.9382030612 2965675.9393328237 0, -1663327.769285614 2965638.6939216475 0, -1663361.490036229 2965616.738735536 0, -1663448.779052874 2965591.0213082884 0, -1663559.3454429738 2965576.8887826274 0, -1663640.0752267477 2965559.5611954783 0, -1663668.2253901486 2965553.518084891 0, -1663733.629209381 2965526.790211123 0, -1663880.5534334064 2965438.480753 0, -1663934.7914855885 2965418.4107965785 0, -1663834.3151137598 2965475.6799948583 0, -1663759.0497988292 2965522.6614214736 0)))</t>
+          <t>MULTIPOLYGON Z (((-2022377.3147742988 2974403.09740933 0, -2022398.8853382058 2974428.3643118157 0, -2022403.2566114787 2974434.113991658 0, -2022459.8146360912 2974476.925170232 0, -2022528.1243986466 2974538.587445689 0, -2022570.7616208917 2974577.4052995346 0, -2022598.740046934 2974636.7288739765 0, -2022624.3954757904 2974668.8455517483 0, -2022642.159423197 2974686.1625958094 0, -2022661.7986063345 2974738.7877075644 0, -2022646.0615444065 2974734.072831868 0, -2022640.2361746407 2974732.3785090167 0, -2022541.0146529807 2974703.5213074395 0, -2022428.9010101797 2975087.7450038083 0, -2022317.5797495937 2975472.193700926 0, -2022705.9353318429 2975585.1392405904 0, -2022594.1421026664 2975969.4455484175 0, -2022538.2459337483 2976161.597220415 0, -2022531.5587934584 2976184.5858256565 0, -2022515.0642586637 2976196.192578154 0, -2022494.024224548 2976218.11697097 0, -2022471.2894866932 2976228.9769758857 0, -2022452.535970978 2976230.530991689 0, -2022444.57218863 2976231.190923296 0, -2022420.097691774 2976224.864681152 0, -2022391.3684990415 2976205.265211491 0, -2022359.0125877908 2976187.7786637316 0, -2022325.9149412876 2976173.1570239933 0, -2022305.424052827 2976157.209021562 0, -2022280.6040477366 2976146.233406032 0, -2022246.7305527579 2976146.600556096 0, -2022214.0280282483 2976138.889554426 0, -2022193.9179536647 2976127.6026913607 0, -2022167.0112498596 2976110.319150268 0, -2022166.686739932 2976109.959489474 0, -2022166.4433775912 2976109.8031345992 0, -2022161.6676595134 2976104.5096097034 0, -2022155.7066692528 2976097.9023979534 0, -2022152.5768778417 2976074.2861615894 0, -2022164.6056061774 2976043.0773203904 0, -2022166.4338388983 2976038.3341261544 0, -2022167.6291961642 2976030.9983204966 0, -2022171.6619896332 2976006.248112531 0, -2022189.103129973 2975963.6050586356 0, -2022193.317922785 2975941.746461309 0, -2022208.3439023497 2975890.1987590105 0, -2022214.4687218065 2975875.337175248 0, -2022217.8560001296 2975869.444019137 0, -2022220.067841656 2975865.5960215465 0, -2022225.2653056274 2975849.895054099 0, -2022227.2568959042 2975843.878384733 0, -2022227.8361377416 2975837.996537856 0, -2022228.090900232 2975835.4120237255 0, -2022230.1367185293 2975814.637024629 0, -2022230.437405515 2975811.583277581 0, -2022229.9383628687 2975808.0463157147 0, -2022228.186881719 2975795.6327760825 0, -2022226.630557727 2975784.6027089804 0, -2022222.8338533377 2975763.745781664 0, -2022221.7820393937 2975739.5901133073 0, -2022227.4433826033 2975714.277198129 0, -2022227.5382744677 2975712.8938861294 0, -2022228.2773114224 2975702.1134002283 0, -2022227.6682758727 2975683.7204428744 0, -2022227.5479842864 2975680.0837781127 0, -2022228.6670184748 2975660.722242781 0, -2022233.1636378197 2975645.436414047 0, -2022237.6084610915 2975639.5469321087 0, -2022241.3629065172 2975628.4190741535 0, -2022243.9756546128 2975620.6752276276 0, -2022245.344470203 2975607.106201788 0, -2022245.399538016 2975606.560500872 0, -2022251.337208646 2975583.785139515 0, -2022258.6506103938 2975555.7331480444 0, -2022259.7238880852 2975551.616281831 0, -2022260.1674704424 2975546.3667625226 0, -2022264.3897412878 2975496.4010210745 0, -2022264.8522323107 2975490.9287130837 0, -2022265.1378469565 2975480.3996026134 0, -2022265.2148387656 2975477.5584638873 0, -2022262.753693705 2975464.3869928424 0, -2022261.975174468 2975462.1571892085 0, -2022253.6741255133 2975438.382067632 0, -2022245.9969177635 2975423.714032733 0, -2022238.3045395731 2975409.0175283873 0, -2022233.7512453739 2975378.9483812936 0, -2022230.7742919622 2975337.6860042163 0, -2022230.7339592134 2975337.1255710986 0, -2022239.9725075113 2975311.041403465 0, -2022242.0776089723 2975305.0979491738 0, -2022247.2266253636 2975285.1312901364 0, -2022262.482573441 2975261.695086388 0, -2022271.3485722868 2975246.676911818 0, -2022273.3759029962 2975243.2426589644 0, -2022281.4407137067 2975232.309251684 0, -2022282.7995369395 2975230.467216447 0, -2022278.5489376185 2975221.4059525016 0, -2022325.9241348677 2975057.8080587997 0, -2022371.554730276 2975071.064272103 0, -2022430.831812876 2974867.2505894126 0, -2022037.0081873392 2974752.708780197 0, -2022042.791874227 2974735.8343377486 0, -2022053.8162527552 2974693.084078516 0, -2022060.4328703424 2974667.4229548476 0, -2022064.6362993266 2974658.7396673835 0, -2022070.2426108338 2974647.1575384904 0, -2022081.9050843397 2974625.8430966735 0, -2022087.7901909503 2974603.029487494 0, -2022091.5508123355 2974572.831553848 0, -2022091.6294089232 2974572.200420241 0, -2022093.7220584734 2974572.8193727504 0, -2022100.5278705973 2974552.2900851807 0, -2022105.5068056947 2974541.302023373 0, -2022114.3952781004 2974525.2384762783 0, -2022121.856591765 2974509.793789283 0, -2022126.8353471216 2974498.805890221 0, -2022130.2226599506 2974486.315647561 0, -2022133.3023462563 2974470.62774974 0, -2022139.3257515836 2974457.8726789197 0, -2022143.1962262644 2974452.785597163 0, -2022148.360766342 2974445.997775775 0, -2022157.163297123 2974437.1629031044 0, -2022169.653544209 2974424.2255676063 0, -2022179.5577045016 2974413.6417207117 0, -2022189.2008531357 2974401.9420306357 0, -2022199.2946997448 2974386.2290255954 0, -2022210.533066156 2974370.8522670064 0, -2022220.1118202151 2974359.1346524945 0, -2022234.1795455955 2974349.7669994617 0, -2022246.2619765159 2974342.931570014 0, -2022262.404031268 2974335.2055705567 0, -2022264.254410031 2974334.4637524188 0, -2022280.352400289 2974328.009098668 0, -2022284.2343091653 2974326.6570565957 0, -2022324.0201035729 2974360.368498534 0, -2022357.5879329306 2974397.998105058 0, -2022377.3147742988 2974403.09740933 0)), ((-2022369.149022734 2976737.60381355 0, -2022263.7087498931 2976706.9315518616 0, -2022247.6045130366 2976702.2469972926 0, -2022249.7940970312 2976700.560832485 0, -2022252.7740648177 2976698.2659858125 0, -2022286.416643166 2976675.0216021314 0, -2022301.562355381 2976654.548447446 0, -2022305.293008606 2976649.505526521 0, -2022310.9079657658 2976627.733221197 0, -2022315.2160602957 2976611.027839996 0, -2022326.3287764883 2976587.399117541 0, -2022335.6131570742 2976567.657928095 0, -2022342.975184214 2976559.2630892694 0, -2022346.5758996473 2976555.1571995807 0, -2022351.1641714869 2976549.925030061 0, -2022352.3083724244 2976548.620300016 0, -2022370.4013405244 2976527.9886640767 0, -2022370.8386288013 2976527.403275572 0, -2022392.2533842996 2976498.7409727275 0, -2022397.4547903787 2976491.7792722015 0, -2022401.3054839866 2976486.625438264 0, -2022405.6145610532 2976480.8579138587 0, -2022440.7549954513 2976467.2962173354 0, -2022459.799366124 2976462.1949356897 0, -2022463.310511482 2976461.342982718 0, -2022474.7188851128 2976458.1986767687 0, -2022475.4288295375 2976458.008532934 0, -2022479.4487442523 2976452.1791328955 0, -2022485.7654679408 2976443.0190728176 0, -2022495.0057567575 2976429.619610154 0, -2022496.4392585915 2976425.623062329 0, -2022504.2584839084 2976403.822260621 0, -2022504.435027158 2976403.330215141 0, -2022505.9848254402 2976399.0091806995 0, -2022508.5926218212 2976394.260632969 0, -2022523.749126702 2976366.6621477343 0, -2022524.3110475475 2976365.9290150274 0, -2022529.5183142074 2976367.443862561 0, -2022870.6836549435 2976466.7101995545 0, -2023263.2470127956 2976568.165741934 0, -2023356.4425675017 2976592.2577558677 0, -2023372.9688632768 2976596.529998495 0, -2023372.3954123778 2976598.597537148 0, -2023363.1576214223 2976614.941286052 0, -2023357.573726966 2976624.794501183 0, -2023343.5954985786 2976671.1902810396 0, -2023324.7134716942 2976701.3298218176 0, -2023312.4656152795 2976733.180826312 0, -2023305.4572751564 2976752.3900292832 0, -2023286.222252146 2976760.415529661 0, -2023247.4258264834 2976785.4047973403 0, -2023229.7099518962 2976818.8395379675 0, -2023219.1954653051 2976836.146255966 0, -2023229.1351348339 2976840.71049126 0, -2023241.9280489571 2976846.0149826715 0, -2023248.0413762352 2976853.6017565695 0, -2023256.5278934555 2976863.8034100262 0, -2023266.4578151198 2976876.3724273187 0, -2023266.6365611234 2976876.3195280507 0, -2023266.667075015 2976876.3581414563 0, -2023272.1113865923 2976874.750521349 0, -2023293.8056726614 2976868.441242324 0, -2023309.8369974284 2976876.5820968836 0, -2023316.9538924983 2976884.412570936 0, -2023324.5135187488 2976890.378188539 0, -2023332.5241425608 2976898.436512635 0, -2023331.9995071676 2976908.3037900864 0, -2023329.0946590507 2976919.573060433 0, -2023325.713151636 2976932.6915180916 0, -2023316.605556433 2976952.3601960205 0, -2023309.9235862116 2976962.630998978 0, -2023310.0777780223 2976977.6845188015 0, -2023310.232808064 2976992.7348027565 0, -2023303.0687048913 2977000.8863632223 0, -2023298.3382268779 2977006.51541246 0, -2023145.288401216 2976961.9757303987 0, -2022757.516656012 2976850.6045143665 0, -2022369.149022734 2976737.60381355 0)), ((-2022513.739813749 2979691.1133844736 0, -2022528.7211059663 2979695.473706297 0, -2022749.1248821886 2979759.6292808857 0, -2023137.5415768432 2979872.7173805605 0, -2023021.749361174 2980269.5700469245 0, -2022676.095311942 2980168.9349389453 0, -2022654.2867567246 2980162.586886195 0, -2022649.4325133453 2980149.50293256 0, -2022648.5387991983 2980147.0944186067 0, -2022642.9541412455 2980136.2620778615 0, -2022642.9021023149 2980136.1610140232 0, -2022633.333263999 2980106.1280230624 0, -2022614.4250224868 2980046.7817877047 0, -2022608.655689065 2980028.674036983 0, -2022594.1663848185 2979964.255827659 0, -2022581.9446664576 2979892.279614118 0, -2022576.9015259366 2979869.1831293856 0, -2022573.090168448 2979851.7283475273 0, -2022572.0010732259 2979846.74019141 0, -2022571.0515447399 2979842.4969200124 0, -2022568.4721702943 2979831.1292888937 0, -2022566.534420757 2979818.374767177 0, -2022558.7339645885 2979791.22872087 0, -2022557.253506465 2979782.547714018 0, -2022544.124024207 2979744.473334384 0, -2022533.3803877374 2979725.9931035214 0, -2022529.3608210615 2979717.916180756 0, -2022527.4640542655 2979714.104949524 0, -2022513.739813749 2979691.1133844736 0)))</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Spokane</t>
+          <t>Squaxin Island</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3585,295 +3585,295 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Common School and Indemnity</t>
+          <t>Administrative Site</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Subsurface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>277.57</v>
       </c>
       <c r="H66" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I66" t="n">
-        <v>18.84</v>
+        <v>52.27</v>
       </c>
       <c r="J66" t="n">
         <v>1</v>
       </c>
       <c r="K66" t="n">
-        <v>18.84</v>
+        <v>329.84</v>
       </c>
       <c r="L66" t="n">
-        <v>158625.43</v>
+        <v>1737.94</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-2022377.3147742988 2974403.09740933 0, -2022398.8853382058 2974428.3643118157 0, -2022403.2566114787 2974434.113991658 0, -2022459.8146360912 2974476.925170232 0, -2022528.1243986466 2974538.587445689 0, -2022570.7616208917 2974577.4052995346 0, -2022598.740046934 2974636.7288739765 0, -2022624.3954757904 2974668.8455517483 0, -2022642.159423197 2974686.1625958094 0, -2022661.7986063345 2974738.7877075644 0, -2022646.0615444065 2974734.072831868 0, -2022640.2361746407 2974732.3785090167 0, -2022541.0146529807 2974703.5213074395 0, -2022428.9010101797 2975087.7450038083 0, -2022317.5797495937 2975472.193700926 0, -2022705.9353318429 2975585.1392405904 0, -2022594.1421026664 2975969.4455484175 0, -2022538.2459337483 2976161.597220415 0, -2022531.5587934584 2976184.5858256565 0, -2022515.0642586637 2976196.192578154 0, -2022494.024224548 2976218.11697097 0, -2022471.2894866932 2976228.9769758857 0, -2022452.535970978 2976230.530991689 0, -2022444.57218863 2976231.190923296 0, -2022420.097691774 2976224.864681152 0, -2022391.3684990415 2976205.265211491 0, -2022359.0125877908 2976187.7786637316 0, -2022325.9149412876 2976173.1570239933 0, -2022305.424052827 2976157.209021562 0, -2022280.6040477366 2976146.233406032 0, -2022246.7305527579 2976146.600556096 0, -2022214.0280282483 2976138.889554426 0, -2022193.9179536647 2976127.6026913607 0, -2022167.0112498596 2976110.319150268 0, -2022166.686739932 2976109.959489474 0, -2022166.4433775912 2976109.8031345992 0, -2022161.6676595134 2976104.5096097034 0, -2022155.7066692528 2976097.9023979534 0, -2022152.5768778417 2976074.2861615894 0, -2022164.6056061774 2976043.0773203904 0, -2022166.4338388983 2976038.3341261544 0, -2022167.6291961642 2976030.9983204966 0, -2022171.6619896332 2976006.248112531 0, -2022189.103129973 2975963.6050586356 0, -2022193.317922785 2975941.746461309 0, -2022208.3439023497 2975890.1987590105 0, -2022214.4687218065 2975875.337175248 0, -2022217.8560001296 2975869.444019137 0, -2022220.067841656 2975865.5960215465 0, -2022225.2653056274 2975849.895054099 0, -2022227.2568959042 2975843.878384733 0, -2022227.8361377416 2975837.996537856 0, -2022228.090900232 2975835.4120237255 0, -2022230.1367185293 2975814.637024629 0, -2022230.437405515 2975811.583277581 0, -2022229.9383628687 2975808.0463157147 0, -2022228.186881719 2975795.6327760825 0, -2022226.630557727 2975784.6027089804 0, -2022222.8338533377 2975763.745781664 0, -2022221.7820393937 2975739.5901133073 0, -2022227.4433826033 2975714.277198129 0, -2022227.5382744677 2975712.8938861294 0, -2022228.2773114224 2975702.1134002283 0, -2022227.6682758727 2975683.7204428744 0, -2022227.5479842864 2975680.0837781127 0, -2022228.6670184748 2975660.722242781 0, -2022233.1636378197 2975645.436414047 0, -2022237.6084610915 2975639.5469321087 0, -2022241.3629065172 2975628.4190741535 0, -2022243.9756546128 2975620.6752276276 0, -2022245.344470203 2975607.106201788 0, -2022245.399538016 2975606.560500872 0, -2022251.337208646 2975583.785139515 0, -2022258.6506103938 2975555.7331480444 0, -2022259.7238880852 2975551.616281831 0, -2022260.1674704424 2975546.3667625226 0, -2022264.3897412878 2975496.4010210745 0, -2022264.8522323107 2975490.9287130837 0, -2022265.1378469565 2975480.3996026134 0, -2022265.2148387656 2975477.5584638873 0, -2022262.753693705 2975464.3869928424 0, -2022261.975174468 2975462.1571892085 0, -2022253.6741255133 2975438.382067632 0, -2022245.9969177635 2975423.714032733 0, -2022238.3045395731 2975409.0175283873 0, -2022233.7512453739 2975378.9483812936 0, -2022230.7742919622 2975337.6860042163 0, -2022230.7339592134 2975337.1255710986 0, -2022239.9725075113 2975311.041403465 0, -2022242.0776089723 2975305.0979491738 0, -2022247.2266253636 2975285.1312901364 0, -2022262.482573441 2975261.695086388 0, -2022271.3485722868 2975246.676911818 0, -2022273.3759029962 2975243.2426589644 0, -2022281.4407137067 2975232.309251684 0, -2022282.7995369395 2975230.467216447 0, -2022278.5489376185 2975221.4059525016 0, -2022325.9241348677 2975057.8080587997 0, -2022371.554730276 2975071.064272103 0, -2022430.831812876 2974867.2505894126 0, -2022037.0081873392 2974752.708780197 0, -2022042.791874227 2974735.8343377486 0, -2022053.8162527552 2974693.084078516 0, -2022060.4328703424 2974667.4229548476 0, -2022064.6362993266 2974658.7396673835 0, -2022070.2426108338 2974647.1575384904 0, -2022081.9050843397 2974625.8430966735 0, -2022087.7901909503 2974603.029487494 0, -2022091.5508123355 2974572.831553848 0, -2022091.6294089232 2974572.200420241 0, -2022093.7220584734 2974572.8193727504 0, -2022100.5278705973 2974552.2900851807 0, -2022105.5068056947 2974541.302023373 0, -2022114.3952781004 2974525.2384762783 0, -2022121.856591765 2974509.793789283 0, -2022126.8353471216 2974498.805890221 0, -2022130.2226599506 2974486.315647561 0, -2022133.3023462563 2974470.62774974 0, -2022139.3257515836 2974457.8726789197 0, -2022143.1962262644 2974452.785597163 0, -2022148.360766342 2974445.997775775 0, -2022157.163297123 2974437.1629031044 0, -2022169.653544209 2974424.2255676063 0, -2022179.5577045016 2974413.6417207117 0, -2022189.2008531357 2974401.9420306357 0, -2022199.2946997448 2974386.2290255954 0, -2022210.533066156 2974370.8522670064 0, -2022220.1118202151 2974359.1346524945 0, -2022234.1795455955 2974349.7669994617 0, -2022246.2619765159 2974342.931570014 0, -2022262.404031268 2974335.2055705567 0, -2022264.254410031 2974334.4637524188 0, -2022280.352400289 2974328.009098668 0, -2022284.2343091653 2974326.6570565957 0, -2022324.0201035729 2974360.368498534 0, -2022357.5879329306 2974397.998105058 0, -2022377.3147742988 2974403.09740933 0)), ((-2022369.149022734 2976737.60381355 0, -2022263.7087498931 2976706.9315518616 0, -2022247.6045130366 2976702.2469972926 0, -2022249.7940970312 2976700.560832485 0, -2022252.7740648177 2976698.2659858125 0, -2022286.416643166 2976675.0216021314 0, -2022301.562355381 2976654.548447446 0, -2022305.293008606 2976649.505526521 0, -2022310.9079657658 2976627.733221197 0, -2022315.2160602957 2976611.027839996 0, -2022326.3287764883 2976587.399117541 0, -2022335.6131570742 2976567.657928095 0, -2022342.975184214 2976559.2630892694 0, -2022346.5758996473 2976555.1571995807 0, -2022351.1641714869 2976549.925030061 0, -2022352.3083724244 2976548.620300016 0, -2022370.4013405244 2976527.9886640767 0, -2022370.8386288013 2976527.403275572 0, -2022392.2533842996 2976498.7409727275 0, -2022397.4547903787 2976491.7792722015 0, -2022401.3054839866 2976486.625438264 0, -2022405.6145610532 2976480.8579138587 0, -2022440.7549954513 2976467.2962173354 0, -2022459.799366124 2976462.1949356897 0, -2022463.310511482 2976461.342982718 0, -2022474.7188851128 2976458.1986767687 0, -2022475.4288295375 2976458.008532934 0, -2022479.4487442523 2976452.1791328955 0, -2022485.7654679408 2976443.0190728176 0, -2022495.0057567575 2976429.619610154 0, -2022496.4392585915 2976425.623062329 0, -2022504.2584839084 2976403.822260621 0, -2022504.435027158 2976403.330215141 0, -2022505.9848254402 2976399.0091806995 0, -2022508.5926218212 2976394.260632969 0, -2022523.749126702 2976366.6621477343 0, -2022524.3110475475 2976365.9290150274 0, -2022529.5183142074 2976367.443862561 0, -2022870.6836549435 2976466.7101995545 0, -2023263.2470127956 2976568.165741934 0, -2023356.4425675017 2976592.2577558677 0, -2023372.9688632768 2976596.529998495 0, -2023372.3954123778 2976598.597537148 0, -2023363.1576214223 2976614.941286052 0, -2023357.573726966 2976624.794501183 0, -2023343.5954985786 2976671.1902810396 0, -2023324.7134716942 2976701.3298218176 0, -2023312.4656152795 2976733.180826312 0, -2023305.4572751564 2976752.3900292832 0, -2023286.222252146 2976760.415529661 0, -2023247.4258264834 2976785.4047973403 0, -2023229.7099518962 2976818.8395379675 0, -2023219.1954653051 2976836.146255966 0, -2023229.1351348339 2976840.71049126 0, -2023241.9280489571 2976846.0149826715 0, -2023248.0413762352 2976853.6017565695 0, -2023256.5278934555 2976863.8034100262 0, -2023266.4578151198 2976876.3724273187 0, -2023266.6365611234 2976876.3195280507 0, -2023266.667075015 2976876.3581414563 0, -2023272.1113865923 2976874.750521349 0, -2023293.8056726614 2976868.441242324 0, -2023309.8369974284 2976876.5820968836 0, -2023316.9538924983 2976884.412570936 0, -2023324.5135187488 2976890.378188539 0, -2023332.5241425608 2976898.436512635 0, -2023331.9995071676 2976908.3037900864 0, -2023329.0946590507 2976919.573060433 0, -2023325.713151636 2976932.6915180916 0, -2023316.605556433 2976952.3601960205 0, -2023309.9235862116 2976962.630998978 0, -2023310.0777780223 2976977.6845188015 0, -2023310.232808064 2976992.7348027565 0, -2023303.0687048913 2977000.8863632223 0, -2023298.3382268779 2977006.51541246 0, -2023145.288401216 2976961.9757303987 0, -2022757.516656012 2976850.6045143665 0, -2022369.149022734 2976737.60381355 0)), ((-2022513.739813749 2979691.1133844736 0, -2022528.7211059663 2979695.473706297 0, -2022749.1248821886 2979759.6292808857 0, -2023137.5415768432 2979872.7173805605 0, -2023021.749361174 2980269.5700469245 0, -2022676.095311942 2980168.9349389453 0, -2022654.2867567246 2980162.586886195 0, -2022649.4325133453 2980149.50293256 0, -2022648.5387991983 2980147.0944186067 0, -2022642.9541412455 2980136.2620778615 0, -2022642.9021023149 2980136.1610140232 0, -2022633.333263999 2980106.1280230624 0, -2022614.4250224868 2980046.7817877047 0, -2022608.655689065 2980028.674036983 0, -2022594.1663848185 2979964.255827659 0, -2022581.9446664576 2979892.279614118 0, -2022576.9015259366 2979869.1831293856 0, -2022573.090168448 2979851.7283475273 0, -2022572.0010732259 2979846.74019141 0, -2022571.0515447399 2979842.4969200124 0, -2022568.4721702943 2979831.1292888937 0, -2022566.534420757 2979818.374767177 0, -2022558.7339645885 2979791.22872087 0, -2022557.253506465 2979782.547714018 0, -2022544.124024207 2979744.473334384 0, -2022533.3803877374 2979725.9931035214 0, -2022529.3608210615 2979717.916180756 0, -2022527.4640542655 2979714.104949524 0, -2022513.739813749 2979691.1133844736 0)))</t>
+          <t>MULTIPOLYGON Z (((-449556.5059218632 2511728.520408616 0, -449176.91746688675 2511705.777670777 0, -449176.1984435866 2511705.733216676 0, -449556.5059218632 2511728.520408616 0)), ((-449982.1299062058 2511754.164890567 0, -449982.1297245475 2511754.167914157 0, -449699.5578025382 2511737.097241653 0, -449982.1299062058 2511754.164890567 0)), ((-449579.1105100217 2511729.8748406926 0, -449579.1429920948 2511729.876786715 0, -449692.63074373675 2511736.678877075 0, -449982.1297245472 2511754.1679141615 0, -449971.4739245098 2511931.527108429 0, -449568.3538073889 2511907.2960243486 0, -449165.2529589046 2511883.0840977235 0, -448762.17476517527 2511858.894686667 0, -448773.2079271766 2511681.583054768 0, -448773.2382601551 2511681.584876002 0, -448871.2507424927 2511687.473799343 0, -448888.1109399908 2511688.486912748 0, -448915.0532655619 2511690.1000152635 0, -449176.12641623017 2511705.7317984854 0, -449176.1676868195 2511705.7342695664 0, -449579.1105100217 2511729.8748406926 0)), ((-463366.30178307346 2512582.8016465153 0, -463334.87706382683 2512580.856246914 0, -463366.30178338743 2512582.8016431336 0, -463405.7509150512 2512585.2358416286 0, -463366.30178307346 2512582.8016465153 0)), ((-464064.27364119334 2512625.8867090484 0, -464170.7422980627 2512632.464345802 0, -464213.54977654974 2512635.13402016 0, -464170.7422882964 2512632.464375655 0, -464064.27364119334 2512625.8867090484 0)), ((-464417.0083980226 2512647.8287448124 0, -464406.96939841536 2512813.1866125953 0, -464005.15649598924 2512788.596259246 0, -463603.3422352082 2512764.027462437 0, -463201.52449667803 2512739.4803704 0, -463211.49494368176 2512573.224213664 0, -463211.5253091886 2512573.226092752 0, -463366.310057336 2512582.8084000037 0, -463613.2370556818 2512598.044970272 0, -463613.2761352741 2512598.047381669 0, -464015.0843742729 2512622.853928947 0, -464015.1124974243 2512622.855665194 0, -464170.7614092613 2512632.4718089625 0, -464417.0083980226 2512647.8287448124 0)), ((-456264.384418507 2513913.2817409043 0, -456311.65716874925 2513126.286220331 0, -456360.0020620866 2512321.4405879593 0, -456361.8088236175 2512291.361745473 0, -457984.09614303196 2512406.6756496173 0, -457932.25081506104 2513225.965336516 0, -457932.2506155181 2513225.9674284193 0, -457893.0983433012 2513844.675265713 0, -457892.23051078035 2513858.3893516134 0, -457891.59300734167 2513868.4635157497 0, -457890.3708778595 2513887.7760617123 0, -457882.31282094686 2514015.1139713754 0, -457881.30541144765 2514015.05057021 0, -456264.384418507 2513913.2817409043 0)), ((-451282.77213509835 2516843.573187387 0, -452881.1286204372 2516941.3567562765 0, -452788.16282210994 2518541.180243185 0, -451193.0181150282 2518454.0908873766 0, -451282.77213509835 2516843.573187387 0)), ((-447775.73130676866 2521466.171663356 0, -447680.4446375186 2523083.00645899 0, -446062.53746012686 2522978.478549137 0, -446149.0682687236 2521383.5954063167 0, -447775.73130676866 2521466.171663356 0)), ((-452263.06508488936 2527420.0165616595 0, -452262.9989986145 2527421.1705014743 0, -452217.3678488886 2528216.499118979 0, -451389.4571952081 2528170.4905104106 0, -451429.1165415427 2527389.9752738457 0, -451432.0658116872 2527378.173895968 0, -451432.0927535317 2527378.066065934 0, -450674.31094751746 2527334.2312229117 0, -450659.6225222654 2527333.820585373 0, -450659.6496749159 2527333.383858899 0, -450711.31631975883 2526504.3601864562 0, -451480.4558586479 2526550.4099000636 0, -451434.6292940259 2527362.1247527148 0, -451433.9890512456 2527378.2706318754 0, -452231.5475172021 2527418.4299013275 0, -452252.6274551624 2527419.4912691237 0, -452263.06508488936 2527420.0165616595 0)), ((-455166.42114959256 2531660.3247363223 0, -455167.23062476097 2531647.0039018453 0, -456801.4756868293 2531730.9629927757 0, -456691.7622620359 2533334.4222966707 0, -455069.8573224605 2533249.725257102 0, -455166.42114959256 2531660.3247363223 0)), ((-451735.24512163736 2536243.317183069 0, -451645.78562387795 2537864.519470849 0, -450021.007770592 2537765.742848979 0, -450116.09840936464 2536144.5834728894 0, -451735.24512163736 2536243.317183069 0)), ((-461322.1501446945 2536845.070964317 0, -461266.4029524177 2537687.653727615 0, -459665.6639103949 2537608.6670449553 0, -459715.99443711824 2536748.6248253267 0, -461322.1501446945 2536845.070964317 0)), ((-454890.8922974969 2542698.1855162326 0, -453281.3780819311 2542600.764220469 0, -453384.07991065923 2540985.658445156 0, -454594.304251081 2541056.715851151 0, -454988.15293683077 2541080.9520675344 0, -454890.8922974969 2542698.1855162326 0)), ((-459524.2299986185 2546204.2215727074 0, -459429.9975628155 2547813.2614215584 0, -457816.4177064228 2547702.894510099 0, -457894.3280349991 2546101.495725701 0, -459524.2299986185 2546204.2215727074 0)), ((-447333.0196933869 2547058.820925809 0, -447227.8717313179 2548665.936131774 0, -446452.08490666316 2548619.788373531 0, -445623.684550666 2548570.683982875 0, -445713.3941800438 2546965.148014899 0, -446547.97513063496 2547014.6210594294 0, -447333.0196933869 2547058.820925809 0)), ((-455693.08488767454 2555626.9297070154 0, -456468.00679758465 2555674.8984094583 0, -456416.7449249867 2556489.9031604244 0, -454802.76577117445 2556376.1514217234 0, -454885.3564354707 2554791.20763069 0, -455740.92444017367 2554843.778459255 0, -455693.08488767454 2555626.9297070154 0)), ((-449276.9794248514 2555236.611581465 0, -449203.3707008164 2556834.7579691587 0, -447593.3605284898 2556738.3556973888 0, -447672.70063963823 2555137.8819685206 0, -449276.9794248514 2555236.611581465 0)), ((-458875.0183390479 2556662.9690301814 0, -458828.2093868158 2557424.049423567 0, -457185.61157180124 2557335.725614214 0, -457303.25758220925 2555726.584222721 0, -458131.4758505402 2555781.6832451886 0, -458083.5253769855 2556616.3136012475 0, -458875.0183390479 2556662.9690301814 0)), ((-452186.6040555831 2560226.9235749864 0, -453804.62321116845 2560336.180691955 0, -453698.7256673469 2561920.4906114456 0, -452074.04850345897 2561828.9798595035 0, -452186.6040555831 2560226.9235749864 0)), ((-449321.9326013234 2564376.2574031744 0, -449321.3769063425 2564386.1416202285 0, -449276.9198393965 2565177.0558428974 0, -449231.9133044314 2565977.837736146 0, -449231.53414914093 2565984.0533565343 0, -449183.4894144431 2566771.4791362807 0, -449182.9648853079 2566780.0764241694 0, -448373.3310903083 2566731.304009236 0, -447563.6950838357 2566682.5144151314 0, -447514.66624011385 2567489.021035307 0, -446705.1953842786 2567440.7313964185 0, -445988.7150911759 2567397.976206695 0, -445909.0247302735 2567388.175121057 0, -445895.8781619955 2567386.558528588 0, -445895.92348154745 2567385.746683493 0, -445895.1590514922 2567385.67234871 0, -445940.1287341057 2566574.7250591344 0, -445941.19318906 2566574.7945829183 0, -445986.07918338495 2565770.789100794 0, -445986.3991030491 2565765.046846068 0, -446034.2458411558 2564974.470302698 0, -446081.848022635 2564187.9879047014 0, -446082.0960329981 2564183.877433263 0, -446175.0936994005 2564189.500664745 0, -446181.23518354836 2564189.8143169554 0, -446892.4000848265 2564226.1902014404 0, -447120.5724311692 2564237.8580566742 0, -447702.7252258939 2564267.693862222 0, -448512.33092102065 2564321.9463786385 0, -448743.30342503305 2564337.4211003976 0, -449321.9326013234 2564376.2574031744 0), (-448467.324070914 2565124.4624965163 0, -447657.7244795784 2565071.8508929783 0, -447612.77113378036 2565875.227558959 0, -448421.53377836954 2565926.115988229 0, -448422.3650867946 2565926.1683864985 0, -448467.324070914 2565124.4624965163 0)), ((-450872.6268687303 2565283.478366009 0, -451680.51605147077 2565331.9210636 0, -451633.04154613346 2566137.5807718737 0, -450834.4153565486 2566092.4419257008 0, -450827.00930416514 2566092.0250950083 0, -450029.46244642325 2566034.939160159 0, -450074.7745231379 2565230.2747832444 0, -450872.6268687303 2565283.478366009 0)), ((-465522.480087164 2566211.0676372 0, -465497.99191343173 2566611.630241336 0, -465480.8451485192 2566892.1531603415 0, -465473.2948586149 2567012.1479260344 0, -465472.71796541277 2567021.4207174475 0, -465472.031586073 2567021.3812373984 0, -465455.0418494883 2567019.6596213793 0, -465448.99211219745 2567018.280112106 0, -465327.7137608106 2567003.131225467 0, -465322.185706256 2567002.8163942015 0, -465347.6779609036 2566601.412719703 0, -465373.0994776094 2566201.1579084056 0, -465398.521134454 2565800.89875415 0, -465423.9451466621 2565400.6366323116 0, -465547.5166171904 2565407.1564568747 0, -465555.2558658541 2565407.657327017 0, -465571.7365829466 2565408.7253705617 0, -465571.6657606916 2565409.8448486715 0, -465547.05419117556 2565810.4818696138 0, -465529.667752618 2566093.4945963905 0, -465522.4895103514 2566210.9134963593 0, -465522.480087164 2566211.0676372 0)), ((-454811.31346071255 2567141.109477066 0, -454855.6294871319 2566337.2350389366 0, -455258.11700768187 2566364.1809276436 0, -455653.93637284345 2566390.676939578 0, -455629.05221015995 2566792.4430512516 0, -455604.16928405856 2567194.205680881 0, -455213.8082963064 2567168.0663915016 0, -454811.31346071255 2567141.109477066 0)), ((-445778.7935746923 2569395.246043825 0, -445773.73187626095 2569498.2577245524 0, -445759.094738161 2569796.1996818786 0, -445369.4413924876 2569772.410528177 0, -445389.7841105851 2569371.470383204 0, -445410.09594294924 2568971.0564951664 0, -445434.51985076955 2568565.8250266635 0, -445458.6746454063 2568165.0839533997 0, -445056.3294193455 2568141.3206398026 0, -444251.63915332005 2568093.7813247424 0, -444299.9785089062 2567292.2843639296 0, -444310.1872706344 2567292.8866332476 0, -445104.64999606746 2567339.8260526597 0, -445506.98577934084 2567363.5917561376 0, -445895.8781619955 2567386.558528588 0, -445895.60333543544 2567391.0871763406 0, -445871.601985927 2567787.2991851103 0, -445847.3282120576 2568188.0355825336 0, -445823.0542726236 2568588.767889601 0, -445798.49213708605 2568994.28689127 0, -445778.7935746923 2569395.246043825 0)), ((-452174.19734232465 2570747.6675056093 0, -452158.0453145773 2571009.3110569436 0, -452157.64718833106 2571015.7608968886 0, -452151.9472461596 2571015.3874891964 0, -451348.75422009744 2570962.814505742 0, -450539.8587676992 2570909.8519592355 0, -450539.9091747104 2570909.024648134 0, -450539.06196779094 2570908.9691903675 0, -450555.61941961234 2570638.495888727 0, -450588.6149749233 2570099.6443992187 0, -450638.17361392797 2569290.297443804 0, -451439.8572009743 2569341.5330177248 0, -452240.91873932607 2569393.2423031386 0, -452240.88616896205 2569393.897006181 0, -452241.76140384376 2569393.953099999 0, -452241.56006396015 2569397.991822121 0, -452205.9345710624 2570111.7782752165 0, -452201.2866546269 2570204.9095945144 0, -452174.19734232465 2570747.6675056093 0)), ((-446568.4550681967 2573951.0915424577 0, -446563.80971174856 2573952.8998985905 0, -446551.8514681421 2573957.555033972 0, -446562.6124286463 2574012.59082663 0, -446565.37551279727 2574026.7223278442 0, -446568.97758666135 2574056.646631005 0, -446625.42937589827 2574067.665254358 0, -446638.2313802044 2574070.1640319084 0, -446697.67873640795 2574081.922251191 0, -446707.6876513473 2574086.7241391297 0, -446714.6893999777 2574091.4392362507 0, -446716.8276809053 2574092.4650806137 0, -446750.1683095114 2574108.4603109276 0, -446784.95938356454 2574131.8839738998 0, -446799.36959451943 2574158.3019924304 0, -446819.34315285203 2574195.813044364 0, -446833.7530955948 2574222.231089865 0, -446853.72635455267 2574259.7421824727 0, -446874.3846494828 2574297.616373964 0, -446900.8587341657 2574347.339388282 0, -446928.68623211666 2574398.3597569247 0, -446916.27634527377 2574427.995409388 0, -446907.2980127922 2574445.9841933427 0, -446885.66267165233 2574454.170303028 0, -446834.9857463377 2574446.780569181 0, -446745.2809730728 2574432.206206241 0, -446694.603883932 2574424.817553702 0, -446676.48620318633 2574422.176331941 0, -446627.87300325214 2574414.278510132 0, -446550.6406528148 2574391.6491387743 0, -446512.7847795553 2574378.09854516 0, -446492.80560379615 2574375.8343219236 0, -446478.4234633957 2574385.0732659595 0, -446431.1496324344 2574422.694776051 0, -446424.6298018589 2574452.140482353 0, -446398.94756617106 2574502.136867927 0, -446340.09982323315 2574560.1016085385 0, -446285.99670345377 2574613.831450595 0, -446278.6087352978 2574624.503452922 0, -446269.89767463866 2574633.0836661397 0, -446270.9608647694 2574615.557296495 0, -446225.9212432688 2574655.5221559913 0, -446214.9682569618 2574654.8433415717 0, -446178.5546935751 2574652.586824033 0, -446178.5546134259 2574652.5869199685 0, -446214.9682506757 2574654.8434831738 0, -446129.2512760676 2574796.1515730764 0, -445989.49300173635 2574948.5913481 0, -445996.2009790698 2575103.6458547325 0, -445956.77361182624 2575108.6720762732 0, -445946.49791766756 2575087.257677356 0, -445921.36968522216 2575044.6333539444 0, -445918.79881303036 2575039.2751104087 0, -445918.79881303024 2575039.2751104087 0, -445905.6137503262 2575011.7946400736 0, -445900.1632744067 2575002.5494192936 0, -445902.4074946497 2574952.3947126777 0, -445899.913273229 2574882.311590769 0, -445893.9836602633 2574842.597457956 0, -445921.7162698178 2574762.8310657055 0, -445951.94644323573 2574667.3735025837 0, -445955.66247839987 2574646.365390554 0, -445954.72250468645 2574644.1635208954 0, -445955.03065915284 2574642.424815998 0, -445953.41247410345 2574638.634799117 0, -445953.4124741035 2574638.634799117 0, -445953.2656972692 2574638.291027136 0, -445953.02043969627 2574637.7165994206 0, -445936.2766363764 2574598.500258093 0, -445928.21034849255 2574575.791354023 0, -445908.6259245545 2574580.4970363365 0, -445891.66946380393 2574593.49464247 0, -445890.2791959668 2574594.560322038 0, -445888.3325162854 2574592.4428514666 0, -445885.50121547433 2574589.363148009 0, -445877.02642133815 2574586.2225874905 0, -445869.65367432754 2574578.2032980197 0, -445868.20082048024 2574576.6230382407 0, -445832.2017305108 2574558.7271710527 0, -445811.4678179631 2574551.0448905793 0, -445774.65136369405 2574537.403744603 0, -445745.5449259613 2574545.3380191578 0, -445743.1645129254 2574546.6865430293 0, -445728.65320356743 2574554.9073210126 0, -445714.51598370774 2574556.52835275 0, -445701.8415694503 2574561.9725715136 0, -445672.98795473785 2574577.9486203967 0, -445652.36112494336 2574615.369621159 0, -445652.260662085 2574615.731640977 0, -445652.0424214849 2574619.333129469 0, -445649.4273990284 2574642.926399384 0, -445647.22935103806 2574698.7794549344 0, -445639.20174341806 2574743.2514613876 0, -445633.4301780968 2574770.0468409318 0, -445626.06384222314 2574774.265435439 0, -445592.0640389263 2574856.1849386683 0, -445569.7662060519 2574911.243892445 0, -445526.85662866797 2574973.9616541793 0, -445505.57474210643 2574986.4271483268 0, -445481.991395397 2574956.311744628 0, -445476.69957869616 2574906.4662741185 0, -445487.9087582305 2574737.260160259 0, -445498.52683381917 2574616.327599229 0, -445498.53442332573 2574616.221544097 0, -445501.02662029344 2574587.838077341 0, -445510.24065185885 2574387.289699773 0, -445516.91910214105 2574278.4432967617 0, -445520.0287879152 2574227.7611629264 0, -445517.53163593437 2574219.3884955756 0, -445516.21309944324 2574214.9675922766 0, -445516.5630488973 2574207.345973943 0, -445516.6752975337 2574204.901288703 0, -445517.0419461239 2574196.915976583 0, -445500.2378451389 2574140.565765194 0, -445494.8548661272 2574122.6799496817 0, -445501.4186812127 2574014.291503234 0, -445516.84541118756 2574004.198597328 0, -445520.0187222175 2574001.5507348306 0, -445560.83336123556 2574017.4222854553 0, -445611.71132416325 2574025.983912797 0, -445663.6098651552 2574046.166564549 0, -445717.5229416513 2574074.1731103915 0, -445740.52318680566 2574090.552032075 0, -445788.76768398494 2574105.7643663273 0, -445828.7094112431 2574111.4429495097 0, -445875.0752445116 2574100.4918937637 0, -445907.2044888619 2574087.663616673 0, -445915.7437630923 2574085.646486602 0, -445919.85222520004 2574084.6759940004 0, -445939.10924534505 2574076.9884381196 0, -445974.8398783625 2574041.5776248965 0, -445999.37579975557 2574002.5589720556 0, -446024.2769612919 2573936.963886998 0, -446042.07678360125 2573881.76528192 0, -446077.3297600856 2573883.9010345708 0, -446093.9672806464 2573885.830022005 0, -446114.94519567984 2573904.7156140115 0, -446159.9014939694 2573915.924581668 0, -446184.9065645396 2573904.292101264 0, -446199.68989141687 2573884.237382285 0, -446200.28617193596 2573883.880797301 0, -446229.0963397115 2573855.7850391716 0, -446227.3448786952 2573844.1857780414 0, -446318.58519534994 2573850.050926444 0, -446698.1780046639 2573874.784120618 0, -446710.4334241953 2573875.528157732 0, -446694.3859729308 2573884.075065285 0, -446681.81349965365 2573910.118912809 0, -446678.2952695306 2573924.7751732552 0, -446628.48430492333 2573944.1648235247 0, -446568.4550681967 2573951.0915424577 0), (-446624.1749220042 2574068.462996698 0, -446624.17492200434 2574068.462996698 0, -446625.42937589827 2574067.665254358 0, -446624.1749220042 2574068.462996698 0)), ((-446950.56243684096 2574198.6320379856 0, -446932.30556629575 2574201.385897007 0, -446908.93935471226 2574176.457900518 0, -446883.80138547975 2574111.1742358143 0, -446863.6045996117 2574054.5049641044 0, -446875.42459873157 2574008.8867512974 0, -446882.9000154899 2573959.3910239553 0, -446876.09148893814 2573931.137323962 0, -446865.8438236706 2573894.418725824 0, -446864.12461474177 2573885.3509173403 0, -447124.44490654866 2573901.9489376843 0, -447108.22404811066 2574142.9668562766 0, -447101.39372117515 2574133.4359606504 0, -447087.50028866966 2574121.831196952 0, -447052.32130097033 2574102.4577116594 0, -447050.1481298079 2574105.75212045 0, -447024.6023644447 2574144.478105517 0, -446997.2296424889 2574184.283265825 0, -446962.1561278046 2574196.8832502966 0, -446950.56243684096 2574198.6320379856 0)), ((-456765.9186664952 2574520.703219268 0, -456766.7534668326 2574520.7562253936 0, -456775.8150063362 2574523.8307035593 0, -456936.0986376184 2574533.4261585367 0, -457573.4196303584 2574571.6560989986 0, -457521.005743965 2575367.450410148 0, -456717.4002130627 2575315.5125296665 0, -456668.05145486625 2576110.2522586337 0, -455863.1617071876 2576062.149205341 0, -455177.45231584826 2576021.155547476 0, -455166.6825075448 2576020.512744768 0, -455069.6986429143 2576016.5006078887 0, -455058.21920649987 2576016.0251637846 0, -455058.282165094 2576015.0817748327 0, -455057.69480324606 2576015.0569460415 0, -455110.6791901181 2575216.2349368795 0, -455164.28176372364 2574417.0104392366 0, -455264.5815672489 2574424.4891094393 0, -455964.7872605663 2574469.126197598 0, -456765.98251743335 2574519.674981475 0, -456765.9186664952 2574520.703219268 0)), ((-463196.45121227956 2574941.5765004004 0, -463993.9246552496 2574981.302344243 0, -463943.32446898887 2575784.3832184738 0, -463918.20070562203 2576183.702619917 0, -463515.8089860782 2576161.4178912505 0, -463113.41681594384 2576139.127593277 0, -463138.301791416 2575744.2873498304 0, -463188.9192366038 2574941.2019163715 0, -463196.45121227956 2574941.5765004004 0)), ((-464937.096481809 2575700.087033282 0, -464928.5530128695 2575837.0287334695 0, -464928.4526466002 2575838.6375712072 0, -464903.51949927624 2576238.3075860483 0, -464887.08327462705 2576501.797045511 0, -464878.39700935816 2576639.4931003833 0, -464878.3431484534 2576640.3824573625 0, -464854.09094255016 2577040.837456766 0, -464838.217164771 2577302.9332062737 0, -464837.0562252017 2577321.3652535304 0, -464811.8891829471 2577321.085257435 0, -464766.82649088395 2577326.1103489115 0, -464755.40941543435 2577334.3433872107 0, -464751.2037088808 2577359.1004940905 0, -464759.70275551005 2577386.9586737705 0, -464773.0340297169 2577424.741107386 0, -464773.0771431283 2577424.862592797 0, -464797.1731942942 2577443.0502988207 0, -464807.56328525895 2577449.673206065 0, -464631.53984982223 2577438.589641639 0, -464631.22398814623 2577443.587782681 0, -464615.29167337413 2577428.4568144553 0, -464576.0646172975 2577397.1888157343 0, -464555.57479544706 2577395.889665911 0, -464524.6199792611 2577422.7116912534 0, -464521.4497953473 2577428.27365366 0, -464514.44614257413 2577434.342532914 0, -464538.9968471909 2577466.3124745665 0, -464562.72751803906 2577493.638865401 0, -464526.389179808 2577549.1250518817 0, -464489.11652091594 2577608.7374029653 0, -464493.6713408025 2577648.7011961546 0, -464492.8433140445 2577702.9044545596 0, -464466.4027872354 2577738.3557627415 0, -464434.40197506174 2577777.065497327 0, -464404.812810613 2577792.169803099 0, -464367.66847528773 2577768.015404443 0, -464342.6809768903 2577724.557705723 0, -464320.66599687096 2577656.6760155717 0, -464295.86255039327 2577601.907708306 0, -464288.0941342627 2577538.082097315 0, -464279.9377086015 2577478.5007729246 0, -464277.9064324353 2577476.794150505 0, -464263.9071737847 2577468.5325357565 0, -464251.9463057986 2577461.4747319506 0, -464249.95473392593 2577459.802275873 0, -464252.5510622925 2577411.0551478895 0, -464218.8431551951 2577409.000187979 0, -464217.78651525057 2577403.2725574877 0, -464209.7549571784 2577359.7271024147 0, -464195.2587707094 2577293.1045055306 0, -464178.698804382 2577281.7068156367 0, -464157.41678466497 2577254.934471376 0, -464186.321640588 2577191.928404721 0, -464222.5097901601 2577143.6309508733 0, -464245.2014497252 2577135.336637269 0, -464265.2189677541 2577140.263590601 0, -464282.6754837639 2577146.4746682304 0, -464287.1030315777 2577147.5649162563 0, -464339.485003487 2577170.942280084 0, -464407.87672958424 2577195.2783001685 0, -464437.7845460607 2577169.9045328535 0, -464483.4159654913 2577116.2338393074 0, -464472.1172339116 2577093.786866766 0, -464437.68294838996 2577057.412049867 0, -464379.71507526276 2577045.2505906043 0, -464319.596377357 2577041.5133966543 0, -464304.40058103704 2577038.3254989535 0, -464297.3545622659 2577028.7823426677 0, -464292.58365757955 2577027.781605413 0, -464289.8096475747 2577024.0247067767 0, -464285.33380089165 2577017.9630467445 0, -464273.68084539607 2577004.189537191 0, -464270.3910880498 2577000.300997528 0, -464266.8004785266 2576995.4363722466 0, -464266.3839822324 2576989.7298110127 0, -464263.14104009303 2576945.3432460255 0, -464255.0198022468 2576895.8779241713 0, -464202.66684775567 2576866.1941167354 0, -464150.96786590706 2576841.200656919 0, -464139.86460662744 2576818.6582911205 0, -464143.9829531782 2576776.6761341197 0, -464142.85249968857 2576726.547589812 0, -464063.6891408286 2576739.7425603513 0, -464014.29669513635 2576749.639661372 0, -463980.3430621567 2576791.996073437 0, -463954.05614179204 2576834.7944496544 0, -463923.30624551146 2576847.566879482 0, -463896.46524345636 2576855.4663607837 0, -463895.59889163164 2576855.8271351433 0, -463883.87232823035 2576859.2774244836 0, -463878.37832621014 2576858.9286823734 0, -463893.0778399444 2576583.0167188225 0, -464295.34907332796 2576607.53743321 0, -464682.56904175243 2576631.13727435 0, -464708.0847137635 2576227.6658522277 0, -464733.5301654517 2575825.334955942 0, -464758.9758257566 2575423.0014905534 0, -464784.4225472731 2575020.6622311734 0, -464794.4157079474 2575021.2268428295 0, -464939.18487480434 2575029.3975207983 0, -464943.71482660837 2575029.707692358 0, -464968.10114058503 2575031.379352574 0, -464978.86292046105 2575032.1186184734 0, -464978.72881342913 2575034.2467949837 0, -464953.62894154043 2575435.655953842 0, -464937.096481809 2575700.087033282 0)), ((-427122.3892649302 2510406.657618777 0, -427121.6073993937 2510406.6083721723 0, -427121.607303883 2510406.6083661583 0, -427121.6074740782 2510406.605239546 0, -427167.29207266384 2510409.4846520214 0, -427477.69133642956 2510424.482990813 0, -427167.2701634584 2510409.4864873113 0, -427167.2702126657 2510409.4864904126 0, -427489.66749348 2510425.061672794 0, -427498.2846000709 2510425.4780471195 0, -427488.6248352047 2510591.0338693755 0, -427112.8165501257 2510568.101098727 0, -427121.60730386025 2510406.608366577 0, -427121.6073213328 2510406.6083676773 0, -427166.7266011812 2510409.4522266914 0, -427122.3892649302 2510406.657618777 0)), ((-428302.7533831593 2510471.4720921647 0, -428293.5116595257 2510636.594242328 0, -427891.0689813323 2510613.801533897 0, -427900.51612006954 2510448.505709506 0, -427970.68001723074 2510452.5260432283 0, -428122.4389314934 2510461.1831019046 0, -427970.98125386966 2510452.5432437616 0, -428302.7533831593 2510471.4720921647 0)), ((-436346.10551138024 2510938.2014115276 0, -436346.1054094166 2510938.2014054214 0, -436260.8903451971 2510933.1025654385 0, -436346.10551316146 2510938.2013793173 0, -436423.0556714865 2510942.8094952027 0, -436346.10551138024 2510938.2014115276 0)), ((-436337.2115463037 2511099.0301875575 0, -435935.1878377702 2511076.165228918 0, -435944.2682461471 2510914.196872157 0, -435944.2725795822 2510914.197129352 0, -436019.43084083596 2510918.661083573 0, -436346.10516805894 2510938.2076197756 0, -436346.11167875346 2510938.2080093427 0, -436747.7785271353 2510962.2613196066 0, -436739.00722823804 2511122.113856621 0, -436337.2115463037 2511099.0301875575 0)), ((-437945.4633888475 2511032.4974911553 0, -438344.8769819778 2511055.7122348617 0, -438349.1716061985 2511055.9619939644 0, -438344.8769817122 2511055.7122394843 0, -438344.8769694131 2511055.712238769 0, -438191.29134578933 2511046.785974206 0, -437945.4633888475 2511032.4974911553 0)), ((-437630.8053028015 2511014.228836478 0, -437942.78666180244 2511032.348041177 0, -437942.7952988941 2511032.3485428006 0, -438344.87663705077 2511055.7182380296 0, -438344.88317202893 2511055.718617854 0, -438436.5255207326 2511061.0482047983 0, -438746.92438312696 2511079.2904069447 0, -438737.5692713429 2511244.521314349 0, -438708.09146898845 2511242.686678195 0, -438641.12810462905 2512855.2839119053 0, -437042.0496653505 2512760.871550386 0, -437136.1836475484 2511123.4523978126 0, -437532.35598531854 2511150.7005817727 0, -437540.67339390906 2511008.9642607914 0, -437540.6777409151 2511008.9645145955 0, -437630.8053028015 2511014.228836478 0)), ((-439149.5913135798 2511103.3541215407 0, -439240.6048005137 2511108.795627342 0, -439552.2067859431 2511127.554180531 0, -439542.82905383897 2511293.0435698433 0, -439140.2008863796 2511268.771542087 0, -439149.5827539224 2511103.3536100066 0, -439149.5913135798 2511103.3541215407 0)), ((-423511.58733838267 2516795.860697203 0, -422312.76373192994 2516733.418483321 0, -422399.4995318504 2515128.1689220434 0, -423623.10174627777 2515195.7103881766 0, -423511.58733838267 2516795.860697203 0)), ((-438174.3331115907 2520886.8578333333 0, -438089.92187792825 2522475.263604186 0, -436474.0111356682 2522378.049033309 0, -436554.3347478653 2520770.822675446 0, -438174.3331115907 2520886.8578333333 0)), ((-440538.10997213115 2535562.1979440977 0, -442145.8851937264 2535670.1549665434 0, -442052.1990970533 2537276.149583939 0, -440436.57473123574 2537166.2334500076 0, -440538.10997213115 2535562.1979440977 0)), ((-424433.8221215985 2539272.0517960135 0, -425858.80544495455 2539354.321771957 0, -426042.7076174558 2539364.6214590515 0, -426000.3251043954 2540171.698450297 0, -425198.13020345493 2540124.357719958 0, -425150.7232410197 2540931.3059425913 0, -424356.8655591133 2540880.5860454924 0, -424433.8221215985 2539272.0517960135 0)), ((-433980.2747087349 2541443.587525573 0, -434077.9976433319 2539841.0195716564 0, -435422.07180602156 2539922.21452343 0, -435687.8193028673 2539937.8840412805 0, -435593.98831040267 2541548.741150996 0, -433980.2747087349 2541443.587525573 0)), ((-445221.8758211143 2542116.0473940196 0, -443609.36413693096 2542010.643948824 0, -443724.2559185373 2540414.178490147 0, -445011.4045750646 2540492.212708913 0, -445334.0316658631 2540511.656936364 0, -445221.8758211143 2542116.0473940196 0)), ((-430483.81379599456 2546068.489295747 0, -428876.86678534385 2545986.869770583 0, -428974.21988311847 2544373.2443760615 0, -429761.11130427127 2544419.7909906157 0, -429739.05529994343 2544779.528298907 0, -430564.12083383923 2544832.9640669976 0, -430483.81379599456 2546068.489295747 0)), ((-425480.6400727827 2548986.52706754 0, -425430.6969382982 2549800.222580658 0, -424598.9474573648 2549755.82807769 0, -424553.6953297701 2550538.651272534 0, -423775.02667608345 2550490.661146024 0, -423859.93340171734 2548888.2040763283 0, -425480.6400727827 2548986.52706754 0)), ((-434275.08783599635 2550281.136577314 0, -435080.07863136154 2550321.9912387785 0, -435056.20641513256 2550737.4739556466 0, -434250.58380005235 2550688.787143192 0, -434275.08783599635 2550281.136577314 0)), ((-444743.72609288245 2550127.3788084257 0, -444646.8909429092 2551734.2035537036 0, -443045.91187862447 2551629.8101939997 0, -443138.36766248266 2550030.7681669304 0, -444743.72609288245 2550127.3788084257 0)), ((-430033.65379390196 2554092.7085277583 0, -429939.73212155275 2555703.016174023 0, -429114.4977130899 2555654.2187654283 0, -429208.16143720975 2554042.0616522403 0, -430033.65379390196 2554092.7085277583 0)), ((-423351.0413268105 2557712.9410724454 0, -423390.8433757743 2556929.712998047 0, -425020.4615986985 2557027.95286503 0, -424974.07251673535 2557811.899534188 0, -426583.6489385309 2557897.5968807926 0, -426530.2388991024 2558724.565606446 0, -424925.27401890064 2558636.616044502 0, -424973.959480343 2557813.8104225034 0, -423351.0413268105 2557712.9410724454 0)), ((-443411.327305519 2558925.4696468185 0, -442620.230223664 2558875.3104349906 0, -442667.3970636231 2558070.3510440984 0, -443463.87689135026 2558116.6695553386 0, -443411.327305519 2558925.4696468185 0)), ((-432008.32069761655 2561507.231298247 0, -431219.4077658447 2561463.038939 0, -431268.61981369683 2560600.434747318 0, -432052.1970686792 2560642.140191054 0, -432008.32069761655 2561507.231298247 0)), ((-426716.81530554 2564624.114100472 0, -426707.52948778763 2564623.5566806584 0, -426692.4828333742 2564614.8672273285 0, -426692.5087301603 2564614.379844563 0, -426691.78988649335 2564613.9495078167 0, -426733.68965493835 2563819.3388428786 0, -426776.64643755584 2563016.7133475426 0, -426799.7086707455 2563018.049594607 0, -427579.00878645526 2563064.951869799 0, -428380.7753124238 2563113.243457345 0, -428380.73552480957 2563113.927417358 0, -428381.6060359371 2563113.979870609 0, -428334.9290819861 2563916.3400202203 0, -428288.2561263625 2564718.683441213 0, -427490.2677354467 2564670.6690188395 0, -426716.81530554 2564624.114100472 0)), ((-434813.6634071391 2563493.2326757205 0, -435617.79621267726 2563541.6064002137 0, -436019.8862331885 2563565.403011668 0, -436425.49723567994 2563589.8554186737 0, -436425.46546135034 2563590.6789542586 0, -436426.48296880024 2563590.739901008 0, -436410.49948270526 2563992.1840610695 0, -436394.68766633986 2564389.3833404593 0, -437200.19668249297 2564433.7771542394 0, -437200.15289863385 2564434.657278908 0, -437200.78255896334 2564434.692071872 0, -437160.9389114734 2565236.5009422502 0, -436402.0176669148 2565192.114209315 0, -436393.7268598631 2565191.6300081937 0, -436362.8367163005 2565189.538800493 0, -436362.86563353776 2565188.812342155 0, -436362.1814346979 2565188.8000458363 0, -436393.90169179055 2564393.5875489637 0, -435980.99398871616 2564368.923160074 0, -435578.9374963974 2564344.902883919 0, -434774.8233555622 2564296.84874285 0, -434774.85987829306 2564296.106550126 0, -434773.9740652296 2564296.0537291938 0, -434774.2416092238 2564291.521798643 0, -433972.84655320656 2564246.8025450376 0, -433972.89941218426 2564245.8250554316 0, -433972.4121819333 2564245.79785903 0, -434015.41325301083 2563445.71849138 0, -434813.6634071391 2563493.2326757205 0)), ((-421756.46215367416 2565939.7167050266 0, -421806.17955510184 2565134.136975296 0, -422614.4160546765 2565178.7852799157 0, -423422.0574774829 2565223.4882375076 0, -423422.0013008767 2565224.4649139903 0, -423422.9813063332 2565224.519108104 0, -423377.15158542315 2566021.330673727 0, -423330.6168102949 2566830.3440194777 0, -423284.0872673842 2567639.34147021 0, -423242.63025312254 2568437.9945767433 0, -423212.2235825094 2569023.8373860703 0, -423199.9920311647 2569236.593043911 0, -423195.68959686905 2569236.320102531 0, -422394.89413102623 2569185.3813387137 0, -421589.7956282559 2569134.1527538174 0, -421589.8393179128 2569133.1811313457 0, -421588.90485162614 2569133.121638298 0, -421593.26696228486 2569056.9531056085 0, -421598.92169992864 2568931.1963351076 0, -421599.2699069732 2568924.6695040325 0, -421630.2338096047 2568345.47384594 0, -421650.8136453823 2567960.5445556445 0, -421671.5662190923 2567555.8997747656 0, -421714.30955632677 2566747.8335770806 0, -4</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Squaxin Island</t>
+          <t>Standing Rock</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>WA</t>
+          <t>SD</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Administrative Site</t>
+          <t>Rural Credit, Indemnity, School and Public Lands, BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, ND SCHOOL OF SCIENCE, CAPITOL BUILDING, VETERANS HOME, MAYVILLE, SCHOOL OF MINES, UNIVERSITY OF ND, ND INDUSTRIAL SCHOOL, ND STATE UNIVERSITY, NDÔøΩSTATEÔøΩUNIVERSITY, ELLENDALE, SCHOOL FOR THE DEAF, STATEÔøΩHOSPITAL, VALLEY/MAYVILLE</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>6</v>
+        <v>739</v>
       </c>
       <c r="G67" t="n">
-        <v>277.57</v>
+        <v>46823.4</v>
       </c>
       <c r="H67" t="n">
-        <v>5</v>
+        <v>217</v>
       </c>
       <c r="I67" t="n">
-        <v>52.27</v>
+        <v>70165.38</v>
       </c>
       <c r="J67" t="n">
-        <v>1</v>
+        <v>522</v>
       </c>
       <c r="K67" t="n">
-        <v>329.84</v>
+        <v>116988.78</v>
       </c>
       <c r="L67" t="n">
-        <v>1737.94</v>
+        <v>2347732.03</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-449556.5059218632 2511728.520408616 0, -449176.91746688675 2511705.777670777 0, -449176.1984435866 2511705.733216676 0, -449556.5059218632 2511728.520408616 0)), ((-449982.1299062058 2511754.164890567 0, -449982.1297245475 2511754.167914157 0, -449699.5578025382 2511737.097241653 0, -449982.1299062058 2511754.164890567 0)), ((-449579.1105100217 2511729.8748406926 0, -449579.1429920948 2511729.876786715 0, -449692.63074373675 2511736.678877075 0, -449982.1297245472 2511754.1679141615 0, -449971.4739245098 2511931.527108429 0, -449568.3538073889 2511907.2960243486 0, -449165.2529589046 2511883.0840977235 0, -448762.17476517527 2511858.894686667 0, -448773.2079271766 2511681.583054768 0, -448773.2382601551 2511681.584876002 0, -448871.2507424927 2511687.473799343 0, -448888.1109399908 2511688.486912748 0, -448915.0532655619 2511690.1000152635 0, -449176.12641623017 2511705.7317984854 0, -449176.1676868195 2511705.7342695664 0, -449579.1105100217 2511729.8748406926 0)), ((-463366.30178307346 2512582.8016465153 0, -463334.87706382683 2512580.856246914 0, -463366.30178338743 2512582.8016431336 0, -463405.7509150512 2512585.2358416286 0, -463366.30178307346 2512582.8016465153 0)), ((-464064.27364119334 2512625.8867090484 0, -464170.7422980627 2512632.464345802 0, -464213.54977654974 2512635.13402016 0, -464170.7422882964 2512632.464375655 0, -464064.27364119334 2512625.8867090484 0)), ((-464417.0083980226 2512647.8287448124 0, -464406.96939841536 2512813.1866125953 0, -464005.15649598924 2512788.596259246 0, -463603.3422352082 2512764.027462437 0, -463201.52449667803 2512739.4803704 0, -463211.49494368176 2512573.224213664 0, -463211.5253091886 2512573.226092752 0, -463366.310057336 2512582.8084000037 0, -463613.2370556818 2512598.044970272 0, -463613.2761352741 2512598.047381669 0, -464015.0843742729 2512622.853928947 0, -464015.1124974243 2512622.855665194 0, -464170.7614092613 2512632.4718089625 0, -464417.0083980226 2512647.8287448124 0)), ((-456264.384418507 2513913.2817409043 0, -456311.65716874925 2513126.286220331 0, -456360.0020620866 2512321.4405879593 0, -456361.8088236175 2512291.361745473 0, -457984.09614303196 2512406.6756496173 0, -457932.25081506104 2513225.965336516 0, -457932.2506155181 2513225.9674284193 0, -457893.0983433012 2513844.675265713 0, -457892.23051078035 2513858.3893516134 0, -457891.59300734167 2513868.4635157497 0, -457890.3708778595 2513887.7760617123 0, -457882.31282094686 2514015.1139713754 0, -457881.30541144765 2514015.05057021 0, -456264.384418507 2513913.2817409043 0)), ((-451282.77213509835 2516843.573187387 0, -452881.1286204372 2516941.3567562765 0, -452788.16282210994 2518541.180243185 0, -451193.0181150282 2518454.0908873766 0, -451282.77213509835 2516843.573187387 0)), ((-447775.73130676866 2521466.171663356 0, -447680.4446375186 2523083.00645899 0, -446062.53746012686 2522978.478549137 0, -446149.0682687236 2521383.5954063167 0, -447775.73130676866 2521466.171663356 0)), ((-452263.06508488936 2527420.0165616595 0, -452262.9989986145 2527421.1705014743 0, -452217.3678488886 2528216.499118979 0, -451389.4571952081 2528170.4905104106 0, -451429.1165415427 2527389.9752738457 0, -451432.0658116872 2527378.173895968 0, -451432.0927535317 2527378.066065934 0, -450674.31094751746 2527334.2312229117 0, -450659.6225222654 2527333.820585373 0, -450659.6496749159 2527333.383858899 0, -450711.31631975883 2526504.3601864562 0, -451480.4558586479 2526550.4099000636 0, -451434.6292940259 2527362.1247527148 0, -451433.9890512456 2527378.2706318754 0, -452231.5475172021 2527418.4299013275 0, -452252.6274551624 2527419.4912691237 0, -452263.06508488936 2527420.0165616595 0)), ((-455166.42114959256 2531660.3247363223 0, -455167.23062476097 2531647.0039018453 0, -456801.4756868293 2531730.9629927757 0, -456691.7622620359 2533334.4222966707 0, -455069.8573224605 2533249.725257102 0, -455166.42114959256 2531660.3247363223 0)), ((-451735.24512163736 2536243.317183069 0, -451645.78562387795 2537864.519470849 0, -450021.007770592 2537765.742848979 0, -450116.09840936464 2536144.5834728894 0, -451735.24512163736 2536243.317183069 0)), ((-461322.1501446945 2536845.070964317 0, -461266.4029524177 2537687.653727615 0, -459665.6639103949 2537608.6670449553 0, -459715.99443711824 2536748.6248253267 0, -461322.1501446945 2536845.070964317 0)), ((-454890.8922974969 2542698.1855162326 0, -453281.3780819311 2542600.764220469 0, -453384.07991065923 2540985.658445156 0, -454594.304251081 2541056.715851151 0, -454988.15293683077 2541080.9520675344 0, -454890.8922974969 2542698.1855162326 0)), ((-459524.2299986185 2546204.2215727074 0, -459429.9975628155 2547813.2614215584 0, -457816.4177064228 2547702.894510099 0, -457894.3280349991 2546101.495725701 0, -459524.2299986185 2546204.2215727074 0)), ((-447333.0196933869 2547058.820925809 0, -447227.8717313179 2548665.936131774 0, -446452.08490666316 2548619.788373531 0, -445623.684550666 2548570.683982875 0, -445713.3941800438 2546965.148014899 0, -446547.97513063496 2547014.6210594294 0, -447333.0196933869 2547058.820925809 0)), ((-455693.08488767454 2555626.9297070154 0, -456468.00679758465 2555674.8984094583 0, -456416.7449249867 2556489.9031604244 0, -454802.76577117445 2556376.1514217234 0, -454885.3564354707 2554791.20763069 0, -455740.92444017367 2554843.778459255 0, -455693.08488767454 2555626.9297070154 0)), ((-449276.9794248514 2555236.611581465 0, -449203.3707008164 2556834.7579691587 0, -447593.3605284898 2556738.3556973888 0, -447672.70063963823 2555137.8819685206 0, -449276.9794248514 2555236.611581465 0)), ((-458875.0183390479 2556662.9690301814 0, -458828.2093868158 2557424.049423567 0, -457185.61157180124 2557335.725614214 0, -457303.25758220925 2555726.584222721 0, -458131.4758505402 2555781.6832451886 0, -458083.5253769855 2556616.3136012475 0, -458875.0183390479 2556662.9690301814 0)), ((-452186.6040555831 2560226.9235749864 0, -453804.62321116845 2560336.180691955 0, -453698.7256673469 2561920.4906114456 0, -452074.04850345897 2561828.9798595035 0, -452186.6040555831 2560226.9235749864 0)), ((-449321.9326013234 2564376.2574031744 0, -449321.3769063425 2564386.1416202285 0, -449276.9198393965 2565177.0558428974 0, -449231.9133044314 2565977.837736146 0, -449231.53414914093 2565984.0533565343 0, -449183.4894144431 2566771.4791362807 0, -449182.9648853079 2566780.0764241694 0, -448373.3310903083 2566731.304009236 0, -447563.6950838357 2566682.5144151314 0, -447514.66624011385 2567489.021035307 0, -446705.1953842786 2567440.7313964185 0, -445988.7150911759 2567397.976206695 0, -445909.0247302735 2567388.175121057 0, -445895.8781619955 2567386.558528588 0, -445895.92348154745 2567385.746683493 0, -445895.1590514922 2567385.67234871 0, -445940.1287341057 2566574.7250591344 0, -445941.19318906 2566574.7945829183 0, -445986.07918338495 2565770.789100794 0, -445986.3991030491 2565765.046846068 0, -446034.2458411558 2564974.470302698 0, -446081.848022635 2564187.9879047014 0, -446082.0960329981 2564183.877433263 0, -446175.0936994005 2564189.500664745 0, -446181.23518354836 2564189.8143169554 0, -446892.4000848265 2564226.1902014404 0, -447120.5724311692 2564237.8580566742 0, -447702.7252258939 2564267.693862222 0, -448512.33092102065 2564321.9463786385 0, -448743.30342503305 2564337.4211003976 0, -449321.9326013234 2564376.2574031744 0), (-448467.324070914 2565124.4624965163 0, -447657.7244795784 2565071.8508929783 0, -447612.77113378036 2565875.227558959 0, -448421.53377836954 2565926.115988229 0, -448422.3650867946 2565926.1683864985 0, -448467.324070914 2565124.4624965163 0)), ((-450872.6268687303 2565283.478366009 0, -451680.51605147077 2565331.9210636 0, -451633.04154613346 2566137.5807718737 0, -450834.4153565486 2566092.4419257008 0, -450827.00930416514 2566092.0250950083 0, -450029.46244642325 2566034.939160159 0, -450074.7745231379 2565230.2747832444 0, -450872.6268687303 2565283.478366009 0)), ((-465522.480087164 2566211.0676372 0, -465497.99191343173 2566611.630241336 0, -465480.8451485192 2566892.1531603415 0, -465473.2948586149 2567012.1479260344 0, -465472.71796541277 2567021.4207174475 0, -465472.031586073 2567021.3812373984 0, -465455.0418494883 2567019.6596213793 0, -465448.99211219745 2567018.280112106 0, -465327.7137608106 2567003.131225467 0, -465322.185706256 2567002.8163942015 0, -465347.6779609036 2566601.412719703 0, -465373.0994776094 2566201.1579084056 0, -465398.521134454 2565800.89875415 0, -465423.9451466621 2565400.6366323116 0, -465547.5166171904 2565407.1564568747 0, -465555.2558658541 2565407.657327017 0, -465571.7365829466 2565408.7253705617 0, -465571.6657606916 2565409.8448486715 0, -465547.05419117556 2565810.4818696138 0, -465529.667752618 2566093.4945963905 0, -465522.4895103514 2566210.9134963593 0, -465522.480087164 2566211.0676372 0)), ((-454811.31346071255 2567141.109477066 0, -454855.6294871319 2566337.2350389366 0, -455258.11700768187 2566364.1809276436 0, -455653.93637284345 2566390.676939578 0, -455629.05221015995 2566792.4430512516 0, -455604.16928405856 2567194.205680881 0, -455213.8082963064 2567168.0663915016 0, -454811.31346071255 2567141.109477066 0)), ((-445778.7935746923 2569395.246043825 0, -445773.73187626095 2569498.2577245524 0, -445759.094738161 2569796.1996818786 0, -445369.4413924876 2569772.410528177 0, -445389.7841105851 2569371.470383204 0, -445410.09594294924 2568971.0564951664 0, -445434.51985076955 2568565.8250266635 0, -445458.6746454063 2568165.0839533997 0, -445056.3294193455 2568141.3206398026 0, -444251.63915332005 2568093.7813247424 0, -444299.9785089062 2567292.2843639296 0, -444310.1872706344 2567292.8866332476 0, -445104.64999606746 2567339.8260526597 0, -445506.98577934084 2567363.5917561376 0, -445895.8781619955 2567386.558528588 0, -445895.60333543544 2567391.0871763406 0, -445871.601985927 2567787.2991851103 0, -445847.3282120576 2568188.0355825336 0, -445823.0542726236 2568588.767889601 0, -445798.49213708605 2568994.28689127 0, -445778.7935746923 2569395.246043825 0)), ((-452174.19734232465 2570747.6675056093 0, -452158.0453145773 2571009.3110569436 0, -452157.64718833106 2571015.7608968886 0, -452151.9472461596 2571015.3874891964 0, -451348.75422009744 2570962.814505742 0, -450539.8587676992 2570909.8519592355 0, -450539.9091747104 2570909.024648134 0, -450539.06196779094 2570908.9691903675 0, -450555.61941961234 2570638.495888727 0, -450588.6149749233 2570099.6443992187 0, -450638.17361392797 2569290.297443804 0, -451439.8572009743 2569341.5330177248 0, -452240.91873932607 2569393.2423031386 0, -452240.88616896205 2569393.897006181 0, -452241.76140384376 2569393.953099999 0, -452241.56006396015 2569397.991822121 0, -452205.9345710624 2570111.7782752165 0, -452201.2866546269 2570204.9095945144 0, -452174.19734232465 2570747.6675056093 0)), ((-446568.4550681967 2573951.0915424577 0, -446563.80971174856 2573952.8998985905 0, -446551.8514681421 2573957.555033972 0, -446562.6124286463 2574012.59082663 0, -446565.37551279727 2574026.7223278442 0, -446568.97758666135 2574056.646631005 0, -446625.42937589827 2574067.665254358 0, -446638.2313802044 2574070.1640319084 0, -446697.67873640795 2574081.922251191 0, -446707.6876513473 2574086.7241391297 0, -446714.6893999777 2574091.4392362507 0, -446716.8276809053 2574092.4650806137 0, -446750.1683095114 2574108.4603109276 0, -446784.95938356454 2574131.8839738998 0, -446799.36959451943 2574158.3019924304 0, -446819.34315285203 2574195.813044364 0, -446833.7530955948 2574222.231089865 0, -446853.72635455267 2574259.7421824727 0, -446874.3846494828 2574297.616373964 0, -446900.8587341657 2574347.339388282 0, -446928.68623211666 2574398.3597569247 0, -446916.27634527377 2574427.995409388 0, -446907.2980127922 2574445.9841933427 0, -446885.66267165233 2574454.170303028 0, -446834.9857463377 2574446.780569181 0, -446745.2809730728 2574432.206206241 0, -446694.603883932 2574424.817553702 0, -446676.48620318633 2574422.176331941 0, -446627.87300325214 2574414.278510132 0, -446550.6406528148 2574391.6491387743 0, -446512.7847795553 2574378.09854516 0, -446492.80560379615 2574375.8343219236 0, -446478.4234633957 2574385.0732659595 0, -446431.1496324344 2574422.694776051 0, -446424.6298018589 2574452.140482353 0, -446398.94756617106 2574502.136867927 0, -446340.09982323315 2574560.1016085385 0, -446285.99670345377 2574613.831450595 0, -446278.6087352978 2574624.503452922 0, -446269.89767463866 2574633.0836661397 0, -446270.9608647694 2574615.557296495 0, -446225.9212432688 2574655.5221559913 0, -446214.9682569618 2574654.8433415717 0, -446178.5546935751 2574652.586824033 0, -446178.5546134259 2574652.5869199685 0, -446214.9682506757 2574654.8434831738 0, -446129.2512760676 2574796.1515730764 0, -445989.49300173635 2574948.5913481 0, -445996.2009790698 2575103.6458547325 0, -445956.77361182624 2575108.6720762732 0, -445946.49791766756 2575087.257677356 0, -445921.36968522216 2575044.6333539444 0, -445918.79881303036 2575039.2751104087 0, -445918.79881303024 2575039.2751104087 0, -445905.6137503262 2575011.7946400736 0, -445900.1632744067 2575002.5494192936 0, -445902.4074946497 2574952.3947126777 0, -445899.913273229 2574882.311590769 0, -445893.9836602633 2574842.597457956 0, -445921.7162698178 2574762.8310657055 0, -445951.94644323573 2574667.3735025837 0, -445955.66247839987 2574646.365390554 0, -445954.72250468645 2574644.1635208954 0, -445955.03065915284 2574642.424815998 0, -445953.41247410345 2574638.634799117 0, -445953.4124741035 2574638.634799117 0, -445953.2656972692 2574638.291027136 0, -445953.02043969627 2574637.7165994206 0, -445936.2766363764 2574598.500258093 0, -445928.21034849255 2574575.791354023 0, -445908.6259245545 2574580.4970363365 0, -445891.66946380393 2574593.49464247 0, -445890.2791959668 2574594.560322038 0, -445888.3325162854 2574592.4428514666 0, -445885.50121547433 2574589.363148009 0, -445877.02642133815 2574586.2225874905 0, -445869.65367432754 2574578.2032980197 0, -445868.20082048024 2574576.6230382407 0, -445832.2017305108 2574558.7271710527 0, -445811.4678179631 2574551.0448905793 0, -445774.65136369405 2574537.403744603 0, -445745.5449259613 2574545.3380191578 0, -445743.1645129254 2574546.6865430293 0, -445728.65320356743 2574554.9073210126 0, -445714.51598370774 2574556.52835275 0, -445701.8415694503 2574561.9725715136 0, -445672.98795473785 2574577.9486203967 0, -445652.36112494336 2574615.369621159 0, -445652.260662085 2574615.731640977 0, -445652.0424214849 2574619.333129469 0, -445649.4273990284 2574642.926399384 0, -445647.22935103806 2574698.7794549344 0, -445639.20174341806 2574743.2514613876 0, -445633.4301780968 2574770.0468409318 0, -445626.06384222314 2574774.265435439 0, -445592.0640389263 2574856.1849386683 0, -445569.7662060519 2574911.243892445 0, -445526.85662866797 2574973.9616541793 0, -445505.57474210643 2574986.4271483268 0, -445481.991395397 2574956.311744628 0, -445476.69957869616 2574906.4662741185 0, -445487.9087582305 2574737.260160259 0, -445498.52683381917 2574616.327599229 0, -445498.53442332573 2574616.221544097 0, -445501.02662029344 2574587.838077341 0, -445510.24065185885 2574387.289699773 0, -445516.91910214105 2574278.4432967617 0, -445520.0287879152 2574227.7611629264 0, -445517.53163593437 2574219.3884955756 0, -445516.21309944324 2574214.9675922766 0, -445516.5630488973 2574207.345973943 0, -445516.6752975337 2574204.901288703 0, -445517.0419461239 2574196.915976583 0, -445500.2378451389 2574140.565765194 0, -445494.8548661272 2574122.6799496817 0, -445501.4186812127 2574014.291503234 0, -445516.84541118756 2574004.198597328 0, -445520.0187222175 2574001.5507348306 0, -445560.83336123556 2574017.4222854553 0, -445611.71132416325 2574025.983912797 0, -445663.6098651552 2574046.166564549 0, -445717.5229416513 2574074.1731103915 0, -445740.52318680566 2574090.552032075 0, -445788.76768398494 2574105.7643663273 0, -445828.7094112431 2574111.4429495097 0, -445875.0752445116 2574100.4918937637 0, -445907.2044888619 2574087.663616673 0, -445915.7437630923 2574085.646486602 0, -445919.85222520004 2574084.6759940004 0, -445939.10924534505 2574076.9884381196 0, -445974.8398783625 2574041.5776248965 0, -445999.37579975557 2574002.5589720556 0, -446024.2769612919 2573936.963886998 0, -446042.07678360125 2573881.76528192 0, -446077.3297600856 2573883.9010345708 0, -446093.9672806464 2573885.830022005 0, -446114.94519567984 2573904.7156140115 0, -446159.9014939694 2573915.924581668 0, -446184.9065645396 2573904.292101264 0, -446199.68989141687 2573884.237382285 0, -446200.28617193596 2573883.880797301 0, -446229.0963397115 2573855.7850391716 0, -446227.3448786952 2573844.1857780414 0, -446318.58519534994 2573850.050926444 0, -446698.1780046639 2573874.784120618 0, -446710.4334241953 2573875.528157732 0, -446694.3859729308 2573884.075065285 0, -446681.81349965365 2573910.118912809 0, -446678.2952695306 2573924.7751732552 0, -446628.48430492333 2573944.1648235247 0, -446568.4550681967 2573951.0915424577 0), (-446624.1749220042 2574068.462996698 0, -446624.17492200434 2574068.462996698 0, -446625.42937589827 2574067.665254358 0, -446624.1749220042 2574068.462996698 0)), ((-446950.56243684096 2574198.6320379856 0, -446932.30556629575 2574201.385897007 0, -446908.93935471226 2574176.457900518 0, -446883.80138547975 2574111.1742358143 0, -446863.6045996117 2574054.5049641044 0, -446875.42459873157 2574008.8867512974 0, -446882.9000154899 2573959.3910239553 0, -446876.09148893814 2573931.137323962 0, -446865.8438236706 2573894.418725824 0, -446864.12461474177 2573885.3509173403 0, -447124.44490654866 2573901.9489376843 0, -447108.22404811066 2574142.9668562766 0, -447101.39372117515 2574133.4359606504 0, -447087.50028866966 2574121.831196952 0, -447052.32130097033 2574102.4577116594 0, -447050.1481298079 2574105.75212045 0, -447024.6023644447 2574144.478105517 0, -446997.2296424889 2574184.283265825 0, -446962.1561278046 2574196.8832502966 0, -446950.56243684096 2574198.6320379856 0)), ((-456765.9186664952 2574520.703219268 0, -456766.7534668326 2574520.7562253936 0, -456775.8150063362 2574523.8307035593 0, -456936.0986376184 2574533.4261585367 0, -457573.4196303584 2574571.6560989986 0, -457521.005743965 2575367.450410148 0, -456717.4002130627 2575315.5125296665 0, -456668.05145486625 2576110.2522586337 0, -455863.1617071876 2576062.149205341 0, -455177.45231584826 2576021.155547476 0, -455166.6825075448 2576020.512744768 0, -455069.6986429143 2576016.5006078887 0, -455058.21920649987 2576016.0251637846 0, -455058.282165094 2576015.0817748327 0, -455057.69480324606 2576015.0569460415 0, -455110.6791901181 2575216.2349368795 0, -455164.28176372364 2574417.0104392366 0, -455264.5815672489 2574424.4891094393 0, -455964.7872605663 2574469.126197598 0, -456765.98251743335 2574519.674981475 0, -456765.9186664952 2574520.703219268 0)), ((-463196.45121227956 2574941.5765004004 0, -463993.9246552496 2574981.302344243 0, -463943.32446898887 2575784.3832184738 0, -463918.20070562203 2576183.702619917 0, -463515.8089860782 2576161.4178912505 0, -463113.41681594384 2576139.127593277 0, -463138.301791416 2575744.2873498304 0, -463188.9192366038 2574941.2019163715 0, -463196.45121227956 2574941.5765004004 0)), ((-464937.096481809 2575700.087033282 0, -464928.5530128695 2575837.0287334695 0, -464928.4526466002 2575838.6375712072 0, -464903.51949927624 2576238.3075860483 0, -464887.08327462705 2576501.797045511 0, -464878.39700935816 2576639.4931003833 0, -464878.3431484534 2576640.3824573625 0, -464854.09094255016 2577040.837456766 0, -464838.217164771 2577302.9332062737 0, -464837.0562252017 2577321.3652535304 0, -464811.8891829471 2577321.085257435 0, -464766.82649088395 2577326.1103489115 0, -464755.40941543435 2577334.3433872107 0, -464751.2037088808 2577359.1004940905 0, -464759.70275551005 2577386.9586737705 0, -464773.0340297169 2577424.741107386 0, -464773.0771431283 2577424.862592797 0, -464797.1731942942 2577443.0502988207 0, -464807.56328525895 2577449.673206065 0, -464631.53984982223 2577438.589641639 0, -464631.22398814623 2577443.587782681 0, -464615.29167337413 2577428.4568144553 0, -464576.0646172975 2577397.1888157343 0, -464555.57479544706 2577395.889665911 0, -464524.6199792611 2577422.7116912534 0, -464521.4497953473 2577428.27365366 0, -464514.44614257413 2577434.342532914 0, -464538.9968471909 2577466.3124745665 0, -464562.72751803906 2577493.638865401 0, -464526.389179808 2577549.1250518817 0, -464489.11652091594 2577608.7374029653 0, -464493.6713408025 2577648.7011961546 0, -464492.8433140445 2577702.9044545596 0, -464466.4027872354 2577738.3557627415 0, -464434.40197506174 2577777.065497327 0, -464404.812810613 2577792.169803099 0, -464367.66847528773 2577768.015404443 0, -464342.6809768903 2577724.557705723 0, -464320.66599687096 2577656.6760155717 0, -464295.86255039327 2577601.907708306 0, -464288.0941342627 2577538.082097315 0, -464279.9377086015 2577478.5007729246 0, -464277.9064324353 2577476.794150505 0, -464263.9071737847 2577468.5325357565 0, -464251.9463057986 2577461.4747319506 0, -464249.95473392593 2577459.802275873 0, -464252.5510622925 2577411.0551478895 0, -464218.8431551951 2577409.000187979 0, -464217.78651525057 2577403.2725574877 0, -464209.7549571784 2577359.7271024147 0, -464195.2587707094 2577293.1045055306 0, -464178.698804382 2577281.7068156367 0, -464157.41678466497 2577254.934471376 0, -464186.321640588 2577191.928404721 0, -464222.5097901601 2577143.6309508733 0, -464245.2014497252 2577135.336637269 0, -464265.2189677541 2577140.263590601 0, -464282.6754837639 2577146.4746682304 0, -464287.1030315777 2577147.5649162563 0, -464339.485003487 2577170.942280084 0, -464407.87672958424 2577195.2783001685 0, -464437.7845460607 2577169.9045328535 0, -464483.4159654913 2577116.2338393074 0, -464472.1172339116 2577093.786866766 0, -464437.68294838996 2577057.412049867 0, -464379.71507526276 2577045.2505906043 0, -464319.596377357 2577041.5133966543 0, -464304.40058103704 2577038.3254989535 0, -464297.3545622659 2577028.7823426677 0, -464292.58365757955 2577027.781605413 0, -464289.8096475747 2577024.0247067767 0, -464285.33380089165 2577017.9630467445 0, -464273.68084539607 2577004.189537191 0, -464270.3910880498 2577000.300997528 0, -464266.8004785266 2576995.4363722466 0, -464266.3839822324 2576989.7298110127 0, -464263.14104009303 2576945.3432460255 0, -464255.0198022468 2576895.8779241713 0, -464202.66684775567 2576866.1941167354 0, -464150.96786590706 2576841.200656919 0, -464139.86460662744 2576818.6582911205 0, -464143.9829531782 2576776.6761341197 0, -464142.85249968857 2576726.547589812 0, -464063.6891408286 2576739.7425603513 0, -464014.29669513635 2576749.639661372 0, -463980.3430621567 2576791.996073437 0, -463954.05614179204 2576834.7944496544 0, -463923.30624551146 2576847.566879482 0, -463896.46524345636 2576855.4663607837 0, -463895.59889163164 2576855.8271351433 0, -463883.87232823035 2576859.2774244836 0, -463878.37832621014 2576858.9286823734 0, -463893.0778399444 2576583.0167188225 0, -464295.34907332796 2576607.53743321 0, -464682.56904175243 2576631.13727435 0, -464708.0847137635 2576227.6658522277 0, -464733.5301654517 2575825.334955942 0, -464758.9758257566 2575423.0014905534 0, -464784.4225472731 2575020.6622311734 0, -464794.4157079474 2575021.2268428295 0, -464939.18487480434 2575029.3975207983 0, -464943.71482660837 2575029.707692358 0, -464968.10114058503 2575031.379352574 0, -464978.86292046105 2575032.1186184734 0, -464978.72881342913 2575034.2467949837 0, -464953.62894154043 2575435.655953842 0, -464937.096481809 2575700.087033282 0)), ((-427122.3892649302 2510406.657618777 0, -427121.6073993937 2510406.6083721723 0, -427121.607303883 2510406.6083661583 0, -427121.6074740782 2510406.605239546 0, -427167.29207266384 2510409.4846520214 0, -427477.69133642956 2510424.482990813 0, -427167.2701634584 2510409.4864873113 0, -427167.2702126657 2510409.4864904126 0, -427489.66749348 2510425.061672794 0, -427498.2846000709 2510425.4780471195 0, -427488.6248352047 2510591.0338693755 0, -427112.8165501257 2510568.101098727 0, -427121.60730386025 2510406.608366577 0, -427121.6073213328 2510406.6083676773 0, -427166.7266011812 2510409.4522266914 0, -427122.3892649302 2510406.657618777 0)), ((-428302.7533831593 2510471.4720921647 0, -428293.5116595257 2510636.594242328 0, -427891.0689813323 2510613.801533897 0, -427900.51612006954 2510448.505709506 0, -427970.68001723074 2510452.5260432283 0, -428122.4389314934 2510461.1831019046 0, -427970.98125386966 2510452.5432437616 0, -428302.7533831593 2510471.4720921647 0)), ((-436346.10551138024 2510938.2014115276 0, -436346.1054094166 2510938.2014054214 0, -436260.8903451971 2510933.1025654385 0, -436346.10551316146 2510938.2013793173 0, -436423.0556714865 2510942.8094952027 0, -436346.10551138024 2510938.2014115276 0)), ((-436337.2115463037 2511099.0301875575 0, -435935.1878377702 2511076.165228918 0, -435944.2682461471 2510914.196872157 0, -435944.2725795822 2510914.197129352 0, -436019.43084083596 2510918.661083573 0, -436346.10516805894 2510938.2076197756 0, -436346.11167875346 2510938.2080093427 0, -436747.7785271353 2510962.2613196066 0, -436739.00722823804 2511122.113856621 0, -436337.2115463037 2511099.0301875575 0)), ((-437945.4633888475 2511032.4974911553 0, -438344.8769819778 2511055.7122348617 0, -438349.1716061985 2511055.9619939644 0, -438344.8769817122 2511055.7122394843 0, -438344.8769694131 2511055.712238769 0, -438191.29134578933 2511046.785974206 0, -437945.4633888475 2511032.4974911553 0)), ((-437630.8053028015 2511014.228836478 0, -437942.78666180244 2511032.348041177 0, -437942.7952988941 2511032.3485428006 0, -438344.87663705077 2511055.7182380296 0, -438344.88317202893 2511055.718617854 0, -438436.5255207326 2511061.0482047983 0, -438746.92438312696 2511079.2904069447 0, -438737.5692713429 2511244.521314349 0, -438708.09146898845 2511242.686678195 0, -438641.12810462905 2512855.2839119053 0, -437042.0496653505 2512760.871550386 0, -437136.1836475484 2511123.4523978126 0, -437532.35598531854 2511150.7005817727 0, -437540.67339390906 2511008.9642607914 0, -437540.6777409151 2511008.9645145955 0, -437630.8053028015 2511014.228836478 0)), ((-439149.5913135798 2511103.3541215407 0, -439240.6048005137 2511108.795627342 0, -439552.2067859431 2511127.554180531 0, -439542.82905383897 2511293.0435698433 0, -439140.2008863796 2511268.771542087 0, -439149.5827539224 2511103.3536100066 0, -439149.5913135798 2511103.3541215407 0)), ((-423511.58733838267 2516795.860697203 0, -422312.76373192994 2516733.418483321 0, -422399.4995318504 2515128.1689220434 0, -423623.10174627777 2515195.7103881766 0, -423511.58733838267 2516795.860697203 0)), ((-438174.3331115907 2520886.8578333333 0, -438089.92187792825 2522475.263604186 0, -436474.0111356682 2522378.049033309 0, -436554.3347478653 2520770.822675446 0, -438174.3331115907 2520886.8578333333 0)), ((-440538.10997213115 2535562.1979440977 0, -442145.8851937264 2535670.1549665434 0, -442052.1990970533 2537276.149583939 0, -440436.57473123574 2537166.2334500076 0, -440538.10997213115 2535562.1979440977 0)), ((-424433.8221215985 2539272.0517960135 0, -425858.80544495455 2539354.321771957 0, -426042.7076174558 2539364.6214590515 0, -426000.3251043954 2540171.698450297 0, -425198.13020345493 2540124.357719958 0, -425150.7232410197 2540931.3059425913 0, -424356.8655591133 2540880.5860454924 0, -424433.8221215985 2539272.0517960135 0)), ((-433980.2747087349 2541443.587525573 0, -434077.9976433319 2539841.0195716564 0, -435422.07180602156 2539922.21452343 0, -435687.8193028673 2539937.8840412805 0, -435593.98831040267 2541548.741150996 0, -433980.2747087349 2541443.587525573 0)), ((-445221.8758211143 2542116.0473940196 0, -443609.36413693096 2542010.643948824 0, -443724.2559185373 2540414.178490147 0, -445011.4045750646 2540492.212708913 0, -445334.0316658631 2540511.656936364 0, -445221.8758211143 2542116.0473940196 0)), ((-430483.81379599456 2546068.489295747 0, -428876.86678534385 2545986.869770583 0, -428974.21988311847 2544373.2443760615 0, -429761.11130427127 2544419.7909906157 0, -429739.05529994343 2544779.528298907 0, -430564.12083383923 2544832.9640669976 0, -430483.81379599456 2546068.489295747 0)), ((-425480.6400727827 2548986.52706754 0, -425430.6969382982 2549800.222580658 0, -424598.9474573648 2549755.82807769 0, -424553.6953297701 2550538.651272534 0, -423775.02667608345 2550490.661146024 0, -423859.93340171734 2548888.2040763283 0, -425480.6400727827 2548986.52706754 0)), ((-434275.08783599635 2550281.136577314 0, -435080.07863136154 2550321.9912387785 0, -435056.20641513256 2550737.4739556466 0, -434250.58380005235 2550688.787143192 0, -434275.08783599635 2550281.136577314 0)), ((-444743.72609288245 2550127.3788084257 0, -444646.8909429092 2551734.2035537036 0, -443045.91187862447 2551629.8101939997 0, -443138.36766248266 2550030.7681669304 0, -444743.72609288245 2550127.3788084257 0)), ((-430033.65379390196 2554092.7085277583 0, -429939.73212155275 2555703.016174023 0, -429114.4977130899 2555654.2187654283 0, -429208.16143720975 2554042.0616522403 0, -430033.65379390196 2554092.7085277583 0)), ((-423351.0413268105 2557712.9410724454 0, -423390.8433757743 2556929.712998047 0, -425020.4615986985 2557027.95286503 0, -424974.07251673535 2557811.899534188 0, -426583.6489385309 2557897.5968807926 0, -426530.2388991024 2558724.565606446 0, -424925.27401890064 2558636.616044502 0, -424973.959480343 2557813.8104225034 0, -423351.0413268105 2557712.9410724454 0)), ((-443411.327305519 2558925.4696468185 0, -442620.230223664 2558875.3104349906 0, -442667.3970636231 2558070.3510440984 0, -443463.87689135026 2558116.6695553386 0, -443411.327305519 2558925.4696468185 0)), ((-432008.32069761655 2561507.231298247 0, -431219.4077658447 2561463.038939 0, -431268.61981369683 2560600.434747318 0, -432052.1970686792 2560642.140191054 0, -432008.32069761655 2561507.231298247 0)), ((-426716.81530554 2564624.114100472 0, -426707.52948778763 2564623.5566806584 0, -426692.4828333742 2564614.8672273285 0, -426692.5087301603 2564614.379844563 0, -426691.78988649335 2564613.9495078167 0, -426733.68965493835 2563819.3388428786 0, -426776.64643755584 2563016.7133475426 0, -426799.7086707455 2563018.049594607 0, -427579.00878645526 2563064.951869799 0, -428380.7753124238 2563113.243457345 0, -428380.73552480957 2563113.927417358 0, -428381.6060359371 2563113.979870609 0, -428334.9290819861 2563916.3400202203 0, -428288.2561263625 2564718.683441213 0, -427490.2677354467 2564670.6690188395 0, -426716.81530554 2564624.114100472 0)), ((-434813.6634071391 2563493.2326757205 0, -435617.79621267726 2563541.6064002137 0, -436019.8862331885 2563565.403011668 0, -436425.49723567994 2563589.8554186737 0, -436425.46546135034 2563590.6789542586 0, -436426.48296880024 2563590.739901008 0, -436410.49948270526 2563992.1840610695 0, -436394.68766633986 2564389.3833404593 0, -437200.19668249297 2564433.7771542394 0, -437200.15289863385 2564434.657278908 0, -437200.78255896334 2564434.692071872 0, -437160.9389114734 2565236.5009422502 0, -436402.0176669148 2565192.114209315 0, -436393.7268598631 2565191.6300081937 0, -436362.8367163005 2565189.538800493 0, -436362.86563353776 2565188.812342155 0, -436362.1814346979 2565188.8000458363 0, -436393.90169179055 2564393.5875489637 0, -435980.99398871616 2564368.923160074 0, -435578.9374963974 2564344.902883919 0, -434774.8233555622 2564296.84874285 0, -434774.85987829306 2564296.106550126 0, -434773.9740652296 2564296.0537291938 0, -434774.2416092238 2564291.521798643 0, -433972.84655320656 2564246.8025450376 0, -433972.89941218426 2564245.8250554316 0, -433972.4121819333 2564245.79785903 0, -434015.41325301083 2563445.71849138 0, -434813.6634071391 2563493.2326757205 0)), ((-421756.46215367416 2565939.7167050266 0, -421806.17955510184 2565134.136975296 0, -422614.4160546765 2565178.7852799157 0, -423422.0574774829 2565223.4882375076 0, -423422.0013008767 2565224.4649139903 0, -423422.9813063332 2565224.519108104 0, -423377.15158542315 2566021.330673727 0, -423330.6168102949 2566830.3440194777 0, -423284.0872673842 2567639.34147021 0, -423242.63025312254 2568437.9945767433 0, -423212.2235825094 2569023.8373860703 0, -423199.9920311647 2569236.593043911 0, -423195.68959686905 2569236.320102531 0, -422394.89413102623 2569185.3813387137 0, -421589.7956282559 2569134.1527538174 0, -421589.8393179128 2569133.1811313457 0, -421588.90485162614 2569133.121638298 0, -421593.26696228486 2569056.9531056085 0, -421598.92169992864 2568931.1963351076 0, -421599.2699069732 2568924.6695040325 0, -421630.2338096047 2568345.47384594 0, -421650.8136453823 2567960.5445556445 0, -421671.5662190923 2567555.8997747656 0, -421714.30955632677 2566747.8335770806 0, -4</t>
+          <t>MULTIPOLYGON Z (((-1468861.5102881684 1062529.544672667 0, -1469017.6210793862 1062555.4110563563 0, -1469129.974785093 1062574.0271501057 0, -1469252.449893471 1062594.3203348885 0, -1469260.0823487265 1062595.5851217243 0, -1469260.0823599044 1062595.5851235767 0, -1469283.173707292 1062599.3663462314 0, -1469642.2312759976 1062658.1631362855 0, -1469644.5357929508 1062658.5420150517 0, -1470024.3775152052 1062720.757761455 0, -1470028.9553121778 1062721.5178974674 0, -1470036.614696355 1062722.7897407915 0, -1470413.0803005649 1062785.259044958 0, -1470413.5090985568 1062785.330216005 0, -1470434.6009114378 1062788.8311073242 0, -1470777.6770908916 1062845.7735343892 0, -1470801.778692093 1062849.7738462705 0, -1470801.7786950548 1062849.7738467618 0, -1470735.291818363 1063247.297021072 0, -1470668.8077412983 1063644.8202214376 0, -1470665.5165512266 1063664.7246222931 0, -1470605.4089253014 1064049.9390719912 0, -1470542.1933719711 1064455.0913720988 0, -1470530.2911529467 1064547.6087893152 0, -1470466.8251287101 1064585.819113063 0, -1470398.8492705273 1064609.9058296997 0, -1470344.2676615152 1064659.9695127506 0, -1470220.7824153055 1064712.4227236935 0, -1470117.9772717974 1064680.9654987962 0, -1470074.4194187138 1064667.6356037075 0, -1470012.878171736 1064611.9488686554 0, -1469981.2567014096 1064594.0036470143 0, -1469904.9436335918 1064618.4355588462 0, -1469867.456967431 1064598.6590498888 0, -1469791.4959079553 1064500.8642470355 0, -1469804.9585004586 1064475.2900794114 0, -1469821.834112315 1064443.2326686454 0, -1469816.7249291502 1064384.524520883 0, -1469812.9904894084 1064341.6145040721 0, -1469811.1894333242 1064334.735605513 0, -1469777.605131138 1064329.0661652733 0, -1469777.6873496468 1064328.532624977 0, -1469789.4935049256 1064251.9189805745 0, -1469789.5006117246 1064251.8726492473 0, -1469789.3708321552 1064251.376711911 0, -1469788.5747998857 1064251.2162895089 0, -1469778.0141272878 1064249.0808299128 0, -1469702.6319516078 1064233.836271017 0, -1469700.7072090243 1064222.2691301936 0, -1469695.323318651 1064189.9152719344 0, -1469641.0308777792 1064172.5543810064 0, -1469589.9364842195 1064156.2161513732 0, -1469580.2220810633 1064136.1836904322 0, -1469578.3887855369 1064132.403009833 0, -1469563.6640393788 1064102.0375518142 0, -1469560.8188364026 1064096.1700240073 0, -1469550.9424646862 1064090.5682925836 0, -1469522.6027439218 1064074.4942171515 0, -1469521.7376082265 1064074.0035687736 0, -1469518.792243473 1064072.332889826 0, -1469518.7249020224 1064072.1973674642 0, -1469494.5615439934 1064023.4539504591 0, -1469427.7809926695 1063998.8150870206 0, -1469395.786498048 1063987.0116526512 0, -1469375.6931782574 1063979.5989675557 0, -1469371.6734833296 1063966.9701128954 0, -1469341.9620892713 1063873.6258968175 0, -1469306.706696515 1063841.1826290756 0, -1469298.967764853 1063834.0602172774 0, -1469289.7784527813 1063838.4524427834 0, -1469276.536821521 1063844.783336913 0, -1469257.2328571894 1063854.0131332797 0, -1469192.3475694433 1063920.157510396 0, -1469161.8019355591 1063932.9952806323 0, -1469149.7209660907 1063938.0728865312 0, -1469137.7064038394 1063951.7945904187 0, -1469108.5820747924 1063985.057432164 0, -1469030.5227920236 1063979.090286098 0, -1469030.5227943866 1063979.0902718552 0, -1469060.0896770647 1063801.4349766506 0, -1469126.045451578 1063405.13122767 0, -1468728.933957707 1063337.2484541982 0, -1468795.2218783214 1062933.398209418 0, -1468857.7885759312 1062528.9281126044 0, -1468861.5102726147 1062529.544767426 0, -1468861.5102881684 1062529.544672667 0)), ((-1470936.141652446 1072177.4399317813 0, -1470956.609938698 1072171.470867857 0, -1470975.5339946318 1072165.9522729167 0, -1470976.333474576 1072165.4015191253 0, -1471017.5148884433 1072137.0258263568 0, -1471050.386111551 1072114.3762780975 0, -1471067.4420601053 1072102.6240930958 0, -1471084.9119592297 1072083.0136674575 0, -1471149.8958743238 1072010.0676796837 0, -1471169.686926693 1071975.458221037 0, -1471185.7446397934 1071947.3774662255 0, -1471191.014199048 1071944.4186051928 0, -1471238.5183119813 1071917.7511584545 0, -1471265.6666654344 1071902.5108701747 0, -1471274.4209054636 1071887.200852194 0, -1471278.7466788962 1071879.6356260723 0, -1471296.989703434 1071847.7311841731 0, -1471308.5035771825 1071827.5945285535 0, -1471353.3414241585 1071749.173591422 0, -1471377.7734401673 1071695.0394602432 0, -1471403.7738109445 1071637.4303359224 0, -1471417.487194447 1071619.213760118 0, -1471417.4872135872 1071619.213734693 0, -1471417.487201225 1071619.213807906 0, -1471357.9532404982 1071971.7344321162 0, -1471291.97526762 1072367.2269985208 0, -1471233.3349821926 1072718.7248871874 0, -1470875.8215589274 1072659.4750318767 0, -1470837.8882755965 1072653.1753064813 0, -1470564.0167686036 1072607.6787556603 0, -1470480.0344672704 1072593.7316797283 0, -1470443.2019366957 1072587.6164524157 0, -1470501.717346761 1072236.8839539203 0, -1470742.030727121 1072277.0534381503 0, -1470742.6141262976 1072276.6007588662 0, -1470755.1501011455 1072266.8721175815 0, -1470755.160569836 1072266.8667452866 0, -1470914.5565615804 1072183.7348585173 0, -1470915.630194244 1072183.4213640604 0, -1470915.6303725615 1072183.4213119927 0, -1470936.141652446 1072177.4399317813 0)), ((-1543541.3070862177 1103619.7923551688 0, -1543471.132541959 1104017.7834517523 0, -1543400.9577496555 1104415.7772416642 0, -1543006.0432961897 1104346.8944055298 0, -1542611.1258225988 1104278.029424674 0, -1542216.2053443387 1104209.1822154725 0, -1541821.2816412267 1104140.3525668217 0, -1541891.0623570846 1103741.9571706527 0, -1541960.8406521182 1103343.5609588125 0, -1542030.6204919585 1102945.17075705 0, -1542100.397894721 1102546.7798312986 0, -1542506.0434976877 1102617.8469586354 0, -1542891.031893279 1102685.266569184 0, -1543286.3435248125 1102754.5333949034 0, -1543681.6515485584 1102823.8207739855 0, -1543611.4784471707 1103221.8035290584 0, -1543541.3070862177 1103619.7923551688 0)), ((-1541031.6997889671 1104002.9700931194 0, -1541426.4922946573 1104071.6524646548 0, -1541821.2816412267 1104140.3525668217 0, -1541751.4321998972 1104538.6853250435 0, -1541681.5821546402 1104937.020687683 0, -1541611.7292000754 1105335.358075126 0, -1541541.8783516525 1105733.6987909738 0, -1541147.1455730456 1105664.8985450075 0, -1540752.409015931 1105596.119028192 0, -1540357.6699156363 1105527.3541561516 0, -1539962.927386934 1105458.6099880957 0, -1540032.7221898055 1105060.3664764278 0, -1540102.516018427 1104662.1286965127 0, -1540172.31262313 1104263.8909204707 0, -1540242.1056809563 1103865.6583494826 0, -1540636.904306417 1103934.3053977208 0, -1541031.6997889671 1104002.9700931194 0)), ((-1547342.5470469545 1105105.3172569699 0, -1547736.7174885585 1105174.4162607584 0, -1548130.8897205284 1105243.5310519938 0, -1548060.8678122961 1105641.9438446802 0, -1547990.845591878 1106040.3594582863 0, -1547920.8222562352 1106438.780509858 0, -1547850.7990700665 1106837.2012610568 0, -1547456.4951831715 1106768.223853697 0, -1547062.190850597 1106699.2613370114 0, -1546667.8870647282 1106630.3163877751 0, -1546273.5808181057 1106561.3860616495 0, -1546343.735389737 1106162.8282205788 0, -1546413.8895459755 1105764.2729044482 0, -1546484.0432420722 1105365.7203685727 0, -1546554.1965213437 1104967.1703658104 0, -1546948.3745847414 1105036.235184688 0, -1547342.5470469545 1105105.3172569699 0)), ((-1544925.5041916769 1109607.9237952072 0, -1545319.5355561916 1109677.1750844913 0, -1545713.5637185103 1109746.4440474745 0, -1545643.4542684052 1110144.7608742642 0, -1545573.3464333003 1110543.0838364991 0, -1545503.2356032194 1110941.408843005 0, -1545433.1268342147 1111339.7369483036 0, -1545039.3780219888 1111270.3692228715 0, -1544645.6255536773 1111201.0221774443 0, -1544251.8730158529 1111131.690055689 0, -1543858.114337918 1111062.3780925348 0, -1543927.9462834024 1110664.149294424 0, -1543997.7751189044 1110265.9226127006 0, -1544067.6060952437 1109867.6989708967 0, -1544137.4346543443 1109469.47446885 0, -1544531.4722247936 1109538.6905486467 0, -1544925.5041916769 1109607.9237952072 0)), ((-1554405.2545278268 1111272.498635714 0, -1554799.5165985026 1111342.3768666137 0, -1555193.7781950636 1111412.2731964616 0, -1555123.1688681673 1111810.2627474642 0, -1555052.5618014392 1112208.2552869038 0, -1554981.9542989044 1112606.2505076707 0, -1554911.346322231 1113004.2481399179 0, -1554516.8998306491 1112934.6555325433 0, -1554122.4497912938 1112865.083517608 0, -1553727.9945172586 1112795.5255847243 0, -1553333.5387672929 1112725.985938102 0, -1553404.334080606 1112327.6849379858 0, -1553475.1316630514 1111929.3869832251 0, -1553545.92672566 1111531.0880411603 0, -1553616.7208285597 1111132.7948632953 0, -1554010.9892628053 1111202.6378513838 0, -1554405.2545278268 1111272.498635714 0)), ((-1540821.1000858005 1112168.1825631203 0, -1541215.5032202355 1112237.2792268265 0, -1541609.9032414798 1112306.3936171948 0, -1542004.3033178374 1112375.5228378773 0, -1541934.5495534237 1112772.449900413 0, -1541864.7957995613 1113169.3765824386 0, -1541794.959892063 1113566.712271437 0, -1541724.3225457717 1113968.6162074856 0, -1541330.043805838 1113899.592810296 0, -1540935.7625170108 1113830.5839519515 0, -1540541.4782218335 1113761.5927436838 0, -1540147.1908377656 1113692.6191710555 0, -1540217.2359593415 1113293.0274753403 0, -1540287.0020580967 1112895.0324329094 0, -1540293.969427788 1112855.2299344921 0, -1540356.840499805 1112497.065358157 0, -1540426.690660166 1112099.1060898788 0, -1540821.1000858005 1112168.1825631203 0)), ((-1551401.8407411405 1114434.772938361 0, -1551330.3865995212 1114832.6475045364 0, -1551259.116941905 1115230.5009309347 0, -1551187.8501687136 1115628.3542240204 0, -1550793.6599560513 1115558.9526567324 0, -1550399.4663589268 1115489.5688436592 0, -1550005.2672562073 1115420.2021529963 0, -1550076.271549637 1115023.8920869136 0, -1549681.9236549835 1114955.0263259395 0, -1549753.2075992275 1114556.8108446607 0, -1550147.8293315996 1114624.4916593872 0, -1550542.1384665174 1114693.89956495 0, -1550936.1860866265 1114763.6996969578 0, -1551007.6152087408 1114365.6667646584 0, -1551401.8407411405 1114434.772938361 0)), ((-1468601.615686918 1063788.0684754087 0, -1468535.0741829383 1063819.1801463002 0, -1468528.7073578194 1063822.156901392 0, -1468502.7962197405 1063815.116886156 0, -1468478.8746527156 1063808.6175396533 0, -1468449.2881214947 1063800.5789912106 0, -1468442.9888689097 1063784.0807156363 0, -1468439.829466776 1063775.8057579244 0, -1468421.9529369222 1063728.9845745459 0, -1468404.6077661994 1063713.4413278988 0, -1468386.5787986477 1063697.2851857617 0, -1468380.0254448703 1063691.4126946828 0, -1468380.2263475517 1063686.7127644774 0, -1468380.6440963955 1063676.9926941614 0, -1468380.7823417233 1063673.7745473245 0, -1468381.8443519762 1063649.052719897 0, -1468346.1375494022 1063556.7575330944 0, -1468317.0841800172 1063481.6602795522 0, -1468329.5057832773 1063434.8410312023 0, -1468342.4687960234 1063418.9478999262 0, -1468370.2285905408 1063384.9135288724 0, -1468324.6108951883 1063320.050833428 0, -1468267.9457064164 1063668.312438764 0, -1468203.235207649 1064066.018831864 0, -1468202.2296142434 1064065.8513758301 0, -1467806.217504514 1063999.9237172224 0, -1467411.2121480687 1063934.1817103429 0, -1467477.2243056681 1063534.9293142157 0, -1467543.3245041664 1063135.1449674314 0, -1467938.0328198047 1063202.606555877 0, -1468310.5765742206 1063266.2857027552 0, -1468310.493354108 1063265.7262026374 0, -1468299.430669261 1063191.3993355876 0, -1468269.1360545233 1063143.598738911 0, -1468267.0946829505 1063140.37760382 0, -1468268.6419386712 1063133.8673546577 0, -1468303.0320962388 1062989.1658948325 0, -1468291.0004253641 1062903.2223146881 0, -1468283.1774665287 1062847.3650625595 0, -1468276.44473341 1062799.2986169462 0, -1468262.5112827518 1062788.9543413199 0, -1468221.6249826727 1062758.6001392917 0, -1468182.9342007223 1062729.8758430292 0, -1468156.0563180307 1062690.570284065 0, -1468134.0870652439 1062658.4430355995 0, -1468091.8939900987 1062645.5733595616 0, -1468095.7168026776 1062639.8473029989 0, -1468128.8270226016 1062590.2502204191 0, -1468145.7972584725 1062511.2885076145 0, -1468137.2458240753 1062459.9532576003 0, -1468133.217049825 1062435.768283414 0, -1468128.753452802 1062408.9728204876 0, -1468275.6936864364 1062432.9568268014 0, -1468462.9383634143 1062463.5195157197 0, -1468397.3814281551 1062866.4442860573 0, -1468331.8213629937 1063269.3711934362 0, -1468728.933957707 1063337.2484541982 0, -1468663.585502209 1063734.527375787 0, -1468648.5095851193 1063826.1798736842 0, -1468648.5087836666 1063826.1792223651 0, -1468601.615686918 1063788.0684754087 0)), ((-1421359.1801524933 1128875.6618870632 0, -1421397.9136396863 1128638.5764640279 0, -1421793.7105461932 1128701.9811103947 0, -1422189.5053045668 1128765.400406615 0, -1422585.2966508765 1128828.8405849081 0, -1422981.0851674736 1128892.2985640552 0, -1422916.7575563558 1129292.1851313629 0, -1422852.429621718 1129692.0740391351 0, -1422788.1010470921 1130091.9656609993 0, -1422723.7722334596 1130491.8596284604 0, -1422326.996357115 1130428.3045470964 0, -1421930.217321748 1130364.7703960943 0, -1421533.435768656 1130301.2511009213 0, -1421136.6488519546 1130237.7493766856 0, -1421201.9675294298 1129837.952657361 0, -1421267.2832773195 1129438.1580246773 0, -1421332.598651699 1129038.3661222346 0, -1421359.1801524933 1128875.6618870632 0)), ((-1463531.2511565369 1188755.4580101734 0, -1463878.2534497501 1188819.6302599178 0, -1463925.9729624768 1188828.4602397683 0, -1464252.5841480803 1188888.8779839652 0, -1464218.961086378 1189079.4634393838 0, -1464182.1281650877 1189288.2826634783 0, -1464148.823761472 1189477.0754685493 0, -1464111.6387284815 1189687.684161974 0, -1464079.4398876503 1189875.444284027 0, -1464042.8443469862 1190088.8203658739 0, -1464011.0906209366 1190273.9858529842 0, -1463974.1054807615 1190489.971261184 0, -1463942.789895234 1190672.5847379053 0, -1463905.3137727934 1190891.1094552637 0, -1463874.4321903992 1191071.1799009135 0, -1463836.5753381876 1191292.2589637707 0, -1463805.9690807331 1191470.7492246598 0, -1463767.8193811495 1191693.2164027032 0, -1463737.4496221736 1191870.3116050353 0, -1463699.113780784 1192094.187835412 0, -1463669.3997288202 1192269.923682783 0, -1463631.1804678114 1192495.972765815 0, -1463601.8214305053 1192669.620079111 0, -1463563.312638796 1192897.7740814928 0, -1463537.505330424 1193050.5814795904 0, -1463495.447004275 1193299.609727551 0, -1463473.1654610978 1193431.544148446 0, -1463467.131492647 1193467.310729348 0, -1463427.6110615314 1193701.4559220355 0, -1463039.2211346093 1193635.722932426 0, -1462645.9246733896 1193569.1766679846 0, -1462253.454596295 1193502.8059261336 0, -1461860.9809928942 1193436.4558941543 0, -1461465.775915477 1193369.3309087444 0, -1461070.5640771105 1193302.2260083114 0, -1460675.35166836 1193235.136159324 0, -1460280.1361796057 1193168.064190211 0, -1460348.9189877973 1192767.698412689 0, -1460417.7015962275 1192367.3348493075 0, -1460486.4818340528 1191966.9702349345 0, -1460555.2638886233 1191566.6115144724 0, -1460624.0968877587 1191166.1222483744 0, -1460654.4481674843 1190989.5241129396 0, -1460693.2947347267 1190763.8966812813 0, -1460762.377094276 1190362.6558866268 0, -1460830.8908553687 1189964.7186480425 0, -1460831.4597193555 1189961.4146086725 0, -1460901.5247094124 1189558.979539018 0, -1460971.5867955305 1189156.546415844 0, -1461041.6488833523 1188754.1159524126 0, -1461111.7107887138 1188351.6875538416 0, -1461161.8645205796 1188359.784572451 0, -1461508.6275839764 1188415.9339920308 0, -1461557.0486800568 1188423.7750625198 0, -1461651.9767357516 1188439.150442345 0, -1461902.7596882635 1188479.8964200392 0, -1461949.4038208523 1188487.8258685207 0, -1462297.8634997874 1188547.408902159 0, -1462344.1805670052 1188555.3295843522 0, -1462692.9540936335 1188614.9808260715 0, -1462738.9863454103 1188622.6580232498 0, -1463089.285219863 1188680.994359118 0, -1463135.1887863597 1188688.6396737194 0, -1463485.61233791 1188747.0162844344 0, -1463531.2511565369 1188755.4580101734 0)))</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Standing Rock</t>
+          <t>Tohono O'odham</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Rural Credit, School and Public Lands, Indemnity, BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, ND SCHOOL OF SCIENCE, CAPITOL BUILDING, VETERANS HOME, MAYVILLE, SCHOOL OF MINES, UNIVERSITY OF ND, ND INDUSTRIAL SCHOOL, ND STATE UNIVERSITY, NDÔøΩSTATEÔøΩUNIVERSITY, ELLENDALE, SCHOOL FOR THE DEAF, STATEÔøΩHOSPITAL, VALLEY/MAYVILLE</t>
+          <t>COUNTY BOND, UNIVERSITY, ST CHRTBL, PENAL &amp; REFORM INST, PERM COMMON SCHLS, SCHOOL OF MINES</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>739</v>
+        <v>33</v>
       </c>
       <c r="G68" t="n">
-        <v>46823.4</v>
+        <v>4903.52</v>
       </c>
       <c r="H68" t="n">
-        <v>217</v>
+        <v>12</v>
       </c>
       <c r="I68" t="n">
-        <v>70165.38</v>
+        <v>9707.76</v>
       </c>
       <c r="J68" t="n">
-        <v>522</v>
+        <v>21</v>
       </c>
       <c r="K68" t="n">
-        <v>116988.78</v>
+        <v>14611.28</v>
       </c>
       <c r="L68" t="n">
-        <v>2347732.03</v>
+        <v>2781661.64</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1468861.5102881684 1062529.544672667 0, -1469017.6210793862 1062555.4110563563 0, -1469129.974785093 1062574.0271501057 0, -1469252.449893471 1062594.3203348885 0, -1469260.0823487265 1062595.5851217243 0, -1469260.0823599044 1062595.5851235767 0, -1469283.173707292 1062599.3663462314 0, -1469642.2312759976 1062658.1631362855 0, -1469644.5357929508 1062658.5420150517 0, -1470024.3775152052 1062720.757761455 0, -1470028.9553121778 1062721.5178974674 0, -1470036.614696355 1062722.7897407915 0, -1470413.0803005649 1062785.259044958 0, -1470413.5090985568 1062785.330216005 0, -1470434.6009114378 1062788.8311073242 0, -1470777.6770908916 1062845.7735343892 0, -1470801.778692093 1062849.7738462705 0, -1470801.7786950548 1062849.7738467618 0, -1470735.291818363 1063247.297021072 0, -1470668.8077412983 1063644.8202214376 0, -1470665.5165512266 1063664.7246222931 0, -1470605.4089253014 1064049.9390719912 0, -1470542.1933719711 1064455.0913720988 0, -1470530.2911529467 1064547.6087893152 0, -1470466.8251287101 1064585.819113063 0, -1470398.8492705273 1064609.9058296997 0, -1470344.2676615152 1064659.9695127506 0, -1470220.7824153055 1064712.4227236935 0, -1470117.9772717974 1064680.9654987962 0, -1470074.4194187138 1064667.6356037075 0, -1470012.878171736 1064611.9488686554 0, -1469981.2567014096 1064594.0036470143 0, -1469904.9436335918 1064618.4355588462 0, -1469867.456967431 1064598.6590498888 0, -1469791.4959079553 1064500.8642470355 0, -1469804.9585004586 1064475.2900794114 0, -1469821.834112315 1064443.2326686454 0, -1469816.7249291502 1064384.524520883 0, -1469812.9904894084 1064341.6145040721 0, -1469811.1894333242 1064334.735605513 0, -1469777.605131138 1064329.0661652733 0, -1469777.6873496468 1064328.532624977 0, -1469789.4935049256 1064251.9189805745 0, -1469789.5006117246 1064251.8726492473 0, -1469789.3708321552 1064251.376711911 0, -1469788.5747998857 1064251.2162895089 0, -1469778.0141272878 1064249.0808299128 0, -1469702.6319516078 1064233.836271017 0, -1469700.7072090243 1064222.2691301936 0, -1469695.323318651 1064189.9152719344 0, -1469641.0308777792 1064172.5543810064 0, -1469589.9364842195 1064156.2161513732 0, -1469580.2220810633 1064136.1836904322 0, -1469578.3887855369 1064132.403009833 0, -1469563.6640393788 1064102.0375518142 0, -1469560.8188364026 1064096.1700240073 0, -1469550.9424646862 1064090.5682925836 0, -1469522.6027439218 1064074.4942171515 0, -1469521.7376082265 1064074.0035687736 0, -1469518.792243473 1064072.332889826 0, -1469518.7249020224 1064072.1973674642 0, -1469494.5615439934 1064023.4539504591 0, -1469427.7809926695 1063998.8150870206 0, -1469395.786498048 1063987.0116526512 0, -1469375.6931782574 1063979.5989675557 0, -1469371.6734833296 1063966.9701128954 0, -1469341.9620892713 1063873.6258968175 0, -1469306.706696515 1063841.1826290756 0, -1469298.967764853 1063834.0602172774 0, -1469289.7784527813 1063838.4524427834 0, -1469276.536821521 1063844.783336913 0, -1469257.2328571894 1063854.0131332797 0, -1469192.3475694433 1063920.157510396 0, -1469161.8019355591 1063932.9952806323 0, -1469149.7209660907 1063938.0728865312 0, -1469137.7064038394 1063951.7945904187 0, -1469108.5820747924 1063985.057432164 0, -1469030.5227920236 1063979.090286098 0, -1469030.5227943866 1063979.0902718552 0, -1469060.0896770647 1063801.4349766506 0, -1469126.045451578 1063405.13122767 0, -1468728.933957707 1063337.2484541982 0, -1468795.2218783214 1062933.398209418 0, -1468857.7885759312 1062528.9281126044 0, -1468861.5102726147 1062529.544767426 0, -1468861.5102881684 1062529.544672667 0)), ((-1470936.141652446 1072177.4399317813 0, -1470956.609938698 1072171.470867857 0, -1470975.5339946318 1072165.9522729167 0, -1470976.333474576 1072165.4015191253 0, -1471017.5148884433 1072137.0258263568 0, -1471050.386111551 1072114.3762780975 0, -1471067.4420601053 1072102.6240930958 0, -1471084.9119592297 1072083.0136674575 0, -1471149.8958743238 1072010.0676796837 0, -1471169.686926693 1071975.458221037 0, -1471185.7446397934 1071947.3774662255 0, -1471191.014199048 1071944.4186051928 0, -1471238.5183119813 1071917.7511584545 0, -1471265.6666654344 1071902.5108701747 0, -1471274.4209054636 1071887.200852194 0, -1471278.7466788962 1071879.6356260723 0, -1471296.989703434 1071847.7311841731 0, -1471308.5035771825 1071827.5945285535 0, -1471353.3414241585 1071749.173591422 0, -1471377.7734401673 1071695.0394602432 0, -1471403.7738109445 1071637.4303359224 0, -1471417.487194447 1071619.213760118 0, -1471417.4872135872 1071619.213734693 0, -1471417.487201225 1071619.213807906 0, -1471357.9532404982 1071971.7344321162 0, -1471291.97526762 1072367.2269985208 0, -1471233.3349821926 1072718.7248871874 0, -1470875.8215589274 1072659.4750318767 0, -1470837.8882755965 1072653.1753064813 0, -1470564.0167686036 1072607.6787556603 0, -1470480.0344672704 1072593.7316797283 0, -1470443.2019366957 1072587.6164524157 0, -1470501.717346761 1072236.8839539203 0, -1470742.030727121 1072277.0534381503 0, -1470742.6141262976 1072276.6007588662 0, -1470755.1501011455 1072266.8721175815 0, -1470755.160569836 1072266.8667452866 0, -1470914.5565615804 1072183.7348585173 0, -1470915.630194244 1072183.4213640604 0, -1470915.6303725615 1072183.4213119927 0, -1470936.141652446 1072177.4399317813 0)), ((-1543541.3070862177 1103619.7923551688 0, -1543471.132541959 1104017.7834517523 0, -1543400.9577496555 1104415.7772416642 0, -1543006.0432961897 1104346.8944055298 0, -1542611.1258225988 1104278.029424674 0, -1542216.2053443387 1104209.1822154725 0, -1541821.2816412267 1104140.3525668217 0, -1541891.0623570846 1103741.9571706527 0, -1541960.8406521182 1103343.5609588125 0, -1542030.6204919585 1102945.17075705 0, -1542100.397894721 1102546.7798312986 0, -1542506.0434976877 1102617.8469586354 0, -1542891.031893279 1102685.266569184 0, -1543286.3435248125 1102754.5333949034 0, -1543681.6515485584 1102823.8207739855 0, -1543611.4784471707 1103221.8035290584 0, -1543541.3070862177 1103619.7923551688 0)), ((-1541031.6997889671 1104002.9700931194 0, -1541426.4922946573 1104071.6524646548 0, -1541821.2816412267 1104140.3525668217 0, -1541751.4321998972 1104538.6853250435 0, -1541681.5821546402 1104937.020687683 0, -1541611.7292000754 1105335.358075126 0, -1541541.8783516525 1105733.6987909738 0, -1541147.1455730456 1105664.8985450075 0, -1540752.409015931 1105596.119028192 0, -1540357.6699156363 1105527.3541561516 0, -1539962.927386934 1105458.6099880957 0, -1540032.7221898055 1105060.3664764278 0, -1540102.516018427 1104662.1286965127 0, -1540172.31262313 1104263.8909204707 0, -1540242.1056809563 1103865.6583494826 0, -1540636.904306417 1103934.3053977208 0, -1541031.6997889671 1104002.9700931194 0)), ((-1547342.5470469545 1105105.3172569699 0, -1547736.7174885585 1105174.4162607584 0, -1548130.8897205284 1105243.5310519938 0, -1548060.8678122961 1105641.9438446802 0, -1547990.845591878 1106040.3594582863 0, -1547920.8222562352 1106438.780509858 0, -1547850.7990700665 1106837.2012610568 0, -1547456.4951831715 1106768.223853697 0, -1547062.190850597 1106699.2613370114 0, -1546667.8870647282 1106630.3163877751 0, -1546273.5808181057 1106561.3860616495 0, -1546343.735389737 1106162.8282205788 0, -1546413.8895459755 1105764.2729044482 0, -1546484.0432420722 1105365.7203685727 0, -1546554.1965213437 1104967.1703658104 0, -1546948.3745847414 1105036.235184688 0, -1547342.5470469545 1105105.3172569699 0)), ((-1544925.5041916769 1109607.9237952072 0, -1545319.5355561916 1109677.1750844913 0, -1545713.5637185103 1109746.4440474745 0, -1545643.4542684052 1110144.7608742642 0, -1545573.3464333003 1110543.0838364991 0, -1545503.2356032194 1110941.408843005 0, -1545433.1268342147 1111339.7369483036 0, -1545039.3780219888 1111270.3692228715 0, -1544645.6255536773 1111201.0221774443 0, -1544251.8730158529 1111131.690055689 0, -1543858.114337918 1111062.3780925348 0, -1543927.9462834024 1110664.149294424 0, -1543997.7751189044 1110265.9226127006 0, -1544067.6060952437 1109867.6989708967 0, -1544137.4346543443 1109469.47446885 0, -1544531.4722247936 1109538.6905486467 0, -1544925.5041916769 1109607.9237952072 0)), ((-1554405.2545278268 1111272.498635714 0, -1554799.5165985026 1111342.3768666137 0, -1555193.7781950636 1111412.2731964616 0, -1555123.1688681673 1111810.2627474642 0, -1555052.5618014392 1112208.2552869038 0, -1554981.9542989044 1112606.2505076707 0, -1554911.346322231 1113004.2481399179 0, -1554516.8998306491 1112934.6555325433 0, -1554122.4497912938 1112865.083517608 0, -1553727.9945172586 1112795.5255847243 0, -1553333.5387672929 1112725.985938102 0, -1553404.334080606 1112327.6849379858 0, -1553475.1316630514 1111929.3869832251 0, -1553545.92672566 1111531.0880411603 0, -1553616.7208285597 1111132.7948632953 0, -1554010.9892628053 1111202.6378513838 0, -1554405.2545278268 1111272.498635714 0)), ((-1540821.1000858005 1112168.1825631203 0, -1541215.5032202355 1112237.2792268265 0, -1541609.9032414798 1112306.3936171948 0, -1542004.3033178374 1112375.5228378773 0, -1541934.5495534237 1112772.449900413 0, -1541864.7957995613 1113169.3765824386 0, -1541794.959892063 1113566.712271437 0, -1541724.3225457717 1113968.6162074856 0, -1541330.043805838 1113899.592810296 0, -1540935.7625170108 1113830.5839519515 0, -1540541.4782218335 1113761.5927436838 0, -1540147.1908377656 1113692.6191710555 0, -1540217.2359593415 1113293.0274753403 0, -1540287.0020580967 1112895.0324329094 0, -1540293.969427788 1112855.2299344921 0, -1540356.840499805 1112497.065358157 0, -1540426.690660166 1112099.1060898788 0, -1540821.1000858005 1112168.1825631203 0)), ((-1551401.8407411405 1114434.772938361 0, -1551330.3865995212 1114832.6475045364 0, -1551259.116941905 1115230.5009309347 0, -1551187.8501687136 1115628.3542240204 0, -1550793.6599560513 1115558.9526567324 0, -1550399.4663589268 1115489.5688436592 0, -1550005.2672562073 1115420.2021529963 0, -1550076.271549637 1115023.8920869136 0, -1549681.9236549835 1114955.0263259395 0, -1549753.2075992275 1114556.8108446607 0, -1550147.8293315996 1114624.4916593872 0, -1550542.1384665174 1114693.89956495 0, -1550936.1860866265 1114763.6996969578 0, -1551007.6152087408 1114365.6667646584 0, -1551401.8407411405 1114434.772938361 0)), ((-1468601.615686918 1063788.0684754087 0, -1468535.0741829383 1063819.1801463002 0, -1468528.7073578194 1063822.156901392 0, -1468502.7962197405 1063815.116886156 0, -1468478.8746527156 1063808.6175396533 0, -1468449.2881214947 1063800.5789912106 0, -1468442.9888689097 1063784.0807156363 0, -1468439.829466776 1063775.8057579244 0, -1468421.9529369222 1063728.9845745459 0, -1468404.6077661994 1063713.4413278988 0, -1468386.5787986477 1063697.2851857617 0, -1468380.0254448703 1063691.4126946828 0, -1468380.2263475517 1063686.7127644774 0, -1468380.6440963955 1063676.9926941614 0, -1468380.7823417233 1063673.7745473245 0, -1468381.8443519762 1063649.052719897 0, -1468346.1375494022 1063556.7575330944 0, -1468317.0841800172 1063481.6602795522 0, -1468329.5057832773 1063434.8410312023 0, -1468342.4687960234 1063418.9478999262 0, -1468370.2285905408 1063384.9135288724 0, -1468324.6108951883 1063320.050833428 0, -1468267.9457064164 1063668.312438764 0, -1468203.235207649 1064066.018831864 0, -1468202.2296142434 1064065.8513758301 0, -1467806.217504514 1063999.9237172224 0, -1467411.2121480687 1063934.1817103429 0, -1467477.2243056681 1063534.9293142157 0, -1467543.3245041664 1063135.1449674314 0, -1467938.0328198047 1063202.606555877 0, -1468310.5765742206 1063266.2857027552 0, -1468310.493354108 1063265.7262026374 0, -1468299.430669261 1063191.3993355876 0, -1468269.1360545233 1063143.598738911 0, -1468267.0946829505 1063140.37760382 0, -1468268.6419386712 1063133.8673546577 0, -1468303.0320962388 1062989.1658948325 0, -1468291.0004253641 1062903.2223146881 0, -1468283.1774665287 1062847.3650625595 0, -1468276.44473341 1062799.2986169462 0, -1468262.5112827518 1062788.9543413199 0, -1468221.6249826727 1062758.6001392917 0, -1468182.9342007223 1062729.8758430292 0, -1468156.0563180307 1062690.570284065 0, -1468134.0870652439 1062658.4430355995 0, -1468091.8939900987 1062645.5733595616 0, -1468095.7168026776 1062639.8473029989 0, -1468128.8270226016 1062590.2502204191 0, -1468145.7972584725 1062511.2885076145 0, -1468137.2458240753 1062459.9532576003 0, -1468133.217049825 1062435.768283414 0, -1468128.753452802 1062408.9728204876 0, -1468275.6936864364 1062432.9568268014 0, -1468462.9383634143 1062463.5195157197 0, -1468397.3814281551 1062866.4442860573 0, -1468331.8213629937 1063269.3711934362 0, -1468728.933957707 1063337.2484541982 0, -1468663.585502209 1063734.527375787 0, -1468648.5095851193 1063826.1798736842 0, -1468648.5087836666 1063826.1792223651 0, -1468601.615686918 1063788.0684754087 0)), ((-1421359.1801524933 1128875.6618870632 0, -1421397.9136396863 1128638.5764640279 0, -1421793.7105461932 1128701.9811103947 0, -1422189.5053045668 1128765.400406615 0, -1422585.2966508765 1128828.8405849081 0, -1422981.0851674736 1128892.2985640552 0, -1422916.7575563558 1129292.1851313629 0, -1422852.429621718 1129692.0740391351 0, -1422788.1010470921 1130091.9656609993 0, -1422723.7722334596 1130491.8596284604 0, -1422326.996357115 1130428.3045470964 0, -1421930.217321748 1130364.7703960943 0, -1421533.435768656 1130301.2511009213 0, -1421136.6488519546 1130237.7493766856 0, -1421201.9675294298 1129837.952657361 0, -1421267.2832773195 1129438.1580246773 0, -1421332.598651699 1129038.3661222346 0, -1421359.1801524933 1128875.6618870632 0)), ((-1463531.2511565369 1188755.4580101734 0, -1463878.2534497501 1188819.6302599178 0, -1463925.9729624768 1188828.4602397683 0, -1464252.5841480803 1188888.8779839652 0, -1464218.961086378 1189079.4634393838 0, -1464182.1281650877 1189288.2826634783 0, -1464148.823761472 1189477.0754685493 0, -1464111.6387284815 1189687.684161974 0, -1464079.4398876503 1189875.444284027 0, -1464042.8443469862 1190088.8203658739 0, -1464011.0906209366 1190273.9858529842 0, -1463974.1054807615 1190489.971261184 0, -1463942.789895234 1190672.5847379053 0, -1463905.3137727934 1190891.1094552637 0, -1463874.4321903992 1191071.1799009135 0, -1463836.5753381876 1191292.2589637707 0, -1463805.9690807331 1191470.7492246598 0, -1463767.8193811495 1191693.2164027032 0, -1463737.4496221736 1191870.3116050353 0, -1463699.113780784 1192094.187835412 0, -1463669.3997288202 1192269.923682783 0, -1463631.1804678114 1192495.972765815 0, -1463601.8214305053 1192669.620079111 0, -1463563.312638796 1192897.7740814928 0, -1463537.505330424 1193050.5814795904 0, -1463495.447004275 1193299.609727551 0, -1463473.1654610978 1193431.544148446 0, -1463467.131492647 1193467.310729348 0, -1463427.6110615314 1193701.4559220355 0, -1463039.2211346093 1193635.722932426 0, -1462645.9246733896 1193569.1766679846 0, -1462253.454596295 1193502.8059261336 0, -1461860.9809928942 1193436.4558941543 0, -1461465.775915477 1193369.3309087444 0, -1461070.5640771105 1193302.2260083114 0, -1460675.35166836 1193235.136159324 0, -1460280.1361796057 1193168.064190211 0, -1460348.9189877973 1192767.698412689 0, -1460417.7015962275 1192367.3348493075 0, -1460486.4818340528 1191966.9702349345 0, -1460555.2638886233 1191566.6115144724 0, -1460624.0968877587 1191166.1222483744 0, -1460654.4481674843 1190989.5241129396 0, -1460693.2947347267 1190763.8966812813 0, -1460762.377094276 1190362.6558866268 0, -1460830.8908553687 1189964.7186480425 0, -1460831.4597193555 1189961.4146086725 0, -1460901.5247094124 1189558.979539018 0, -1460971.5867955305 1189156.546415844 0, -1461041.6488833523 1188754.1159524126 0, -1461111.7107887138 1188351.6875538416 0, -1461161.8645205796 1188359.784572451 0, -1461508.6275839764 1188415.9339920308 0, -1461557.0486800568 1188423.7750625198 0, -1461651.9767357516 1188439.150442345 0, -1461902.7596882635 1188479.8964200392 0, -1461949.4038208523 1188487.8258685207 0, -1462297.8634997874 1188547.408902159 0, -1462344.1805670052 1188555.3295843522 0, -1462692.9540936335 1188614.9808260715 0, -1462738.9863454103 1188622.6580232498 0, -1463089.285219863 1188680.994359118 0, -1463135.1887863597 1188688.6396737194 0, -1463485.61233791 1188747.0162844344 0, -1463531.2511565369 1188755.4580101734 0)))</t>
+          <t>MULTIPOLYGON Z (((-126428.62322647788 1506590.4673863722 0, -126419.5078889794 1506995.0315194267 0, -126013.29182701427 1506990.0060043542 0, -125615.9628336914 1506985.244362261 0, -125218.6161798179 1506980.4788590758 0, -124839.35714439845 1506976.0109209418 0, -124846.02256163236 1506571.3431001147 0, -124852.72540050365 1506164.1532511492 0, -125229.91695981652 1506169.7056386427 0, -125609.17162482155 1506175.2883957503 0, -125628.21110767208 1506175.5707156293 0, -126026.51557175932 1506181.4768249998 0, -126437.7088187951 1506187.5740508868 0, -126428.62322647788 1506590.4673863722 0)), ((-126328.47366274262 1512654.7900340538 0, -125925.11772182248 1512656.1815480343 0, -125528.95547502476 1512657.5649384318 0, -125132.83774524032 1512658.9789293592 0, -124746.9258310655 1512660.3609926691 0, -124751.6730561306 1512248.1914185893 0, -124756.35842910505 1511841.9823246961 0, -125144.36193426771 1511843.644976366 0, -125540.86080873317 1511845.37364449 0, -125546.79751200859 1511439.7551722657 0, -125150.13354273964 1511437.72160729 0, -124761.03469939323 1511435.7739310288 0, -124765.75185726258 1511026.2057185778 0, -125155.92106849636 1511030.7236763998 0, -125552.7341746498 1511035.3250618821 0, -125949.5470047659 1511039.9563562071 0, -126348.57424852277 1511044.6283226218 0, -126343.58969136687 1511443.8854637193 0, -126338.53614343535 1511848.9123334696 0, -126333.47375256877 1512253.9286938282 0, -126328.47366274262 1512654.7900340538 0)), ((-126268.68125744934 1515917.5458290786 0, -126270.36793947153 1516325.9654369245 0, -126272.04018153538 1516732.346466401 0, -126273.70401740653 1517138.0558186683 0, -126275.36985405014 1517541.8166029404 0, -125867.81269531592 1517534.8634892956 0, -125468.27418382304 1517528.0608032343 0, -125068.73533762619 1517521.2771920671 0, -124676.36541358086 1517514.6297736473 0, -124676.58106027775 1517118.5400189376 0, -124676.80695083256 1516712.7707200558 0, -125072.12608191653 1516717.7020674224 0, -125472.88230528434 1516722.5874150866 0, -125475.24808324069 1516316.5699905695 0, -125477.62148531683 1515910.0156483965 0, -125877.44107624413 1515913.8075593114 0, -126268.68125744934 1515917.5458290786 0)), ((-126224.89516022889 1521194.6489400552 0, -126217.79956318598 1521599.372847899 0, -126210.71311489711 1522004.0752571216 0, -126203.5678509434 1522411.533865739 0, -125809.20984091918 1522408.6090121903 0, -125410.36621002032 1522405.6806337943 0, -125011.52270265628 1522402.76000022 0, -124618.70411357592 1522399.9026395646 0, -124622.13115635276 1521982.047332273 0, -124625.46167313609 1521577.2445741813 0, -124628.78268918867 1521172.464893381 0, -124632.09194657534 1520769.0639375413 0, -125034.69622160662 1520774.194629696 0, -125434.06195500019 1520779.296377248 0, -125833.42755836768 1520784.417087296 0, -126231.99660111818 1520789.5449003836 0, -126224.89516022889 1521194.6489400552 0)), ((-120847.64143212377 1506105.5732457587 0, -120844.3304654017 1506520.8640379936 0, -120445.64522029008 1506516.708205814 0, -120449.20874109371 1506101.6004871374 0, -120462.5576369535 1506101.7238225874 0, -120847.64143212377 1506105.5732457587 0)), ((-121240.08536453794 1506930.3648465348 0, -121243.02427341757 1506525.0500728537 0, -121666.25969838328 1506529.5528248027 0, -121660.75708829418 1506934.819746684 0, -121240.08536453794 1506930.3648465348 0)), ((-120837.94142515396 1507331.464363735 0, -120841.13574773929 1506926.1861657395 0, -121240.08536453794 1506930.3648465348 0, -121237.14669844387 1507335.647000029 0, -120837.94142515396 1507331.464363735 0)), ((-120374.48354121138 1511780.0335297228 0, -120382.1560054831 1511375.079419753 0, -120782.70172135768 1511379.9353246607 0, -121183.24702740194 1511384.832745308 0, -121175.54034185561 1511789.4950272364 0, -121167.83391822259 1512194.1468786737 0, -120767.3225307569 1512189.563704962 0, -120775.02066180098 1511784.766116763 0, -120374.48354121138 1511780.0335297228 0)), ((-120707.8534847224 1515856.5487732443 0, -120702.4572395265 1516259.605987525 0, -120697.05644867805 1516665.442556123 0, -120691.63862696686 1517071.2348002568 0, -120686.17998507353 1517480.4781508537 0, -120288.620272845 1517476.4821538334 0, -119893.47711048658 1517472.5168218843 0, -119899.96158757615 1517066.2460947693 0, -119906.4623708097 1516658.8336174053 0, -119912.96324728672 1516251.4220112301 0, -119919.33105734637 1515852.0985516747 0, -120311.13087643796 1515854.3016815225 0, -120707.8534847224 1515856.5487732443 0)), ((-121423.27919263708 1521123.6379134287 0, -121418.10893474067 1521529.2408057053 0, -121826.29440331022 1521536.1366622106 0, -122224.86296199447 1521542.9015232115 0, -122220.13127017854 1521948.5342373766 0, -122215.45736674874 1522350.1908891867 0, -121815.89131574231 1522342.234943161 0, -121407.84184039342 1522334.1419623222 0, -121018.52061237377 1522336.06356573 0, -120620.82032566948 1522338.0399300922 0, -120223.12029071625 1522340.0462541622 0, -119814.56364879261 1522342.1186002165 0, -119821.43015230344 1521932.5722585346 0, -119828.23087917826 1521527.653247194 0, -119835.02279326417 1521122.7348988163 0, -119841.69247015512 1520725.1543634795 0, -120244.46853500957 1520723.1114406264 0, -120642.7226717468 1520721.1014950145 0, -121040.99494318612 1520719.1106676604 0, -121428.46142744238 1520717.1956556789 0, -121423.27919263708 1521123.6379134287 0)), ((-116471.45640800915 1506060.2624132033 0, -116594.54191503269 1506061.0267343943 0, -116882.40405810311 1506065.8006737737 0, -116889.51687631683 1506065.9232600555 0, -116885.6696075123 1506463.6173947568 0, -116881.76229939541 1506867.5384234276 0, -116467.95463077669 1506861.6245820164 0, -116469.72981176751 1506457.2484630274 0, -116071.6503314145 1506451.0002098747 0, -116073.25528882556 1506056.8939392562 0, -116189.72593021201 1506058.2336734035 0, -116335.80511972874 1506059.1296684262 0, -116354.05844230119 1506059.7179110707 0, -116388.71931142654 1506059.7486425918 0, -116471.45640800915 1506060.2624132033 0)), ((-120054.01589803868 1507323.6422674174 0, -120064.85478750731 1506918.5741732598 0, -120075.69404072672 1506513.5179867279 0, -120445.64522029008 1506516.708205814 0, -120442.1863253491 1506922.003984145 0, -120438.73599286917 1507327.3119527982 0, -120054.01589803868 1507323.6422674174 0)), ((-116068.32066701987 1507260.6183581767 0, -116066.55903039787 1507671.7629631455 0, -115668.82447392556 1507665.8735412485 0, -115285.09936666551 1507660.2167836893 0, -115288.32614014135 1507249.9890117033 0, -115291.51705574054 1506844.2990662323 0, -115672.01610032438 1506850.0344130418 0, -116069.98528544577 1506855.83690274 0, -116068.32066701987 1507260.6183581767 0)), ((-116846.39151474854 1510924.704217221 0, -116845.16462299743 1511324.9405872498 0, -116843.9271629774 1511729.7374744387 0, -116842.68046339208 1512134.5351659828 0, -116841.42182462315 1512545.260208008 0, -116426.63213803283 1512538.220543904 0, -116029.19096976993 1512531.4961158284 0, -115792.77013346601 1512527.5053387107 0, -115861.56410122562 1512116.4430048715 0, -115874.71515635849 1512039.5643073677 0, -115824.2898662478 1511712.8981180622 0, -115800.93082433454 1511561.5284411449 0, -115707.14755079916 1511430.8375939096 0, -115638.51462219845 1511394.1334878106 0, -115464.3698573541 1511301.0411959954 0, -115243.8402278692 1511181.561052207 0, -115245.96735315837 1510911.1889799149 0, -115642.91094529454 1510914.5070823168 0, -116041.67928666784 1510917.8690668375 0, -116440.43872641968 1510921.2497684301 0, -116846.39151474854 1510924.704217221 0)), ((-119984.91059292722 1511775.5321362126 0, -120374.48354121138 1511780.0335297228 0, -120366.82009955254 1512184.9886002117 0, -119977.45822824458 1512180.6582820406 0, -119984.91059292722 1511775.5321362126 0)), ((-116663.71292682382 1522325.186876025 0, -116273.24848322617 1522314.3152888955 0, -115877.1758424719 1522303.3061685655 0, -115480.91674428737 1522292.3131322623 0, -115079.40322824946 1522281.188541352 0, -115084.04238776764 1521866.3125016468 0, -115088.59057512072 1521460.6571707528 0, -115093.12967776295 1521055.013615643 0, -115097.57815085424 1520657.2685002252 0, -115500.7912924653 1520667.5419716476 0, -115899.46532991882 1520677.7273618353 0, -116298.12107991171 1520687.9203425033 0, -116694.44956562693 1520698.0774491972 0, -116687.05813663924 1521089.4854640688 0, -116679.37966499559 1521495.8478743378 0, -116671.701530671 1521902.1999256238 0, -116663.71292682382 1522325.186876025 0)), ((-111693.47827975018 1506791.7373515991 0, -111690.67166922861 1507196.837033738 0, -111291.84376854908 1507191.0281420343 0, -111295.02150904168 1506785.9000619962 0, -111298.19956011556 1506380.739163877 0, -110900.09626867746 1506374.880627077 0, -110526.69017948666 1506369.3524212283 0, -110531.69889082109 1505988.0124887344 0, -110903.36823473191 1505992.0725870694 0, -111301.12811380504 1505996.4363694172 0, -111698.88782772499 1506000.8188656422 0, -112110.03137877685 1506005.3643421577 0, -112109.39633769491 1506392.4092545758 0, -112108.73343015161 1506797.480731412 0, -111693.47827975018 1506791.7373515991 0)), ((-115294.70735200212 1506438.632235053 0, -115297.80474291745 1506044.632829943 0, -115298.11684014743 1506044.6370991848 0, -115507.43099867749 1506049.857698452 0, -115675.06780216953 1506050.369341692 0, -115673.57021314393 1506444.781974076 0, -115294.70735200212 1506438.632235053 0)), ((-110893.03322813392 1507185.238518913 0, -111291.84376854908 1507191.0281420343 0, -111288.49301764238 1507615.2455195594 0, -110889.2896443036 1507612.5313155309 0, -110510.39547663584 1507609.9780101487 0, -110516.04636656727 1507179.7414623227 0, -110893.03322813392 1507185.238518913 0)), ((-111687.6964802307 1507617.967321089 0, -111690.67166922861 1507196.837033738 0, -112108.07038293855 1507202.5305956076 0, -112107.38954065862 1507620.857122165 0, -111687.6964802307 1507617.967321089 0)), ((-115239.74303067155 1511703.0603429652 0, -115629.54393633179 1511709.641905785 0, -115635.44894134508 1511735.704398272 0, -115706.24141109285 1512047.9832236923 0, -115704.1622780216 1512113.4742729727 0, -115632.96689429639 1512112.1387424502 0, -115236.58908618204 1512104.6040311817 0, -115239.74303067155 1511703.0603429652 0)), ((-111914.36779684611 1520593.843441507 0, -111907.99874313743 1520996.2340475866 0, -111901.57447392131 1521402.1091506225 0, -111895.15037167615 1521807.9851056247 0, -111888.66682726864 1522217.659301615 0, -111493.40769582988 1522213.6686086245 0, -111095.11402961217 1522209.667588022 0, -110696.82028878036 1522205.6855196028 0, -110303.8783094667 1522201.780405798 0, -110307.50071021168 1521797.9286285667 0, -110311.14072355286 1521392.0498372915 0, -110314.78940902809 1520986.172076282 0, -110318.38811167254 1520584.764788481 0, -110720.25922364488 1520587.0278309209 0, -111118.56376665241 1520589.2843575063 0, -111516.86848876557 1520591.5486326523 0, -111914.36779684611 1520593.843441507 0)))</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Tohono O'odham</t>
+          <t>Tonkawa</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>COUNTY BOND, UNIVERSITY, ST CHRTBL, PENAL &amp; REFORM INST, PERM COMMON SCHLS, SCHOOL OF MINES</t>
+          <t>Public Building, Common Schools, Oklahoma State University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>33</v>
+        <v>152</v>
       </c>
       <c r="G69" t="n">
-        <v>4903.52</v>
+        <v>186.91</v>
       </c>
       <c r="H69" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I69" t="n">
-        <v>9707.76</v>
+        <v>5810.78</v>
       </c>
       <c r="J69" t="n">
-        <v>21</v>
+        <v>146</v>
       </c>
       <c r="K69" t="n">
-        <v>14611.28</v>
+        <v>5997.69</v>
       </c>
       <c r="L69" t="n">
-        <v>2781661.64</v>
+        <v>91880.64999999999</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-126428.62322647788 1506590.4673863722 0, -126419.5078889794 1506995.0315194267 0, -126013.29182701427 1506990.0060043542 0, -125615.9628336914 1506985.244362261 0, -125218.6161798179 1506980.4788590758 0, -124839.35714439845 1506976.0109209418 0, -124846.02256163236 1506571.3431001147 0, -124852.72540050365 1506164.1532511492 0, -125229.91695981652 1506169.7056386427 0, -125609.17162482155 1506175.2883957503 0, -125628.21110767208 1506175.5707156293 0, -126026.51557175932 1506181.4768249998 0, -126437.7088187951 1506187.5740508868 0, -126428.62322647788 1506590.4673863722 0)), ((-126328.47366274262 1512654.7900340538 0, -125925.11772182248 1512656.1815480343 0, -125528.95547502476 1512657.5649384318 0, -125132.83774524032 1512658.9789293592 0, -124746.9258310655 1512660.3609926691 0, -124751.6730561306 1512248.1914185893 0, -124756.35842910505 1511841.9823246961 0, -125144.36193426771 1511843.644976366 0, -125540.86080873317 1511845.37364449 0, -125546.79751200859 1511439.7551722657 0, -125150.13354273964 1511437.72160729 0, -124761.03469939323 1511435.7739310288 0, -124765.75185726258 1511026.2057185778 0, -125155.92106849636 1511030.7236763998 0, -125552.7341746498 1511035.3250618821 0, -125949.5470047659 1511039.9563562071 0, -126348.57424852277 1511044.6283226218 0, -126343.58969136687 1511443.8854637193 0, -126338.53614343535 1511848.9123334696 0, -126333.47375256877 1512253.9286938282 0, -126328.47366274262 1512654.7900340538 0)), ((-126268.68125744934 1515917.5458290786 0, -126270.36793947153 1516325.9654369245 0, -126272.04018153538 1516732.346466401 0, -126273.70401740653 1517138.0558186683 0, -126275.36985405014 1517541.8166029404 0, -125867.81269531592 1517534.8634892956 0, -125468.27418382304 1517528.0608032343 0, -125068.73533762619 1517521.2771920671 0, -124676.36541358086 1517514.6297736473 0, -124676.58106027775 1517118.5400189376 0, -124676.80695083256 1516712.7707200558 0, -125072.12608191653 1516717.7020674224 0, -125472.88230528434 1516722.5874150866 0, -125475.24808324069 1516316.5699905695 0, -125477.62148531683 1515910.0156483965 0, -125877.44107624413 1515913.8075593114 0, -126268.68125744934 1515917.5458290786 0)), ((-126224.89516022889 1521194.6489400552 0, -126217.79956318598 1521599.372847899 0, -126210.71311489711 1522004.0752571216 0, -126203.5678509434 1522411.533865739 0, -125809.20984091918 1522408.6090121903 0, -125410.36621002032 1522405.6806337943 0, -125011.52270265628 1522402.76000022 0, -124618.70411357592 1522399.9026395646 0, -124622.13115635276 1521982.047332273 0, -124625.46167313609 1521577.2445741813 0, -124628.78268918867 1521172.464893381 0, -124632.09194657534 1520769.0639375413 0, -125034.69622160662 1520774.194629696 0, -125434.06195500019 1520779.296377248 0, -125833.42755836768 1520784.417087296 0, -126231.99660111818 1520789.5449003836 0, -126224.89516022889 1521194.6489400552 0)), ((-120847.64143212377 1506105.5732457587 0, -120844.3304654017 1506520.8640379936 0, -120445.64522029008 1506516.708205814 0, -120449.20874109371 1506101.6004871374 0, -120462.5576369535 1506101.7238225874 0, -120847.64143212377 1506105.5732457587 0)), ((-121240.08536453794 1506930.3648465348 0, -121243.02427341757 1506525.0500728537 0, -121666.25969838328 1506529.5528248027 0, -121660.75708829418 1506934.819746684 0, -121240.08536453794 1506930.3648465348 0)), ((-120837.94142515396 1507331.464363735 0, -120841.13574773929 1506926.1861657395 0, -121240.08536453794 1506930.3648465348 0, -121237.14669844387 1507335.647000029 0, -120837.94142515396 1507331.464363735 0)), ((-120374.48354121138 1511780.0335297228 0, -120382.1560054831 1511375.079419753 0, -120782.70172135768 1511379.9353246607 0, -121183.24702740194 1511384.832745308 0, -121175.54034185561 1511789.4950272364 0, -121167.83391822259 1512194.1468786737 0, -120767.3225307569 1512189.563704962 0, -120775.02066180098 1511784.766116763 0, -120374.48354121138 1511780.0335297228 0)), ((-120707.8534847224 1515856.5487732443 0, -120702.4572395265 1516259.605987525 0, -120697.05644867805 1516665.442556123 0, -120691.63862696686 1517071.2348002568 0, -120686.17998507353 1517480.4781508537 0, -120288.620272845 1517476.4821538334 0, -119893.47711048658 1517472.5168218843 0, -119899.96158757615 1517066.2460947693 0, -119906.4623708097 1516658.8336174053 0, -119912.96324728672 1516251.4220112301 0, -119919.33105734637 1515852.0985516747 0, -120311.13087643796 1515854.3016815225 0, -120707.8534847224 1515856.5487732443 0)), ((-121423.27919263708 1521123.6379134287 0, -121418.10893474067 1521529.2408057053 0, -121826.29440331022 1521536.1366622106 0, -122224.86296199447 1521542.9015232115 0, -122220.13127017854 1521948.5342373766 0, -122215.45736674874 1522350.1908891867 0, -121815.89131574231 1522342.234943161 0, -121407.84184039342 1522334.1419623222 0, -121018.52061237377 1522336.06356573 0, -120620.82032566948 1522338.0399300922 0, -120223.12029071625 1522340.0462541622 0, -119814.56364879261 1522342.1186002165 0, -119821.43015230344 1521932.5722585346 0, -119828.23087917826 1521527.653247194 0, -119835.02279326417 1521122.7348988163 0, -119841.69247015512 1520725.1543634795 0, -120244.46853500957 1520723.1114406264 0, -120642.7226717468 1520721.1014950145 0, -121040.99494318612 1520719.1106676604 0, -121428.46142744238 1520717.1956556789 0, -121423.27919263708 1521123.6379134287 0)), ((-116471.45640800915 1506060.2624132033 0, -116594.54191503269 1506061.0267343943 0, -116882.40405810311 1506065.8006737737 0, -116889.51687631683 1506065.9232600555 0, -116885.6696075123 1506463.6173947568 0, -116881.76229939541 1506867.5384234276 0, -116467.95463077669 1506861.6245820164 0, -116469.72981176751 1506457.2484630274 0, -116071.6503314145 1506451.0002098747 0, -116073.25528882556 1506056.8939392562 0, -116189.72593021201 1506058.2336734035 0, -116335.80511972874 1506059.1296684262 0, -116354.05844230119 1506059.7179110707 0, -116388.71931142654 1506059.7486425918 0, -116471.45640800915 1506060.2624132033 0)), ((-120054.01589803868 1507323.6422674174 0, -120064.85478750731 1506918.5741732598 0, -120075.69404072672 1506513.5179867279 0, -120445.64522029008 1506516.708205814 0, -120442.1863253491 1506922.003984145 0, -120438.73599286917 1507327.3119527982 0, -120054.01589803868 1507323.6422674174 0)), ((-116068.32066701987 1507260.6183581767 0, -116066.55903039787 1507671.7629631455 0, -115668.82447392556 1507665.8735412485 0, -115285.09936666551 1507660.2167836893 0, -115288.32614014135 1507249.9890117033 0, -115291.51705574054 1506844.2990662323 0, -115672.01610032438 1506850.0344130418 0, -116069.98528544577 1506855.83690274 0, -116068.32066701987 1507260.6183581767 0)), ((-116846.39151474854 1510924.704217221 0, -116845.16462299743 1511324.9405872498 0, -116843.9271629774 1511729.7374744387 0, -116842.68046339208 1512134.5351659828 0, -116841.42182462315 1512545.260208008 0, -116426.63213803283 1512538.220543904 0, -116029.19096976993 1512531.4961158284 0, -115792.77013346601 1512527.5053387107 0, -115861.56410122562 1512116.4430048715 0, -115874.71515635849 1512039.5643073677 0, -115824.2898662478 1511712.8981180622 0, -115800.93082433454 1511561.5284411449 0, -115707.14755079916 1511430.8375939096 0, -115638.51462219845 1511394.1334878106 0, -115464.3698573541 1511301.0411959954 0, -115243.8402278692 1511181.561052207 0, -115245.96735315837 1510911.1889799149 0, -115642.91094529454 1510914.5070823168 0, -116041.67928666784 1510917.8690668375 0, -116440.43872641968 1510921.2497684301 0, -116846.39151474854 1510924.704217221 0)), ((-119984.91059292722 1511775.5321362126 0, -120374.48354121138 1511780.0335297228 0, -120366.82009955254 1512184.9886002117 0, -119977.45822824458 1512180.6582820406 0, -119984.91059292722 1511775.5321362126 0)), ((-116663.71292682382 1522325.186876025 0, -116273.24848322617 1522314.3152888955 0, -115877.1758424719 1522303.3061685655 0, -115480.91674428737 1522292.3131322623 0, -115079.40322824946 1522281.188541352 0, -115084.04238776764 1521866.3125016468 0, -115088.59057512072 1521460.6571707528 0, -115093.12967776295 1521055.013615643 0, -115097.57815085424 1520657.2685002252 0, -115500.7912924653 1520667.5419716476 0, -115899.46532991882 1520677.7273618353 0, -116298.12107991171 1520687.9203425033 0, -116694.44956562693 1520698.0774491972 0, -116687.05813663924 1521089.4854640688 0, -116679.37966499559 1521495.8478743378 0, -116671.701530671 1521902.1999256238 0, -116663.71292682382 1522325.186876025 0)), ((-111693.47827975018 1506791.7373515991 0, -111690.67166922861 1507196.837033738 0, -111291.84376854908 1507191.0281420343 0, -111295.02150904168 1506785.9000619962 0, -111298.19956011556 1506380.739163877 0, -110900.09626867746 1506374.880627077 0, -110526.69017948666 1506369.3524212283 0, -110531.69889082109 1505988.0124887344 0, -110903.36823473191 1505992.0725870694 0, -111301.12811380504 1505996.4363694172 0, -111698.88782772499 1506000.8188656422 0, -112110.03137877685 1506005.3643421577 0, -112109.39633769491 1506392.4092545758 0, -112108.73343015161 1506797.480731412 0, -111693.47827975018 1506791.7373515991 0)), ((-115294.70735200212 1506438.632235053 0, -115297.80474291745 1506044.632829943 0, -115298.11684014743 1506044.6370991848 0, -115507.43099867749 1506049.857698452 0, -115675.06780216953 1506050.369341692 0, -115673.57021314393 1506444.781974076 0, -115294.70735200212 1506438.632235053 0)), ((-110893.03322813392 1507185.238518913 0, -111291.84376854908 1507191.0281420343 0, -111288.49301764238 1507615.2455195594 0, -110889.2896443036 1507612.5313155309 0, -110510.39547663584 1507609.9780101487 0, -110516.04636656727 1507179.7414623227 0, -110893.03322813392 1507185.238518913 0)), ((-111687.6964802307 1507617.967321089 0, -111690.67166922861 1507196.837033738 0, -112108.07038293855 1507202.5305956076 0, -112107.38954065862 1507620.857122165 0, -111687.6964802307 1507617.967321089 0)), ((-115239.74303067155 1511703.0603429652 0, -115629.54393633179 1511709.641905785 0, -115635.44894134508 1511735.704398272 0, -115706.24141109285 1512047.9832236923 0, -115704.1622780216 1512113.4742729727 0, -115632.96689429639 1512112.1387424502 0, -115236.58908618204 1512104.6040311817 0, -115239.74303067155 1511703.0603429652 0)), ((-111914.36779684611 1520593.843441507 0, -111907.99874313743 1520996.2340475866 0, -111901.57447392131 1521402.1091506225 0, -111895.15037167615 1521807.9851056247 0, -111888.66682726864 1522217.659301615 0, -111493.40769582988 1522213.6686086245 0, -111095.11402961217 1522209.667588022 0, -110696.82028878036 1522205.6855196028 0, -110303.8783094667 1522201.780405798 0, -110307.50071021168 1521797.9286285667 0, -110311.14072355286 1521392.0498372915 0, -110314.78940902809 1520986.172076282 0, -110318.38811167254 1520584.764788481 0, -110720.25922364488 1520587.0278309209 0, -111118.56376665241 1520589.2843575063 0, -111516.86848876557 1520591.5486326523 0, -111914.36779684611 1520593.843441507 0)))</t>
+          <t>MULTIPOLYGON Z (((-1200949.4146035248 1986131.3865049854 0, -1201008.5640779603 1985729.7722811436 0, -1200614.5012370858 1985673.7686730388 0, -1200669.6533357725 1985271.2897667151 0, -1201066.493713974 1985328.1256063147 0, -1201124.4264467019 1984926.4579796004 0, -1201524.0432644722 1984984.1342984058 0, -1201587.8614740546 1984581.7502122638 0, -1201985.2307194718 1984639.351418582 0, -1202382.6020516898 1984696.9409601807 0, -1202323.2590749203 1985099.5400278254 0, -1202257.5025131584 1985498.7310964514 0, -1202191.7442448295 1985897.9311084636 0, -1201797.1904774976 1985841.8542835591 0, -1201402.6258149387 1985785.7841837544 0, -1201341.8535774376 1986187.0676920137 0, -1200949.4146035248 1986131.3865049854 0)), ((-1199313.8102938333 1988900.7280749313 0, -1198924.411766142 1988843.6943137369 0, -1198985.113375903 1988444.5957812008 0, -1199375.1571254837 1988503.367987584 0, -1199436.503853103 1988106.0068802263 0, -1199827.1983496007 1988166.547356416 0, -1199888.7259280758 1987770.6245739467 0, -1200280.5990791349 1987832.833716148 0, -1200343.3062871008 1987438.5702774525 0, -1200734.5698639639 1987496.4786489669 0, -1201125.8437221616 1987554.3869302985 0, -1201065.402010298 1987951.2005946347 0, -1200673.0051892675 1987892.0187706524 0, -1200611.4306241132 1988287.5563193974 0, -1200217.890172515 1988227.106117349 0, -1200154.5920585152 1988620.8540026043 0, -1199764.8849283112 1988562.1083989786 0, -1199702.5616101853 1988957.666862466 0, -1199313.8102938333 1988900.7280749313 0)), ((-1223143.436401538 1989881.719152336 0, -1223419.4352111868 1989923.7774424125 0, -1223535.9816394616 1989941.6531504765 0, -1223812.1357923334 1989983.7452325672 0, -1223928.5534829786 1990001.6100994176 0, -1224204.8433981768 1990043.7328470063 0, -1224139.843618964 1990444.944148744 0, -1224074.8536150574 1990846.1559898094 0, -1223683.6110876764 1990782.5072356572 0, -1223292.3787798015 1990718.858378817 0, -1222901.1371126957 1990655.2062944588 0, -1222509.8958780668 1990591.5525453805 0, -1222571.9559296 1990197.724306925 0, -1222634.015968297 1989803.8950855925 0, -1222750.8590300886 1989821.7987297545 0, -1223026.7220759718 1989863.826351641 0, -1223143.436401538 1989881.719152336 0)), ((-1222542.1489198531 1995514.436441026 0, -1222155.7781050908 1995451.2022305646 0, -1221769.4045387236 1995387.986314855 0, -1221836.504233702 1994990.4565124046 0, -1221903.6023083215 1994592.9356454306 0, -1222288.3583468322 1994653.879323529 0, -1222673.1116197156 1994714.8413128022 0, -1222607.6310736444 1995114.6344123706 0, -1222542.1489198531 1995514.436441026 0)), ((-1201659.4476120977 1996675.8534731867 0, -1201744.9832824129 1996662.408207222 0, -1201835.2855395805 1996648.2221966062 0, -1201868.6205855391 1996654.307126532 0, -1201949.4849365936 1996795.4842738025 0, -1202011.3662478626 1996779.085643789 0, -1202066.0289064448 1996803.4623602377 0, -1202124.5704391345 1996848.7081638963 0, -1202089.9396841028 1997077.5244327018 0, -1202028.971132923 1997475.37670198 0, -1201631.711433702 1997414.6150895464 0, -1201234.646459388 1997353.8929998917 0, -1201294.6483140206 1996954.8134063454 0, -1201354.0538059068 1996554.2472903777 0, -1201453.4910764284 1996191.6643473764 0, -1201859.681803924 1996257.7183014518 0, -1201751.6667690177 1996617.4994862182 0, -1201690.0623007054 1996607.5600724139 0, -1201513.1361385188 1996579.7178727558 0, -1201566.3729970062 1996664.9414722568 0, -1201659.4476120977 1996675.8534731867 0)), ((-1223783.3877977077 1996529.6031083053 0, -1223982.4632963662 1996557.8789112386 0, -1223921.3039287934 1996958.2968418167 0, -1223719.7676918844 1996928.9535949833 0, -1223783.3877977077 1996529.6031083053 0)), ((-1226224.4013266957 1997734.1563803519 0, -1226164.75220724 1998132.4426223265 0, -1225771.418804286 1998069.1362751452 0, -1225378.0858237073 1998005.8282160312 0, -1225438.9652518556 1997605.3160135497 0, -1225499.8510547597 1997204.762899866 0, -1225891.9505479299 1997270.3168557796 0, -1226284.0488838982 1997335.87908203 0, -1226224.4013266957 1997734.1563803519 0)), ((-1224011.6469405184 1999021.8959077331 0, -1224041.4676897498 1998825.9433438212 0, -1224072.6007326506 1998621.3173565797 0, -1224175.176919924 1998637.1867835436 0, -1224219.6011097645 1998644.061814488 0, -1224283.7478828828 1998243.9815083751 0, -1224133.5659189047 1998220.7293548975 0, -1224195.1988720312 1997819.1633783365 0, -1224591.4049895727 1997879.2452730516 0, -1224529.290479228 1998282.0122576081 0, -1224923.2498256515 1998344.1667091553 0, -1224862.1799927137 1998744.6054138567 0, -1225255.9658451523 1998806.658980719 0, -1225194.7237044915 1999206.9875076083 0, -1224801.1117659858 1999145.0331064777 0, -1224407.5100378783 1999083.0785490803 0, -1224011.6469405184 1999021.8959077331 0)), ((-1211938.199385719 1999251.9292097052 0, -1211708.2860837039 1999217.054850042 0, -1211739.7245894852 1999019.934832633 0, -1211793.9822809868 1998848.1292916932 0, -1211801.5882713445 1998824.0457813325 0, -1211761.4914027578 1998665.1450358173 0, -1211743.4844433214 1998593.7942208254 0, -1211723.6454804663 1998519.074035636 0, -1211697.5921301139 1998420.9349449435 0, -1211667.7705426493 1998416.1714279458 0, -1211671.6267437972 1998391.8670954371 0, -1211736.120784928 1997991.4536868574 0, -1211759.7685744949 1997995.016372625 0, -1212130.3548239018 1998054.7113660679 0, -1212361.1455087503 1998088.7947185356 0, -1212497.7644001434 1998267.784060639 0, -1212394.8303602547 1998910.8103656892 0, -1212002.221016313 1998851.4524695664 0, -1212001.4851433197 1998851.3451502009 0, -1211938.199385719 1999251.9292097052 0)), ((-1211625.379728793 2001256.687723491 0, -1211233.2807288296 2001198.2464947454 0, -1211295.7737314815 2000796.9178301052 0, -1211358.2666912023 2000395.5880874582 0, -1211750.2268920816 2000454.0680641413 0, -1212142.187544372 2000512.5463302468 0, -1212079.8317922114 2000913.847289778 0, -1212017.476001224 2001315.1471723234 0, -1211625.379728793 2001256.687723491 0)), ((-1239286.9752013446 2000957.7813093676 0, -1239233.9397241138 2001365.6879314126 0, -1238841.929181456 2001305.8821331554 0, -1238743.3460844427 2001290.8404238424 0, -1238796.4796279324 2000884.595153859 0, -1238503.2533085248 2000840.8426608983 0, -1238556.5909239606 2000435.589719444 0, -1238747.5856001636 2000463.4427302745 0, -1238718.9932655112 2000664.4696718368 0, -1238921.958696769 2000694.067133627 0, -1238948.3022853793 2000492.7225605128 0, -1239340.0026043046 2000549.8621019782 0, -1239731.709873227 2000607.021433765 0, -1239680.696164114 2001016.5496067496 0, -1239286.9752013446 2000957.7813093676 0)), ((-1199488.400481616 2003700.7845815797 0, -1199446.2541140798 2004018.886376972 0, -1199435.6734278726 2004097.0835830967 0, -1199392.7873951585 2004421.0149994013 0, -1199382.0074318317 2004493.476731145 0, -1199012.6275708398 2004434.6261367777 0, -1198616.147769523 2004371.3797959967 0, -1198219.6751145 2004308.1531906656 0, -1197823.19002622 2004244.9431902638 0, -1197880.7325412876 2003843.6001293233 0, -1197937.5119648324 2003442.6961403133 0, -1198332.0451085707 2003508.4350993743 0, -1198277.3532443237 2003908.3443222241 0, -1198673.963112886 2003973.0951545911 0, -1199070.5687549158 2004037.8741253703 0, -1199121.113285039 2003639.9691604427 0, -1199488.400481616 2003700.7845815797 0)), ((-1250198.876306713 2005962.3489113243 0, -1250590.909210174 2006023.710049164 0, -1250528.2781075302 2006423.9168497787 0, -1250921.141191029 2006485.7457691838 0, -1251314.0143797263 2006547.5745069631 0, -1251251.2997013847 2006947.9407636316 0, -1250858.469156953 2006886.026792026 0, -1250465.6389268648 2006824.1110779692 0, -1250073.1321132244 2006761.8669079489 0, -1249680.6158270082 2006699.6194389884 0, -1249617.6377757322 2007098.082292455 0, -1249221.292169128 2007037.8089200025 0, -1248824.9437029413 2006977.5537103121 0, -1248890.3705293871 2006577.723025546 0, -1248492.1883682916 2006515.8758622867 0, -1248094.006535081 2006454.0269105784 0, -1248159.4489725113 2006053.16543721 0, -1247761.2891187842 2005990.8071546177 0, -1247363.1198071872 2005928.445525758 0, -1247428.6104098717 2005526.538003521 0, -1247826.7580702042 2005589.4071762606 0, -1248224.906066516 2005652.2745642345 0, -1248623.0610138224 2005715.1616635385 0, -1249021.2065024893 2005778.0454177293 0, -1249414.0249507115 2005839.5165988407 0, -1249806.8437167546 2005900.9860418532 0, -1250198.876306713 2005962.3489113243 0)), ((-1247566.6694429861 2007195.5715515325 0, -1247630.3480796162 2006793.562503844 0, -1248028.555996695 2006854.8757994352 0, -1248426.751274466 2006916.2056816863 0, -1248824.9437029413 2006977.5537103121 0, -1248760.0966418097 2007379.7958559261 0, -1248362.2845145166 2007318.385699903 0, -1247964.4840919334 2007256.965347405 0, -1247566.6694429861 2007195.5715515325 0)), ((-1214884.9514026928 2011587.7699811428 0, -1214823.6887198512 2011988.554887671 0, -1214432.1813166821 2011931.952489681 0, -1214038.8685967259 2011871.3089509988 0, -1214100.2322876945 2011470.785835063 0, -1213707.0202478133 2011410.4633386673 0, -1213808.1304391075 2010762.22808278 0, -1214140.6939690532 2010810.974031074 0, -1214177.9683250245 2010911.4998709369 0, -1214475.6776406844 2010971.7266713823 0, -1214536.4578955977 2011112.1671980636 0, -1214529.8486618707 2011293.5120795213 0, -1214530.434687362 2011296.0075491248 0, -1214493.431810409 2011531.124937915 0, -1214884.9514026928 2011587.7699811428 0)), ((-1203414.773080094 2017818.9878087633 0, -1203021.3449131686 2017761.423441275 0, -1202627.9140480196 2017703.8772140818 0, -1202687.8143944452 2017300.7751719146 0, -1202746.846823229 2016900.4051773595 0, -1203141.0981948192 2016958.5215804302 0, -1203535.3370808254 2017016.654554963 0, -1203475.0921401458 2017416.7085512585 0, -1203414.773080094 2017818.9878087633 0)), ((-1229885.7531415808 2017938.892345719 0, -1230278.27186139 2017998.945235504 0, -1230670.7893786563 2018059.0063095205 0, -1230607.6603637964 2018455.4002416127 0, -1230544.5329900116 2018851.7831042658 0, -1230149.4687500696 2018791.2440430394 0, -1229754.4017251895 2018730.7231066062 0, -1229359.3303284014 2018670.2302620958 0, -1228965.276372797 2018609.9693858812 0, -1228571.2294262208 2018549.7282063698 0, -1228177.178109552 2018489.5151287275 0, -1227783.1142206467 2018429.3186240913 0, -1227852.942872487 2018036.5505560231 0, -1227922.7731155031 2017643.7714194034 0, -1228315.3855124349 2017702.5402665238 0, -1228708.0080880623 2017761.3088930578 0, -1229100.6212568304 2017820.0741747317 0, -1229493.2461895708 2017878.8292683167 0, -1229885.7531415808 2017938.892345719 0)), ((-1206105.5278482453 2018606.1810173478 0, -1205713.8515176112 2018553.733399309 0, -1205322.1610654704 2018501.312333519 0, -1205382.0702499007 2018099.805695467 0, -1205772.3526640234 2018152.7374070461 0, -1206162.6421304154 2018205.688848611 0, -1206552.9174745223 2018258.66685713 0, -1206497.211229256 2018658.6483505857 0, -1206105.5278482453 2018606.1810173478 0)), ((-1206272.1471640056 2020272.094377161 0, -1206319.771786443 2019860.462891817 0, -1205928.7723013028 2019814.0727765951 0, -1205995.245163187 2019409.7445033374 0, -1206390.0777057828 2019459.2916460761 0, -1206746.3742502234 2019504.7952211872 0, -1206687.703592044 2019904.6677672267 0, -1207082.5781711931 2019963.9683060655 0, -1207023.2084410943 2020364.5151582565 0, -1206628.6340526156 2020304.7104994433 0, -1206272.1471640056 2020272.094377161 0)), ((-1204575.983485033 2020844.4712396988 0, -1204182.154224872 2020786.848793847 0, -1203788.3026792211 2020729.241342847 0, -1203849.091208816 2020342.5179917072 0, -1203909.415305679 2019961.4732845365 0, -1204302.928527725 2020020.9987176163 0, -1204696.4390576784 2020080.5422823506 0, -1204637.0053456717 2020457.0897676328 0, -1204575.983485033 2020844.4712396988 0)), ((-1209332.818848822 2021125.1684327514 0, -1209272.771639584 2021530.6954869886 0, -1209213.2751222092 2021936.483071149 0, -1209154.272241546 2022338.985942864 0, -1208759.8565809361 2022277.5207135705 0, -1208818.5156753226 2021875.2288204296 0, -1208877.468430193 2021470.5911785201 0, -1208937.3975810385 2021065.4338153556 0, -1208997.3876847923 2020661.2150426162 0, -1209392.596071574 2020719.8219105892 0, -1209332.818848822 2021125.1684327514 0)), ((-1205302.2244544607 2021349.971451156 0, -1205242.567928354 2021749.6392183537 0, -1205178.4817013156 2022150.0696602145 0, -1204787.0127856692 2022091.9792527887 0, -1204848.2562035522 2021692.4437968323 0, -1204908.9907677753 2021294.9005438634 0, -1205302.2244544607 2021349.971451156 0)), ((-1232957.6495970143 2022111.1251855183 0, -1232957.7353560326 2022110.5869775526 0, -1233085.527546776 2021308.5850659579 0, -1233085.8372327816 2021306.6415261528 0, -1233371.2401876114 2021352.1115497453 0, -1233307.3027463725 2021754.1336854794 0, -1233243.3685518657 2022156.1347434698 0, -1232957.6495970143 2022111.1251855183 0)), ((-1203666.8994157643 2021513.3005405762 0, -1204060.6213631586 2021572.9930481655 0, -1203999.0077779 2021970.680419623 0, -1203938.3219586762 2022369.915049777 0, -1203543.2228862923 2022309.399046005 0, -1203605.0004523103 2021910.0631655224 0, -1203666.8994157643 2021513.3005405762 0)), ((-1240824.7997962106 2022116.7025246206 0, -1241216.3239648386 2022181.4804448355 0, -1241607.8551180388 2022246.2780687707 0, -1242000.8346198548 2022311.7543284777 0, -1242393.8211085119 2022377.250277791 0, -1242786.79499762 2022442.7627955063 0, -1243179.7758707441 2022508.2950022228 0, -1243570.5444152341 2022566.472135946 0, -1243961.319898175 2022624.6689802737 0, -1244352.090938294 2022682.893941753 0, -1244704.043135988 2022735.6987950618 0, -1245100.672702718 2022800.8936539893 0, -1245497.2994534615 2022866.106606608 0, -1245893.9315920607 2022931.3491798039 0, -1246290.5511192465 2022996.608286078 0, -1246688.3028421644 2023060.3697814473 0, -1246854.222548723 2023086.9641918603 0, -1247086.04194313 2023124.147799671 0, -1247483.7782132423 2023187.9439005193 0, -1247881.5198564983 2023251.769610707 0, -1248274.3760642011 2023317.2067196239 0, -1248667.2376472114 2023382.673481462 0, -1249060.0866059994 2023448.1568093183 0, -1249452.9441114145 2023513.649855215 0, -1249847.316838842 2023578.7078421412 0, -1250241.6965216782 2023643.7854998587 0, -1250636.0749527814 2023708.8713013076 0, -1251030.439164145 2023773.983621087 0, -1251420.8377171035 2023834.0475751222 0, -1251811.2447756436 2023894.1212700573 0, -1252201.6375792723 2023954.2215212677 0, -1252592.029092959 2024014.329953608 0, -1252985.8073247832 2024079.3396748095 0, -1253379.5745004576 2024144.3559842452 0, -1253773.3388244524 2024209.3904081208 0, -1254143.464578902 2024270.4652805342 0, -1254540.4336789472 2024330.5693503893 0, -1254480.561012865 2024733.1099419487 0, -1254420.6803270606 2025135.637883956 0, -1254816.070587661 2025195.8975025956 0, -1254755.42314183 2025598.4555184136 0, -1254694.7676744922 2026001.0008800384 0, -1255088.582258263 2026061.396129427 0, -1255482.3939579725 2026121.8094874748 0, -1255875.4416704772 2026186.391620376 0, -1256268.4767259322 2026250.9903073946 0, -1256661.508915793 2026315.607107215 0, -1256600.6694906123 2026716.9467298146 0, -1256993.89299775 2026782.4505437952 0, -1256933.229952671 2027184.6448551298 0, -1257324.2901272497 2027244.9481369173 0, -1257263.0153584753 2027646.8293020562 0, -1257653.4458903556 2027706.8056826259 0, -1257591.5413923927 2028108.3606214274 0, -1257525.2230301008 2028505.7883454151 0, -1257458.904829029 2028903.2149502914 0, -1257850.185653451 2028965.0621591632 0, -1258241.4651761076 2029026.91752068 0, -1258176.6170405287 2029426.4777840169 0, -1258111.7772884814 2029826.048442068 0, -1258047.1366058583 2030226.3240997333 0, -1258439.619044347 2030290.1063409834 0, -1258374.5898588668 2030690.7482105817 0, -1258309.5722330518 2031091.3805298947 0, -1258244.5481669626 2031491.9902132635 0, -1258180.9745911143 2031890.4893605306 0, -1257789.5470117969 2031825.7917771202 0, -1257397.058731641 2031763.089979814 0, -1257004.5707433224 2031700.386345697 0, -1256940.962613132 2032099.522656034 0, -1256548.5191066172 2032037.1001378882 0, -1256484.946862812 2032436.4453752316 0, -1256092.5330086597 2032374.2709517737 0, -1255700.510181279 2032314.1189771222 0, -1255308.4974309984 2032253.9667281853 0, -1255371.759463026 2031853.4377977676 0, -1254979.6008854692 2031792.8210392797 0, -1254587.4425973361 2031732.2024480815 0, -1254191.95264393 2031670.182949536 0, -1253796.4531999393 2031608.1600279238 0, -1253859.6203336667 2031207.246962477 0, -1253464.2134179117 2031145.5332332975 0, -1253068.8181858058 2031083.8092356243 0, -1253132.1585524387 2030683.5255467219 0, -1252768.9144148913 2030625.1608824118 0, -1252375.8307867476 2030562.0435614423 0, -1251983.2787089215 2030499.1827182607 0, -1251590.7221853412 2030436.3499428467 0, -1251193.902099216 2030371.5998309178 0, -1250797.0791710068 2030306.8677798829 0, -1250400.2518153617 2030242.1637567105 0, -1250003.4134142431 2030177.466268665 0, -1249607.731750929 2030113.1350200824 0, -1249212.0374554251 2030048.820284649 0, -1248816.3501153798 2029984.5251818541 0, -1248420.6501460623 2029920.2465926132 0, -1248026.4912020147 2029856.1910947484 0, -1247632.327835281 2029792.1636517057 0, -1247238.1632212957 2029728.1443303619 0, -1246843.9941874365 2029664.153064309 0, -1246452.892148137 2029596.1620961318 0, -1246061.7888863166 2029528.179277119 0, -1245670.67143612 2029460.2229808578 0, -1245279.5609720952 2029392.2863610035 0, -1244880.4399652374 2029333.035713487 0, -1244481.3047312102 2029273.811517816 0, -1244082.1764446825 2029214.6069278538 0, -1243683.0339338758 2029155.428789975 0, -1243339.3741954616 2029101.0827773253 0, -1242946.7681836765 2029039.0079999948 0, -1242555.324435895 2028977.0756579326 0, -1242163.8860647916 2028915.172960424 0, -1241770.1254374017 2028851.3960662757 0, -1241376.3831700536 2028787.6304226187 0, -1240984.2828058784 2028724.77858945 0, -1240592.181212203 2028661.9349018326 0, -1240200.7532791651 2028598.6448393282 0, -1239809.322533992 2028535.3728955484 0, -1239417.8873904916 2028472.1290372899 0, -1239026.4510252296 2028408.8933316357 0, -1239090.6484675815 2028005.5682271295 0, -1239154.8476013097 2027602.2319856184 0, -1239219.0468385175 2027198.894575455 0, -1239283.246178932 2026795.5559984501 0, -1239345.920694454 2026394.4770470175 0, -1239408.5969054077 2025993.3869810896 0, -1239471.2814289166 2025592.307296627 0, -1239533.9578545913 2025191.2149403521 0, -1239593.4783309621 2024791.9689913124 0, -1239652.9891357217 2024392.7203571005 0, -1239712.500061204 2023993.4706002155 0, -1239772.020899634 2023594.2212831436 0, -1239839.4509167261 2023192.4704520234 0, -1239906.8810148402 2022790.7184735409 0, -1239974.3096060858 2022388.97531649 0, -1240041.7398655603 2021987.221048717 0, -1240433.2712334564 2022051.952714843 0, -1240824.7997962106 2022116.7025246206 0), (-1248679.1504517798 2028318.3355548251 0, -1248281.1012414123 2028253.2007077434 0, -1247883.0409976325 2028188.072392038 0, -1247950.8550266984 2027790.3148147415 0, -1248018.6691689556 2027392.5561029816 0, -1247620.1990256833 2027328.9447225698 0, -1247221.739016179 2027265.3330268385 0, -1247154.3271923906 2027661.6227578027 0, -1247086.9170654146 2028057.9013955873 0, -1247026.186511067 2028459.4635404407 0, -1247423.2705223358 2028524.297168386 0, -1247820.3564682123 2028589.1189620579 0, -1248217.437998981 2028653.9687882473 0, -1248614.5296671642 2028718.8183060996 0, -1248549.9008149747 2029119.28838522 0, -1248944.6187334761 2029183.6659870485 0, -1249339.338575796 2029248.0317741423 0, -1249734.0587533587 2029312.3957129922 0, -1250128.7792645586 2029376.757803301 0, -1250191.4583207741 2028976.396093616 0, -1250254.137532732 2028576.0332437023 0, -1249860.397470757 2028511.5820652237 0, -1249466.644774831 2028447.147424419 0, -1249072.89903236 2028382.7324407294 0, -1248679.1504517798 2028318.3355548251 0), (-1248417.1298585548 2027456.164048192 0, -1248815.6006786304 2027519.7716774573 0, -1248883.826760444 2027120.4830428087 0, -1248952.0415787275 2026721.2016760434 0, -1248553.179836742 2026659.0546324335 0, -1248154.3120755805 2026596.9455808732 0, -1248086.4913593903 2026994.7464240948 0, -1248018.6691689556 2027392.5561029816 0, -1248417.1298585548 2027456.164048192 0)), ((-1205613.2579564946 2024675.5960363327 0, -1205675.5244646221 2024274.1660020929 0, -1206032.660344529 2024329.3412408892 0, -1206428.4227780085 2024389.8282359694 0, -1206370.059889674 2024791.7290923826 0, -1206311.8148573178 2025194.5265068624 0, -1205915.429507019 2025133.01981894 0, -1205553.0379621363 2025077.3519040926 0, -1205613.2579564946 2024675.5960363327 0)), ((-1210826.6896727383 2024644.9510114104 0, -1210766.8396209527 2025048.7023286093 0, -1210708.0706603783 2025452.7886553959 0, -1210652.5090646092 2025859.0519228405 0, -1210259.6466006862 2025799.2429971588 0, -1210315.3310209601 2025393.224340328 0, -1210373.7644687237 2024988.9823952538 0, -1210433.3022160495 2024585.559505433 0, -1210493.3687443314 2024183.793758386 0, -1210887.3913352073 2024243.2252126785 0, -1210826.6896727383 2024644.9510114104 0)), ((-1200231.0400632427 2025535.3340568452 0, -1200285.8945334961 2025124.8883061956 0, -1200680.5298244192 2025181.563982954 0, -1201074.9665822696 2025238.2264538677 0, -1201019.0329055046 2025649.0315278738 0, -1200625.0378307404 2025592.1737410005 0, -1200231.0400632427 2025535.3340568452 0)), ((-1321280.6173853083 2058083.5737533076 0, -1321664.5810077875 2058142.4762339485 0, -1322062.3611194459 2058210.5236693362 0, -1321995.9126071483 2058609.6128780514 0, -1321995.8019652606 2058610.2773933143 0, -1321599.448249967 2058543.876546212 0, -1321202.0510165088 2058477.2808153273 0, -1321280.6173853083 2058083.5737533076 0)), ((-1179105.2869066224 1888617.7273695231 0, -1179115.9710953655 1888616.9338675025 0, -1179055.91134986 1888996.7362096165 0, -1178665.555186845 1888942.4659631737 0, -1178602.9243309263 1888933.7580948023 0, -1178615.1686528765 1888924.7423638906 0, -1178628.521187138 1888912.6537212462 0, -1178668.8000334883 1888876.6469856459 0, -1178678.9045889655 1888867.7110062523 0, -1178680.0172958132 1888866.726883542 0, -1178726.2427016278 1888560.2434908405 0, -1179102.3208169893 1888617.9476949621 0, -1179105.2869066224 1888617.7273695231 0)), ((-1186874.038604841 1890491.4992944147 0, -1186872.9404039271 1890491.6713313425 0, -1186872.9499457758 1890491.6069984068 0, -1186874.038604841 1890491.4992944147 0)), ((-1187740.3863162966 1890499.7574263406 0, -1187748.0021001725 1890497.9372015141 0, -1187756.097569647 1890501.0593707971 0, -1187769.8049647976 1890517.7187150263 0, -1187735.7767808228 1890537.4623593946 0, -1187735.0307261655 1890521.9647945906 0, -1187736.0798005583 1890507.8447073444 0, -1187740.3863162966 1890499.7574263406 0)), ((-1186876.2157106234 1890491.1582433505 0, -1186886.8172234602 1890419.606674067 0, -1187725.3433674988 1890543.515976666 0, -1187690.2819010757 1890563.8591464516 0, -1187667.5501648362 1890568.6700683476 0, -1187429.897759995 1890618.9811750606 0, -1187382.6620204141 1890677.4576822075 0, -1187278.4854413432 1890612.248134321 0, -1187259.0582802685 1890605.7146222093 0, -1186904.8840154533 1890486.6672553835 0, -1186876.2157106234 1890491.1582433505 0)), ((-1188123.1064447055 1890600.9546276894 0, -1188128.0039866117 1890603.014600695 0, -1188138.3730090496 1890604.5467761555 0, -1188144.3265888842 1890601.825143622 0, -1188151.8937026053 1890596.8258572621 0, -1188174.7378867653 1890576.1840846913 0, -1188205.3639952096 1890556.6926516807 0, -1188230.8611510843 1890550.2649717983 0, -1188272.4515197284 1890561.8512074805 0, -1188298.2323615844 1890572.7998664386 0, -1188312.1030920038 1890581.8746381055 0, -1188315.9869673569 1890591.8521417447 0, -1188313.110770919 1890609.5541057098 0, -1188315.5454941096 1890630.726273488 0, -1188461.169951352 1890652.2442963165 0, -1188450.3049999387 1890725.5993665976 0, -1188421.50489671 1890726.4331994643 0, -1188378.9585863028 1890727.7680660281 0, -1188266.312074268 1890640.1686700091 0, -1188061.9755397409 1890626.546116768 0, -1187894.4421532732 1890615.3684420993 0, -1187830.581959661 1890559.0666487284 0, -1188068.9253935083 1890594.2850415143 0, -1188072.961564745 1890592.8631398568 0, -1188095.3008167378 1890590.840211846 0, -1188104.430743351 1890591.0567089948 0, -1188123.1064447055 1890600.9546276894 0)), ((-1194406.0165086838 1892277.5862176022 0, -1194465.4208935194 1891875.9678030992 0, -1194524.8234477565 1891474.3587166604 0, -1194918.1344180182 1891532.8403313872 0, -1195311.4329493698 1891591.3390325352 0, -1195704.7370191833 1891649.8679212425 0, -1196098.0400220633 1891708.4054882715 0, -1196038.6754803476 1892109.6026921868 0, -1195979.3091151244 1892510.8092263872 0, -1195919.94410731 1892912.0051446112 0, -1195860.587061192 1893313.2119541636 0, -1195467.2460356867 1893255.0862772418 0, -1195073.9039429305 1893196.9692714587 0, -1194680.5576036887 1893138.8808814313 0, -1194287.2183944033 1893080.812699648 0, -1194346.6216684908 1892679.2055507903 0, -1194406.0165086838 1892277.5862176022 0)), ((-1178359.9781860579 1893376.8770570161 0, -1178415.8113924572 1892979.0734418454 0, -1178471.6427189133 1892581.279152106 0, -1178527.4851311543 1892183.4758120168 0, -1178927.6116216248 1892242.5125736254 0, -1179327.7485048182 1892301.5495577876 0, -1179727.8698472194 1892360.6235194542 0, -1180127.990204148 1892419.7061092216 0, -1180516.993823687 1892535.830099272 0, -1180456.068967295 1892950.6668688487 0, -1180066.9659569485 1892838.8728355994 0, -1180005.9413891886 1893258.038840582 0, -1179944.9165011777 1893677.204122247 0, -1179883.9010774507 1894096.3702444974 0, -1179488.9723053728 1894015.9258636925 0, -1179094.0441929265 1893935.480196685 0, -1178699.0892185145 1893855.079970265 0, -1178304.1462819271 1893774.6700527072 0, -1178359.9781860579 1893376.8770570161 0)), ((-1190778.829093544 1895026.871992526 0, -1190839.760251897 1894625.2293031116 0, -1190900.7009389747 1894223.587514901 0, -1191295.2800924832 1894282.1221429226 0, -1191689.858199118 1894340.6654296252 0, -1192084.4320763815 1894399.2373190005 0, -1192479.0017228236 1894457.8378109236 0, -1192416.8089803848 1894859.2296450553 0, -1192354.6257699209 1895260.6223786166 0, -1192292.579050568 1895661.9749551334 0, -1192229.6659854073 1896068.94580703 0, -1191836.1569407692 1896011.2293614007 0, -1191442.6452515044 1895953.5315459068 0, -1191049.1407037235 1895895.8539255825 0, -1190655.623729621 1895838.1933708163 0, -1190717.8532868377 1895428.4148791246 0, -1190778.829093544 1895026.871992526 0)), ((-1195711.515713946 1896991.7734474617 0, -1195651.6267974805 1897393.2779463765 0, -1195591.7503743176 1897794.7020027523 0, -1195531.8753121055 1898196.1154197033 0, -1195137.8224340407 1898138.2517039974 0, -1195197.746987196 1897736.8465314081 0, -1195257.6713091212 1897335.4406911351 0, -1195317.5953995492 1896934.0341848754 0, -1195377.5290429997 1896532.6285788429 0, -1195771.4044003438 1896590.2682842822 0, -1195711.515713946 1896991.7734474617 0)), ((-1193082.5478134777 1901109.9753088155 0, -1193475.8960802914 1901170.3934988985 0, -1193415.7913449106 1901571.7017512866 0, -1193022.3988302003 1901511.3681873989 0, -1193082.5478134777 1901109.9753088155 0)), ((-1177752.4872717867 1903502.8787994755 0, -1177359.8021421588 1903441.4241137463 0, -1176967.1144337156 1903379.9880371129 0, -1177021.8245550608 1902987.4604622647 0, -1177076.5328122007 1902594.9421904658 0, -1177131.2521716019 1902202.414847007 0, -1177185.9696662202 1901809.8968097374 0, -1177577.428125001 1901876.44191709 0, -1177968.8758242452 1901942.994117986 0, -1178360.3193647412 1902009.5749209428 0, -1178751.771711725 1902076.1659491605 0, -1178698.2916188638 1902463.5864314684 0, -1178644.809676144 1902851.0162392645 0, -1178591.329066001 1903238.4354284331 0, -1178537.8481976374 1903625.853968784 0, -1178145.1698211322 1903564.3520941334 0, -1177752.4872717867 1903502.8787994755 0)), ((-1190908.3198422568 1904888.1385654486 0, -1190848.7425799756 1905289.809262526 0, -1190788.5411628187 1905695.7050735203 0, -1190395.0807721363 1905635.6361323004 0, -1190001.6177493844 1905575.5857850604 0, -1189608.1423110566 1905515.5524668305 0, -1189214.664243633 1905455.5377428497 0, -1189219.171575706 1905425.0182571036 0, -1189274.2901261137 1905051.8827897592 0, -1189667.9235759 1905111.3595901635 0, -1190061.5477913003 1905170.8334764433 0, -1190121.0204423175 1904769.1978609448 0, -1189727.318542925 1904709.7118929208 0, -1189333.6156033983 1904650.2345486004 0, -1189392.9622375325 1904248.6401592877 0, -1189452.308626869 1903847.0450700808 0, -1189481.2739230653 1903851.350970904 0, -1189846.1548405404 1903906.3707972832 0, -1190239.997073223 1903965.786488621 0, -1190633.8205257917 1904025.2590989687 0, -1191027.6413443335 1904084.7503066773 0, -1190967.981508196 1904486.4398003086 0, -1190908.3198422568 1904888.1385654486 0)), ((-1179945.6358764141 1905066.5924320498 0, -1179970.7189541813 1904895.560016338 0, -1180004.802821503 1904663.150277138 0, -1180029.770264339 1904493.847700341 0, -1180064.1989814092 1904260.4701743908 0, -1180089.0169855845 1904092.16599216 0, -1180463.5398180843 1904147.3500395033 0, -1180838.0486198857 1904202.5612151208 0, -1180878.008857196 1904208.4552150238 0, -1181212.5481627237 1904257.76960505 0, -1181272.4486707496 1904266.6091266726 0, -1181587.0532416308 1904313.0082548873 0, -1181666.8890657434 1904324.7616849826 0, -1181607.6338308388 1904726.5765007597 0, -1181548.3685356055 1905128.389039277 0, -1181489.1029650006 1905530.20086466 0, -1181429.8484950538 1905932.0035698146 0, -1181035.713326319 1905873.7449473573 0, -1180641.5755574198 1905815.5049099228 0, -1180247.435189834 1905757.2834576652 0, -1179853.2922250433 1905699.0805907263 0, -1179886.4784328507 1905470.0354333818 0, -1179911.8043482066 1905297.293543197 0, -1179945.6358764141 1905066.5924320498 0)), ((-1186223.0697855402 1906234.524458163 0, -1186281.9241700133 1905832.3458637698 0, -1186310.932549742 1905635.0445003845 0, -1186340.9403507034 1905430.3458742376 0, -1186399.8568370268 1905028.3394933036 0, -1186650.132388549 1905066.2523844785 0, -1186793.9930118804 1905088.0505190296 0, -1186980.189869192 1905116.2634695985 0, -1187188.126569116 1905147.7801355016 0, -1187310.2845728302 1905166.105655993 0, -1187640.4078231023 1905215.6446172167 0, -1187581.8276503226 1905617.3173266833 0, -1187545.3951083054 1905867.138556 0, -1187523.0010153102 1906018.9601683628 0, -1187464.6224085458 1906420.6228855937 0, -1187406.2435549675 1906822.2848942888 0, -1187112.8000172758 1906778.50026626 0, -1186952.5913249126 1906754.6289590811 0, -1186558.4045455763 1906695.6563583014 0, -1186164.2151470624 1906636.7023404115 0, -1186223.0697855402 1906234.524458163 0)), ((-1178469.7116424306 1906896.4162612902 0, -1178863.3891631283 1906952.1983750868 0, -1178802.8822249305 1907355.4621336507 0, -1178409.1200194932 1907299.0116164312 0, -1178469.7116424306 1906896.4162612902 0)), ((-1184852.3185068783 1948696.343759482 0, -1184911.3826322686 1948294.7235612997 0, -1185306.3286445949 1948353.1609087712 0, -1185701.2720399515 1948411.6166631556 0, -1186096.2030299772 1948470.0892582536 0, -1186491.139595801 1948528.5917956394 0, -1186431.7017706153 1948930.5624904055 0, -1186372.2637454076 1949332.5322974538 0, -1186312.8157335003 1949734.49964899 0, -1186253.3773090634 1950136.4676753902 0, -1185859.758994891 1950077.796469102 0, -1185466.1282724966 1950019.1421073962 0, -1185070.6222038823 1949960.1655721343 0, -1184675.103735667 1949901.2058671056 0, -1184734.1684757974 1949499.5883326414 0, -1184793.2443894309 1949097.9615052918 0, -1184852.3185068783 1948696.343759482 0)), ((-1181884.3401847018 1952349.62141396 0, -1181489.663253396 1952290.7109749934 0, -1181094.9837210989 1952231.818929109 0, -1181153.606980693 1951837.930128558 0, -1181213.7998061194 1951436.4704010205 0, -1181273.9826235292 1951035.008202347 0, -1181668.533676252 1951093.7457282406 0, -1182063.0805350034 1951152.511622226 0, -1182457.6345766736 1951211.2974813473 0, -1182852.1680303665 1951270.088636811 0, -1182792.2110123308 1951671.7928474464 0, -1182732.245585199 1952073.4846184973 0, -1182673.696025463 1952467.4990369854 0, -1182279.0145135478 1952408.550245857 0, -1181884.3401847018 1952349.62141396 0)), ((-1179515.3458221497 1951996.3120427965 0, -1179910.2526456257 1952055.1550170188 0, -1180305.1650700283 1952114.0279190429 0, -1180700.0764899934 1952172.9092436894 0, -1181094.9837210989 1952231.818929109 0, -1181035.5736542786 1952633.4635708747 0, -1180976.1535832637 1953035.105737911 0, -1180916.74467373 1953436.7385926174 0, -1</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Tonkawa</t>
+          <t>Uintah and Ouray</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>UT</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Public Building, Common Schools, Oklahoma State University, State Educational Institutions</t>
+          <t>Public Schools, Recreation Exchange, Multi-Beneficiary, College of Mines and Earth Sciences, UtahÔøΩStateÔøΩHospital, Reservoirs, UtahÔøΩSchools for the Deaf, University ofÔøΩUtah, UtahÔøΩStateÔøΩUniversity, Juvenile Justice Services, UtahÔøΩSchools for the Blind, Teaching Colleges at Public Universities, Public Buildings, Miners Hospital</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>subsurface, surface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>152</v>
+        <v>1463</v>
       </c>
       <c r="G70" t="n">
-        <v>186.91</v>
+        <v>230995.4</v>
       </c>
       <c r="H70" t="n">
-        <v>6</v>
+        <v>672</v>
       </c>
       <c r="I70" t="n">
-        <v>5810.78</v>
+        <v>280566.13</v>
       </c>
       <c r="J70" t="n">
-        <v>146</v>
+        <v>791</v>
       </c>
       <c r="K70" t="n">
-        <v>5997.69</v>
+        <v>511561.53</v>
       </c>
       <c r="L70" t="n">
-        <v>91880.64999999999</v>
+        <v>4504964.31</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1200949.4146035248 1986131.3865049854 0, -1201008.5640779603 1985729.7722811436 0, -1200614.5012370858 1985673.7686730388 0, -1200669.6533357725 1985271.2897667151 0, -1201066.493713974 1985328.1256063147 0, -1201124.4264467019 1984926.4579796004 0, -1201524.0432644722 1984984.1342984058 0, -1201587.8614740546 1984581.7502122638 0, -1201985.2307194718 1984639.351418582 0, -1202382.6020516898 1984696.9409601807 0, -1202323.2590749203 1985099.5400278254 0, -1202257.5025131584 1985498.7310964514 0, -1202191.7442448295 1985897.9311084636 0, -1201797.1904774976 1985841.8542835591 0, -1201402.6258149387 1985785.7841837544 0, -1201341.8535774376 1986187.0676920137 0, -1200949.4146035248 1986131.3865049854 0)), ((-1199313.8102938333 1988900.7280749313 0, -1198924.411766142 1988843.6943137369 0, -1198985.113375903 1988444.5957812008 0, -1199375.1571254837 1988503.367987584 0, -1199436.503853103 1988106.0068802263 0, -1199827.1983496007 1988166.547356416 0, -1199888.7259280758 1987770.6245739467 0, -1200280.5990791349 1987832.833716148 0, -1200343.3062871008 1987438.5702774525 0, -1200734.5698639639 1987496.4786489669 0, -1201125.8437221616 1987554.3869302985 0, -1201065.402010298 1987951.2005946347 0, -1200673.0051892675 1987892.0187706524 0, -1200611.4306241132 1988287.5563193974 0, -1200217.890172515 1988227.106117349 0, -1200154.5920585152 1988620.8540026043 0, -1199764.8849283112 1988562.1083989786 0, -1199702.5616101853 1988957.666862466 0, -1199313.8102938333 1988900.7280749313 0)), ((-1223143.436401538 1989881.719152336 0, -1223419.4352111868 1989923.7774424125 0, -1223535.9816394616 1989941.6531504765 0, -1223812.1357923334 1989983.7452325672 0, -1223928.5534829786 1990001.6100994176 0, -1224204.8433981768 1990043.7328470063 0, -1224139.843618964 1990444.944148744 0, -1224074.8536150574 1990846.1559898094 0, -1223683.6110876764 1990782.5072356572 0, -1223292.3787798015 1990718.858378817 0, -1222901.1371126957 1990655.2062944588 0, -1222509.8958780668 1990591.5525453805 0, -1222571.9559296 1990197.724306925 0, -1222634.015968297 1989803.8950855925 0, -1222750.8590300886 1989821.7987297545 0, -1223026.7220759718 1989863.826351641 0, -1223143.436401538 1989881.719152336 0)), ((-1222542.1489198531 1995514.436441026 0, -1222155.7781050908 1995451.2022305646 0, -1221769.4045387236 1995387.986314855 0, -1221836.504233702 1994990.4565124046 0, -1221903.6023083215 1994592.9356454306 0, -1222288.3583468322 1994653.879323529 0, -1222673.1116197156 1994714.8413128022 0, -1222607.6310736444 1995114.6344123706 0, -1222542.1489198531 1995514.436441026 0)), ((-1201659.4476120977 1996675.8534731867 0, -1201744.9832824129 1996662.408207222 0, -1201835.2855395805 1996648.2221966062 0, -1201868.6205855391 1996654.307126532 0, -1201949.4849365936 1996795.4842738025 0, -1202011.3662478626 1996779.085643789 0, -1202066.0289064448 1996803.4623602377 0, -1202124.5704391345 1996848.7081638963 0, -1202089.9396841028 1997077.5244327018 0, -1202028.971132923 1997475.37670198 0, -1201631.711433702 1997414.6150895464 0, -1201234.646459388 1997353.8929998917 0, -1201294.6483140206 1996954.8134063454 0, -1201354.0538059068 1996554.2472903777 0, -1201453.4910764284 1996191.6643473764 0, -1201859.681803924 1996257.7183014518 0, -1201751.6667690177 1996617.4994862182 0, -1201690.0623007054 1996607.5600724139 0, -1201513.1361385188 1996579.7178727558 0, -1201566.3729970062 1996664.9414722568 0, -1201659.4476120977 1996675.8534731867 0)), ((-1223783.3877977077 1996529.6031083053 0, -1223982.4632963662 1996557.8789112386 0, -1223921.3039287934 1996958.2968418167 0, -1223719.7676918844 1996928.9535949833 0, -1223783.3877977077 1996529.6031083053 0)), ((-1226224.4013266957 1997734.1563803519 0, -1226164.75220724 1998132.4426223265 0, -1225771.418804286 1998069.1362751452 0, -1225378.0858237073 1998005.8282160312 0, -1225438.9652518556 1997605.3160135497 0, -1225499.8510547597 1997204.762899866 0, -1225891.9505479299 1997270.3168557796 0, -1226284.0488838982 1997335.87908203 0, -1226224.4013266957 1997734.1563803519 0)), ((-1224011.6469405184 1999021.8959077331 0, -1224041.4676897498 1998825.9433438212 0, -1224072.6007326506 1998621.3173565797 0, -1224175.176919924 1998637.1867835436 0, -1224219.6011097645 1998644.061814488 0, -1224283.7478828828 1998243.9815083751 0, -1224133.5659189047 1998220.7293548975 0, -1224195.1988720312 1997819.1633783365 0, -1224591.4049895727 1997879.2452730516 0, -1224529.290479228 1998282.0122576081 0, -1224923.2498256515 1998344.1667091553 0, -1224862.1799927137 1998744.6054138567 0, -1225255.9658451523 1998806.658980719 0, -1225194.7237044915 1999206.9875076083 0, -1224801.1117659858 1999145.0331064777 0, -1224407.5100378783 1999083.0785490803 0, -1224011.6469405184 1999021.8959077331 0)), ((-1211938.199385719 1999251.9292097052 0, -1211708.2860837039 1999217.054850042 0, -1211739.7245894852 1999019.934832633 0, -1211793.9822809868 1998848.1292916932 0, -1211801.5882713445 1998824.0457813325 0, -1211761.4914027578 1998665.1450358173 0, -1211743.4844433214 1998593.7942208254 0, -1211723.6454804663 1998519.074035636 0, -1211697.5921301139 1998420.9349449435 0, -1211667.7705426493 1998416.1714279458 0, -1211671.6267437972 1998391.8670954371 0, -1211736.120784928 1997991.4536868574 0, -1211759.7685744949 1997995.016372625 0, -1212130.3548239018 1998054.7113660679 0, -1212361.1455087503 1998088.7947185356 0, -1212497.7644001434 1998267.784060639 0, -1212394.8303602547 1998910.8103656892 0, -1212002.221016313 1998851.4524695664 0, -1212001.4851433197 1998851.3451502009 0, -1211938.199385719 1999251.9292097052 0)), ((-1211625.379728793 2001256.687723491 0, -1211233.2807288296 2001198.2464947454 0, -1211295.7737314815 2000796.9178301052 0, -1211358.2666912023 2000395.5880874582 0, -1211750.2268920816 2000454.0680641413 0, -1212142.187544372 2000512.5463302468 0, -1212079.8317922114 2000913.847289778 0, -1212017.476001224 2001315.1471723234 0, -1211625.379728793 2001256.687723491 0)), ((-1239286.9752013446 2000957.7813093676 0, -1239233.9397241138 2001365.6879314126 0, -1238841.929181456 2001305.8821331554 0, -1238743.3460844427 2001290.8404238424 0, -1238796.4796279324 2000884.595153859 0, -1238503.2533085248 2000840.8426608983 0, -1238556.5909239606 2000435.589719444 0, -1238747.5856001636 2000463.4427302745 0, -1238718.9932655112 2000664.4696718368 0, -1238921.958696769 2000694.067133627 0, -1238948.3022853793 2000492.7225605128 0, -1239340.0026043046 2000549.8621019782 0, -1239731.709873227 2000607.021433765 0, -1239680.696164114 2001016.5496067496 0, -1239286.9752013446 2000957.7813093676 0)), ((-1199488.400481616 2003700.7845815797 0, -1199446.2541140798 2004018.886376972 0, -1199435.6734278726 2004097.0835830967 0, -1199392.7873951585 2004421.0149994013 0, -1199382.0074318317 2004493.476731145 0, -1199012.6275708398 2004434.6261367777 0, -1198616.147769523 2004371.3797959967 0, -1198219.6751145 2004308.1531906656 0, -1197823.19002622 2004244.9431902638 0, -1197880.7325412876 2003843.6001293233 0, -1197937.5119648324 2003442.6961403133 0, -1198332.0451085707 2003508.4350993743 0, -1198277.3532443237 2003908.3443222241 0, -1198673.963112886 2003973.0951545911 0, -1199070.5687549158 2004037.8741253703 0, -1199121.113285039 2003639.9691604427 0, -1199488.400481616 2003700.7845815797 0)), ((-1250198.876306713 2005962.3489113243 0, -1250590.909210174 2006023.710049164 0, -1250528.2781075302 2006423.9168497787 0, -1250921.141191029 2006485.7457691838 0, -1251314.0143797263 2006547.5745069631 0, -1251251.2997013847 2006947.9407636316 0, -1250858.469156953 2006886.026792026 0, -1250465.6389268648 2006824.1110779692 0, -1250073.1321132244 2006761.8669079489 0, -1249680.6158270082 2006699.6194389884 0, -1249617.6377757322 2007098.082292455 0, -1249221.292169128 2007037.8089200025 0, -1248824.9437029413 2006977.5537103121 0, -1248890.3705293871 2006577.723025546 0, -1248492.1883682916 2006515.8758622867 0, -1248094.006535081 2006454.0269105784 0, -1248159.4489725113 2006053.16543721 0, -1247761.2891187842 2005990.8071546177 0, -1247363.1198071872 2005928.445525758 0, -1247428.6104098717 2005526.538003521 0, -1247826.7580702042 2005589.4071762606 0, -1248224.906066516 2005652.2745642345 0, -1248623.0610138224 2005715.1616635385 0, -1249021.2065024893 2005778.0454177293 0, -1249414.0249507115 2005839.5165988407 0, -1249806.8437167546 2005900.9860418532 0, -1250198.876306713 2005962.3489113243 0)), ((-1247566.6694429861 2007195.5715515325 0, -1247630.3480796162 2006793.562503844 0, -1248028.555996695 2006854.8757994352 0, -1248426.751274466 2006916.2056816863 0, -1248824.9437029413 2006977.5537103121 0, -1248760.0966418097 2007379.7958559261 0, -1248362.2845145166 2007318.385699903 0, -1247964.4840919334 2007256.965347405 0, -1247566.6694429861 2007195.5715515325 0)), ((-1214884.9514026928 2011587.7699811428 0, -1214823.6887198512 2011988.554887671 0, -1214432.1813166821 2011931.952489681 0, -1214038.8685967259 2011871.3089509988 0, -1214100.2322876945 2011470.785835063 0, -1213707.0202478133 2011410.4633386673 0, -1213808.1304391075 2010762.22808278 0, -1214140.6939690532 2010810.974031074 0, -1214177.9683250245 2010911.4998709369 0, -1214475.6776406844 2010971.7266713823 0, -1214536.4578955977 2011112.1671980636 0, -1214529.8486618707 2011293.5120795213 0, -1214530.434687362 2011296.0075491248 0, -1214493.431810409 2011531.124937915 0, -1214884.9514026928 2011587.7699811428 0)), ((-1203414.773080094 2017818.9878087633 0, -1203021.3449131686 2017761.423441275 0, -1202627.9140480196 2017703.8772140818 0, -1202687.8143944452 2017300.7751719146 0, -1202746.846823229 2016900.4051773595 0, -1203141.0981948192 2016958.5215804302 0, -1203535.3370808254 2017016.654554963 0, -1203475.0921401458 2017416.7085512585 0, -1203414.773080094 2017818.9878087633 0)), ((-1229885.7531415808 2017938.892345719 0, -1230278.27186139 2017998.945235504 0, -1230670.7893786563 2018059.0063095205 0, -1230607.6603637964 2018455.4002416127 0, -1230544.5329900116 2018851.7831042658 0, -1230149.4687500696 2018791.2440430394 0, -1229754.4017251895 2018730.7231066062 0, -1229359.3303284014 2018670.2302620958 0, -1228965.276372797 2018609.9693858812 0, -1228571.2294262208 2018549.7282063698 0, -1228177.178109552 2018489.5151287275 0, -1227783.1142206467 2018429.3186240913 0, -1227852.942872487 2018036.5505560231 0, -1227922.7731155031 2017643.7714194034 0, -1228315.3855124349 2017702.5402665238 0, -1228708.0080880623 2017761.3088930578 0, -1229100.6212568304 2017820.0741747317 0, -1229493.2461895708 2017878.8292683167 0, -1229885.7531415808 2017938.892345719 0)), ((-1206105.5278482453 2018606.1810173478 0, -1205713.8515176112 2018553.733399309 0, -1205322.1610654704 2018501.312333519 0, -1205382.0702499007 2018099.805695467 0, -1205772.3526640234 2018152.7374070461 0, -1206162.6421304154 2018205.688848611 0, -1206552.9174745223 2018258.66685713 0, -1206497.211229256 2018658.6483505857 0, -1206105.5278482453 2018606.1810173478 0)), ((-1206272.1471640056 2020272.094377161 0, -1206319.771786443 2019860.462891817 0, -1205928.7723013028 2019814.0727765951 0, -1205995.245163187 2019409.7445033374 0, -1206390.0777057828 2019459.2916460761 0, -1206746.3742502234 2019504.7952211872 0, -1206687.703592044 2019904.6677672267 0, -1207082.5781711931 2019963.9683060655 0, -1207023.2084410943 2020364.5151582565 0, -1206628.6340526156 2020304.7104994433 0, -1206272.1471640056 2020272.094377161 0)), ((-1204575.983485033 2020844.4712396988 0, -1204182.154224872 2020786.848793847 0, -1203788.3026792211 2020729.241342847 0, -1203849.091208816 2020342.5179917072 0, -1203909.415305679 2019961.4732845365 0, -1204302.928527725 2020020.9987176163 0, -1204696.4390576784 2020080.5422823506 0, -1204637.0053456717 2020457.0897676328 0, -1204575.983485033 2020844.4712396988 0)), ((-1209332.818848822 2021125.1684327514 0, -1209272.771639584 2021530.6954869886 0, -1209213.2751222092 2021936.483071149 0, -1209154.272241546 2022338.985942864 0, -1208759.8565809361 2022277.5207135705 0, -1208818.5156753226 2021875.2288204296 0, -1208877.468430193 2021470.5911785201 0, -1208937.3975810385 2021065.4338153556 0, -1208997.3876847923 2020661.2150426162 0, -1209392.596071574 2020719.8219105892 0, -1209332.818848822 2021125.1684327514 0)), ((-1205302.2244544607 2021349.971451156 0, -1205242.567928354 2021749.6392183537 0, -1205178.4817013156 2022150.0696602145 0, -1204787.0127856692 2022091.9792527887 0, -1204848.2562035522 2021692.4437968323 0, -1204908.9907677753 2021294.9005438634 0, -1205302.2244544607 2021349.971451156 0)), ((-1232957.6495970143 2022111.1251855183 0, -1232957.7353560326 2022110.5869775526 0, -1233085.527546776 2021308.5850659579 0, -1233085.8372327816 2021306.6415261528 0, -1233371.2401876114 2021352.1115497453 0, -1233307.3027463725 2021754.1336854794 0, -1233243.3685518657 2022156.1347434698 0, -1232957.6495970143 2022111.1251855183 0)), ((-1203666.8994157643 2021513.3005405762 0, -1204060.6213631586 2021572.9930481655 0, -1203999.0077779 2021970.680419623 0, -1203938.3219586762 2022369.915049777 0, -1203543.2228862923 2022309.399046005 0, -1203605.0004523103 2021910.0631655224 0, -1203666.8994157643 2021513.3005405762 0)), ((-1240824.7997962106 2022116.7025246206 0, -1241216.3239648386 2022181.4804448355 0, -1241607.8551180388 2022246.2780687707 0, -1242000.8346198548 2022311.7543284777 0, -1242393.8211085119 2022377.250277791 0, -1242786.79499762 2022442.7627955063 0, -1243179.7758707441 2022508.2950022228 0, -1243570.5444152341 2022566.472135946 0, -1243961.319898175 2022624.6689802737 0, -1244352.090938294 2022682.893941753 0, -1244704.043135988 2022735.6987950618 0, -1245100.672702718 2022800.8936539893 0, -1245497.2994534615 2022866.106606608 0, -1245893.9315920607 2022931.3491798039 0, -1246290.5511192465 2022996.608286078 0, -1246688.3028421644 2023060.3697814473 0, -1246854.222548723 2023086.9641918603 0, -1247086.04194313 2023124.147799671 0, -1247483.7782132423 2023187.9439005193 0, -1247881.5198564983 2023251.769610707 0, -1248274.3760642011 2023317.2067196239 0, -1248667.2376472114 2023382.673481462 0, -1249060.0866059994 2023448.1568093183 0, -1249452.9441114145 2023513.649855215 0, -1249847.316838842 2023578.7078421412 0, -1250241.6965216782 2023643.7854998587 0, -1250636.0749527814 2023708.8713013076 0, -1251030.439164145 2023773.983621087 0, -1251420.8377171035 2023834.0475751222 0, -1251811.2447756436 2023894.1212700573 0, -1252201.6375792723 2023954.2215212677 0, -1252592.029092959 2024014.329953608 0, -1252985.8073247832 2024079.3396748095 0, -1253379.5745004576 2024144.3559842452 0, -1253773.3388244524 2024209.3904081208 0, -1254143.464578902 2024270.4652805342 0, -1254540.4336789472 2024330.5693503893 0, -1254480.561012865 2024733.1099419487 0, -1254420.6803270606 2025135.637883956 0, -1254816.070587661 2025195.8975025956 0, -1254755.42314183 2025598.4555184136 0, -1254694.7676744922 2026001.0008800384 0, -1255088.582258263 2026061.396129427 0, -1255482.3939579725 2026121.8094874748 0, -1255875.4416704772 2026186.391620376 0, -1256268.4767259322 2026250.9903073946 0, -1256661.508915793 2026315.607107215 0, -1256600.6694906123 2026716.9467298146 0, -1256993.89299775 2026782.4505437952 0, -1256933.229952671 2027184.6448551298 0, -1257324.2901272497 2027244.9481369173 0, -1257263.0153584753 2027646.8293020562 0, -1257653.4458903556 2027706.8056826259 0, -1257591.5413923927 2028108.3606214274 0, -1257525.2230301008 2028505.7883454151 0, -1257458.904829029 2028903.2149502914 0, -1257850.185653451 2028965.0621591632 0, -1258241.4651761076 2029026.91752068 0, -1258176.6170405287 2029426.4777840169 0, -1258111.7772884814 2029826.048442068 0, -1258047.1366058583 2030226.3240997333 0, -1258439.619044347 2030290.1063409834 0, -1258374.5898588668 2030690.7482105817 0, -1258309.5722330518 2031091.3805298947 0, -1258244.5481669626 2031491.9902132635 0, -1258180.9745911143 2031890.4893605306 0, -1257789.5470117969 2031825.7917771202 0, -1257397.058731641 2031763.089979814 0, -1257004.5707433224 2031700.386345697 0, -1256940.962613132 2032099.522656034 0, -1256548.5191066172 2032037.1001378882 0, -1256484.946862812 2032436.4453752316 0, -1256092.5330086597 2032374.2709517737 0, -1255700.510181279 2032314.1189771222 0, -1255308.4974309984 2032253.9667281853 0, -1255371.759463026 2031853.4377977676 0, -1254979.6008854692 2031792.8210392797 0, -1254587.4425973361 2031732.2024480815 0, -1254191.95264393 2031670.182949536 0, -1253796.4531999393 2031608.1600279238 0, -1253859.6203336667 2031207.246962477 0, -1253464.2134179117 2031145.5332332975 0, -1253068.8181858058 2031083.8092356243 0, -1253132.1585524387 2030683.5255467219 0, -1252768.9144148913 2030625.1608824118 0, -1252375.8307867476 2030562.0435614423 0, -1251983.2787089215 2030499.1827182607 0, -1251590.7221853412 2030436.3499428467 0, -1251193.902099216 2030371.5998309178 0, -1250797.0791710068 2030306.8677798829 0, -1250400.2518153617 2030242.1637567105 0, -1250003.4134142431 2030177.466268665 0, -1249607.731750929 2030113.1350200824 0, -1249212.0374554251 2030048.820284649 0, -1248816.3501153798 2029984.5251818541 0, -1248420.6501460623 2029920.2465926132 0, -1248026.4912020147 2029856.1910947484 0, -1247632.327835281 2029792.1636517057 0, -1247238.1632212957 2029728.1443303619 0, -1246843.9941874365 2029664.153064309 0, -1246452.892148137 2029596.1620961318 0, -1246061.7888863166 2029528.179277119 0, -1245670.67143612 2029460.2229808578 0, -1245279.5609720952 2029392.2863610035 0, -1244880.4399652374 2029333.035713487 0, -1244481.3047312102 2029273.811517816 0, -1244082.1764446825 2029214.6069278538 0, -1243683.0339338758 2029155.428789975 0, -1243339.3741954616 2029101.0827773253 0, -1242946.7681836765 2029039.0079999948 0, -1242555.324435895 2028977.0756579326 0, -1242163.8860647916 2028915.172960424 0, -1241770.1254374017 2028851.3960662757 0, -1241376.3831700536 2028787.6304226187 0, -1240984.2828058784 2028724.77858945 0, -1240592.181212203 2028661.9349018326 0, -1240200.7532791651 2028598.6448393282 0, -1239809.322533992 2028535.3728955484 0, -1239417.8873904916 2028472.1290372899 0, -1239026.4510252296 2028408.8933316357 0, -1239090.6484675815 2028005.5682271295 0, -1239154.8476013097 2027602.2319856184 0, -1239219.0468385175 2027198.894575455 0, -1239283.246178932 2026795.5559984501 0, -1239345.920694454 2026394.4770470175 0, -1239408.5969054077 2025993.3869810896 0, -1239471.2814289166 2025592.307296627 0, -1239533.9578545913 2025191.2149403521 0, -1239593.4783309621 2024791.9689913124 0, -1239652.9891357217 2024392.7203571005 0, -1239712.500061204 2023993.4706002155 0, -1239772.020899634 2023594.2212831436 0, -1239839.4509167261 2023192.4704520234 0, -1239906.8810148402 2022790.7184735409 0, -1239974.3096060858 2022388.97531649 0, -1240041.7398655603 2021987.221048717 0, -1240433.2712334564 2022051.952714843 0, -1240824.7997962106 2022116.7025246206 0), (-1248679.1504517798 2028318.3355548251 0, -1248281.1012414123 2028253.2007077434 0, -1247883.0409976325 2028188.072392038 0, -1247950.8550266984 2027790.3148147415 0, -1248018.6691689556 2027392.5561029816 0, -1247620.1990256833 2027328.9447225698 0, -1247221.739016179 2027265.3330268385 0, -1247154.3271923906 2027661.6227578027 0, -1247086.9170654146 2028057.9013955873 0, -1247026.186511067 2028459.4635404407 0, -1247423.2705223358 2028524.297168386 0, -1247820.3564682123 2028589.1189620579 0, -1248217.437998981 2028653.9687882473 0, -1248614.5296671642 2028718.8183060996 0, -1248549.9008149747 2029119.28838522 0, -1248944.6187334761 2029183.6659870485 0, -1249339.338575796 2029248.0317741423 0, -1249734.0587533587 2029312.3957129922 0, -1250128.7792645586 2029376.757803301 0, -1250191.4583207741 2028976.396093616 0, -1250254.137532732 2028576.0332437023 0, -1249860.397470757 2028511.5820652237 0, -1249466.644774831 2028447.147424419 0, -1249072.89903236 2028382.7324407294 0, -1248679.1504517798 2028318.3355548251 0), (-1248417.1298585548 2027456.164048192 0, -1248815.6006786304 2027519.7716774573 0, -1248883.826760444 2027120.4830428087 0, -1248952.0415787275 2026721.2016760434 0, -1248553.179836742 2026659.0546324335 0, -1248154.3120755805 2026596.9455808732 0, -1248086.4913593903 2026994.7464240948 0, -1248018.6691689556 2027392.5561029816 0, -1248417.1298585548 2027456.164048192 0)), ((-1205613.2579564946 2024675.5960363327 0, -1205675.5244646221 2024274.1660020929 0, -1206032.660344529 2024329.3412408892 0, -1206428.4227780085 2024389.8282359694 0, -1206370.059889674 2024791.7290923826 0, -1206311.8148573178 2025194.5265068624 0, -1205915.429507019 2025133.01981894 0, -1205553.0379621363 2025077.3519040926 0, -1205613.2579564946 2024675.5960363327 0)), ((-1210826.6896727383 2024644.9510114104 0, -1210766.8396209527 2025048.7023286093 0, -1210708.0706603783 2025452.7886553959 0, -1210652.5090646092 2025859.0519228405 0, -1210259.6466006862 2025799.2429971588 0, -1210315.3310209601 2025393.224340328 0, -1210373.7644687237 2024988.9823952538 0, -1210433.3022160495 2024585.559505433 0, -1210493.3687443314 2024183.793758386 0, -1210887.3913352073 2024243.2252126785 0, -1210826.6896727383 2024644.9510114104 0)), ((-1200231.0400632427 2025535.3340568452 0, -1200285.8945334961 2025124.8883061956 0, -1200680.5298244192 2025181.563982954 0, -1201074.9665822696 2025238.2264538677 0, -1201019.0329055046 2025649.0315278738 0, -1200625.0378307404 2025592.1737410005 0, -1200231.0400632427 2025535.3340568452 0)), ((-1321280.6173853083 2058083.5737533076 0, -1321664.5810077875 2058142.4762339485 0, -1322062.3611194459 2058210.5236693362 0, -1321995.9126071483 2058609.6128780514 0, -1321995.8019652606 2058610.2773933143 0, -1321599.448249967 2058543.876546212 0, -1321202.0510165088 2058477.2808153273 0, -1321280.6173853083 2058083.5737533076 0)), ((-1179105.2869066224 1888617.7273695231 0, -1179115.9710953655 1888616.9338675025 0, -1179055.91134986 1888996.7362096165 0, -1178665.555186845 1888942.4659631737 0, -1178602.9243309263 1888933.7580948023 0, -1178615.1686528765 1888924.7423638906 0, -1178628.521187138 1888912.6537212462 0, -1178668.8000334883 1888876.6469856459 0, -1178678.9045889655 1888867.7110062523 0, -1178680.0172958132 1888866.726883542 0, -1178726.2427016278 1888560.2434908405 0, -1179102.3208169893 1888617.9476949621 0, -1179105.2869066224 1888617.7273695231 0)), ((-1186872.9404039271 1890491.6713313425 0, -1186872.9499457758 1890491.6069984068 0, -1186874.038604841 1890491.4992944147 0, -1186872.9404039271 1890491.6713313425 0)), ((-1187740.3863162966 1890499.7574263406 0, -1187748.0021001725 1890497.9372015141 0, -1187756.097569647 1890501.0593707971 0, -1187769.8049647976 1890517.7187150263 0, -1187735.7767808228 1890537.4623593946 0, -1187735.0307261655 1890521.9647945906 0, -1187736.0798005583 1890507.8447073444 0, -1187740.3863162966 1890499.7574263406 0)), ((-1187667.5501648362 1890568.6700683476 0, -1187429.897759995 1890618.9811750606 0, -1187382.6620204141 1890677.4576822075 0, -1187278.4854413432 1890612.248134321 0, -1187259.0582802685 1890605.7146222093 0, -1186904.8840154533 1890486.6672553835 0, -1186876.2157106234 1890491.1582433505 0, -1186886.8172234602 1890419.606674067 0, -1187725.3433674988 1890543.515976666 0, -1187690.2819010757 1890563.8591464516 0, -1187667.5501648362 1890568.6700683476 0)), ((-1188123.1064447055 1890600.9546276894 0, -1188128.0039866117 1890603.014600695 0, -1188138.3730090496 1890604.5467761555 0, -1188144.3265888842 1890601.825143622 0, -1188151.8937026053 1890596.8258572621 0, -1188174.7378867653 1890576.1840846913 0, -1188205.3639952096 1890556.6926516807 0, -1188230.8611510843 1890550.2649717983 0, -1188272.4515197284 1890561.8512074805 0, -1188298.2323615844 1890572.7998664386 0, -1188312.1030920038 1890581.8746381055 0, -1188315.9869673569 1890591.8521417447 0, -1188313.110770919 1890609.5541057098 0, -1188315.5454941096 1890630.726273488 0, -1188461.169951352 1890652.2442963165 0, -1188450.3049999387 1890725.5993665976 0, -1188421.50489671 1890726.4331994643 0, -1188378.9585863028 1890727.7680660281 0, -1188266.312074268 1890640.1686700091 0, -1188061.9755397409 1890626.546116768 0, -1187894.4421532732 1890615.3684420993 0, -1187830.581959661 1890559.0666487284 0, -1188068.9253935083 1890594.2850415143 0, -1188072.961564745 1890592.8631398568 0, -1188095.3008167378 1890590.840211846 0, -1188104.430743351 1890591.0567089948 0, -1188123.1064447055 1890600.9546276894 0)), ((-1194406.0165086838 1892277.5862176022 0, -1194465.4208935194 1891875.9678030992 0, -1194524.8234477565 1891474.3587166604 0, -1194918.1344180182 1891532.8403313872 0, -1195311.4329493698 1891591.3390325352 0, -1195704.7370191833 1891649.8679212425 0, -1196098.0400220633 1891708.4054882715 0, -1196038.6754803476 1892109.6026921868 0, -1195979.3091151244 1892510.8092263872 0, -1195919.94410731 1892912.0051446112 0, -1195860.587061192 1893313.2119541636 0, -1195467.2460356867 1893255.0862772418 0, -1195073.9039429305 1893196.9692714587 0, -1194680.5576036887 1893138.8808814313 0, -1194287.2183944033 1893080.812699648 0, -1194346.6216684908 1892679.2055507903 0, -1194406.0165086838 1892277.5862176022 0)), ((-1178359.9781860579 1893376.8770570161 0, -1178415.8113924572 1892979.0734418454 0, -1178471.6427189133 1892581.279152106 0, -1178527.4851311543 1892183.4758120168 0, -1178927.6116216248 1892242.5125736254 0, -1179327.7485048182 1892301.5495577876 0, -1179727.8698472194 1892360.6235194542 0, -1180127.990204148 1892419.7061092216 0, -1180516.993823687 1892535.830099272 0, -1180456.068967295 1892950.6668688487 0, -1180066.9659569485 1892838.8728355994 0, -1180005.9413891886 1893258.038840582 0, -1179944.9165011777 1893677.204122247 0, -1179883.9010774507 1894096.3702444974 0, -1179488.9723053728 1894015.9258636925 0, -1179094.0441929265 1893935.480196685 0, -1178699.0892185145 1893855.079970265 0, -1178304.1462819271 1893774.6700527072 0, -1178359.9781860579 1893376.8770570161 0)), ((-1190778.829093544 1895026.871992526 0, -1190839.760251897 1894625.2293031116 0, -1190900.7009389747 1894223.587514901 0, -1191295.2800924832 1894282.1221429226 0, -1191689.858199118 1894340.6654296252 0, -1192084.4320763815 1894399.2373190005 0, -1192479.0017228236 1894457.8378109236 0, -1192416.8089803848 1894859.2296450553 0, -1192354.6257699209 1895260.6223786166 0, -1192292.579050568 1895661.9749551334 0, -1192229.6659854073 1896068.94580703 0, -1191836.1569407692 1896011.2293614007 0, -1191442.6452515044 1895953.5315459068 0, -1191049.1407037235 1895895.8539255825 0, -1190655.623729621 1895838.1933708163 0, -1190717.8532868377 1895428.4148791246 0, -1190778.829093544 1895026.871992526 0)), ((-1195711.515713946 1896991.7734474617 0, -1195651.6267974805 1897393.2779463765 0, -1195591.7503743176 1897794.7020027523 0, -1195531.8753121055 1898196.1154197033 0, -1195137.8224340407 1898138.2517039974 0, -1195197.746987196 1897736.8465314081 0, -1195257.6713091212 1897335.4406911351 0, -1195317.5953995492 1896934.0341848754 0, -1195377.5290429997 1896532.6285788429 0, -1195771.4044003438 1896590.2682842822 0, -1195711.515713946 1896991.7734474617 0)), ((-1193082.5478134777 1901109.9753088155 0, -1193475.8960802914 1901170.3934988985 0, -1193415.7913449106 1901571.7017512866 0, -1193022.3988302003 1901511.3681873989 0, -1193082.5478134777 1901109.9753088155 0)), ((-1177752.4872717867 1903502.8787994755 0, -1177359.8021421588 1903441.4241137463 0, -1176967.1144337156 1903379.9880371129 0, -1177021.8245550608 1902987.4604622647 0, -1177076.5328122007 1902594.9421904658 0, -1177131.2521716019 1902202.414847007 0, -1177185.9696662202 1901809.8968097374 0, -1177577.428125001 1901876.44191709 0, -1177968.8758242452 1901942.994117986 0, -1178360.3193647412 1902009.5749209428 0, -1178751.771711725 1902076.1659491605 0, -1178698.2916188638 1902463.5864314684 0, -1178644.809676144 1902851.0162392645 0, -1178591.329066001 1903238.4354284331 0, -1178537.8481976374 1903625.853968784 0, -1178145.1698211322 1903564.3520941334 0, -1177752.4872717867 1903502.8787994755 0)), ((-1190908.3198422568 1904888.1385654486 0, -1190848.7425799756 1905289.809262526 0, -1190788.5411628187 1905695.7050735203 0, -1190395.0807721363 1905635.6361323004 0, -1190001.6177493844 1905575.5857850604 0, -1189608.1423110566 1905515.5524668305 0, -1189214.664243633 1905455.5377428497 0, -1189219.171575706 1905425.0182571036 0, -1189274.2901261137 1905051.8827897592 0, -1189667.9235759 1905111.3595901635 0, -1190061.5477913003 1905170.8334764433 0, -1190121.0204423175 1904769.1978609448 0, -1189727.318542925 1904709.7118929208 0, -1189333.6156033983 1904650.2345486004 0, -1189392.9622375325 1904248.6401592877 0, -1189452.308626869 1903847.0450700808 0, -1189481.2739230653 1903851.350970904 0, -1189846.1548405404 1903906.3707972832 0, -1190239.997073223 1903965.786488621 0, -1190633.8205257917 1904025.2590989687 0, -1191027.6413443335 1904084.7503066773 0, -1190967.981508196 1904486.4398003086 0, -1190908.3198422568 1904888.1385654486 0)), ((-1179945.6358764141 1905066.5924320498 0, -1179970.7189541813 1904895.560016338 0, -1180004.802821503 1904663.150277138 0, -1180029.770264339 1904493.847700341 0, -1180064.1989814092 1904260.4701743908 0, -1180089.0169855845 1904092.16599216 0, -1180463.5398180843 1904147.3500395033 0, -1180838.0486198857 1904202.5612151208 0, -1180878.008857196 1904208.4552150238 0, -1181212.5481627237 1904257.76960505 0, -1181272.4486707496 1904266.6091266726 0, -1181587.0532416308 1904313.0082548873 0, -1181666.8890657434 1904324.7616849826 0, -1181607.6338308388 1904726.5765007597 0, -1181548.3685356055 1905128.389039277 0, -1181489.1029650006 1905530.20086466 0, -1181429.8484950538 1905932.0035698146 0, -1181035.713326319 1905873.7449473573 0, -1180641.5755574198 1905815.5049099228 0, -1180247.435189834 1905757.2834576652 0, -1179853.2922250433 1905699.0805907263 0, -1179886.4784328507 1905470.0354333818 0, -1179911.8043482066 1905297.293543197 0, -1179945.6358764141 1905066.5924320498 0)), ((-1186223.0697855402 1906234.524458163 0, -1186281.9241700133 1905832.3458637698 0, -1186310.932549742 1905635.0445003845 0, -1186340.9403507034 1905430.3458742376 0, -1186399.8568370268 1905028.3394933036 0, -1186650.132388549 1905066.2523844785 0, -1186793.9930118804 1905088.0505190296 0, -1186980.189869192 1905116.2634695985 0, -1187188.126569116 1905147.7801355016 0, -1187310.2845728302 1905166.105655993 0, -1187640.4078231023 1905215.6446172167 0, -1187581.8276503226 1905617.3173266833 0, -1187545.3951083054 1905867.138556 0, -1187523.0010153102 1906018.9601683628 0, -1187464.6224085458 1906420.6228855937 0, -1187406.2435549675 1906822.2848942888 0, -1187112.8000172758 1906778.50026626 0, -1186952.5913249126 1906754.6289590811 0, -1186558.4045455763 1906695.6563583014 0, -1186164.2151470624 1906636.7023404115 0, -1186223.0697855402 1906234.524458163 0)), ((-1178469.7116424306 1906896.4162612902 0, -1178863.3891631283 1906952.1983750868 0, -1178802.8822249305 1907355.4621336507 0, -1178409.1200194932 1907299.0116164312 0, -1178469.7116424306 1906896.4162612902 0)), ((-1184852.3185068783 1948696.343759482 0, -1184911.3826322686 1948294.7235612997 0, -1185306.3286445949 1948353.1609087712 0, -1185701.2720399515 1948411.6166631556 0, -1186096.2030299772 1948470.0892582536 0, -1186491.139595801 1948528.5917956394 0, -1186431.7017706153 1948930.5624904055 0, -1186372.2637454076 1949332.5322974538 0, -1186312.8157335003 1949734.49964899 0, -1186253.3773090634 1950136.4676753902 0, -1185859.758994891 1950077.796469102 0, -1185466.1282724966 1950019.1421073962 0, -1185070.6222038823 1949960.1655721343 0, -1184675.103735667 1949901.2058671056 0, -1184734.1684757974 1949499.5883326414 0, -1184793.2443894309 1949097.9615052918 0, -1184852.3185068783 1948696.343759482 0)), ((-1181884.3401847018 1952349.62141396 0, -1181489.663253396 1952290.7109749934 0, -1181094.9837210989 1952231.818929109 0, -1181153.606980693 1951837.930128558 0, -1181213.7998061194 1951436.4704010205 0, -1181273.9826235292 1951035.008202347 0, -1181668.533676252 1951093.7457282406 0, -1182063.0805350034 1951152.511622226 0, -1182457.6345766736 1951211.2974813473 0, -1182852.1680303665 1951270.088636811 0, -1182792.2110123308 1951671.7928474464 0, -1182732.245585199 1952073.4846184973 0, -1182673.696025463 1952467.4990369854 0, -1182279.0145135478 1952408.550245857 0, -1181884.3401847018 1952349.62141396 0)), ((-1179456.0682277712 1952398.0480524653 0, -1179515.3458221497 1951996.3120427965 0, -1179910.2526456257 1952055.1550170188 0, -1180305.1650700283 1952114.0279190429 0, -1180700.0764899934 1952172.9092436894 0, -1181094.9837210989 1952231.818929109 0, -1181035.5736542786 1952633.4635708747 0, -1180976.1535832637 1953035.105737911 0,</t>
+          <t>POLYGON Z ((-1735957.5288111183 2709325.7336960486 0, -1735894.7669745085 2709579.947660815 0, -1735560.4508488195 2709498.6150810597 0, -1735873.2193062378 2709024.509133888 0, -1735957.5288111183 2709325.7336960486 0))</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Uintah and Ouray</t>
+          <t>Umatilla</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>UT</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Public Schools, Recreation Exchange, Multi-Beneficiary, College of Mines and Earth Sciences, UtahÔøΩStateÔøΩHospital, Reservoirs, UtahÔøΩSchools for the Deaf, University ofÔøΩUtah, UtahÔøΩStateÔøΩUniversity, Juvenile Justice Services, UtahÔøΩSchools for the Blind, Teaching Colleges at Public Universities, Public Buildings, Miners Hospital</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>1463</v>
+        <v>1</v>
       </c>
       <c r="G71" t="n">
-        <v>230995.4</v>
+        <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="I71" t="n">
-        <v>280566.13</v>
+        <v>27.71</v>
       </c>
       <c r="J71" t="n">
-        <v>791</v>
+        <v>1</v>
       </c>
       <c r="K71" t="n">
-        <v>511561.53</v>
+        <v>27.71</v>
       </c>
       <c r="L71" t="n">
-        <v>4504964.31</v>
+        <v>293080.11</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>POLYGON Z ((-1735957.5288111183 2709325.7336960486 0, -1735894.7669745085 2709579.947660815 0, -1735560.4508488195 2709498.6150810597 0, -1735873.2193062378 2709024.509133888 0, -1735957.5288111183 2709325.7336960486 0))</t>
+          <t>MULTIPOLYGON Z (((-1193003.2095425471 1695774.3584740828 0, -1192984.9212274093 1695900.7692824828 0, -1192945.0435830269 1696176.3015231234 0, -1192886.8559896317 1696578.25154202 0, -1192881.9343917111 1696577.5376560343 0, -1192492.216327342 1696521.5778199872 0, -1192097.5544728765 1696464.9204099888 0, -1191702.8981870324 1696408.293970237 0, -1191310.6498185473 1696352.0224191104 0, -1191367.5662472763 1695958.1387066147 0, -1191425.6036585008 1695556.607454057 0, -1191484.279965398 1695154.292625367 0, -1191542.9719370164 1694751.9805008422 0, -1191599.5623806964 1694760.1283922999 0, -1191936.8302557205 1694808.7758680845 0, -1192330.6857806419 1694865.5900618492 0, -1192725.2076363482 1694922.6423065949 0, -1193021.7043253863 1694965.511388046 0, -1193118.2409867113 1694979.5181527494 0, -1193099.2474606927 1695110.749390148 0, -1193061.394581745 1695372.418666538 0, -1193003.2095425471 1695774.3584740828 0)), ((-1175136.4566705169 1700196.8519050677 0, -1175355.6007487734 1700231.1283220071 0, -1175392.9283744611 1700237.0265294942 0, -1175435.9682477617 1700243.7402009661 0, -1175914.600607573 1700318.5815734565 0, -1175921.385623749 1700319.6179123465 0, -1175869.8664627378 1700677.2443388063 0, -1175813.2255560244 1701079.2291578047 0, -1175419.2740635977 1701023.5417064158 0, -1175025.3900617007 1700967.8746278076 0, -1174967.7857207288 1701369.7353618878 0, -1174911.9834876428 1701759.8501871168 0, -1174762.074135036 1701742.6522933922 0, -1174824.6026744395 1701349.4990872564 0, -1174820.4623422304 1701348.9197408815 0, -1174857.8606624247 1701001.4230639348 0, -1174921.1802547355 1700543.1526606646 0, -1175082.984075629 1700566.0124138736 0, -1175136.4566705169 1700196.8519050677 0)))</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Umatilla</t>
+          <t>Ute Mountain Ute</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>OR</t>
+          <t>UT</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Common Schools</t>
+          <t>Public Schools, UtahÔøΩSchools for the Blind, UtahÔøΩStateÔøΩUniversity</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G72" t="n">
         <v>0</v>
@@ -3891,37 +3891,37 @@
         <v>0</v>
       </c>
       <c r="I72" t="n">
-        <v>27.71</v>
+        <v>834.13</v>
       </c>
       <c r="J72" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K72" t="n">
-        <v>27.71</v>
+        <v>834.13</v>
       </c>
       <c r="L72" t="n">
-        <v>293080.11</v>
+        <v>598651.62</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1193003.2095425471 1695774.3584740828 0, -1192984.9212274093 1695900.7692824828 0, -1192945.0435830269 1696176.3015231234 0, -1192886.8559896317 1696578.25154202 0, -1192881.9343917111 1696577.5376560343 0, -1192492.216327342 1696521.5778199872 0, -1192097.5544728765 1696464.9204099888 0, -1191702.8981870324 1696408.293970237 0, -1191310.6498185473 1696352.0224191104 0, -1191367.5662472763 1695958.1387066147 0, -1191425.6036585008 1695556.607454057 0, -1191484.279965398 1695154.292625367 0, -1191542.9719370164 1694751.9805008422 0, -1191599.5623806964 1694760.1283922999 0, -1191936.8302557205 1694808.7758680845 0, -1192330.6857806419 1694865.5900618492 0, -1192725.2076363482 1694922.6423065949 0, -1193021.7043253863 1694965.511388046 0, -1193118.2409867113 1694979.5181527494 0, -1193099.2474606927 1695110.749390148 0, -1193061.394581745 1695372.418666538 0, -1193003.2095425471 1695774.3584740828 0)), ((-1175136.4566705169 1700196.8519050677 0, -1175355.6007487734 1700231.1283220071 0, -1175392.9283744611 1700237.0265294942 0, -1175435.9682477617 1700243.7402009661 0, -1175914.600607573 1700318.5815734565 0, -1175921.385623749 1700319.6179123465 0, -1175869.8664627378 1700677.2443388063 0, -1175813.2255560244 1701079.2291578047 0, -1175419.2740635977 1701023.5417064158 0, -1175025.3900617007 1700967.8746278076 0, -1174967.7857207288 1701369.7353618878 0, -1174911.9834876428 1701759.8501871168 0, -1174762.074135036 1701742.6522933922 0, -1174824.6026744395 1701349.4990872564 0, -1174820.4623422304 1701348.9197408815 0, -1174857.8606624247 1701001.4230639348 0, -1174921.1802547355 1700543.1526606646 0, -1175082.984075629 1700566.0124138736 0, -1175136.4566705169 1700196.8519050677 0)))</t>
+          <t>MULTIPOLYGON Z (((-1992631.9944673681 2670926.464298897 0, -1992938.932462263 2671012.287260834 0, -1992936.7828719348 2671019.243412175 0, -1992825.3261720703 2671379.902557449 0, -1992904.8151096767 2671402.274419125 0, -1992901.0677554947 2671414.7063132157 0, -1993201.0460950553 2671494.2228502235 0, -1993088.1247060255 2671871.201701455 0, -1993058.3305977758 2671970.7121474133 0, -1993003.2970318634 2671939.513304314 0, -1992996.262628254 2671934.9114480624 0, -1992994.1999950157 2671934.3561421246 0, -1992804.3193770477 2671826.711734401 0, -1992723.4052418773 2671721.186190158 0, -1992677.6417616934 2671644.2716992777 0, -1992617.7862502602 2671606.288020065 0, -1992610.2707793624 2671598.969549228 0, -1992596.140810236 2671582.9898940483 0, -1992580.6040879954 2671566.6810664223 0, -1992567.0944994588 2671553.8842298975 0, -1992517.154220667 2671508.2119610617 0, -1992441.4175795135 2671299.07597776 0, -1992377.5585912424 2671152.7685074173 0, -1992361.3805807908 2671131.2579916352 0, -1992330.831970632 2671092.735895415 0, -1992298.4242728483 2671019.456564848 0, -1992257.486781599 2670929.531273581 0, -1992248.0455779533 2670895.511296295 0, -1992241.546146979 2670876.8117774087 0, -1992232.9681949937 2670862.147679242 0, -1992222.3049043599 2670842.983375668 0, -1992209.3735253057 2670819.7423042394 0, -1992568.143237446 2670902.140877451 0, -1992633.9366475567 2670919.403673451 0, -1992631.9944673681 2670926.464298897 0)), ((-1971019.1127336344 2680570.723298427 0, -1971409.0781579274 2680679.934139636 0, -1971798.3806258538 2680792.5859385673 0, -1971574.33247729 2681567.2272357335 0, -1971367.0090841458 2682338.5522929113 0, -1970979.1211007498 2682234.321961667 0, -1970584.2668008404 2682123.7649993724 0, -1970801.6881515817 2681347.2510244963 0, -1971019.1127336344 2680570.723298427 0)))</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Ute Mountain Ute</t>
+          <t>Warm Springs</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>UT</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Public Schools, UtahÔøΩSchools for the Blind, UtahÔøΩStateÔøΩUniversity</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -3930,7 +3930,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G73" t="n">
         <v>0</v>
@@ -3939,277 +3939,277 @@
         <v>0</v>
       </c>
       <c r="I73" t="n">
-        <v>834.13</v>
+        <v>441.49</v>
       </c>
       <c r="J73" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K73" t="n">
-        <v>834.13</v>
+        <v>441.49</v>
       </c>
       <c r="L73" t="n">
-        <v>598651.62</v>
+        <v>657110.6</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1992631.9944673681 2670926.464298897 0, -1992938.932462263 2671012.287260834 0, -1992936.7828719348 2671019.243412175 0, -1992825.3261720703 2671379.902557449 0, -1992904.8151096767 2671402.274419125 0, -1992901.0677554947 2671414.7063132157 0, -1993201.0460950553 2671494.2228502235 0, -1993088.1247060255 2671871.201701455 0, -1993058.3305977758 2671970.7121474133 0, -1993003.2970318634 2671939.513304314 0, -1992996.262628254 2671934.9114480624 0, -1992994.1999950157 2671934.3561421246 0, -1992804.3193770477 2671826.711734401 0, -1992723.4052418773 2671721.186190158 0, -1992677.6417616934 2671644.2716992777 0, -1992617.7862502602 2671606.288020065 0, -1992610.2707793624 2671598.969549228 0, -1992596.140810236 2671582.9898940483 0, -1992580.6040879954 2671566.6810664223 0, -1992567.0944994588 2671553.8842298975 0, -1992517.154220667 2671508.2119610617 0, -1992441.4175795135 2671299.07597776 0, -1992377.5585912424 2671152.7685074173 0, -1992361.3805807908 2671131.2579916352 0, -1992330.831970632 2671092.735895415 0, -1992298.4242728483 2671019.456564848 0, -1992257.486781599 2670929.531273581 0, -1992248.0455779533 2670895.511296295 0, -1992241.546146979 2670876.8117774087 0, -1992232.9681949937 2670862.147679242 0, -1992222.3049043599 2670842.983375668 0, -1992209.3735253057 2670819.7423042394 0, -1992568.143237446 2670902.140877451 0, -1992633.9366475567 2670919.403673451 0, -1992631.9944673681 2670926.464298897 0)), ((-1971019.1127336344 2680570.723298427 0, -1971409.0781579274 2680679.934139636 0, -1971798.3806258538 2680792.5859385673 0, -1971574.33247729 2681567.2272357335 0, -1971367.0090841458 2682338.5522929113 0, -1970979.1211007498 2682234.321961667 0, -1970584.2668008404 2682123.7649993724 0, -1970801.6881515817 2681347.2510244963 0, -1971019.1127336344 2680570.723298427 0)))</t>
+          <t>MULTIPOLYGON Z (((1383.5353677989615 2665597.0389574743 0, 1787.8362839817985 2665595.1437992966 0, 1789.5667013662242 2665192.0752311223 0, 1612.6779454421549 2665193.079095202 0, 1499.3286985567952 2665193.722393299 0, 1434.7197709316813 2665194.088678773 0, 1384.9421352758486 2665194.370903259 0, 1100.0312463793368 2665193.814237008 0, 986.5166697160986 2665196.539836616 0, 980.3181917673943 2665196.688671415 0, 979.234695915162 2665598.9298086413 0, 1383.5353677989615 2665597.0389574743 0)), ((1630.4892621535892 2666577.227090937 0, 1782.7804459670808 2666773.125752292 0, 1784.3763232551087 2666401.2862598463 0, 1631.4780851873477 2666401.6276745563 0, 1630.4892621535892 2666577.227090937 0)), ((-1043.9127356924253 2667205.017103878 0, -1044.3824041522014 2667606.73599305 0, -640.1260951447346 2667608.1508072903 0, -639.6571572228979 2667206.2935517295 0, -1043.9127356924253 2667205.017103878 0)), ((3412.4767253203277 2670802.752104579 0, 3413.0752287707783 2671204.0885676933 0, 3820.3192275613037 2671204.3768943134 0, 3819.07616086587 2670803.339855818 0, 3412.4767253203277 2670802.752104579 0)), ((981.2231380002734 2671211.303034148 0, 980.6184513733934 2671613.6781696626 0, 1384.406988532018 2671609.0994988997 0, 1385.6794557510357 2671207.1844922407 0, 981.2231380002734 2671211.303034148 0)), ((576.8307485585088 2671618.2796248817 0, 571.6782034535402 2672021.0900131185 0, 977.3368457358474 2672016.9964574035 0, 980.6184513733934 2671613.6781696626 0, 576.8307485585088 2671618.2796248817 0)), ((974.0551698998473 2672420.309051253 0, 970.7736638072345 2672823.562984495 0, 1380.1735619965264 2672820.506616753 0, 1381.5849194588827 2672416.7318239957 0, 974.0551698998473 2672420.309051253 0)), ((5912.8415571091955 2674827.5905595156 0, 5915.34731046087 2674406.918686161 0, 5917.757013608493 2674002.4214660246 0, 6319.887350455133 2673997.197710027 0, 6722.018009562836 2673991.969764447 0, 6722.4135626571415 2674391.254104146 0, 7124.713803093802 2674393.2473753593 0, 7123.474072854011 2673992.1342754653 0, 7122.229005335942 2673590.968537697 0, 6721.62239690647 2673592.6807247777 0, 6320.893763014451 2673595.4109512526 0, 6321.899885734936 2673193.6058778767 0, 5922.573267334203 2673193.847145713 0, 5523.246700266753 2673194.1099877832 0, 5038.264683324756 2673194.458879093 0, 5037.04495268615 2673604.163529869 0, 5035.82506100801 2674013.8633151893 0, 5034.605529452809 2674423.5577543243 0, 5033.386049244274 2674833.2470321404 0, 5507.842197286466 2674830.182107177 0, 5912.8415571091955 2674827.5905595156 0)), ((1017.9204615395657 2682065.7481912365 0, 1022.4606315108377 2682467.562998352 0, 1027.0012276590394 2682869.3724264596 0, 1424.8994874822993 2682871.3093063678 0, 1421.3919521954385 2682468.6672865455 0, 1820.3229625971003 2682469.7673309087 0, 1817.8481141545 2682066.261951393 0, 1417.8844088355 2682066.0070054685 0, 1017.9204615395657 2682065.7481912365 0)), ((2248.8362833070732 2683670.6256722473 0, 2239.947981889339 2683272.2181566656 0, 2231.0597428386955 2682873.7922004396 0, 2227.761508969853 2682470.349425693 0, 1820.3229625971003 2682469.7673309087 0, 1822.7975564517574 2682873.267853401 0, 1424.8994874822993 2682871.3093063678 0, 1432.5442688101505 2683270.57538892 0, 1440.1888607093929 2683669.823295923 0, 1447.8314432683142 2684069.040314768 0, 1850.7439922273386 2684069.591119776 0, 2257.722988909524 2684069.000448099 0, 2248.8362833070732 2683670.6256722473 0)), ((3455.8455431892626 2682875.5030630757 0, 3463.4532388986904 2683272.759969386 0, 3870.5289121893675 2683267.5784294275 0, 3863.606664061292 2682869.5188334202 0, 3455.8455431892626 2682875.5030630757 0)), ((236.47474820775284 2683666.8031992353 0, 637.7116523797454 2683667.8139777663 0, 633.4070456116638 2683267.644938588 0, 233.83955206538675 2683266.1862250827 0, 236.47474820775284 2683666.8031992353 0)), ((-3417.6777773818003 2683274.60055734 0, -3416.0135255833156 2683676.514065591 0, -3014.1754051494845 2683676.7827926064 0, -3018.1874508010887 2683274.4760140674 0, -3417.6777773818003 2683274.60055734 0)), ((5101.588751731198 2684052.7620926443 0, 4695.839099557662 2684056.7940946138 0, 4701.457836598618 2684456.942234662 0, 5106.486014164929 2684453.1049528564 0, 5104.037477161907 2684252.934147923 0, 5101.588751731198 2684052.7620926443 0)), ((2673.689484060182 2684861.4009187645 0, 3080.3520430623566 2684861.0919844564 0, 3487.014895776545 2684860.7783419285 0, 3486.149774040266 2684458.1455836007 0, 3079.580141260864 2684458.6700031054 0, 2673.0103286512626 2684459.21737087 0, 2673.689484060182 2684861.4009187645 0)), ((2675.0446514598357 2685663.893965721 0, 2674.368651619193 2685263.5796309058 0, 2673.689484060182 2684861.4009187645 0, 2267.2950769636245 2684861.7325346717 0, 2266.440650033938 2684459.787399877 0, 1859.871102576042 2684460.380189284 0, 1860.9009774007502 2684862.05915012 0, 1861.9307817363458 2685263.7329876428 0, 1862.960411386893 2685665.40179497 0, 2269.0021928041383 2685664.65012255 0, 2675.0446514598357 2685663.893965721 0)), ((3082.5759505649357 2687264.07062505 0, 3082.907939134586 2687664.441864723 0, 3487.3440335022947 2687665.704985281 0, 3487.3676324344483 2687264.647758527 0, 3082.5759505649357 2687264.07062505 0)), ((998.2684010510346 2706066.267530266 0, 998.7142267459749 2706469.0704515167 0, 1402.1458548675744 2706475.293432962 0, 1402.6529933882593 2706072.394173808 0, 998.2684010510346 2706066.267530266 0)), ((3841.172606768769 2706087.964316507 0, 3839.521796802324 2706490.616138839 0, 4246.285195752414 2706489.0255209506 0, 4247.581830900716 2706087.3651774214 0, 3841.172606768769 2706087.964316507 0)), ((1804.1155716580497 2706884.50227363 0, 2210.7754551222692 2706887.3022113666 0, 2212.372712894733 2706484.177774412 0, 1805.5767395007708 2706481.5115015535 0, 1804.1155716580497 2706884.50227363 0)), ((2212.012694327966 2707686.8354237806 0, 2212.6314143693453 2708086.559291596 0, 2619.2511251877418 2708090.21324856 0, 3025.870455191995 2708093.8901692806 0, 3432.4895729825143 2708097.5624091453 0, 3431.910851741838 2707696.9932933724 0, 3025.2783066424413 2707693.6123147793 0, 2618.6457542894213 2707690.226364632 0, 2212.012694327966 2707686.8354237806 0)), ((3838.7793070041766 2707694.586730474 0, 3839.233353306072 2708095.213191078 0, 4245.977480480861 2708092.8587930105 0, 4245.647694677946 2707692.175268233 0, 3838.7793070041766 2707694.586730474 0)), ((-5106.651918404079 2711281.7034740294 0, -5107.501617508913 2711470.620925021 0, -5108.455607399276 2711682.7534461278 0, -4675.295503652894 2711682.844125988 0, -4677.184035010697 2711282.4189093523 0, -4679.073494315028 2710881.953594931 0, -4680.967637594464 2710480.7067106846 0, -4682.862738058344 2710079.4280649396 0, -5101.240216921132 2710078.5229432643 0, -5103.044339564015 2710479.58835322 0, -5104.848454811948 2710880.6487840856 0, -5105.228836937038 2710965.2330671665 0, -5106.651918333609 2711281.703458358 0, -5106.651918404079 2711281.7034740294 0)), ((4255.021903333384 2710498.7436810127 0, 3850.3880491768778 2710505.0583903505 0, 3843.870118786147 2710903.2411668384 0, 3842.4519574278183 2711305.4453184055 0, 4250.698685929169 2711303.448886601 0, 4252.865565825576 2710900.1591316117 0, 4661.6574063913 2710897.072262254 0, 4663.773030244654 2710497.092572416 0, 4255.021903333384 2710498.7436810127 0)), ((-4269.70831925989 2712890.655111386 0, -4676.320287089962 2712890.688614873 0, -5117.132716128869 2712890.719593824 0, -5120.02311810595 2713293.179542048 0, -5118.382633689577 2713293.369323318 0, -5118.382320941198 2713293.3693243014 0, -5118.392643909606 2713287.748213695 0, -4676.631346000081 2713290.5845160163 0, -4674.896648937593 2713290.5956852036 0, -4270.4090715393495 2713293.2166674216 0, -4268.579073213473 2713293.228477472 0, -3864.1897983730737 2713295.871765018 0, -3862.261885126718 2713295.8843135983 0, -3457.9707959306834 2713297.989240222 0, -3457.0075923977965 2713297.9942313256 0, -3051.7535045864397 2713300.127124115 0, -3049.932240095481 2712889.8907292085 0, -2644.888321633176 2712890.535121375 0, -2239.8440697577216 2712891.1747652455 0, -2238.445368673496 2712490.284288044 0, -2643.2956807531045 2712488.9904344073 0, -2643.535803263525 2712090.1510578045 0, -3046.3605262186784 2712085.4875751836 0, -3048.145940448636 2712487.691730232 0, -3455.1020574277586 2712487.776043136 0, -3862.058160765678 2712487.855847102 0, -4269.007270750511 2712487.9303149693 0, -4269.70831925989 2712890.655111386 0)), ((4258.5777549818595 2712505.44122695 0, 4658.248838942368 2712500.2307842523 0, 4658.348320051825 2712100.523392187 0, 4253.635103178385 2712105.807845356 0, 4258.5777549818595 2712505.44122695 0)), ((-1836.0148288950045 2713296.0281345397 0, -1430.7683162261403 2713294.707195535 0, -1427.9208151375617 2712892.491884259 0, -1425.0914209221282 2712492.868953733 0, -1831.7684270770046 2712491.579166733 0, -1833.8809975115978 2712891.8356715976 0, -1836.0148288950045 2713296.0281345397 0)), ((3033.2239233042237 2713286.675944311 0, 3439.5777274196394 2713285.9191595083 0, 3434.609641684605 2712914.106807696 0, 3030.1547177381285 2712913.115378526 0, 3032.876518482947 2713286.6765549146 0, 3033.2239233042237 2713286.675944311 0)), ((191.24675436282772 2713682.2688071155 0, 188.1100455757981 2713281.8331672493 0, -216.60997828050702 2713285.017712498 0, -621.3299425510596 2713288.2247412466 0, -618.8584316213498 2713688.351987669 0, -213.8058691205999 2713685.313281258 0, -211.0013515317427 2714085.5898771165 0, 194.38379128553382 2714082.7006832794 0, 191.24675436282772 2713682.2688071155 0)), ((-1649.9456180682266 2715295.421635402 0, -1618.1799364685733 2715495.3742659106 0, -1582.7676239280281 2715597.3847823306 0, -1702.5530287301283 2715689.4910429125 0, -1703.783319452899 2715696.3169638338 0, -1720.2774801544037 2715787.8343663174 0, -1781.052836937852 2715879.9153260333 0, -1781.240398412982 2715999.763944685 0, -1710.7693077944662 2716092.3242227477 0, -1711.6825030898558 2716095.916031599 0, -1747.717082071063 2716237.6539940974 0, -1852.8649537851527 2716255.7991800443 0, -1856.8632074523973 2716498.0741839157 0, -1453.9115417504436 2716496.8841965348 0, -1438.9683756533925 2716092.8599919737 0, -1032.640313329464 2716090.7936810893 0, -1030.0297502254796 2715692.5462534055 0, -621.3591906385346 2715688.702142325 0, -616.3861447072471 2715289.2109832875 0, -611.4437058543614 2714888.647759559 0, -613.9151646126546 2714488.5635543303 0, -1019.6342010151255 2714491.2756021745 0, -1021.7725612321208 2714091.3539768253 0, -1023.9110516341043 2713691.413760786 0, -1428.962687071269 2713694.469403211 0, -1427.1582102463103 2714094.2285999577 0, -1425.3525812221044 2714493.9824845614 0, -1423.5471298473424 2714893.73160047 0, -1431.1394687405632 2715294.5275185746 0, -1649.9456180682266 2715295.421635402 0)), ((-2402.352077579976 2716099.334853069 0, -2413.36844541935 2716093.0382219893 0, -2294.4589538125874 2715931.276844202 0, -2323.360583455664 2715698.643016867 0, -2653.4612891532324 2715699.8776385793 0, -2658.113847241481 2716100.2091913237 0, -2662.766312008028 2716500.5218182127 0, -2259.814975757727 2716499.286982927 0, -2255.5264929878385 2716194.363314527 0, -2276.609240628882 2716171.2053056955 0, -2402.352077579976 2716099.334853069 0)), ((-5114.516344134941 2715699.591771844 0, -5114.1675727356105 2716099.560706577 0, -5114.174559426497 2716101.073244287 0, -5115.874814454032 2716469.1587783494 0, -5115.884030242105 2716502.5500650387 0, -4686.082284763518 2716502.3401412563 0, -4683.377929902097 2716101.1767004402 0, -4680.674335148573 2715699.9810619885 0, -5114.516344134941 2715699.591771844 0)), ((-3875.8999535398907 2716502.014269519 0, -3470.8088823478374 2716501.8857303634 0, -3065.717853351423 2716501.7795600616 0, -3062.045100201077 2716101.586174578 0, -3467.378483349269 2716101.4740142776 0, -3872.711936780993 2716101.356873321 0, -3875.8999535398907 2716502.014269519 0)), ((4259.173389040151 2716499.602358147 0, 4257.897788135917 2716900.911863932 0, 4663.67512608057 2716902.714408253 0, 4664.329278431304 2716501.0692761866 0, 4259.173389040151 2716499.602358147 0)), ((-1858.049349993421 2716904.4505387424 0, -1859.2356445559512 2717310.808105758 0, -1456.0861838246765 2717311.674963512 0, -1454.9990194379297 2716904.2820678363 0, -1858.049349993421 2716904.4505387424 0)), ((-225.4412341625802 2717696.122938931 0, -225.44136625068052 2717696.249909394 0, -224.62921019346118 2717696.1078722137 0, -221.7764295375716 2717695.6090442045 0, 45.99379118113641 2717632.0475321608 0, 138.95106175224706 2717689.342302194 0, 184.31465186959124 2717688.4978438085 0, 183.39742742500147 2717287.304102903 0, -225.2399847123634 2717293.385876797 0, -633.8775431778841 2717299.4627628666 0, -635.1967975754217 2717703.743030767 0, -225.4412341625802 2717696.122938931 0)), ((15079.501850495779 2667400.911845348 0, 15125.666890252996 2667311.980604434 0, 15191.120772676088 2667284.6512994124 0, 15210.063621884934 2667269.0161402402 0, 15210.858954446136 2667181.2885950194 0, 14765.698578201169 2667179.4144756533 0, 14762.364038258156 2667582.408584772 0, 14847.975366687539 2667583.0539863487 0, 14841.385369952295 2667452.791058091 0, 15079.501850495779 2667400.911845348 0)), ((16250.437263109736 2667185.688715323 0, 16212.863384605109 2667216.180548536 0, 16107.166205849237 2667337.9112681528 0, 16023.860067014903 2667301.8384443605 0, 16019.831808211695 2667265.730373721 0, 16016.703916299599 2667591.844295529 0, 16421.459554043173 2667594.8802448865 0, 16425.48372246775 2667186.4313854077 0, 16250.437263109736 2667185.688715323 0)), ((13948.867468892431 2667984.6879084967 0, 14353.948960351807 2667985.0449518133 0, 14356.537747320093 2667581.979590327 0, 13950.711097539757 2667581.5463382415 0, 13544.88449625694 2667581.1087441025 0, 13543.786105052044 2667984.353232905 0, 13948.867468892431 2667984.6879084967 0)), ((15495.80898399944 2667993.3461896866 0, 15608.162694162504 2667994.556954945 0, 16012.799302952984 2667998.9426411623 0, 16016.703916299599 2667591.844295529 0, 15611.948077044612 2667588.8040282903 0, 15339.127594443033 2667586.7523486507 0, 15341.644186387613 2667594.4185282057 0, 15354.556646538535 2667638.9483704814 0, 15387.566679094865 2667696.8993172334 0, 15432.158450588911 2667778.4519989695 0, 15526.672760607735 2667825.8039362514 0, 15495.80898399944 2667993.3461896866 0)), ((17830.08146852741 2669760.683438869 0, 17649.05768640751 2669777.0741732577 0, 17631.565247529103 2669617.8104476244 0, 17633.997077992266 2670020.34696265 0, 18037.79208556993 2670022.324691535 0, 18035.31636994485 2669619.136690924 0, 17875.953747805626 2669618.6137737106 0, 17830.08146852741 2669760.683438869 0)), ((14768.977026613255 2670388.4224988976 0, 14770.948934927701 2669988.3990127323 0, 14361.0257746289 2669995.3652410023 0, 14188.502483820428 2669998.3039836264 0, 14305.200836025242 2670054.2689221795 0, 14360.454752604344 2670104.4469125723 0, 14459.501902742279 2670194.3941970877 0, 14392.330452011978 2670240.163269429 0, 14359.827510695948 2670224.2641465412 0, 14358.931950126587 2670395.300505628 0, 14768.977026613255 2670388.4224988976 0)), ((15982.398502089718 2671996.7309447806 0, 16386.891446308186 2672004.6743460796 0, 16390.790187731553 2671611.734047498 0, 15986.386770171996 2671605.9186339066 0, 15982.398502089718 2671996.7309447806 0)), ((14352.435077189672 2671983.181671434 0, 14352.224013645891 2672371.435161358 0, 14759.808406016065 2672357.1248954944 0, 14761.435499449008 2671972.796652494 0, 14352.435077189672 2671983.181671434 0)), ((17639.318406072478 2675987.607339894 0, 17643.392109364686 2676387.886543175 0, 18046.26375822212 2676389.8389650537 0, 18042.45093777533 2675989.1689838255 0, 17639.318406072478 2675987.607339894 0)), ((14413.950944558499 2676344.7981293434 0, 14419.429425159593 2676743.432690209 0, 14830.110234988155 2676735.110527663 0, 14823.781228980388 2676335.599639608 0, 14413.950944558499 2676344.7981293434 0)), ((5043.858294920456 2677630.709189919 0, 5538.680446440614 2677627.831867304 0, 5944.22467263026 2677625.4685462583 0, 5938.965806168243 2677226.9173046453 0, 5534.944850585622 2677228.6367265102 0, 5043.958277677374 2677230.7203423693 0, 5043.858294920456 2677630.709189919 0)), ((14458.96357176142 2680338.908785741 0, 14459.992977810683 2680740.223605747 0, 14870.501341395266 2680736.0568875275 0, 14870.820254864704 2680333.8588010394 0, 14458.96357176142 2680338.908785741 0)), ((16050.83168322219 2684343.462719235 0, 16044.58080873297 2684743.49997516 0, 16448.26209559142 2684745.254399555 0, 16455.014089451728 2684345.5851647467 0, 16050.83168322219 2684343.462719235 0)), ((18064.93140508903 2684773.3330952954 0, 18056.64674919042 2685174.1869721995 0, 18455.458325242198 2685173.716147613 0, 18462.604457031957 2684772.805884849 0, 18064.93140508903 2684773.3330952954 0)), ((6399.911934908316 2684824.6959309313 0, 5990.868503157693 2684833.7125557074 0, 5987.686570742631 2685231.4931133687 0, 5984.505287553653 2685629.2170933248 0, 6392.278881404925 2685617.948536389 0, 6396.095641197958 2685221.337491395 0, 6804.5040338186 2685211.177146352 0, 6808.955447117598 2684815.6740054963 0, 6399.911934908316 2684824.6959309313 0)), ((5576.73096105953 2685640.5076097576 0, 5574.186618246233 2686039.3547491203 0, 5981.323657273146 2686026.9363154173 0, 5984.505287553653 2685629.2170933248 0, 5576.73096105953 2685640.5076097576 0)), ((18094.60930537767 2686272.6232533487 0, 18136.337536053034 2686109.609611235 0, 18100.22394129301 2686054.099339751 0, 18039.11985384811 2686093.1248439457 0, 18036.793375254492 2686377.4029910318 0, 18438.40066455692 2686377.0248764483 0, 18441.197964693434 2685975.454465967 0, 18411.85774471977 2685975.484722507 0, 18414.281707821112 2686075.47883292 0, 18438.61011432442 2686180.806094717 0, 18328.79169006953 2686319.1780334767 0, 18293.469005068087 2686367.92355676 0, 18216.312201170203 2686352.106225105 0, 18174.496124258203 2686303.269197429 0, 18084.434667421552 2686315.498731412 0, 18094.60930537767 2686272.6232533487 0)), ((9757.617694161461 2687748.8867081027 0, 9752.912573017042 2687812.3713740297 0, 9809.99251404404 2687868.836168498 0, 9842.736504109951 2687888.670693366 0, 9866.846198967809 2687918.1370489956 0, 9868.55862330926 2687927.8645071695 0, 10025.266346764902 2687923.554683998 0, 10030.775277616185 2687525.8802808467 0, 9626.302538349495 2687535.950591208 0, 9625.222165730322 2687621.2640673453 0, 9688.71839456967 2687557.789856814 0, 9769.461858185103 2687564.7714799345 0, 9821.699850100742 2687598.9525585975 0, 9855.846723816974 2687660.001203148 0, 9829.586884813207 2687713.693975444 0, 9780.221945131274 2687723.534390778 0, 9757.617694161461 2687748.8867081027 0)), ((20443.3028628736 2687586.371680449 0, 20041.32598418925 2687583.5210404084 0, 20040.29140951473 2687982.3402563483 0, 20039.256856533208 2688381.1406538524 0, 20440.432441648754 2688384.847955336 0, 20441.867668474377 2687985.612067682 0, 20443.3028628736 2687586.371680449 0)), ((17832.1715950558 2690039.5518426816 0, 17873.625918772523 2690071.73188395 0, 17863.72857082412 2690141.080796169 0, 17894.80372434661 2690225.8250616076 0, 17952.78078221775 2690307.9989660927 0, 18006.783260803368 2690343.534066388 0, 18007.86092477352 2689973.4960319065 0, 17608.94248657115 2689968.850090002 0, 17607.954287781853 2690223.1475237035 0, 17727.31607366602 2690050.051828257 0, 17832.1715950558 2690039.5518426816 0)), ((5962.16379607039 2690841.1623292356 0, 5959.722312819952 2691241.1190262316 0, 6365.8830732785145 2691229.7663953453 0, 6367.586316556753 2690829.6923118155 0, 5962.16379607039 2690841.1623292356 0)), ((8383.09897757985 2691978.113463563 0, 8380.675440758812 2692378.948162184 0, 7977.433821210296 2692392.439634175 0, 7978.304519062915 2692789.062010852 0, 8381.457501985777 2692779.7847833694 0, 8787.765956236552 2692764.539263972 0, 8783.749577303544 2692363.6513578077 0, 8786.605085872568 2691963.149060149 0, 8383.09897757985 2691978.113463563 0)), ((10006.656624822906 2692743.5703330548 0, 10006.148483262275 2693167.8273011874 0, 10409.87651692492 2693166.7346429247 0, 10410.531604089409 2692744.273491583 0, 10006.656624822906 2692743.5703330548 0)), ((12820.230571030992 2693987.1397618665 0, 13220.698438218798 2693978.8834125823 0, 13220.438750020374 2693560.731732215 0, 12820.317281149624 2693565.659423673 0, 12820.230571030992 2693987.1397618665 0)), ((13215.127118235887 2700399.666562965 0, 13215.227855665682 2700802.1199340294 0, 13619.990253904578 2700795.658400593 0, 13620.88687039511 2700393.2762028207 0, 13215.127118235887 2700399.666562965 0)), ((16392.840605276408 2703596.5060888682 0, 16383.125101629521 2703997.62602151 0, 16785.850806478826 2703997.951237007 0, 16795.870516859217 2703596.94585355 0, 16392.840605276408 2703596.5060888682 0)), ((15975.207072759222 2703997.9543919303 0, 15965.459065785224 2704399.226921988 0, 16373.410834087772 2704398.741124809 0, 16383.125101629521 2703997.62602151 0, 15975.207072759222 2703997.9543919303 0)), ((14827.086485329473 2706384.7014311543 0, 14827.310022861895 2706777.6348382668 0, 15131.254753312056 2706780.614523737 0, 15130.551474041911 2706386.371219829 0, 14827.086485329473 2706384.7014311543 0)), ((7522.227589090743 2708066.9255449134 0, 7520.158680293587 2708467.9552760525 0, 7923.556393586471 2708466.0656237192 0, 7925.689286587144 2708064.3484900966 0, 7522.227589090743 2708066.9255449134 0)), ((16745.75995483178 2709988.8745242865 0, 16746.667418866586 2710393.857344907 0, 17153.54681341561 2710392.589243589 0, 17152.271366804034 2709987.066847501 0, 16745.75995483178 2709988.8745242865 0)), ((6304.264438979591 2712077.884363088 0, 6709.28915354734 2712072.1646806276 0, 6708.662774980455 2711672.191079046 0, 6304.349176872272 2711677.7776579163 0, 5900.0361394553265 2711683.3870479646 0, 5899.240417419743 2712083.6000901195 0, 6304.264438979591 2712077.884363088 0)), ((5067.319587614606 2712095.3252380895 0, 5066.277108903527 2712495.7629549075 0, 5494.685530606004 2712492.570208957 0, 5495.203892548303 2712090.776470419 0, 5067.319587614606 2712095.3252380895 0)), ((14802.43948004929 2714817.140624798 0, 14799.629966355671 2715216.3170601483 0, 14796.820658031116 2715615.4887292874 0, 15106.672545318035 2715616.7386727654 0, 15515.044486057697 2715618.3820719235 0, 15519.28731555198 2715220.1142183505 0, 15523.530421567928 2714821.841619475 0, 15119.104680751328 2714819.1961925817 0, 14802.43948004929 2714817.140624798 0)), ((12785.367357945022 2714839.243365424 0, 12778.028915937308 2715236.0972862532 0, 13181.373092528867 2715227.4012877173 0, 13189.212136702059 2714828.9145913515 0, 12785.367357945022 2714839.243365424 0)), ((19994.04610420238 2715185.5830227 0, 19991.993523887522 2715584.4885022948 0, 20397.81477682427 2715588.3003217042 0, 20397.63390720022 2715188.541757956 0, 19994.04610420238 2715185.5830227 0)), ((19171.838315983867 2716377.6469778386 0, 19168.059939930412 2716789.0019131415 0, 19576.440094002144 2716781.513537892 0, 19581.203435945397 2716369.2471883143 0, 19171.838315983867 2716377.6469778386 0)), ((20377.201750580276 2717598.8714839485 0, 20384.210267780993 2717193.925981193 0, 20013.00878703776 2717193.859437133 0, 20090.18921685623 2717263.3915806734 0, 19988.472462192796 2717548.6466629165 0, 19955.256397845413 2717602.601635659 0, 19972.05813135294 2717602.4532160163 0, 19966.17255585521 2718011.0342926322 0, 20370.193050922833 2718003.8116252488 0, 20377.201750580276 2717598.8714839485 0)), ((7880.287644520213 2717686.3839548663 0, 7877.502471846527 2718086.0268312832 0, 8283.264371112695 2718079.7193653136 0, 8285.493700064386 2717684.7793571926 0, 7880.287644520213 2717686.3839548663 0)), ((17143.136432501247 2718851.854545071 0, 17144.202373201148 2719250.693087528 0, 17145.268861881665 2719649.526274158 0, 17138.22853807499 2720049.3402349 0, 17536.18847418455 2720047.1827014093 0, 17540.601504212802 2719647.0594305797 0, 17540.63320173533 2719246.571066197 0, 17540.665010196175 2718846.0642567384 0, 17143.136432501247 2718851.854545071 0)), ((14365.029125951763 2719623.039628195 0, 13958.362885241737 2719629.1218747017 0, 13957.991485826433 2720032.389292792 0, 13957.619754289239 2720435.6511978353 0, 14362.950120561516 2720431.214218232 0, 14364.122307525207 2720028.861460987 0, 14365.029125951763 2719623.039628195 0)), ((9491.60155904921 2721276.076987971 0, 9489.432853290962 2721679.294584789 0, 9894.283104601725 2721674.779063306 0, 9897.325460810427 2721271.338466534 0, 9491.60155904921 2721276.076987971 0)), ((18736.208666899285 2721676.6144660674 0, 18734.891654079587 2722051.826046071 0, 19136.588965145314 2722056.2822198295 0, 19139.57401460323 2721654.9095463166 0, 18790.92133692967 2721651.352431548 0, 18746.635856455418 2721676.7592725707 0, 18736.208666899285 2721676.6144660674 0)), ((21672.095659978957 2665350.4282260244 0, 21672.086531502355 2665372.293954613 0, 21672.002551113914 2665572.198931443 0, 22059.960606851728 2665564.6437839186 0, 22059.51012393185 2665167.59760149 0, 22042.28568617821 2665168.139391153 0, 21979.807829336783 2665167.291337973 0, 21994.721507906586 2665202.3508685934 0, 22029.89727967998 2665381.3843977274 0, 21931.68197265437 2665532.912427275 0, 21812.327495206817 2665534.558848511 0, 21765.219748988056 2665459.200083126 0, 21729.44806997073 2665442.17642127 0, 21672.095659978957 2665350.4282260244 0)), ((22526.39306199842 2668392.650090327 0, 22571.531054147057 2668431.9261325086 0, 22601.43999812779 2668557.036422714 0, 22467.527157841312 2668601.5973549234 0, 22362.588536156494 2668636.5161758307 0, 22265.193535352802 2668608.130263837 0, 22186.23592688549 2668589.485017691 0, 22136.24419039 2668513.050294867 0, 22066.49272276504 2668462.3599507613 0, 22068.446639537877 2668726.159225186 0, 22468.719284162424 2668724.630279338 0, 22472.577107835903 2669122.7334815585 0, 22476.43435871928 2669520.8054370214 0, 22878.516806908323 2669518.220935466 0, 22873.75495539628 2669120.661552744 0, 22868.992262921827 2668723.0972213857 0, 22864.22911954068 2668325.528257113 0, 22464.861288350457 2668326.509093097 0, 22461.436513251225 2667936.855417234 0, 22458.011782350834 2667547.184071324 0, 22063.41142481525 2667548.628132555 0, 22064.452367454378 2667938.072487041 0, 22064.866843109572 2668093.024994244 0, 22087.812256035013 2668099.9010696686 0, 22251.251893170476 2668178.331044052 0, 22318.909450994066 2668238.3963519 0, 22336.464665231382 2668326.8292036676 0, 22377.00661620023 2668455.2155561815 0, 22526.39306199842 2668392.650090327 0)), ((21238.062742160102 2672362.930049306 0, 21642.699803803214 2672353.536105773 0, 21649.843835256223 2671955.7597573567 0, 21656.987634893936 2671557.964977879 0, 21252.146787717928 2671569.7579869293 0, 21245.104343659616 2671966.3461281485 0, 21238.062742160102 2672362.930049306 0)), ((23233.557563243914 2677306.346060751 0, 23082.518714103106 2677307.2123584705 0, 22932.835304386874 2677442.3850612105 0, 22930.10024565291 2677482.6121738856 0, 22873.135289436876 2677539.7261577803 0, 22873.45513215189 2677603.2231258126 0, 23277.6756393173 2677600.10813607 0, 23276.291406722252 2677269.08311469 0, 23233.557563243914 2677306.346060751 0)), ((22361.541615464164 2678131.308724134 0, 22443.312103270844 2678138.6495944164 0, 22465.556612685996 2678205.6963616014 0, 22466.659101666002 2678285.9859404014 0, 22460.191065290033 2678325.510705349 0, 22449.944183092568 2678374.4871553318 0, 22450.21983220639 2678394.559488821 0, 22448.53386465906 2678399.633472604 0, 22468.488240851788 2678399.6887218244 0, 22462.815185186064 2678003.6075812285 0, 22050.144745821603 2678000.862586919 0, 22053.310914273978 2678181.018962657 0, 22088.65612681045 2678163.2921830253 0, 22127.28547799425 2678149.778922786 0, 22159.78535174015 2678108.4195764763 0, 22219.17341173864 2678092.642262964 0, 22266.327219458064 2678094.8594078356 0, 22321.71368324477 2678121.444521027 0, 22361.541615464164 2678131.308724134 0)), ((21248.36970233172 2685980.628674969 0, 21652.294354918202 2685978.034577255 0, 21653.517930722817 2685578.1925358097 0, 21249.516926402557 2685581.2547017853 0, 21248.36970233172 2685980.628674969 0)), ((20846.84784678621 2686381.608176658 0, 20846.324936369674 2686784.181338925 0, 21247.81286830698 2686786.3944675643 0, 21248.09128594254 2686383.514008659 0, 20846.84784678621 2686381.608176658 0)), ((21649.88512991329 2688388.9431185103 0, 21647.96200389764 2688788.7994424985 0, 22055.228065565476 2688785.2986972253 0, 22056.887436198034 2688385.6325590163 0, 21649.88512991329 2688388.9431185103 0)), ((21240.695987252886 2688792.294844053 0, 21240.013952181373 2688917.108323467 0, 21283.321607611946 2688954.86373636 0, 21273.553858226376 2689054.4134390554 0, 21312.608422000754 2689135.3807898764 0, 21291.7948801089 2689191.8511573537 0, 21646.03889336303 2689188.636614877 0, 21647.96200389764 2688788.7994424985 0, 21240.695987252886 2688792.294844053 0)), ((21644.23998371618 2689578.272499468 0, 22051.509184007904 2689575.0818125755 0, 22053.56858350532 2689184.9598181364 0, 21646.03889336303 2689188.636614877 0, 21644.23998371618 2689578.272499468 0)), ((21232.34872532887 2690750.746599673 0, 21638.837245605 2690748.503476382 0, 22045.326068598206 2690746.283301461 0, 22047.387821246793 2690355.7437071516 0, 21640.639157350506 2690358.206040195 0, 21233.890748772475 2690360.6634465405 0, 21232.34872532887 2690750.746599673 0)), ((21639.208461658516 2691147.4002783964 0, 21639.579752169004 2691546.278047918 0, 22045.07389786588 2691544.0359015004 0, 22045.199926743804 2691145.1618523286 0, 21639.208461658516 2691147.4002783964 0)), ((23226.575169089832 2696036.708609112 0, 23150.430370563205 2696200.070948086 0, 23009.39260196048 2696310.0075473674 0, 23224.045232100492 2696311.012287523 0, 23627.058679142625 2696312.8949512797 0, 23633.279092870616 2695915.5534111713 0, 23326.99086647538 2695915.184468969 0, 23226.575169089832 2696036.708609112 0)), ((22002.504304606646 2696705.3661034345 0, 21596.743107050333 2696706.235865666 0, 21589.651204900736 2697102.605961009 0, 21591.713483730593 2697501.296876686 0, 21997.38648802732 2697501.3579260954 0, 22403.059959762424 2697501.4416328142 0, 22401.231345531633 2697099.6485378286 0, 22408.265644450326 2696704.5189842856 0, 22002.504304606646 2696705.3661034345 0)), ((22401.794765157432 2706780.4998695026 0, 21997.848440500948 2706787.234221662 0, 22000.680687837634 2707189.2289537825 0, 22003.513038443056 2707591.21841288 0, 22406.005657508904 2707583.3601349206 0, 22403.90025830444 2707181.939450402 0, 22401.794765157432 2706780.4998695026 0)), ((22410.54812813725 2708786.4320440646 0, 22401.8252175175 2708390.768550851 0, 22394.40303404622 2708385.338074282 0, 22009.165428940538 2708393.413618841 0, 22012.350819990817 2708792.0905121784 0, 22410.54812813725 2708786.4320440646 0)), ((22828.434004623694 2709588.7140895724 0, 22977.127390372654 2709482.18863001 0, 22973.449147104748 2709402.0783697325 0, 23098.609703089154 2709377.6827498274 0, 23192.482053936867 2709428.1301585827 0, 23233.27105311363 2709502.1027587685 0, 23226.52107775667 2709174.941936698 0, 22823.25449040109 2709184.677679324 0, 22828.434004623694 2709588.7140895724 0)), ((22013.055636146997 2711588.19436297 0, 22420.166229923485 2711583.5662361635 0, 22422.07034114094 2711184.656227873 0, 22015.277082351273 2711187.6367293787 0, 22013.055636146997 2711588.19436297 0)), ((22420.166229923485 2711583.5662361635 0, 22423.312718587167 2711982.7058012057 0, 22832.492621021636 2711977.354743092 0, 22827.27733910165 2711578.9613630553 0, 22420.166229923485 2711583.5662361635 0)), ((20802.38715176861 2712405.3168605864 0, 21202.086186972207 2712399.907491889 0, 21200.461495763215 2711998.715649977 0, 21607.297157999412 2711993.3862271537 0, 21605.945782625487 2711592.845154835 0, 21198.83635357114 2711597.5189974555 0, 20800.035805611144 2711609.255313006 0, 20401.23662399326 2711621.0135896066 0, 20401.96246907941 2712015.8698570635 0, 20402.688063687085 2712410.721382355 0, 20802.38715176861 2712405.3168605864 0)), ((22017.362462900226 2713185.8663945086 0, 22425.72653559047 2713187.6505632205 0, 22426.09508279207 2712782.2914511976 0, 22016.287898943185 2712787.3123977995 0, 22017.362462900226 2713185.8663945086 0)), ((21205.28140417238 2713189.095065119 0, 21206.765638147455 2713588.43038808 0, 21612.04103255767 2713587.915965496 0, 21611.321773924778 2713187.4694403093 0, 21205.28140417238 2713189.095065119 0)), ((21610.71529260665 2714390.403757304 0, 22017.22492195067 2714390.378172485 0, 22017.270712843423 2713988.9213646604 0, 22017.316423672222 2713587.3964814483 0, 21612.04103255767 2713587.915965496 0, 21612.76016174718 2713</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Warm Springs</t>
+          <t>White Earth</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>OR</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Common Schools</t>
+          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>5</v>
+        <v>1141</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>17197.01</v>
       </c>
       <c r="H74" t="n">
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="I74" t="n">
-        <v>441.49</v>
+        <v>27174.74</v>
       </c>
       <c r="J74" t="n">
-        <v>5</v>
+        <v>701</v>
       </c>
       <c r="K74" t="n">
-        <v>441.49</v>
+        <v>44371.75</v>
       </c>
       <c r="L74" t="n">
-        <v>657110.6</v>
+        <v>747912.54</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((1383.5353677989615 2665597.0389574743 0, 1787.8362839817985 2665595.1437992966 0, 1789.5667013662242 2665192.0752311223 0, 1612.6779454421549 2665193.079095202 0, 1499.3286985567952 2665193.722393299 0, 1434.7197709316813 2665194.088678773 0, 1384.9421352758486 2665194.370903259 0, 1100.0312463793368 2665193.814237008 0, 986.5166697160986 2665196.539836616 0, 980.3181917673943 2665196.688671415 0, 979.234695915162 2665598.9298086413 0, 1383.5353677989615 2665597.0389574743 0)), ((1630.4892621535892 2666577.227090937 0, 1782.7804459670808 2666773.125752292 0, 1784.3763232551087 2666401.2862598463 0, 1631.4780851873477 2666401.6276745563 0, 1630.4892621535892 2666577.227090937 0)), ((-1043.9127356924253 2667205.017103878 0, -1044.3824041522014 2667606.73599305 0, -640.1260951447346 2667608.1508072903 0, -639.6571572228979 2667206.2935517295 0, -1043.9127356924253 2667205.017103878 0)), ((3412.4767253203277 2670802.752104579 0, 3413.0752287707783 2671204.0885676933 0, 3820.3192275613037 2671204.3768943134 0, 3819.07616086587 2670803.339855818 0, 3412.4767253203277 2670802.752104579 0)), ((981.2231380002734 2671211.303034148 0, 980.6184513733934 2671613.6781696626 0, 1384.406988532018 2671609.0994988997 0, 1385.6794557510357 2671207.1844922407 0, 981.2231380002734 2671211.303034148 0)), ((576.8307485585088 2671618.2796248817 0, 571.6782034535402 2672021.0900131185 0, 977.3368457358474 2672016.9964574035 0, 980.6184513733934 2671613.6781696626 0, 576.8307485585088 2671618.2796248817 0)), ((974.0551698998473 2672420.309051253 0, 970.7736638072345 2672823.562984495 0, 1380.1735619965264 2672820.506616753 0, 1381.5849194588827 2672416.7318239957 0, 974.0551698998473 2672420.309051253 0)), ((5912.8415571091955 2674827.5905595156 0, 5915.34731046087 2674406.918686161 0, 5917.757013608493 2674002.4214660246 0, 6319.887350455133 2673997.197710027 0, 6722.018009562836 2673991.969764447 0, 6722.4135626571415 2674391.254104146 0, 7124.713803093802 2674393.2473753593 0, 7123.474072854011 2673992.1342754653 0, 7122.229005335942 2673590.968537697 0, 6721.62239690647 2673592.6807247777 0, 6320.893763014451 2673595.4109512526 0, 6321.899885734936 2673193.6058778767 0, 5922.573267334203 2673193.847145713 0, 5523.246700266753 2673194.1099877832 0, 5038.264683324756 2673194.458879093 0, 5037.04495268615 2673604.163529869 0, 5035.82506100801 2674013.8633151893 0, 5034.605529452809 2674423.5577543243 0, 5033.386049244274 2674833.2470321404 0, 5507.842197286466 2674830.182107177 0, 5912.8415571091955 2674827.5905595156 0)), ((1017.9204615395657 2682065.7481912365 0, 1022.4606315108377 2682467.562998352 0, 1027.0012276590394 2682869.3724264596 0, 1424.8994874822993 2682871.3093063678 0, 1421.3919521954385 2682468.6672865455 0, 1820.3229625971003 2682469.7673309087 0, 1817.8481141545 2682066.261951393 0, 1417.8844088355 2682066.0070054685 0, 1017.9204615395657 2682065.7481912365 0)), ((2248.8362833070732 2683670.6256722473 0, 2239.947981889339 2683272.2181566656 0, 2231.0597428386955 2682873.7922004396 0, 2227.761508969853 2682470.349425693 0, 1820.3229625971003 2682469.7673309087 0, 1822.7975564517574 2682873.267853401 0, 1424.8994874822993 2682871.3093063678 0, 1432.5442688101505 2683270.57538892 0, 1440.1888607093929 2683669.823295923 0, 1447.8314432683142 2684069.040314768 0, 1850.7439922273386 2684069.591119776 0, 2257.722988909524 2684069.000448099 0, 2248.8362833070732 2683670.6256722473 0)), ((3455.8455431892626 2682875.5030630757 0, 3463.4532388986904 2683272.759969386 0, 3870.5289121893675 2683267.5784294275 0, 3863.606664061292 2682869.5188334202 0, 3455.8455431892626 2682875.5030630757 0)), ((236.47474820775284 2683666.8031992353 0, 637.7116523797454 2683667.8139777663 0, 633.4070456116638 2683267.644938588 0, 233.83955206538675 2683266.1862250827 0, 236.47474820775284 2683666.8031992353 0)), ((-3417.6777773818003 2683274.60055734 0, -3416.0135255833156 2683676.514065591 0, -3014.1754051494845 2683676.7827926064 0, -3018.1874508010887 2683274.4760140674 0, -3417.6777773818003 2683274.60055734 0)), ((5101.588751731198 2684052.7620926443 0, 4695.839099557662 2684056.7940946138 0, 4701.457836598618 2684456.942234662 0, 5106.486014164929 2684453.1049528564 0, 5104.037477161907 2684252.934147923 0, 5101.588751731198 2684052.7620926443 0)), ((2673.689484060182 2684861.4009187645 0, 3080.3520430623566 2684861.0919844564 0, 3487.014895776545 2684860.7783419285 0, 3486.149774040266 2684458.1455836007 0, 3079.580141260864 2684458.6700031054 0, 2673.0103286512626 2684459.21737087 0, 2673.689484060182 2684861.4009187645 0)), ((2675.0446514598357 2685663.893965721 0, 2674.368651619193 2685263.5796309058 0, 2673.689484060182 2684861.4009187645 0, 2267.2950769636245 2684861.7325346717 0, 2266.440650033938 2684459.787399877 0, 1859.871102576042 2684460.380189284 0, 1860.9009774007502 2684862.05915012 0, 1861.9307817363458 2685263.7329876428 0, 1862.960411386893 2685665.40179497 0, 2269.0021928041383 2685664.65012255 0, 2675.0446514598357 2685663.893965721 0)), ((3082.5759505649357 2687264.07062505 0, 3082.907939134586 2687664.441864723 0, 3487.3440335022947 2687665.704985281 0, 3487.3676324344483 2687264.647758527 0, 3082.5759505649357 2687264.07062505 0)), ((998.2684010510346 2706066.267530266 0, 998.7142267459749 2706469.0704515167 0, 1402.1458548675744 2706475.293432962 0, 1402.6529933882593 2706072.394173808 0, 998.2684010510346 2706066.267530266 0)), ((3841.172606768769 2706087.964316507 0, 3839.521796802324 2706490.616138839 0, 4246.285195752414 2706489.0255209506 0, 4247.581830900716 2706087.3651774214 0, 3841.172606768769 2706087.964316507 0)), ((1804.1155716580497 2706884.50227363 0, 2210.7754551222692 2706887.3022113666 0, 2212.372712894733 2706484.177774412 0, 1805.5767395007708 2706481.5115015535 0, 1804.1155716580497 2706884.50227363 0)), ((2212.012694327966 2707686.8354237806 0, 2212.6314143693453 2708086.559291596 0, 2619.2511251877418 2708090.21324856 0, 3025.870455191995 2708093.8901692806 0, 3432.4895729825143 2708097.5624091453 0, 3431.910851741838 2707696.9932933724 0, 3025.2783066424413 2707693.6123147793 0, 2618.6457542894213 2707690.226364632 0, 2212.012694327966 2707686.8354237806 0)), ((3838.7793070041766 2707694.586730474 0, 3839.233353306072 2708095.213191078 0, 4245.977480480861 2708092.8587930105 0, 4245.647694677946 2707692.175268233 0, 3838.7793070041766 2707694.586730474 0)), ((-5106.651918404079 2711281.7034740294 0, -5107.501617508913 2711470.620925021 0, -5108.455607399276 2711682.7534461278 0, -4675.295503652894 2711682.844125988 0, -4677.184035010697 2711282.4189093523 0, -4679.073494315028 2710881.953594931 0, -4680.967637594464 2710480.7067106846 0, -4682.862738058344 2710079.4280649396 0, -5101.240216921132 2710078.5229432643 0, -5103.044339564015 2710479.58835322 0, -5104.848454811948 2710880.6487840856 0, -5105.228836937038 2710965.2330671665 0, -5106.651918333609 2711281.703458358 0, -5106.651918404079 2711281.7034740294 0)), ((4255.021903333384 2710498.7436810127 0, 3850.3880491768778 2710505.0583903505 0, 3843.870118786147 2710903.2411668384 0, 3842.4519574278183 2711305.4453184055 0, 4250.698685929169 2711303.448886601 0, 4252.865565825576 2710900.1591316117 0, 4661.6574063913 2710897.072262254 0, 4663.773030244654 2710497.092572416 0, 4255.021903333384 2710498.7436810127 0)), ((-4269.70831925989 2712890.655111386 0, -4676.320287089962 2712890.688614873 0, -5117.132716128869 2712890.719593824 0, -5120.02311810595 2713293.179542048 0, -5118.382633689577 2713293.369323318 0, -5118.382320941198 2713293.3693243014 0, -5118.392643909606 2713287.748213695 0, -4676.631346000081 2713290.5845160163 0, -4674.896648937593 2713290.5956852036 0, -4270.4090715393495 2713293.2166674216 0, -4268.579073213473 2713293.228477472 0, -3864.1897983730737 2713295.871765018 0, -3862.261885126718 2713295.8843135983 0, -3457.9707959306834 2713297.989240222 0, -3457.0075923977965 2713297.9942313256 0, -3051.7535045864397 2713300.127124115 0, -3049.932240095481 2712889.8907292085 0, -2644.888321633176 2712890.535121375 0, -2239.8440697577216 2712891.1747652455 0, -2238.445368673496 2712490.284288044 0, -2643.2956807531045 2712488.9904344073 0, -2643.535803263525 2712090.1510578045 0, -3046.3605262186784 2712085.4875751836 0, -3048.145940448636 2712487.691730232 0, -3455.1020574277586 2712487.776043136 0, -3862.058160765678 2712487.855847102 0, -4269.007270750511 2712487.9303149693 0, -4269.70831925989 2712890.655111386 0)), ((4258.5777549818595 2712505.44122695 0, 4658.248838942368 2712500.2307842523 0, 4658.348320051825 2712100.523392187 0, 4253.635103178385 2712105.807845356 0, 4258.5777549818595 2712505.44122695 0)), ((-1836.0148288950045 2713296.0281345397 0, -1430.7683162261403 2713294.707195535 0, -1427.9208151375617 2712892.491884259 0, -1425.0914209221282 2712492.868953733 0, -1831.7684270770046 2712491.579166733 0, -1833.8809975115978 2712891.8356715976 0, -1836.0148288950045 2713296.0281345397 0)), ((3033.2239233042237 2713286.675944311 0, 3439.5777274196394 2713285.9191595083 0, 3434.609641684605 2712914.106807696 0, 3030.1547177381285 2712913.115378526 0, 3032.876518482947 2713286.6765549146 0, 3033.2239233042237 2713286.675944311 0)), ((191.24675436282772 2713682.2688071155 0, 188.1100455757981 2713281.8331672493 0, -216.60997828050702 2713285.017712498 0, -621.3299425510596 2713288.2247412466 0, -618.8584316213498 2713688.351987669 0, -213.8058691205999 2713685.313281258 0, -211.0013515317427 2714085.5898771165 0, 194.38379128553382 2714082.7006832794 0, 191.24675436282772 2713682.2688071155 0)), ((-1649.9456180682266 2715295.421635402 0, -1618.1799364685733 2715495.3742659106 0, -1582.7676239280281 2715597.3847823306 0, -1702.5530287301283 2715689.4910429125 0, -1703.783319452899 2715696.3169638338 0, -1720.2774801544037 2715787.8343663174 0, -1781.052836937852 2715879.9153260333 0, -1781.240398412982 2715999.763944685 0, -1710.7693077944662 2716092.3242227477 0, -1711.6825030898558 2716095.916031599 0, -1747.717082071063 2716237.6539940974 0, -1852.8649537851527 2716255.7991800443 0, -1856.8632074523973 2716498.0741839157 0, -1453.9115417504436 2716496.8841965348 0, -1438.9683756533925 2716092.8599919737 0, -1032.640313329464 2716090.7936810893 0, -1030.0297502254796 2715692.5462534055 0, -621.3591906385346 2715688.702142325 0, -616.3861447072471 2715289.2109832875 0, -611.4437058543614 2714888.647759559 0, -613.9151646126546 2714488.5635543303 0, -1019.6342010151255 2714491.2756021745 0, -1021.7725612321208 2714091.3539768253 0, -1023.9110516341043 2713691.413760786 0, -1428.962687071269 2713694.469403211 0, -1427.1582102463103 2714094.2285999577 0, -1425.3525812221044 2714493.9824845614 0, -1423.5471298473424 2714893.73160047 0, -1431.1394687405632 2715294.5275185746 0, -1649.9456180682266 2715295.421635402 0)), ((-2402.352077579976 2716099.334853069 0, -2413.36844541935 2716093.0382219893 0, -2294.4589538125874 2715931.276844202 0, -2323.360583455664 2715698.643016867 0, -2653.4612891532324 2715699.8776385793 0, -2658.113847241481 2716100.2091913237 0, -2662.766312008028 2716500.5218182127 0, -2259.814975757727 2716499.286982927 0, -2255.5264929878385 2716194.363314527 0, -2276.609240628882 2716171.2053056955 0, -2402.352077579976 2716099.334853069 0)), ((-5114.516344134941 2715699.591771844 0, -5114.1675727356105 2716099.560706577 0, -5114.174559426497 2716101.073244287 0, -5115.874814454032 2716469.1587783494 0, -5115.884030242105 2716502.5500650387 0, -4686.082284763518 2716502.3401412563 0, -4683.377929902097 2716101.1767004402 0, -4680.674335148573 2715699.9810619885 0, -5114.516344134941 2715699.591771844 0)), ((-3875.8999535398907 2716502.014269519 0, -3470.8088823478374 2716501.8857303634 0, -3065.717853351423 2716501.7795600616 0, -3062.045100201077 2716101.586174578 0, -3467.378483349269 2716101.4740142776 0, -3872.711936780993 2716101.356873321 0, -3875.8999535398907 2716502.014269519 0)), ((4259.173389040151 2716499.602358147 0, 4257.897788135917 2716900.911863932 0, 4663.67512608057 2716902.714408253 0, 4664.329278431304 2716501.0692761866 0, 4259.173389040151 2716499.602358147 0)), ((-1858.049349993421 2716904.4505387424 0, -1859.2356445559512 2717310.808105758 0, -1456.0861838246765 2717311.674963512 0, -1454.9990194379297 2716904.2820678363 0, -1858.049349993421 2716904.4505387424 0)), ((-225.4412341625802 2717696.122938931 0, -225.44136625068052 2717696.249909394 0, -224.62921019346118 2717696.1078722137 0, -221.7764295375716 2717695.6090442045 0, 45.99379118113641 2717632.0475321608 0, 138.95106175224706 2717689.342302194 0, 184.31465186959124 2717688.4978438085 0, 183.39742742500147 2717287.304102903 0, -225.2399847123634 2717293.385876797 0, -633.8775431778841 2717299.4627628666 0, -635.1967975754217 2717703.743030767 0, -225.4412341625802 2717696.122938931 0)), ((15079.501850495779 2667400.911845348 0, 15125.666890252996 2667311.980604434 0, 15191.120772676088 2667284.6512994124 0, 15210.063621884934 2667269.0161402402 0, 15210.858954446136 2667181.2885950194 0, 14765.698578201169 2667179.4144756533 0, 14762.364038258156 2667582.408584772 0, 14847.975366687539 2667583.0539863487 0, 14841.385369952295 2667452.791058091 0, 15079.501850495779 2667400.911845348 0)), ((16250.437263109736 2667185.688715323 0, 16212.863384605109 2667216.180548536 0, 16107.166205849237 2667337.9112681528 0, 16023.860067014903 2667301.8384443605 0, 16019.831808211695 2667265.730373721 0, 16016.703916299599 2667591.844295529 0, 16421.459554043173 2667594.8802448865 0, 16425.48372246775 2667186.4313854077 0, 16250.437263109736 2667185.688715323 0)), ((13948.867468892431 2667984.6879084967 0, 14353.948960351807 2667985.0449518133 0, 14356.537747320093 2667581.979590327 0, 13950.711097539757 2667581.5463382415 0, 13544.88449625694 2667581.1087441025 0, 13543.786105052044 2667984.353232905 0, 13948.867468892431 2667984.6879084967 0)), ((15495.80898399944 2667993.3461896866 0, 15608.162694162504 2667994.556954945 0, 16012.799302952984 2667998.9426411623 0, 16016.703916299599 2667591.844295529 0, 15611.948077044612 2667588.8040282903 0, 15339.127594443033 2667586.7523486507 0, 15341.644186387613 2667594.4185282057 0, 15354.556646538535 2667638.9483704814 0, 15387.566679094865 2667696.8993172334 0, 15432.158450588911 2667778.4519989695 0, 15526.672760607735 2667825.8039362514 0, 15495.80898399944 2667993.3461896866 0)), ((17830.08146852741 2669760.683438869 0, 17649.05768640751 2669777.0741732577 0, 17631.565247529103 2669617.8104476244 0, 17633.997077992266 2670020.34696265 0, 18037.79208556993 2670022.324691535 0, 18035.31636994485 2669619.136690924 0, 17875.953747805626 2669618.6137737106 0, 17830.08146852741 2669760.683438869 0)), ((14768.977026613255 2670388.4224988976 0, 14770.948934927701 2669988.3990127323 0, 14361.0257746289 2669995.3652410023 0, 14188.502483820428 2669998.3039836264 0, 14305.200836025242 2670054.2689221795 0, 14360.454752604344 2670104.4469125723 0, 14459.501902742279 2670194.3941970877 0, 14392.330452011978 2670240.163269429 0, 14359.827510695948 2670224.2641465412 0, 14358.931950126587 2670395.300505628 0, 14768.977026613255 2670388.4224988976 0)), ((15982.398502089718 2671996.7309447806 0, 16386.891446308186 2672004.6743460796 0, 16390.790187731553 2671611.734047498 0, 15986.386770171996 2671605.9186339066 0, 15982.398502089718 2671996.7309447806 0)), ((14352.435077189672 2671983.181671434 0, 14352.224013645891 2672371.435161358 0, 14759.808406016065 2672357.1248954944 0, 14761.435499449008 2671972.796652494 0, 14352.435077189672 2671983.181671434 0)), ((17639.318406072478 2675987.607339894 0, 17643.392109364686 2676387.886543175 0, 18046.26375822212 2676389.8389650537 0, 18042.45093777533 2675989.1689838255 0, 17639.318406072478 2675987.607339894 0)), ((14413.950944558499 2676344.7981293434 0, 14419.429425159593 2676743.432690209 0, 14830.110234988155 2676735.110527663 0, 14823.781228980388 2676335.599639608 0, 14413.950944558499 2676344.7981293434 0)), ((5043.858294920456 2677630.709189919 0, 5538.680446440614 2677627.831867304 0, 5944.22467263026 2677625.4685462583 0, 5938.965806168243 2677226.9173046453 0, 5534.944850585622 2677228.6367265102 0, 5043.958277677374 2677230.7203423693 0, 5043.858294920456 2677630.709189919 0)), ((14458.96357176142 2680338.908785741 0, 14459.992977810683 2680740.223605747 0, 14870.501341395266 2680736.0568875275 0, 14870.820254864704 2680333.8588010394 0, 14458.96357176142 2680338.908785741 0)), ((16050.83168322219 2684343.462719235 0, 16044.58080873297 2684743.49997516 0, 16448.26209559142 2684745.254399555 0, 16455.014089451728 2684345.5851647467 0, 16050.83168322219 2684343.462719235 0)), ((18064.93140508903 2684773.3330952954 0, 18056.64674919042 2685174.1869721995 0, 18455.458325242198 2685173.716147613 0, 18462.604457031957 2684772.805884849 0, 18064.93140508903 2684773.3330952954 0)), ((6399.911934908316 2684824.6959309313 0, 5990.868503157693 2684833.7125557074 0, 5987.686570742631 2685231.4931133687 0, 5984.505287553653 2685629.2170933248 0, 6392.278881404925 2685617.948536389 0, 6396.095641197958 2685221.337491395 0, 6804.5040338186 2685211.177146352 0, 6808.955447117598 2684815.6740054963 0, 6399.911934908316 2684824.6959309313 0)), ((5576.73096105953 2685640.5076097576 0, 5574.186618246233 2686039.3547491203 0, 5981.323657273146 2686026.9363154173 0, 5984.505287553653 2685629.2170933248 0, 5576.73096105953 2685640.5076097576 0)), ((18094.60930537767 2686272.6232533487 0, 18136.337536053034 2686109.609611235 0, 18100.22394129301 2686054.099339751 0, 18039.11985384811 2686093.1248439457 0, 18036.793375254492 2686377.4029910318 0, 18438.40066455692 2686377.0248764483 0, 18441.197964693434 2685975.454465967 0, 18411.85774471977 2685975.484722507 0, 18414.281707821112 2686075.47883292 0, 18438.61011432442 2686180.806094717 0, 18328.79169006953 2686319.1780334767 0, 18293.469005068087 2686367.92355676 0, 18216.312201170203 2686352.106225105 0, 18174.496124258203 2686303.269197429 0, 18084.434667421552 2686315.498731412 0, 18094.60930537767 2686272.6232533487 0)), ((9757.617694161461 2687748.8867081027 0, 9752.912573017042 2687812.3713740297 0, 9809.99251404404 2687868.836168498 0, 9842.736504109951 2687888.670693366 0, 9866.846198967809 2687918.1370489956 0, 9868.55862330926 2687927.8645071695 0, 10025.266346764902 2687923.554683998 0, 10030.775277616185 2687525.8802808467 0, 9626.302538349495 2687535.950591208 0, 9625.222165730322 2687621.2640673453 0, 9688.71839456967 2687557.789856814 0, 9769.461858185103 2687564.7714799345 0, 9821.699850100742 2687598.9525585975 0, 9855.846723816974 2687660.001203148 0, 9829.586884813207 2687713.693975444 0, 9780.221945131274 2687723.534390778 0, 9757.617694161461 2687748.8867081027 0)), ((20443.3028628736 2687586.371680449 0, 20041.32598418925 2687583.5210404084 0, 20040.29140951473 2687982.3402563483 0, 20039.256856533208 2688381.1406538524 0, 20440.432441648754 2688384.847955336 0, 20441.867668474377 2687985.612067682 0, 20443.3028628736 2687586.371680449 0)), ((17832.1715950558 2690039.5518426816 0, 17873.625918772523 2690071.73188395 0, 17863.72857082412 2690141.080796169 0, 17894.80372434661 2690225.8250616076 0, 17952.78078221775 2690307.9989660927 0, 18006.783260803368 2690343.534066388 0, 18007.86092477352 2689973.4960319065 0, 17608.94248657115 2689968.850090002 0, 17607.954287781853 2690223.1475237035 0, 17727.31607366602 2690050.051828257 0, 17832.1715950558 2690039.5518426816 0)), ((5962.16379607039 2690841.1623292356 0, 5959.722312819952 2691241.1190262316 0, 6365.8830732785145 2691229.7663953453 0, 6367.586316556753 2690829.6923118155 0, 5962.16379607039 2690841.1623292356 0)), ((8383.09897757985 2691978.113463563 0, 8380.675440758812 2692378.948162184 0, 7977.433821210296 2692392.439634175 0, 7978.304519062915 2692789.062010852 0, 8381.457501985777 2692779.7847833694 0, 8787.765956236552 2692764.539263972 0, 8783.749577303544 2692363.6513578077 0, 8786.605085872568 2691963.149060149 0, 8383.09897757985 2691978.113463563 0)), ((10006.656624822906 2692743.5703330548 0, 10006.148483262275 2693167.8273011874 0, 10409.87651692492 2693166.7346429247 0, 10410.531604089409 2692744.273491583 0, 10006.656624822906 2692743.5703330548 0)), ((12820.230571030992 2693987.1397618665 0, 13220.698438218798 2693978.8834125823 0, 13220.438750020374 2693560.731732215 0, 12820.317281149624 2693565.659423673 0, 12820.230571030992 2693987.1397618665 0)), ((13215.127118235887 2700399.666562965 0, 13215.227855665682 2700802.1199340294 0, 13619.990253904578 2700795.658400593 0, 13620.88687039511 2700393.2762028207 0, 13215.127118235887 2700399.666562965 0)), ((16392.840605276408 2703596.5060888682 0, 16383.125101629521 2703997.62602151 0, 16785.850806478826 2703997.951237007 0, 16795.870516859217 2703596.94585355 0, 16392.840605276408 2703596.5060888682 0)), ((15975.207072759222 2703997.9543919303 0, 15965.459065785224 2704399.226921988 0, 16373.410834087772 2704398.741124809 0, 16383.125101629521 2703997.62602151 0, 15975.207072759222 2703997.9543919303 0)), ((14827.086485329473 2706384.7014311543 0, 14827.310022861895 2706777.6348382668 0, 15131.254753312056 2706780.614523737 0, 15130.551474041911 2706386.371219829 0, 14827.086485329473 2706384.7014311543 0)), ((7522.227589090743 2708066.9255449134 0, 7520.158680293587 2708467.9552760525 0, 7923.556393586471 2708466.0656237192 0, 7925.689286587144 2708064.3484900966 0, 7522.227589090743 2708066.9255449134 0)), ((16745.75995483178 2709988.8745242865 0, 16746.667418866586 2710393.857344907 0, 17153.54681341561 2710392.589243589 0, 17152.271366804034 2709987.066847501 0, 16745.75995483178 2709988.8745242865 0)), ((6304.264438979591 2712077.884363088 0, 6709.28915354734 2712072.1646806276 0, 6708.662774980455 2711672.191079046 0, 6304.349176872272 2711677.7776579163 0, 5900.0361394553265 2711683.3870479646 0, 5899.240417419743 2712083.6000901195 0, 6304.264438979591 2712077.884363088 0)), ((5067.319587614606 2712095.3252380895 0, 5066.277108903527 2712495.7629549075 0, 5494.685530606004 2712492.570208957 0, 5495.203892548303 2712090.776470419 0, 5067.319587614606 2712095.3252380895 0)), ((14802.43948004929 2714817.140624798 0, 14799.629966355671 2715216.3170601483 0, 14796.820658031116 2715615.4887292874 0, 15106.672545318035 2715616.7386727654 0, 15515.044486057697 2715618.3820719235 0, 15519.28731555198 2715220.1142183505 0, 15523.530421567928 2714821.841619475 0, 15119.104680751328 2714819.1961925817 0, 14802.43948004929 2714817.140624798 0)), ((12785.367357945022 2714839.243365424 0, 12778.028915937308 2715236.0972862532 0, 13181.373092528867 2715227.4012877173 0, 13189.212136702059 2714828.9145913515 0, 12785.367357945022 2714839.243365424 0)), ((19994.04610420238 2715185.5830227 0, 19991.993523887522 2715584.4885022948 0, 20397.81477682427 2715588.3003217042 0, 20397.63390720022 2715188.541757956 0, 19994.04610420238 2715185.5830227 0)), ((19171.838315983867 2716377.6469778386 0, 19168.059939930412 2716789.0019131415 0, 19576.440094002144 2716781.513537892 0, 19581.203435945397 2716369.2471883143 0, 19171.838315983867 2716377.6469778386 0)), ((20377.201750580276 2717598.8714839485 0, 20384.210267780993 2717193.925981193 0, 20013.00878703776 2717193.859437133 0, 20090.18921685623 2717263.3915806734 0, 19988.472462192796 2717548.6466629165 0, 19955.256397845413 2717602.601635659 0, 19972.05813135294 2717602.4532160163 0, 19966.17255585521 2718011.0342926322 0, 20370.193050922833 2718003.8116252488 0, 20377.201750580276 2717598.8714839485 0)), ((7880.287644520213 2717686.3839548663 0, 7877.502471846527 2718086.0268312832 0, 8283.264371112695 2718079.7193653136 0, 8285.493700064386 2717684.7793571926 0, 7880.287644520213 2717686.3839548663 0)), ((17143.136432501247 2718851.854545071 0, 17144.202373201148 2719250.693087528 0, 17145.268861881665 2719649.526274158 0, 17138.22853807499 2720049.3402349 0, 17536.18847418455 2720047.1827014093 0, 17540.601504212802 2719647.0594305797 0, 17540.63320173533 2719246.571066197 0, 17540.665010196175 2718846.0642567384 0, 17143.136432501247 2718851.854545071 0)), ((14365.029125951763 2719623.039628195 0, 13958.362885241737 2719629.1218747017 0, 13957.991485826433 2720032.389292792 0, 13957.619754289239 2720435.6511978353 0, 14362.950120561516 2720431.214218232 0, 14364.122307525207 2720028.861460987 0, 14365.029125951763 2719623.039628195 0)), ((9491.60155904921 2721276.076987971 0, 9489.432853290962 2721679.294584789 0, 9894.283104601725 2721674.779063306 0, 9897.325460810427 2721271.338466534 0, 9491.60155904921 2721276.076987971 0)), ((18736.208666899285 2721676.6144660674 0, 18734.891654079587 2722051.826046071 0, 19136.588965145314 2722056.2822198295 0, 19139.57401460323 2721654.9095463166 0, 18790.92133692967 2721651.352431548 0, 18746.635856455418 2721676.7592725707 0, 18736.208666899285 2721676.6144660674 0)), ((21672.095659978957 2665350.4282260244 0, 21672.086531502355 2665372.293954613 0, 21672.002551113914 2665572.198931443 0, 22059.960606851728 2665564.6437839186 0, 22059.51012393185 2665167.59760149 0, 22042.28568617821 2665168.139391153 0, 21979.807829336783 2665167.291337973 0, 21994.721507906586 2665202.3508685934 0, 22029.89727967998 2665381.3843977274 0, 21931.68197265437 2665532.912427275 0, 21812.327495206817 2665534.558848511 0, 21765.219748988056 2665459.200083126 0, 21729.44806997073 2665442.17642127 0, 21672.095659978957 2665350.4282260244 0)), ((22526.39306199842 2668392.650090327 0, 22571.531054147057 2668431.9261325086 0, 22601.43999812779 2668557.036422714 0, 22467.527157841312 2668601.5973549234 0, 22362.588536156494 2668636.5161758307 0, 22265.193535352802 2668608.130263837 0, 22186.23592688549 2668589.485017691 0, 22136.24419039 2668513.050294867 0, 22066.49272276504 2668462.3599507613 0, 22068.446639537877 2668726.159225186 0, 22468.719284162424 2668724.630279338 0, 22472.577107835903 2669122.7334815585 0, 22476.43435871928 2669520.8054370214 0, 22878.516806908323 2669518.220935466 0, 22873.75495539628 2669120.661552744 0, 22868.992262921827 2668723.0972213857 0, 22864.22911954068 2668325.528257113 0, 22464.861288350457 2668326.509093097 0, 22461.436513251225 2667936.855417234 0, 22458.011782350834 2667547.184071324 0, 22063.41142481525 2667548.628132555 0, 22064.452367454378 2667938.072487041 0, 22064.866843109572 2668093.024994244 0, 22087.812256035013 2668099.9010696686 0, 22251.251893170476 2668178.331044052 0, 22318.909450994066 2668238.3963519 0, 22336.464665231382 2668326.8292036676 0, 22377.00661620023 2668455.2155561815 0, 22526.39306199842 2668392.650090327 0)), ((21238.062742160102 2672362.930049306 0, 21642.699803803214 2672353.536105773 0, 21649.843835256223 2671955.7597573567 0, 21656.987634893936 2671557.964977879 0, 21252.146787717928 2671569.7579869293 0, 21245.104343659616 2671966.3461281485 0, 21238.062742160102 2672362.930049306 0)), ((23233.557563243914 2677306.346060751 0, 23082.518714103106 2677307.2123584705 0, 22932.835304386874 2677442.3850612105 0, 22930.10024565291 2677482.6121738856 0, 22873.135289436876 2677539.7261577803 0, 22873.45513215189 2677603.2231258126 0, 23277.6756393173 2677600.10813607 0, 23276.291406722252 2677269.08311469 0, 23233.557563243914 2677306.346060751 0)), ((22361.541615464164 2678131.308724134 0, 22443.312103270844 2678138.6495944164 0, 22465.556612685996 2678205.6963616014 0, 22466.659101666002 2678285.9859404014 0, 22460.191065290033 2678325.510705349 0, 22449.944183092568 2678374.4871553318 0, 22450.21983220639 2678394.559488821 0, 22448.53386465906 2678399.633472604 0, 22468.488240851788 2678399.6887218244 0, 22462.815185186064 2678003.6075812285 0, 22050.144745821603 2678000.862586919 0, 22053.310914273978 2678181.018962657 0, 22088.65612681045 2678163.2921830253 0, 22127.28547799425 2678149.778922786 0, 22159.78535174015 2678108.4195764763 0, 22219.17341173864 2678092.642262964 0, 22266.327219458064 2678094.8594078356 0, 22321.71368324477 2678121.444521027 0, 22361.541615464164 2678131.308724134 0)), ((21248.36970233172 2685980.628674969 0, 21652.294354918202 2685978.034577255 0, 21653.517930722817 2685578.1925358097 0, 21249.516926402557 2685581.2547017853 0, 21248.36970233172 2685980.628674969 0)), ((20846.84784678621 2686381.608176658 0, 20846.324936369674 2686784.181338925 0, 21247.81286830698 2686786.3944675643 0, 21248.09128594254 2686383.514008659 0, 20846.84784678621 2686381.608176658 0)), ((21649.88512991329 2688388.9431185103 0, 21647.96200389764 2688788.7994424985 0, 22055.228065565476 2688785.2986972253 0, 22056.887436198034 2688385.6325590163 0, 21649.88512991329 2688388.9431185103 0)), ((21240.695987252886 2688792.294844053 0, 21240.013952181373 2688917.108323467 0, 21283.321607611946 2688954.86373636 0, 21273.553858226376 2689054.4134390554 0, 21312.608422000754 2689135.3807898764 0, 21291.7948801089 2689191.8511573537 0, 21646.03889336303 2689188.636614877 0, 21647.96200389764 2688788.7994424985 0, 21240.695987252886 2688792.294844053 0)), ((21644.23998371618 2689578.272499468 0, 22051.509184007904 2689575.0818125755 0, 22053.56858350532 2689184.9598181364 0, 21646.03889336303 2689188.636614877 0, 21644.23998371618 2689578.272499468 0)), ((21232.34872532887 2690750.746599673 0, 21638.837245605 2690748.503476382 0, 22045.326068598206 2690746.283301461 0, 22047.387821246793 2690355.7437071516 0, 21640.639157350506 2690358.206040195 0, 21233.890748772475 2690360.6634465405 0, 21232.34872532887 2690750.746599673 0)), ((21639.208461658516 2691147.4002783964 0, 21639.579752169004 2691546.278047918 0, 22045.07389786588 2691544.0359015004 0, 22045.199926743804 2691145.1618523286 0, 21639.208461658516 2691147.4002783964 0)), ((23226.575169089832 2696036.708609112 0, 23150.430370563205 2696200.070948086 0, 23009.39260196048 2696310.0075473674 0, 23224.045232100492 2696311.012287523 0, 23627.058679142625 2696312.8949512797 0, 23633.279092870616 2695915.5534111713 0, 23326.99086647538 2695915.184468969 0, 23226.575169089832 2696036.708609112 0)), ((22002.504304606646 2696705.3661034345 0, 21596.743107050333 2696706.235865666 0, 21589.651204900736 2697102.605961009 0, 21591.713483730593 2697501.296876686 0, 21997.38648802732 2697501.3579260954 0, 22403.059959762424 2697501.4416328142 0, 22401.231345531633 2697099.6485378286 0, 22408.265644450326 2696704.5189842856 0, 22002.504304606646 2696705.3661034345 0)), ((22401.794765157432 2706780.4998695026 0, 21997.848440500948 2706787.234221662 0, 22000.680687837634 2707189.2289537825 0, 22003.513038443056 2707591.21841288 0, 22406.005657508904 2707583.3601349206 0, 22403.90025830444 2707181.939450402 0, 22401.794765157432 2706780.4998695026 0)), ((22410.54812813725 2708786.4320440646 0, 22401.8252175175 2708390.768550851 0, 22394.40303404622 2708385.338074282 0, 22009.165428940538 2708393.413618841 0, 22012.350819990817 2708792.0905121784 0, 22410.54812813725 2708786.4320440646 0)), ((22828.434004623694 2709588.7140895724 0, 22977.127390372654 2709482.18863001 0, 22973.449147104748 2709402.0783697325 0, 23098.609703089154 2709377.6827498274 0, 23192.482053936867 2709428.1301585827 0, 23233.27105311363 2709502.1027587685 0, 23226.52107775667 2709174.941936698 0, 22823.25449040109 2709184.677679324 0, 22828.434004623694 2709588.7140895724 0)), ((22013.055636146997 2711588.19436297 0, 22420.166229923485 2711583.5662361635 0, 22422.07034114094 2711184.656227873 0, 22015.277082351273 2711187.6367293787 0, 22013.055636146997 2711588.19436297 0)), ((22420.166229923485 2711583.5662361635 0, 22423.312718587167 2711982.7058012057 0, 22832.492621021636 2711977.354743092 0, 22827.27733910165 2711578.9613630553 0, 22420.166229923485 2711583.5662361635 0)), ((20802.38715176861 2712405.3168605864 0, 21202.086186972207 2712399.907491889 0, 21200.461495763215 2711998.715649977 0, 21607.297157999412 2711993.3862271537 0, 21605.945782625487 2711592.845154835 0, 21198.83635357114 2711597.5189974555 0, 20800.035805611144 2711609.255313006 0, 20401.23662399326 2711621.0135896066 0, 20401.96246907941 2712015.8698570635 0, 20402.688063687085 2712410.721382355 0, 20802.38715176861 2712405.3168605864 0)), ((22017.362462900226 2713185.8663945086 0, 22425.72653559047 2713187.6505632205 0, 22426.09508279207 2712782.2914511976 0, 22016.287898943185 2712787.3123977995 0, 22017.362462900226 2713185.8663945086 0)), ((21205.28140417238 2713189.095065119 0, 21206.765638147455 2713588.43038808 0, 21612.04103255767 2713587.915965496 0, 21611.321773924778 2713187.4694403093 0, 21205.28140417238 2713189.095065119 0)), ((21610.71529260665 2714390.403757304 0, 22017.22492195067 2714390.378172485 0, 22017.270712843423 2713988.9213646604 0, 22017.316423672222 2713587.3964814483 0, 21612.04103255767 2713587.915965496 0, 21612.76016174718 2713</t>
+          <t>MULTIPOLYGON Z (((-1050634.2762595804 2312278.921033107 0, -1050692.1496858974 2311878.8901095935 0, -1050749.8418575835 2311480.125285387 0, -1050805.7506747406 2311081.4597527836 0, -1050861.6613238936 2310682.782564328 0, -1051255.859984779 2310743.4741963 0, -1051200.1037733245 2311141.4396161498 0, -1051144.3479498741 2311539.4029425895 0, -1051088.5929212286 2311937.360776254 0, -1051032.8378361643 2312335.3193941107 0, -1050634.2762595804 2312278.921033107 0)), ((-1042827.6080114043 2324641.903880159 0, -1042429.0177734202 2324582.6384197455 0, -1042031.3687667405 2324523.506086521 0, -1042088.8292028453 2324128.4938440737 0, -1042087.857374831 2324128.3551963973 0, -1042088.6925061723 2324122.6112281634 0, -1041689.879792263 2324063.533034388 0, -1041292.0584445689 2324004.6261834027 0, -1041350.0240442571 2323614.889880292 0, -1041351.4699388619 2323605.1686712345 0, -1041409.4806173473 2323215.144439011 0, -1041410.9986382548 2323205.724764946 0, -1041473.7604708544 2322816.272943921 0, -1041472.3642102741 2322816.089643594 0, -1041473.7990416642 2322807.2053701356 0, -1041125.9567855056 2322761.754220014 0, -1040731.5802114733 2322710.2174758688 0, -1040791.3933385293 2322318.3149438472 0, -1040792.477179104 2322310.396591345 0, -1040846.3585751874 2321916.7483948767 0, -1040845.4352658397 2321916.6246562605 0, -1040846.3829309222 2321909.7169102994 0, -1041243.1470202254 2321962.8195580887 0, -1041593.576394404 2322009.7149099344 0, -1041991.033277303 2322068.01460237 0, -1042388.4929601529 2322126.307653034 0, -1042333.4848828288 2322526.274883522 0, -1041935.8066824579 2322467.5824857615 0, -1041873.028642868 2322866.373482969 0, -1041810.2530178527 2323265.1530656577 0, -1042211.0342654212 2323324.8051944994 0, -1042607.2119206154 2323383.7695842357 0, -1042547.2426509934 2323783.4970818204 0, -1042944.6907629055 2323842.7817654843 0, -1042886.3057913377 2324240.829846611 0, -1043285.130652052 2324298.636963205 0, -1043226.2979992016 2324699.977115077 0, -1042827.6080114043 2324641.903880159 0)), ((-1046247.5562064119 2329220.6481662146 0, -1046191.3633868239 2329622.789430642 0, -1046593.9948730316 2329678.6363939364 0, -1046534.9886577296 2330080.588037373 0, -1046475.9821583936 2330482.5278504863 0, -1046073.6083994912 2330426.0280175335 0, -1046132.4852626884 2330024.4114558683 0, -1045729.9819064847 2329968.257709795 0, -1045788.7291921459 2329566.9681130997 0, -1045845.5922356682 2329165.063035892 0, -1045443.6285155453 2329109.4754572785 0, -1045501.1639552393 2328707.7760154633 0, -1045558.6997935177 2328306.0742610637 0, -1045616.2362395419 2327904.37012149 0, -1045617.0326782259 2327904.479360659 0, -1045616.9327830005 2327905.1956020826 0, -1046016.0937759206 2327959.9533524564 0, -1045959.3246830138 2328361.192974082 0, -1045902.4578365213 2328763.1402011085 0, -1046303.7496655369 2328818.5044084494 0, -1046247.5562064119 2329220.6481662146 0)), ((-1059727.8355241397 2337697.3455502763 0, -1059668.8527381408 2338098.124818296 0, -1060067.131052015 2338153.3211093354 0, -1060465.4090640997 2338208.5355003844 0, -1060410.0971186836 2338610.1316959243 0, -1060354.7856983019 2339011.7223898345 0, -1059956.6096501015 2338955.955333517 0, -1059558.4318289415 2338900.184331322 0, -1059613.6421632078 2338499.155718323 0, -1059215.414667514 2338443.6841478753 0, -1058817.1846679002 2338388.2147207656 0, -1058872.287569143 2337987.7950442224 0, -1058931.3390659136 2337587.2694612537 0, -1058534.796627428 2337532.90503816 0, -1058592.9067027688 2337132.182809552 0, -1058194.7240368775 2337077.520104881 0, -1058252.2701342073 2336676.4067847277 0, -1058650.7321761935 2336731.296394675 0, -1059049.4432704628 2336786.216981644 0, -1058990.3909251 2337186.7443455644 0, -1059388.6021759196 2337241.6571514467 0, -1059329.5859732355 2337642.3091146755 0, -1059727.8355241397 2337697.3455502763 0)), ((-1066371.9632855507 2339438.2108617574 0, -1066373.429756151 2339438.414318711 0, -1066325.9659184492 2339779.1937124613 0, -1066316.6288095424 2339775.4830386983 0, -1066201.70517481 2339740.4795712177 0, -1066022.4006281008 2339615.323439348 0, -1065949.3493714838 2339578.6985750943 0, -1065929.2570379518 2339568.627267384 0, -1065850.4238185033 2339539.308687006 0, -1065748.3028524022 2339468.346541264 0, -1065676.2207522886 2339424.8367052525 0, -1065654.1213722434 2339415.392399067 0, -1065606.175104046 2339412.400131573 0, -1065571.9863841333 2339376.9328016816 0, -1065578.765703502 2339328.3709718734 0, -1065775.329001942 2339355.539352133 0, -1065828.8039514287 2338960.7937077926 0, -1066028.005994407 2338986.8329564976 0, -1066000.9377325266 2339187.759105069 0, -1066398.6148282972 2339240.822932089 0, -1066371.9632855507 2339438.2108617574 0)), ((-1061837.3204676933 2340034.6030477574 0, -1061780.3655670825 2340436.5922139487 0, -1061723.408817523 2340838.5788117982 0, -1061325.3843199636 2340783.392501526 0, -1060927.3602048056 2340728.202607241 0, -1060529.3384876326 2340673.0124064325 0, -1060131.31556903 2340617.8150917715 0, -1060187.739295776 2340216.35853855 0, -1060244.1628082008 2339814.9025566597 0, -1060299.4740761493 2339413.3136684936 0, -1060354.7856983019 2339011.7223898345 0, -1060752.5765780364 2339066.2638833597 0, -1061150.3704149113 2339120.8020020006 0, -1061548.164748814 2339175.3363516834 0, -1061945.959765405 2339229.8670557295 0, -1061891.6412659038 2339632.23640928 0, -1061837.3204676933 2340034.6030477574 0)), ((-1035118.4999299524 2281190.209319271 0, -1035513.4719348657 2281246.333069391 0, -1035908.4437363615 2281302.455823209 0, -1035850.9664973858 2281705.0788636506 0, -1035456.3629951405 2281647.737895494 0, -1035061.7616243811 2281590.3958082073 0, -1035118.4999299524 2281190.209319271 0)), ((-1016227.3939126243 2286441.674483058 0, -1016170.7846368499 2286843.4743179535 0, -1016116.572680074 2287240.187457348 0, -1015719.7979054934 2287188.6790665807 0, -1015774.9398044108 2286789.754045181 0, -1015830.8571983477 2286390.9832253153 0, -1016227.3939126243 2286441.674483058 0)), ((-1033898.8322515577 2287115.5060672923 0, -1034294.5248291742 2287171.182248576 0, -1034242.4095084692 2287571.8515250664 0, -1034188.3680121511 2287971.6597832455 0, -1033792.6131830172 2287916.5542716077 0, -1033846.4969216322 2287516.1923875464 0, -1033898.8322515577 2287115.5060672923 0)), ((-1035482.4640965455 2287333.0698815673 0, -1035431.1532593278 2287732.771150824 0, -1035380.0460347141 2288135.9017904988 0, -1034981.6506295949 2288083.604406882 0, -1035034.2370944343 2287683.1639975063 0, -1035085.9019275007 2287282.590195216 0, -1035482.4640965455 2287333.0698815673 0)), ((-1031335.8145355216 2288032.690707102 0, -1031735.973979156 2288083.6424779366 0, -1031684.4242973576 2288486.76042762 0, -1031283.7416613278 2288434.873665544 0, -1030883.0524479783 2288383.0092891282 0, -1030935.6500580298 2287981.7333433605 0, -1031335.8145355216 2288032.690707102 0)), ((-1029690.6327695481 2288227.9861841374 0, -1030081.6691394955 2288279.3375122994 0, -1030031.1897501762 2288680.060399877 0, -1029980.707957195 2289080.780604471 0, -1029580.5337932236 2289031.2535202373 0, -1029632.4103333049 2288630.7904119412 0, -1029690.6327695481 2288227.9861841374 0)), ((-1019437.7014199753 2308499.869161773 0, -1019385.3452084363 2308902.469899386 0, -1018988.0279197779 2308849.793594077 0, -1019040.5066439967 2308447.541076709 0, -1019437.7014199753 2308499.869161773 0)), ((-1015746.4921843759 2314958.970178708 0, -1015693.6757171493 2315360.0135502284 0, -1015496.280137871 2315334.935964606 0, -1015549.3098236041 2314933.92679566 0, -1015746.4921843759 2314958.970178708 0)), ((-1016826.8467043939 2315911.7043980435 0, -1016432.4276351677 2315861.5429225443 0, -1016486.7752965459 2315461.576262847 0, -1016486.8862928433 2315460.7593977996 0, -1016514.1169489527 2315260.3583780047 0, -1016541.2452727675 2315060.7104614796 0, -1016540.278824313 2315060.5877280417 0, -1016540.3865441052 2315059.796102671 0, -1016740.1515403495 2315085.1658760984 0, -1016712.3379686448 2315285.539725222 0, -1016811.9507220382 2315298.1938166893 0, -1016911.5634863044 2315310.847821505 0, -1016883.2160986736 2315511.120703014 0, -1016883.3611283406 2315511.1391318156 0, -1016826.8467043939 2315911.7043980435 0)), ((-1016088.5754403418 2315410.1455756347 0, -1016089.4892584289 2315410.2616955633 0, -1016089.3836509151 2315411.0698238383 0, -1016037.0835551982 2315811.281564955 0, -1016036.1696450292 2315811.1653767275 0, -1015640.8272461377 2315760.928157282 0, -1015693.6841488682 2315359.9842735534 0, -1015746.5446647434 2314959.029045533 0, -1016140.983925117 2315009.120498495 0, -1016088.5754403418 2315410.1455756347 0)), ((-1027155.3452638367 2316411.786709581 0, -1027099.3060001228 2316814.926257049 0, -1027043.2648768441 2317218.0630884925 0, -1026644.7072264659 2317166.6641910076 0, -1026246.1444279129 2317115.289097042 0, -1026301.8767193094 2316714.5768864295 0, -1026357.6113957331 2316313.8658440644 0, -1026413.3443055688 2315913.1521339053 0, -1026469.0776228255 2315512.4360198975 0, -1026474.1921480831 2315513.058994836 0, -1026474.157555098 2315513.316376404 0, -1026871.760588797 2315561.5732183787 0, -1027078.1453079201 2315586.632985187 0, -1027266.8527822931 2315609.6269936697 0, -1027211.099731914 2316010.7096340056 0, -1027155.3452638367 2316411.786709581 0)), ((-1025287.2500278767 2318219.881490436 0, -1025233.7673048442 2318619.0690635266 0, -1025036.6764289986 2318595.601747828 0, -1025043.9946522627 2318452.6497306363 0, -1024460.203644346 2318386.780092331 0, -1024550.039398206 2317716.8354266207 0, -1024948.6598177875 2317765.867653209 0, -1024893.4948594307 2318171.132183464 0, -1025287.2500278767 2318219.881490436 0)), ((-1014849.3035981857 2318610.752736169 0, -1014835.8670853045 2318710.77994911 0, -1014808.9939054567 2318910.834037035 0, -1014808.1539995833 2318917.0210857503 0, -1014414.5562884181 2318863.378070875 0, -1014015.7704339768 2318809.04622694 0, -1013615.4254839027 2318758.0232241508 0, -1013550.772978898 2318749.786416855 0, -1013609.6767885035 2318757.0489088283 0, -1013610.3754804195 2318751.8921359894 0, -1013215.7460878228 2318702.1602814947 0, -1013270.3161568193 2318305.2298836303 0, -1013270.981068162 2318300.3937520864 0, -1013668.3551273596 2318351.655942579 0, -1013667.6468856283 2318356.8909093654 0, -1014063.7056366887 2318406.8852371457 0, -1014050.3463598335 2318506.779348246 0, -1014449.826788734 2318558.767781257 0, -1014849.3035981857 2318610.752736169 0), (-1014037.285272602 2318604.443743791 0, -1014010.2686532065 2318806.460754792 0, -1014036.9870937357 2318606.673387476 0, -1014037.285272602 2318604.443743791 0)), ((-1014672.4252685239 2319910.521527098 0, -1014273.4849611721 2319859.6864720886 0, -1014244.5833741965 2320058.227364899 0, -1013850.0849239003 2320009.065353609 0, -1013905.9635467671 2319613.4271603054 0, -1013957.7778587915 2319209.892514499 0, -1013962.933897664 2319210.485891009 0, -1014360.2488984851 2319264.227305992 0, -1014306.4781407012 2319665.4990265067 0, -1014700.2199382108 2319717.20804532 0, -1014672.4252685239 2319910.521527098 0)), ((-1019844.4605516114 2367828.7181895296 0, -1019836.6832047377 2367828.6566944965 0, -1019844.1631092988 2367827.1020178064 0, -1019844.4605516114 2367828.7181895296 0)), ((-1019749.8586578161 2367846.7029273226 0, -1019730.4547369138 2367862.7044856353 0, -1019721.1015328282 2367852.680013197 0, -1019749.8586578161 2367846.7029273226 0)), ((-1019489.243215159 2367941.975031009 0, -1019589.486000852 2367857.0802320065 0, -1019591.1965935136 2367855.6316565396 0, -1019597.1352694286 2367850.602627461 0, -1019661.9165680929 2367823.0492214714 0, -1019712.3063310208 2367869.2079813634 0, -1019849.1142427962 2367835.4914042763 0, -1019869.2018001195 2367828.7689682436 0, -1020002.4213520194 2367846.9370946446 0, -1019971.7302186178 2368059.401858848 0, -1019569.4784886269 2368009.641163103 0, -1019568.6378645014 2368009.5371733913 0, -1019542.0667056023 2368203.846304738 0, -1019139.8706920221 2368154.1615764936 0, -1019150.3566583431 2368077.039244164 0, -1019152.6926239136 2368077.2998635396 0, -1019489.243215159 2367941.975031009 0)), ((-1003973.5743517822 2287706.1898662974 0, -1004025.5718877799 2287305.1669149064 0, -1004424.7817649296 2287357.397890239 0, -1004346.5417785074 2287950.361873327 0, -1003948.9173469689 2287896.3566977885 0, -1003973.5743517822 2287706.1898662974 0)), ((-1003901.1989418323 2288116.2585630426 0, -1003890.8487933791 2288114.9201946543 0, -1003883.605893194 2288174.411962796 0, -1003862.1054485671 2288171.600248244 0, -1003860.2304077749 2288184.957091726 0, -1003823.7950634706 2288181.0176527454 0, -1003781.916172518 2288501.9038193477 0, -1003475.6863386785 2288461.2584242583 0, -1003522.6738056624 2288067.3118181056 0, -1003502.4747744225 2288064.6998995417 0, -1003447.9683762782 2288465.462530355 0, -1003050.0397184071 2288414.0294446526 0, -1003103.747842437 2288013.1618786035 0, -1003154.9964387836 2287612.0738458135 0, -1003553.2501116302 2287663.7089973115 0, -1003951.5011944886 2287715.3650219887 0, -1003901.1989418323 2288116.2585630426 0)), ((-1009087.5148740095 2305865.370139448 0, -1009136.258259307 2305916.103084611 0, -1009136.5330183754 2305954.5286968364 0, -1009154.2122259465 2305981.045586549 0, -1009134.447688086 2306029.7765306416 0, -1009156.1677302218 2306060.736313041 0, -1009147.0279683745 2306158.2603304214 0, -1010042.1916633627 2306270.799617838 0, -1010014.2160898889 2306474.1360758375 0, -1009865.6718125867 2306454.892116094 0, -1009844.0995549656 2306610.806528638 0, -1009993.1410792228 2306627.320265293 0, -1009958.7902933572 2306878.827137127 0, -1008372.5172130546 2306669.6925328304 0, -1008477.6478298152 2305870.324516675 0, -1008504.3609385635 2305667.190937402 0, -1008902.3516348937 2305719.1747760354 0, -1008894.8853314016 2305776.1156096156 0, -1008907.9652613336 2305792.846865982 0, -1008963.7418124018 2305829.481909031 0, -1009086.796717778 2305844.6904211 0, -1009087.5148740095 2305865.370139448 0)), ((-1012080.1657174543 2306225.495257412 0, -1012066.2181388165 2306326.0104286755 0, -1011667.9346320677 2306274.120442113 0, -1011682.0397675895 2306173.623383318 0, -1012080.1657174543 2306225.495257412 0)), ((-995185.4699424236 2362232.4418430002 0, -995580.9063635829 2362284.6914323024 0, -995977.6564756974 2362337.1076862775 0, -995924.85988683 2362737.1121919192 0, -995528.3288417512 2362684.8342794636 0, -995133.4475070041 2362632.7698034365 0, -995185.3293791463 2362233.5235670325 0, -995185.4699424236 2362232.4418430002 0)), ((-1001947.4908209293 2369990.034007098 0, -1001895.5755670936 2370390.1016204013 0, -1001880.763366087 2370388.3296251586 0, -1001504.4080491482 2370340.030472195 0, -1001105.0060704153 2370288.7919512643 0, -1001154.8635472904 2369895.589450522 0, -1001548.4682520501 2369942.488806778 0, -1001947.4908209293 2369990.034007098 0)))</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>White Earth</t>
+          <t>Wind River</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>WY</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
+          <t>Farm Loan, Department of Environmental Quality, Escheat, Board of Charities and Reform, Game and Fish Commission, Acquired Farm Loan, State Charitable, Educational, Penal &amp; Reform Inst, Common School</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F75" t="n">
-        <v>1141</v>
+        <v>89</v>
       </c>
       <c r="G75" t="n">
-        <v>17197.01</v>
+        <v>3665.45</v>
       </c>
       <c r="H75" t="n">
-        <v>440</v>
+        <v>50</v>
       </c>
       <c r="I75" t="n">
-        <v>27174.74</v>
+        <v>2301.95</v>
       </c>
       <c r="J75" t="n">
-        <v>701</v>
+        <v>39</v>
       </c>
       <c r="K75" t="n">
-        <v>44371.75</v>
+        <v>5967.4</v>
       </c>
       <c r="L75" t="n">
-        <v>747912.54</v>
+        <v>2066861.74</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1050634.2762595804 2312278.921033107 0, -1050692.1496858974 2311878.8901095935 0, -1050749.8418575835 2311480.125285387 0, -1050805.7506747406 2311081.4597527836 0, -1050861.6613238936 2310682.782564328 0, -1051255.859984779 2310743.4741963 0, -1051200.1037733245 2311141.4396161498 0, -1051144.3479498741 2311539.4029425895 0, -1051088.5929212286 2311937.360776254 0, -1051032.8378361643 2312335.3193941107 0, -1050634.2762595804 2312278.921033107 0)), ((-1042827.6080114043 2324641.903880159 0, -1042429.0177734202 2324582.6384197455 0, -1042031.3687667405 2324523.506086521 0, -1042088.8292028453 2324128.4938440737 0, -1042087.857374831 2324128.3551963973 0, -1042088.6925061723 2324122.6112281634 0, -1041689.879792263 2324063.533034388 0, -1041292.0584445689 2324004.6261834027 0, -1041350.0240442571 2323614.889880292 0, -1041351.4699388619 2323605.1686712345 0, -1041409.4806173473 2323215.144439011 0, -1041410.9986382548 2323205.724764946 0, -1041473.7604708544 2322816.272943921 0, -1041472.3642102741 2322816.089643594 0, -1041473.7990416642 2322807.2053701356 0, -1041125.9567855056 2322761.754220014 0, -1040731.5802114733 2322710.2174758688 0, -1040791.3933385293 2322318.3149438472 0, -1040792.477179104 2322310.396591345 0, -1040846.3585751874 2321916.7483948767 0, -1040845.4352658397 2321916.6246562605 0, -1040846.3829309222 2321909.7169102994 0, -1041243.1470202254 2321962.8195580887 0, -1041593.576394404 2322009.7149099344 0, -1041991.033277303 2322068.01460237 0, -1042388.4929601529 2322126.307653034 0, -1042333.4848828288 2322526.274883522 0, -1041935.8066824579 2322467.5824857615 0, -1041873.028642868 2322866.373482969 0, -1041810.2530178527 2323265.1530656577 0, -1042211.0342654212 2323324.8051944994 0, -1042607.2119206154 2323383.7695842357 0, -1042547.2426509934 2323783.4970818204 0, -1042944.6907629055 2323842.7817654843 0, -1042886.3057913377 2324240.829846611 0, -1043285.130652052 2324298.636963205 0, -1043226.2979992016 2324699.977115077 0, -1042827.6080114043 2324641.903880159 0)), ((-1046247.5562064119 2329220.6481662146 0, -1046191.3633868239 2329622.789430642 0, -1046593.9948730316 2329678.6363939364 0, -1046534.9886577296 2330080.588037373 0, -1046475.9821583936 2330482.5278504863 0, -1046073.6083994912 2330426.0280175335 0, -1046132.4852626884 2330024.4114558683 0, -1045729.9819064847 2329968.257709795 0, -1045788.7291921459 2329566.9681130997 0, -1045845.5922356682 2329165.063035892 0, -1045443.6285155453 2329109.4754572785 0, -1045501.1639552393 2328707.7760154633 0, -1045558.6997935177 2328306.0742610637 0, -1045616.2362395419 2327904.37012149 0, -1045617.0326782259 2327904.479360659 0, -1045616.9327830005 2327905.1956020826 0, -1046016.0937759206 2327959.9533524564 0, -1045959.3246830138 2328361.192974082 0, -1045902.4578365213 2328763.1402011085 0, -1046303.7496655369 2328818.5044084494 0, -1046247.5562064119 2329220.6481662146 0)), ((-1059727.8355241397 2337697.3455502763 0, -1059668.8527381408 2338098.124818296 0, -1060067.131052015 2338153.3211093354 0, -1060465.4090640997 2338208.5355003844 0, -1060410.0971186836 2338610.1316959243 0, -1060354.7856983019 2339011.7223898345 0, -1059956.6096501015 2338955.955333517 0, -1059558.4318289415 2338900.184331322 0, -1059613.6421632078 2338499.155718323 0, -1059215.414667514 2338443.6841478753 0, -1058817.1846679002 2338388.2147207656 0, -1058872.287569143 2337987.7950442224 0, -1058931.3390659136 2337587.2694612537 0, -1058534.796627428 2337532.90503816 0, -1058592.9067027688 2337132.182809552 0, -1058194.7240368775 2337077.520104881 0, -1058252.2701342073 2336676.4067847277 0, -1058650.7321761935 2336731.296394675 0, -1059049.4432704628 2336786.216981644 0, -1058990.3909251 2337186.7443455644 0, -1059388.6021759196 2337241.6571514467 0, -1059329.5859732355 2337642.3091146755 0, -1059727.8355241397 2337697.3455502763 0)), ((-1066371.9632855507 2339438.2108617574 0, -1066373.429756151 2339438.414318711 0, -1066325.9659184492 2339779.1937124613 0, -1066316.6288095424 2339775.4830386983 0, -1066201.70517481 2339740.4795712177 0, -1066022.4006281008 2339615.323439348 0, -1065949.3493714838 2339578.6985750943 0, -1065929.2570379518 2339568.627267384 0, -1065850.4238185033 2339539.308687006 0, -1065748.3028524022 2339468.346541264 0, -1065676.2207522886 2339424.8367052525 0, -1065654.1213722434 2339415.392399067 0, -1065606.175104046 2339412.400131573 0, -1065571.9863841333 2339376.9328016816 0, -1065578.765703502 2339328.3709718734 0, -1065775.329001942 2339355.539352133 0, -1065828.8039514287 2338960.7937077926 0, -1066028.005994407 2338986.8329564976 0, -1066000.9377325266 2339187.759105069 0, -1066398.6148282972 2339240.822932089 0, -1066371.9632855507 2339438.2108617574 0)), ((-1061837.3204676933 2340034.6030477574 0, -1061780.3655670825 2340436.5922139487 0, -1061723.408817523 2340838.5788117982 0, -1061325.3843199636 2340783.392501526 0, -1060927.3602048056 2340728.202607241 0, -1060529.3384876326 2340673.0124064325 0, -1060131.31556903 2340617.8150917715 0, -1060187.739295776 2340216.35853855 0, -1060244.1628082008 2339814.9025566597 0, -1060299.4740761493 2339413.3136684936 0, -1060354.7856983019 2339011.7223898345 0, -1060752.5765780364 2339066.2638833597 0, -1061150.3704149113 2339120.8020020006 0, -1061548.164748814 2339175.3363516834 0, -1061945.959765405 2339229.8670557295 0, -1061891.6412659038 2339632.23640928 0, -1061837.3204676933 2340034.6030477574 0)), ((-1035118.4999299524 2281190.209319271 0, -1035513.4719348657 2281246.333069391 0, -1035908.4437363615 2281302.455823209 0, -1035850.9664973858 2281705.0788636506 0, -1035456.3629951405 2281647.737895494 0, -1035061.7616243811 2281590.3958082073 0, -1035118.4999299524 2281190.209319271 0)), ((-1016227.3939126243 2286441.674483058 0, -1016170.7846368499 2286843.4743179535 0, -1016116.572680074 2287240.187457348 0, -1015719.7979054934 2287188.6790665807 0, -1015774.9398044108 2286789.754045181 0, -1015830.8571983477 2286390.9832253153 0, -1016227.3939126243 2286441.674483058 0)), ((-1033898.8322515577 2287115.5060672923 0, -1034294.5248291742 2287171.182248576 0, -1034242.4095084692 2287571.8515250664 0, -1034188.3680121511 2287971.6597832455 0, -1033792.6131830172 2287916.5542716077 0, -1033846.4969216322 2287516.1923875464 0, -1033898.8322515577 2287115.5060672923 0)), ((-1035482.4640965455 2287333.0698815673 0, -1035431.1532593278 2287732.771150824 0, -1035380.0460347141 2288135.9017904988 0, -1034981.6506295949 2288083.604406882 0, -1035034.2370944343 2287683.1639975063 0, -1035085.9019275007 2287282.590195216 0, -1035482.4640965455 2287333.0698815673 0)), ((-1031335.8145355216 2288032.690707102 0, -1031735.973979156 2288083.6424779366 0, -1031684.4242973576 2288486.76042762 0, -1031283.7416613278 2288434.873665544 0, -1030883.0524479783 2288383.0092891282 0, -1030935.6500580298 2287981.7333433605 0, -1031335.8145355216 2288032.690707102 0)), ((-1029690.6327695481 2288227.9861841374 0, -1030081.6691394955 2288279.3375122994 0, -1030031.1897501762 2288680.060399877 0, -1029980.707957195 2289080.780604471 0, -1029580.5337932236 2289031.2535202373 0, -1029632.4103333049 2288630.7904119412 0, -1029690.6327695481 2288227.9861841374 0)), ((-1019437.7014199753 2308499.869161773 0, -1019385.3452084363 2308902.469899386 0, -1018988.0279197779 2308849.793594077 0, -1019040.5066439967 2308447.541076709 0, -1019437.7014199753 2308499.869161773 0)), ((-1015746.4921843759 2314958.970178708 0, -1015693.6757171493 2315360.0135502284 0, -1015496.280137871 2315334.935964606 0, -1015549.3098236041 2314933.92679566 0, -1015746.4921843759 2314958.970178708 0)), ((-1016826.8467043939 2315911.7043980435 0, -1016432.4276351677 2315861.5429225443 0, -1016486.7752965459 2315461.576262847 0, -1016486.8862928433 2315460.7593977996 0, -1016514.1169489527 2315260.3583780047 0, -1016541.2452727675 2315060.7104614796 0, -1016540.278824313 2315060.5877280417 0, -1016540.3865441052 2315059.796102671 0, -1016740.1515403495 2315085.1658760984 0, -1016712.3379686448 2315285.539725222 0, -1016811.9507220382 2315298.1938166893 0, -1016911.5634863044 2315310.847821505 0, -1016883.2160986736 2315511.120703014 0, -1016883.3611283406 2315511.1391318156 0, -1016826.8467043939 2315911.7043980435 0)), ((-1016088.5754403418 2315410.1455756347 0, -1016089.4892584289 2315410.2616955633 0, -1016089.3836509151 2315411.0698238383 0, -1016037.0835551982 2315811.281564955 0, -1016036.1696450292 2315811.1653767275 0, -1015640.8272461377 2315760.928157282 0, -1015693.6841488682 2315359.9842735534 0, -1015746.5446647434 2314959.029045533 0, -1016140.983925117 2315009.120498495 0, -1016088.5754403418 2315410.1455756347 0)), ((-1027155.3452638367 2316411.786709581 0, -1027099.3060001228 2316814.926257049 0, -1027043.2648768441 2317218.0630884925 0, -1026644.7072264659 2317166.6641910076 0, -1026246.1444279129 2317115.289097042 0, -1026301.8767193094 2316714.5768864295 0, -1026357.6113957331 2316313.8658440644 0, -1026413.3443055688 2315913.1521339053 0, -1026469.0776228255 2315512.4360198975 0, -1026474.1921480831 2315513.058994836 0, -1026474.157555098 2315513.316376404 0, -1026871.760588797 2315561.5732183787 0, -1027078.1453079201 2315586.632985187 0, -1027266.8527822931 2315609.6269936697 0, -1027211.099731914 2316010.7096340056 0, -1027155.3452638367 2316411.786709581 0)), ((-1025287.2500278767 2318219.881490436 0, -1025233.7673048442 2318619.0690635266 0, -1025036.6764289986 2318595.601747828 0, -1025043.9946522627 2318452.6497306363 0, -1024460.203644346 2318386.780092331 0, -1024550.039398206 2317716.8354266207 0, -1024948.6598177875 2317765.867653209 0, -1024893.4948594307 2318171.132183464 0, -1025287.2500278767 2318219.881490436 0)), ((-1014849.3035981857 2318610.752736169 0, -1014835.8670853045 2318710.77994911 0, -1014808.9939054567 2318910.834037035 0, -1014808.1539995833 2318917.0210857503 0, -1014414.5562884181 2318863.378070875 0, -1014015.7704339768 2318809.04622694 0, -1013615.4254839027 2318758.0232241508 0, -1013550.772978898 2318749.786416855 0, -1013609.6767885035 2318757.0489088283 0, -1013610.3754804195 2318751.8921359894 0, -1013215.7460878228 2318702.1602814947 0, -1013270.3161568193 2318305.2298836303 0, -1013270.981068162 2318300.3937520864 0, -1013668.3551273596 2318351.655942579 0, -1013667.6468856283 2318356.8909093654 0, -1014063.7056366887 2318406.8852371457 0, -1014050.3463598335 2318506.779348246 0, -1014449.826788734 2318558.767781257 0, -1014849.3035981857 2318610.752736169 0), (-1014037.285272602 2318604.443743791 0, -1014010.2686532065 2318806.460754792 0, -1014036.9870937357 2318606.673387476 0, -1014037.285272602 2318604.443743791 0)), ((-1014672.4252685239 2319910.521527098 0, -1014273.4849611721 2319859.6864720886 0, -1014244.5833741965 2320058.227364899 0, -1013850.0849239003 2320009.065353609 0, -1013905.9635467671 2319613.4271603054 0, -1013957.7778587915 2319209.892514499 0, -1013962.933897664 2319210.485891009 0, -1014360.2488984851 2319264.227305992 0, -1014306.4781407012 2319665.4990265067 0, -1014700.2199382108 2319717.20804532 0, -1014672.4252685239 2319910.521527098 0)), ((-1019844.4605516114 2367828.7181895296 0, -1019836.6832047377 2367828.6566944965 0, -1019844.1631092988 2367827.1020178064 0, -1019844.4605516114 2367828.7181895296 0)), ((-1019749.8586578161 2367846.7029273226 0, -1019730.4547369138 2367862.7044856353 0, -1019721.1015328282 2367852.680013197 0, -1019749.8586578161 2367846.7029273226 0)), ((-1019489.243215159 2367941.975031009 0, -1019589.486000852 2367857.0802320065 0, -1019591.1965935136 2367855.6316565396 0, -1019597.1352694286 2367850.602627461 0, -1019661.9165680929 2367823.0492214714 0, -1019712.3063310208 2367869.2079813634 0, -1019849.1142427962 2367835.4914042763 0, -1019869.2018001195 2367828.7689682436 0, -1020002.4213520194 2367846.9370946446 0, -1019971.7302186178 2368059.401858848 0, -1019569.4784886269 2368009.641163103 0, -1019568.6378645014 2368009.5371733913 0, -1019542.0667056023 2368203.846304738 0, -1019139.8706920221 2368154.1615764936 0, -1019150.3566583431 2368077.039244164 0, -1019152.6926239136 2368077.2998635396 0, -1019489.243215159 2367941.975031009 0)), ((-1003973.5743517822 2287706.1898662974 0, -1004025.5718877799 2287305.1669149064 0, -1004424.7817649296 2287357.397890239 0, -1004346.5417785074 2287950.361873327 0, -1003948.9173469689 2287896.3566977885 0, -1003973.5743517822 2287706.1898662974 0)), ((-1003901.1989418323 2288116.2585630426 0, -1003890.8487933791 2288114.9201946543 0, -1003883.605893194 2288174.411962796 0, -1003862.1054485671 2288171.600248244 0, -1003860.2304077749 2288184.957091726 0, -1003823.7950634706 2288181.0176527454 0, -1003781.916172518 2288501.9038193477 0, -1003475.6863386785 2288461.2584242583 0, -1003522.6738056624 2288067.3118181056 0, -1003502.4747744225 2288064.6998995417 0, -1003447.9683762782 2288465.462530355 0, -1003050.0397184071 2288414.0294446526 0, -1003103.747842437 2288013.1618786035 0, -1003154.9964387836 2287612.0738458135 0, -1003553.2501116302 2287663.7089973115 0, -1003951.5011944886 2287715.3650219887 0, -1003901.1989418323 2288116.2585630426 0)), ((-1009087.5148740095 2305865.370139448 0, -1009136.258259307 2305916.103084611 0, -1009136.5330183754 2305954.5286968364 0, -1009154.2122259465 2305981.045586549 0, -1009134.447688086 2306029.7765306416 0, -1009156.1677302218 2306060.736313041 0, -1009147.0279683745 2306158.2603304214 0, -1010042.1916633627 2306270.799617838 0, -1010014.2160898889 2306474.1360758375 0, -1009865.6718125867 2306454.892116094 0, -1009844.0995549656 2306610.806528638 0, -1009993.1410792228 2306627.320265293 0, -1009958.7902933572 2306878.827137127 0, -1008372.5172130546 2306669.6925328304 0, -1008477.6478298152 2305870.324516675 0, -1008504.3609385635 2305667.190937402 0, -1008902.3516348937 2305719.1747760354 0, -1008894.8853314016 2305776.1156096156 0, -1008907.9652613336 2305792.846865982 0, -1008963.7418124018 2305829.481909031 0, -1009086.796717778 2305844.6904211 0, -1009087.5148740095 2305865.370139448 0)), ((-1012080.1657174543 2306225.495257412 0, -1012066.2181388165 2306326.0104286755 0, -1011667.9346320677 2306274.120442113 0, -1011682.0397675895 2306173.623383318 0, -1012080.1657174543 2306225.495257412 0)), ((-995185.4699424236 2362232.4418430002 0, -995580.9063635829 2362284.6914323024 0, -995977.6564756974 2362337.1076862775 0, -995924.85988683 2362737.1121919192 0, -995528.3288417512 2362684.8342794636 0, -995133.4475070041 2362632.7698034365 0, -995185.3293791463 2362233.5235670325 0, -995185.4699424236 2362232.4418430002 0)), ((-1001947.4908209293 2369990.034007098 0, -1001895.5755670936 2370390.1016204013 0, -1001880.763366087 2370388.3296251586 0, -1001504.4080491482 2370340.030472195 0, -1001105.0060704153 2370288.7919512643 0, -1001154.8635472904 2369895.589450522 0, -1001548.4682520501 2369942.488806778 0, -1001947.4908209293 2369990.034007098 0)))</t>
+          <t>POLYGON Z ((-2000691.670389903 2331962.4047491485 0, -2000297.120530334 2331863.8366929404 0, -2000378.7610276425 2331555.6632454637 0, -2000383.52788925 2331550.664125949 0, -2000404.2332826294 2331528.949865917 0, -2000436.5508040052 2331496.630248958 0, -2000457.0939019124 2331482.942588032 0, -2000524.6099901185 2331437.9570213845 0, -2000623.547944883 2331521.1411316423 0, -2000642.2051764121 2331455.954080666 0, -2000783.0149527532 2331525.924893335 0, -2000794.6718260078 2331570.5907869237 0, -2000795.608453972 2331574.17969693 0, -2000856.417264013 2331807.1811536797 0, -2000936.3358951204 2331898.801343468 0, -2001108.5968959765 2331976.922216007 0, -2001147.7393053952 2331994.673259766 0, -2001155.817165279 2332078.3893294954 0, -2001086.2153794249 2332060.9932991057 0, -2000691.670389903 2331962.4047491485 0))</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Wind River</t>
+          <t>XL Ranch</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>WY</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Department of Environmental Quality, Farm Loan, Escheat, Board of Charities and Reform, Game and Fish Commission, Acquired Farm Loan, State Charitable, Educational, Penal &amp; Reform Inst, Common School</t>
+          <t>School Lands</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="G76" t="n">
-        <v>3665.45</v>
+        <v>62.54</v>
       </c>
       <c r="H76" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="I76" t="n">
-        <v>2301.95</v>
+        <v>62.54</v>
       </c>
       <c r="J76" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="K76" t="n">
-        <v>5967.4</v>
+        <v>125.08</v>
       </c>
       <c r="L76" t="n">
-        <v>2066861.74</v>
+        <v>9807.360000000001</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>POLYGON Z ((-2000691.670389903 2331962.4047491485 0, -2000297.120530334 2331863.8366929404 0, -2000378.7610276425 2331555.6632454637 0, -2000383.52788925 2331550.664125949 0, -2000404.2332826294 2331528.949865917 0, -2000436.5508040052 2331496.630248958 0, -2000457.0939019124 2331482.942588032 0, -2000524.6099901185 2331437.9570213845 0, -2000623.547944883 2331521.1411316423 0, -2000642.2051764121 2331455.954080666 0, -2000783.0149527532 2331525.924893335 0, -2000794.6718260078 2331570.5907869237 0, -2000795.608453972 2331574.17969693 0, -2000856.417264013 2331807.1811536797 0, -2000936.3358951204 2331898.801343468 0, -2001108.5968959765 2331976.922216007 0, -2001147.7393053952 2331994.673259766 0, -2001155.817165279 2332078.3893294954 0, -2001086.2153794249 2332060.9932991057 0, -2000691.670389903 2331962.4047491485 0))</t>
+          <t xml:space="preserve">MULTIPOLYGON Z (((-1947124.5557107623 2807295.7237508334 0, -1947196.7819263288 2807274.393608224 0, -1947193.1458702104 2807288.599900207 0, -1947059.5372636789 2807810.6141429264 0, -1946853.3734672957 2808596.0136770844 0, -1946745.5648815252 2808986.612934126 0, -1946341.8260397688 2808874.4829723123 0, -1945948.194095369 2808765.148187057 0, -1945556.2480824378 2808656.277029655 0, -1945447.281745532 2809049.883998759 0, -1945055.775332241 2808942.2476052986 0, -1944671.1240387606 2808836.5816436727 0, -1944285.9715556526 2808729.451306282 0, -1944182.7006740377 2808700.8373704124 0, -1944175.258183883 2808698.7751340363 0, -1944205.97409468 2808691.593999012 0, -1944239.832728101 2808683.6780427233 0, -1944297.1865183178 2808670.268832043 0, -1944326.1207686376 2808663.504190235 0, -1944341.9027250202 2808643.0757502136 0, -1944450.3186288457 2808502.7405995512 0, -1944484.6290076356 2808458.3283272255 0, -1944531.3559075892 2808450.5231368784 0, -1944533.2475823362 2808450.207102876 0, -1944742.3493571964 2808415.2779346644 0, -1944782.5304498996 2808408.56573509 0, -1944825.9314816992 2808401.315558442 0, -1944846.4419707358 2808397.889270128 0, -1944932.4650723806 2808383.518803587 0, -1945120.8879312954 2808352.0413803793 0, -1945232.340665698 2808300.193092651 0, -1945233.011146676 2808299.8811820387 0, -1945234.1767156126 2808299.338971333 0, -1945367.0666779706 2808239.105563168 0, -1945403.2525988873 2808189.1273322944 0, -1945406.8244306557 2808184.194092287 0, -1945434.3286187563 2808146.206466028 0, -1945452.2644826355 2808121.434357619 0, -1945517.6448988912 2808031.1333648274 0, -1945708.4753189383 2807935.2428929717 0, -1945743.469064124 2807917.658688479 0, -1945773.6058255532 2807875.803767459 0, -1945783.8263632155 2807861.609515513 0, -1945794.803288026 2807846.364457131 0, -1945805.1034344905 2807832.0591395595 0, -1945838.5799746306 2807785.5660434654 0, -1945999.7991482161 2807667.234313057 0, -1946006.4658096721 2807662.3410324776 0, -1946060.3811198939 2807650.8228329164 0, -1946249.9701467785 2807610.3188651903 0, -1946270.8384821936 2807605.860535518 0, -1946329.3806055868 2807593.353076714 0, -1946424.2470437514 2807573.08506474 0, -1946682.5545190827 2807536.241129031 0, -1946715.8717711887 2807531.488632948 0, -1946735.830111049 2807528.641718737 0, -1946811.206861308 2807517.889765267 0, -1946845.9224203727 2807472.3194938726 0, -1946907.4433662225 2807391.5624610432 0, -1946950.1763059627 2807335.467485209 0, -1946961.8711610327 2807337.088222957 0, -1947066.3557622277 2807351.5676600714 0, -1947124.5557107623 2807295.7237508334 0)), ((-1953386.7879867416 2809957.2616419047 0, -1953122.7670257601 2809888.019521383 0, -1953193.010530159 2809596.6558950776 0, -1953203.577075884 2809552.826982933 0, -1953281.4916945917 2809558.277206182 0, -1953292.17934746 2809749.786360986 0, -1953293.2236294863 2809768.4961081003 0, -1953296.9640707995 2809835.516895046 0, -1953482.0649389857 2809967.511132979 0, -1953484.7584606395 2809969.4318917906 0, -1953487.6914903347 2809983.723829882 0, -1953386.7879867416 2809957.2616419047 0)), ((-1946614.9078962246 2811885.370776785 0, -1946633.8647125496 2811896.64560381 0, -1946653.0110561145 2811912.1504938467 0, -1946684.166303763 2811937.3803751133 0, -1946689.2998346796 2811942.553062524 0, -1946690.5019310338 2811943.7641511704 0, -1946698.197141594 2811951.5179146877 0, -1946715.1627968417 2811971.3295670627 0, -1946730.0721239133 2811985.5084807114 0, -1946745.232731864 2811995.7451126017 0, -1946751.3168938763 2811998.816866132 0, -1946821.3437366372 2812034.169959289 0, -1946845.616608355 2812045.7422609036 0, -1946879.5990443504 2812061.9438724904 0, -1946879.8500397133 2812062.0636778786 0, -1946910.9144404363 2812076.8738750056 0, -1946947.7533411365 2812094.4371382394 0, -1947060.7872370374 2812153.652763408 0, -1947139.5149107124 2812191.1254910952 0, -1947153.044659055 2812194.2237642687 0, -1947176.9299978777 2812105.4381115045 0, -1947178.3598672908 2812088.189209279 0, -1947180.6096412572 2812076.401427918 0, -1947184.6021095074 2812055.484020593 0, -1947199.007831662 2811996.7596786823 0, -1947205.7505111548 2811998.307882489 0, -1947601.865979837 2812089.2656746367 0, -1947161.8444363042 2813724.908500826 0, -1947938.7742716009 2813946.868101684 0, -1948716.0669331742 2814153.7326147486 0, -1948508.1692716295 2814936.5808169744 0, -1948296.06130565 2815711.6417853036 0, -1948085.8615166286 2816490.051731219 0, -1947887.1532080339 2817263.7317802105 0, -1947110.1819699025 2817045.1674422114 0, -1946333.2349266736 2816826.5353467013 0, -1946536.5120191795 2816052.253474633 0, -1946743.038038953 2815275.9633118263 0, -1945965.8537946267 2815058.6734601483 0, -1945187.38250786 2814847.511176291 0, -1945390.6584151017 2814070.8353690077 0, -1945593.9390024608 2813294.1439373647 0, -1945806.4183397717 2812512.0426953356 0, -1946017.4099203725 2811725.407987297 0, -1946413.5226287036 2811816.379077322 0, -1946413.1175892442 2811817.8873744495 0, -1946429.5205681976 2811823.0182974017 0, -1946430.5705775602 2811823.3468920225 0, -1946441.4127719733 2811826.7384116566 0, -1946460.0693028378 2811832.573924255 0, -1946546.4250696348 2811858.060609156 0, -1946584.401309241 2811872.0030026874 0, -1946614.9078962246 2811885.370776785 0)), ((-1948900.588521401 2813349.774017343 0, -1948809.1497083865 2813748.171309886 0, -1948240.7924339913 2813580.0435008793 0, -1948345.2341088098 2813173.972558003 0, -1948900.588521401 2813349.774017343 0)), ((-1952221.214135054 2813417.0188169414 0, -1952606.9522442534 2813525.2989367954 0, -1952609.412323701 2813525.9894720893 0, -1952608.7617625473 2813528.576734444 0, -1952521.005898842 2813877.601366205 0, -1952461.1719096894 2813882.468296462 0, -1952404.91447361 2813887.0441548065 0, -1952125.3607299807 2813809.319979971 0, -1952221.214135054 2813417.0188169414 0)), ((-1951109.403211928 2817706.2222447176 0, -1950981.9253401442 2817755.7212553616 0, -1950915.0461234644 2817781.5329516055 0, -1950878.459851005 2817795.653069836 0, -1950813.5889805139 2817754.9988670424 0, -1950714.747913343 2817693.0551435365 0, -1950696.3781159038 2817681.5429214216 0, -1950634.842756184 2817642.978246047 0, -1950475.0732963716 2817794.2712869965 0, -1950350.9850651731 2817911.774685636 0, -1950229.4130995688 2817877.218136361 0, -1949459.3219813337 2817655.629660831 0, -1949675.1280854722 2816881.8744489173 0, -1949882.0230697875 2816121.976450482 0, -1951048.5181664268 2816443.4519810094 0, -1951135.8725615966 2816045.698412492 0, -1951397.6412383653 2816122.326121462 0, -1951398.2366670764 2816140.6499513793 0, -1951429.1657775978 2816344.5042031966 0, -1951458.0132103665 2816395.444446804 0, -1951458.6854130586 2816396.631445679 0, -1951419.2681869979 2816543.478137624 0, -1951245.4248171826 2817266.2006058693 0, -1951115.3352282133 2817703.9188853893 0, -1951109.403211928 2817706.2222447176 0)), ((-1948800.0774710595 2820079.056871323 0, -1948755.4657172174 2820088.8711917084 0, -1948729.7918133228 2820094.519223721 0, -1948749.6901557706 2819981.7351393187 0, -1949029.2966877047 2819219.0309122363 0, -1949216.1317151315 2819267.1190779125 0, -1949122.1522565759 2819352.187155631 0, -1949068.056106266 2819432.4726366717 0, -1949023.0329906945 2819505.4548712545 0, -1949044.0199872083 2819623.3749157335 0, -1949075.2662473642 2819798.93361861 0, -1948965.0742484073 2819994.7351705506 0, -1948901.8355726646 2820027.0534498193 0, -1948800.0774710595 2820079.056871323 0)), ((-1947711.056209912 2823037.388546394 0, -1947710.3908040728 2823052.360373251 0, -1947703.6130837516 2823204.87018648 0, -1947635.7493479564 2823448.7215245077 0, -1947632.6231846497 2823459.954442923 0, -1947651.3765163652 2823799.3043881706 0, -1947622.273734997 2823892.2555906605 0, -1947617.236901387 2823908.3427039455 0, -1947519.7118047255 2824219.8324208586 0, -1947474.1677948614 2824286.46855595 0, -1947457.4749831655 2824310.895477439 0, -1947392.8850046801 2824501.2802619715 0, -1947285.5751249949 2824652.8274717364 0, -1947282.93064712 2824656.5636720136 0, -1947144.512593157 2824804.2110868483 0, -1947222.884602449 2824860.459899903 0, -1947266.2238187243 2824978.8393854517 0, -1947343.8223486969 2824953.2193777794 0, -1947334.0825702942 2825080.905190541 0, -1947321.0618002464 2825251.6351106544 0, -1947253.1551944956 2825475.1227064123 0, -1947248.8139849745 2825482.088473379 0, -1946516.2152451943 2825292.499795915 0, -1945735.8521312105 2825090.6417997656 0, -1945524.0930363676 2825864.6570646428 0, -1945314.7721398615 2826639.52506426 0, -1945088.7128367843 2827410.705539773 0, -1944876.2513827144 2828185.515469902 0, -1944086.5716233156 2827974.060117378 0, -1943708.4311984438 2827856.921258917 0, -1943313.7750874953 2827749.8342451244 0, -1942552.8778908548 2827565.478069011 0, -1942433.8878418936 2827952.8691948676 0, -1942115.2148576651 2829110.296337552 0, -1941740.247006324 2829021.677830297 0, -1941364.8913283464 2828934.2149304776 0, -1940614.4885814935 2828717.4324106015 0, -1940380.7262877997 2829491.0634633354 0, -1941157.3486816953 2829714.164489239 0, -1940962.5406810332 2830480.7188912537 0, -1942461.70950291 2830885.848456556 0, -1942692.6805440595 2830137.7557435655 0, -1942793.6901436509 2829709.63596787 0, -1942894.7014358174 2829281.5114808935 0, -1943664.6776832102 2829494.2014161125 0, -1944444.5162852963 2829727.3526395317 0, -1944240.9796830066 2830537.874774691 0, -1944046.067697474 2831315.9714416503 0, -1943848.50376597 2832102.6996421823 0, -1943743.83154259 2832479.2347885496 0, -1943644.3767330595 2832837.0025605005 0, -1943581.2039236382 2832819.7384977685 0, -1942869.1977661247 2832625.1609020308 0, -1942803.9323556963 2832608.7278774576 0, -1942095.9751251442 2832430.4740522504 0, -1942023.432910939 2832411.589677251 0, -1941320.4345445875 2832228.5872334125 0, -1941241.4812423058 2832213.40905601 0, -1940518.8604381077 2832067.5301795797 0, -1940427.6025438693 2832041.979955196 0, -1939719.1298166327 2831844.149645808 0, -1939650.2813025315 2831823.7800045474 0, -1939008.2927350795 2831633.9075519615 0, -1938937.8182702172 2831612.9978779657 0, -1938875.459023381 2831595.8261597687 0, -1938155.5847200237 2831397.7635465516 0, -1938098.1574108254 2831382.171489841 0, -1937367.725195407 2831183.8592544473 0, -1937319.7935790198 2831170.7466271804 0, -1936592.1479990568 2830970.5633796058 0, -1936551.782240904 2830958.459755302 0, -1935919.8841535791 2830768.979581447 0, -1935853.7424633587 2830666.800432577 0, -1936043.9285566418 2829974.059544721 0, -1936145.9669096095 2829606.0232871436 0, -1936248.0642732342 2829237.7809193237 0, -1936459.6332089452 2828420.087475266 0, -1936671.1932913214 2827602.744161404 0, -1935901.1673248971 2827404.963971848 0, -1935131.6484503855 2827207.345645183 0, -1934737.3642994917 2827104.054830973 0, -1934342.5261924486 2827000.6324797366 0, -1933553.2220813956 2826793.841596687 0, -1933761.5091981522 2826019.775546707 0, -1933975.9384614483 2825234.8236955265 0, -1933583.8297440552 2825126.270168573 0, -1933192.1269479976 2825017.8277554675 0, -1933406.247326265 2824251.320284405 0, -1933484.1597564383 2824270.6364715467 0, -1933560.93079583 2824065.5594003047 0, -1933557.1777476843 2823669.876861863 0, -1933632.168574466 2823445.1023491654 0, -1933233.0538895007 2823344.3789825863 0, -1932833.940247076 2823243.6511097113 0, -1932372.995906775 2823117.950424193 0, -1932730.2121003186 2821547.4664698183 0, -1933252.3690630475 2820001.953830233 0, -1932875.059471353 2819895.6085127 0, -1932120.5151176807 2819683.5672394563 0, -1930577.5733440355 2819261.3804175365 0, -1929696.1913390842 2819055.4839692526 0, -1929845.6354374762 2818625.467116351 0, -1929872.7544179265 2818547.434736694 0, -1929874.57124737 2818542.207133 0, -1929880.1351356034 2818526.1975715207 0, -1929881.7522122038 2818521.5443381337 0, -1929983.0851736646 2818229.966494045 0, -1929619.2157681047 2818130.8872940643 0, -1929736.580766636 2817750.492223993 0, -1929360.2837025973 2817657.226028599 0, -1929354.5875267424 2817678.947000758 0, -1929353.228261422 2817684.129774841 0, -1929341.3386348058 2817729.4691167814 0, -1929339.8485104665 2817735.151194868 0, -1929337.815666145 2817742.9028611216 0, -1929255.3412267803 2818031.826646187 0, -1928918.8246952381 2818810.952408313 0, -1928122.7990207672 2818594.244171984 0, -1928024.642395889 2818569.0576784485 0, -1927630.2863546014 2817947.253782771 0, -1927551.1817190184 2817823.047702654 0, -1927201.5305156272 2817274.0244157608 0, -1927013.8005473418 2816985.972721535 0, -1927170.6971796076 2816600.8326979834 0, -1927186.888627717 2816605.135812899 0, -1927955.1064756506 2816810.1267357282 0, -1928062.8644512328 2816410.767847923 0, -1928170.6236448651 2816011.404500228 0, -1928170.6519277014 2816011.3002163935 0, -1928335.5725609951 2816060.678830224 0, -1928340.479160045 2816062.14773463 0, -1928358.8299043912 2816067.6420136616 0, -1928363.9512381542 2816069.1753942226 0, -1928547.897408099 2816124.249284745 0, -1928652.450982854 2815747.538075545 0, -1928287.6432609076 2815609.2405163767 0, -1928283.2752051004 2815607.584605435 0, -1928279.9276287449 2815606.3154997323 0, -1928283.612778869 2815594.6022822983 0, -1928288.215822168 2815577.514176424 0, -1928388.6672126406 2815203.3196104844 0, -1928756.3313858095 2815373.2517059958 0, -1929123.7263016994 2815543.083117765 0, -1929897.3229792737 2815749.610247387 0, -1929707.9124916464 2816449.4440081026 0, -1929470.2812261013 2817237.773556349 0, -1929860.56049845 2817348.6562962593 0, -1930250.833378816 2817459.560403357 0, -1930641.143404357 2817570.4991767206 0, -1931031.4472574294 2817681.459688435 0, -1931805.2503211931 2817905.5667042457 0, -1932594.1915322812 2818127.825577896 0, -1932811.8928143983 2817356.7666764436 0, -1933022.8681155671 2816578.4116334063 0, -1933795.9299697948 2816792.540353066 0, -1934163.8246629832 2816898.246070321 0, -1934550.1172213496 2817009.2331912736 0, -1934334.2296709986 2817788.790593405 0, -1934108.049074308 2818561.261530009 0, -1934909.250632951 2818782.6145231696 0, -1935116.7927075562 2818006.531720954 0, -1935916.8198173607 2818229.1149338917 0, -1936676.3996078675 2818437.897329563 0, -1936462.9739085813 2819219.5778062106 0, -1936353.5000564817 2819609.4351670644 0, -1936243.9917860483 2819999.2792242086 0, -1936632.7686874776 2820105.6482482827 0, -1937021.5500128125 2820212.013846692 0, -1937413.318937494 2820320.6705608866 0, -1937805.0901551058 2820429.3200657633 0, -1937698.353795431 2820820.401979242 0, -1937592.4233251668 2821208.550592578 0, -1937985.3208603768 2821315.5024794503 0, -1937786.438834566 2822105.703372242 0, -1937572.007178126 2822882.830218352 0, -1937947.7030090205 2822971.5158543093 0, -1938378.049721953 2821422.3454312244 0, -1938770.257508245 2821532.227865583 0, -1938981.1579699456 2820755.2587466994 0, -1938588.1487450716 2820646.4371728147 0, -1938799.1743406628 2819864.585701209 0, -1939022.6444431625 2819088.687467256 0, -1939242.4706204562 2818309.8925407636 0, -1939462.8863154226 2817539.1384911337 0, -1939684.5868446275 2816755.1590106944 0, -1940481.046967366 2816953.4827664336 0, -1941277.4698106893 2817151.7884277906 0, -1941666.9750141355 2817255.678148611 0, -1942056.4813348188 2817359.563572374 0, -1942799.6122432877 2817584.255998529 0, -1942579.2484212103 2818370.2245898014 0, -1942358.8900397797 2819156.175726435 0, -1942255.0990678044 2819547.3025721707 0, -1942151.236367304 2819938.450738095 0, -1942043.4314071736 2820328.0719141285 0, -1941935.5920665667 2820717.6798253707 0, -1943517.0213170212 2821089.9273377797 0, -1943289.8592308573 2821862.5371859185 0, -1943073.3554806781 2822728.562133121 0, -1943834.9354735375 2822914.7426675498 0, -1944612.9373131827 2823120.186971993 0, -1945390.9473912406 2823325.61012788 0, -1945779.9519991863 2823428.3177299947 0, -1946168.9579114623 2823531.02142024 0, -1946284.3938566889 2823110.445017022 0, -1946397.9609839355 2822700.6624759194 0, -1947185.9908282983 2822901.5805788804 0, -1947711.056209912 2823037.388546394 0), (-1934758.975706155 2825446.512897815 0, -1934653.0218455815 2825841.932409918 0, -1935043.4589296302 2825948.790364581 0, -1935150.4415958782 2825552.3993304996 0, -1935541.7468236985 2825658.256978833 0, -1935646.7138191978 2825263.1583201904 0, -1936029.8489498126 2825363.6139364857 0, -1936413.00537298 2825464.090523153 0, -1936487.7773941478 2825192.6720164535 0, -1936433.7728069306 2825054.5628216825 0, -1936135.5340307557 2824973.1069335695 0, -1936245.3051296428 2824573.794055444 0, -1935862.1415192464 2824473.3424840486 0, -1935969.817728062 2824082.0210779584 0, -1936084.9942129245 2823647.682375033 0, -1936174.577011313 2823309.8599834703 0, -1935399.411184608 2823094.9130661804 0, -1935501.0654255731 2822711.01071649 0, -1935124.0544510153 2822606.820595831 0, -1934963.3254915304 2822562.4005034817 0, -1934958.4332583307 2822369.333828692 0, -1934828.3273453016 2822114.356937905 0, -1934728.9298708765 2822497.6198299667 0, -1934629.6000918266 2822880.6597541803 0, -1934467.1727870738 2822838.0632362305 0, -1934237.4196847486 2822777.8091885406 0, -1934031.2843016037 2823545.8212093497 0, -1933917.7880985364 2823517.1802627076 0, -1933790.0503903565 2823747.4732142584 0, -1933761.194117387 2824123.826363364 0, -1933680.13984651 2824319.2227905844 0, -1934217.7233894903 2824452.4925112473 0, -1933975.9384614483 2825234.8236955265 0, -1934758.975706155 2825446.512897815 0), (-1939585.1471896607 2829261.4028389654 0, -1939818.2940440194 2828487.400401368 0, -1938649.617593449 2828181.742712182 0, -1938258.7925312018 2828077.720105118 0, -1938143.3234812513 2828440.935519226 0, -1938027.8552433995 2828804.146640231 0, -1937825.555195848 2829570.0810287166 0, -1939374.8838128757 2829997.759182874 0, -1939585.1471896607 2829261.4028389654 0), (-1930920.3377759478 2818068.226708838 0, -1930518.6474033971 2817956.4985622237 0, -1930396.1606221455 2818342.4661825285 0, -1930766.5858791282 2818443.3733610176 0, -1930776.1682660037 2818445.983636517 0, -1930809.2299065518 2818454.9896017592 0, -1930813.003602764 2818441.853874067 0, -1930814.3485153364 2818437.1717314213 0, -1930920.3377759478 2818068.226708838 0), (-1930255.115148408 2817883.195627018 0, -1930236.724376213 2817878.080051084 0, -1930012.3089755394 2818237.925762199 0, -1930030.7570267974 2818242.950074561 0, -1930255.115148408 2817883.195627018 0)), ((-1941975.4751981073 2808840.0696086613 0, -1941997.1538114115 2808836.4567134576 0, -1942073.5637378213 2808823.722606744 0, -1942131.7629030917 2808808.992433286 0, -1942208.4989129088 2808789.57058315 0, -1942416.180367779 2808737.0050345478 0, -1942455.87754672 2808717.4955143197 0, -1942544.9733916684 2808673.708611994 0, -1942610.5539401006 2808641.478167417 0, -1942620.1244321063 2808636.774620107 0, -1942663.400072895 2808615.5060951007 0, -1942753.6674295608 2808571.1424578154 0, -1942869.51606919 2808688.9877995523 0, -1942888.4225879675 2808708.219790584 0, -1942889.654890738 2808709.4734285926 0, -1942895.2061948585 2808710.0261795996 0, -1943049.4737258072 2808725.3855749154 0, -1943082.0811213637 2808728.6318694507 0, -1943105.6422018444 2808759.283847976 0, -1943160.5267339058 2808830.685657026 0, -1943205.0386135392 2808888.592700042 0, -1943276.3573062862 2809003.8482864983 0, -1943377.1216596877 2809067.6060874094 0, -1943381.3177654438 2809070.2610881724 0, -1943377.6567924723 2809086.5898198485 0, -1943328.4432893663 2809306.0939921406 0, -1942477.1866891305 2809087.429074342 0, -1941793.930382525 2808892.4903800027 0, -1941789.0354423348 2808891.0937741525 0, -1941800.329167384 2808887.565882612 0, -1941827.8367050479 2808878.973043119 0, -1941869.040369248 2808866.101807077 0, -1941925.9578423577 2808848.3217931706 0, -1941933.5939346517 2808847.0492320075 0, -1941975.4751981073 2808840.0696086613 0)), ((-1944058.723598079 2816226.208026141 0, -1943942.488938613 2816616.768198294 0, -1943547.2736266737 2816516.6943910923 0, -1943663.3560512534 2816121.164155373 0, -1944058.723598079 2816226.208026141 0)), ((-1943034.0998549613 2816804.0528895273 0, -1943429.9347577845 2816916.434716266 0, -1943190.0135548415 2817682.717167016 0, -1942799.6122432877 2817584.255998529 0, -1943034.0998549613 2816804.0528895273 0)), ((-1943581.524175765 2817781.7749560145 0, -1943822.2347943233 2817004.9033741523 0, -1944560.3858638655 2817171.3886290533 0, -1944344.9823447221 2817974.9235633775 0, -1943581.524175765 2817781.7749560145 0)), ((-1936153.4484906516 2811585.839009829 0, -1936174.945166137 2811575.6432904634 0, -1936331.8753854744 2811520.53820495 0, -1936485.3815387331 2811478.6248240764 0, -1936535.956110518 2811464.8157760906 0, -1936570.6387233243 2811455.3457541857 0, -1936691.344574958 2811344.07207154 0, -1936797.7922188782 2811318.367799899 0, -1936864.795513821 2811302.187914356 0, -1936932.0140674335 2811261.923055901 0, -1936967.2226207997 2811240.832516306 0, -1936988.2531909542 2811228.234803959 0, -1937110.3845130322 2811121.5474925996 0, -1937331.5234054446 2811029.662503699 0, -1937825.614099507 2811136.749395092 0, -1937626.9716735017 2811921.5246444508 0, -1937428.2562024964 2812706.7988925623 0, -1936631.9254041116 2812517.482568833 0, -1935835.3500741445 2812328.5873463713 0, -1936019.0369716408 2811654.632357626 0, -1936020.6140379785 2811648.8460765434 0, -1936023.788997826 2811647.3343533343 0, -1936153.4484906516 2811585.839009829 0)), ((-1934629.6000918266 2822880.6597541803 0, -1935014.5051893676 2822987.7885432597 0, -1934920.3375659534 2823381.8329619314 0, -1934530.000007294 2823263.5995747233 0, -1934629.6000918266 2822880.6597541803 0)), ((-1928802.6239436434 2813711.292642901 0, -1928695.4713545218 2814099.5714198337 0, -1928588.319572293 2814487.8458844405 0, -1928486.0163505543 2814883.946014951 0, -1928047.7060741284 2814765.1291601956 0, -1928169.909786337 2814374.937847502 0, -1928291.2333748734 2813991.870427505 0, -1928411.9188028697 2813610.815898007 0, -1928802.6239436434 2813711.292642901 0)), ((-1930344.3252405708 2814131.2391046174 0, -1931145.4264724182 2814216.068519604 0, -1931897.6967454187 2814520.078997948 0, -1931677.669010281 2815348.565582413 0, -1931455.9990515015 2816177.889569845 0, -1930679.8917686564 2815963.721800876 0, -1929897.3229792737 2815749.610247387 0, -1930101.4035317835 2814982.196513081 0, -1930344.3252405708 2814131.2391046174 0), (-1931176.4831238952 2815664.0622126306 0, -1931285.0219405617 2815257.3089883183 0, -1930496.8888091063 2815074.1259574196 0, -1930392.7472309952 2815465.399057443 0, -1930786.1327697122 2815564.888445243 0, -1931176.4831238952 2815664.0622126306 0)), ((-1932625.004395147 2824019.372009379 0, -1933015.4430826395 2824135.5915850047 0, -1932800.8537718498 2824906.077624436 0, -1932409.581895042 2824794.323167323 0, -1932625.004395147 2824019.372009379 0)), ((-1920878.2998509065 2864462.17655 0, -1919339.6526715388 2863911.015689175 0, -1919499.2762970189 2863216.3909553443 0, -1919730.7560771785 2862646.1294262023 0, -1921234.9285229577 2863201.991168637 0, -1920878.2998509065 2864462.17655 0)), ((-1922638.7562835668 2863745.317361907 0, -1924153.195741897 2864306.7299528057 0, -1923888.6471772937 2865271.213071534 0, -1922316.4412968731 2864845.7317742375 0, -1922638.7562835668 2863745.317361907 0)), ((-1926037.7249022147 2865457.6752195945 0, -1926036.5113501642 2865458.052518688 0, -1925975.9532681934 2865453.9122872567 0, -1925930.7511069255 2865465.3310377323 0, -1925799.5858269983 2865498.4620929626 0, -1925670.3957903862 2865546.158560157 0, -1925466.1884740398 2865642.7213355713 0, -1925454.2712138693 2865648.3563584513 0, -1925407.9209830656 2865656.2345184283 0, -1925416.9028312895 2865626.803323347 0, -1925647.9816289446 2864883.8372634226 0, -1926426.6688185155 2865162.56099678 0, -1926346.923875304 2865447.8805387504 0, -1926344.6599197036 2865455.9786466183 0, -1926286.1722074042 2865450.0294201733 0, -1926239.953681523 2865433.6989291757 0, -1926194.1290867266 2865409.05764377 0, -1926102.589071288 2865437.5118282633 0, -1926037.7249022147 2865457.6752195945 0)), ((-1920878.2998509065 2864462.17655 0, -1922316.4412968731 2864845.7317742375 0, -1921937.9880175826 2866328.2418175107 0, -1920493.8236914861 2865916.736179924 0, -1920878.2998509065 2864462.17655 0)), ((-1923905.1909504859 2866062.0840243534 0, -1923694.2456817098 2865994.054471567 0, -1923888.6471772937 2865271.213071534 0, -1924647.095419721 2865525.620003377 0, -1924553.537377164 2865901.4384199167 0, -1924430.9460681241 2865941.608395081 0, -1924323.7107533982 2865938.42827042 0, -1924230.5070588181 2866006.112174293 0, -1924104.4933114254 2866035.8790831277 0, -1924100.3231105062 2866036.8642222416 0, -1923905.1909504859 2866062.0840243534 0)), ((-1919701.1799191511 2865692.628450287 0, -1920493.8236914861 2865916.736179924 0, -1920282.5159418776 2866689.6695956476 0, -1920063.0392874023 2867437.0951254596 0, -1918519.0079381303 2867049.4514382277 0, -1918727.2580562208 2866291.9558586976 0, -1918935.992267362 2865493.9974696813 0, -1919701.1799191511 2865692.628450287 0)), ((-1920484.2790882466 2868891.2747279843 0, -1920457.821402454 2868892.4005715097 0, -1920423.629405119 2868893.855391192 0, -1920360.068046492 2868917.624331222 0, -1920298.8876387314 2868971.2923594313 0, -1920288.32324321 2868985.276912684 0, -1920253.0264786195 2869031.9994208585 0, -1920198.3077958673 2869072.7124186186 0, -1920172.056477208 2869092.2443947084 0, -1920070.8849752592 2869120.7112222956 0, -1920069.5049013162 2869120.347357614 0, -1919656.880719714 2869011.5518553834 0, -1920063.0392874023 2867437.0951254596 0, -1921505.7355209019 2867841.2034891616 0, -1921303.6114292133 2868629.609526721 0, -1920661.5235922271 2868452.082035754 0, -1920552.1579890763 2868882.1221683607 0, -1920551.1712253771 2868885.8993717683 0, -1920537.0033777482 2868887.4095733752 0, -1920516.0798756713 2868889.640050298 0, -1920511.680168411 2868890.1066194465 0, -1920484.2790882466 2868891.2747279843 0)), ((-1918281.6149233957 2869427.129881711 0, -1918180.6272271832 2869429.0710308147 0, -1918157.0973496847 2869429.5232212557 0, -1918121.4546746355 2869422.962137803 0, -1918109.0596553606 2869420.68110986 0, -1918105.0060209925 2869419.538707551 0, -1917882.2714684121 2869356.764865057 0, -1918095.5308712325 2868585.0459888475 0, -1918867.7827164773 2868791.986355689 0, -1918726.0367620673 2869308.9572289637 0, -1918725.9448960554 2869309.2774270247 0, -1918677.5162904623 2869380.159117461 0, -1918636.2236785386 2869440.596596778 0, -1918596.5901848478 2869421.0781514556 0, -1918460.091061805 2869423.70111539 0, -1918281.6149233957 2869427.129881711 0)), ((-1896662.1291620622 2805250.3423015014 0, -1896617.8490537708 2805417.656135391 0, -1896839.5872408089 2805526.699763196 0, -1896981.9109618014 2805599.2744929465 0, -1897118.6617120001 2805669.0071706297 0, -1897394.0270403055 2805732.1153340274 0, -1897405.6310079533 2805734.7171778316 0, -1897403.2774505315 2805741.8933131336 0, -1897160.6182358935 2805690.3540516123 0, -1896836.4849928634 2805560.3781644492 0, -1896796.3253876953 2805542.363626464 0, -1896664.9456934035 2805486.5652625123 0, -1896474.0382321659 2805390.3940137057 0, -1896027.2588527822 2805152.2507861634 0, -1895895.7028750055 2805075.2363432255 0, -1895897.5966885793 2805066.959958494 0, -1896037.0741669147 2805145.6315296795 0, -1896115.9962219296 2805170.8494562437 0, -1896252.7791996817 2805238.118718162 0, -1896253.7904080655 2805238.615882762 0, -1896257.1900887035 2805225.622883738 0, -1896278.2708206922 2805145.0768309115 0, -1896280.8100677126 2805145.7731968067 0, -1896662.1291620622 2805250.3423015014 0)), ((-1848363.6882150844 2809557.9256321383 0, -1847565.2008195755 2809347.35479946 0, -1847753.0180932435 2808570.847165622 0, -1848168.1485670605 2808679.627370943 0, -1848066.2456815925 2809060.0568930204 0, -1848467.2445381596 2809166.4507369203 0, -1848363.6882150844 2809557.9256321383 0)), ((-1855995.3764377357 2824711.132278971 0, -1856596.2530270615 2824860.499229959 0, -1856502.6217058415 2825243.653543744 0, -1855917.2237804504 2825098.7500604456 0, -1855902.085931869 2825094.751325446 0, -1855995.3764377357 2824711.132278971 0)), ((-1912910.4701252922 2825105.470172096 0, -1913690.2678639877 2825318.0513913846 0, -1913475.602772493 2826091.513492878 0, -1912695.934640716 2825879.9739590874 0, -1912910.4701252922 2825105.470172096 0)), ((-1911069.7715516498 2859288.2712812563 0, -1911118.0394319408 2859292.194786913 0, -1911148.3038582413 2859299.7011281266 0, -1911204.6475025443 2859323.4398436164 0, -1911433.145370624 2859457.0825968017 0, -1911475.0160240466 2859469.7359355534 0, -1911566.2282880305 2859484.6296004737 0, -1911624.1042513992 2859503.7192126443 0, -1911655.2056487277 2859524.9016695837 0, -1911672.238303252 2859550.3286137334 0, -1911693.0234700018 2859608.4402489266 0, -1911711.5377839655 2859633.0364471176 0, -1911787.3753059297 2859681.2531758402 0, -1911873.8105411069 2859711.941820578 0, -1912024.2322820295 2859744.469130588 0, -1912118.6433898045 2859778.4844851773 0, -1912533.2117745362 2859944.8979557194 0, -1913643.2050348504 2860347.8959560236 0, -1913527.9301741994 2860756.2311121295 0, -1915082.0788809326 2861183.9764312278 0, -1914655.1870602483 2862736.5331034884 0, -1913105.016828101 2862299.3443285665 0, -1913060.4700790537 2862471.6502935244 0, -1912992.565783229 2862453.340604565 0, -1913072.2428802666 2862365.9101331043 0, -1913086.8815983618 2862321.335075575 0, -1913093.0844607016 2862302.4471131875 0, -1913095.7141809722 2862294.442648306 0, -1913093.0009326101 2862222.036124531 0, -1913098.4926566228 2862078.558125645 0, -1913099.0955059526 2862062.8152301223 0, -1913026.3898837257 2862009.91471713 0, -1913014.0192889408 2861978.061959087 0, -1912974.4306614639 2861876.1249502343 0, -1912977.757394028 2861858.5793345035 0, -1912996.705049017 2861758.6463654567 0, -1913076.2420588923 2861721.586656786 0, -1913124.9517082511 2861698.8959120987 0, -1913139.4522744163 2861676.030208984 0, -1913223.418938074 2861543.628482523 0, -1913222.8707171988 2861534.6809602724 0, -1913221.1860840458 2861507.18803523 0, -1913214.856270181 2861403.8810550272 0, -1913207.2930252783 2861280.4406802733 0, -1913185.6124821394 2860926.5160575625 0, -1913157.2245225396 2860853.5992868417 0, -1913155.6716720276 2860849.6110518365 0, -1913125.3692025102 2860771.784262498 0, -1913131.7364428965 2860669.004731093 0, -1913131.782236189 2860668.72819048 0, -1913143.5723766568 2860477.931809763 0, -1913131.619344249 2860430.3780944976 0, -1913124.8165809885 2860403.3147919704 0, -1912941.4974071295 2860292.591562632 0, -1912833.3460024307 2860227.2493567374 0, -1912474.2022318812 2860010.26171056 0, -1912432.4013694355 2859985.0065007173 0, -1912356.966638263 2860217.7809732584 0, -1912335.8611494561 2860282.906388533 0, -1912390.8543641644 2860318.422930044 0, -1912504.0346987934 2860391.516893893 0, -1912597.268442078 2860512.76332725 0, -1912631.4741167298 2860526.0990556735 0, -1912663.9295307714 2860567.4074183432 0, -1912688.5321914845 2860613.0776181757 0, -1912718.59309723 2860651.3639282566 0, -1912718.9211642176 2860651.781943132 0, -1912752.8300348427 2860671.8267409485 0, -1912792.7016657135 2860715.319400522 0, -1912801.0621218358 2860751.8794533582 0, -1912802.8163927726 2860759.5508336276 0, -1912811.3612939587 2860771.9968697843 0, -1912860.9368616662 2860844.1748114796 0, -1912881.9719934592 2860850.586878815 0, -1912914.2566657045 2860887.3722070316 0, -1912951.5542474554 2860901.672441451 0, -1912997.136471682 2861061.497576031 0, -1912972.5083661168 2861121.6599827837 0, -1912976.572345268 2861168.462726313 0, -1912955.1807925128 2861213.557281548 0, -1912938.9904720702 2861247.6880313484 0, -1912914.4718112536 2861303.540262284 0, -1912900.9537771847 2861346.3993542246 0, -1912905.2138733114 2861372.9690812184 0, -1912885.3924334827 2861432.7661755173 0, -1912848.3822755567 2861450.0640992844 0, -1912807.5578270198 2861463.233480185 0, -1912779.958603024 2861482.7017999063 0, -1912706.106748129 2861489.606784551 0, -1912649.7560292801 2861492.86930673 0, -1912589.126544637 2861465.8263269123 0, -1912573.697175786 2861458.9442121834 0, -1912533.597625341 2861427.459699995 0, -1912509.6031612083 2861417.4320082692 0, -1912497.6881110407 2861412.4511158867 0, -1912435.0815359554 2861427.8055061647 0, -1912412.7539228862 2861448.3456075285 0, -1912370.034183779 2861438.8233540137 0, -1912300.3260759236 2861435.998505672 0, -1912283.3518890105 2861420.8285070877 0, -1912226.1528728916 2861434.1905212556 0, -1912214.300237075 2861436.959300874 0, -1912150.424289445 2861464.1960276156 0, -1912116.9846162822 2861465.5227756826 </t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>XL Ranch</t>
+          <t>Yakama</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>WA</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>School Lands</t>
+          <t>Common School and Indemnity, State Forest Transfer, Escheat, Scientific School, Community Forest Trust, Normal School, Natural Resources Conservation Area, Charitable/Educational/Penal &amp; Reformatory Instit., University - Transferred</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>2</v>
+        <v>304</v>
       </c>
       <c r="G77" t="n">
-        <v>62.54</v>
+        <v>46922.33</v>
       </c>
       <c r="H77" t="n">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="I77" t="n">
-        <v>62.54</v>
+        <v>44906.36</v>
       </c>
       <c r="J77" t="n">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="K77" t="n">
-        <v>125.08</v>
+        <v>91828.69</v>
       </c>
       <c r="L77" t="n">
-        <v>9807.360000000001</v>
+        <v>1376779.33</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t xml:space="preserve">MULTIPOLYGON Z (((-1947124.5557107623 2807295.7237508334 0, -1947196.7819263288 2807274.393608224 0, -1947193.1458702104 2807288.599900207 0, -1947059.5372636789 2807810.6141429264 0, -1946853.3734672957 2808596.0136770844 0, -1946745.5648815252 2808986.612934126 0, -1946341.8260397688 2808874.4829723123 0, -1945948.194095369 2808765.148187057 0, -1945556.2480824378 2808656.277029655 0, -1945447.281745532 2809049.883998759 0, -1945055.775332241 2808942.2476052986 0, -1944671.1240387606 2808836.5816436727 0, -1944285.9715556526 2808729.451306282 0, -1944182.7006740377 2808700.8373704124 0, -1944175.258183883 2808698.7751340363 0, -1944205.97409468 2808691.593999012 0, -1944239.832728101 2808683.6780427233 0, -1944297.1865183178 2808670.268832043 0, -1944326.1207686376 2808663.504190235 0, -1944341.9027250202 2808643.0757502136 0, -1944450.3186288457 2808502.7405995512 0, -1944484.6290076356 2808458.3283272255 0, -1944531.3559075892 2808450.5231368784 0, -1944533.2475823362 2808450.207102876 0, -1944742.3493571964 2808415.2779346644 0, -1944782.5304498996 2808408.56573509 0, -1944825.9314816992 2808401.315558442 0, -1944846.4419707358 2808397.889270128 0, -1944932.4650723806 2808383.518803587 0, -1945120.8879312954 2808352.0413803793 0, -1945232.340665698 2808300.193092651 0, -1945233.011146676 2808299.8811820387 0, -1945234.1767156126 2808299.338971333 0, -1945367.0666779706 2808239.105563168 0, -1945403.2525988873 2808189.1273322944 0, -1945406.8244306557 2808184.194092287 0, -1945434.3286187563 2808146.206466028 0, -1945452.2644826355 2808121.434357619 0, -1945517.6448988912 2808031.1333648274 0, -1945708.4753189383 2807935.2428929717 0, -1945743.469064124 2807917.658688479 0, -1945773.6058255532 2807875.803767459 0, -1945783.8263632155 2807861.609515513 0, -1945794.803288026 2807846.364457131 0, -1945805.1034344905 2807832.0591395595 0, -1945838.5799746306 2807785.5660434654 0, -1945999.7991482161 2807667.234313057 0, -1946006.4658096721 2807662.3410324776 0, -1946060.3811198939 2807650.8228329164 0, -1946249.9701467785 2807610.3188651903 0, -1946270.8384821936 2807605.860535518 0, -1946329.3806055868 2807593.353076714 0, -1946424.2470437514 2807573.08506474 0, -1946682.5545190827 2807536.241129031 0, -1946715.8717711887 2807531.488632948 0, -1946735.830111049 2807528.641718737 0, -1946811.206861308 2807517.889765267 0, -1946845.9224203727 2807472.3194938726 0, -1946907.4433662225 2807391.5624610432 0, -1946950.1763059627 2807335.467485209 0, -1946961.8711610327 2807337.088222957 0, -1947066.3557622277 2807351.5676600714 0, -1947124.5557107623 2807295.7237508334 0)), ((-1953386.7879867416 2809957.2616419047 0, -1953122.7670257601 2809888.019521383 0, -1953193.010530159 2809596.6558950776 0, -1953203.577075884 2809552.826982933 0, -1953281.4916945917 2809558.277206182 0, -1953292.17934746 2809749.786360986 0, -1953293.2236294863 2809768.4961081003 0, -1953296.9640707995 2809835.516895046 0, -1953482.0649389857 2809967.511132979 0, -1953484.7584606395 2809969.4318917906 0, -1953487.6914903347 2809983.723829882 0, -1953386.7879867416 2809957.2616419047 0)), ((-1946614.9078962246 2811885.370776785 0, -1946633.8647125496 2811896.64560381 0, -1946653.0110561145 2811912.1504938467 0, -1946684.166303763 2811937.3803751133 0, -1946689.2998346796 2811942.553062524 0, -1946690.5019310338 2811943.7641511704 0, -1946698.197141594 2811951.5179146877 0, -1946715.1627968417 2811971.3295670627 0, -1946730.0721239133 2811985.5084807114 0, -1946745.232731864 2811995.7451126017 0, -1946751.3168938763 2811998.816866132 0, -1946821.3437366372 2812034.169959289 0, -1946845.616608355 2812045.7422609036 0, -1946879.5990443504 2812061.9438724904 0, -1946879.8500397133 2812062.0636778786 0, -1946910.9144404363 2812076.8738750056 0, -1946947.7533411365 2812094.4371382394 0, -1947060.7872370374 2812153.652763408 0, -1947139.5149107124 2812191.1254910952 0, -1947153.044659055 2812194.2237642687 0, -1947176.9299978777 2812105.4381115045 0, -1947178.3598672908 2812088.189209279 0, -1947180.6096412572 2812076.401427918 0, -1947184.6021095074 2812055.484020593 0, -1947199.007831662 2811996.7596786823 0, -1947205.7505111548 2811998.307882489 0, -1947601.865979837 2812089.2656746367 0, -1947161.8444363042 2813724.908500826 0, -1947938.7742716009 2813946.868101684 0, -1948716.0669331742 2814153.7326147486 0, -1948508.1692716295 2814936.5808169744 0, -1948296.06130565 2815711.6417853036 0, -1948085.8615166286 2816490.051731219 0, -1947887.1532080339 2817263.7317802105 0, -1947110.1819699025 2817045.1674422114 0, -1946333.2349266736 2816826.5353467013 0, -1946536.5120191795 2816052.253474633 0, -1946743.038038953 2815275.9633118263 0, -1945965.8537946267 2815058.6734601483 0, -1945187.38250786 2814847.511176291 0, -1945390.6584151017 2814070.8353690077 0, -1945593.9390024608 2813294.1439373647 0, -1945806.4183397717 2812512.0426953356 0, -1946017.4099203725 2811725.407987297 0, -1946413.5226287036 2811816.379077322 0, -1946413.1175892442 2811817.8873744495 0, -1946429.5205681976 2811823.0182974017 0, -1946430.5705775602 2811823.3468920225 0, -1946441.4127719733 2811826.7384116566 0, -1946460.0693028378 2811832.573924255 0, -1946546.4250696348 2811858.060609156 0, -1946584.401309241 2811872.0030026874 0, -1946614.9078962246 2811885.370776785 0)), ((-1948900.588521401 2813349.774017343 0, -1948809.1497083865 2813748.171309886 0, -1948240.7924339913 2813580.0435008793 0, -1948345.2341088098 2813173.972558003 0, -1948900.588521401 2813349.774017343 0)), ((-1952221.214135054 2813417.0188169414 0, -1952606.9522442534 2813525.2989367954 0, -1952609.412323701 2813525.9894720893 0, -1952608.7617625473 2813528.576734444 0, -1952521.005898842 2813877.601366205 0, -1952461.1719096894 2813882.468296462 0, -1952404.91447361 2813887.0441548065 0, -1952125.3607299807 2813809.319979971 0, -1952221.214135054 2813417.0188169414 0)), ((-1951109.403211928 2817706.2222447176 0, -1950981.9253401442 2817755.7212553616 0, -1950915.0461234644 2817781.5329516055 0, -1950878.459851005 2817795.653069836 0, -1950813.5889805139 2817754.9988670424 0, -1950714.747913343 2817693.0551435365 0, -1950696.3781159038 2817681.5429214216 0, -1950634.842756184 2817642.978246047 0, -1950475.0732963716 2817794.2712869965 0, -1950350.9850651731 2817911.774685636 0, -1950229.4130995688 2817877.218136361 0, -1949459.3219813337 2817655.629660831 0, -1949675.1280854722 2816881.8744489173 0, -1949882.0230697875 2816121.976450482 0, -1951048.5181664268 2816443.4519810094 0, -1951135.8725615966 2816045.698412492 0, -1951397.6412383653 2816122.326121462 0, -1951398.2366670764 2816140.6499513793 0, -1951429.1657775978 2816344.5042031966 0, -1951458.0132103665 2816395.444446804 0, -1951458.6854130586 2816396.631445679 0, -1951419.2681869979 2816543.478137624 0, -1951245.4248171826 2817266.2006058693 0, -1951115.3352282133 2817703.9188853893 0, -1951109.403211928 2817706.2222447176 0)), ((-1948800.0774710595 2820079.056871323 0, -1948755.4657172174 2820088.8711917084 0, -1948729.7918133228 2820094.519223721 0, -1948749.6901557706 2819981.7351393187 0, -1949029.2966877047 2819219.0309122363 0, -1949216.1317151315 2819267.1190779125 0, -1949122.1522565759 2819352.187155631 0, -1949068.056106266 2819432.4726366717 0, -1949023.0329906945 2819505.4548712545 0, -1949044.0199872083 2819623.3749157335 0, -1949075.2662473642 2819798.93361861 0, -1948965.0742484073 2819994.7351705506 0, -1948901.8355726646 2820027.0534498193 0, -1948800.0774710595 2820079.056871323 0)), ((-1947711.056209912 2823037.388546394 0, -1947710.3908040728 2823052.360373251 0, -1947703.6130837516 2823204.87018648 0, -1947635.7493479564 2823448.7215245077 0, -1947632.6231846497 2823459.954442923 0, -1947651.3765163652 2823799.3043881706 0, -1947622.273734997 2823892.2555906605 0, -1947617.236901387 2823908.3427039455 0, -1947519.7118047255 2824219.8324208586 0, -1947474.1677948614 2824286.46855595 0, -1947457.4749831655 2824310.895477439 0, -1947392.8850046801 2824501.2802619715 0, -1947285.5751249949 2824652.8274717364 0, -1947282.93064712 2824656.5636720136 0, -1947144.512593157 2824804.2110868483 0, -1947222.884602449 2824860.459899903 0, -1947266.2238187243 2824978.8393854517 0, -1947343.8223486969 2824953.2193777794 0, -1947334.0825702942 2825080.905190541 0, -1947321.0618002464 2825251.6351106544 0, -1947253.1551944956 2825475.1227064123 0, -1947248.8139849745 2825482.088473379 0, -1946516.2152451943 2825292.499795915 0, -1945735.8521312105 2825090.6417997656 0, -1945524.0930363676 2825864.6570646428 0, -1945314.7721398615 2826639.52506426 0, -1945088.7128367843 2827410.705539773 0, -1944876.2513827144 2828185.515469902 0, -1944086.5716233156 2827974.060117378 0, -1943708.4311984438 2827856.921258917 0, -1943313.7750874953 2827749.8342451244 0, -1942552.8778908548 2827565.478069011 0, -1942433.8878418936 2827952.8691948676 0, -1942115.2148576651 2829110.296337552 0, -1941740.247006324 2829021.677830297 0, -1941364.8913283464 2828934.2149304776 0, -1940614.4885814935 2828717.4324106015 0, -1940380.7262877997 2829491.0634633354 0, -1941157.3486816953 2829714.164489239 0, -1940962.5406810332 2830480.7188912537 0, -1942461.70950291 2830885.848456556 0, -1942692.6805440595 2830137.7557435655 0, -1942793.6901436509 2829709.63596787 0, -1942894.7014358174 2829281.5114808935 0, -1943664.6776832102 2829494.2014161125 0, -1944444.5162852963 2829727.3526395317 0, -1944240.9796830066 2830537.874774691 0, -1944046.067697474 2831315.9714416503 0, -1943848.50376597 2832102.6996421823 0, -1943743.83154259 2832479.2347885496 0, -1943644.3767330595 2832837.0025605005 0, -1943581.2039236382 2832819.7384977685 0, -1942869.1977661247 2832625.1609020308 0, -1942803.9323556963 2832608.7278774576 0, -1942095.9751251442 2832430.4740522504 0, -1942023.432910939 2832411.589677251 0, -1941320.4345445875 2832228.5872334125 0, -1941241.4812423058 2832213.40905601 0, -1940518.8604381077 2832067.5301795797 0, -1940427.6025438693 2832041.979955196 0, -1939719.1298166327 2831844.149645808 0, -1939650.2813025315 2831823.7800045474 0, -1939008.2927350795 2831633.9075519615 0, -1938937.8182702172 2831612.9978779657 0, -1938875.459023381 2831595.8261597687 0, -1938155.5847200237 2831397.7635465516 0, -1938098.1574108254 2831382.171489841 0, -1937367.725195407 2831183.8592544473 0, -1937319.7935790198 2831170.7466271804 0, -1936592.1479990568 2830970.5633796058 0, -1936551.782240904 2830958.459755302 0, -1935919.8841535791 2830768.979581447 0, -1935853.7424633587 2830666.800432577 0, -1936043.9285566418 2829974.059544721 0, -1936145.9669096095 2829606.0232871436 0, -1936248.0642732342 2829237.7809193237 0, -1936459.6332089452 2828420.087475266 0, -1936671.1932913214 2827602.744161404 0, -1935901.1673248971 2827404.963971848 0, -1935131.6484503855 2827207.345645183 0, -1934737.3642994917 2827104.054830973 0, -1934342.5261924486 2827000.6324797366 0, -1933553.2220813956 2826793.841596687 0, -1933761.5091981522 2826019.775546707 0, -1933975.9384614483 2825234.8236955265 0, -1933583.8297440552 2825126.270168573 0, -1933192.1269479976 2825017.8277554675 0, -1933406.247326265 2824251.320284405 0, -1933484.1597564383 2824270.6364715467 0, -1933560.93079583 2824065.5594003047 0, -1933557.1777476843 2823669.876861863 0, -1933632.168574466 2823445.1023491654 0, -1933233.0538895007 2823344.3789825863 0, -1932833.940247076 2823243.6511097113 0, -1932372.995906775 2823117.950424193 0, -1932730.2121003186 2821547.4664698183 0, -1933252.3690630475 2820001.953830233 0, -1932875.059471353 2819895.6085127 0, -1932120.5151176807 2819683.5672394563 0, -1930577.5733440355 2819261.3804175365 0, -1929696.1913390842 2819055.4839692526 0, -1929845.6354374762 2818625.467116351 0, -1929872.7544179265 2818547.434736694 0, -1929874.57124737 2818542.207133 0, -1929880.1351356034 2818526.1975715207 0, -1929881.7522122038 2818521.5443381337 0, -1929983.0851736646 2818229.966494045 0, -1929619.2157681047 2818130.8872940643 0, -1929736.580766636 2817750.492223993 0, -1929360.2837025973 2817657.226028599 0, -1929354.5875267424 2817678.947000758 0, -1929353.228261422 2817684.129774841 0, -1929341.3386348058 2817729.4691167814 0, -1929339.8485104665 2817735.151194868 0, -1929337.815666145 2817742.9028611216 0, -1929255.3412267803 2818031.826646187 0, -1928918.8246952381 2818810.952408313 0, -1928122.7990207672 2818594.244171984 0, -1928024.642395889 2818569.0576784485 0, -1927630.2863546014 2817947.253782771 0, -1927551.1817190184 2817823.047702654 0, -1927201.5305156272 2817274.0244157608 0, -1927013.8005473418 2816985.972721535 0, -1927170.6971796076 2816600.8326979834 0, -1927186.888627717 2816605.135812899 0, -1927955.1064756506 2816810.1267357282 0, -1928062.8644512328 2816410.767847923 0, -1928170.6236448651 2816011.404500228 0, -1928170.6519277014 2816011.3002163935 0, -1928335.5725609951 2816060.678830224 0, -1928340.479160045 2816062.14773463 0, -1928358.8299043912 2816067.6420136616 0, -1928363.9512381542 2816069.1753942226 0, -1928547.897408099 2816124.249284745 0, -1928652.450982854 2815747.538075545 0, -1928287.6432609076 2815609.2405163767 0, -1928283.2752051004 2815607.584605435 0, -1928279.9276287449 2815606.3154997323 0, -1928283.612778869 2815594.6022822983 0, -1928288.215822168 2815577.514176424 0, -1928388.6672126406 2815203.3196104844 0, -1928756.3313858095 2815373.2517059958 0, -1929123.7263016994 2815543.083117765 0, -1929897.3229792737 2815749.610247387 0, -1929707.9124916464 2816449.4440081026 0, -1929470.2812261013 2817237.773556349 0, -1929860.56049845 2817348.6562962593 0, -1930250.833378816 2817459.560403357 0, -1930641.143404357 2817570.4991767206 0, -1931031.4472574294 2817681.459688435 0, -1931805.2503211931 2817905.5667042457 0, -1932594.1915322812 2818127.825577896 0, -1932811.8928143983 2817356.7666764436 0, -1933022.8681155671 2816578.4116334063 0, -1933795.9299697948 2816792.540353066 0, -1934163.8246629832 2816898.246070321 0, -1934550.1172213496 2817009.2331912736 0, -1934334.2296709986 2817788.790593405 0, -1934108.049074308 2818561.261530009 0, -1934909.250632951 2818782.6145231696 0, -1935116.7927075562 2818006.531720954 0, -1935916.8198173607 2818229.1149338917 0, -1936676.3996078675 2818437.897329563 0, -1936462.9739085813 2819219.5778062106 0, -1936353.5000564817 2819609.4351670644 0, -1936243.9917860483 2819999.2792242086 0, -1936632.7686874776 2820105.6482482827 0, -1937021.5500128125 2820212.013846692 0, -1937413.318937494 2820320.6705608866 0, -1937805.0901551058 2820429.3200657633 0, -1937698.353795431 2820820.401979242 0, -1937592.4233251668 2821208.550592578 0, -1937985.3208603768 2821315.5024794503 0, -1937786.438834566 2822105.703372242 0, -1937572.007178126 2822882.830218352 0, -1937947.7030090205 2822971.5158543093 0, -1938378.049721953 2821422.3454312244 0, -1938770.257508245 2821532.227865583 0, -1938981.1579699456 2820755.2587466994 0, -1938588.1487450716 2820646.4371728147 0, -1938799.1743406628 2819864.585701209 0, -1939022.6444431625 2819088.687467256 0, -1939242.4706204562 2818309.8925407636 0, -1939462.8863154226 2817539.1384911337 0, -1939684.5868446275 2816755.1590106944 0, -1940481.046967366 2816953.4827664336 0, -1941277.4698106893 2817151.7884277906 0, -1941666.9750141355 2817255.678148611 0, -1942056.4813348188 2817359.563572374 0, -1942799.6122432877 2817584.255998529 0, -1942579.2484212103 2818370.2245898014 0, -1942358.8900397797 2819156.175726435 0, -1942255.0990678044 2819547.3025721707 0, -1942151.236367304 2819938.450738095 0, -1942043.4314071736 2820328.0719141285 0, -1941935.5920665667 2820717.6798253707 0, -1943517.0213170212 2821089.9273377797 0, -1943289.8592308573 2821862.5371859185 0, -1943073.3554806781 2822728.562133121 0, -1943834.9354735375 2822914.7426675498 0, -1944612.9373131827 2823120.186971993 0, -1945390.9473912406 2823325.61012788 0, -1945779.9519991863 2823428.3177299947 0, -1946168.9579114623 2823531.02142024 0, -1946284.3938566889 2823110.445017022 0, -1946397.9609839355 2822700.6624759194 0, -1947185.9908282983 2822901.5805788804 0, -1947711.056209912 2823037.388546394 0), (-1934758.975706155 2825446.512897815 0, -1934653.0218455815 2825841.932409918 0, -1935043.4589296302 2825948.790364581 0, -1935150.4415958782 2825552.3993304996 0, -1935541.7468236985 2825658.256978833 0, -1935646.7138191978 2825263.1583201904 0, -1936029.8489498126 2825363.6139364857 0, -1936413.00537298 2825464.090523153 0, -1936487.7773941478 2825192.6720164535 0, -1936433.7728069306 2825054.5628216825 0, -1936135.5340307557 2824973.1069335695 0, -1936245.3051296428 2824573.794055444 0, -1935862.1415192464 2824473.3424840486 0, -1935969.817728062 2824082.0210779584 0, -1936084.9942129245 2823647.682375033 0, -1936174.577011313 2823309.8599834703 0, -1935399.411184608 2823094.9130661804 0, -1935501.0654255731 2822711.01071649 0, -1935124.0544510153 2822606.820595831 0, -1934963.3254915304 2822562.4005034817 0, -1934958.4332583307 2822369.333828692 0, -1934828.3273453016 2822114.356937905 0, -1934728.9298708765 2822497.6198299667 0, -1934629.6000918266 2822880.6597541803 0, -1934467.1727870738 2822838.0632362305 0, -1934237.4196847486 2822777.8091885406 0, -1934031.2843016037 2823545.8212093497 0, -1933917.7880985364 2823517.1802627076 0, -1933790.0503903565 2823747.4732142584 0, -1933761.194117387 2824123.826363364 0, -1933680.13984651 2824319.2227905844 0, -1934217.7233894903 2824452.4925112473 0, -1933975.9384614483 2825234.8236955265 0, -1934758.975706155 2825446.512897815 0), (-1939585.1471896607 2829261.4028389654 0, -1939818.2940440194 2828487.400401368 0, -1938649.617593449 2828181.742712182 0, -1938258.7925312018 2828077.720105118 0, -1938143.3234812513 2828440.935519226 0, -1938027.8552433995 2828804.146640231 0, -1937825.555195848 2829570.0810287166 0, -1939374.8838128757 2829997.759182874 0, -1939585.1471896607 2829261.4028389654 0), (-1930920.3377759478 2818068.226708838 0, -1930518.6474033971 2817956.4985622237 0, -1930396.1606221455 2818342.4661825285 0, -1930766.5858791282 2818443.3733610176 0, -1930776.1682660037 2818445.983636517 0, -1930809.2299065518 2818454.9896017592 0, -1930813.003602764 2818441.853874067 0, -1930814.3485153364 2818437.1717314213 0, -1930920.3377759478 2818068.226708838 0), (-1930255.115148408 2817883.195627018 0, -1930236.724376213 2817878.080051084 0, -1930012.3089755394 2818237.925762199 0, -1930030.7570267974 2818242.950074561 0, -1930255.115148408 2817883.195627018 0)), ((-1941975.4751981073 2808840.0696086613 0, -1941997.1538114115 2808836.4567134576 0, -1942073.5637378213 2808823.722606744 0, -1942131.7629030917 2808808.992433286 0, -1942208.4989129088 2808789.57058315 0, -1942416.180367779 2808737.0050345478 0, -1942455.87754672 2808717.4955143197 0, -1942544.9733916684 2808673.708611994 0, -1942610.5539401006 2808641.478167417 0, -1942620.1244321063 2808636.774620107 0, -1942663.400072895 2808615.5060951007 0, -1942753.6674295608 2808571.1424578154 0, -1942869.51606919 2808688.9877995523 0, -1942888.4225879675 2808708.219790584 0, -1942889.654890738 2808709.4734285926 0, -1942895.2061948585 2808710.0261795996 0, -1943049.4737258072 2808725.3855749154 0, -1943082.0811213637 2808728.6318694507 0, -1943105.6422018444 2808759.283847976 0, -1943160.5267339058 2808830.685657026 0, -1943205.0386135392 2808888.592700042 0, -1943276.3573062862 2809003.8482864983 0, -1943377.1216596877 2809067.6060874094 0, -1943381.3177654438 2809070.2610881724 0, -1943377.6567924723 2809086.5898198485 0, -1943328.4432893663 2809306.0939921406 0, -1942477.1866891305 2809087.429074342 0, -1941793.930382525 2808892.4903800027 0, -1941789.0354423348 2808891.0937741525 0, -1941800.329167384 2808887.565882612 0, -1941827.8367050479 2808878.973043119 0, -1941869.040369248 2808866.101807077 0, -1941925.9578423577 2808848.3217931706 0, -1941933.5939346517 2808847.0492320075 0, -1941975.4751981073 2808840.0696086613 0)), ((-1944058.723598079 2816226.208026141 0, -1943942.488938613 2816616.768198294 0, -1943547.2736266737 2816516.6943910923 0, -1943663.3560512534 2816121.164155373 0, -1944058.723598079 2816226.208026141 0)), ((-1943034.0998549613 2816804.0528895273 0, -1943429.9347577845 2816916.434716266 0, -1943190.0135548415 2817682.717167016 0, -1942799.6122432877 2817584.255998529 0, -1943034.0998549613 2816804.0528895273 0)), ((-1943581.524175765 2817781.7749560145 0, -1943822.2347943233 2817004.9033741523 0, -1944560.3858638655 2817171.3886290533 0, -1944344.9823447221 2817974.9235633775 0, -1943581.524175765 2817781.7749560145 0)), ((-1936153.4484906516 2811585.839009829 0, -1936174.945166137 2811575.6432904634 0, -1936331.8753854744 2811520.53820495 0, -1936485.3815387331 2811478.6248240764 0, -1936535.956110518 2811464.8157760906 0, -1936570.6387233243 2811455.3457541857 0, -1936691.344574958 2811344.07207154 0, -1936797.7922188782 2811318.367799899 0, -1936864.795513821 2811302.187914356 0, -1936932.0140674335 2811261.923055901 0, -1936967.2226207997 2811240.832516306 0, -1936988.2531909542 2811228.234803959 0, -1937110.3845130322 2811121.5474925996 0, -1937331.5234054446 2811029.662503699 0, -1937825.614099507 2811136.749395092 0, -1937626.9716735017 2811921.5246444508 0, -1937428.2562024964 2812706.7988925623 0, -1936631.9254041116 2812517.482568833 0, -1935835.3500741445 2812328.5873463713 0, -1936019.0369716408 2811654.632357626 0, -1936020.6140379785 2811648.8460765434 0, -1936023.788997826 2811647.3343533343 0, -1936153.4484906516 2811585.839009829 0)), ((-1934629.6000918266 2822880.6597541803 0, -1935014.5051893676 2822987.7885432597 0, -1934920.3375659534 2823381.8329619314 0, -1934530.000007294 2823263.5995747233 0, -1934629.6000918266 2822880.6597541803 0)), ((-1928802.6239436434 2813711.292642901 0, -1928695.4713545218 2814099.5714198337 0, -1928588.319572293 2814487.8458844405 0, -1928486.0163505543 2814883.946014951 0, -1928047.7060741284 2814765.1291601956 0, -1928169.909786337 2814374.937847502 0, -1928291.2333748734 2813991.870427505 0, -1928411.9188028697 2813610.815898007 0, -1928802.6239436434 2813711.292642901 0)), ((-1930344.3252405708 2814131.2391046174 0, -1931145.4264724182 2814216.068519604 0, -1931897.6967454187 2814520.078997948 0, -1931677.669010281 2815348.565582413 0, -1931455.9990515015 2816177.889569845 0, -1930679.8917686564 2815963.721800876 0, -1929897.3229792737 2815749.610247387 0, -1930101.4035317835 2814982.196513081 0, -1930344.3252405708 2814131.2391046174 0), (-1931176.4831238952 2815664.0622126306 0, -1931285.0219405617 2815257.3089883183 0, -1930496.8888091063 2815074.1259574196 0, -1930392.7472309952 2815465.399057443 0, -1930786.1327697122 2815564.888445243 0, -1931176.4831238952 2815664.0622126306 0)), ((-1932625.004395147 2824019.372009379 0, -1933015.4430826395 2824135.5915850047 0, -1932800.8537718498 2824906.077624436 0, -1932409.581895042 2824794.323167323 0, -1932625.004395147 2824019.372009379 0)), ((-1920878.2998509065 2864462.17655 0, -1919339.6526715388 2863911.015689175 0, -1919499.2762970189 2863216.3909553443 0, -1919730.7560771785 2862646.1294262023 0, -1921234.9285229577 2863201.991168637 0, -1920878.2998509065 2864462.17655 0)), ((-1922638.7562835668 2863745.317361907 0, -1924153.195741897 2864306.7299528057 0, -1923888.6471772937 2865271.213071534 0, -1922316.4412968731 2864845.7317742375 0, -1922638.7562835668 2863745.317361907 0)), ((-1926037.7249022147 2865457.6752195945 0, -1926036.5113501642 2865458.052518688 0, -1925975.9532681934 2865453.9122872567 0, -1925930.7511069255 2865465.3310377323 0, -1925799.5858269983 2865498.4620929626 0, -1925670.3957903862 2865546.158560157 0, -1925466.1884740398 2865642.7213355713 0, -1925454.2712138693 2865648.3563584513 0, -1925407.9209830656 2865656.2345184283 0, -1925416.9028312895 2865626.803323347 0, -1925647.9816289446 2864883.8372634226 0, -1926426.6688185155 2865162.56099678 0, -1926346.923875304 2865447.8805387504 0, -1926344.6599197036 2865455.9786466183 0, -1926286.1722074042 2865450.0294201733 0, -1926239.953681523 2865433.6989291757 0, -1926194.1290867266 2865409.05764377 0, -1926102.589071288 2865437.5118282633 0, -1926037.7249022147 2865457.6752195945 0)), ((-1920878.2998509065 2864462.17655 0, -1922316.4412968731 2864845.7317742375 0, -1921937.9880175826 2866328.2418175107 0, -1920493.8236914861 2865916.736179924 0, -1920878.2998509065 2864462.17655 0)), ((-1923905.1909504859 2866062.0840243534 0, -1923694.2456817098 2865994.054471567 0, -1923888.6471772937 2865271.213071534 0, -1924647.095419721 2865525.620003377 0, -1924553.537377164 2865901.4384199167 0, -1924430.9460681241 2865941.608395081 0, -1924323.7107533982 2865938.42827042 0, -1924230.5070588181 2866006.112174293 0, -1924104.4933114254 2866035.8790831277 0, -1924100.3231105062 2866036.8642222416 0, -1923905.1909504859 2866062.0840243534 0)), ((-1919701.1799191511 2865692.628450287 0, -1920493.8236914861 2865916.736179924 0, -1920282.5159418776 2866689.6695956476 0, -1920063.0392874023 2867437.0951254596 0, -1918519.0079381303 2867049.4514382277 0, -1918727.2580562208 2866291.9558586976 0, -1918935.992267362 2865493.9974696813 0, -1919701.1799191511 2865692.628450287 0)), ((-1920484.2790882466 2868891.2747279843 0, -1920457.821402454 2868892.4005715097 0, -1920423.629405119 2868893.855391192 0, -1920360.068046492 2868917.624331222 0, -1920298.8876387314 2868971.2923594313 0, -1920288.32324321 2868985.276912684 0, -1920253.0264786195 2869031.9994208585 0, -1920198.3077958673 2869072.7124186186 0, -1920172.056477208 2869092.2443947084 0, -1920070.8849752592 2869120.7112222956 0, -1920069.5049013162 2869120.347357614 0, -1919656.880719714 2869011.5518553834 0, -1920063.0392874023 2867437.0951254596 0, -1921505.7355209019 2867841.2034891616 0, -1921303.6114292133 2868629.609526721 0, -1920661.5235922271 2868452.082035754 0, -1920552.1579890763 2868882.1221683607 0, -1920551.1712253771 2868885.8993717683 0, -1920537.0033777482 2868887.4095733752 0, -1920516.0798756713 2868889.640050298 0, -1920511.680168411 2868890.1066194465 0, -1920484.2790882466 2868891.2747279843 0)), ((-1918281.6149233957 2869427.129881711 0, -1918180.6272271832 2869429.0710308147 0, -1918157.0973496847 2869429.5232212557 0, -1918121.4546746355 2869422.962137803 0, -1918109.0596553606 2869420.68110986 0, -1918105.0060209925 2869419.538707551 0, -1917882.2714684121 2869356.764865057 0, -1918095.5308712325 2868585.0459888475 0, -1918867.7827164773 2868791.986355689 0, -1918726.0367620673 2869308.9572289637 0, -1918725.9448960554 2869309.2774270247 0, -1918677.5162904623 2869380.159117461 0, -1918636.2236785386 2869440.596596778 0, -1918596.5901848478 2869421.0781514556 0, -1918460.091061805 2869423.70111539 0, -1918281.6149233957 2869427.129881711 0)), ((-1896662.1291620622 2805250.3423015014 0, -1896617.8490537708 2805417.656135391 0, -1896839.5872408089 2805526.699763196 0, -1896981.9109618014 2805599.2744929465 0, -1897118.6617120001 2805669.0071706297 0, -1897394.0270403055 2805732.1153340274 0, -1897405.6310079533 2805734.7171778316 0, -1897403.2774505315 2805741.8933131336 0, -1897160.6182358935 2805690.3540516123 0, -1896836.4849928634 2805560.3781644492 0, -1896796.3253876953 2805542.363626464 0, -1896664.9456934035 2805486.5652625123 0, -1896474.0382321659 2805390.3940137057 0, -1896027.2588527822 2805152.2507861634 0, -1895895.7028750055 2805075.2363432255 0, -1895897.5966885793 2805066.959958494 0, -1896037.0741669147 2805145.6315296795 0, -1896115.9962219296 2805170.8494562437 0, -1896252.7791996817 2805238.118718162 0, -1896253.7904080655 2805238.615882762 0, -1896257.1900887035 2805225.622883738 0, -1896278.2708206922 2805145.0768309115 0, -1896280.8100677126 2805145.7731968067 0, -1896662.1291620622 2805250.3423015014 0)), ((-1848363.6882150844 2809557.9256321383 0, -1847565.2008195755 2809347.35479946 0, -1847753.0180932435 2808570.847165622 0, -1848168.1485670605 2808679.627370943 0, -1848066.2456815925 2809060.0568930204 0, -1848467.2445381596 2809166.4507369203 0, -1848363.6882150844 2809557.9256321383 0)), ((-1855995.3764377357 2824711.132278971 0, -1856596.2530270615 2824860.499229959 0, -1856502.6217058415 2825243.653543744 0, -1855917.2237804504 2825098.7500604456 0, -1855902.085931869 2825094.751325446 0, -1855995.3764377357 2824711.132278971 0)), ((-1912910.4701252922 2825105.470172096 0, -1913690.2678639877 2825318.0513913846 0, -1913475.602772493 2826091.513492878 0, -1912695.934640716 2825879.9739590874 0, -1912910.4701252922 2825105.470172096 0)), ((-1911069.7715516498 2859288.2712812563 0, -1911118.0394319408 2859292.194786913 0, -1911148.3038582413 2859299.7011281266 0, -1911204.6475025443 2859323.4398436164 0, -1911433.145370624 2859457.0825968017 0, -1911475.0160240466 2859469.7359355534 0, -1911566.2282880305 2859484.6296004737 0, -1911624.1042513992 2859503.7192126443 0, -1911655.2056487277 2859524.9016695837 0, -1911672.238303252 2859550.3286137334 0, -1911693.0234700018 2859608.4402489266 0, -1911711.5377839655 2859633.0364471176 0, -1911787.3753059297 2859681.2531758402 0, -1911873.8105411069 2859711.941820578 0, -1912024.2322820295 2859744.469130588 0, -1912118.6433898045 2859778.4844851773 0, -1912533.2117745362 2859944.8979557194 0, -1913643.2050348504 2860347.8959560236 0, -1913527.9301741994 2860756.2311121295 0, -1915082.0788809326 2861183.9764312278 0, -1914655.1870602483 2862736.5331034884 0, -1913105.016828101 2862299.3443285665 0, -1913060.4700790537 2862471.6502935244 0, -1912992.565783229 2862453.340604565 0, -1913072.2428802666 2862365.9101331043 0, -1913086.8815983618 2862321.335075575 0, -1913093.0844607016 2862302.4471131875 0, -1913095.7141809722 2862294.442648306 0, -1913093.0009326101 2862222.036124531 0, -1913098.4926566228 2862078.558125645 0, -1913099.0955059526 2862062.8152301223 0, -1913026.3898837257 2862009.91471713 0, -1913014.0192889408 2861978.061959087 0, -1912974.4306614639 2861876.1249502343 0, -1912977.757394028 2861858.5793345035 0, -1912996.705049017 2861758.6463654567 0, -1913076.2420588923 2861721.586656786 0, -1913124.9517082511 2861698.8959120987 0, -1913139.4522744163 2861676.030208984 0, -1913223.418938074 2861543.628482523 0, -1913222.8707171988 2861534.6809602724 0, -1913221.1860840458 2861507.18803523 0, -1913214.856270181 2861403.8810550272 0, -1913207.2930252783 2861280.4406802733 0, -1913185.6124821394 2860926.5160575625 0, -1913157.2245225396 2860853.5992868417 0, -1913155.6716720276 2860849.6110518365 0, -1913125.3692025102 2860771.784262498 0, -1913131.7364428965 2860669.004731093 0, -1913131.782236189 2860668.72819048 0, -1913143.5723766568 2860477.931809763 0, -1913131.619344249 2860430.3780944976 0, -1913124.8165809885 2860403.3147919704 0, -1912941.4974071295 2860292.591562632 0, -1912833.3460024307 2860227.2493567374 0, -1912474.2022318812 2860010.26171056 0, -1912432.4013694355 2859985.0065007173 0, -1912356.966638263 2860217.7809732584 0, -1912335.8611494561 2860282.906388533 0, -1912390.8543641644 2860318.422930044 0, -1912504.0346987934 2860391.516893893 0, -1912597.268442078 2860512.76332725 0, -1912631.4741167298 2860526.0990556735 0, -1912663.9295307714 2860567.4074183432 0, -1912688.5321914845 2860613.0776181757 0, -1912718.59309723 2860651.3639282566 0, -1912718.9211642176 2860651.781943132 0, -1912752.8300348427 2860671.8267409485 0, -1912792.7016657135 2860715.319400522 0, -1912801.0621218358 2860751.8794533582 0, -1912802.8163927726 2860759.5508336276 0, -1912811.3612939587 2860771.9968697843 0, -1912860.9368616662 2860844.1748114796 0, -1912881.9719934592 2860850.586878815 0, -1912914.2566657045 2860887.3722070316 0, -1912951.5542474554 2860901.672441451 0, -1912997.136471682 2861061.497576031 0, -1912972.5083661168 2861121.6599827837 0, -1912976.572345268 2861168.462726313 0, -1912955.1807925128 2861213.557281548 0, -1912938.9904720702 2861247.6880313484 0, -1912914.4718112536 2861303.540262284 0, -1912900.9537771847 2861346.3993542246 0, -1912905.2138733114 2861372.9690812184 0, -1912885.3924334827 2861432.7661755173 0, -1912848.3822755567 2861450.0640992844 0, -1912807.5578270198 2861463.233480185 0, -1912779.958603024 2861482.7017999063 0, -1912706.106748129 2861489.606784551 0, -1912649.7560292801 2861492.86930673 0, -1912589.126544637 2861465.8263269123 0, -1912573.697175786 2861458.9442121834 0, -1912533.597625341 2861427.459699995 0, -1912509.6031612083 2861417.4320082692 0, -1912497.6881110407 2861412.4511158867 0, -1912435.0815359554 2861427.8055061647 0, -1912412.7539228862 2861448.3456075285 0, -1912370.034183779 2861438.8233540137 0, -1912300.3260759236 2861435.998505672 0, -1912283.3518890105 2861420.8285070877 0, -1912226.1528728916 2861434.1905212556 0, -1912214.300237075 2861436.959300874 0, -1912150.424289445 2861464.1960276156 0, -1912116.9846162822 2861465.5227756826 </t>
+          <t>MULTIPOLYGON Z (((-201157.89714606619 2226817.235233947 0, -201150.4477368668 2227219.438475946 0, -200753.3026580403 2227209.6763946763 0, -200761.2634767131 2226807.28490224 0, -200769.14780959437 2226405.0503807156 0, -200774.72665332502 2226003.684905638 0, -200780.4616888446 2225601.4149824106 0, -201173.2890220301 2225612.9101912207 0, -201169.26346164412 2226014.247476004 0, -201165.3147526024 2226415.1188031007 0, -201157.89714606619 2226817.235233947 0)), ((-200676.61833697834 2245072.9570895853 0, -200665.50219727602 2245477.002334861 0, -200654.41287032556 2245882.0017014216 0, -200253.06813058004 2245868.06750964 0, -200264.80304160324 2245464.127465126 0, -200276.0542363167 2245060.042299942 0, -200676.61833697834 2245072.9570895853 0)), ((-195578.19880497677 2240443.3940137667 0, -195588.7887579272 2240039.0023805574 0, -195990.64187128432 2240050.3519468727 0, -195979.83454412993 2240455.3803870333 0, -195969.04419966493 2240859.482109948 0, -195567.5232243485 2240846.6419790983 0, -195578.19880497677 2240443.3940137667 0)), ((-195094.1654991865 2243651.0130477655 0, -195495.08877752116 2243663.273893927 0, -195484.58355444393 2244090.3184903734 0, -195083.88341866044 2244078.4668051726 0, -195094.1654991865 2243651.0130477655 0)), ((-194940.4916684473 2250262.022545632 0, -195003.14344391183 2250153.274088545 0, -195323.60931402224 2250162.274926262 0, -195313.63431049834 2250560.801723744 0, -194913.45908245555 2250548.03897212 0, -194513.28320715865 2250535.2967868103 0, -194920.3943810987 2250274.8795906464 0, -194940.4916684473 2250262.022545632 0)))</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Yakama</t>
+          <t>Yankton</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>WA</t>
+          <t>SD</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Common School and Indemnity, State Forest Transfer, Escheat, Scientific School, Community Forest Trust, Normal School, Natural Resources Conservation Area, Charitable/Educational/Penal &amp; Reformatory Instit., University - Transferred</t>
+          <t>Rural Credit, Common School</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>304</v>
+        <v>11</v>
       </c>
       <c r="G78" t="n">
-        <v>46922.33</v>
+        <v>0</v>
       </c>
       <c r="H78" t="n">
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="I78" t="n">
-        <v>44906.36</v>
+        <v>411.47</v>
       </c>
       <c r="J78" t="n">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="K78" t="n">
-        <v>91828.69</v>
+        <v>411.47</v>
       </c>
       <c r="L78" t="n">
-        <v>1376779.33</v>
+        <v>441528.7</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-201157.89714606619 2226817.235233947 0, -201150.4477368668 2227219.438475946 0, -200753.3026580403 2227209.6763946763 0, -200761.2634767131 2226807.28490224 0, -200769.14780959437 2226405.0503807156 0, -200774.72665332502 2226003.684905638 0, -200780.4616888446 2225601.4149824106 0, -201173.2890220301 2225612.9101912207 0, -201169.26346164412 2226014.247476004 0, -201165.3147526024 2226415.1188031007 0, -201157.89714606619 2226817.235233947 0)), ((-200676.61833697834 2245072.9570895853 0, -200665.50219727602 2245477.002334861 0, -200654.41287032556 2245882.0017014216 0, -200253.06813058004 2245868.06750964 0, -200264.80304160324 2245464.127465126 0, -200276.0542363167 2245060.042299942 0, -200676.61833697834 2245072.9570895853 0)), ((-195578.19880497677 2240443.3940137667 0, -195588.7887579272 2240039.0023805574 0, -195990.64187128432 2240050.3519468727 0, -195979.83454412993 2240455.3803870333 0, -195969.04419966493 2240859.482109948 0, -195567.5232243485 2240846.6419790983 0, -195578.19880497677 2240443.3940137667 0)), ((-195094.1654991865 2243651.0130477655 0, -195495.08877752116 2243663.273893927 0, -195484.58355444393 2244090.3184903734 0, -195083.88341866044 2244078.4668051726 0, -195094.1654991865 2243651.0130477655 0)), ((-194940.4916684473 2250262.022545632 0, -195003.14344391183 2250153.274088545 0, -195323.60931402224 2250162.274926262 0, -195313.63431049834 2250560.801723744 0, -194913.45908245555 2250548.03897212 0, -194513.28320715865 2250535.2967868103 0, -194920.3943810987 2250274.8795906464 0, -194940.4916684473 2250262.022545632 0)))</t>
+          <t>MULTIPOLYGON Z (((-963268.8443002809 1430363.758449293 0, -963314.768776577 1429960.686608801 0, -963712.0928119401 1430005.2204112052 0, -964109.4149344104 1430049.7727536343 0, -964506.7349353305 1430094.3437174025 0, -964904.050499542 1430138.9532507225 0, -964857.8234155204 1430542.153026707 0, -964811.5983582808 1430945.3339162313 0, -964765.3870148513 1431348.538080399 0, -964719.1596053746 1431751.7416974963 0, -964322.1604582192 1431707.0262301438 0, -963925.1432217385 1431662.3276507275 0, -963528.1377355896 1431617.6691773336 0, -963131.1162792982 1431573.0076248609 0, -963177.0249580408 1431169.9300062372 0, -963222.935745118 1430766.833605139 0, -963268.8443002809 1430363.758449293 0)), ((-967876.2163708522 1435408.6258091806 0, -967898.5115904618 1435410.9029027203 0, -968024.1492157216 1435423.7205935058 0, -968272.4248065699 1435449.0805621415 0, -968420.5530298074 1435465.1779594878 0, -968668.6124218298 1435491.7214209768 0, -968816.8661406672 1435507.5765224646 0, -969064.811744366 1435534.1185812366 0, -969019.2277263771 1435940.26696611 0, -968973.6274765375 1436346.4146844898 0, -968928.0430966188 1436752.5655057395 0, -968882.460746101 1437158.697634772 0, -968487.2379654302 1437113.5522262396 0, -968092.0154913071 1437068.4051628842 0, -967696.7885802072 1437023.2965345103 0, -967301.5779261262 1436978.1881779493 0, -967346.1711293819 1436575.7762582644 0, -967390.7641289367 1436173.3655807443 0, -967435.3569149923 1435770.9562472757 0, -967479.9492996859 1435368.5481400448 0, -967627.6342112896 1435383.2426118369 0, -967876.2163708522 1435408.6258091806 0)), ((-960653.0446861065 1425166.016569518 0, -960607.207696015 1425569.36785534 0, -960561.0948636045 1425972.8516395423 0, -960514.9819931365 1426376.3368287787 0, -960116.7787778581 1426331.3044214197 0, -959718.5757645215 1426286.2707026964 0, -959321.3485803383 1426241.4065627086 0, -958926.1302420439 1426196.807988672 0, -958935.754727946 1426107.382628779 0, -958967.4774739698 1425812.6336601684 0, -958968.9143523972 1425799.3134923284 0, -959010.972017595 1425408.6922006202 0, -959011.6981147537 1425401.8201261768 0, -959056.0033996366 1425005.0064636632 0, -959056.4447545457 1425001.0928834502 0, -959056.7416672814 1424998.4600985888 0, -959101.0828541025 1424601.3289680968 0, -959172.6533876254 1424608.8375537123 0, -959490.5010221126 1424642.1898751282 0, -959888.511958673 1424683.9590740039 0, -959895.4770753954 1424684.7715973589 0, -959899.2016164239 1424685.2104734667 0, -959899.2026799689 1424685.2105960224 0, -960080.0348917983 1424706.0484719486 0, -960292.8598894889 1424730.578138235 0, -960295.0851773646 1424730.8294062922 0, -960298.2058799788 1424731.1890148665 0, -960298.2068716306 1424731.189129193 0, -960501.5159544711 1424754.6284201655 0, -960697.2077411973 1424777.196489024 0, -960653.0446861065 1425166.016569518 0)), ((-961324.0386378516 1433411.4759536136 0, -960928.6425412277 1433366.544296997 0, -960533.037416067 1433321.5874915635 0, -960137.7060290826 1433276.6597803393 0, -959742.0207926851 1433231.6905779922 0, -959787.7854994311 1432828.8331621452 0, -960183.1167977916 1432873.6407322495 0, -960578.4437900083 1432918.4867662687 0, -960973.7709123844 1432963.3312459562 0, -961369.0959684617 1433008.1939289172 0, -961324.0386378516 1433411.4759536136 0)))</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Yankton</t>
+          <t>Zia</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>NM</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Rural Credit, Common School</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -4218,7 +4218,7 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="G79" t="n">
         <v>0</v>
@@ -4227,111 +4227,63 @@
         <v>0</v>
       </c>
       <c r="I79" t="n">
-        <v>411.47</v>
+        <v>2078.97</v>
       </c>
       <c r="J79" t="n">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="K79" t="n">
-        <v>411.47</v>
+        <v>2078.97</v>
       </c>
       <c r="L79" t="n">
-        <v>441528.7</v>
+        <v>134256.19</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-963268.8443002809 1430363.758449293 0, -963314.768776577 1429960.686608801 0, -963712.0928119401 1430005.2204112052 0, -964109.4149344104 1430049.7727536343 0, -964506.7349353305 1430094.3437174025 0, -964904.050499542 1430138.9532507225 0, -964857.8234155204 1430542.153026707 0, -964811.5983582808 1430945.3339162313 0, -964765.3870148513 1431348.538080399 0, -964719.1596053746 1431751.7416974963 0, -964322.1604582192 1431707.0262301438 0, -963925.1432217385 1431662.3276507275 0, -963528.1377355896 1431617.6691773336 0, -963131.1162792982 1431573.0076248609 0, -963177.0249580408 1431169.9300062372 0, -963222.935745118 1430766.833605139 0, -963268.8443002809 1430363.758449293 0)), ((-967876.2163708522 1435408.6258091806 0, -967898.5115904618 1435410.9029027203 0, -968024.1492157216 1435423.7205935058 0, -968272.4248065699 1435449.0805621415 0, -968420.5530298074 1435465.1779594878 0, -968668.6124218298 1435491.7214209768 0, -968816.8661406672 1435507.5765224646 0, -969064.811744366 1435534.1185812366 0, -969019.2277263771 1435940.26696611 0, -968973.6274765375 1436346.4146844898 0, -968928.0430966188 1436752.5655057395 0, -968882.460746101 1437158.697634772 0, -968487.2379654302 1437113.5522262396 0, -968092.0154913071 1437068.4051628842 0, -967696.7885802072 1437023.2965345103 0, -967301.5779261262 1436978.1881779493 0, -967346.1711293819 1436575.7762582644 0, -967390.7641289367 1436173.3655807443 0, -967435.3569149923 1435770.9562472757 0, -967479.9492996859 1435368.5481400448 0, -967627.6342112896 1435383.2426118369 0, -967876.2163708522 1435408.6258091806 0)), ((-960653.0446861065 1425166.016569518 0, -960607.207696015 1425569.36785534 0, -960561.0948636045 1425972.8516395423 0, -960514.9819931365 1426376.3368287787 0, -960116.7787778581 1426331.3044214197 0, -959718.5757645215 1426286.2707026964 0, -959321.3485803383 1426241.4065627086 0, -958926.1302420439 1426196.807988672 0, -958935.754727946 1426107.382628779 0, -958967.4774739698 1425812.6336601684 0, -958968.9143523972 1425799.3134923284 0, -959010.972017595 1425408.6922006202 0, -959011.6981147537 1425401.8201261768 0, -959056.0033996366 1425005.0064636632 0, -959056.4447545457 1425001.0928834502 0, -959056.7416672814 1424998.4600985888 0, -959101.0828541025 1424601.3289680968 0, -959172.6533876254 1424608.8375537123 0, -959490.5010221126 1424642.1898751282 0, -959888.511958673 1424683.9590740039 0, -959895.4770753954 1424684.7715973589 0, -959899.2016164239 1424685.2104734667 0, -959899.2026799689 1424685.2105960224 0, -960080.0348917983 1424706.0484719486 0, -960292.8598894889 1424730.578138235 0, -960295.0851773646 1424730.8294062922 0, -960298.2058799788 1424731.1890148665 0, -960298.2068716306 1424731.189129193 0, -960501.5159544711 1424754.6284201655 0, -960697.2077411973 1424777.196489024 0, -960653.0446861065 1425166.016569518 0)), ((-961324.0386378516 1433411.4759536136 0, -960928.6425412277 1433366.544296997 0, -960533.037416067 1433321.5874915635 0, -960137.7060290826 1433276.6597803393 0, -959742.0207926851 1433231.6905779922 0, -959787.7854994311 1432828.8331621452 0, -960183.1167977916 1432873.6407322495 0, -960578.4437900083 1432918.4867662687 0, -960973.7709123844 1432963.3312459562 0, -961369.0959684617 1433008.1939289172 0, -961324.0386378516 1433411.4759536136 0)))</t>
+          <t>MULTIPOLYGON Z (((-1230650.156670046 1366226.2121109671 0, -1231028.9950256061 1366267.9902809532 0, -1231434.9410266553 1366312.7802076074 0, -1231553.7829297276 1366325.8982821826 0, -1231860.339186602 1366362.0613912167 0, -1232246.1631810844 1366407.5938032246 0, -1232193.9459687504 1366815.4479508896 0, -1232141.0641802193 1367228.4859656875 0, -1232088.184509508 1367641.522767267 0, -1232035.6589074172 1368051.7703597795 0, -1231637.5983343583 1367995.2436863934 0, -1231238.7788168278 1367938.6251752558 0, -1230839.959229202 1367882.0254403732 0, -1230441.1340725517 1367825.4471172183 0, -1230493.6114402523 1367423.947975173 0, -1230546.0880157726 1367022.4503648307 0, -1230598.5639603366 1366620.954313936 0, -1230650.156670046 1366226.2121109671 0)), ((-1179406.438675978 1391598.4780311848 0, -1179376.687082965 1391813.8626402074 0, -1179010.4326745963 1391763.4625733264 0, -1179065.7797230636 1391362.0123873388 0, -1179319.6081469771 1391396.9113365898 0, -1179432.1469314967 1391412.3850173734 0, -1179406.438675978 1391598.4780311848 0)), ((-1175305.599237999 1392944.4259394954 0, -1175621.874753935 1392989.2567373854 0, -1175621.8809291632 1392989.2576126994 0, -1175910.2924798438 1393030.1499464114 0, -1176014.9073974208 1393044.985994756 0, -1176031.103019932 1393047.2170488585 0, -1176046.4939471069 1393049.3403368995 0, -1176012.7306980283 1393060.7847225934 0, -1175736.8256427709 1393154.0499050894 0, -1175592.5168004592 1393202.6557926997 0, -1175589.648874361 1393203.6227490243 0, -1175323.7911327295 1393293.1614621235 0, -1175172.3955430223 1393343.8675344859 0, -1175170.7525365737 1393344.4340099616 0, -1174752.3127354553 1393484.6127173828 0, -1174745.9919210786 1393486.7307787493 0, -1174332.2999252037 1393625.3644597516 0, -1174379.2882461646 1393283.846637234 0, -1174387.5275870538 1393223.9615068294 0, -1174442.7906177957 1392822.1808368226 0, -1174442.797383291 1392822.1817798174 0, -1174508.347529387 1392831.467321712 0, -1174835.821363174 1392877.8660369725 0, -1175228.8553593291 1392933.549978982 0, -1175305.599237999 1392944.4259394954 0)), ((-1175498.48855562 1411715.7205234338 0, -1175441.8983347837 1412118.5051669523 0, -1175385.3242070945 1412521.2934287016 0, -1174988.4403513533 1412467.4704269178 0, -1174591.5674526324 1412413.6881112035 0, -1174194.6786928598 1412359.9022091634 0, -1173797.7847071388 1412306.15462643 0, -1173821.9412342522 1412130.3965524095 0, -1174114.0481024592 1412035.6636411452 0, -1174245.7611750644 1411992.951309675 0, -1174323.0265613003 1411967.9030613736 0, -1174647.7320901754 1412011.9211541049 0, -1174669.5860315608 1411855.4850039117 0, -1174952.3221461347 1411763.7958221657 0, -1175093.4321466126 1411717.8781879004 0, -1175177.930924187 1411690.378694991 0, -1175217.4038987628 1411677.6287058126 0, -1175498.48855562 1411715.7205234338 0)), ((-1173751.581436906 1412710.9424306303 0, -1173705.3932026997 1413115.7338729296 0, -1173659.2128793285 1413520.2228657487 0, -1173613.0315028783 1413924.7131335821 0, -1173205.9243093685 1413868.355277904 0, -1172798.8011752826 1413811.9948493536 0, -1172391.688647008 1413755.6758929698 0, -1171984.5673369104 1413699.353434267 0, -1172041.4165952036 1413295.2357265905 0, -1172098.2496506604 1412891.117114005 0, -1172127.4563667192 1412680.2118645296 0, -1172127.835877648 1412680.0813261492 0, -1172436.2533071206 1412579.7565870732 0, -1172545.9688739832 1412544.0760245186 0, -1172554.7766014778 1412545.2885085973 0, -1172947.894318748 1412599.699872987 0, -1172971.7267977002 1412405.7625562567 0, -1173041.902875316 1412383.0617254323 0, -1173276.6135359607 1412307.0915113334 0, -1173399.2328404363 1412267.424644406 0, -1173434.7959754285 1412255.9174583415 0, -1173508.7881769352 1412266.151749508 0, -1173797.7847071388 1412306.15462643 0, -1173751.581436906 1412710.9424306303 0)), ((-1173580.6659229193 1420491.9394159773 0, -1173988.2226527212 1420545.8410660995 0, -1174395.7767336085 1420599.7620567963 0, -1174340.3669349628 1421002.050548744 0, -1174284.9568995119 1421404.340637009 0, -1174229.1714013966 1421806.376833381 0, -1174172.9946762586 1422211.2476761562 0, -1173760.3094233195 1422155.459276981 0, -1173347.6054191792 1422099.6885641788 0, -1172934.9122025375 1422043.9601368255 0, -1172522.2189816942 1421988.231668506 0, -1172581.7721226283 1421584.965266842 0, -1172640.9633129588 1421184.0901085644 0, -1172703.2446664653 1420784.1505723682 0, -1172765.5425179063 1420384.2146920348 0, -1173173.104076678 1420438.0773112255 0, -1173580.6659229193 1420491.9394159773 0)), ((-1172931.5229131742 1392610.821508625 0, -1172868.1889384773 1393074.6264596726 0, -1172813.3253800871 1393476.5471046895 0, -1172758.4452655197 1393878.467051319 0, -1172718.5168001745 1394170.8544220314 0, -1172664.2858641562 1394189.1357508404 0, -1172482.8464786327 1394250.2482840049 0, -1172307.9466047282 1394226.2442566087 0, -1171912.611488917 1394172.0763804908 0, -1171517.1442191983 1394118.030874152 0, -1171121.674581965 1394064.0037918896 0, -1171176.4501409233 1393662.16961251 0, -1171231.2254442002 1393260.3369106937 0, -1171286.006078273 1392858.4658545179 0, -1171348.3640234817 1392401.1326202895 0, -1171701.545907671 1392447.8108679873 0, -1171744.1627877895 1392453.456954902 0, -1172097.0675940812 1392500.1139375262 0, -1172139.9537026782 1392505.839576628 0, -1172492.5493494605 1392552.4705798456 0, -1172535.7639712938 1392558.2027700492 0, -1172888.0502426925 1392604.8079744328 0, -1172931.5229131742 1392610.821508625 0)), ((-1172428.4447664267 1422802.9976639973 0, -1172381.5574290259 1423210.3726671918 0, -1172334.6690533226 1423617.749033902 0, -1171934.255366138 1423566.6582560865 0, -1171533.8233525308 1423515.5840813902 0, -1171133.3919443616 1423464.5089000766 0, -1170732.9746686113 1423413.4756065952 0, -1170785.9002174437 1423010.5717117349 0, -1170838.8280762054 1422607.6491881046 0, -1170891.7527453594 1422204.748089802 0, -1170944.6958408337 1421801.8304217265 0, -1171339.0711084942 1421848.4121627612 0, -1171733.4511185244 1421894.9930114867 0, -1172127.8264853735 1421941.612038815 0, -1172522.2189816942 1421988.231668506 0, -1172475.3337117848 1422395.6040405133 0, -1172428.4447664267 1422802.9976639973 0)), ((-1166379.8580742273 1393412.7984702166 0, -1165984.229424639 1393358.8500000613 0, -1165588.61172215 1393304.9417828736 0, -1165192.9780163325 1393251.0298344865 0, -1164797.3552512976 1393197.1582403914 0, -1164851.7833524747 1392795.2767565313 0, -1164906.213813485 1392393.3768613848 0, -1164960.8570348632 1391991.4870388547 0, -1165015.4839551386 1391589.5966411936 0, -1165411.0337512083 1391641.1819036664 0, -1165806.565017187 1391692.7833502255 0, -1166204.1803047655 1391744.566076178 0, -1166601.8120934765 1391796.3495493892 0, -1166545.4010741839 1392207.2434767624 0, -1166490.2246998842 1392609.1010301283 0, -1166435.0510008365 1393010.940109647 0, -1166379.8580742273 1393412.7984702166 0)), ((-1168346.2402175646 1416938.950836989 0, -1168291.8866725499 1417344.4231284817 0, -1168237.535633526 1417749.876955446 0, -1168183.181422921 1418155.3521491783 0, -1167782.2249332508 1418106.2680156042 0, -1167381.2637183075 1418057.2224765148 0, -1166980.303220909 1418008.1760811964 0, -1166579.3244220777 1417959.1463298993 0, -1166631.40375167 1417552.5665601827 0, -1166683.4825636602 1417145.987956514 0, -1166735.563563827 1416739.3909451917 0, -1166787.641173089 1416332.8153704344 0, -1167190.8791227962 1416382.9472842843 0, -1167594.1120814949 1416433.1182798971 0, -1167997.3457350433 1416483.2884237745 0, -1168400.577237942 1416533.4776820375 0, -1168346.2402175646 1416938.950836989 0)), ((-1169364.0171739731 1421592.1376663186 0, -1169309.5614646836 1421994.908155483 0, -1169255.1082735094 1422397.6599490184 0, -1169200.6547376886 1422800.4132128763 0, -1169146.2009559378 1423203.1679550996 0, -1168735.3866428486 1423150.8022123748 0, -1168324.551193241 1423098.4740808965 0, -1167913.7323020592 1423046.1480197525 0, -1167502.908178204 1422993.8618082106 0, -1167558.5688820183 1422589.8698776641 0, -1167614.2268096716 1422185.8993378947 0, -1167669.8844984479 1421781.9302947018 0, -1167725.5419775494 1421377.9624487595 0, -1168135.1590305243 1421431.4862235263 0, -1168544.792575077 1421485.0117535614 0, -1168954.404688972 1421538.5748606836 0, -1169364.0171739731 1421592.1376663186 0)), ((-1164634.1081047873 1420190.6300656113 0, -1164576.9766307764 1420593.5399584575 0, -1164519.8452037955 1420996.4513851749 0, -1164129.5886527759 1420948.558849198 0, -1163739.33284891 1420900.664002819 0, -1163349.072364934 1420852.8072118475 0, -1162958.8127199542 1420804.9482208462 0, -1163010.6734844977 1420403.775606886 0, -1163062.5175730835 1420002.6020558227 0, -1163111.2830547593 1419602.2085557617 0, -1163160.0611932212 1419201.8385708327 0, -1163558.1923093174 1419247.0732339686 0, -1163956.3350437784 1419292.3488860107 0, -1164354.4761687422 1419337.6430014072 0, -1164752.6182990842 1419382.9358940723 0, -1164693.3537539684 1419786.791009418 0, -1164634.1081047873 1420190.6300656113 0)), ((-1162554.3179741418 1420760.8343401507 0, -1162958.8127199542 1420804.9482208462 0, -1162907.1421569402 1421206.1687318848 0, -1162855.45500648 1421607.3884115983 0, -1162803.7673767486 1422008.6094145814 0, -1162752.0954645814 1422409.8340048988 0, -1162357.0406865175 1422364.2244797307 0, -1161961.9869693308 1422318.6134074237 0, -1161566.9315708561 1422273.0207662575 0, -1161171.8717686632 1422227.4663342931 0, -1161214.1050098995 1421827.7387250643 0, -1161256.3504611242 1421428.034624433 0, -1161298.5812155544 1421028.3095464534 0, -1161340.8077851892 1420628.6056951552 0, -1161745.3234605545 1420672.66414543 0, -1162149.8214223213 1420716.7396355853 0, -1162554.3179741418 1420760.8343401507 0)), ((-1160555.835367265 1342362.4724318008 0, -1160639.0989210666 1342372.8008393203 0, -1160639.1025707817 1342372.8012920392 0, -1161067.547138715 1342425.9465278913 0, -1161084.0594122906 1342427.9948507575 0, -1161084.0625698133 1342427.995312719 0, -1161086.8509861662 1342428.4032720837 0, -1161481.30990815 1342486.1245715774 0, -1161471.8016836355 1342557.7932392866 0, -1161426.9593904626 1342895.7342120272 0, -1161426.9583758549 1342895.741858687 0, -1161382.1573930888 1343233.3875231277 0, -1161372.6084341146 1343305.3411579954 0, -1161345.5917563364 1343502.4844921895 0, -1161317.9007638758 1343704.535456809 0, -1161174.6171993 1343681.4754627682 0, -1160918.0771163949 1343640.1857298138 0, -1160918.0768122156 1343640.1879653856 0, -1160918.07595339 1343640.1878271666 0, -1160863.1124110003 1344044.1219970598 0, -1160419.319074915 1343987.2959846682 0, -1160200.1974385392 1343959.2410356097 0, -1160021.8329877972 1343936.4005959847 0, -1160021.8323116223 1343936.4005094012 0, -1159742.2525162355 1343900.6005991232 0, -1159622.9155582127 1343885.3180074997 0, -1159677.0775108382 1343481.2768438656 0, -1159677.0776918822 1343481.2754933028 0, -1159708.191035808 1343249.174230714 0, -1159731.2444110706 1343077.2353770316 0, -1159751.1380842498 1342911.234984098 0, -1159779.4919498912 1342674.6956624135 0, -1159779.4923405426 1342674.6924034243 0, -1159827.7437912773 1342272.1571615706 0, -1159970.3261369911 1342289.8435207168 0, -1160239.2273022288 1342323.2090227657 0, -1160555.835367265 1342362.4724318008 0)), ((-1157166.6133341766 1418425.5600141888 0, -1157168.564336575 1418425.8454011441 0, -1157164.0956349513 1418429.9739014811 0, -1156969.451975769 1418609.2781745216 0, -1156914.1249898104 1418692.372831359 0, -1156868.3254176043 1418797.4147460205 0, -1156722.0185353474 1418776.390662088 0, -1156767.2325033643 1418367.0227464072 0, -1156990.915978495 1418399.808372859 0, -1157164.6204906022 1418425.2685328429 0, -1157166.6133341766 1418425.5600141888 0)), ((-1159678.263049038 1421200.6842120434 0, -1159633.407860968 1421589.500756771 0, -1159588.551875587 1421978.318575145 0, -1159194.6171948852 1421940.5322140078 0, -1158800.694781235 1421902.7862226758 0, -1158406.7553600164 1421865.0563305682 0, -1158012.8336763529 1421827.3270519462 0, -1158053.6318724658 1421424.379318485 0, -1158094.425684959 1421021.4527952771 0, -1158135.2369948642 1420618.5098106978 0, -1158176.0279103909 1420215.5858927795 0, -1158574.0130461846 1420267.42473959 0, -1158971.9958590274 1420319.282030556 0, -1159369.9924167069 1420371.1603221798 0, -1159767.9705395217 1420423.0549011857 0, -1159723.1172424308 1420811.8689232648 0, -1159678.263049038 1421200.6842120434 0)))</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Zia</t>
+          <t>Zuni</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>NM</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Common Schools</t>
+          <t>PERM CMN SCHLS (INDMTY SELEC), Saline Lands, University of New Mexico, Common Schools, New Mexico School for the Visually Handicapped</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>52</v>
+        <v>189</v>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>62.57</v>
       </c>
       <c r="H80" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I80" t="n">
-        <v>2078.97</v>
+        <v>8070.27</v>
       </c>
       <c r="J80" t="n">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="K80" t="n">
-        <v>2078.97</v>
+        <v>8132.84</v>
       </c>
       <c r="L80" t="n">
-        <v>134256.19</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON Z (((-1230650.156670046 1366226.2121109671 0, -1231028.9950256061 1366267.9902809532 0, -1231434.9410266553 1366312.7802076074 0, -1231553.7829297276 1366325.8982821826 0, -1231860.339186602 1366362.0613912167 0, -1232246.1631810844 1366407.5938032246 0, -1232193.9459687504 1366815.4479508896 0, -1232141.0641802193 1367228.4859656875 0, -1232088.184509508 1367641.522767267 0, -1232035.6589074172 1368051.7703597795 0, -1231637.5983343583 1367995.2436863934 0, -1231238.7788168278 1367938.6251752558 0, -1230839.959229202 1367882.0254403732 0, -1230441.1340725517 1367825.4471172183 0, -1230493.6114402523 1367423.947975173 0, -1230546.0880157726 1367022.4503648307 0, -1230598.5639603366 1366620.954313936 0, -1230650.156670046 1366226.2121109671 0)), ((-1179406.438675978 1391598.4780311848 0, -1179376.687082965 1391813.8626402074 0, -1179010.4326745963 1391763.4625733264 0, -1179065.7797230636 1391362.0123873388 0, -1179319.6081469771 1391396.9113365898 0, -1179432.1469314967 1391412.3850173734 0, -1179406.438675978 1391598.4780311848 0)), ((-1175305.599237999 1392944.4259394954 0, -1175621.874753935 1392989.2567373854 0, -1175621.8809291632 1392989.2576126994 0, -1175910.2924798438 1393030.1499464114 0, -1176014.9073974208 1393044.985994756 0, -1176031.103019932 1393047.2170488585 0, -1176046.4939471069 1393049.3403368995 0, -1176012.7306980283 1393060.7847225934 0, -1175736.8256427709 1393154.0499050894 0, -1175592.5168004592 1393202.6557926997 0, -1175589.648874361 1393203.6227490243 0, -1175323.7911327295 1393293.1614621235 0, -1175172.3955430223 1393343.8675344859 0, -1175170.7525365737 1393344.4340099616 0, -1174752.3127354553 1393484.6127173828 0, -1174745.9919210786 1393486.7307787493 0, -1174332.2999252037 1393625.3644597516 0, -1174379.2882461646 1393283.846637234 0, -1174387.5275870538 1393223.9615068294 0, -1174442.7906177957 1392822.1808368226 0, -1174442.797383291 1392822.1817798174 0, -1174508.347529387 1392831.467321712 0, -1174835.821363174 1392877.8660369725 0, -1175228.8553593291 1392933.549978982 0, -1175305.599237999 1392944.4259394954 0)), ((-1175498.48855562 1411715.7205234338 0, -1175441.8983347837 1412118.5051669523 0, -1175385.3242070945 1412521.2934287016 0, -1174988.4403513533 1412467.4704269178 0, -1174591.5674526324 1412413.6881112035 0, -1174194.6786928598 1412359.9022091634 0, -1173797.7847071388 1412306.15462643 0, -1173821.9412342522 1412130.3965524095 0, -1174114.0481024592 1412035.6636411452 0, -1174245.7611750644 1411992.951309675 0, -1174323.0265613003 1411967.9030613736 0, -1174647.7320901754 1412011.9211541049 0, -1174669.5860315608 1411855.4850039117 0, -1174952.3221461347 1411763.7958221657 0, -1175093.4321466126 1411717.8781879004 0, -1175177.930924187 1411690.378694991 0, -1175217.4038987628 1411677.6287058126 0, -1175498.48855562 1411715.7205234338 0)), ((-1173751.581436906 1412710.9424306303 0, -1173705.3932026997 1413115.7338729296 0, -1173659.2128793285 1413520.2228657487 0, -1173613.0315028783 1413924.7131335821 0, -1173205.9243093685 1413868.355277904 0, -1172798.8011752826 1413811.9948493536 0, -1172391.688647008 1413755.6758929698 0, -1171984.5673369104 1413699.353434267 0, -1172041.4165952036 1413295.2357265905 0, -1172098.2496506604 1412891.117114005 0, -1172127.4563667192 1412680.2118645296 0, -1172127.835877648 1412680.0813261492 0, -1172436.2533071206 1412579.7565870732 0, -1172545.9688739832 1412544.0760245186 0, -1172554.7766014778 1412545.2885085973 0, -1172947.894318748 1412599.699872987 0, -1172971.7267977002 1412405.7625562567 0, -1173041.902875316 1412383.0617254323 0, -1173276.6135359607 1412307.0915113334 0, -1173399.2328404363 1412267.424644406 0, -1173434.7959754285 1412255.9174583415 0, -1173508.7881769352 1412266.151749508 0, -1173797.7847071388 1412306.15462643 0, -1173751.581436906 1412710.9424306303 0)), ((-1173580.6659229193 1420491.9394159773 0, -1173988.2226527212 1420545.8410660995 0, -1174395.7767336085 1420599.7620567963 0, -1174340.3669349628 1421002.050548744 0, -1174284.9568995119 1421404.340637009 0, -1174229.1714013966 1421806.376833381 0, -1174172.9946762586 1422211.2476761562 0, -1173760.3094233195 1422155.459276981 0, -1173347.6054191792 1422099.6885641788 0, -1172934.9122025375 1422043.9601368255 0, -1172522.2189816942 1421988.231668506 0, -1172581.7721226283 1421584.965266842 0, -1172640.9633129588 1421184.0901085644 0, -1172703.2446664653 1420784.1505723682 0, -1172765.5425179063 1420384.2146920348 0, -1173173.104076678 1420438.0773112255 0, -1173580.6659229193 1420491.9394159773 0)), ((-1172931.5229131742 1392610.821508625 0, -1172868.1889384773 1393074.6264596726 0, -1172813.3253800871 1393476.5471046895 0, -1172758.4452655197 1393878.467051319 0, -1172718.5168001745 1394170.8544220314 0, -1172664.2858641562 1394189.1357508404 0, -1172482.8464786327 1394250.2482840049 0, -1172307.9466047282 1394226.2442566087 0, -1171912.611488917 1394172.0763804908 0, -1171517.1442191983 1394118.030874152 0, -1171121.674581965 1394064.0037918896 0, -1171176.4501409233 1393662.16961251 0, -1171231.2254442002 1393260.3369106937 0, -1171286.006078273 1392858.4658545179 0, -1171348.3640234817 1392401.1326202895 0, -1171701.545907671 1392447.8108679873 0, -1171744.1627877895 1392453.456954902 0, -1172097.0675940812 1392500.1139375262 0, -1172139.9537026782 1392505.839576628 0, -1172492.5493494605 1392552.4705798456 0, -1172535.7639712938 1392558.2027700492 0, -1172888.0502426925 1392604.8079744328 0, -1172931.5229131742 1392610.821508625 0)), ((-1172428.4447664267 1422802.9976639973 0, -1172381.5574290259 1423210.3726671918 0, -1172334.6690533226 1423617.749033902 0, -1171934.255366138 1423566.6582560865 0, -1171533.8233525308 1423515.5840813902 0, -1171133.3919443616 1423464.5089000766 0, -1170732.9746686113 1423413.4756065952 0, -1170785.9002174437 1423010.5717117349 0, -1170838.8280762054 1422607.6491881046 0, -1170891.7527453594 1422204.748089802 0, -1170944.6958408337 1421801.8304217265 0, -1171339.0711084942 1421848.4121627612 0, -1171733.4511185244 1421894.9930114867 0, -1172127.8264853735 1421941.612038815 0, -1172522.2189816942 1421988.231668506 0, -1172475.3337117848 1422395.6040405133 0, -1172428.4447664267 1422802.9976639973 0)), ((-1166379.8580742273 1393412.7984702166 0, -1165984.229424639 1393358.8500000613 0, -1165588.61172215 1393304.9417828736 0, -1165192.9780163325 1393251.0298344865 0, -1164797.3552512976 1393197.1582403914 0, -1164851.7833524747 1392795.2767565313 0, -1164906.213813485 1392393.3768613848 0, -1164960.8570348632 1391991.4870388547 0, -1165015.4839551386 1391589.5966411936 0, -1165411.0337512083 1391641.1819036664 0, -1165806.565017187 1391692.7833502255 0, -1166204.1803047655 1391744.566076178 0, -1166601.8120934765 1391796.3495493892 0, -1166545.4010741839 1392207.2434767624 0, -1166490.2246998842 1392609.1010301283 0, -1166435.0510008365 1393010.940109647 0, -1166379.8580742273 1393412.7984702166 0)), ((-1168346.2402175646 1416938.950836989 0, -1168291.8866725499 1417344.4231284817 0, -1168237.535633526 1417749.876955446 0, -1168183.181422921 1418155.3521491783 0, -1167782.2249332508 1418106.2680156042 0, -1167381.2637183075 1418057.2224765148 0, -1166980.303220909 1418008.1760811964 0, -1166579.3244220777 1417959.1463298993 0, -1166631.40375167 1417552.5665601827 0, -1166683.4825636602 1417145.987956514 0, -1166735.563563827 1416739.3909451917 0, -1166787.641173089 1416332.8153704344 0, -1167190.8791227962 1416382.9472842843 0, -1167594.1120814949 1416433.1182798971 0, -1167997.3457350433 1416483.2884237745 0, -1168400.577237942 1416533.4776820375 0, -1168346.2402175646 1416938.950836989 0)), ((-1169364.0171739731 1421592.1376663186 0, -1169309.5614646836 1421994.908155483 0, -1169255.1082735094 1422397.6599490184 0, -1169200.6547376886 1422800.4132128763 0, -1169146.2009559378 1423203.1679550996 0, -1168735.3866428486 1423150.8022123748 0, -1168324.551193241 1423098.4740808965 0, -1167913.7323020592 1423046.1480197525 0, -1167502.908178204 1422993.8618082106 0, -1167558.5688820183 1422589.8698776641 0, -1167614.2268096716 1422185.8993378947 0, -1167669.8844984479 1421781.9302947018 0, -1167725.5419775494 1421377.9624487595 0, -1168135.1590305243 1421431.4862235263 0, -1168544.792575077 1421485.0117535614 0, -1168954.404688972 1421538.5748606836 0, -1169364.0171739731 1421592.1376663186 0)), ((-1164634.1081047873 1420190.6300656113 0, -1164576.9766307764 1420593.5399584575 0, -1164519.8452037955 1420996.4513851749 0, -1164129.5886527759 1420948.558849198 0, -1163739.33284891 1420900.664002819 0, -1163349.072364934 1420852.8072118475 0, -1162958.8127199542 1420804.9482208462 0, -1163010.6734844977 1420403.775606886 0, -1163062.5175730835 1420002.6020558227 0, -1163111.2830547593 1419602.2085557617 0, -1163160.0611932212 1419201.8385708327 0, -1163558.1923093174 1419247.0732339686 0, -1163956.3350437784 1419292.3488860107 0, -1164354.4761687422 1419337.6430014072 0, -1164752.6182990842 1419382.9358940723 0, -1164693.3537539684 1419786.791009418 0, -1164634.1081047873 1420190.6300656113 0)), ((-1162554.3179741418 1420760.8343401507 0, -1162958.8127199542 1420804.9482208462 0, -1162907.1421569402 1421206.1687318848 0, -1162855.45500648 1421607.3884115983 0, -1162803.7673767486 1422008.6094145814 0, -1162752.0954645814 1422409.8340048988 0, -1162357.0406865175 1422364.2244797307 0, -1161961.9869693308 1422318.6134074237 0, -1161566.9315708561 1422273.0207662575 0, -1161171.8717686632 1422227.4663342931 0, -1161214.1050098995 1421827.7387250643 0, -1161256.3504611242 1421428.034624433 0, -1161298.5812155544 1421028.3095464534 0, -1161340.8077851892 1420628.6056951552 0, -1161745.3234605545 1420672.66414543 0, -1162149.8214223213 1420716.7396355853 0, -1162554.3179741418 1420760.8343401507 0)), ((-1160555.835367265 1342362.4724318008 0, -1160639.0989210666 1342372.8008393203 0, -1160639.1025707817 1342372.8012920392 0, -1161067.547138715 1342425.9465278913 0, -1161084.0594122906 1342427.9948507575 0, -1161084.0625698133 1342427.995312719 0, -1161086.8509861662 1342428.4032720837 0, -1161481.30990815 1342486.1245715774 0, -1161471.8016836355 1342557.7932392866 0, -1161426.9593904626 1342895.7342120272 0, -1161426.9583758549 1342895.741858687 0, -1161382.1573930888 1343233.3875231277 0, -1161372.6084341146 1343305.3411579954 0, -1161345.5917563364 1343502.4844921895 0, -1161317.9007638758 1343704.535456809 0, -1161174.6171993 1343681.4754627682 0, -1160918.0771163949 1343640.1857298138 0, -1160918.0768122156 1343640.1879653856 0, -1160918.07595339 1343640.1878271666 0, -1160863.1124110003 1344044.1219970598 0, -1160419.319074915 1343987.2959846682 0, -1160200.1974385392 1343959.2410356097 0, -1160021.8329877972 1343936.4005959847 0, -1160021.8323116223 1343936.4005094012 0, -1159742.2525162355 1343900.6005991232 0, -1159622.9155582127 1343885.3180074997 0, -1159677.0775108382 1343481.2768438656 0, -1159677.0776918822 1343481.2754933028 0, -1159708.191035808 1343249.174230714 0, -1159731.2444110706 1343077.2353770316 0, -1159751.1380842498 1342911.234984098 0, -1159779.4919498912 1342674.6956624135 0, -1159779.4923405426 1342674.6924034243 0, -1159827.7437912773 1342272.1571615706 0, -1159970.3261369911 1342289.8435207168 0, -1160239.2273022288 1342323.2090227657 0, -1160555.835367265 1342362.4724318008 0)), ((-1157166.6133341766 1418425.5600141888 0, -1157168.564336575 1418425.8454011441 0, -1157164.0956349513 1418429.9739014811 0, -1156969.451975769 1418609.2781745216 0, -1156914.1249898104 1418692.372831359 0, -1156868.3254176043 1418797.4147460205 0, -1156722.0185353474 1418776.390662088 0, -1156767.2325033643 1418367.0227464072 0, -1156990.915978495 1418399.808372859 0, -1157164.6204906022 1418425.2685328429 0, -1157166.6133341766 1418425.5600141888 0)), ((-1159678.263049038 1421200.6842120434 0, -1159633.407860968 1421589.500756771 0, -1159588.551875587 1421978.318575145 0, -1159194.6171948852 1421940.5322140078 0, -1158800.694781235 1421902.7862226758 0, -1158406.7553600164 1421865.0563305682 0, -1158012.8336763529 1421827.3270519462 0, -1158053.6318724658 1421424.379318485 0, -1158094.425684959 1421021.4527952771 0, -1158135.2369948642 1420618.5098106978 0, -1158176.0279103909 1420215.5858927795 0, -1158574.0130461846 1420267.42473959 0, -1158971.9958590274 1420319.282030556 0, -1159369.9924167069 1420371.1603221798 0, -1159767.9705395217 1420423.0549011857 0, -1159723.1172424308 1420811.8689232648 0, -1159678.263049038 1421200.6842120434 0)))</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Zuni</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>AZ</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>PERM CMN SCHLS (INDMTY SELEC), Saline Lands, University of New Mexico, Common Schools, New Mexico School for the Visually Handicapped</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Subsurface, Surface</t>
-        </is>
-      </c>
-      <c r="F81" t="n">
-        <v>189</v>
-      </c>
-      <c r="G81" t="n">
-        <v>62.57</v>
-      </c>
-      <c r="H81" t="n">
-        <v>2</v>
-      </c>
-      <c r="I81" t="n">
-        <v>8070.27</v>
-      </c>
-      <c r="J81" t="n">
-        <v>187</v>
-      </c>
-      <c r="K81" t="n">
-        <v>8132.84</v>
-      </c>
-      <c r="L81" t="n">
         <v>462553.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove border-river sliver polygons (#18)
---------

Co-authored-by: parkerziegler <parkerellisziegler@gmail.com>
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,7 +546,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1215734.4919286212 2919412.348803906 0, -1215739.2418993178 2919415.854489744 0, -1215752.301648532 2919425.0016529365 0, -1215801.1184896445 2919460.5409494657 0, -1215880.1351253951 2919458.194114684 0, -1215935.7465738817 2919456.662823337 0, -1216017.514904797 2919424.4208201505 0, -1216301.6985192918 2919383.909817556 0, -1216379.7725044978 2919372.857053071 0, -1216421.4827175136 2919404.798627857 0, -1216469.9646424958 2919466.6185278543 0, -1216487.0923211551 2919489.0687451703 0, -1216593.3096698693 2919789.9906576937 0, -1216651.6264636929 2919845.8770137485 0, -1216722.102225036 2919913.20975236 0, -1216831.1752236811 2920017.569721035 0, -1216842.6006949407 2920051.4157221178 0, -1216862.8363486752 2920111.6435212083 0, -1216862.7034745696 2920112.4260375807 0, -1216853.6560083632 2920085.5366167566 0, -1216843.1038769977 2920059.6028733077 0, -1216788.3014150327 2920007.3321183003 0, -1216697.798992958 2919912.0946244993 0, -1216633.1836969352 2919850.462773938 0, -1216599.6502633595 2919815.1742660655 0, -1216567.797031382 2919770.1383114094 0, -1216565.3659194517 2919760.2612490105 0, -1216511.7640747712 2919615.50416238 0, -1216496.3529543676 2919552.8790510045 0, -1216472.969075556 2919514.3247987595 0, -1216439.8650943723 2919472.5683507663 0, -1216418.8132326123 2919456.8300753315 0, -1216358.015127779 2919455.0348798954 0, -1216318.5462705519 2919461.0072452463 0, -1216263.0451418571 2919466.0366023434 0, -1216119.5758356226 2919487.7435471755 0, -1216003.1941593739 2919521.9833337013 0, -1215961.895446596 2919538.5249132873 0, -1215933.7719486097 2919539.620839089 0, -1215858.3285944469 2919530.32260102 0, -1215818.4702780903 2919531.876578283 0, -1215803.123633326 2919510.222797078 0, -1215726.7621123476 2919429.118585371 0, -1215704.0221886155 2919391.4580905 0, -1215619.2137624647 2919251.0013917703 0, -1215629.2988838274 2919241.1229922394 0, -1215629.3130592303 2919241.146159707 0, -1215734.4919286212 2919412.348803906 0)), ((-1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0)))</t>
+          <t>POLYGON Z ((-1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0))</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -561,22 +561,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Common Schools, Dept. of Transportation, None Listed</t>
+          <t>Dept. of Transportation, None Listed</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Surface, subsurface, Subsurface</t>
+          <t>subsurface, Subsurface</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>17.01</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>81.20999999999999</v>
@@ -585,7 +585,7 @@
         <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>98.22</v>
+        <v>81.20999999999999</v>
       </c>
       <c r="L3" t="n">
         <v>1534569.87</v>
@@ -657,7 +657,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Public Building, Common Schools, State Educational Institutions, Oklahoma State University, University Preparatory, University of Oklahoma, Normal Schools</t>
+          <t>Common Schools, Oklahoma State University, State Educational Institutions, Public Building, University Preparatory, University of Oklahoma, Normal Schools</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Common Schools, Oklahoma State University, Normal Schools, University Preparatory, Connors State College, Langston University, State Educational Institutions</t>
+          <t>Common Schools, Normal Schools, University Preparatory, Connors State College, Oklahoma State University, Langston University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Rural Credit, School and Public Lands, Common School, Indemnity</t>
+          <t>Common School, Rural Credit, School and Public Lands, Indemnity</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Oklahoma State University, University of Oklahoma, Common Schools, Greer 33, State Educational Institutions, Normal Schools, University Preparatory, Langston University, Wildlife Conservation, Redlands Community College, University Hospitals Authority &amp; Trust</t>
+          <t>Oklahoma State University, University of Oklahoma, Common Schools, State Educational Institutions, Greer 33, Normal Schools, University Preparatory, Langston University, Wildlife Conservation, Redlands Community College, University Hospitals Authority &amp; Trust</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -945,7 +945,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, University Preparatory, Oklahoma State University, Other Agency, Wildlife Conservation, Normal Schools, Aeronautics Commission</t>
+          <t>Oklahoma State University, Common Schools, Normal Schools, State Educational Institutions, University Preparatory, Other Agency, Wildlife Conservation, Aeronautics Commission</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -993,7 +993,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, University of Oklahoma, Langston University, Oklahoma State University, Normal Schools, University Preparatory, Other Agency, Wildlife Conservation</t>
+          <t>University of Oklahoma, State Educational Institutions, Common Schools, Normal Schools, University Preparatory, Oklahoma State University, Langston University, Other Agency, Wildlife Conservation</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dept. of Parks and Recreation, 100.00% Dept. of Parks and Recreation, Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), 100.00% Normal School, 100.00% University of Idaho, State Hospital South (Insane Asylum), Normal School, Agricultural College, 100.00% Dept. of Fish and Game, General Fund, 100.00% General Fund</t>
+          <t>Dept. of Parks and Recreation, 100.00% Dept. of Parks and Recreation, Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), 100.00% Normal School, 100.00% University of Idaho, State Hospital South (Insane Asylum), Normal School, Agricultural College, 100.00% Dept. of Fish and Game, 100.00% General Fund, General Fund</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Rural Credit, Common School</t>
+          <t>Common School, Rural Credit</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1362,7 +1362,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1406379.8180101914 2835502.9676008387 0, -1406473.9785516895 2835521.734531294 0, -1406778.7770429626 2835582.4882667917 0, -1406872.8312997553 2835601.148932945 0, -1406791.7645722493 2835992.9266004586 0, -1406710.698745883 2836384.702508994 0, -1406629.6366764735 2836776.4711096287 0, -1406548.5739271764 2837168.2345223785 0, -1406152.1431418383 2837088.956904065 0, -1406087.6405494164 2837076.280484532 0, -1405796.91670816 2837018.1569047323 0, -1405755.7083628573 2837009.698301688 0, -1405535.803621465 2836965.9663151815 0, -1405487.176097592 2836956.2471401114 0, -1405359.2691901615 2836930.461773824 0, -1405080.115136758 2836874.9046132243 0, -1404962.8255844747 2836851.2476163614 0, -1405025.8156075906 2836537.4335374683 0, -1405029.769174486 2836517.7370062955 0, -1405041.4965421397 2836459.306839623 0, -1405041.4965422011 2836459.306839316 0, -1405081.6600892353 2836258.4058300443 0, -1405108.2831449925 2836126.578187748 0, -1405120.0309416638 2836067.337313631 0, -1405133.2551556446 2836000.645850542 0, -1405186.659309687 2835735.386966785 0, -1405188.114813715 2835727.329112005 0, -1405192.8804176834 2835703.5856685042 0, -1405198.701406638 2835675.389715876 0, -1405261.8129454285 2835360.1547357994 0, -1405265.1738896933 2835344.2151984107 0, -1405277.2234497615 2835283.407895384 0, -1405277.2234497755 2835283.4078953867 0, -1405277.2234497757 2835283.4078953853 0, -1405581.9305416776 2835344.089946119 0, -1405676.1759969064 2835362.862839606 0, -1405980.8366573509 2835423.550296702 0, -1406075.138144352 2835442.2583379205 0, -1406202.3274685177 2835467.601562032 0, -1406379.8180101914 2835502.9676008387 0)), ((-1399306.9140826785 2840269.7509606453 0, -1399308.926485363 2840259.6770075844 0, -1399310.6939220119 2840250.9220541627 0, -1399335.4899758273 2840125.914068922 0, -1399347.1961440216 2840066.79943821 0, -1399356.4079068387 2840020.2810208434 0, -1399368.1809894112 2839960.4057747424 0, -1399384.6546780465 2839877.227700831 0, -1399462.396458146 2839484.6995438226 0, -1399540.139008013 2839092.1665506647 0, -1399542.905688448 2839092.835199241 0, -1399556.3294038298 2839095.3861888293 0, -1399556.329404045 2839095.3861888703 0, -1399561.6720821362 2839096.376602012 0, -1399582.007635379 2839100.423022579 0, -1399599.5649045492 2839103.916675662 0, -1399623.3376730068 2839108.6470440533 0, -1399644.5027693652 2839112.8586522965 0, -1399667.8546858106 2839117.505222619 0, -1399689.9714188937 2839121.9060038663 0, -1399712.3326666437 2839126.3553711157 0, -1399735.4324632378 2839130.9517879887 0, -1399753.6615634388 2839134.578885354 0, -1399780.8692110055 2839139.992492276 0, -1399798.1407629494 2839143.429084783 0, -1399826.33910559 2839149.039729029 0, -1399842.651850635 2839152.2853515954 0, -1399871.8019453995 2839158.085069711 0, -1399883.9572934853 2839160.5036009005 0, -1399916.771608468 2839167.0324040405 0, -1399928.497425498 2839169.3652046104 0, -1399934.4273121587 2839170.492037641 0, -1399937.3344581702 2839171.1505293464 0, -1399937.334458662 2839171.150529451 0, -1399937.3344694409 2839171.1505315923 0, -1399961.7740465652 2839175.991441545 0, -1399972.9727293379 2839178.2173738675 0, -1400007.6713144428 2839185.123969481 0, -1400014.3015124146 2839186.44347234 0, -1400053.0843019113 2839194.164184724 0, -1400059.1674090049 2839195.3749906607 0, -1400062.5253671096 2839196.043416641 0, -1400098.5195565978 2839203.2079879213 0, -1400103.2938011107 2839204.1582646235 0, -1400135.8492566794 2839210.638179495 0, -1400135.84925794 2839210.638179746 0, -1400143.9549004098 2839212.251141099 0, -1400147.7740981488 2839213.0111707496 0, -1400189.1188868866 2839221.238374427 0, -1400322.934807602 2839247.8660599813 0, -1400331.4578416802 2839249.561483696 0, -1400334.5232879098 2839250.1564733693 0, -1400337.289539137 2839250.8269082224 0, -1400438.6676987924 2839270.9013746134 0, -1400616.4727830754 2839306.2846389473 0, -1400666.7624768384 2839316.2673303704 0, -1400731.7096861927 2839329.18493668 0, -1400734.4720727175 2839329.8709867066 0, -1400774.2737872985 2839337.662505503 0, -1400819.7837660834 2839346.7515740218 0, -1401125.8721471464 2839407.6680866037 0, -1401128.8917457967 2839408.235767459 0, -1401123.9478869513 2839432.9798185662 0, -1401114.9923184975 2839478.068050874 0, -1401105.4885421125 2839525.9158027335 0, -1401103.154785328 2839537.809666259 0, -1401103.15478518 2839537.809667019 0, -1401067.6565216575 2839720.071360423 0, -1401063.830226231 2839739.28926802 0, -1401063.2021711767 2839742.434400068 0, -1401053.3518599859 2839788.545631688 0, -1401050.9229196983 2839800.7740466096 0, -1401050.9229196971 2839800.7740466157 0, -1401053.6475980359 2839801.596686764 0, -1400999.4443926136 2840062.6907491884 0, -1400998.724069705 2840066.308780294 0, -1400989.0886561542 2840114.569291522 0, -1400975.3905077311 2840183.1795261377 0, -1400973.5361308318 2840190.382025044 0, -1400973.536130806 2840190.382025154 0, -1400972.9550610757 2840193.3075143024 0, -1400954.6895441287 2840190.4323968505 0, -1400920.226759528 2840183.5676653488 0, -1400578.8062332084 2840115.124226884 0, -1400575.8805057171 2840114.2936359607 0, -1400575.7633936796 2840117.3285491103 0, -1400574.844702643 2840122.2522871094 0, -1400574.022585394 2840126.3318334757 0, -1400566.8949736727 2840162.4611979346 0, -1400542.6533913193 2840284.271411241 0, -1400539.2966141847 2840301.1361504267 0, -1400517.715227514 2840409.5622253655 0, -1400512.0344126902 2840438.1135863895 0, -1400502.104311991 2840485.9874962857 0, -1400497.9721403266 2840506.8058186676 0, -1400497.390664912 2840509.80477352 0, -1400452.1259811474 2840738.4564959686 0, -1400451.4587958015 2840741.808285925 0, -1400428.6235849268 2840856.2023643884 0, -1400420.8018900126 2840895.468983268 0, -1400420.069223923 2840899.301431375 0, -1400274.7199397993 2840870.543052567 0, -1400213.4646311947 2840858.3298914144 0, -1400023.1088309977 2840820.26744506 0, -1400022.4191629284 2840823.311960139 0, -1399739.523394895 2840764.6045222455 0, -1399736.5386692584 2840764.0057220142 0, -1399709.2365354546 2840758.5145079345 0, -1399626.1434866686 2840741.2589619365 0, -1399229.1764102448 2840662.2699850057 0, -1399306.9140804114 2840269.750971841 0, -1399306.9140826785 2840269.7509606453 0)), ((-1399229.1764102448 2840662.2699850057 0, -1399151.2946448606 2841054.7992079007 0, -1398754.3652302015 2840975.7562494082 0, -1398357.4368467703 2840896.7085765144 0, -1398434.9954991627 2840504.121791033 0, -1398832.0885730598 2840583.1832069866 0, -1399229.1764102448 2840662.2699850057 0)), ((-1410207.0886851817 2841171.569820003 0, -1410292.106862424 2841187.9271961376 0, -1410693.8600138929 2841265.8675316847 0, -1410641.7045664315 2841528.5669757756 0, -1410634.2942596902 2841565.9644431355 0, -1410616.0088154103 2841658.7990578404 0, -1410598.9623274822 2841744.276462479 0, -1410583.5237163594 2841822.194011335 0, -1410567.3071516913 2841904.0386808235 0, -1410550.4485024924 2841989.125877908 0, -1410546.7760295542 2842007.661339168 0, -1410538.1586854516 2842051.725978964 0, -1410475.0699257555 2842369.6151062693 0, -1410460.3759917119 2842444.344847481 0, -1410410.353163191 2842696.3028291394 0, -1410373.9500720813 2842880.5766738653 0, -1410314.8445090398 2842868.6933648163 0, -1410314.8445067066 2842868.6933643688 0, -1410074.8976017982 2842822.7379557453 0, -1409974.2514204897 2842803.210860995 0, -1409926.9607263294 2842794.120359546 0, -1409574.4517075391 2842726.364992527 0, -1409539.7596685698 2842719.476227892 0, -1409539.1167997618 2842719.3485740544 0, -1409539.1167996211 2842719.3485740265 0, -1409407.3427740564 2842693.406117487 0, -1409174.87310327 2842647.185105116 0, -1409135.3708942847 2842639.3610066515 0, -1408775.2871312238 2842568.0429873103 0, -1408775.2871312243 2842568.042987308 0, -1408775.2871312224 2842568.0429873075 0, -1408791.982561276 2842482.1825481723 0, -1408859.431612287 2842135.3088754904 0, -1408936.0102514483 2841742.172147534 0, -1409010.5622617726 2841352.679039439 0, -1409011.4184577104 2841348.2058882047 0, -1409086.8267116826 2840954.237889088 0, -1409107.1392109245 2840958.307386213 0, -1409374.2239804657 2841010.0749029545 0, -1409488.590801991 2841032.1093411823 0, -1409488.590810442 2841032.1093428046 0, -1409488.5908287365 2841032.1093463674 0, -1409735.5629954843 2841080.1273449566 0, -1409890.3520447423 2841110.0070721535 0, -1410027.3861210642 2841136.7169916257 0, -1410207.0886851817 2841171.569820003 0)), ((-1404413.0040087868 2845598.7170888362 0, -1404411.9634668445 2845599.4135239385 0, -1404403.6665685656 2845604.966773168 0, -1404367.6175215868 2845629.094281301 0, -1404365.3857084531 2845630.5880346466 0, -1404365.3856752666 2845630.588048675 0, -1404359.7842581766 2845634.337058641 0, -1404209.994285118 2845697.6924938657 0, -1403967.0449391939 2845739.4757514074 0, -1403962.6991410798 2845740.222877639 0, -1403925.888990231 2845756.5350805065 0, -1403811.697381762 2845808.3746001213 0, -1403763.0290770517 2845813.871618658 0, -1403678.995867877 2845799.875162555 0, -1403644.1093635445 2845787.7281875107 0, -1403561.9104531568 2845792.578875461 0, -1403546.0403714462 2845795.453029865 0, -1403471.1140033456 2845809.0260385834 0, -1403350.954397719 2845815.8751161206 0, -1403137.9662648952 2845786.6090687537 0, -1403161.1101112196 2845669.769369071 0, -1403161.3519901694 2845669.741687514 0, -1403161.3953671006 2845669.522701863 0, -1403166.1869040276 2845668.9743470913 0, -1403166.6076956226 2845666.871903373 0, -1403587.2478790737 2845618.1462674816 0, -1403645.7782884282 2845611.3678443404 0, -1403671.7299334654 2845608.36233764 0, -1403654.8238005526 2845469.124905376 0, -1403609.740873767 2845474.285456348 0, -1403190.3208668637 2845522.3126093117 0, -1403267.3277244826 2845133.712013439 0, -1403345.307317196 2844741.3896947694 0, -1403345.3073174688 2844741.3896933924 0, -1403351.278613076 2844742.575062426 0, -1403351.9856773617 2844739.030921994 0, -1403739.775040757 2844819.6959529603 0, -1403739.7750432093 2844819.695953447 0, -1403739.775176096 2844819.695979834 0, -1404142.2220031724 2844899.538941732 0, -1404538.6548402628 2844972.33059754 0, -1404934.1430632109 2845049.787531759 0, -1404468.8456640067 2845562.344196431 0, -1404413.0040087868 2845598.7170888362 0)), ((-1404384.173923037 2845913.506921877 0, -1404460.723088921 2845877.299411543 0, -1404498.694650209 2845842.6323788343 0, -1404543.1465726472 2845794.266376779 0, -1404553.1898897956 2845768.42480921 0, -1404560.4058094958 2845767.591449572 0, -1404562.263610549 2845762.872978879 0, -1404602.726522319 2845758.1884405124 0, -1404617.3759774447 2845736.0786963697 0, -1404641.038383801 2845700.366122346 0, -1404770.6570928784 2845608.785523316 0, -1404825.8077152742 2845544.414600234 0, -1404824.4991240369 2845551.0100588636 0, -1404835.93094067 2845538.743090079 0, -1404776.9849010152 2845832.7790643815 0, -1404698.3157223004 2846224.9341655592 0, -1404619.6501308896 2846617.0814418728 0, -1404613.1333087308 2846615.800988013 0, -1404611.440918708 2846624.325265719 0, -1404217.1673162603 2846545.7387325265 0, -1403822.8913253082 2846467.1743903724 0, -1403428.6090668149 2846388.631626333 0, -1403034.3220979962 2846310.11094714 0, -1403053.4782844791 2846213.634980691 0, -1403098.5972614503 2845986.403067261 0, -1403102.6692528867 2845986.22169955 0, -1403103.248347781 2845983.290500964 0, -1403194.7240722105 2845979.1141459174 0, -1403449.0559606147 2846028.010740485 0, -1403504.9632931324 2846028.6813831767 0, -1403799.7788403556 2846032.221859208 0, -1403917.369560205 2846021.144461339 0, -1404023.201279463 2846011.177178477 0, -1404120.1833968922 2845982.644777186 0, -1404347.9635557476 2845922.9921767535 0, -1404384.173923037 2845913.506921877 0)), ((-1397408.2962231054 2850092.3249010867 0, -1397368.4896856248 2850084.068534674 0, -1397446.3713279825 2849691.2643500497 0, -1397505.381414212 2849392.6996998107 0, -1397510.6108350344 2849365.822199518 0, -1397524.2513040218 2849298.457697818 0, -1397541.4491653107 2849211.7165610585 0, -1397541.458220491 2849211.6708892966 0, -1397542.5345600036 2849206.2421379318 0, -1397543.8495907197 2849199.6533351694 0, -1397552.4185829689 2849156.451312542 0, -1397575.9850958055 2849037.5695722825 0, -1397592.0332196734 2848956.627131109 0, -1397592.679842527 2848953.3228822346 0, -1397592.6798425396 2848953.3228821703 0, -1397602.13302944 2848905.6434157547 0, -1397665.8361152133 2848583.3899085936 0, -1397680.0171525239 2848512.827412834 0, -1397680.0171525334 2848512.8274127864 0, -1397929.700960232 2848562.7028559577 0, -1397929.7009632865 2848562.702856566 0, -1397948.4323890347 2848566.4242267665 0, -1397957.4309592475 2848568.2419514772 0, -1397957.4309620752 2848568.241952046 0, -1398077.2551434217 2848592.176531594 0, -1398141.5814011388 2848605.029787731 0, -1398239.0745437716 2848624.510235964 0, -1398247.1236719787 2848626.1050571734 0, -1398282.7133075856 2848633.219462183 0, -1398287.580911698 2848634.192208714 0, -1398327.5059190358 2848642.169873064 0, -1398332.0947335428 2848643.086969197 0, -1398372.692625795 2848651.1939333444 0, -1398377.8822906353 2848652.2453921833 0, -1398377.8822907384 2848652.2453922043 0, -1398377.8822960923 2848652.2453932827 0, -1398474.4887164899 2848671.5479072505 0, -1398871.7176727587 2848750.941513455 0, -1398936.6503813192 2848763.925655422 0, -1398962.2122963727 2848769.0345055317 0, -1399102.7436877913 2848797.11353484 0, -1399111.7925354156 2848798.9398238114 0, -1399113.3217560383 2848799.2471367856 0, -1399268.9442821615 2848830.357851166 0, -1399266.4973957373 2848842.226063975 0, -1399231.7310575226 2849019.0364407757 0, -1399231.7310429218 2849019.036515031 0, -1399221.9107939033 2849069.0883870637 0, -1399215.8337490482 2849099.6392980004 0, -1399215.8337490472 2849099.639298005 0, -1399215.833740717 2849099.639340032 0, -1399191.420180221 2849223.420864117 0, -1399191.322303488 2849223.9171182876 0, -1399113.7035125983 2849617.4718418084 0, -1399036.0835453114 2850011.0212396816 0, -1398958.4665678807 2850404.5660594977 0, -1398945.88544305 2850402.2433631923 0, -1398647.0857153283 2850341.77419907 0, -1398647.0857049285 2850341.774196965 0, -1398647.085704724 2850341.7741969237 0, -1398622.6991095608 2850336.8458357486 0, -1398618.7863314683 2850336.06729265 0, -1398618.7863266538 2850336.0672917007 0, -1398560.9794564047 2850324.409822854 0, -1398193.5005080379 2850250.547556947 0, -1398163.4883337207 2850244.272879605 0, -1397765.99050446 2850164.157983164 0, -1397408.2962231054 2850092.3249010867 0)), ((-1408499.7917902402 2851897.0108265877 0, -1408421.0447701633 2852289.2328041033 0, -1408208.4406804384 2852246.8743553446 0, -1408024.111393916 2852209.763787432 0, -1407803.8467946316 2852165.883525409 0, -1407627.1719187878 2852130.313602257 0, -1407230.2294260436 2852050.8889755737 0, -1407230.2294255465 2852050.888975477 0, -1407206.2683501462 2852046.303831964 0, -1406833.2804088348 2851971.486434671 0, -1406833.280408835 2851971.4864346697 0, -1406911.933817793 2851579.414764962 0, -1406921.6758014641 2851530.0046396935 0, -1406934.686355972 2851465.14776617 0, -1406956.335386052 2851357.2290452607 0, -1406990.586042128 2851187.337697579 0, -1406990.5860421804 2851187.3376973188 0, -1406990.5860422545 2851187.3376969495 0, -1407041.0215364834 2850935.08214724 0, -1407069.2414205894 2850795.256210503 0, -1407069.2414206765 2850795.2562100706 0, -1407069.2414206867 2850795.2562100184 0, -1407073.5684860025 2850772.8424741207 0, -1407147.89795659 2850403.1700436547 0, -1407147.8979565974 2850403.170043656 0, -1407147.897956598 2850403.1700436533 0, -1407506.3690000873 2850474.723267223 0, -1407544.9384991385 2850482.421997814 0, -1407941.9745221676 2850561.6962001207 0, -1408339.0062130108 2850640.9927756977 0, -1408736.0331859435 2850720.3115733187 0, -1408657.41158823 2851111.919579926 0, -1408657.2847018465 2851112.5515910415 0, -1408578.5377025602 2851504.7836576267 0, -1408499.7917902402 2851897.0108265877 0)), ((-1402322.4997742055 2855962.8549554977 0, -1401926.2423490663 2855884.0684591965 0, -1401529.9818892553 2855805.3075370626 0, -1401133.7178690603 2855726.5661011315 0, -1401213.211228292 2855335.412905123 0, -1401292.708138397 2854944.2551045995 0, -1401372.2039204885 2854553.0919847465 0, -1401451.7031004892 2854161.9246495627 0, -1401847.939906079 2854240.6579817794 0, -1402244.174336076 2854319.414166907 0, -1402640.4039476456 2854398.195590499 0, -1403036.6295266182 2854476.9962373967 0, -1402957.1582407928 2854868.1687561497 0, -1402877.6877139623 2855259.339419323 0, -1402798.2189316931 2855650.5022341553 0, -1402718.750697533 2856041.6632575803 0, -1402322.4997742055 2855962.8549554977 0)), ((-1411751.5853603992 2856418.185144432 0, -1411754.7571084467 2856429.033555226 0, -1411767.7582414288 2856473.501728358 0, -1411817.3561956498 2856643.1425894992 0, -1411842.2963358818 2856728.4480426703 0, -1411857.2971659566 2856779.7566173365 0, -1411866.2335776836 2856810.323187832 0, -1411899.5147161097 2856924.1581729716 0, -1411899.2923966853 2856930.5015921816 0, -1411897.9417615307 2856969.061157462 0, -1411894.9402896597 2857054.74085981 0, -1411894.5358408932 2857066.285733073 0, -1411894.0926921885 2857078.934847568 0, -1411893.5171049975 2857095.3595575998 0, -1411891.713688685 2857146.8214332475 0, -1411889.994330014 2857195.9125946364 0, -1411889.699684305 2857204.325522127 0, -1411880.874398725 2857470.4536910965 0, -1411878.0360349421 2857552.343632654 0, -1411875.6033314364 2857624.912060565 0, -1411877.2522324275 2857628.9538111114 0, -1411915.182499596 2857721.932867112 0, -1411933.3960081232 2857766.5799572086 0, -1411978.6628281383 2857877.543262183 0, -1411987.1789034253 2857898.418955808 0, -1411967.8125782465 2857894.7388543542 0, -1411940.9460620254 2857889.3657909026 0, -1411827.0057558136 2857866.5978943333 0, -1411816.2609931997 2857864.4504358424 0, -1411785.6653254726 2857858.335715912 0, -1411778.7458917818 2857856.7582134116 0, -1411778.7458915478 2857856.758213361 0, -1411594.861806844 2857819.9848252423 0, -1411383.7384575654 2857777.7640921324 0, -1411367.0593044949 2857774.617511555 0, -1410990.311091655 2857698.9297966924 0, -1410858.0004306268 2857672.622335774 0, -1410596.879148821 2857620.1174235255 0, -1410621.9852533883 2857491.62132465 0, -1410633.7672996472 2857431.7274165326 0, -1410674.0526222952 2857227.8057096056 0, -1410674.0526223222 2857227.805709468 0, -1410751.224144693 2856835.4917604737 0, -1410757.8768594344 2856800.8060144023 0, -1410820.825048066 2856480.8087421665 0, -1410828.3986047867 2856443.173116284 0, -1410828.3986047988 2856443.1731162234 0, -1410828.3986048105 2856443.173116164 0, -1410842.1263099334 2856372.5611441107 0, -1410905.5745906155 2856050.8465852523 0, -1411295.5805096321 2856130.8219032804 0, -1411432.25054098 2856158.360234526 0, -1411432.2505409804 2856158.360234527 0, -1411432.3744690558 2856158.659060573 0, -1411528.0464481325 2856236.440972607 0, -1411560.3916010382 2856262.7377897943 0, -1411667.3655141646 2856349.7080069594 0, -1411702.6279902614 2856378.379090404 0, -1411740.73912433 2856409.366361044 0, -1411751.5853603992 2856418.185144432 0)), ((-1405261.3863524538 2859814.963898068 0, -1405651.2703595373 2859892.5344997076 0, -1406048.3939748404 2859971.7027081377 0, -1406445.5149132037 2860050.8938099025 0, -1406842.6286486182 2860130.1098150183 0, -1406842.628648618 2860130.1098150196 0, -1406764.8265913033 2860522.0183203532 0, -1406688.7504382622 2860905.23269522 0, -1406687.0248609448 2860913.924854412 0, -1406687.0248609437 2860913.924854418 0, -1406415.590490284 2860859.6128464383 0, -1406290.115452382 2860834.5054980735 0, -1405897.4905057237 2860756.1532146623 0, -1405893.2084571854 2860755.084839173 0, -1405815.6258750965 2861146.7138585607 0, -1406212.4251978938 2861226.269456487 0, -1406609.224541734 2861305.8234384237 0, -1406531.4236872834 2861697.717321509 0, -1406531.4236872534 2861697.717321503 0, -1406531.4236872522 2861697.717321509 0, -1406134.7369737187 2861618.013712855 0, -1405738.045266009 2861538.3353076545 0, -1405341.3495085759 2861458.6764138103 0, -1404944.6466850971 2861379.042249062 0, -1405022.0205961196 2860987.6359433997 0, -1405099.3936611253 2860596.2250118344 0, -1405176.7677404573 2860204.8092027605 0, -1404780.8769870354 2860124.730539985 0, -1404858.3628771487 2859733.3601081683 0, -1404935.3719751574 2859342.672009466 0, -1405331.1001697828 2859423.1280607716 0, -1405254.1434443628 2859813.3853914333 0, -1405261.3863524538 2859814.963898068 0)), ((-1402682.2020684432 2864118.7237778557 0, -1402695.4529211784 2864121.2283095215 0, -1402695.4529211782 2864121.228309523 0, -1402616.8936437613 2864513.0297153555 0, -1402538.3358605783 2864904.823133617 0, -1402499.8153482743 2865096.9325434817 0, -1402459.7765047003 2865296.6141715446 0, -1402419.7474271564 2865496.252592065 0, -1402381.2202299368 2865688.4006322375 0, -1402381.2202299358 2865688.4006322417 0, -1401983.5451695155 2865608.8553613233 0, -1401712.7970666003 2865554.720197429 0, -1401585.8632989998 2865529.3320246567 0, -1401188.179284525 2865449.831439479 0, -1401188.1792117932 2865449.831424936 0, -1401097.3997936426 2865431.6841614405 0, -1401084.8622124526 2865429.1840025107 0, -1400799.226584094 2865372.3078978863 0, -1400790.4886198821 2865370.35311039 0, -1400868.6112097064 2864978.9369326024 0, -1400945.8802026587 2864590.1986702695 0, -1400946.7321918367 2864587.5186793273 0, -1401024.8546978398 2864196.092250667 0, -1401100.9681356936 2863813.8579939683 0, -1401102.9804730942 2863804.661391134 0, -1401161.397036985 2863816.255982978 0, -1401501.1095115985 2863883.7670430006 0, -1401558.569074346 2863895.1879364145 0, -1401899.2323785443 2863962.904431385 0, -1401955.7386749384 2863974.1206539576 0, -1402297.3480475233 2864042.044840975 0, -1402352.9085788366 2864053.0954119097 0, -1402682.2020684432 2864118.7237778557 0)), ((-1411465.037336772 2865648.779537992 0, -1411463.8557415532 2865655.0362547883 0, -1411467.7572204815 2865655.390586278 0, -1411528.471929807 2865656.642773342 0, -1411528.4719302277 2865656.6427733493 0, -1411528.471930238 2865656.6427733507 0, -1411528.4719302412 2865656.6427733507 0, -1411569.6250164183 2865661.9779159166 0, -1411578.782938681 2865663.366841497 0, -1411605.6501287578 2865674.490354063 0, -1411625.477942975 2865682.6947615296 0, -1411631.7469223023 2865685.3064114386 0, -1411632.7949084023 2865685.7423111056 0, -1411635.878725861 2865685.393298609 0, -1411647.15672865 2865684.1156663178 0, -1411652.734374543 2865683.483661498 0, -1411663.069627925 2865682.308265712 0, -1411676.9610435506 2865680.725924123 0, -1411731.4632386134 2865723.2860093727 0, -1411740.6671240507 2865730.519389325 0, -1411822.090020838 2865718.2191672903 0, -1411838.3978266304 2865715.9588456973 0, -1411841.073689812 2865717.1605165387 0, -1411983.169821221 2865779.4717531553 0, -1411983.1698278135 2865779.4717560387 0, -1411999.7797165555 2865786.7246760647 0, -1412158.2912243297 2865835.9466782827 0, -1412170.146075653 2865836.9489773572 0, -1412170.146076222 2865836.9489774047 0, -1412229.6105864234 2865841.7906655665 0, -1412229.6105864223 2865841.790665572 0, -1412229.6105864225 2865841.790665572 0, -1412229.6105863927 2865841.7906657173 0, -1412219.1846687484 2865892.884224412 0, -1412162.0192036116 2866176.968186281 0, -1412082.825008011 2866569.0058447286 0, -1412002.6728112134 2866961.1972452626 0, -1411922.5221962316 2867353.380643108 0, -1411922.5221962258 2867353.3806431065 0, -1411922.522196224 2867353.3806431163 0, -1411583.5471875449 2867284.2856640294 0, -1411524.470183467 2867272.0276043857 0, -1411445.3103906135 2867256.03696549 0, -1411360.55465754 2867238.708295354 0, -1411126.4154879246 2867190.697131833 0, -1411025.867544467 2867170.3460400575 0, -1410917.9101386506 2867148.296874894 0, -1410817.3561835214 2867127.759786799 0, -1410728.3555018317 2867109.3920901567 0, -1410728.3549554553 2867109.3919785875 0, -1410610.287801935 2867085.2829328044 0, -1410330.3074244468 2867028.109796696 0, -1410330.291306805 2867028.1065054135 0, -1410361.2985384562 2866873.7711350676 0, -1410409.33354803 2866634.6905706557 0, -1410420.9139694646 2866577.055654584 0, -1410440.2146718572 2866480.997461124 0, -1410440.2146719096 2866480.9974608603 0, -1410456.6149111663 2866398.174093309 0, -1410463.2236422338 2866365.1634405 0, -1410488.222008319 2866241.2386903674 0, -1410504.0888303516 2866161.32310462 0, -1410519.0021884008 2866088.0397656164 0, -1410519.002188406 2866088.0397655913 0, -1410566.296370515 2865852.6473873486 0, -1410597.9484032183 2865695.10541922 0, -1410644.2002541109 2865464.0360314716 0, -1410644.2099788839 2865464.0379698332 0, -1410644.2113585516 2865464.0310786646 0, -1410684.423421186 2865472.053394944 0, -1411044.5673082075 2865544.3390496573 0, -1411064.664278303 2865548.3758619865 0, -1411303.885356992 2865596.5309854182 0, -1411444.901632407 2865624.715773975 0, -1411454.7045603914 2865626.808822695 0, -1411468.8876433342 2865629.512212369 0, -1411468.8876433324 2865629.512212379 0, -1411465.037336772 2865648.779537992 0)), ((-1405352.3578766033 2869543.935077524 0, -1405359.1363504976 2869545.2042935197 0, -1405436.3132154464 2869560.2322490425 0, -1405502.746418892 2869573.2515146 0, -1405502.7464338238 2869573.2515175208 0, -1405720.6097105232 2869615.720096893 0, -1406118.040747909 2869693.2168943826 0, -1406295.4979188778 2869727.8309028526 0, -1406335.326025477 2869735.548965003 0, -1406368.3830205046 2869742.047260953 0, -1406368.3830230972 2869742.047261461 0, -1406515.4696160685 2869770.7362509747 0, -1406515.4696160683 2869770.736250976 0, -1406515.3518045028 2869771.324431194 0, -1406436.8880400027 2870163.058756294 0, -1406358.3075719213 2870555.3763669888 0, -1406349.6235684261 2870598.7326819636 0, -1406349.6235644566 2870598.7327020443 0, -1406348.2495920586 2870605.7389051924 0, -1406343.9503185805 2870627.2036582665 0, -1406334.9120333896 2870672.1828832966 0, -1406279.7301098744 2870947.689329546 0, -1406259.8342604002 2871047.0207821187 0, -1406256.6776818188 2871062.9237264954 0, -1406248.9494264596 2871101.3638142054 0, -1406201.1516861857 2871339.9969154075 0, -1405935.8783990357 2871288.0464658416 0, -1405919.2268095443 2871284.7765399343 0, -1405859.9066085038 2871273.1582050133 0, -1405856.2419319113 2871272.450294864 0, -1405856.241927392 2871272.4502939982 0, -1405803.751681128 2871262.170407299 0, -1405658.300430607 2871233.6943604634 0, -1405644.932170153 2871231.0641286485 0, -1405623.858496985 2871226.937981929 0, -1405605.0992181995 2871223.278679066 0, -1405605.0992040872 2871223.278676319 0, -1405406.3471053601 2871184.366241646 0, -1405435.624495818 2871038.2277601827 0, -1405437.0592010934 2871031.0664098286 0, -1405441.9988417523 2871006.4998400114 0, -1405484.3701475295 2870794.999082076 0, -1405484.9057895474 2870792.2393457848 0, -1405479.7815442246 2870791.226744264 0, -1405424.8324013767 2870780.4771098006 0, -1405420.8968640964 2870779.7077110303 0, -1405370.7645056879 2870769.9052323746 0, -1405367.6517246566 2870769.2986274436 0, -1405283.9653302229 2870752.933274581 0, -1405255.9106829148 2870747.465511902 0, -1405255.9106593088 2870747.46550731 0, -1405205.8767456764 2870737.7331411466 0, -1405087.490981406 2870714.534637766 0, -1405066.3558166963 2870710.5732503003 0, -1404937.6800193107 2870685.241462984 0, -1404912.420841931 2870680.2812086833 0, -1404873.690080004 2870672.728276086 0, -1404690.0778117212 2870636.8252614536 0, -1404690.077166699 2870636.8251353293 0, -1404690.0771666993 2870636.825135328 0, -1404708.0471434693 2870547.146432178 0, -1404710.958022651 2870532.710837276 0, -1404753.5632293806 2870320.0914300634 0, -1404767.9136741732 2870248.445385562 0, -1404768.6279536458 2870244.8196088024 0, -1404768.6279536616 2870244.819608721 0, -1404775.7641339956 2870209.20661129 0, -1404775.7641365211 2870209.206598999 0, -1404776.9359453998 2870203.4499911657 0, -1404809.6746020482 2870040.0693464084 0, -1404828.469240713 2869946.2757398025 0, -1404829.4227403163 2869941.5171959335 0, -1404831.863324543 2869929.2458460294 0, -1404847.1798434148 2869852.8091909704 0, -1404851.4089969185 2869831.7039236957 0, -1404851.4422845743 2869831.5378041933 0, -1404852.1575244702 2869828.0605850974 0, -1404853.231110614 2869822.7023808896 0, -1404856.9175901003 2869804.3054733314 0, -1404883.9239550708 2869669.5310635734 0, -1404889.6944281512 2869640.6415555426 0, -1404889.6944321946 2869640.6415352616 0, -1404925.732661221 2869460.793662609 0, -1405323.1722710785 2869538.245600288 0, -1405352.3578766033 2869543.935077524 0)), ((-1403270.9110435373 2873607.989720598 0, -1403195.57265247 2873987.095011088 0, -1402798.6169425067 2873907.8261163756 0, -1402874.1480264233 2873528.383814522 0, -1402952.0604383987 2873136.965264704 0, -1403348.7412445976 2873216.3452473097 0, -1403270.9110435373 2873607.989720598 0)), ((-1400722.020211627 2873987.416916897 0, -1400659.8349719865 2874300.9579526847 0, -1400582.1008802357 2874692.897713141 0, -1400504.368199048 2875084.8295678613 0, -1400504.3681990472 2875084.8295678655 0, -1400306.06796822 2875046.0779310446 0, -1400108.2805656404 2875006.994913384 0, -1399712.1886875827 2874929.1824742686 0, -1399316.0923516774 2874851.392322538 0, -1398919.9918312414 2874773.6246947986 0, -1398997.4825770769 2874381.3695183387 0, -1399074.9721307347 2873989.109292349 0, -1399152.464837142 2873596.8441945347 0, -1399229.9583728071 2873204.574122286 0, -1399626.3009079173 2873282.6651033484 0, -1400022.6398035127 2873360.7752654627 0, -1400418.9757098868 2873438.911310901 0, -1400341.2951306698 2873830.9661018522 0, -1400408.590619487 2873844.220564607 0, -1400737.569628418 2873909.015992905 0, -1400737.5696284168 2873909.0159929106 0, -1400737.5696284187 2873909.015992911 0, -1400722.020211627 2873987.416916897 0)), ((-1409103.6964492481 2875025.2421185113 0, -1409141.8900567754 2875032.891256656 0, -1409213.6801065572 2875047.2731291484 0, -1409213.6801090706 2875047.273129647 0, -1409229.77988655 2875050.449152512 0, -1409285.8021089113 2875061.721309533 0, -1409285.8021396676 2875061.7213157113 0, -1409535.654514666 2875111.773087116 0, -1409929.4117891053 2875190.679700427 0, -1409971.24784557 2875199.065926775 0, -1409971.2478463105 2875199.065926921 0, -1409978.7519803427 2875200.531137577 0, -1410108.979261336 2875226.637376353 0, -1410140.157719893 2875232.924347864 0, -1410323.172103583 2875269.6090371227 0, -1410323.1721035815 2875269.609037131 0, -1410323.1721035817 2875269.609037131 0, -1410280.0390395173 2875485.7118710545 0, -1410275.657886319 2875507.7470515314 0, -1410272.7716184133 2875522.122472482 0, -1410244.8465344294 2875662.031449576 0, -1410244.846486525 2875662.031689817 0, -1410238.80266182 2875692.360027673 0, -1410188.7019879804 2875943.3155002077 0, -1410185.8364133637 2875957.6702931076 0, -1410166.5198291473 2876054.448420859 0, -1410154.9493124203 2876112.3908099523 0, -1410129.6492050847 2876239.1153764776 0, -1410097.0531707695 2876404.0092286854 0, -1410096.267817752 2876406.490527884 0, -1410095.9545911942 2876406.9131187014 0, -1410092.6124654415 2876411.4155137967 0, -1410071.9405331241 2876439.594348282 0, -1410067.334844834 2876445.872557595 0, -1410044.8896179674 2876476.467052874 0, -1410017.2528691767 2876514.1379344515 0, -1410017.2528691764 2876514.1379344515 0, -1410017.2513635792 2876514.139986689 0, -1409975.5495828802 2876541.3013308863 0, -1409950.1803787204 2876557.8212493835 0, -1409908.6595203627 2876584.8949637697 0, -1409866.487935356 2876612.392758426 0, -1409766.4990217146 2876677.5969618005 0, -1409766.4997185215 2876677.6499651307 0, -1409766.2500051307 2876677.812799691 0, -1409766.6451122717 2876704.2036529 0, -1409767.1408562034 2876737.3104113834 0, -1409767.507660834 2876761.8052125834 0, -1409769.9336998635 2876795.1547505893 0, -1409764.5592822868 2876794.095048755 0, -1409627.5944055112 2876766.6532114935 0, -1409510.6739233304 2876743.2241767757 0, -1409446.8540509548 2876730.4106893907 0, -1409310.6548475022 2876703.0646280306 0, -1409263.1621494931 2876693.52887364 0, -1409260.287299188 2876692.9515570784 0, -1409230.218035185 2876686.8663708684 0, -1408832.1384908531 2876608.0227922006 0, -1408774.6639410295 2876596.8008374856 0, -1408728.6500602255 2876587.657983948 0, -1408514.9915482828 2876545.2276930353 0, -1408514.9915142735 2876545.2276862813 0, -1408455.7443594562 2876533.474764181 0, -1408452.775912659 2876532.908685063 0, -1408434.0567597842 2876529.2021547086 0, -1408446.2223965924 2876468.189760085 0, -1408486.3784147138 2876266.7236018917 0, -1408489.3887333323 2876251.6218461953 0, -1408512.5581591323</t>
+          <t>MULTIPOLYGON Z (((-1406379.8180101914 2835502.9676008387 0, -1406473.9785516895 2835521.734531294 0, -1406778.7770429626 2835582.4882667917 0, -1406872.8312997553 2835601.148932945 0, -1406791.7645722493 2835992.9266004586 0, -1406710.698745883 2836384.702508994 0, -1406629.6366764735 2836776.4711096287 0, -1406548.5739271764 2837168.2345223785 0, -1406152.1431418383 2837088.956904065 0, -1406087.6405494164 2837076.280484532 0, -1405796.91670816 2837018.1569047323 0, -1405755.7083628573 2837009.698301688 0, -1405535.803621465 2836965.9663151815 0, -1405487.176097592 2836956.2471401114 0, -1405359.2691901615 2836930.461773824 0, -1405080.115136758 2836874.9046132243 0, -1404962.8255844747 2836851.2476163614 0, -1405025.8156075906 2836537.4335374683 0, -1405029.769174486 2836517.7370062955 0, -1405041.4965421397 2836459.306839623 0, -1405041.4965422011 2836459.306839316 0, -1405081.6600892353 2836258.4058300443 0, -1405108.2831449925 2836126.578187748 0, -1405120.0309416638 2836067.337313631 0, -1405133.2551556446 2836000.645850542 0, -1405186.659309687 2835735.386966785 0, -1405188.114813715 2835727.329112005 0, -1405192.8804176834 2835703.5856685042 0, -1405198.701406638 2835675.389715876 0, -1405261.8129454285 2835360.1547357994 0, -1405265.1738896933 2835344.2151984107 0, -1405277.2234497615 2835283.407895384 0, -1405277.2234497755 2835283.4078953867 0, -1405277.2234497757 2835283.4078953853 0, -1405581.9305416776 2835344.089946119 0, -1405676.1759969064 2835362.862839606 0, -1405980.8366573509 2835423.550296702 0, -1406075.138144352 2835442.2583379205 0, -1406202.3274685177 2835467.601562032 0, -1406379.8180101914 2835502.9676008387 0)), ((-1399356.4079068387 2840020.2810208434 0, -1399368.1809894112 2839960.4057747424 0, -1399384.6546780465 2839877.227700831 0, -1399462.396458146 2839484.6995438226 0, -1399540.139008013 2839092.1665506647 0, -1399542.905688448 2839092.835199241 0, -1399556.3294038298 2839095.3861888293 0, -1399556.3294040805 2839095.3861888773 0, -1399561.6720821362 2839096.376602012 0, -1399582.007635379 2839100.423022579 0, -1399599.5649045492 2839103.916675662 0, -1399623.3376730068 2839108.6470440533 0, -1399644.5027693652 2839112.8586522965 0, -1399667.8546858106 2839117.505222619 0, -1399689.9714188937 2839121.9060038663 0, -1399712.3326666437 2839126.3553711157 0, -1399735.4324632378 2839130.9517879887 0, -1399753.6615634388 2839134.578885354 0, -1399780.8692110055 2839139.992492276 0, -1399798.1407629494 2839143.429084783 0, -1399826.33910559 2839149.039729029 0, -1399842.651850635 2839152.2853515954 0, -1399871.8019453995 2839158.085069711 0, -1399883.9572934853 2839160.5036009005 0, -1399916.771608468 2839167.0324040405 0, -1399928.497425498 2839169.3652046104 0, -1399934.4273121587 2839170.492037641 0, -1399937.3344581702 2839171.1505293464 0, -1399937.334458662 2839171.150529451 0, -1399937.3344698094 2839171.1505316654 0, -1399961.7740465652 2839175.991441545 0, -1399972.9727293379 2839178.2173738675 0, -1400007.6713144428 2839185.123969481 0, -1400014.3015124146 2839186.44347234 0, -1400053.0843019113 2839194.164184724 0, -1400059.1674090049 2839195.3749906607 0, -1400062.5253671096 2839196.043416641 0, -1400098.5195565978 2839203.2079879213 0, -1400103.2938011107 2839204.1582646235 0, -1400135.8492566794 2839210.638179495 0, -1400143.9549004098 2839212.251141099 0, -1400147.7740981488 2839213.0111707496 0, -1400189.1188868866 2839221.238374427 0, -1400322.934807602 2839247.8660599813 0, -1400331.4578416802 2839249.561483696 0, -1400334.5232879098 2839250.1564733693 0, -1400337.289539137 2839250.8269082224 0, -1400438.6676987924 2839270.9013746134 0, -1400616.4727830754 2839306.2846389473 0, -1400666.7624768384 2839316.2673303704 0, -1400731.7096861927 2839329.18493668 0, -1400734.4720727175 2839329.8709867066 0, -1400774.2737872985 2839337.662505503 0, -1400819.7837660834 2839346.7515740218 0, -1401125.8721471464 2839407.6680866037 0, -1401128.8917457967 2839408.235767459 0, -1401123.9478869513 2839432.9798185662 0, -1401114.9923184975 2839478.068050874 0, -1401105.4885421125 2839525.9158027335 0, -1401103.154785328 2839537.809666259 0, -1401103.15478518 2839537.809667019 0, -1401067.6565216575 2839720.071360423 0, -1401063.830226231 2839739.28926802 0, -1401063.2021711767 2839742.434400068 0, -1401053.3518599859 2839788.545631688 0, -1401050.9229196983 2839800.7740466096 0, -1401050.9229196971 2839800.7740466157 0, -1401053.6475980359 2839801.596686764 0, -1400999.4443926136 2840062.6907491884 0, -1400998.724069705 2840066.308780294 0, -1400989.0886561542 2840114.569291522 0, -1400975.3905077311 2840183.1795261377 0, -1400973.5361308325 2840190.3820250407 0, -1400973.536130806 2840190.382025154 0, -1400972.9550610757 2840193.3075143024 0, -1400954.6895441287 2840190.4323968505 0, -1400920.226759528 2840183.5676653488 0, -1400578.8062332084 2840115.124226884 0, -1400575.8805057171 2840114.2936359607 0, -1400575.7633936796 2840117.3285491103 0, -1400574.844702643 2840122.2522871094 0, -1400574.022585394 2840126.3318334757 0, -1400566.8949736727 2840162.4611979346 0, -1400542.6533913193 2840284.271411241 0, -1400539.2966141847 2840301.1361504267 0, -1400517.715227514 2840409.5622253655 0, -1400512.0344126902 2840438.1135863895 0, -1400502.104311991 2840485.9874962857 0, -1400497.9721403266 2840506.8058186676 0, -1400497.390664912 2840509.80477352 0, -1400452.1259811474 2840738.4564959686 0, -1400451.4587958015 2840741.808285925 0, -1400428.6235849268 2840856.2023643884 0, -1400420.8018900126 2840895.468983268 0, -1400420.069223923 2840899.301431375 0, -1400274.7199397993 2840870.543052567 0, -1400213.4646311947 2840858.3298914144 0, -1400023.1088309977 2840820.26744506 0, -1400022.4191629284 2840823.311960139 0, -1399739.523394895 2840764.6045222455 0, -1399736.5386692584 2840764.0057220142 0, -1399709.2365354546 2840758.5145079345 0, -1399626.1434866686 2840741.2589619365 0, -1399229.1764102448 2840662.2699850057 0, -1399306.9140804114 2840269.750971841 0, -1399306.9140826785 2840269.7509606453 0, -1399308.926485363 2840259.6770075844 0, -1399310.6939220119 2840250.9220541627 0, -1399335.4899758273 2840125.914068922 0, -1399347.1961440216 2840066.79943821 0, -1399356.4079068387 2840020.2810208434 0)), ((-1399229.1764102448 2840662.2699850057 0, -1399151.2946448606 2841054.7992079007 0, -1398754.3652302015 2840975.7562494082 0, -1398357.4368467703 2840896.7085765144 0, -1398434.9954991627 2840504.121791033 0, -1398832.0885730598 2840583.1832069866 0, -1399229.1764102448 2840662.2699850057 0)), ((-1410207.0886851817 2841171.569820003 0, -1410292.106862424 2841187.9271961376 0, -1410693.8600138929 2841265.8675316847 0, -1410641.7045664315 2841528.5669757756 0, -1410634.2942596902 2841565.9644431355 0, -1410616.0088154103 2841658.7990578404 0, -1410598.9623274822 2841744.276462479 0, -1410583.5237163594 2841822.194011335 0, -1410567.3071516913 2841904.0386808235 0, -1410550.4485024924 2841989.125877908 0, -1410546.7760295542 2842007.661339168 0, -1410538.1586854516 2842051.725978964 0, -1410475.0699257555 2842369.6151062693 0, -1410460.3759917119 2842444.344847481 0, -1410410.353163191 2842696.3028291394 0, -1410373.9500720813 2842880.5766738653 0, -1410314.8445090398 2842868.6933648163 0, -1410314.8445067066 2842868.6933643688 0, -1410074.8976017982 2842822.7379557453 0, -1409974.2514204897 2842803.210860995 0, -1409926.9607263294 2842794.120359546 0, -1409574.4517075391 2842726.364992527 0, -1409539.7596685698 2842719.476227892 0, -1409539.1167997618 2842719.3485740544 0, -1409539.1167996211 2842719.3485740265 0, -1409407.3427740564 2842693.406117487 0, -1409174.87310327 2842647.185105116 0, -1409135.3708942847 2842639.3610066515 0, -1408775.2871312238 2842568.0429873103 0, -1408775.2871312243 2842568.042987308 0, -1408775.2871312224 2842568.0429873075 0, -1408791.982561276 2842482.1825481723 0, -1408859.431612287 2842135.3088754904 0, -1408936.0102514483 2841742.172147534 0, -1409010.5622617726 2841352.679039439 0, -1409011.4184577104 2841348.2058882047 0, -1409086.8267116826 2840954.237889088 0, -1409107.1392109245 2840958.307386213 0, -1409374.2239804657 2841010.0749029545 0, -1409488.590801991 2841032.1093411823 0, -1409488.590810442 2841032.1093428046 0, -1409488.5908287365 2841032.1093463674 0, -1409735.5629954843 2841080.1273449566 0, -1409890.3520447423 2841110.0070721535 0, -1410027.3861210642 2841136.7169916257 0, -1410207.0886851817 2841171.569820003 0)), ((-1404413.0040087868 2845598.7170888362 0, -1404411.9634668445 2845599.4135239385 0, -1404403.6665685656 2845604.966773168 0, -1404367.6175215868 2845629.094281301 0, -1404365.3857084531 2845630.5880346466 0, -1404365.3856752666 2845630.588048675 0, -1404359.7842581766 2845634.337058641 0, -1404209.994285118 2845697.6924938657 0, -1403967.0449391939 2845739.4757514074 0, -1403962.6991410798 2845740.222877639 0, -1403925.888990231 2845756.5350805065 0, -1403811.697381762 2845808.3746001213 0, -1403763.0290770517 2845813.871618658 0, -1403678.995867877 2845799.875162555 0, -1403644.1093635445 2845787.7281875107 0, -1403561.9104531568 2845792.578875461 0, -1403546.0403714462 2845795.453029865 0, -1403471.1140033456 2845809.0260385834 0, -1403350.954397719 2845815.8751161206 0, -1403137.9662648952 2845786.6090687537 0, -1403161.1101112196 2845669.769369071 0, -1403161.3519901694 2845669.741687514 0, -1403161.3953671006 2845669.522701863 0, -1403166.1869040276 2845668.9743470913 0, -1403166.6076956226 2845666.871903373 0, -1403587.2478790737 2845618.1462674816 0, -1403645.7782884282 2845611.3678443404 0, -1403671.7299334654 2845608.36233764 0, -1403654.8238005526 2845469.124905376 0, -1403609.740873767 2845474.285456348 0, -1403190.3208668637 2845522.3126093117 0, -1403267.3277244826 2845133.712013439 0, -1403345.307317196 2844741.3896947694 0, -1403345.3073174688 2844741.3896933924 0, -1403351.278613076 2844742.575062426 0, -1403351.9856773617 2844739.030921994 0, -1403739.775040757 2844819.6959529603 0, -1403739.7750432093 2844819.695953447 0, -1403739.775176096 2844819.695979834 0, -1404142.2220031724 2844899.538941732 0, -1404538.6548402628 2844972.33059754 0, -1404934.1430632109 2845049.787531759 0, -1404468.8456640067 2845562.344196431 0, -1404413.0040087868 2845598.7170888362 0)), ((-1404384.173923037 2845913.506921877 0, -1404460.723088921 2845877.299411543 0, -1404498.694650209 2845842.6323788343 0, -1404543.1465726472 2845794.266376779 0, -1404553.1898897956 2845768.42480921 0, -1404560.4058094958 2845767.591449572 0, -1404562.263610549 2845762.872978879 0, -1404602.726522319 2845758.1884405124 0, -1404617.3759774447 2845736.0786963697 0, -1404641.038383801 2845700.366122346 0, -1404770.6570928784 2845608.785523316 0, -1404825.8077152742 2845544.414600234 0, -1404824.4991240369 2845551.0100588636 0, -1404835.93094067 2845538.743090079 0, -1404776.9849010152 2845832.7790643815 0, -1404698.3157223004 2846224.9341655592 0, -1404619.6501308896 2846617.0814418728 0, -1404613.1333087308 2846615.800988013 0, -1404611.440918708 2846624.325265719 0, -1404217.1673162603 2846545.7387325265 0, -1403822.8913253082 2846467.1743903724 0, -1403428.6090668149 2846388.631626333 0, -1403034.3220979962 2846310.11094714 0, -1403053.4782844791 2846213.634980691 0, -1403098.5972614503 2845986.403067261 0, -1403102.6692528867 2845986.22169955 0, -1403103.248347781 2845983.290500964 0, -1403194.7240722105 2845979.1141459174 0, -1403449.0559606147 2846028.010740485 0, -1403504.9632931324 2846028.6813831767 0, -1403799.7788403556 2846032.221859208 0, -1403917.369560205 2846021.144461339 0, -1404023.201279463 2846011.177178477 0, -1404120.1833968922 2845982.644777186 0, -1404347.9635557476 2845922.9921767535 0, -1404384.173923037 2845913.506921877 0)), ((-1397408.2962231054 2850092.3249010867 0, -1397368.4896856248 2850084.068534674 0, -1397446.3713279825 2849691.2643500497 0, -1397505.381414212 2849392.6996998107 0, -1397510.6108350344 2849365.822199518 0, -1397524.2513040218 2849298.457697818 0, -1397541.4491653107 2849211.7165610585 0, -1397541.458220491 2849211.6708892966 0, -1397542.5345600036 2849206.2421379318 0, -1397543.8495907197 2849199.6533351694 0, -1397552.4185829689 2849156.451312542 0, -1397575.9850958055 2849037.5695722825 0, -1397592.0332196734 2848956.627131109 0, -1397592.679842527 2848953.3228822346 0, -1397592.6798425396 2848953.3228821703 0, -1397602.13302944 2848905.6434157547 0, -1397665.8361152133 2848583.3899085936 0, -1397680.0171525239 2848512.827412834 0, -1397680.0171525334 2848512.8274127864 0, -1397929.700960232 2848562.7028559577 0, -1397929.7009632865 2848562.702856566 0, -1397948.4323890347 2848566.4242267665 0, -1397957.4309592475 2848568.2419514772 0, -1397957.4309620752 2848568.241952046 0, -1398077.2551434217 2848592.176531594 0, -1398141.5814011388 2848605.029787731 0, -1398239.0745437716 2848624.510235964 0, -1398247.1236719787 2848626.1050571734 0, -1398282.7133075856 2848633.219462183 0, -1398287.580911698 2848634.192208714 0, -1398327.5059190358 2848642.169873064 0, -1398332.0947335428 2848643.086969197 0, -1398372.692625795 2848651.1939333444 0, -1398377.8822906353 2848652.2453921833 0, -1398377.8822907384 2848652.2453922043 0, -1398377.8822960923 2848652.2453932827 0, -1398474.4887164899 2848671.5479072505 0, -1398871.7176727587 2848750.941513455 0, -1398936.6503813192 2848763.925655422 0, -1398962.2122963727 2848769.0345055317 0, -1399102.7436877913 2848797.11353484 0, -1399111.7925354156 2848798.9398238114 0, -1399113.3217560383 2848799.2471367856 0, -1399268.9442821615 2848830.357851166 0, -1399266.4973957373 2848842.226063975 0, -1399231.7310575226 2849019.0364407757 0, -1399231.7310429218 2849019.036515031 0, -1399221.9107939033 2849069.0883870637 0, -1399215.8337490482 2849099.6392980004 0, -1399215.8337490472 2849099.639298005 0, -1399215.833740717 2849099.639340032 0, -1399191.420180221 2849223.420864117 0, -1399191.322303488 2849223.9171182876 0, -1399113.7035125983 2849617.4718418084 0, -1399036.0835453114 2850011.0212396816 0, -1398958.4665678807 2850404.5660594977 0, -1398945.88544305 2850402.2433631923 0, -1398647.0857153283 2850341.77419907 0, -1398647.0857049285 2850341.774196965 0, -1398647.085704724 2850341.7741969237 0, -1398622.6991095608 2850336.8458357486 0, -1398618.7863314683 2850336.06729265 0, -1398618.7863266538 2850336.0672917007 0, -1398560.9794564047 2850324.409822854 0, -1398193.5005080379 2850250.547556947 0, -1398163.4883337207 2850244.272879605 0, -1397765.99050446 2850164.157983164 0, -1397408.2962231054 2850092.3249010867 0)), ((-1408499.7917902402 2851897.0108265877 0, -1408421.0447701633 2852289.2328041033 0, -1408208.4406804384 2852246.8743553446 0, -1408024.111393916 2852209.763787432 0, -1407803.8467946316 2852165.883525409 0, -1407627.1719187878 2852130.313602257 0, -1407230.2294260436 2852050.8889755737 0, -1407230.2294255465 2852050.888975477 0, -1407206.2683501462 2852046.303831964 0, -1406833.2804088348 2851971.486434671 0, -1406833.280408835 2851971.4864346697 0, -1406911.933817793 2851579.414764962 0, -1406921.6758014641 2851530.0046396935 0, -1406934.686355972 2851465.14776617 0, -1406956.335386052 2851357.2290452607 0, -1406990.586042128 2851187.337697579 0, -1406990.5860421804 2851187.3376973188 0, -1406990.5860422545 2851187.3376969495 0, -1407041.0215364834 2850935.08214724 0, -1407069.2414205894 2850795.256210503 0, -1407069.2414206765 2850795.2562100706 0, -1407069.2414206867 2850795.2562100184 0, -1407073.5684860025 2850772.8424741207 0, -1407147.89795659 2850403.1700436547 0, -1407147.8979565974 2850403.170043656 0, -1407147.897956598 2850403.1700436533 0, -1407506.3690000873 2850474.723267223 0, -1407544.9384991385 2850482.421997814 0, -1407941.9745221676 2850561.6962001207 0, -1408339.0062130108 2850640.9927756977 0, -1408736.0331859435 2850720.3115733187 0, -1408657.41158823 2851111.919579926 0, -1408657.2847018465 2851112.5515910415 0, -1408578.5377025602 2851504.7836576267 0, -1408499.7917902402 2851897.0108265877 0)), ((-1402322.4997742055 2855962.8549554977 0, -1401926.2423490663 2855884.0684591965 0, -1401529.9818892553 2855805.3075370626 0, -1401133.7178690603 2855726.5661011315 0, -1401213.211228292 2855335.412905123 0, -1401292.708138397 2854944.2551045995 0, -1401372.2039204885 2854553.0919847465 0, -1401451.7031004892 2854161.9246495627 0, -1401847.939906079 2854240.6579817794 0, -1402244.174336076 2854319.414166907 0, -1402640.4039476456 2854398.195590499 0, -1403036.6295266182 2854476.9962373967 0, -1402957.1582407928 2854868.1687561497 0, -1402877.6877139623 2855259.339419323 0, -1402798.2189316931 2855650.5022341553 0, -1402718.750697533 2856041.6632575803 0, -1402322.4997742055 2855962.8549554977 0)), ((-1411751.5853603992 2856418.185144432 0, -1411754.7571084467 2856429.033555226 0, -1411767.7582414288 2856473.501728358 0, -1411817.3561956498 2856643.1425894992 0, -1411842.2963358818 2856728.4480426703 0, -1411857.2971659566 2856779.7566173365 0, -1411866.2335776836 2856810.323187832 0, -1411899.5147161097 2856924.1581729716 0, -1411899.2923966853 2856930.5015921816 0, -1411897.9417615307 2856969.061157462 0, -1411894.9402896597 2857054.74085981 0, -1411894.5358408932 2857066.285733073 0, -1411894.0926921885 2857078.934847568 0, -1411893.5171049975 2857095.3595575998 0, -1411891.713688685 2857146.8214332475 0, -1411889.994330014 2857195.9125946364 0, -1411889.699684305 2857204.325522127 0, -1411880.874398725 2857470.4536910965 0, -1411878.0360349421 2857552.343632654 0, -1411875.6033314364 2857624.912060565 0, -1411877.2522324275 2857628.9538111114 0, -1411915.182499596 2857721.932867112 0, -1411933.3960081232 2857766.5799572086 0, -1411978.6628281383 2857877.543262183 0, -1411987.1789034253 2857898.418955808 0, -1411967.8125782465 2857894.7388543542 0, -1411940.9460620254 2857889.3657909026 0, -1411827.0057558136 2857866.5978943333 0, -1411816.2609931997 2857864.4504358424 0, -1411785.6653254726 2857858.335715912 0, -1411778.7458917818 2857856.7582134116 0, -1411778.7458915478 2857856.758213361 0, -1411594.861806844 2857819.9848252423 0, -1411383.7384575654 2857777.7640921324 0, -1411367.0593044949 2857774.617511555 0, -1410990.311091655 2857698.9297966924 0, -1410858.0004306268 2857672.622335774 0, -1410596.879148821 2857620.1174235255 0, -1410621.9852533883 2857491.62132465 0, -1410633.7672996472 2857431.7274165326 0, -1410674.0526222952 2857227.8057096056 0, -1410674.0526223222 2857227.805709468 0, -1410751.224144693 2856835.4917604737 0, -1410757.8768594344 2856800.8060144023 0, -1410820.825048066 2856480.8087421665 0, -1410828.3986047867 2856443.173116284 0, -1410828.3986047988 2856443.1731162234 0, -1410828.3986048105 2856443.173116164 0, -1410842.1263099334 2856372.5611441107 0, -1410905.5745906155 2856050.8465852523 0, -1411295.5805096321 2856130.8219032804 0, -1411432.25054098 2856158.360234526 0, -1411432.2505409804 2856158.360234527 0, -1411432.3744690558 2856158.659060573 0, -1411528.0464481325 2856236.440972607 0, -1411560.3916010382 2856262.7377897943 0, -1411667.3655141646 2856349.7080069594 0, -1411702.6279902614 2856378.379090404 0, -1411740.73912433 2856409.366361044 0, -1411751.5853603992 2856418.185144432 0)), ((-1405261.3863524538 2859814.963898068 0, -1405651.2703595373 2859892.5344997076 0, -1406048.3939748404 2859971.7027081377 0, -1406445.5149132037 2860050.8938099025 0, -1406842.6286486182 2860130.1098150183 0, -1406842.628648618 2860130.1098150196 0, -1406764.8265913033 2860522.0183203532 0, -1406688.7504382622 2860905.23269522 0, -1406687.0248609448 2860913.924854412 0, -1406687.0248609437 2860913.924854418 0, -1406415.590490284 2860859.6128464383 0, -1406290.115452382 2860834.5054980735 0, -1405897.4905057237 2860756.1532146623 0, -1405893.2084571854 2860755.084839173 0, -1405815.6258750965 2861146.7138585607 0, -1406212.4251978938 2861226.269456487 0, -1406609.224541734 2861305.8234384237 0, -1406531.4236872834 2861697.717321509 0, -1406531.4236872534 2861697.717321503 0, -1406531.4236872522 2861697.717321509 0, -1406134.7369737187 2861618.013712855 0, -1405738.045266009 2861538.3353076545 0, -1405341.3495085759 2861458.6764138103 0, -1404944.6466850971 2861379.042249062 0, -1405022.0205961196 2860987.6359433997 0, -1405099.3936611253 2860596.2250118344 0, -1405176.7677404573 2860204.8092027605 0, -1404780.8769870354 2860124.730539985 0, -1404858.3628771487 2859733.3601081683 0, -1404935.3719751574 2859342.672009466 0, -1405331.1001697828 2859423.1280607716 0, -1405254.1434443628 2859813.3853914333 0, -1405261.3863524538 2859814.963898068 0)), ((-1402682.2020684432 2864118.7237778557 0, -1402695.4529211784 2864121.2283095215 0, -1402695.4529211782 2864121.228309523 0, -1402616.8936437613 2864513.0297153555 0, -1402538.3358605783 2864904.823133617 0, -1402499.8153482743 2865096.9325434817 0, -1402459.7765047003 2865296.6141715446 0, -1402419.7474271564 2865496.252592065 0, -1402381.2202299368 2865688.4006322375 0, -1402381.2202299358 2865688.4006322417 0, -1401983.5451695155 2865608.8553613233 0, -1401712.7970666003 2865554.720197429 0, -1401585.8632989998 2865529.3320246567 0, -1401188.179284525 2865449.831439479 0, -1401188.1792117932 2865449.831424936 0, -1401097.3997936426 2865431.6841614405 0, -1401084.8622124526 2865429.1840025107 0, -1400799.226584094 2865372.3078978863 0, -1400790.4886198821 2865370.35311039 0, -1400868.6112097064 2864978.9369326024 0, -1400945.8802026587 2864590.1986702695 0, -1400946.7321918367 2864587.5186793273 0, -1401024.8546978398 2864196.092250667 0, -1401100.9681356936 2863813.8579939683 0, -1401102.9804730942 2863804.661391134 0, -1401161.397036985 2863816.255982978 0, -1401501.1095115985 2863883.7670430006 0, -1401558.569074346 2863895.1879364145 0, -1401899.2323785443 2863962.904431385 0, -1401955.7386749384 2863974.1206539576 0, -1402297.3480475233 2864042.044840975 0, -1402352.9085788366 2864053.0954119097 0, -1402682.2020684432 2864118.7237778557 0)), ((-1411465.037336772 2865648.779537992 0, -1411463.8557415532 2865655.0362547883 0, -1411467.7572204815 2865655.390586278 0, -1411528.471929807 2865656.642773342 0, -1411528.4719302277 2865656.6427733493 0, -1411528.471930238 2865656.6427733507 0, -1411528.4719302412 2865656.6427733507 0, -1411569.6250164183 2865661.9779159166 0, -1411578.782938681 2865663.366841497 0, -1411605.6501287578 2865674.490354063 0, -1411625.477942975 2865682.6947615296 0, -1411631.7469223023 2865685.3064114386 0, -1411632.7949084023 2865685.7423111056 0, -1411635.878725861 2865685.393298609 0, -1411647.15672865 2865684.1156663178 0, -1411652.734374543 2865683.483661498 0, -1411663.069627925 2865682.308265712 0, -1411676.9610435506 2865680.725924123 0, -1411731.4632386134 2865723.2860093727 0, -1411740.6671240507 2865730.519389325 0, -1411822.090020838 2865718.2191672903 0, -1411838.3978266304 2865715.9588456973 0, -1411841.073689812 2865717.1605165387 0, -1411983.169821221 2865779.4717531553 0, -1411983.1698278135 2865779.4717560387 0, -1411999.7797165555 2865786.7246760647 0, -1412158.2912243297 2865835.9466782827 0, -1412170.146075653 2865836.9489773572 0, -1412170.146076222 2865836.9489774047 0, -1412229.6105864234 2865841.7906655665 0, -1412229.6105864223 2865841.790665572 0, -1412229.6105864225 2865841.790665572 0, -1412229.6105863927 2865841.7906657173 0, -1412219.1846687484 2865892.884224412 0, -1412162.0192036116 2866176.968186281 0, -1412082.825008011 2866569.0058447286 0, -1412002.6728112134 2866961.1972452626 0, -1411922.5221962316 2867353.380643108 0, -1411922.5221962258 2867353.3806431065 0, -1411922.522196224 2867353.3806431163 0, -1411583.5471875449 2867284.2856640294 0, -1411524.470183467 2867272.0276043857 0, -1411445.3103906135 2867256.03696549 0, -1411360.55465754 2867238.708295354 0, -1411126.4154879246 2867190.697131833 0, -1411025.867544467 2867170.3460400575 0, -1410917.9101386506 2867148.296874894 0, -1410817.3561835214 2867127.759786799 0, -1410728.3555018317 2867109.3920901567 0, -1410728.3549554553 2867109.3919785875 0, -1410610.287801935 2867085.2829328044 0, -1410330.3074244468 2867028.109796696 0, -1410330.291306805 2867028.1065054135 0, -1410361.2985384562 2866873.7711350676 0, -1410409.33354803 2866634.6905706557 0, -1410420.9139694646 2866577.055654584 0, -1410440.2146718572 2866480.997461124 0, -1410440.2146719096 2866480.9974608603 0, -1410456.6149111663 2866398.174093309 0, -1410463.2236422338 2866365.1634405 0, -1410488.222008319 2866241.2386903674 0, -1410504.0888303516 2866161.32310462 0, -1410519.0021884008 2866088.0397656164 0, -1410519.002188406 2866088.0397655913 0, -1410566.296370515 2865852.6473873486 0, -1410597.9484032183 2865695.10541922 0, -1410644.2002541109 2865464.0360314716 0, -1410644.2099788839 2865464.0379698332 0, -1410644.2113585516 2865464.0310786646 0, -1410684.423421186 2865472.053394944 0, -1411044.5673082075 2865544.3390496573 0, -1411064.664278303 2865548.3758619865 0, -1411303.885356992 2865596.5309854182 0, -1411444.901632407 2865624.715773975 0, -1411454.7045603914 2865626.808822695 0, -1411468.8876433342 2865629.512212369 0, -1411468.8876433324 2865629.512212379 0, -1411465.037336772 2865648.779537992 0)), ((-1405352.3578766033 2869543.935077524 0, -1405359.1363504976 2869545.2042935197 0, -1405436.3132154464 2869560.2322490425 0, -1405502.746418892 2869573.2515146 0, -1405502.7464338238 2869573.2515175208 0, -1405720.6097105232 2869615.720096893 0, -1406118.040747909 2869693.2168943826 0, -1406295.4979188778 2869727.8309028526 0, -1406335.326025477 2869735.548965003 0, -1406368.3830205046 2869742.047260953 0, -1406368.3830230972 2869742.047261461 0, -1406515.4696160685 2869770.7362509747 0, -1406515.4696160683 2869770.736250976 0, -1406515.3518045028 2869771.324431194 0, -1406436.8880400027 2870163.058756294 0, -1406358.3075719213 2870555.3763669888 0, -1406349.6235684261 2870598.7326819636 0, -1406349.6235644566 2870598.7327020443 0, -1406348.2495920586 2870605.7389051924 0, -1406343.9503185805 2870627.2036582665 0, -1406334.9120333896 2870672.1828832966 0, -1406279.7301098744 2870947.689329546 0, -1406259.8342604002 2871047.0207821187 0, -1406256.6776818188 2871062.9237264954 0, -1406248.9494264596 2871101.3638142054 0, -1406201.1516861857 2871339.9969154075 0, -1405935.8783990357 2871288.0464658416 0, -1405919.2268095443 2871284.7765399343 0, -1405859.9066085038 2871273.1582050133 0, -1405856.2419319113 2871272.450294864 0, -1405856.241927392 2871272.4502939982 0, -1405803.751681128 2871262.170407299 0, -1405658.300430607 2871233.6943604634 0, -1405644.932170153 2871231.0641286485 0, -1405623.858496985 2871226.937981929 0, -1405605.0992181995 2871223.278679066 0, -1405605.0992040872 2871223.278676319 0, -1405406.3471053601 2871184.366241646 0, -1405435.624495818 2871038.2277601827 0, -1405437.0592010934 2871031.0664098286 0, -1405441.9988417523 2871006.4998400114 0, -1405484.3701475295 2870794.999082076 0, -1405484.9057895474 2870792.2393457848 0, -1405479.7815442246 2870791.226744264 0, -1405424.8324013767 2870780.4771098006 0, -1405420.8968640964 2870779.7077110303 0, -1405370.7645056879 2870769.9052323746 0, -1405367.6517246566 2870769.2986274436 0, -1405283.9653302229 2870752.933274581 0, -1405255.9106829148 2870747.465511902 0, -1405255.9106593088 2870747.46550731 0, -1405205.8767456764 2870737.7331411466 0, -1405087.490981406 2870714.534637766 0, -1405066.3558166963 2870710.5732503003 0, -1404937.6800193107 2870685.241462984 0, -1404912.420841931 2870680.2812086833 0, -1404873.690080004 2870672.728276086 0, -1404690.0778117212 2870636.8252614536 0, -1404690.077166699 2870636.8251353293 0, -1404690.0771666993 2870636.825135328 0, -1404708.0471434693 2870547.146432178 0, -1404710.958022651 2870532.710837276 0, -1404753.5632293806 2870320.0914300634 0, -1404767.9136741732 2870248.445385562 0, -1404768.6279536458 2870244.8196088024 0, -1404768.6279536616 2870244.819608721 0, -1404775.7641339956 2870209.20661129 0, -1404775.7641365211 2870209.206598999 0, -1404776.9359453998 2870203.4499911657 0, -1404809.6746020482 2870040.0693464084 0, -1404828.469240713 2869946.2757398025 0, -1404829.4227403163 2869941.5171959335 0, -1404831.863324543 2869929.2458460294 0, -1404847.1798434148 2869852.8091909704 0, -1404851.4089969185 2869831.7039236957 0, -1404851.4422845743 2869831.5378041933 0, -1404852.1575244702 2869828.0605850974 0, -1404853.231110614 2869822.7023808896 0, -1404856.9175901003 2869804.3054733314 0, -1404883.9239550708 2869669.5310635734 0, -1404889.6944281512 2869640.6415555426 0, -1404889.6944321946 2869640.6415352616 0, -1404925.732661221 2869460.793662609 0, -1405323.1722710785 2869538.245600288 0, -1405352.3578766033 2869543.935077524 0)), ((-1403270.9110435373 2873607.989720598 0, -1403195.57265247 2873987.095011088 0, -1402798.6169425067 2873907.8261163756 0, -1402874.1480264233 2873528.383814522 0, -1402952.0604383987 2873136.965264704 0, -1403348.7412445976 2873216.3452473097 0, -1403270.9110435373 2873607.989720598 0)), ((-1400722.020211627 2873987.416916897 0, -1400659.8349719865 2874300.9579526847 0, -1400582.1008802357 2874692.897713141 0, -1400504.368199048 2875084.8295678613 0, -1400504.3681990472 2875084.8295678655 0, -1400306.06796822 2875046.0779310446 0, -1400108.2805656404 2875006.994913384 0, -1399712.1886875827 2874929.1824742686 0, -1399316.0923516774 2874851.392322538 0, -1398919.9918312414 2874773.6246947986 0, -1398997.4825770769 2874381.3695183387 0, -1399074.9721307347 2873989.109292349 0, -1399152.464837142 2873596.8441945347 0, -1399229.9583728071 2873204.574122286 0, -1399626.3009079173 2873282.6651033484 0, -1400022.6398035127 2873360.7752654627 0, -1400418.9757098868 2873438.911310901 0, -1400341.2951306698 2873830.9661018522 0, -1400408.590619487 2873844.220564607 0, -1400737.569628418 2873909.015992905 0, -1400737.5696284168 2873909.0159929106 0, -1400737.5696284187 2873909.015992911 0, -1400722.020211627 2873987.416916897 0)), ((-1409103.6964492481 2875025.2421185113 0, -1409141.8900567754 2875032.891256656 0, -1409213.6801065572 2875047.2731291484 0, -1409213.6801090706 2875047.273129647 0, -1409229.77988655 2875050.449152512 0, -1409285.8021089113 2875061.721309533 0, -1409285.8021396676 2875061.7213157113 0, -1409535.654514666 2875111.773087116 0, -1409929.4117891053 2875190.679700427 0, -1409971.24784557 2875199.065926775 0, -1409971.2478463105 2875199.065926921 0, -1409978.7519803427 2875200.531137577 0, -1410108.979261336 2875226.637376353 0, -1410140.157719893 2875232.924347864 0, -1410323.172103583 2875269.6090371227 0, -1410323.1721035815 2875269.609037131 0, -1410323.1721035817 2875269.609037131 0, -1410280.0390395173 2875485.7118710545 0, -1410275.657886319 2875507.7470515314 0, -1410272.7716184133 2875522.122472482 0, -1410244.8465344294 2875662.031449576 0, -1410244.846486525 2875662.031689817 0, -1410238.80266182 2875692.360027673 0, -1410188.7019879804 2875943.3155002077 0, -1410185.8364133637 2875957.6702931076 0, -1410166.5198291473 2876054.448420859 0, -1410154.9493124203 2876112.3908099523 0, -1410129.6492050847 2876239.1153764776 0, -1410097.0531707695 2876404.0092286854 0, -1410096.267817752 2876406.490527884 0, -1410095.9545911942 2876406.9131187014 0, -1410092.6124654415 2876411.4155137967 0, -1410071.9405331241 2876439.594348282 0, -1410067.334844834 2876445.872557595 0, -1410044.8896179674 2876476.467052874 0, -1410017.2528691767 2876514.1379344515 0, -1410017.2528691764 2876514.1379344515 0, -1410017.2513635792 2876514.139986689 0, -1409975.5495828802 2876541.3013308863 0, -1409950.1803787204 2876557.8212493835 0, -1409908.6595203627 2876584.8949637697 0, -1409866.487935356 2876612.392758426 0, -1409766.4990217146 2876677.5969618005 0, -1409766.4997185215 2876677.6499651307 0, -1409766.2500051307 2876677.812799691 0, -1409766.6451122717 2876704.2036529 0, -1409767.1408562034 2876737.3104113834 0, -1409767.507660834 2876761.8052125834 0, -1409769.9336998635 2876795.1547505893 0, -1409764.5592822868 2876794.095048755 0, -1409627.5944055112 2876766.6532114935 0, -1409510.6739233304 2876743.2241767757 0, -1409446.8540509548 2876730.4106893907 0, -1409310.6548475022 2876703.0646280306 0, -1409263.1621494931 2876693.52887364 0, -1409260.287299188 2876692.9515570784 0, -1409230.218035185 2876686.8663708684 0, -1408832.1384908531 2876608.0227922006 0, -1408774.6639410295 2876596.8008374856 0, -1408728.6500602255 2876587.657983948 0, -1408514.9915482828 2876545.2276930353 0, -1408514.9915142735 2876545.2276862813 0, -1408455.7443594562 2876533.474764181 0, -1408452.775912659 2876532.908685063 0, -1408434.0567597842 2876529.2021547086 0, -1408446.2223965924 2876468.189760085 0, -1408486.3784147138 2876266.7236018917 0, -1408489.3887333323 2876251.6218461953 0, -1408512.5581591323 2876135.3886321625 0, -1408529.94382</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>BANK OFÔøΩNORTHÔøΩDAKOTA, SOVEREIGNÔøΩLANDS, COMMON SCHOOLS, NDÔøΩSTATEÔøΩUNIVERSITY, ND INDUSTRIAL SCHOOL, SCHOOL OF MINES, ELLENDALE, SCHOOL FOR THE BLIND, ND SCHOOL OF SCIENCE, UNIVERSITY OF ND, NDÔøΩSTATEÔøΩTREASURER, MAYVILLE, VALLEY CITY</t>
+          <t>SOVEREIGNÔøΩLANDS, COMMON SCHOOLS, BANK OFÔøΩNORTHÔøΩDAKOTA, NDÔøΩSTATEÔøΩUNIVERSITY, ND INDUSTRIAL SCHOOL, SCHOOL OF MINES, ELLENDALE, SCHOOL FOR THE BLIND, ND SCHOOL OF SCIENCE, UNIVERSITY OF ND, NDÔøΩSTATEÔøΩTREASURER, MAYVILLE, VALLEY CITY</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Dept. of Transportation, 100.00% State Hospital South (Insane Asylum), Public School (Indemnity, Schools, Common Schools)</t>
+          <t>Public School (Indemnity, Schools, Common Schools), Dept. of Transportation, 100.00% State Hospital South (Insane Asylum)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1650,7 +1650,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-778111.123129531 2849966.4205661775 0, -778152.0380063502 2849995.857612358 0, -778232.4635076745 2850022.7648026235 0, -778232.4635694196 2850022.7648232784 0, -778272.3694730203 2850005.137503722 0, -778286.1607537577 2849979.6017443314 0, -778296.920254595 2849936.9769389974 0, -778336.2231786009 2849907.0715158912 0, -778393.8367818684 2849849.3580969116 0, -778393.8430354721 2849849.360552195 0, -778393.8430511502 2849849.360536491 0, -778403.6653998105 2849853.216998893 0, -778428.6853912089 2849863.0403224714 0, -778428.6854091042 2849863.040385179 0, -778428.6991688223 2849863.0457875365 0, -778443.4649263347 2849914.8092266163 0, -778414.1937640968 2849949.001410578 0, -778371.7344926831 2850017.615826767 0, -778382.3051193785 2850074.338933517 0, -778398.5470595541 2850082.064149347 0, -778403.3046900313 2850084.3265774795 0, -778446.810059922 2850176.3057739446 0, -778447.2446485488 2850181.0248513315 0, -778455.2041889131 2850268.246773478 0, -778429.6688173915 2850307.581051144 0, -778392.1623876267 2850337.822753677 0, -778391.2678431092 2850381.5535695823 0, -778409.1754104488 2850423.8003512262 0, -778443.3267647222 2850418.882471604 0, -778472.0479189741 2850425.3049393725 0, -778472.0487260116 2850425.3051198344 0, -778472.1538681126 2850425.351573998 0, -778539.5934494556 2850455.1479067337 0, -778539.5934506133 2850455.1479104175 0, -778539.6047455587 2850455.1529007806 0, -778556.6351373835 2850509.3733091513 0, -778560.1761920195 2850560.9527782807 0, -778547.8672037215 2850595.660859155 0, -778537.9140969089 2850606.129185271 0, -778520.642783997 2850623.4954078286 0, -778493.3349725715 2850650.953595447 0, -778451.0096472857 2850697.8333630995 0, -778412.2927054393 2850735.7666474488 0, -778332.2267194751 2850801.4565049415 0, -778302.6506236638 2850831.477270452 0, -778261.3214377748 2850858.485909124 0, -778219.6404445403 2850879.0038987314 0, -778186.4701389986 2850893.9341213712 0, -778155.5423610273 2850942.964488242 0, -778155.3875860953 2850943.902271544 0, -778153.8866063681 2850952.996727043 0, -778144.8386589016 2851007.818732372 0, -778144.838656444 2851007.8187473714 0, -778143.8777997025 2851013.701355991 0, -778149.8737242838 2851080.1654093326 0, -778164.1845627591 2851163.640269842 0, -778188.4564350559 2851188.1242920617 0, -778205.9905316551 2851205.810038239 0, -778226.8356577648 2851241.215181279 0, -778255.9156079143 2851286.877953428 0, -778270.0726153597 2851365.3265308696 0, -778270.072638942 2851365.326661501 0, -778270.0726389335 2851365.3266615 0, -778270.0726389342 2851365.326661504 0, -778094.4605108831 2851346.208892302 0, -777690.6850503956 2851302.830592308 0, -777690.6850503958 2851302.8305923063 0, -777690.6850503882 2851302.8305923054 0, -777733.9628193304 2850906.4917634716 0, -777777.2388194209 2850510.150120197 0, -777820.9831457793 2850114.3101011575 0, -777864.7277990956 2849718.467504392 0, -777460.6128714907 2849673.6653484977 0, -777056.4934434132 2849628.885801183 0, -777056.4934434134 2849628.885801181 0, -777056.4934434058 2849628.8858011803 0, -777099.6764418286 2849232.3232875033 0, -777503.5643492694 2849277.22811051 0, -777690.8115454458 2849298.045287109 0, -777908.4311447623 2849322.23911069 0, -777951.249948151 2848933.928056874 0, -777951.249948158 2848933.92805688 0, -777951.2499481585 2848933.9280568752 0, -777951.4898512964 2848934.1258694273 0, -778018.9447448857 2848989.745918616 0, -778066.8683336076 2849016.709277986 0, -778107.8935463295 2849031.885046103 0, -778107.8935678903 2849031.885071271 0, -778107.8998301893 2849031.887387773 0, -778165.2545033393 2849098.842157993 0, -778111.3076032304 2849130.168651748 0, -778087.6126041275 2849186.3163977806 0, -778126.6375942499 2849232.727695082 0, -778223.3552550377 2849265.8186636334 0, -778254.8962661957 2849265.7881828006 0, -778317.3286196977 2849256.3805453232 0, -778320.3206548779 2849255.9305497576 0, -778382.8332636404 2849238.0703015476 0, -778423.6735988836 2849259.0496166716 0, -778428.9827689723 2849261.776760421 0, -778454.2196999231 2849278.691583925 0, -778488.0754617819 2849356.2284987266 0, -778488.6501968709 2849382.5362317674 0, -778489.152936014 2849406.1901539196 0, -778450.2355246089 2849445.274848413 0, -778352.5313618146 2849449.953824687 0, -778312.1611298464 2849447.1315117213 0, -778292.6974834282 2849465.247074199 0, -778251.9586401515 2849503.1628931905 0, -778240.67791667 2849566.0853533074 0, -778195.7662688775 2849622.488102977 0, -778177.5478470904 2849623.076913356 0, -778120.4627838772 2849639.9752028664 0, -778096.8846394607 2849645.720705325 0, -778000.5748267936 2849733.491153451 0, -778000.5748146558 2849733.491172231 0, -777995.0456996908 2849742.0505981613 0, -778024.6618800078 2849822.4492694708 0, -778065.4236408372 2849893.553183616 0, -778095.0547552725 2849940.7998997993 0, -778111.123129531 2849966.4205661775 0)), ((-779039.152479286 2865439.924130304 0, -779023.0279794952 2865448.293106738 0, -778993.7520421153 2865463.826756115 0, -778970.6611095731 2865476.0778305396 0, -778968.6561214548 2865477.1415926316 0, -778956.4113200627 2865482.241545986 0, -778946.6793083777 2865486.32109739 0, -778934.1801994797 2865491.5606448776 0, -778917.3725716695 2865498.641953889 0, -778939.3769872008 2865584.7747839727 0, -778976.8123785012 2865626.5557441814 0, -779070.4881821149 2865731.398700857 0, -779138.7121427488 2865757.6186342165 0, -779193.8966056061 2865744.298193133 0, -779227.2728923232 2865741.3936695904 0, -779262.9244508899 2865760.6726428876 0, -779323.3717550738 2865789.4067152063 0, -779310.5830200284 2865837.322463818 0, -779310.5830133609 2865837.322488929 0, -779309.2371529589 2865842.397671633 0, -779304.6237460255 2865848.684998582 0, -779292.6560994192 2865864.9949638876 0, -779287.2914060361 2865886.224715173 0, -779291.490815091 2865924.855617001 0, -779300.0528537801 2865939.7354915333 0, -779325.8083980508 2865984.182716592 0, -779329.5936830095 2865990.877125187 0, -779335.7647028733 2866001.3645638414 0, -779340.7360346571 2866009.9421461234 0, -779342.2131859002 2866012.3954330594 0, -779342.2131859086 2866012.3954330618 0, -779342.2131859087 2866012.395433061 0, -779342.2131880341 2866012.395433664 0, -779372.151402374 2866020.876621468 0, -779379.3495333014 2866022.90937798 0, -779387.2382461597 2866026.0080900206 0, -779414.3932899326 2866036.6744328826 0, -779419.9555692682 2866038.8594160196 0, -779469.6521037758 2866035.7577639148 0, -779505.5638708652 2866029.304145113 0, -779509.6160760403 2866028.57596547 0, -779586.2511909457 2866048.736966126 0, -779617.6114337902 2866070.9433910954 0, -779668.0572842329 2866133.4988183226 0, -779713.5557304206 2866181.3759299745 0, -779699.7635778274 2866250.2194864987 0, -779699.6693577461 2866250.696038443 0, -779673.6980300663 2866306.686730672 0, -779666.9540606847 2866309.5274188924 0, -779658.3149942142 2866313.166358084 0, -779631.6438362749 2866328.9537691833 0, -779599.8944918101 2866347.747102227 0, -779591.8881338246 2866352.7793916864 0, -779591.8881273797 2866352.7793957484 0, -779583.9506848671 2866357.808552827 0, -779568.3500247455 2866367.6919736937 0, -779554.0057215543 2866376.817223519 0, -779553.0384076122 2866378.842453414 0, -779551.4617086295 2866382.143530564 0, -779551.4617066641 2866382.1435346873 0, -779528.7638745711 2866429.7637730306 0, -779525.9447666332 2866449.6653061714 0, -779525.1477111776 2866455.5680601005 0, -779509.1860784377 2866573.1947606048 0, -779549.4492355619 2866622.156958724 0, -779585.8910487035 2866644.055816147 0, -779617.0343096714 2866656.3589980225 0, -779657.055098304 2866678.170773459 0, -779675.9214310695 2866702.196313196 0, -779686.9074296867 2866716.193585674 0, -779688.6923568146 2866718.467497366 0, -779731.2478500814 2866748.2971152854 0, -779735.0626553502 2866750.8928653626 0, -779745.1792336187 2866773.911404346 0, -779746.3262182855 2866776.5126066078 0, -779756.6804523873 2866780.2930155494 0, -779760.5911791024 2866781.6816453673 0, -779765.1353403393 2866783.4185599373 0, -779780.7410285155 2866801.9090242246 0, -779782.5802469932 2866804.0885802833 0, -779783.9213599105 2866811.0940339374 0, -779783.9907325234 2866811.4505314506 0, -779788.6696253056 2866835.16151928 0, -779793.970550902 2866838.8543598186 0, -779793.9705511765 2866838.8543600063 0, -779796.9830574616 2866840.9154834338 0, -779799.3910429042 2866842.5239838576 0, -779809.7036107051 2866849.3774993685 0, -779814.9315585205 2866854.655198107 0, -779817.2558039882 2866857.0005583656 0, -779849.9090321712 2866890.2079449045 0, -779851.6497902453 2866891.9764218726 0, -779851.9474376016 2866892.2784973974 0, -779851.948620692 2866892.2796980888 0, -779855.1715612088 2866893.450912427 0, -779855.1715615301 2866893.450912543 0, -779883.5784008092 2866903.5945362016 0, -779889.4830955303 2866906.0520811765 0, -779889.4830956871 2866906.052081239 0, -779899.4872820814 2866910.0145255593 0, -779902.7661595201 2866909.1573240245 0, -779903.06432163 2866909.0727239456 0, -779941.7597677703 2866901.0007285383 0, -779945.6779448233 2866900.181854022 0, -779990.7910749582 2866884.045822849 0, -780030.6135322689 2866836.682446488 0, -780033.2684257341 2866833.597392254 0, -780033.2684354124 2866833.59738504 0, -780035.5375477438 2866831.904521111 0, -780057.7257643872 2866815.6568061677 0, -780064.1461269036 2866818.502320128 0, -780090.9366377833 2866830.3917377423 0, -780133.89057774 2866842.597644402 0, -780150.4058261721 2866852.3191592274 0, -780150.411989451 2866852.3350040643 0, -780150.4600618072 2866852.3633030327 0, -780175.428586096 2866916.474325607 0, -780189.5268056914 2866982.7689993717 0, -780182.4600024628 2867001.0239812057 0, -780182.3555241922 2867001.0592753175 0, -780182.3460716568 2867001.083688821 0, -780171.1883500539 2867004.8316912395 0, -780171.188347239 2867004.8316921904 0, -780149.7691617253 2867012.024510049 0, -780113.6291492814 2867097.1966597107 0, -780112.5635850911 2867179.7537893984 0, -780119.5752173394 2867199.9731411543 0, -780119.5752190775 2867199.973146141 0, -780124.6908509599 2867214.502216883 0, -780127.9139902004 2867223.6557753137 0, -780127.913991517 2867223.6557789934 0, -780137.4979773352 2867250.2324645696 0, -780178.9906645096 2867279.6379998005 0, -780179.1848188583 2867279.775487024 0, -780196.6391077609 2867292.1453208667 0, -780196.6444624714 2867292.154038222 0, -780196.7084945008 2867292.1994353007 0, -780219.2578227344 2867328.912949185 0, -780235.8500057842 2867380.125415139 0, -780235.0224535076 2867424.9112286805 0, -780223.0311947786 2867462.8745537414 0, -780214.7739112539 2867483.972928059 0, -780212.2158848194 2867490.689476867 0, -780211.8137265675 2867491.3326835395 0, -780210.2229013377 2867493.8770287107 0, -780210.222900861 2867493.877029491 0, -780203.9572028025 2867504.257186381 0, -780187.6526605099 2867515.9848600714 0, -780172.9110753008 2867540.9148804476 0, -780108.4302354697 2867585.6731637605 0, -780108.3680211534 2867585.63938935 0, -780108.3545303716 2867585.648749364 0, -780086.1618562269 2867573.594301091 0, -780064.7922477692 2867543.212531911 0, -780015.172118825 2867545.1532341493 0, -779981.4447819251 2867558.5686488766 0, -779960.3008234018 2867566.992400341 0, -779954.7320235713 2867569.1731972136 0, -779952.0898931359 2867570.228046003 0, -779952.0898924158 2867570.228046878 0, -779933.4884271858 2867592.9712232375 0, -779931.8133636253 2867595.2339429366 0, -779920.4619358924 2867613.6809061766 0, -779914.5769850386 2867623.4378382144 0, -779906.2403500113 2867637.2861757823 0, -779909.7839589368 2867660.69840403 0, -779910.8196514907 2867667.540766627 0, -779910.819651789 2867667.540768598 0, -779913.2101330699 2867683.2267922917 0, -779921.0107550346 2867694.4813809455 0, -779921.0107599307 2867694.481387992 0, -779935.6925738538 2867715.5333454106 0, -779941.7260559902 2867722.2085948098 0, -779938.8574386678 2867732.09062936 0, -779942.7537764932 2867738.28435054 0, -779953.4220376707 2867755.2412652266 0, -779958.6876414513 2867760.5741329957 0, -779986.6780746016 2867788.9244766654 0, -779994.4211631832 2867833.4695059485 0, -779996.0619575984 2867843.330221665 0, -780011.4805325873 2867878.64794406 0, -780016.4294372235 2867889.9838030394 0, -780021.2511991784 2867901.2779533747 0, -780035.1559595682 2867933.8245187956 0, -780067.3044794233 2867958.099728915 0, -780092.3876133718 2867976.934358336 0, -780129.5150795655 2867976.8573418804 0, -780143.2501499564 2867976.7104670755 0, -780154.1347760144 2867970.2724514757 0, -780162.0250643261 2867966.2409890736 0, -780175.9838638561 2867959.2371197087 0, -780208.9271376494 2867942.498026442 0, -780211.8219856764 2867941.0769677185 0, -780230.718415916 2867961.4392033685 0, -780257.9387566276 2867990.4320396497 0, -780270.7877296533 2868008.664862903 0, -780271.4156469837 2868030.8659969084 0, -780271.5125259771 2868035.891481801 0, -780271.6917727466 2868042.667724333 0, -780271.1457061982 2868045.415702571 0, -780267.2596377166 2868048.030826591 0, -780253.6413667245 2868058.8683116804 0, -780257.2126298236 2868082.1137912082 0, -780258.9307758686 2868093.286304257 0, -780258.1532994827 2868103.3527499135 0, -780256.0195743253 2868131.016723943 0, -780267.8618371518 2868157.734759952 0, -780275.7022799109 2868175.388378105 0, -780283.7983055882 2868179.5489601586 0, -780292.6615983079 2868183.7742528054 0, -780354.078242831 2868213.054084066 0, -780369.8741598591 2868209.5798874223 0, -780390.6740443747 2868205.0054862285 0, -780430.7194506521 2868157.6157531324 0, -780465.6122176911 2868123.0502816536 0, -780499.7822652165 2868108.0142097017 0, -780530.2662878109 2868100.6320033004 0, -780561.2797663695 2868096.1173576936 0, -780585.229592231 2868116.792696185 0, -780591.0638451594 2868121.8172028866 0, -780624.0195790911 2868153.9296654146 0, -780643.824291495 2868181.95309038 0, -780674.2701028391 2868231.3114375924 0, -780667.647170231 2868287.642819418 0, -780616.1934146394 2868341.3145533646 0, -780507.0768621111 2868362.4499460557 0, -780457.2872171006 2868398.598726522 0, -780449.404758897 2868423.2172151553 0, -780437.8880136701 2868459.33193768 0, -780438.5095848306 2868483.186428469 0, -780439.0009394187 2868500.6547144447 0, -780439.8144682248 2868530.312555635 0, -780468.3067455092 2868558.260272274 0, -780500.407432749 2868589.6802325044 0, -780508.0750506903 2868590.5639736885 0, -780529.5642923648 2868593.031618096 0, -780607.6072858134 2868608.3802648797 0, -780638.321222069 2868629.9391305605 0, -780647.700380725 2868636.5278843227 0, -780651.56526434 2868643.8651430532 0, -780652.9061471489 2868646.433761697 0, -780655.1950769854 2868650.9467331795 0, -780660.1665794743 2868660.6458233334 0, -780679.864017195 2868676.355004451 0, -780714.946225137 2868699.9128579376 0, -780743.0561164145 2868725.705022825 0, -780758.935581237 2868737.913406749 0, -780771.7703215113 2868755.5970413806 0, -780782.0069733132 2868771.081739324 0, -780758.0237120664 2868806.7965130196 0, -780741.8468468265 2868788.8999802982 0, -780733.2992106574 2868779.4440627513 0, -780678.7923149357 2868764.3483426278 0, -780660.1429525369 2868758.9684430636 0, -780658.5017949716 2868756.0317070684 0, -780656.7962791208 2868752.9729189766 0, -780649.5004004847 2868739.8882335406 0, -780642.4107917225 2868741.3814160144 0, -780614.7483967241 2868747.16278265 0, -780620.0283193644 2868770.6165203536 0, -780621.9438328906 2868779.125455868 0, -780617.1331207319 2868794.1621076036 0, -780608.5842629903 2868820.8827284453 0, -780610.4017453694 2868829.684730192 0, -780620.786809104 2868879.735953714 0, -780623.0206860149 2868890.5036827917 0, -780623.7801947279 2868894.1227484457 0, -780624.8843686173 2868899.486581847 0, -780629.1621139545 2868906.5911678923 0, -780645.4627844561 2868933.6927095293 0, -780665.7848580597 2868946.047142861 0, -780673.2674873873 2868950.5959313135 0, -780711.3980113654 2868978.7783207335 0, -780729.7938893085 2868998.102228022 0, -780806.5890987276 2869042.5713849533 0, -780829.2104213691 2869055.652398372 0, -780846.7317857399 2869077.7908078814 0, -780849.6888465665 2869093.1635548575 0, -780851.2444533325 2869101.205827288 0, -780859.1080571082 2869106.840241632 0, -780880.0671380667 2869121.6901659234 0, -780904.5848287079 2869147.0680197002 0, -780921.8018630006 2869228.848461901 0, -780933.9451154479 2869278.0984647786 0, -780937.0773687472 2869290.7618271643 0, -780932.6817647588 2869314.222176287 0, -780592.4494464375 2869276.510103586 0, -780581.8633916792 2869275.322169444 0, -780567.0906029015 2869273.687439044 0, -780379.9151030026 2869252.798227524 0, -780381.1025343707 2869240.0205894937 0, -780383.0646016569 2869217.729473123 0, -780399.8209768042 2869054.593767323 0, -780199.4815631429 2869031.6136801844 0, -780203.080664142 2868998.261281361 0, -780204.655392828 2868983.713981458 0, -780220.9781707377 2868835.5410523666 0, -780218.0416167416 2868835.220864358 0, -780018.8788017232 2868813.224142559 0, -780040.9544328884 2868615.3333827914 0, -779839.1214824963 2868592.593344387 0, -779860.9283054336 2868395.968623219 0, -779860.828353818 2868395.9572289027 0, -779860.8258508032 2868395.9799712407 0, -779796.6513697552 2868388.657097032 0, -779840.3492388529 2867994.546192049 0, -779830.6159661649 2867993.376086266 0, -779721.0984120859 2867980.393429644 0, -779721.0738629557 2867980.3909338894 0, -779721.0739095071 2867980.3905237895 0, -779538.1912544267 2867958.699190479 0, -779567.3780728334 2867697.7170125665 0, -779583.1859263789 2867557.450209374 0, -779583.1859263411 2867557.45020937 0, -779583.3632852 2867554.6543739727 0, -779621.887920612 2867195.499852003 0, -779626.0347395401 2867161.275451751 0, -779423.8093009266 2867139.980027611 0, -779423.8585457572 2867139.514386206 0, -779423.78805035 2867139.5064977612 0, -779443.4744816157 2866953.0341884177 0, -779446.6159386438 2866923.454483797 0, -779465.5197998745 2866745.580134709 0, -779302.7630156983 2866727.718068347 0, -779302.7629729796 2866727.7180636683 0, -779264.7313398954 2866723.53681002 0, -779264.5992211195 2866723.5222846875 0, -779264.7791592191 2866720.7265381604 0, -779307.7513682813 2866327.328534183 0, -779304.9079350996 2866327.0745835477 0, -779300.9590657263 2866326.6702074828 0, -779153.7570984508 2866310.424541069 0, -779126.2156186483 2866307.361045627 0, -779125.8700102569 2866307.315473458 0, -779106.148184011 2866305.145636247 0, -779106.194800808 2866304.721086294 0, -779105.9362982546 2866304.6869999627 0, -779107.8416011414 2866287.525426021 0, -779118.403661055 2866192.183078766 0, -779121.943787134 2866160.692226106 0, -779122.7684254933 2866153.3506462113 0, -779125.2419485286 2866131.254306182 0, -779149.6119593101 2865909.3109809356 0, -779145.2762115606 2865908.8863971997 0, -779144.4407769815 2865908.8045861954 0, -779140.3282349799 2865908.3484188453 0, -779130.3583803957 2865907.2381662573 0, -779051.6946062817 2865898.477727759 0, -778947.9796811765 2865887.046657124 0, -778925.8803831866 2865884.459117109 0, -778745.9815095876 2865864.2462161575 0, -778748.0973385327 2865839.5907291775 0, -778788.7313347592 2865472.488801352 0, -778789.1232820231 2865468.892843553 0, -778782.8493347741 2865468.133675343 0, -778770.8662202087 2865466.777084145 0, -778587.2785353988 2865446.6961526177 0, -778630.5060057266 2865050.817523389 0, -778795.9364610518 2865069.071144758 0, -778829.1488904493 2865072.7371318964 0, -778832.1191208631 2865073.0992569556 0, -778875.3544676013 2864677.2069002697 0, -778821.0044294996 2864671.1840836187 0, -778673.6318773903 2864654.931451717 0, -778716.7582594071 2864259.0396635346 0, -778846.0666581673 2864273.1639524833 0, -778919.5771365796 2864281.3721959386 0, -778923.4298074759 2864281.7881243434 0, -779011.2024317926 2864291.481546741 0, -779021.4239533767 2864292.7003727993 0, -779040.0241077212 2864294.802851747 0, -779048.0950406332 2864304.9275779794 0, -779081.51011605 2864346.6919513326 0, -779103.2222831812 2864379.2385333944 0, -779110.4115474825 2864400.7378377835 0, -779145.2388073046 2864504.909856213 0, -779145.2373684415 2864504.9142325423 0, -779145.2398763419 2864504.9217334674 0, -779105.4091129539 2864626.054522275 0, -779107.6021636605 2864666.8165470483 0, -779114.191915418 2864703.5070613227 0, -779120.2681808715 2864737.406605333 0, -779152.3886458386 2864800.707789942 0, -779192.2797327498 2864828.211610813 0, -779215.7149021933 2864853.127852828 0, -779262.4077841557 2864910.8684776765 0, -779262.4055274363 2864910.876613737 0, -779262.4090644304 2864910.8809871553 0, -779254.9582020501 2864937.7329249955 0, -779267.8374664417 2864984.89326154 0, -779271.255752108 2865019.5770358304 0, -779271.2549658094 2865019.584497317 0, -779271.2558011949 2865019.592966862 0, -779268.6462162543 2865044.3403834435 0, -779243.0937434582 2865062.3057162617 0, -779231.5169619516 2865081.0065179598 0, -779228.8898344346 2865104.702292179 0, -779214.1056601275 2865115.198077089 0, -779205.6575091856 2865125.4143026145 0, -779202.9635111759 2865130.8248968916 0, -779202.909264674 2865130.8649468077 0, -779202.1647279778 2865131.4146344624 0, -779201.4792949216 2865131.9206862 0, -779201.3140513613 2865132.04268468 0, -779196.9972393411 2865134.977016463 0, -779181.7520377578 2865145.3398674186 0, -779181.7306119628 2865145.3444808493 0, -779176.4806674288 2865146.474905855 0, -779168.5528792638 2865148.175910826 0, -779157.1356959858 2865152.3430054043 0, -779146.6797055126 2865156.1514428747 0, -779139.7253875722 2865157.584441535 0, -779134.2441885404 2865158.71260292 0, -779134.0559668748 2865158.7513434244 0, -779125.9651313591 2865159.8935043905 0, -779079.2908318003 2865206.865736912 0, -779053.740847804 2865248.6332662883 0, -779060.3669293413 2865293.016810817 0, -779072.521815128 2865371.894083655 0, -779072.5202583339 2865371.897731961 0, -779072.5223159426 2865371.911083353 0, -779070.2483823916 2865377.2218135255 0, -779057.6609545639 2865406.748632715 0, -779042.7205976748 2865433.5028620926 0, -779039.152479286 2865439.924130304 0), (-779150.1806210199 2865909.373383448 0, -779150.1813775826 2865909.366741886 0, -779149.6119593101 2865909.3109809356 0, -779150.1806210199 2865909.373383448 0), (-779861.8286988554 2868386.8681159625 0, -779862.8004075689 2868378.804957592 0, -779861.8286988555 2868386.868115961 0, -779861.8286988554 2868386.8681159625 0), (-779174.191770332 2865911.9384812503 0, -779174.1917702062 2865911.9384812354 0, -779172.9852149499 2865911.798587795 0, -779174.191770332 2865911.9384812503 0)), ((-785071.1520494085 2884237.5328455777 0, -785074.0743182834 2884251.245471162 0, -785074.0743187336 2884251.245473275 0, -785072.8350446203 2884251.8137203488 0, -785059.5933640503 2884257.886078278 0, -785058.4655225205 2884258.4033064526 0, -785029.9331651429 2884271.4876718954 0, -784982.5444845094 2884293.218891352 0, -784982.5329867667 2884293.224081307 0, -784981.2149508686 2884293.828500253 0, -784981.2147696365 2884293.8286640937 0, -784981.1467549306 2884293.859853873 0, -784981.1130963754 2884293.9201835813 0, -784981.1126494949 2884293.9209845713 0, -784942.4933314892 2884328.8343114667 0, -784938.2966815983 2884346.38967372 0, -784936.6179760093 2884353.4133089255 0, -784936.4155603364 2884354.2629710403 0, -784935.9100860038 2884356.388015854 0, -784928.5993805551 2884386.991325736 0, -784993.285410236 2884560.2029558844 0, -785012.5606098194 2884631.6563191717 0, -785012.5606306553 2884631.6563964025 0, -785012.56075832 2884631.6565387323 0, -785100.1409543537 2884729.2930047493 0, -785100.1382688797 2884729.2942893715 0, -785100.1383894685 2884729.2944238125 0, -785100.0426378414 2884729.3402275466 0, -785100.0479940528 2884729.3461995577 0, -784865.9550747823 2884841.3273328207 0, -784870.340734311 2884898.9978950107 0, -785089.1225307342 2885040.6966766133 0, -785137.4241029804 2885071.9800291564 0, -785137.4241168518 2885071.9800381204 0, -785144.7563596909 2885076.7156066117 0, -785149.5507473459 2885089.185002046 0, -785149.5507482933 2885089.1850045086 0, -785181.1397999076 2885171.1300373194 0, -785181.053034548 2885171.1755495123 0, -785181.0546302543 2885171.1796889217 0, -785068.2787474302 2885230.336112334 0, -785090.9109817881 2885300.809213529 0, -785167.8188858558 2885335.1925203144 0, -785137.469540249 2885398.2045503845 0, -785134.704310118 2885449.9587178538 0, -785134.6223183037 2885449.9492915287 0, -785134.6191365693 2885450.009068597 0, -784753.0042645405 2885403.7581594787 0, -784796.9568533582 2885008.159964477 0, -784840.9078724972 2884612.558932737 0, -784887.075394753 2884217.026761061 0, -784911.6030819823 2884002.4308323604 0, -784911.6851222854 2884002.415955814 0, -784911.6851257501 2884002.415925501 0, -784944.0389234985 2883996.549170707 0, -784952.7095800161 2883994.9769096673 0, -784952.8177494847 2883994.957295599 0, -784952.8177494848 2883994.957295599 0, -784967.5701537884 2883992.282283246 0, -785000.7248227113 2884032.8557939967 0, -784985.4464197728 2884082.796609726 0, -784985.4170368295 2884082.8926543295 0, -784985.4169973311 2884082.892783439 0, -784985.4749725992 2884082.943058755 0, -784986.1639220841 2884083.540505809 0, -784987.2354451539 2884084.469715156 0, -784987.2354451566 2884084.4697151585 0, -785018.3869469 2884111.4838480535 0, -785018.3869469035 2884111.4838480563 0, -785020.9831284193 2884113.7352192122 0, -785050.1615275689 2884139.0394245973 0, -785065.6032716993 2884211.4965632465 0, -785071.1520494085 2884237.5328455777 0)), ((-677953.8032069259 2817491.995393068 0, -678069.7167141542 2817509.6469280994 0, -678217.8576353688 2817488.848912527 0, -678360.5968406689 2817380.5145609425 0, -678422.363924916 2817266.043436793 0, -678472.6245951293 2817096.2507114923 0, -678561.0224409284 2817067.0342389997 0, -678545.320390724 2817204.245976727 0, -678491.7559608689 2817388.0985640883 0, -678341.5493091701 2817544.846515532 0, -678153.6668712639 2817578.174609607 0, -677972.3188691082 2817569.1404563193 0, -677884.9331917596 2817555.833059413 0, -677953.8032069259 2817491.995393068 0)), ((-677231.108041418 2817868.8189695026 0, -677243.7302638481 2817848.087077101 0, -677302.6825308974 2817777.5864733313 0, -677371.2711007164 2817664.9247852275 0, -677400.605370943 2817672.2437291546 0, -677343.919459624 2817721.1919580186 0, -677257.1413748725 2817875.2061114036 0, -677199.6587318564 2818002.712525519 0, -677137.3316518572 2818079.93129337 0, -677140.9925296828 2817942.3201913605 0, -677201.7502498041 2817918.0844985824 0, -677231.108041418 2817868.8189695026 0)), ((-684318.6846920928 2819500.932570692 0, -684372.1220427881 2819423.543772798 0, -684378.6398463694 2819238.7881175373 0, -684378.9312386372 2819230.7932612128 0, -684379.3043926465 2819228.0124945026 0, -684392.8650749848 2818848.5049169254 0, -684393.3477382112 2818835.2632447104 0, -684633.7653833054 2818860.799628752 0, -684627.3292304148 2818944.117061264 0, -684620.1144404393 2819141.882059492 0, -684519.2542157422 2819443.795445804 0, -684466.7083714664 2819447.0300505226 0, -684318.6846920928 2819500.932570692 0)), ((-758564.3085984066 2818681.459485316 0, -758612.9349165041 2818669.7694761525 0, -758683.0315532052 2818659.023409713 0, -758684.2664664839 2818658.954652578 0, -758690.4925450943 2818658.607998822 0, -758705.2007471576 2818864.2361701773 0, -758703.6352082351 2818877.7171009136 0, -758702.3916274216 2818888.419208434 0, -758698.6599958367 2818888.360734387 0, -758673.240844335 2819122.967706949 0, -758671.1253143873 2819142.654787704 0, -758662.8618090664 2819219.5519139674 0, -758662.0386418796 2819227.72897034 0, -758660.8380965086 2819238.730063153 0, -758659.9974660431 2819245.63617677 0, -758654.9995410803 2819291.004841916 0, -758652.8177214448 2819311.114481737 0, -758649.6994803348 2819339.5311173634 0, -758648.8960344149 2819346.865086477 0, -758646.4922947071 2819369.0005113664 0, -758631.8576979493 2819379.1870485577 0, -758536.064134595 2819446.324745872 0, -758514.8718126633 2819461.2477754466 0, -758485.6581259697 2819504.5401307573 0, -758478.5390067782 2819503.793334076 0, -758387.1776951574 2819494.239560099 0, -758383.9344536605 2819501.2761283335 0, -758294.8821531541 2819698.4999611787 0, -758222.8901628957 2819794.6144463588 0, -758219.1547436661 2819795.8039818443 0, -758135.0313326333 2819821.8674609046 0, -758066.521909814 2819843.067383866 0, -757828.6292486495 2819916.503110772 0, -757799.3222543218 2819925.9983771066 0, -757755.6494078401 2819941.3006530274 0, -757752.8907657883 2819942.5764507395 0, -757704.5660675837 2819959.9000758203 0, -757701.6393355912 2819959.065462002 0, -757699.643904292 2819961.551829715 0, -757561.1458225977 2820074.960448736 0, -757555.8430975865 2820070.8414156293 0, -757550.9735694206 2820074.982238254 0, -757481.9404218218 2820018.2084677597 0, -757482.4561308704 2820013.8361315764 0, -757482.4561308703 2820013.8361315764 0, -757492.1058916934 2819932.0225614556 0, -757503.4412317734 2819842.025062935 0, -757501.9678061336 2819800.163542735 0, -757517.7576863117 2819733.44784273 0, -757623.4385056113 2819484.6797583695 0, -757637.5009377657 2819425.2618666664 0, -757661.7956097596 2819370.4721926623 0, -757696.0177974278 2819292.0024861433 0, -757721.922390823 2819205.035827121 0, -757736.6275908743 2819174.638084911 0, -757737.0165452119 2819173.334920214 0, -757741.4280077589 2819166.1500806683 0, -757741.428007759 2819166.1500806683 0, -757759.8850263678 2819136.089592614 0, -758197.1008297182 2818993.8735601115 0, -758327.2708448981 2818883.1271426165 0, -758362.0488636584 2818801.7491274294 0, -758377.9835691601 2818772.7022241666 0, -758394.1881798329 2818730.436357328 0, -758398.940881438 2818721.82847353 0, -758419.1923586403 2818716.3461524355 0, -758564.3085984066 2818681.459485316 0)), ((-685406.7749890666 2820150.9731799574 0, -685400.3319445832 2820348.786152655 0, -685393.7911048346 2820549.7388392347 0, -684839.8720346185 2820545.634140948 0, -684839.8720105918 2820545.621117336 0, -684840.3312223172 2820441.6714656926 0, -684871.2681394718 2820357.0635166476 0, -684910.5715663977 2820275.264069664 0, -684992.4791806015 2820152.7612019363 0, -685041.0750198234 2820020.280271287 0, -685041.077481309 2820020.273531119 0, -685064.4136583988 2819956.652698548 0, -685086.3190185177 2819896.9329020516 0, -685138.9726904748 2819842.5020072707 0, -685194.0354687502 2819799.1662575803 0, -685236.5853367789 2819768.847604989 0, -685236.550166813 2819768.8443257883 0, -685236.5450051151 2819768.843828265 0, -684916.6440199587 2819739.5957859433 0, -684916.6440229195 2819739.595781044 0, -684945.6328751008 2819692.7802545377 0, -684945.6625750877 2819692.73131614 0, -684967.7097781891 2819656.4264919492 0, -684997.8398916608 2819621.014111073 0, -685028.3835677358 2819585.1347657465 0, -685028.3999501476 2819585.1155179623 0, -685037.9384010277 2819582.1730363164 0, -685039.1387194602 2819581.802820588 0, -685103.4861764351 2819561.9635363007 0, -685137.0040355758 2819558.360435938 0, -685179.2472731313 2819551.5159108536 0, -685249.391375077 2819527.3632100928 0, -685306.5188882543 2819512.9642430195 0, -685362.1588061354 2819484.907158246 0, -685431.8660218114 2819453.3149557426 0, -685468.9920896178 2819440.5144576817 0, -685563.888679765 2819407.7955109654 0, -685636.2613541516 2819379.6873441306 0, -685640.6739805538 2819377.9735447094 0, -685702.3709854203 2819361.1076629325 0, -685728.2820672604 2819354.0240989714 0, -685728.9251393601 2819353.8482212727 0, -685806.5335374678 2819363.7610720047 0, -685853.7612179846 2819381.721241745 0, -685888.7005642356 2819397.951743835 0, -685922.4854385246 2819418.581234686 0, -685945.6799238139 2819433.9883979373 0, -685869.4123479467 2819821.0368117904 0, -685863.1288250255 2819823.518940691 0, -685864.1816556539 2819827.1815945944 0, -685540.204894181 2819957.386556406 0, -685415.1722053345 2820100.280244374 0, -685408.1481832038 2820108.339061455 0, -685406.7749890666 2820150.9731799574 0)), ((-684408.1490245973 2819867.199147018 0, -684403.7568967363 2819871.7894599894 0, -684366.1728107164 2819918.800327894 0, -684341.6640185011 2819940.294274738 0, -683920.27431122 2820381.750421679 0, -683913.815141469 2820393.1697519096 0, -683817.1119588523 2820564.133764186 0, -683798.7212036223 2820574.091676301 0, -683734.6547211821 2820608.784698552 0, -683729.2433599001 2820611.71585344 0, -683724.973466479 2820619.263663777 0, -683663.3630113038 2820646.328719441 0, -683606.6740045693 2820746.548567463 0, -683551.2397670313 2820767.638794945 0, -683489.7714684663 2820795.144686282 0, -683480.872286895 2820888.9620507676 0, -683290.4365471886 2821207.273167537 0, -683311.2688215015 2821326.1315004327 0, -683303.2284282156 2821410.9116964876 0, -683382.457</t>
+          <t>MULTIPOLYGON Z (((-779304.9079350996 2866327.0745835477 0, -779300.9590657263 2866326.6702074828 0, -779153.7570984508 2866310.424541069 0, -779126.2156186483 2866307.361045627 0, -779125.8700102569 2866307.315473458 0, -779106.148184011 2866305.145636247 0, -779106.194800808 2866304.721086294 0, -779105.9362982546 2866304.6869999627 0, -779107.8416011414 2866287.525426021 0, -779118.403661055 2866192.183078766 0, -779121.943787134 2866160.692226106 0, -779122.7684254933 2866153.3506462113 0, -779125.2419485286 2866131.254306182 0, -779149.6119593101 2865909.3109809356 0, -779150.1806210199 2865909.373383448 0, -779150.1813775826 2865909.366741886 0, -779145.2762115606 2865908.8863971997 0, -779144.4407769815 2865908.8045861954 0, -779140.3282349799 2865908.3484188453 0, -779130.3583803957 2865907.2381662573 0, -779051.6946062817 2865898.477727759 0, -778947.9796811765 2865887.046657124 0, -778925.8803831866 2865884.459117109 0, -778745.9815095876 2865864.2462161575 0, -778748.0973385327 2865839.5907291775 0, -778788.7313347592 2865472.488801352 0, -778789.1232820227 2865468.8928435566 0, -778782.8493347741 2865468.133675343 0, -778770.8662202087 2865466.777084145 0, -778587.2785353988 2865446.6961526177 0, -778630.5060057266 2865050.817523389 0, -778795.9364610518 2865069.071144758 0, -778829.1488904493 2865072.7371318964 0, -778832.1191208631 2865073.0992569556 0, -778875.3544676013 2864677.2069002697 0, -778821.0044294996 2864671.1840836187 0, -778673.6318773903 2864654.931451717 0, -778716.7582594071 2864259.0396635346 0, -778846.0666581673 2864273.1639524833 0, -778919.5771365796 2864281.3721959386 0, -778923.4298074759 2864281.7881243434 0, -779011.2024317926 2864291.481546741 0, -779021.4239533767 2864292.7003727993 0, -779040.0241077212 2864294.802851747 0, -779040.0241161513 2864294.802862341 0, -779048.0950406332 2864304.9275779794 0, -779081.5100963196 2864346.691926683 0, -779081.51011605 2864346.6919513326 0, -779081.5101339425 2864346.6919781645 0, -779103.2222831812 2864379.2385333944 0, -779110.4115474825 2864400.7378377835 0, -779145.2388073046 2864504.909856213 0, -779145.2373684414 2864504.9142325423 0, -779145.2398763419 2864504.9217334674 0, -779145.239876338 2864504.921733479 0, -779145.2398763392 2864504.9217334827 0, -779105.4091129539 2864626.054522275 0, -779107.6021636605 2864666.8165470483 0, -779114.1918241585 2864703.506553551 0, -779114.191915418 2864703.5070613227 0, -779114.1920173957 2864703.5076306025 0, -779120.2681808715 2864737.406605333 0, -779152.3886458386 2864800.707789942 0, -779192.2797327498 2864828.211610813 0, -779215.7149021933 2864853.127852828 0, -779262.4077841557 2864910.8684776765 0, -779262.4055274364 2864910.876613737 0, -779262.4090644304 2864910.8809871553 0, -779254.9582020501 2864937.7329249955 0, -779267.8374664417 2864984.89326154 0, -779271.255752108 2865019.5770358304 0, -779271.2549658094 2865019.584497317 0, -779271.2558011949 2865019.592966862 0, -779268.6462162543 2865044.3403834435 0, -779268.6462162522 2865044.340383445 0, -779268.6462162477 2865044.3403834878 0, -779243.0937434582 2865062.3057162617 0, -779231.5169619516 2865081.0065179598 0, -779228.8898344346 2865104.702292179 0, -779214.1056601275 2865115.198077089 0, -779205.6575091856 2865125.4143026145 0, -779202.9635111759 2865130.8248968916 0, -779202.9092646397 2865130.8649468333 0, -779201.9461432174 2865131.5760144787 0, -779201.3687132479 2865132.002328087 0, -779201.3140513613 2865132.04268468 0, -779196.9972393411 2865134.977016463 0, -779181.7520377578 2865145.3398674186 0, -779181.7448222385 2865145.341421074 0, -779181.7306119628 2865145.3444808493 0, -779176.4806674288 2865146.474905855 0, -779168.5528792638 2865148.175910826 0, -779157.1356959858 2865152.3430054043 0, -779146.6797055126 2865156.1514428747 0, -779139.7253875722 2865157.584441535 0, -779134.0559668748 2865158.7513434244 0, -779134.0559668734 2865158.7513434244 0, -779134.0559668269 2865158.751343434 0, -779125.9651313591 2865159.8935043905 0, -779079.2908318003 2865206.865736912 0, -779053.740847804 2865248.6332662883 0, -779060.3669293413 2865293.016810817 0, -779072.521815128 2865371.894083655 0, -779072.5202583339 2865371.897731961 0, -779072.5223159426 2865371.911083353 0, -779070.2483823916 2865377.2218135255 0, -779057.6609545639 2865406.748632715 0, -779042.7205976748 2865433.5028620926 0, -779039.152479286 2865439.924130304 0, -779023.0279794952 2865448.293106738 0, -778993.7520421153 2865463.826756115 0, -778970.6611095731 2865476.0778305396 0, -778968.6561214548 2865477.1415926316 0, -778956.4113200627 2865482.241545986 0, -778946.6793083777 2865486.32109739 0, -778946.6793082762 2865486.3210973786 0, -778934.1801994797 2865491.5606448776 0, -778917.3725716695 2865498.641953889 0, -778939.3769872008 2865584.7747839727 0, -778976.8123785012 2865626.5557441814 0, -779070.4881821149 2865731.398700857 0, -779138.7121427488 2865757.6186342165 0, -779193.8966056061 2865744.298193133 0, -779227.2728923232 2865741.3936695904 0, -779262.9244508899 2865760.6726428876 0, -779323.3717550738 2865789.4067152063 0, -779310.5830200284 2865837.322463818 0, -779310.5830133636 2865837.3224889184 0, -779309.2371529589 2865842.397671633 0, -779309.2371529434 2865842.397671654 0, -779309.2371529362 2865842.3976716814 0, -779304.6237460255 2865848.684998582 0, -779292.6560994192 2865864.9949638876 0, -779287.2914060361 2865886.2247151732 0, -779291.490815091 2865924.855617001 0, -779300.0528537801 2865939.7354915333 0, -779325.8083980508 2865984.182716592 0, -779329.5936830095 2865990.877125187 0, -779335.7647028733 2866001.3645638414 0, -779340.7360346571 2866009.9421461234 0, -779342.2131859002 2866012.3954330594 0, -779342.2131859086 2866012.3954330618 0, -779342.2131859087 2866012.395433061 0, -779342.2131880341 2866012.395433664 0, -779372.151402374 2866020.876621468 0, -779379.3495333014 2866022.90937798 0, -779387.2382461597 2866026.0080900206 0, -779414.3932899326 2866036.6744328826 0, -779419.9555692682 2866038.8594160196 0, -779469.6521037758 2866035.7577639148 0, -779505.5638708652 2866029.304145113 0, -779509.6160760403 2866028.57596547 0, -779586.2511909457 2866048.736966126 0, -779617.6114337902 2866070.9433910954 0, -779668.0572842329 2866133.4988183226 0, -779713.5557304206 2866181.3759299745 0, -779699.7635778274 2866250.2194864987 0, -779699.6693577461 2866250.696038443 0, -779673.6980300663 2866306.686730672 0, -779666.9540606847 2866309.5274188924 0, -779658.3149942142 2866313.166358084 0, -779631.6438362749 2866328.9537691833 0, -779599.8944918101 2866347.747102227 0, -779591.8881338246 2866352.7793916864 0, -779591.8881273797 2866352.7793957484 0, -779583.9506848671 2866357.808552827 0, -779568.3500247455 2866367.6919736937 0, -779554.0057215543 2866376.817223519 0, -779553.0384076122 2866378.842453414 0, -779551.4617086295 2866382.143530564 0, -779551.4617066641 2866382.1435346873 0, -779528.7638745711 2866429.7637730306 0, -779525.9447666332 2866449.6653061714 0, -779525.1477111776 2866455.5680601005 0, -779509.1860784377 2866573.1947606048 0, -779549.4492355619 2866622.156958724 0, -779585.8910487035 2866644.055816147 0, -779617.0343096714 2866656.3589980225 0, -779657.055098304 2866678.170773459 0, -779675.9214310695 2866702.196313196 0, -779686.9074296867 2866716.193585674 0, -779688.6923568146 2866718.467497366 0, -779731.2478500814 2866748.2971152854 0, -779735.0626553502 2866750.8928653626 0, -779745.1792336187 2866773.911404346 0, -779746.3262182855 2866776.5126066078 0, -779756.6804523873 2866780.2930155494 0, -779760.5911791024 2866781.6816453673 0, -779765.1353403393 2866783.4185599373 0, -779780.7410285155 2866801.9090242246 0, -779782.5802469932 2866804.0885802833 0, -779783.9213599105 2866811.0940339374 0, -779783.9907325234 2866811.4505314506 0, -779788.6696253056 2866835.16151928 0, -779793.970550902 2866838.8543598186 0, -779793.9705511765 2866838.8543600063 0, -779796.9830574616 2866840.9154834338 0, -779799.3910429042 2866842.5239838576 0, -779809.7036107051 2866849.3774993685 0, -779814.9315585205 2866854.655198107 0, -779817.2558039882 2866857.0005583656 0, -779849.9090321712 2866890.2079449045 0, -779851.6497902453 2866891.9764218726 0, -779851.9474376016 2866892.2784973974 0, -779851.948620692 2866892.2796980888 0, -779855.1715612088 2866893.450912427 0, -779855.1715615301 2866893.450912543 0, -779883.5784008092 2866903.5945362016 0, -779889.4830955303 2866906.0520811765 0, -779889.4830956871 2866906.052081239 0, -779899.4872820814 2866910.0145255593 0, -779902.7661595201 2866909.1573240245 0, -779903.06432163 2866909.0727239456 0, -779941.7597677703 2866901.0007285383 0, -779945.6779448233 2866900.181854022 0, -779990.7910749582 2866884.045822849 0, -780030.6135322689 2866836.682446488 0, -780033.2684257341 2866833.597392254 0, -780033.2684354124 2866833.59738504 0, -780035.5375477438 2866831.904521111 0, -780057.7257643872 2866815.6568061677 0, -780064.1461269036 2866818.502320128 0, -780090.9366377833 2866830.3917377423 0, -780133.89057774 2866842.597644402 0, -780150.4058261721 2866852.3191592274 0, -780150.411989451 2866852.3350040643 0, -780150.4600618072 2866852.3633030327 0, -780175.428586096 2866916.474325607 0, -780189.5268056914 2866982.7689993717 0, -780182.4600024628 2867001.0239812057 0, -780182.3555241922 2867001.0592753175 0, -780182.3460716568 2867001.083688821 0, -780171.1883500539 2867004.8316912395 0, -780171.188347239 2867004.8316921904 0, -780149.7691617253 2867012.024510049 0, -780113.6291492814 2867097.1966597107 0, -780112.5635850911 2867179.7537893984 0, -780119.5752173394 2867199.9731411543 0, -780119.5752190775 2867199.973146141 0, -780124.6908509599 2867214.502216883 0, -780127.9139902004 2867223.6557753137 0, -780127.913991517 2867223.6557789934 0, -780137.4979773352 2867250.2324645696 0, -780178.9906645096 2867279.6379998005 0, -780179.1848188583 2867279.775487024 0, -780196.6391077609 2867292.1453208667 0, -780196.6444624714 2867292.154038222 0, -780196.7084945008 2867292.1994353007 0, -780219.2578227344 2867328.912949185 0, -780235.8500057842 2867380.125415139 0, -780235.0224535076 2867424.9112286805 0, -780223.0311947786 2867462.8745537414 0, -780214.7739112539 2867483.972928059 0, -780212.2158848194 2867490.689476867 0, -780211.8137265675 2867491.3326835395 0, -780210.2229013377 2867493.8770287107 0, -780210.222900861 2867493.877029491 0, -780203.9572028025 2867504.257186381 0, -780187.6526605099 2867515.9848600714 0, -780172.9110753008 2867540.9148804476 0, -780108.4302354697 2867585.6731637605 0, -780108.3680211534 2867585.63938935 0, -780108.3545303716 2867585.648749364 0, -780086.1618562269 2867573.594301091 0, -780064.7922477692 2867543.212531911 0, -780015.172118825 2867545.1532341493 0, -779981.4447819251 2867558.5686488766 0, -779960.3008234018 2867566.992400341 0, -779954.7320235713 2867569.1731972136 0, -779952.0898931359 2867570.228046003 0, -779952.0898924158 2867570.228046878 0, -779933.4884271858 2867592.9712232375 0, -779931.8133636253 2867595.2339429366 0, -779920.4619358924 2867613.6809061766 0, -779914.5769850386 2867623.4378382144 0, -779906.2403500113 2867637.2861757823 0, -779909.7839589368 2867660.69840403 0, -779910.8196514907 2867667.540766627 0, -779910.819651789 2867667.540768598 0, -779913.2101330699 2867683.2267922917 0, -779921.0107550346 2867694.4813809455 0, -779921.0107599307 2867694.481387992 0, -779935.6925738538 2867715.5333454106 0, -779941.7260559902 2867722.2085948098 0, -779938.8574386678 2867732.09062936 0, -779942.7537764932 2867738.28435054 0, -779953.4220376707 2867755.2412652266 0, -779958.6876414513 2867760.5741329957 0, -779986.6780746016 2867788.9244766654 0, -779994.4211631832 2867833.4695059485 0, -779996.0619575984 2867843.330221665 0, -780011.4805325873 2867878.64794406 0, -780016.4294372235 2867889.9838030394 0, -780021.2511991784 2867901.2779533747 0, -780035.1559595682 2867933.8245187956 0, -780067.3044794233 2867958.099728915 0, -780092.3876133718 2867976.934358336 0, -780129.5150795655 2867976.8573418804 0, -780143.2501499564 2867976.7104670755 0, -780154.1347760144 2867970.2724514757 0, -780162.0250643261 2867966.2409890736 0, -780175.9838638561 2867959.2371197087 0, -780208.9271376494 2867942.498026442 0, -780211.8219856764 2867941.0769677185 0, -780230.718415916 2867961.4392033685 0, -780257.9387566276 2867990.4320396497 0, -780270.7877296533 2868008.664862903 0, -780271.4156469837 2868030.8659969084 0, -780271.5125259771 2868035.891481801 0, -780271.6917727466 2868042.667724333 0, -780271.1457061982 2868045.415702571 0, -780267.2596377166 2868048.030826591 0, -780253.6413667245 2868058.8683116804 0, -780257.2126298236 2868082.1137912082 0, -780258.9307758686 2868093.286304257 0, -780258.1532994827 2868103.3527499135 0, -780256.0195743253 2868131.016723943 0, -780267.8618371518 2868157.734759952 0, -780275.7022799109 2868175.388378105 0, -780283.7983055882 2868179.5489601586 0, -780292.6615983079 2868183.7742528054 0, -780354.078242831 2868213.054084066 0, -780369.8741598591 2868209.5798874223 0, -780390.6740443747 2868205.0054862285 0, -780430.7194506521 2868157.6157531324 0, -780465.6122176911 2868123.0502816536 0, -780499.7822652165 2868108.0142097017 0, -780530.2662878109 2868100.6320033004 0, -780561.2797663695 2868096.1173576936 0, -780585.229592231 2868116.792696185 0, -780591.0638451594 2868121.8172028866 0, -780624.0195790911 2868153.9296654146 0, -780643.824291495 2868181.95309038 0, -780674.2701028391 2868231.3114375924 0, -780667.647170231 2868287.642819418 0, -780616.1934146394 2868341.3145533646 0, -780507.0768621111 2868362.4499460557 0, -780457.2872171006 2868398.598726522 0, -780449.404758897 2868423.2172151553 0, -780437.8880136701 2868459.33193768 0, -780438.5095848306 2868483.186428469 0, -780439.0009394187 2868500.6547144447 0, -780439.8144682248 2868530.312555635 0, -780468.3067455092 2868558.260272274 0, -780500.407432749 2868589.6802325044 0, -780508.0750506903 2868590.5639736885 0, -780529.5642923648 2868593.031618096 0, -780607.6072858134 2868608.3802648797 0, -780638.321222069 2868629.9391305605 0, -780647.700380725 2868636.5278843227 0, -780651.56526434 2868643.8651430532 0, -780652.9061471489 2868646.433761697 0, -780655.1950769854 2868650.9467331795 0, -780660.1665794743 2868660.6458233334 0, -780679.864017195 2868676.355004451 0, -780714.946225137 2868699.9128579376 0, -780743.0561164145 2868725.705022825 0, -780758.935581237 2868737.913406749 0, -780771.7703215113 2868755.5970413806 0, -780782.0069733132 2868771.081739324 0, -780758.0237120664 2868806.7965130196 0, -780741.8468468265 2868788.8999802982 0, -780733.2992106574 2868779.4440627513 0, -780678.7923149357 2868764.3483426278 0, -780660.1429525369 2868758.9684430636 0, -780658.5017949716 2868756.0317070684 0, -780656.7962791208 2868752.9729189766 0, -780649.5004004847 2868739.8882335406 0, -780642.4107917225 2868741.3814160144 0, -780614.7483967241 2868747.16278265 0, -780620.0283193644 2868770.6165203536 0, -780621.9438328906 2868779.125455868 0, -780617.1331207319 2868794.1621076036 0, -780608.5842629903 2868820.8827284453 0, -780610.4017453694 2868829.684730192 0, -780620.786809104 2868879.735953714 0, -780623.0206860149 2868890.5036827917 0, -780623.7801947279 2868894.1227484457 0, -780624.8843686173 2868899.486581847 0, -780629.1621139545 2868906.5911678923 0, -780645.4627844561 2868933.6927095293 0, -780665.7848580597 2868946.047142861 0, -780673.2674873873 2868950.5959313135 0, -780711.3980113654 2868978.7783207335 0, -780729.7938893085 2868998.102228022 0, -780806.5890987276 2869042.5713849533 0, -780829.2104213691 2869055.652398372 0, -780846.7317857399 2869077.7908078814 0, -780849.6888465665 2869093.1635548575 0, -780851.2444533325 2869101.205827288 0, -780859.1080571082 2869106.840241632 0, -780880.0671380667 2869121.6901659234 0, -780904.5848287079 2869147.0680197002 0, -780921.8018630006 2869228.848461901 0, -780933.9451154479 2869278.0984647786 0, -780937.0773687472 2869290.7618271643 0, -780932.6817647588 2869314.222176287 0, -780592.4494464375 2869276.510103586 0, -780581.8633916792 2869275.322169444 0, -780567.0906029015 2869273.687439044 0, -780379.9151030026 2869252.798227524 0, -780381.1025343707 2869240.0205894937 0, -780383.0646016569 2869217.729473123 0, -780399.8209768042 2869054.593767323 0, -780199.4815631429 2869031.6136801844 0, -780203.080664142 2868998.261281361 0, -780204.655392828 2868983.713981458 0, -780220.9781707377 2868835.5410523666 0, -780218.0416167416 2868835.220864358 0, -780018.8788017232 2868813.224142559 0, -780040.9544328884 2868615.3333827914 0, -779839.1214824963 2868592.593344387 0, -779860.9283054336 2868395.968623219 0, -779860.828353818 2868395.9572289027 0, -779860.8258508032 2868395.9799712407 0, -779796.6513697552 2868388.657097032 0, -779840.3492388529 2867994.546192049 0, -779830.6159661649 2867993.376086266 0, -779721.0984120859 2867980.393429644 0, -779721.0738629557 2867980.3909338894 0, -779721.0739095071 2867980.3905237895 0, -779538.1912544267 2867958.699190479 0, -779567.3780728334 2867697.7170125665 0, -779583.1859263789 2867557.450209374 0, -779583.1859263411 2867557.45020937 0, -779583.3632852 2867554.6543739727 0, -779621.887920612 2867195.499852003 0, -779626.0347395401 2867161.275451751 0, -779423.8093009266 2867139.980027611 0, -779423.8585457572 2867139.514386206 0, -779423.78805035 2867139.5064977612 0, -779443.4744816157 2866953.0341884177 0, -779446.6159386438 2866923.454483797 0, -779465.5197998745 2866745.580134709 0, -779302.7630156983 2866727.718068347 0, -779302.7629729796 2866727.7180636683 0, -779264.7313398954 2866723.53681002 0, -779264.5992211195 2866723.5222846875 0, -779264.7791592191 2866720.7265381604 0, -779307.7513682813 2866327.328534183 0, -779304.9079350996 2866327.0745835477 0), (-779174.191770332 2865911.9384812503 0, -779174.1917702062 2865911.9384812354 0, -779172.9852149499 2865911.798587795 0, -779174.191770332 2865911.9384812503 0)), ((-785065.6032716993 2884211.4965632465 0, -785071.1520494085 2884237.5328455777 0, -785074.0743182834 2884251.245471162 0, -785074.0743187336 2884251.245473275 0, -785072.8350446203 2884251.8137203488 0, -785059.5933640503 2884257.886078278 0, -785058.4655225205 2884258.4033064526 0, -785029.9331651429 2884271.4876718954 0, -784982.5444845094 2884293.218891352 0, -784982.5329867667 2884293.224081307 0, -784981.2149508686 2884293.828500253 0, -784981.2147696365 2884293.8286640937 0, -784981.1467549306 2884293.859853873 0, -784981.1130963754 2884293.9201835813 0, -784981.1126494949 2884293.9209845713 0, -784942.4933314892 2884328.8343114667 0, -784938.2966815983 2884346.38967372 0, -784936.6179760093 2884353.4133089255 0, -784936.4155603364 2884354.2629710403 0, -784935.9100860038 2884356.388015854 0, -784928.5993805551 2884386.991325736 0, -784993.285410236 2884560.2029558844 0, -785012.5606098194 2884631.6563191717 0, -785012.5606306553 2884631.6563964025 0, -785012.56075832 2884631.6565387323 0, -785100.1409543537 2884729.2930047493 0, -785100.1382688797 2884729.2942893715 0, -785100.1383894685 2884729.2944238125 0, -785100.0426378414 2884729.3402275466 0, -785100.0479940528 2884729.3461995577 0, -784865.9550747823 2884841.3273328207 0, -784870.340734311 2884898.9978950107 0, -785089.1225307342 2885040.6966766133 0, -785137.4241029804 2885071.9800291564 0, -785137.4241168518 2885071.9800381204 0, -785144.7563596909 2885076.7156066117 0, -785149.5507473459 2885089.185002046 0, -785149.5507482933 2885089.1850045086 0, -785181.1397999076 2885171.1300373194 0, -785181.053034548 2885171.1755495123 0, -785181.0546302543 2885171.1796889217 0, -785068.2787474302 2885230.336112334 0, -785090.9109817881 2885300.809213529 0, -785167.8188858558 2885335.1925203144 0, -785137.469540249 2885398.2045503845 0, -785134.704310118 2885449.9587178538 0, -785134.6223183037 2885449.9492915287 0, -785134.6191365693 2885450.009068597 0, -784753.0042645405 2885403.7581594787 0, -784796.9568533582 2885008.159964477 0, -784840.9078724972 2884612.558932737 0, -784887.075394753 2884217.026761061 0, -784911.6030819823 2884002.4308323604 0, -784911.6851222854 2884002.415955814 0, -784911.6851257501 2884002.415925501 0, -784944.0389234985 2883996.549170707 0, -784952.7095800161 2883994.9769096673 0, -784952.8177494847 2883994.957295599 0, -784952.8177494848 2883994.957295599 0, -784967.5701537884 2883992.282283246 0, -785000.7248227113 2884032.8557939967 0, -784985.4464197728 2884082.796609726 0, -784985.4170368295 2884082.8926543295 0, -784985.4169973311 2884082.892783439 0, -784985.4749725992 2884082.943058755 0, -784986.1639220841 2884083.540505809 0, -784987.2354451539 2884084.469715156 0, -784987.2354451566 2884084.4697151585 0, -785018.3869469 2884111.4838480535 0, -785018.3869469035 2884111.4838480563 0, -785020.9831284193 2884113.7352192122 0, -785050.1615275689 2884139.0394245973 0, -785065.6032716993 2884211.4965632465 0)), ((-778018.9447448857 2848989.745918616 0, -778066.8683336076 2849016.709277986 0, -778107.8935463295 2849031.885046103 0, -778107.8935678903 2849031.885071271 0, -778107.8998301893 2849031.887387773 0, -778165.2545033393 2849098.842157993 0, -778111.3076032304 2849130.168651748 0, -778087.6126041275 2849186.3163977806 0, -778126.6375942499 2849232.727695082 0, -778223.3552550377 2849265.8186636334 0, -778254.8962661957 2849265.7881828006 0, -778317.3286196977 2849256.3805453232 0, -778320.3206548779 2849255.9305497576 0, -778382.8332636404 2849238.0703015476 0, -778423.6735988836 2849259.0496166716 0, -778428.9827689723 2849261.776760421 0, -778454.2196999231 2849278.691583925 0, -778488.0754617819 2849356.2284987266 0, -778488.6501968709 2849382.5362317674 0, -778489.152936014 2849406.1901539196 0, -778450.2355246089 2849445.274848413 0, -778352.5313618146 2849449.953824687 0, -778312.1611298464 2849447.1315117213 0, -778292.6974834282 2849465.247074199 0, -778251.9586401515 2849503.1628931905 0, -778240.67791667 2849566.0853533074 0, -778195.7662688775 2849622.488102977 0, -778177.5478470904 2849623.076913356 0, -778120.4627838772 2849639.9752028664 0, -778096.8846394607 2849645.720705325 0, -778000.5748267936 2849733.491153451 0, -778000.5748146558 2849733.491172231 0, -777995.0456996908 2849742.0505981613 0, -778024.6618800078 2849822.4492694708 0, -778065.4236408372 2849893.553183616 0, -778095.0547552725 2849940.7998997993 0, -778111.123129531 2849966.4205661775 0, -778152.0380063502 2849995.857612358 0, -778232.4635076745 2850022.7648026235 0, -778232.4635694196 2850022.7648232784 0, -778272.3694730203 2850005.137503722 0, -778286.1607537577 2849979.6017443314 0, -778296.920254595 2849936.9769389974 0, -778336.2231786009 2849907.0715158912 0, -778393.8367818684 2849849.3580969116 0, -778393.8430354721 2849849.360552195 0, -778393.8430511502 2849849.360536491 0, -778403.6653998105 2849853.216998893 0, -778428.6853912089 2849863.0403224714 0, -778428.6854091042 2849863.040385179 0, -778428.6991688223 2849863.0457875365 0, -778443.4649263347 2849914.8092266163 0, -778414.1937640968 2849949.001410578 0, -778371.7344926831 2850017.615826767 0, -778382.3051193785 2850074.338933517 0, -778398.5470595541 2850082.064149347 0, -778403.3046900313 2850084.3265774795 0, -778446.810059922 2850176.3057739446 0, -778447.2446485488 2850181.0248513315 0, -778455.2041889131 2850268.246773478 0, -778429.6688173915 2850307.581051144 0, -778392.1623876267 2850337.822753677 0, -778391.2678431092 2850381.5535695823 0, -778409.1754104488 2850423.8003512262 0, -778443.3267647222 2850418.882471604 0, -778472.0479189741 2850425.3049393725 0, -778472.0487260116 2850425.3051198344 0, -778472.1538681126 2850425.351573998 0, -778539.5934494556 2850455.1479067337 0, -778539.5934506133 2850455.1479104175 0, -778539.6047455587 2850455.1529007806 0, -778556.6351373835 2850509.3733091513 0, -778560.1761920195 2850560.9527782807 0, -778547.8672037215 2850595.660859155 0, -778537.9140969089 2850606.129185271 0, -778520.642783997 2850623.4954078286 0, -778493.3349725715 2850650.953595447 0, -778451.0096472857 2850697.8333630995 0, -778412.2927054393 2850735.7666474488 0, -778332.2267194751 2850801.4565049415 0, -778302.6506236638 2850831.477270452 0, -778261.3214377748 2850858.485909124 0, -778219.6404445403 2850879.0038987314 0, -778186.4701389986 2850893.9341213712 0, -778155.5423610273 2850942.964488242 0, -778155.3875860953 2850943.902271544 0, -778153.8866063681 2850952.996727043 0, -778144.8386589016 2851007.818732372 0, -778144.838656444 2851007.8187473714 0, -778143.8777997025 2851013.701355991 0, -778149.8737242838 2851080.1654093326 0, -778164.1845627591 2851163.640269842 0, -778188.4564350559 2851188.1242920617 0, -778205.9905316551 2851205.810038239 0, -778226.8356577648 2851241.215181279 0, -778255.9156079143 2851286.877953428 0, -778270.0726153597 2851365.3265308696 0, -778270.072638942 2851365.326661501 0, -778270.0726389335 2851365.3266615 0, -778270.0726389342 2851365.326661504 0, -778094.4605108831 2851346.208892302 0, -777690.6850503956 2851302.830592308 0, -777690.6850503958 2851302.8305923063 0, -777690.6850503882 2851302.8305923054 0, -777733.9628193304 2850906.4917634716 0, -777777.2388194209 2850510.150120197 0, -777820.9831457793 2850114.3101011575 0, -777864.7277990956 2849718.467504392 0, -777460.6128714907 2849673.6653484977 0, -777056.4934434132 2849628.885801183 0, -777056.4934434134 2849628.885801181 0, -777056.4934434058 2849628.8858011803 0, -777099.6764418286 2849232.3232875033 0, -777503.5643492694 2849277.22811051 0, -777690.8115454458 2849298.045287109 0, -777908.4311447623 2849322.23911069 0, -777951.249948151 2848933.928056874 0, -777951.249948158 2848933.92805688 0, -777951.2499481585 2848933.9280568752 0, -777951.4898512964 2848934.1258694273 0, -778018.9447448857 2848989.745918616 0)), ((-775704.8974972891 2861917.3864071863 0, -775748.9644106021 2861520.776052916 0, -776152.9127795845 2861565.5854092953 0, -776152.9127961973 2861565.5854111384 0, -776553.9168441865 2861610.0682845274 0, -776556.8636252692 2861610.390778591 0, -776512.039852616 2862006.354712643 0, -776467.216922884 2862402.3131001843 0, -776466.9929051308 2862404.3219294287 0, -776423.0514987482 2862798.356692091 0, -776019.7807803612 2862754.2477628333 0, -775616.5129932838 2862710.1317281877 0, -775616.7509383601 2862707.339991846 0, -775660.8313339656 2862313.9912819895 0, -775661.0604045603 2862311.1987747676 0, -775704.8974972891 2861917.3864071863 0)))</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1665,31 +1665,31 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>None Listed, Common Schools, Public Land Trust Income - Navigable Rivers</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Subsurface, subsurface, Surface</t>
+          <t>subsurface, Surface</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="G26" t="n">
-        <v>1809.4</v>
+        <v>1183.38</v>
       </c>
       <c r="H26" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I26" t="n">
-        <v>1725.02</v>
+        <v>1054.27</v>
       </c>
       <c r="J26" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="K26" t="n">
-        <v>3534.42</v>
+        <v>2237.65</v>
       </c>
       <c r="L26" t="n">
         <v>2110405.94</v>
@@ -1698,7 +1698,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1722347.3590887182 1241236.1226395366 0, -1722378.978481109 1241226.6656640186 0, -1722458.0590248206 1241214.3619041357 0, -1722511.0244963982 1241209.64816162 0, -1722554.9108853338 1241209.2290898764 0, -1722573.2574028883 1241209.0540111328 0, -1722619.8481824573 1241210.135066921 0, -1722651.3319137658 1241215.0706257604 0, -1722682.5981761983 1241220.9879581626 0, -1722708.2435573405 1241227.6669537546 0, -1722709.5477916386 1241228.0066600225 0, -1722745.0125975516 1241237.9475634922 0, -1722776.2787327354 1241243.8649960575 0, -1722784.8158541396 1241246.5779228427 0, -1722808.6150244088 1241254.1408575638 0, -1722845.5848813362 1241266.4767380522 0, -1722851.2141634866 1241269.2062787032 0, -1722904.4176961277 1241295.0027672967 0, -1722931.0321193866 1241308.1281024928 0, -1722956.3408534867 1241327.1445511675 0, -1722983.8075472587 1241345.6103498647 0, -1723012.7796750604 1241366.4711491766 0, -1723056.3874646388 1241403.976641978 0, -1723075.4393329283 1241423.663191418 0, -1723077.4803774995 1241425.9903314833 0, -1723099.0068817858 1241450.5344244046 0, -1723124.515092653 1241477.8367388353 0, -1723147.4297913224 1241507.6535189159 0, -1723165.4931102102 1241536.392342372 0, -1723193.8396936913 1241601.412638931 0, -1723209.8264970898 1241644.112965642 0, -1723218.0693761532 1241675.8206161677 0, -1723223.1834689046 1241707.8632057626 0, -1723227.110158572 1241740.6721114677 0, -1723227.3697827994 1241758.299072991 0, -1723227.490938815 1241766.511721777 0, -1723223.1203431368 1241795.4164874577 0, -1723216.591583556 1241824.8717889888 0, -1723194.2481291608 1241888.9307157993 0, -1723191.2465811328 1241898.1658365303 0, -1723181.4444746135 1241928.3238711308 0, -1723169.9463166813 1241961.8260648944 0, -1723156.9700882272 1242034.1478473837 0, -1723154.20692709 1242069.5589382623 0, -1723153.6513406222 1242076.6790162898 0, -1723152.7261972136 1242108.4100066365 0, -1723152.7500927413 1242108.7320616634 0, -1723150.208765948 1242110.7701281658 0, -1723106.6430053764 1242145.714618138 0, -1723094.3103107193 1242391.8233115352 0, -1723111.9207210592 1242612.7974887264 0, -1723223.9138330873 1242782.587060279 0, -1723029.603357652 1242879.8031119374 0, -1723029.602232531 1242879.8028472173 0, -1723029.585444656 1242879.8112464237 0, -1722884.2021506082 1242845.6052545607 0, -1722884.0032644228 1242845.6278090398 0, -1722757.3192187187 1242863.5770453282 0, -1722733.3568359872 1242879.1896421772 0, -1722733.3527278912 1242879.1889246006 0, -1722733.3389890755 1242879.197876182 0, -1722559.6401527082 1243013.8007383328 0, -1722381.6339916687 1242949.53811921 0, -1722232.672660665 1242832.3087205358 0, -1722211.1041122193 1242787.965799454 0, -1721996.7433034913 1242750.5225927236 0, -1722003.6491573025 1242716.5649391306 0, -1722003.4785811466 1242716.544707561 0, -1722073.9175046657 1242361.0715618066 0, -1722080.7294661691 1242326.694809999 0, -1722153.0310744173 1241961.8344069486 0, -1721764.424998388 1241891.068965686 0, -1721366.1294605085 1241818.5546973892 0, -1720979.3183402896 1241748.1524682967 0, -1720972.6732262475 1241746.9431201753 0, -1720586.7628300434 1241676.72268317 0, -1720406.9748293536 1241642.9505246803 0, -1720355.4043134027 1241635.7290223027 0, -1720331.8072004942 1241631.964132609 0, -1720266.5560556562 1241619.4766118755 0, -1720264.2451736396 1241616.33845115 0, -1720240.328073899 1241583.8592163166 0, -1720213.1145884478 1241545.876842757 0, -1720206.239817999 1241537.1404345052 0, -1720175.7812797052 1241498.4348461167 0, -1720117.2735897598 1241413.3225018526 0, -1720074.5715069098 1241353.3557109775 0, -1720068.2504339456 1241331.347701848 0, -1720067.8685424912 1241305.5083018334 0, -1720071.2679676383 1241276.3881464894 0, -1720083.61689073 1241248.2264821115 0, -1720108.2617918705 1241219.7063913245 0, -1720130.295560692 1241202.9680343617 0, -1720197.6765641028 1241186.2199534823 0, -1720273.1628833918 1241200.430675972 0, -1720343.965099368 1241213.7592215824 0, -1720387.9010476028 1241230.3286424568 0, -1720442.8701737248 1241248.7231904976 0, -1720502.2555709393 1241270.1592070626 0, -1720569.2850051324 1241298.4448821677 0, -1720631.3635780402 1241321.509484366 0, -1720656.1041292115 1241328.8255317586 0, -1720656.1919981353 1241328.8515153455 0, -1720673.4018369738 1241333.9406108344 0, -1720751.3217416313 1241363.6157461514 0, -1720779.1239249345 1241375.9743005778 0, -1720839.6970031105 1241396.6443093063 0, -1720867.6166970753 1241403.8781641305 0, -1720909.0201827416 1241409.987069465 0, -1720971.8690523116 1241424.9817720288 0, -1721025.7679832708 1241439.018070436 0, -1721040.422373618 1241441.1608262327 0, -1721080.0024789404 1241446.948017187 0, -1721118.0598608023 1241454.3739352655 0, -1721168.6308853503 1241460.4596318211 0, -1721213.380481255 1241465.2518001262 0, -1721286.802439242 1241478.4752963868 0, -1721324.2250700656 1241479.579163603 0, -1721403.93976753 1241473.5970794298 0, -1721440.4980931187 1241473.9168606205 0, -1721481.1606803727 1241474.2725525228 0, -1721556.1418710703 1241462.0877432576 0, -1721597.1462023102 1241451.62527158 0, -1721616.9167840271 1241448.386496333 0, -1721647.8530407362 1241443.3186712575 0, -1721689.3924369845 1241435.0353536338 0, -1721730.8318611628 1241422.6091250256 0, -1721812.840776079 1241401.6841761821 0, -1721854.4980541016 1241388.276426463 0, -1721863.7109090104 1241385.9255508024 0, -1721884.7117926555 1241380.5671934842 0, -1721916.3311244752 1241371.1099750742 0, -1721970.5019116465 1241356.3617224116 0, -1722005.9024231657 1241343.6242233745 0, -1722048.7475203713 1241329.449915905 0, -1722080.1492643817 1241320.9747471123 0, -1722098.284799741 1241312.6421258582 0, -1722119.33101951 1241304.9563377919 0, -1722143.406089291 1241292.7925285716 0, -1722175.4606723138 1241281.3717397756 0, -1722216.9003799972 1241268.9456731929 0, -1722262.5322767175 1241255.7107134452 0, -1722283.2675461078 1241249.6965605556 0, -1722295.9735278878 1241247.0056232987 0, -1722299.0169854849 1241246.361047292 0, -1722347.3590887182 1241236.1226395366 0), (-1723009.6320559324 1241731.4823028664 0, -1723015.5545509255 1241746.463191892 0, -1723014.774587201 1241744.489667424 0, -1723011.709418197 1241736.7367974606 0, -1723009.6320559324 1241731.4823028664 0), (-1722610.5526441797 1241224.6314802137 0, -1722708.167260696 1241245.7283784277 0, -1722705.0190924767 1241245.047048451 0, -1722702.9337487202 1241244.5958083365 0, -1722610.5526441797 1241224.6314802137 0), (-1722454.2543153085 1241304.430653828 0, -1722454.2543160145 1241304.4306540184 0, -1722454.98907467 1241304.055503984 0, -1722454.2543153085 1241304.430653828 0), (-1722414.2925843324 1241324.8341496456 0, -1722400.8516707958 1241359.638348673 0, -1722378.0255372766 1241418.7451582972 0, -1722414.2925843324 1241324.8341496456 0)), ((-1726744.1875113233 1247804.5482547088 0, -1726667.2191239798 1248203.6930200334 0, -1726272.475200279 1248126.9230959278 0, -1726349.5557299664 1247727.7893932688 0, -1726744.1875113233 1247804.5482547088 0)))</t>
+          <t>MULTIPOLYGON Z (((-1720266.5560556562 1241619.4766118755 0, -1720264.2451736396 1241616.33845115 0, -1720240.328073899 1241583.8592163166 0, -1720213.1145884478 1241545.876842757 0, -1720206.239817999 1241537.1404345052 0, -1720175.7812797052 1241498.4348461167 0, -1720117.2735897598 1241413.3225018526 0, -1720074.5715069098 1241353.3557109775 0, -1720068.2504339456 1241331.347701848 0, -1720067.8685424912 1241305.5083018334 0, -1720071.2679676383 1241276.3881464894 0, -1720083.61689073 1241248.2264821115 0, -1720108.2617918705 1241219.7063913245 0, -1720130.295560692 1241202.9680343617 0, -1720197.6765641028 1241186.2199534823 0, -1720273.1628833918 1241200.430675972 0, -1720343.965099368 1241213.7592215824 0, -1720387.9010476028 1241230.3286424568 0, -1720442.8701737248 1241248.7231904976 0, -1720502.2555709393 1241270.1592070626 0, -1720569.2850051324 1241298.4448821677 0, -1720631.3635780402 1241321.509484366 0, -1720656.1041292115 1241328.8255317586 0, -1720656.1919981353 1241328.8515153455 0, -1720673.4018369738 1241333.9406108344 0, -1720751.3217416313 1241363.6157461514 0, -1720779.1239249345 1241375.9743005778 0, -1720839.6970031105 1241396.6443093063 0, -1720867.6166970753 1241403.8781641305 0, -1720909.0201827416 1241409.987069465 0, -1720971.8690523116 1241424.9817720288 0, -1721025.7679832708 1241439.018070436 0, -1721040.422373618 1241441.1608262327 0, -1721080.0024789404 1241446.948017187 0, -1721118.0598608023 1241454.3739352655 0, -1721168.6308853503 1241460.4596318211 0, -1721213.380481255 1241465.2518001262 0, -1721286.802439242 1241478.4752963868 0, -1721324.2250700656 1241479.579163603 0, -1721403.93976753 1241473.5970794298 0, -1721440.4980931187 1241473.9168606205 0, -1721481.1606803727 1241474.2725525228 0, -1721556.1418710703 1241462.0877432576 0, -1721597.1462023102 1241451.62527158 0, -1721616.9167840271 1241448.386496333 0, -1721647.8530407362 1241443.3186712575 0, -1721689.3924369845 1241435.0353536338 0, -1721730.8318611628 1241422.6091250256 0, -1721812.840776079 1241401.6841761821 0, -1721854.4980541016 1241388.276426463 0, -1721863.7109090104 1241385.9255508024 0, -1721884.7117926555 1241380.5671934842 0, -1721916.3311244752 1241371.1099750742 0, -1721970.5019116465 1241356.3617224116 0, -1722005.9024231657 1241343.6242233745 0, -1722048.7475203713 1241329.449915905 0, -1722080.1492643817 1241320.9747471123 0, -1722098.284799741 1241312.6421258582 0, -1722119.33101951 1241304.9563377919 0, -1722143.406089291 1241292.7925285716 0, -1722175.4606723138 1241281.3717397756 0, -1722216.9003799972 1241268.9456731929 0, -1722262.5322767175 1241255.7107134452 0, -1722283.2675461078 1241249.6965605556 0, -1722295.9735278878 1241247.0056232987 0, -1722299.0169854849 1241246.361047292 0, -1722252.9485856215 1241478.6413275711 0, -1722272.6254606016 1241475.3149359988 0, -1722378.0255372766 1241418.7451582972 0, -1722414.2925843324 1241324.8341496456 0, -1722454.1728438796 1241304.4086799675 0, -1722454.2543160145 1241304.4306540184 0, -1722454.98907467 1241304.055503984 0, -1722610.5526441797 1241224.6314802137 0, -1722708.167260696 1241245.7283784277 0, -1722769.9371245964 1241296.428067863 0, -1722919.9237587042 1241484.540896977 0, -1722964.7576367015 1241617.9722237035 0, -1723002.2130112445 1241712.7152698801 0, -1723009.6320559324 1241731.4823028664 0, -1723015.5545509255 1241746.463191892 0, -1723191.6603304711 1241896.8928183888 0, -1723191.2465811328 1241898.1658365303 0, -1723181.4444746135 1241928.3238711308 0, -1723169.9463166813 1241961.8260648944 0, -1723156.9700882272 1242034.1478473837 0, -1723153.6513406222 1242076.6790162898 0, -1723152.7261972136 1242108.4100066365 0, -1723152.7500927413 1242108.7320616634 0, -1723150.208765948 1242110.7701281658 0, -1723106.6430053764 1242145.714618138 0, -1723094.3103107193 1242391.8233115352 0, -1723111.9207210592 1242612.7974887264 0, -1723223.9138330873 1242782.587060279 0, -1723029.603357652 1242879.8031119374 0, -1723029.602232531 1242879.8028472173 0, -1723029.585444656 1242879.8112464237 0, -1722884.2021506082 1242845.6052545607 0, -1722884.0032644228 1242845.6278090398 0, -1722757.3192187187 1242863.5770453282 0, -1722733.3568359872 1242879.1896421772 0, -1722733.3527278912 1242879.1889246006 0, -1722733.3389890755 1242879.197876182 0, -1722559.6401527082 1243013.8007383328 0, -1722381.6339916687 1242949.53811921 0, -1722232.672660665 1242832.3087205358 0, -1722211.1041122193 1242787.965799454 0, -1721996.7433034913 1242750.5225927236 0, -1722003.6491573025 1242716.5649391306 0, -1722003.4785811466 1242716.544707561 0, -1722073.9175046657 1242361.0715618066 0, -1722080.7294661691 1242326.694809999 0, -1722153.0310744173 1241961.8344069486 0, -1721764.424998388 1241891.068965686 0, -1721366.1294605085 1241818.5546973892 0, -1720979.3183402896 1241748.1524682967 0, -1720972.6732262475 1241746.9431201753 0, -1720586.7628300434 1241676.72268317 0, -1720406.9748293536 1241642.9505246803 0, -1720355.4043134027 1241635.7290223027 0, -1720331.8072004942 1241631.964132609 0, -1720266.5560556562 1241619.4766118755 0)), ((-1726349.5557299664 1247727.7893932688 0, -1726744.1875113233 1247804.5482547088 0, -1726667.2191239798 1248203.6930200334 0, -1726272.475200279 1248126.9230959278 0, -1726349.5557299664 1247727.7893932688 0)))</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1713,22 +1713,22 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PENITENTIARY LAND FUND, NAVIGABLE STREAMBEDS, School Lands</t>
+          <t>PENITENTIARY LAND FUND, School Lands</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G27" t="n">
-        <v>536.51</v>
+        <v>367.17</v>
       </c>
       <c r="H27" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I27" t="n">
         <v>619.86</v>
@@ -1737,7 +1737,7 @@
         <v>5</v>
       </c>
       <c r="K27" t="n">
-        <v>1156.37</v>
+        <v>987.03</v>
       </c>
       <c r="L27" t="n">
         <v>52129.25</v>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1905,12 +1905,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Oklahoma State University, Common Schools, Other Agency</t>
+          <t>Common Schools, Oklahoma State University, Other Agency</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>surface, subsurface</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -2097,12 +2097,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>State Educational Institutions, Oklahoma State University, Common Schools, Public Building</t>
+          <t>Oklahoma State University, Common Schools, State Educational Institutions, Public Building</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>subsurface, surface</t>
+          <t>surface, subsurface</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, Public Building, Oklahoma State University</t>
+          <t>Common Schools, Public Building, State Educational Institutions, Oklahoma State University</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Common Schools, Greer 33, Oklahoma State University, State Educational Institutions, University Preparatory, Public Building, Normal Schools</t>
+          <t>Common Schools, Greer 33, Oklahoma State University, State Educational Institutions, University Preparatory, Normal Schools, Public Building</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>State Educational Institutions, Common Schools, Public Building, Oklahoma State University</t>
+          <t>Common Schools, State Educational Institutions, Public Building, Oklahoma State University</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), Dept. of Fish and Game, 100.00% Agricultural College, 100.00% Charitable Institute, 100.00% Normal School, 100.00% Forest Purposes (Dept. of Forestry), 100.00% University of Idaho, 100.00% Dept. of Fish and Game, 100.00% Dept. of Health and Welfare, Dept. of Health and Welfare, 100.00% General Fund, 100.00% Dept. of Transportation</t>
+          <t>Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), Dept. of Fish and Game, 100.00% Agricultural College, 100.00% Dept. of Transportation, 100.00% Charitable Institute, 100.00% Normal School, 100.00% Forest Purposes (Dept. of Forestry), 100.00% University of Idaho, 100.00% Dept. of Fish and Game, 100.00% Dept. of Health and Welfare, Dept. of Health and Welfare, 100.00% General Fund</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, STATE HOSPITAL, VALLEY/MAYVILLE, SCHOOL FOR THE DEAF, ND STATE UNIVERSITY, ND SCHOOL OF SCIENCE, VALLEY CITY, VETERANS HOME, ELLENDALE, MAYVILLE, ND INDUSTRIAL SCHOOL</t>
+          <t>COMMON SCHOOLS, BANK OFÔøΩNORTHÔøΩDAKOTA, STATE HOSPITAL, VALLEY/MAYVILLE, SCHOOL FOR THE DEAF, ND STATE UNIVERSITY, ND SCHOOL OF SCIENCE, VALLEY CITY, VETERANS HOME, ELLENDALE, MAYVILLE, ND INDUSTRIAL SCHOOL</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3570,12 +3570,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1664100.0121284036 2965338.7654427923 0, -1663999.4695497244 2965379.7210711455 0, -1664020.5066267399 2965362.712489979 0, -1664113.950854609 2965324.4462060267 0, -1664114.2313182952 2965324.367111401 0, -1664111.1788303582 2965337.0181473573 0, -1664100.0121284036 2965338.7654427923 0)), ((-1663759.0497988292 2965522.6614214736 0, -1663622.6939214163 2965600.2512186817 0, -1663556.8513078566 2965632.399373433 0, -1663422.5190301985 2965672.6931485054 0, -1663333.18452634 2965691.5473255995 0, -1663254.4814397362 2965705.207975173 0, -1663180.884130269 2965726.798973366 0, -1663098.5475386158 2965746.8080340233 0, -1663025.1290540951 2965778.7546608355 0, -1662910.0294940504 2965820.8421138846 0, -1662861.863442064 2965838.7155494974 0, -1662726.9999577163 2965903.080960916 0, -1662665.0101153927 2965935.511776588 0, -1662575.2567217865 2966011.5176111967 0, -1662512.4478622496 2966052.1918395762 0, -1662408.1118847448 2966135.649747651 0, -1662363.65538063 2966200.7205385747 0, -1662304.0634256515 2966310.2496420993 0, -1662271.6141911214 2966362.8314835713 0, -1662241.0140750348 2966400.381565996 0, -1662199.6818378742 2966427.783666996 0, -1662176.794089121 2966435.7822622946 0, -1662181.8431938915 2966418.5055073504 0, -1662198.101661121 2966396.4603498555 0, -1662243.9333120761 2966357.3526089326 0, -1662268.1700962489 2966313.6442167456 0, -1662285.0021017974 2966277.407075364 0, -1662305.1251161357 2966236.0901758783 0, -1662325.7425396738 2966197.253899609 0, -1662352.9994726032 2966155.324634322 0, -1662363.3754003395 2966123.008460601 0, -1662366.880078718 2966115.1412538616 0, -1662385.3321085796 2966073.7339914837 0, -1662487.7458373671 2966030.730320794 0, -1662607.3782301024 2965908.913562891 0, -1662683.7728323797 2965860.1873174678 0, -1662738.5967986537 2965847.0115358024 0, -1662848.444701723 2965820.6111051645 0, -1662920.3638127327 2965803.32496469 0, -1663118.9152078175 2965703.4399412116 0, -1663194.674353364 2965678.2584710866 0, -1663214.8318499771 2965671.5586890937 0, -1663244.9382030612 2965675.9393328237 0, -1663327.769285614 2965638.6939216475 0, -1663361.490036229 2965616.738735536 0, -1663448.779052874 2965591.0213082884 0, -1663559.3454429738 2965576.8887826274 0, -1663640.0752267477 2965559.5611954783 0, -1663668.2253901486 2965553.518084891 0, -1663733.629209381 2965526.790211123 0, -1663880.5534334064 2965438.480753 0, -1663934.7914855885 2965418.4107965785 0, -1663834.3151137598 2965475.6799948583 0, -1663759.0497988292 2965522.6614214736 0)))</t>
+          <t>MULTIPOLYGON Z (((-2022377.3147742988 2974403.09740933 0, -2022398.8853382058 2974428.3643118157 0, -2022403.2566114787 2974434.113991658 0, -2022459.8146360912 2974476.925170232 0, -2022528.1243986466 2974538.587445689 0, -2022570.7616208917 2974577.4052995346 0, -2022598.740046934 2974636.7288739765 0, -2022624.3954757904 2974668.8455517483 0, -2022642.159423197 2974686.1625958094 0, -2022661.7986063345 2974738.7877075644 0, -2022646.0615444065 2974734.072831868 0, -2022640.2361746407 2974732.3785090167 0, -2022541.0146529807 2974703.5213074395 0, -2022428.9010101797 2975087.7450038083 0, -2022317.5797495937 2975472.193700926 0, -2022705.9353318429 2975585.1392405904 0, -2022594.1421026664 2975969.4455484175 0, -2022538.2459337483 2976161.597220415 0, -2022531.5587934584 2976184.5858256565 0, -2022515.0642586637 2976196.192578154 0, -2022494.024224548 2976218.11697097 0, -2022471.2894866932 2976228.9769758857 0, -2022452.535970978 2976230.530991689 0, -2022444.57218863 2976231.190923296 0, -2022420.097691774 2976224.864681152 0, -2022391.3684990415 2976205.265211491 0, -2022359.0125877908 2976187.7786637316 0, -2022325.9149412876 2976173.1570239933 0, -2022305.424052827 2976157.209021562 0, -2022280.6040477366 2976146.233406032 0, -2022246.7305527579 2976146.600556096 0, -2022214.0280282483 2976138.889554426 0, -2022193.9179536647 2976127.6026913607 0, -2022167.0112498596 2976110.319150268 0, -2022166.686739932 2976109.959489474 0, -2022166.4433775912 2976109.8031345992 0, -2022161.6676595134 2976104.5096097034 0, -2022155.7066692528 2976097.9023979534 0, -2022152.5768778417 2976074.2861615894 0, -2022164.6056061774 2976043.0773203904 0, -2022166.4338388983 2976038.3341261544 0, -2022167.6291961642 2976030.9983204966 0, -2022171.6619896332 2976006.248112531 0, -2022189.103129973 2975963.6050586356 0, -2022193.317922785 2975941.746461309 0, -2022208.3439023497 2975890.1987590105 0, -2022214.4687218065 2975875.337175248 0, -2022217.8560001296 2975869.444019137 0, -2022220.067841656 2975865.5960215465 0, -2022225.2653056274 2975849.895054099 0, -2022227.2568959042 2975843.878384733 0, -2022227.8361377416 2975837.996537856 0, -2022228.090900232 2975835.4120237255 0, -2022230.1367185293 2975814.637024629 0, -2022230.437405515 2975811.583277581 0, -2022229.9383628687 2975808.0463157147 0, -2022228.186881719 2975795.6327760825 0, -2022226.630557727 2975784.6027089804 0, -2022222.8338533377 2975763.745781664 0, -2022221.7820393937 2975739.5901133073 0, -2022227.4433826033 2975714.277198129 0, -2022227.5382744677 2975712.8938861294 0, -2022228.2773114224 2975702.1134002283 0, -2022227.6682758727 2975683.7204428744 0, -2022227.5479842864 2975680.0837781127 0, -2022228.6670184748 2975660.722242781 0, -2022233.1636378197 2975645.436414047 0, -2022237.6084610915 2975639.5469321087 0, -2022241.3629065172 2975628.4190741535 0, -2022243.9756546128 2975620.6752276276 0, -2022245.344470203 2975607.106201788 0, -2022245.399538016 2975606.560500872 0, -2022251.337208646 2975583.785139515 0, -2022258.6506103938 2975555.7331480444 0, -2022259.7238880852 2975551.616281831 0, -2022260.1674704424 2975546.3667625226 0, -2022264.3897412878 2975496.4010210745 0, -2022264.8522323107 2975490.9287130837 0, -2022265.1378469565 2975480.3996026134 0, -2022265.2148387656 2975477.5584638873 0, -2022262.753693705 2975464.3869928424 0, -2022261.975174468 2975462.1571892085 0, -2022253.6741255133 2975438.382067632 0, -2022245.9969177635 2975423.714032733 0, -2022238.3045395731 2975409.0175283873 0, -2022233.7512453739 2975378.9483812936 0, -2022230.7742919622 2975337.6860042163 0, -2022230.7339592134 2975337.1255710986 0, -2022239.9725075113 2975311.041403465 0, -2022242.0776089723 2975305.0979491738 0, -2022247.2266253636 2975285.1312901364 0, -2022262.482573441 2975261.695086388 0, -2022271.3485722868 2975246.676911818 0, -2022273.3759029962 2975243.2426589644 0, -2022281.4407137067 2975232.309251684 0, -2022282.7995369395 2975230.467216447 0, -2022278.5489376185 2975221.4059525016 0, -2022325.9241348677 2975057.8080587997 0, -2022371.554730276 2975071.064272103 0, -2022430.831812876 2974867.2505894126 0, -2022037.0081873392 2974752.708780197 0, -2022042.791874227 2974735.8343377486 0, -2022053.8162527552 2974693.084078516 0, -2022060.4328703424 2974667.4229548476 0, -2022064.6362993266 2974658.7396673835 0, -2022070.2426108338 2974647.1575384904 0, -2022081.9050843397 2974625.8430966735 0, -2022087.7901909503 2974603.029487494 0, -2022091.5508123355 2974572.831553848 0, -2022091.6294089232 2974572.200420241 0, -2022093.7220584734 2974572.8193727504 0, -2022100.5278705973 2974552.2900851807 0, -2022105.5068056947 2974541.302023373 0, -2022114.3952781004 2974525.2384762783 0, -2022121.856591765 2974509.793789283 0, -2022126.8353471216 2974498.805890221 0, -2022130.2226599506 2974486.315647561 0, -2022133.3023462563 2974470.62774974 0, -2022139.3257515836 2974457.8726789197 0, -2022143.1962262644 2974452.785597163 0, -2022148.360766342 2974445.997775775 0, -2022157.163297123 2974437.1629031044 0, -2022169.653544209 2974424.2255676063 0, -2022179.5577045016 2974413.6417207117 0, -2022189.2008531357 2974401.9420306357 0, -2022199.2946997448 2974386.2290255954 0, -2022210.533066156 2974370.8522670064 0, -2022220.1118202151 2974359.1346524945 0, -2022234.1795455955 2974349.7669994617 0, -2022246.2619765159 2974342.931570014 0, -2022262.404031268 2974335.2055705567 0, -2022264.254410031 2974334.4637524188 0, -2022280.352400289 2974328.009098668 0, -2022284.2343091653 2974326.6570565957 0, -2022324.0201035729 2974360.368498534 0, -2022357.5879329306 2974397.998105058 0, -2022377.3147742988 2974403.09740933 0)), ((-2022369.149022734 2976737.60381355 0, -2022263.7087498931 2976706.9315518616 0, -2022247.6045130366 2976702.2469972926 0, -2022249.7940970312 2976700.560832485 0, -2022252.7740648177 2976698.2659858125 0, -2022286.416643166 2976675.0216021314 0, -2022301.562355381 2976654.548447446 0, -2022305.293008606 2976649.505526521 0, -2022310.9079657658 2976627.733221197 0, -2022315.2160602957 2976611.027839996 0, -2022326.3287764883 2976587.399117541 0, -2022335.6131570742 2976567.657928095 0, -2022342.975184214 2976559.2630892694 0, -2022346.5758996473 2976555.1571995807 0, -2022351.1641714869 2976549.925030061 0, -2022352.3083724244 2976548.620300016 0, -2022370.4013405244 2976527.9886640767 0, -2022370.8386288013 2976527.403275572 0, -2022392.2533842996 2976498.7409727275 0, -2022397.4547903787 2976491.7792722015 0, -2022401.3054839866 2976486.625438264 0, -2022405.6145610532 2976480.8579138587 0, -2022440.7549954513 2976467.2962173354 0, -2022459.799366124 2976462.1949356897 0, -2022463.310511482 2976461.342982718 0, -2022474.7188851128 2976458.1986767687 0, -2022475.4288295375 2976458.008532934 0, -2022479.4487442523 2976452.1791328955 0, -2022485.7654679408 2976443.0190728176 0, -2022495.0057567575 2976429.619610154 0, -2022496.4392585915 2976425.623062329 0, -2022504.2584839084 2976403.822260621 0, -2022504.435027158 2976403.330215141 0, -2022505.9848254402 2976399.0091806995 0, -2022508.5926218212 2976394.260632969 0, -2022523.749126702 2976366.6621477343 0, -2022524.3110475475 2976365.9290150274 0, -2022529.5183142074 2976367.443862561 0, -2022870.6836549435 2976466.7101995545 0, -2023263.2470127956 2976568.165741934 0, -2023356.4425675017 2976592.2577558677 0, -2023372.9688632768 2976596.529998495 0, -2023372.3954123778 2976598.597537148 0, -2023363.1576214223 2976614.941286052 0, -2023357.573726966 2976624.794501183 0, -2023343.5954985786 2976671.1902810396 0, -2023324.7134716942 2976701.3298218176 0, -2023312.4656152795 2976733.180826312 0, -2023305.4572751564 2976752.3900292832 0, -2023286.222252146 2976760.415529661 0, -2023247.4258264834 2976785.4047973403 0, -2023229.7099518962 2976818.8395379675 0, -2023219.1954653051 2976836.146255966 0, -2023229.1351348339 2976840.71049126 0, -2023241.9280489571 2976846.0149826715 0, -2023248.0413762352 2976853.6017565695 0, -2023256.5278934555 2976863.8034100262 0, -2023266.4578151198 2976876.3724273187 0, -2023266.6365611234 2976876.3195280507 0, -2023266.667075015 2976876.3581414563 0, -2023272.1113865923 2976874.750521349 0, -2023293.8056726614 2976868.441242324 0, -2023309.8369974284 2976876.5820968836 0, -2023316.9538924983 2976884.412570936 0, -2023324.5135187488 2976890.378188539 0, -2023332.5241425608 2976898.436512635 0, -2023331.9995071676 2976908.3037900864 0, -2023329.0946590507 2976919.573060433 0, -2023325.713151636 2976932.6915180916 0, -2023316.605556433 2976952.3601960205 0, -2023309.9235862116 2976962.630998978 0, -2023310.0777780223 2976977.6845188015 0, -2023310.232808064 2976992.7348027565 0, -2023303.0687048913 2977000.8863632223 0, -2023298.3382268779 2977006.51541246 0, -2023145.288401216 2976961.9757303987 0, -2022757.516656012 2976850.6045143665 0, -2022369.149022734 2976737.60381355 0)), ((-2022513.739813749 2979691.1133844736 0, -2022528.7211059663 2979695.473706297 0, -2022749.1248821886 2979759.6292808857 0, -2023137.5415768432 2979872.7173805605 0, -2023021.749361174 2980269.5700469245 0, -2022676.095311942 2980168.9349389453 0, -2022654.2867567246 2980162.586886195 0, -2022649.4325133453 2980149.50293256 0, -2022648.5387991983 2980147.0944186067 0, -2022642.9541412455 2980136.2620778615 0, -2022642.9021023149 2980136.1610140232 0, -2022633.333263999 2980106.1280230624 0, -2022614.4250224868 2980046.7817877047 0, -2022608.655689065 2980028.674036983 0, -2022594.1663848185 2979964.255827659 0, -2022581.9446664576 2979892.279614118 0, -2022576.9015259366 2979869.1831293856 0, -2022573.090168448 2979851.7283475273 0, -2022572.0010732259 2979846.74019141 0, -2022571.0515447399 2979842.4969200124 0, -2022568.4721702943 2979831.1292888937 0, -2022566.534420757 2979818.374767177 0, -2022558.7339645885 2979791.22872087 0, -2022557.253506465 2979782.547714018 0, -2022544.124024207 2979744.473334384 0, -2022533.3803877374 2979725.9931035214 0, -2022529.3608210615 2979717.916180756 0, -2022527.4640542655 2979714.104949524 0, -2022513.739813749 2979691.1133844736 0)))</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Spokane</t>
+          <t>Squaxin Island</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3585,295 +3585,295 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Common School and Indemnity</t>
+          <t>Administrative Site</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Subsurface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>277.57</v>
       </c>
       <c r="H66" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I66" t="n">
-        <v>18.84</v>
+        <v>52.27</v>
       </c>
       <c r="J66" t="n">
         <v>1</v>
       </c>
       <c r="K66" t="n">
-        <v>18.84</v>
+        <v>329.84</v>
       </c>
       <c r="L66" t="n">
-        <v>158625.43</v>
+        <v>1737.94</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-2022377.3147742988 2974403.09740933 0, -2022398.8853382058 2974428.3643118157 0, -2022403.2566114787 2974434.113991658 0, -2022459.8146360912 2974476.925170232 0, -2022528.1243986466 2974538.587445689 0, -2022570.7616208917 2974577.4052995346 0, -2022598.740046934 2974636.7288739765 0, -2022624.3954757904 2974668.8455517483 0, -2022642.159423197 2974686.1625958094 0, -2022661.7986063345 2974738.7877075644 0, -2022646.0615444065 2974734.072831868 0, -2022640.2361746407 2974732.3785090167 0, -2022541.0146529807 2974703.5213074395 0, -2022428.9010101797 2975087.7450038083 0, -2022317.5797495937 2975472.193700926 0, -2022705.9353318429 2975585.1392405904 0, -2022594.1421026664 2975969.4455484175 0, -2022538.2459337483 2976161.597220415 0, -2022531.5587934584 2976184.5858256565 0, -2022515.0642586637 2976196.192578154 0, -2022494.024224548 2976218.11697097 0, -2022471.2894866932 2976228.9769758857 0, -2022452.535970978 2976230.530991689 0, -2022444.57218863 2976231.190923296 0, -2022420.097691774 2976224.864681152 0, -2022391.3684990415 2976205.265211491 0, -2022359.0125877908 2976187.7786637316 0, -2022325.9149412876 2976173.1570239933 0, -2022305.424052827 2976157.209021562 0, -2022280.6040477366 2976146.233406032 0, -2022246.7305527579 2976146.600556096 0, -2022214.0280282483 2976138.889554426 0, -2022193.9179536647 2976127.6026913607 0, -2022167.0112498596 2976110.319150268 0, -2022166.686739932 2976109.959489474 0, -2022166.4433775912 2976109.8031345992 0, -2022161.6676595134 2976104.5096097034 0, -2022155.7066692528 2976097.9023979534 0, -2022152.5768778417 2976074.2861615894 0, -2022164.6056061774 2976043.0773203904 0, -2022166.4338388983 2976038.3341261544 0, -2022167.6291961642 2976030.9983204966 0, -2022171.6619896332 2976006.248112531 0, -2022189.103129973 2975963.6050586356 0, -2022193.317922785 2975941.746461309 0, -2022208.3439023497 2975890.1987590105 0, -2022214.4687218065 2975875.337175248 0, -2022217.8560001296 2975869.444019137 0, -2022220.067841656 2975865.5960215465 0, -2022225.2653056274 2975849.895054099 0, -2022227.2568959042 2975843.878384733 0, -2022227.8361377416 2975837.996537856 0, -2022228.090900232 2975835.4120237255 0, -2022230.1367185293 2975814.637024629 0, -2022230.437405515 2975811.583277581 0, -2022229.9383628687 2975808.0463157147 0, -2022228.186881719 2975795.6327760825 0, -2022226.630557727 2975784.6027089804 0, -2022222.8338533377 2975763.745781664 0, -2022221.7820393937 2975739.5901133073 0, -2022227.4433826033 2975714.277198129 0, -2022227.5382744677 2975712.8938861294 0, -2022228.2773114224 2975702.1134002283 0, -2022227.6682758727 2975683.7204428744 0, -2022227.5479842864 2975680.0837781127 0, -2022228.6670184748 2975660.722242781 0, -2022233.1636378197 2975645.436414047 0, -2022237.6084610915 2975639.5469321087 0, -2022241.3629065172 2975628.4190741535 0, -2022243.9756546128 2975620.6752276276 0, -2022245.344470203 2975607.106201788 0, -2022245.399538016 2975606.560500872 0, -2022251.337208646 2975583.785139515 0, -2022258.6506103938 2975555.7331480444 0, -2022259.7238880852 2975551.616281831 0, -2022260.1674704424 2975546.3667625226 0, -2022264.3897412878 2975496.4010210745 0, -2022264.8522323107 2975490.9287130837 0, -2022265.1378469565 2975480.3996026134 0, -2022265.2148387656 2975477.5584638873 0, -2022262.753693705 2975464.3869928424 0, -2022261.975174468 2975462.1571892085 0, -2022253.6741255133 2975438.382067632 0, -2022245.9969177635 2975423.714032733 0, -2022238.3045395731 2975409.0175283873 0, -2022233.7512453739 2975378.9483812936 0, -2022230.7742919622 2975337.6860042163 0, -2022230.7339592134 2975337.1255710986 0, -2022239.9725075113 2975311.041403465 0, -2022242.0776089723 2975305.0979491738 0, -2022247.2266253636 2975285.1312901364 0, -2022262.482573441 2975261.695086388 0, -2022271.3485722868 2975246.676911818 0, -2022273.3759029962 2975243.2426589644 0, -2022281.4407137067 2975232.309251684 0, -2022282.7995369395 2975230.467216447 0, -2022278.5489376185 2975221.4059525016 0, -2022325.9241348677 2975057.8080587997 0, -2022371.554730276 2975071.064272103 0, -2022430.831812876 2974867.2505894126 0, -2022037.0081873392 2974752.708780197 0, -2022042.791874227 2974735.8343377486 0, -2022053.8162527552 2974693.084078516 0, -2022060.4328703424 2974667.4229548476 0, -2022064.6362993266 2974658.7396673835 0, -2022070.2426108338 2974647.1575384904 0, -2022081.9050843397 2974625.8430966735 0, -2022087.7901909503 2974603.029487494 0, -2022091.5508123355 2974572.831553848 0, -2022091.6294089232 2974572.200420241 0, -2022093.7220584734 2974572.8193727504 0, -2022100.5278705973 2974552.2900851807 0, -2022105.5068056947 2974541.302023373 0, -2022114.3952781004 2974525.2384762783 0, -2022121.856591765 2974509.793789283 0, -2022126.8353471216 2974498.805890221 0, -2022130.2226599506 2974486.315647561 0, -2022133.3023462563 2974470.62774974 0, -2022139.3257515836 2974457.8726789197 0, -2022143.1962262644 2974452.785597163 0, -2022148.360766342 2974445.997775775 0, -2022157.163297123 2974437.1629031044 0, -2022169.653544209 2974424.2255676063 0, -2022179.5577045016 2974413.6417207117 0, -2022189.2008531357 2974401.9420306357 0, -2022199.2946997448 2974386.2290255954 0, -2022210.533066156 2974370.8522670064 0, -2022220.1118202151 2974359.1346524945 0, -2022234.1795455955 2974349.7669994617 0, -2022246.2619765159 2974342.931570014 0, -2022262.404031268 2974335.2055705567 0, -2022264.254410031 2974334.4637524188 0, -2022280.352400289 2974328.009098668 0, -2022284.2343091653 2974326.6570565957 0, -2022324.0201035729 2974360.368498534 0, -2022357.5879329306 2974397.998105058 0, -2022377.3147742988 2974403.09740933 0)), ((-2022369.149022734 2976737.60381355 0, -2022263.7087498931 2976706.9315518616 0, -2022247.6045130366 2976702.2469972926 0, -2022249.7940970312 2976700.560832485 0, -2022252.7740648177 2976698.2659858125 0, -2022286.416643166 2976675.0216021314 0, -2022301.562355381 2976654.548447446 0, -2022305.293008606 2976649.505526521 0, -2022310.9079657658 2976627.733221197 0, -2022315.2160602957 2976611.027839996 0, -2022326.3287764883 2976587.399117541 0, -2022335.6131570742 2976567.657928095 0, -2022342.975184214 2976559.2630892694 0, -2022346.5758996473 2976555.1571995807 0, -2022351.1641714869 2976549.925030061 0, -2022352.3083724244 2976548.620300016 0, -2022370.4013405244 2976527.9886640767 0, -2022370.8386288013 2976527.403275572 0, -2022392.2533842996 2976498.7409727275 0, -2022397.4547903787 2976491.7792722015 0, -2022401.3054839866 2976486.625438264 0, -2022405.6145610532 2976480.8579138587 0, -2022440.7549954513 2976467.2962173354 0, -2022459.799366124 2976462.1949356897 0, -2022463.310511482 2976461.342982718 0, -2022474.7188851128 2976458.1986767687 0, -2022475.4288295375 2976458.008532934 0, -2022479.4487442523 2976452.1791328955 0, -2022485.7654679408 2976443.0190728176 0, -2022495.0057567575 2976429.619610154 0, -2022496.4392585915 2976425.623062329 0, -2022504.2584839084 2976403.822260621 0, -2022504.435027158 2976403.330215141 0, -2022505.9848254402 2976399.0091806995 0, -2022508.5926218212 2976394.260632969 0, -2022523.749126702 2976366.6621477343 0, -2022524.3110475475 2976365.9290150274 0, -2022529.5183142074 2976367.443862561 0, -2022870.6836549435 2976466.7101995545 0, -2023263.2470127956 2976568.165741934 0, -2023356.4425675017 2976592.2577558677 0, -2023372.9688632768 2976596.529998495 0, -2023372.3954123778 2976598.597537148 0, -2023363.1576214223 2976614.941286052 0, -2023357.573726966 2976624.794501183 0, -2023343.5954985786 2976671.1902810396 0, -2023324.7134716942 2976701.3298218176 0, -2023312.4656152795 2976733.180826312 0, -2023305.4572751564 2976752.3900292832 0, -2023286.222252146 2976760.415529661 0, -2023247.4258264834 2976785.4047973403 0, -2023229.7099518962 2976818.8395379675 0, -2023219.1954653051 2976836.146255966 0, -2023229.1351348339 2976840.71049126 0, -2023241.9280489571 2976846.0149826715 0, -2023248.0413762352 2976853.6017565695 0, -2023256.5278934555 2976863.8034100262 0, -2023266.4578151198 2976876.3724273187 0, -2023266.6365611234 2976876.3195280507 0, -2023266.667075015 2976876.3581414563 0, -2023272.1113865923 2976874.750521349 0, -2023293.8056726614 2976868.441242324 0, -2023309.8369974284 2976876.5820968836 0, -2023316.9538924983 2976884.412570936 0, -2023324.5135187488 2976890.378188539 0, -2023332.5241425608 2976898.436512635 0, -2023331.9995071676 2976908.3037900864 0, -2023329.0946590507 2976919.573060433 0, -2023325.713151636 2976932.6915180916 0, -2023316.605556433 2976952.3601960205 0, -2023309.9235862116 2976962.630998978 0, -2023310.0777780223 2976977.6845188015 0, -2023310.232808064 2976992.7348027565 0, -2023303.0687048913 2977000.8863632223 0, -2023298.3382268779 2977006.51541246 0, -2023145.288401216 2976961.9757303987 0, -2022757.516656012 2976850.6045143665 0, -2022369.149022734 2976737.60381355 0)), ((-2022513.739813749 2979691.1133844736 0, -2022528.7211059663 2979695.473706297 0, -2022749.1248821886 2979759.6292808857 0, -2023137.5415768432 2979872.7173805605 0, -2023021.749361174 2980269.5700469245 0, -2022676.095311942 2980168.9349389453 0, -2022654.2867567246 2980162.586886195 0, -2022649.4325133453 2980149.50293256 0, -2022648.5387991983 2980147.0944186067 0, -2022642.9541412455 2980136.2620778615 0, -2022642.9021023149 2980136.1610140232 0, -2022633.333263999 2980106.1280230624 0, -2022614.4250224868 2980046.7817877047 0, -2022608.655689065 2980028.674036983 0, -2022594.1663848185 2979964.255827659 0, -2022581.9446664576 2979892.279614118 0, -2022576.9015259366 2979869.1831293856 0, -2022573.090168448 2979851.7283475273 0, -2022572.0010732259 2979846.74019141 0, -2022571.0515447399 2979842.4969200124 0, -2022568.4721702943 2979831.1292888937 0, -2022566.534420757 2979818.374767177 0, -2022558.7339645885 2979791.22872087 0, -2022557.253506465 2979782.547714018 0, -2022544.124024207 2979744.473334384 0, -2022533.3803877374 2979725.9931035214 0, -2022529.3608210615 2979717.916180756 0, -2022527.4640542655 2979714.104949524 0, -2022513.739813749 2979691.1133844736 0)))</t>
+          <t>MULTIPOLYGON Z (((-449556.5059218632 2511728.520408616 0, -449176.91746688675 2511705.777670777 0, -449176.1984435866 2511705.733216676 0, -449556.5059218632 2511728.520408616 0)), ((-449982.1299062058 2511754.164890567 0, -449982.1297245475 2511754.167914157 0, -449699.5578025382 2511737.097241653 0, -449982.1299062058 2511754.164890567 0)), ((-449579.1105100217 2511729.8748406926 0, -449579.1429920948 2511729.876786715 0, -449692.63074373675 2511736.678877075 0, -449982.1297245472 2511754.1679141615 0, -449971.4739245098 2511931.527108429 0, -449568.3538073889 2511907.2960243486 0, -449165.2529589046 2511883.0840977235 0, -448762.17476517527 2511858.894686667 0, -448773.2079271766 2511681.583054768 0, -448773.2382601551 2511681.584876002 0, -448871.2507424927 2511687.473799343 0, -448888.1109399908 2511688.486912748 0, -448915.0532655619 2511690.1000152635 0, -449176.12641623017 2511705.7317984854 0, -449176.1676868195 2511705.7342695664 0, -449579.1105100217 2511729.8748406926 0)), ((-463366.30178307346 2512582.8016465153 0, -463334.87706382683 2512580.856246914 0, -463366.30178338743 2512582.8016431336 0, -463405.7509150512 2512585.2358416286 0, -463366.30178307346 2512582.8016465153 0)), ((-464064.27364119334 2512625.8867090484 0, -464170.7422980627 2512632.464345802 0, -464213.54977654974 2512635.13402016 0, -464170.7422882964 2512632.464375655 0, -464064.27364119334 2512625.8867090484 0)), ((-464417.0083980226 2512647.8287448124 0, -464406.96939841536 2512813.1866125953 0, -464005.15649598924 2512788.596259246 0, -463603.3422352082 2512764.027462437 0, -463201.52449667803 2512739.4803704 0, -463211.49494368176 2512573.224213664 0, -463211.5253091886 2512573.226092752 0, -463366.310057336 2512582.8084000037 0, -463613.2370556818 2512598.044970272 0, -463613.2761352741 2512598.047381669 0, -464015.0843742729 2512622.853928947 0, -464015.1124974243 2512622.855665194 0, -464170.7614092613 2512632.4718089625 0, -464417.0083980226 2512647.8287448124 0)), ((-456264.384418507 2513913.2817409043 0, -456311.65716874925 2513126.286220331 0, -456360.0020620866 2512321.4405879593 0, -456361.8088236175 2512291.361745473 0, -457984.09614303196 2512406.6756496173 0, -457932.25081506104 2513225.965336516 0, -457932.2506155181 2513225.9674284193 0, -457893.0983433012 2513844.675265713 0, -457892.23051078035 2513858.3893516134 0, -457891.59300734167 2513868.4635157497 0, -457890.3708778595 2513887.7760617123 0, -457882.31282094686 2514015.1139713754 0, -457881.30541144765 2514015.05057021 0, -456264.384418507 2513913.2817409043 0)), ((-451282.77213509835 2516843.573187387 0, -452881.1286204372 2516941.3567562765 0, -452788.16282210994 2518541.180243185 0, -451193.0181150282 2518454.0908873766 0, -451282.77213509835 2516843.573187387 0)), ((-447775.73130676866 2521466.171663356 0, -447680.4446375186 2523083.00645899 0, -446062.53746012686 2522978.478549137 0, -446149.0682687236 2521383.5954063167 0, -447775.73130676866 2521466.171663356 0)), ((-452263.06508488936 2527420.0165616595 0, -452262.9989986145 2527421.1705014743 0, -452217.3678488886 2528216.499118979 0, -451389.4571952081 2528170.4905104106 0, -451429.1165415427 2527389.9752738457 0, -451432.0658116872 2527378.173895968 0, -451432.0927535317 2527378.066065934 0, -450674.31094751746 2527334.2312229117 0, -450659.6225222654 2527333.820585373 0, -450659.6496749159 2527333.383858899 0, -450711.31631975883 2526504.3601864562 0, -451480.4558586479 2526550.4099000636 0, -451434.6292940259 2527362.1247527148 0, -451433.9890512456 2527378.2706318754 0, -452231.5475172021 2527418.4299013275 0, -452252.6274551624 2527419.4912691237 0, -452263.06508488936 2527420.0165616595 0)), ((-455166.42114959256 2531660.3247363223 0, -455167.23062476097 2531647.0039018453 0, -456801.4756868293 2531730.9629927757 0, -456691.7622620359 2533334.4222966707 0, -455069.8573224605 2533249.725257102 0, -455166.42114959256 2531660.3247363223 0)), ((-451735.24512163736 2536243.317183069 0, -451645.78562387795 2537864.519470849 0, -450021.007770592 2537765.742848979 0, -450116.09840936464 2536144.5834728894 0, -451735.24512163736 2536243.317183069 0)), ((-461322.1501446945 2536845.070964317 0, -461266.4029524177 2537687.653727615 0, -459665.6639103949 2537608.6670449553 0, -459715.99443711824 2536748.6248253267 0, -461322.1501446945 2536845.070964317 0)), ((-454890.8922974969 2542698.1855162326 0, -453281.3780819311 2542600.764220469 0, -453384.07991065923 2540985.658445156 0, -454594.304251081 2541056.715851151 0, -454988.15293683077 2541080.9520675344 0, -454890.8922974969 2542698.1855162326 0)), ((-459524.2299986185 2546204.2215727074 0, -459429.9975628155 2547813.2614215584 0, -457816.4177064228 2547702.894510099 0, -457894.3280349991 2546101.495725701 0, -459524.2299986185 2546204.2215727074 0)), ((-447333.0196933869 2547058.820925809 0, -447227.8717313179 2548665.936131774 0, -446452.08490666316 2548619.788373531 0, -445623.684550666 2548570.683982875 0, -445713.3941800438 2546965.148014899 0, -446547.97513063496 2547014.6210594294 0, -447333.0196933869 2547058.820925809 0)), ((-455693.08488767454 2555626.9297070154 0, -456468.00679758465 2555674.8984094583 0, -456416.7449249867 2556489.9031604244 0, -454802.76577117445 2556376.1514217234 0, -454885.3564354707 2554791.20763069 0, -455740.92444017367 2554843.778459255 0, -455693.08488767454 2555626.9297070154 0)), ((-449276.9794248514 2555236.611581465 0, -449203.3707008164 2556834.7579691587 0, -447593.3605284898 2556738.3556973888 0, -447672.70063963823 2555137.8819685206 0, -449276.9794248514 2555236.611581465 0)), ((-458875.0183390479 2556662.9690301814 0, -458828.2093868158 2557424.049423567 0, -457185.61157180124 2557335.725614214 0, -457303.25758220925 2555726.584222721 0, -458131.4758505402 2555781.6832451886 0, -458083.5253769855 2556616.3136012475 0, -458875.0183390479 2556662.9690301814 0)), ((-452186.6040555831 2560226.9235749864 0, -453804.62321116845 2560336.180691955 0, -453698.7256673469 2561920.4906114456 0, -452074.04850345897 2561828.9798595035 0, -452186.6040555831 2560226.9235749864 0)), ((-449321.9326013234 2564376.2574031744 0, -449321.3769063425 2564386.1416202285 0, -449276.9198393965 2565177.0558428974 0, -449231.9133044314 2565977.837736146 0, -449231.53414914093 2565984.0533565343 0, -449183.4894144431 2566771.4791362807 0, -449182.9648853079 2566780.0764241694 0, -448373.3310903083 2566731.304009236 0, -447563.6950838357 2566682.5144151314 0, -447514.66624011385 2567489.021035307 0, -446705.1953842786 2567440.7313964185 0, -445988.7150911759 2567397.976206695 0, -445909.0247302735 2567388.175121057 0, -445895.8781619955 2567386.558528588 0, -445895.92348154745 2567385.746683493 0, -445895.1590514922 2567385.67234871 0, -445940.1287341057 2566574.7250591344 0, -445941.19318906 2566574.7945829183 0, -445986.07918338495 2565770.789100794 0, -445986.3991030491 2565765.046846068 0, -446034.2458411558 2564974.470302698 0, -446081.848022635 2564187.9879047014 0, -446082.0960329981 2564183.877433263 0, -446175.0936994005 2564189.500664745 0, -446181.23518354836 2564189.8143169554 0, -446892.4000848265 2564226.1902014404 0, -447120.5724311692 2564237.8580566742 0, -447702.7252258939 2564267.693862222 0, -448512.33092102065 2564321.9463786385 0, -448743.30342503305 2564337.4211003976 0, -449321.9326013234 2564376.2574031744 0), (-448467.324070914 2565124.4624965163 0, -447657.7244795784 2565071.8508929783 0, -447612.77113378036 2565875.227558959 0, -448421.53377836954 2565926.115988229 0, -448422.3650867946 2565926.1683864985 0, -448467.324070914 2565124.4624965163 0)), ((-450872.6268687303 2565283.478366009 0, -451680.51605147077 2565331.9210636 0, -451633.04154613346 2566137.5807718737 0, -450834.4153565486 2566092.4419257008 0, -450827.00930416514 2566092.0250950083 0, -450029.46244642325 2566034.939160159 0, -450074.7745231379 2565230.2747832444 0, -450872.6268687303 2565283.478366009 0)), ((-465522.480087164 2566211.0676372 0, -465497.99191343173 2566611.630241336 0, -465480.8451485192 2566892.1531603415 0, -465473.2948586149 2567012.1479260344 0, -465472.71796541277 2567021.4207174475 0, -465472.031586073 2567021.3812373984 0, -465455.0418494883 2567019.6596213793 0, -465448.99211219745 2567018.280112106 0, -465327.7137608106 2567003.131225467 0, -465322.185706256 2567002.8163942015 0, -465347.6779609036 2566601.412719703 0, -465373.0994776094 2566201.1579084056 0, -465398.521134454 2565800.89875415 0, -465423.9451466621 2565400.6366323116 0, -465547.5166171904 2565407.1564568747 0, -465555.2558658541 2565407.657327017 0, -465571.7365829466 2565408.7253705617 0, -465571.6657606916 2565409.8448486715 0, -465547.05419117556 2565810.4818696138 0, -465529.667752618 2566093.4945963905 0, -465522.4895103514 2566210.9134963593 0, -465522.480087164 2566211.0676372 0)), ((-454811.31346071255 2567141.109477066 0, -454855.6294871319 2566337.2350389366 0, -455258.11700768187 2566364.1809276436 0, -455653.93637284345 2566390.676939578 0, -455629.05221015995 2566792.4430512516 0, -455604.16928405856 2567194.205680881 0, -455213.8082963064 2567168.0663915016 0, -454811.31346071255 2567141.109477066 0)), ((-445778.7935746923 2569395.246043825 0, -445773.73187626095 2569498.2577245524 0, -445759.094738161 2569796.1996818786 0, -445369.4413924876 2569772.410528177 0, -445389.7841105851 2569371.470383204 0, -445410.09594294924 2568971.0564951664 0, -445434.51985076955 2568565.8250266635 0, -445458.6746454063 2568165.0839533997 0, -445056.3294193455 2568141.3206398026 0, -444251.63915332005 2568093.7813247424 0, -444299.9785089062 2567292.2843639296 0, -444310.1872706344 2567292.8866332476 0, -445104.64999606746 2567339.8260526597 0, -445506.98577934084 2567363.5917561376 0, -445895.8781619955 2567386.558528588 0, -445895.60333543544 2567391.0871763406 0, -445871.601985927 2567787.2991851103 0, -445847.3282120576 2568188.0355825336 0, -445823.0542726236 2568588.767889601 0, -445798.49213708605 2568994.28689127 0, -445778.7935746923 2569395.246043825 0)), ((-452174.19734232465 2570747.6675056093 0, -452158.0453145773 2571009.3110569436 0, -452157.64718833106 2571015.7608968886 0, -452151.9472461596 2571015.3874891964 0, -451348.75422009744 2570962.814505742 0, -450539.8587676992 2570909.8519592355 0, -450539.9091747104 2570909.024648134 0, -450539.06196779094 2570908.9691903675 0, -450555.61941961234 2570638.495888727 0, -450588.6149749233 2570099.6443992187 0, -450638.17361392797 2569290.297443804 0, -451439.8572009743 2569341.5330177248 0, -452240.91873932607 2569393.2423031386 0, -452240.88616896205 2569393.897006181 0, -452241.76140384376 2569393.953099999 0, -452241.56006396015 2569397.991822121 0, -452205.9345710624 2570111.7782752165 0, -452201.2866546269 2570204.9095945144 0, -452174.19734232465 2570747.6675056093 0)), ((-446568.4550681967 2573951.0915424577 0, -446563.80971174856 2573952.8998985905 0, -446551.8514681421 2573957.555033972 0, -446562.6124286463 2574012.59082663 0, -446565.37551279727 2574026.7223278442 0, -446568.97758666135 2574056.646631005 0, -446625.42937589827 2574067.665254358 0, -446638.2313802044 2574070.1640319084 0, -446697.67873640795 2574081.922251191 0, -446707.6876513473 2574086.7241391297 0, -446714.6893999777 2574091.4392362507 0, -446716.8276809053 2574092.4650806137 0, -446750.1683095114 2574108.4603109276 0, -446784.95938356454 2574131.8839738998 0, -446799.36959451943 2574158.3019924304 0, -446819.34315285203 2574195.813044364 0, -446833.7530955948 2574222.231089865 0, -446853.72635455267 2574259.7421824727 0, -446874.3846494828 2574297.616373964 0, -446900.8587341657 2574347.339388282 0, -446928.68623211666 2574398.3597569247 0, -446916.27634527377 2574427.995409388 0, -446907.2980127922 2574445.9841933427 0, -446885.66267165233 2574454.170303028 0, -446834.9857463377 2574446.780569181 0, -446745.2809730728 2574432.206206241 0, -446694.603883932 2574424.817553702 0, -446676.48620318633 2574422.176331941 0, -446627.87300325214 2574414.278510132 0, -446550.6406528148 2574391.6491387743 0, -446512.7847795553 2574378.09854516 0, -446492.80560379615 2574375.8343219236 0, -446478.4234633957 2574385.0732659595 0, -446431.1496324344 2574422.694776051 0, -446424.6298018589 2574452.140482353 0, -446398.94756617106 2574502.136867927 0, -446340.09982323315 2574560.1016085385 0, -446285.99670345377 2574613.831450595 0, -446278.6087352978 2574624.503452922 0, -446269.89767463866 2574633.0836661397 0, -446270.9608647694 2574615.557296495 0, -446225.9212432688 2574655.5221559913 0, -446214.9682569618 2574654.8433415717 0, -446178.5546935751 2574652.586824033 0, -446178.5546134259 2574652.5869199685 0, -446214.9682506757 2574654.8434831738 0, -446129.2512760676 2574796.1515730764 0, -445989.49300173635 2574948.5913481 0, -445996.2009790698 2575103.6458547325 0, -445956.77361182624 2575108.6720762732 0, -445946.49791766756 2575087.257677356 0, -445921.36968522216 2575044.6333539444 0, -445918.79881303036 2575039.2751104087 0, -445918.79881303024 2575039.2751104087 0, -445905.6137503262 2575011.7946400736 0, -445900.1632744067 2575002.5494192936 0, -445902.4074946497 2574952.3947126777 0, -445899.913273229 2574882.311590769 0, -445893.9836602633 2574842.597457956 0, -445921.7162698178 2574762.8310657055 0, -445951.94644323573 2574667.3735025837 0, -445955.66247839987 2574646.365390554 0, -445954.72250468645 2574644.1635208954 0, -445955.03065915284 2574642.424815998 0, -445953.41247410345 2574638.634799117 0, -445953.4124741035 2574638.634799117 0, -445953.2656972692 2574638.291027136 0, -445953.02043969627 2574637.7165994206 0, -445936.2766363764 2574598.500258093 0, -445928.21034849255 2574575.791354023 0, -445908.6259245545 2574580.4970363365 0, -445891.66946380393 2574593.49464247 0, -445890.2791959668 2574594.560322038 0, -445888.3325162854 2574592.4428514666 0, -445885.50121547433 2574589.363148009 0, -445877.02642133815 2574586.2225874905 0, -445869.65367432754 2574578.2032980197 0, -445868.20082048024 2574576.6230382407 0, -445832.2017305108 2574558.7271710527 0, -445811.4678179631 2574551.0448905793 0, -445774.65136369405 2574537.403744603 0, -445745.5449259613 2574545.3380191578 0, -445743.1645129254 2574546.6865430293 0, -445728.65320356743 2574554.9073210126 0, -445714.51598370774 2574556.52835275 0, -445701.8415694503 2574561.9725715136 0, -445672.98795473785 2574577.9486203967 0, -445652.36112494336 2574615.369621159 0, -445652.260662085 2574615.731640977 0, -445652.0424214849 2574619.333129469 0, -445649.4273990284 2574642.926399384 0, -445647.22935103806 2574698.7794549344 0, -445639.20174341806 2574743.2514613876 0, -445633.4301780968 2574770.0468409318 0, -445626.06384222314 2574774.265435439 0, -445592.0640389263 2574856.1849386683 0, -445569.7662060519 2574911.243892445 0, -445526.85662866797 2574973.9616541793 0, -445505.57474210643 2574986.4271483268 0, -445481.991395397 2574956.311744628 0, -445476.69957869616 2574906.4662741185 0, -445487.9087582305 2574737.260160259 0, -445498.52683381917 2574616.327599229 0, -445498.53442332573 2574616.221544097 0, -445501.02662029344 2574587.838077341 0, -445510.24065185885 2574387.289699773 0, -445516.91910214105 2574278.4432967617 0, -445520.0287879152 2574227.7611629264 0, -445517.53163593437 2574219.3884955756 0, -445516.21309944324 2574214.9675922766 0, -445516.5630488973 2574207.345973943 0, -445516.6752975337 2574204.901288703 0, -445517.0419461239 2574196.915976583 0, -445500.2378451389 2574140.565765194 0, -445494.8548661272 2574122.6799496817 0, -445501.4186812127 2574014.291503234 0, -445516.84541118756 2574004.198597328 0, -445520.0187222175 2574001.5507348306 0, -445560.83336123556 2574017.4222854553 0, -445611.71132416325 2574025.983912797 0, -445663.6098651552 2574046.166564549 0, -445717.5229416513 2574074.1731103915 0, -445740.52318680566 2574090.552032075 0, -445788.76768398494 2574105.7643663273 0, -445828.7094112431 2574111.4429495097 0, -445875.0752445116 2574100.4918937637 0, -445907.2044888619 2574087.663616673 0, -445915.7437630923 2574085.646486602 0, -445919.85222520004 2574084.6759940004 0, -445939.10924534505 2574076.9884381196 0, -445974.8398783625 2574041.5776248965 0, -445999.37579975557 2574002.5589720556 0, -446024.2769612919 2573936.963886998 0, -446042.07678360125 2573881.76528192 0, -446077.3297600856 2573883.9010345708 0, -446093.9672806464 2573885.830022005 0, -446114.94519567984 2573904.7156140115 0, -446159.9014939694 2573915.924581668 0, -446184.9065645396 2573904.292101264 0, -446199.68989141687 2573884.237382285 0, -446200.28617193596 2573883.880797301 0, -446229.0963397115 2573855.7850391716 0, -446227.3448786952 2573844.1857780414 0, -446318.58519534994 2573850.050926444 0, -446698.1780046639 2573874.784120618 0, -446710.4334241953 2573875.528157732 0, -446694.3859729308 2573884.075065285 0, -446681.81349965365 2573910.118912809 0, -446678.2952695306 2573924.7751732552 0, -446628.48430492333 2573944.1648235247 0, -446568.4550681967 2573951.0915424577 0), (-446624.1749220042 2574068.462996698 0, -446624.17492200434 2574068.462996698 0, -446625.42937589827 2574067.665254358 0, -446624.1749220042 2574068.462996698 0)), ((-446950.56243684096 2574198.6320379856 0, -446932.30556629575 2574201.385897007 0, -446908.93935471226 2574176.457900518 0, -446883.80138547975 2574111.1742358143 0, -446863.6045996117 2574054.5049641044 0, -446875.42459873157 2574008.8867512974 0, -446882.9000154899 2573959.3910239553 0, -446876.09148893814 2573931.137323962 0, -446865.8438236706 2573894.418725824 0, -446864.12461474177 2573885.3509173403 0, -447124.44490654866 2573901.9489376843 0, -447108.22404811066 2574142.9668562766 0, -447101.39372117515 2574133.4359606504 0, -447087.50028866966 2574121.831196952 0, -447052.32130097033 2574102.4577116594 0, -447050.1481298079 2574105.75212045 0, -447024.6023644447 2574144.478105517 0, -446997.2296424889 2574184.283265825 0, -446962.1561278046 2574196.8832502966 0, -446950.56243684096 2574198.6320379856 0)), ((-456765.9186664952 2574520.703219268 0, -456766.7534668326 2574520.7562253936 0, -456775.8150063362 2574523.8307035593 0, -456936.0986376184 2574533.4261585367 0, -457573.4196303584 2574571.6560989986 0, -457521.005743965 2575367.450410148 0, -456717.4002130627 2575315.5125296665 0, -456668.05145486625 2576110.2522586337 0, -455863.1617071876 2576062.149205341 0, -455177.45231584826 2576021.155547476 0, -455166.6825075448 2576020.512744768 0, -455069.6986429143 2576016.5006078887 0, -455058.21920649987 2576016.0251637846 0, -455058.282165094 2576015.0817748327 0, -455057.69480324606 2576015.0569460415 0, -455110.6791901181 2575216.2349368795 0, -455164.28176372364 2574417.0104392366 0, -455264.5815672489 2574424.4891094393 0, -455964.7872605663 2574469.126197598 0, -456765.98251743335 2574519.674981475 0, -456765.9186664952 2574520.703219268 0)), ((-463196.45121227956 2574941.5765004004 0, -463993.9246552496 2574981.302344243 0, -463943.32446898887 2575784.3832184738 0, -463918.20070562203 2576183.702619917 0, -463515.8089860782 2576161.4178912505 0, -463113.41681594384 2576139.127593277 0, -463138.301791416 2575744.2873498304 0, -463188.9192366038 2574941.2019163715 0, -463196.45121227956 2574941.5765004004 0)), ((-464937.096481809 2575700.087033282 0, -464928.5530128695 2575837.0287334695 0, -464928.4526466002 2575838.6375712072 0, -464903.51949927624 2576238.3075860483 0, -464887.08327462705 2576501.797045511 0, -464878.39700935816 2576639.4931003833 0, -464878.3431484534 2576640.3824573625 0, -464854.09094255016 2577040.837456766 0, -464838.217164771 2577302.9332062737 0, -464837.0562252017 2577321.3652535304 0, -464811.8891829471 2577321.085257435 0, -464766.82649088395 2577326.1103489115 0, -464755.40941543435 2577334.3433872107 0, -464751.2037088808 2577359.1004940905 0, -464759.70275551005 2577386.9586737705 0, -464773.0340297169 2577424.741107386 0, -464773.0771431283 2577424.862592797 0, -464797.1731942942 2577443.0502988207 0, -464807.56328525895 2577449.673206065 0, -464631.53984982223 2577438.589641639 0, -464631.22398814623 2577443.587782681 0, -464615.29167337413 2577428.4568144553 0, -464576.0646172975 2577397.1888157343 0, -464555.57479544706 2577395.889665911 0, -464524.6199792611 2577422.7116912534 0, -464521.4497953473 2577428.27365366 0, -464514.44614257413 2577434.342532914 0, -464538.9968471909 2577466.3124745665 0, -464562.72751803906 2577493.638865401 0, -464526.389179808 2577549.1250518817 0, -464489.11652091594 2577608.7374029653 0, -464493.6713408025 2577648.7011961546 0, -464492.8433140445 2577702.9044545596 0, -464466.4027872354 2577738.3557627415 0, -464434.40197506174 2577777.065497327 0, -464404.812810613 2577792.169803099 0, -464367.66847528773 2577768.015404443 0, -464342.6809768903 2577724.557705723 0, -464320.66599687096 2577656.6760155717 0, -464295.86255039327 2577601.907708306 0, -464288.0941342627 2577538.082097315 0, -464279.9377086015 2577478.5007729246 0, -464277.9064324353 2577476.794150505 0, -464263.9071737847 2577468.5325357565 0, -464251.9463057986 2577461.4747319506 0, -464249.95473392593 2577459.802275873 0, -464252.5510622925 2577411.0551478895 0, -464218.8431551951 2577409.000187979 0, -464217.78651525057 2577403.2725574877 0, -464209.7549571784 2577359.7271024147 0, -464195.2587707094 2577293.1045055306 0, -464178.698804382 2577281.7068156367 0, -464157.41678466497 2577254.934471376 0, -464186.321640588 2577191.928404721 0, -464222.5097901601 2577143.6309508733 0, -464245.2014497252 2577135.336637269 0, -464265.2189677541 2577140.263590601 0, -464282.6754837639 2577146.4746682304 0, -464287.1030315777 2577147.5649162563 0, -464339.485003487 2577170.942280084 0, -464407.87672958424 2577195.2783001685 0, -464437.7845460607 2577169.9045328535 0, -464483.4159654913 2577116.2338393074 0, -464472.1172339116 2577093.786866766 0, -464437.68294838996 2577057.412049867 0, -464379.71507526276 2577045.2505906043 0, -464319.596377357 2577041.5133966543 0, -464304.40058103704 2577038.3254989535 0, -464297.3545622659 2577028.7823426677 0, -464292.58365757955 2577027.781605413 0, -464289.8096475747 2577024.0247067767 0, -464285.33380089165 2577017.9630467445 0, -464273.68084539607 2577004.189537191 0, -464270.3910880498 2577000.300997528 0, -464266.8004785266 2576995.4363722466 0, -464266.3839822324 2576989.7298110127 0, -464263.14104009303 2576945.3432460255 0, -464255.0198022468 2576895.8779241713 0, -464202.66684775567 2576866.1941167354 0, -464150.96786590706 2576841.200656919 0, -464139.86460662744 2576818.6582911205 0, -464143.9829531782 2576776.6761341197 0, -464142.85249968857 2576726.547589812 0, -464063.6891408286 2576739.7425603513 0, -464014.29669513635 2576749.639661372 0, -463980.3430621567 2576791.996073437 0, -463954.05614179204 2576834.7944496544 0, -463923.30624551146 2576847.566879482 0, -463896.46524345636 2576855.4663607837 0, -463895.59889163164 2576855.8271351433 0, -463883.87232823035 2576859.2774244836 0, -463878.37832621014 2576858.9286823734 0, -463893.0778399444 2576583.0167188225 0, -464295.34907332796 2576607.53743321 0, -464682.56904175243 2576631.13727435 0, -464708.0847137635 2576227.6658522277 0, -464733.5301654517 2575825.334955942 0, -464758.9758257566 2575423.0014905534 0, -464784.4225472731 2575020.6622311734 0, -464794.4157079474 2575021.2268428295 0, -464939.18487480434 2575029.3975207983 0, -464943.71482660837 2575029.707692358 0, -464968.10114058503 2575031.379352574 0, -464978.86292046105 2575032.1186184734 0, -464978.72881342913 2575034.2467949837 0, -464953.62894154043 2575435.655953842 0, -464937.096481809 2575700.087033282 0)), ((-427122.3892649302 2510406.657618777 0, -427121.6073993937 2510406.6083721723 0, -427121.607303883 2510406.6083661583 0, -427121.6074740782 2510406.605239546 0, -427167.29207266384 2510409.4846520214 0, -427477.69133642956 2510424.482990813 0, -427167.2701634584 2510409.4864873113 0, -427167.2702126657 2510409.4864904126 0, -427489.66749348 2510425.061672794 0, -427498.2846000709 2510425.4780471195 0, -427488.6248352047 2510591.0338693755 0, -427112.8165501257 2510568.101098727 0, -427121.60730386025 2510406.608366577 0, -427121.6073213328 2510406.6083676773 0, -427166.7266011812 2510409.4522266914 0, -427122.3892649302 2510406.657618777 0)), ((-428302.7533831593 2510471.4720921647 0, -428293.5116595257 2510636.594242328 0, -427891.0689813323 2510613.801533897 0, -427900.51612006954 2510448.505709506 0, -427970.68001723074 2510452.5260432283 0, -428122.4389314934 2510461.1831019046 0, -427970.98125386966 2510452.5432437616 0, -428302.7533831593 2510471.4720921647 0)), ((-436346.10551138024 2510938.2014115276 0, -436346.1054094166 2510938.2014054214 0, -436260.8903451971 2510933.1025654385 0, -436346.10551316146 2510938.2013793173 0, -436423.0556714865 2510942.8094952027 0, -436346.10551138024 2510938.2014115276 0)), ((-436337.2115463037 2511099.0301875575 0, -435935.1878377702 2511076.165228918 0, -435944.2682461471 2510914.196872157 0, -435944.2725795822 2510914.197129352 0, -436019.43084083596 2510918.661083573 0, -436346.10516805894 2510938.2076197756 0, -436346.11167875346 2510938.2080093427 0, -436747.7785271353 2510962.2613196066 0, -436739.00722823804 2511122.113856621 0, -436337.2115463037 2511099.0301875575 0)), ((-437945.4633888475 2511032.4974911553 0, -438344.8769819778 2511055.7122348617 0, -438349.1716061985 2511055.9619939644 0, -438344.8769817122 2511055.7122394843 0, -438344.8769694131 2511055.712238769 0, -438191.29134578933 2511046.785974206 0, -437945.4633888475 2511032.4974911553 0)), ((-437630.8053028015 2511014.228836478 0, -437942.78666180244 2511032.348041177 0, -437942.7952988941 2511032.3485428006 0, -438344.87663705077 2511055.7182380296 0, -438344.88317202893 2511055.718617854 0, -438436.5255207326 2511061.0482047983 0, -438746.92438312696 2511079.2904069447 0, -438737.5692713429 2511244.521314349 0, -438708.09146898845 2511242.686678195 0, -438641.12810462905 2512855.2839119053 0, -437042.0496653505 2512760.871550386 0, -437136.1836475484 2511123.4523978126 0, -437532.35598531854 2511150.7005817727 0, -437540.67339390906 2511008.9642607914 0, -437540.6777409151 2511008.9645145955 0, -437630.8053028015 2511014.228836478 0)), ((-439149.5913135798 2511103.3541215407 0, -439240.6048005137 2511108.795627342 0, -439552.2067859431 2511127.554180531 0, -439542.82905383897 2511293.0435698433 0, -439140.2008863796 2511268.771542087 0, -439149.5827539224 2511103.3536100066 0, -439149.5913135798 2511103.3541215407 0)), ((-423511.58733838267 2516795.860697203 0, -422312.76373192994 2516733.418483321 0, -422399.4995318504 2515128.1689220434 0, -423623.10174627777 2515195.7103881766 0, -423511.58733838267 2516795.860697203 0)), ((-438174.3331115907 2520886.8578333333 0, -438089.92187792825 2522475.263604186 0, -436474.0111356682 2522378.049033309 0, -436554.3347478653 2520770.822675446 0, -438174.3331115907 2520886.8578333333 0)), ((-440538.10997213115 2535562.1979440977 0, -442145.8851937264 2535670.1549665434 0, -442052.1990970533 2537276.149583939 0, -440436.57473123574 2537166.2334500076 0, -440538.10997213115 2535562.1979440977 0)), ((-424433.8221215985 2539272.0517960135 0, -425858.80544495455 2539354.321771957 0, -426042.7076174558 2539364.6214590515 0, -426000.3251043954 2540171.698450297 0, -425198.13020345493 2540124.357719958 0, -425150.7232410197 2540931.3059425913 0, -424356.8655591133 2540880.5860454924 0, -424433.8221215985 2539272.0517960135 0)), ((-433980.2747087349 2541443.587525573 0, -434077.9976433319 2539841.0195716564 0, -435422.07180602156 2539922.21452343 0, -435687.8193028673 2539937.8840412805 0, -435593.98831040267 2541548.741150996 0, -433980.2747087349 2541443.587525573 0)), ((-445221.8758211143 2542116.0473940196 0, -443609.36413693096 2542010.643948824 0, -443724.2559185373 2540414.178490147 0, -445011.4045750646 2540492.212708913 0, -445334.0316658631 2540511.656936364 0, -445221.8758211143 2542116.0473940196 0)), ((-430483.81379599456 2546068.489295747 0, -428876.86678534385 2545986.869770583 0, -428974.21988311847 2544373.2443760615 0, -429761.11130427127 2544419.7909906157 0, -429739.05529994343 2544779.528298907 0, -430564.12083383923 2544832.9640669976 0, -430483.81379599456 2546068.489295747 0)), ((-425480.6400727827 2548986.52706754 0, -425430.6969382982 2549800.222580658 0, -424598.9474573648 2549755.82807769 0, -424553.6953297701 2550538.651272534 0, -423775.02667608345 2550490.661146024 0, -423859.93340171734 2548888.2040763283 0, -425480.6400727827 2548986.52706754 0)), ((-434275.08783599635 2550281.136577314 0, -435080.07863136154 2550321.9912387785 0, -435056.20641513256 2550737.4739556466 0, -434250.58380005235 2550688.787143192 0, -434275.08783599635 2550281.136577314 0)), ((-444743.72609288245 2550127.3788084257 0, -444646.8909429092 2551734.2035537036 0, -443045.91187862447 2551629.8101939997 0, -443138.36766248266 2550030.7681669304 0, -444743.72609288245 2550127.3788084257 0)), ((-430033.65379390196 2554092.7085277583 0, -429939.73212155275 2555703.016174023 0, -429114.4977130899 2555654.2187654283 0, -429208.16143720975 2554042.0616522403 0, -430033.65379390196 2554092.7085277583 0)), ((-423351.0413268105 2557712.9410724454 0, -423390.8433757743 2556929.712998047 0, -425020.4615986985 2557027.95286503 0, -424974.07251673535 2557811.899534188 0, -426583.6489385309 2557897.5968807926 0, -426530.2388991024 2558724.565606446 0, -424925.27401890064 2558636.616044502 0, -424973.959480343 2557813.8104225034 0, -423351.0413268105 2557712.9410724454 0)), ((-443411.327305519 2558925.4696468185 0, -442620.230223664 2558875.3104349906 0, -442667.3970636231 2558070.3510440984 0, -443463.87689135026 2558116.6695553386 0, -443411.327305519 2558925.4696468185 0)), ((-432008.32069761655 2561507.231298247 0, -431219.4077658447 2561463.038939 0, -431268.61981369683 2560600.434747318 0, -432052.1970686792 2560642.140191054 0, -432008.32069761655 2561507.231298247 0)), ((-426716.81530554 2564624.114100472 0, -426707.52948778763 2564623.5566806584 0, -426692.4828333742 2564614.8672273285 0, -426692.5087301603 2564614.379844563 0, -426691.78988649335 2564613.9495078167 0, -426733.68965493835 2563819.3388428786 0, -426776.64643755584 2563016.7133475426 0, -426799.7086707455 2563018.049594607 0, -427579.00878645526 2563064.951869799 0, -428380.7753124238 2563113.243457345 0, -428380.73552480957 2563113.927417358 0, -428381.6060359371 2563113.979870609 0, -428334.9290819861 2563916.3400202203 0, -428288.2561263625 2564718.683441213 0, -427490.2677354467 2564670.6690188395 0, -426716.81530554 2564624.114100472 0)), ((-434813.6634071391 2563493.2326757205 0, -435617.79621267726 2563541.6064002137 0, -436019.8862331885 2563565.403011668 0, -436425.49723567994 2563589.8554186737 0, -436425.46546135034 2563590.6789542586 0, -436426.48296880024 2563590.739901008 0, -436410.49948270526 2563992.1840610695 0, -436394.68766633986 2564389.3833404593 0, -437200.19668249297 2564433.7771542394 0, -437200.15289863385 2564434.657278908 0, -437200.78255896334 2564434.692071872 0, -437160.9389114734 2565236.5009422502 0, -436402.0176669148 2565192.114209315 0, -436393.7268598631 2565191.6300081937 0, -436362.8367163005 2565189.538800493 0, -436362.86563353776 2565188.812342155 0, -436362.1814346979 2565188.8000458363 0, -436393.90169179055 2564393.5875489637 0, -435980.99398871616 2564368.923160074 0, -435578.9374963974 2564344.902883919 0, -434774.8233555622 2564296.84874285 0, -434774.85987829306 2564296.106550126 0, -434773.9740652296 2564296.0537291938 0, -434774.2416092238 2564291.521798643 0, -433972.84655320656 2564246.8025450376 0, -433972.89941218426 2564245.8250554316 0, -433972.4121819333 2564245.79785903 0, -434015.41325301083 2563445.71849138 0, -434813.6634071391 2563493.2326757205 0)), ((-421756.46215367416 2565939.7167050266 0, -421806.17955510184 2565134.136975296 0, -422614.4160546765 2565178.7852799157 0, -423422.0574774829 2565223.4882375076 0, -423422.0013008767 2565224.4649139903 0, -423422.9813063332 2565224.519108104 0, -423377.15158542315 2566021.330673727 0, -423330.6168102949 2566830.3440194777 0, -423284.0872673842 2567639.34147021 0, -423242.63025312254 2568437.9945767433 0, -423212.2235825094 2569023.8373860703 0, -423199.9920311647 2569236.593043911 0, -423195.68959686905 2569236.320102531 0, -422394.89413102623 2569185.3813387137 0, -421589.7956282559 2569134.1527538174 0, -421589.8393179128 2569133.1811313457 0, -421588.90485162614 2569133.121638298 0, -421593.26696228486 2569056.9531056085 0, -421598.92169992864 2568931.1963351076 0, -421599.2699069732 2568924.6695040325 0, -421630.2338096047 2568345.47384594 0, -421650.8136453823 2567960.5445556445 0, -421671.5662190923 2567555.8997747656 0, -421714.30955632677 2566747.8335770806 0, -4</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Squaxin Island</t>
+          <t>Standing Rock</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>WA</t>
+          <t>SD</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Administrative Site</t>
+          <t>Rural Credit, Indemnity, School and Public Lands, BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, ND SCHOOL OF SCIENCE, CAPITOL BUILDING, VETERANS HOME, MAYVILLE, SCHOOL OF MINES, UNIVERSITY OF ND, ND INDUSTRIAL SCHOOL, ND STATE UNIVERSITY, NDÔøΩSTATEÔøΩUNIVERSITY, ELLENDALE, SCHOOL FOR THE DEAF, STATEÔøΩHOSPITAL, VALLEY/MAYVILLE</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>6</v>
+        <v>739</v>
       </c>
       <c r="G67" t="n">
-        <v>277.57</v>
+        <v>46823.4</v>
       </c>
       <c r="H67" t="n">
-        <v>5</v>
+        <v>217</v>
       </c>
       <c r="I67" t="n">
-        <v>52.27</v>
+        <v>70165.38</v>
       </c>
       <c r="J67" t="n">
-        <v>1</v>
+        <v>522</v>
       </c>
       <c r="K67" t="n">
-        <v>329.84</v>
+        <v>116988.78</v>
       </c>
       <c r="L67" t="n">
-        <v>1737.94</v>
+        <v>2347732.03</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-449556.5059218632 2511728.520408616 0, -449176.91746688675 2511705.777670777 0, -449176.1984435866 2511705.733216676 0, -449556.5059218632 2511728.520408616 0)), ((-449982.1299062058 2511754.164890567 0, -449982.1297245475 2511754.167914157 0, -449699.5578025382 2511737.097241653 0, -449982.1299062058 2511754.164890567 0)), ((-449579.1105100217 2511729.8748406926 0, -449579.1429920948 2511729.876786715 0, -449692.63074373675 2511736.678877075 0, -449982.1297245472 2511754.1679141615 0, -449971.4739245098 2511931.527108429 0, -449568.3538073889 2511907.2960243486 0, -449165.2529589046 2511883.0840977235 0, -448762.17476517527 2511858.894686667 0, -448773.2079271766 2511681.583054768 0, -448773.2382601551 2511681.584876002 0, -448871.2507424927 2511687.473799343 0, -448888.1109399908 2511688.486912748 0, -448915.0532655619 2511690.1000152635 0, -449176.12641623017 2511705.7317984854 0, -449176.1676868195 2511705.7342695664 0, -449579.1105100217 2511729.8748406926 0)), ((-463366.30178307346 2512582.8016465153 0, -463334.87706382683 2512580.856246914 0, -463366.30178338743 2512582.8016431336 0, -463405.7509150512 2512585.2358416286 0, -463366.30178307346 2512582.8016465153 0)), ((-464064.27364119334 2512625.8867090484 0, -464170.7422980627 2512632.464345802 0, -464213.54977654974 2512635.13402016 0, -464170.7422882964 2512632.464375655 0, -464064.27364119334 2512625.8867090484 0)), ((-464417.0083980226 2512647.8287448124 0, -464406.96939841536 2512813.1866125953 0, -464005.15649598924 2512788.596259246 0, -463603.3422352082 2512764.027462437 0, -463201.52449667803 2512739.4803704 0, -463211.49494368176 2512573.224213664 0, -463211.5253091886 2512573.226092752 0, -463366.310057336 2512582.8084000037 0, -463613.2370556818 2512598.044970272 0, -463613.2761352741 2512598.047381669 0, -464015.0843742729 2512622.853928947 0, -464015.1124974243 2512622.855665194 0, -464170.7614092613 2512632.4718089625 0, -464417.0083980226 2512647.8287448124 0)), ((-456264.384418507 2513913.2817409043 0, -456311.65716874925 2513126.286220331 0, -456360.0020620866 2512321.4405879593 0, -456361.8088236175 2512291.361745473 0, -457984.09614303196 2512406.6756496173 0, -457932.25081506104 2513225.965336516 0, -457932.2506155181 2513225.9674284193 0, -457893.0983433012 2513844.675265713 0, -457892.23051078035 2513858.3893516134 0, -457891.59300734167 2513868.4635157497 0, -457890.3708778595 2513887.7760617123 0, -457882.31282094686 2514015.1139713754 0, -457881.30541144765 2514015.05057021 0, -456264.384418507 2513913.2817409043 0)), ((-451282.77213509835 2516843.573187387 0, -452881.1286204372 2516941.3567562765 0, -452788.16282210994 2518541.180243185 0, -451193.0181150282 2518454.0908873766 0, -451282.77213509835 2516843.573187387 0)), ((-447775.73130676866 2521466.171663356 0, -447680.4446375186 2523083.00645899 0, -446062.53746012686 2522978.478549137 0, -446149.0682687236 2521383.5954063167 0, -447775.73130676866 2521466.171663356 0)), ((-452263.06508488936 2527420.0165616595 0, -452262.9989986145 2527421.1705014743 0, -452217.3678488886 2528216.499118979 0, -451389.4571952081 2528170.4905104106 0, -451429.1165415427 2527389.9752738457 0, -451432.0658116872 2527378.173895968 0, -451432.0927535317 2527378.066065934 0, -450674.31094751746 2527334.2312229117 0, -450659.6225222654 2527333.820585373 0, -450659.6496749159 2527333.383858899 0, -450711.31631975883 2526504.3601864562 0, -451480.4558586479 2526550.4099000636 0, -451434.6292940259 2527362.1247527148 0, -451433.9890512456 2527378.2706318754 0, -452231.5475172021 2527418.4299013275 0, -452252.6274551624 2527419.4912691237 0, -452263.06508488936 2527420.0165616595 0)), ((-455166.42114959256 2531660.3247363223 0, -455167.23062476097 2531647.0039018453 0, -456801.4756868293 2531730.9629927757 0, -456691.7622620359 2533334.4222966707 0, -455069.8573224605 2533249.725257102 0, -455166.42114959256 2531660.3247363223 0)), ((-451735.24512163736 2536243.317183069 0, -451645.78562387795 2537864.519470849 0, -450021.007770592 2537765.742848979 0, -450116.09840936464 2536144.5834728894 0, -451735.24512163736 2536243.317183069 0)), ((-461322.1501446945 2536845.070964317 0, -461266.4029524177 2537687.653727615 0, -459665.6639103949 2537608.6670449553 0, -459715.99443711824 2536748.6248253267 0, -461322.1501446945 2536845.070964317 0)), ((-454890.8922974969 2542698.1855162326 0, -453281.3780819311 2542600.764220469 0, -453384.07991065923 2540985.658445156 0, -454594.304251081 2541056.715851151 0, -454988.15293683077 2541080.9520675344 0, -454890.8922974969 2542698.1855162326 0)), ((-459524.2299986185 2546204.2215727074 0, -459429.9975628155 2547813.2614215584 0, -457816.4177064228 2547702.894510099 0, -457894.3280349991 2546101.495725701 0, -459524.2299986185 2546204.2215727074 0)), ((-447333.0196933869 2547058.820925809 0, -447227.8717313179 2548665.936131774 0, -446452.08490666316 2548619.788373531 0, -445623.684550666 2548570.683982875 0, -445713.3941800438 2546965.148014899 0, -446547.97513063496 2547014.6210594294 0, -447333.0196933869 2547058.820925809 0)), ((-455693.08488767454 2555626.9297070154 0, -456468.00679758465 2555674.8984094583 0, -456416.7449249867 2556489.9031604244 0, -454802.76577117445 2556376.1514217234 0, -454885.3564354707 2554791.20763069 0, -455740.92444017367 2554843.778459255 0, -455693.08488767454 2555626.9297070154 0)), ((-449276.9794248514 2555236.611581465 0, -449203.3707008164 2556834.7579691587 0, -447593.3605284898 2556738.3556973888 0, -447672.70063963823 2555137.8819685206 0, -449276.9794248514 2555236.611581465 0)), ((-458875.0183390479 2556662.9690301814 0, -458828.2093868158 2557424.049423567 0, -457185.61157180124 2557335.725614214 0, -457303.25758220925 2555726.584222721 0, -458131.4758505402 2555781.6832451886 0, -458083.5253769855 2556616.3136012475 0, -458875.0183390479 2556662.9690301814 0)), ((-452186.6040555831 2560226.9235749864 0, -453804.62321116845 2560336.180691955 0, -453698.7256673469 2561920.4906114456 0, -452074.04850345897 2561828.9798595035 0, -452186.6040555831 2560226.9235749864 0)), ((-449321.9326013234 2564376.2574031744 0, -449321.3769063425 2564386.1416202285 0, -449276.9198393965 2565177.0558428974 0, -449231.9133044314 2565977.837736146 0, -449231.53414914093 2565984.0533565343 0, -449183.4894144431 2566771.4791362807 0, -449182.9648853079 2566780.0764241694 0, -448373.3310903083 2566731.304009236 0, -447563.6950838357 2566682.5144151314 0, -447514.66624011385 2567489.021035307 0, -446705.1953842786 2567440.7313964185 0, -445988.7150911759 2567397.976206695 0, -445909.0247302735 2567388.175121057 0, -445895.8781619955 2567386.558528588 0, -445895.92348154745 2567385.746683493 0, -445895.1590514922 2567385.67234871 0, -445940.1287341057 2566574.7250591344 0, -445941.19318906 2566574.7945829183 0, -445986.07918338495 2565770.789100794 0, -445986.3991030491 2565765.046846068 0, -446034.2458411558 2564974.470302698 0, -446081.848022635 2564187.9879047014 0, -446082.0960329981 2564183.877433263 0, -446175.0936994005 2564189.500664745 0, -446181.23518354836 2564189.8143169554 0, -446892.4000848265 2564226.1902014404 0, -447120.5724311692 2564237.8580566742 0, -447702.7252258939 2564267.693862222 0, -448512.33092102065 2564321.9463786385 0, -448743.30342503305 2564337.4211003976 0, -449321.9326013234 2564376.2574031744 0), (-448467.324070914 2565124.4624965163 0, -447657.7244795784 2565071.8508929783 0, -447612.77113378036 2565875.227558959 0, -448421.53377836954 2565926.115988229 0, -448422.3650867946 2565926.1683864985 0, -448467.324070914 2565124.4624965163 0)), ((-450872.6268687303 2565283.478366009 0, -451680.51605147077 2565331.9210636 0, -451633.04154613346 2566137.5807718737 0, -450834.4153565486 2566092.4419257008 0, -450827.00930416514 2566092.0250950083 0, -450029.46244642325 2566034.939160159 0, -450074.7745231379 2565230.2747832444 0, -450872.6268687303 2565283.478366009 0)), ((-465522.480087164 2566211.0676372 0, -465497.99191343173 2566611.630241336 0, -465480.8451485192 2566892.1531603415 0, -465473.2948586149 2567012.1479260344 0, -465472.71796541277 2567021.4207174475 0, -465472.031586073 2567021.3812373984 0, -465455.0418494883 2567019.6596213793 0, -465448.99211219745 2567018.280112106 0, -465327.7137608106 2567003.131225467 0, -465322.185706256 2567002.8163942015 0, -465347.6779609036 2566601.412719703 0, -465373.0994776094 2566201.1579084056 0, -465398.521134454 2565800.89875415 0, -465423.9451466621 2565400.6366323116 0, -465547.5166171904 2565407.1564568747 0, -465555.2558658541 2565407.657327017 0, -465571.7365829466 2565408.7253705617 0, -465571.6657606916 2565409.8448486715 0, -465547.05419117556 2565810.4818696138 0, -465529.667752618 2566093.4945963905 0, -465522.4895103514 2566210.9134963593 0, -465522.480087164 2566211.0676372 0)), ((-454811.31346071255 2567141.109477066 0, -454855.6294871319 2566337.2350389366 0, -455258.11700768187 2566364.1809276436 0, -455653.93637284345 2566390.676939578 0, -455629.05221015995 2566792.4430512516 0, -455604.16928405856 2567194.205680881 0, -455213.8082963064 2567168.0663915016 0, -454811.31346071255 2567141.109477066 0)), ((-445778.7935746923 2569395.246043825 0, -445773.73187626095 2569498.2577245524 0, -445759.094738161 2569796.1996818786 0, -445369.4413924876 2569772.410528177 0, -445389.7841105851 2569371.470383204 0, -445410.09594294924 2568971.0564951664 0, -445434.51985076955 2568565.8250266635 0, -445458.6746454063 2568165.0839533997 0, -445056.3294193455 2568141.3206398026 0, -444251.63915332005 2568093.7813247424 0, -444299.9785089062 2567292.2843639296 0, -444310.1872706344 2567292.8866332476 0, -445104.64999606746 2567339.8260526597 0, -445506.98577934084 2567363.5917561376 0, -445895.8781619955 2567386.558528588 0, -445895.60333543544 2567391.0871763406 0, -445871.601985927 2567787.2991851103 0, -445847.3282120576 2568188.0355825336 0, -445823.0542726236 2568588.767889601 0, -445798.49213708605 2568994.28689127 0, -445778.7935746923 2569395.246043825 0)), ((-452174.19734232465 2570747.6675056093 0, -452158.0453145773 2571009.3110569436 0, -452157.64718833106 2571015.7608968886 0, -452151.9472461596 2571015.3874891964 0, -451348.75422009744 2570962.814505742 0, -450539.8587676992 2570909.8519592355 0, -450539.9091747104 2570909.024648134 0, -450539.06196779094 2570908.9691903675 0, -450555.61941961234 2570638.495888727 0, -450588.6149749233 2570099.6443992187 0, -450638.17361392797 2569290.297443804 0, -451439.8572009743 2569341.5330177248 0, -452240.91873932607 2569393.2423031386 0, -452240.88616896205 2569393.897006181 0, -452241.76140384376 2569393.953099999 0, -452241.56006396015 2569397.991822121 0, -452205.9345710624 2570111.7782752165 0, -452201.2866546269 2570204.9095945144 0, -452174.19734232465 2570747.6675056093 0)), ((-446568.4550681967 2573951.0915424577 0, -446563.80971174856 2573952.8998985905 0, -446551.8514681421 2573957.555033972 0, -446562.6124286463 2574012.59082663 0, -446565.37551279727 2574026.7223278442 0, -446568.97758666135 2574056.646631005 0, -446625.42937589827 2574067.665254358 0, -446638.2313802044 2574070.1640319084 0, -446697.67873640795 2574081.922251191 0, -446707.6876513473 2574086.7241391297 0, -446714.6893999777 2574091.4392362507 0, -446716.8276809053 2574092.4650806137 0, -446750.1683095114 2574108.4603109276 0, -446784.95938356454 2574131.8839738998 0, -446799.36959451943 2574158.3019924304 0, -446819.34315285203 2574195.813044364 0, -446833.7530955948 2574222.231089865 0, -446853.72635455267 2574259.7421824727 0, -446874.3846494828 2574297.616373964 0, -446900.8587341657 2574347.339388282 0, -446928.68623211666 2574398.3597569247 0, -446916.27634527377 2574427.995409388 0, -446907.2980127922 2574445.9841933427 0, -446885.66267165233 2574454.170303028 0, -446834.9857463377 2574446.780569181 0, -446745.2809730728 2574432.206206241 0, -446694.603883932 2574424.817553702 0, -446676.48620318633 2574422.176331941 0, -446627.87300325214 2574414.278510132 0, -446550.6406528148 2574391.6491387743 0, -446512.7847795553 2574378.09854516 0, -446492.80560379615 2574375.8343219236 0, -446478.4234633957 2574385.0732659595 0, -446431.1496324344 2574422.694776051 0, -446424.6298018589 2574452.140482353 0, -446398.94756617106 2574502.136867927 0, -446340.09982323315 2574560.1016085385 0, -446285.99670345377 2574613.831450595 0, -446278.6087352978 2574624.503452922 0, -446269.89767463866 2574633.0836661397 0, -446270.9608647694 2574615.557296495 0, -446225.9212432688 2574655.5221559913 0, -446214.9682569618 2574654.8433415717 0, -446178.5546935751 2574652.586824033 0, -446178.5546134259 2574652.5869199685 0, -446214.9682506757 2574654.8434831738 0, -446129.2512760676 2574796.1515730764 0, -445989.49300173635 2574948.5913481 0, -445996.2009790698 2575103.6458547325 0, -445956.77361182624 2575108.6720762732 0, -445946.49791766756 2575087.257677356 0, -445921.36968522216 2575044.6333539444 0, -445918.79881303036 2575039.2751104087 0, -445918.79881303024 2575039.2751104087 0, -445905.6137503262 2575011.7946400736 0, -445900.1632744067 2575002.5494192936 0, -445902.4074946497 2574952.3947126777 0, -445899.913273229 2574882.311590769 0, -445893.9836602633 2574842.597457956 0, -445921.7162698178 2574762.8310657055 0, -445951.94644323573 2574667.3735025837 0, -445955.66247839987 2574646.365390554 0, -445954.72250468645 2574644.1635208954 0, -445955.03065915284 2574642.424815998 0, -445953.41247410345 2574638.634799117 0, -445953.4124741035 2574638.634799117 0, -445953.2656972692 2574638.291027136 0, -445953.02043969627 2574637.7165994206 0, -445936.2766363764 2574598.500258093 0, -445928.21034849255 2574575.791354023 0, -445908.6259245545 2574580.4970363365 0, -445891.66946380393 2574593.49464247 0, -445890.2791959668 2574594.560322038 0, -445888.3325162854 2574592.4428514666 0, -445885.50121547433 2574589.363148009 0, -445877.02642133815 2574586.2225874905 0, -445869.65367432754 2574578.2032980197 0, -445868.20082048024 2574576.6230382407 0, -445832.2017305108 2574558.7271710527 0, -445811.4678179631 2574551.0448905793 0, -445774.65136369405 2574537.403744603 0, -445745.5449259613 2574545.3380191578 0, -445743.1645129254 2574546.6865430293 0, -445728.65320356743 2574554.9073210126 0, -445714.51598370774 2574556.52835275 0, -445701.8415694503 2574561.9725715136 0, -445672.98795473785 2574577.9486203967 0, -445652.36112494336 2574615.369621159 0, -445652.260662085 2574615.731640977 0, -445652.0424214849 2574619.333129469 0, -445649.4273990284 2574642.926399384 0, -445647.22935103806 2574698.7794549344 0, -445639.20174341806 2574743.2514613876 0, -445633.4301780968 2574770.0468409318 0, -445626.06384222314 2574774.265435439 0, -445592.0640389263 2574856.1849386683 0, -445569.7662060519 2574911.243892445 0, -445526.85662866797 2574973.9616541793 0, -445505.57474210643 2574986.4271483268 0, -445481.991395397 2574956.311744628 0, -445476.69957869616 2574906.4662741185 0, -445487.9087582305 2574737.260160259 0, -445498.52683381917 2574616.327599229 0, -445498.53442332573 2574616.221544097 0, -445501.02662029344 2574587.838077341 0, -445510.24065185885 2574387.289699773 0, -445516.91910214105 2574278.4432967617 0, -445520.0287879152 2574227.7611629264 0, -445517.53163593437 2574219.3884955756 0, -445516.21309944324 2574214.9675922766 0, -445516.5630488973 2574207.345973943 0, -445516.6752975337 2574204.901288703 0, -445517.0419461239 2574196.915976583 0, -445500.2378451389 2574140.565765194 0, -445494.8548661272 2574122.6799496817 0, -445501.4186812127 2574014.291503234 0, -445516.84541118756 2574004.198597328 0, -445520.0187222175 2574001.5507348306 0, -445560.83336123556 2574017.4222854553 0, -445611.71132416325 2574025.983912797 0, -445663.6098651552 2574046.166564549 0, -445717.5229416513 2574074.1731103915 0, -445740.52318680566 2574090.552032075 0, -445788.76768398494 2574105.7643663273 0, -445828.7094112431 2574111.4429495097 0, -445875.0752445116 2574100.4918937637 0, -445907.2044888619 2574087.663616673 0, -445915.7437630923 2574085.646486602 0, -445919.85222520004 2574084.6759940004 0, -445939.10924534505 2574076.9884381196 0, -445974.8398783625 2574041.5776248965 0, -445999.37579975557 2574002.5589720556 0, -446024.2769612919 2573936.963886998 0, -446042.07678360125 2573881.76528192 0, -446077.3297600856 2573883.9010345708 0, -446093.9672806464 2573885.830022005 0, -446114.94519567984 2573904.7156140115 0, -446159.9014939694 2573915.924581668 0, -446184.9065645396 2573904.292101264 0, -446199.68989141687 2573884.237382285 0, -446200.28617193596 2573883.880797301 0, -446229.0963397115 2573855.7850391716 0, -446227.3448786952 2573844.1857780414 0, -446318.58519534994 2573850.050926444 0, -446698.1780046639 2573874.784120618 0, -446710.4334241953 2573875.528157732 0, -446694.3859729308 2573884.075065285 0, -446681.81349965365 2573910.118912809 0, -446678.2952695306 2573924.7751732552 0, -446628.48430492333 2573944.1648235247 0, -446568.4550681967 2573951.0915424577 0), (-446624.1749220042 2574068.462996698 0, -446624.17492200434 2574068.462996698 0, -446625.42937589827 2574067.665254358 0, -446624.1749220042 2574068.462996698 0)), ((-446950.56243684096 2574198.6320379856 0, -446932.30556629575 2574201.385897007 0, -446908.93935471226 2574176.457900518 0, -446883.80138547975 2574111.1742358143 0, -446863.6045996117 2574054.5049641044 0, -446875.42459873157 2574008.8867512974 0, -446882.9000154899 2573959.3910239553 0, -446876.09148893814 2573931.137323962 0, -446865.8438236706 2573894.418725824 0, -446864.12461474177 2573885.3509173403 0, -447124.44490654866 2573901.9489376843 0, -447108.22404811066 2574142.9668562766 0, -447101.39372117515 2574133.4359606504 0, -447087.50028866966 2574121.831196952 0, -447052.32130097033 2574102.4577116594 0, -447050.1481298079 2574105.75212045 0, -447024.6023644447 2574144.478105517 0, -446997.2296424889 2574184.283265825 0, -446962.1561278046 2574196.8832502966 0, -446950.56243684096 2574198.6320379856 0)), ((-456765.9186664952 2574520.703219268 0, -456766.7534668326 2574520.7562253936 0, -456775.8150063362 2574523.8307035593 0, -456936.0986376184 2574533.4261585367 0, -457573.4196303584 2574571.6560989986 0, -457521.005743965 2575367.450410148 0, -456717.4002130627 2575315.5125296665 0, -456668.05145486625 2576110.2522586337 0, -455863.1617071876 2576062.149205341 0, -455177.45231584826 2576021.155547476 0, -455166.6825075448 2576020.512744768 0, -455069.6986429143 2576016.5006078887 0, -455058.21920649987 2576016.0251637846 0, -455058.282165094 2576015.0817748327 0, -455057.69480324606 2576015.0569460415 0, -455110.6791901181 2575216.2349368795 0, -455164.28176372364 2574417.0104392366 0, -455264.5815672489 2574424.4891094393 0, -455964.7872605663 2574469.126197598 0, -456765.98251743335 2574519.674981475 0, -456765.9186664952 2574520.703219268 0)), ((-463196.45121227956 2574941.5765004004 0, -463993.9246552496 2574981.302344243 0, -463943.32446898887 2575784.3832184738 0, -463918.20070562203 2576183.702619917 0, -463515.8089860782 2576161.4178912505 0, -463113.41681594384 2576139.127593277 0, -463138.301791416 2575744.2873498304 0, -463188.9192366038 2574941.2019163715 0, -463196.45121227956 2574941.5765004004 0)), ((-464937.096481809 2575700.087033282 0, -464928.5530128695 2575837.0287334695 0, -464928.4526466002 2575838.6375712072 0, -464903.51949927624 2576238.3075860483 0, -464887.08327462705 2576501.797045511 0, -464878.39700935816 2576639.4931003833 0, -464878.3431484534 2576640.3824573625 0, -464854.09094255016 2577040.837456766 0, -464838.217164771 2577302.9332062737 0, -464837.0562252017 2577321.3652535304 0, -464811.8891829471 2577321.085257435 0, -464766.82649088395 2577326.1103489115 0, -464755.40941543435 2577334.3433872107 0, -464751.2037088808 2577359.1004940905 0, -464759.70275551005 2577386.9586737705 0, -464773.0340297169 2577424.741107386 0, -464773.0771431283 2577424.862592797 0, -464797.1731942942 2577443.0502988207 0, -464807.56328525895 2577449.673206065 0, -464631.53984982223 2577438.589641639 0, -464631.22398814623 2577443.587782681 0, -464615.29167337413 2577428.4568144553 0, -464576.0646172975 2577397.1888157343 0, -464555.57479544706 2577395.889665911 0, -464524.6199792611 2577422.7116912534 0, -464521.4497953473 2577428.27365366 0, -464514.44614257413 2577434.342532914 0, -464538.9968471909 2577466.3124745665 0, -464562.72751803906 2577493.638865401 0, -464526.389179808 2577549.1250518817 0, -464489.11652091594 2577608.7374029653 0, -464493.6713408025 2577648.7011961546 0, -464492.8433140445 2577702.9044545596 0, -464466.4027872354 2577738.3557627415 0, -464434.40197506174 2577777.065497327 0, -464404.812810613 2577792.169803099 0, -464367.66847528773 2577768.015404443 0, -464342.6809768903 2577724.557705723 0, -464320.66599687096 2577656.6760155717 0, -464295.86255039327 2577601.907708306 0, -464288.0941342627 2577538.082097315 0, -464279.9377086015 2577478.5007729246 0, -464277.9064324353 2577476.794150505 0, -464263.9071737847 2577468.5325357565 0, -464251.9463057986 2577461.4747319506 0, -464249.95473392593 2577459.802275873 0, -464252.5510622925 2577411.0551478895 0, -464218.8431551951 2577409.000187979 0, -464217.78651525057 2577403.2725574877 0, -464209.7549571784 2577359.7271024147 0, -464195.2587707094 2577293.1045055306 0, -464178.698804382 2577281.7068156367 0, -464157.41678466497 2577254.934471376 0, -464186.321640588 2577191.928404721 0, -464222.5097901601 2577143.6309508733 0, -464245.2014497252 2577135.336637269 0, -464265.2189677541 2577140.263590601 0, -464282.6754837639 2577146.4746682304 0, -464287.1030315777 2577147.5649162563 0, -464339.485003487 2577170.942280084 0, -464407.87672958424 2577195.2783001685 0, -464437.7845460607 2577169.9045328535 0, -464483.4159654913 2577116.2338393074 0, -464472.1172339116 2577093.786866766 0, -464437.68294838996 2577057.412049867 0, -464379.71507526276 2577045.2505906043 0, -464319.596377357 2577041.5133966543 0, -464304.40058103704 2577038.3254989535 0, -464297.3545622659 2577028.7823426677 0, -464292.58365757955 2577027.781605413 0, -464289.8096475747 2577024.0247067767 0, -464285.33380089165 2577017.9630467445 0, -464273.68084539607 2577004.189537191 0, -464270.3910880498 2577000.300997528 0, -464266.8004785266 2576995.4363722466 0, -464266.3839822324 2576989.7298110127 0, -464263.14104009303 2576945.3432460255 0, -464255.0198022468 2576895.8779241713 0, -464202.66684775567 2576866.1941167354 0, -464150.96786590706 2576841.200656919 0, -464139.86460662744 2576818.6582911205 0, -464143.9829531782 2576776.6761341197 0, -464142.85249968857 2576726.547589812 0, -464063.6891408286 2576739.7425603513 0, -464014.29669513635 2576749.639661372 0, -463980.3430621567 2576791.996073437 0, -463954.05614179204 2576834.7944496544 0, -463923.30624551146 2576847.566879482 0, -463896.46524345636 2576855.4663607837 0, -463895.59889163164 2576855.8271351433 0, -463883.87232823035 2576859.2774244836 0, -463878.37832621014 2576858.9286823734 0, -463893.0778399444 2576583.0167188225 0, -464295.34907332796 2576607.53743321 0, -464682.56904175243 2576631.13727435 0, -464708.0847137635 2576227.6658522277 0, -464733.5301654517 2575825.334955942 0, -464758.9758257566 2575423.0014905534 0, -464784.4225472731 2575020.6622311734 0, -464794.4157079474 2575021.2268428295 0, -464939.18487480434 2575029.3975207983 0, -464943.71482660837 2575029.707692358 0, -464968.10114058503 2575031.379352574 0, -464978.86292046105 2575032.1186184734 0, -464978.72881342913 2575034.2467949837 0, -464953.62894154043 2575435.655953842 0, -464937.096481809 2575700.087033282 0)), ((-427122.3892649302 2510406.657618777 0, -427121.6073993937 2510406.6083721723 0, -427121.607303883 2510406.6083661583 0, -427121.6074740782 2510406.605239546 0, -427167.29207266384 2510409.4846520214 0, -427477.69133642956 2510424.482990813 0, -427167.2701634584 2510409.4864873113 0, -427167.2702126657 2510409.4864904126 0, -427489.66749348 2510425.061672794 0, -427498.2846000709 2510425.4780471195 0, -427488.6248352047 2510591.0338693755 0, -427112.8165501257 2510568.101098727 0, -427121.60730386025 2510406.608366577 0, -427121.6073213328 2510406.6083676773 0, -427166.7266011812 2510409.4522266914 0, -427122.3892649302 2510406.657618777 0)), ((-428302.7533831593 2510471.4720921647 0, -428293.5116595257 2510636.594242328 0, -427891.0689813323 2510613.801533897 0, -427900.51612006954 2510448.505709506 0, -427970.68001723074 2510452.5260432283 0, -428122.4389314934 2510461.1831019046 0, -427970.98125386966 2510452.5432437616 0, -428302.7533831593 2510471.4720921647 0)), ((-436346.10551138024 2510938.2014115276 0, -436346.1054094166 2510938.2014054214 0, -436260.8903451971 2510933.1025654385 0, -436346.10551316146 2510938.2013793173 0, -436423.0556714865 2510942.8094952027 0, -436346.10551138024 2510938.2014115276 0)), ((-436337.2115463037 2511099.0301875575 0, -435935.1878377702 2511076.165228918 0, -435944.2682461471 2510914.196872157 0, -435944.2725795822 2510914.197129352 0, -436019.43084083596 2510918.661083573 0, -436346.10516805894 2510938.2076197756 0, -436346.11167875346 2510938.2080093427 0, -436747.7785271353 2510962.2613196066 0, -436739.00722823804 2511122.113856621 0, -436337.2115463037 2511099.0301875575 0)), ((-437945.4633888475 2511032.4974911553 0, -438344.8769819778 2511055.7122348617 0, -438349.1716061985 2511055.9619939644 0, -438344.8769817122 2511055.7122394843 0, -438344.8769694131 2511055.712238769 0, -438191.29134578933 2511046.785974206 0, -437945.4633888475 2511032.4974911553 0)), ((-437630.8053028015 2511014.228836478 0, -437942.78666180244 2511032.348041177 0, -437942.7952988941 2511032.3485428006 0, -438344.87663705077 2511055.7182380296 0, -438344.88317202893 2511055.718617854 0, -438436.5255207326 2511061.0482047983 0, -438746.92438312696 2511079.2904069447 0, -438737.5692713429 2511244.521314349 0, -438708.09146898845 2511242.686678195 0, -438641.12810462905 2512855.2839119053 0, -437042.0496653505 2512760.871550386 0, -437136.1836475484 2511123.4523978126 0, -437532.35598531854 2511150.7005817727 0, -437540.67339390906 2511008.9642607914 0, -437540.6777409151 2511008.9645145955 0, -437630.8053028015 2511014.228836478 0)), ((-439149.5913135798 2511103.3541215407 0, -439240.6048005137 2511108.795627342 0, -439552.2067859431 2511127.554180531 0, -439542.82905383897 2511293.0435698433 0, -439140.2008863796 2511268.771542087 0, -439149.5827539224 2511103.3536100066 0, -439149.5913135798 2511103.3541215407 0)), ((-423511.58733838267 2516795.860697203 0, -422312.76373192994 2516733.418483321 0, -422399.4995318504 2515128.1689220434 0, -423623.10174627777 2515195.7103881766 0, -423511.58733838267 2516795.860697203 0)), ((-438174.3331115907 2520886.8578333333 0, -438089.92187792825 2522475.263604186 0, -436474.0111356682 2522378.049033309 0, -436554.3347478653 2520770.822675446 0, -438174.3331115907 2520886.8578333333 0)), ((-440538.10997213115 2535562.1979440977 0, -442145.8851937264 2535670.1549665434 0, -442052.1990970533 2537276.149583939 0, -440436.57473123574 2537166.2334500076 0, -440538.10997213115 2535562.1979440977 0)), ((-424433.8221215985 2539272.0517960135 0, -425858.80544495455 2539354.321771957 0, -426042.7076174558 2539364.6214590515 0, -426000.3251043954 2540171.698450297 0, -425198.13020345493 2540124.357719958 0, -425150.7232410197 2540931.3059425913 0, -424356.8655591133 2540880.5860454924 0, -424433.8221215985 2539272.0517960135 0)), ((-433980.2747087349 2541443.587525573 0, -434077.9976433319 2539841.0195716564 0, -435422.07180602156 2539922.21452343 0, -435687.8193028673 2539937.8840412805 0, -435593.98831040267 2541548.741150996 0, -433980.2747087349 2541443.587525573 0)), ((-445221.8758211143 2542116.0473940196 0, -443609.36413693096 2542010.643948824 0, -443724.2559185373 2540414.178490147 0, -445011.4045750646 2540492.212708913 0, -445334.0316658631 2540511.656936364 0, -445221.8758211143 2542116.0473940196 0)), ((-430483.81379599456 2546068.489295747 0, -428876.86678534385 2545986.869770583 0, -428974.21988311847 2544373.2443760615 0, -429761.11130427127 2544419.7909906157 0, -429739.05529994343 2544779.528298907 0, -430564.12083383923 2544832.9640669976 0, -430483.81379599456 2546068.489295747 0)), ((-425480.6400727827 2548986.52706754 0, -425430.6969382982 2549800.222580658 0, -424598.9474573648 2549755.82807769 0, -424553.6953297701 2550538.651272534 0, -423775.02667608345 2550490.661146024 0, -423859.93340171734 2548888.2040763283 0, -425480.6400727827 2548986.52706754 0)), ((-434275.08783599635 2550281.136577314 0, -435080.07863136154 2550321.9912387785 0, -435056.20641513256 2550737.4739556466 0, -434250.58380005235 2550688.787143192 0, -434275.08783599635 2550281.136577314 0)), ((-444743.72609288245 2550127.3788084257 0, -444646.8909429092 2551734.2035537036 0, -443045.91187862447 2551629.8101939997 0, -443138.36766248266 2550030.7681669304 0, -444743.72609288245 2550127.3788084257 0)), ((-430033.65379390196 2554092.7085277583 0, -429939.73212155275 2555703.016174023 0, -429114.4977130899 2555654.2187654283 0, -429208.16143720975 2554042.0616522403 0, -430033.65379390196 2554092.7085277583 0)), ((-423351.0413268105 2557712.9410724454 0, -423390.8433757743 2556929.712998047 0, -425020.4615986985 2557027.95286503 0, -424974.07251673535 2557811.899534188 0, -426583.6489385309 2557897.5968807926 0, -426530.2388991024 2558724.565606446 0, -424925.27401890064 2558636.616044502 0, -424973.959480343 2557813.8104225034 0, -423351.0413268105 2557712.9410724454 0)), ((-443411.327305519 2558925.4696468185 0, -442620.230223664 2558875.3104349906 0, -442667.3970636231 2558070.3510440984 0, -443463.87689135026 2558116.6695553386 0, -443411.327305519 2558925.4696468185 0)), ((-432008.32069761655 2561507.231298247 0, -431219.4077658447 2561463.038939 0, -431268.61981369683 2560600.434747318 0, -432052.1970686792 2560642.140191054 0, -432008.32069761655 2561507.231298247 0)), ((-426716.81530554 2564624.114100472 0, -426707.52948778763 2564623.5566806584 0, -426692.4828333742 2564614.8672273285 0, -426692.5087301603 2564614.379844563 0, -426691.78988649335 2564613.9495078167 0, -426733.68965493835 2563819.3388428786 0, -426776.64643755584 2563016.7133475426 0, -426799.7086707455 2563018.049594607 0, -427579.00878645526 2563064.951869799 0, -428380.7753124238 2563113.243457345 0, -428380.73552480957 2563113.927417358 0, -428381.6060359371 2563113.979870609 0, -428334.9290819861 2563916.3400202203 0, -428288.2561263625 2564718.683441213 0, -427490.2677354467 2564670.6690188395 0, -426716.81530554 2564624.114100472 0)), ((-434813.6634071391 2563493.2326757205 0, -435617.79621267726 2563541.6064002137 0, -436019.8862331885 2563565.403011668 0, -436425.49723567994 2563589.8554186737 0, -436425.46546135034 2563590.6789542586 0, -436426.48296880024 2563590.739901008 0, -436410.49948270526 2563992.1840610695 0, -436394.68766633986 2564389.3833404593 0, -437200.19668249297 2564433.7771542394 0, -437200.15289863385 2564434.657278908 0, -437200.78255896334 2564434.692071872 0, -437160.9389114734 2565236.5009422502 0, -436402.0176669148 2565192.114209315 0, -436393.7268598631 2565191.6300081937 0, -436362.8367163005 2565189.538800493 0, -436362.86563353776 2565188.812342155 0, -436362.1814346979 2565188.8000458363 0, -436393.90169179055 2564393.5875489637 0, -435980.99398871616 2564368.923160074 0, -435578.9374963974 2564344.902883919 0, -434774.8233555622 2564296.84874285 0, -434774.85987829306 2564296.106550126 0, -434773.9740652296 2564296.0537291938 0, -434774.2416092238 2564291.521798643 0, -433972.84655320656 2564246.8025450376 0, -433972.89941218426 2564245.8250554316 0, -433972.4121819333 2564245.79785903 0, -434015.41325301083 2563445.71849138 0, -434813.6634071391 2563493.2326757205 0)), ((-421756.46215367416 2565939.7167050266 0, -421806.17955510184 2565134.136975296 0, -422614.4160546765 2565178.7852799157 0, -423422.0574774829 2565223.4882375076 0, -423422.0013008767 2565224.4649139903 0, -423422.9813063332 2565224.519108104 0, -423377.15158542315 2566021.330673727 0, -423330.6168102949 2566830.3440194777 0, -423284.0872673842 2567639.34147021 0, -423242.63025312254 2568437.9945767433 0, -423212.2235825094 2569023.8373860703 0, -423199.9920311647 2569236.593043911 0, -423195.68959686905 2569236.320102531 0, -422394.89413102623 2569185.3813387137 0, -421589.7956282559 2569134.1527538174 0, -421589.8393179128 2569133.1811313457 0, -421588.90485162614 2569133.121638298 0, -421593.26696228486 2569056.9531056085 0, -421598.92169992864 2568931.1963351076 0, -421599.2699069732 2568924.6695040325 0, -421630.2338096047 2568345.47384594 0, -421650.8136453823 2567960.5445556445 0, -421671.5662190923 2567555.8997747656 0, -421714.30955632677 2566747.8335770806 0, -4</t>
+          <t>MULTIPOLYGON Z (((-1468861.5102881684 1062529.544672667 0, -1469017.6210793862 1062555.4110563563 0, -1469129.974785093 1062574.0271501057 0, -1469252.449893471 1062594.3203348885 0, -1469260.0823487265 1062595.5851217243 0, -1469260.0823599044 1062595.5851235767 0, -1469283.173707292 1062599.3663462314 0, -1469642.2312759976 1062658.1631362855 0, -1469644.5357929508 1062658.5420150517 0, -1470024.3775152052 1062720.757761455 0, -1470028.9553121778 1062721.5178974674 0, -1470036.614696355 1062722.7897407915 0, -1470413.0803005649 1062785.259044958 0, -1470413.5090985568 1062785.330216005 0, -1470434.6009114378 1062788.8311073242 0, -1470777.6770908916 1062845.7735343892 0, -1470801.778692093 1062849.7738462705 0, -1470801.7786950548 1062849.7738467618 0, -1470735.291818363 1063247.297021072 0, -1470668.8077412983 1063644.8202214376 0, -1470665.5165512266 1063664.7246222931 0, -1470605.4089253014 1064049.9390719912 0, -1470542.1933719711 1064455.0913720988 0, -1470530.2911529467 1064547.6087893152 0, -1470466.8251287101 1064585.819113063 0, -1470398.8492705273 1064609.9058296997 0, -1470344.2676615152 1064659.9695127506 0, -1470220.7824153055 1064712.4227236935 0, -1470117.9772717974 1064680.9654987962 0, -1470074.4194187138 1064667.6356037075 0, -1470012.878171736 1064611.9488686554 0, -1469981.2567014096 1064594.0036470143 0, -1469904.9436335918 1064618.4355588462 0, -1469867.456967431 1064598.6590498888 0, -1469791.4959079553 1064500.8642470355 0, -1469804.9585004586 1064475.2900794114 0, -1469821.834112315 1064443.2326686454 0, -1469816.7249291502 1064384.524520883 0, -1469812.9904894084 1064341.6145040721 0, -1469811.1894333242 1064334.735605513 0, -1469777.605131138 1064329.0661652733 0, -1469777.6873496468 1064328.532624977 0, -1469789.4935049256 1064251.9189805745 0, -1469789.5006117246 1064251.8726492473 0, -1469789.3708321552 1064251.376711911 0, -1469788.5747998857 1064251.2162895089 0, -1469778.0141272878 1064249.0808299128 0, -1469702.6319516078 1064233.836271017 0, -1469700.7072090243 1064222.2691301936 0, -1469695.323318651 1064189.9152719344 0, -1469641.0308777792 1064172.5543810064 0, -1469589.9364842195 1064156.2161513732 0, -1469580.2220810633 1064136.1836904322 0, -1469578.3887855369 1064132.403009833 0, -1469563.6640393788 1064102.0375518142 0, -1469560.8188364026 1064096.1700240073 0, -1469550.9424646862 1064090.5682925836 0, -1469522.6027439218 1064074.4942171515 0, -1469521.7376082265 1064074.0035687736 0, -1469518.792243473 1064072.332889826 0, -1469518.7249020224 1064072.1973674642 0, -1469494.5615439934 1064023.4539504591 0, -1469427.7809926695 1063998.8150870206 0, -1469395.786498048 1063987.0116526512 0, -1469375.6931782574 1063979.5989675557 0, -1469371.6734833296 1063966.9701128954 0, -1469341.9620892713 1063873.6258968175 0, -1469306.706696515 1063841.1826290756 0, -1469298.967764853 1063834.0602172774 0, -1469289.7784527813 1063838.4524427834 0, -1469276.536821521 1063844.783336913 0, -1469257.2328571894 1063854.0131332797 0, -1469192.3475694433 1063920.157510396 0, -1469161.8019355591 1063932.9952806323 0, -1469149.7209660907 1063938.0728865312 0, -1469137.7064038394 1063951.7945904187 0, -1469108.5820747924 1063985.057432164 0, -1469030.5227920236 1063979.090286098 0, -1469030.5227943866 1063979.0902718552 0, -1469060.0896770647 1063801.4349766506 0, -1469126.045451578 1063405.13122767 0, -1468728.933957707 1063337.2484541982 0, -1468795.2218783214 1062933.398209418 0, -1468857.7885759312 1062528.9281126044 0, -1468861.5102726147 1062529.544767426 0, -1468861.5102881684 1062529.544672667 0)), ((-1470936.141652446 1072177.4399317813 0, -1470956.609938698 1072171.470867857 0, -1470975.5339946318 1072165.9522729167 0, -1470976.333474576 1072165.4015191253 0, -1471017.5148884433 1072137.0258263568 0, -1471050.386111551 1072114.3762780975 0, -1471067.4420601053 1072102.6240930958 0, -1471084.9119592297 1072083.0136674575 0, -1471149.8958743238 1072010.0676796837 0, -1471169.686926693 1071975.458221037 0, -1471185.7446397934 1071947.3774662255 0, -1471191.014199048 1071944.4186051928 0, -1471238.5183119813 1071917.7511584545 0, -1471265.6666654344 1071902.5108701747 0, -1471274.4209054636 1071887.200852194 0, -1471278.7466788962 1071879.6356260723 0, -1471296.989703434 1071847.7311841731 0, -1471308.5035771825 1071827.5945285535 0, -1471353.3414241585 1071749.173591422 0, -1471377.7734401673 1071695.0394602432 0, -1471403.7738109445 1071637.4303359224 0, -1471417.487194447 1071619.213760118 0, -1471417.4872135872 1071619.213734693 0, -1471417.487201225 1071619.213807906 0, -1471357.9532404982 1071971.7344321162 0, -1471291.97526762 1072367.2269985208 0, -1471233.3349821926 1072718.7248871874 0, -1470875.8215589274 1072659.4750318767 0, -1470837.8882755965 1072653.1753064813 0, -1470564.0167686036 1072607.6787556603 0, -1470480.0344672704 1072593.7316797283 0, -1470443.2019366957 1072587.6164524157 0, -1470501.717346761 1072236.8839539203 0, -1470742.030727121 1072277.0534381503 0, -1470742.6141262976 1072276.6007588662 0, -1470755.1501011455 1072266.8721175815 0, -1470755.160569836 1072266.8667452866 0, -1470914.5565615804 1072183.7348585173 0, -1470915.630194244 1072183.4213640604 0, -1470915.6303725615 1072183.4213119927 0, -1470936.141652446 1072177.4399317813 0)), ((-1543541.3070862177 1103619.7923551688 0, -1543471.132541959 1104017.7834517523 0, -1543400.9577496555 1104415.7772416642 0, -1543006.0432961897 1104346.8944055298 0, -1542611.1258225988 1104278.029424674 0, -1542216.2053443387 1104209.1822154725 0, -1541821.2816412267 1104140.3525668217 0, -1541891.0623570846 1103741.9571706527 0, -1541960.8406521182 1103343.5609588125 0, -1542030.6204919585 1102945.17075705 0, -1542100.397894721 1102546.7798312986 0, -1542506.0434976877 1102617.8469586354 0, -1542891.031893279 1102685.266569184 0, -1543286.3435248125 1102754.5333949034 0, -1543681.6515485584 1102823.8207739855 0, -1543611.4784471707 1103221.8035290584 0, -1543541.3070862177 1103619.7923551688 0)), ((-1541031.6997889671 1104002.9700931194 0, -1541426.4922946573 1104071.6524646548 0, -1541821.2816412267 1104140.3525668217 0, -1541751.4321998972 1104538.6853250435 0, -1541681.5821546402 1104937.020687683 0, -1541611.7292000754 1105335.358075126 0, -1541541.8783516525 1105733.6987909738 0, -1541147.1455730456 1105664.8985450075 0, -1540752.409015931 1105596.119028192 0, -1540357.6699156363 1105527.3541561516 0, -1539962.927386934 1105458.6099880957 0, -1540032.7221898055 1105060.3664764278 0, -1540102.516018427 1104662.1286965127 0, -1540172.31262313 1104263.8909204707 0, -1540242.1056809563 1103865.6583494826 0, -1540636.904306417 1103934.3053977208 0, -1541031.6997889671 1104002.9700931194 0)), ((-1547342.5470469545 1105105.3172569699 0, -1547736.7174885585 1105174.4162607584 0, -1548130.8897205284 1105243.5310519938 0, -1548060.8678122961 1105641.9438446802 0, -1547990.845591878 1106040.3594582863 0, -1547920.8222562352 1106438.780509858 0, -1547850.7990700665 1106837.2012610568 0, -1547456.4951831715 1106768.223853697 0, -1547062.190850597 1106699.2613370114 0, -1546667.8870647282 1106630.3163877751 0, -1546273.5808181057 1106561.3860616495 0, -1546343.735389737 1106162.8282205788 0, -1546413.8895459755 1105764.2729044482 0, -1546484.0432420722 1105365.7203685727 0, -1546554.1965213437 1104967.1703658104 0, -1546948.3745847414 1105036.235184688 0, -1547342.5470469545 1105105.3172569699 0)), ((-1544925.5041916769 1109607.9237952072 0, -1545319.5355561916 1109677.1750844913 0, -1545713.5637185103 1109746.4440474745 0, -1545643.4542684052 1110144.7608742642 0, -1545573.3464333003 1110543.0838364991 0, -1545503.2356032194 1110941.408843005 0, -1545433.1268342147 1111339.7369483036 0, -1545039.3780219888 1111270.3692228715 0, -1544645.6255536773 1111201.0221774443 0, -1544251.8730158529 1111131.690055689 0, -1543858.114337918 1111062.3780925348 0, -1543927.9462834024 1110664.149294424 0, -1543997.7751189044 1110265.9226127006 0, -1544067.6060952437 1109867.6989708967 0, -1544137.4346543443 1109469.47446885 0, -1544531.4722247936 1109538.6905486467 0, -1544925.5041916769 1109607.9237952072 0)), ((-1554405.2545278268 1111272.498635714 0, -1554799.5165985026 1111342.3768666137 0, -1555193.7781950636 1111412.2731964616 0, -1555123.1688681673 1111810.2627474642 0, -1555052.5618014392 1112208.2552869038 0, -1554981.9542989044 1112606.2505076707 0, -1554911.346322231 1113004.2481399179 0, -1554516.8998306491 1112934.6555325433 0, -1554122.4497912938 1112865.083517608 0, -1553727.9945172586 1112795.5255847243 0, -1553333.5387672929 1112725.985938102 0, -1553404.334080606 1112327.6849379858 0, -1553475.1316630514 1111929.3869832251 0, -1553545.92672566 1111531.0880411603 0, -1553616.7208285597 1111132.7948632953 0, -1554010.9892628053 1111202.6378513838 0, -1554405.2545278268 1111272.498635714 0)), ((-1540821.1000858005 1112168.1825631203 0, -1541215.5032202355 1112237.2792268265 0, -1541609.9032414798 1112306.3936171948 0, -1542004.3033178374 1112375.5228378773 0, -1541934.5495534237 1112772.449900413 0, -1541864.7957995613 1113169.3765824386 0, -1541794.959892063 1113566.712271437 0, -1541724.3225457717 1113968.6162074856 0, -1541330.043805838 1113899.592810296 0, -1540935.7625170108 1113830.5839519515 0, -1540541.4782218335 1113761.5927436838 0, -1540147.1908377656 1113692.6191710555 0, -1540217.2359593415 1113293.0274753403 0, -1540287.0020580967 1112895.0324329094 0, -1540293.969427788 1112855.2299344921 0, -1540356.840499805 1112497.065358157 0, -1540426.690660166 1112099.1060898788 0, -1540821.1000858005 1112168.1825631203 0)), ((-1551401.8407411405 1114434.772938361 0, -1551330.3865995212 1114832.6475045364 0, -1551259.116941905 1115230.5009309347 0, -1551187.8501687136 1115628.3542240204 0, -1550793.6599560513 1115558.9526567324 0, -1550399.4663589268 1115489.5688436592 0, -1550005.2672562073 1115420.2021529963 0, -1550076.271549637 1115023.8920869136 0, -1549681.9236549835 1114955.0263259395 0, -1549753.2075992275 1114556.8108446607 0, -1550147.8293315996 1114624.4916593872 0, -1550542.1384665174 1114693.89956495 0, -1550936.1860866265 1114763.6996969578 0, -1551007.6152087408 1114365.6667646584 0, -1551401.8407411405 1114434.772938361 0)), ((-1468601.615686918 1063788.0684754087 0, -1468535.0741829383 1063819.1801463002 0, -1468528.7073578194 1063822.156901392 0, -1468502.7962197405 1063815.116886156 0, -1468478.8746527156 1063808.6175396533 0, -1468449.2881214947 1063800.5789912106 0, -1468442.9888689097 1063784.0807156363 0, -1468439.829466776 1063775.8057579244 0, -1468421.9529369222 1063728.9845745459 0, -1468404.6077661994 1063713.4413278988 0, -1468386.5787986477 1063697.2851857617 0, -1468380.0254448703 1063691.4126946828 0, -1468380.2263475517 1063686.7127644774 0, -1468380.6440963955 1063676.9926941614 0, -1468380.7823417233 1063673.7745473245 0, -1468381.8443519762 1063649.052719897 0, -1468346.1375494022 1063556.7575330944 0, -1468317.0841800172 1063481.6602795522 0, -1468329.5057832773 1063434.8410312023 0, -1468342.4687960234 1063418.9478999262 0, -1468370.2285905408 1063384.9135288724 0, -1468324.6108951883 1063320.050833428 0, -1468267.9457064164 1063668.312438764 0, -1468203.235207649 1064066.018831864 0, -1468202.2296142434 1064065.8513758301 0, -1467806.217504514 1063999.9237172224 0, -1467411.2121480687 1063934.1817103429 0, -1467477.2243056681 1063534.9293142157 0, -1467543.3245041664 1063135.1449674314 0, -1467938.0328198047 1063202.606555877 0, -1468310.5765742206 1063266.2857027552 0, -1468310.493354108 1063265.7262026374 0, -1468299.430669261 1063191.3993355876 0, -1468269.1360545233 1063143.598738911 0, -1468267.0946829505 1063140.37760382 0, -1468268.6419386712 1063133.8673546577 0, -1468303.0320962388 1062989.1658948325 0, -1468291.0004253641 1062903.2223146881 0, -1468283.1774665287 1062847.3650625595 0, -1468276.44473341 1062799.2986169462 0, -1468262.5112827518 1062788.9543413199 0, -1468221.6249826727 1062758.6001392917 0, -1468182.9342007223 1062729.8758430292 0, -1468156.0563180307 1062690.570284065 0, -1468134.0870652439 1062658.4430355995 0, -1468091.8939900987 1062645.5733595616 0, -1468095.7168026776 1062639.8473029989 0, -1468128.8270226016 1062590.2502204191 0, -1468145.7972584725 1062511.2885076145 0, -1468137.2458240753 1062459.9532576003 0, -1468133.217049825 1062435.768283414 0, -1468128.753452802 1062408.9728204876 0, -1468275.6936864364 1062432.9568268014 0, -1468462.9383634143 1062463.5195157197 0, -1468397.3814281551 1062866.4442860573 0, -1468331.8213629937 1063269.3711934362 0, -1468728.933957707 1063337.2484541982 0, -1468663.585502209 1063734.527375787 0, -1468648.5095851193 1063826.1798736842 0, -1468648.5087836666 1063826.1792223651 0, -1468601.615686918 1063788.0684754087 0)), ((-1421359.1801524933 1128875.6618870632 0, -1421397.9136396863 1128638.5764640279 0, -1421793.7105461932 1128701.9811103947 0, -1422189.5053045668 1128765.400406615 0, -1422585.2966508765 1128828.8405849081 0, -1422981.0851674736 1128892.2985640552 0, -1422916.7575563558 1129292.1851313629 0, -1422852.429621718 1129692.0740391351 0, -1422788.1010470921 1130091.9656609993 0, -1422723.7722334596 1130491.8596284604 0, -1422326.996357115 1130428.3045470964 0, -1421930.217321748 1130364.7703960943 0, -1421533.435768656 1130301.2511009213 0, -1421136.6488519546 1130237.7493766856 0, -1421201.9675294298 1129837.952657361 0, -1421267.2832773195 1129438.1580246773 0, -1421332.598651699 1129038.3661222346 0, -1421359.1801524933 1128875.6618870632 0)), ((-1463531.2511565369 1188755.4580101734 0, -1463878.2534497501 1188819.6302599178 0, -1463925.9729624768 1188828.4602397683 0, -1464252.5841480803 1188888.8779839652 0, -1464218.961086378 1189079.4634393838 0, -1464182.1281650877 1189288.2826634783 0, -1464148.823761472 1189477.0754685493 0, -1464111.6387284815 1189687.684161974 0, -1464079.4398876503 1189875.444284027 0, -1464042.8443469862 1190088.8203658739 0, -1464011.0906209366 1190273.9858529842 0, -1463974.1054807615 1190489.971261184 0, -1463942.789895234 1190672.5847379053 0, -1463905.3137727934 1190891.1094552637 0, -1463874.4321903992 1191071.1799009135 0, -1463836.5753381876 1191292.2589637707 0, -1463805.9690807331 1191470.7492246598 0, -1463767.8193811495 1191693.2164027032 0, -1463737.4496221736 1191870.3116050353 0, -1463699.113780784 1192094.187835412 0, -1463669.3997288202 1192269.923682783 0, -1463631.1804678114 1192495.972765815 0, -1463601.8214305053 1192669.620079111 0, -1463563.312638796 1192897.7740814928 0, -1463537.505330424 1193050.5814795904 0, -1463495.447004275 1193299.609727551 0, -1463473.1654610978 1193431.544148446 0, -1463467.131492647 1193467.310729348 0, -1463427.6110615314 1193701.4559220355 0, -1463039.2211346093 1193635.722932426 0, -1462645.9246733896 1193569.1766679846 0, -1462253.454596295 1193502.8059261336 0, -1461860.9809928942 1193436.4558941543 0, -1461465.775915477 1193369.3309087444 0, -1461070.5640771105 1193302.2260083114 0, -1460675.35166836 1193235.136159324 0, -1460280.1361796057 1193168.064190211 0, -1460348.9189877973 1192767.698412689 0, -1460417.7015962275 1192367.3348493075 0, -1460486.4818340528 1191966.9702349345 0, -1460555.2638886233 1191566.6115144724 0, -1460624.0968877587 1191166.1222483744 0, -1460654.4481674843 1190989.5241129396 0, -1460693.2947347267 1190763.8966812813 0, -1460762.377094276 1190362.6558866268 0, -1460830.8908553687 1189964.7186480425 0, -1460831.4597193555 1189961.4146086725 0, -1460901.5247094124 1189558.979539018 0, -1460971.5867955305 1189156.546415844 0, -1461041.6488833523 1188754.1159524126 0, -1461111.7107887138 1188351.6875538416 0, -1461161.8645205796 1188359.784572451 0, -1461508.6275839764 1188415.9339920308 0, -1461557.0486800568 1188423.7750625198 0, -1461651.9767357516 1188439.150442345 0, -1461902.7596882635 1188479.8964200392 0, -1461949.4038208523 1188487.8258685207 0, -1462297.8634997874 1188547.408902159 0, -1462344.1805670052 1188555.3295843522 0, -1462692.9540936335 1188614.9808260715 0, -1462738.9863454103 1188622.6580232498 0, -1463089.285219863 1188680.994359118 0, -1463135.1887863597 1188688.6396737194 0, -1463485.61233791 1188747.0162844344 0, -1463531.2511565369 1188755.4580101734 0)))</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Standing Rock</t>
+          <t>Tohono O'odham</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Rural Credit, School and Public Lands, Indemnity, BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, ND SCHOOL OF SCIENCE, CAPITOL BUILDING, VETERANS HOME, MAYVILLE, SCHOOL OF MINES, UNIVERSITY OF ND, ND INDUSTRIAL SCHOOL, ND STATE UNIVERSITY, NDÔøΩSTATEÔøΩUNIVERSITY, ELLENDALE, SCHOOL FOR THE DEAF, STATEÔøΩHOSPITAL, VALLEY/MAYVILLE</t>
+          <t>COUNTY BOND, UNIVERSITY, ST CHRTBL, PENAL &amp; REFORM INST, PERM COMMON SCHLS, SCHOOL OF MINES</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>739</v>
+        <v>33</v>
       </c>
       <c r="G68" t="n">
-        <v>46823.4</v>
+        <v>4903.52</v>
       </c>
       <c r="H68" t="n">
-        <v>217</v>
+        <v>12</v>
       </c>
       <c r="I68" t="n">
-        <v>70165.38</v>
+        <v>9707.76</v>
       </c>
       <c r="J68" t="n">
-        <v>522</v>
+        <v>21</v>
       </c>
       <c r="K68" t="n">
-        <v>116988.78</v>
+        <v>14611.28</v>
       </c>
       <c r="L68" t="n">
-        <v>2347732.03</v>
+        <v>2781661.64</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1468861.5102881684 1062529.544672667 0, -1469017.6210793862 1062555.4110563563 0, -1469129.974785093 1062574.0271501057 0, -1469252.449893471 1062594.3203348885 0, -1469260.0823487265 1062595.5851217243 0, -1469260.0823599044 1062595.5851235767 0, -1469283.173707292 1062599.3663462314 0, -1469642.2312759976 1062658.1631362855 0, -1469644.5357929508 1062658.5420150517 0, -1470024.3775152052 1062720.757761455 0, -1470028.9553121778 1062721.5178974674 0, -1470036.614696355 1062722.7897407915 0, -1470413.0803005649 1062785.259044958 0, -1470413.5090985568 1062785.330216005 0, -1470434.6009114378 1062788.8311073242 0, -1470777.6770908916 1062845.7735343892 0, -1470801.778692093 1062849.7738462705 0, -1470801.7786950548 1062849.7738467618 0, -1470735.291818363 1063247.297021072 0, -1470668.8077412983 1063644.8202214376 0, -1470665.5165512266 1063664.7246222931 0, -1470605.4089253014 1064049.9390719912 0, -1470542.1933719711 1064455.0913720988 0, -1470530.2911529467 1064547.6087893152 0, -1470466.8251287101 1064585.819113063 0, -1470398.8492705273 1064609.9058296997 0, -1470344.2676615152 1064659.9695127506 0, -1470220.7824153055 1064712.4227236935 0, -1470117.9772717974 1064680.9654987962 0, -1470074.4194187138 1064667.6356037075 0, -1470012.878171736 1064611.9488686554 0, -1469981.2567014096 1064594.0036470143 0, -1469904.9436335918 1064618.4355588462 0, -1469867.456967431 1064598.6590498888 0, -1469791.4959079553 1064500.8642470355 0, -1469804.9585004586 1064475.2900794114 0, -1469821.834112315 1064443.2326686454 0, -1469816.7249291502 1064384.524520883 0, -1469812.9904894084 1064341.6145040721 0, -1469811.1894333242 1064334.735605513 0, -1469777.605131138 1064329.0661652733 0, -1469777.6873496468 1064328.532624977 0, -1469789.4935049256 1064251.9189805745 0, -1469789.5006117246 1064251.8726492473 0, -1469789.3708321552 1064251.376711911 0, -1469788.5747998857 1064251.2162895089 0, -1469778.0141272878 1064249.0808299128 0, -1469702.6319516078 1064233.836271017 0, -1469700.7072090243 1064222.2691301936 0, -1469695.323318651 1064189.9152719344 0, -1469641.0308777792 1064172.5543810064 0, -1469589.9364842195 1064156.2161513732 0, -1469580.2220810633 1064136.1836904322 0, -1469578.3887855369 1064132.403009833 0, -1469563.6640393788 1064102.0375518142 0, -1469560.8188364026 1064096.1700240073 0, -1469550.9424646862 1064090.5682925836 0, -1469522.6027439218 1064074.4942171515 0, -1469521.7376082265 1064074.0035687736 0, -1469518.792243473 1064072.332889826 0, -1469518.7249020224 1064072.1973674642 0, -1469494.5615439934 1064023.4539504591 0, -1469427.7809926695 1063998.8150870206 0, -1469395.786498048 1063987.0116526512 0, -1469375.6931782574 1063979.5989675557 0, -1469371.6734833296 1063966.9701128954 0, -1469341.9620892713 1063873.6258968175 0, -1469306.706696515 1063841.1826290756 0, -1469298.967764853 1063834.0602172774 0, -1469289.7784527813 1063838.4524427834 0, -1469276.536821521 1063844.783336913 0, -1469257.2328571894 1063854.0131332797 0, -1469192.3475694433 1063920.157510396 0, -1469161.8019355591 1063932.9952806323 0, -1469149.7209660907 1063938.0728865312 0, -1469137.7064038394 1063951.7945904187 0, -1469108.5820747924 1063985.057432164 0, -1469030.5227920236 1063979.090286098 0, -1469030.5227943866 1063979.0902718552 0, -1469060.0896770647 1063801.4349766506 0, -1469126.045451578 1063405.13122767 0, -1468728.933957707 1063337.2484541982 0, -1468795.2218783214 1062933.398209418 0, -1468857.7885759312 1062528.9281126044 0, -1468861.5102726147 1062529.544767426 0, -1468861.5102881684 1062529.544672667 0)), ((-1470936.141652446 1072177.4399317813 0, -1470956.609938698 1072171.470867857 0, -1470975.5339946318 1072165.9522729167 0, -1470976.333474576 1072165.4015191253 0, -1471017.5148884433 1072137.0258263568 0, -1471050.386111551 1072114.3762780975 0, -1471067.4420601053 1072102.6240930958 0, -1471084.9119592297 1072083.0136674575 0, -1471149.8958743238 1072010.0676796837 0, -1471169.686926693 1071975.458221037 0, -1471185.7446397934 1071947.3774662255 0, -1471191.014199048 1071944.4186051928 0, -1471238.5183119813 1071917.7511584545 0, -1471265.6666654344 1071902.5108701747 0, -1471274.4209054636 1071887.200852194 0, -1471278.7466788962 1071879.6356260723 0, -1471296.989703434 1071847.7311841731 0, -1471308.5035771825 1071827.5945285535 0, -1471353.3414241585 1071749.173591422 0, -1471377.7734401673 1071695.0394602432 0, -1471403.7738109445 1071637.4303359224 0, -1471417.487194447 1071619.213760118 0, -1471417.4872135872 1071619.213734693 0, -1471417.487201225 1071619.213807906 0, -1471357.9532404982 1071971.7344321162 0, -1471291.97526762 1072367.2269985208 0, -1471233.3349821926 1072718.7248871874 0, -1470875.8215589274 1072659.4750318767 0, -1470837.8882755965 1072653.1753064813 0, -1470564.0167686036 1072607.6787556603 0, -1470480.0344672704 1072593.7316797283 0, -1470443.2019366957 1072587.6164524157 0, -1470501.717346761 1072236.8839539203 0, -1470742.030727121 1072277.0534381503 0, -1470742.6141262976 1072276.6007588662 0, -1470755.1501011455 1072266.8721175815 0, -1470755.160569836 1072266.8667452866 0, -1470914.5565615804 1072183.7348585173 0, -1470915.630194244 1072183.4213640604 0, -1470915.6303725615 1072183.4213119927 0, -1470936.141652446 1072177.4399317813 0)), ((-1543541.3070862177 1103619.7923551688 0, -1543471.132541959 1104017.7834517523 0, -1543400.9577496555 1104415.7772416642 0, -1543006.0432961897 1104346.8944055298 0, -1542611.1258225988 1104278.029424674 0, -1542216.2053443387 1104209.1822154725 0, -1541821.2816412267 1104140.3525668217 0, -1541891.0623570846 1103741.9571706527 0, -1541960.8406521182 1103343.5609588125 0, -1542030.6204919585 1102945.17075705 0, -1542100.397894721 1102546.7798312986 0, -1542506.0434976877 1102617.8469586354 0, -1542891.031893279 1102685.266569184 0, -1543286.3435248125 1102754.5333949034 0, -1543681.6515485584 1102823.8207739855 0, -1543611.4784471707 1103221.8035290584 0, -1543541.3070862177 1103619.7923551688 0)), ((-1541031.6997889671 1104002.9700931194 0, -1541426.4922946573 1104071.6524646548 0, -1541821.2816412267 1104140.3525668217 0, -1541751.4321998972 1104538.6853250435 0, -1541681.5821546402 1104937.020687683 0, -1541611.7292000754 1105335.358075126 0, -1541541.8783516525 1105733.6987909738 0, -1541147.1455730456 1105664.8985450075 0, -1540752.409015931 1105596.119028192 0, -1540357.6699156363 1105527.3541561516 0, -1539962.927386934 1105458.6099880957 0, -1540032.7221898055 1105060.3664764278 0, -1540102.516018427 1104662.1286965127 0, -1540172.31262313 1104263.8909204707 0, -1540242.1056809563 1103865.6583494826 0, -1540636.904306417 1103934.3053977208 0, -1541031.6997889671 1104002.9700931194 0)), ((-1547342.5470469545 1105105.3172569699 0, -1547736.7174885585 1105174.4162607584 0, -1548130.8897205284 1105243.5310519938 0, -1548060.8678122961 1105641.9438446802 0, -1547990.845591878 1106040.3594582863 0, -1547920.8222562352 1106438.780509858 0, -1547850.7990700665 1106837.2012610568 0, -1547456.4951831715 1106768.223853697 0, -1547062.190850597 1106699.2613370114 0, -1546667.8870647282 1106630.3163877751 0, -1546273.5808181057 1106561.3860616495 0, -1546343.735389737 1106162.8282205788 0, -1546413.8895459755 1105764.2729044482 0, -1546484.0432420722 1105365.7203685727 0, -1546554.1965213437 1104967.1703658104 0, -1546948.3745847414 1105036.235184688 0, -1547342.5470469545 1105105.3172569699 0)), ((-1544925.5041916769 1109607.9237952072 0, -1545319.5355561916 1109677.1750844913 0, -1545713.5637185103 1109746.4440474745 0, -1545643.4542684052 1110144.7608742642 0, -1545573.3464333003 1110543.0838364991 0, -1545503.2356032194 1110941.408843005 0, -1545433.1268342147 1111339.7369483036 0, -1545039.3780219888 1111270.3692228715 0, -1544645.6255536773 1111201.0221774443 0, -1544251.8730158529 1111131.690055689 0, -1543858.114337918 1111062.3780925348 0, -1543927.9462834024 1110664.149294424 0, -1543997.7751189044 1110265.9226127006 0, -1544067.6060952437 1109867.6989708967 0, -1544137.4346543443 1109469.47446885 0, -1544531.4722247936 1109538.6905486467 0, -1544925.5041916769 1109607.9237952072 0)), ((-1554405.2545278268 1111272.498635714 0, -1554799.5165985026 1111342.3768666137 0, -1555193.7781950636 1111412.2731964616 0, -1555123.1688681673 1111810.2627474642 0, -1555052.5618014392 1112208.2552869038 0, -1554981.9542989044 1112606.2505076707 0, -1554911.346322231 1113004.2481399179 0, -1554516.8998306491 1112934.6555325433 0, -1554122.4497912938 1112865.083517608 0, -1553727.9945172586 1112795.5255847243 0, -1553333.5387672929 1112725.985938102 0, -1553404.334080606 1112327.6849379858 0, -1553475.1316630514 1111929.3869832251 0, -1553545.92672566 1111531.0880411603 0, -1553616.7208285597 1111132.7948632953 0, -1554010.9892628053 1111202.6378513838 0, -1554405.2545278268 1111272.498635714 0)), ((-1540821.1000858005 1112168.1825631203 0, -1541215.5032202355 1112237.2792268265 0, -1541609.9032414798 1112306.3936171948 0, -1542004.3033178374 1112375.5228378773 0, -1541934.5495534237 1112772.449900413 0, -1541864.7957995613 1113169.3765824386 0, -1541794.959892063 1113566.712271437 0, -1541724.3225457717 1113968.6162074856 0, -1541330.043805838 1113899.592810296 0, -1540935.7625170108 1113830.5839519515 0, -1540541.4782218335 1113761.5927436838 0, -1540147.1908377656 1113692.6191710555 0, -1540217.2359593415 1113293.0274753403 0, -1540287.0020580967 1112895.0324329094 0, -1540293.969427788 1112855.2299344921 0, -1540356.840499805 1112497.065358157 0, -1540426.690660166 1112099.1060898788 0, -1540821.1000858005 1112168.1825631203 0)), ((-1551401.8407411405 1114434.772938361 0, -1551330.3865995212 1114832.6475045364 0, -1551259.116941905 1115230.5009309347 0, -1551187.8501687136 1115628.3542240204 0, -1550793.6599560513 1115558.9526567324 0, -1550399.4663589268 1115489.5688436592 0, -1550005.2672562073 1115420.2021529963 0, -1550076.271549637 1115023.8920869136 0, -1549681.9236549835 1114955.0263259395 0, -1549753.2075992275 1114556.8108446607 0, -1550147.8293315996 1114624.4916593872 0, -1550542.1384665174 1114693.89956495 0, -1550936.1860866265 1114763.6996969578 0, -1551007.6152087408 1114365.6667646584 0, -1551401.8407411405 1114434.772938361 0)), ((-1468601.615686918 1063788.0684754087 0, -1468535.0741829383 1063819.1801463002 0, -1468528.7073578194 1063822.156901392 0, -1468502.7962197405 1063815.116886156 0, -1468478.8746527156 1063808.6175396533 0, -1468449.2881214947 1063800.5789912106 0, -1468442.9888689097 1063784.0807156363 0, -1468439.829466776 1063775.8057579244 0, -1468421.9529369222 1063728.9845745459 0, -1468404.6077661994 1063713.4413278988 0, -1468386.5787986477 1063697.2851857617 0, -1468380.0254448703 1063691.4126946828 0, -1468380.2263475517 1063686.7127644774 0, -1468380.6440963955 1063676.9926941614 0, -1468380.7823417233 1063673.7745473245 0, -1468381.8443519762 1063649.052719897 0, -1468346.1375494022 1063556.7575330944 0, -1468317.0841800172 1063481.6602795522 0, -1468329.5057832773 1063434.8410312023 0, -1468342.4687960234 1063418.9478999262 0, -1468370.2285905408 1063384.9135288724 0, -1468324.6108951883 1063320.050833428 0, -1468267.9457064164 1063668.312438764 0, -1468203.235207649 1064066.018831864 0, -1468202.2296142434 1064065.8513758301 0, -1467806.217504514 1063999.9237172224 0, -1467411.2121480687 1063934.1817103429 0, -1467477.2243056681 1063534.9293142157 0, -1467543.3245041664 1063135.1449674314 0, -1467938.0328198047 1063202.606555877 0, -1468310.5765742206 1063266.2857027552 0, -1468310.493354108 1063265.7262026374 0, -1468299.430669261 1063191.3993355876 0, -1468269.1360545233 1063143.598738911 0, -1468267.0946829505 1063140.37760382 0, -1468268.6419386712 1063133.8673546577 0, -1468303.0320962388 1062989.1658948325 0, -1468291.0004253641 1062903.2223146881 0, -1468283.1774665287 1062847.3650625595 0, -1468276.44473341 1062799.2986169462 0, -1468262.5112827518 1062788.9543413199 0, -1468221.6249826727 1062758.6001392917 0, -1468182.9342007223 1062729.8758430292 0, -1468156.0563180307 1062690.570284065 0, -1468134.0870652439 1062658.4430355995 0, -1468091.8939900987 1062645.5733595616 0, -1468095.7168026776 1062639.8473029989 0, -1468128.8270226016 1062590.2502204191 0, -1468145.7972584725 1062511.2885076145 0, -1468137.2458240753 1062459.9532576003 0, -1468133.217049825 1062435.768283414 0, -1468128.753452802 1062408.9728204876 0, -1468275.6936864364 1062432.9568268014 0, -1468462.9383634143 1062463.5195157197 0, -1468397.3814281551 1062866.4442860573 0, -1468331.8213629937 1063269.3711934362 0, -1468728.933957707 1063337.2484541982 0, -1468663.585502209 1063734.527375787 0, -1468648.5095851193 1063826.1798736842 0, -1468648.5087836666 1063826.1792223651 0, -1468601.615686918 1063788.0684754087 0)), ((-1421359.1801524933 1128875.6618870632 0, -1421397.9136396863 1128638.5764640279 0, -1421793.7105461932 1128701.9811103947 0, -1422189.5053045668 1128765.400406615 0, -1422585.2966508765 1128828.8405849081 0, -1422981.0851674736 1128892.2985640552 0, -1422916.7575563558 1129292.1851313629 0, -1422852.429621718 1129692.0740391351 0, -1422788.1010470921 1130091.9656609993 0, -1422723.7722334596 1130491.8596284604 0, -1422326.996357115 1130428.3045470964 0, -1421930.217321748 1130364.7703960943 0, -1421533.435768656 1130301.2511009213 0, -1421136.6488519546 1130237.7493766856 0, -1421201.9675294298 1129837.952657361 0, -1421267.2832773195 1129438.1580246773 0, -1421332.598651699 1129038.3661222346 0, -1421359.1801524933 1128875.6618870632 0)), ((-1463531.2511565369 1188755.4580101734 0, -1463878.2534497501 1188819.6302599178 0, -1463925.9729624768 1188828.4602397683 0, -1464252.5841480803 1188888.8779839652 0, -1464218.961086378 1189079.4634393838 0, -1464182.1281650877 1189288.2826634783 0, -1464148.823761472 1189477.0754685493 0, -1464111.6387284815 1189687.684161974 0, -1464079.4398876503 1189875.444284027 0, -1464042.8443469862 1190088.8203658739 0, -1464011.0906209366 1190273.9858529842 0, -1463974.1054807615 1190489.971261184 0, -1463942.789895234 1190672.5847379053 0, -1463905.3137727934 1190891.1094552637 0, -1463874.4321903992 1191071.1799009135 0, -1463836.5753381876 1191292.2589637707 0, -1463805.9690807331 1191470.7492246598 0, -1463767.8193811495 1191693.2164027032 0, -1463737.4496221736 1191870.3116050353 0, -1463699.113780784 1192094.187835412 0, -1463669.3997288202 1192269.923682783 0, -1463631.1804678114 1192495.972765815 0, -1463601.8214305053 1192669.620079111 0, -1463563.312638796 1192897.7740814928 0, -1463537.505330424 1193050.5814795904 0, -1463495.447004275 1193299.609727551 0, -1463473.1654610978 1193431.544148446 0, -1463467.131492647 1193467.310729348 0, -1463427.6110615314 1193701.4559220355 0, -1463039.2211346093 1193635.722932426 0, -1462645.9246733896 1193569.1766679846 0, -1462253.454596295 1193502.8059261336 0, -1461860.9809928942 1193436.4558941543 0, -1461465.775915477 1193369.3309087444 0, -1461070.5640771105 1193302.2260083114 0, -1460675.35166836 1193235.136159324 0, -1460280.1361796057 1193168.064190211 0, -1460348.9189877973 1192767.698412689 0, -1460417.7015962275 1192367.3348493075 0, -1460486.4818340528 1191966.9702349345 0, -1460555.2638886233 1191566.6115144724 0, -1460624.0968877587 1191166.1222483744 0, -1460654.4481674843 1190989.5241129396 0, -1460693.2947347267 1190763.8966812813 0, -1460762.377094276 1190362.6558866268 0, -1460830.8908553687 1189964.7186480425 0, -1460831.4597193555 1189961.4146086725 0, -1460901.5247094124 1189558.979539018 0, -1460971.5867955305 1189156.546415844 0, -1461041.6488833523 1188754.1159524126 0, -1461111.7107887138 1188351.6875538416 0, -1461161.8645205796 1188359.784572451 0, -1461508.6275839764 1188415.9339920308 0, -1461557.0486800568 1188423.7750625198 0, -1461651.9767357516 1188439.150442345 0, -1461902.7596882635 1188479.8964200392 0, -1461949.4038208523 1188487.8258685207 0, -1462297.8634997874 1188547.408902159 0, -1462344.1805670052 1188555.3295843522 0, -1462692.9540936335 1188614.9808260715 0, -1462738.9863454103 1188622.6580232498 0, -1463089.285219863 1188680.994359118 0, -1463135.1887863597 1188688.6396737194 0, -1463485.61233791 1188747.0162844344 0, -1463531.2511565369 1188755.4580101734 0)))</t>
+          <t>MULTIPOLYGON Z (((-126428.62322647788 1506590.4673863722 0, -126419.5078889794 1506995.0315194267 0, -126013.29182701427 1506990.0060043542 0, -125615.9628336914 1506985.244362261 0, -125218.6161798179 1506980.4788590758 0, -124839.35714439845 1506976.0109209418 0, -124846.02256163236 1506571.3431001147 0, -124852.72540050365 1506164.1532511492 0, -125229.91695981652 1506169.7056386427 0, -125609.17162482155 1506175.2883957503 0, -125628.21110767208 1506175.5707156293 0, -126026.51557175932 1506181.4768249998 0, -126437.7088187951 1506187.5740508868 0, -126428.62322647788 1506590.4673863722 0)), ((-126328.47366274262 1512654.7900340538 0, -125925.11772182248 1512656.1815480343 0, -125528.95547502476 1512657.5649384318 0, -125132.83774524032 1512658.9789293592 0, -124746.9258310655 1512660.3609926691 0, -124751.6730561306 1512248.1914185893 0, -124756.35842910505 1511841.9823246961 0, -125144.36193426771 1511843.644976366 0, -125540.86080873317 1511845.37364449 0, -125546.79751200859 1511439.7551722657 0, -125150.13354273964 1511437.72160729 0, -124761.03469939323 1511435.7739310288 0, -124765.75185726258 1511026.2057185778 0, -125155.92106849636 1511030.7236763998 0, -125552.7341746498 1511035.3250618821 0, -125949.5470047659 1511039.9563562071 0, -126348.57424852277 1511044.6283226218 0, -126343.58969136687 1511443.8854637193 0, -126338.53614343535 1511848.9123334696 0, -126333.47375256877 1512253.9286938282 0, -126328.47366274262 1512654.7900340538 0)), ((-126268.68125744934 1515917.5458290786 0, -126270.36793947153 1516325.9654369245 0, -126272.04018153538 1516732.346466401 0, -126273.70401740653 1517138.0558186683 0, -126275.36985405014 1517541.8166029404 0, -125867.81269531592 1517534.8634892956 0, -125468.27418382304 1517528.0608032343 0, -125068.73533762619 1517521.2771920671 0, -124676.36541358086 1517514.6297736473 0, -124676.58106027775 1517118.5400189376 0, -124676.80695083256 1516712.7707200558 0, -125072.12608191653 1516717.7020674224 0, -125472.88230528434 1516722.5874150866 0, -125475.24808324069 1516316.5699905695 0, -125477.62148531683 1515910.0156483965 0, -125877.44107624413 1515913.8075593114 0, -126268.68125744934 1515917.5458290786 0)), ((-126224.89516022889 1521194.6489400552 0, -126217.79956318598 1521599.372847899 0, -126210.71311489711 1522004.0752571216 0, -126203.5678509434 1522411.533865739 0, -125809.20984091918 1522408.6090121903 0, -125410.36621002032 1522405.6806337943 0, -125011.52270265628 1522402.76000022 0, -124618.70411357592 1522399.9026395646 0, -124622.13115635276 1521982.047332273 0, -124625.46167313609 1521577.2445741813 0, -124628.78268918867 1521172.464893381 0, -124632.09194657534 1520769.0639375413 0, -125034.69622160662 1520774.194629696 0, -125434.06195500019 1520779.296377248 0, -125833.42755836768 1520784.417087296 0, -126231.99660111818 1520789.5449003836 0, -126224.89516022889 1521194.6489400552 0)), ((-120847.64143212377 1506105.5732457587 0, -120844.3304654017 1506520.8640379936 0, -120445.64522029008 1506516.708205814 0, -120449.20874109371 1506101.6004871374 0, -120462.5576369535 1506101.7238225874 0, -120847.64143212377 1506105.5732457587 0)), ((-121240.08536453794 1506930.3648465348 0, -121243.02427341757 1506525.0500728537 0, -121666.25969838328 1506529.5528248027 0, -121660.75708829418 1506934.819746684 0, -121240.08536453794 1506930.3648465348 0)), ((-120837.94142515396 1507331.464363735 0, -120841.13574773929 1506926.1861657395 0, -121240.08536453794 1506930.3648465348 0, -121237.14669844387 1507335.647000029 0, -120837.94142515396 1507331.464363735 0)), ((-120374.48354121138 1511780.0335297228 0, -120382.1560054831 1511375.079419753 0, -120782.70172135768 1511379.9353246607 0, -121183.24702740194 1511384.832745308 0, -121175.54034185561 1511789.4950272364 0, -121167.83391822259 1512194.1468786737 0, -120767.3225307569 1512189.563704962 0, -120775.02066180098 1511784.766116763 0, -120374.48354121138 1511780.0335297228 0)), ((-120707.8534847224 1515856.5487732443 0, -120702.4572395265 1516259.605987525 0, -120697.05644867805 1516665.442556123 0, -120691.63862696686 1517071.2348002568 0, -120686.17998507353 1517480.4781508537 0, -120288.620272845 1517476.4821538334 0, -119893.47711048658 1517472.5168218843 0, -119899.96158757615 1517066.2460947693 0, -119906.4623708097 1516658.8336174053 0, -119912.96324728672 1516251.4220112301 0, -119919.33105734637 1515852.0985516747 0, -120311.13087643796 1515854.3016815225 0, -120707.8534847224 1515856.5487732443 0)), ((-121423.27919263708 1521123.6379134287 0, -121418.10893474067 1521529.2408057053 0, -121826.29440331022 1521536.1366622106 0, -122224.86296199447 1521542.9015232115 0, -122220.13127017854 1521948.5342373766 0, -122215.45736674874 1522350.1908891867 0, -121815.89131574231 1522342.234943161 0, -121407.84184039342 1522334.1419623222 0, -121018.52061237377 1522336.06356573 0, -120620.82032566948 1522338.0399300922 0, -120223.12029071625 1522340.0462541622 0, -119814.56364879261 1522342.1186002165 0, -119821.43015230344 1521932.5722585346 0, -119828.23087917826 1521527.653247194 0, -119835.02279326417 1521122.7348988163 0, -119841.69247015512 1520725.1543634795 0, -120244.46853500957 1520723.1114406264 0, -120642.7226717468 1520721.1014950145 0, -121040.99494318612 1520719.1106676604 0, -121428.46142744238 1520717.1956556789 0, -121423.27919263708 1521123.6379134287 0)), ((-116471.45640800915 1506060.2624132033 0, -116594.54191503269 1506061.0267343943 0, -116882.40405810311 1506065.8006737737 0, -116889.51687631683 1506065.9232600555 0, -116885.6696075123 1506463.6173947568 0, -116881.76229939541 1506867.5384234276 0, -116467.95463077669 1506861.6245820164 0, -116469.72981176751 1506457.2484630274 0, -116071.6503314145 1506451.0002098747 0, -116073.25528882556 1506056.8939392562 0, -116189.72593021201 1506058.2336734035 0, -116335.80511972874 1506059.1296684262 0, -116354.05844230119 1506059.7179110707 0, -116388.71931142654 1506059.7486425918 0, -116471.45640800915 1506060.2624132033 0)), ((-120054.01589803868 1507323.6422674174 0, -120064.85478750731 1506918.5741732598 0, -120075.69404072672 1506513.5179867279 0, -120445.64522029008 1506516.708205814 0, -120442.1863253491 1506922.003984145 0, -120438.73599286917 1507327.3119527982 0, -120054.01589803868 1507323.6422674174 0)), ((-116068.32066701987 1507260.6183581767 0, -116066.55903039787 1507671.7629631455 0, -115668.82447392556 1507665.8735412485 0, -115285.09936666551 1507660.2167836893 0, -115288.32614014135 1507249.9890117033 0, -115291.51705574054 1506844.2990662323 0, -115672.01610032438 1506850.0344130418 0, -116069.98528544577 1506855.83690274 0, -116068.32066701987 1507260.6183581767 0)), ((-116846.39151474854 1510924.704217221 0, -116845.16462299743 1511324.9405872498 0, -116843.9271629774 1511729.7374744387 0, -116842.68046339208 1512134.5351659828 0, -116841.42182462315 1512545.260208008 0, -116426.63213803283 1512538.220543904 0, -116029.19096976993 1512531.4961158284 0, -115792.77013346601 1512527.5053387107 0, -115861.56410122562 1512116.4430048715 0, -115874.71515635849 1512039.5643073677 0, -115824.2898662478 1511712.8981180622 0, -115800.93082433454 1511561.5284411449 0, -115707.14755079916 1511430.8375939096 0, -115638.51462219845 1511394.1334878106 0, -115464.3698573541 1511301.0411959954 0, -115243.8402278692 1511181.561052207 0, -115245.96735315837 1510911.1889799149 0, -115642.91094529454 1510914.5070823168 0, -116041.67928666784 1510917.8690668375 0, -116440.43872641968 1510921.2497684301 0, -116846.39151474854 1510924.704217221 0)), ((-119984.91059292722 1511775.5321362126 0, -120374.48354121138 1511780.0335297228 0, -120366.82009955254 1512184.9886002117 0, -119977.45822824458 1512180.6582820406 0, -119984.91059292722 1511775.5321362126 0)), ((-116663.71292682382 1522325.186876025 0, -116273.24848322617 1522314.3152888955 0, -115877.1758424719 1522303.3061685655 0, -115480.91674428737 1522292.3131322623 0, -115079.40322824946 1522281.188541352 0, -115084.04238776764 1521866.3125016468 0, -115088.59057512072 1521460.6571707528 0, -115093.12967776295 1521055.013615643 0, -115097.57815085424 1520657.2685002252 0, -115500.7912924653 1520667.5419716476 0, -115899.46532991882 1520677.7273618353 0, -116298.12107991171 1520687.9203425033 0, -116694.44956562693 1520698.0774491972 0, -116687.05813663924 1521089.4854640688 0, -116679.37966499559 1521495.8478743378 0, -116671.701530671 1521902.1999256238 0, -116663.71292682382 1522325.186876025 0)), ((-111693.47827975018 1506791.7373515991 0, -111690.67166922861 1507196.837033738 0, -111291.84376854908 1507191.0281420343 0, -111295.02150904168 1506785.9000619962 0, -111298.19956011556 1506380.739163877 0, -110900.09626867746 1506374.880627077 0, -110526.69017948666 1506369.3524212283 0, -110531.69889082109 1505988.0124887344 0, -110903.36823473191 1505992.0725870694 0, -111301.12811380504 1505996.4363694172 0, -111698.88782772499 1506000.8188656422 0, -112110.03137877685 1506005.3643421577 0, -112109.39633769491 1506392.4092545758 0, -112108.73343015161 1506797.480731412 0, -111693.47827975018 1506791.7373515991 0)), ((-115294.70735200212 1506438.632235053 0, -115297.80474291745 1506044.632829943 0, -115298.11684014743 1506044.6370991848 0, -115507.43099867749 1506049.857698452 0, -115675.06780216953 1506050.369341692 0, -115673.57021314393 1506444.781974076 0, -115294.70735200212 1506438.632235053 0)), ((-110893.03322813392 1507185.238518913 0, -111291.84376854908 1507191.0281420343 0, -111288.49301764238 1507615.2455195594 0, -110889.2896443036 1507612.5313155309 0, -110510.39547663584 1507609.9780101487 0, -110516.04636656727 1507179.7414623227 0, -110893.03322813392 1507185.238518913 0)), ((-111687.6964802307 1507617.967321089 0, -111690.67166922861 1507196.837033738 0, -112108.07038293855 1507202.5305956076 0, -112107.38954065862 1507620.857122165 0, -111687.6964802307 1507617.967321089 0)), ((-115239.74303067155 1511703.0603429652 0, -115629.54393633179 1511709.641905785 0, -115635.44894134508 1511735.704398272 0, -115706.24141109285 1512047.9832236923 0, -115704.1622780216 1512113.4742729727 0, -115632.96689429639 1512112.1387424502 0, -115236.58908618204 1512104.6040311817 0, -115239.74303067155 1511703.0603429652 0)), ((-111914.36779684611 1520593.843441507 0, -111907.99874313743 1520996.2340475866 0, -111901.57447392131 1521402.1091506225 0, -111895.15037167615 1521807.9851056247 0, -111888.66682726864 1522217.659301615 0, -111493.40769582988 1522213.6686086245 0, -111095.11402961217 1522209.667588022 0, -110696.82028878036 1522205.6855196028 0, -110303.8783094667 1522201.780405798 0, -110307.50071021168 1521797.9286285667 0, -110311.14072355286 1521392.0498372915 0, -110314.78940902809 1520986.172076282 0, -110318.38811167254 1520584.764788481 0, -110720.25922364488 1520587.0278309209 0, -111118.56376665241 1520589.2843575063 0, -111516.86848876557 1520591.5486326523 0, -111914.36779684611 1520593.843441507 0)))</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Tohono O'odham</t>
+          <t>Tonkawa</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>COUNTY BOND, UNIVERSITY, ST CHRTBL, PENAL &amp; REFORM INST, PERM COMMON SCHLS, SCHOOL OF MINES</t>
+          <t>Public Building, Common Schools, Oklahoma State University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>33</v>
+        <v>152</v>
       </c>
       <c r="G69" t="n">
-        <v>4903.52</v>
+        <v>186.91</v>
       </c>
       <c r="H69" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I69" t="n">
-        <v>9707.76</v>
+        <v>5810.78</v>
       </c>
       <c r="J69" t="n">
-        <v>21</v>
+        <v>146</v>
       </c>
       <c r="K69" t="n">
-        <v>14611.28</v>
+        <v>5997.69</v>
       </c>
       <c r="L69" t="n">
-        <v>2781661.64</v>
+        <v>91880.64999999999</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-126428.62322647788 1506590.4673863722 0, -126419.5078889794 1506995.0315194267 0, -126013.29182701427 1506990.0060043542 0, -125615.9628336914 1506985.244362261 0, -125218.6161798179 1506980.4788590758 0, -124839.35714439845 1506976.0109209418 0, -124846.02256163236 1506571.3431001147 0, -124852.72540050365 1506164.1532511492 0, -125229.91695981652 1506169.7056386427 0, -125609.17162482155 1506175.2883957503 0, -125628.21110767208 1506175.5707156293 0, -126026.51557175932 1506181.4768249998 0, -126437.7088187951 1506187.5740508868 0, -126428.62322647788 1506590.4673863722 0)), ((-126328.47366274262 1512654.7900340538 0, -125925.11772182248 1512656.1815480343 0, -125528.95547502476 1512657.5649384318 0, -125132.83774524032 1512658.9789293592 0, -124746.9258310655 1512660.3609926691 0, -124751.6730561306 1512248.1914185893 0, -124756.35842910505 1511841.9823246961 0, -125144.36193426771 1511843.644976366 0, -125540.86080873317 1511845.37364449 0, -125546.79751200859 1511439.7551722657 0, -125150.13354273964 1511437.72160729 0, -124761.03469939323 1511435.7739310288 0, -124765.75185726258 1511026.2057185778 0, -125155.92106849636 1511030.7236763998 0, -125552.7341746498 1511035.3250618821 0, -125949.5470047659 1511039.9563562071 0, -126348.57424852277 1511044.6283226218 0, -126343.58969136687 1511443.8854637193 0, -126338.53614343535 1511848.9123334696 0, -126333.47375256877 1512253.9286938282 0, -126328.47366274262 1512654.7900340538 0)), ((-126268.68125744934 1515917.5458290786 0, -126270.36793947153 1516325.9654369245 0, -126272.04018153538 1516732.346466401 0, -126273.70401740653 1517138.0558186683 0, -126275.36985405014 1517541.8166029404 0, -125867.81269531592 1517534.8634892956 0, -125468.27418382304 1517528.0608032343 0, -125068.73533762619 1517521.2771920671 0, -124676.36541358086 1517514.6297736473 0, -124676.58106027775 1517118.5400189376 0, -124676.80695083256 1516712.7707200558 0, -125072.12608191653 1516717.7020674224 0, -125472.88230528434 1516722.5874150866 0, -125475.24808324069 1516316.5699905695 0, -125477.62148531683 1515910.0156483965 0, -125877.44107624413 1515913.8075593114 0, -126268.68125744934 1515917.5458290786 0)), ((-126224.89516022889 1521194.6489400552 0, -126217.79956318598 1521599.372847899 0, -126210.71311489711 1522004.0752571216 0, -126203.5678509434 1522411.533865739 0, -125809.20984091918 1522408.6090121903 0, -125410.36621002032 1522405.6806337943 0, -125011.52270265628 1522402.76000022 0, -124618.70411357592 1522399.9026395646 0, -124622.13115635276 1521982.047332273 0, -124625.46167313609 1521577.2445741813 0, -124628.78268918867 1521172.464893381 0, -124632.09194657534 1520769.0639375413 0, -125034.69622160662 1520774.194629696 0, -125434.06195500019 1520779.296377248 0, -125833.42755836768 1520784.417087296 0, -126231.99660111818 1520789.5449003836 0, -126224.89516022889 1521194.6489400552 0)), ((-120847.64143212377 1506105.5732457587 0, -120844.3304654017 1506520.8640379936 0, -120445.64522029008 1506516.708205814 0, -120449.20874109371 1506101.6004871374 0, -120462.5576369535 1506101.7238225874 0, -120847.64143212377 1506105.5732457587 0)), ((-121240.08536453794 1506930.3648465348 0, -121243.02427341757 1506525.0500728537 0, -121666.25969838328 1506529.5528248027 0, -121660.75708829418 1506934.819746684 0, -121240.08536453794 1506930.3648465348 0)), ((-120837.94142515396 1507331.464363735 0, -120841.13574773929 1506926.1861657395 0, -121240.08536453794 1506930.3648465348 0, -121237.14669844387 1507335.647000029 0, -120837.94142515396 1507331.464363735 0)), ((-120374.48354121138 1511780.0335297228 0, -120382.1560054831 1511375.079419753 0, -120782.70172135768 1511379.9353246607 0, -121183.24702740194 1511384.832745308 0, -121175.54034185561 1511789.4950272364 0, -121167.83391822259 1512194.1468786737 0, -120767.3225307569 1512189.563704962 0, -120775.02066180098 1511784.766116763 0, -120374.48354121138 1511780.0335297228 0)), ((-120707.8534847224 1515856.5487732443 0, -120702.4572395265 1516259.605987525 0, -120697.05644867805 1516665.442556123 0, -120691.63862696686 1517071.2348002568 0, -120686.17998507353 1517480.4781508537 0, -120288.620272845 1517476.4821538334 0, -119893.47711048658 1517472.5168218843 0, -119899.96158757615 1517066.2460947693 0, -119906.4623708097 1516658.8336174053 0, -119912.96324728672 1516251.4220112301 0, -119919.33105734637 1515852.0985516747 0, -120311.13087643796 1515854.3016815225 0, -120707.8534847224 1515856.5487732443 0)), ((-121423.27919263708 1521123.6379134287 0, -121418.10893474067 1521529.2408057053 0, -121826.29440331022 1521536.1366622106 0, -122224.86296199447 1521542.9015232115 0, -122220.13127017854 1521948.5342373766 0, -122215.45736674874 1522350.1908891867 0, -121815.89131574231 1522342.234943161 0, -121407.84184039342 1522334.1419623222 0, -121018.52061237377 1522336.06356573 0, -120620.82032566948 1522338.0399300922 0, -120223.12029071625 1522340.0462541622 0, -119814.56364879261 1522342.1186002165 0, -119821.43015230344 1521932.5722585346 0, -119828.23087917826 1521527.653247194 0, -119835.02279326417 1521122.7348988163 0, -119841.69247015512 1520725.1543634795 0, -120244.46853500957 1520723.1114406264 0, -120642.7226717468 1520721.1014950145 0, -121040.99494318612 1520719.1106676604 0, -121428.46142744238 1520717.1956556789 0, -121423.27919263708 1521123.6379134287 0)), ((-116471.45640800915 1506060.2624132033 0, -116594.54191503269 1506061.0267343943 0, -116882.40405810311 1506065.8006737737 0, -116889.51687631683 1506065.9232600555 0, -116885.6696075123 1506463.6173947568 0, -116881.76229939541 1506867.5384234276 0, -116467.95463077669 1506861.6245820164 0, -116469.72981176751 1506457.2484630274 0, -116071.6503314145 1506451.0002098747 0, -116073.25528882556 1506056.8939392562 0, -116189.72593021201 1506058.2336734035 0, -116335.80511972874 1506059.1296684262 0, -116354.05844230119 1506059.7179110707 0, -116388.71931142654 1506059.7486425918 0, -116471.45640800915 1506060.2624132033 0)), ((-120054.01589803868 1507323.6422674174 0, -120064.85478750731 1506918.5741732598 0, -120075.69404072672 1506513.5179867279 0, -120445.64522029008 1506516.708205814 0, -120442.1863253491 1506922.003984145 0, -120438.73599286917 1507327.3119527982 0, -120054.01589803868 1507323.6422674174 0)), ((-116068.32066701987 1507260.6183581767 0, -116066.55903039787 1507671.7629631455 0, -115668.82447392556 1507665.8735412485 0, -115285.09936666551 1507660.2167836893 0, -115288.32614014135 1507249.9890117033 0, -115291.51705574054 1506844.2990662323 0, -115672.01610032438 1506850.0344130418 0, -116069.98528544577 1506855.83690274 0, -116068.32066701987 1507260.6183581767 0)), ((-116846.39151474854 1510924.704217221 0, -116845.16462299743 1511324.9405872498 0, -116843.9271629774 1511729.7374744387 0, -116842.68046339208 1512134.5351659828 0, -116841.42182462315 1512545.260208008 0, -116426.63213803283 1512538.220543904 0, -116029.19096976993 1512531.4961158284 0, -115792.77013346601 1512527.5053387107 0, -115861.56410122562 1512116.4430048715 0, -115874.71515635849 1512039.5643073677 0, -115824.2898662478 1511712.8981180622 0, -115800.93082433454 1511561.5284411449 0, -115707.14755079916 1511430.8375939096 0, -115638.51462219845 1511394.1334878106 0, -115464.3698573541 1511301.0411959954 0, -115243.8402278692 1511181.561052207 0, -115245.96735315837 1510911.1889799149 0, -115642.91094529454 1510914.5070823168 0, -116041.67928666784 1510917.8690668375 0, -116440.43872641968 1510921.2497684301 0, -116846.39151474854 1510924.704217221 0)), ((-119984.91059292722 1511775.5321362126 0, -120374.48354121138 1511780.0335297228 0, -120366.82009955254 1512184.9886002117 0, -119977.45822824458 1512180.6582820406 0, -119984.91059292722 1511775.5321362126 0)), ((-116663.71292682382 1522325.186876025 0, -116273.24848322617 1522314.3152888955 0, -115877.1758424719 1522303.3061685655 0, -115480.91674428737 1522292.3131322623 0, -115079.40322824946 1522281.188541352 0, -115084.04238776764 1521866.3125016468 0, -115088.59057512072 1521460.6571707528 0, -115093.12967776295 1521055.013615643 0, -115097.57815085424 1520657.2685002252 0, -115500.7912924653 1520667.5419716476 0, -115899.46532991882 1520677.7273618353 0, -116298.12107991171 1520687.9203425033 0, -116694.44956562693 1520698.0774491972 0, -116687.05813663924 1521089.4854640688 0, -116679.37966499559 1521495.8478743378 0, -116671.701530671 1521902.1999256238 0, -116663.71292682382 1522325.186876025 0)), ((-111693.47827975018 1506791.7373515991 0, -111690.67166922861 1507196.837033738 0, -111291.84376854908 1507191.0281420343 0, -111295.02150904168 1506785.9000619962 0, -111298.19956011556 1506380.739163877 0, -110900.09626867746 1506374.880627077 0, -110526.69017948666 1506369.3524212283 0, -110531.69889082109 1505988.0124887344 0, -110903.36823473191 1505992.0725870694 0, -111301.12811380504 1505996.4363694172 0, -111698.88782772499 1506000.8188656422 0, -112110.03137877685 1506005.3643421577 0, -112109.39633769491 1506392.4092545758 0, -112108.73343015161 1506797.480731412 0, -111693.47827975018 1506791.7373515991 0)), ((-115294.70735200212 1506438.632235053 0, -115297.80474291745 1506044.632829943 0, -115298.11684014743 1506044.6370991848 0, -115507.43099867749 1506049.857698452 0, -115675.06780216953 1506050.369341692 0, -115673.57021314393 1506444.781974076 0, -115294.70735200212 1506438.632235053 0)), ((-110893.03322813392 1507185.238518913 0, -111291.84376854908 1507191.0281420343 0, -111288.49301764238 1507615.2455195594 0, -110889.2896443036 1507612.5313155309 0, -110510.39547663584 1507609.9780101487 0, -110516.04636656727 1507179.7414623227 0, -110893.03322813392 1507185.238518913 0)), ((-111687.6964802307 1507617.967321089 0, -111690.67166922861 1507196.837033738 0, -112108.07038293855 1507202.5305956076 0, -112107.38954065862 1507620.857122165 0, -111687.6964802307 1507617.967321089 0)), ((-115239.74303067155 1511703.0603429652 0, -115629.54393633179 1511709.641905785 0, -115635.44894134508 1511735.704398272 0, -115706.24141109285 1512047.9832236923 0, -115704.1622780216 1512113.4742729727 0, -115632.96689429639 1512112.1387424502 0, -115236.58908618204 1512104.6040311817 0, -115239.74303067155 1511703.0603429652 0)), ((-111914.36779684611 1520593.843441507 0, -111907.99874313743 1520996.2340475866 0, -111901.57447392131 1521402.1091506225 0, -111895.15037167615 1521807.9851056247 0, -111888.66682726864 1522217.659301615 0, -111493.40769582988 1522213.6686086245 0, -111095.11402961217 1522209.667588022 0, -110696.82028878036 1522205.6855196028 0, -110303.8783094667 1522201.780405798 0, -110307.50071021168 1521797.9286285667 0, -110311.14072355286 1521392.0498372915 0, -110314.78940902809 1520986.172076282 0, -110318.38811167254 1520584.764788481 0, -110720.25922364488 1520587.0278309209 0, -111118.56376665241 1520589.2843575063 0, -111516.86848876557 1520591.5486326523 0, -111914.36779684611 1520593.843441507 0)))</t>
+          <t>MULTIPOLYGON Z (((-1200949.4146035248 1986131.3865049854 0, -1201008.5640779603 1985729.7722811436 0, -1200614.5012370858 1985673.7686730388 0, -1200669.6533357725 1985271.2897667151 0, -1201066.493713974 1985328.1256063147 0, -1201124.4264467019 1984926.4579796004 0, -1201524.0432644722 1984984.1342984058 0, -1201587.8614740546 1984581.7502122638 0, -1201985.2307194718 1984639.351418582 0, -1202382.6020516898 1984696.9409601807 0, -1202323.2590749203 1985099.5400278254 0, -1202257.5025131584 1985498.7310964514 0, -1202191.7442448295 1985897.9311084636 0, -1201797.1904774976 1985841.8542835591 0, -1201402.6258149387 1985785.7841837544 0, -1201341.8535774376 1986187.0676920137 0, -1200949.4146035248 1986131.3865049854 0)), ((-1199313.8102938333 1988900.7280749313 0, -1198924.411766142 1988843.6943137369 0, -1198985.113375903 1988444.5957812008 0, -1199375.1571254837 1988503.367987584 0, -1199436.503853103 1988106.0068802263 0, -1199827.1983496007 1988166.547356416 0, -1199888.7259280758 1987770.6245739467 0, -1200280.5990791349 1987832.833716148 0, -1200343.3062871008 1987438.5702774525 0, -1200734.5698639639 1987496.4786489669 0, -1201125.8437221616 1987554.3869302985 0, -1201065.402010298 1987951.2005946347 0, -1200673.0051892675 1987892.0187706524 0, -1200611.4306241132 1988287.5563193974 0, -1200217.890172515 1988227.106117349 0, -1200154.5920585152 1988620.8540026043 0, -1199764.8849283112 1988562.1083989786 0, -1199702.5616101853 1988957.666862466 0, -1199313.8102938333 1988900.7280749313 0)), ((-1223143.436401538 1989881.719152336 0, -1223419.4352111868 1989923.7774424125 0, -1223535.9816394616 1989941.6531504765 0, -1223812.1357923334 1989983.7452325672 0, -1223928.5534829786 1990001.6100994176 0, -1224204.8433981768 1990043.7328470063 0, -1224139.843618964 1990444.944148744 0, -1224074.8536150574 1990846.1559898094 0, -1223683.6110876764 1990782.5072356572 0, -1223292.3787798015 1990718.858378817 0, -1222901.1371126957 1990655.2062944588 0, -1222509.8958780668 1990591.5525453805 0, -1222571.9559296 1990197.724306925 0, -1222634.015968297 1989803.8950855925 0, -1222750.8590300886 1989821.7987297545 0, -1223026.7220759718 1989863.826351641 0, -1223143.436401538 1989881.719152336 0)), ((-1222542.1489198531 1995514.436441026 0, -1222155.7781050908 1995451.2022305646 0, -1221769.4045387236 1995387.986314855 0, -1221836.504233702 1994990.4565124046 0, -1221903.6023083215 1994592.9356454306 0, -1222288.3583468322 1994653.879323529 0, -1222673.1116197156 1994714.8413128022 0, -1222607.6310736444 1995114.6344123706 0, -1222542.1489198531 1995514.436441026 0)), ((-1201659.4476120977 1996675.8534731867 0, -1201744.9832824129 1996662.408207222 0, -1201835.2855395805 1996648.2221966062 0, -1201868.6205855391 1996654.307126532 0, -1201949.4849365936 1996795.4842738025 0, -1202011.3662478626 1996779.085643789 0, -1202066.0289064448 1996803.4623602377 0, -1202124.5704391345 1996848.7081638963 0, -1202089.9396841028 1997077.5244327018 0, -1202028.971132923 1997475.37670198 0, -1201631.711433702 1997414.6150895464 0, -1201234.646459388 1997353.8929998917 0, -1201294.6483140206 1996954.8134063454 0, -1201354.0538059068 1996554.2472903777 0, -1201453.4910764284 1996191.6643473764 0, -1201859.681803924 1996257.7183014518 0, -1201751.6667690177 1996617.4994862182 0, -1201690.0623007054 1996607.5600724139 0, -1201513.1361385188 1996579.7178727558 0, -1201566.3729970062 1996664.9414722568 0, -1201659.4476120977 1996675.8534731867 0)), ((-1223783.3877977077 1996529.6031083053 0, -1223982.4632963662 1996557.8789112386 0, -1223921.3039287934 1996958.2968418167 0, -1223719.7676918844 1996928.9535949833 0, -1223783.3877977077 1996529.6031083053 0)), ((-1226224.4013266957 1997734.1563803519 0, -1226164.75220724 1998132.4426223265 0, -1225771.418804286 1998069.1362751452 0, -1225378.0858237073 1998005.8282160312 0, -1225438.9652518556 1997605.3160135497 0, -1225499.8510547597 1997204.762899866 0, -1225891.9505479299 1997270.3168557796 0, -1226284.0488838982 1997335.87908203 0, -1226224.4013266957 1997734.1563803519 0)), ((-1224011.6469405184 1999021.8959077331 0, -1224041.4676897498 1998825.9433438212 0, -1224072.6007326506 1998621.3173565797 0, -1224175.176919924 1998637.1867835436 0, -1224219.6011097645 1998644.061814488 0, -1224283.7478828828 1998243.9815083751 0, -1224133.5659189047 1998220.7293548975 0, -1224195.1988720312 1997819.1633783365 0, -1224591.4049895727 1997879.2452730516 0, -1224529.290479228 1998282.0122576081 0, -1224923.2498256515 1998344.1667091553 0, -1224862.1799927137 1998744.6054138567 0, -1225255.9658451523 1998806.658980719 0, -1225194.7237044915 1999206.9875076083 0, -1224801.1117659858 1999145.0331064777 0, -1224407.5100378783 1999083.0785490803 0, -1224011.6469405184 1999021.8959077331 0)), ((-1211938.199385719 1999251.9292097052 0, -1211708.2860837039 1999217.054850042 0, -1211739.7245894852 1999019.934832633 0, -1211793.9822809868 1998848.1292916932 0, -1211801.5882713445 1998824.0457813325 0, -1211761.4914027578 1998665.1450358173 0, -1211743.4844433214 1998593.7942208254 0, -1211723.6454804663 1998519.074035636 0, -1211697.5921301139 1998420.9349449435 0, -1211667.7705426493 1998416.1714279458 0, -1211671.6267437972 1998391.8670954371 0, -1211736.120784928 1997991.4536868574 0, -1211759.7685744949 1997995.016372625 0, -1212130.3548239018 1998054.7113660679 0, -1212361.1455087503 1998088.7947185356 0, -1212497.7644001434 1998267.784060639 0, -1212394.8303602547 1998910.8103656892 0, -1212002.221016313 1998851.4524695664 0, -1212001.4851433197 1998851.3451502009 0, -1211938.199385719 1999251.9292097052 0)), ((-1211625.379728793 2001256.687723491 0, -1211233.2807288296 2001198.2464947454 0, -1211295.7737314815 2000796.9178301052 0, -1211358.2666912023 2000395.5880874582 0, -1211750.2268920816 2000454.0680641413 0, -1212142.187544372 2000512.5463302468 0, -1212079.8317922114 2000913.847289778 0, -1212017.476001224 2001315.1471723234 0, -1211625.379728793 2001256.687723491 0)), ((-1239286.9752013446 2000957.7813093676 0, -1239233.9397241138 2001365.6879314126 0, -1238841.929181456 2001305.8821331554 0, -1238743.3460844427 2001290.8404238424 0, -1238796.4796279324 2000884.595153859 0, -1238503.2533085248 2000840.8426608983 0, -1238556.5909239606 2000435.589719444 0, -1238747.5856001636 2000463.4427302745 0, -1238718.9932655112 2000664.4696718368 0, -1238921.958696769 2000694.067133627 0, -1238948.3022853793 2000492.7225605128 0, -1239340.0026043046 2000549.8621019782 0, -1239731.709873227 2000607.021433765 0, -1239680.696164114 2001016.5496067496 0, -1239286.9752013446 2000957.7813093676 0)), ((-1199488.400481616 2003700.7845815797 0, -1199446.2541140798 2004018.886376972 0, -1199435.6734278726 2004097.0835830967 0, -1199392.7873951585 2004421.0149994013 0, -1199382.0074318317 2004493.476731145 0, -1199012.6275708398 2004434.6261367777 0, -1198616.147769523 2004371.3797959967 0, -1198219.6751145 2004308.1531906656 0, -1197823.19002622 2004244.9431902638 0, -1197880.7325412876 2003843.6001293233 0, -1197937.5119648324 2003442.6961403133 0, -1198332.0451085707 2003508.4350993743 0, -1198277.3532443237 2003908.3443222241 0, -1198673.963112886 2003973.0951545911 0, -1199070.5687549158 2004037.8741253703 0, -1199121.113285039 2003639.9691604427 0, -1199488.400481616 2003700.7845815797 0)), ((-1250198.876306713 2005962.3489113243 0, -1250590.909210174 2006023.710049164 0, -1250528.2781075302 2006423.9168497787 0, -1250921.141191029 2006485.7457691838 0, -1251314.0143797263 2006547.5745069631 0, -1251251.2997013847 2006947.9407636316 0, -1250858.469156953 2006886.026792026 0, -1250465.6389268648 2006824.1110779692 0, -1250073.1321132244 2006761.8669079489 0, -1249680.6158270082 2006699.6194389884 0, -1249617.6377757322 2007098.082292455 0, -1249221.292169128 2007037.8089200025 0, -1248824.9437029413 2006977.5537103121 0, -1248890.3705293871 2006577.723025546 0, -1248492.1883682916 2006515.8758622867 0, -1248094.006535081 2006454.0269105784 0, -1248159.4489725113 2006053.16543721 0, -1247761.2891187842 2005990.8071546177 0, -1247363.1198071872 2005928.445525758 0, -1247428.6104098717 2005526.538003521 0, -1247826.7580702042 2005589.4071762606 0, -1248224.906066516 2005652.2745642345 0, -1248623.0610138224 2005715.1616635385 0, -1249021.2065024893 2005778.0454177293 0, -1249414.0249507115 2005839.5165988407 0, -1249806.8437167546 2005900.9860418532 0, -1250198.876306713 2005962.3489113243 0)), ((-1247566.6694429861 2007195.5715515325 0, -1247630.3480796162 2006793.562503844 0, -1248028.555996695 2006854.8757994352 0, -1248426.751274466 2006916.2056816863 0, -1248824.9437029413 2006977.5537103121 0, -1248760.0966418097 2007379.7958559261 0, -1248362.2845145166 2007318.385699903 0, -1247964.4840919334 2007256.965347405 0, -1247566.6694429861 2007195.5715515325 0)), ((-1214884.9514026928 2011587.7699811428 0, -1214823.6887198512 2011988.554887671 0, -1214432.1813166821 2011931.952489681 0, -1214038.8685967259 2011871.3089509988 0, -1214100.2322876945 2011470.785835063 0, -1213707.0202478133 2011410.4633386673 0, -1213808.1304391075 2010762.22808278 0, -1214140.6939690532 2010810.974031074 0, -1214177.9683250245 2010911.4998709369 0, -1214475.6776406844 2010971.7266713823 0, -1214536.4578955977 2011112.1671980636 0, -1214529.8486618707 2011293.5120795213 0, -1214530.434687362 2011296.0075491248 0, -1214493.431810409 2011531.124937915 0, -1214884.9514026928 2011587.7699811428 0)), ((-1203414.773080094 2017818.9878087633 0, -1203021.3449131686 2017761.423441275 0, -1202627.9140480196 2017703.8772140818 0, -1202687.8143944452 2017300.7751719146 0, -1202746.846823229 2016900.4051773595 0, -1203141.0981948192 2016958.5215804302 0, -1203535.3370808254 2017016.654554963 0, -1203475.0921401458 2017416.7085512585 0, -1203414.773080094 2017818.9878087633 0)), ((-1229885.7531415808 2017938.892345719 0, -1230278.27186139 2017998.945235504 0, -1230670.7893786563 2018059.0063095205 0, -1230607.6603637964 2018455.4002416127 0, -1230544.5329900116 2018851.7831042658 0, -1230149.4687500696 2018791.2440430394 0, -1229754.4017251895 2018730.7231066062 0, -1229359.3303284014 2018670.2302620958 0, -1228965.276372797 2018609.9693858812 0, -1228571.2294262208 2018549.7282063698 0, -1228177.178109552 2018489.5151287275 0, -1227783.1142206467 2018429.3186240913 0, -1227852.942872487 2018036.5505560231 0, -1227922.7731155031 2017643.7714194034 0, -1228315.3855124349 2017702.5402665238 0, -1228708.0080880623 2017761.3088930578 0, -1229100.6212568304 2017820.0741747317 0, -1229493.2461895708 2017878.8292683167 0, -1229885.7531415808 2017938.892345719 0)), ((-1206105.5278482453 2018606.1810173478 0, -1205713.8515176112 2018553.733399309 0, -1205322.1610654704 2018501.312333519 0, -1205382.0702499007 2018099.805695467 0, -1205772.3526640234 2018152.7374070461 0, -1206162.6421304154 2018205.688848611 0, -1206552.9174745223 2018258.66685713 0, -1206497.211229256 2018658.6483505857 0, -1206105.5278482453 2018606.1810173478 0)), ((-1206272.1471640056 2020272.094377161 0, -1206319.771786443 2019860.462891817 0, -1205928.7723013028 2019814.0727765951 0, -1205995.245163187 2019409.7445033374 0, -1206390.0777057828 2019459.2916460761 0, -1206746.3742502234 2019504.7952211872 0, -1206687.703592044 2019904.6677672267 0, -1207082.5781711931 2019963.9683060655 0, -1207023.2084410943 2020364.5151582565 0, -1206628.6340526156 2020304.7104994433 0, -1206272.1471640056 2020272.094377161 0)), ((-1204575.983485033 2020844.4712396988 0, -1204182.154224872 2020786.848793847 0, -1203788.3026792211 2020729.241342847 0, -1203849.091208816 2020342.5179917072 0, -1203909.415305679 2019961.4732845365 0, -1204302.928527725 2020020.9987176163 0, -1204696.4390576784 2020080.5422823506 0, -1204637.0053456717 2020457.0897676328 0, -1204575.983485033 2020844.4712396988 0)), ((-1209332.818848822 2021125.1684327514 0, -1209272.771639584 2021530.6954869886 0, -1209213.2751222092 2021936.483071149 0, -1209154.272241546 2022338.985942864 0, -1208759.8565809361 2022277.5207135705 0, -1208818.5156753226 2021875.2288204296 0, -1208877.468430193 2021470.5911785201 0, -1208937.3975810385 2021065.4338153556 0, -1208997.3876847923 2020661.2150426162 0, -1209392.596071574 2020719.8219105892 0, -1209332.818848822 2021125.1684327514 0)), ((-1205302.2244544607 2021349.971451156 0, -1205242.567928354 2021749.6392183537 0, -1205178.4817013156 2022150.0696602145 0, -1204787.0127856692 2022091.9792527887 0, -1204848.2562035522 2021692.4437968323 0, -1204908.9907677753 2021294.9005438634 0, -1205302.2244544607 2021349.971451156 0)), ((-1232957.6495970143 2022111.1251855183 0, -1232957.7353560326 2022110.5869775526 0, -1233085.527546776 2021308.5850659579 0, -1233085.8372327816 2021306.6415261528 0, -1233371.2401876114 2021352.1115497453 0, -1233307.3027463725 2021754.1336854794 0, -1233243.3685518657 2022156.1347434698 0, -1232957.6495970143 2022111.1251855183 0)), ((-1203666.8994157643 2021513.3005405762 0, -1204060.6213631586 2021572.9930481655 0, -1203999.0077779 2021970.680419623 0, -1203938.3219586762 2022369.915049777 0, -1203543.2228862923 2022309.399046005 0, -1203605.0004523103 2021910.0631655224 0, -1203666.8994157643 2021513.3005405762 0)), ((-1240824.7997962106 2022116.7025246206 0, -1241216.3239648386 2022181.4804448355 0, -1241607.8551180388 2022246.2780687707 0, -1242000.8346198548 2022311.7543284777 0, -1242393.8211085119 2022377.250277791 0, -1242786.79499762 2022442.7627955063 0, -1243179.7758707441 2022508.2950022228 0, -1243570.5444152341 2022566.472135946 0, -1243961.319898175 2022624.6689802737 0, -1244352.090938294 2022682.893941753 0, -1244704.043135988 2022735.6987950618 0, -1245100.672702718 2022800.8936539893 0, -1245497.2994534615 2022866.106606608 0, -1245893.9315920607 2022931.3491798039 0, -1246290.5511192465 2022996.608286078 0, -1246688.3028421644 2023060.3697814473 0, -1246854.222548723 2023086.9641918603 0, -1247086.04194313 2023124.147799671 0, -1247483.7782132423 2023187.9439005193 0, -1247881.5198564983 2023251.769610707 0, -1248274.3760642011 2023317.2067196239 0, -1248667.2376472114 2023382.673481462 0, -1249060.0866059994 2023448.1568093183 0, -1249452.9441114145 2023513.649855215 0, -1249847.316838842 2023578.7078421412 0, -1250241.6965216782 2023643.7854998587 0, -1250636.0749527814 2023708.8713013076 0, -1251030.439164145 2023773.983621087 0, -1251420.8377171035 2023834.0475751222 0, -1251811.2447756436 2023894.1212700573 0, -1252201.6375792723 2023954.2215212677 0, -1252592.029092959 2024014.329953608 0, -1252985.8073247832 2024079.3396748095 0, -1253379.5745004576 2024144.3559842452 0, -1253773.3388244524 2024209.3904081208 0, -1254143.464578902 2024270.4652805342 0, -1254540.4336789472 2024330.5693503893 0, -1254480.561012865 2024733.1099419487 0, -1254420.6803270606 2025135.637883956 0, -1254816.070587661 2025195.8975025956 0, -1254755.42314183 2025598.4555184136 0, -1254694.7676744922 2026001.0008800384 0, -1255088.582258263 2026061.396129427 0, -1255482.3939579725 2026121.8094874748 0, -1255875.4416704772 2026186.391620376 0, -1256268.4767259322 2026250.9903073946 0, -1256661.508915793 2026315.607107215 0, -1256600.6694906123 2026716.9467298146 0, -1256993.89299775 2026782.4505437952 0, -1256933.229952671 2027184.6448551298 0, -1257324.2901272497 2027244.9481369173 0, -1257263.0153584753 2027646.8293020562 0, -1257653.4458903556 2027706.8056826259 0, -1257591.5413923927 2028108.3606214274 0, -1257525.2230301008 2028505.7883454151 0, -1257458.904829029 2028903.2149502914 0, -1257850.185653451 2028965.0621591632 0, -1258241.4651761076 2029026.91752068 0, -1258176.6170405287 2029426.4777840169 0, -1258111.7772884814 2029826.048442068 0, -1258047.1366058583 2030226.3240997333 0, -1258439.619044347 2030290.1063409834 0, -1258374.5898588668 2030690.7482105817 0, -1258309.5722330518 2031091.3805298947 0, -1258244.5481669626 2031491.9902132635 0, -1258180.9745911143 2031890.4893605306 0, -1257789.5470117969 2031825.7917771202 0, -1257397.058731641 2031763.089979814 0, -1257004.5707433224 2031700.386345697 0, -1256940.962613132 2032099.522656034 0, -1256548.5191066172 2032037.1001378882 0, -1256484.946862812 2032436.4453752316 0, -1256092.5330086597 2032374.2709517737 0, -1255700.510181279 2032314.1189771222 0, -1255308.4974309984 2032253.9667281853 0, -1255371.759463026 2031853.4377977676 0, -1254979.6008854692 2031792.8210392797 0, -1254587.4425973361 2031732.2024480815 0, -1254191.95264393 2031670.182949536 0, -1253796.4531999393 2031608.1600279238 0, -1253859.6203336667 2031207.246962477 0, -1253464.2134179117 2031145.5332332975 0, -1253068.8181858058 2031083.8092356243 0, -1253132.1585524387 2030683.5255467219 0, -1252768.9144148913 2030625.1608824118 0, -1252375.8307867476 2030562.0435614423 0, -1251983.2787089215 2030499.1827182607 0, -1251590.7221853412 2030436.3499428467 0, -1251193.902099216 2030371.5998309178 0, -1250797.0791710068 2030306.8677798829 0, -1250400.2518153617 2030242.1637567105 0, -1250003.4134142431 2030177.466268665 0, -1249607.731750929 2030113.1350200824 0, -1249212.0374554251 2030048.820284649 0, -1248816.3501153798 2029984.5251818541 0, -1248420.6501460623 2029920.2465926132 0, -1248026.4912020147 2029856.1910947484 0, -1247632.327835281 2029792.1636517057 0, -1247238.1632212957 2029728.1443303619 0, -1246843.9941874365 2029664.153064309 0, -1246452.892148137 2029596.1620961318 0, -1246061.7888863166 2029528.179277119 0, -1245670.67143612 2029460.2229808578 0, -1245279.5609720952 2029392.2863610035 0, -1244880.4399652374 2029333.035713487 0, -1244481.3047312102 2029273.811517816 0, -1244082.1764446825 2029214.6069278538 0, -1243683.0339338758 2029155.428789975 0, -1243339.3741954616 2029101.0827773253 0, -1242946.7681836765 2029039.0079999948 0, -1242555.324435895 2028977.0756579326 0, -1242163.8860647916 2028915.172960424 0, -1241770.1254374017 2028851.3960662757 0, -1241376.3831700536 2028787.6304226187 0, -1240984.2828058784 2028724.77858945 0, -1240592.181212203 2028661.9349018326 0, -1240200.7532791651 2028598.6448393282 0, -1239809.322533992 2028535.3728955484 0, -1239417.8873904916 2028472.1290372899 0, -1239026.4510252296 2028408.8933316357 0, -1239090.6484675815 2028005.5682271295 0, -1239154.8476013097 2027602.2319856184 0, -1239219.0468385175 2027198.894575455 0, -1239283.246178932 2026795.5559984501 0, -1239345.920694454 2026394.4770470175 0, -1239408.5969054077 2025993.3869810896 0, -1239471.2814289166 2025592.307296627 0, -1239533.9578545913 2025191.2149403521 0, -1239593.4783309621 2024791.9689913124 0, -1239652.9891357217 2024392.7203571005 0, -1239712.500061204 2023993.4706002155 0, -1239772.020899634 2023594.2212831436 0, -1239839.4509167261 2023192.4704520234 0, -1239906.8810148402 2022790.7184735409 0, -1239974.3096060858 2022388.97531649 0, -1240041.7398655603 2021987.221048717 0, -1240433.2712334564 2022051.952714843 0, -1240824.7997962106 2022116.7025246206 0), (-1248679.1504517798 2028318.3355548251 0, -1248281.1012414123 2028253.2007077434 0, -1247883.0409976325 2028188.072392038 0, -1247950.8550266984 2027790.3148147415 0, -1248018.6691689556 2027392.5561029816 0, -1247620.1990256833 2027328.9447225698 0, -1247221.739016179 2027265.3330268385 0, -1247154.3271923906 2027661.6227578027 0, -1247086.9170654146 2028057.9013955873 0, -1247026.186511067 2028459.4635404407 0, -1247423.2705223358 2028524.297168386 0, -1247820.3564682123 2028589.1189620579 0, -1248217.437998981 2028653.9687882473 0, -1248614.5296671642 2028718.8183060996 0, -1248549.9008149747 2029119.28838522 0, -1248944.6187334761 2029183.6659870485 0, -1249339.338575796 2029248.0317741423 0, -1249734.0587533587 2029312.3957129922 0, -1250128.7792645586 2029376.757803301 0, -1250191.4583207741 2028976.396093616 0, -1250254.137532732 2028576.0332437023 0, -1249860.397470757 2028511.5820652237 0, -1249466.644774831 2028447.147424419 0, -1249072.89903236 2028382.7324407294 0, -1248679.1504517798 2028318.3355548251 0), (-1248417.1298585548 2027456.164048192 0, -1248815.6006786304 2027519.7716774573 0, -1248883.826760444 2027120.4830428087 0, -1248952.0415787275 2026721.2016760434 0, -1248553.179836742 2026659.0546324335 0, -1248154.3120755805 2026596.9455808732 0, -1248086.4913593903 2026994.7464240948 0, -1248018.6691689556 2027392.5561029816 0, -1248417.1298585548 2027456.164048192 0)), ((-1205613.2579564946 2024675.5960363327 0, -1205675.5244646221 2024274.1660020929 0, -1206032.660344529 2024329.3412408892 0, -1206428.4227780085 2024389.8282359694 0, -1206370.059889674 2024791.7290923826 0, -1206311.8148573178 2025194.5265068624 0, -1205915.429507019 2025133.01981894 0, -1205553.0379621363 2025077.3519040926 0, -1205613.2579564946 2024675.5960363327 0)), ((-1210826.6896727383 2024644.9510114104 0, -1210766.8396209527 2025048.7023286093 0, -1210708.0706603783 2025452.7886553959 0, -1210652.5090646092 2025859.0519228405 0, -1210259.6466006862 2025799.2429971588 0, -1210315.3310209601 2025393.224340328 0, -1210373.7644687237 2024988.9823952538 0, -1210433.3022160495 2024585.559505433 0, -1210493.3687443314 2024183.793758386 0, -1210887.3913352073 2024243.2252126785 0, -1210826.6896727383 2024644.9510114104 0)), ((-1200231.0400632427 2025535.3340568452 0, -1200285.8945334961 2025124.8883061956 0, -1200680.5298244192 2025181.563982954 0, -1201074.9665822696 2025238.2264538677 0, -1201019.0329055046 2025649.0315278738 0, -1200625.0378307404 2025592.1737410005 0, -1200231.0400632427 2025535.3340568452 0)), ((-1321280.6173853083 2058083.5737533076 0, -1321664.5810077875 2058142.4762339485 0, -1322062.3611194459 2058210.5236693362 0, -1321995.9126071483 2058609.6128780514 0, -1321995.8019652606 2058610.2773933143 0, -1321599.448249967 2058543.876546212 0, -1321202.0510165088 2058477.2808153273 0, -1321280.6173853083 2058083.5737533076 0)), ((-1179105.2869066224 1888617.7273695231 0, -1179115.9710953655 1888616.9338675025 0, -1179055.91134986 1888996.7362096165 0, -1178665.555186845 1888942.4659631737 0, -1178602.9243309263 1888933.7580948023 0, -1178615.1686528765 1888924.7423638906 0, -1178628.521187138 1888912.6537212462 0, -1178668.8000334883 1888876.6469856459 0, -1178678.9045889655 1888867.7110062523 0, -1178680.0172958132 1888866.726883542 0, -1178726.2427016278 1888560.2434908405 0, -1179102.3208169893 1888617.9476949621 0, -1179105.2869066224 1888617.7273695231 0)), ((-1186874.038604841 1890491.4992944147 0, -1186872.9404039271 1890491.6713313425 0, -1186872.9499457758 1890491.6069984068 0, -1186874.038604841 1890491.4992944147 0)), ((-1187740.3863162966 1890499.7574263406 0, -1187748.0021001725 1890497.9372015141 0, -1187756.097569647 1890501.0593707971 0, -1187769.8049647976 1890517.7187150263 0, -1187735.7767808228 1890537.4623593946 0, -1187735.0307261655 1890521.9647945906 0, -1187736.0798005583 1890507.8447073444 0, -1187740.3863162966 1890499.7574263406 0)), ((-1186876.2157106234 1890491.1582433505 0, -1186886.8172234602 1890419.606674067 0, -1187725.3433674988 1890543.515976666 0, -1187690.2819010757 1890563.8591464516 0, -1187667.5501648362 1890568.6700683476 0, -1187429.897759995 1890618.9811750606 0, -1187382.6620204141 1890677.4576822075 0, -1187278.4854413432 1890612.248134321 0, -1187259.0582802685 1890605.7146222093 0, -1186904.8840154533 1890486.6672553835 0, -1186876.2157106234 1890491.1582433505 0)), ((-1188123.1064447055 1890600.9546276894 0, -1188128.0039866117 1890603.014600695 0, -1188138.3730090496 1890604.5467761555 0, -1188144.3265888842 1890601.825143622 0, -1188151.8937026053 1890596.8258572621 0, -1188174.7378867653 1890576.1840846913 0, -1188205.3639952096 1890556.6926516807 0, -1188230.8611510843 1890550.2649717983 0, -1188272.4515197284 1890561.8512074805 0, -1188298.2323615844 1890572.7998664386 0, -1188312.1030920038 1890581.8746381055 0, -1188315.9869673569 1890591.8521417447 0, -1188313.110770919 1890609.5541057098 0, -1188315.5454941096 1890630.726273488 0, -1188461.169951352 1890652.2442963165 0, -1188450.3049999387 1890725.5993665976 0, -1188421.50489671 1890726.4331994643 0, -1188378.9585863028 1890727.7680660281 0, -1188266.312074268 1890640.1686700091 0, -1188061.9755397409 1890626.546116768 0, -1187894.4421532732 1890615.3684420993 0, -1187830.581959661 1890559.0666487284 0, -1188068.9253935083 1890594.2850415143 0, -1188072.961564745 1890592.8631398568 0, -1188095.3008167378 1890590.840211846 0, -1188104.430743351 1890591.0567089948 0, -1188123.1064447055 1890600.9546276894 0)), ((-1194406.0165086838 1892277.5862176022 0, -1194465.4208935194 1891875.9678030992 0, -1194524.8234477565 1891474.3587166604 0, -1194918.1344180182 1891532.8403313872 0, -1195311.4329493698 1891591.3390325352 0, -1195704.7370191833 1891649.8679212425 0, -1196098.0400220633 1891708.4054882715 0, -1196038.6754803476 1892109.6026921868 0, -1195979.3091151244 1892510.8092263872 0, -1195919.94410731 1892912.0051446112 0, -1195860.587061192 1893313.2119541636 0, -1195467.2460356867 1893255.0862772418 0, -1195073.9039429305 1893196.9692714587 0, -1194680.5576036887 1893138.8808814313 0, -1194287.2183944033 1893080.812699648 0, -1194346.6216684908 1892679.2055507903 0, -1194406.0165086838 1892277.5862176022 0)), ((-1178359.9781860579 1893376.8770570161 0, -1178415.8113924572 1892979.0734418454 0, -1178471.6427189133 1892581.279152106 0, -1178527.4851311543 1892183.4758120168 0, -1178927.6116216248 1892242.5125736254 0, -1179327.7485048182 1892301.5495577876 0, -1179727.8698472194 1892360.6235194542 0, -1180127.990204148 1892419.7061092216 0, -1180516.993823687 1892535.830099272 0, -1180456.068967295 1892950.6668688487 0, -1180066.9659569485 1892838.8728355994 0, -1180005.9413891886 1893258.038840582 0, -1179944.9165011777 1893677.204122247 0, -1179883.9010774507 1894096.3702444974 0, -1179488.9723053728 1894015.9258636925 0, -1179094.0441929265 1893935.480196685 0, -1178699.0892185145 1893855.079970265 0, -1178304.1462819271 1893774.6700527072 0, -1178359.9781860579 1893376.8770570161 0)), ((-1190778.829093544 1895026.871992526 0, -1190839.760251897 1894625.2293031116 0, -1190900.7009389747 1894223.587514901 0, -1191295.2800924832 1894282.1221429226 0, -1191689.858199118 1894340.6654296252 0, -1192084.4320763815 1894399.2373190005 0, -1192479.0017228236 1894457.8378109236 0, -1192416.8089803848 1894859.2296450553 0, -1192354.6257699209 1895260.6223786166 0, -1192292.579050568 1895661.9749551334 0, -1192229.6659854073 1896068.94580703 0, -1191836.1569407692 1896011.2293614007 0, -1191442.6452515044 1895953.5315459068 0, -1191049.1407037235 1895895.8539255825 0, -1190655.623729621 1895838.1933708163 0, -1190717.8532868377 1895428.4148791246 0, -1190778.829093544 1895026.871992526 0)), ((-1195711.515713946 1896991.7734474617 0, -1195651.6267974805 1897393.2779463765 0, -1195591.7503743176 1897794.7020027523 0, -1195531.8753121055 1898196.1154197033 0, -1195137.8224340407 1898138.2517039974 0, -1195197.746987196 1897736.8465314081 0, -1195257.6713091212 1897335.4406911351 0, -1195317.5953995492 1896934.0341848754 0, -1195377.5290429997 1896532.6285788429 0, -1195771.4044003438 1896590.2682842822 0, -1195711.515713946 1896991.7734474617 0)), ((-1193082.5478134777 1901109.9753088155 0, -1193475.8960802914 1901170.3934988985 0, -1193415.7913449106 1901571.7017512866 0, -1193022.3988302003 1901511.3681873989 0, -1193082.5478134777 1901109.9753088155 0)), ((-1177752.4872717867 1903502.8787994755 0, -1177359.8021421588 1903441.4241137463 0, -1176967.1144337156 1903379.9880371129 0, -1177021.8245550608 1902987.4604622647 0, -1177076.5328122007 1902594.9421904658 0, -1177131.2521716019 1902202.414847007 0, -1177185.9696662202 1901809.8968097374 0, -1177577.428125001 1901876.44191709 0, -1177968.8758242452 1901942.994117986 0, -1178360.3193647412 1902009.5749209428 0, -1178751.771711725 1902076.1659491605 0, -1178698.2916188638 1902463.5864314684 0, -1178644.809676144 1902851.0162392645 0, -1178591.329066001 1903238.4354284331 0, -1178537.8481976374 1903625.853968784 0, -1178145.1698211322 1903564.3520941334 0, -1177752.4872717867 1903502.8787994755 0)), ((-1190908.3198422568 1904888.1385654486 0, -1190848.7425799756 1905289.809262526 0, -1190788.5411628187 1905695.7050735203 0, -1190395.0807721363 1905635.6361323004 0, -1190001.6177493844 1905575.5857850604 0, -1189608.1423110566 1905515.5524668305 0, -1189214.664243633 1905455.5377428497 0, -1189219.171575706 1905425.0182571036 0, -1189274.2901261137 1905051.8827897592 0, -1189667.9235759 1905111.3595901635 0, -1190061.5477913003 1905170.8334764433 0, -1190121.0204423175 1904769.1978609448 0, -1189727.318542925 1904709.7118929208 0, -1189333.6156033983 1904650.2345486004 0, -1189392.9622375325 1904248.6401592877 0, -1189452.308626869 1903847.0450700808 0, -1189481.2739230653 1903851.350970904 0, -1189846.1548405404 1903906.3707972832 0, -1190239.997073223 1903965.786488621 0, -1190633.8205257917 1904025.2590989687 0, -1191027.6413443335 1904084.7503066773 0, -1190967.981508196 1904486.4398003086 0, -1190908.3198422568 1904888.1385654486 0)), ((-1179945.6358764141 1905066.5924320498 0, -1179970.7189541813 1904895.560016338 0, -1180004.802821503 1904663.150277138 0, -1180029.770264339 1904493.847700341 0, -1180064.1989814092 1904260.4701743908 0, -1180089.0169855845 1904092.16599216 0, -1180463.5398180843 1904147.3500395033 0, -1180838.0486198857 1904202.5612151208 0, -1180878.008857196 1904208.4552150238 0, -1181212.5481627237 1904257.76960505 0, -1181272.4486707496 1904266.6091266726 0, -1181587.0532416308 1904313.0082548873 0, -1181666.8890657434 1904324.7616849826 0, -1181607.6338308388 1904726.5765007597 0, -1181548.3685356055 1905128.389039277 0, -1181489.1029650006 1905530.20086466 0, -1181429.8484950538 1905932.0035698146 0, -1181035.713326319 1905873.7449473573 0, -1180641.5755574198 1905815.5049099228 0, -1180247.435189834 1905757.2834576652 0, -1179853.2922250433 1905699.0805907263 0, -1179886.4784328507 1905470.0354333818 0, -1179911.8043482066 1905297.293543197 0, -1179945.6358764141 1905066.5924320498 0)), ((-1186223.0697855402 1906234.524458163 0, -1186281.9241700133 1905832.3458637698 0, -1186310.932549742 1905635.0445003845 0, -1186340.9403507034 1905430.3458742376 0, -1186399.8568370268 1905028.3394933036 0, -1186650.132388549 1905066.2523844785 0, -1186793.9930118804 1905088.0505190296 0, -1186980.189869192 1905116.2634695985 0, -1187188.126569116 1905147.7801355016 0, -1187310.2845728302 1905166.105655993 0, -1187640.4078231023 1905215.6446172167 0, -1187581.8276503226 1905617.3173266833 0, -1187545.3951083054 1905867.138556 0, -1187523.0010153102 1906018.9601683628 0, -1187464.6224085458 1906420.6228855937 0, -1187406.2435549675 1906822.2848942888 0, -1187112.8000172758 1906778.50026626 0, -1186952.5913249126 1906754.6289590811 0, -1186558.4045455763 1906695.6563583014 0, -1186164.2151470624 1906636.7023404115 0, -1186223.0697855402 1906234.524458163 0)), ((-1178469.7116424306 1906896.4162612902 0, -1178863.3891631283 1906952.1983750868 0, -1178802.8822249305 1907355.4621336507 0, -1178409.1200194932 1907299.0116164312 0, -1178469.7116424306 1906896.4162612902 0)), ((-1184852.3185068783 1948696.343759482 0, -1184911.3826322686 1948294.7235612997 0, -1185306.3286445949 1948353.1609087712 0, -1185701.2720399515 1948411.6166631556 0, -1186096.2030299772 1948470.0892582536 0, -1186491.139595801 1948528.5917956394 0, -1186431.7017706153 1948930.5624904055 0, -1186372.2637454076 1949332.5322974538 0, -1186312.8157335003 1949734.49964899 0, -1186253.3773090634 1950136.4676753902 0, -1185859.758994891 1950077.796469102 0, -1185466.1282724966 1950019.1421073962 0, -1185070.6222038823 1949960.1655721343 0, -1184675.103735667 1949901.2058671056 0, -1184734.1684757974 1949499.5883326414 0, -1184793.2443894309 1949097.9615052918 0, -1184852.3185068783 1948696.343759482 0)), ((-1181884.3401847018 1952349.62141396 0, -1181489.663253396 1952290.7109749934 0, -1181094.9837210989 1952231.818929109 0, -1181153.606980693 1951837.930128558 0, -1181213.7998061194 1951436.4704010205 0, -1181273.9826235292 1951035.008202347 0, -1181668.533676252 1951093.7457282406 0, -1182063.0805350034 1951152.511622226 0, -1182457.6345766736 1951211.2974813473 0, -1182852.1680303665 1951270.088636811 0, -1182792.2110123308 1951671.7928474464 0, -1182732.245585199 1952073.4846184973 0, -1182673.696025463 1952467.4990369854 0, -1182279.0145135478 1952408.550245857 0, -1181884.3401847018 1952349.62141396 0)), ((-1179515.3458221497 1951996.3120427965 0, -1179910.2526456257 1952055.1550170188 0, -1180305.1650700283 1952114.0279190429 0, -1180700.0764899934 1952172.9092436894 0, -1181094.9837210989 1952231.818929109 0, -1181035.5736542786 1952633.4635708747 0, -1180976.1535832637 1953035.105737911 0, -1180916.74467373 1953436.7385926174 0, -1</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Tonkawa</t>
+          <t>Uintah and Ouray</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>UT</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Public Building, Common Schools, Oklahoma State University, State Educational Institutions</t>
+          <t>Public Schools, Recreation Exchange, Multi-Beneficiary, College of Mines and Earth Sciences, UtahÔøΩStateÔøΩHospital, Reservoirs, UtahÔøΩSchools for the Deaf, University ofÔøΩUtah, UtahÔøΩStateÔøΩUniversity, Juvenile Justice Services, UtahÔøΩSchools for the Blind, Teaching Colleges at Public Universities, Public Buildings, Miners Hospital</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>subsurface, surface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>152</v>
+        <v>1463</v>
       </c>
       <c r="G70" t="n">
-        <v>186.91</v>
+        <v>230995.4</v>
       </c>
       <c r="H70" t="n">
-        <v>6</v>
+        <v>672</v>
       </c>
       <c r="I70" t="n">
-        <v>5810.78</v>
+        <v>280566.13</v>
       </c>
       <c r="J70" t="n">
-        <v>146</v>
+        <v>791</v>
       </c>
       <c r="K70" t="n">
-        <v>5997.69</v>
+        <v>511561.53</v>
       </c>
       <c r="L70" t="n">
-        <v>91880.64999999999</v>
+        <v>4504964.31</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1200949.4146035248 1986131.3865049854 0, -1201008.5640779603 1985729.7722811436 0, -1200614.5012370858 1985673.7686730388 0, -1200669.6533357725 1985271.2897667151 0, -1201066.493713974 1985328.1256063147 0, -1201124.4264467019 1984926.4579796004 0, -1201524.0432644722 1984984.1342984058 0, -1201587.8614740546 1984581.7502122638 0, -1201985.2307194718 1984639.351418582 0, -1202382.6020516898 1984696.9409601807 0, -1202323.2590749203 1985099.5400278254 0, -1202257.5025131584 1985498.7310964514 0, -1202191.7442448295 1985897.9311084636 0, -1201797.1904774976 1985841.8542835591 0, -1201402.6258149387 1985785.7841837544 0, -1201341.8535774376 1986187.0676920137 0, -1200949.4146035248 1986131.3865049854 0)), ((-1199313.8102938333 1988900.7280749313 0, -1198924.411766142 1988843.6943137369 0, -1198985.113375903 1988444.5957812008 0, -1199375.1571254837 1988503.367987584 0, -1199436.503853103 1988106.0068802263 0, -1199827.1983496007 1988166.547356416 0, -1199888.7259280758 1987770.6245739467 0, -1200280.5990791349 1987832.833716148 0, -1200343.3062871008 1987438.5702774525 0, -1200734.5698639639 1987496.4786489669 0, -1201125.8437221616 1987554.3869302985 0, -1201065.402010298 1987951.2005946347 0, -1200673.0051892675 1987892.0187706524 0, -1200611.4306241132 1988287.5563193974 0, -1200217.890172515 1988227.106117349 0, -1200154.5920585152 1988620.8540026043 0, -1199764.8849283112 1988562.1083989786 0, -1199702.5616101853 1988957.666862466 0, -1199313.8102938333 1988900.7280749313 0)), ((-1223143.436401538 1989881.719152336 0, -1223419.4352111868 1989923.7774424125 0, -1223535.9816394616 1989941.6531504765 0, -1223812.1357923334 1989983.7452325672 0, -1223928.5534829786 1990001.6100994176 0, -1224204.8433981768 1990043.7328470063 0, -1224139.843618964 1990444.944148744 0, -1224074.8536150574 1990846.1559898094 0, -1223683.6110876764 1990782.5072356572 0, -1223292.3787798015 1990718.858378817 0, -1222901.1371126957 1990655.2062944588 0, -1222509.8958780668 1990591.5525453805 0, -1222571.9559296 1990197.724306925 0, -1222634.015968297 1989803.8950855925 0, -1222750.8590300886 1989821.7987297545 0, -1223026.7220759718 1989863.826351641 0, -1223143.436401538 1989881.719152336 0)), ((-1222542.1489198531 1995514.436441026 0, -1222155.7781050908 1995451.2022305646 0, -1221769.4045387236 1995387.986314855 0, -1221836.504233702 1994990.4565124046 0, -1221903.6023083215 1994592.9356454306 0, -1222288.3583468322 1994653.879323529 0, -1222673.1116197156 1994714.8413128022 0, -1222607.6310736444 1995114.6344123706 0, -1222542.1489198531 1995514.436441026 0)), ((-1201659.4476120977 1996675.8534731867 0, -1201744.9832824129 1996662.408207222 0, -1201835.2855395805 1996648.2221966062 0, -1201868.6205855391 1996654.307126532 0, -1201949.4849365936 1996795.4842738025 0, -1202011.3662478626 1996779.085643789 0, -1202066.0289064448 1996803.4623602377 0, -1202124.5704391345 1996848.7081638963 0, -1202089.9396841028 1997077.5244327018 0, -1202028.971132923 1997475.37670198 0, -1201631.711433702 1997414.6150895464 0, -1201234.646459388 1997353.8929998917 0, -1201294.6483140206 1996954.8134063454 0, -1201354.0538059068 1996554.2472903777 0, -1201453.4910764284 1996191.6643473764 0, -1201859.681803924 1996257.7183014518 0, -1201751.6667690177 1996617.4994862182 0, -1201690.0623007054 1996607.5600724139 0, -1201513.1361385188 1996579.7178727558 0, -1201566.3729970062 1996664.9414722568 0, -1201659.4476120977 1996675.8534731867 0)), ((-1223783.3877977077 1996529.6031083053 0, -1223982.4632963662 1996557.8789112386 0, -1223921.3039287934 1996958.2968418167 0, -1223719.7676918844 1996928.9535949833 0, -1223783.3877977077 1996529.6031083053 0)), ((-1226224.4013266957 1997734.1563803519 0, -1226164.75220724 1998132.4426223265 0, -1225771.418804286 1998069.1362751452 0, -1225378.0858237073 1998005.8282160312 0, -1225438.9652518556 1997605.3160135497 0, -1225499.8510547597 1997204.762899866 0, -1225891.9505479299 1997270.3168557796 0, -1226284.0488838982 1997335.87908203 0, -1226224.4013266957 1997734.1563803519 0)), ((-1224011.6469405184 1999021.8959077331 0, -1224041.4676897498 1998825.9433438212 0, -1224072.6007326506 1998621.3173565797 0, -1224175.176919924 1998637.1867835436 0, -1224219.6011097645 1998644.061814488 0, -1224283.7478828828 1998243.9815083751 0, -1224133.5659189047 1998220.7293548975 0, -1224195.1988720312 1997819.1633783365 0, -1224591.4049895727 1997879.2452730516 0, -1224529.290479228 1998282.0122576081 0, -1224923.2498256515 1998344.1667091553 0, -1224862.1799927137 1998744.6054138567 0, -1225255.9658451523 1998806.658980719 0, -1225194.7237044915 1999206.9875076083 0, -1224801.1117659858 1999145.0331064777 0, -1224407.5100378783 1999083.0785490803 0, -1224011.6469405184 1999021.8959077331 0)), ((-1211938.199385719 1999251.9292097052 0, -1211708.2860837039 1999217.054850042 0, -1211739.7245894852 1999019.934832633 0, -1211793.9822809868 1998848.1292916932 0, -1211801.5882713445 1998824.0457813325 0, -1211761.4914027578 1998665.1450358173 0, -1211743.4844433214 1998593.7942208254 0, -1211723.6454804663 1998519.074035636 0, -1211697.5921301139 1998420.9349449435 0, -1211667.7705426493 1998416.1714279458 0, -1211671.6267437972 1998391.8670954371 0, -1211736.120784928 1997991.4536868574 0, -1211759.7685744949 1997995.016372625 0, -1212130.3548239018 1998054.7113660679 0, -1212361.1455087503 1998088.7947185356 0, -1212497.7644001434 1998267.784060639 0, -1212394.8303602547 1998910.8103656892 0, -1212002.221016313 1998851.4524695664 0, -1212001.4851433197 1998851.3451502009 0, -1211938.199385719 1999251.9292097052 0)), ((-1211625.379728793 2001256.687723491 0, -1211233.2807288296 2001198.2464947454 0, -1211295.7737314815 2000796.9178301052 0, -1211358.2666912023 2000395.5880874582 0, -1211750.2268920816 2000454.0680641413 0, -1212142.187544372 2000512.5463302468 0, -1212079.8317922114 2000913.847289778 0, -1212017.476001224 2001315.1471723234 0, -1211625.379728793 2001256.687723491 0)), ((-1239286.9752013446 2000957.7813093676 0, -1239233.9397241138 2001365.6879314126 0, -1238841.929181456 2001305.8821331554 0, -1238743.3460844427 2001290.8404238424 0, -1238796.4796279324 2000884.595153859 0, -1238503.2533085248 2000840.8426608983 0, -1238556.5909239606 2000435.589719444 0, -1238747.5856001636 2000463.4427302745 0, -1238718.9932655112 2000664.4696718368 0, -1238921.958696769 2000694.067133627 0, -1238948.3022853793 2000492.7225605128 0, -1239340.0026043046 2000549.8621019782 0, -1239731.709873227 2000607.021433765 0, -1239680.696164114 2001016.5496067496 0, -1239286.9752013446 2000957.7813093676 0)), ((-1199488.400481616 2003700.7845815797 0, -1199446.2541140798 2004018.886376972 0, -1199435.6734278726 2004097.0835830967 0, -1199392.7873951585 2004421.0149994013 0, -1199382.0074318317 2004493.476731145 0, -1199012.6275708398 2004434.6261367777 0, -1198616.147769523 2004371.3797959967 0, -1198219.6751145 2004308.1531906656 0, -1197823.19002622 2004244.9431902638 0, -1197880.7325412876 2003843.6001293233 0, -1197937.5119648324 2003442.6961403133 0, -1198332.0451085707 2003508.4350993743 0, -1198277.3532443237 2003908.3443222241 0, -1198673.963112886 2003973.0951545911 0, -1199070.5687549158 2004037.8741253703 0, -1199121.113285039 2003639.9691604427 0, -1199488.400481616 2003700.7845815797 0)), ((-1250198.876306713 2005962.3489113243 0, -1250590.909210174 2006023.710049164 0, -1250528.2781075302 2006423.9168497787 0, -1250921.141191029 2006485.7457691838 0, -1251314.0143797263 2006547.5745069631 0, -1251251.2997013847 2006947.9407636316 0, -1250858.469156953 2006886.026792026 0, -1250465.6389268648 2006824.1110779692 0, -1250073.1321132244 2006761.8669079489 0, -1249680.6158270082 2006699.6194389884 0, -1249617.6377757322 2007098.082292455 0, -1249221.292169128 2007037.8089200025 0, -1248824.9437029413 2006977.5537103121 0, -1248890.3705293871 2006577.723025546 0, -1248492.1883682916 2006515.8758622867 0, -1248094.006535081 2006454.0269105784 0, -1248159.4489725113 2006053.16543721 0, -1247761.2891187842 2005990.8071546177 0, -1247363.1198071872 2005928.445525758 0, -1247428.6104098717 2005526.538003521 0, -1247826.7580702042 2005589.4071762606 0, -1248224.906066516 2005652.2745642345 0, -1248623.0610138224 2005715.1616635385 0, -1249021.2065024893 2005778.0454177293 0, -1249414.0249507115 2005839.5165988407 0, -1249806.8437167546 2005900.9860418532 0, -1250198.876306713 2005962.3489113243 0)), ((-1247566.6694429861 2007195.5715515325 0, -1247630.3480796162 2006793.562503844 0, -1248028.555996695 2006854.8757994352 0, -1248426.751274466 2006916.2056816863 0, -1248824.9437029413 2006977.5537103121 0, -1248760.0966418097 2007379.7958559261 0, -1248362.2845145166 2007318.385699903 0, -1247964.4840919334 2007256.965347405 0, -1247566.6694429861 2007195.5715515325 0)), ((-1214884.9514026928 2011587.7699811428 0, -1214823.6887198512 2011988.554887671 0, -1214432.1813166821 2011931.952489681 0, -1214038.8685967259 2011871.3089509988 0, -1214100.2322876945 2011470.785835063 0, -1213707.0202478133 2011410.4633386673 0, -1213808.1304391075 2010762.22808278 0, -1214140.6939690532 2010810.974031074 0, -1214177.9683250245 2010911.4998709369 0, -1214475.6776406844 2010971.7266713823 0, -1214536.4578955977 2011112.1671980636 0, -1214529.8486618707 2011293.5120795213 0, -1214530.434687362 2011296.0075491248 0, -1214493.431810409 2011531.124937915 0, -1214884.9514026928 2011587.7699811428 0)), ((-1203414.773080094 2017818.9878087633 0, -1203021.3449131686 2017761.423441275 0, -1202627.9140480196 2017703.8772140818 0, -1202687.8143944452 2017300.7751719146 0, -1202746.846823229 2016900.4051773595 0, -1203141.0981948192 2016958.5215804302 0, -1203535.3370808254 2017016.654554963 0, -1203475.0921401458 2017416.7085512585 0, -1203414.773080094 2017818.9878087633 0)), ((-1229885.7531415808 2017938.892345719 0, -1230278.27186139 2017998.945235504 0, -1230670.7893786563 2018059.0063095205 0, -1230607.6603637964 2018455.4002416127 0, -1230544.5329900116 2018851.7831042658 0, -1230149.4687500696 2018791.2440430394 0, -1229754.4017251895 2018730.7231066062 0, -1229359.3303284014 2018670.2302620958 0, -1228965.276372797 2018609.9693858812 0, -1228571.2294262208 2018549.7282063698 0, -1228177.178109552 2018489.5151287275 0, -1227783.1142206467 2018429.3186240913 0, -1227852.942872487 2018036.5505560231 0, -1227922.7731155031 2017643.7714194034 0, -1228315.3855124349 2017702.5402665238 0, -1228708.0080880623 2017761.3088930578 0, -1229100.6212568304 2017820.0741747317 0, -1229493.2461895708 2017878.8292683167 0, -1229885.7531415808 2017938.892345719 0)), ((-1206105.5278482453 2018606.1810173478 0, -1205713.8515176112 2018553.733399309 0, -1205322.1610654704 2018501.312333519 0, -1205382.0702499007 2018099.805695467 0, -1205772.3526640234 2018152.7374070461 0, -1206162.6421304154 2018205.688848611 0, -1206552.9174745223 2018258.66685713 0, -1206497.211229256 2018658.6483505857 0, -1206105.5278482453 2018606.1810173478 0)), ((-1206272.1471640056 2020272.094377161 0, -1206319.771786443 2019860.462891817 0, -1205928.7723013028 2019814.0727765951 0, -1205995.245163187 2019409.7445033374 0, -1206390.0777057828 2019459.2916460761 0, -1206746.3742502234 2019504.7952211872 0, -1206687.703592044 2019904.6677672267 0, -1207082.5781711931 2019963.9683060655 0, -1207023.2084410943 2020364.5151582565 0, -1206628.6340526156 2020304.7104994433 0, -1206272.1471640056 2020272.094377161 0)), ((-1204575.983485033 2020844.4712396988 0, -1204182.154224872 2020786.848793847 0, -1203788.3026792211 2020729.241342847 0, -1203849.091208816 2020342.5179917072 0, -1203909.415305679 2019961.4732845365 0, -1204302.928527725 2020020.9987176163 0, -1204696.4390576784 2020080.5422823506 0, -1204637.0053456717 2020457.0897676328 0, -1204575.983485033 2020844.4712396988 0)), ((-1209332.818848822 2021125.1684327514 0, -1209272.771639584 2021530.6954869886 0, -1209213.2751222092 2021936.483071149 0, -1209154.272241546 2022338.985942864 0, -1208759.8565809361 2022277.5207135705 0, -1208818.5156753226 2021875.2288204296 0, -1208877.468430193 2021470.5911785201 0, -1208937.3975810385 2021065.4338153556 0, -1208997.3876847923 2020661.2150426162 0, -1209392.596071574 2020719.8219105892 0, -1209332.818848822 2021125.1684327514 0)), ((-1205302.2244544607 2021349.971451156 0, -1205242.567928354 2021749.6392183537 0, -1205178.4817013156 2022150.0696602145 0, -1204787.0127856692 2022091.9792527887 0, -1204848.2562035522 2021692.4437968323 0, -1204908.9907677753 2021294.9005438634 0, -1205302.2244544607 2021349.971451156 0)), ((-1232957.6495970143 2022111.1251855183 0, -1232957.7353560326 2022110.5869775526 0, -1233085.527546776 2021308.5850659579 0, -1233085.8372327816 2021306.6415261528 0, -1233371.2401876114 2021352.1115497453 0, -1233307.3027463725 2021754.1336854794 0, -1233243.3685518657 2022156.1347434698 0, -1232957.6495970143 2022111.1251855183 0)), ((-1203666.8994157643 2021513.3005405762 0, -1204060.6213631586 2021572.9930481655 0, -1203999.0077779 2021970.680419623 0, -1203938.3219586762 2022369.915049777 0, -1203543.2228862923 2022309.399046005 0, -1203605.0004523103 2021910.0631655224 0, -1203666.8994157643 2021513.3005405762 0)), ((-1240824.7997962106 2022116.7025246206 0, -1241216.3239648386 2022181.4804448355 0, -1241607.8551180388 2022246.2780687707 0, -1242000.8346198548 2022311.7543284777 0, -1242393.8211085119 2022377.250277791 0, -1242786.79499762 2022442.7627955063 0, -1243179.7758707441 2022508.2950022228 0, -1243570.5444152341 2022566.472135946 0, -1243961.319898175 2022624.6689802737 0, -1244352.090938294 2022682.893941753 0, -1244704.043135988 2022735.6987950618 0, -1245100.672702718 2022800.8936539893 0, -1245497.2994534615 2022866.106606608 0, -1245893.9315920607 2022931.3491798039 0, -1246290.5511192465 2022996.608286078 0, -1246688.3028421644 2023060.3697814473 0, -1246854.222548723 2023086.9641918603 0, -1247086.04194313 2023124.147799671 0, -1247483.7782132423 2023187.9439005193 0, -1247881.5198564983 2023251.769610707 0, -1248274.3760642011 2023317.2067196239 0, -1248667.2376472114 2023382.673481462 0, -1249060.0866059994 2023448.1568093183 0, -1249452.9441114145 2023513.649855215 0, -1249847.316838842 2023578.7078421412 0, -1250241.6965216782 2023643.7854998587 0, -1250636.0749527814 2023708.8713013076 0, -1251030.439164145 2023773.983621087 0, -1251420.8377171035 2023834.0475751222 0, -1251811.2447756436 2023894.1212700573 0, -1252201.6375792723 2023954.2215212677 0, -1252592.029092959 2024014.329953608 0, -1252985.8073247832 2024079.3396748095 0, -1253379.5745004576 2024144.3559842452 0, -1253773.3388244524 2024209.3904081208 0, -1254143.464578902 2024270.4652805342 0, -1254540.4336789472 2024330.5693503893 0, -1254480.561012865 2024733.1099419487 0, -1254420.6803270606 2025135.637883956 0, -1254816.070587661 2025195.8975025956 0, -1254755.42314183 2025598.4555184136 0, -1254694.7676744922 2026001.0008800384 0, -1255088.582258263 2026061.396129427 0, -1255482.3939579725 2026121.8094874748 0, -1255875.4416704772 2026186.391620376 0, -1256268.4767259322 2026250.9903073946 0, -1256661.508915793 2026315.607107215 0, -1256600.6694906123 2026716.9467298146 0, -1256993.89299775 2026782.4505437952 0, -1256933.229952671 2027184.6448551298 0, -1257324.2901272497 2027244.9481369173 0, -1257263.0153584753 2027646.8293020562 0, -1257653.4458903556 2027706.8056826259 0, -1257591.5413923927 2028108.3606214274 0, -1257525.2230301008 2028505.7883454151 0, -1257458.904829029 2028903.2149502914 0, -1257850.185653451 2028965.0621591632 0, -1258241.4651761076 2029026.91752068 0, -1258176.6170405287 2029426.4777840169 0, -1258111.7772884814 2029826.048442068 0, -1258047.1366058583 2030226.3240997333 0, -1258439.619044347 2030290.1063409834 0, -1258374.5898588668 2030690.7482105817 0, -1258309.5722330518 2031091.3805298947 0, -1258244.5481669626 2031491.9902132635 0, -1258180.9745911143 2031890.4893605306 0, -1257789.5470117969 2031825.7917771202 0, -1257397.058731641 2031763.089979814 0, -1257004.5707433224 2031700.386345697 0, -1256940.962613132 2032099.522656034 0, -1256548.5191066172 2032037.1001378882 0, -1256484.946862812 2032436.4453752316 0, -1256092.5330086597 2032374.2709517737 0, -1255700.510181279 2032314.1189771222 0, -1255308.4974309984 2032253.9667281853 0, -1255371.759463026 2031853.4377977676 0, -1254979.6008854692 2031792.8210392797 0, -1254587.4425973361 2031732.2024480815 0, -1254191.95264393 2031670.182949536 0, -1253796.4531999393 2031608.1600279238 0, -1253859.6203336667 2031207.246962477 0, -1253464.2134179117 2031145.5332332975 0, -1253068.8181858058 2031083.8092356243 0, -1253132.1585524387 2030683.5255467219 0, -1252768.9144148913 2030625.1608824118 0, -1252375.8307867476 2030562.0435614423 0, -1251983.2787089215 2030499.1827182607 0, -1251590.7221853412 2030436.3499428467 0, -1251193.902099216 2030371.5998309178 0, -1250797.0791710068 2030306.8677798829 0, -1250400.2518153617 2030242.1637567105 0, -1250003.4134142431 2030177.466268665 0, -1249607.731750929 2030113.1350200824 0, -1249212.0374554251 2030048.820284649 0, -1248816.3501153798 2029984.5251818541 0, -1248420.6501460623 2029920.2465926132 0, -1248026.4912020147 2029856.1910947484 0, -1247632.327835281 2029792.1636517057 0, -1247238.1632212957 2029728.1443303619 0, -1246843.9941874365 2029664.153064309 0, -1246452.892148137 2029596.1620961318 0, -1246061.7888863166 2029528.179277119 0, -1245670.67143612 2029460.2229808578 0, -1245279.5609720952 2029392.2863610035 0, -1244880.4399652374 2029333.035713487 0, -1244481.3047312102 2029273.811517816 0, -1244082.1764446825 2029214.6069278538 0, -1243683.0339338758 2029155.428789975 0, -1243339.3741954616 2029101.0827773253 0, -1242946.7681836765 2029039.0079999948 0, -1242555.324435895 2028977.0756579326 0, -1242163.8860647916 2028915.172960424 0, -1241770.1254374017 2028851.3960662757 0, -1241376.3831700536 2028787.6304226187 0, -1240984.2828058784 2028724.77858945 0, -1240592.181212203 2028661.9349018326 0, -1240200.7532791651 2028598.6448393282 0, -1239809.322533992 2028535.3728955484 0, -1239417.8873904916 2028472.1290372899 0, -1239026.4510252296 2028408.8933316357 0, -1239090.6484675815 2028005.5682271295 0, -1239154.8476013097 2027602.2319856184 0, -1239219.0468385175 2027198.894575455 0, -1239283.246178932 2026795.5559984501 0, -1239345.920694454 2026394.4770470175 0, -1239408.5969054077 2025993.3869810896 0, -1239471.2814289166 2025592.307296627 0, -1239533.9578545913 2025191.2149403521 0, -1239593.4783309621 2024791.9689913124 0, -1239652.9891357217 2024392.7203571005 0, -1239712.500061204 2023993.4706002155 0, -1239772.020899634 2023594.2212831436 0, -1239839.4509167261 2023192.4704520234 0, -1239906.8810148402 2022790.7184735409 0, -1239974.3096060858 2022388.97531649 0, -1240041.7398655603 2021987.221048717 0, -1240433.2712334564 2022051.952714843 0, -1240824.7997962106 2022116.7025246206 0), (-1248679.1504517798 2028318.3355548251 0, -1248281.1012414123 2028253.2007077434 0, -1247883.0409976325 2028188.072392038 0, -1247950.8550266984 2027790.3148147415 0, -1248018.6691689556 2027392.5561029816 0, -1247620.1990256833 2027328.9447225698 0, -1247221.739016179 2027265.3330268385 0, -1247154.3271923906 2027661.6227578027 0, -1247086.9170654146 2028057.9013955873 0, -1247026.186511067 2028459.4635404407 0, -1247423.2705223358 2028524.297168386 0, -1247820.3564682123 2028589.1189620579 0, -1248217.437998981 2028653.9687882473 0, -1248614.5296671642 2028718.8183060996 0, -1248549.9008149747 2029119.28838522 0, -1248944.6187334761 2029183.6659870485 0, -1249339.338575796 2029248.0317741423 0, -1249734.0587533587 2029312.3957129922 0, -1250128.7792645586 2029376.757803301 0, -1250191.4583207741 2028976.396093616 0, -1250254.137532732 2028576.0332437023 0, -1249860.397470757 2028511.5820652237 0, -1249466.644774831 2028447.147424419 0, -1249072.89903236 2028382.7324407294 0, -1248679.1504517798 2028318.3355548251 0), (-1248417.1298585548 2027456.164048192 0, -1248815.6006786304 2027519.7716774573 0, -1248883.826760444 2027120.4830428087 0, -1248952.0415787275 2026721.2016760434 0, -1248553.179836742 2026659.0546324335 0, -1248154.3120755805 2026596.9455808732 0, -1248086.4913593903 2026994.7464240948 0, -1248018.6691689556 2027392.5561029816 0, -1248417.1298585548 2027456.164048192 0)), ((-1205613.2579564946 2024675.5960363327 0, -1205675.5244646221 2024274.1660020929 0, -1206032.660344529 2024329.3412408892 0, -1206428.4227780085 2024389.8282359694 0, -1206370.059889674 2024791.7290923826 0, -1206311.8148573178 2025194.5265068624 0, -1205915.429507019 2025133.01981894 0, -1205553.0379621363 2025077.3519040926 0, -1205613.2579564946 2024675.5960363327 0)), ((-1210826.6896727383 2024644.9510114104 0, -1210766.8396209527 2025048.7023286093 0, -1210708.0706603783 2025452.7886553959 0, -1210652.5090646092 2025859.0519228405 0, -1210259.6466006862 2025799.2429971588 0, -1210315.3310209601 2025393.224340328 0, -1210373.7644687237 2024988.9823952538 0, -1210433.3022160495 2024585.559505433 0, -1210493.3687443314 2024183.793758386 0, -1210887.3913352073 2024243.2252126785 0, -1210826.6896727383 2024644.9510114104 0)), ((-1200231.0400632427 2025535.3340568452 0, -1200285.8945334961 2025124.8883061956 0, -1200680.5298244192 2025181.563982954 0, -1201074.9665822696 2025238.2264538677 0, -1201019.0329055046 2025649.0315278738 0, -1200625.0378307404 2025592.1737410005 0, -1200231.0400632427 2025535.3340568452 0)), ((-1321280.6173853083 2058083.5737533076 0, -1321664.5810077875 2058142.4762339485 0, -1322062.3611194459 2058210.5236693362 0, -1321995.9126071483 2058609.6128780514 0, -1321995.8019652606 2058610.2773933143 0, -1321599.448249967 2058543.876546212 0, -1321202.0510165088 2058477.2808153273 0, -1321280.6173853083 2058083.5737533076 0)), ((-1179105.2869066224 1888617.7273695231 0, -1179115.9710953655 1888616.9338675025 0, -1179055.91134986 1888996.7362096165 0, -1178665.555186845 1888942.4659631737 0, -1178602.9243309263 1888933.7580948023 0, -1178615.1686528765 1888924.7423638906 0, -1178628.521187138 1888912.6537212462 0, -1178668.8000334883 1888876.6469856459 0, -1178678.9045889655 1888867.7110062523 0, -1178680.0172958132 1888866.726883542 0, -1178726.2427016278 1888560.2434908405 0, -1179102.3208169893 1888617.9476949621 0, -1179105.2869066224 1888617.7273695231 0)), ((-1186872.9404039271 1890491.6713313425 0, -1186872.9499457758 1890491.6069984068 0, -1186874.038604841 1890491.4992944147 0, -1186872.9404039271 1890491.6713313425 0)), ((-1187740.3863162966 1890499.7574263406 0, -1187748.0021001725 1890497.9372015141 0, -1187756.097569647 1890501.0593707971 0, -1187769.8049647976 1890517.7187150263 0, -1187735.7767808228 1890537.4623593946 0, -1187735.0307261655 1890521.9647945906 0, -1187736.0798005583 1890507.8447073444 0, -1187740.3863162966 1890499.7574263406 0)), ((-1187667.5501648362 1890568.6700683476 0, -1187429.897759995 1890618.9811750606 0, -1187382.6620204141 1890677.4576822075 0, -1187278.4854413432 1890612.248134321 0, -1187259.0582802685 1890605.7146222093 0, -1186904.8840154533 1890486.6672553835 0, -1186876.2157106234 1890491.1582433505 0, -1186886.8172234602 1890419.606674067 0, -1187725.3433674988 1890543.515976666 0, -1187690.2819010757 1890563.8591464516 0, -1187667.5501648362 1890568.6700683476 0)), ((-1188123.1064447055 1890600.9546276894 0, -1188128.0039866117 1890603.014600695 0, -1188138.3730090496 1890604.5467761555 0, -1188144.3265888842 1890601.825143622 0, -1188151.8937026053 1890596.8258572621 0, -1188174.7378867653 1890576.1840846913 0, -1188205.3639952096 1890556.6926516807 0, -1188230.8611510843 1890550.2649717983 0, -1188272.4515197284 1890561.8512074805 0, -1188298.2323615844 1890572.7998664386 0, -1188312.1030920038 1890581.8746381055 0, -1188315.9869673569 1890591.8521417447 0, -1188313.110770919 1890609.5541057098 0, -1188315.5454941096 1890630.726273488 0, -1188461.169951352 1890652.2442963165 0, -1188450.3049999387 1890725.5993665976 0, -1188421.50489671 1890726.4331994643 0, -1188378.9585863028 1890727.7680660281 0, -1188266.312074268 1890640.1686700091 0, -1188061.9755397409 1890626.546116768 0, -1187894.4421532732 1890615.3684420993 0, -1187830.581959661 1890559.0666487284 0, -1188068.9253935083 1890594.2850415143 0, -1188072.961564745 1890592.8631398568 0, -1188095.3008167378 1890590.840211846 0, -1188104.430743351 1890591.0567089948 0, -1188123.1064447055 1890600.9546276894 0)), ((-1194406.0165086838 1892277.5862176022 0, -1194465.4208935194 1891875.9678030992 0, -1194524.8234477565 1891474.3587166604 0, -1194918.1344180182 1891532.8403313872 0, -1195311.4329493698 1891591.3390325352 0, -1195704.7370191833 1891649.8679212425 0, -1196098.0400220633 1891708.4054882715 0, -1196038.6754803476 1892109.6026921868 0, -1195979.3091151244 1892510.8092263872 0, -1195919.94410731 1892912.0051446112 0, -1195860.587061192 1893313.2119541636 0, -1195467.2460356867 1893255.0862772418 0, -1195073.9039429305 1893196.9692714587 0, -1194680.5576036887 1893138.8808814313 0, -1194287.2183944033 1893080.812699648 0, -1194346.6216684908 1892679.2055507903 0, -1194406.0165086838 1892277.5862176022 0)), ((-1178359.9781860579 1893376.8770570161 0, -1178415.8113924572 1892979.0734418454 0, -1178471.6427189133 1892581.279152106 0, -1178527.4851311543 1892183.4758120168 0, -1178927.6116216248 1892242.5125736254 0, -1179327.7485048182 1892301.5495577876 0, -1179727.8698472194 1892360.6235194542 0, -1180127.990204148 1892419.7061092216 0, -1180516.993823687 1892535.830099272 0, -1180456.068967295 1892950.6668688487 0, -1180066.9659569485 1892838.8728355994 0, -1180005.9413891886 1893258.038840582 0, -1179944.9165011777 1893677.204122247 0, -1179883.9010774507 1894096.3702444974 0, -1179488.9723053728 1894015.9258636925 0, -1179094.0441929265 1893935.480196685 0, -1178699.0892185145 1893855.079970265 0, -1178304.1462819271 1893774.6700527072 0, -1178359.9781860579 1893376.8770570161 0)), ((-1190778.829093544 1895026.871992526 0, -1190839.760251897 1894625.2293031116 0, -1190900.7009389747 1894223.587514901 0, -1191295.2800924832 1894282.1221429226 0, -1191689.858199118 1894340.6654296252 0, -1192084.4320763815 1894399.2373190005 0, -1192479.0017228236 1894457.8378109236 0, -1192416.8089803848 1894859.2296450553 0, -1192354.6257699209 1895260.6223786166 0, -1192292.579050568 1895661.9749551334 0, -1192229.6659854073 1896068.94580703 0, -1191836.1569407692 1896011.2293614007 0, -1191442.6452515044 1895953.5315459068 0, -1191049.1407037235 1895895.8539255825 0, -1190655.623729621 1895838.1933708163 0, -1190717.8532868377 1895428.4148791246 0, -1190778.829093544 1895026.871992526 0)), ((-1195711.515713946 1896991.7734474617 0, -1195651.6267974805 1897393.2779463765 0, -1195591.7503743176 1897794.7020027523 0, -1195531.8753121055 1898196.1154197033 0, -1195137.8224340407 1898138.2517039974 0, -1195197.746987196 1897736.8465314081 0, -1195257.6713091212 1897335.4406911351 0, -1195317.5953995492 1896934.0341848754 0, -1195377.5290429997 1896532.6285788429 0, -1195771.4044003438 1896590.2682842822 0, -1195711.515713946 1896991.7734474617 0)), ((-1193082.5478134777 1901109.9753088155 0, -1193475.8960802914 1901170.3934988985 0, -1193415.7913449106 1901571.7017512866 0, -1193022.3988302003 1901511.3681873989 0, -1193082.5478134777 1901109.9753088155 0)), ((-1177752.4872717867 1903502.8787994755 0, -1177359.8021421588 1903441.4241137463 0, -1176967.1144337156 1903379.9880371129 0, -1177021.8245550608 1902987.4604622647 0, -1177076.5328122007 1902594.9421904658 0, -1177131.2521716019 1902202.414847007 0, -1177185.9696662202 1901809.8968097374 0, -1177577.428125001 1901876.44191709 0, -1177968.8758242452 1901942.994117986 0, -1178360.3193647412 1902009.5749209428 0, -1178751.771711725 1902076.1659491605 0, -1178698.2916188638 1902463.5864314684 0, -1178644.809676144 1902851.0162392645 0, -1178591.329066001 1903238.4354284331 0, -1178537.8481976374 1903625.853968784 0, -1178145.1698211322 1903564.3520941334 0, -1177752.4872717867 1903502.8787994755 0)), ((-1190908.3198422568 1904888.1385654486 0, -1190848.7425799756 1905289.809262526 0, -1190788.5411628187 1905695.7050735203 0, -1190395.0807721363 1905635.6361323004 0, -1190001.6177493844 1905575.5857850604 0, -1189608.1423110566 1905515.5524668305 0, -1189214.664243633 1905455.5377428497 0, -1189219.171575706 1905425.0182571036 0, -1189274.2901261137 1905051.8827897592 0, -1189667.9235759 1905111.3595901635 0, -1190061.5477913003 1905170.8334764433 0, -1190121.0204423175 1904769.1978609448 0, -1189727.318542925 1904709.7118929208 0, -1189333.6156033983 1904650.2345486004 0, -1189392.9622375325 1904248.6401592877 0, -1189452.308626869 1903847.0450700808 0, -1189481.2739230653 1903851.350970904 0, -1189846.1548405404 1903906.3707972832 0, -1190239.997073223 1903965.786488621 0, -1190633.8205257917 1904025.2590989687 0, -1191027.6413443335 1904084.7503066773 0, -1190967.981508196 1904486.4398003086 0, -1190908.3198422568 1904888.1385654486 0)), ((-1179945.6358764141 1905066.5924320498 0, -1179970.7189541813 1904895.560016338 0, -1180004.802821503 1904663.150277138 0, -1180029.770264339 1904493.847700341 0, -1180064.1989814092 1904260.4701743908 0, -1180089.0169855845 1904092.16599216 0, -1180463.5398180843 1904147.3500395033 0, -1180838.0486198857 1904202.5612151208 0, -1180878.008857196 1904208.4552150238 0, -1181212.5481627237 1904257.76960505 0, -1181272.4486707496 1904266.6091266726 0, -1181587.0532416308 1904313.0082548873 0, -1181666.8890657434 1904324.7616849826 0, -1181607.6338308388 1904726.5765007597 0, -1181548.3685356055 1905128.389039277 0, -1181489.1029650006 1905530.20086466 0, -1181429.8484950538 1905932.0035698146 0, -1181035.713326319 1905873.7449473573 0, -1180641.5755574198 1905815.5049099228 0, -1180247.435189834 1905757.2834576652 0, -1179853.2922250433 1905699.0805907263 0, -1179886.4784328507 1905470.0354333818 0, -1179911.8043482066 1905297.293543197 0, -1179945.6358764141 1905066.5924320498 0)), ((-1186223.0697855402 1906234.524458163 0, -1186281.9241700133 1905832.3458637698 0, -1186310.932549742 1905635.0445003845 0, -1186340.9403507034 1905430.3458742376 0, -1186399.8568370268 1905028.3394933036 0, -1186650.132388549 1905066.2523844785 0, -1186793.9930118804 1905088.0505190296 0, -1186980.189869192 1905116.2634695985 0, -1187188.126569116 1905147.7801355016 0, -1187310.2845728302 1905166.105655993 0, -1187640.4078231023 1905215.6446172167 0, -1187581.8276503226 1905617.3173266833 0, -1187545.3951083054 1905867.138556 0, -1187523.0010153102 1906018.9601683628 0, -1187464.6224085458 1906420.6228855937 0, -1187406.2435549675 1906822.2848942888 0, -1187112.8000172758 1906778.50026626 0, -1186952.5913249126 1906754.6289590811 0, -1186558.4045455763 1906695.6563583014 0, -1186164.2151470624 1906636.7023404115 0, -1186223.0697855402 1906234.524458163 0)), ((-1178469.7116424306 1906896.4162612902 0, -1178863.3891631283 1906952.1983750868 0, -1178802.8822249305 1907355.4621336507 0, -1178409.1200194932 1907299.0116164312 0, -1178469.7116424306 1906896.4162612902 0)), ((-1184852.3185068783 1948696.343759482 0, -1184911.3826322686 1948294.7235612997 0, -1185306.3286445949 1948353.1609087712 0, -1185701.2720399515 1948411.6166631556 0, -1186096.2030299772 1948470.0892582536 0, -1186491.139595801 1948528.5917956394 0, -1186431.7017706153 1948930.5624904055 0, -1186372.2637454076 1949332.5322974538 0, -1186312.8157335003 1949734.49964899 0, -1186253.3773090634 1950136.4676753902 0, -1185859.758994891 1950077.796469102 0, -1185466.1282724966 1950019.1421073962 0, -1185070.6222038823 1949960.1655721343 0, -1184675.103735667 1949901.2058671056 0, -1184734.1684757974 1949499.5883326414 0, -1184793.2443894309 1949097.9615052918 0, -1184852.3185068783 1948696.343759482 0)), ((-1181884.3401847018 1952349.62141396 0, -1181489.663253396 1952290.7109749934 0, -1181094.9837210989 1952231.818929109 0, -1181153.606980693 1951837.930128558 0, -1181213.7998061194 1951436.4704010205 0, -1181273.9826235292 1951035.008202347 0, -1181668.533676252 1951093.7457282406 0, -1182063.0805350034 1951152.511622226 0, -1182457.6345766736 1951211.2974813473 0, -1182852.1680303665 1951270.088636811 0, -1182792.2110123308 1951671.7928474464 0, -1182732.245585199 1952073.4846184973 0, -1182673.696025463 1952467.4990369854 0, -1182279.0145135478 1952408.550245857 0, -1181884.3401847018 1952349.62141396 0)), ((-1179456.0682277712 1952398.0480524653 0, -1179515.3458221497 1951996.3120427965 0, -1179910.2526456257 1952055.1550170188 0, -1180305.1650700283 1952114.0279190429 0, -1180700.0764899934 1952172.9092436894 0, -1181094.9837210989 1952231.818929109 0, -1181035.5736542786 1952633.4635708747 0, -1180976.1535832637 1953035.105737911 0,</t>
+          <t>POLYGON Z ((-1735957.5288111183 2709325.7336960486 0, -1735894.7669745085 2709579.947660815 0, -1735560.4508488195 2709498.6150810597 0, -1735873.2193062378 2709024.509133888 0, -1735957.5288111183 2709325.7336960486 0))</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Uintah and Ouray</t>
+          <t>Umatilla</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>UT</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Public Schools, Recreation Exchange, Multi-Beneficiary, College of Mines and Earth Sciences, UtahÔøΩStateÔøΩHospital, Reservoirs, UtahÔøΩSchools for the Deaf, University ofÔøΩUtah, UtahÔøΩStateÔøΩUniversity, Juvenile Justice Services, UtahÔøΩSchools for the Blind, Teaching Colleges at Public Universities, Public Buildings, Miners Hospital</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>1463</v>
+        <v>1</v>
       </c>
       <c r="G71" t="n">
-        <v>230995.4</v>
+        <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="I71" t="n">
-        <v>280566.13</v>
+        <v>27.71</v>
       </c>
       <c r="J71" t="n">
-        <v>791</v>
+        <v>1</v>
       </c>
       <c r="K71" t="n">
-        <v>511561.53</v>
+        <v>27.71</v>
       </c>
       <c r="L71" t="n">
-        <v>4504964.31</v>
+        <v>293080.11</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>POLYGON Z ((-1735957.5288111183 2709325.7336960486 0, -1735894.7669745085 2709579.947660815 0, -1735560.4508488195 2709498.6150810597 0, -1735873.2193062378 2709024.509133888 0, -1735957.5288111183 2709325.7336960486 0))</t>
+          <t>MULTIPOLYGON Z (((-1193003.2095425471 1695774.3584740828 0, -1192984.9212274093 1695900.7692824828 0, -1192945.0435830269 1696176.3015231234 0, -1192886.8559896317 1696578.25154202 0, -1192881.9343917111 1696577.5376560343 0, -1192492.216327342 1696521.5778199872 0, -1192097.5544728765 1696464.9204099888 0, -1191702.8981870324 1696408.293970237 0, -1191310.6498185473 1696352.0224191104 0, -1191367.5662472763 1695958.1387066147 0, -1191425.6036585008 1695556.607454057 0, -1191484.279965398 1695154.292625367 0, -1191542.9719370164 1694751.9805008422 0, -1191599.5623806964 1694760.1283922999 0, -1191936.8302557205 1694808.7758680845 0, -1192330.6857806419 1694865.5900618492 0, -1192725.2076363482 1694922.6423065949 0, -1193021.7043253863 1694965.511388046 0, -1193118.2409867113 1694979.5181527494 0, -1193099.2474606927 1695110.749390148 0, -1193061.394581745 1695372.418666538 0, -1193003.2095425471 1695774.3584740828 0)), ((-1175136.4566705169 1700196.8519050677 0, -1175355.6007487734 1700231.1283220071 0, -1175392.9283744611 1700237.0265294942 0, -1175435.9682477617 1700243.7402009661 0, -1175914.600607573 1700318.5815734565 0, -1175921.385623749 1700319.6179123465 0, -1175869.8664627378 1700677.2443388063 0, -1175813.2255560244 1701079.2291578047 0, -1175419.2740635977 1701023.5417064158 0, -1175025.3900617007 1700967.8746278076 0, -1174967.7857207288 1701369.7353618878 0, -1174911.9834876428 1701759.8501871168 0, -1174762.074135036 1701742.6522933922 0, -1174824.6026744395 1701349.4990872564 0, -1174820.4623422304 1701348.9197408815 0, -1174857.8606624247 1701001.4230639348 0, -1174921.1802547355 1700543.1526606646 0, -1175082.984075629 1700566.0124138736 0, -1175136.4566705169 1700196.8519050677 0)))</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Umatilla</t>
+          <t>Ute Mountain Ute</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>OR</t>
+          <t>UT</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Common Schools</t>
+          <t>Public Schools, UtahÔøΩSchools for the Blind, UtahÔøΩStateÔøΩUniversity</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G72" t="n">
         <v>0</v>
@@ -3891,37 +3891,37 @@
         <v>0</v>
       </c>
       <c r="I72" t="n">
-        <v>27.71</v>
+        <v>834.13</v>
       </c>
       <c r="J72" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K72" t="n">
-        <v>27.71</v>
+        <v>834.13</v>
       </c>
       <c r="L72" t="n">
-        <v>293080.11</v>
+        <v>598651.62</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1193003.2095425471 1695774.3584740828 0, -1192984.9212274093 1695900.7692824828 0, -1192945.0435830269 1696176.3015231234 0, -1192886.8559896317 1696578.25154202 0, -1192881.9343917111 1696577.5376560343 0, -1192492.216327342 1696521.5778199872 0, -1192097.5544728765 1696464.9204099888 0, -1191702.8981870324 1696408.293970237 0, -1191310.6498185473 1696352.0224191104 0, -1191367.5662472763 1695958.1387066147 0, -1191425.6036585008 1695556.607454057 0, -1191484.279965398 1695154.292625367 0, -1191542.9719370164 1694751.9805008422 0, -1191599.5623806964 1694760.1283922999 0, -1191936.8302557205 1694808.7758680845 0, -1192330.6857806419 1694865.5900618492 0, -1192725.2076363482 1694922.6423065949 0, -1193021.7043253863 1694965.511388046 0, -1193118.2409867113 1694979.5181527494 0, -1193099.2474606927 1695110.749390148 0, -1193061.394581745 1695372.418666538 0, -1193003.2095425471 1695774.3584740828 0)), ((-1175136.4566705169 1700196.8519050677 0, -1175355.6007487734 1700231.1283220071 0, -1175392.9283744611 1700237.0265294942 0, -1175435.9682477617 1700243.7402009661 0, -1175914.600607573 1700318.5815734565 0, -1175921.385623749 1700319.6179123465 0, -1175869.8664627378 1700677.2443388063 0, -1175813.2255560244 1701079.2291578047 0, -1175419.2740635977 1701023.5417064158 0, -1175025.3900617007 1700967.8746278076 0, -1174967.7857207288 1701369.7353618878 0, -1174911.9834876428 1701759.8501871168 0, -1174762.074135036 1701742.6522933922 0, -1174824.6026744395 1701349.4990872564 0, -1174820.4623422304 1701348.9197408815 0, -1174857.8606624247 1701001.4230639348 0, -1174921.1802547355 1700543.1526606646 0, -1175082.984075629 1700566.0124138736 0, -1175136.4566705169 1700196.8519050677 0)))</t>
+          <t>MULTIPOLYGON Z (((-1992631.9944673681 2670926.464298897 0, -1992938.932462263 2671012.287260834 0, -1992936.7828719348 2671019.243412175 0, -1992825.3261720703 2671379.902557449 0, -1992904.8151096767 2671402.274419125 0, -1992901.0677554947 2671414.7063132157 0, -1993201.0460950553 2671494.2228502235 0, -1993088.1247060255 2671871.201701455 0, -1993058.3305977758 2671970.7121474133 0, -1993003.2970318634 2671939.513304314 0, -1992996.262628254 2671934.9114480624 0, -1992994.1999950157 2671934.3561421246 0, -1992804.3193770477 2671826.711734401 0, -1992723.4052418773 2671721.186190158 0, -1992677.6417616934 2671644.2716992777 0, -1992617.7862502602 2671606.288020065 0, -1992610.2707793624 2671598.969549228 0, -1992596.140810236 2671582.9898940483 0, -1992580.6040879954 2671566.6810664223 0, -1992567.0944994588 2671553.8842298975 0, -1992517.154220667 2671508.2119610617 0, -1992441.4175795135 2671299.07597776 0, -1992377.5585912424 2671152.7685074173 0, -1992361.3805807908 2671131.2579916352 0, -1992330.831970632 2671092.735895415 0, -1992298.4242728483 2671019.456564848 0, -1992257.486781599 2670929.531273581 0, -1992248.0455779533 2670895.511296295 0, -1992241.546146979 2670876.8117774087 0, -1992232.9681949937 2670862.147679242 0, -1992222.3049043599 2670842.983375668 0, -1992209.3735253057 2670819.7423042394 0, -1992568.143237446 2670902.140877451 0, -1992633.9366475567 2670919.403673451 0, -1992631.9944673681 2670926.464298897 0)), ((-1971019.1127336344 2680570.723298427 0, -1971409.0781579274 2680679.934139636 0, -1971798.3806258538 2680792.5859385673 0, -1971574.33247729 2681567.2272357335 0, -1971367.0090841458 2682338.5522929113 0, -1970979.1211007498 2682234.321961667 0, -1970584.2668008404 2682123.7649993724 0, -1970801.6881515817 2681347.2510244963 0, -1971019.1127336344 2680570.723298427 0)))</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Ute Mountain Ute</t>
+          <t>Warm Springs</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>UT</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Public Schools, UtahÔøΩSchools for the Blind, UtahÔøΩStateÔøΩUniversity</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -3930,7 +3930,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G73" t="n">
         <v>0</v>
@@ -3939,277 +3939,277 @@
         <v>0</v>
       </c>
       <c r="I73" t="n">
-        <v>834.13</v>
+        <v>441.49</v>
       </c>
       <c r="J73" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K73" t="n">
-        <v>834.13</v>
+        <v>441.49</v>
       </c>
       <c r="L73" t="n">
-        <v>598651.62</v>
+        <v>657110.6</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1992631.9944673681 2670926.464298897 0, -1992938.932462263 2671012.287260834 0, -1992936.7828719348 2671019.243412175 0, -1992825.3261720703 2671379.902557449 0, -1992904.8151096767 2671402.274419125 0, -1992901.0677554947 2671414.7063132157 0, -1993201.0460950553 2671494.2228502235 0, -1993088.1247060255 2671871.201701455 0, -1993058.3305977758 2671970.7121474133 0, -1993003.2970318634 2671939.513304314 0, -1992996.262628254 2671934.9114480624 0, -1992994.1999950157 2671934.3561421246 0, -1992804.3193770477 2671826.711734401 0, -1992723.4052418773 2671721.186190158 0, -1992677.6417616934 2671644.2716992777 0, -1992617.7862502602 2671606.288020065 0, -1992610.2707793624 2671598.969549228 0, -1992596.140810236 2671582.9898940483 0, -1992580.6040879954 2671566.6810664223 0, -1992567.0944994588 2671553.8842298975 0, -1992517.154220667 2671508.2119610617 0, -1992441.4175795135 2671299.07597776 0, -1992377.5585912424 2671152.7685074173 0, -1992361.3805807908 2671131.2579916352 0, -1992330.831970632 2671092.735895415 0, -1992298.4242728483 2671019.456564848 0, -1992257.486781599 2670929.531273581 0, -1992248.0455779533 2670895.511296295 0, -1992241.546146979 2670876.8117774087 0, -1992232.9681949937 2670862.147679242 0, -1992222.3049043599 2670842.983375668 0, -1992209.3735253057 2670819.7423042394 0, -1992568.143237446 2670902.140877451 0, -1992633.9366475567 2670919.403673451 0, -1992631.9944673681 2670926.464298897 0)), ((-1971019.1127336344 2680570.723298427 0, -1971409.0781579274 2680679.934139636 0, -1971798.3806258538 2680792.5859385673 0, -1971574.33247729 2681567.2272357335 0, -1971367.0090841458 2682338.5522929113 0, -1970979.1211007498 2682234.321961667 0, -1970584.2668008404 2682123.7649993724 0, -1970801.6881515817 2681347.2510244963 0, -1971019.1127336344 2680570.723298427 0)))</t>
+          <t>MULTIPOLYGON Z (((1383.5353677989615 2665597.0389574743 0, 1787.8362839817985 2665595.1437992966 0, 1789.5667013662242 2665192.0752311223 0, 1612.6779454421549 2665193.079095202 0, 1499.3286985567952 2665193.722393299 0, 1434.7197709316813 2665194.088678773 0, 1384.9421352758486 2665194.370903259 0, 1100.0312463793368 2665193.814237008 0, 986.5166697160986 2665196.539836616 0, 980.3181917673943 2665196.688671415 0, 979.234695915162 2665598.9298086413 0, 1383.5353677989615 2665597.0389574743 0)), ((1630.4892621535892 2666577.227090937 0, 1782.7804459670808 2666773.125752292 0, 1784.3763232551087 2666401.2862598463 0, 1631.4780851873477 2666401.6276745563 0, 1630.4892621535892 2666577.227090937 0)), ((-1043.9127356924253 2667205.017103878 0, -1044.3824041522014 2667606.73599305 0, -640.1260951447346 2667608.1508072903 0, -639.6571572228979 2667206.2935517295 0, -1043.9127356924253 2667205.017103878 0)), ((3412.4767253203277 2670802.752104579 0, 3413.0752287707783 2671204.0885676933 0, 3820.3192275613037 2671204.3768943134 0, 3819.07616086587 2670803.339855818 0, 3412.4767253203277 2670802.752104579 0)), ((981.2231380002734 2671211.303034148 0, 980.6184513733934 2671613.6781696626 0, 1384.406988532018 2671609.0994988997 0, 1385.6794557510357 2671207.1844922407 0, 981.2231380002734 2671211.303034148 0)), ((576.8307485585088 2671618.2796248817 0, 571.6782034535402 2672021.0900131185 0, 977.3368457358474 2672016.9964574035 0, 980.6184513733934 2671613.6781696626 0, 576.8307485585088 2671618.2796248817 0)), ((974.0551698998473 2672420.309051253 0, 970.7736638072345 2672823.562984495 0, 1380.1735619965264 2672820.506616753 0, 1381.5849194588827 2672416.7318239957 0, 974.0551698998473 2672420.309051253 0)), ((5912.8415571091955 2674827.5905595156 0, 5915.34731046087 2674406.918686161 0, 5917.757013608493 2674002.4214660246 0, 6319.887350455133 2673997.197710027 0, 6722.018009562836 2673991.969764447 0, 6722.4135626571415 2674391.254104146 0, 7124.713803093802 2674393.2473753593 0, 7123.474072854011 2673992.1342754653 0, 7122.229005335942 2673590.968537697 0, 6721.62239690647 2673592.6807247777 0, 6320.893763014451 2673595.4109512526 0, 6321.899885734936 2673193.6058778767 0, 5922.573267334203 2673193.847145713 0, 5523.246700266753 2673194.1099877832 0, 5038.264683324756 2673194.458879093 0, 5037.04495268615 2673604.163529869 0, 5035.82506100801 2674013.8633151893 0, 5034.605529452809 2674423.5577543243 0, 5033.386049244274 2674833.2470321404 0, 5507.842197286466 2674830.182107177 0, 5912.8415571091955 2674827.5905595156 0)), ((1017.9204615395657 2682065.7481912365 0, 1022.4606315108377 2682467.562998352 0, 1027.0012276590394 2682869.3724264596 0, 1424.8994874822993 2682871.3093063678 0, 1421.3919521954385 2682468.6672865455 0, 1820.3229625971003 2682469.7673309087 0, 1817.8481141545 2682066.261951393 0, 1417.8844088355 2682066.0070054685 0, 1017.9204615395657 2682065.7481912365 0)), ((2248.8362833070732 2683670.6256722473 0, 2239.947981889339 2683272.2181566656 0, 2231.0597428386955 2682873.7922004396 0, 2227.761508969853 2682470.349425693 0, 1820.3229625971003 2682469.7673309087 0, 1822.7975564517574 2682873.267853401 0, 1424.8994874822993 2682871.3093063678 0, 1432.5442688101505 2683270.57538892 0, 1440.1888607093929 2683669.823295923 0, 1447.8314432683142 2684069.040314768 0, 1850.7439922273386 2684069.591119776 0, 2257.722988909524 2684069.000448099 0, 2248.8362833070732 2683670.6256722473 0)), ((3455.8455431892626 2682875.5030630757 0, 3463.4532388986904 2683272.759969386 0, 3870.5289121893675 2683267.5784294275 0, 3863.606664061292 2682869.5188334202 0, 3455.8455431892626 2682875.5030630757 0)), ((236.47474820775284 2683666.8031992353 0, 637.7116523797454 2683667.8139777663 0, 633.4070456116638 2683267.644938588 0, 233.83955206538675 2683266.1862250827 0, 236.47474820775284 2683666.8031992353 0)), ((-3417.6777773818003 2683274.60055734 0, -3416.0135255833156 2683676.514065591 0, -3014.1754051494845 2683676.7827926064 0, -3018.1874508010887 2683274.4760140674 0, -3417.6777773818003 2683274.60055734 0)), ((5101.588751731198 2684052.7620926443 0, 4695.839099557662 2684056.7940946138 0, 4701.457836598618 2684456.942234662 0, 5106.486014164929 2684453.1049528564 0, 5104.037477161907 2684252.934147923 0, 5101.588751731198 2684052.7620926443 0)), ((2673.689484060182 2684861.4009187645 0, 3080.3520430623566 2684861.0919844564 0, 3487.014895776545 2684860.7783419285 0, 3486.149774040266 2684458.1455836007 0, 3079.580141260864 2684458.6700031054 0, 2673.0103286512626 2684459.21737087 0, 2673.689484060182 2684861.4009187645 0)), ((2675.0446514598357 2685663.893965721 0, 2674.368651619193 2685263.5796309058 0, 2673.689484060182 2684861.4009187645 0, 2267.2950769636245 2684861.7325346717 0, 2266.440650033938 2684459.787399877 0, 1859.871102576042 2684460.380189284 0, 1860.9009774007502 2684862.05915012 0, 1861.9307817363458 2685263.7329876428 0, 1862.960411386893 2685665.40179497 0, 2269.0021928041383 2685664.65012255 0, 2675.0446514598357 2685663.893965721 0)), ((3082.5759505649357 2687264.07062505 0, 3082.907939134586 2687664.441864723 0, 3487.3440335022947 2687665.704985281 0, 3487.3676324344483 2687264.647758527 0, 3082.5759505649357 2687264.07062505 0)), ((998.2684010510346 2706066.267530266 0, 998.7142267459749 2706469.0704515167 0, 1402.1458548675744 2706475.293432962 0, 1402.6529933882593 2706072.394173808 0, 998.2684010510346 2706066.267530266 0)), ((3841.172606768769 2706087.964316507 0, 3839.521796802324 2706490.616138839 0, 4246.285195752414 2706489.0255209506 0, 4247.581830900716 2706087.3651774214 0, 3841.172606768769 2706087.964316507 0)), ((1804.1155716580497 2706884.50227363 0, 2210.7754551222692 2706887.3022113666 0, 2212.372712894733 2706484.177774412 0, 1805.5767395007708 2706481.5115015535 0, 1804.1155716580497 2706884.50227363 0)), ((2212.012694327966 2707686.8354237806 0, 2212.6314143693453 2708086.559291596 0, 2619.2511251877418 2708090.21324856 0, 3025.870455191995 2708093.8901692806 0, 3432.4895729825143 2708097.5624091453 0, 3431.910851741838 2707696.9932933724 0, 3025.2783066424413 2707693.6123147793 0, 2618.6457542894213 2707690.226364632 0, 2212.012694327966 2707686.8354237806 0)), ((3838.7793070041766 2707694.586730474 0, 3839.233353306072 2708095.213191078 0, 4245.977480480861 2708092.8587930105 0, 4245.647694677946 2707692.175268233 0, 3838.7793070041766 2707694.586730474 0)), ((-5106.651918404079 2711281.7034740294 0, -5107.501617508913 2711470.620925021 0, -5108.455607399276 2711682.7534461278 0, -4675.295503652894 2711682.844125988 0, -4677.184035010697 2711282.4189093523 0, -4679.073494315028 2710881.953594931 0, -4680.967637594464 2710480.7067106846 0, -4682.862738058344 2710079.4280649396 0, -5101.240216921132 2710078.5229432643 0, -5103.044339564015 2710479.58835322 0, -5104.848454811948 2710880.6487840856 0, -5105.228836937038 2710965.2330671665 0, -5106.651918333609 2711281.703458358 0, -5106.651918404079 2711281.7034740294 0)), ((4255.021903333384 2710498.7436810127 0, 3850.3880491768778 2710505.0583903505 0, 3843.870118786147 2710903.2411668384 0, 3842.4519574278183 2711305.4453184055 0, 4250.698685929169 2711303.448886601 0, 4252.865565825576 2710900.1591316117 0, 4661.6574063913 2710897.072262254 0, 4663.773030244654 2710497.092572416 0, 4255.021903333384 2710498.7436810127 0)), ((-4269.70831925989 2712890.655111386 0, -4676.320287089962 2712890.688614873 0, -5117.132716128869 2712890.719593824 0, -5120.02311810595 2713293.179542048 0, -5118.382633689577 2713293.369323318 0, -5118.382320941198 2713293.3693243014 0, -5118.392643909606 2713287.748213695 0, -4676.631346000081 2713290.5845160163 0, -4674.896648937593 2713290.5956852036 0, -4270.4090715393495 2713293.2166674216 0, -4268.579073213473 2713293.228477472 0, -3864.1897983730737 2713295.871765018 0, -3862.261885126718 2713295.8843135983 0, -3457.9707959306834 2713297.989240222 0, -3457.0075923977965 2713297.9942313256 0, -3051.7535045864397 2713300.127124115 0, -3049.932240095481 2712889.8907292085 0, -2644.888321633176 2712890.535121375 0, -2239.8440697577216 2712891.1747652455 0, -2238.445368673496 2712490.284288044 0, -2643.2956807531045 2712488.9904344073 0, -2643.535803263525 2712090.1510578045 0, -3046.3605262186784 2712085.4875751836 0, -3048.145940448636 2712487.691730232 0, -3455.1020574277586 2712487.776043136 0, -3862.058160765678 2712487.855847102 0, -4269.007270750511 2712487.9303149693 0, -4269.70831925989 2712890.655111386 0)), ((4258.5777549818595 2712505.44122695 0, 4658.248838942368 2712500.2307842523 0, 4658.348320051825 2712100.523392187 0, 4253.635103178385 2712105.807845356 0, 4258.5777549818595 2712505.44122695 0)), ((-1836.0148288950045 2713296.0281345397 0, -1430.7683162261403 2713294.707195535 0, -1427.9208151375617 2712892.491884259 0, -1425.0914209221282 2712492.868953733 0, -1831.7684270770046 2712491.579166733 0, -1833.8809975115978 2712891.8356715976 0, -1836.0148288950045 2713296.0281345397 0)), ((3033.2239233042237 2713286.675944311 0, 3439.5777274196394 2713285.9191595083 0, 3434.609641684605 2712914.106807696 0, 3030.1547177381285 2712913.115378526 0, 3032.876518482947 2713286.6765549146 0, 3033.2239233042237 2713286.675944311 0)), ((191.24675436282772 2713682.2688071155 0, 188.1100455757981 2713281.8331672493 0, -216.60997828050702 2713285.017712498 0, -621.3299425510596 2713288.2247412466 0, -618.8584316213498 2713688.351987669 0, -213.8058691205999 2713685.313281258 0, -211.0013515317427 2714085.5898771165 0, 194.38379128553382 2714082.7006832794 0, 191.24675436282772 2713682.2688071155 0)), ((-1649.9456180682266 2715295.421635402 0, -1618.1799364685733 2715495.3742659106 0, -1582.7676239280281 2715597.3847823306 0, -1702.5530287301283 2715689.4910429125 0, -1703.783319452899 2715696.3169638338 0, -1720.2774801544037 2715787.8343663174 0, -1781.052836937852 2715879.9153260333 0, -1781.240398412982 2715999.763944685 0, -1710.7693077944662 2716092.3242227477 0, -1711.6825030898558 2716095.916031599 0, -1747.717082071063 2716237.6539940974 0, -1852.8649537851527 2716255.7991800443 0, -1856.8632074523973 2716498.0741839157 0, -1453.9115417504436 2716496.8841965348 0, -1438.9683756533925 2716092.8599919737 0, -1032.640313329464 2716090.7936810893 0, -1030.0297502254796 2715692.5462534055 0, -621.3591906385346 2715688.702142325 0, -616.3861447072471 2715289.2109832875 0, -611.4437058543614 2714888.647759559 0, -613.9151646126546 2714488.5635543303 0, -1019.6342010151255 2714491.2756021745 0, -1021.7725612321208 2714091.3539768253 0, -1023.9110516341043 2713691.413760786 0, -1428.962687071269 2713694.469403211 0, -1427.1582102463103 2714094.2285999577 0, -1425.3525812221044 2714493.9824845614 0, -1423.5471298473424 2714893.73160047 0, -1431.1394687405632 2715294.5275185746 0, -1649.9456180682266 2715295.421635402 0)), ((-2402.352077579976 2716099.334853069 0, -2413.36844541935 2716093.0382219893 0, -2294.4589538125874 2715931.276844202 0, -2323.360583455664 2715698.643016867 0, -2653.4612891532324 2715699.8776385793 0, -2658.113847241481 2716100.2091913237 0, -2662.766312008028 2716500.5218182127 0, -2259.814975757727 2716499.286982927 0, -2255.5264929878385 2716194.363314527 0, -2276.609240628882 2716171.2053056955 0, -2402.352077579976 2716099.334853069 0)), ((-5114.516344134941 2715699.591771844 0, -5114.1675727356105 2716099.560706577 0, -5114.174559426497 2716101.073244287 0, -5115.874814454032 2716469.1587783494 0, -5115.884030242105 2716502.5500650387 0, -4686.082284763518 2716502.3401412563 0, -4683.377929902097 2716101.1767004402 0, -4680.674335148573 2715699.9810619885 0, -5114.516344134941 2715699.591771844 0)), ((-3875.8999535398907 2716502.014269519 0, -3470.8088823478374 2716501.8857303634 0, -3065.717853351423 2716501.7795600616 0, -3062.045100201077 2716101.586174578 0, -3467.378483349269 2716101.4740142776 0, -3872.711936780993 2716101.356873321 0, -3875.8999535398907 2716502.014269519 0)), ((4259.173389040151 2716499.602358147 0, 4257.897788135917 2716900.911863932 0, 4663.67512608057 2716902.714408253 0, 4664.329278431304 2716501.0692761866 0, 4259.173389040151 2716499.602358147 0)), ((-1858.049349993421 2716904.4505387424 0, -1859.2356445559512 2717310.808105758 0, -1456.0861838246765 2717311.674963512 0, -1454.9990194379297 2716904.2820678363 0, -1858.049349993421 2716904.4505387424 0)), ((-225.4412341625802 2717696.122938931 0, -225.44136625068052 2717696.249909394 0, -224.62921019346118 2717696.1078722137 0, -221.7764295375716 2717695.6090442045 0, 45.99379118113641 2717632.0475321608 0, 138.95106175224706 2717689.342302194 0, 184.31465186959124 2717688.4978438085 0, 183.39742742500147 2717287.304102903 0, -225.2399847123634 2717293.385876797 0, -633.8775431778841 2717299.4627628666 0, -635.1967975754217 2717703.743030767 0, -225.4412341625802 2717696.122938931 0)), ((15079.501850495779 2667400.911845348 0, 15125.666890252996 2667311.980604434 0, 15191.120772676088 2667284.6512994124 0, 15210.063621884934 2667269.0161402402 0, 15210.858954446136 2667181.2885950194 0, 14765.698578201169 2667179.4144756533 0, 14762.364038258156 2667582.408584772 0, 14847.975366687539 2667583.0539863487 0, 14841.385369952295 2667452.791058091 0, 15079.501850495779 2667400.911845348 0)), ((16250.437263109736 2667185.688715323 0, 16212.863384605109 2667216.180548536 0, 16107.166205849237 2667337.9112681528 0, 16023.860067014903 2667301.8384443605 0, 16019.831808211695 2667265.730373721 0, 16016.703916299599 2667591.844295529 0, 16421.459554043173 2667594.8802448865 0, 16425.48372246775 2667186.4313854077 0, 16250.437263109736 2667185.688715323 0)), ((13948.867468892431 2667984.6879084967 0, 14353.948960351807 2667985.0449518133 0, 14356.537747320093 2667581.979590327 0, 13950.711097539757 2667581.5463382415 0, 13544.88449625694 2667581.1087441025 0, 13543.786105052044 2667984.353232905 0, 13948.867468892431 2667984.6879084967 0)), ((15495.80898399944 2667993.3461896866 0, 15608.162694162504 2667994.556954945 0, 16012.799302952984 2667998.9426411623 0, 16016.703916299599 2667591.844295529 0, 15611.948077044612 2667588.8040282903 0, 15339.127594443033 2667586.7523486507 0, 15341.644186387613 2667594.4185282057 0, 15354.556646538535 2667638.9483704814 0, 15387.566679094865 2667696.8993172334 0, 15432.158450588911 2667778.4519989695 0, 15526.672760607735 2667825.8039362514 0, 15495.80898399944 2667993.3461896866 0)), ((17830.08146852741 2669760.683438869 0, 17649.05768640751 2669777.0741732577 0, 17631.565247529103 2669617.8104476244 0, 17633.997077992266 2670020.34696265 0, 18037.79208556993 2670022.324691535 0, 18035.31636994485 2669619.136690924 0, 17875.953747805626 2669618.6137737106 0, 17830.08146852741 2669760.683438869 0)), ((14768.977026613255 2670388.4224988976 0, 14770.948934927701 2669988.3990127323 0, 14361.0257746289 2669995.3652410023 0, 14188.502483820428 2669998.3039836264 0, 14305.200836025242 2670054.2689221795 0, 14360.454752604344 2670104.4469125723 0, 14459.501902742279 2670194.3941970877 0, 14392.330452011978 2670240.163269429 0, 14359.827510695948 2670224.2641465412 0, 14358.931950126587 2670395.300505628 0, 14768.977026613255 2670388.4224988976 0)), ((15982.398502089718 2671996.7309447806 0, 16386.891446308186 2672004.6743460796 0, 16390.790187731553 2671611.734047498 0, 15986.386770171996 2671605.9186339066 0, 15982.398502089718 2671996.7309447806 0)), ((14352.435077189672 2671983.181671434 0, 14352.224013645891 2672371.435161358 0, 14759.808406016065 2672357.1248954944 0, 14761.435499449008 2671972.796652494 0, 14352.435077189672 2671983.181671434 0)), ((17639.318406072478 2675987.607339894 0, 17643.392109364686 2676387.886543175 0, 18046.26375822212 2676389.8389650537 0, 18042.45093777533 2675989.1689838255 0, 17639.318406072478 2675987.607339894 0)), ((14413.950944558499 2676344.7981293434 0, 14419.429425159593 2676743.432690209 0, 14830.110234988155 2676735.110527663 0, 14823.781228980388 2676335.599639608 0, 14413.950944558499 2676344.7981293434 0)), ((5043.858294920456 2677630.709189919 0, 5538.680446440614 2677627.831867304 0, 5944.22467263026 2677625.4685462583 0, 5938.965806168243 2677226.9173046453 0, 5534.944850585622 2677228.6367265102 0, 5043.958277677374 2677230.7203423693 0, 5043.858294920456 2677630.709189919 0)), ((14458.96357176142 2680338.908785741 0, 14459.992977810683 2680740.223605747 0, 14870.501341395266 2680736.0568875275 0, 14870.820254864704 2680333.8588010394 0, 14458.96357176142 2680338.908785741 0)), ((16050.83168322219 2684343.462719235 0, 16044.58080873297 2684743.49997516 0, 16448.26209559142 2684745.254399555 0, 16455.014089451728 2684345.5851647467 0, 16050.83168322219 2684343.462719235 0)), ((18064.93140508903 2684773.3330952954 0, 18056.64674919042 2685174.1869721995 0, 18455.458325242198 2685173.716147613 0, 18462.604457031957 2684772.805884849 0, 18064.93140508903 2684773.3330952954 0)), ((6399.911934908316 2684824.6959309313 0, 5990.868503157693 2684833.7125557074 0, 5987.686570742631 2685231.4931133687 0, 5984.505287553653 2685629.2170933248 0, 6392.278881404925 2685617.948536389 0, 6396.095641197958 2685221.337491395 0, 6804.5040338186 2685211.177146352 0, 6808.955447117598 2684815.6740054963 0, 6399.911934908316 2684824.6959309313 0)), ((5576.73096105953 2685640.5076097576 0, 5574.186618246233 2686039.3547491203 0, 5981.323657273146 2686026.9363154173 0, 5984.505287553653 2685629.2170933248 0, 5576.73096105953 2685640.5076097576 0)), ((18094.60930537767 2686272.6232533487 0, 18136.337536053034 2686109.609611235 0, 18100.22394129301 2686054.099339751 0, 18039.11985384811 2686093.1248439457 0, 18036.793375254492 2686377.4029910318 0, 18438.40066455692 2686377.0248764483 0, 18441.197964693434 2685975.454465967 0, 18411.85774471977 2685975.484722507 0, 18414.281707821112 2686075.47883292 0, 18438.61011432442 2686180.806094717 0, 18328.79169006953 2686319.1780334767 0, 18293.469005068087 2686367.92355676 0, 18216.312201170203 2686352.106225105 0, 18174.496124258203 2686303.269197429 0, 18084.434667421552 2686315.498731412 0, 18094.60930537767 2686272.6232533487 0)), ((9757.617694161461 2687748.8867081027 0, 9752.912573017042 2687812.3713740297 0, 9809.99251404404 2687868.836168498 0, 9842.736504109951 2687888.670693366 0, 9866.846198967809 2687918.1370489956 0, 9868.55862330926 2687927.8645071695 0, 10025.266346764902 2687923.554683998 0, 10030.775277616185 2687525.8802808467 0, 9626.302538349495 2687535.950591208 0, 9625.222165730322 2687621.2640673453 0, 9688.71839456967 2687557.789856814 0, 9769.461858185103 2687564.7714799345 0, 9821.699850100742 2687598.9525585975 0, 9855.846723816974 2687660.001203148 0, 9829.586884813207 2687713.693975444 0, 9780.221945131274 2687723.534390778 0, 9757.617694161461 2687748.8867081027 0)), ((20443.3028628736 2687586.371680449 0, 20041.32598418925 2687583.5210404084 0, 20040.29140951473 2687982.3402563483 0, 20039.256856533208 2688381.1406538524 0, 20440.432441648754 2688384.847955336 0, 20441.867668474377 2687985.612067682 0, 20443.3028628736 2687586.371680449 0)), ((17832.1715950558 2690039.5518426816 0, 17873.625918772523 2690071.73188395 0, 17863.72857082412 2690141.080796169 0, 17894.80372434661 2690225.8250616076 0, 17952.78078221775 2690307.9989660927 0, 18006.783260803368 2690343.534066388 0, 18007.86092477352 2689973.4960319065 0, 17608.94248657115 2689968.850090002 0, 17607.954287781853 2690223.1475237035 0, 17727.31607366602 2690050.051828257 0, 17832.1715950558 2690039.5518426816 0)), ((5962.16379607039 2690841.1623292356 0, 5959.722312819952 2691241.1190262316 0, 6365.8830732785145 2691229.7663953453 0, 6367.586316556753 2690829.6923118155 0, 5962.16379607039 2690841.1623292356 0)), ((8383.09897757985 2691978.113463563 0, 8380.675440758812 2692378.948162184 0, 7977.433821210296 2692392.439634175 0, 7978.304519062915 2692789.062010852 0, 8381.457501985777 2692779.7847833694 0, 8787.765956236552 2692764.539263972 0, 8783.749577303544 2692363.6513578077 0, 8786.605085872568 2691963.149060149 0, 8383.09897757985 2691978.113463563 0)), ((10006.656624822906 2692743.5703330548 0, 10006.148483262275 2693167.8273011874 0, 10409.87651692492 2693166.7346429247 0, 10410.531604089409 2692744.273491583 0, 10006.656624822906 2692743.5703330548 0)), ((12820.230571030992 2693987.1397618665 0, 13220.698438218798 2693978.8834125823 0, 13220.438750020374 2693560.731732215 0, 12820.317281149624 2693565.659423673 0, 12820.230571030992 2693987.1397618665 0)), ((13215.127118235887 2700399.666562965 0, 13215.227855665682 2700802.1199340294 0, 13619.990253904578 2700795.658400593 0, 13620.88687039511 2700393.2762028207 0, 13215.127118235887 2700399.666562965 0)), ((16392.840605276408 2703596.5060888682 0, 16383.125101629521 2703997.62602151 0, 16785.850806478826 2703997.951237007 0, 16795.870516859217 2703596.94585355 0, 16392.840605276408 2703596.5060888682 0)), ((15975.207072759222 2703997.9543919303 0, 15965.459065785224 2704399.226921988 0, 16373.410834087772 2704398.741124809 0, 16383.125101629521 2703997.62602151 0, 15975.207072759222 2703997.9543919303 0)), ((14827.086485329473 2706384.7014311543 0, 14827.310022861895 2706777.6348382668 0, 15131.254753312056 2706780.614523737 0, 15130.551474041911 2706386.371219829 0, 14827.086485329473 2706384.7014311543 0)), ((7522.227589090743 2708066.9255449134 0, 7520.158680293587 2708467.9552760525 0, 7923.556393586471 2708466.0656237192 0, 7925.689286587144 2708064.3484900966 0, 7522.227589090743 2708066.9255449134 0)), ((16745.75995483178 2709988.8745242865 0, 16746.667418866586 2710393.857344907 0, 17153.54681341561 2710392.589243589 0, 17152.271366804034 2709987.066847501 0, 16745.75995483178 2709988.8745242865 0)), ((6304.264438979591 2712077.884363088 0, 6709.28915354734 2712072.1646806276 0, 6708.662774980455 2711672.191079046 0, 6304.349176872272 2711677.7776579163 0, 5900.0361394553265 2711683.3870479646 0, 5899.240417419743 2712083.6000901195 0, 6304.264438979591 2712077.884363088 0)), ((5067.319587614606 2712095.3252380895 0, 5066.277108903527 2712495.7629549075 0, 5494.685530606004 2712492.570208957 0, 5495.203892548303 2712090.776470419 0, 5067.319587614606 2712095.3252380895 0)), ((14802.43948004929 2714817.140624798 0, 14799.629966355671 2715216.3170601483 0, 14796.820658031116 2715615.4887292874 0, 15106.672545318035 2715616.7386727654 0, 15515.044486057697 2715618.3820719235 0, 15519.28731555198 2715220.1142183505 0, 15523.530421567928 2714821.841619475 0, 15119.104680751328 2714819.1961925817 0, 14802.43948004929 2714817.140624798 0)), ((12785.367357945022 2714839.243365424 0, 12778.028915937308 2715236.0972862532 0, 13181.373092528867 2715227.4012877173 0, 13189.212136702059 2714828.9145913515 0, 12785.367357945022 2714839.243365424 0)), ((19994.04610420238 2715185.5830227 0, 19991.993523887522 2715584.4885022948 0, 20397.81477682427 2715588.3003217042 0, 20397.63390720022 2715188.541757956 0, 19994.04610420238 2715185.5830227 0)), ((19171.838315983867 2716377.6469778386 0, 19168.059939930412 2716789.0019131415 0, 19576.440094002144 2716781.513537892 0, 19581.203435945397 2716369.2471883143 0, 19171.838315983867 2716377.6469778386 0)), ((20377.201750580276 2717598.8714839485 0, 20384.210267780993 2717193.925981193 0, 20013.00878703776 2717193.859437133 0, 20090.18921685623 2717263.3915806734 0, 19988.472462192796 2717548.6466629165 0, 19955.256397845413 2717602.601635659 0, 19972.05813135294 2717602.4532160163 0, 19966.17255585521 2718011.0342926322 0, 20370.193050922833 2718003.8116252488 0, 20377.201750580276 2717598.8714839485 0)), ((7880.287644520213 2717686.3839548663 0, 7877.502471846527 2718086.0268312832 0, 8283.264371112695 2718079.7193653136 0, 8285.493700064386 2717684.7793571926 0, 7880.287644520213 2717686.3839548663 0)), ((17143.136432501247 2718851.854545071 0, 17144.202373201148 2719250.693087528 0, 17145.268861881665 2719649.526274158 0, 17138.22853807499 2720049.3402349 0, 17536.18847418455 2720047.1827014093 0, 17540.601504212802 2719647.0594305797 0, 17540.63320173533 2719246.571066197 0, 17540.665010196175 2718846.0642567384 0, 17143.136432501247 2718851.854545071 0)), ((14365.029125951763 2719623.039628195 0, 13958.362885241737 2719629.1218747017 0, 13957.991485826433 2720032.389292792 0, 13957.619754289239 2720435.6511978353 0, 14362.950120561516 2720431.214218232 0, 14364.122307525207 2720028.861460987 0, 14365.029125951763 2719623.039628195 0)), ((9491.60155904921 2721276.076987971 0, 9489.432853290962 2721679.294584789 0, 9894.283104601725 2721674.779063306 0, 9897.325460810427 2721271.338466534 0, 9491.60155904921 2721276.076987971 0)), ((18736.208666899285 2721676.6144660674 0, 18734.891654079587 2722051.826046071 0, 19136.588965145314 2722056.2822198295 0, 19139.57401460323 2721654.9095463166 0, 18790.92133692967 2721651.352431548 0, 18746.635856455418 2721676.7592725707 0, 18736.208666899285 2721676.6144660674 0)), ((21672.095659978957 2665350.4282260244 0, 21672.086531502355 2665372.293954613 0, 21672.002551113914 2665572.198931443 0, 22059.960606851728 2665564.6437839186 0, 22059.51012393185 2665167.59760149 0, 22042.28568617821 2665168.139391153 0, 21979.807829336783 2665167.291337973 0, 21994.721507906586 2665202.3508685934 0, 22029.89727967998 2665381.3843977274 0, 21931.68197265437 2665532.912427275 0, 21812.327495206817 2665534.558848511 0, 21765.219748988056 2665459.200083126 0, 21729.44806997073 2665442.17642127 0, 21672.095659978957 2665350.4282260244 0)), ((22526.39306199842 2668392.650090327 0, 22571.531054147057 2668431.9261325086 0, 22601.43999812779 2668557.036422714 0, 22467.527157841312 2668601.5973549234 0, 22362.588536156494 2668636.5161758307 0, 22265.193535352802 2668608.130263837 0, 22186.23592688549 2668589.485017691 0, 22136.24419039 2668513.050294867 0, 22066.49272276504 2668462.3599507613 0, 22068.446639537877 2668726.159225186 0, 22468.719284162424 2668724.630279338 0, 22472.577107835903 2669122.7334815585 0, 22476.43435871928 2669520.8054370214 0, 22878.516806908323 2669518.220935466 0, 22873.75495539628 2669120.661552744 0, 22868.992262921827 2668723.0972213857 0, 22864.22911954068 2668325.528257113 0, 22464.861288350457 2668326.509093097 0, 22461.436513251225 2667936.855417234 0, 22458.011782350834 2667547.184071324 0, 22063.41142481525 2667548.628132555 0, 22064.452367454378 2667938.072487041 0, 22064.866843109572 2668093.024994244 0, 22087.812256035013 2668099.9010696686 0, 22251.251893170476 2668178.331044052 0, 22318.909450994066 2668238.3963519 0, 22336.464665231382 2668326.8292036676 0, 22377.00661620023 2668455.2155561815 0, 22526.39306199842 2668392.650090327 0)), ((21238.062742160102 2672362.930049306 0, 21642.699803803214 2672353.536105773 0, 21649.843835256223 2671955.7597573567 0, 21656.987634893936 2671557.964977879 0, 21252.146787717928 2671569.7579869293 0, 21245.104343659616 2671966.3461281485 0, 21238.062742160102 2672362.930049306 0)), ((23233.557563243914 2677306.346060751 0, 23082.518714103106 2677307.2123584705 0, 22932.835304386874 2677442.3850612105 0, 22930.10024565291 2677482.6121738856 0, 22873.135289436876 2677539.7261577803 0, 22873.45513215189 2677603.2231258126 0, 23277.6756393173 2677600.10813607 0, 23276.291406722252 2677269.08311469 0, 23233.557563243914 2677306.346060751 0)), ((22361.541615464164 2678131.308724134 0, 22443.312103270844 2678138.6495944164 0, 22465.556612685996 2678205.6963616014 0, 22466.659101666002 2678285.9859404014 0, 22460.191065290033 2678325.510705349 0, 22449.944183092568 2678374.4871553318 0, 22450.21983220639 2678394.559488821 0, 22448.53386465906 2678399.633472604 0, 22468.488240851788 2678399.6887218244 0, 22462.815185186064 2678003.6075812285 0, 22050.144745821603 2678000.862586919 0, 22053.310914273978 2678181.018962657 0, 22088.65612681045 2678163.2921830253 0, 22127.28547799425 2678149.778922786 0, 22159.78535174015 2678108.4195764763 0, 22219.17341173864 2678092.642262964 0, 22266.327219458064 2678094.8594078356 0, 22321.71368324477 2678121.444521027 0, 22361.541615464164 2678131.308724134 0)), ((21248.36970233172 2685980.628674969 0, 21652.294354918202 2685978.034577255 0, 21653.517930722817 2685578.1925358097 0, 21249.516926402557 2685581.2547017853 0, 21248.36970233172 2685980.628674969 0)), ((20846.84784678621 2686381.608176658 0, 20846.324936369674 2686784.181338925 0, 21247.81286830698 2686786.3944675643 0, 21248.09128594254 2686383.514008659 0, 20846.84784678621 2686381.608176658 0)), ((21649.88512991329 2688388.9431185103 0, 21647.96200389764 2688788.7994424985 0, 22055.228065565476 2688785.2986972253 0, 22056.887436198034 2688385.6325590163 0, 21649.88512991329 2688388.9431185103 0)), ((21240.695987252886 2688792.294844053 0, 21240.013952181373 2688917.108323467 0, 21283.321607611946 2688954.86373636 0, 21273.553858226376 2689054.4134390554 0, 21312.608422000754 2689135.3807898764 0, 21291.7948801089 2689191.8511573537 0, 21646.03889336303 2689188.636614877 0, 21647.96200389764 2688788.7994424985 0, 21240.695987252886 2688792.294844053 0)), ((21644.23998371618 2689578.272499468 0, 22051.509184007904 2689575.0818125755 0, 22053.56858350532 2689184.9598181364 0, 21646.03889336303 2689188.636614877 0, 21644.23998371618 2689578.272499468 0)), ((21232.34872532887 2690750.746599673 0, 21638.837245605 2690748.503476382 0, 22045.326068598206 2690746.283301461 0, 22047.387821246793 2690355.7437071516 0, 21640.639157350506 2690358.206040195 0, 21233.890748772475 2690360.6634465405 0, 21232.34872532887 2690750.746599673 0)), ((21639.208461658516 2691147.4002783964 0, 21639.579752169004 2691546.278047918 0, 22045.07389786588 2691544.0359015004 0, 22045.199926743804 2691145.1618523286 0, 21639.208461658516 2691147.4002783964 0)), ((23226.575169089832 2696036.708609112 0, 23150.430370563205 2696200.070948086 0, 23009.39260196048 2696310.0075473674 0, 23224.045232100492 2696311.012287523 0, 23627.058679142625 2696312.8949512797 0, 23633.279092870616 2695915.5534111713 0, 23326.99086647538 2695915.184468969 0, 23226.575169089832 2696036.708609112 0)), ((22002.504304606646 2696705.3661034345 0, 21596.743107050333 2696706.235865666 0, 21589.651204900736 2697102.605961009 0, 21591.713483730593 2697501.296876686 0, 21997.38648802732 2697501.3579260954 0, 22403.059959762424 2697501.4416328142 0, 22401.231345531633 2697099.6485378286 0, 22408.265644450326 2696704.5189842856 0, 22002.504304606646 2696705.3661034345 0)), ((22401.794765157432 2706780.4998695026 0, 21997.848440500948 2706787.234221662 0, 22000.680687837634 2707189.2289537825 0, 22003.513038443056 2707591.21841288 0, 22406.005657508904 2707583.3601349206 0, 22403.90025830444 2707181.939450402 0, 22401.794765157432 2706780.4998695026 0)), ((22410.54812813725 2708786.4320440646 0, 22401.8252175175 2708390.768550851 0, 22394.40303404622 2708385.338074282 0, 22009.165428940538 2708393.413618841 0, 22012.350819990817 2708792.0905121784 0, 22410.54812813725 2708786.4320440646 0)), ((22828.434004623694 2709588.7140895724 0, 22977.127390372654 2709482.18863001 0, 22973.449147104748 2709402.0783697325 0, 23098.609703089154 2709377.6827498274 0, 23192.482053936867 2709428.1301585827 0, 23233.27105311363 2709502.1027587685 0, 23226.52107775667 2709174.941936698 0, 22823.25449040109 2709184.677679324 0, 22828.434004623694 2709588.7140895724 0)), ((22013.055636146997 2711588.19436297 0, 22420.166229923485 2711583.5662361635 0, 22422.07034114094 2711184.656227873 0, 22015.277082351273 2711187.6367293787 0, 22013.055636146997 2711588.19436297 0)), ((22420.166229923485 2711583.5662361635 0, 22423.312718587167 2711982.7058012057 0, 22832.492621021636 2711977.354743092 0, 22827.27733910165 2711578.9613630553 0, 22420.166229923485 2711583.5662361635 0)), ((20802.38715176861 2712405.3168605864 0, 21202.086186972207 2712399.907491889 0, 21200.461495763215 2711998.715649977 0, 21607.297157999412 2711993.3862271537 0, 21605.945782625487 2711592.845154835 0, 21198.83635357114 2711597.5189974555 0, 20800.035805611144 2711609.255313006 0, 20401.23662399326 2711621.0135896066 0, 20401.96246907941 2712015.8698570635 0, 20402.688063687085 2712410.721382355 0, 20802.38715176861 2712405.3168605864 0)), ((22017.362462900226 2713185.8663945086 0, 22425.72653559047 2713187.6505632205 0, 22426.09508279207 2712782.2914511976 0, 22016.287898943185 2712787.3123977995 0, 22017.362462900226 2713185.8663945086 0)), ((21205.28140417238 2713189.095065119 0, 21206.765638147455 2713588.43038808 0, 21612.04103255767 2713587.915965496 0, 21611.321773924778 2713187.4694403093 0, 21205.28140417238 2713189.095065119 0)), ((21610.71529260665 2714390.403757304 0, 22017.22492195067 2714390.378172485 0, 22017.270712843423 2713988.9213646604 0, 22017.316423672222 2713587.3964814483 0, 21612.04103255767 2713587.915965496 0, 21612.76016174718 2713</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Warm Springs</t>
+          <t>White Earth</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>OR</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Common Schools</t>
+          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>5</v>
+        <v>1141</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>17197.01</v>
       </c>
       <c r="H74" t="n">
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="I74" t="n">
-        <v>441.49</v>
+        <v>27174.74</v>
       </c>
       <c r="J74" t="n">
-        <v>5</v>
+        <v>701</v>
       </c>
       <c r="K74" t="n">
-        <v>441.49</v>
+        <v>44371.75</v>
       </c>
       <c r="L74" t="n">
-        <v>657110.6</v>
+        <v>747912.54</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((1383.5353677989615 2665597.0389574743 0, 1787.8362839817985 2665595.1437992966 0, 1789.5667013662242 2665192.0752311223 0, 1612.6779454421549 2665193.079095202 0, 1499.3286985567952 2665193.722393299 0, 1434.7197709316813 2665194.088678773 0, 1384.9421352758486 2665194.370903259 0, 1100.0312463793368 2665193.814237008 0, 986.5166697160986 2665196.539836616 0, 980.3181917673943 2665196.688671415 0, 979.234695915162 2665598.9298086413 0, 1383.5353677989615 2665597.0389574743 0)), ((1630.4892621535892 2666577.227090937 0, 1782.7804459670808 2666773.125752292 0, 1784.3763232551087 2666401.2862598463 0, 1631.4780851873477 2666401.6276745563 0, 1630.4892621535892 2666577.227090937 0)), ((-1043.9127356924253 2667205.017103878 0, -1044.3824041522014 2667606.73599305 0, -640.1260951447346 2667608.1508072903 0, -639.6571572228979 2667206.2935517295 0, -1043.9127356924253 2667205.017103878 0)), ((3412.4767253203277 2670802.752104579 0, 3413.0752287707783 2671204.0885676933 0, 3820.3192275613037 2671204.3768943134 0, 3819.07616086587 2670803.339855818 0, 3412.4767253203277 2670802.752104579 0)), ((981.2231380002734 2671211.303034148 0, 980.6184513733934 2671613.6781696626 0, 1384.406988532018 2671609.0994988997 0, 1385.6794557510357 2671207.1844922407 0, 981.2231380002734 2671211.303034148 0)), ((576.8307485585088 2671618.2796248817 0, 571.6782034535402 2672021.0900131185 0, 977.3368457358474 2672016.9964574035 0, 980.6184513733934 2671613.6781696626 0, 576.8307485585088 2671618.2796248817 0)), ((974.0551698998473 2672420.309051253 0, 970.7736638072345 2672823.562984495 0, 1380.1735619965264 2672820.506616753 0, 1381.5849194588827 2672416.7318239957 0, 974.0551698998473 2672420.309051253 0)), ((5912.8415571091955 2674827.5905595156 0, 5915.34731046087 2674406.918686161 0, 5917.757013608493 2674002.4214660246 0, 6319.887350455133 2673997.197710027 0, 6722.018009562836 2673991.969764447 0, 6722.4135626571415 2674391.254104146 0, 7124.713803093802 2674393.2473753593 0, 7123.474072854011 2673992.1342754653 0, 7122.229005335942 2673590.968537697 0, 6721.62239690647 2673592.6807247777 0, 6320.893763014451 2673595.4109512526 0, 6321.899885734936 2673193.6058778767 0, 5922.573267334203 2673193.847145713 0, 5523.246700266753 2673194.1099877832 0, 5038.264683324756 2673194.458879093 0, 5037.04495268615 2673604.163529869 0, 5035.82506100801 2674013.8633151893 0, 5034.605529452809 2674423.5577543243 0, 5033.386049244274 2674833.2470321404 0, 5507.842197286466 2674830.182107177 0, 5912.8415571091955 2674827.5905595156 0)), ((1017.9204615395657 2682065.7481912365 0, 1022.4606315108377 2682467.562998352 0, 1027.0012276590394 2682869.3724264596 0, 1424.8994874822993 2682871.3093063678 0, 1421.3919521954385 2682468.6672865455 0, 1820.3229625971003 2682469.7673309087 0, 1817.8481141545 2682066.261951393 0, 1417.8844088355 2682066.0070054685 0, 1017.9204615395657 2682065.7481912365 0)), ((2248.8362833070732 2683670.6256722473 0, 2239.947981889339 2683272.2181566656 0, 2231.0597428386955 2682873.7922004396 0, 2227.761508969853 2682470.349425693 0, 1820.3229625971003 2682469.7673309087 0, 1822.7975564517574 2682873.267853401 0, 1424.8994874822993 2682871.3093063678 0, 1432.5442688101505 2683270.57538892 0, 1440.1888607093929 2683669.823295923 0, 1447.8314432683142 2684069.040314768 0, 1850.7439922273386 2684069.591119776 0, 2257.722988909524 2684069.000448099 0, 2248.8362833070732 2683670.6256722473 0)), ((3455.8455431892626 2682875.5030630757 0, 3463.4532388986904 2683272.759969386 0, 3870.5289121893675 2683267.5784294275 0, 3863.606664061292 2682869.5188334202 0, 3455.8455431892626 2682875.5030630757 0)), ((236.47474820775284 2683666.8031992353 0, 637.7116523797454 2683667.8139777663 0, 633.4070456116638 2683267.644938588 0, 233.83955206538675 2683266.1862250827 0, 236.47474820775284 2683666.8031992353 0)), ((-3417.6777773818003 2683274.60055734 0, -3416.0135255833156 2683676.514065591 0, -3014.1754051494845 2683676.7827926064 0, -3018.1874508010887 2683274.4760140674 0, -3417.6777773818003 2683274.60055734 0)), ((5101.588751731198 2684052.7620926443 0, 4695.839099557662 2684056.7940946138 0, 4701.457836598618 2684456.942234662 0, 5106.486014164929 2684453.1049528564 0, 5104.037477161907 2684252.934147923 0, 5101.588751731198 2684052.7620926443 0)), ((2673.689484060182 2684861.4009187645 0, 3080.3520430623566 2684861.0919844564 0, 3487.014895776545 2684860.7783419285 0, 3486.149774040266 2684458.1455836007 0, 3079.580141260864 2684458.6700031054 0, 2673.0103286512626 2684459.21737087 0, 2673.689484060182 2684861.4009187645 0)), ((2675.0446514598357 2685663.893965721 0, 2674.368651619193 2685263.5796309058 0, 2673.689484060182 2684861.4009187645 0, 2267.2950769636245 2684861.7325346717 0, 2266.440650033938 2684459.787399877 0, 1859.871102576042 2684460.380189284 0, 1860.9009774007502 2684862.05915012 0, 1861.9307817363458 2685263.7329876428 0, 1862.960411386893 2685665.40179497 0, 2269.0021928041383 2685664.65012255 0, 2675.0446514598357 2685663.893965721 0)), ((3082.5759505649357 2687264.07062505 0, 3082.907939134586 2687664.441864723 0, 3487.3440335022947 2687665.704985281 0, 3487.3676324344483 2687264.647758527 0, 3082.5759505649357 2687264.07062505 0)), ((998.2684010510346 2706066.267530266 0, 998.7142267459749 2706469.0704515167 0, 1402.1458548675744 2706475.293432962 0, 1402.6529933882593 2706072.394173808 0, 998.2684010510346 2706066.267530266 0)), ((3841.172606768769 2706087.964316507 0, 3839.521796802324 2706490.616138839 0, 4246.285195752414 2706489.0255209506 0, 4247.581830900716 2706087.3651774214 0, 3841.172606768769 2706087.964316507 0)), ((1804.1155716580497 2706884.50227363 0, 2210.7754551222692 2706887.3022113666 0, 2212.372712894733 2706484.177774412 0, 1805.5767395007708 2706481.5115015535 0, 1804.1155716580497 2706884.50227363 0)), ((2212.012694327966 2707686.8354237806 0, 2212.6314143693453 2708086.559291596 0, 2619.2511251877418 2708090.21324856 0, 3025.870455191995 2708093.8901692806 0, 3432.4895729825143 2708097.5624091453 0, 3431.910851741838 2707696.9932933724 0, 3025.2783066424413 2707693.6123147793 0, 2618.6457542894213 2707690.226364632 0, 2212.012694327966 2707686.8354237806 0)), ((3838.7793070041766 2707694.586730474 0, 3839.233353306072 2708095.213191078 0, 4245.977480480861 2708092.8587930105 0, 4245.647694677946 2707692.175268233 0, 3838.7793070041766 2707694.586730474 0)), ((-5106.651918404079 2711281.7034740294 0, -5107.501617508913 2711470.620925021 0, -5108.455607399276 2711682.7534461278 0, -4675.295503652894 2711682.844125988 0, -4677.184035010697 2711282.4189093523 0, -4679.073494315028 2710881.953594931 0, -4680.967637594464 2710480.7067106846 0, -4682.862738058344 2710079.4280649396 0, -5101.240216921132 2710078.5229432643 0, -5103.044339564015 2710479.58835322 0, -5104.848454811948 2710880.6487840856 0, -5105.228836937038 2710965.2330671665 0, -5106.651918333609 2711281.703458358 0, -5106.651918404079 2711281.7034740294 0)), ((4255.021903333384 2710498.7436810127 0, 3850.3880491768778 2710505.0583903505 0, 3843.870118786147 2710903.2411668384 0, 3842.4519574278183 2711305.4453184055 0, 4250.698685929169 2711303.448886601 0, 4252.865565825576 2710900.1591316117 0, 4661.6574063913 2710897.072262254 0, 4663.773030244654 2710497.092572416 0, 4255.021903333384 2710498.7436810127 0)), ((-4269.70831925989 2712890.655111386 0, -4676.320287089962 2712890.688614873 0, -5117.132716128869 2712890.719593824 0, -5120.02311810595 2713293.179542048 0, -5118.382633689577 2713293.369323318 0, -5118.382320941198 2713293.3693243014 0, -5118.392643909606 2713287.748213695 0, -4676.631346000081 2713290.5845160163 0, -4674.896648937593 2713290.5956852036 0, -4270.4090715393495 2713293.2166674216 0, -4268.579073213473 2713293.228477472 0, -3864.1897983730737 2713295.871765018 0, -3862.261885126718 2713295.8843135983 0, -3457.9707959306834 2713297.989240222 0, -3457.0075923977965 2713297.9942313256 0, -3051.7535045864397 2713300.127124115 0, -3049.932240095481 2712889.8907292085 0, -2644.888321633176 2712890.535121375 0, -2239.8440697577216 2712891.1747652455 0, -2238.445368673496 2712490.284288044 0, -2643.2956807531045 2712488.9904344073 0, -2643.535803263525 2712090.1510578045 0, -3046.3605262186784 2712085.4875751836 0, -3048.145940448636 2712487.691730232 0, -3455.1020574277586 2712487.776043136 0, -3862.058160765678 2712487.855847102 0, -4269.007270750511 2712487.9303149693 0, -4269.70831925989 2712890.655111386 0)), ((4258.5777549818595 2712505.44122695 0, 4658.248838942368 2712500.2307842523 0, 4658.348320051825 2712100.523392187 0, 4253.635103178385 2712105.807845356 0, 4258.5777549818595 2712505.44122695 0)), ((-1836.0148288950045 2713296.0281345397 0, -1430.7683162261403 2713294.707195535 0, -1427.9208151375617 2712892.491884259 0, -1425.0914209221282 2712492.868953733 0, -1831.7684270770046 2712491.579166733 0, -1833.8809975115978 2712891.8356715976 0, -1836.0148288950045 2713296.0281345397 0)), ((3033.2239233042237 2713286.675944311 0, 3439.5777274196394 2713285.9191595083 0, 3434.609641684605 2712914.106807696 0, 3030.1547177381285 2712913.115378526 0, 3032.876518482947 2713286.6765549146 0, 3033.2239233042237 2713286.675944311 0)), ((191.24675436282772 2713682.2688071155 0, 188.1100455757981 2713281.8331672493 0, -216.60997828050702 2713285.017712498 0, -621.3299425510596 2713288.2247412466 0, -618.8584316213498 2713688.351987669 0, -213.8058691205999 2713685.313281258 0, -211.0013515317427 2714085.5898771165 0, 194.38379128553382 2714082.7006832794 0, 191.24675436282772 2713682.2688071155 0)), ((-1649.9456180682266 2715295.421635402 0, -1618.1799364685733 2715495.3742659106 0, -1582.7676239280281 2715597.3847823306 0, -1702.5530287301283 2715689.4910429125 0, -1703.783319452899 2715696.3169638338 0, -1720.2774801544037 2715787.8343663174 0, -1781.052836937852 2715879.9153260333 0, -1781.240398412982 2715999.763944685 0, -1710.7693077944662 2716092.3242227477 0, -1711.6825030898558 2716095.916031599 0, -1747.717082071063 2716237.6539940974 0, -1852.8649537851527 2716255.7991800443 0, -1856.8632074523973 2716498.0741839157 0, -1453.9115417504436 2716496.8841965348 0, -1438.9683756533925 2716092.8599919737 0, -1032.640313329464 2716090.7936810893 0, -1030.0297502254796 2715692.5462534055 0, -621.3591906385346 2715688.702142325 0, -616.3861447072471 2715289.2109832875 0, -611.4437058543614 2714888.647759559 0, -613.9151646126546 2714488.5635543303 0, -1019.6342010151255 2714491.2756021745 0, -1021.7725612321208 2714091.3539768253 0, -1023.9110516341043 2713691.413760786 0, -1428.962687071269 2713694.469403211 0, -1427.1582102463103 2714094.2285999577 0, -1425.3525812221044 2714493.9824845614 0, -1423.5471298473424 2714893.73160047 0, -1431.1394687405632 2715294.5275185746 0, -1649.9456180682266 2715295.421635402 0)), ((-2402.352077579976 2716099.334853069 0, -2413.36844541935 2716093.0382219893 0, -2294.4589538125874 2715931.276844202 0, -2323.360583455664 2715698.643016867 0, -2653.4612891532324 2715699.8776385793 0, -2658.113847241481 2716100.2091913237 0, -2662.766312008028 2716500.5218182127 0, -2259.814975757727 2716499.286982927 0, -2255.5264929878385 2716194.363314527 0, -2276.609240628882 2716171.2053056955 0, -2402.352077579976 2716099.334853069 0)), ((-5114.516344134941 2715699.591771844 0, -5114.1675727356105 2716099.560706577 0, -5114.174559426497 2716101.073244287 0, -5115.874814454032 2716469.1587783494 0, -5115.884030242105 2716502.5500650387 0, -4686.082284763518 2716502.3401412563 0, -4683.377929902097 2716101.1767004402 0, -4680.674335148573 2715699.9810619885 0, -5114.516344134941 2715699.591771844 0)), ((-3875.8999535398907 2716502.014269519 0, -3470.8088823478374 2716501.8857303634 0, -3065.717853351423 2716501.7795600616 0, -3062.045100201077 2716101.586174578 0, -3467.378483349269 2716101.4740142776 0, -3872.711936780993 2716101.356873321 0, -3875.8999535398907 2716502.014269519 0)), ((4259.173389040151 2716499.602358147 0, 4257.897788135917 2716900.911863932 0, 4663.67512608057 2716902.714408253 0, 4664.329278431304 2716501.0692761866 0, 4259.173389040151 2716499.602358147 0)), ((-1858.049349993421 2716904.4505387424 0, -1859.2356445559512 2717310.808105758 0, -1456.0861838246765 2717311.674963512 0, -1454.9990194379297 2716904.2820678363 0, -1858.049349993421 2716904.4505387424 0)), ((-225.4412341625802 2717696.122938931 0, -225.44136625068052 2717696.249909394 0, -224.62921019346118 2717696.1078722137 0, -221.7764295375716 2717695.6090442045 0, 45.99379118113641 2717632.0475321608 0, 138.95106175224706 2717689.342302194 0, 184.31465186959124 2717688.4978438085 0, 183.39742742500147 2717287.304102903 0, -225.2399847123634 2717293.385876797 0, -633.8775431778841 2717299.4627628666 0, -635.1967975754217 2717703.743030767 0, -225.4412341625802 2717696.122938931 0)), ((15079.501850495779 2667400.911845348 0, 15125.666890252996 2667311.980604434 0, 15191.120772676088 2667284.6512994124 0, 15210.063621884934 2667269.0161402402 0, 15210.858954446136 2667181.2885950194 0, 14765.698578201169 2667179.4144756533 0, 14762.364038258156 2667582.408584772 0, 14847.975366687539 2667583.0539863487 0, 14841.385369952295 2667452.791058091 0, 15079.501850495779 2667400.911845348 0)), ((16250.437263109736 2667185.688715323 0, 16212.863384605109 2667216.180548536 0, 16107.166205849237 2667337.9112681528 0, 16023.860067014903 2667301.8384443605 0, 16019.831808211695 2667265.730373721 0, 16016.703916299599 2667591.844295529 0, 16421.459554043173 2667594.8802448865 0, 16425.48372246775 2667186.4313854077 0, 16250.437263109736 2667185.688715323 0)), ((13948.867468892431 2667984.6879084967 0, 14353.948960351807 2667985.0449518133 0, 14356.537747320093 2667581.979590327 0, 13950.711097539757 2667581.5463382415 0, 13544.88449625694 2667581.1087441025 0, 13543.786105052044 2667984.353232905 0, 13948.867468892431 2667984.6879084967 0)), ((15495.80898399944 2667993.3461896866 0, 15608.162694162504 2667994.556954945 0, 16012.799302952984 2667998.9426411623 0, 16016.703916299599 2667591.844295529 0, 15611.948077044612 2667588.8040282903 0, 15339.127594443033 2667586.7523486507 0, 15341.644186387613 2667594.4185282057 0, 15354.556646538535 2667638.9483704814 0, 15387.566679094865 2667696.8993172334 0, 15432.158450588911 2667778.4519989695 0, 15526.672760607735 2667825.8039362514 0, 15495.80898399944 2667993.3461896866 0)), ((17830.08146852741 2669760.683438869 0, 17649.05768640751 2669777.0741732577 0, 17631.565247529103 2669617.8104476244 0, 17633.997077992266 2670020.34696265 0, 18037.79208556993 2670022.324691535 0, 18035.31636994485 2669619.136690924 0, 17875.953747805626 2669618.6137737106 0, 17830.08146852741 2669760.683438869 0)), ((14768.977026613255 2670388.4224988976 0, 14770.948934927701 2669988.3990127323 0, 14361.0257746289 2669995.3652410023 0, 14188.502483820428 2669998.3039836264 0, 14305.200836025242 2670054.2689221795 0, 14360.454752604344 2670104.4469125723 0, 14459.501902742279 2670194.3941970877 0, 14392.330452011978 2670240.163269429 0, 14359.827510695948 2670224.2641465412 0, 14358.931950126587 2670395.300505628 0, 14768.977026613255 2670388.4224988976 0)), ((15982.398502089718 2671996.7309447806 0, 16386.891446308186 2672004.6743460796 0, 16390.790187731553 2671611.734047498 0, 15986.386770171996 2671605.9186339066 0, 15982.398502089718 2671996.7309447806 0)), ((14352.435077189672 2671983.181671434 0, 14352.224013645891 2672371.435161358 0, 14759.808406016065 2672357.1248954944 0, 14761.435499449008 2671972.796652494 0, 14352.435077189672 2671983.181671434 0)), ((17639.318406072478 2675987.607339894 0, 17643.392109364686 2676387.886543175 0, 18046.26375822212 2676389.8389650537 0, 18042.45093777533 2675989.1689838255 0, 17639.318406072478 2675987.607339894 0)), ((14413.950944558499 2676344.7981293434 0, 14419.429425159593 2676743.432690209 0, 14830.110234988155 2676735.110527663 0, 14823.781228980388 2676335.599639608 0, 14413.950944558499 2676344.7981293434 0)), ((5043.858294920456 2677630.709189919 0, 5538.680446440614 2677627.831867304 0, 5944.22467263026 2677625.4685462583 0, 5938.965806168243 2677226.9173046453 0, 5534.944850585622 2677228.6367265102 0, 5043.958277677374 2677230.7203423693 0, 5043.858294920456 2677630.709189919 0)), ((14458.96357176142 2680338.908785741 0, 14459.992977810683 2680740.223605747 0, 14870.501341395266 2680736.0568875275 0, 14870.820254864704 2680333.8588010394 0, 14458.96357176142 2680338.908785741 0)), ((16050.83168322219 2684343.462719235 0, 16044.58080873297 2684743.49997516 0, 16448.26209559142 2684745.254399555 0, 16455.014089451728 2684345.5851647467 0, 16050.83168322219 2684343.462719235 0)), ((18064.93140508903 2684773.3330952954 0, 18056.64674919042 2685174.1869721995 0, 18455.458325242198 2685173.716147613 0, 18462.604457031957 2684772.805884849 0, 18064.93140508903 2684773.3330952954 0)), ((6399.911934908316 2684824.6959309313 0, 5990.868503157693 2684833.7125557074 0, 5987.686570742631 2685231.4931133687 0, 5984.505287553653 2685629.2170933248 0, 6392.278881404925 2685617.948536389 0, 6396.095641197958 2685221.337491395 0, 6804.5040338186 2685211.177146352 0, 6808.955447117598 2684815.6740054963 0, 6399.911934908316 2684824.6959309313 0)), ((5576.73096105953 2685640.5076097576 0, 5574.186618246233 2686039.3547491203 0, 5981.323657273146 2686026.9363154173 0, 5984.505287553653 2685629.2170933248 0, 5576.73096105953 2685640.5076097576 0)), ((18094.60930537767 2686272.6232533487 0, 18136.337536053034 2686109.609611235 0, 18100.22394129301 2686054.099339751 0, 18039.11985384811 2686093.1248439457 0, 18036.793375254492 2686377.4029910318 0, 18438.40066455692 2686377.0248764483 0, 18441.197964693434 2685975.454465967 0, 18411.85774471977 2685975.484722507 0, 18414.281707821112 2686075.47883292 0, 18438.61011432442 2686180.806094717 0, 18328.79169006953 2686319.1780334767 0, 18293.469005068087 2686367.92355676 0, 18216.312201170203 2686352.106225105 0, 18174.496124258203 2686303.269197429 0, 18084.434667421552 2686315.498731412 0, 18094.60930537767 2686272.6232533487 0)), ((9757.617694161461 2687748.8867081027 0, 9752.912573017042 2687812.3713740297 0, 9809.99251404404 2687868.836168498 0, 9842.736504109951 2687888.670693366 0, 9866.846198967809 2687918.1370489956 0, 9868.55862330926 2687927.8645071695 0, 10025.266346764902 2687923.554683998 0, 10030.775277616185 2687525.8802808467 0, 9626.302538349495 2687535.950591208 0, 9625.222165730322 2687621.2640673453 0, 9688.71839456967 2687557.789856814 0, 9769.461858185103 2687564.7714799345 0, 9821.699850100742 2687598.9525585975 0, 9855.846723816974 2687660.001203148 0, 9829.586884813207 2687713.693975444 0, 9780.221945131274 2687723.534390778 0, 9757.617694161461 2687748.8867081027 0)), ((20443.3028628736 2687586.371680449 0, 20041.32598418925 2687583.5210404084 0, 20040.29140951473 2687982.3402563483 0, 20039.256856533208 2688381.1406538524 0, 20440.432441648754 2688384.847955336 0, 20441.867668474377 2687985.612067682 0, 20443.3028628736 2687586.371680449 0)), ((17832.1715950558 2690039.5518426816 0, 17873.625918772523 2690071.73188395 0, 17863.72857082412 2690141.080796169 0, 17894.80372434661 2690225.8250616076 0, 17952.78078221775 2690307.9989660927 0, 18006.783260803368 2690343.534066388 0, 18007.86092477352 2689973.4960319065 0, 17608.94248657115 2689968.850090002 0, 17607.954287781853 2690223.1475237035 0, 17727.31607366602 2690050.051828257 0, 17832.1715950558 2690039.5518426816 0)), ((5962.16379607039 2690841.1623292356 0, 5959.722312819952 2691241.1190262316 0, 6365.8830732785145 2691229.7663953453 0, 6367.586316556753 2690829.6923118155 0, 5962.16379607039 2690841.1623292356 0)), ((8383.09897757985 2691978.113463563 0, 8380.675440758812 2692378.948162184 0, 7977.433821210296 2692392.439634175 0, 7978.304519062915 2692789.062010852 0, 8381.457501985777 2692779.7847833694 0, 8787.765956236552 2692764.539263972 0, 8783.749577303544 2692363.6513578077 0, 8786.605085872568 2691963.149060149 0, 8383.09897757985 2691978.113463563 0)), ((10006.656624822906 2692743.5703330548 0, 10006.148483262275 2693167.8273011874 0, 10409.87651692492 2693166.7346429247 0, 10410.531604089409 2692744.273491583 0, 10006.656624822906 2692743.5703330548 0)), ((12820.230571030992 2693987.1397618665 0, 13220.698438218798 2693978.8834125823 0, 13220.438750020374 2693560.731732215 0, 12820.317281149624 2693565.659423673 0, 12820.230571030992 2693987.1397618665 0)), ((13215.127118235887 2700399.666562965 0, 13215.227855665682 2700802.1199340294 0, 13619.990253904578 2700795.658400593 0, 13620.88687039511 2700393.2762028207 0, 13215.127118235887 2700399.666562965 0)), ((16392.840605276408 2703596.5060888682 0, 16383.125101629521 2703997.62602151 0, 16785.850806478826 2703997.951237007 0, 16795.870516859217 2703596.94585355 0, 16392.840605276408 2703596.5060888682 0)), ((15975.207072759222 2703997.9543919303 0, 15965.459065785224 2704399.226921988 0, 16373.410834087772 2704398.741124809 0, 16383.125101629521 2703997.62602151 0, 15975.207072759222 2703997.9543919303 0)), ((14827.086485329473 2706384.7014311543 0, 14827.310022861895 2706777.6348382668 0, 15131.254753312056 2706780.614523737 0, 15130.551474041911 2706386.371219829 0, 14827.086485329473 2706384.7014311543 0)), ((7522.227589090743 2708066.9255449134 0, 7520.158680293587 2708467.9552760525 0, 7923.556393586471 2708466.0656237192 0, 7925.689286587144 2708064.3484900966 0, 7522.227589090743 2708066.9255449134 0)), ((16745.75995483178 2709988.8745242865 0, 16746.667418866586 2710393.857344907 0, 17153.54681341561 2710392.589243589 0, 17152.271366804034 2709987.066847501 0, 16745.75995483178 2709988.8745242865 0)), ((6304.264438979591 2712077.884363088 0, 6709.28915354734 2712072.1646806276 0, 6708.662774980455 2711672.191079046 0, 6304.349176872272 2711677.7776579163 0, 5900.0361394553265 2711683.3870479646 0, 5899.240417419743 2712083.6000901195 0, 6304.264438979591 2712077.884363088 0)), ((5067.319587614606 2712095.3252380895 0, 5066.277108903527 2712495.7629549075 0, 5494.685530606004 2712492.570208957 0, 5495.203892548303 2712090.776470419 0, 5067.319587614606 2712095.3252380895 0)), ((14802.43948004929 2714817.140624798 0, 14799.629966355671 2715216.3170601483 0, 14796.820658031116 2715615.4887292874 0, 15106.672545318035 2715616.7386727654 0, 15515.044486057697 2715618.3820719235 0, 15519.28731555198 2715220.1142183505 0, 15523.530421567928 2714821.841619475 0, 15119.104680751328 2714819.1961925817 0, 14802.43948004929 2714817.140624798 0)), ((12785.367357945022 2714839.243365424 0, 12778.028915937308 2715236.0972862532 0, 13181.373092528867 2715227.4012877173 0, 13189.212136702059 2714828.9145913515 0, 12785.367357945022 2714839.243365424 0)), ((19994.04610420238 2715185.5830227 0, 19991.993523887522 2715584.4885022948 0, 20397.81477682427 2715588.3003217042 0, 20397.63390720022 2715188.541757956 0, 19994.04610420238 2715185.5830227 0)), ((19171.838315983867 2716377.6469778386 0, 19168.059939930412 2716789.0019131415 0, 19576.440094002144 2716781.513537892 0, 19581.203435945397 2716369.2471883143 0, 19171.838315983867 2716377.6469778386 0)), ((20377.201750580276 2717598.8714839485 0, 20384.210267780993 2717193.925981193 0, 20013.00878703776 2717193.859437133 0, 20090.18921685623 2717263.3915806734 0, 19988.472462192796 2717548.6466629165 0, 19955.256397845413 2717602.601635659 0, 19972.05813135294 2717602.4532160163 0, 19966.17255585521 2718011.0342926322 0, 20370.193050922833 2718003.8116252488 0, 20377.201750580276 2717598.8714839485 0)), ((7880.287644520213 2717686.3839548663 0, 7877.502471846527 2718086.0268312832 0, 8283.264371112695 2718079.7193653136 0, 8285.493700064386 2717684.7793571926 0, 7880.287644520213 2717686.3839548663 0)), ((17143.136432501247 2718851.854545071 0, 17144.202373201148 2719250.693087528 0, 17145.268861881665 2719649.526274158 0, 17138.22853807499 2720049.3402349 0, 17536.18847418455 2720047.1827014093 0, 17540.601504212802 2719647.0594305797 0, 17540.63320173533 2719246.571066197 0, 17540.665010196175 2718846.0642567384 0, 17143.136432501247 2718851.854545071 0)), ((14365.029125951763 2719623.039628195 0, 13958.362885241737 2719629.1218747017 0, 13957.991485826433 2720032.389292792 0, 13957.619754289239 2720435.6511978353 0, 14362.950120561516 2720431.214218232 0, 14364.122307525207 2720028.861460987 0, 14365.029125951763 2719623.039628195 0)), ((9491.60155904921 2721276.076987971 0, 9489.432853290962 2721679.294584789 0, 9894.283104601725 2721674.779063306 0, 9897.325460810427 2721271.338466534 0, 9491.60155904921 2721276.076987971 0)), ((18736.208666899285 2721676.6144660674 0, 18734.891654079587 2722051.826046071 0, 19136.588965145314 2722056.2822198295 0, 19139.57401460323 2721654.9095463166 0, 18790.92133692967 2721651.352431548 0, 18746.635856455418 2721676.7592725707 0, 18736.208666899285 2721676.6144660674 0)), ((21672.095659978957 2665350.4282260244 0, 21672.086531502355 2665372.293954613 0, 21672.002551113914 2665572.198931443 0, 22059.960606851728 2665564.6437839186 0, 22059.51012393185 2665167.59760149 0, 22042.28568617821 2665168.139391153 0, 21979.807829336783 2665167.291337973 0, 21994.721507906586 2665202.3508685934 0, 22029.89727967998 2665381.3843977274 0, 21931.68197265437 2665532.912427275 0, 21812.327495206817 2665534.558848511 0, 21765.219748988056 2665459.200083126 0, 21729.44806997073 2665442.17642127 0, 21672.095659978957 2665350.4282260244 0)), ((22526.39306199842 2668392.650090327 0, 22571.531054147057 2668431.9261325086 0, 22601.43999812779 2668557.036422714 0, 22467.527157841312 2668601.5973549234 0, 22362.588536156494 2668636.5161758307 0, 22265.193535352802 2668608.130263837 0, 22186.23592688549 2668589.485017691 0, 22136.24419039 2668513.050294867 0, 22066.49272276504 2668462.3599507613 0, 22068.446639537877 2668726.159225186 0, 22468.719284162424 2668724.630279338 0, 22472.577107835903 2669122.7334815585 0, 22476.43435871928 2669520.8054370214 0, 22878.516806908323 2669518.220935466 0, 22873.75495539628 2669120.661552744 0, 22868.992262921827 2668723.0972213857 0, 22864.22911954068 2668325.528257113 0, 22464.861288350457 2668326.509093097 0, 22461.436513251225 2667936.855417234 0, 22458.011782350834 2667547.184071324 0, 22063.41142481525 2667548.628132555 0, 22064.452367454378 2667938.072487041 0, 22064.866843109572 2668093.024994244 0, 22087.812256035013 2668099.9010696686 0, 22251.251893170476 2668178.331044052 0, 22318.909450994066 2668238.3963519 0, 22336.464665231382 2668326.8292036676 0, 22377.00661620023 2668455.2155561815 0, 22526.39306199842 2668392.650090327 0)), ((21238.062742160102 2672362.930049306 0, 21642.699803803214 2672353.536105773 0, 21649.843835256223 2671955.7597573567 0, 21656.987634893936 2671557.964977879 0, 21252.146787717928 2671569.7579869293 0, 21245.104343659616 2671966.3461281485 0, 21238.062742160102 2672362.930049306 0)), ((23233.557563243914 2677306.346060751 0, 23082.518714103106 2677307.2123584705 0, 22932.835304386874 2677442.3850612105 0, 22930.10024565291 2677482.6121738856 0, 22873.135289436876 2677539.7261577803 0, 22873.45513215189 2677603.2231258126 0, 23277.6756393173 2677600.10813607 0, 23276.291406722252 2677269.08311469 0, 23233.557563243914 2677306.346060751 0)), ((22361.541615464164 2678131.308724134 0, 22443.312103270844 2678138.6495944164 0, 22465.556612685996 2678205.6963616014 0, 22466.659101666002 2678285.9859404014 0, 22460.191065290033 2678325.510705349 0, 22449.944183092568 2678374.4871553318 0, 22450.21983220639 2678394.559488821 0, 22448.53386465906 2678399.633472604 0, 22468.488240851788 2678399.6887218244 0, 22462.815185186064 2678003.6075812285 0, 22050.144745821603 2678000.862586919 0, 22053.310914273978 2678181.018962657 0, 22088.65612681045 2678163.2921830253 0, 22127.28547799425 2678149.778922786 0, 22159.78535174015 2678108.4195764763 0, 22219.17341173864 2678092.642262964 0, 22266.327219458064 2678094.8594078356 0, 22321.71368324477 2678121.444521027 0, 22361.541615464164 2678131.308724134 0)), ((21248.36970233172 2685980.628674969 0, 21652.294354918202 2685978.034577255 0, 21653.517930722817 2685578.1925358097 0, 21249.516926402557 2685581.2547017853 0, 21248.36970233172 2685980.628674969 0)), ((20846.84784678621 2686381.608176658 0, 20846.324936369674 2686784.181338925 0, 21247.81286830698 2686786.3944675643 0, 21248.09128594254 2686383.514008659 0, 20846.84784678621 2686381.608176658 0)), ((21649.88512991329 2688388.9431185103 0, 21647.96200389764 2688788.7994424985 0, 22055.228065565476 2688785.2986972253 0, 22056.887436198034 2688385.6325590163 0, 21649.88512991329 2688388.9431185103 0)), ((21240.695987252886 2688792.294844053 0, 21240.013952181373 2688917.108323467 0, 21283.321607611946 2688954.86373636 0, 21273.553858226376 2689054.4134390554 0, 21312.608422000754 2689135.3807898764 0, 21291.7948801089 2689191.8511573537 0, 21646.03889336303 2689188.636614877 0, 21647.96200389764 2688788.7994424985 0, 21240.695987252886 2688792.294844053 0)), ((21644.23998371618 2689578.272499468 0, 22051.509184007904 2689575.0818125755 0, 22053.56858350532 2689184.9598181364 0, 21646.03889336303 2689188.636614877 0, 21644.23998371618 2689578.272499468 0)), ((21232.34872532887 2690750.746599673 0, 21638.837245605 2690748.503476382 0, 22045.326068598206 2690746.283301461 0, 22047.387821246793 2690355.7437071516 0, 21640.639157350506 2690358.206040195 0, 21233.890748772475 2690360.6634465405 0, 21232.34872532887 2690750.746599673 0)), ((21639.208461658516 2691147.4002783964 0, 21639.579752169004 2691546.278047918 0, 22045.07389786588 2691544.0359015004 0, 22045.199926743804 2691145.1618523286 0, 21639.208461658516 2691147.4002783964 0)), ((23226.575169089832 2696036.708609112 0, 23150.430370563205 2696200.070948086 0, 23009.39260196048 2696310.0075473674 0, 23224.045232100492 2696311.012287523 0, 23627.058679142625 2696312.8949512797 0, 23633.279092870616 2695915.5534111713 0, 23326.99086647538 2695915.184468969 0, 23226.575169089832 2696036.708609112 0)), ((22002.504304606646 2696705.3661034345 0, 21596.743107050333 2696706.235865666 0, 21589.651204900736 2697102.605961009 0, 21591.713483730593 2697501.296876686 0, 21997.38648802732 2697501.3579260954 0, 22403.059959762424 2697501.4416328142 0, 22401.231345531633 2697099.6485378286 0, 22408.265644450326 2696704.5189842856 0, 22002.504304606646 2696705.3661034345 0)), ((22401.794765157432 2706780.4998695026 0, 21997.848440500948 2706787.234221662 0, 22000.680687837634 2707189.2289537825 0, 22003.513038443056 2707591.21841288 0, 22406.005657508904 2707583.3601349206 0, 22403.90025830444 2707181.939450402 0, 22401.794765157432 2706780.4998695026 0)), ((22410.54812813725 2708786.4320440646 0, 22401.8252175175 2708390.768550851 0, 22394.40303404622 2708385.338074282 0, 22009.165428940538 2708393.413618841 0, 22012.350819990817 2708792.0905121784 0, 22410.54812813725 2708786.4320440646 0)), ((22828.434004623694 2709588.7140895724 0, 22977.127390372654 2709482.18863001 0, 22973.449147104748 2709402.0783697325 0, 23098.609703089154 2709377.6827498274 0, 23192.482053936867 2709428.1301585827 0, 23233.27105311363 2709502.1027587685 0, 23226.52107775667 2709174.941936698 0, 22823.25449040109 2709184.677679324 0, 22828.434004623694 2709588.7140895724 0)), ((22013.055636146997 2711588.19436297 0, 22420.166229923485 2711583.5662361635 0, 22422.07034114094 2711184.656227873 0, 22015.277082351273 2711187.6367293787 0, 22013.055636146997 2711588.19436297 0)), ((22420.166229923485 2711583.5662361635 0, 22423.312718587167 2711982.7058012057 0, 22832.492621021636 2711977.354743092 0, 22827.27733910165 2711578.9613630553 0, 22420.166229923485 2711583.5662361635 0)), ((20802.38715176861 2712405.3168605864 0, 21202.086186972207 2712399.907491889 0, 21200.461495763215 2711998.715649977 0, 21607.297157999412 2711993.3862271537 0, 21605.945782625487 2711592.845154835 0, 21198.83635357114 2711597.5189974555 0, 20800.035805611144 2711609.255313006 0, 20401.23662399326 2711621.0135896066 0, 20401.96246907941 2712015.8698570635 0, 20402.688063687085 2712410.721382355 0, 20802.38715176861 2712405.3168605864 0)), ((22017.362462900226 2713185.8663945086 0, 22425.72653559047 2713187.6505632205 0, 22426.09508279207 2712782.2914511976 0, 22016.287898943185 2712787.3123977995 0, 22017.362462900226 2713185.8663945086 0)), ((21205.28140417238 2713189.095065119 0, 21206.765638147455 2713588.43038808 0, 21612.04103255767 2713587.915965496 0, 21611.321773924778 2713187.4694403093 0, 21205.28140417238 2713189.095065119 0)), ((21610.71529260665 2714390.403757304 0, 22017.22492195067 2714390.378172485 0, 22017.270712843423 2713988.9213646604 0, 22017.316423672222 2713587.3964814483 0, 21612.04103255767 2713587.915965496 0, 21612.76016174718 2713</t>
+          <t>MULTIPOLYGON Z (((-1050634.2762595804 2312278.921033107 0, -1050692.1496858974 2311878.8901095935 0, -1050749.8418575835 2311480.125285387 0, -1050805.7506747406 2311081.4597527836 0, -1050861.6613238936 2310682.782564328 0, -1051255.859984779 2310743.4741963 0, -1051200.1037733245 2311141.4396161498 0, -1051144.3479498741 2311539.4029425895 0, -1051088.5929212286 2311937.360776254 0, -1051032.8378361643 2312335.3193941107 0, -1050634.2762595804 2312278.921033107 0)), ((-1042827.6080114043 2324641.903880159 0, -1042429.0177734202 2324582.6384197455 0, -1042031.3687667405 2324523.506086521 0, -1042088.8292028453 2324128.4938440737 0, -1042087.857374831 2324128.3551963973 0, -1042088.6925061723 2324122.6112281634 0, -1041689.879792263 2324063.533034388 0, -1041292.0584445689 2324004.6261834027 0, -1041350.0240442571 2323614.889880292 0, -1041351.4699388619 2323605.1686712345 0, -1041409.4806173473 2323215.144439011 0, -1041410.9986382548 2323205.724764946 0, -1041473.7604708544 2322816.272943921 0, -1041472.3642102741 2322816.089643594 0, -1041473.7990416642 2322807.2053701356 0, -1041125.9567855056 2322761.754220014 0, -1040731.5802114733 2322710.2174758688 0, -1040791.3933385293 2322318.3149438472 0, -1040792.477179104 2322310.396591345 0, -1040846.3585751874 2321916.7483948767 0, -1040845.4352658397 2321916.6246562605 0, -1040846.3829309222 2321909.7169102994 0, -1041243.1470202254 2321962.8195580887 0, -1041593.576394404 2322009.7149099344 0, -1041991.033277303 2322068.01460237 0, -1042388.4929601529 2322126.307653034 0, -1042333.4848828288 2322526.274883522 0, -1041935.8066824579 2322467.5824857615 0, -1041873.028642868 2322866.373482969 0, -1041810.2530178527 2323265.1530656577 0, -1042211.0342654212 2323324.8051944994 0, -1042607.2119206154 2323383.7695842357 0, -1042547.2426509934 2323783.4970818204 0, -1042944.6907629055 2323842.7817654843 0, -1042886.3057913377 2324240.829846611 0, -1043285.130652052 2324298.636963205 0, -1043226.2979992016 2324699.977115077 0, -1042827.6080114043 2324641.903880159 0)), ((-1046247.5562064119 2329220.6481662146 0, -1046191.3633868239 2329622.789430642 0, -1046593.9948730316 2329678.6363939364 0, -1046534.9886577296 2330080.588037373 0, -1046475.9821583936 2330482.5278504863 0, -1046073.6083994912 2330426.0280175335 0, -1046132.4852626884 2330024.4114558683 0, -1045729.9819064847 2329968.257709795 0, -1045788.7291921459 2329566.9681130997 0, -1045845.5922356682 2329165.063035892 0, -1045443.6285155453 2329109.4754572785 0, -1045501.1639552393 2328707.7760154633 0, -1045558.6997935177 2328306.0742610637 0, -1045616.2362395419 2327904.37012149 0, -1045617.0326782259 2327904.479360659 0, -1045616.9327830005 2327905.1956020826 0, -1046016.0937759206 2327959.9533524564 0, -1045959.3246830138 2328361.192974082 0, -1045902.4578365213 2328763.1402011085 0, -1046303.7496655369 2328818.5044084494 0, -1046247.5562064119 2329220.6481662146 0)), ((-1059727.8355241397 2337697.3455502763 0, -1059668.8527381408 2338098.124818296 0, -1060067.131052015 2338153.3211093354 0, -1060465.4090640997 2338208.5355003844 0, -1060410.0971186836 2338610.1316959243 0, -1060354.7856983019 2339011.7223898345 0, -1059956.6096501015 2338955.955333517 0, -1059558.4318289415 2338900.184331322 0, -1059613.6421632078 2338499.155718323 0, -1059215.414667514 2338443.6841478753 0, -1058817.1846679002 2338388.2147207656 0, -1058872.287569143 2337987.7950442224 0, -1058931.3390659136 2337587.2694612537 0, -1058534.796627428 2337532.90503816 0, -1058592.9067027688 2337132.182809552 0, -1058194.7240368775 2337077.520104881 0, -1058252.2701342073 2336676.4067847277 0, -1058650.7321761935 2336731.296394675 0, -1059049.4432704628 2336786.216981644 0, -1058990.3909251 2337186.7443455644 0, -1059388.6021759196 2337241.6571514467 0, -1059329.5859732355 2337642.3091146755 0, -1059727.8355241397 2337697.3455502763 0)), ((-1066371.9632855507 2339438.2108617574 0, -1066373.429756151 2339438.414318711 0, -1066325.9659184492 2339779.1937124613 0, -1066316.6288095424 2339775.4830386983 0, -1066201.70517481 2339740.4795712177 0, -1066022.4006281008 2339615.323439348 0, -1065949.3493714838 2339578.6985750943 0, -1065929.2570379518 2339568.627267384 0, -1065850.4238185033 2339539.308687006 0, -1065748.3028524022 2339468.346541264 0, -1065676.2207522886 2339424.8367052525 0, -1065654.1213722434 2339415.392399067 0, -1065606.175104046 2339412.400131573 0, -1065571.9863841333 2339376.9328016816 0, -1065578.765703502 2339328.3709718734 0, -1065775.329001942 2339355.539352133 0, -1065828.8039514287 2338960.7937077926 0, -1066028.005994407 2338986.8329564976 0, -1066000.9377325266 2339187.759105069 0, -1066398.6148282972 2339240.822932089 0, -1066371.9632855507 2339438.2108617574 0)), ((-1061837.3204676933 2340034.6030477574 0, -1061780.3655670825 2340436.5922139487 0, -1061723.408817523 2340838.5788117982 0, -1061325.3843199636 2340783.392501526 0, -1060927.3602048056 2340728.202607241 0, -1060529.3384876326 2340673.0124064325 0, -1060131.31556903 2340617.8150917715 0, -1060187.739295776 2340216.35853855 0, -1060244.1628082008 2339814.9025566597 0, -1060299.4740761493 2339413.3136684936 0, -1060354.7856983019 2339011.7223898345 0, -1060752.5765780364 2339066.2638833597 0, -1061150.3704149113 2339120.8020020006 0, -1061548.164748814 2339175.3363516834 0, -1061945.959765405 2339229.8670557295 0, -1061891.6412659038 2339632.23640928 0, -1061837.3204676933 2340034.6030477574 0)), ((-1035118.4999299524 2281190.209319271 0, -1035513.4719348657 2281246.333069391 0, -1035908.4437363615 2281302.455823209 0, -1035850.9664973858 2281705.0788636506 0, -1035456.3629951405 2281647.737895494 0, -1035061.7616243811 2281590.3958082073 0, -1035118.4999299524 2281190.209319271 0)), ((-1016227.3939126243 2286441.674483058 0, -1016170.7846368499 2286843.4743179535 0, -1016116.572680074 2287240.187457348 0, -1015719.7979054934 2287188.6790665807 0, -1015774.9398044108 2286789.754045181 0, -1015830.8571983477 2286390.9832253153 0, -1016227.3939126243 2286441.674483058 0)), ((-1033898.8322515577 2287115.5060672923 0, -1034294.5248291742 2287171.182248576 0, -1034242.4095084692 2287571.8515250664 0, -1034188.3680121511 2287971.6597832455 0, -1033792.6131830172 2287916.5542716077 0, -1033846.4969216322 2287516.1923875464 0, -1033898.8322515577 2287115.5060672923 0)), ((-1035482.4640965455 2287333.0698815673 0, -1035431.1532593278 2287732.771150824 0, -1035380.0460347141 2288135.9017904988 0, -1034981.6506295949 2288083.604406882 0, -1035034.2370944343 2287683.1639975063 0, -1035085.9019275007 2287282.590195216 0, -1035482.4640965455 2287333.0698815673 0)), ((-1031335.8145355216 2288032.690707102 0, -1031735.973979156 2288083.6424779366 0, -1031684.4242973576 2288486.76042762 0, -1031283.7416613278 2288434.873665544 0, -1030883.0524479783 2288383.0092891282 0, -1030935.6500580298 2287981.7333433605 0, -1031335.8145355216 2288032.690707102 0)), ((-1029690.6327695481 2288227.9861841374 0, -1030081.6691394955 2288279.3375122994 0, -1030031.1897501762 2288680.060399877 0, -1029980.707957195 2289080.780604471 0, -1029580.5337932236 2289031.2535202373 0, -1029632.4103333049 2288630.7904119412 0, -1029690.6327695481 2288227.9861841374 0)), ((-1019437.7014199753 2308499.869161773 0, -1019385.3452084363 2308902.469899386 0, -1018988.0279197779 2308849.793594077 0, -1019040.5066439967 2308447.541076709 0, -1019437.7014199753 2308499.869161773 0)), ((-1015746.4921843759 2314958.970178708 0, -1015693.6757171493 2315360.0135502284 0, -1015496.280137871 2315334.935964606 0, -1015549.3098236041 2314933.92679566 0, -1015746.4921843759 2314958.970178708 0)), ((-1016826.8467043939 2315911.7043980435 0, -1016432.4276351677 2315861.5429225443 0, -1016486.7752965459 2315461.576262847 0, -1016486.8862928433 2315460.7593977996 0, -1016514.1169489527 2315260.3583780047 0, -1016541.2452727675 2315060.7104614796 0, -1016540.278824313 2315060.5877280417 0, -1016540.3865441052 2315059.796102671 0, -1016740.1515403495 2315085.1658760984 0, -1016712.3379686448 2315285.539725222 0, -1016811.9507220382 2315298.1938166893 0, -1016911.5634863044 2315310.847821505 0, -1016883.2160986736 2315511.120703014 0, -1016883.3611283406 2315511.1391318156 0, -1016826.8467043939 2315911.7043980435 0)), ((-1016088.5754403418 2315410.1455756347 0, -1016089.4892584289 2315410.2616955633 0, -1016089.3836509151 2315411.0698238383 0, -1016037.0835551982 2315811.281564955 0, -1016036.1696450292 2315811.1653767275 0, -1015640.8272461377 2315760.928157282 0, -1015693.6841488682 2315359.9842735534 0, -1015746.5446647434 2314959.029045533 0, -1016140.983925117 2315009.120498495 0, -1016088.5754403418 2315410.1455756347 0)), ((-1027155.3452638367 2316411.786709581 0, -1027099.3060001228 2316814.926257049 0, -1027043.2648768441 2317218.0630884925 0, -1026644.7072264659 2317166.6641910076 0, -1026246.1444279129 2317115.289097042 0, -1026301.8767193094 2316714.5768864295 0, -1026357.6113957331 2316313.8658440644 0, -1026413.3443055688 2315913.1521339053 0, -1026469.0776228255 2315512.4360198975 0, -1026474.1921480831 2315513.058994836 0, -1026474.157555098 2315513.316376404 0, -1026871.760588797 2315561.5732183787 0, -1027078.1453079201 2315586.632985187 0, -1027266.8527822931 2315609.6269936697 0, -1027211.099731914 2316010.7096340056 0, -1027155.3452638367 2316411.786709581 0)), ((-1025287.2500278767 2318219.881490436 0, -1025233.7673048442 2318619.0690635266 0, -1025036.6764289986 2318595.601747828 0, -1025043.9946522627 2318452.6497306363 0, -1024460.203644346 2318386.780092331 0, -1024550.039398206 2317716.8354266207 0, -1024948.6598177875 2317765.867653209 0, -1024893.4948594307 2318171.132183464 0, -1025287.2500278767 2318219.881490436 0)), ((-1014849.3035981857 2318610.752736169 0, -1014835.8670853045 2318710.77994911 0, -1014808.9939054567 2318910.834037035 0, -1014808.1539995833 2318917.0210857503 0, -1014414.5562884181 2318863.378070875 0, -1014015.7704339768 2318809.04622694 0, -1013615.4254839027 2318758.0232241508 0, -1013550.772978898 2318749.786416855 0, -1013609.6767885035 2318757.0489088283 0, -1013610.3754804195 2318751.8921359894 0, -1013215.7460878228 2318702.1602814947 0, -1013270.3161568193 2318305.2298836303 0, -1013270.981068162 2318300.3937520864 0, -1013668.3551273596 2318351.655942579 0, -1013667.6468856283 2318356.8909093654 0, -1014063.7056366887 2318406.8852371457 0, -1014050.3463598335 2318506.779348246 0, -1014449.826788734 2318558.767781257 0, -1014849.3035981857 2318610.752736169 0), (-1014037.285272602 2318604.443743791 0, -1014010.2686532065 2318806.460754792 0, -1014036.9870937357 2318606.673387476 0, -1014037.285272602 2318604.443743791 0)), ((-1014672.4252685239 2319910.521527098 0, -1014273.4849611721 2319859.6864720886 0, -1014244.5833741965 2320058.227364899 0, -1013850.0849239003 2320009.065353609 0, -1013905.9635467671 2319613.4271603054 0, -1013957.7778587915 2319209.892514499 0, -1013962.933897664 2319210.485891009 0, -1014360.2488984851 2319264.227305992 0, -1014306.4781407012 2319665.4990265067 0, -1014700.2199382108 2319717.20804532 0, -1014672.4252685239 2319910.521527098 0)), ((-1019844.4605516114 2367828.7181895296 0, -1019836.6832047377 2367828.6566944965 0, -1019844.1631092988 2367827.1020178064 0, -1019844.4605516114 2367828.7181895296 0)), ((-1019749.8586578161 2367846.7029273226 0, -1019730.4547369138 2367862.7044856353 0, -1019721.1015328282 2367852.680013197 0, -1019749.8586578161 2367846.7029273226 0)), ((-1019489.243215159 2367941.975031009 0, -1019589.486000852 2367857.0802320065 0, -1019591.1965935136 2367855.6316565396 0, -1019597.1352694286 2367850.602627461 0, -1019661.9165680929 2367823.0492214714 0, -1019712.3063310208 2367869.2079813634 0, -1019849.1142427962 2367835.4914042763 0, -1019869.2018001195 2367828.7689682436 0, -1020002.4213520194 2367846.9370946446 0, -1019971.7302186178 2368059.401858848 0, -1019569.4784886269 2368009.641163103 0, -1019568.6378645014 2368009.5371733913 0, -1019542.0667056023 2368203.846304738 0, -1019139.8706920221 2368154.1615764936 0, -1019150.3566583431 2368077.039244164 0, -1019152.6926239136 2368077.2998635396 0, -1019489.243215159 2367941.975031009 0)), ((-1003973.5743517822 2287706.1898662974 0, -1004025.5718877799 2287305.1669149064 0, -1004424.7817649296 2287357.397890239 0, -1004346.5417785074 2287950.361873327 0, -1003948.9173469689 2287896.3566977885 0, -1003973.5743517822 2287706.1898662974 0)), ((-1003901.1989418323 2288116.2585630426 0, -1003890.8487933791 2288114.9201946543 0, -1003883.605893194 2288174.411962796 0, -1003862.1054485671 2288171.600248244 0, -1003860.2304077749 2288184.957091726 0, -1003823.7950634706 2288181.0176527454 0, -1003781.916172518 2288501.9038193477 0, -1003475.6863386785 2288461.2584242583 0, -1003522.6738056624 2288067.3118181056 0, -1003502.4747744225 2288064.6998995417 0, -1003447.9683762782 2288465.462530355 0, -1003050.0397184071 2288414.0294446526 0, -1003103.747842437 2288013.1618786035 0, -1003154.9964387836 2287612.0738458135 0, -1003553.2501116302 2287663.7089973115 0, -1003951.5011944886 2287715.3650219887 0, -1003901.1989418323 2288116.2585630426 0)), ((-1009087.5148740095 2305865.370139448 0, -1009136.258259307 2305916.103084611 0, -1009136.5330183754 2305954.5286968364 0, -1009154.2122259465 2305981.045586549 0, -1009134.447688086 2306029.7765306416 0, -1009156.1677302218 2306060.736313041 0, -1009147.0279683745 2306158.2603304214 0, -1010042.1916633627 2306270.799617838 0, -1010014.2160898889 2306474.1360758375 0, -1009865.6718125867 2306454.892116094 0, -1009844.0995549656 2306610.806528638 0, -1009993.1410792228 2306627.320265293 0, -1009958.7902933572 2306878.827137127 0, -1008372.5172130546 2306669.6925328304 0, -1008477.6478298152 2305870.324516675 0, -1008504.3609385635 2305667.190937402 0, -1008902.3516348937 2305719.1747760354 0, -1008894.8853314016 2305776.1156096156 0, -1008907.9652613336 2305792.846865982 0, -1008963.7418124018 2305829.481909031 0, -1009086.796717778 2305844.6904211 0, -1009087.5148740095 2305865.370139448 0)), ((-1012080.1657174543 2306225.495257412 0, -1012066.2181388165 2306326.0104286755 0, -1011667.9346320677 2306274.120442113 0, -1011682.0397675895 2306173.623383318 0, -1012080.1657174543 2306225.495257412 0)), ((-995185.4699424236 2362232.4418430002 0, -995580.9063635829 2362284.6914323024 0, -995977.6564756974 2362337.1076862775 0, -995924.85988683 2362737.1121919192 0, -995528.3288417512 2362684.8342794636 0, -995133.4475070041 2362632.7698034365 0, -995185.3293791463 2362233.5235670325 0, -995185.4699424236 2362232.4418430002 0)), ((-1001947.4908209293 2369990.034007098 0, -1001895.5755670936 2370390.1016204013 0, -1001880.763366087 2370388.3296251586 0, -1001504.4080491482 2370340.030472195 0, -1001105.0060704153 2370288.7919512643 0, -1001154.8635472904 2369895.589450522 0, -1001548.4682520501 2369942.488806778 0, -1001947.4908209293 2369990.034007098 0)))</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>White Earth</t>
+          <t>Wind River</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>WY</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
+          <t>Farm Loan, Department of Environmental Quality, Escheat, Board of Charities and Reform, Game and Fish Commission, Acquired Farm Loan, State Charitable, Educational, Penal &amp; Reform Inst, Common School</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F75" t="n">
-        <v>1141</v>
+        <v>89</v>
       </c>
       <c r="G75" t="n">
-        <v>17197.01</v>
+        <v>3665.45</v>
       </c>
       <c r="H75" t="n">
-        <v>440</v>
+        <v>50</v>
       </c>
       <c r="I75" t="n">
-        <v>27174.74</v>
+        <v>2301.95</v>
       </c>
       <c r="J75" t="n">
-        <v>701</v>
+        <v>39</v>
       </c>
       <c r="K75" t="n">
-        <v>44371.75</v>
+        <v>5967.4</v>
       </c>
       <c r="L75" t="n">
-        <v>747912.54</v>
+        <v>2066861.74</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1050634.2762595804 2312278.921033107 0, -1050692.1496858974 2311878.8901095935 0, -1050749.8418575835 2311480.125285387 0, -1050805.7506747406 2311081.4597527836 0, -1050861.6613238936 2310682.782564328 0, -1051255.859984779 2310743.4741963 0, -1051200.1037733245 2311141.4396161498 0, -1051144.3479498741 2311539.4029425895 0, -1051088.5929212286 2311937.360776254 0, -1051032.8378361643 2312335.3193941107 0, -1050634.2762595804 2312278.921033107 0)), ((-1042827.6080114043 2324641.903880159 0, -1042429.0177734202 2324582.6384197455 0, -1042031.3687667405 2324523.506086521 0, -1042088.8292028453 2324128.4938440737 0, -1042087.857374831 2324128.3551963973 0, -1042088.6925061723 2324122.6112281634 0, -1041689.879792263 2324063.533034388 0, -1041292.0584445689 2324004.6261834027 0, -1041350.0240442571 2323614.889880292 0, -1041351.4699388619 2323605.1686712345 0, -1041409.4806173473 2323215.144439011 0, -1041410.9986382548 2323205.724764946 0, -1041473.7604708544 2322816.272943921 0, -1041472.3642102741 2322816.089643594 0, -1041473.7990416642 2322807.2053701356 0, -1041125.9567855056 2322761.754220014 0, -1040731.5802114733 2322710.2174758688 0, -1040791.3933385293 2322318.3149438472 0, -1040792.477179104 2322310.396591345 0, -1040846.3585751874 2321916.7483948767 0, -1040845.4352658397 2321916.6246562605 0, -1040846.3829309222 2321909.7169102994 0, -1041243.1470202254 2321962.8195580887 0, -1041593.576394404 2322009.7149099344 0, -1041991.033277303 2322068.01460237 0, -1042388.4929601529 2322126.307653034 0, -1042333.4848828288 2322526.274883522 0, -1041935.8066824579 2322467.5824857615 0, -1041873.028642868 2322866.373482969 0, -1041810.2530178527 2323265.1530656577 0, -1042211.0342654212 2323324.8051944994 0, -1042607.2119206154 2323383.7695842357 0, -1042547.2426509934 2323783.4970818204 0, -1042944.6907629055 2323842.7817654843 0, -1042886.3057913377 2324240.829846611 0, -1043285.130652052 2324298.636963205 0, -1043226.2979992016 2324699.977115077 0, -1042827.6080114043 2324641.903880159 0)), ((-1046247.5562064119 2329220.6481662146 0, -1046191.3633868239 2329622.789430642 0, -1046593.9948730316 2329678.6363939364 0, -1046534.9886577296 2330080.588037373 0, -1046475.9821583936 2330482.5278504863 0, -1046073.6083994912 2330426.0280175335 0, -1046132.4852626884 2330024.4114558683 0, -1045729.9819064847 2329968.257709795 0, -1045788.7291921459 2329566.9681130997 0, -1045845.5922356682 2329165.063035892 0, -1045443.6285155453 2329109.4754572785 0, -1045501.1639552393 2328707.7760154633 0, -1045558.6997935177 2328306.0742610637 0, -1045616.2362395419 2327904.37012149 0, -1045617.0326782259 2327904.479360659 0, -1045616.9327830005 2327905.1956020826 0, -1046016.0937759206 2327959.9533524564 0, -1045959.3246830138 2328361.192974082 0, -1045902.4578365213 2328763.1402011085 0, -1046303.7496655369 2328818.5044084494 0, -1046247.5562064119 2329220.6481662146 0)), ((-1059727.8355241397 2337697.3455502763 0, -1059668.8527381408 2338098.124818296 0, -1060067.131052015 2338153.3211093354 0, -1060465.4090640997 2338208.5355003844 0, -1060410.0971186836 2338610.1316959243 0, -1060354.7856983019 2339011.7223898345 0, -1059956.6096501015 2338955.955333517 0, -1059558.4318289415 2338900.184331322 0, -1059613.6421632078 2338499.155718323 0, -1059215.414667514 2338443.6841478753 0, -1058817.1846679002 2338388.2147207656 0, -1058872.287569143 2337987.7950442224 0, -1058931.3390659136 2337587.2694612537 0, -1058534.796627428 2337532.90503816 0, -1058592.9067027688 2337132.182809552 0, -1058194.7240368775 2337077.520104881 0, -1058252.2701342073 2336676.4067847277 0, -1058650.7321761935 2336731.296394675 0, -1059049.4432704628 2336786.216981644 0, -1058990.3909251 2337186.7443455644 0, -1059388.6021759196 2337241.6571514467 0, -1059329.5859732355 2337642.3091146755 0, -1059727.8355241397 2337697.3455502763 0)), ((-1066371.9632855507 2339438.2108617574 0, -1066373.429756151 2339438.414318711 0, -1066325.9659184492 2339779.1937124613 0, -1066316.6288095424 2339775.4830386983 0, -1066201.70517481 2339740.4795712177 0, -1066022.4006281008 2339615.323439348 0, -1065949.3493714838 2339578.6985750943 0, -1065929.2570379518 2339568.627267384 0, -1065850.4238185033 2339539.308687006 0, -1065748.3028524022 2339468.346541264 0, -1065676.2207522886 2339424.8367052525 0, -1065654.1213722434 2339415.392399067 0, -1065606.175104046 2339412.400131573 0, -1065571.9863841333 2339376.9328016816 0, -1065578.765703502 2339328.3709718734 0, -1065775.329001942 2339355.539352133 0, -1065828.8039514287 2338960.7937077926 0, -1066028.005994407 2338986.8329564976 0, -1066000.9377325266 2339187.759105069 0, -1066398.6148282972 2339240.822932089 0, -1066371.9632855507 2339438.2108617574 0)), ((-1061837.3204676933 2340034.6030477574 0, -1061780.3655670825 2340436.5922139487 0, -1061723.408817523 2340838.5788117982 0, -1061325.3843199636 2340783.392501526 0, -1060927.3602048056 2340728.202607241 0, -1060529.3384876326 2340673.0124064325 0, -1060131.31556903 2340617.8150917715 0, -1060187.739295776 2340216.35853855 0, -1060244.1628082008 2339814.9025566597 0, -1060299.4740761493 2339413.3136684936 0, -1060354.7856983019 2339011.7223898345 0, -1060752.5765780364 2339066.2638833597 0, -1061150.3704149113 2339120.8020020006 0, -1061548.164748814 2339175.3363516834 0, -1061945.959765405 2339229.8670557295 0, -1061891.6412659038 2339632.23640928 0, -1061837.3204676933 2340034.6030477574 0)), ((-1035118.4999299524 2281190.209319271 0, -1035513.4719348657 2281246.333069391 0, -1035908.4437363615 2281302.455823209 0, -1035850.9664973858 2281705.0788636506 0, -1035456.3629951405 2281647.737895494 0, -1035061.7616243811 2281590.3958082073 0, -1035118.4999299524 2281190.209319271 0)), ((-1016227.3939126243 2286441.674483058 0, -1016170.7846368499 2286843.4743179535 0, -1016116.572680074 2287240.187457348 0, -1015719.7979054934 2287188.6790665807 0, -1015774.9398044108 2286789.754045181 0, -1015830.8571983477 2286390.9832253153 0, -1016227.3939126243 2286441.674483058 0)), ((-1033898.8322515577 2287115.5060672923 0, -1034294.5248291742 2287171.182248576 0, -1034242.4095084692 2287571.8515250664 0, -1034188.3680121511 2287971.6597832455 0, -1033792.6131830172 2287916.5542716077 0, -1033846.4969216322 2287516.1923875464 0, -1033898.8322515577 2287115.5060672923 0)), ((-1035482.4640965455 2287333.0698815673 0, -1035431.1532593278 2287732.771150824 0, -1035380.0460347141 2288135.9017904988 0, -1034981.6506295949 2288083.604406882 0, -1035034.2370944343 2287683.1639975063 0, -1035085.9019275007 2287282.590195216 0, -1035482.4640965455 2287333.0698815673 0)), ((-1031335.8145355216 2288032.690707102 0, -1031735.973979156 2288083.6424779366 0, -1031684.4242973576 2288486.76042762 0, -1031283.7416613278 2288434.873665544 0, -1030883.0524479783 2288383.0092891282 0, -1030935.6500580298 2287981.7333433605 0, -1031335.8145355216 2288032.690707102 0)), ((-1029690.6327695481 2288227.9861841374 0, -1030081.6691394955 2288279.3375122994 0, -1030031.1897501762 2288680.060399877 0, -1029980.707957195 2289080.780604471 0, -1029580.5337932236 2289031.2535202373 0, -1029632.4103333049 2288630.7904119412 0, -1029690.6327695481 2288227.9861841374 0)), ((-1019437.7014199753 2308499.869161773 0, -1019385.3452084363 2308902.469899386 0, -1018988.0279197779 2308849.793594077 0, -1019040.5066439967 2308447.541076709 0, -1019437.7014199753 2308499.869161773 0)), ((-1015746.4921843759 2314958.970178708 0, -1015693.6757171493 2315360.0135502284 0, -1015496.280137871 2315334.935964606 0, -1015549.3098236041 2314933.92679566 0, -1015746.4921843759 2314958.970178708 0)), ((-1016826.8467043939 2315911.7043980435 0, -1016432.4276351677 2315861.5429225443 0, -1016486.7752965459 2315461.576262847 0, -1016486.8862928433 2315460.7593977996 0, -1016514.1169489527 2315260.3583780047 0, -1016541.2452727675 2315060.7104614796 0, -1016540.278824313 2315060.5877280417 0, -1016540.3865441052 2315059.796102671 0, -1016740.1515403495 2315085.1658760984 0, -1016712.3379686448 2315285.539725222 0, -1016811.9507220382 2315298.1938166893 0, -1016911.5634863044 2315310.847821505 0, -1016883.2160986736 2315511.120703014 0, -1016883.3611283406 2315511.1391318156 0, -1016826.8467043939 2315911.7043980435 0)), ((-1016088.5754403418 2315410.1455756347 0, -1016089.4892584289 2315410.2616955633 0, -1016089.3836509151 2315411.0698238383 0, -1016037.0835551982 2315811.281564955 0, -1016036.1696450292 2315811.1653767275 0, -1015640.8272461377 2315760.928157282 0, -1015693.6841488682 2315359.9842735534 0, -1015746.5446647434 2314959.029045533 0, -1016140.983925117 2315009.120498495 0, -1016088.5754403418 2315410.1455756347 0)), ((-1027155.3452638367 2316411.786709581 0, -1027099.3060001228 2316814.926257049 0, -1027043.2648768441 2317218.0630884925 0, -1026644.7072264659 2317166.6641910076 0, -1026246.1444279129 2317115.289097042 0, -1026301.8767193094 2316714.5768864295 0, -1026357.6113957331 2316313.8658440644 0, -1026413.3443055688 2315913.1521339053 0, -1026469.0776228255 2315512.4360198975 0, -1026474.1921480831 2315513.058994836 0, -1026474.157555098 2315513.316376404 0, -1026871.760588797 2315561.5732183787 0, -1027078.1453079201 2315586.632985187 0, -1027266.8527822931 2315609.6269936697 0, -1027211.099731914 2316010.7096340056 0, -1027155.3452638367 2316411.786709581 0)), ((-1025287.2500278767 2318219.881490436 0, -1025233.7673048442 2318619.0690635266 0, -1025036.6764289986 2318595.601747828 0, -1025043.9946522627 2318452.6497306363 0, -1024460.203644346 2318386.780092331 0, -1024550.039398206 2317716.8354266207 0, -1024948.6598177875 2317765.867653209 0, -1024893.4948594307 2318171.132183464 0, -1025287.2500278767 2318219.881490436 0)), ((-1014849.3035981857 2318610.752736169 0, -1014835.8670853045 2318710.77994911 0, -1014808.9939054567 2318910.834037035 0, -1014808.1539995833 2318917.0210857503 0, -1014414.5562884181 2318863.378070875 0, -1014015.7704339768 2318809.04622694 0, -1013615.4254839027 2318758.0232241508 0, -1013550.772978898 2318749.786416855 0, -1013609.6767885035 2318757.0489088283 0, -1013610.3754804195 2318751.8921359894 0, -1013215.7460878228 2318702.1602814947 0, -1013270.3161568193 2318305.2298836303 0, -1013270.981068162 2318300.3937520864 0, -1013668.3551273596 2318351.655942579 0, -1013667.6468856283 2318356.8909093654 0, -1014063.7056366887 2318406.8852371457 0, -1014050.3463598335 2318506.779348246 0, -1014449.826788734 2318558.767781257 0, -1014849.3035981857 2318610.752736169 0), (-1014037.285272602 2318604.443743791 0, -1014010.2686532065 2318806.460754792 0, -1014036.9870937357 2318606.673387476 0, -1014037.285272602 2318604.443743791 0)), ((-1014672.4252685239 2319910.521527098 0, -1014273.4849611721 2319859.6864720886 0, -1014244.5833741965 2320058.227364899 0, -1013850.0849239003 2320009.065353609 0, -1013905.9635467671 2319613.4271603054 0, -1013957.7778587915 2319209.892514499 0, -1013962.933897664 2319210.485891009 0, -1014360.2488984851 2319264.227305992 0, -1014306.4781407012 2319665.4990265067 0, -1014700.2199382108 2319717.20804532 0, -1014672.4252685239 2319910.521527098 0)), ((-1019844.4605516114 2367828.7181895296 0, -1019836.6832047377 2367828.6566944965 0, -1019844.1631092988 2367827.1020178064 0, -1019844.4605516114 2367828.7181895296 0)), ((-1019749.8586578161 2367846.7029273226 0, -1019730.4547369138 2367862.7044856353 0, -1019721.1015328282 2367852.680013197 0, -1019749.8586578161 2367846.7029273226 0)), ((-1019489.243215159 2367941.975031009 0, -1019589.486000852 2367857.0802320065 0, -1019591.1965935136 2367855.6316565396 0, -1019597.1352694286 2367850.602627461 0, -1019661.9165680929 2367823.0492214714 0, -1019712.3063310208 2367869.2079813634 0, -1019849.1142427962 2367835.4914042763 0, -1019869.2018001195 2367828.7689682436 0, -1020002.4213520194 2367846.9370946446 0, -1019971.7302186178 2368059.401858848 0, -1019569.4784886269 2368009.641163103 0, -1019568.6378645014 2368009.5371733913 0, -1019542.0667056023 2368203.846304738 0, -1019139.8706920221 2368154.1615764936 0, -1019150.3566583431 2368077.039244164 0, -1019152.6926239136 2368077.2998635396 0, -1019489.243215159 2367941.975031009 0)), ((-1003973.5743517822 2287706.1898662974 0, -1004025.5718877799 2287305.1669149064 0, -1004424.7817649296 2287357.397890239 0, -1004346.5417785074 2287950.361873327 0, -1003948.9173469689 2287896.3566977885 0, -1003973.5743517822 2287706.1898662974 0)), ((-1003901.1989418323 2288116.2585630426 0, -1003890.8487933791 2288114.9201946543 0, -1003883.605893194 2288174.411962796 0, -1003862.1054485671 2288171.600248244 0, -1003860.2304077749 2288184.957091726 0, -1003823.7950634706 2288181.0176527454 0, -1003781.916172518 2288501.9038193477 0, -1003475.6863386785 2288461.2584242583 0, -1003522.6738056624 2288067.3118181056 0, -1003502.4747744225 2288064.6998995417 0, -1003447.9683762782 2288465.462530355 0, -1003050.0397184071 2288414.0294446526 0, -1003103.747842437 2288013.1618786035 0, -1003154.9964387836 2287612.0738458135 0, -1003553.2501116302 2287663.7089973115 0, -1003951.5011944886 2287715.3650219887 0, -1003901.1989418323 2288116.2585630426 0)), ((-1009087.5148740095 2305865.370139448 0, -1009136.258259307 2305916.103084611 0, -1009136.5330183754 2305954.5286968364 0, -1009154.2122259465 2305981.045586549 0, -1009134.447688086 2306029.7765306416 0, -1009156.1677302218 2306060.736313041 0, -1009147.0279683745 2306158.2603304214 0, -1010042.1916633627 2306270.799617838 0, -1010014.2160898889 2306474.1360758375 0, -1009865.6718125867 2306454.892116094 0, -1009844.0995549656 2306610.806528638 0, -1009993.1410792228 2306627.320265293 0, -1009958.7902933572 2306878.827137127 0, -1008372.5172130546 2306669.6925328304 0, -1008477.6478298152 2305870.324516675 0, -1008504.3609385635 2305667.190937402 0, -1008902.3516348937 2305719.1747760354 0, -1008894.8853314016 2305776.1156096156 0, -1008907.9652613336 2305792.846865982 0, -1008963.7418124018 2305829.481909031 0, -1009086.796717778 2305844.6904211 0, -1009087.5148740095 2305865.370139448 0)), ((-1012080.1657174543 2306225.495257412 0, -1012066.2181388165 2306326.0104286755 0, -1011667.9346320677 2306274.120442113 0, -1011682.0397675895 2306173.623383318 0, -1012080.1657174543 2306225.495257412 0)), ((-995185.4699424236 2362232.4418430002 0, -995580.9063635829 2362284.6914323024 0, -995977.6564756974 2362337.1076862775 0, -995924.85988683 2362737.1121919192 0, -995528.3288417512 2362684.8342794636 0, -995133.4475070041 2362632.7698034365 0, -995185.3293791463 2362233.5235670325 0, -995185.4699424236 2362232.4418430002 0)), ((-1001947.4908209293 2369990.034007098 0, -1001895.5755670936 2370390.1016204013 0, -1001880.763366087 2370388.3296251586 0, -1001504.4080491482 2370340.030472195 0, -1001105.0060704153 2370288.7919512643 0, -1001154.8635472904 2369895.589450522 0, -1001548.4682520501 2369942.488806778 0, -1001947.4908209293 2369990.034007098 0)))</t>
+          <t>POLYGON Z ((-2000691.670389903 2331962.4047491485 0, -2000297.120530334 2331863.8366929404 0, -2000378.7610276425 2331555.6632454637 0, -2000383.52788925 2331550.664125949 0, -2000404.2332826294 2331528.949865917 0, -2000436.5508040052 2331496.630248958 0, -2000457.0939019124 2331482.942588032 0, -2000524.6099901185 2331437.9570213845 0, -2000623.547944883 2331521.1411316423 0, -2000642.2051764121 2331455.954080666 0, -2000783.0149527532 2331525.924893335 0, -2000794.6718260078 2331570.5907869237 0, -2000795.608453972 2331574.17969693 0, -2000856.417264013 2331807.1811536797 0, -2000936.3358951204 2331898.801343468 0, -2001108.5968959765 2331976.922216007 0, -2001147.7393053952 2331994.673259766 0, -2001155.817165279 2332078.3893294954 0, -2001086.2153794249 2332060.9932991057 0, -2000691.670389903 2331962.4047491485 0))</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Wind River</t>
+          <t>XL Ranch</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>WY</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Department of Environmental Quality, Farm Loan, Escheat, Board of Charities and Reform, Game and Fish Commission, Acquired Farm Loan, State Charitable, Educational, Penal &amp; Reform Inst, Common School</t>
+          <t>School Lands</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="G76" t="n">
-        <v>3665.45</v>
+        <v>62.54</v>
       </c>
       <c r="H76" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="I76" t="n">
-        <v>2301.95</v>
+        <v>62.54</v>
       </c>
       <c r="J76" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="K76" t="n">
-        <v>5967.4</v>
+        <v>125.08</v>
       </c>
       <c r="L76" t="n">
-        <v>2066861.74</v>
+        <v>9807.360000000001</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>POLYGON Z ((-2000691.670389903 2331962.4047491485 0, -2000297.120530334 2331863.8366929404 0, -2000378.7610276425 2331555.6632454637 0, -2000383.52788925 2331550.664125949 0, -2000404.2332826294 2331528.949865917 0, -2000436.5508040052 2331496.630248958 0, -2000457.0939019124 2331482.942588032 0, -2000524.6099901185 2331437.9570213845 0, -2000623.547944883 2331521.1411316423 0, -2000642.2051764121 2331455.954080666 0, -2000783.0149527532 2331525.924893335 0, -2000794.6718260078 2331570.5907869237 0, -2000795.608453972 2331574.17969693 0, -2000856.417264013 2331807.1811536797 0, -2000936.3358951204 2331898.801343468 0, -2001108.5968959765 2331976.922216007 0, -2001147.7393053952 2331994.673259766 0, -2001155.817165279 2332078.3893294954 0, -2001086.2153794249 2332060.9932991057 0, -2000691.670389903 2331962.4047491485 0))</t>
+          <t xml:space="preserve">MULTIPOLYGON Z (((-1947124.5557107623 2807295.7237508334 0, -1947196.7819263288 2807274.393608224 0, -1947193.1458702104 2807288.599900207 0, -1947059.5372636789 2807810.6141429264 0, -1946853.3734672957 2808596.0136770844 0, -1946745.5648815252 2808986.612934126 0, -1946341.8260397688 2808874.4829723123 0, -1945948.194095369 2808765.148187057 0, -1945556.2480824378 2808656.277029655 0, -1945447.281745532 2809049.883998759 0, -1945055.775332241 2808942.2476052986 0, -1944671.1240387606 2808836.5816436727 0, -1944285.9715556526 2808729.451306282 0, -1944182.7006740377 2808700.8373704124 0, -1944175.258183883 2808698.7751340363 0, -1944205.97409468 2808691.593999012 0, -1944239.832728101 2808683.6780427233 0, -1944297.1865183178 2808670.268832043 0, -1944326.1207686376 2808663.504190235 0, -1944341.9027250202 2808643.0757502136 0, -1944450.3186288457 2808502.7405995512 0, -1944484.6290076356 2808458.3283272255 0, -1944531.3559075892 2808450.5231368784 0, -1944533.2475823362 2808450.207102876 0, -1944742.3493571964 2808415.2779346644 0, -1944782.5304498996 2808408.56573509 0, -1944825.9314816992 2808401.315558442 0, -1944846.4419707358 2808397.889270128 0, -1944932.4650723806 2808383.518803587 0, -1945120.8879312954 2808352.0413803793 0, -1945232.340665698 2808300.193092651 0, -1945233.011146676 2808299.8811820387 0, -1945234.1767156126 2808299.338971333 0, -1945367.0666779706 2808239.105563168 0, -1945403.2525988873 2808189.1273322944 0, -1945406.8244306557 2808184.194092287 0, -1945434.3286187563 2808146.206466028 0, -1945452.2644826355 2808121.434357619 0, -1945517.6448988912 2808031.1333648274 0, -1945708.4753189383 2807935.2428929717 0, -1945743.469064124 2807917.658688479 0, -1945773.6058255532 2807875.803767459 0, -1945783.8263632155 2807861.609515513 0, -1945794.803288026 2807846.364457131 0, -1945805.1034344905 2807832.0591395595 0, -1945838.5799746306 2807785.5660434654 0, -1945999.7991482161 2807667.234313057 0, -1946006.4658096721 2807662.3410324776 0, -1946060.3811198939 2807650.8228329164 0, -1946249.9701467785 2807610.3188651903 0, -1946270.8384821936 2807605.860535518 0, -1946329.3806055868 2807593.353076714 0, -1946424.2470437514 2807573.08506474 0, -1946682.5545190827 2807536.241129031 0, -1946715.8717711887 2807531.488632948 0, -1946735.830111049 2807528.641718737 0, -1946811.206861308 2807517.889765267 0, -1946845.9224203727 2807472.3194938726 0, -1946907.4433662225 2807391.5624610432 0, -1946950.1763059627 2807335.467485209 0, -1946961.8711610327 2807337.088222957 0, -1947066.3557622277 2807351.5676600714 0, -1947124.5557107623 2807295.7237508334 0)), ((-1953386.7879867416 2809957.2616419047 0, -1953122.7670257601 2809888.019521383 0, -1953193.010530159 2809596.6558950776 0, -1953203.577075884 2809552.826982933 0, -1953281.4916945917 2809558.277206182 0, -1953292.17934746 2809749.786360986 0, -1953293.2236294863 2809768.4961081003 0, -1953296.9640707995 2809835.516895046 0, -1953482.0649389857 2809967.511132979 0, -1953484.7584606395 2809969.4318917906 0, -1953487.6914903347 2809983.723829882 0, -1953386.7879867416 2809957.2616419047 0)), ((-1946614.9078962246 2811885.370776785 0, -1946633.8647125496 2811896.64560381 0, -1946653.0110561145 2811912.1504938467 0, -1946684.166303763 2811937.3803751133 0, -1946689.2998346796 2811942.553062524 0, -1946690.5019310338 2811943.7641511704 0, -1946698.197141594 2811951.5179146877 0, -1946715.1627968417 2811971.3295670627 0, -1946730.0721239133 2811985.5084807114 0, -1946745.232731864 2811995.7451126017 0, -1946751.3168938763 2811998.816866132 0, -1946821.3437366372 2812034.169959289 0, -1946845.616608355 2812045.7422609036 0, -1946879.5990443504 2812061.9438724904 0, -1946879.8500397133 2812062.0636778786 0, -1946910.9144404363 2812076.8738750056 0, -1946947.7533411365 2812094.4371382394 0, -1947060.7872370374 2812153.652763408 0, -1947139.5149107124 2812191.1254910952 0, -1947153.044659055 2812194.2237642687 0, -1947176.9299978777 2812105.4381115045 0, -1947178.3598672908 2812088.189209279 0, -1947180.6096412572 2812076.401427918 0, -1947184.6021095074 2812055.484020593 0, -1947199.007831662 2811996.7596786823 0, -1947205.7505111548 2811998.307882489 0, -1947601.865979837 2812089.2656746367 0, -1947161.8444363042 2813724.908500826 0, -1947938.7742716009 2813946.868101684 0, -1948716.0669331742 2814153.7326147486 0, -1948508.1692716295 2814936.5808169744 0, -1948296.06130565 2815711.6417853036 0, -1948085.8615166286 2816490.051731219 0, -1947887.1532080339 2817263.7317802105 0, -1947110.1819699025 2817045.1674422114 0, -1946333.2349266736 2816826.5353467013 0, -1946536.5120191795 2816052.253474633 0, -1946743.038038953 2815275.9633118263 0, -1945965.8537946267 2815058.6734601483 0, -1945187.38250786 2814847.511176291 0, -1945390.6584151017 2814070.8353690077 0, -1945593.9390024608 2813294.1439373647 0, -1945806.4183397717 2812512.0426953356 0, -1946017.4099203725 2811725.407987297 0, -1946413.5226287036 2811816.379077322 0, -1946413.1175892442 2811817.8873744495 0, -1946429.5205681976 2811823.0182974017 0, -1946430.5705775602 2811823.3468920225 0, -1946441.4127719733 2811826.7384116566 0, -1946460.0693028378 2811832.573924255 0, -1946546.4250696348 2811858.060609156 0, -1946584.401309241 2811872.0030026874 0, -1946614.9078962246 2811885.370776785 0)), ((-1948900.588521401 2813349.774017343 0, -1948809.1497083865 2813748.171309886 0, -1948240.7924339913 2813580.0435008793 0, -1948345.2341088098 2813173.972558003 0, -1948900.588521401 2813349.774017343 0)), ((-1952221.214135054 2813417.0188169414 0, -1952606.9522442534 2813525.2989367954 0, -1952609.412323701 2813525.9894720893 0, -1952608.7617625473 2813528.576734444 0, -1952521.005898842 2813877.601366205 0, -1952461.1719096894 2813882.468296462 0, -1952404.91447361 2813887.0441548065 0, -1952125.3607299807 2813809.319979971 0, -1952221.214135054 2813417.0188169414 0)), ((-1951109.403211928 2817706.2222447176 0, -1950981.9253401442 2817755.7212553616 0, -1950915.0461234644 2817781.5329516055 0, -1950878.459851005 2817795.653069836 0, -1950813.5889805139 2817754.9988670424 0, -1950714.747913343 2817693.0551435365 0, -1950696.3781159038 2817681.5429214216 0, -1950634.842756184 2817642.978246047 0, -1950475.0732963716 2817794.2712869965 0, -1950350.9850651731 2817911.774685636 0, -1950229.4130995688 2817877.218136361 0, -1949459.3219813337 2817655.629660831 0, -1949675.1280854722 2816881.8744489173 0, -1949882.0230697875 2816121.976450482 0, -1951048.5181664268 2816443.4519810094 0, -1951135.8725615966 2816045.698412492 0, -1951397.6412383653 2816122.326121462 0, -1951398.2366670764 2816140.6499513793 0, -1951429.1657775978 2816344.5042031966 0, -1951458.0132103665 2816395.444446804 0, -1951458.6854130586 2816396.631445679 0, -1951419.2681869979 2816543.478137624 0, -1951245.4248171826 2817266.2006058693 0, -1951115.3352282133 2817703.9188853893 0, -1951109.403211928 2817706.2222447176 0)), ((-1948800.0774710595 2820079.056871323 0, -1948755.4657172174 2820088.8711917084 0, -1948729.7918133228 2820094.519223721 0, -1948749.6901557706 2819981.7351393187 0, -1949029.2966877047 2819219.0309122363 0, -1949216.1317151315 2819267.1190779125 0, -1949122.1522565759 2819352.187155631 0, -1949068.056106266 2819432.4726366717 0, -1949023.0329906945 2819505.4548712545 0, -1949044.0199872083 2819623.3749157335 0, -1949075.2662473642 2819798.93361861 0, -1948965.0742484073 2819994.7351705506 0, -1948901.8355726646 2820027.0534498193 0, -1948800.0774710595 2820079.056871323 0)), ((-1947711.056209912 2823037.388546394 0, -1947710.3908040728 2823052.360373251 0, -1947703.6130837516 2823204.87018648 0, -1947635.7493479564 2823448.7215245077 0, -1947632.6231846497 2823459.954442923 0, -1947651.3765163652 2823799.3043881706 0, -1947622.273734997 2823892.2555906605 0, -1947617.236901387 2823908.3427039455 0, -1947519.7118047255 2824219.8324208586 0, -1947474.1677948614 2824286.46855595 0, -1947457.4749831655 2824310.895477439 0, -1947392.8850046801 2824501.2802619715 0, -1947285.5751249949 2824652.8274717364 0, -1947282.93064712 2824656.5636720136 0, -1947144.512593157 2824804.2110868483 0, -1947222.884602449 2824860.459899903 0, -1947266.2238187243 2824978.8393854517 0, -1947343.8223486969 2824953.2193777794 0, -1947334.0825702942 2825080.905190541 0, -1947321.0618002464 2825251.6351106544 0, -1947253.1551944956 2825475.1227064123 0, -1947248.8139849745 2825482.088473379 0, -1946516.2152451943 2825292.499795915 0, -1945735.8521312105 2825090.6417997656 0, -1945524.0930363676 2825864.6570646428 0, -1945314.7721398615 2826639.52506426 0, -1945088.7128367843 2827410.705539773 0, -1944876.2513827144 2828185.515469902 0, -1944086.5716233156 2827974.060117378 0, -1943708.4311984438 2827856.921258917 0, -1943313.7750874953 2827749.8342451244 0, -1942552.8778908548 2827565.478069011 0, -1942433.8878418936 2827952.8691948676 0, -1942115.2148576651 2829110.296337552 0, -1941740.247006324 2829021.677830297 0, -1941364.8913283464 2828934.2149304776 0, -1940614.4885814935 2828717.4324106015 0, -1940380.7262877997 2829491.0634633354 0, -1941157.3486816953 2829714.164489239 0, -1940962.5406810332 2830480.7188912537 0, -1942461.70950291 2830885.848456556 0, -1942692.6805440595 2830137.7557435655 0, -1942793.6901436509 2829709.63596787 0, -1942894.7014358174 2829281.5114808935 0, -1943664.6776832102 2829494.2014161125 0, -1944444.5162852963 2829727.3526395317 0, -1944240.9796830066 2830537.874774691 0, -1944046.067697474 2831315.9714416503 0, -1943848.50376597 2832102.6996421823 0, -1943743.83154259 2832479.2347885496 0, -1943644.3767330595 2832837.0025605005 0, -1943581.2039236382 2832819.7384977685 0, -1942869.1977661247 2832625.1609020308 0, -1942803.9323556963 2832608.7278774576 0, -1942095.9751251442 2832430.4740522504 0, -1942023.432910939 2832411.589677251 0, -1941320.4345445875 2832228.5872334125 0, -1941241.4812423058 2832213.40905601 0, -1940518.8604381077 2832067.5301795797 0, -1940427.6025438693 2832041.979955196 0, -1939719.1298166327 2831844.149645808 0, -1939650.2813025315 2831823.7800045474 0, -1939008.2927350795 2831633.9075519615 0, -1938937.8182702172 2831612.9978779657 0, -1938875.459023381 2831595.8261597687 0, -1938155.5847200237 2831397.7635465516 0, -1938098.1574108254 2831382.171489841 0, -1937367.725195407 2831183.8592544473 0, -1937319.7935790198 2831170.7466271804 0, -1936592.1479990568 2830970.5633796058 0, -1936551.782240904 2830958.459755302 0, -1935919.8841535791 2830768.979581447 0, -1935853.7424633587 2830666.800432577 0, -1936043.9285566418 2829974.059544721 0, -1936145.9669096095 2829606.0232871436 0, -1936248.0642732342 2829237.7809193237 0, -1936459.6332089452 2828420.087475266 0, -1936671.1932913214 2827602.744161404 0, -1935901.1673248971 2827404.963971848 0, -1935131.6484503855 2827207.345645183 0, -1934737.3642994917 2827104.054830973 0, -1934342.5261924486 2827000.6324797366 0, -1933553.2220813956 2826793.841596687 0, -1933761.5091981522 2826019.775546707 0, -1933975.9384614483 2825234.8236955265 0, -1933583.8297440552 2825126.270168573 0, -1933192.1269479976 2825017.8277554675 0, -1933406.247326265 2824251.320284405 0, -1933484.1597564383 2824270.6364715467 0, -1933560.93079583 2824065.5594003047 0, -1933557.1777476843 2823669.876861863 0, -1933632.168574466 2823445.1023491654 0, -1933233.0538895007 2823344.3789825863 0, -1932833.940247076 2823243.6511097113 0, -1932372.995906775 2823117.950424193 0, -1932730.2121003186 2821547.4664698183 0, -1933252.3690630475 2820001.953830233 0, -1932875.059471353 2819895.6085127 0, -1932120.5151176807 2819683.5672394563 0, -1930577.5733440355 2819261.3804175365 0, -1929696.1913390842 2819055.4839692526 0, -1929845.6354374762 2818625.467116351 0, -1929872.7544179265 2818547.434736694 0, -1929874.57124737 2818542.207133 0, -1929880.1351356034 2818526.1975715207 0, -1929881.7522122038 2818521.5443381337 0, -1929983.0851736646 2818229.966494045 0, -1929619.2157681047 2818130.8872940643 0, -1929736.580766636 2817750.492223993 0, -1929360.2837025973 2817657.226028599 0, -1929354.5875267424 2817678.947000758 0, -1929353.228261422 2817684.129774841 0, -1929341.3386348058 2817729.4691167814 0, -1929339.8485104665 2817735.151194868 0, -1929337.815666145 2817742.9028611216 0, -1929255.3412267803 2818031.826646187 0, -1928918.8246952381 2818810.952408313 0, -1928122.7990207672 2818594.244171984 0, -1928024.642395889 2818569.0576784485 0, -1927630.2863546014 2817947.253782771 0, -1927551.1817190184 2817823.047702654 0, -1927201.5305156272 2817274.0244157608 0, -1927013.8005473418 2816985.972721535 0, -1927170.6971796076 2816600.8326979834 0, -1927186.888627717 2816605.135812899 0, -1927955.1064756506 2816810.1267357282 0, -1928062.8644512328 2816410.767847923 0, -1928170.6236448651 2816011.404500228 0, -1928170.6519277014 2816011.3002163935 0, -1928335.5725609951 2816060.678830224 0, -1928340.479160045 2816062.14773463 0, -1928358.8299043912 2816067.6420136616 0, -1928363.9512381542 2816069.1753942226 0, -1928547.897408099 2816124.249284745 0, -1928652.450982854 2815747.538075545 0, -1928287.6432609076 2815609.2405163767 0, -1928283.2752051004 2815607.584605435 0, -1928279.9276287449 2815606.3154997323 0, -1928283.612778869 2815594.6022822983 0, -1928288.215822168 2815577.514176424 0, -1928388.6672126406 2815203.3196104844 0, -1928756.3313858095 2815373.2517059958 0, -1929123.7263016994 2815543.083117765 0, -1929897.3229792737 2815749.610247387 0, -1929707.9124916464 2816449.4440081026 0, -1929470.2812261013 2817237.773556349 0, -1929860.56049845 2817348.6562962593 0, -1930250.833378816 2817459.560403357 0, -1930641.143404357 2817570.4991767206 0, -1931031.4472574294 2817681.459688435 0, -1931805.2503211931 2817905.5667042457 0, -1932594.1915322812 2818127.825577896 0, -1932811.8928143983 2817356.7666764436 0, -1933022.8681155671 2816578.4116334063 0, -1933795.9299697948 2816792.540353066 0, -1934163.8246629832 2816898.246070321 0, -1934550.1172213496 2817009.2331912736 0, -1934334.2296709986 2817788.790593405 0, -1934108.049074308 2818561.261530009 0, -1934909.250632951 2818782.6145231696 0, -1935116.7927075562 2818006.531720954 0, -1935916.8198173607 2818229.1149338917 0, -1936676.3996078675 2818437.897329563 0, -1936462.9739085813 2819219.5778062106 0, -1936353.5000564817 2819609.4351670644 0, -1936243.9917860483 2819999.2792242086 0, -1936632.7686874776 2820105.6482482827 0, -1937021.5500128125 2820212.013846692 0, -1937413.318937494 2820320.6705608866 0, -1937805.0901551058 2820429.3200657633 0, -1937698.353795431 2820820.401979242 0, -1937592.4233251668 2821208.550592578 0, -1937985.3208603768 2821315.5024794503 0, -1937786.438834566 2822105.703372242 0, -1937572.007178126 2822882.830218352 0, -1937947.7030090205 2822971.5158543093 0, -1938378.049721953 2821422.3454312244 0, -1938770.257508245 2821532.227865583 0, -1938981.1579699456 2820755.2587466994 0, -1938588.1487450716 2820646.4371728147 0, -1938799.1743406628 2819864.585701209 0, -1939022.6444431625 2819088.687467256 0, -1939242.4706204562 2818309.8925407636 0, -1939462.8863154226 2817539.1384911337 0, -1939684.5868446275 2816755.1590106944 0, -1940481.046967366 2816953.4827664336 0, -1941277.4698106893 2817151.7884277906 0, -1941666.9750141355 2817255.678148611 0, -1942056.4813348188 2817359.563572374 0, -1942799.6122432877 2817584.255998529 0, -1942579.2484212103 2818370.2245898014 0, -1942358.8900397797 2819156.175726435 0, -1942255.0990678044 2819547.3025721707 0, -1942151.236367304 2819938.450738095 0, -1942043.4314071736 2820328.0719141285 0, -1941935.5920665667 2820717.6798253707 0, -1943517.0213170212 2821089.9273377797 0, -1943289.8592308573 2821862.5371859185 0, -1943073.3554806781 2822728.562133121 0, -1943834.9354735375 2822914.7426675498 0, -1944612.9373131827 2823120.186971993 0, -1945390.9473912406 2823325.61012788 0, -1945779.9519991863 2823428.3177299947 0, -1946168.9579114623 2823531.02142024 0, -1946284.3938566889 2823110.445017022 0, -1946397.9609839355 2822700.6624759194 0, -1947185.9908282983 2822901.5805788804 0, -1947711.056209912 2823037.388546394 0), (-1934758.975706155 2825446.512897815 0, -1934653.0218455815 2825841.932409918 0, -1935043.4589296302 2825948.790364581 0, -1935150.4415958782 2825552.3993304996 0, -1935541.7468236985 2825658.256978833 0, -1935646.7138191978 2825263.1583201904 0, -1936029.8489498126 2825363.6139364857 0, -1936413.00537298 2825464.090523153 0, -1936487.7773941478 2825192.6720164535 0, -1936433.7728069306 2825054.5628216825 0, -1936135.5340307557 2824973.1069335695 0, -1936245.3051296428 2824573.794055444 0, -1935862.1415192464 2824473.3424840486 0, -1935969.817728062 2824082.0210779584 0, -1936084.9942129245 2823647.682375033 0, -1936174.577011313 2823309.8599834703 0, -1935399.411184608 2823094.9130661804 0, -1935501.0654255731 2822711.01071649 0, -1935124.0544510153 2822606.820595831 0, -1934963.3254915304 2822562.4005034817 0, -1934958.4332583307 2822369.333828692 0, -1934828.3273453016 2822114.356937905 0, -1934728.9298708765 2822497.6198299667 0, -1934629.6000918266 2822880.6597541803 0, -1934467.1727870738 2822838.0632362305 0, -1934237.4196847486 2822777.8091885406 0, -1934031.2843016037 2823545.8212093497 0, -1933917.7880985364 2823517.1802627076 0, -1933790.0503903565 2823747.4732142584 0, -1933761.194117387 2824123.826363364 0, -1933680.13984651 2824319.2227905844 0, -1934217.7233894903 2824452.4925112473 0, -1933975.9384614483 2825234.8236955265 0, -1934758.975706155 2825446.512897815 0), (-1939585.1471896607 2829261.4028389654 0, -1939818.2940440194 2828487.400401368 0, -1938649.617593449 2828181.742712182 0, -1938258.7925312018 2828077.720105118 0, -1938143.3234812513 2828440.935519226 0, -1938027.8552433995 2828804.146640231 0, -1937825.555195848 2829570.0810287166 0, -1939374.8838128757 2829997.759182874 0, -1939585.1471896607 2829261.4028389654 0), (-1930920.3377759478 2818068.226708838 0, -1930518.6474033971 2817956.4985622237 0, -1930396.1606221455 2818342.4661825285 0, -1930766.5858791282 2818443.3733610176 0, -1930776.1682660037 2818445.983636517 0, -1930809.2299065518 2818454.9896017592 0, -1930813.003602764 2818441.853874067 0, -1930814.3485153364 2818437.1717314213 0, -1930920.3377759478 2818068.226708838 0), (-1930255.115148408 2817883.195627018 0, -1930236.724376213 2817878.080051084 0, -1930012.3089755394 2818237.925762199 0, -1930030.7570267974 2818242.950074561 0, -1930255.115148408 2817883.195627018 0)), ((-1941975.4751981073 2808840.0696086613 0, -1941997.1538114115 2808836.4567134576 0, -1942073.5637378213 2808823.722606744 0, -1942131.7629030917 2808808.992433286 0, -1942208.4989129088 2808789.57058315 0, -1942416.180367779 2808737.0050345478 0, -1942455.87754672 2808717.4955143197 0, -1942544.9733916684 2808673.708611994 0, -1942610.5539401006 2808641.478167417 0, -1942620.1244321063 2808636.774620107 0, -1942663.400072895 2808615.5060951007 0, -1942753.6674295608 2808571.1424578154 0, -1942869.51606919 2808688.9877995523 0, -1942888.4225879675 2808708.219790584 0, -1942889.654890738 2808709.4734285926 0, -1942895.2061948585 2808710.0261795996 0, -1943049.4737258072 2808725.3855749154 0, -1943082.0811213637 2808728.6318694507 0, -1943105.6422018444 2808759.283847976 0, -1943160.5267339058 2808830.685657026 0, -1943205.0386135392 2808888.592700042 0, -1943276.3573062862 2809003.8482864983 0, -1943377.1216596877 2809067.6060874094 0, -1943381.3177654438 2809070.2610881724 0, -1943377.6567924723 2809086.5898198485 0, -1943328.4432893663 2809306.0939921406 0, -1942477.1866891305 2809087.429074342 0, -1941793.930382525 2808892.4903800027 0, -1941789.0354423348 2808891.0937741525 0, -1941800.329167384 2808887.565882612 0, -1941827.8367050479 2808878.973043119 0, -1941869.040369248 2808866.101807077 0, -1941925.9578423577 2808848.3217931706 0, -1941933.5939346517 2808847.0492320075 0, -1941975.4751981073 2808840.0696086613 0)), ((-1944058.723598079 2816226.208026141 0, -1943942.488938613 2816616.768198294 0, -1943547.2736266737 2816516.6943910923 0, -1943663.3560512534 2816121.164155373 0, -1944058.723598079 2816226.208026141 0)), ((-1943034.0998549613 2816804.0528895273 0, -1943429.9347577845 2816916.434716266 0, -1943190.0135548415 2817682.717167016 0, -1942799.6122432877 2817584.255998529 0, -1943034.0998549613 2816804.0528895273 0)), ((-1943581.524175765 2817781.7749560145 0, -1943822.2347943233 2817004.9033741523 0, -1944560.3858638655 2817171.3886290533 0, -1944344.9823447221 2817974.9235633775 0, -1943581.524175765 2817781.7749560145 0)), ((-1936153.4484906516 2811585.839009829 0, -1936174.945166137 2811575.6432904634 0, -1936331.8753854744 2811520.53820495 0, -1936485.3815387331 2811478.6248240764 0, -1936535.956110518 2811464.8157760906 0, -1936570.6387233243 2811455.3457541857 0, -1936691.344574958 2811344.07207154 0, -1936797.7922188782 2811318.367799899 0, -1936864.795513821 2811302.187914356 0, -1936932.0140674335 2811261.923055901 0, -1936967.2226207997 2811240.832516306 0, -1936988.2531909542 2811228.234803959 0, -1937110.3845130322 2811121.5474925996 0, -1937331.5234054446 2811029.662503699 0, -1937825.614099507 2811136.749395092 0, -1937626.9716735017 2811921.5246444508 0, -1937428.2562024964 2812706.7988925623 0, -1936631.9254041116 2812517.482568833 0, -1935835.3500741445 2812328.5873463713 0, -1936019.0369716408 2811654.632357626 0, -1936020.6140379785 2811648.8460765434 0, -1936023.788997826 2811647.3343533343 0, -1936153.4484906516 2811585.839009829 0)), ((-1934629.6000918266 2822880.6597541803 0, -1935014.5051893676 2822987.7885432597 0, -1934920.3375659534 2823381.8329619314 0, -1934530.000007294 2823263.5995747233 0, -1934629.6000918266 2822880.6597541803 0)), ((-1928802.6239436434 2813711.292642901 0, -1928695.4713545218 2814099.5714198337 0, -1928588.319572293 2814487.8458844405 0, -1928486.0163505543 2814883.946014951 0, -1928047.7060741284 2814765.1291601956 0, -1928169.909786337 2814374.937847502 0, -1928291.2333748734 2813991.870427505 0, -1928411.9188028697 2813610.815898007 0, -1928802.6239436434 2813711.292642901 0)), ((-1930344.3252405708 2814131.2391046174 0, -1931145.4264724182 2814216.068519604 0, -1931897.6967454187 2814520.078997948 0, -1931677.669010281 2815348.565582413 0, -1931455.9990515015 2816177.889569845 0, -1930679.8917686564 2815963.721800876 0, -1929897.3229792737 2815749.610247387 0, -1930101.4035317835 2814982.196513081 0, -1930344.3252405708 2814131.2391046174 0), (-1931176.4831238952 2815664.0622126306 0, -1931285.0219405617 2815257.3089883183 0, -1930496.8888091063 2815074.1259574196 0, -1930392.7472309952 2815465.399057443 0, -1930786.1327697122 2815564.888445243 0, -1931176.4831238952 2815664.0622126306 0)), ((-1932625.004395147 2824019.372009379 0, -1933015.4430826395 2824135.5915850047 0, -1932800.8537718498 2824906.077624436 0, -1932409.581895042 2824794.323167323 0, -1932625.004395147 2824019.372009379 0)), ((-1920878.2998509065 2864462.17655 0, -1919339.6526715388 2863911.015689175 0, -1919499.2762970189 2863216.3909553443 0, -1919730.7560771785 2862646.1294262023 0, -1921234.9285229577 2863201.991168637 0, -1920878.2998509065 2864462.17655 0)), ((-1922638.7562835668 2863745.317361907 0, -1924153.195741897 2864306.7299528057 0, -1923888.6471772937 2865271.213071534 0, -1922316.4412968731 2864845.7317742375 0, -1922638.7562835668 2863745.317361907 0)), ((-1926037.7249022147 2865457.6752195945 0, -1926036.5113501642 2865458.052518688 0, -1925975.9532681934 2865453.9122872567 0, -1925930.7511069255 2865465.3310377323 0, -1925799.5858269983 2865498.4620929626 0, -1925670.3957903862 2865546.158560157 0, -1925466.1884740398 2865642.7213355713 0, -1925454.2712138693 2865648.3563584513 0, -1925407.9209830656 2865656.2345184283 0, -1925416.9028312895 2865626.803323347 0, -1925647.9816289446 2864883.8372634226 0, -1926426.6688185155 2865162.56099678 0, -1926346.923875304 2865447.8805387504 0, -1926344.6599197036 2865455.9786466183 0, -1926286.1722074042 2865450.0294201733 0, -1926239.953681523 2865433.6989291757 0, -1926194.1290867266 2865409.05764377 0, -1926102.589071288 2865437.5118282633 0, -1926037.7249022147 2865457.6752195945 0)), ((-1920878.2998509065 2864462.17655 0, -1922316.4412968731 2864845.7317742375 0, -1921937.9880175826 2866328.2418175107 0, -1920493.8236914861 2865916.736179924 0, -1920878.2998509065 2864462.17655 0)), ((-1923905.1909504859 2866062.0840243534 0, -1923694.2456817098 2865994.054471567 0, -1923888.6471772937 2865271.213071534 0, -1924647.095419721 2865525.620003377 0, -1924553.537377164 2865901.4384199167 0, -1924430.9460681241 2865941.608395081 0, -1924323.7107533982 2865938.42827042 0, -1924230.5070588181 2866006.112174293 0, -1924104.4933114254 2866035.8790831277 0, -1924100.3231105062 2866036.8642222416 0, -1923905.1909504859 2866062.0840243534 0)), ((-1919701.1799191511 2865692.628450287 0, -1920493.8236914861 2865916.736179924 0, -1920282.5159418776 2866689.6695956476 0, -1920063.0392874023 2867437.0951254596 0, -1918519.0079381303 2867049.4514382277 0, -1918727.2580562208 2866291.9558586976 0, -1918935.992267362 2865493.9974696813 0, -1919701.1799191511 2865692.628450287 0)), ((-1920484.2790882466 2868891.2747279843 0, -1920457.821402454 2868892.4005715097 0, -1920423.629405119 2868893.855391192 0, -1920360.068046492 2868917.624331222 0, -1920298.8876387314 2868971.2923594313 0, -1920288.32324321 2868985.276912684 0, -1920253.0264786195 2869031.9994208585 0, -1920198.3077958673 2869072.7124186186 0, -1920172.056477208 2869092.2443947084 0, -1920070.8849752592 2869120.7112222956 0, -1920069.5049013162 2869120.347357614 0, -1919656.880719714 2869011.5518553834 0, -1920063.0392874023 2867437.0951254596 0, -1921505.7355209019 2867841.2034891616 0, -1921303.6114292133 2868629.609526721 0, -1920661.5235922271 2868452.082035754 0, -1920552.1579890763 2868882.1221683607 0, -1920551.1712253771 2868885.8993717683 0, -1920537.0033777482 2868887.4095733752 0, -1920516.0798756713 2868889.640050298 0, -1920511.680168411 2868890.1066194465 0, -1920484.2790882466 2868891.2747279843 0)), ((-1918281.6149233957 2869427.129881711 0, -1918180.6272271832 2869429.0710308147 0, -1918157.0973496847 2869429.5232212557 0, -1918121.4546746355 2869422.962137803 0, -1918109.0596553606 2869420.68110986 0, -1918105.0060209925 2869419.538707551 0, -1917882.2714684121 2869356.764865057 0, -1918095.5308712325 2868585.0459888475 0, -1918867.7827164773 2868791.986355689 0, -1918726.0367620673 2869308.9572289637 0, -1918725.9448960554 2869309.2774270247 0, -1918677.5162904623 2869380.159117461 0, -1918636.2236785386 2869440.596596778 0, -1918596.5901848478 2869421.0781514556 0, -1918460.091061805 2869423.70111539 0, -1918281.6149233957 2869427.129881711 0)), ((-1896662.1291620622 2805250.3423015014 0, -1896617.8490537708 2805417.656135391 0, -1896839.5872408089 2805526.699763196 0, -1896981.9109618014 2805599.2744929465 0, -1897118.6617120001 2805669.0071706297 0, -1897394.0270403055 2805732.1153340274 0, -1897405.6310079533 2805734.7171778316 0, -1897403.2774505315 2805741.8933131336 0, -1897160.6182358935 2805690.3540516123 0, -1896836.4849928634 2805560.3781644492 0, -1896796.3253876953 2805542.363626464 0, -1896664.9456934035 2805486.5652625123 0, -1896474.0382321659 2805390.3940137057 0, -1896027.2588527822 2805152.2507861634 0, -1895895.7028750055 2805075.2363432255 0, -1895897.5966885793 2805066.959958494 0, -1896037.0741669147 2805145.6315296795 0, -1896115.9962219296 2805170.8494562437 0, -1896252.7791996817 2805238.118718162 0, -1896253.7904080655 2805238.615882762 0, -1896257.1900887035 2805225.622883738 0, -1896278.2708206922 2805145.0768309115 0, -1896280.8100677126 2805145.7731968067 0, -1896662.1291620622 2805250.3423015014 0)), ((-1848363.6882150844 2809557.9256321383 0, -1847565.2008195755 2809347.35479946 0, -1847753.0180932435 2808570.847165622 0, -1848168.1485670605 2808679.627370943 0, -1848066.2456815925 2809060.0568930204 0, -1848467.2445381596 2809166.4507369203 0, -1848363.6882150844 2809557.9256321383 0)), ((-1855995.3764377357 2824711.132278971 0, -1856596.2530270615 2824860.499229959 0, -1856502.6217058415 2825243.653543744 0, -1855917.2237804504 2825098.7500604456 0, -1855902.085931869 2825094.751325446 0, -1855995.3764377357 2824711.132278971 0)), ((-1912910.4701252922 2825105.470172096 0, -1913690.2678639877 2825318.0513913846 0, -1913475.602772493 2826091.513492878 0, -1912695.934640716 2825879.9739590874 0, -1912910.4701252922 2825105.470172096 0)), ((-1911069.7715516498 2859288.2712812563 0, -1911118.0394319408 2859292.194786913 0, -1911148.3038582413 2859299.7011281266 0, -1911204.6475025443 2859323.4398436164 0, -1911433.145370624 2859457.0825968017 0, -1911475.0160240466 2859469.7359355534 0, -1911566.2282880305 2859484.6296004737 0, -1911624.1042513992 2859503.7192126443 0, -1911655.2056487277 2859524.9016695837 0, -1911672.238303252 2859550.3286137334 0, -1911693.0234700018 2859608.4402489266 0, -1911711.5377839655 2859633.0364471176 0, -1911787.3753059297 2859681.2531758402 0, -1911873.8105411069 2859711.941820578 0, -1912024.2322820295 2859744.469130588 0, -1912118.6433898045 2859778.4844851773 0, -1912533.2117745362 2859944.8979557194 0, -1913643.2050348504 2860347.8959560236 0, -1913527.9301741994 2860756.2311121295 0, -1915082.0788809326 2861183.9764312278 0, -1914655.1870602483 2862736.5331034884 0, -1913105.016828101 2862299.3443285665 0, -1913060.4700790537 2862471.6502935244 0, -1912992.565783229 2862453.340604565 0, -1913072.2428802666 2862365.9101331043 0, -1913086.8815983618 2862321.335075575 0, -1913093.0844607016 2862302.4471131875 0, -1913095.7141809722 2862294.442648306 0, -1913093.0009326101 2862222.036124531 0, -1913098.4926566228 2862078.558125645 0, -1913099.0955059526 2862062.8152301223 0, -1913026.3898837257 2862009.91471713 0, -1913014.0192889408 2861978.061959087 0, -1912974.4306614639 2861876.1249502343 0, -1912977.757394028 2861858.5793345035 0, -1912996.705049017 2861758.6463654567 0, -1913076.2420588923 2861721.586656786 0, -1913124.9517082511 2861698.8959120987 0, -1913139.4522744163 2861676.030208984 0, -1913223.418938074 2861543.628482523 0, -1913222.8707171988 2861534.6809602724 0, -1913221.1860840458 2861507.18803523 0, -1913214.856270181 2861403.8810550272 0, -1913207.2930252783 2861280.4406802733 0, -1913185.6124821394 2860926.5160575625 0, -1913157.2245225396 2860853.5992868417 0, -1913155.6716720276 2860849.6110518365 0, -1913125.3692025102 2860771.784262498 0, -1913131.7364428965 2860669.004731093 0, -1913131.782236189 2860668.72819048 0, -1913143.5723766568 2860477.931809763 0, -1913131.619344249 2860430.3780944976 0, -1913124.8165809885 2860403.3147919704 0, -1912941.4974071295 2860292.591562632 0, -1912833.3460024307 2860227.2493567374 0, -1912474.2022318812 2860010.26171056 0, -1912432.4013694355 2859985.0065007173 0, -1912356.966638263 2860217.7809732584 0, -1912335.8611494561 2860282.906388533 0, -1912390.8543641644 2860318.422930044 0, -1912504.0346987934 2860391.516893893 0, -1912597.268442078 2860512.76332725 0, -1912631.4741167298 2860526.0990556735 0, -1912663.9295307714 2860567.4074183432 0, -1912688.5321914845 2860613.0776181757 0, -1912718.59309723 2860651.3639282566 0, -1912718.9211642176 2860651.781943132 0, -1912752.8300348427 2860671.8267409485 0, -1912792.7016657135 2860715.319400522 0, -1912801.0621218358 2860751.8794533582 0, -1912802.8163927726 2860759.5508336276 0, -1912811.3612939587 2860771.9968697843 0, -1912860.9368616662 2860844.1748114796 0, -1912881.9719934592 2860850.586878815 0, -1912914.2566657045 2860887.3722070316 0, -1912951.5542474554 2860901.672441451 0, -1912997.136471682 2861061.497576031 0, -1912972.5083661168 2861121.6599827837 0, -1912976.572345268 2861168.462726313 0, -1912955.1807925128 2861213.557281548 0, -1912938.9904720702 2861247.6880313484 0, -1912914.4718112536 2861303.540262284 0, -1912900.9537771847 2861346.3993542246 0, -1912905.2138733114 2861372.9690812184 0, -1912885.3924334827 2861432.7661755173 0, -1912848.3822755567 2861450.0640992844 0, -1912807.5578270198 2861463.233480185 0, -1912779.958603024 2861482.7017999063 0, -1912706.106748129 2861489.606784551 0, -1912649.7560292801 2861492.86930673 0, -1912589.126544637 2861465.8263269123 0, -1912573.697175786 2861458.9442121834 0, -1912533.597625341 2861427.459699995 0, -1912509.6031612083 2861417.4320082692 0, -1912497.6881110407 2861412.4511158867 0, -1912435.0815359554 2861427.8055061647 0, -1912412.7539228862 2861448.3456075285 0, -1912370.034183779 2861438.8233540137 0, -1912300.3260759236 2861435.998505672 0, -1912283.3518890105 2861420.8285070877 0, -1912226.1528728916 2861434.1905212556 0, -1912214.300237075 2861436.959300874 0, -1912150.424289445 2861464.1960276156 0, -1912116.9846162822 2861465.5227756826 </t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>XL Ranch</t>
+          <t>Yakama</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>WA</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>School Lands</t>
+          <t>Common School and Indemnity, State Forest Transfer, Escheat, Scientific School, Community Forest Trust, Normal School, Natural Resources Conservation Area, Charitable/Educational/Penal &amp; Reformatory Instit., University - Transferred</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>2</v>
+        <v>304</v>
       </c>
       <c r="G77" t="n">
-        <v>62.54</v>
+        <v>46922.33</v>
       </c>
       <c r="H77" t="n">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="I77" t="n">
-        <v>62.54</v>
+        <v>44906.36</v>
       </c>
       <c r="J77" t="n">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="K77" t="n">
-        <v>125.08</v>
+        <v>91828.69</v>
       </c>
       <c r="L77" t="n">
-        <v>9807.360000000001</v>
+        <v>1376779.33</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t xml:space="preserve">MULTIPOLYGON Z (((-1947124.5557107623 2807295.7237508334 0, -1947196.7819263288 2807274.393608224 0, -1947193.1458702104 2807288.599900207 0, -1947059.5372636789 2807810.6141429264 0, -1946853.3734672957 2808596.0136770844 0, -1946745.5648815252 2808986.612934126 0, -1946341.8260397688 2808874.4829723123 0, -1945948.194095369 2808765.148187057 0, -1945556.2480824378 2808656.277029655 0, -1945447.281745532 2809049.883998759 0, -1945055.775332241 2808942.2476052986 0, -1944671.1240387606 2808836.5816436727 0, -1944285.9715556526 2808729.451306282 0, -1944182.7006740377 2808700.8373704124 0, -1944175.258183883 2808698.7751340363 0, -1944205.97409468 2808691.593999012 0, -1944239.832728101 2808683.6780427233 0, -1944297.1865183178 2808670.268832043 0, -1944326.1207686376 2808663.504190235 0, -1944341.9027250202 2808643.0757502136 0, -1944450.3186288457 2808502.7405995512 0, -1944484.6290076356 2808458.3283272255 0, -1944531.3559075892 2808450.5231368784 0, -1944533.2475823362 2808450.207102876 0, -1944742.3493571964 2808415.2779346644 0, -1944782.5304498996 2808408.56573509 0, -1944825.9314816992 2808401.315558442 0, -1944846.4419707358 2808397.889270128 0, -1944932.4650723806 2808383.518803587 0, -1945120.8879312954 2808352.0413803793 0, -1945232.340665698 2808300.193092651 0, -1945233.011146676 2808299.8811820387 0, -1945234.1767156126 2808299.338971333 0, -1945367.0666779706 2808239.105563168 0, -1945403.2525988873 2808189.1273322944 0, -1945406.8244306557 2808184.194092287 0, -1945434.3286187563 2808146.206466028 0, -1945452.2644826355 2808121.434357619 0, -1945517.6448988912 2808031.1333648274 0, -1945708.4753189383 2807935.2428929717 0, -1945743.469064124 2807917.658688479 0, -1945773.6058255532 2807875.803767459 0, -1945783.8263632155 2807861.609515513 0, -1945794.803288026 2807846.364457131 0, -1945805.1034344905 2807832.0591395595 0, -1945838.5799746306 2807785.5660434654 0, -1945999.7991482161 2807667.234313057 0, -1946006.4658096721 2807662.3410324776 0, -1946060.3811198939 2807650.8228329164 0, -1946249.9701467785 2807610.3188651903 0, -1946270.8384821936 2807605.860535518 0, -1946329.3806055868 2807593.353076714 0, -1946424.2470437514 2807573.08506474 0, -1946682.5545190827 2807536.241129031 0, -1946715.8717711887 2807531.488632948 0, -1946735.830111049 2807528.641718737 0, -1946811.206861308 2807517.889765267 0, -1946845.9224203727 2807472.3194938726 0, -1946907.4433662225 2807391.5624610432 0, -1946950.1763059627 2807335.467485209 0, -1946961.8711610327 2807337.088222957 0, -1947066.3557622277 2807351.5676600714 0, -1947124.5557107623 2807295.7237508334 0)), ((-1953386.7879867416 2809957.2616419047 0, -1953122.7670257601 2809888.019521383 0, -1953193.010530159 2809596.6558950776 0, -1953203.577075884 2809552.826982933 0, -1953281.4916945917 2809558.277206182 0, -1953292.17934746 2809749.786360986 0, -1953293.2236294863 2809768.4961081003 0, -1953296.9640707995 2809835.516895046 0, -1953482.0649389857 2809967.511132979 0, -1953484.7584606395 2809969.4318917906 0, -1953487.6914903347 2809983.723829882 0, -1953386.7879867416 2809957.2616419047 0)), ((-1946614.9078962246 2811885.370776785 0, -1946633.8647125496 2811896.64560381 0, -1946653.0110561145 2811912.1504938467 0, -1946684.166303763 2811937.3803751133 0, -1946689.2998346796 2811942.553062524 0, -1946690.5019310338 2811943.7641511704 0, -1946698.197141594 2811951.5179146877 0, -1946715.1627968417 2811971.3295670627 0, -1946730.0721239133 2811985.5084807114 0, -1946745.232731864 2811995.7451126017 0, -1946751.3168938763 2811998.816866132 0, -1946821.3437366372 2812034.169959289 0, -1946845.616608355 2812045.7422609036 0, -1946879.5990443504 2812061.9438724904 0, -1946879.8500397133 2812062.0636778786 0, -1946910.9144404363 2812076.8738750056 0, -1946947.7533411365 2812094.4371382394 0, -1947060.7872370374 2812153.652763408 0, -1947139.5149107124 2812191.1254910952 0, -1947153.044659055 2812194.2237642687 0, -1947176.9299978777 2812105.4381115045 0, -1947178.3598672908 2812088.189209279 0, -1947180.6096412572 2812076.401427918 0, -1947184.6021095074 2812055.484020593 0, -1947199.007831662 2811996.7596786823 0, -1947205.7505111548 2811998.307882489 0, -1947601.865979837 2812089.2656746367 0, -1947161.8444363042 2813724.908500826 0, -1947938.7742716009 2813946.868101684 0, -1948716.0669331742 2814153.7326147486 0, -1948508.1692716295 2814936.5808169744 0, -1948296.06130565 2815711.6417853036 0, -1948085.8615166286 2816490.051731219 0, -1947887.1532080339 2817263.7317802105 0, -1947110.1819699025 2817045.1674422114 0, -1946333.2349266736 2816826.5353467013 0, -1946536.5120191795 2816052.253474633 0, -1946743.038038953 2815275.9633118263 0, -1945965.8537946267 2815058.6734601483 0, -1945187.38250786 2814847.511176291 0, -1945390.6584151017 2814070.8353690077 0, -1945593.9390024608 2813294.1439373647 0, -1945806.4183397717 2812512.0426953356 0, -1946017.4099203725 2811725.407987297 0, -1946413.5226287036 2811816.379077322 0, -1946413.1175892442 2811817.8873744495 0, -1946429.5205681976 2811823.0182974017 0, -1946430.5705775602 2811823.3468920225 0, -1946441.4127719733 2811826.7384116566 0, -1946460.0693028378 2811832.573924255 0, -1946546.4250696348 2811858.060609156 0, -1946584.401309241 2811872.0030026874 0, -1946614.9078962246 2811885.370776785 0)), ((-1948900.588521401 2813349.774017343 0, -1948809.1497083865 2813748.171309886 0, -1948240.7924339913 2813580.0435008793 0, -1948345.2341088098 2813173.972558003 0, -1948900.588521401 2813349.774017343 0)), ((-1952221.214135054 2813417.0188169414 0, -1952606.9522442534 2813525.2989367954 0, -1952609.412323701 2813525.9894720893 0, -1952608.7617625473 2813528.576734444 0, -1952521.005898842 2813877.601366205 0, -1952461.1719096894 2813882.468296462 0, -1952404.91447361 2813887.0441548065 0, -1952125.3607299807 2813809.319979971 0, -1952221.214135054 2813417.0188169414 0)), ((-1951109.403211928 2817706.2222447176 0, -1950981.9253401442 2817755.7212553616 0, -1950915.0461234644 2817781.5329516055 0, -1950878.459851005 2817795.653069836 0, -1950813.5889805139 2817754.9988670424 0, -1950714.747913343 2817693.0551435365 0, -1950696.3781159038 2817681.5429214216 0, -1950634.842756184 2817642.978246047 0, -1950475.0732963716 2817794.2712869965 0, -1950350.9850651731 2817911.774685636 0, -1950229.4130995688 2817877.218136361 0, -1949459.3219813337 2817655.629660831 0, -1949675.1280854722 2816881.8744489173 0, -1949882.0230697875 2816121.976450482 0, -1951048.5181664268 2816443.4519810094 0, -1951135.8725615966 2816045.698412492 0, -1951397.6412383653 2816122.326121462 0, -1951398.2366670764 2816140.6499513793 0, -1951429.1657775978 2816344.5042031966 0, -1951458.0132103665 2816395.444446804 0, -1951458.6854130586 2816396.631445679 0, -1951419.2681869979 2816543.478137624 0, -1951245.4248171826 2817266.2006058693 0, -1951115.3352282133 2817703.9188853893 0, -1951109.403211928 2817706.2222447176 0)), ((-1948800.0774710595 2820079.056871323 0, -1948755.4657172174 2820088.8711917084 0, -1948729.7918133228 2820094.519223721 0, -1948749.6901557706 2819981.7351393187 0, -1949029.2966877047 2819219.0309122363 0, -1949216.1317151315 2819267.1190779125 0, -1949122.1522565759 2819352.187155631 0, -1949068.056106266 2819432.4726366717 0, -1949023.0329906945 2819505.4548712545 0, -1949044.0199872083 2819623.3749157335 0, -1949075.2662473642 2819798.93361861 0, -1948965.0742484073 2819994.7351705506 0, -1948901.8355726646 2820027.0534498193 0, -1948800.0774710595 2820079.056871323 0)), ((-1947711.056209912 2823037.388546394 0, -1947710.3908040728 2823052.360373251 0, -1947703.6130837516 2823204.87018648 0, -1947635.7493479564 2823448.7215245077 0, -1947632.6231846497 2823459.954442923 0, -1947651.3765163652 2823799.3043881706 0, -1947622.273734997 2823892.2555906605 0, -1947617.236901387 2823908.3427039455 0, -1947519.7118047255 2824219.8324208586 0, -1947474.1677948614 2824286.46855595 0, -1947457.4749831655 2824310.895477439 0, -1947392.8850046801 2824501.2802619715 0, -1947285.5751249949 2824652.8274717364 0, -1947282.93064712 2824656.5636720136 0, -1947144.512593157 2824804.2110868483 0, -1947222.884602449 2824860.459899903 0, -1947266.2238187243 2824978.8393854517 0, -1947343.8223486969 2824953.2193777794 0, -1947334.0825702942 2825080.905190541 0, -1947321.0618002464 2825251.6351106544 0, -1947253.1551944956 2825475.1227064123 0, -1947248.8139849745 2825482.088473379 0, -1946516.2152451943 2825292.499795915 0, -1945735.8521312105 2825090.6417997656 0, -1945524.0930363676 2825864.6570646428 0, -1945314.7721398615 2826639.52506426 0, -1945088.7128367843 2827410.705539773 0, -1944876.2513827144 2828185.515469902 0, -1944086.5716233156 2827974.060117378 0, -1943708.4311984438 2827856.921258917 0, -1943313.7750874953 2827749.8342451244 0, -1942552.8778908548 2827565.478069011 0, -1942433.8878418936 2827952.8691948676 0, -1942115.2148576651 2829110.296337552 0, -1941740.247006324 2829021.677830297 0, -1941364.8913283464 2828934.2149304776 0, -1940614.4885814935 2828717.4324106015 0, -1940380.7262877997 2829491.0634633354 0, -1941157.3486816953 2829714.164489239 0, -1940962.5406810332 2830480.7188912537 0, -1942461.70950291 2830885.848456556 0, -1942692.6805440595 2830137.7557435655 0, -1942793.6901436509 2829709.63596787 0, -1942894.7014358174 2829281.5114808935 0, -1943664.6776832102 2829494.2014161125 0, -1944444.5162852963 2829727.3526395317 0, -1944240.9796830066 2830537.874774691 0, -1944046.067697474 2831315.9714416503 0, -1943848.50376597 2832102.6996421823 0, -1943743.83154259 2832479.2347885496 0, -1943644.3767330595 2832837.0025605005 0, -1943581.2039236382 2832819.7384977685 0, -1942869.1977661247 2832625.1609020308 0, -1942803.9323556963 2832608.7278774576 0, -1942095.9751251442 2832430.4740522504 0, -1942023.432910939 2832411.589677251 0, -1941320.4345445875 2832228.5872334125 0, -1941241.4812423058 2832213.40905601 0, -1940518.8604381077 2832067.5301795797 0, -1940427.6025438693 2832041.979955196 0, -1939719.1298166327 2831844.149645808 0, -1939650.2813025315 2831823.7800045474 0, -1939008.2927350795 2831633.9075519615 0, -1938937.8182702172 2831612.9978779657 0, -1938875.459023381 2831595.8261597687 0, -1938155.5847200237 2831397.7635465516 0, -1938098.1574108254 2831382.171489841 0, -1937367.725195407 2831183.8592544473 0, -1937319.7935790198 2831170.7466271804 0, -1936592.1479990568 2830970.5633796058 0, -1936551.782240904 2830958.459755302 0, -1935919.8841535791 2830768.979581447 0, -1935853.7424633587 2830666.800432577 0, -1936043.9285566418 2829974.059544721 0, -1936145.9669096095 2829606.0232871436 0, -1936248.0642732342 2829237.7809193237 0, -1936459.6332089452 2828420.087475266 0, -1936671.1932913214 2827602.744161404 0, -1935901.1673248971 2827404.963971848 0, -1935131.6484503855 2827207.345645183 0, -1934737.3642994917 2827104.054830973 0, -1934342.5261924486 2827000.6324797366 0, -1933553.2220813956 2826793.841596687 0, -1933761.5091981522 2826019.775546707 0, -1933975.9384614483 2825234.8236955265 0, -1933583.8297440552 2825126.270168573 0, -1933192.1269479976 2825017.8277554675 0, -1933406.247326265 2824251.320284405 0, -1933484.1597564383 2824270.6364715467 0, -1933560.93079583 2824065.5594003047 0, -1933557.1777476843 2823669.876861863 0, -1933632.168574466 2823445.1023491654 0, -1933233.0538895007 2823344.3789825863 0, -1932833.940247076 2823243.6511097113 0, -1932372.995906775 2823117.950424193 0, -1932730.2121003186 2821547.4664698183 0, -1933252.3690630475 2820001.953830233 0, -1932875.059471353 2819895.6085127 0, -1932120.5151176807 2819683.5672394563 0, -1930577.5733440355 2819261.3804175365 0, -1929696.1913390842 2819055.4839692526 0, -1929845.6354374762 2818625.467116351 0, -1929872.7544179265 2818547.434736694 0, -1929874.57124737 2818542.207133 0, -1929880.1351356034 2818526.1975715207 0, -1929881.7522122038 2818521.5443381337 0, -1929983.0851736646 2818229.966494045 0, -1929619.2157681047 2818130.8872940643 0, -1929736.580766636 2817750.492223993 0, -1929360.2837025973 2817657.226028599 0, -1929354.5875267424 2817678.947000758 0, -1929353.228261422 2817684.129774841 0, -1929341.3386348058 2817729.4691167814 0, -1929339.8485104665 2817735.151194868 0, -1929337.815666145 2817742.9028611216 0, -1929255.3412267803 2818031.826646187 0, -1928918.8246952381 2818810.952408313 0, -1928122.7990207672 2818594.244171984 0, -1928024.642395889 2818569.0576784485 0, -1927630.2863546014 2817947.253782771 0, -1927551.1817190184 2817823.047702654 0, -1927201.5305156272 2817274.0244157608 0, -1927013.8005473418 2816985.972721535 0, -1927170.6971796076 2816600.8326979834 0, -1927186.888627717 2816605.135812899 0, -1927955.1064756506 2816810.1267357282 0, -1928062.8644512328 2816410.767847923 0, -1928170.6236448651 2816011.404500228 0, -1928170.6519277014 2816011.3002163935 0, -1928335.5725609951 2816060.678830224 0, -1928340.479160045 2816062.14773463 0, -1928358.8299043912 2816067.6420136616 0, -1928363.9512381542 2816069.1753942226 0, -1928547.897408099 2816124.249284745 0, -1928652.450982854 2815747.538075545 0, -1928287.6432609076 2815609.2405163767 0, -1928283.2752051004 2815607.584605435 0, -1928279.9276287449 2815606.3154997323 0, -1928283.612778869 2815594.6022822983 0, -1928288.215822168 2815577.514176424 0, -1928388.6672126406 2815203.3196104844 0, -1928756.3313858095 2815373.2517059958 0, -1929123.7263016994 2815543.083117765 0, -1929897.3229792737 2815749.610247387 0, -1929707.9124916464 2816449.4440081026 0, -1929470.2812261013 2817237.773556349 0, -1929860.56049845 2817348.6562962593 0, -1930250.833378816 2817459.560403357 0, -1930641.143404357 2817570.4991767206 0, -1931031.4472574294 2817681.459688435 0, -1931805.2503211931 2817905.5667042457 0, -1932594.1915322812 2818127.825577896 0, -1932811.8928143983 2817356.7666764436 0, -1933022.8681155671 2816578.4116334063 0, -1933795.9299697948 2816792.540353066 0, -1934163.8246629832 2816898.246070321 0, -1934550.1172213496 2817009.2331912736 0, -1934334.2296709986 2817788.790593405 0, -1934108.049074308 2818561.261530009 0, -1934909.250632951 2818782.6145231696 0, -1935116.7927075562 2818006.531720954 0, -1935916.8198173607 2818229.1149338917 0, -1936676.3996078675 2818437.897329563 0, -1936462.9739085813 2819219.5778062106 0, -1936353.5000564817 2819609.4351670644 0, -1936243.9917860483 2819999.2792242086 0, -1936632.7686874776 2820105.6482482827 0, -1937021.5500128125 2820212.013846692 0, -1937413.318937494 2820320.6705608866 0, -1937805.0901551058 2820429.3200657633 0, -1937698.353795431 2820820.401979242 0, -1937592.4233251668 2821208.550592578 0, -1937985.3208603768 2821315.5024794503 0, -1937786.438834566 2822105.703372242 0, -1937572.007178126 2822882.830218352 0, -1937947.7030090205 2822971.5158543093 0, -1938378.049721953 2821422.3454312244 0, -1938770.257508245 2821532.227865583 0, -1938981.1579699456 2820755.2587466994 0, -1938588.1487450716 2820646.4371728147 0, -1938799.1743406628 2819864.585701209 0, -1939022.6444431625 2819088.687467256 0, -1939242.4706204562 2818309.8925407636 0, -1939462.8863154226 2817539.1384911337 0, -1939684.5868446275 2816755.1590106944 0, -1940481.046967366 2816953.4827664336 0, -1941277.4698106893 2817151.7884277906 0, -1941666.9750141355 2817255.678148611 0, -1942056.4813348188 2817359.563572374 0, -1942799.6122432877 2817584.255998529 0, -1942579.2484212103 2818370.2245898014 0, -1942358.8900397797 2819156.175726435 0, -1942255.0990678044 2819547.3025721707 0, -1942151.236367304 2819938.450738095 0, -1942043.4314071736 2820328.0719141285 0, -1941935.5920665667 2820717.6798253707 0, -1943517.0213170212 2821089.9273377797 0, -1943289.8592308573 2821862.5371859185 0, -1943073.3554806781 2822728.562133121 0, -1943834.9354735375 2822914.7426675498 0, -1944612.9373131827 2823120.186971993 0, -1945390.9473912406 2823325.61012788 0, -1945779.9519991863 2823428.3177299947 0, -1946168.9579114623 2823531.02142024 0, -1946284.3938566889 2823110.445017022 0, -1946397.9609839355 2822700.6624759194 0, -1947185.9908282983 2822901.5805788804 0, -1947711.056209912 2823037.388546394 0), (-1934758.975706155 2825446.512897815 0, -1934653.0218455815 2825841.932409918 0, -1935043.4589296302 2825948.790364581 0, -1935150.4415958782 2825552.3993304996 0, -1935541.7468236985 2825658.256978833 0, -1935646.7138191978 2825263.1583201904 0, -1936029.8489498126 2825363.6139364857 0, -1936413.00537298 2825464.090523153 0, -1936487.7773941478 2825192.6720164535 0, -1936433.7728069306 2825054.5628216825 0, -1936135.5340307557 2824973.1069335695 0, -1936245.3051296428 2824573.794055444 0, -1935862.1415192464 2824473.3424840486 0, -1935969.817728062 2824082.0210779584 0, -1936084.9942129245 2823647.682375033 0, -1936174.577011313 2823309.8599834703 0, -1935399.411184608 2823094.9130661804 0, -1935501.0654255731 2822711.01071649 0, -1935124.0544510153 2822606.820595831 0, -1934963.3254915304 2822562.4005034817 0, -1934958.4332583307 2822369.333828692 0, -1934828.3273453016 2822114.356937905 0, -1934728.9298708765 2822497.6198299667 0, -1934629.6000918266 2822880.6597541803 0, -1934467.1727870738 2822838.0632362305 0, -1934237.4196847486 2822777.8091885406 0, -1934031.2843016037 2823545.8212093497 0, -1933917.7880985364 2823517.1802627076 0, -1933790.0503903565 2823747.4732142584 0, -1933761.194117387 2824123.826363364 0, -1933680.13984651 2824319.2227905844 0, -1934217.7233894903 2824452.4925112473 0, -1933975.9384614483 2825234.8236955265 0, -1934758.975706155 2825446.512897815 0), (-1939585.1471896607 2829261.4028389654 0, -1939818.2940440194 2828487.400401368 0, -1938649.617593449 2828181.742712182 0, -1938258.7925312018 2828077.720105118 0, -1938143.3234812513 2828440.935519226 0, -1938027.8552433995 2828804.146640231 0, -1937825.555195848 2829570.0810287166 0, -1939374.8838128757 2829997.759182874 0, -1939585.1471896607 2829261.4028389654 0), (-1930920.3377759478 2818068.226708838 0, -1930518.6474033971 2817956.4985622237 0, -1930396.1606221455 2818342.4661825285 0, -1930766.5858791282 2818443.3733610176 0, -1930776.1682660037 2818445.983636517 0, -1930809.2299065518 2818454.9896017592 0, -1930813.003602764 2818441.853874067 0, -1930814.3485153364 2818437.1717314213 0, -1930920.3377759478 2818068.226708838 0), (-1930255.115148408 2817883.195627018 0, -1930236.724376213 2817878.080051084 0, -1930012.3089755394 2818237.925762199 0, -1930030.7570267974 2818242.950074561 0, -1930255.115148408 2817883.195627018 0)), ((-1941975.4751981073 2808840.0696086613 0, -1941997.1538114115 2808836.4567134576 0, -1942073.5637378213 2808823.722606744 0, -1942131.7629030917 2808808.992433286 0, -1942208.4989129088 2808789.57058315 0, -1942416.180367779 2808737.0050345478 0, -1942455.87754672 2808717.4955143197 0, -1942544.9733916684 2808673.708611994 0, -1942610.5539401006 2808641.478167417 0, -1942620.1244321063 2808636.774620107 0, -1942663.400072895 2808615.5060951007 0, -1942753.6674295608 2808571.1424578154 0, -1942869.51606919 2808688.9877995523 0, -1942888.4225879675 2808708.219790584 0, -1942889.654890738 2808709.4734285926 0, -1942895.2061948585 2808710.0261795996 0, -1943049.4737258072 2808725.3855749154 0, -1943082.0811213637 2808728.6318694507 0, -1943105.6422018444 2808759.283847976 0, -1943160.5267339058 2808830.685657026 0, -1943205.0386135392 2808888.592700042 0, -1943276.3573062862 2809003.8482864983 0, -1943377.1216596877 2809067.6060874094 0, -1943381.3177654438 2809070.2610881724 0, -1943377.6567924723 2809086.5898198485 0, -1943328.4432893663 2809306.0939921406 0, -1942477.1866891305 2809087.429074342 0, -1941793.930382525 2808892.4903800027 0, -1941789.0354423348 2808891.0937741525 0, -1941800.329167384 2808887.565882612 0, -1941827.8367050479 2808878.973043119 0, -1941869.040369248 2808866.101807077 0, -1941925.9578423577 2808848.3217931706 0, -1941933.5939346517 2808847.0492320075 0, -1941975.4751981073 2808840.0696086613 0)), ((-1944058.723598079 2816226.208026141 0, -1943942.488938613 2816616.768198294 0, -1943547.2736266737 2816516.6943910923 0, -1943663.3560512534 2816121.164155373 0, -1944058.723598079 2816226.208026141 0)), ((-1943034.0998549613 2816804.0528895273 0, -1943429.9347577845 2816916.434716266 0, -1943190.0135548415 2817682.717167016 0, -1942799.6122432877 2817584.255998529 0, -1943034.0998549613 2816804.0528895273 0)), ((-1943581.524175765 2817781.7749560145 0, -1943822.2347943233 2817004.9033741523 0, -1944560.3858638655 2817171.3886290533 0, -1944344.9823447221 2817974.9235633775 0, -1943581.524175765 2817781.7749560145 0)), ((-1936153.4484906516 2811585.839009829 0, -1936174.945166137 2811575.6432904634 0, -1936331.8753854744 2811520.53820495 0, -1936485.3815387331 2811478.6248240764 0, -1936535.956110518 2811464.8157760906 0, -1936570.6387233243 2811455.3457541857 0, -1936691.344574958 2811344.07207154 0, -1936797.7922188782 2811318.367799899 0, -1936864.795513821 2811302.187914356 0, -1936932.0140674335 2811261.923055901 0, -1936967.2226207997 2811240.832516306 0, -1936988.2531909542 2811228.234803959 0, -1937110.3845130322 2811121.5474925996 0, -1937331.5234054446 2811029.662503699 0, -1937825.614099507 2811136.749395092 0, -1937626.9716735017 2811921.5246444508 0, -1937428.2562024964 2812706.7988925623 0, -1936631.9254041116 2812517.482568833 0, -1935835.3500741445 2812328.5873463713 0, -1936019.0369716408 2811654.632357626 0, -1936020.6140379785 2811648.8460765434 0, -1936023.788997826 2811647.3343533343 0, -1936153.4484906516 2811585.839009829 0)), ((-1934629.6000918266 2822880.6597541803 0, -1935014.5051893676 2822987.7885432597 0, -1934920.3375659534 2823381.8329619314 0, -1934530.000007294 2823263.5995747233 0, -1934629.6000918266 2822880.6597541803 0)), ((-1928802.6239436434 2813711.292642901 0, -1928695.4713545218 2814099.5714198337 0, -1928588.319572293 2814487.8458844405 0, -1928486.0163505543 2814883.946014951 0, -1928047.7060741284 2814765.1291601956 0, -1928169.909786337 2814374.937847502 0, -1928291.2333748734 2813991.870427505 0, -1928411.9188028697 2813610.815898007 0, -1928802.6239436434 2813711.292642901 0)), ((-1930344.3252405708 2814131.2391046174 0, -1931145.4264724182 2814216.068519604 0, -1931897.6967454187 2814520.078997948 0, -1931677.669010281 2815348.565582413 0, -1931455.9990515015 2816177.889569845 0, -1930679.8917686564 2815963.721800876 0, -1929897.3229792737 2815749.610247387 0, -1930101.4035317835 2814982.196513081 0, -1930344.3252405708 2814131.2391046174 0), (-1931176.4831238952 2815664.0622126306 0, -1931285.0219405617 2815257.3089883183 0, -1930496.8888091063 2815074.1259574196 0, -1930392.7472309952 2815465.399057443 0, -1930786.1327697122 2815564.888445243 0, -1931176.4831238952 2815664.0622126306 0)), ((-1932625.004395147 2824019.372009379 0, -1933015.4430826395 2824135.5915850047 0, -1932800.8537718498 2824906.077624436 0, -1932409.581895042 2824794.323167323 0, -1932625.004395147 2824019.372009379 0)), ((-1920878.2998509065 2864462.17655 0, -1919339.6526715388 2863911.015689175 0, -1919499.2762970189 2863216.3909553443 0, -1919730.7560771785 2862646.1294262023 0, -1921234.9285229577 2863201.991168637 0, -1920878.2998509065 2864462.17655 0)), ((-1922638.7562835668 2863745.317361907 0, -1924153.195741897 2864306.7299528057 0, -1923888.6471772937 2865271.213071534 0, -1922316.4412968731 2864845.7317742375 0, -1922638.7562835668 2863745.317361907 0)), ((-1926037.7249022147 2865457.6752195945 0, -1926036.5113501642 2865458.052518688 0, -1925975.9532681934 2865453.9122872567 0, -1925930.7511069255 2865465.3310377323 0, -1925799.5858269983 2865498.4620929626 0, -1925670.3957903862 2865546.158560157 0, -1925466.1884740398 2865642.7213355713 0, -1925454.2712138693 2865648.3563584513 0, -1925407.9209830656 2865656.2345184283 0, -1925416.9028312895 2865626.803323347 0, -1925647.9816289446 2864883.8372634226 0, -1926426.6688185155 2865162.56099678 0, -1926346.923875304 2865447.8805387504 0, -1926344.6599197036 2865455.9786466183 0, -1926286.1722074042 2865450.0294201733 0, -1926239.953681523 2865433.6989291757 0, -1926194.1290867266 2865409.05764377 0, -1926102.589071288 2865437.5118282633 0, -1926037.7249022147 2865457.6752195945 0)), ((-1920878.2998509065 2864462.17655 0, -1922316.4412968731 2864845.7317742375 0, -1921937.9880175826 2866328.2418175107 0, -1920493.8236914861 2865916.736179924 0, -1920878.2998509065 2864462.17655 0)), ((-1923905.1909504859 2866062.0840243534 0, -1923694.2456817098 2865994.054471567 0, -1923888.6471772937 2865271.213071534 0, -1924647.095419721 2865525.620003377 0, -1924553.537377164 2865901.4384199167 0, -1924430.9460681241 2865941.608395081 0, -1924323.7107533982 2865938.42827042 0, -1924230.5070588181 2866006.112174293 0, -1924104.4933114254 2866035.8790831277 0, -1924100.3231105062 2866036.8642222416 0, -1923905.1909504859 2866062.0840243534 0)), ((-1919701.1799191511 2865692.628450287 0, -1920493.8236914861 2865916.736179924 0, -1920282.5159418776 2866689.6695956476 0, -1920063.0392874023 2867437.0951254596 0, -1918519.0079381303 2867049.4514382277 0, -1918727.2580562208 2866291.9558586976 0, -1918935.992267362 2865493.9974696813 0, -1919701.1799191511 2865692.628450287 0)), ((-1920484.2790882466 2868891.2747279843 0, -1920457.821402454 2868892.4005715097 0, -1920423.629405119 2868893.855391192 0, -1920360.068046492 2868917.624331222 0, -1920298.8876387314 2868971.2923594313 0, -1920288.32324321 2868985.276912684 0, -1920253.0264786195 2869031.9994208585 0, -1920198.3077958673 2869072.7124186186 0, -1920172.056477208 2869092.2443947084 0, -1920070.8849752592 2869120.7112222956 0, -1920069.5049013162 2869120.347357614 0, -1919656.880719714 2869011.5518553834 0, -1920063.0392874023 2867437.0951254596 0, -1921505.7355209019 2867841.2034891616 0, -1921303.6114292133 2868629.609526721 0, -1920661.5235922271 2868452.082035754 0, -1920552.1579890763 2868882.1221683607 0, -1920551.1712253771 2868885.8993717683 0, -1920537.0033777482 2868887.4095733752 0, -1920516.0798756713 2868889.640050298 0, -1920511.680168411 2868890.1066194465 0, -1920484.2790882466 2868891.2747279843 0)), ((-1918281.6149233957 2869427.129881711 0, -1918180.6272271832 2869429.0710308147 0, -1918157.0973496847 2869429.5232212557 0, -1918121.4546746355 2869422.962137803 0, -1918109.0596553606 2869420.68110986 0, -1918105.0060209925 2869419.538707551 0, -1917882.2714684121 2869356.764865057 0, -1918095.5308712325 2868585.0459888475 0, -1918867.7827164773 2868791.986355689 0, -1918726.0367620673 2869308.9572289637 0, -1918725.9448960554 2869309.2774270247 0, -1918677.5162904623 2869380.159117461 0, -1918636.2236785386 2869440.596596778 0, -1918596.5901848478 2869421.0781514556 0, -1918460.091061805 2869423.70111539 0, -1918281.6149233957 2869427.129881711 0)), ((-1896662.1291620622 2805250.3423015014 0, -1896617.8490537708 2805417.656135391 0, -1896839.5872408089 2805526.699763196 0, -1896981.9109618014 2805599.2744929465 0, -1897118.6617120001 2805669.0071706297 0, -1897394.0270403055 2805732.1153340274 0, -1897405.6310079533 2805734.7171778316 0, -1897403.2774505315 2805741.8933131336 0, -1897160.6182358935 2805690.3540516123 0, -1896836.4849928634 2805560.3781644492 0, -1896796.3253876953 2805542.363626464 0, -1896664.9456934035 2805486.5652625123 0, -1896474.0382321659 2805390.3940137057 0, -1896027.2588527822 2805152.2507861634 0, -1895895.7028750055 2805075.2363432255 0, -1895897.5966885793 2805066.959958494 0, -1896037.0741669147 2805145.6315296795 0, -1896115.9962219296 2805170.8494562437 0, -1896252.7791996817 2805238.118718162 0, -1896253.7904080655 2805238.615882762 0, -1896257.1900887035 2805225.622883738 0, -1896278.2708206922 2805145.0768309115 0, -1896280.8100677126 2805145.7731968067 0, -1896662.1291620622 2805250.3423015014 0)), ((-1848363.6882150844 2809557.9256321383 0, -1847565.2008195755 2809347.35479946 0, -1847753.0180932435 2808570.847165622 0, -1848168.1485670605 2808679.627370943 0, -1848066.2456815925 2809060.0568930204 0, -1848467.2445381596 2809166.4507369203 0, -1848363.6882150844 2809557.9256321383 0)), ((-1855995.3764377357 2824711.132278971 0, -1856596.2530270615 2824860.499229959 0, -1856502.6217058415 2825243.653543744 0, -1855917.2237804504 2825098.7500604456 0, -1855902.085931869 2825094.751325446 0, -1855995.3764377357 2824711.132278971 0)), ((-1912910.4701252922 2825105.470172096 0, -1913690.2678639877 2825318.0513913846 0, -1913475.602772493 2826091.513492878 0, -1912695.934640716 2825879.9739590874 0, -1912910.4701252922 2825105.470172096 0)), ((-1911069.7715516498 2859288.2712812563 0, -1911118.0394319408 2859292.194786913 0, -1911148.3038582413 2859299.7011281266 0, -1911204.6475025443 2859323.4398436164 0, -1911433.145370624 2859457.0825968017 0, -1911475.0160240466 2859469.7359355534 0, -1911566.2282880305 2859484.6296004737 0, -1911624.1042513992 2859503.7192126443 0, -1911655.2056487277 2859524.9016695837 0, -1911672.238303252 2859550.3286137334 0, -1911693.0234700018 2859608.4402489266 0, -1911711.5377839655 2859633.0364471176 0, -1911787.3753059297 2859681.2531758402 0, -1911873.8105411069 2859711.941820578 0, -1912024.2322820295 2859744.469130588 0, -1912118.6433898045 2859778.4844851773 0, -1912533.2117745362 2859944.8979557194 0, -1913643.2050348504 2860347.8959560236 0, -1913527.9301741994 2860756.2311121295 0, -1915082.0788809326 2861183.9764312278 0, -1914655.1870602483 2862736.5331034884 0, -1913105.016828101 2862299.3443285665 0, -1913060.4700790537 2862471.6502935244 0, -1912992.565783229 2862453.340604565 0, -1913072.2428802666 2862365.9101331043 0, -1913086.8815983618 2862321.335075575 0, -1913093.0844607016 2862302.4471131875 0, -1913095.7141809722 2862294.442648306 0, -1913093.0009326101 2862222.036124531 0, -1913098.4926566228 2862078.558125645 0, -1913099.0955059526 2862062.8152301223 0, -1913026.3898837257 2862009.91471713 0, -1913014.0192889408 2861978.061959087 0, -1912974.4306614639 2861876.1249502343 0, -1912977.757394028 2861858.5793345035 0, -1912996.705049017 2861758.6463654567 0, -1913076.2420588923 2861721.586656786 0, -1913124.9517082511 2861698.8959120987 0, -1913139.4522744163 2861676.030208984 0, -1913223.418938074 2861543.628482523 0, -1913222.8707171988 2861534.6809602724 0, -1913221.1860840458 2861507.18803523 0, -1913214.856270181 2861403.8810550272 0, -1913207.2930252783 2861280.4406802733 0, -1913185.6124821394 2860926.5160575625 0, -1913157.2245225396 2860853.5992868417 0, -1913155.6716720276 2860849.6110518365 0, -1913125.3692025102 2860771.784262498 0, -1913131.7364428965 2860669.004731093 0, -1913131.782236189 2860668.72819048 0, -1913143.5723766568 2860477.931809763 0, -1913131.619344249 2860430.3780944976 0, -1913124.8165809885 2860403.3147919704 0, -1912941.4974071295 2860292.591562632 0, -1912833.3460024307 2860227.2493567374 0, -1912474.2022318812 2860010.26171056 0, -1912432.4013694355 2859985.0065007173 0, -1912356.966638263 2860217.7809732584 0, -1912335.8611494561 2860282.906388533 0, -1912390.8543641644 2860318.422930044 0, -1912504.0346987934 2860391.516893893 0, -1912597.268442078 2860512.76332725 0, -1912631.4741167298 2860526.0990556735 0, -1912663.9295307714 2860567.4074183432 0, -1912688.5321914845 2860613.0776181757 0, -1912718.59309723 2860651.3639282566 0, -1912718.9211642176 2860651.781943132 0, -1912752.8300348427 2860671.8267409485 0, -1912792.7016657135 2860715.319400522 0, -1912801.0621218358 2860751.8794533582 0, -1912802.8163927726 2860759.5508336276 0, -1912811.3612939587 2860771.9968697843 0, -1912860.9368616662 2860844.1748114796 0, -1912881.9719934592 2860850.586878815 0, -1912914.2566657045 2860887.3722070316 0, -1912951.5542474554 2860901.672441451 0, -1912997.136471682 2861061.497576031 0, -1912972.5083661168 2861121.6599827837 0, -1912976.572345268 2861168.462726313 0, -1912955.1807925128 2861213.557281548 0, -1912938.9904720702 2861247.6880313484 0, -1912914.4718112536 2861303.540262284 0, -1912900.9537771847 2861346.3993542246 0, -1912905.2138733114 2861372.9690812184 0, -1912885.3924334827 2861432.7661755173 0, -1912848.3822755567 2861450.0640992844 0, -1912807.5578270198 2861463.233480185 0, -1912779.958603024 2861482.7017999063 0, -1912706.106748129 2861489.606784551 0, -1912649.7560292801 2861492.86930673 0, -1912589.126544637 2861465.8263269123 0, -1912573.697175786 2861458.9442121834 0, -1912533.597625341 2861427.459699995 0, -1912509.6031612083 2861417.4320082692 0, -1912497.6881110407 2861412.4511158867 0, -1912435.0815359554 2861427.8055061647 0, -1912412.7539228862 2861448.3456075285 0, -1912370.034183779 2861438.8233540137 0, -1912300.3260759236 2861435.998505672 0, -1912283.3518890105 2861420.8285070877 0, -1912226.1528728916 2861434.1905212556 0, -1912214.300237075 2861436.959300874 0, -1912150.424289445 2861464.1960276156 0, -1912116.9846162822 2861465.5227756826 </t>
+          <t>MULTIPOLYGON Z (((-201157.89714606619 2226817.235233947 0, -201150.4477368668 2227219.438475946 0, -200753.3026580403 2227209.6763946763 0, -200761.2634767131 2226807.28490224 0, -200769.14780959437 2226405.0503807156 0, -200774.72665332502 2226003.684905638 0, -200780.4616888446 2225601.4149824106 0, -201173.2890220301 2225612.9101912207 0, -201169.26346164412 2226014.247476004 0, -201165.3147526024 2226415.1188031007 0, -201157.89714606619 2226817.235233947 0)), ((-200676.61833697834 2245072.9570895853 0, -200665.50219727602 2245477.002334861 0, -200654.41287032556 2245882.0017014216 0, -200253.06813058004 2245868.06750964 0, -200264.80304160324 2245464.127465126 0, -200276.0542363167 2245060.042299942 0, -200676.61833697834 2245072.9570895853 0)), ((-195578.19880497677 2240443.3940137667 0, -195588.7887579272 2240039.0023805574 0, -195990.64187128432 2240050.3519468727 0, -195979.83454412993 2240455.3803870333 0, -195969.04419966493 2240859.482109948 0, -195567.5232243485 2240846.6419790983 0, -195578.19880497677 2240443.3940137667 0)), ((-195094.1654991865 2243651.0130477655 0, -195495.08877752116 2243663.273893927 0, -195484.58355444393 2244090.3184903734 0, -195083.88341866044 2244078.4668051726 0, -195094.1654991865 2243651.0130477655 0)), ((-194940.4916684473 2250262.022545632 0, -195003.14344391183 2250153.274088545 0, -195323.60931402224 2250162.274926262 0, -195313.63431049834 2250560.801723744 0, -194913.45908245555 2250548.03897212 0, -194513.28320715865 2250535.2967868103 0, -194920.3943810987 2250274.8795906464 0, -194940.4916684473 2250262.022545632 0)))</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Yakama</t>
+          <t>Yankton</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>WA</t>
+          <t>SD</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Common School and Indemnity, State Forest Transfer, Escheat, Scientific School, Community Forest Trust, Normal School, Natural Resources Conservation Area, Charitable/Educational/Penal &amp; Reformatory Instit., University - Transferred</t>
+          <t>Rural Credit, Common School</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Subsurface</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>304</v>
+        <v>11</v>
       </c>
       <c r="G78" t="n">
-        <v>46922.33</v>
+        <v>0</v>
       </c>
       <c r="H78" t="n">
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="I78" t="n">
-        <v>44906.36</v>
+        <v>411.47</v>
       </c>
       <c r="J78" t="n">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="K78" t="n">
-        <v>91828.69</v>
+        <v>411.47</v>
       </c>
       <c r="L78" t="n">
-        <v>1376779.33</v>
+        <v>441528.7</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-201157.89714606619 2226817.235233947 0, -201150.4477368668 2227219.438475946 0, -200753.3026580403 2227209.6763946763 0, -200761.2634767131 2226807.28490224 0, -200769.14780959437 2226405.0503807156 0, -200774.72665332502 2226003.684905638 0, -200780.4616888446 2225601.4149824106 0, -201173.2890220301 2225612.9101912207 0, -201169.26346164412 2226014.247476004 0, -201165.3147526024 2226415.1188031007 0, -201157.89714606619 2226817.235233947 0)), ((-200676.61833697834 2245072.9570895853 0, -200665.50219727602 2245477.002334861 0, -200654.41287032556 2245882.0017014216 0, -200253.06813058004 2245868.06750964 0, -200264.80304160324 2245464.127465126 0, -200276.0542363167 2245060.042299942 0, -200676.61833697834 2245072.9570895853 0)), ((-195578.19880497677 2240443.3940137667 0, -195588.7887579272 2240039.0023805574 0, -195990.64187128432 2240050.3519468727 0, -195979.83454412993 2240455.3803870333 0, -195969.04419966493 2240859.482109948 0, -195567.5232243485 2240846.6419790983 0, -195578.19880497677 2240443.3940137667 0)), ((-195094.1654991865 2243651.0130477655 0, -195495.08877752116 2243663.273893927 0, -195484.58355444393 2244090.3184903734 0, -195083.88341866044 2244078.4668051726 0, -195094.1654991865 2243651.0130477655 0)), ((-194940.4916684473 2250262.022545632 0, -195003.14344391183 2250153.274088545 0, -195323.60931402224 2250162.274926262 0, -195313.63431049834 2250560.801723744 0, -194913.45908245555 2250548.03897212 0, -194513.28320715865 2250535.2967868103 0, -194920.3943810987 2250274.8795906464 0, -194940.4916684473 2250262.022545632 0)))</t>
+          <t>MULTIPOLYGON Z (((-963268.8443002809 1430363.758449293 0, -963314.768776577 1429960.686608801 0, -963712.0928119401 1430005.2204112052 0, -964109.4149344104 1430049.7727536343 0, -964506.7349353305 1430094.3437174025 0, -964904.050499542 1430138.9532507225 0, -964857.8234155204 1430542.153026707 0, -964811.5983582808 1430945.3339162313 0, -964765.3870148513 1431348.538080399 0, -964719.1596053746 1431751.7416974963 0, -964322.1604582192 1431707.0262301438 0, -963925.1432217385 1431662.3276507275 0, -963528.1377355896 1431617.6691773336 0, -963131.1162792982 1431573.0076248609 0, -963177.0249580408 1431169.9300062372 0, -963222.935745118 1430766.833605139 0, -963268.8443002809 1430363.758449293 0)), ((-967876.2163708522 1435408.6258091806 0, -967898.5115904618 1435410.9029027203 0, -968024.1492157216 1435423.7205935058 0, -968272.4248065699 1435449.0805621415 0, -968420.5530298074 1435465.1779594878 0, -968668.6124218298 1435491.7214209768 0, -968816.8661406672 1435507.5765224646 0, -969064.811744366 1435534.1185812366 0, -969019.2277263771 1435940.26696611 0, -968973.6274765375 1436346.4146844898 0, -968928.0430966188 1436752.5655057395 0, -968882.460746101 1437158.697634772 0, -968487.2379654302 1437113.5522262396 0, -968092.0154913071 1437068.4051628842 0, -967696.7885802072 1437023.2965345103 0, -967301.5779261262 1436978.1881779493 0, -967346.1711293819 1436575.7762582644 0, -967390.7641289367 1436173.3655807443 0, -967435.3569149923 1435770.9562472757 0, -967479.9492996859 1435368.5481400448 0, -967627.6342112896 1435383.2426118369 0, -967876.2163708522 1435408.6258091806 0)), ((-960653.0446861065 1425166.016569518 0, -960607.207696015 1425569.36785534 0, -960561.0948636045 1425972.8516395423 0, -960514.9819931365 1426376.3368287787 0, -960116.7787778581 1426331.3044214197 0, -959718.5757645215 1426286.2707026964 0, -959321.3485803383 1426241.4065627086 0, -958926.1302420439 1426196.807988672 0, -958935.754727946 1426107.382628779 0, -958967.4774739698 1425812.6336601684 0, -958968.9143523972 1425799.3134923284 0, -959010.972017595 1425408.6922006202 0, -959011.6981147537 1425401.8201261768 0, -959056.0033996366 1425005.0064636632 0, -959056.4447545457 1425001.0928834502 0, -959056.7416672814 1424998.4600985888 0, -959101.0828541025 1424601.3289680968 0, -959172.6533876254 1424608.8375537123 0, -959490.5010221126 1424642.1898751282 0, -959888.511958673 1424683.9590740039 0, -959895.4770753954 1424684.7715973589 0, -959899.2016164239 1424685.2104734667 0, -959899.2026799689 1424685.2105960224 0, -960080.0348917983 1424706.0484719486 0, -960292.8598894889 1424730.578138235 0, -960295.0851773646 1424730.8294062922 0, -960298.2058799788 1424731.1890148665 0, -960298.2068716306 1424731.189129193 0, -960501.5159544711 1424754.6284201655 0, -960697.2077411973 1424777.196489024 0, -960653.0446861065 1425166.016569518 0)), ((-961324.0386378516 1433411.4759536136 0, -960928.6425412277 1433366.544296997 0, -960533.037416067 1433321.5874915635 0, -960137.7060290826 1433276.6597803393 0, -959742.0207926851 1433231.6905779922 0, -959787.7854994311 1432828.8331621452 0, -960183.1167977916 1432873.6407322495 0, -960578.4437900083 1432918.4867662687 0, -960973.7709123844 1432963.3312459562 0, -961369.0959684617 1433008.1939289172 0, -961324.0386378516 1433411.4759536136 0)))</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Yankton</t>
+          <t>Zia</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>NM</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Rural Credit, Common School</t>
+          <t>Common Schools</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -4218,7 +4218,7 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="G79" t="n">
         <v>0</v>
@@ -4227,111 +4227,63 @@
         <v>0</v>
       </c>
       <c r="I79" t="n">
-        <v>411.47</v>
+        <v>2078.97</v>
       </c>
       <c r="J79" t="n">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="K79" t="n">
-        <v>411.47</v>
+        <v>2078.97</v>
       </c>
       <c r="L79" t="n">
-        <v>441528.7</v>
+        <v>134256.19</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-963268.8443002809 1430363.758449293 0, -963314.768776577 1429960.686608801 0, -963712.0928119401 1430005.2204112052 0, -964109.4149344104 1430049.7727536343 0, -964506.7349353305 1430094.3437174025 0, -964904.050499542 1430138.9532507225 0, -964857.8234155204 1430542.153026707 0, -964811.5983582808 1430945.3339162313 0, -964765.3870148513 1431348.538080399 0, -964719.1596053746 1431751.7416974963 0, -964322.1604582192 1431707.0262301438 0, -963925.1432217385 1431662.3276507275 0, -963528.1377355896 1431617.6691773336 0, -963131.1162792982 1431573.0076248609 0, -963177.0249580408 1431169.9300062372 0, -963222.935745118 1430766.833605139 0, -963268.8443002809 1430363.758449293 0)), ((-967876.2163708522 1435408.6258091806 0, -967898.5115904618 1435410.9029027203 0, -968024.1492157216 1435423.7205935058 0, -968272.4248065699 1435449.0805621415 0, -968420.5530298074 1435465.1779594878 0, -968668.6124218298 1435491.7214209768 0, -968816.8661406672 1435507.5765224646 0, -969064.811744366 1435534.1185812366 0, -969019.2277263771 1435940.26696611 0, -968973.6274765375 1436346.4146844898 0, -968928.0430966188 1436752.5655057395 0, -968882.460746101 1437158.697634772 0, -968487.2379654302 1437113.5522262396 0, -968092.0154913071 1437068.4051628842 0, -967696.7885802072 1437023.2965345103 0, -967301.5779261262 1436978.1881779493 0, -967346.1711293819 1436575.7762582644 0, -967390.7641289367 1436173.3655807443 0, -967435.3569149923 1435770.9562472757 0, -967479.9492996859 1435368.5481400448 0, -967627.6342112896 1435383.2426118369 0, -967876.2163708522 1435408.6258091806 0)), ((-960653.0446861065 1425166.016569518 0, -960607.207696015 1425569.36785534 0, -960561.0948636045 1425972.8516395423 0, -960514.9819931365 1426376.3368287787 0, -960116.7787778581 1426331.3044214197 0, -959718.5757645215 1426286.2707026964 0, -959321.3485803383 1426241.4065627086 0, -958926.1302420439 1426196.807988672 0, -958935.754727946 1426107.382628779 0, -958967.4774739698 1425812.6336601684 0, -958968.9143523972 1425799.3134923284 0, -959010.972017595 1425408.6922006202 0, -959011.6981147537 1425401.8201261768 0, -959056.0033996366 1425005.0064636632 0, -959056.4447545457 1425001.0928834502 0, -959056.7416672814 1424998.4600985888 0, -959101.0828541025 1424601.3289680968 0, -959172.6533876254 1424608.8375537123 0, -959490.5010221126 1424642.1898751282 0, -959888.511958673 1424683.9590740039 0, -959895.4770753954 1424684.7715973589 0, -959899.2016164239 1424685.2104734667 0, -959899.2026799689 1424685.2105960224 0, -960080.0348917983 1424706.0484719486 0, -960292.8598894889 1424730.578138235 0, -960295.0851773646 1424730.8294062922 0, -960298.2058799788 1424731.1890148665 0, -960298.2068716306 1424731.189129193 0, -960501.5159544711 1424754.6284201655 0, -960697.2077411973 1424777.196489024 0, -960653.0446861065 1425166.016569518 0)), ((-961324.0386378516 1433411.4759536136 0, -960928.6425412277 1433366.544296997 0, -960533.037416067 1433321.5874915635 0, -960137.7060290826 1433276.6597803393 0, -959742.0207926851 1433231.6905779922 0, -959787.7854994311 1432828.8331621452 0, -960183.1167977916 1432873.6407322495 0, -960578.4437900083 1432918.4867662687 0, -960973.7709123844 1432963.3312459562 0, -961369.0959684617 1433008.1939289172 0, -961324.0386378516 1433411.4759536136 0)))</t>
+          <t>MULTIPOLYGON Z (((-1230650.156670046 1366226.2121109671 0, -1231028.9950256061 1366267.9902809532 0, -1231434.9410266553 1366312.7802076074 0, -1231553.7829297276 1366325.8982821826 0, -1231860.339186602 1366362.0613912167 0, -1232246.1631810844 1366407.5938032246 0, -1232193.9459687504 1366815.4479508896 0, -1232141.0641802193 1367228.4859656875 0, -1232088.184509508 1367641.522767267 0, -1232035.6589074172 1368051.7703597795 0, -1231637.5983343583 1367995.2436863934 0, -1231238.7788168278 1367938.6251752558 0, -1230839.959229202 1367882.0254403732 0, -1230441.1340725517 1367825.4471172183 0, -1230493.6114402523 1367423.947975173 0, -1230546.0880157726 1367022.4503648307 0, -1230598.5639603366 1366620.954313936 0, -1230650.156670046 1366226.2121109671 0)), ((-1179406.438675978 1391598.4780311848 0, -1179376.687082965 1391813.8626402074 0, -1179010.4326745963 1391763.4625733264 0, -1179065.7797230636 1391362.0123873388 0, -1179319.6081469771 1391396.9113365898 0, -1179432.1469314967 1391412.3850173734 0, -1179406.438675978 1391598.4780311848 0)), ((-1175305.599237999 1392944.4259394954 0, -1175621.874753935 1392989.2567373854 0, -1175621.8809291632 1392989.2576126994 0, -1175910.2924798438 1393030.1499464114 0, -1176014.9073974208 1393044.985994756 0, -1176031.103019932 1393047.2170488585 0, -1176046.4939471069 1393049.3403368995 0, -1176012.7306980283 1393060.7847225934 0, -1175736.8256427709 1393154.0499050894 0, -1175592.5168004592 1393202.6557926997 0, -1175589.648874361 1393203.6227490243 0, -1175323.7911327295 1393293.1614621235 0, -1175172.3955430223 1393343.8675344859 0, -1175170.7525365737 1393344.4340099616 0, -1174752.3127354553 1393484.6127173828 0, -1174745.9919210786 1393486.7307787493 0, -1174332.2999252037 1393625.3644597516 0, -1174379.2882461646 1393283.846637234 0, -1174387.5275870538 1393223.9615068294 0, -1174442.7906177957 1392822.1808368226 0, -1174442.797383291 1392822.1817798174 0, -1174508.347529387 1392831.467321712 0, -1174835.821363174 1392877.8660369725 0, -1175228.8553593291 1392933.549978982 0, -1175305.599237999 1392944.4259394954 0)), ((-1175498.48855562 1411715.7205234338 0, -1175441.8983347837 1412118.5051669523 0, -1175385.3242070945 1412521.2934287016 0, -1174988.4403513533 1412467.4704269178 0, -1174591.5674526324 1412413.6881112035 0, -1174194.6786928598 1412359.9022091634 0, -1173797.7847071388 1412306.15462643 0, -1173821.9412342522 1412130.3965524095 0, -1174114.0481024592 1412035.6636411452 0, -1174245.7611750644 1411992.951309675 0, -1174323.0265613003 1411967.9030613736 0, -1174647.7320901754 1412011.9211541049 0, -1174669.5860315608 1411855.4850039117 0, -1174952.3221461347 1411763.7958221657 0, -1175093.4321466126 1411717.8781879004 0, -1175177.930924187 1411690.378694991 0, -1175217.4038987628 1411677.6287058126 0, -1175498.48855562 1411715.7205234338 0)), ((-1173751.581436906 1412710.9424306303 0, -1173705.3932026997 1413115.7338729296 0, -1173659.2128793285 1413520.2228657487 0, -1173613.0315028783 1413924.7131335821 0, -1173205.9243093685 1413868.355277904 0, -1172798.8011752826 1413811.9948493536 0, -1172391.688647008 1413755.6758929698 0, -1171984.5673369104 1413699.353434267 0, -1172041.4165952036 1413295.2357265905 0, -1172098.2496506604 1412891.117114005 0, -1172127.4563667192 1412680.2118645296 0, -1172127.835877648 1412680.0813261492 0, -1172436.2533071206 1412579.7565870732 0, -1172545.9688739832 1412544.0760245186 0, -1172554.7766014778 1412545.2885085973 0, -1172947.894318748 1412599.699872987 0, -1172971.7267977002 1412405.7625562567 0, -1173041.902875316 1412383.0617254323 0, -1173276.6135359607 1412307.0915113334 0, -1173399.2328404363 1412267.424644406 0, -1173434.7959754285 1412255.9174583415 0, -1173508.7881769352 1412266.151749508 0, -1173797.7847071388 1412306.15462643 0, -1173751.581436906 1412710.9424306303 0)), ((-1173580.6659229193 1420491.9394159773 0, -1173988.2226527212 1420545.8410660995 0, -1174395.7767336085 1420599.7620567963 0, -1174340.3669349628 1421002.050548744 0, -1174284.9568995119 1421404.340637009 0, -1174229.1714013966 1421806.376833381 0, -1174172.9946762586 1422211.2476761562 0, -1173760.3094233195 1422155.459276981 0, -1173347.6054191792 1422099.6885641788 0, -1172934.9122025375 1422043.9601368255 0, -1172522.2189816942 1421988.231668506 0, -1172581.7721226283 1421584.965266842 0, -1172640.9633129588 1421184.0901085644 0, -1172703.2446664653 1420784.1505723682 0, -1172765.5425179063 1420384.2146920348 0, -1173173.104076678 1420438.0773112255 0, -1173580.6659229193 1420491.9394159773 0)), ((-1172931.5229131742 1392610.821508625 0, -1172868.1889384773 1393074.6264596726 0, -1172813.3253800871 1393476.5471046895 0, -1172758.4452655197 1393878.467051319 0, -1172718.5168001745 1394170.8544220314 0, -1172664.2858641562 1394189.1357508404 0, -1172482.8464786327 1394250.2482840049 0, -1172307.9466047282 1394226.2442566087 0, -1171912.611488917 1394172.0763804908 0, -1171517.1442191983 1394118.030874152 0, -1171121.674581965 1394064.0037918896 0, -1171176.4501409233 1393662.16961251 0, -1171231.2254442002 1393260.3369106937 0, -1171286.006078273 1392858.4658545179 0, -1171348.3640234817 1392401.1326202895 0, -1171701.545907671 1392447.8108679873 0, -1171744.1627877895 1392453.456954902 0, -1172097.0675940812 1392500.1139375262 0, -1172139.9537026782 1392505.839576628 0, -1172492.5493494605 1392552.4705798456 0, -1172535.7639712938 1392558.2027700492 0, -1172888.0502426925 1392604.8079744328 0, -1172931.5229131742 1392610.821508625 0)), ((-1172428.4447664267 1422802.9976639973 0, -1172381.5574290259 1423210.3726671918 0, -1172334.6690533226 1423617.749033902 0, -1171934.255366138 1423566.6582560865 0, -1171533.8233525308 1423515.5840813902 0, -1171133.3919443616 1423464.5089000766 0, -1170732.9746686113 1423413.4756065952 0, -1170785.9002174437 1423010.5717117349 0, -1170838.8280762054 1422607.6491881046 0, -1170891.7527453594 1422204.748089802 0, -1170944.6958408337 1421801.8304217265 0, -1171339.0711084942 1421848.4121627612 0, -1171733.4511185244 1421894.9930114867 0, -1172127.8264853735 1421941.612038815 0, -1172522.2189816942 1421988.231668506 0, -1172475.3337117848 1422395.6040405133 0, -1172428.4447664267 1422802.9976639973 0)), ((-1166379.8580742273 1393412.7984702166 0, -1165984.229424639 1393358.8500000613 0, -1165588.61172215 1393304.9417828736 0, -1165192.9780163325 1393251.0298344865 0, -1164797.3552512976 1393197.1582403914 0, -1164851.7833524747 1392795.2767565313 0, -1164906.213813485 1392393.3768613848 0, -1164960.8570348632 1391991.4870388547 0, -1165015.4839551386 1391589.5966411936 0, -1165411.0337512083 1391641.1819036664 0, -1165806.565017187 1391692.7833502255 0, -1166204.1803047655 1391744.566076178 0, -1166601.8120934765 1391796.3495493892 0, -1166545.4010741839 1392207.2434767624 0, -1166490.2246998842 1392609.1010301283 0, -1166435.0510008365 1393010.940109647 0, -1166379.8580742273 1393412.7984702166 0)), ((-1168346.2402175646 1416938.950836989 0, -1168291.8866725499 1417344.4231284817 0, -1168237.535633526 1417749.876955446 0, -1168183.181422921 1418155.3521491783 0, -1167782.2249332508 1418106.2680156042 0, -1167381.2637183075 1418057.2224765148 0, -1166980.303220909 1418008.1760811964 0, -1166579.3244220777 1417959.1463298993 0, -1166631.40375167 1417552.5665601827 0, -1166683.4825636602 1417145.987956514 0, -1166735.563563827 1416739.3909451917 0, -1166787.641173089 1416332.8153704344 0, -1167190.8791227962 1416382.9472842843 0, -1167594.1120814949 1416433.1182798971 0, -1167997.3457350433 1416483.2884237745 0, -1168400.577237942 1416533.4776820375 0, -1168346.2402175646 1416938.950836989 0)), ((-1169364.0171739731 1421592.1376663186 0, -1169309.5614646836 1421994.908155483 0, -1169255.1082735094 1422397.6599490184 0, -1169200.6547376886 1422800.4132128763 0, -1169146.2009559378 1423203.1679550996 0, -1168735.3866428486 1423150.8022123748 0, -1168324.551193241 1423098.4740808965 0, -1167913.7323020592 1423046.1480197525 0, -1167502.908178204 1422993.8618082106 0, -1167558.5688820183 1422589.8698776641 0, -1167614.2268096716 1422185.8993378947 0, -1167669.8844984479 1421781.9302947018 0, -1167725.5419775494 1421377.9624487595 0, -1168135.1590305243 1421431.4862235263 0, -1168544.792575077 1421485.0117535614 0, -1168954.404688972 1421538.5748606836 0, -1169364.0171739731 1421592.1376663186 0)), ((-1164634.1081047873 1420190.6300656113 0, -1164576.9766307764 1420593.5399584575 0, -1164519.8452037955 1420996.4513851749 0, -1164129.5886527759 1420948.558849198 0, -1163739.33284891 1420900.664002819 0, -1163349.072364934 1420852.8072118475 0, -1162958.8127199542 1420804.9482208462 0, -1163010.6734844977 1420403.775606886 0, -1163062.5175730835 1420002.6020558227 0, -1163111.2830547593 1419602.2085557617 0, -1163160.0611932212 1419201.8385708327 0, -1163558.1923093174 1419247.0732339686 0, -1163956.3350437784 1419292.3488860107 0, -1164354.4761687422 1419337.6430014072 0, -1164752.6182990842 1419382.9358940723 0, -1164693.3537539684 1419786.791009418 0, -1164634.1081047873 1420190.6300656113 0)), ((-1162554.3179741418 1420760.8343401507 0, -1162958.8127199542 1420804.9482208462 0, -1162907.1421569402 1421206.1687318848 0, -1162855.45500648 1421607.3884115983 0, -1162803.7673767486 1422008.6094145814 0, -1162752.0954645814 1422409.8340048988 0, -1162357.0406865175 1422364.2244797307 0, -1161961.9869693308 1422318.6134074237 0, -1161566.9315708561 1422273.0207662575 0, -1161171.8717686632 1422227.4663342931 0, -1161214.1050098995 1421827.7387250643 0, -1161256.3504611242 1421428.034624433 0, -1161298.5812155544 1421028.3095464534 0, -1161340.8077851892 1420628.6056951552 0, -1161745.3234605545 1420672.66414543 0, -1162149.8214223213 1420716.7396355853 0, -1162554.3179741418 1420760.8343401507 0)), ((-1160555.835367265 1342362.4724318008 0, -1160639.0989210666 1342372.8008393203 0, -1160639.1025707817 1342372.8012920392 0, -1161067.547138715 1342425.9465278913 0, -1161084.0594122906 1342427.9948507575 0, -1161084.0625698133 1342427.995312719 0, -1161086.8509861662 1342428.4032720837 0, -1161481.30990815 1342486.1245715774 0, -1161471.8016836355 1342557.7932392866 0, -1161426.9593904626 1342895.7342120272 0, -1161426.9583758549 1342895.741858687 0, -1161382.1573930888 1343233.3875231277 0, -1161372.6084341146 1343305.3411579954 0, -1161345.5917563364 1343502.4844921895 0, -1161317.9007638758 1343704.535456809 0, -1161174.6171993 1343681.4754627682 0, -1160918.0771163949 1343640.1857298138 0, -1160918.0768122156 1343640.1879653856 0, -1160918.07595339 1343640.1878271666 0, -1160863.1124110003 1344044.1219970598 0, -1160419.319074915 1343987.2959846682 0, -1160200.1974385392 1343959.2410356097 0, -1160021.8329877972 1343936.4005959847 0, -1160021.8323116223 1343936.4005094012 0, -1159742.2525162355 1343900.6005991232 0, -1159622.9155582127 1343885.3180074997 0, -1159677.0775108382 1343481.2768438656 0, -1159677.0776918822 1343481.2754933028 0, -1159708.191035808 1343249.174230714 0, -1159731.2444110706 1343077.2353770316 0, -1159751.1380842498 1342911.234984098 0, -1159779.4919498912 1342674.6956624135 0, -1159779.4923405426 1342674.6924034243 0, -1159827.7437912773 1342272.1571615706 0, -1159970.3261369911 1342289.8435207168 0, -1160239.2273022288 1342323.2090227657 0, -1160555.835367265 1342362.4724318008 0)), ((-1157166.6133341766 1418425.5600141888 0, -1157168.564336575 1418425.8454011441 0, -1157164.0956349513 1418429.9739014811 0, -1156969.451975769 1418609.2781745216 0, -1156914.1249898104 1418692.372831359 0, -1156868.3254176043 1418797.4147460205 0, -1156722.0185353474 1418776.390662088 0, -1156767.2325033643 1418367.0227464072 0, -1156990.915978495 1418399.808372859 0, -1157164.6204906022 1418425.2685328429 0, -1157166.6133341766 1418425.5600141888 0)), ((-1159678.263049038 1421200.6842120434 0, -1159633.407860968 1421589.500756771 0, -1159588.551875587 1421978.318575145 0, -1159194.6171948852 1421940.5322140078 0, -1158800.694781235 1421902.7862226758 0, -1158406.7553600164 1421865.0563305682 0, -1158012.8336763529 1421827.3270519462 0, -1158053.6318724658 1421424.379318485 0, -1158094.425684959 1421021.4527952771 0, -1158135.2369948642 1420618.5098106978 0, -1158176.0279103909 1420215.5858927795 0, -1158574.0130461846 1420267.42473959 0, -1158971.9958590274 1420319.282030556 0, -1159369.9924167069 1420371.1603221798 0, -1159767.9705395217 1420423.0549011857 0, -1159723.1172424308 1420811.8689232648 0, -1159678.263049038 1421200.6842120434 0)))</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Zia</t>
+          <t>Zuni</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>NM</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Common Schools</t>
+          <t>PERM CMN SCHLS (INDMTY SELEC), Saline Lands, University of New Mexico, Common Schools, New Mexico School for the Visually Handicapped</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>52</v>
+        <v>189</v>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>62.57</v>
       </c>
       <c r="H80" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I80" t="n">
-        <v>2078.97</v>
+        <v>8070.27</v>
       </c>
       <c r="J80" t="n">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="K80" t="n">
-        <v>2078.97</v>
+        <v>8132.84</v>
       </c>
       <c r="L80" t="n">
-        <v>134256.19</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON Z (((-1230650.156670046 1366226.2121109671 0, -1231028.9950256061 1366267.9902809532 0, -1231434.9410266553 1366312.7802076074 0, -1231553.7829297276 1366325.8982821826 0, -1231860.339186602 1366362.0613912167 0, -1232246.1631810844 1366407.5938032246 0, -1232193.9459687504 1366815.4479508896 0, -1232141.0641802193 1367228.4859656875 0, -1232088.184509508 1367641.522767267 0, -1232035.6589074172 1368051.7703597795 0, -1231637.5983343583 1367995.2436863934 0, -1231238.7788168278 1367938.6251752558 0, -1230839.959229202 1367882.0254403732 0, -1230441.1340725517 1367825.4471172183 0, -1230493.6114402523 1367423.947975173 0, -1230546.0880157726 1367022.4503648307 0, -1230598.5639603366 1366620.954313936 0, -1230650.156670046 1366226.2121109671 0)), ((-1179406.438675978 1391598.4780311848 0, -1179376.687082965 1391813.8626402074 0, -1179010.4326745963 1391763.4625733264 0, -1179065.7797230636 1391362.0123873388 0, -1179319.6081469771 1391396.9113365898 0, -1179432.1469314967 1391412.3850173734 0, -1179406.438675978 1391598.4780311848 0)), ((-1175305.599237999 1392944.4259394954 0, -1175621.874753935 1392989.2567373854 0, -1175621.8809291632 1392989.2576126994 0, -1175910.2924798438 1393030.1499464114 0, -1176014.9073974208 1393044.985994756 0, -1176031.103019932 1393047.2170488585 0, -1176046.4939471069 1393049.3403368995 0, -1176012.7306980283 1393060.7847225934 0, -1175736.8256427709 1393154.0499050894 0, -1175592.5168004592 1393202.6557926997 0, -1175589.648874361 1393203.6227490243 0, -1175323.7911327295 1393293.1614621235 0, -1175172.3955430223 1393343.8675344859 0, -1175170.7525365737 1393344.4340099616 0, -1174752.3127354553 1393484.6127173828 0, -1174745.9919210786 1393486.7307787493 0, -1174332.2999252037 1393625.3644597516 0, -1174379.2882461646 1393283.846637234 0, -1174387.5275870538 1393223.9615068294 0, -1174442.7906177957 1392822.1808368226 0, -1174442.797383291 1392822.1817798174 0, -1174508.347529387 1392831.467321712 0, -1174835.821363174 1392877.8660369725 0, -1175228.8553593291 1392933.549978982 0, -1175305.599237999 1392944.4259394954 0)), ((-1175498.48855562 1411715.7205234338 0, -1175441.8983347837 1412118.5051669523 0, -1175385.3242070945 1412521.2934287016 0, -1174988.4403513533 1412467.4704269178 0, -1174591.5674526324 1412413.6881112035 0, -1174194.6786928598 1412359.9022091634 0, -1173797.7847071388 1412306.15462643 0, -1173821.9412342522 1412130.3965524095 0, -1174114.0481024592 1412035.6636411452 0, -1174245.7611750644 1411992.951309675 0, -1174323.0265613003 1411967.9030613736 0, -1174647.7320901754 1412011.9211541049 0, -1174669.5860315608 1411855.4850039117 0, -1174952.3221461347 1411763.7958221657 0, -1175093.4321466126 1411717.8781879004 0, -1175177.930924187 1411690.378694991 0, -1175217.4038987628 1411677.6287058126 0, -1175498.48855562 1411715.7205234338 0)), ((-1173751.581436906 1412710.9424306303 0, -1173705.3932026997 1413115.7338729296 0, -1173659.2128793285 1413520.2228657487 0, -1173613.0315028783 1413924.7131335821 0, -1173205.9243093685 1413868.355277904 0, -1172798.8011752826 1413811.9948493536 0, -1172391.688647008 1413755.6758929698 0, -1171984.5673369104 1413699.353434267 0, -1172041.4165952036 1413295.2357265905 0, -1172098.2496506604 1412891.117114005 0, -1172127.4563667192 1412680.2118645296 0, -1172127.835877648 1412680.0813261492 0, -1172436.2533071206 1412579.7565870732 0, -1172545.9688739832 1412544.0760245186 0, -1172554.7766014778 1412545.2885085973 0, -1172947.894318748 1412599.699872987 0, -1172971.7267977002 1412405.7625562567 0, -1173041.902875316 1412383.0617254323 0, -1173276.6135359607 1412307.0915113334 0, -1173399.2328404363 1412267.424644406 0, -1173434.7959754285 1412255.9174583415 0, -1173508.7881769352 1412266.151749508 0, -1173797.7847071388 1412306.15462643 0, -1173751.581436906 1412710.9424306303 0)), ((-1173580.6659229193 1420491.9394159773 0, -1173988.2226527212 1420545.8410660995 0, -1174395.7767336085 1420599.7620567963 0, -1174340.3669349628 1421002.050548744 0, -1174284.9568995119 1421404.340637009 0, -1174229.1714013966 1421806.376833381 0, -1174172.9946762586 1422211.2476761562 0, -1173760.3094233195 1422155.459276981 0, -1173347.6054191792 1422099.6885641788 0, -1172934.9122025375 1422043.9601368255 0, -1172522.2189816942 1421988.231668506 0, -1172581.7721226283 1421584.965266842 0, -1172640.9633129588 1421184.0901085644 0, -1172703.2446664653 1420784.1505723682 0, -1172765.5425179063 1420384.2146920348 0, -1173173.104076678 1420438.0773112255 0, -1173580.6659229193 1420491.9394159773 0)), ((-1172931.5229131742 1392610.821508625 0, -1172868.1889384773 1393074.6264596726 0, -1172813.3253800871 1393476.5471046895 0, -1172758.4452655197 1393878.467051319 0, -1172718.5168001745 1394170.8544220314 0, -1172664.2858641562 1394189.1357508404 0, -1172482.8464786327 1394250.2482840049 0, -1172307.9466047282 1394226.2442566087 0, -1171912.611488917 1394172.0763804908 0, -1171517.1442191983 1394118.030874152 0, -1171121.674581965 1394064.0037918896 0, -1171176.4501409233 1393662.16961251 0, -1171231.2254442002 1393260.3369106937 0, -1171286.006078273 1392858.4658545179 0, -1171348.3640234817 1392401.1326202895 0, -1171701.545907671 1392447.8108679873 0, -1171744.1627877895 1392453.456954902 0, -1172097.0675940812 1392500.1139375262 0, -1172139.9537026782 1392505.839576628 0, -1172492.5493494605 1392552.4705798456 0, -1172535.7639712938 1392558.2027700492 0, -1172888.0502426925 1392604.8079744328 0, -1172931.5229131742 1392610.821508625 0)), ((-1172428.4447664267 1422802.9976639973 0, -1172381.5574290259 1423210.3726671918 0, -1172334.6690533226 1423617.749033902 0, -1171934.255366138 1423566.6582560865 0, -1171533.8233525308 1423515.5840813902 0, -1171133.3919443616 1423464.5089000766 0, -1170732.9746686113 1423413.4756065952 0, -1170785.9002174437 1423010.5717117349 0, -1170838.8280762054 1422607.6491881046 0, -1170891.7527453594 1422204.748089802 0, -1170944.6958408337 1421801.8304217265 0, -1171339.0711084942 1421848.4121627612 0, -1171733.4511185244 1421894.9930114867 0, -1172127.8264853735 1421941.612038815 0, -1172522.2189816942 1421988.231668506 0, -1172475.3337117848 1422395.6040405133 0, -1172428.4447664267 1422802.9976639973 0)), ((-1166379.8580742273 1393412.7984702166 0, -1165984.229424639 1393358.8500000613 0, -1165588.61172215 1393304.9417828736 0, -1165192.9780163325 1393251.0298344865 0, -1164797.3552512976 1393197.1582403914 0, -1164851.7833524747 1392795.2767565313 0, -1164906.213813485 1392393.3768613848 0, -1164960.8570348632 1391991.4870388547 0, -1165015.4839551386 1391589.5966411936 0, -1165411.0337512083 1391641.1819036664 0, -1165806.565017187 1391692.7833502255 0, -1166204.1803047655 1391744.566076178 0, -1166601.8120934765 1391796.3495493892 0, -1166545.4010741839 1392207.2434767624 0, -1166490.2246998842 1392609.1010301283 0, -1166435.0510008365 1393010.940109647 0, -1166379.8580742273 1393412.7984702166 0)), ((-1168346.2402175646 1416938.950836989 0, -1168291.8866725499 1417344.4231284817 0, -1168237.535633526 1417749.876955446 0, -1168183.181422921 1418155.3521491783 0, -1167782.2249332508 1418106.2680156042 0, -1167381.2637183075 1418057.2224765148 0, -1166980.303220909 1418008.1760811964 0, -1166579.3244220777 1417959.1463298993 0, -1166631.40375167 1417552.5665601827 0, -1166683.4825636602 1417145.987956514 0, -1166735.563563827 1416739.3909451917 0, -1166787.641173089 1416332.8153704344 0, -1167190.8791227962 1416382.9472842843 0, -1167594.1120814949 1416433.1182798971 0, -1167997.3457350433 1416483.2884237745 0, -1168400.577237942 1416533.4776820375 0, -1168346.2402175646 1416938.950836989 0)), ((-1169364.0171739731 1421592.1376663186 0, -1169309.5614646836 1421994.908155483 0, -1169255.1082735094 1422397.6599490184 0, -1169200.6547376886 1422800.4132128763 0, -1169146.2009559378 1423203.1679550996 0, -1168735.3866428486 1423150.8022123748 0, -1168324.551193241 1423098.4740808965 0, -1167913.7323020592 1423046.1480197525 0, -1167502.908178204 1422993.8618082106 0, -1167558.5688820183 1422589.8698776641 0, -1167614.2268096716 1422185.8993378947 0, -1167669.8844984479 1421781.9302947018 0, -1167725.5419775494 1421377.9624487595 0, -1168135.1590305243 1421431.4862235263 0, -1168544.792575077 1421485.0117535614 0, -1168954.404688972 1421538.5748606836 0, -1169364.0171739731 1421592.1376663186 0)), ((-1164634.1081047873 1420190.6300656113 0, -1164576.9766307764 1420593.5399584575 0, -1164519.8452037955 1420996.4513851749 0, -1164129.5886527759 1420948.558849198 0, -1163739.33284891 1420900.664002819 0, -1163349.072364934 1420852.8072118475 0, -1162958.8127199542 1420804.9482208462 0, -1163010.6734844977 1420403.775606886 0, -1163062.5175730835 1420002.6020558227 0, -1163111.2830547593 1419602.2085557617 0, -1163160.0611932212 1419201.8385708327 0, -1163558.1923093174 1419247.0732339686 0, -1163956.3350437784 1419292.3488860107 0, -1164354.4761687422 1419337.6430014072 0, -1164752.6182990842 1419382.9358940723 0, -1164693.3537539684 1419786.791009418 0, -1164634.1081047873 1420190.6300656113 0)), ((-1162554.3179741418 1420760.8343401507 0, -1162958.8127199542 1420804.9482208462 0, -1162907.1421569402 1421206.1687318848 0, -1162855.45500648 1421607.3884115983 0, -1162803.7673767486 1422008.6094145814 0, -1162752.0954645814 1422409.8340048988 0, -1162357.0406865175 1422364.2244797307 0, -1161961.9869693308 1422318.6134074237 0, -1161566.9315708561 1422273.0207662575 0, -1161171.8717686632 1422227.4663342931 0, -1161214.1050098995 1421827.7387250643 0, -1161256.3504611242 1421428.034624433 0, -1161298.5812155544 1421028.3095464534 0, -1161340.8077851892 1420628.6056951552 0, -1161745.3234605545 1420672.66414543 0, -1162149.8214223213 1420716.7396355853 0, -1162554.3179741418 1420760.8343401507 0)), ((-1160555.835367265 1342362.4724318008 0, -1160639.0989210666 1342372.8008393203 0, -1160639.1025707817 1342372.8012920392 0, -1161067.547138715 1342425.9465278913 0, -1161084.0594122906 1342427.9948507575 0, -1161084.0625698133 1342427.995312719 0, -1161086.8509861662 1342428.4032720837 0, -1161481.30990815 1342486.1245715774 0, -1161471.8016836355 1342557.7932392866 0, -1161426.9593904626 1342895.7342120272 0, -1161426.9583758549 1342895.741858687 0, -1161382.1573930888 1343233.3875231277 0, -1161372.6084341146 1343305.3411579954 0, -1161345.5917563364 1343502.4844921895 0, -1161317.9007638758 1343704.535456809 0, -1161174.6171993 1343681.4754627682 0, -1160918.0771163949 1343640.1857298138 0, -1160918.0768122156 1343640.1879653856 0, -1160918.07595339 1343640.1878271666 0, -1160863.1124110003 1344044.1219970598 0, -1160419.319074915 1343987.2959846682 0, -1160200.1974385392 1343959.2410356097 0, -1160021.8329877972 1343936.4005959847 0, -1160021.8323116223 1343936.4005094012 0, -1159742.2525162355 1343900.6005991232 0, -1159622.9155582127 1343885.3180074997 0, -1159677.0775108382 1343481.2768438656 0, -1159677.0776918822 1343481.2754933028 0, -1159708.191035808 1343249.174230714 0, -1159731.2444110706 1343077.2353770316 0, -1159751.1380842498 1342911.234984098 0, -1159779.4919498912 1342674.6956624135 0, -1159779.4923405426 1342674.6924034243 0, -1159827.7437912773 1342272.1571615706 0, -1159970.3261369911 1342289.8435207168 0, -1160239.2273022288 1342323.2090227657 0, -1160555.835367265 1342362.4724318008 0)), ((-1157166.6133341766 1418425.5600141888 0, -1157168.564336575 1418425.8454011441 0, -1157164.0956349513 1418429.9739014811 0, -1156969.451975769 1418609.2781745216 0, -1156914.1249898104 1418692.372831359 0, -1156868.3254176043 1418797.4147460205 0, -1156722.0185353474 1418776.390662088 0, -1156767.2325033643 1418367.0227464072 0, -1156990.915978495 1418399.808372859 0, -1157164.6204906022 1418425.2685328429 0, -1157166.6133341766 1418425.5600141888 0)), ((-1159678.263049038 1421200.6842120434 0, -1159633.407860968 1421589.500756771 0, -1159588.551875587 1421978.318575145 0, -1159194.6171948852 1421940.5322140078 0, -1158800.694781235 1421902.7862226758 0, -1158406.7553600164 1421865.0563305682 0, -1158012.8336763529 1421827.3270519462 0, -1158053.6318724658 1421424.379318485 0, -1158094.425684959 1421021.4527952771 0, -1158135.2369948642 1420618.5098106978 0, -1158176.0279103909 1420215.5858927795 0, -1158574.0130461846 1420267.42473959 0, -1158971.9958590274 1420319.282030556 0, -1159369.9924167069 1420371.1603221798 0, -1159767.9705395217 1420423.0549011857 0, -1159723.1172424308 1420811.8689232648 0, -1159678.263049038 1421200.6842120434 0)))</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Zuni</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>AZ</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>PERM CMN SCHLS (INDMTY SELEC), Saline Lands, University of New Mexico, Common Schools, New Mexico School for the Visually Handicapped</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Subsurface, Surface</t>
-        </is>
-      </c>
-      <c r="F81" t="n">
-        <v>189</v>
-      </c>
-      <c r="G81" t="n">
-        <v>62.57</v>
-      </c>
-      <c r="H81" t="n">
-        <v>2</v>
-      </c>
-      <c r="I81" t="n">
-        <v>8070.27</v>
-      </c>
-      <c r="J81" t="n">
-        <v>187</v>
-      </c>
-      <c r="K81" t="n">
-        <v>8132.84</v>
-      </c>
-      <c r="L81" t="n">
         <v>462553.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Integrate Nebraska subsurface parcels.
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -546,7 +546,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>POLYGON Z ((-1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0))</t>
+          <t>POLYGON Z ((-1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0))</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -561,12 +561,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dept. of Transportation, None Listed</t>
+          <t>None Listed, Dept. of Transportation</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>subsurface, Subsurface</t>
+          <t>Subsurface, subsurface</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -758,7 +758,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -801,7 +801,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Common Schools, Normal Schools, University Preparatory, Connors State College, Oklahoma State University, Langston University, State Educational Institutions</t>
+          <t>Common Schools, Oklahoma State University, Normal Schools, Connors State College, University Preparatory, Langston University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dept. of Parks and Recreation, 100.00% Dept. of Parks and Recreation, Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), 100.00% Normal School, 100.00% University of Idaho, State Hospital South (Insane Asylum), Normal School, Agricultural College, 100.00% Dept. of Fish and Game, 100.00% General Fund, General Fund</t>
+          <t>Dept. of Parks and Recreation, 100.00% Dept. of Parks and Recreation, Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), 100.00% Normal School, 100.00% University of Idaho, State Hospital South (Insane Asylum), Normal School, Agricultural College, 100.00% Dept. of Fish and Game, General Fund, 100.00% General Fund</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1905,12 +1905,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Common Schools, Oklahoma State University, Other Agency</t>
+          <t>Oklahoma State University, Common Schools, Other Agency</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>subsurface, surface</t>
+          <t>surface, subsurface</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2390,7 +2390,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2721,12 +2721,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Oklahoma State University, Common Schools, Public Building, State Educational Institutions, Other Agency</t>
+          <t>Common Schools, Oklahoma State University, Public Building, State Educational Institutions, Other Agency</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>surface, subsurface</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -3330,7 +3330,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-150654.51162035248 2180758.678847399 0, -150727.67552972207 2180759.685291849 0, -151058.23785022597 2180767.194620998 0, -151050.6643970744 2181169.403240565 0, -150647.36731614405 2181162.756169655 0, -150654.51162035248 2180758.678847399 0)), ((-144985.75394429002 2186761.1955177807 0, -144993.57760826222 2186358.8521826295 0, -145001.40205040292 2185956.507569622 0, -145399.94308498083 2185961.978390855 0, -145391.28270177462 2186365.0471574035 0, -145382.62273704054 2186768.1136125233 0, -144985.75394429002 2186761.1955177807 0)), ((-155804.6157940152 2185751.5754990443 0, -156213.95280016185 2185771.815552367 0, -156194.81600412223 2186180.9574394897 0, -156176.03287459628 2186582.5349008576 0, -156157.59366610707 2186976.756056978 0, -156139.48908621314 2187363.8209823803 0, -155744.84600765648 2187348.445937388 0, -155348.1509325643 2187332.9886809853 0, -154949.3876756076 2187317.4484555325 0, -154548.54004262667 2187301.8247038866 0, -154552.12219585586 2186910.1019930975 0, -154555.77139012987 2186511.059859929 0, -154559.48947036255 2186104.491345304 0, -154563.2783467011 2185690.181225061 0, -154979.2966338558 2185710.759282247 0, -155393.06976225073 2185731.2236910015 0, -155804.6157940152 2185751.5754990443 0)), ((-146166.02163888028 2187186.444051743 0, -146176.35634732372 2186781.936397038 0, -146186.68968903017 2186377.4237080743 0, -146584.39309958878 2186383.6114961575 0, -146573.22349830132 2186788.8468318544 0, -146562.05367514814 2187194.0780807077 0, -146166.02163888028 2187186.444051743 0)), ((-150394.06204562637 2191642.5065784375 0, -150383.6975485528 2192048.570456311 0, -149985.44773027493 2192037.957515076 0, -149604.66534376488 2192027.8079793444 0, -149617.6731232064 2191624.1751634963 0, -149623.36915654116 2191447.4289275855 0, -149642.32078511678 2191298.056048375 0, -149657.298111479 2191222.1884050462 0, -149692.36435896214 2191044.5601496864 0, -149675.98934608878 2191015.215095343 0, -149620.52489968407 2190931.2250189628 0, -149623.67058447894 2190819.8473241213 0, -149635.45273980167 2190820.0542867915 0, -149646.50565726828 2190435.131514635 0, -150028.3764674055 2190441.381687129 0, -150424.5544889028 2190447.8637507427 0, -150414.70544404458 2190833.735152485 0, -150404.3979716605 2191237.5631112135 0, -150394.06204562637 2191642.5065784375 0)), ((-154357.67009668285 2195394.6561956443 0, -154756.49514332798 2195401.4538690597 0, -155153.7515568258 2195408.221370756 0, -155553.12051018604 2195415.229121782 0, -155950.92415796503 2195422.2057534335 0, -155947.17202052783 2195827.355199152 0, -155943.4074702889 2196233.814884058 0, -155941.47868866843 2196637.651863205 0, -155939.54341035578 2197042.7984314207 0, -155541.2189184494 2197040.569327221 0, -155353.65413790673 2197039.518888024 0, -155396.12102644477 2196817.527901084 0, -155160.51979592125 2196817.2483607503 0, -155161.41836884365 2197038.4414134705 0, -155141.31684328214 2197038.3286947077 0, -154739.82762817875 2197036.076583675 0, -154336.74182022538 2197033.8129475242 0, -154341.998905905 2196622.0189541783 0, -154347.23910693155 2196211.5658134827 0, -154352.46280488887 2195802.447130641 0, -154357.67009668285 2195394.6561956443 0)), ((-151058.50384008256 2201573.53086171 0, -150662.53300438932 2201565.8143678103 0, -150265.73542722332 2201558.079416251 0, -150266.11107496227 2201956.7167395214 0, -149870.38817961563 2201949.4151801527 0, -149473.8411775989 2201942.0961809494 0, -149469.64870493274 2201542.554079617 0, -149465.41586004765 2201139.138079935 0, -149461.14186428962 2200731.7913708803 0, -149456.82626367526 2200320.456549403 0, -149861.1348939628 2200329.6388499835 0, -150264.58700048906 2200338.799250088 0, -150667.18486721066 2200347.937866776 0, -151068.93166755023 2200357.0549574546 0, -151065.42192813862 2200766.4810241363 0, -151061.94612094056 2201171.95410604 0, -151058.50384008256 2201573.53086171 0)))</t>
+          <t>MULTIPOLYGON Z (((-150727.67552972207 2180759.685291849 0, -151058.23785022597 2180767.194620998 0, -151050.6643970744 2181169.403240565 0, -150647.36731614405 2181162.756169655 0, -150654.51162035248 2180758.678847399 0, -150727.67552972207 2180759.685291849 0)), ((-156213.95280016185 2185771.815552367 0, -156194.81600412223 2186180.9574394897 0, -156176.03287459628 2186582.5349008576 0, -156157.59366610707 2186976.756056978 0, -156139.48908621314 2187363.8209823803 0, -155744.84600765648 2187348.445937388 0, -155348.1509325643 2187332.9886809853 0, -154949.3876756076 2187317.4484555325 0, -154548.54004262667 2187301.8247038866 0, -154552.12219585586 2186910.1019930975 0, -154555.77139012987 2186511.059859929 0, -154559.48947036255 2186104.491345304 0, -154563.2783467011 2185690.181225061 0, -154979.2966338558 2185710.759282247 0, -155393.06976225073 2185731.2236910015 0, -155804.6157940152 2185751.5754990443 0, -156213.95280016185 2185771.815552367 0)), ((-154756.49514332798 2195401.4538690597 0, -155153.7515568258 2195408.221370756 0, -155553.12051018604 2195415.229121782 0, -155950.92415796503 2195422.2057534335 0, -155947.17202052783 2195827.355199152 0, -155943.4074702889 2196233.814884058 0, -155941.47868866843 2196637.651863205 0, -155939.54341035578 2197042.7984314207 0, -155541.2189184494 2197040.569327221 0, -155353.65413790673 2197039.518888024 0, -155396.12102644477 2196817.527901084 0, -155160.51979592125 2196817.2483607503 0, -155161.41836884365 2197038.4414134705 0, -155141.31684328214 2197038.3286947077 0, -154739.82762817875 2197036.076583675 0, -154336.74182022538 2197033.8129475242 0, -154341.998905905 2196622.0189541783 0, -154347.23910693155 2196211.5658134827 0, -154352.46280488887 2195802.447130641 0, -154357.67009668285 2195394.6561956443 0, -154756.49514332798 2195401.4538690597 0)), ((-150662.53300438932 2201565.8143678103 0, -150265.73542722332 2201558.079416251 0, -150266.11107496227 2201956.7167395214 0, -149870.38817961563 2201949.4151801527 0, -149473.8411775989 2201942.0961809494 0, -149469.64870493274 2201542.554079617 0, -149465.41586004765 2201139.138079935 0, -149461.14186428962 2200731.7913708803 0, -149456.82626367526 2200320.456549403 0, -149861.1348939628 2200329.6388499835 0, -150264.58700048906 2200338.799250088 0, -150667.18486721066 2200347.937866776 0, -151068.93166755023 2200357.0549574546 0, -151065.42192813862 2200766.4810241363 0, -151061.94612094056 2201171.95410604 0, -151058.50384008256 2201573.53086171 0, -150662.53300438932 2201565.8143678103 0)), ((-144985.75394429002 2186761.1955177807 0, -144993.57760826222 2186358.8521826295 0, -145001.40205040292 2185956.507569622 0, -145399.94308498083 2185961.978390855 0, -145391.28270177462 2186365.0471574035 0, -145382.62273704054 2186768.1136125233 0, -144985.75394429002 2186761.1955177807 0)), ((-146176.35634732372 2186781.936397038 0, -146186.68968903017 2186377.4237080743 0, -146584.39309958878 2186383.6114961575 0, -146573.22349830132 2186788.8468318544 0, -146562.05367514814 2187194.0780807077 0, -146166.02163888028 2187186.444051743 0, -146176.35634732372 2186781.936397038 0)), ((-150383.6975485528 2192048.570456311 0, -149985.44773027493 2192037.957515076 0, -149604.66534376488 2192027.8079793444 0, -149617.6731232064 2191624.1751634963 0, -149623.36915654116 2191447.4289275855 0, -149642.32078511678 2191298.056048375 0, -149657.298111479 2191222.1884050462 0, -149692.36435896214 2191044.5601496864 0, -149675.98934608878 2191015.215095343 0, -149620.52489968407 2190931.2250189628 0, -149623.67058447894 2190819.8473241213 0, -149635.45273980167 2190820.0542867915 0, -149646.50565726828 2190435.131514635 0, -150028.3764674055 2190441.381687129 0, -150424.5544889028 2190447.8637507427 0, -150414.70544404458 2190833.735152485 0, -150404.3979716605 2191237.5631112135 0, -150394.06204562637 2191642.5065784375 0, -150383.6975485528 2192048.570456311 0)))</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3350,11 +3350,11 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G61" t="n">
         <v>2337.21</v>
@@ -3363,13 +3363,13 @@
         <v>6</v>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>2337.21</v>
       </c>
       <c r="J61" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K61" t="n">
-        <v>2337.21</v>
+        <v>4674.42</v>
       </c>
       <c r="L61" t="n">
         <v>117388.4</v>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -4118,7 +4118,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F77" t="n">

</xml_diff>

<commit_message>
feat: Integrate Nebraska subsurface parcels. (#20)
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -546,7 +546,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>POLYGON Z ((-1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0))</t>
+          <t>POLYGON Z ((-1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0))</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -561,12 +561,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dept. of Transportation, None Listed</t>
+          <t>None Listed, Dept. of Transportation</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>subsurface, Subsurface</t>
+          <t>Subsurface, subsurface</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -758,7 +758,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -801,7 +801,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Common Schools, Normal Schools, University Preparatory, Connors State College, Oklahoma State University, Langston University, State Educational Institutions</t>
+          <t>Common Schools, Oklahoma State University, Normal Schools, Connors State College, University Preparatory, Langston University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dept. of Parks and Recreation, 100.00% Dept. of Parks and Recreation, Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), 100.00% Normal School, 100.00% University of Idaho, State Hospital South (Insane Asylum), Normal School, Agricultural College, 100.00% Dept. of Fish and Game, 100.00% General Fund, General Fund</t>
+          <t>Dept. of Parks and Recreation, 100.00% Dept. of Parks and Recreation, Public School (Indemnity, Schools, Common Schools), 100.00% Public School (Indemnity, Schools, Common Schools), 100.00% Normal School, 100.00% University of Idaho, State Hospital South (Insane Asylum), Normal School, Agricultural College, 100.00% Dept. of Fish and Game, General Fund, 100.00% General Fund</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1905,12 +1905,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Common Schools, Oklahoma State University, Other Agency</t>
+          <t>Oklahoma State University, Common Schools, Other Agency</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>subsurface, surface</t>
+          <t>surface, subsurface</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2390,7 +2390,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2721,12 +2721,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Oklahoma State University, Common Schools, Public Building, State Educational Institutions, Other Agency</t>
+          <t>Common Schools, Oklahoma State University, Public Building, State Educational Institutions, Other Agency</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>surface, subsurface</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -3330,7 +3330,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-150654.51162035248 2180758.678847399 0, -150727.67552972207 2180759.685291849 0, -151058.23785022597 2180767.194620998 0, -151050.6643970744 2181169.403240565 0, -150647.36731614405 2181162.756169655 0, -150654.51162035248 2180758.678847399 0)), ((-144985.75394429002 2186761.1955177807 0, -144993.57760826222 2186358.8521826295 0, -145001.40205040292 2185956.507569622 0, -145399.94308498083 2185961.978390855 0, -145391.28270177462 2186365.0471574035 0, -145382.62273704054 2186768.1136125233 0, -144985.75394429002 2186761.1955177807 0)), ((-155804.6157940152 2185751.5754990443 0, -156213.95280016185 2185771.815552367 0, -156194.81600412223 2186180.9574394897 0, -156176.03287459628 2186582.5349008576 0, -156157.59366610707 2186976.756056978 0, -156139.48908621314 2187363.8209823803 0, -155744.84600765648 2187348.445937388 0, -155348.1509325643 2187332.9886809853 0, -154949.3876756076 2187317.4484555325 0, -154548.54004262667 2187301.8247038866 0, -154552.12219585586 2186910.1019930975 0, -154555.77139012987 2186511.059859929 0, -154559.48947036255 2186104.491345304 0, -154563.2783467011 2185690.181225061 0, -154979.2966338558 2185710.759282247 0, -155393.06976225073 2185731.2236910015 0, -155804.6157940152 2185751.5754990443 0)), ((-146166.02163888028 2187186.444051743 0, -146176.35634732372 2186781.936397038 0, -146186.68968903017 2186377.4237080743 0, -146584.39309958878 2186383.6114961575 0, -146573.22349830132 2186788.8468318544 0, -146562.05367514814 2187194.0780807077 0, -146166.02163888028 2187186.444051743 0)), ((-150394.06204562637 2191642.5065784375 0, -150383.6975485528 2192048.570456311 0, -149985.44773027493 2192037.957515076 0, -149604.66534376488 2192027.8079793444 0, -149617.6731232064 2191624.1751634963 0, -149623.36915654116 2191447.4289275855 0, -149642.32078511678 2191298.056048375 0, -149657.298111479 2191222.1884050462 0, -149692.36435896214 2191044.5601496864 0, -149675.98934608878 2191015.215095343 0, -149620.52489968407 2190931.2250189628 0, -149623.67058447894 2190819.8473241213 0, -149635.45273980167 2190820.0542867915 0, -149646.50565726828 2190435.131514635 0, -150028.3764674055 2190441.381687129 0, -150424.5544889028 2190447.8637507427 0, -150414.70544404458 2190833.735152485 0, -150404.3979716605 2191237.5631112135 0, -150394.06204562637 2191642.5065784375 0)), ((-154357.67009668285 2195394.6561956443 0, -154756.49514332798 2195401.4538690597 0, -155153.7515568258 2195408.221370756 0, -155553.12051018604 2195415.229121782 0, -155950.92415796503 2195422.2057534335 0, -155947.17202052783 2195827.355199152 0, -155943.4074702889 2196233.814884058 0, -155941.47868866843 2196637.651863205 0, -155939.54341035578 2197042.7984314207 0, -155541.2189184494 2197040.569327221 0, -155353.65413790673 2197039.518888024 0, -155396.12102644477 2196817.527901084 0, -155160.51979592125 2196817.2483607503 0, -155161.41836884365 2197038.4414134705 0, -155141.31684328214 2197038.3286947077 0, -154739.82762817875 2197036.076583675 0, -154336.74182022538 2197033.8129475242 0, -154341.998905905 2196622.0189541783 0, -154347.23910693155 2196211.5658134827 0, -154352.46280488887 2195802.447130641 0, -154357.67009668285 2195394.6561956443 0)), ((-151058.50384008256 2201573.53086171 0, -150662.53300438932 2201565.8143678103 0, -150265.73542722332 2201558.079416251 0, -150266.11107496227 2201956.7167395214 0, -149870.38817961563 2201949.4151801527 0, -149473.8411775989 2201942.0961809494 0, -149469.64870493274 2201542.554079617 0, -149465.41586004765 2201139.138079935 0, -149461.14186428962 2200731.7913708803 0, -149456.82626367526 2200320.456549403 0, -149861.1348939628 2200329.6388499835 0, -150264.58700048906 2200338.799250088 0, -150667.18486721066 2200347.937866776 0, -151068.93166755023 2200357.0549574546 0, -151065.42192813862 2200766.4810241363 0, -151061.94612094056 2201171.95410604 0, -151058.50384008256 2201573.53086171 0)))</t>
+          <t>MULTIPOLYGON Z (((-150727.67552972207 2180759.685291849 0, -151058.23785022597 2180767.194620998 0, -151050.6643970744 2181169.403240565 0, -150647.36731614405 2181162.756169655 0, -150654.51162035248 2180758.678847399 0, -150727.67552972207 2180759.685291849 0)), ((-156213.95280016185 2185771.815552367 0, -156194.81600412223 2186180.9574394897 0, -156176.03287459628 2186582.5349008576 0, -156157.59366610707 2186976.756056978 0, -156139.48908621314 2187363.8209823803 0, -155744.84600765648 2187348.445937388 0, -155348.1509325643 2187332.9886809853 0, -154949.3876756076 2187317.4484555325 0, -154548.54004262667 2187301.8247038866 0, -154552.12219585586 2186910.1019930975 0, -154555.77139012987 2186511.059859929 0, -154559.48947036255 2186104.491345304 0, -154563.2783467011 2185690.181225061 0, -154979.2966338558 2185710.759282247 0, -155393.06976225073 2185731.2236910015 0, -155804.6157940152 2185751.5754990443 0, -156213.95280016185 2185771.815552367 0)), ((-154756.49514332798 2195401.4538690597 0, -155153.7515568258 2195408.221370756 0, -155553.12051018604 2195415.229121782 0, -155950.92415796503 2195422.2057534335 0, -155947.17202052783 2195827.355199152 0, -155943.4074702889 2196233.814884058 0, -155941.47868866843 2196637.651863205 0, -155939.54341035578 2197042.7984314207 0, -155541.2189184494 2197040.569327221 0, -155353.65413790673 2197039.518888024 0, -155396.12102644477 2196817.527901084 0, -155160.51979592125 2196817.2483607503 0, -155161.41836884365 2197038.4414134705 0, -155141.31684328214 2197038.3286947077 0, -154739.82762817875 2197036.076583675 0, -154336.74182022538 2197033.8129475242 0, -154341.998905905 2196622.0189541783 0, -154347.23910693155 2196211.5658134827 0, -154352.46280488887 2195802.447130641 0, -154357.67009668285 2195394.6561956443 0, -154756.49514332798 2195401.4538690597 0)), ((-150662.53300438932 2201565.8143678103 0, -150265.73542722332 2201558.079416251 0, -150266.11107496227 2201956.7167395214 0, -149870.38817961563 2201949.4151801527 0, -149473.8411775989 2201942.0961809494 0, -149469.64870493274 2201542.554079617 0, -149465.41586004765 2201139.138079935 0, -149461.14186428962 2200731.7913708803 0, -149456.82626367526 2200320.456549403 0, -149861.1348939628 2200329.6388499835 0, -150264.58700048906 2200338.799250088 0, -150667.18486721066 2200347.937866776 0, -151068.93166755023 2200357.0549574546 0, -151065.42192813862 2200766.4810241363 0, -151061.94612094056 2201171.95410604 0, -151058.50384008256 2201573.53086171 0, -150662.53300438932 2201565.8143678103 0)), ((-144985.75394429002 2186761.1955177807 0, -144993.57760826222 2186358.8521826295 0, -145001.40205040292 2185956.507569622 0, -145399.94308498083 2185961.978390855 0, -145391.28270177462 2186365.0471574035 0, -145382.62273704054 2186768.1136125233 0, -144985.75394429002 2186761.1955177807 0)), ((-146176.35634732372 2186781.936397038 0, -146186.68968903017 2186377.4237080743 0, -146584.39309958878 2186383.6114961575 0, -146573.22349830132 2186788.8468318544 0, -146562.05367514814 2187194.0780807077 0, -146166.02163888028 2187186.444051743 0, -146176.35634732372 2186781.936397038 0)), ((-150383.6975485528 2192048.570456311 0, -149985.44773027493 2192037.957515076 0, -149604.66534376488 2192027.8079793444 0, -149617.6731232064 2191624.1751634963 0, -149623.36915654116 2191447.4289275855 0, -149642.32078511678 2191298.056048375 0, -149657.298111479 2191222.1884050462 0, -149692.36435896214 2191044.5601496864 0, -149675.98934608878 2191015.215095343 0, -149620.52489968407 2190931.2250189628 0, -149623.67058447894 2190819.8473241213 0, -149635.45273980167 2190820.0542867915 0, -149646.50565726828 2190435.131514635 0, -150028.3764674055 2190441.381687129 0, -150424.5544889028 2190447.8637507427 0, -150414.70544404458 2190833.735152485 0, -150404.3979716605 2191237.5631112135 0, -150394.06204562637 2191642.5065784375 0, -150383.6975485528 2192048.570456311 0)))</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3350,11 +3350,11 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G61" t="n">
         <v>2337.21</v>
@@ -3363,13 +3363,13 @@
         <v>6</v>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>2337.21</v>
       </c>
       <c r="J61" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K61" t="n">
-        <v>2337.21</v>
+        <v>4674.42</v>
       </c>
       <c r="L61" t="n">
         <v>117388.4</v>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -4118,7 +4118,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F77" t="n">

</xml_diff>

<commit_message>
feat: Update trust names in ND, MN, and AZ.
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -609,7 +609,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TRUST FUND: SCHOOL</t>
+          <t>Trust Fund: School</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>TRUST FUND: SCHOOL</t>
+          <t>Trust Fund: School</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>SOVEREIGNÔøΩLANDS, COMMON SCHOOLS, BANK OFÔøΩNORTHÔøΩDAKOTA, NDÔøΩSTATEÔøΩUNIVERSITY, ND INDUSTRIAL SCHOOL, SCHOOL OF MINES, ELLENDALE, SCHOOL FOR THE BLIND, ND SCHOOL OF SCIENCE, UNIVERSITY OF ND, NDÔøΩSTATEÔøΩTREASURER, MAYVILLE, VALLEY CITY</t>
+          <t>Sovereign Lands, Common Schools, Strategic Investment and Improvement Fund, ND State University, ND Industrial School, School of Mines, Ellendale, School for the Blind, ND School of Science, University of ND, ND State Treasurer, Mayville, Valley City</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PENITENTIARY LAND FUND, School Lands</t>
+          <t>Penitentiary Land Fund, School Lands</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>TRUST FUND: UNIVERSITY, TRUST FUND: SWAMP, TRUST FUND: SCHOOL</t>
+          <t>Trust Fund: University, Trust Fund: Swamp, Trust Fund: School</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>PERM CMN SCHLS (INDMTY SELEC), PERM COMMON SCHLS</t>
+          <t>Perm Cmn Schls (Indmty Selec), Perm Common Schls</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>PERM COMMON SCHLS, AGRICULTURE &amp; MECHANICAL CLLGE</t>
+          <t>Perm Common Schls, Agriculture &amp; Mechanical Cllge</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
+          <t>Trust Fund: Swamp, Trust Fund: School, Trust Fund: Ind School</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
+          <t>Trust Fund: School, Trust Fund: Ind School</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>PERM COMMON SCHLS, PERM CMN SCHLS (INDMTY SELEC), COUNTY BOND, New Mexico Institute of Mining and Technology, Common Schools, Public Schools</t>
+          <t>Perm Common Schls, Perm Cmn Schls (Indmty Selec), County Bond, New Mexico Institute of Mining and Technology, Common Schools, Public Schools</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>TRUST FUND: SCHOOL</t>
+          <t>Trust Fund: School</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>TRUST FUND: IND SCHOOL, TRUST FUND: SWAMP</t>
+          <t>Trust Fund: Ind School, Trust Fund: Swamp</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>PERM CMN SCHLS (INDMTY SELEC), 02-90-0021 FED PATENT</t>
+          <t>Perm Cmn Schls (Indmty Selec), 02-90-0021 Fed Patent</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>PERM COMMON SCHLS</t>
+          <t>Perm Common Schls</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>COMMON SCHOOLS, BANK OFÔøΩNORTHÔøΩDAKOTA, STATE HOSPITAL, VALLEY/MAYVILLE, SCHOOL FOR THE DEAF, ND STATE UNIVERSITY, ND SCHOOL OF SCIENCE, VALLEY CITY, VETERANS HOME, ELLENDALE, MAYVILLE, ND INDUSTRIAL SCHOOL</t>
+          <t>Common Schools, Strategic Investment and Improvement Fund, State Hospital, Valley/Mayville, School for the Deaf, ND State University, ND School of Science, Valley City, Veterans Home, Ellendale, Mayville, ND Industrial School</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Rural Credit, Indemnity, School and Public Lands, BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, ND SCHOOL OF SCIENCE, CAPITOL BUILDING, VETERANS HOME, MAYVILLE, SCHOOL OF MINES, UNIVERSITY OF ND, ND INDUSTRIAL SCHOOL, ND STATE UNIVERSITY, NDÔøΩSTATEÔøΩUNIVERSITY, ELLENDALE, SCHOOL FOR THE DEAF, STATEÔøΩHOSPITAL, VALLEY/MAYVILLE</t>
+          <t>Rural Credit, Indemnity, School and Public Lands, Strategic Investment and Improvement Fund, Common Schools, ND School of Science, Capitol Building, Veterans Home, Mayville, School of Mines, University of ND, ND Industrial School, ND State University, Ellendale, School for the Deaf, State Hospital, Valley/Mayville</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>COUNTY BOND, UNIVERSITY, ST CHRTBL, PENAL &amp; REFORM INST, PERM COMMON SCHLS, SCHOOL OF MINES</t>
+          <t>County Bond, University, St Chrtbl, Penal &amp; Reform Inst, Perm Common Schls, School of Mines</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
+          <t>Trust Fund: Swamp, Trust Fund: School, Trust Fund: Ind School</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>PERM CMN SCHLS (INDMTY SELEC), Saline Lands, University of New Mexico, Common Schools, New Mexico School for the Visually Handicapped</t>
+          <t>Perm Cmn Schls (Indmty Selec), Saline Lands, University of New Mexico, Common Schools, New Mexico School for the Visually Handicapped</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">

</xml_diff>

<commit_message>
feat: Update trust names in ND, MN, and AZ. (#21)
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -609,7 +609,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TRUST FUND: SCHOOL</t>
+          <t>Trust Fund: School</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>TRUST FUND: SCHOOL</t>
+          <t>Trust Fund: School</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>SOVEREIGNÔøΩLANDS, COMMON SCHOOLS, BANK OFÔøΩNORTHÔøΩDAKOTA, NDÔøΩSTATEÔøΩUNIVERSITY, ND INDUSTRIAL SCHOOL, SCHOOL OF MINES, ELLENDALE, SCHOOL FOR THE BLIND, ND SCHOOL OF SCIENCE, UNIVERSITY OF ND, NDÔøΩSTATEÔøΩTREASURER, MAYVILLE, VALLEY CITY</t>
+          <t>Sovereign Lands, Common Schools, Strategic Investment and Improvement Fund, ND State University, ND Industrial School, School of Mines, Ellendale, School for the Blind, ND School of Science, University of ND, ND State Treasurer, Mayville, Valley City</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PENITENTIARY LAND FUND, School Lands</t>
+          <t>Penitentiary Land Fund, School Lands</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>TRUST FUND: UNIVERSITY, TRUST FUND: SWAMP, TRUST FUND: SCHOOL</t>
+          <t>Trust Fund: University, Trust Fund: Swamp, Trust Fund: School</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>PERM CMN SCHLS (INDMTY SELEC), PERM COMMON SCHLS</t>
+          <t>Perm Cmn Schls (Indmty Selec), Perm Common Schls</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>PERM COMMON SCHLS, AGRICULTURE &amp; MECHANICAL CLLGE</t>
+          <t>Perm Common Schls, Agriculture &amp; Mechanical Cllge</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
+          <t>Trust Fund: Swamp, Trust Fund: School, Trust Fund: Ind School</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
+          <t>Trust Fund: School, Trust Fund: Ind School</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>PERM COMMON SCHLS, PERM CMN SCHLS (INDMTY SELEC), COUNTY BOND, New Mexico Institute of Mining and Technology, Common Schools, Public Schools</t>
+          <t>Perm Common Schls, Perm Cmn Schls (Indmty Selec), County Bond, New Mexico Institute of Mining and Technology, Common Schools, Public Schools</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>TRUST FUND: SCHOOL</t>
+          <t>Trust Fund: School</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>TRUST FUND: IND SCHOOL, TRUST FUND: SWAMP</t>
+          <t>Trust Fund: Ind School, Trust Fund: Swamp</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>PERM CMN SCHLS (INDMTY SELEC), 02-90-0021 FED PATENT</t>
+          <t>Perm Cmn Schls (Indmty Selec), 02-90-0021 Fed Patent</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>PERM COMMON SCHLS</t>
+          <t>Perm Common Schls</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>COMMON SCHOOLS, BANK OFÔøΩNORTHÔøΩDAKOTA, STATE HOSPITAL, VALLEY/MAYVILLE, SCHOOL FOR THE DEAF, ND STATE UNIVERSITY, ND SCHOOL OF SCIENCE, VALLEY CITY, VETERANS HOME, ELLENDALE, MAYVILLE, ND INDUSTRIAL SCHOOL</t>
+          <t>Common Schools, Strategic Investment and Improvement Fund, State Hospital, Valley/Mayville, School for the Deaf, ND State University, ND School of Science, Valley City, Veterans Home, Ellendale, Mayville, ND Industrial School</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Rural Credit, Indemnity, School and Public Lands, BANK OFÔøΩNORTHÔøΩDAKOTA, COMMON SCHOOLS, ND SCHOOL OF SCIENCE, CAPITOL BUILDING, VETERANS HOME, MAYVILLE, SCHOOL OF MINES, UNIVERSITY OF ND, ND INDUSTRIAL SCHOOL, ND STATE UNIVERSITY, NDÔøΩSTATEÔøΩUNIVERSITY, ELLENDALE, SCHOOL FOR THE DEAF, STATEÔøΩHOSPITAL, VALLEY/MAYVILLE</t>
+          <t>Rural Credit, Indemnity, School and Public Lands, Strategic Investment and Improvement Fund, Common Schools, ND School of Science, Capitol Building, Veterans Home, Mayville, School of Mines, University of ND, ND Industrial School, ND State University, Ellendale, School for the Deaf, State Hospital, Valley/Mayville</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>COUNTY BOND, UNIVERSITY, ST CHRTBL, PENAL &amp; REFORM INST, PERM COMMON SCHLS, SCHOOL OF MINES</t>
+          <t>County Bond, University, St Chrtbl, Penal &amp; Reform Inst, Perm Common Schls, School of Mines</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>TRUST FUND: SWAMP, TRUST FUND: SCHOOL, TRUST FUND: IND SCHOOL</t>
+          <t>Trust Fund: Swamp, Trust Fund: School, Trust Fund: Ind School</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>PERM CMN SCHLS (INDMTY SELEC), Saline Lands, University of New Mexico, Common Schools, New Mexico School for the Visually Handicapped</t>
+          <t>Perm Cmn Schls (Indmty Selec), Saline Lands, University of New Mexico, Common Schools, New Mexico School for the Visually Handicapped</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">

</xml_diff>

<commit_message>
fix: Remove OK parcels with "Aeronautics Commission", "Other Agency", "University Hospitals Authority & Trust", or "Wildlife Conservation" trust_name.
</commit_message>
<xml_diff>
--- a/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
+++ b/public_data/05_Final-Dataset/01_STLs-on-Reservations-by-Reservation.xlsx
@@ -546,7 +546,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>POLYGON Z ((-1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0))</t>
+          <t>POLYGON Z ((-1268746.656403215 2958669.4221782363 0, -1269148.7719312687 2958739.0154197128 0, -1269547.4615757428 2958814.6065749167 0, -1269546.6619563145 2958817.763578659 0, -1269474.6916636892 2959210.0765392943 0, -1269075.0058828911 2959137.6925412486 0, -1268673.8272412254 2959065.033669607 0, -1268745.8565798467 2958672.5777471345 0, -1268746.656403215 2958669.4221782363 0))</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -561,12 +561,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dept. of Transportation, None Listed</t>
+          <t>None Listed, Dept. of Transportation</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>subsurface, Subsurface</t>
+          <t>Subsurface, subsurface</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -657,7 +657,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, Normal Schools, Public Building, Oklahoma State University, University Preparatory, University of Oklahoma</t>
+          <t>Common Schools, State Educational Institutions, Public Building, Oklahoma State University, University Preparatory, Normal Schools, University of Oklahoma</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Common Schools, Oklahoma State University, Normal Schools, Connors State College, University Preparatory, State Educational Institutions, Langston University</t>
+          <t>Normal Schools, Oklahoma State University, Connors State College, Common Schools, University Preparatory, Langston University, State Educational Institutions</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -849,12 +849,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>School and Public Lands, Rural Credit, Common School, Indemnity</t>
+          <t>Common School, School and Public Lands, Rural Credit, Indemnity</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -882,7 +882,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-357801.5254078213 1344905.6837980137 0, -357819.7813741029 1344500.6385781919 0, -357837.9461128943 1344097.7861179465 0, -358238.3795021891 1344116.1991087764 0, -358221.53217823076 1344516.9562831922 0, -358204.5089800107 1344921.9297024182 0, -357801.5254078213 1344905.6837980137 0)), ((-355817.1438377021 1344822.5767877724 0, -356192.3206674648 1344837.5196446632 0, -356170.9744176764 1345242.7738757702 0, -356150.45549275127 1345632.2392934079 0, -355784.3258817538 1345617.05570784 0, -355385.30022062804 1345600.5256966979 0, -355401.4895024438 1345211.6423526665 0, -355800.39435997873 1345228.0328843403 0, -355817.1438377021 1344822.5767877724 0)), ((-356492.7974237927 1347695.012585433 0, -356510.87549364264 1347264.5720195188 0, -356909.82662284037 1347273.9088334735 0, -356891.55644370994 1347711.5314927895 0, -356492.7974237927 1347695.012585433 0)), ((-357659.26413695083 1347743.1696422533 0, -357640.7186669393 1348147.8222976355 0, -357622.163819644 1348552.4871537504 0, -357255.7905134044 1348537.8295405135 0, -357273.0523890364 1348132.954159144 0, -357290.3147160633 1347728.0689817243 0, -357659.26413695083 1347743.1696422533 0)), ((-356441.3910590585 1348896.6962962754 0, -356458.16752986953 1348505.4293759149 0, -356856.974705646 1348521.6255712162 0, -356840.2718644965 1348911.9885101218 0, -356441.3910590585 1348896.6962962754 0)), ((-352776.81700003677 1350388.8219333305 0, -352760.62431139336 1350790.7813189148 0, -352744.2869625499 1351196.4767546572 0, -352727.9495858058 1351602.173574781 0, -352711.6684112581 1352006.2838402814 0, -352323.3775849207 1351988.6776163653 0, -352340.211365484 1351585.8557566707 0, -352357.1722433722 1351180.1622097993 0, -352374.14339090075 1350774.4368619784 0, -352390.99767125765 1350371.3400573279 0, -352776.81700003677 1350388.8219333305 0)), ((-356293.07562019554 1352561.2261443897 0, -356309.752733045 1352136.219551802 0, -356708.1808269701 1352157.900147144 0, -356691.6088914508 1352578.1624770577 0, -356293.07562019554 1352561.2261443897 0)), ((-357074.13182791 1353001.6173415012 0, -357090.14095807 1352595.1284598762 0, -357486.2359831532 1352612.0003487691 0, -357471.02916397265 1353018.9596132175 0, -357074.13182791 1353001.6173415012 0)), ((-357442.1053178831 1353793.2174804166 0, -357043.31814070564 1353780.4442563402 0, -357058.1140250918 1353408.0961251466 0, -357455.8311478643 1353425.9206436945 0, -357442.1053178831 1353793.2174804166 0)), ((-347847.4595934799 1357553.0443838078 0, -347449.16478902934 1357536.7756948087 0, -347466.29814592085 1357131.2030211596 0, -347483.6032865532 1356721.3939454856 0, -347738.730805186 1356731.7409423897 0, -347881.57620768 1356740.9646807353 0, -347864.4904633793 1357147.5683108286 0, -347847.4595934799 1357553.0443838078 0)), ((-359297.29753420234 1357219.2749062034 0, -359443.0900664448 1357224.9063832841 0, -359696.06486753083 1357235.5196004468 0, -359831.22039591917 1357241.1929491353 0, -359814.238527892 1357642.7742239118 0, -359797.077253654 1358048.415189146 0, -359407.8827726577 1358031.2326209673 0, -358999.90043192107 1358014.143237385 0, -359016.99002120824 1357608.0177139184 0, -359033.7779137578 1357209.094205264 0, -359297.29753420234 1357219.2749062034 0)), ((-351270.8017206167 1361748.2628893526 0, -351288.3413908767 1361353.243297764 0, -351306.36751743325 1360947.45884278 0, -351694.42529263464 1360963.460190764 0, -352093.6874091619 1360979.9844625439 0, -352492.9406986409 1360996.5044930095 0, -352899.4685926382 1361013.3541745322 0, -352882.0807381286 1361418.9074092212 0, -352864.6485749161 1361825.7594670148 0, -352459.39748882724 1361806.0276758445 0, -352059.940405738 1361786.5980778746 0, -351660.4821784091 1361767.187089537 0, -351270.8017206167 1361748.2628893526 0)), ((-354424.65131061 1362294.773071838 0, -354408.20124209835 1362700.8249301065 0, -354015.7150691202 1362684.5142586315 0, -354033.09612832806 1362278.6464530088 0, -354050.04812724976 1361882.336925241 0, -354440.6126000446 1361901.0211186607 0, -354424.65131061 1362294.773071838 0)), ((-357473.947476606 1365291.5016070085 0, -357459.62449225865 1365674.1181109415 0, -357078.60873583413 1365658.8350642982 0, -356681.1793443605 1365642.9748502166 0, -356698.93782114284 1365259.1797455663 0, -357096.1393811552 1365275.7363124103 0, -357473.947476606 1365291.5016070085 0)), ((-357873.21971875464 1365691.9560075493 0, -358270.38363140216 1365709.2046618902 0, -358252.79299782147 1366114.6931972597 0, -358235.21367921255 1366520.12749701 0, -357837.46152221074 1366502.3054830607 0, -357429.3093563812 1366484.101384524 0, -357444.47470284847 1366078.9245816981 0, -357459.62449225865 1365674.1181109415 0, -357873.21971875464 1365691.9560075493 0)), ((-348660.282804362 1366932.2975763981 0, -348676.46502220124 1366543.18852855 0, -349074.2820011688 1366564.0710639488 0, -349059.9344129219 1366948.6849072697 0, -348660.282804362 1366932.2975763981 0)), ((-357397.9916733659 1367293.868953829 0, -357413.4577528418 1366907.6658822547 0, -357818.88116476673 1366925.0278789743 0, -357801.8454937258 1367312.9351737169 0, -357397.9916733659 1367293.868953829 0)), ((-358200.0593048811 1367331.7620508755 0, -358216.9251348344 1366942.08910748 0, -358614.9678924947 1366959.1800282802 0, -358597.54068866116 1367350.8345066137 0, -358200.0593048811 1367331.7620508755 0)), ((-353372.4720056694 1368351.6774324747 0, -353391.0150068847 1367942.7579636874 0, -353789.5047035531 1367960.1377027866 0, -353771.2464242833 1368371.5331147136 0, -353372.4720056694 1368351.6774324747 0)), ((-347687.5396211228 1370950.8598156471 0, -347705.00175835413 1370545.7607001553 0, -348109.3719902935 1370563.0411290487 0, -348091.781302927 1370967.9445063812 0, -347687.5396211228 1370950.8598156471 0)), ((-349755.5066175441 1378759.992180404 0, -349772.295284719 1378354.9302033514 0, -350170.6027937253 1378371.5814273914 0, -350153.8408328068 1378776.4091730039 0, -349755.5066175441 1378759.992180404 0)), ((-346817.15529319266 1382291.8851551288 0, -346833.7295586715 1381886.399112779 0, -347211.554953689 1381902.7596700615 0, -347197.15536544897 1382308.378918614 0, -346817.15529319266 1382291.8851551288 0)), ((-354717.6469380916 1383434.7708101235 0, -355109.7107669407 1383451.6149904262 0, -355090.52058009495 1383856.771498326 0, -355496.18665894936 1383873.1464426564 0, -355894.54523188854 1383889.1467156415 0, -355876.57681959815 1384294.332607935 0, -355478.03890379204 1384278.3361831154 0, -355071.33997259726 1384261.918373973 0, -354681.4486774456 1384245.2766223864 0, -354699.54261558375 1383840.0396270151 0, -354717.6469380916 1383434.7708101235 0)), ((-350542.21304843505 1387728.8903621482 0, -350559.96972634003 1387322.629726069 0, -350958.8867659312 1387338.8547332073 0, -350941.21447320527 1387746.1046110156 0, -350542.21304843505 1387728.8903621482 0)), ((-351340.21552578005 1387763.326283671 0, -351357.7845907379 1387355.1087823967 0, -351747.9172067287 1387371.0429147827 0, -351732.8164146267 1387780.3029814872 0, -351340.21552578005 1387763.326283671 0)), ((-353696.8589999303 1388669.939378815 0, -353714.1796983275 1388264.6110539115 0, -354112.52048784273 1388281.2300513396 0, -354095.15150745376 1388686.612328041 0, -353696.8589999303 1388669.939378815 0)), ((-356477.7443976425 1388785.475961282 0, -356492.32325303997 1388379.3390252984 0, -356900.9627433467 1388396.8319157565 0, -356883.57240180305 1388802.7841161329 0, -356477.7443976425 1388785.475961282 0)), ((-353661.8262649351 1389488.52661755 0, -353282.6077046209 1389469.950351536 0, -353291.29145057936 1389058.6269033318 0, -353679.5300948229 1389075.246176343 0, -353661.8262649351 1389488.52661755 0)), ((-348407.88163971197 1391697.2612485385 0, -348392.05328470294 1392102.2264325675 0, -348007.9749739478 1392086.2695230446 0, -347608.6422700115 1392069.708717478 0, -347625.88360492187 1391664.4874593369 0, -348025.1216067826 1391681.1899792918 0, -348407.88163971197 1391697.2612485385 0)), ((-355532.6399913388 1392402.7768669496 0, -355549.8375729409 1391997.510224203 0, -355948.00830165227 1392014.9764385358 0, -355930.8801632781 1392420.2796652473 0, -355532.6399913388 1392402.7768669496 0)), ((-355115.1116125206 1392841.0467951794 0, -354713.1800568097 1392825.1869997384 0, -354733.73397034826 1392367.6705122732 0, -355134.39942643075 1392385.28157189 0, -355115.1116125206 1392841.0467951794 0)), ((-348329.5256154085 1393726.4002683775 0, -348345.08864940243 1393320.0075596853 0, -348360.66055985086 1392913.6165689405 0, -348375.8090843845 1392518.0430112684 0, -348787.9468124709 1392538.50221225 0, -349186.15655104857 1392558.2771554294 0, -349170.08305611735 1392948.928327773 0, -349153.3125517046 1393354.6429300876 0, -349551.665762811 1393371.753541793 0, -349534.9051223101 1393777.2009643163 0, -349517.046501679 1394205.5157084002 0, -349118.8701624145 1394184.8161240076 0, -349136.5337751835 1393760.56015241 0, -348738.19989919744 1393743.65954547 0, -348329.5256154085 1393726.4002683775 0)), ((-351711.4353606546 1401528.1259935389 0, -351729.2336429809 1401122.8436259546 0, -352126.7728349011 1401139.450112515 0, -352108.6963418144 1401544.6984636858 0, -351711.4353606546 1401528.1259935389 0)), ((-348008.1567221181 1404219.0299562518 0, -348024.7499558863 1403810.4509366164 0, -348421.1604141024 1403827.9078839866 0, -348405.021139808 1404235.6874635674 0, -348008.1567221181 1404219.0299562518 0)), ((-347123.46775164246 1406202.6003402423 0, -347491.3053225818 1406218.0928346743 0, -347470.4041352478 1406622.6828833793 0, -347449.32853422535 1407030.4604055476 0, -347083.03003610106 1407015.535289719 0, -346684.9139218934 1406999.331504781 0, -346286.79699508625 1406983.1464610733 0, -345844.2178804622 1406965.1756277063 0, -345867.2192612666 1406552.5341596862 0, -345889.7436118823 1406148.345018375 0, -345912.2684441618 1405744.1571821545 0, -345935.010934434 1405336.1699430896 0, -346368.7683103965 1405353.7837066324 0, -346766.40530349367 1405369.9501869874 0, -346745.8836935247 1405780.8842287003 0, -346725.624441341 1406185.3764335453 0, -347123.46775164246 1406202.6003402423 0)), ((-348695.42086405825 1406676.1972816356 0, -348715.3237081502 1406271.0851836922 0, -349091.4769303675 1406286.8638828169 0, -349070.0785561751 1406692.0825219816 0, -348695.42086405825 1406676.1972816356 0)), ((-347003.893684781 1408636.5159532179 0, -347372.30107684643 1408651.526345813 0, -347353.6388574002 1409051.2513625193 0, -347334.740736428 1409456.110942918 0, -346964.997256089 1409439.9259129746 0, -346567.5977578113 1409422.363094277 0, -346587.0567698071 1409017.828587732 0, -346606.2209480094 1408620.3309691842 0, -347003.893684781 1408636.5159532179 0)), ((-356873.3493111362 1409863.7026592577 0, -356891.6818188939 1409458.979536657 0, -357317.7298844178 1409476.0853097995 0, -357299.3961189424 1409880.9986555127 0, -356873.3493111362 1409863.7026592577 0)), ((-355224.0502692145 1411008.9416083568 0, -355241.7573319244 1410608.771321979 0, -355670.1325873775 1410624.807051414 0, -355652.1639219354 1411027.5323561318 0, -355224.0502692145 1411008.9416083568 0)), ((-356049.7527283597 1411044.7454744605 0, -356067.75576661574 1410639.7135129182 0, -356465.38732174423 1410654.6388935337 0, -356447.341140399 1411061.9661195907 0, -356049.7527283597 1411044.7454744605 0)), ((-354839.1738298257 1411397.732531105 0, -354857.33571466134 1410992.907355637 0, -355224.0502692145 1411008.9416083568 0, -355206.1317225063 1411413.7543825363 0, -354839.1738298257 1411397.732531105 0)), ((-355188.2123615047 1411818.5907162693 0, -355206.1317225063 1411413.7543825363 0, -355634.11657352693 1411432.3620669418 0, -355616.06122956896 1411837.1702722742 0, -355188.2123615047 1411818.5907162693 0)), ((-356411.46797655127 1411871.6019979452 0, -356429.3993107161 1411466.800072399 0, -356792.5799965783 1411481.8919451416 0, -356770.54732132587 1411886.4548459747 0, -356411.46797655127 1411871.6019979452 0)), ((-348360.21644791716 1413559.594939356 0, -347964.1878763282 1413541.6906920564 0, -347983.950479413 1413130.4118596665 0, -348003.3930837916 1412726.3147021506 0, -348399.87269641826 1412744.4395201094 0, -348766.35575836373 1412760.2900713126 0, -348740.9308342871 1413164.4780370304 0, -348715.058814354 1413575.6631823056 0, -348360.21644791716 1413559.594939356 0)), ((-346722.75356198533 1414692.6055146086 0, -346325.8964156597 1414675.2569416263 0, -345928.81429065444 1414657.9179484423 0, -345944.9573532146 1414253.1657256628 0, -345961.39735369437 1413849.2784336288 0, -345977.05834741297 1413467.221423721 0, -346375.44168994646 1413479.974607463 0, -346773.82453416137 1413492.7465218005 0, -346757.06482423027 1413883.9356210881 0, -346739.8671542056 1414287.8704604353 0, -346722.75356198533 1414692.6055146086 0)), ((-354118.10199398984 1419078.2133150047 0, -354134.11917277594 1418700.50468748 0, -354533.3095714249 1418717.5374399722 0, -354517.42658010306 1419094.4000600972 0, -354118.10199398984 1419078.2133150047 0)), ((-353684.2354638857 1419872.6064042423 0, -353701.505658522 1419467.3364129893 0, -354100.9330146703 1419483.3966548406 0, -354083.7563947924 1419888.5471587286 0, -353684.2354638857 1419872.6064042423 0)), ((-354065.83622214454 1420311.7879888718 0, -354083.7563947924 1419888.5471587286 0, -354483.2675635586 1419904.506421962 0, -354465.424729406 1420327.9968572203 0, -354065.83622214454 1420311.7879888718 0)), ((-348025.463406294 1420836.1086869314 0, -348041.53962860245 1420430.6854239649 0, -348426.68665312266 1420453.3152277546 0, -348415.5384656027 1420858.6154446949 0, -348025.463406294 1420836.1086869314 0)), ((-354752.6658573873 1423153.059072331 0, -354771.8774517418 1422749.911501092 0, -355160.4615968746 1422766.0464488377 0, -355143.4081668078 1423169.4632624118 0, -354752.6658573873 1423153.059072331 0)), ((-357481.67610300274 1424481.3435530642 0, -357498.5536899574 1424077.7702274134 0, -357905.831372728 1424094.4938023358 0, -357890.94891877763 1424497.7028040465 0, -357481.67610300274 1424481.3435530642 0)), ((-350668.2946377912 1425028.8661579809 0, -351068.15334199637 1425044.9471145743 0, -351468.67390004173 1425061.0630969177 0, -351452.0744898809 1425455.0139780398 0, -351434.9950174119 1425860.1523877648 0, -351034.11502877454 1425842.800234286 0, -350634.6934922263 1425825.5046070383 0, -350651.7702399814 1425420.377342054 0, -350668.2946377912 1425028.8661579809 0)), ((-349029.9255381937 1425753.9336475662 0, -349046.05618212954 1425348.5881110544 0, -349444.5642389892 1425366.9920935426 0, -349428.39186113706 1425772.2350828093 0, -349029.9255381937 1425753.9336475662 0)), ((-352161.1064046387 1427513.0234934015 0, -352143.83785809303 1427918.1374389369 0, -351745.6649810806 1427901.9915139768 0, -351762.8175462715 1427496.8392070443 0, -351779.9884874296 1427091.677581022 0, -352178.36785600433 1427107.8656894905 0, -352161.1064046387 1427513.0234934015 0)), ((-348164.38240724464 1427744.2994552937 0, -348178.9385128509 1427339.0742825416 0, -348566.62502079806 1427356.8297654947 0, -348550.342897298 1427762.1747602886 0, -348164.38240724464 1427744.2994552937 0)), ((-350230.8223324763 1445875.9999094566 0, -350248.37302386295 1445442.739409267 0, -350646.9239416059 1445460.523727007 0, -350629.40674311947 1445890.7484154105 0, -350230.8223324763 1445875.9999094566 0)), ((-354838.6553428664 1450517.9471484432 0, -354853.83655417344 1450111.9818005834 0, -355251.92480748164 1450128.9414715187 0, -355236.98129094596 1450534.7488335774 0, -354838.6553428664 1450517.9471484432 0)), ((-355620.12947804976 1450966.5364257703 0, -355635.2971191326 1450551.5799998227 0, -356000.3316821585 1450566.8757307483 0, -355981.6724153701 1450986.023187938 0, -355620.12947804976 1450966.5364257703 0)), ((-354807.67728060915 1451330.4830263734 0, -354823.4852046381 1450923.645091325 0, -355221.80369747564 1450945.0755959547 0, -355206.1505550897 1451347.548941065 0, -354807.67728060915 1451330.4830263734 0)), ((-348389.8106483252 1452295.3684782349 0, -348407.4266693561 1451876.218079681 0, -348805.6747593268 1451892.6275055222 0, -348787.3184284985 1452316.9143551881 0, -348389.8106483252 1452295.3684782349 0)), ((-351142.60133101285 1452805.1546824405 0, -351161.3749024862 1452428.462809134 0, -351571.2959469255 1452440.6224147517 0, -351555.46592494147 1452822.3790739346 0, -351142.60133101285 1452805.1546824405 0)), ((-349930.8961596085 1453566.3630178545 0, -349510.99900394725 1453548.186396057 0, -349529.4427887525 1453142.438189612 0, -349947.20200318896 1453160.5153243535 0, -349930.8961596085 1453566.3630178545 0)), ((-350280.25106129213 1454801.014190131 0, -350296.1677086838 1454394.6765530207 0, -350693.9919418809 1454411.4312017092 0, -350678.4096056654 1454817.8612900588 0, -350280.25106129213 1454801.014190131 0)), ((-350662.846357255 1455224.2595562523 0, -350678.4096056654 1454817.8612900588 0, -351056.847353793 1454834.2239497942 0, -351044.447383277 1455240.7981939812 0, -350662.846357255 1455224.2595562523 0)), ((-351843.51982631 1455688.29057269 0, -351858.7485328112 1455274.7709105567 0, -352257.44366374187 1455291.5697279382 0, -352242.41031523165 1455703.5732049684 0, -351843.51982631 1455688.29057269 0)), ((-346969.18978681305 1458323.8229245085 0, -346570.700375131 1458307.9141672119 0, -346586.4165548162 1457902.0863561668 0, -346602.1414244961 1457496.2599147782 0, -347000.57691500767 1457512.0205547437 0, -346984.88231883367 1457917.949240597 0, -346969.18978681305 1458323.8229245085 0)), ((-350115.36667721387 1459269.4369634266 0, -349715.0099568234 1459252.3261245366 0, -349729.6036264148 1458856.6265498945 0, -350129.6127423112 1458876.9847469658 0, -350115.36667721387 1459269.4369634266 0)), ((-346937.73634376767 1459135.492216159 0, -347336.0914732778 1459151.7843275242 0, -347320.21083438 1459557.8552156815 0, -346921.98470325454 1459541.2770024491 0, -346523.75877064344 1459524.6950247176 0, -346539.37148178974 1459119.2185542292 0, -346937.73634376767 1459135.492216159 0)), ((-349936.66028010513 1463705.187592036 0, -350333.93352318247 1463719.926289244 0, -350337.515488424 1463720.0521339818 0, -350757.12427452975 1463735.6341429213 0, -350734.86403182475 1464175.2029000216 0, -350727.1610888539 1464327.3657469398 0, -350307.9088828024 1464314.9481103728 0, -350194.9177407775 1464311.6014781625 0, -349910.86979118193 1464299.0031514687 0, -349917.9166273989 1464137.5602397716 0, -349936.66028010513 1463705.187592036 0)), ((-342841.1119918173 1340632.8637823046 0, -342824.3076344522 1341038.0108424642 0, -342425.2988937983 1341020.861646638 0, -342442.07448514656 1340615.7359850365 0, -342460.6459103588 1340172.1510842622 0, -342859.57056067494 1340192.3986456948 0, -342841.1119918173 1340632.8637823046 0)), ((-345140.9918017979 1341920.508097555 0, -345157.2557233199 1341540.3530836098 0, -345174.6185909283 1341134.4315884863 0, -345191.981407407 1340728.5115147133 0, -345209.79870890256 1340311.9618774182 0, -345648.49624270713 1340327.2749385322 0, -346047.53628352174 1340341.2141825373 0, -346029.97228601924 1340762.824623058 0, -345631.0548593376 1340746.5497945012 0, -345614.1299151223 1341152.3194379532 0, -345597.1976300247 1341558.0455516647 0, -345581.2937218333 1341938.2151379136 0, -345140.9918017979 1341920.508097555 0)), ((-343567.364092724 1341475.53907294 0, -343549.612151009 1341861.849379169 0, -343190.32350818557 1341848.648402978 0, -342791.25206229615 1341833.9975858508 0, -342392.1890544817 1341819.3656692682 0, -342408.5146746234 1341425.977246004 0, -342807.51452379476 1341443.1037557158 0, -343206.51358036016 1341460.2487691753 0, -343567.364092724 1341475.53907294 0)), ((-343458.35092139174 1343907.5892299209 0, -343470.7760278855 1343488.8299505985 0, -343919.5971428533 1343511.1187815068 0, -343902.5440715328 1343925.5944250748 0, -343885.8885799567 1344331.4982611246 0, -343446.29649084527 1344313.6770053855 0, -343458.35092139174 1343907.5892299209 0)), ((-342176.333127305 1347107.9038847473 0, -342192.88253073563 1346693.911832327 0, -342590.96282975515 1346705.9520534985 0, -342574.09787235287 1347123.5151336843 0, -342176.333127305 1347107.9038847473 0)), ((-342955.1820634155 1347544.801544837 0, -342971.86239083664 1347139.1337758112 0, -343341.0886031171 1347153.6513152218 0, -343325.2035261862 1347559.1270751476 0, -342955.1820634155 1347544.801544837 0)), ((-342013.47716455837 1351165.0940395673 0, -342029.6918228652 1350759.4956530817 0, -342426.89655603445 1350775.1526136629 0, -342410.6151158646 1351180.5916005028 0, -342013.47716455837 1351165.0940395673 0)), ((-344994.82985854853 1356162.1732665733 0, -344573.50844120356 1356144.9687277474 0, -344589.813440057 1355739.2444343232 0, -344606.12744614785 1355333.2978831504 0, -345029.01590181206 1355350.5093214312 0, -345427.04025114607 1355366.7061175613 0, -345409.99986517086 1355772.6682895813 0, -345807.82373454917 1355788.8867577168 0, -346176.48575458466 1355803.5876765575 0, -346157.10198400303 1356209.1768285248 0, -345790.9450225855 1356194.6330347736 0, -345392.9581951006 1356178.4415963513 0, -344994.82985854853 1356162.1732665733 0)), ((-341283.0262273813 1362171.040049678 0, -341266.51905991114 1362576.4876883903 0, -341250.1071516174 1362979.3196337237 0, -340851.5096170965 1362967.7698017969 0, -340867.9206153428 1362563.5825670965 0, -340884.3436855282 1362158.411502429 0, -341283.0262273813 1362171.040049678 0)), ((-340368.3405678828 1374702.528704076 0, -340383.3609665003 1374301.988174039 0, -340781.81042570295 1374319.1638477154 0, -340766.6387609196 1374720.3144716925 0, -340751.3025726853 1375125.369039317 0, -340353.1187008209 1375107.6774550283 0, -340368.3405678828 1374702.528704076 0)), ((-344121.3756386842 1380144.0009456384 0, -344135.27865748905 1379738.469479155 0, -344529.7654317961 1379755.7259424091 0, -344513.069789827 1380161.2233191975 0, -344121.3756386842 1380144.0009456384 0)), ((-340922.0202294746 1380409.9732110247 0, -340906.25508266763 1380832.324753256 0, -340524.6781668231 1380810.83038884 0, -340508.2186719182 1381204.7142695847 0, -340109.7615425989 1381188.3342901908 0, -339711.29063051404 1381171.849157207 0, -339728.0619542611 1380766.0140956528 0, -339348.0450811503 1380744.6680040872 0, -339363.9110429375 1380344.8471468957 0, -339379.982923474 1379939.8381771157 0, -339759.14410311804 1379955.5046300765 0, -340157.6289554072 1379971.9343324383 0, -340556.09600387886 1379988.3596279428 0, -340937.16659181804 1380004.0425070876 0, -340922.0202294746 1380409.9732110247 0)), ((-344878.1483756385 1380982.2527074562 0, -344894.4474772146 1380584.152432693 0, -345292.5188371152 1380601.6238125055 0, -345276.3043799941 1380999.6265122788 0, -344878.1483756385 1380982.2527074562 0)), ((-345207.52771767805 1382639.6053506676 0, -345585.0650542109 1382657.7432602337 0, -345569.8139299514 1383051.31048828 0, -345190.86118456634 1383034.750900587 0, -344793.20966751425 1383017.4985788283 0, -344809.74244653963 1382620.5215218433 0, -345207.52771767805 1382639.6053506676 0)), ((-345066.30847864936 1398408.6408999928 0, -344642.6851108595 1398393.219284141 0, -344658.7209222365 1397987.704672577 0, -345083.58321694814 1398003.8935036052 0, -345066.30847864936 1398408.6408999928 0)), ((-345465.684327352 1398423.1240414022 0, -345482.7879678646 1398019.0755668976 0, -345881.98345621413 1398034.2648332508 0, -345865.0684907993 1398437.6262531297 0, -345465.684327352 1398423.1240414022 0)), ((-341876.77152334526 1398278.2418595853 0, -342273.8355395169 1398295.2051671294 0, -342256.3478088118 1398700.9542483406 0, -342239.4476560443 1399105.2828931536 0, -341842.5295894404 1399088.3144151075 0, -341859.38069039135 1398682.0454870034 0, -341876.77152334526 1398278.2418595853 0)), ((-340638.0911691787 1399445.6980949338 0, -340620.72515622806 1399850.526226411 0, -340603.04242367914 1400266.8938196686 0, -340205.32143577555 1400258.4149165906 0, -339808.46281444904 1400249.966519819 0, -339831.3228318947 1399820.6744445744 0, -339428.584161946 1399803.6299457243 0, -339445.6395202424 1399398.6323314465 0, -339462.7051056934 1398993.602721615 0, -339479.3587053041 1398598.7081489614 0, -339895.48909513635 1398615.7151477942 0, -340274.62398019526 1398627.0540899008 0, -340672.7063960766 1398638.9761529872 0, -340655.44109253195 1399041.0497994921 0, -340638.0911691787 1399445.6980949338 0)), ((-342636.35647675116 1399122.258260717 0, -342653.3135758737 1398719.8925664052 0, -343022.63075729815 1398737.5247592917 0, -343007.5354047162 1399138.3183066058 0, -342636.35647675116 1399122.258260717 0)), ((-341342.4916148999 1401092.897813271 0, -341355.93487557484 1400688.6261757205 0, -341774.6881077003 1400706.3601315005 0, -341757.1298013605 1401110.7695320407 0, -341342.4916148999 1401092.897813271 0)), ((-343247.7710604982 1403617.1635324513 0, -342838.1736146872 1403598.9131773629 0, -342850.2072338024 1403187.3505506825 0, -343264.9033698708 1403205.3353939906 0, -343247.7710604982 1403617.1635324513 0)), ((-339870.1649730208 1407922.203352726 0, -339888.49578716926 1407518.7671617086 0, -340286.26887479814 1407535.2120291828 0, -340304.36010001914 1407131.9580457902 0, -340702.33325170807 1407148.1382843032 0, -340684.32908456627 1407551.6644661804 0, -340666.31967764045 1407955.3260661766 0, -340268.1491926431 1407938.734904692 0, -339870.1649730208 1407922.203352726 0)), ((-346247.9670798881 1407786.4941878766 0, -346645.8201518031 1407803.8223594844 0, -346626.1635088715 1408208.5580263122 0, -346228.42658896185 1408191.268497852 0, -345802.3720339995 1408173.094835538 0, -345433.00469636556 1408156.948935821 0, -345035.31090906216 1408139.918623091 0, -345015.64152360446 1408549.9554787027 0, -344996.61168193567 1408948.6357003283 0, -345394.33315879374 1408965.8236967118 0, -345770.66748386074 1408982.027884845 0, -345752.90011232597 1409386.3288852144 0, -345735.13290618424 1409790.6310598035 0, -345716.77404238534 1410208.4120195876 0, -345335.98430017295 1410193.372097704 0, -344938.1520471706 1410177.6816061637 0, -344958.0753859025 1409757.1289551663 0, -344977.3386638479 1409352.8871418906 0, -344579.616953587 1409335.729115382 0, -344166.849856294 1409318.0043719218 0, -343784.0478287569 1409302.2930294177 0, -343386.2179976331 1409286.0267386187 0, -343405.7698970168 1408882.3348835513 0, -343425.5895086238 1408472.8959652386 0, -343823.0140721051 1408492.3618964383 0, -344197.4123954481 1408510.7034136688 0, -344216.9066691419 1408104.6926269128 0, -344637.6341516515 1408122.9075098906 0, -344657.05210852646 1407718.6206526163 0, -345054.7451216327 1407735.4756642699 0, -345452.4382479587 1407752.3268210804 0, -345816.4036151787 1407768.119297683 0, -346247.9670798881 1407786.4941878766 0)), ((-342232.2456999183 1408415.8328396617 0, -342251.20168313495 1408024.69007037 0, -342633.0801790554 1408041.5033950997 0, -342613.661897842 1408433.2099763302 0, -342232.2456999183 1408415.8328396617 0)), ((-340229.9926343114 1408746.3575773109 0, -340249.8654157816 1408349.7480834918 0, -340648.3951632625 1408355.5189963714 0, -340628.2790211926 1408762.9195044443 0, -340229.9926343114 1408746.3575773109 0)), ((-341394.7861058384 1409200.480017132 0, -341414.75091705786 1408796.893348834 0, -341813.28227504826 1408814.7305489664 0, -341793.3769847323 1409218.1513685295 0, -341394.7861058384 1409200.480017132 0)), ((-340189.87556168414 1409554.7583447332 0, -340209.937477618 1409150.4679064595 0, -340608.24752550916 1409166.8624452765 0, -340588.2051832871 1409570.8621599749 0, -340567.8395292777 1409983.4102936746 0, -340169.45275954565 1409968.7722235362 0, -340189.87556168414 1409554.7583447332 0)), ((-340943.757611454 1409997.246302414 0, -340964.34459648543 1409585.9061182565 0, -341374.8313825132 1409604.0458560777 0, -341354.31428205146 1410018.9740127448 0, -340943.757611454 1409997.246302414 0)), ((-341752.8456458819 1410040.0823027717 0, -341773.4733260696 1409621.5397792314 0, -342172.1233875785 1409639.0527147471 0, -342151.35741088085 1410061.2197270521 0, -341752.8456458819 1410040.0823027717 0)), ((-341295.6899582391 1411217.1830032198 0, -341315.42150696437 1410813.9956491112 0, -341714.2326547699 1410831.0027304366 0, -341694.57000477024 1411234.013420732 0, -341295.6899582391 1411217.1830032198 0)), ((-340857.5851405858 1412005.3255519627 0, -340875.57805844577 1411598.211593418 0, -341276.01546856196 1411619.3991900957 0, -341256.39696708706 1412022.2461524508 0, -340857.5851405858 1412005.3255519627 0)), ((-342017.12861457776 1412860.9707734026 0, -342036.0396851789 1412458.5640298661 0, -342054.9335399395 1412056.146478906 0, -342451.05728952045 1412072.9368059956 0, -342432.1348355964 1412475.5994607469 0, -342413.2125393507 1412878.2632718477 0, -342017.12861457776 1412860.9707734026 0)), ((-342288.46965569444 1415299.557578831 0, -342309.6265927482 1414907.5537957386 0, -342728.69513802195 1414925.7662906835 0, -342708.0364654197 1415318.7310265675 0, -342288.46965569444 1415299.557578831 0)), ((-341093.84846998606 1415649.51457269 0, -341112.626062274 1415246.0966882883 0, -341511.60121303174 1415264.3413924437 0, -341492.1317843788 1415667.5297177257 0, -341472.6461528557 1416070.6849413887 0, -341075.0713863812 1416052.9225069566 0, -341093.84846998606 1415649.51457269 0)), ((-341890.3967321589 1415685.551496792 0, -341910.5846393012 1415282.5938803065 0, -342288.46965569444 1415299.557578831 0, -342266.73286666913 1415702.206168663 0, -341890.3967321589 1415685.551496792 0)), ((-342245.00545663363 1416104.8564021925 0, -342266.73286666913 1415702.206168663 0, -342686.96553434426 1415721.5069476827 0, -342665.89542482805 1416124.2729297816 0, -342245.00545663363 1416104.8564021925 0)), ((-341453.4935543765 1416465.7646827723 0, -341472.6461528557 1416070.6849413887 0, -341870.2283866334 1416088.4774484204 0, -341850.4493658072 1416481.2684777866 0, -341453.4935543765 1416465.7646827723 0)), ((-344235.4406224039 1416606.5112660357 0, -344257.56470035476 1416197.064708848 0, -344654.9743995496 1416215.7649027384 0, -344632.3928176994 1416631.1649907243 0, -344612.01726633956 1417021.3320227156 0, -344214.61608383316 1417002.6886667702 0, -344235.4406224039 1416606.5112660357 0)), ((-346052.03838083055 1420323.7215362722 0, -346070.1133486577 1419894.8157591738 0, -346468.53318228025 1419912.7298333382 0, -346450.3329771588 1420342.8967375774 0, -346052.03838083055 1420323.7215362722 0)), ((-345231.2792150368 1420689.7486846386 0, -345249.0465732472 1420285.1113357048 0, -345653.73384955747 1420304.5646276753 0, -345636.7558976912 1420709.6036824018 0, -345231.2792150368 1420689.7486846386 0)), ((-346001.41042557085 1421528.3774480198 0, -346017.9193507657 1421134.4553692716 0, -346416.0573851456 1421154.341318056 0, -346399.4620596688 1421548.8314686015 0, -346001.41042557085 1421528.3774480198 0)), ((-343993.1292071387 1421853.642363438 0, -344010.39866362844 1421447.9391295684 0, -344408.6583404756 1421461.058222714 0, -344391.4430687855 1421870.4949712337 0, -343993.1292071387 1421853.642363438 0)), ((-343958.61173849425 1422664.7505184505 0, -343975.8657560828 1422259.2012829315 0, -344374.3768456535 1422275.8041104088 0, -344357.3022249994 1422681.1028981893 0, -343958.61173849425 1422664.7505184505 0)), ((-344739.1851728616 1423101.003025634 0, -344756.0012790888 1422697.4631436786 0, -345146.5099317879 1422713.4986350536 0, -345130.2000715515 1423115.591044668 0, -344739.1851728616 1423101.003025634 0)), ((-341226.3356192942 1431053.7071600927 0, -341242.08306449116 1430652.4771845983 0, -341620.11884193955 1430669.6354140968 0, -341605.2708941855 1431072.9971029009 0, -341226.3356192942 1431053.7071600927 0)), ((-340213.1564386973 1435396.5121018137 0, -340231.0214376499 1434990.3793355639 0, -339828.2895830553 1434975.5258258528 0, -339757.6919452463 1434640.0977227513 0, -339691.0554744319 1434563.975529186 0, -339850.4455809276 1434569.74501426 0, -340248.8812272845 1434584.1578984833 0, -340605.5225451439 1434597.507583827 0, -340592.9295309687 1435004.1306148195 0, -340580.33605210437 1435410.7548076266 0, -340213.1564386973 1435396.5121018137 0)), ((-343312.3659997066 1438333.0040433246 0, -342912.0090136283 1438322.4981403698 0, -342926.83478493 1437915.3837327522 0, -343326.973428204 1437925.7910365951 0, -343312.3659997066 1438333.0040433246 0)), ((-343297.7687086868 1438740.1850085407 0, -343312.3659997066 1438333.0040433246 0, -343715.1191248843 1438343.5810134464 0, -343701.41866796766 1438750.8991207564 0, -343297.7687086868 1438740.1850085407 0)), ((-344084.72178318526 1439150.9532293137 0, -344098.1710782253 1438763.784886659 0, -344497.9798800907 1438776.7795799167 0, -344484.2697039125 1439169.7090403608 0, -344084.72178318526 1439150.953229</t>
+          <t xml:space="preserve">MULTIPOLYGON Z (((-357801.5254078213 1344905.6837980137 0, -357819.7813741029 1344500.6385781919 0, -357837.9461128943 1344097.7861179465 0, -358238.3795021891 1344116.1991087764 0, -358221.53217823076 1344516.9562831922 0, -358204.5089800107 1344921.9297024182 0, -357801.5254078213 1344905.6837980137 0)), ((-355817.1438377021 1344822.5767877724 0, -356192.3206674648 1344837.5196446632 0, -356170.9744176764 1345242.7738757702 0, -356150.45549275127 1345632.2392934079 0, -355784.3258817538 1345617.05570784 0, -355385.30022062804 1345600.5256966979 0, -355401.4895024438 1345211.6423526665 0, -355800.39435997873 1345228.0328843403 0, -355817.1438377021 1344822.5767877724 0)), ((-356492.7974237927 1347695.012585433 0, -356510.87549364264 1347264.5720195188 0, -356909.82662284037 1347273.9088334735 0, -356891.55644370994 1347711.5314927895 0, -356492.7974237927 1347695.012585433 0)), ((-357659.26413695083 1347743.1696422533 0, -357640.7186669393 1348147.8222976355 0, -357622.163819644 1348552.4871537504 0, -357255.7905134044 1348537.8295405135 0, -357273.0523890364 1348132.954159144 0, -357290.3147160633 1347728.0689817243 0, -357659.26413695083 1347743.1696422533 0)), ((-356441.3910590585 1348896.6962962754 0, -356458.16752986953 1348505.4293759149 0, -356856.974705646 1348521.6255712162 0, -356840.2718644965 1348911.9885101218 0, -356441.3910590585 1348896.6962962754 0)), ((-352776.81700003677 1350388.8219333305 0, -352760.62431139336 1350790.7813189148 0, -352744.2869625499 1351196.4767546572 0, -352727.9495858058 1351602.173574781 0, -352711.6684112581 1352006.2838402814 0, -352323.3775849207 1351988.6776163653 0, -352340.211365484 1351585.8557566707 0, -352357.1722433722 1351180.1622097993 0, -352374.14339090075 1350774.4368619784 0, -352390.99767125765 1350371.3400573279 0, -352776.81700003677 1350388.8219333305 0)), ((-356293.07562019554 1352561.2261443897 0, -356309.752733045 1352136.219551802 0, -356708.1808269701 1352157.900147144 0, -356691.6088914508 1352578.1624770577 0, -356293.07562019554 1352561.2261443897 0)), ((-357074.13182791 1353001.6173415012 0, -357090.14095807 1352595.1284598762 0, -357486.2359831532 1352612.0003487691 0, -357471.02916397265 1353018.9596132175 0, -357074.13182791 1353001.6173415012 0)), ((-357442.1053178831 1353793.2174804166 0, -357043.31814070564 1353780.4442563402 0, -357058.1140250918 1353408.0961251466 0, -357455.8311478643 1353425.9206436945 0, -357442.1053178831 1353793.2174804166 0)), ((-347847.4595934799 1357553.0443838078 0, -347449.16478902934 1357536.7756948087 0, -347466.29814592085 1357131.2030211596 0, -347483.6032865532 1356721.3939454856 0, -347738.730805186 1356731.7409423897 0, -347881.57620768 1356740.9646807353 0, -347864.4904633793 1357147.5683108286 0, -347847.4595934799 1357553.0443838078 0)), ((-359297.29753420234 1357219.2749062034 0, -359443.0900664448 1357224.9063832841 0, -359696.06486753083 1357235.5196004468 0, -359831.22039591917 1357241.1929491353 0, -359814.238527892 1357642.7742239118 0, -359797.077253654 1358048.415189146 0, -359407.8827726577 1358031.2326209673 0, -358999.90043192107 1358014.143237385 0, -359016.99002120824 1357608.0177139184 0, -359033.7779137578 1357209.094205264 0, -359297.29753420234 1357219.2749062034 0)), ((-351270.8017206167 1361748.2628893526 0, -351288.3413908767 1361353.243297764 0, -351306.36751743325 1360947.45884278 0, -351694.42529263464 1360963.460190764 0, -352093.6874091619 1360979.9844625439 0, -352492.9406986409 1360996.5044930095 0, -352899.4685926382 1361013.3541745322 0, -352882.0807381286 1361418.9074092212 0, -352864.6485749161 1361825.7594670148 0, -352459.39748882724 1361806.0276758445 0, -352059.940405738 1361786.5980778746 0, -351660.4821784091 1361767.187089537 0, -351270.8017206167 1361748.2628893526 0)), ((-354424.65131061 1362294.773071838 0, -354408.20124209835 1362700.8249301065 0, -354015.7150691202 1362684.5142586315 0, -354033.09612832806 1362278.6464530088 0, -354050.04812724976 1361882.336925241 0, -354440.6126000446 1361901.0211186607 0, -354424.65131061 1362294.773071838 0)), ((-357473.947476606 1365291.5016070085 0, -357459.62449225865 1365674.1181109415 0, -357078.60873583413 1365658.8350642982 0, -356681.1793443605 1365642.9748502166 0, -356698.93782114284 1365259.1797455663 0, -357096.1393811552 1365275.7363124103 0, -357473.947476606 1365291.5016070085 0)), ((-357873.21971875464 1365691.9560075493 0, -358270.38363140216 1365709.2046618902 0, -358252.79299782147 1366114.6931972597 0, -358235.21367921255 1366520.12749701 0, -357837.46152221074 1366502.3054830607 0, -357429.3093563812 1366484.101384524 0, -357444.47470284847 1366078.9245816981 0, -357459.62449225865 1365674.1181109415 0, -357873.21971875464 1365691.9560075493 0)), ((-348660.282804362 1366932.2975763981 0, -348676.46502220124 1366543.18852855 0, -349074.2820011688 1366564.0710639488 0, -349059.9344129219 1366948.6849072697 0, -348660.282804362 1366932.2975763981 0)), ((-357397.9916733659 1367293.868953829 0, -357413.4577528418 1366907.6658822547 0, -357818.88116476673 1366925.0278789743 0, -357801.8454937258 1367312.9351737169 0, -357397.9916733659 1367293.868953829 0)), ((-358200.0593048811 1367331.7620508755 0, -358216.9251348344 1366942.08910748 0, -358614.9678924947 1366959.1800282802 0, -358597.54068866116 1367350.8345066137 0, -358200.0593048811 1367331.7620508755 0)), ((-353372.4720056694 1368351.6774324747 0, -353391.0150068847 1367942.7579636874 0, -353789.5047035531 1367960.1377027866 0, -353771.2464242833 1368371.5331147136 0, -353372.4720056694 1368351.6774324747 0)), ((-347687.5396211228 1370950.8598156471 0, -347705.00175835413 1370545.7607001553 0, -348109.3719902935 1370563.0411290487 0, -348091.781302927 1370967.9445063812 0, -347687.5396211228 1370950.8598156471 0)), ((-349755.5066175441 1378759.992180404 0, -349772.295284719 1378354.9302033514 0, -350170.6027937253 1378371.5814273914 0, -350153.8408328068 1378776.4091730039 0, -349755.5066175441 1378759.992180404 0)), ((-346817.15529319266 1382291.8851551288 0, -346833.7295586715 1381886.399112779 0, -347211.554953689 1381902.7596700615 0, -347197.15536544897 1382308.378918614 0, -346817.15529319266 1382291.8851551288 0)), ((-354717.6469380916 1383434.7708101235 0, -355109.7107669407 1383451.6149904262 0, -355090.52058009495 1383856.771498326 0, -355496.18665894936 1383873.1464426564 0, -355894.54523188854 1383889.1467156415 0, -355876.57681959815 1384294.332607935 0, -355478.03890379204 1384278.3361831154 0, -355071.33997259726 1384261.918373973 0, -354681.4486774456 1384245.2766223864 0, -354699.54261558375 1383840.0396270151 0, -354717.6469380916 1383434.7708101235 0)), ((-350542.21304843505 1387728.8903621482 0, -350559.96972634003 1387322.629726069 0, -350958.8867659312 1387338.8547332073 0, -350941.21447320527 1387746.1046110156 0, -350542.21304843505 1387728.8903621482 0)), ((-351340.21552578005 1387763.326283671 0, -351357.7845907379 1387355.1087823967 0, -351747.9172067287 1387371.0429147827 0, -351732.8164146267 1387780.3029814872 0, -351340.21552578005 1387763.326283671 0)), ((-353696.8589999303 1388669.939378815 0, -353714.1796983275 1388264.6110539115 0, -354112.52048784273 1388281.2300513396 0, -354095.15150745376 1388686.612328041 0, -353696.8589999303 1388669.939378815 0)), ((-356477.7443976425 1388785.475961282 0, -356492.32325303997 1388379.3390252984 0, -356900.9627433467 1388396.8319157565 0, -356883.57240180305 1388802.7841161329 0, -356477.7443976425 1388785.475961282 0)), ((-353661.8262649351 1389488.52661755 0, -353282.6077046209 1389469.950351536 0, -353291.29145057936 1389058.6269033318 0, -353679.5300948229 1389075.246176343 0, -353661.8262649351 1389488.52661755 0)), ((-348407.88163971197 1391697.2612485385 0, -348392.05328470294 1392102.2264325675 0, -348007.9749739478 1392086.2695230446 0, -347608.6422700115 1392069.708717478 0, -347625.88360492187 1391664.4874593369 0, -348025.1216067826 1391681.1899792918 0, -348407.88163971197 1391697.2612485385 0)), ((-355532.6399913388 1392402.7768669496 0, -355549.8375729409 1391997.510224203 0, -355948.00830165227 1392014.9764385358 0, -355930.8801632781 1392420.2796652473 0, -355532.6399913388 1392402.7768669496 0)), ((-355115.1116125206 1392841.0467951794 0, -354713.1800568097 1392825.1869997384 0, -354733.73397034826 1392367.6705122732 0, -355134.39942643075 1392385.28157189 0, -355115.1116125206 1392841.0467951794 0)), ((-348329.5256154085 1393726.4002683775 0, -348345.08864940243 1393320.0075596853 0, -348360.66055985086 1392913.6165689405 0, -348375.8090843845 1392518.0430112684 0, -348787.9468124709 1392538.50221225 0, -349186.15655104857 1392558.2771554294 0, -349170.08305611735 1392948.928327773 0, -349153.3125517046 1393354.6429300876 0, -349551.665762811 1393371.753541793 0, -349534.9051223101 1393777.2009643163 0, -349517.046501679 1394205.5157084002 0, -349118.8701624145 1394184.8161240076 0, -349136.5337751835 1393760.56015241 0, -348738.19989919744 1393743.65954547 0, -348329.5256154085 1393726.4002683775 0)), ((-351711.4353606546 1401528.1259935389 0, -351729.2336429809 1401122.8436259546 0, -352126.7728349011 1401139.450112515 0, -352108.6963418144 1401544.6984636858 0, -351711.4353606546 1401528.1259935389 0)), ((-348008.1567221181 1404219.0299562518 0, -348024.7499558863 1403810.4509366164 0, -348421.1604141024 1403827.9078839866 0, -348405.021139808 1404235.6874635674 0, -348008.1567221181 1404219.0299562518 0)), ((-347123.46775164246 1406202.6003402423 0, -347491.3053225818 1406218.0928346743 0, -347470.4041352478 1406622.6828833793 0, -347449.32853422535 1407030.4604055476 0, -347083.03003610106 1407015.535289719 0, -346684.9139218934 1406999.331504781 0, -346286.79699508625 1406983.1464610733 0, -345844.2178804622 1406965.1756277063 0, -345867.2192612666 1406552.5341596862 0, -345889.7436118823 1406148.345018375 0, -345912.2684441618 1405744.1571821545 0, -345935.010934434 1405336.1699430896 0, -346368.7683103965 1405353.7837066324 0, -346766.40530349367 1405369.9501869874 0, -346745.8836935247 1405780.8842287003 0, -346725.624441341 1406185.3764335453 0, -347123.46775164246 1406202.6003402423 0)), ((-348695.42086405825 1406676.1972816356 0, -348715.3237081502 1406271.0851836922 0, -349091.4769303675 1406286.8638828169 0, -349070.0785561751 1406692.0825219816 0, -348695.42086405825 1406676.1972816356 0)), ((-345802.3720339995 1408173.094835538 0, -345433.00469636556 1408156.948935821 0, -345035.31090906216 1408139.918623091 0, -345015.64152360446 1408549.9554787027 0, -344996.61168193567 1408948.6357003283 0, -345394.33315879374 1408965.8236967118 0, -345770.66748386074 1408982.027884845 0, -345752.90011232597 1409386.3288852144 0, -345735.13290618424 1409790.6310598035 0, -345716.77404238534 1410208.4120195876 0, -345335.98430017295 1410193.372097704 0, -344938.1520471706 1410177.6816061637 0, -344958.0753859025 1409757.1289551663 0, -344977.3386638479 1409352.8871418906 0, -344579.616953587 1409335.729115382 0, -344166.849856294 1409318.0043719218 0, -343784.0478287569 1409302.2930294177 0, -343386.2179976331 1409286.0267386187 0, -343405.7698970168 1408882.3348835513 0, -343425.5895086238 1408472.8959652386 0, -343823.0140721051 1408492.3618964383 0, -344197.4123954481 1408510.7034136688 0, -344216.9066691419 1408104.6926269128 0, -344637.6341516515 1408122.9075098906 0, -344657.05210852646 1407718.6206526163 0, -345054.7451216327 1407735.4756642699 0, -345452.4382479587 1407752.3268210804 0, -345816.4036151787 1407768.119297683 0, -346247.9670798881 1407786.4941878766 0, -346645.8201518031 1407803.8223594844 0, -346626.1635088715 1408208.5580263122 0, -346228.42658896185 1408191.268497852 0, -345802.3720339995 1408173.094835538 0)), ((-346587.0567698071 1409017.828587732 0, -346606.2209480094 1408620.3309691842 0, -347003.893684781 1408636.5159532179 0, -347372.30107684643 1408651.526345813 0, -347353.6388574002 1409051.2513625193 0, -347334.740736428 1409456.110942918 0, -346964.997256089 1409439.9259129746 0, -346567.5977578113 1409422.363094277 0, -346587.0567698071 1409017.828587732 0)), ((-356873.3493111362 1409863.7026592577 0, -356891.6818188939 1409458.979536657 0, -357317.7298844178 1409476.0853097995 0, -357299.3961189424 1409880.9986555127 0, -356873.3493111362 1409863.7026592577 0)), ((-355224.0502692145 1411008.9416083568 0, -355241.7573319244 1410608.771321979 0, -355670.1325873775 1410624.807051414 0, -355652.1639219354 1411027.5323561318 0, -355224.0502692145 1411008.9416083568 0)), ((-356049.7527283597 1411044.7454744605 0, -356067.75576661574 1410639.7135129182 0, -356465.38732174423 1410654.6388935337 0, -356447.341140399 1411061.9661195907 0, -356049.7527283597 1411044.7454744605 0)), ((-354839.1738298257 1411397.732531105 0, -354857.33571466134 1410992.907355637 0, -355224.0502692145 1411008.9416083568 0, -355206.1317225063 1411413.7543825363 0, -354839.1738298257 1411397.732531105 0)), ((-355188.2123615047 1411818.5907162693 0, -355206.1317225063 1411413.7543825363 0, -355634.11657352693 1411432.3620669418 0, -355616.06122956896 1411837.1702722742 0, -355188.2123615047 1411818.5907162693 0)), ((-356411.46797655127 1411871.6019979452 0, -356429.3993107161 1411466.800072399 0, -356792.5799965783 1411481.8919451416 0, -356770.54732132587 1411886.4548459747 0, -356411.46797655127 1411871.6019979452 0)), ((-348766.35575836373 1412760.2900713126 0, -348740.9308342871 1413164.4780370304 0, -348715.058814354 1413575.6631823056 0, -348360.21644791716 1413559.594939356 0, -347964.1878763282 1413541.6906920564 0, -347983.950479413 1413130.4118596665 0, -348003.3930837916 1412726.3147021506 0, -348399.87269641826 1412744.4395201094 0, -348766.35575836373 1412760.2900713126 0)), ((-345944.9573532146 1414253.1657256628 0, -345961.39735369437 1413849.2784336288 0, -345977.05834741297 1413467.221423721 0, -346375.44168994646 1413479.974607463 0, -346773.82453416137 1413492.7465218005 0, -346757.06482423027 1413883.9356210881 0, -346739.8671542056 1414287.8704604353 0, -346722.75356198533 1414692.6055146086 0, -346325.8964156597 1414675.2569416263 0, -345928.81429065444 1414657.9179484423 0, -345944.9573532146 1414253.1657256628 0)), ((-354118.10199398984 1419078.2133150047 0, -354134.11917277594 1418700.50468748 0, -354533.3095714249 1418717.5374399722 0, -354517.42658010306 1419094.4000600972 0, -354118.10199398984 1419078.2133150047 0)), ((-353684.2354638857 1419872.6064042423 0, -353701.505658522 1419467.3364129893 0, -354100.9330146703 1419483.3966548406 0, -354083.7563947924 1419888.5471587286 0, -353684.2354638857 1419872.6064042423 0)), ((-354065.83622214454 1420311.7879888718 0, -354083.7563947924 1419888.5471587286 0, -354483.2675635586 1419904.506421962 0, -354465.424729406 1420327.9968572203 0, -354065.83622214454 1420311.7879888718 0)), ((-346052.03838083055 1420323.7215362722 0, -346070.1133486577 1419894.8157591738 0, -346468.53318228025 1419912.7298333382 0, -346450.3329771588 1420342.8967375774 0, -346052.03838083055 1420323.7215362722 0)), ((-348025.463406294 1420836.1086869314 0, -348041.53962860245 1420430.6854239649 0, -348426.68665312266 1420453.3152277546 0, -348415.5384656027 1420858.6154446949 0, -348025.463406294 1420836.1086869314 0)), ((-346001.41042557085 1421528.3774480198 0, -346017.9193507657 1421134.4553692716 0, -346416.0573851456 1421154.341318056 0, -346399.4620596688 1421548.8314686015 0, -346001.41042557085 1421528.3774480198 0)), ((-354752.6658573873 1423153.059072331 0, -354771.8774517418 1422749.911501092 0, -355160.4615968746 1422766.0464488377 0, -355143.4081668078 1423169.4632624118 0, -354752.6658573873 1423153.059072331 0)), ((-357481.67610300274 1424481.3435530642 0, -357498.5536899574 1424077.7702274134 0, -357905.831372728 1424094.4938023358 0, -357890.94891877763 1424497.7028040465 0, -357481.67610300274 1424481.3435530642 0)), ((-350668.2946377912 1425028.8661579809 0, -351068.15334199637 1425044.9471145743 0, -351468.67390004173 1425061.0630969177 0, -351452.0744898809 1425455.0139780398 0, -351434.9950174119 1425860.1523877648 0, -351034.11502877454 1425842.800234286 0, -350634.6934922263 1425825.5046070383 0, -350651.7702399814 1425420.377342054 0, -350668.2946377912 1425028.8661579809 0)), ((-349029.9255381937 1425753.9336475662 0, -349046.05618212954 1425348.5881110544 0, -349444.5642389892 1425366.9920935426 0, -349428.39186113706 1425772.2350828093 0, -349029.9255381937 1425753.9336475662 0)), ((-352178.36785600433 1427107.8656894905 0, -352161.1064046387 1427513.0234934015 0, -352143.83785809303 1427918.1374389369 0, -351745.6649810806 1427901.9915139768 0, -351762.8175462715 1427496.8392070443 0, -351779.9884874296 1427091.677581022 0, -352178.36785600433 1427107.8656894905 0)), ((-348164.38240724464 1427744.2994552937 0, -348178.9385128509 1427339.0742825416 0, -348566.62502079806 1427356.8297654947 0, -348550.342897298 1427762.1747602886 0, -348164.38240724464 1427744.2994552937 0)), ((-346235.23410652525 1446091.9792850977 0, -345830.9783168082 1446070.9518629392 0, -345814.5154433621 1446475.9675088117 0, -345413.2601418669 1446455.4962533272 0, -345017.11258891906 1446435.173393346 0, -344611.5502534447 1446414.621045567 0, -344211.18409721926 1446394.242920429 0, -343810.8529261694 1446373.8738984803 0, -343817.3926997089 1446208.0686848569 0, -343980.37208429986 1446146.4674142573 0, -344224.29113195447 1446059.6974000416 0, -344631.04726695153 1445914.9930020897 0, -344730.52660267445 1445879.6182937291 0, -345039.550292268 1445815.2193496209 0, -345031.8017203849 1446029.3011293616 0, -345429.3810166217 1446050.063324085 0, -345440.1026757518 1445725.8550735612 0, -345526.7499216841 1445707.562497297 0, -345843.23656160344 1445769.0979079106 0, -345874.19687807764 1445784.7841153156 0, -346090.6879857239 1445739.267253177 0, -346399.1800506631 1445291.1949497655 0, -346714.04477292026 1445301.89240218 0, -346703.8682969567 1445773.7838963736 0, -346249.8868085602 1445748.2284954276 0, -346235.23410652525 1446091.9792850977 0)), ((-350230.8223324763 1445875.9999094566 0, -350248.37302386295 1445442.739409267 0, -350646.9239416059 1445460.523727007 0, -350629.40674311947 1445890.7484154105 0, -350230.8223324763 1445875.9999094566 0)), ((-354838.6553428664 1450517.9471484432 0, -354853.83655417344 1450111.9818005834 0, -355251.92480748164 1450128.9414715187 0, -355236.98129094596 1450534.7488335774 0, -354838.6553428664 1450517.9471484432 0)), ((-355620.12947804976 1450966.5364257703 0, -355635.2971191326 1450551.5799998227 0, -356000.3316821585 1450566.8757307483 0, -355981.6724153701 1450986.023187938 0, -355620.12947804976 1450966.5364257703 0)), ((-354807.67728060915 1451330.4830263734 0, -354823.4852046381 1450923.645091325 0, -355221.80369747564 1450945.0755959547 0, -355206.1505550897 1451347.548941065 0, -354807.67728060915 1451330.4830263734 0)), ((-350662.846357255 1455224.2595562523 0, -350678.4096056654 1454817.8612900588 0, -351056.847353793 1454834.2239497942 0, -351044.447383277 1455240.7981939812 0, -350662.846357255 1455224.2595562523 0)), ((-346969.18978681305 1458323.8229245085 0, -346570.700375131 1458307.9141672119 0, -346586.4165548162 1457902.0863561668 0, -346602.1414244961 1457496.2599147782 0, -347000.57691500767 1457512.0205547437 0, -346984.88231883367 1457917.949240597 0, -346969.18978681305 1458323.8229245085 0)), ((-350115.36667721387 1459269.4369634266 0, -349715.0099568234 1459252.3261245366 0, -349729.6036264148 1458856.6265498945 0, -350129.6127423112 1458876.9847469658 0, -350115.36667721387 1459269.4369634266 0)), ((-346937.73634376767 1459135.492216159 0, -347336.0914732778 1459151.7843275242 0, -347320.21083438 1459557.8552156815 0, -346921.98470325454 1459541.2770024491 0, -346523.75877064344 1459524.6950247176 0, -346539.37148178974 1459119.2185542292 0, -346937.73634376767 1459135.492216159 0)), ((-349936.66028010513 1463705.187592036 0, -350333.93352318247 1463719.926289244 0, -350337.515488424 1463720.0521339818 0, -350757.12427452975 1463735.6341429213 0, -350734.86403182475 1464175.2029000216 0, -350727.1610888539 1464327.3657469398 0, -350307.9088828024 1464314.9481103728 0, -350194.9177407775 1464311.6014781625 0, -349910.86979118193 1464299.0031514687 0, -349917.9166273989 1464137.5602397716 0, -349936.66028010513 1463705.187592036 0)), ((-342841.1119918173 1340632.8637823046 0, -342824.3076344522 1341038.0108424642 0, -342425.2988937983 1341020.861646638 0, -342442.07448514656 1340615.7359850365 0, -342460.6459103588 1340172.1510842622 0, -342859.57056067494 1340192.3986456948 0, -342841.1119918173 1340632.8637823046 0)), ((-345140.9918017979 1341920.508097555 0, -345157.2557233199 1341540.3530836098 0, -345174.6185909283 1341134.4315884863 0, -345191.981407407 1340728.5115147133 0, -345209.79870890256 1340311.9618774182 0, -345648.49624270713 1340327.2749385322 0, -346047.53628352174 1340341.2141825373 0, -346029.97228601924 1340762.824623058 0, -345631.0548593376 1340746.5497945012 0, -345614.1299151223 1341152.3194379532 0, -345597.1976300247 1341558.0455516647 0, -345581.2937218333 1341938.2151379136 0, -345140.9918017979 1341920.508097555 0)), ((-343206.51358036016 1341460.2487691753 0, -343567.364092724 1341475.53907294 0, -343549.612151009 1341861.849379169 0, -343190.32350818557 1341848.648402978 0, -342791.25206229615 1341833.9975858508 0, -342392.1890544817 1341819.3656692682 0, -342408.5146746234 1341425.977246004 0, -342807.51452379476 1341443.1037557158 0, -343206.51358036016 1341460.2487691753 0)), ((-343458.35092139174 1343907.5892299209 0, -343470.7760278855 1343488.8299505985 0, -343919.5971428533 1343511.1187815068 0, -343902.5440715328 1343925.5944250748 0, -343885.8885799567 1344331.4982611246 0, -343446.29649084527 1344313.6770053855 0, -343458.35092139174 1343907.5892299209 0)), ((-342176.333127305 1347107.9038847473 0, -342192.88253073563 1346693.911832327 0, -342590.96282975515 1346705.9520534985 0, -342574.09787235287 1347123.5151336843 0, -342176.333127305 1347107.9038847473 0)), ((-342955.1820634155 1347544.801544837 0, -342971.86239083664 1347139.1337758112 0, -343341.0886031171 1347153.6513152218 0, -343325.2035261862 1347559.1270751476 0, -342955.1820634155 1347544.801544837 0)), ((-340114.499890167 1349057.2078276132 0, -340125.73802572803 1348651.5989460791 0, -340544.31690338027 1348668.3588085552 0, -340528.0716648638 1349073.8588849332 0, -340114.499890167 1349057.2078276132 0)), ((-342013.47716455837 1351165.0940395673 0, -342029.6918228652 1350759.4956530817 0, -342426.89655603445 1350775.1526136629 0, -342410.6151158646 1351180.5916005028 0, -342013.47716455837 1351165.0940395673 0)), ((-345409.99986517086 1355772.6682895813 0, -345807.82373454917 1355788.8867577168 0, -346176.48575458466 1355803.5876765575 0, -346157.10198400303 1356209.1768285248 0, -345790.9450225855 1356194.6330347736 0, -345392.9581951006 1356178.4415963513 0, -344994.82985854853 1356162.1732665733 0, -344573.50844120356 1356144.9687277474 0, -344589.813440057 1355739.2444343232 0, -344606.12744614785 1355333.2978831504 0, -345029.01590181206 1355350.5093214312 0, -345427.04025114607 1355366.7061175613 0, -345409.99986517086 1355772.6682895813 0)), ((-341266.51905991114 1362576.4876883903 0, -341250.1071516174 1362979.3196337237 0, -340851.5096170965 1362967.7698017969 0, -340867.9206153428 1362563.5825670965 0, -340884.3436855282 1362158.411502429 0, -341283.0262273813 1362171.040049678 0, -341266.51905991114 1362576.4876883903 0)), ((-339893.89626669866 1366573.1096507814 0, -339909.113563356 1366189.6168995781 0, -340315.9751982418 1366204.447412866 0, -340299.3923740316 1366589.8234169253 0, -339893.89626669866 1366573.1096507814 0)), ((-340368.3405678828 1374702.528704076 0, -340383.3609665003 1374301.988174039 0, -340781.81042570295 1374319.1638477154 0, -340766.6387609196 1374720.3144716925 0, -340751.3025726853 1375125.369039317 0, -340353.1187008209 1375107.6774550283 0, -340368.3405678828 1374702.528704076 0)), ((-344121.3756386842 1380144.0009456384 0, -344135.27865748905 1379738.469479155 0, -344529.7654317961 1379755.7259424091 0, -344513.069789827 1380161.2233191975 0, -344121.3756386842 1380144.0009456384 0)), ((-339711.29063051404 1381171.849157207 0, -339728.0619542611 1380766.0140956528 0, -339348.0450811503 1380744.6680040872 0, -339363.9110429375 1380344.8471468957 0, -339379.982923474 1379939.8381771157 0, -339759.14410311804 1379955.5046300765 0, -340157.6289554072 1379971.9343324383 0, -340556.09600387886 1379988.3596279428 0, -340937.16659181804 1380004.0425070876 0, -340922.0202294746 1380409.9732110247 0, -340906.25508266763 1380832.324753256 0, -340524.6781668231 1380810.83038884 0, -340508.2186719182 1381204.7142695847 0, -340109.7615425989 1381188.3342901908 0, -339711.29063051404 1381171.849157207 0)), ((-344878.1483756385 1380982.2527074562 0, -344894.4474772146 1380584.152432693 0, -345292.5188371152 1380601.6238125055 0, -345276.3043799941 1380999.6265122788 0, -344878.1483756385 1380982.2527074562 0)), ((-345585.0650542109 1382657.7432602337 0, -345569.8139299514 1383051.31048828 0, -345190.86118456634 1383034.750900587 0, -344793.20966751425 1383017.4985788283 0, -344809.74244653963 1382620.5215218433 0, -345207.52771767805 1382639.6053506676 0, -345585.0650542109 1382657.7432602337 0)), ((-345066.30847864936 1398408.6408999928 0, -344642.6851108595 1398393.219284141 0, -344658.7209222365 1397987.704672577 0, -345083.58321694814 1398003.8935036052 0, -345066.30847864936 1398408.6408999928 0)), ((-345465.684327352 1398423.1240414022 0, -345482.7879678646 1398019.0755668976 0, -345881.98345621413 1398034.2648332508 0, -345865.0684907993 1398437.6262531297 0, -345465.684327352 1398423.1240414022 0)), ((-341842.5295894404 1399088.3144151075 0, -341859.38069039135 1398682.0454870034 0, -341876.77152334526 1398278.2418595853 0, -342273.8355395169 1398295.2051671294 0, -342256.3478088118 1398700.9542483406 0, -342239.4476560443 1399105.2828931536 0, -341842.5295894404 1399088.3144151075 0)), ((-339808.46281444904 1400249.966519819 0, -339831.3228318947 1399820.6744445744 0, -339428.584161946 1399803.6299457243 0, -339445.6395202424 1399398.6323314465 0, -339462.7051056934 1398993.602721615 0, -339479.3587053041 1398598.7081489614 0, -339895.48909513635 1398615.7151477942 0, -340274.62398019526 1398627.0540899008 0, -340672.7063960766 1398638.9761529872 0, -340655.44109253195 1399041.0497994921 0, -340638.0911691787 1399445.6980949338 0, -340620.72515622806 1399850.526226411 0, -340603.04242367914 1400266.8938196686 0, -340205.32143577555 1400258.4149165906 0, -339808.46281444904 1400249.966519819 0)), ((-342636.35647675116 1399122.258260717 0, -342653.3135758737 1398719.8925664052 0, -343022.63075729815 1398737.5247592917 0, -343007.5354047162 1399138.3183066058 0, -342636.35647675116 1399122.258260717 0)), ((-341342.4916148999 1401092.897813271 0, -341355.93487557484 1400688.6261757205 0, -341774.6881077003 1400706.3601315005 0, -341757.1298013605 1401110.7695320407 0, -341342.4916148999 1401092.897813271 0)), ((-343247.7710604982 1403617.1635324513 0, -342838.1736146872 1403598.9131773629 0, -342850.2072338024 1403187.3505506825 0, -343264.9033698708 1403205.3353939906 0, -343247.7710604982 1403617.1635324513 0)), ((-339870.1649730208 1407922.203352726 0, -339888.49578716926 1407518.7671617086 0, -340286.26887479814 1407535.2120291828 0, -340304.36010001914 1407131.9580457902 0, -340702.33325170807 1407148.1382843032 0, -340684.32908456627 1407551.6644661804 0, -340666.31967764045 1407955.3260661766 0, -340268.1491926431 1407938.734904692 0, -339870.1649730208 1407922.203352726 0)), ((-342232.2456999183 1408415.8328396617 0, -342251.20168313495 1408024.69007037 0, -342633.0801790554 1408041.5033950997 0, -342613.661897842 1408433.2099763302 0, -342232.2456999183 1408415.8328396617 0)), ((-340229.9926343114 1408746.3575773109 0, -340249.8654157816 1408349.7480834918 0, -340648.3951632625 1408355.5189963714 0, -340628.2790211926 1408762.9195044443 0, -340229.9926343114 1408746.3575773109 0)), ((-341394.7861058384 1409200.480017132 0, -341414.75091705786 1408796.893348834 0, -341813.28227504826 1408814.7305489664 0, -341793.3769847323 1409218.1513685295 0, -341394.7861058384 1409200.480017132 0)), ((-340588.2051832871 1409570.8621599749 0, -340567.8395292777 1409983.4102936746 0, -340169.45275954565 1409968.7722235362 0, -340189.87556168414 1409554.7583447332 0, -340209.937477618 1409150.4679064595 0, -340608.24752550916 1409166.8624452765 0, -340588.2051832871 1409570.8621599749 0)), ((-340943.757611454 1409997.246302414 0, -340964.34459648543 1409585.9061182565 0, -341374.8313825132 1409604.0458560777 0, -341354.31428205146 1410018.9740127448 0, -340943.757611454 1409997.246302414 0)), ((-341752.8456458819 1410040.0823027717 0, -341773.4733260696 1409621.5397792314 0, -342172.1233875785 1409639.0527147471 0, -342151.35741088085 1410061.2197270521 0, -341752.8456458819 1410040.0823027717 0)), ((-341295.6899582391 1411217.1830032198 0, -341315.42150696437 1410813.9956491112 0, -341714.2326547699 1410831.0027304366 0, -341694.57000477024 1411234.013420732 0, -341295.6899582391 1411217.1830032198 0)), ((-340857.5851405858 1412005.3255519627 0, -340875.57805844577 1411598.211593418 0, -341276.01546856196 1411619.3991900957 0, -341256.39696708706 1412022.2461524508 0, -340857.5851405858 1412005.3255519627 0)), ((-342017.12861457776 1412860.9707734026 0, -342036.0396851789 1412458.5640298661 0, -342054.9335399395 1412056.146478906 0, -342451.05728952045 1412072.9368059956 0, -342432.1348355964 1412475.5994607469 0, -342413.2125393507 1412878.2632718477 0, -342017.12861457776 1412860.9707734026 0)), ((-342288.46965569444 1415299.557578831 0, -342309.6265927482 1414907.5537957386 0, -342728.69513802195 1414925.7662906835 0, -342708.0364654197 1415318.7310265675 0, -342288.46965569444 1415299.557578831 0)), ((-341093.84846998606 1415649.51457269 0, -341112.626062274 1415246.0966882883 0, -341511.60121303174 1415264.3413924437 0, -341492.1317843788 1415667.5297177257 0, -341472.6461528557 1416070.6849413887 0, -341075.0713863812 1416052.9225069566 0, -341093.84846998606 1415649.51457269 0)), ((-341890.3967321589 1415685.551496792 0, -341910.5846393012 1415282.5938803065 0, -342288.46965569444 1415299.557578831 0, -342266.73286666913 1415702.206168663 0, -341890.3967321589 1415685.551496792 0)), ((-342245.00545663363 1416104.8564021925 0, -342266.73286666913 1415702.206168663 0, -342686.96553434426 1415721.5069476827 0, -342665.89542482805 1416124.2729297816 0, -342245.00545663363 1416104.8564021925 0)), ((-341453.4935543765 1416465.7646827723 0, -341472.6461528557 1416070.6849413887 0, -341870.2283866334 1416088.4774484204 0, -341850.4493658072 1416481.2684777866 0, -341453.4935543765 1416465.7646827723 0)), ((-344235.4406224039 1416606.5112660357 0, -344257.56470035476 1416197.064708848 0, -344654.9743995496 1416215.7649027384 0, -344632.3928176994 1416631.1649907243 0, -344612.01726633956 1417021.3320227156 0, -344214.61608383316 1417002.6886667702 0, -344235.4406224039 1416606.5112660357 0)), ((-345231.2792150368 1420689.7486846386 0, -345249.0465732472 1420285.1113357048 0, -345653.73384955747 1420304.5646276753 0, -345636.7558976912 1420709.6036824018 0, -345231.2792150368 1420689.7486846386 0)), ((-343993.1292071387 1421853.642363438 0, -344010.39866362844 1421447.9391295684 0, -344408.6583404756 1421461.058222714 0, -344391.4430687855 1421870.4949712337 0, -343993.1292071387 1421853.642363438 0)), ((-343958.61173849425 1422664.7505184505 0, -343975.8657560828 1422259.2012829315 0, -344374.3768456535 1422275.8041104088 0, -344357.3022249994 1422681.1028981893 0, -343958.61173849425 1422664.7505184505 0)), ((-344739.1851728616 1423101.003025634 0, -344756.0012790888 1422697.4631436786 0, -345146.5099317879 1422713.4986350536 0, -345130.2000715515 1423115.591044668 0, -344739.1851728616 1423101.003025634 0)), ((-341226.3356192942 1431053.7071600927 0, -341242.08306449116 1430652.4771845983 0, -341620.11884193955 1430669.6354140968 0, -341605.2708941855 1431072.9971029009 0, -341226.3356192942 1431053.7071600927 0)), ((-340213.1564386973 1435396.5121018137 0, -340231.0214376499 1434990.3793355639 0, -339828.2895830553 1434975.5258258528 0, -339757.6919452463 1434640.0977227513 0, -339691.0554744319 1434563.975529186 0, -339850.4455809276 1434569.74501426 0, -340248.8812272845 1434584.1578984833 0, -340605.5225451439 1434597.507583827 0, -340592.9295309687 1435004.1306148195 0, -340580.33605210437 1435410.7548076266 0, -340213.1564386973 1435396.5121018137 0)), ((-343312.3659997066 1438333.0040433246 0, -342912.0090136283 1438322.4981403698 0, -342926.83478493 1437915.3837327522 0, -343326.973428204 1437925.7910365951 0, </t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Oklahoma State University, University of Oklahoma, Common Schools, Greer 33, State Educational Institutions, University Preparatory, Normal Schools, Langston University, Wildlife Conservation, University Hospitals Authority &amp; Trust, Redlands Community College</t>
+          <t>Oklahoma State University, University of Oklahoma, State Educational Institutions, Common Schools, Greer 33, University Preparatory, Normal Schools, Langston University, Redlands Community College</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1978</v>
+        <v>1970</v>
       </c>
       <c r="G10" t="n">
         <v>8928.620000000001</v>
@@ -915,13 +915,13 @@
         <v>235</v>
       </c>
       <c r="I10" t="n">
-        <v>67019.86</v>
+        <v>66702.03</v>
       </c>
       <c r="J10" t="n">
-        <v>1743</v>
+        <v>1735</v>
       </c>
       <c r="K10" t="n">
-        <v>75948.48</v>
+        <v>75630.64999999999</v>
       </c>
       <c r="L10" t="n">
         <v>5232808.01</v>
@@ -930,7 +930,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-175943.71283896 1212106.3037297826 0, -175935.79532105886 1212512.5733073968 0, -175536.08848253996 1212504.426624654 0, -175544.1594031835 1212098.271906859 0, -175943.71283896 1212106.3037297826 0)), ((-181700.78384793104 1285368.4640731735 0, -181692.73354630606 1285774.2279579418 0, -181298.48571137796 1285765.2698804617 0, -181307.22258078412 1285359.29660042 0, -181700.78384793104 1285368.4640731735 0)), ((-177519.82736241954 1295447.3905718534 0, -177120.1367204274 1295438.2893821509 0, -177131.22501268188 1295032.2023772858 0, -177142.19103232567 1294630.7681567878 0, -177537.56031274592 1294641.872728787 0, -177528.77445184242 1295041.1478030116 0, -177519.82736241954 1295447.3905718534 0)), ((-166711.9329116557 1297668.1456837556 0, -166312.31739866122 1297660.4392632516 0, -165911.04839525977 1297652.7195881458 0, -165904.20617210446 1298044.3488438388 0, -165504.3948566682 1298035.948586059 0, -165512.93539193086 1297642.942385881 0, -165521.87973214872 1297223.1748894467 0, -165919.4957754316 1297231.4547340714 0, -165927.6366133453 1296825.1985452406 0, -166329.91634444712 1296833.8550246235 0, -166729.3168636199 1296842.441181488 0, -167128.7169466071 1296851.04570791 0, -167120.2446458109 1297257.4296628565 0, -166720.74608208291 1297248.7784411104 0, -166711.9329116557 1297668.1456837556 0)), ((-181415.31756465684 1299184.0383990002 0, -181016.3042165501 1299175.8301672598 0, -180617.19971178332 1299167.6385792592 0, -180626.03963073913 1298762.7777868316 0, -181025.05565840437 1298770.8780416844 0, -181424.01732632934 1298778.9732833093 0, -181415.31756465684 1299184.0383990002 0)), ((-169830.76779149592 1301383.450634181 0, -169838.87213207252 1300990.8478482347 0, -170237.6983258694 1301006.994852677 0, -170229.76076715748 1301392.0606305823 0, -170221.13594984202 1301798.1692645918 0, -170212.52524437272 1302204.0225707788 0, -169813.65865044043 1302195.0572226327 0, -169822.21204499074 1301789.3146728901 0, -169423.0069198787 1301780.4394204812 0, -169431.524140447 1301374.652920801 0, -169830.76779149592 1301383.450634181 0)), ((-169788.86160126817 1303413.6650749452 0, -169389.98181696117 1303404.9978022866 0, -168981.86264853785 1303396.1232943535 0, -168591.80600117214 1303387.5874084446 0, -168600.10481799682 1302981.7566239857 0, -168200.82677309972 1302972.9802964502 0, -168208.99494014232 1302574.2862726857 0, -168608.2576082851 1302582.9392895256 0, -169000.36669939946 1302591.4706914916 0, -169406.24505310657 1302599.865100548 0, -169800.97622297762 1302608.048108155 0, -169804.97027133533 1302608.1267051154 0, -170203.7767726697 1302616.4082887543 0, -170195.8283428422 1303016.3147130327 0, -170187.74171083848 1303422.3061118794 0, -169788.86160126817 1303413.6650749452 0)), ((-170942.24319836902 1304268.5136714405 0, -170530.3995460436 1304260.3640199222 0, -170540.21671339264 1303836.1115285608 0, -170549.60967512644 1303430.1220329597 0, -170959.66042125976 1303438.6502908848 0, -170968.20262940569 1303032.578499056 0, -170976.60806430024 1302632.5022333097 0, -171375.94893308158 1302640.848620011 0, -171367.5551198576 1303040.7796541722 0, -171359.01996390708 1303446.918691137 0, -171350.5038038494 1303853.0148543965 0, -171341.625637845 1304276.4355201125 0, -170942.24319836902 1304268.5136714405 0)), ((-172890.40280191824 1306729.3321700757 0, -172881.9206606126 1307135.4190319115 0, -172481.66521688006 1307127.3276678263 0, -172490.10260625373 1306721.1728267525 0, -172890.40280191824 1306729.3321700757 0)), ((-173247.37758807736 1308767.6725587486 0, -172847.28258171518 1308759.4206617458 0, -172855.9976194669 1308353.477750135 0, -173256.1402540953 1308361.652404969 0, -173654.8311616236 1308369.8163153199 0, -173646.65608828366 1308775.915436199 0, -173247.37758807736 1308767.6725587486 0)), ((-177427.57266913127 1313615.4914161863 0, -177436.69472270043 1313208.4093691164 0, -177445.82652484815 1312801.2955308848 0, -177454.65771123077 1312407.4694556496 0, -177562.54396094198 1312409.8252800247 0, -177853.48931695626 1312416.192000791 0, -177961.87395196344 1312418.5742428903 0, -178252.17528498083 1312424.9412420623 0, -178243.3729212048 1312816.485219252 0, -178234.23457366994 1313223.8448711818 0, -178225.08817224612 1313631.161178124 0, -177826.34851557473 1313623.328654295 0, -177427.57266913127 1313615.4914161863 0)), ((-166214.51319871837 1315431.8296019 0, -166206.37969640837 1315842.3437449534 0, -166198.35842515825 1316248.4532250927 0, -166190.31929299276 1316654.5526442274 0, -165786.2170489032 1316647.2833973987 0, -165391.71779996052 1316641.3250859359 0, -165399.70927637056 1316235.2805723276 0, -165407.69195749695 1315829.215078176 0, -165415.85381046106 1315414.7627328401 0, -165815.98861440568 1315422.4520768158 0, -166214.51319871837 1315431.8296019 0)), ((-175318.52035623518 1318461.9104561047 0, -175309.29431087075 1318864.5461170557 0, -174922.10745709657 1318859.6074760954 0, -174522.5874871394 1318854.53708477 0, -174531.10492345627 1318446.1355614138 0, -174131.74327217424 1318438.1328185203 0, -174140.35635534214 1318031.234057544 0, -174148.9700038597 1317624.3144026555 0, -174157.4860605784 1317222.2169809998 0, -174556.4852565153 1317229.865680886 0, -174955.48408520847 1317237.532768946 0, -174947.20538393813 1317639.937023618 0, -174938.82184958446 1318047.0626794752 0, -174930.45683278897 1318454.167801143 0, -175318.52035623518 1318461.9104561047 0)), ((-179669.31573975112 1321407.2658184378 0, -179270.06716808988 1321399.3266712248 0, -179277.5681826787 1320991.924711194 0, -179676.56784325987 1321000.5412793288 0, -179669.31573975112 1321407.2658184378 0)), ((-173045.73774925352 1332652.892716459 0, -173037.65899207807 1333059.345837976 0, -172637.87555580688 1333051.2121156424 0, -172238.09174489122 1333043.0971236012 0, -172246.46689737157 1332636.6723558058 0, -172646.10682314547 1332644.7845589102 0, -172654.33919258622 1332238.30245773 0, -172254.84250905522 1332230.22673438 0, -172263.1550242012 1331827.3847325481 0, -172662.5084145642 1331834.9652462706 0, -173061.85206936652 1331842.5753031168 0, -173469.39190715915 1331850.357938232 0, -173462.94802872138 1332254.6699356202 0, -173053.82589179816 1332246.4189196844 0, -173045.73774925352 1332652.892716459 0)), ((-171789.32883007283 1335069.6679535052 0, -171399.80857682804 1335060.6311684356 0, -171407.60770866153 1334652.1619048263 0, -171800.28550075658 1334660.3106362945 0, -171789.32883007283 1335069.6679535052 0)), ((-171399.80857682804 1335060.6311684356 0, -171391.1730348959 1335464.7652869667 0, -170992.67448215908 1335456.406894264 0, -171001.77857086583 1335051.4203000162 0, -171399.80857682804 1335060.6311684356 0)), ((-168603.86251440516 1335815.838597261 0, -168209.1341206244 1335808.5334665133 0, -168215.45309209675 1335402.3490952235 0, -168613.2118206783 1335409.6912505527 0, -168603.86251440516 1335815.838597261 0)), ((-174149.02501426663 1337148.257244764 0, -173749.01359806658 1337139.2799883648 0, -173757.98255604412 1336734.0501666393 0, -174157.97685709526 1336743.0158799295 0, -174149.02501426663 1337148.257244764 0)), ((-174531.09440898293 1337969.9777784895 0, -174131.0607312339 1337960.8471441225 0, -174140.0333637393 1337554.5737474703 0, -174149.02501426663 1337148.257244764 0, -174549.02667559774 1337157.2642293086 0, -174540.06945298254 1337563.6260234802 0, -174531.09440898293 1337969.9777784895 0)), ((-166531.05064138706 1340245.2043401864 0, -166131.48671424444 1340237.6843571982 0, -166138.57701623806 1339844.3025036508 0, -166538.26030580953 1339850.3363781278 0, -166531.05064138706 1340245.2043401864 0)), ((-177924.32001138572 1352651.4520921558 0, -177531.66751574012 1352643.1299813164 0, -177539.60728712505 1352236.7057207413 0, -177547.53728480323 1351830.3162388531 0, -177933.60306564363 1351838.4570458084 0, -177928.96633726385 1352244.948328299 0, -177924.32001138572 1352651.4520921558 0)), ((-172727.89095030742 1353358.0248979128 0, -172329.01525733987 1353349.9045962747 0, -172337.3779199937 1352938.0577529087 0, -172736.2019338599 1352945.66220058 0, -172727.89095030742 1353358.0248979128 0)), ((-171896.72846093695 1354964.9050773887 0, -171888.29363013318 1355370.5005559528 0, -171482.97650396972 1355361.9976007862 0, -171492.4556019558 1354956.4789137857 0, -171896.72846093695 1354964.9050773887 0)), ((-172279.20231218045 1355784.4996053241 0, -171879.84082857828 1355776.0970254324 0, -171888.29363013318 1355370.5005559528 0, -172287.566444225 1355378.867745847 0, -172279.20231218045 1355784.4996053241 0)), ((-169835.47313990362 1358576.5516512757 0, -169443.92142799436 1358569.522864897 0, -169450.53675244324 1358164.0320933273 0, -169838.02849845815 1358171.081165173 0, -169835.47313990362 1358576.5516512757 0)), ((-180176.51978652005 1360002.6721153068 0, -180167.2158318822 1360408.8637633454 0, -179767.77191739547 1360400.9719492304 0, -179776.79150236165 1359995.3899140768 0, -180176.51978652005 1360002.6721153068 0)), ((-168595.28370776202 1361394.442381945 0, -168227.56071239134 1361388.024900765 0, -168235.52634394265 1360982.193007978 0, -168603.56927655888 1360990.6539787045 0, -168595.28370776202 1361394.442381945 0)), ((-168570.11374468 1362621.7380692349 0, -168203.45499178141 1362616.158706952 0, -168211.63592106712 1362199.3572157256 0, -168578.6216929984 1362205.7265712805 0, -168570.11374468 1362621.7380692349 0)), ((-174913.7308303282 1363548.545377046 0, -174904.9750124603 1363954.514866465 0, -174504.31655040843 1363947.3328408299 0, -174513.6202447151 1363541.4192655685 0, -174913.7308303282 1363548.545377046 0)), ((-174099.36983850287 1364353.093090298 0, -173701.08528966803 1364346.7352481862 0, -173709.4643063541 1363932.0925851122 0, -174107.86810484927 1363939.740122899 0, -174099.36983850287 1364353.093090298 0)), ((-153215.0175010142 1242969.5947690236 0, -153615.9754351269 1242977.2900949293 0, -153623.67599931773 1242571.6961415 0, -154027.01343899211 1242579.2845108828 0, -154019.46488250766 1242985.0376654444 0, -154011.91058188947 1243390.6024957732 0, -153608.3501508337 1243382.7641784525 0, -153207.30286158103 1243374.9778435475 0, -153215.0175010142 1242969.5947690236 0)), ((-162817.3801144094 1243150.7745979107 0, -163217.3973464473 1243158.3154715241 0, -163610.46730043937 1243165.7774644892 0, -163604.55339088276 1243571.552269511 0, -163209.83851955028 1243564.0593338464 0, -162809.82194226366 1243556.507319417 0, -162817.3801144094 1243150.7745979107 0)), ((-160359.9012970106 1245537.615322755 0, -159977.59192745638 1245530.5638024416 0, -159576.8692091762 1245523.191895592 0, -159584.70338458187 1245121.1926338114 0, -159985.33124037087 1245128.7641475056 0, -160369.0641162158 1245135.920217078 0, -160359.9012970106 1245537.615322755 0)), ((-152216.75322093457 1253910.4537251112 0, -152206.5273128618 1254315.335269746 0, -151838.45177776896 1254308.819883611 0, -151845.02504084533 1253903.4827835227 0, -152216.75322093457 1253910.4537251112 0)), ((-152186.14304921476 1255122.3428848654 0, -151825.30817169257 1255118.7947019294 0, -151831.87700120764 1254714.2368156444 0, -152196.301943496 1254720.207436628 0, -152186.14304921476 1255122.3428848654 0)), ((-157983.34755768956 1295853.4281711378 0, -158382.07729223545 1295864.140621129 0, -158780.08882858077 1295874.8583381465 0, -158772.30953818254 1296274.3055458148 0, -158374.23212556896 1296266.2044292989 0, -157975.9459392016 1296258.084232003 0, -157983.34755768956 1295853.4281711378 0)), ((-163653.1310199901 1310997.8152320355 0, -163660.8818023161 1310589.3479996864 0, -163668.55099643348 1310186.139380371 0, -164086.80746085395 1310193.942777795 0, -164084.25042091103 1310598.7478604529 0, -164072.11903125813 1311006.1023095907 0, -163653.1310199901 1310997.8152320355 0)), ((-162550.2254389613 1319032.015734088 0, -162148.42503825494 1319026.5475952884 0, -162157.15575879705 1318615.091773267 0, -162165.33965226883 1318214.4025009258 0, -162565.8519518942 1318220.0142986386 0, -162556.95352377798 1318619.63827458 0, -162550.2254389613 1319032.015734088 0)), ((-152932.92099863235 1320085.8918196873 0, -153341.3310235734 1320093.151814407 0, -153740.88985343307 1320100.273132569 0, -153734.664098569 1320502.4828813542 0, -153334.88262986054 1320497.7072252622 0, -152930.5616179454 1320492.9366910174 0, -152932.92099863235 1320085.8918196873 0)), ((-153328.39216819522 1320904.1207910858 0, -153321.89951349344 1321310.1443134542 0, -152925.85277630598 1321305.3639816998 0, -152928.20413718335 1320899.3341226527 0, -153328.39216819522 1320904.1207910858 0)), ((-154093.20713756562 1322946.9156327373 0, -153692.85484692265 1322940.3543913355 0, -153700.4999713324 1322533.763593273 0, -154100.86046577114 1322540.4145138732 0, -154093.20713756562 1322946.9156327373 0)), ((-154839.5692750221 1325806.973036847 0, -155240.35054086844 1325815.5672947324 0, -155232.82127561062 1326222.1049964302 0, -155225.2855029517 1326629.505836762 0, -154824.51335926063 1326621.0011945614 0, -154832.04185527054 1326213.4548934444 0, -154429.2343154817 1326204.775760451 0, -154435.82736405553 1325798.333135726 0, -154839.5692750221 1325806.973036847 0)), ((-159230.52179247924 1327104.1398283392 0, -159217.77822971952 1327511.6486867382 0, -158814.24570231294 1327504.9214155392 0, -158821.70056296527 1327097.404303562 0, -159230.52179247924 1327104.1398283392 0)), ((-159606.72725558787 1327926.933928233 0, -159614.3708805533 1327519.586606882 0, -159622.00504865064 1327112.2519599325 0, -160021.47804103562 1327120.6645602852 0, -160013.71421555907 1327527.6163674663 0, -160005.94011452116 1327934.6366322683 0, -159606.72725558787 1327926.933928233 0)), ((-147216.60607805848 1328940.5430697792 0, -147209.4665911311 1329346.777728987 0, -146809.073429069 1329340.7545623088 0, -146816.43162154453 1328934.3892698882 0, -147216.60607805848 1328940.5430697792 0)), ((-160374.6998251148 1329569.3442793237 0, -159975.65580557435 1329561.491869007 0, -159983.16438059925 1329154.760077558 0, -160382.17750341076 1329162.3657044237 0, -160374.6998251148 1329569.3442793237 0)), ((-150346.34284573808 1332643.7158480035 0, -150352.85367283705 1332237.5702835622 0, -150359.3592450211 1331831.20224705 0, -150365.98700833853 1331416.2884148022 0, -150764.7965045753 1331421.097169029 0, -150758.22027965143 1331837.1309649998 0, -150751.774090154 1332243.164365835 0, -151126.35902318076 1332248.3941068486 0, -151119.2312503611 1332654.0924993681 0, -150745.33875430524 1332649.0874178354 0, -150346.34284573808 1332643.7158480035 0)), ((-147940.26375886716 1333007.6192090078 0, -147547.11485829687 1333003.7983143027 0, -147553.7576516025 1332602.823734389 0, -147947.11979710546 1332608.9982825897 0, -147940.26375886716 1333007.6192090078 0)), ((-154678.532832025 1335157.084999092 0, -154272.21939837653 1335148.8683594975 0, -154278.12002236737 1334742.8480410725 0, -154686.01566518855 1334750.1755503293 0, -154678.532832025 1335157.084999092 0)), ((-155469.3755933252 1335579.780797964 0, -155462.0267408171 1335986.1920075733 0, -155062.80131452228 1335977.8079761812 0, -155070.21021053058 1335571.5321538919 0, -155469.3755933252 1335579.780797964 0)), ((-154254.50936181424 1336366.3332816497 0, -153856.85964110345 1336360.8980306394 0, -153864.4003283596 1335954.7014575093 0, -154260.40602981093 1335961.0583532727 0, -154254.50936181424 1336366.3332816497 0)), ((-155055.45901774327 1336379.8899300178 0, -154656.13266013938 1336373.1229481855 0, -154663.56621552716 1335969.453571963 0, -155062.80131452228 1335977.8079761812 0, -155055.45901774327 1336379.8899300178 0)), ((-155843.92925139275 1336393.3173925595 0, -155839.2255570788 1336807.4566159938 0, -155447.08402105645 1336799.059216686 0, -155454.78483779175 1336386.6866166233 0, -155843.92925139275 1336393.3173925595 0)), ((-153427.18060698203 1337972.0459149135 0, -153028.06810671612 1337966.6552639122 0, -153035.2195628425 1337567.999827459 0, -153434.52511141027 1337574.2557381268 0, -153833.83052199156 1337580.5189529632 0, -153826.3018018914 1337977.466547696 0, -153427.18060698203 1337972.0459149135 0)), ((-153826.3018018914 1337977.466547696 0, -154219.98951167185 1337982.8193956506 0, -154213.91534702264 1338399.9944404592 0, -153818.76080926618 1338393.7983247596 0, -153826.3018018914 1337977.466547696 0)), ((-155009.1547133005 1338822.911460389 0, -154609.76684636995 1338814.834079961 0, -154617.36113392762 1338408.2492493305 0, -155016.89196970733 1338416.4747248052 0, -155009.1547133005 1338822.911460389 0)), ((-156206.19136721594 1338845.9476902375 0, -155807.17068206743 1338839.0747537075 0, -155816.26017470998 1338432.9534301544 0, -156214.01723597976 1338439.7476310013 0, -156206.19136721594 1338845.9476902375 0)), ((-156198.35672434646 1339252.137990731 0, -156190.6354712538 1339653.0830245882 0, -155789.13589395312 1339645.3705042982 0, -155798.09022928137 1339245.1976703575 0, -156198.35672434646 1339252.137990731 0)), ((-147831.51555332803 1340333.865928966 0, -147419.90795926438 1340327.9033265659 0, -147427.86958277982 1339921.7328666248 0, -147839.54300877076 1339927.6293664617 0, -147831.51555332803 1340333.865928966 0)), ((-163667.65051926434 1344670.7142616373 0, -163254.24097146775 1344662.8477049796 0, -163262.35052098683 1344249.0671734721 0, -163674.82578318458 1344256.7369317363 0, -163667.65051926434 1344670.7142616373 0)), ((-152101.23189219472 1344868.142414273 0, -151702.14957268618 1344861.3868170383 0, -151303.04867891027 1344854.6606295847 0, -151310.6510733763 1344439.5037653856 0, -151709.62548874057 1344450.391082684 0, -152108.62637045985 1344461.2974167615 0, -152101.23189219472 1344868.142414273 0)), ((-162433.4104174998 1345858.263872705 0, -162041.7395721198 1345851.0783356146 0, -162048.0286997655 1345445.0152543068 0, -162441.632219718 1345452.2707738655 0, -162433.4104174998 1345858.263872705 0)), ((-152056.34573203544 1347306.4130121074 0, -152048.8935703995 1347705.2982626064 0, -151649.8222583555 1347698.2407525964 0, -151657.2479042241 1347300.3174988267 0, -152056.34573203544 1347306.4130121074 0)), ((-154837.31606037813 1348165.9023316095 0, -154438.93645708536 1348158.6151754947 0, -154446.6596687272 1347749.8620370426 0, -154844.85458771526 1347760.4363562535 0, -154837.31606037813 1348165.9023316095 0)), ((-155228.24129324564 1348579.4602952788 0, -154829.77068477182 1348572.2537974995 0, -154837.31606037813 1348165.9023316095 0, -155235.6956106203 1348173.1967511538 0, -155228.24129324564 1348579.4602952788 0)), ((-154431.27309903636 1348565.0429208998 0, -154423.61023557428 1348971.4496555608 0, -154019.48736618 1348964.2122469456 0, -154027.4845532631 1348557.7331650024 0, -154431.27309903636 1348565.0429208998 0)), ((-155612.44293623764 1348992.6477535865 0, -155220.7963930565 1348985.70310651 0, -155228.24129324564 1348579.4602952788 0, -155622.23405740855 1348586.548243629 0, -155612.44293623764 1348992.6477535865 0)), ((-149244.3618468017 1349702.683281918 0, -148849.7489068089 1349696.0780549971 0, -148856.9858320523 1349280.7855524893 0, -149250.50807761765 1349288.893930589 0, -149244.3618468017 1349702.683281918 0)), ((-156408.9365036002 1349407.7381076575 0, -156401.66776029047 1349817.557229275 0, -156003.25455303933 1349811.3034675561 0, -156010.51852226187 1349402.1893399984 0, -156408.9365036002 1349407.7381076575 0)), ((-149639.7934934366 1350115.0934686544 0, -149238.3350083157 1350108.5633078576 0, -149244.3618468017 1349702.683281918 0, -149646.87073823885 1349709.1086215752 0, -149639.7934934366 1350115.0934686544 0)), ((-155585.15069978265 1350210.7910502413 0, -155198.8488123306 1350203.9991811563 0, -155206.10020083666 1349797.972603298 0, -155593.90091683116 1349804.7916059187 0, -155585.15069978265 1350210.7910502413 0)), ((-149639.7934934366 1350115.0934686544 0, -150038.50739124487 1350121.5944305244 0, -150031.50275469752 1350527.5148864177 0, -149632.81768050426 1350520.9583980623 0, -149639.7934934366 1350115.0934686544 0)), ((-155184.54669782813 1350997.656169277 0, -154789.398449124 1350992.4790538661 0, -154794.5060017364 1350602.0409136314 0, -155195.37636356743 1350613.2084270788 0, -155184.54669782813 1350997.656169277 0)), ((-155198.63116829252 1352222.2248564686 0, -155206.1772473879 1351815.9726843506 0, -155596.63651353068 1351822.9982890885 0, -156003.9188370007 1351829.877387308 0, -155996.4987495789 1352236.0535013853 0, -155591.69786506644 1352229.3201215023 0, -155198.63116829252 1352222.2248564686 0)), ((-157593.08784688235 1352262.953108527 0, -157189.16517546648 1352256.0708515148 0, -156795.0157294149 1352249.4310476887 0, -156802.24397557 1351843.4752076555 0, -157195.56205515377 1351850.1894254172 0, -157600.17852866193 1351857.2074340805 0, -157593.08784688235 1352262.953108527 0)), ((-152802.86055196647 1352572.748382288 0, -152795.68063321002 1352991.679811784 0, -152393.38345242525 1352984.402580458 0, -152397.6431043266 1352565.117169408 0, -152802.86055196647 1352572.748382288 0)), ((-157174.28696595167 1353068.2698622567 0, -156780.58934995392 1353061.671794447 0, -156787.871183984 1352652.2893103384 0, -157182.7743720142 1352661.6180000193 0, -157586.02288138567 1352667.3014826218 0, -157578.7242227329 1353075.0272221325 0, -157174.28696595167 1353068.2698622567 0)), ((-157165.80511167276 1353474.6209384834 0, -157157.3228821247 1353880.9958755823 0, -156766.15742719386 1353874.2091516515 0, -156773.373311206 1353467.9453401759 0, -157165.80511167276 1353474.6209384834 0)), ((-153966.08582144798 1353826.3144078031 0, -153960.36854565542 1354218.8505520849 0, -153569.98322517873 1354211.8540566787 0, -153576.7454523844 1353818.944907566 0, -153966.08582144798 1353826.3144078031 0)), ((-155960.04629387095 1354257.6206781897 0, -155952.6439078706 1354672.2560051081 0, -155541.35849916993 1354665.1363230979 0, -155546.44924047423 1354247.4594699736 0, -155960.04629387095 1354257.6206781897 0)), ((-156359.5229409861 1354267.4661267216 0, -156759.01726149913 1354277.3192752271 0, -156751.63432391797 1354686.3026390863 0, -156352.14353495612 1354679.281290819 0, -156359.5229409861 1354267.4661267216 0)), ((-156295.14384288268 1357926.2296338114 0, -155896.26341427167 1357919.786561152 0, -155903.17504087288 1357523.7727790687 0, -156302.17417032074 1357530.162059324 0, -156295.14384288268 1357926.2296338114 0)), ((-159088.34330247532 1357973.646932964 0, -158718.66444835864 1357966.4845812207 0, -158725.53052986585 1357578.0366991628 0, -159094.9096434183 1357583.290563462 0, -159088.34330247532 1357973.646932964 0)), ((-153927.54773803763 1357888.1095035025 0, -153921.628849752 1358294.205226988 0, -153497.46541507126 1358286.5579619068 0, -153504.6450566326 1357880.473668274 0, -153927.54773803763 1357888.1095035025 0)), ((-156686.7181276296 1358338.3809343532 0, -156287.93741160425 1358331.9547787134 0, -156295.14384288268 1357926.2296338114 0, -156694.02406843836 1357932.6912303197 0, -156686.7181276296 1358338.3809343532 0)), ((-147117.43157852665 1358582.3374349228 0, -146718.79077246223 1358575.7544239631 0, -146320.14053286315 1358569.2009492368 0, -146327.0534902763 1358163.5458822388 0, -146725.7316913923 1358170.0999134446 0, -147124.40962667338 1358176.672463058 0, -147117.43157852665 1358582.3374349228 0)), ((-147542.9253715189 1358589.0987587327 0, -147538.5978381123 1359004.1679376068 0, -147110.30092198015 1358996.373509068 0, -147117.43157852665 1358582.3374349228 0, -147542.9253715189 1358589.0987587327 0)), ((-149121.4605762462 1359834.1038132894 0, -149116.80190434528 1360239.8701716722 0, -148687.4866014962 1360232.403753368 0, -148288.84240719103 1360225.1757654941 0, -148294.84831593322 1359819.5558019162 0, -148300.85253878497 1359414.0267659102 0, -148306.7633879843 1359014.933385587 0, -148705.6722404669 1359020.554306121 0, -149130.73489886665 1359026.558987703 0, -149126.11824317276 1359428.3834874744 0, -149121.4605762462 1359834.1038132894 0)), ((-147098.5899586273 1359798.817022618 0, -146699.90422644696 1359792.3788411694 0, -146705.877141481 1359386.893891728 0, -147104.52635541573 1359393.4098595302 0, -147098.5899586273 1359798.817022618 0)), ((-137345.52076110264 1234567.930088222 0, -137338.98380080552 1234973.945429173 0, -136939.11983145314 1234966.8112361876 0, -136945.572516736 1234560.8953305294 0, -137345.52076110264 1234567.930088222 0)), ((-137732.19155236293 1235389.29187156 0, -137332.37907850774 1235384.254182857 0, -137338.98380080552 1234973.945429173 0, -137738.85495487796 1234981.0968554765 0, -137732.19155236293 1235389.29187156 0)), ((-146004.95270369758 1244464.298553648 0, -145605.57868785976 1244458.1538807123 0, -145612.44363430905 1244052.4161532205 0, -146012.81103504924 1244058.7675813201 0, -146004.95270369758 1244464.298553648 0)), ((-128770.17265130593 1245387.9655853468 0, -129169.46761859793 1245393.5263106502 0, -129163.34686924885 1245799.6421268254 0, -128763.95134848665 1245794.1135002414 0, -128770.17265130593 1245387.9655853468 0)), ((-140779.7429531961 1270345.7012183582 0, -140377.93219366448 1270339.192467016 0, -140384.5308523573 1269932.69079566 0, -140785.66373684147 1269938.8866375468 0, -140779.7429531961 1270345.7012183582 0)), ((-129122.61563460238 1278694.7199382484 0, -128723.53329968442 1278688.2169841693 0, -128729.38828536043 1278282.326534239 0, -129128.53531133535 1278288.796981107 0, -129122.61563460238 1278694.7199382484 0)), ((-145252.20096160527 1282216.197520876 0, -145215.58625032182 1282215.7239599524 0, -145205.75055320252 1282627.1191624103 0, -144623.43420937622 1282612.792210075 0, -144628.6590024141 1282207.9544320994 0, -144628.49701549913 1282207.952264684 0, -144629.19479837845 1282166.438826393 0, -144631.24020497318 1282007.9525753856 0, -144426.22189661642 1282005.5134918517 0, -144433.54119046146 1281801.1314159958 0, -144635.3115773361 1281802.531179298 0, -144635.3165924723 1281802.2328120647 0, -144635.65947211778 1281802.237400236 0, -144640.33425885698 1281602.4275720576 0, -143818.28457170606 1281591.6801632915 0, -143841.9575044904 1280168.3065773223 0, -145449.22263697928 1280189.2587877952 0, -145414.09446047482 1282220.02749221 0, -145252.20096160527 1282216.197520876 0)), ((-129037.42694387684 1284778.8946705274 0, -128637.65499772798 1284772.1917113666 0, -128643.29451767255 1284366.128022969 0, -129042.9674064857 1284372.8071368106 0, -129037.42694387684 1284778.8946705274 0)), ((-126614.50808183597 1286364.3077194658 0, -126192.1874438171 1286357.6553052745 0, -126199.49465913615 1285951.698787946 0, -126206.85838485227 1285542.501059177 0, -126626.13762203927 1285547.7221436817 0, -126620.28940837563 1285958.2953769616 0, -126614.50808183597 1286364.3077194658 0)), ((-134537.91641483316 1289343.6235207387 0, -134130.60135332463 1289335.3606228917 0, -134134.82259705357 1288926.7964526922 0, -134544.2962866867 1288933.1577272648 0, -134537.91641483316 1289343.6235207387 0)), ((-134937.2935306726 1289351.826463831 0, -134930.9557333717 1289757.7977986427 0, -134531.60007962736 1289749.4162629638 0, -134537.91641483316 1289343.6235207387 0, -134937.2935306726 1289351.826463831 0)), ((-134525.28414022498 1290155.188314266 0, -134122.2044262647 1290146.5885801543 0, -134126.39847725205 1289740.9736664027 0, -134531.60007962736 1289749.4162629638 0, -134525.28414022498 1290155.188314266 0)), ((-134079.6883778616 1292572.3127820236 0, -133688.64116096977 1292565.9094625292 0, -133695.05577487996 1292149.5697654448 0, -134084.77668025435 1292151.8585555125 0, -134079.6883778616 1292572.3127820236 0)), ((-133688.64116096977 1292565.9094625292 0, -133682.32739647356 1292971.6145047047 0, -133676.01402571143 1293377.2988434085 0, -133669.9228074871 1293768.6254107016 0, -133269.63777509658 1293762.444135176 0, -133275.9034998461 1293370.4156000693 0, -132875.79243836482 1293363.562027714 0, -132882.4169060993 1292958.2515840302 0, -133282.36778666414 1292964.9236646255 0, -133288.85076028825 1292559.4001895112 0, -133688.64116096977 1292565.9094625292 0)), ((-132105.7497757779 1293352.0049368362 0, -132099.3518351936 1293748.4277406142 0, -131700.38987692518 1293746.6908600759 0, -131706.7384877057 1293346.9337726904 0, -132105.7497757779 1293352.0049368362 0)), ((-132875.79243836482 1293363.562027714 0, -132869.36157527668 1293756.2816187704 0, -132462.34283650547 1293750.0343869794 0, -132469.72982872513 1293356.5799136753 0, -132875.79243836482 1293363.562027714 0)), ((-126873.31005762635 1296526.9378338892 0, -126474.05027020945 1296521.2193321225 0, -126479.65268876923 1296115.0633938138 0, -126878.96674273346 1296120.8386488124 0, -126873.31005762635 1296526.9378338892 0)), ((-146359.18168692812 1298476.2636290384 0, -145959.89247033958 1298468.433158988 0, -145966.6009965479 1298062.4459685492 0, -146365.88454495426 1298070.1085416565 0, -146359.18168692812 1298476.2636290384 0)), ((-136713.27875432523 1303176.3946085982 0, -137105.49451181374 1303182.8046719744 0, -137100.4690950279 1303586.0432593564 0, -136707.06806424246 1303579.3905864523 0, -136701.16278207707 1303988.3108931258 0, -136303.54643248214 1303981.8780328168 0, -136309.4825533003 1303572.6785587189 0, -136315.3986023686 1303169.9241440573 0, -136713.27875432523 1303176.3946085982 0)), ((-133893.09407836397 1304751.9413546915 0, -133887.04354756486 1305164.1306788137 0, -133491.3404844265 1305157.588880618 0, -133497.37769181907 1304746.204896057 0, -133893.09407836397 1304751.9413546915 0)), ((-142989.45688318764 1308969.580860934 0, -142590.4745520935 1308961.656802017 0, -142597.7858748713 1308546.262398 0, -142996.78813341475 1308554.142016431 0, -142989.45688318764 1308969.580860934 0)), ((-141407.8490834323 1309749.9982035072 0, -141008.89170567057 1309741.6996568395 0, -141014.65703192184 1309335.7863935425 0, -141413.58809457015 1309344.062073828 0, -141407.8490834323 1309749.9982035072 0)), ((-140205.85312624054 1309724.9515690322 0, -140198.3716098655 1310122.6823183054 0, -139804.97549499408 1310118.8369902407 0, -139810.703236529 1309719.6009644438 0, -140205.85312624054 1309724.9515690322 0)), ((-137100.7977474412 1313321.6666433956 0, -136699.65104940033 1313314.4361723603 0, -136705.83734350637 1312912.8573782397 0, -137107.8599163462 1312919.7884243997 0, -137100.7977474412 1313321.6666433956 0)), ((-130308.81360761348 1313213.3286096363 0, -130302.47462487727 1313626.7100577322 0, -130296.21464684955 1314033.0681423673 0, -129896.42411079406 1314027.0710105351 0, -129902.72970966011 1313620.6465247157 0, -129909.0895354794 1313209.4246535252 0, -130308.81360761348 1313213.3286096363 0)), ((-130283.63422203531 1314849.7821925324 0, -130289.9550967352 1314439.3942504218 0, -130296.21464684955 1314033.0681423673 0, -130692.97746949394 1314039.015654003 0, -130686.81810582144 1314445.2760366432 0, -130680.5686062979 1314857.4775282682 0, -130283.63422203531 1314849.7821925324 0)), ((-136282.55101588773 1314529.6101039622 0, -136276.42789069767 1314938.11031696 0, -136675.76083340234 1314944.0180789041 0, -136669.4026778369 1315348.4211931974 0, -136270.02841539227 1315341.1478201828 0, -135870.6461883922 1315333.8932045393 0, -135877.1049963062 1314932.2328676383 0, -135883.3656347428 1314522.437010701 0, -136282.55101588773 1314529.6101039622 0)), ((-133783.33468803097 1320577.908223658 0, -133390.1033258306 1320574.4307267813 0, -133396.78129673997 1320168.3569447359 0, -133788.26915563343 1320172.1094459286 0, -133783.33468803097 1320577.908223658 0)), ((-133783.33468803097 1320577.908223658 0, -134189.0857350929 1320584.4517344353 0, -134182.1216138577 1320990.1868695873 0, -133778.41021299968 1320983.6414908948 0, -133783.33468803097 1320577.908223658 0)), ((-128910.81865287777 1326611.9775393459 0, -128512.64715223933 1326606.4182682214 0, -128517.99072722287 1326201.8122814873 0, -128914.12430106499 1326209.8697929264 0, -128910.81865287777 1326611.9775393459 0)), ((-141655.39036514505 1326816.9646126637 0, -142060.67995831466 1326823.9233051282 0, -142459.03541628056 1326830.7863080618 0, -142451.9799867155 1327237.9521963922 0, -142053.6049712687 1327231.223070673 0, -141648.68552814057 1327224.3936069396 0, -141655.39036514505 1326816.9646126637 0)), ((-128904.13108198957 1327424.8568851964 0, -128501.877413403 1327419.3372129477 0, -128507.26677592589 1327012.8826966698 0, -128907.47497546455 1327018.4164790905 0, -128904.13108198957 1327424.8568851964 0)), ((-134068.4886943904 1328310.645318157 0, -133666.82018088922 1328303.6616706066 0, -133269.43961086072 1328299.2025184166 0, -133275.8620412256 1327897.8154941974 0, -132876.18007423234 1327894.637166521 0, -132476.48899451602 1327891.47739667 0, -132483.1261542321 1327477.9232214198 0, -132882.73384462358 1327482.4469228457 0, -132889.21079555576 1327076.4</t>
+          <t>MULTIPOLYGON Z (((-175943.71283896 1212106.3037297826 0, -175935.79532105886 1212512.5733073968 0, -175536.08848253996 1212504.426624654 0, -175544.1594031835 1212098.271906859 0, -175943.71283896 1212106.3037297826 0)), ((-163610.46730043937 1243165.7774644892 0, -163604.55339088276 1243571.552269511 0, -163209.83851955028 1243564.0593338464 0, -162809.82194226366 1243556.507319417 0, -162817.3801144094 1243150.7745979107 0, -163217.3973464473 1243158.3154715241 0, -163610.46730043937 1243165.7774644892 0)), ((-160359.9012970106 1245537.615322755 0, -159977.59192745638 1245530.5638024416 0, -159576.8692091762 1245523.191895592 0, -159584.70338458187 1245121.1926338114 0, -159985.33124037087 1245128.7641475056 0, -160369.0641162158 1245135.920217078 0, -160359.9012970106 1245537.615322755 0)), ((-181700.78384793104 1285368.4640731735 0, -181692.73354630606 1285774.2279579418 0, -181298.48571137796 1285765.2698804617 0, -181307.22258078412 1285359.29660042 0, -181700.78384793104 1285368.4640731735 0)), ((-177120.1367204274 1295438.2893821509 0, -177131.22501268188 1295032.2023772858 0, -177142.19103232567 1294630.7681567878 0, -177537.56031274592 1294641.872728787 0, -177528.77445184242 1295041.1478030116 0, -177519.82736241954 1295447.3905718534 0, -177120.1367204274 1295438.2893821509 0)), ((-158772.30953818254 1296274.3055458148 0, -158374.23212556896 1296266.2044292989 0, -157975.9459392016 1296258.084232003 0, -157983.34755768956 1295853.4281711378 0, -158382.07729223545 1295864.140621129 0, -158780.08882858077 1295874.8583381465 0, -158772.30953818254 1296274.3055458148 0)), ((-166711.9329116557 1297668.1456837556 0, -166312.31739866122 1297660.4392632516 0, -165911.04839525977 1297652.7195881458 0, -165904.20617210446 1298044.3488438388 0, -165504.3948566682 1298035.948586059 0, -165512.93539193086 1297642.942385881 0, -165521.87973214872 1297223.1748894467 0, -165919.4957754316 1297231.4547340714 0, -165927.6366133453 1296825.1985452406 0, -166329.91634444712 1296833.8550246235 0, -166729.3168636199 1296842.441181488 0, -167128.7169466071 1296851.04570791 0, -167120.2446458109 1297257.4296628565 0, -166720.74608208291 1297248.7784411104 0, -166711.9329116557 1297668.1456837556 0)), ((-181016.3042165501 1299175.8301672598 0, -180617.19971178332 1299167.6385792592 0, -180626.03963073913 1298762.7777868316 0, -181025.05565840437 1298770.8780416844 0, -181424.01732632934 1298778.9732833093 0, -181415.31756465684 1299184.0383990002 0, -181016.3042165501 1299175.8301672598 0)), ((-172890.40280191824 1306729.3321700757 0, -172881.9206606126 1307135.4190319115 0, -172481.66521688006 1307127.3276678263 0, -172490.10260625373 1306721.1728267525 0, -172890.40280191824 1306729.3321700757 0)), ((-173247.37758807736 1308767.6725587486 0, -172847.28258171518 1308759.4206617458 0, -172855.9976194669 1308353.477750135 0, -173256.1402540953 1308361.652404969 0, -173654.8311616236 1308369.8163153199 0, -173646.65608828366 1308775.915436199 0, -173247.37758807736 1308767.6725587486 0)), ((-164072.11903125813 1311006.1023095907 0, -163653.1310199901 1310997.8152320355 0, -163660.8818023161 1310589.3479996864 0, -163668.55099643348 1310186.139380371 0, -164086.80746085395 1310193.942777795 0, -164084.25042091103 1310598.7478604529 0, -164072.11903125813 1311006.1023095907 0)), ((-165407.69195749695 1315829.215078176 0, -165415.85381046106 1315414.7627328401 0, -165815.98861440568 1315422.4520768158 0, -166214.51319871837 1315431.8296019 0, -166206.37969640837 1315842.3437449534 0, -166198.35842515825 1316248.4532250927 0, -166190.31929299276 1316654.5526442274 0, -165786.2170489032 1316647.2833973987 0, -165391.71779996052 1316641.3250859359 0, -165399.70927637056 1316235.2805723276 0, -165407.69195749695 1315829.215078176 0)), ((-174922.10745709657 1318859.6074760954 0, -174522.5874871394 1318854.53708477 0, -174531.10492345627 1318446.1355614138 0, -174131.74327217424 1318438.1328185203 0, -174140.35635534214 1318031.234057544 0, -174148.9700038597 1317624.3144026555 0, -174157.4860605784 1317222.2169809998 0, -174556.4852565153 1317229.865680886 0, -174955.48408520847 1317237.532768946 0, -174947.20538393813 1317639.937023618 0, -174938.82184958446 1318047.0626794752 0, -174930.45683278897 1318454.167801143 0, -175318.52035623518 1318461.9104561047 0, -175309.29431087075 1318864.5461170557 0, -174922.10745709657 1318859.6074760954 0)), ((-162157.15575879705 1318615.091773267 0, -162165.33965226883 1318214.4025009258 0, -162565.8519518942 1318220.0142986386 0, -162556.95352377798 1318619.63827458 0, -162550.2254389613 1319032.015734088 0, -162148.42503825494 1319026.5475952884 0, -162157.15575879705 1318615.091773267 0)), ((-179676.56784325987 1321000.5412793288 0, -179669.31573975112 1321407.2658184378 0, -179270.06716808988 1321399.3266712248 0, -179277.5681826787 1320991.924711194 0, -179676.56784325987 1321000.5412793288 0)), ((-159230.52179247924 1327104.1398283392 0, -159217.77822971952 1327511.6486867382 0, -158814.24570231294 1327504.9214155392 0, -158821.70056296527 1327097.404303562 0, -159230.52179247924 1327104.1398283392 0)), ((-159606.72725558787 1327926.933928233 0, -159614.3708805533 1327519.586606882 0, -159622.00504865064 1327112.2519599325 0, -160021.47804103562 1327120.6645602852 0, -160013.71421555907 1327527.6163674663 0, -160005.94011452116 1327934.6366322683 0, -159606.72725558787 1327926.933928233 0)), ((-160382.17750341076 1329162.3657044237 0, -160374.6998251148 1329569.3442793237 0, -159975.65580557435 1329561.491869007 0, -159983.16438059925 1329154.760077558 0, -160382.17750341076 1329162.3657044237 0)), ((-173045.73774925352 1332652.892716459 0, -173037.65899207807 1333059.345837976 0, -172637.87555580688 1333051.2121156424 0, -172238.09174489122 1333043.0971236012 0, -172246.46689737157 1332636.6723558058 0, -172646.10682314547 1332644.7845589102 0, -172654.33919258622 1332238.30245773 0, -172254.84250905522 1332230.22673438 0, -172263.1550242012 1331827.3847325481 0, -172662.5084145642 1331834.9652462706 0, -173061.85206936652 1331842.5753031168 0, -173469.39190715915 1331850.357938232 0, -173462.94802872138 1332254.6699356202 0, -173053.82589179816 1332246.4189196844 0, -173045.73774925352 1332652.892716459 0)), ((-171800.28550075658 1334660.3106362945 0, -171789.32883007283 1335069.6679535052 0, -171399.80857682804 1335060.6311684356 0, -171407.60770866153 1334652.1619048263 0, -171800.28550075658 1334660.3106362945 0)), ((-171399.80857682804 1335060.6311684356 0, -171391.1730348959 1335464.7652869667 0, -170992.67448215908 1335456.406894264 0, -171001.77857086583 1335051.4203000162 0, -171399.80857682804 1335060.6311684356 0)), ((-168603.86251440516 1335815.838597261 0, -168209.1341206244 1335808.5334665133 0, -168215.45309209675 1335402.3490952235 0, -168613.2118206783 1335409.6912505527 0, -168603.86251440516 1335815.838597261 0)), ((-174149.02501426663 1337148.257244764 0, -173749.01359806658 1337139.2799883648 0, -173757.98255604412 1336734.0501666393 0, -174157.97685709526 1336743.0158799295 0, -174149.02501426663 1337148.257244764 0)), ((-174531.09440898293 1337969.9777784895 0, -174131.0607312339 1337960.8471441225 0, -174140.0333637393 1337554.5737474703 0, -174149.02501426663 1337148.257244764 0, -174549.02667559774 1337157.2642293086 0, -174540.06945298254 1337563.6260234802 0, -174531.09440898293 1337969.9777784895 0)), ((-166531.05064138706 1340245.2043401864 0, -166131.48671424444 1340237.6843571982 0, -166138.57701623806 1339844.3025036508 0, -166538.26030580953 1339850.3363781278 0, -166531.05064138706 1340245.2043401864 0)), ((-163674.82578318458 1344256.7369317363 0, -163667.65051926434 1344670.7142616373 0, -163254.24097146775 1344662.8477049796 0, -163262.35052098683 1344249.0671734721 0, -163674.82578318458 1344256.7369317363 0)), ((-162433.4104174998 1345858.263872705 0, -162041.7395721198 1345851.0783356146 0, -162048.0286997655 1345445.0152543068 0, -162441.632219718 1345452.2707738655 0, -162433.4104174998 1345858.263872705 0)), ((-177547.53728480323 1351830.3162388531 0, -177933.60306564363 1351838.4570458084 0, -177928.96633726385 1352244.948328299 0, -177924.32001138572 1352651.4520921558 0, -177531.66751574012 1352643.1299813164 0, -177539.60728712505 1352236.7057207413 0, -177547.53728480323 1351830.3162388531 0)), ((-156795.0157294149 1352249.4310476887 0, -156802.24397557 1351843.4752076555 0, -157195.56205515377 1351850.1894254172 0, -157600.17852866193 1351857.2074340805 0, -157593.08784688235 1352262.953108527 0, -157189.16517546648 1352256.0708515148 0, -156795.0157294149 1352249.4310476887 0)), ((-156787.871183984 1352652.2893103384 0, -157182.7743720142 1352661.6180000193 0, -157586.02288138567 1352667.3014826218 0, -157578.7242227329 1353075.0272221325 0, -157174.28696595167 1353068.2698622567 0, -156780.58934995392 1353061.671794447 0, -156787.871183984 1352652.2893103384 0)), ((-172727.89095030742 1353358.0248979128 0, -172329.01525733987 1353349.9045962747 0, -172337.3779199937 1352938.0577529087 0, -172736.2019338599 1352945.66220058 0, -172727.89095030742 1353358.0248979128 0)), ((-171888.29363013318 1355370.5005559528 0, -171482.97650396972 1355361.9976007862 0, -171492.4556019558 1354956.4789137857 0, -171896.72846093695 1354964.9050773887 0, -171888.29363013318 1355370.5005559528 0)), ((-172287.566444225 1355378.867745847 0, -172279.20231218045 1355784.4996053241 0, -171879.84082857828 1355776.0970254324 0, -171888.29363013318 1355370.5005559528 0, -172287.566444225 1355378.867745847 0)), ((-159088.34330247532 1357973.646932964 0, -158718.66444835864 1357966.4845812207 0, -158725.53052986585 1357578.0366991628 0, -159094.9096434183 1357583.290563462 0, -159088.34330247532 1357973.646932964 0)), ((-169835.47313990362 1358576.5516512757 0, -169443.92142799436 1358569.522864897 0, -169450.53675244324 1358164.0320933273 0, -169838.02849845815 1358171.081165173 0, -169835.47313990362 1358576.5516512757 0)), ((-180176.51978652005 1360002.6721153068 0, -180167.2158318822 1360408.8637633454 0, -179767.77191739547 1360400.9719492304 0, -179776.79150236165 1359995.3899140768 0, -180176.51978652005 1360002.6721153068 0)), ((-168595.28370776202 1361394.442381945 0, -168227.56071239134 1361388.024900765 0, -168235.52634394265 1360982.193007978 0, -168603.56927655888 1360990.6539787045 0, -168595.28370776202 1361394.442381945 0)), ((-168570.11374468 1362621.7380692349 0, -168203.45499178141 1362616.158706952 0, -168211.63592106712 1362199.3572157256 0, -168578.6216929984 1362205.7265712805 0, -168570.11374468 1362621.7380692349 0)), ((-174913.7308303282 1363548.545377046 0, -174904.9750124603 1363954.514866465 0, -174504.31655040843 1363947.3328408299 0, -174513.6202447151 1363541.4192655685 0, -174913.7308303282 1363548.545377046 0)), ((-174107.86810484927 1363939.740122899 0, -174099.36983850287 1364353.093090298 0, -173701.08528966803 1364346.7352481862 0, -173709.4643063541 1363932.0925851122 0, -174107.86810484927 1363939.740122899 0)), ((-153215.0175010142 1242969.5947690236 0, -153615.9754351269 1242977.2900949293 0, -153623.67599931773 1242571.6961415 0, -154027.01343899211 1242579.2845108828 0, -154019.46488250766 1242985.0376654444 0, -154011.91058188947 1243390.6024957732 0, -153608.3501508337 1243382.7641784525 0, -153207.30286158103 1243374.9778435475 0, -153215.0175010142 1242969.5947690236 0)), ((-146012.81103504924 1244058.7675813201 0, -146004.95270369758 1244464.298553648 0, -145605.57868785976 1244458.1538807123 0, -145612.44363430905 1244052.4161532205 0, -146012.81103504924 1244058.7675813201 0)), ((-152206.5273128618 1254315.335269746 0, -151838.45177776896 1254308.819883611 0, -151845.02504084533 1253903.4827835227 0, -152216.75322093457 1253910.4537251112 0, -152206.5273128618 1254315.335269746 0)), ((-152186.14304921476 1255122.3428848654 0, -151825.30817169257 1255118.7947019294 0, -151831.87700120764 1254714.2368156444 0, -152196.301943496 1254720.207436628 0, -152186.14304921476 1255122.3428848654 0)), ((-144635.65947211778 1281802.237400236 0, -144640.33425885698 1281602.4275720576 0, -143818.28457170606 1281591.6801632915 0, -143841.9575044904 1280168.3065773223 0, -145449.22263697928 1280189.2587877952 0, -145414.09446047482 1282220.02749221 0, -145252.20096160527 1282216.197520876 0, -145215.58625032182 1282215.7239599524 0, -145205.75055320252 1282627.1191624103 0, -144623.43420937622 1282612.792210075 0, -144628.6590024141 1282207.9544320994 0, -144628.49701549913 1282207.952264684 0, -144629.19479837845 1282166.438826393 0, -144631.24020497318 1282007.9525753856 0, -144426.22189661642 1282005.5134918517 0, -144433.54119046146 1281801.1314159958 0, -144635.3115773361 1281802.531179298 0, -144635.3165924723 1281802.2328120647 0, -144635.65947211778 1281802.237400236 0)), ((-146365.88454495426 1298070.1085416565 0, -146359.18168692812 1298476.2636290384 0, -145959.89247033958 1298468.433158988 0, -145966.6009965479 1298062.4459685492 0, -146365.88454495426 1298070.1085416565 0)), ((-153334.88262986054 1320497.7072252622 0, -152930.5616179454 1320492.9366910174 0, -152932.92099863235 1320085.8918196873 0, -153341.3310235734 1320093.151814407 0, -153740.88985343307 1320100.273132569 0, -153734.664098569 1320502.4828813542 0, -153334.88262986054 1320497.7072252622 0)), ((-152928.20413718335 1320899.3341226527 0, -153328.39216819522 1320904.1207910858 0, -153321.89951349344 1321310.1443134542 0, -152925.85277630598 1321305.3639816998 0, -152928.20413718335 1320899.3341226527 0)), ((-154093.20713756562 1322946.9156327373 0, -153692.85484692265 1322940.3543913355 0, -153700.4999713324 1322533.763593273 0, -154100.86046577114 1322540.4145138732 0, -154093.20713756562 1322946.9156327373 0)), ((-154832.04185527054 1326213.4548934444 0, -154429.2343154817 1326204.775760451 0, -154435.82736405553 1325798.333135726 0, -154839.5692750221 1325806.973036847 0, -155240.35054086844 1325815.5672947324 0, -155232.82127561062 1326222.1049964302 0, -155225.2855029517 1326629.505836762 0, -154824.51335926063 1326621.0011945614 0, -154832.04185527054 1326213.4548934444 0)), ((-146823.78065994848 1328528.0253479884 0, -146816.43162154453 1328934.3892698882 0, -146415.75931633505 1328928.2344914298 0, -146423.72522453536 1328521.7467751517 0, -146823.78065994848 1328528.0253479884 0)), ((-147209.4665911311 1329346.777728987 0, -146809.073429069 1329340.7545623088 0, -146816.43162154453 1328934.3892698882 0, -147216.60607805848 1328940.5430697792 0, -147209.4665911311 1329346.777728987 0)), ((-146399.88031887476 1329738.652703942 0, -146002.11274848995 1329733.181461774 0, -146009.47857243635 1329328.9297116688 0, -146407.7937217798 1329334.7125688149 0, -146399.88031887476 1329738.652703942 0)), ((-150359.3592450211 1331831.20224705 0, -150365.98700833853 1331416.2884148022 0, -150764.7965045753 1331421.097169029 0, -150758.22027965143 1331837.1309649998 0, -150751.774090154 1332243.164365835 0, -151126.35902318076 1332248.3941068486 0, -151119.2312503611 1332654.0924993681 0, -150745.33875430524 1332649.0874178354 0, -150346.34284573808 1332643.7158480035 0, -150352.85367283705 1332237.5702835622 0, -150359.3592450211 1331831.20224705 0)), ((-147940.26375886716 1333007.6192090078 0, -147547.11485829687 1333003.7983143027 0, -147553.7576516025 1332602.823734389 0, -147947.11979710546 1332608.9982825897 0, -147940.26375886716 1333007.6192090078 0)), ((-154686.01566518855 1334750.1755503293 0, -154678.532832025 1335157.084999092 0, -154272.21939837653 1335148.8683594975 0, -154278.12002236737 1334742.8480410725 0, -154686.01566518855 1334750.1755503293 0)), ((-144316.75082181906 1334992.179136188 0, -144710.21701864712 1334999.4737627455 0, -144701.65843617864 1335405.9641072804 0, -144309.66903486208 1335398.5600022823 0, -144316.75082181906 1334992.179136188 0)), ((-144309.66903486208 1335398.5600022823 0, -144302.56964861142 1335804.9196488785 0, -143902.88027996547 1335797.1584011673 0, -143910.03914550686 1335390.97877305 0, -144309.66903486208 1335398.5600022823 0)), ((-155462.0267408171 1335986.1920075733 0, -155062.80131452228 1335977.8079761812 0, -155070.21021053058 1335571.5321538919 0, -155469.3755933252 1335579.780797964 0, -155462.0267408171 1335986.1920075733 0)), ((-154254.50936181424 1336366.3332816497 0, -153856.85964110345 1336360.8980306394 0, -153864.4003283596 1335954.7014575093 0, -154260.40602981093 1335961.0583532727 0, -154254.50936181424 1336366.3332816497 0)), ((-155062.80131452228 1335977.8079761812 0, -155055.45901774327 1336379.8899300178 0, -154656.13266013938 1336373.1229481855 0, -154663.56621552716 1335969.453571963 0, -155062.80131452228 1335977.8079761812 0)), ((-155839.2255570788 1336807.4566159938 0, -155447.08402105645 1336799.059216686 0, -155454.78483779175 1336386.6866166233 0, -155843.92925139275 1336393.3173925595 0, -155839.2255570788 1336807.4566159938 0)), ((-153035.2195628425 1337567.999827459 0, -153434.52511141027 1337574.2557381268 0, -153833.83052199156 1337580.5189529632 0, -153826.3018018914 1337977.466547696 0, -153427.18060698203 1337972.0459149135 0, -153028.06810671612 1337966.6552639122 0, -153035.2195628425 1337567.999827459 0)), ((-154219.98951167185 1337982.8193956506 0, -154213.91534702264 1338399.9944404592 0, -153818.76080926618 1338393.7983247596 0, -153826.3018018914 1337977.466547696 0, -154219.98951167185 1337982.8193956506 0)), ((-155009.1547133005 1338822.911460389 0, -154609.76684636995 1338814.834079961 0, -154617.36113392762 1338408.2492493305 0, -155016.89196970733 1338416.4747248052 0, -155009.1547133005 1338822.911460389 0)), ((-156214.01723597976 1338439.7476310013 0, -156206.19136721594 1338845.9476902375 0, -155807.17068206743 1338839.0747537075 0, -155816.26017470998 1338432.9534301544 0, -156214.01723597976 1338439.7476310013 0)), ((-156198.35672434646 1339252.137990731 0, -156190.6354712538 1339653.0830245882 0, -155789.13589395312 1339645.3705042982 0, -155798.09022928137 1339245.1976703575 0, -156198.35672434646 1339252.137990731 0)), ((-147839.54300877076 1339927.6293664617 0, -147831.51555332803 1340333.865928966 0, -147419.90795926438 1340327.9033265659 0, -147427.86958277982 1339921.7328666248 0, -147839.54300877076 1339927.6293664617 0)), ((-151702.14957268618 1344861.3868170383 0, -151303.04867891027 1344854.6606295847 0, -151310.6510733763 1344439.5037653856 0, -151709.62548874057 1344450.391082684 0, -152108.62637045985 1344461.2974167615 0, -152101.23189219472 1344868.142414273 0, -151702.14957268618 1344861.3868170383 0)), ((-152056.34573203544 1347306.4130121074 0, -152048.8935703995 1347705.2982626064 0, -151649.8222583555 1347698.2407525964 0, -151657.2479042241 1347300.3174988267 0, -152056.34573203544 1347306.4130121074 0)), ((-154837.31606037813 1348165.9023316095 0, -154438.93645708536 1348158.6151754947 0, -154446.6596687272 1347749.8620370426 0, -154844.85458771526 1347760.4363562535 0, -154837.31606037813 1348165.9023316095 0)), ((-155228.24129324564 1348579.4602952788 0, -154829.77068477182 1348572.2537974995 0, -154837.31606037813 1348165.9023316095 0, -155235.6956106203 1348173.1967511538 0, -155228.24129324564 1348579.4602952788 0)), ((-154431.27309903636 1348565.0429208998 0, -154423.61023557428 1348971.4496555608 0, -154019.48736618 1348964.2122469456 0, -154027.4845532631 1348557.7331650024 0, -154431.27309903636 1348565.0429208998 0)), ((-155612.44293623764 1348992.6477535865 0, -155220.7963930565 1348985.70310651 0, -155228.24129324564 1348579.4602952788 0, -155622.23405740855 1348586.548243629 0, -155612.44293623764 1348992.6477535865 0)), ((-146864.1687501368 1349248.6000839875 0, -146465.6865890268 1349244.8143187116 0, -146472.48223450372 1348846.4715961681 0, -146871.0464352838 1348852.351734472 0, -146864.1687501368 1349248.6000839875 0)), ((-149250.50807761765 1349288.893930589 0, -149244.3618468017 1349702.683281918 0, -148849.7489068089 1349696.0780549971 0, -148856.9858320523 1349280.7855524893 0, -149250.50807761765 1349288.893930589 0)), ((-156408.9365036002 1349407.7381076575 0, -156401.66776029047 1349817.557229275 0, -156003.25455303933 1349811.3034675561 0, -156010.51852226187 1349402.1893399984 0, -156408.9365036002 1349407.7381076575 0)), ((-149646.87073823885 1349709.1086215752 0, -149639.7934934366 1350115.0934686544 0, -149238.3350083157 1350108.5633078576 0, -149244.3618468017 1349702.683281918 0, -149646.87073823885 1349709.1086215752 0)), ((-155585.15069978265 1350210.7910502413 0, -155198.8488123306 1350203.9991811563 0, -155206.10020083666 1349797.972603298 0, -155593.90091683116 1349804.7916059187 0, -155585.15069978265 1350210.7910502413 0)), ((-150038.50739124487 1350121.5944305244 0, -150031.50275469752 1350527.5148864177 0, -149632.81768050426 1350520.9583980623 0, -149639.7934934366 1350115.0934686544 0, -150038.50739124487 1350121.5944305244 0)), ((-155195.37636356743 1350613.2084270788 0, -155184.54669782813 1350997.656169277 0, -154789.398449124 1350992.4790538661 0, -154794.5060017364 1350602.0409136314 0, -155195.37636356743 1350613.2084270788 0)), ((-155996.4987495789 1352236.0535013853 0, -155591.69786506644 1352229.3201215023 0, -155198.63116829252 1352222.2248564686 0, -155206.1772473879 1351815.9726843506 0, -155596.63651353068 1351822.9982890885 0, -156003.9188370007 1351829.877387308 0, -155996.4987495789 1352236.0535013853 0)), ((-152795.68063321002 1352991.679811784 0, -152393.38345242525 1352984.402580458 0, -152397.6431043266 1352565.117169408 0, -152802.86055196647 1352572.748382288 0, -152795.68063321002 1352991.679811784 0)), ((-157165.80511167276 1353474.6209384834 0, -157157.3228821247 1353880.9958755823 0, -156766.15742719386 1353874.2091516515 0, -156773.373311206 1353467.9453401759 0, -157165.80511167276 1353474.6209384834 0)), ((-153576.7454523844 1353818.944907566 0, -153966.08582144798 1353826.3144078031 0, -153960.36854565542 1354218.8505520849 0, -153569.98322517873 1354211.8540566787 0, -153576.7454523844 1353818.944907566 0)), ((-155546.44924047423 1354247.4594699736 0, -155960.04629387095 1354257.6206781897 0, -155952.6439078706 1354672.2560051081 0, -155541.35849916993 1354665.1363230979 0, -155546.44924047423 1354247.4594699736 0)), ((-156759.01726149913 1354277.3192752271 0, -156751.63432391797 1354686.3026390863 0, -156352.14353495612 1354679.281290819 0, -156359.5229409861 1354267.4661267216 0, -156759.01726149913 1354277.3192752271 0)), ((-156295.14384288268 1357926.2296338114 0, -155896.26341427167 1357919.786561152 0, -155903.17504087288 1357523.7727790687 0, -156302.17417032074 1357530.162059324 0, -156295.14384288268 1357926.2296338114 0)), ((-153927.54773803763 1357888.1095035025 0, -153921.628849752 1358294.205226988 0, -153497.46541507126 1358286.5579619068 0, -153504.6450566326 1357880.473668274 0, -153927.54773803763 1357888.1095035025 0)), ((-156686.7181276296 1358338.3809343532 0, -156287.93741160425 1358331.9547787134 0, -156295.14384288268 1357926.2296338114 0, -156694.02406843836 1357932.6912303197 0, -156686.7181276296 1358338.3809343532 0)), ((-146327.0534902763 1358163.5458822388 0, -146725.7316913923 1358170.0999134446 0, -147124.40962667338 1358176.672463058 0, -147117.43157852665 1358582.3374349228 0, -146718.79077246223 1358575.7544239631 0, -146320.14053286315 1358569.2009492368 0, -146327.0534902763 1358163.5458822388 0)), ((-147538.5978381123 1359004.1679376068 0, -147110.30092198015 1358996.373509068 0, -147117.43157852665 1358582.3374349228 0, -147542.9253715189 1358589.0987587327 0, -147538.5978381123 1359004.1679376068 0)), ((-149121.4605762462 1359834.1038132894 0, -149116.80190434528 1360239.8701716722 0, -148687.4866014962 1360232.403753368 0, -148288.84240719103 1360225.1757654941 0, -148294.84831593322 1359819.5558019162 0, -148300.85253878497 1359414.0267659102 0, -148306.7633879843 1359014.933385587 0, -148705.6722404669 1359020.554306121 0, -149130.73489886665 1359026.558987703 0, -149126.11824317276 1359428.3834874744 0, -149121.4605762462 1359834.1038132894 0)), ((-147104.52635541573 1359393.4098595302 0, -147098.5899586273 1359798.817022618 0, -146699.90422644696 1359792.3788411694 0, -146705.877141481 1359386.893891728 0, -147104.52635541573 1359393.4098595302 0)), ((-137338.98380080552 1234973.945429173 0, -136939.11983145314 1234966.8112361876 0, -136945.572516736 1234560.8953305294 0, -137345.52076110264 1234567.930088222 0, -137338.98380080552 1234973.945429173 0)), ((-137738.85495487796 1234981.0968554765 0, -137732.19155236293 1235389.29187156 0, -137332.37907850774 1235384.254182857 0, -137338.98380080552 1234973.945429173 0, -137738.85495487796 1234981.0968554765 0)), ((-129169.46761859793 1245393.5263106502 0, -129163.34686924885 1245799.6421268254 0, -128763.95134848665 1245794.1135002414 0, -128770.17265130593 1245387.9655853468 0, -129169.46761859793 1245393.5263106502 0)), ((-140779.7429531961 1270345.7012183582 0, -140377.93219366448 1270339.192467016 0, -140384.5308523573 1269932.69079566 0, -140785.66373684147 1269938.8866375468 0, -140779.7429531961 1270345.7012183582 0)), ((-122026.4768970869 1272493.381808247 0, -122420.38820990089 1272500.2150434542 0, -122426.38182790914 1272500.3108489884 0, -122819.8645824935 1272507.1562028509 0, -122814.32780570837 1272913.0172200245 0, -122414.95625319544 1272907.0728843687 0, -122015.25937432279 1272900.9410113492 0, -122020.49265035699 1272493.2751074557 0, -122026.4768970869 1272493.381808247 0)), ((-125580.94302113118 1274984.4320478467 0, -125181.51849999817 1274977.9330902863 0, -125187.4107042767 1274572.2814955763 0, -125586.77390338219 1274578.6453963707 0, -125580.94302113118 1274984.4320478467 0)), ((-125140.85847847998 1277819.215613086 0, -125134.90567507969 1278225.2821594477 0, -124727.17580067285 1278218.5593556939 0, -124733.72837937086 1277812.5124438612 0, -125140.85847847998 1277819.215613086 0)), ((-129128.53531133535 1278288.796981107 0, -129122.61563460238 1278694.7199382484 0, -128723.53329968442 1278688.2169841693 0, -128729.38828536043 1278282.326534239 0, -129128.53531133535 1278288.796981107 0)), ((-123827.49092526261 1285524.2889669826 0, -123428.25776962508 1285518.1585560646 0, -123434.26955455272 1285102.0412873365 0, -123440.12131234386 1284695.8667190017 0, -123445.98240368116 1284289.6828563996 0, -123451.73706180132 1283890.3105028553 0, -123850.78167704101 1283896.4384220329 0, -124249.81691540833 1283902.584570939 0, -124244.18336706693 1284301.0860859558 0, -123845.06937117598 1284295.3749979127 0, -123839.271270085 1284701.5710158295 0, -123833.4555087105 1285107.734814738 0, -124232.65009981027 1285113.45811755 0, -124226.72382986367 1285530.437782408 0, -123827.49092526261 1285524.2889669826 0)), ((-129042.9674064857 1284372.8071368106 0, -129037.42694387684 1284778.8946705274 0, -128637.65499772798 1284772.1917113666 0, -128643.29451767255 1284366.128022969 0, -129042.9674064857 1284372.8071368106 0)), ((-126192.1874438171 1286357.6553052745 0, -126199.49465913615 1285951.698787946 0, -126206.85838485227 1285542.501059177 0, -126626.13762203927 1285547.7221436817 0, -126620.28940837563 1285958.2953769616 0, -126614.50808183597 1286364.3077194658 0, -126192.1874438171 1286357.6553052745 0)), ((-134544.2962866867 1288933.1577272648 0, -134537.91641483316 1289343.6235207387 0, -134130.60135332463 1289335.3606228917 0, -134134.82259705357 1288926.7964526922 0, -134544.2962866867 1288933.1577272648 0)), ((-134937.2935306726 1289351.826463831 0, -134930.9557333717 1289757.7977986427 0, -134531.60007962736 1289749.4162629638 0, -134537.91641483316 1289343.6235207387 0, -134937.2935306726 1289351.826463831 0)), ((-134531.60007962736 1289749.4162629638 0, -134525.28414022498 1290155.188314266 0, -134122.2044262647 1290146.5885801543 0, -134126.39847725205 1289740.9736664027 0, -134531.60007962736 1289749.4162629638 0)), ((-134079.6883778616 1292572.3127820236 0, -133688.64116096977 1292565.9094625292 0, -133695.05577487996 1292149.5697654448 0, -134084.77668025435 1292151.8585555125 0, -134079.6883778616 1292572.3127820236 0)), ((-133275.9034998461 1293370.4156000693 0, -132875.79243836482 1293363.562027714 0, -132882.4169060993 1292958.2515840302 0, -133282.36778666414 1292964.9236646255 0, -133288.85076028825 1292559.4001895112 0, -133688.64116096977 1292565.9094625292 0, -133682.32739647356 1292971.6145047047 0, -133676.01402571143 1293377.2988434085 0, -133669.9228074871 1293768.6254107016 0, -133269.63777509658 1293762.444135176 0, -133275.9034998461 1293370.4156000693 0)), ((-132099.3518351936 1293748.4277406142 0, -131700.38987692518 1293746.6908600759 0, -131706.7384877057 1293346.9337726904 0, -132105.7497757779 1293352.0049368362 0, -132099.3518351936 1293748.4277406142 0)), ((-132875.79243836482 1293363.562027714 0, -132869.36157527668 1293756.2816187704 0, -132462.34283650547 1293750.0343869794 0, -132469.72982872513 1293356.5799136753 0, -132875.79243836482 1293363.562027714 0)), ((-126873.31005762635 1296526.9378338892 0, -126474.05027020945 1296521.2193321225 0, -126479.65268876923 1296115.0633938138 0, -126878.96674273346 1296120.8386488124 0, -126873.31005762635 1296526.9378338892 0)), ((-126468.39176976836 1296931.8282304714 0, -126462.67424921041 1297333.4328748183 0, -126056.36731075917 1297327.6188907253 0, -126061.50046388266 1296928.030410143 0, -126468.39176976836 1296931.8282304714 0)), ((-136309.4825533003 1303572.6785587189 0, -136315.3986023686 1303169.9241440573 0, -136713.27875432523 1303176.3946085982 0, -137105.49451181374 1303182.8046719744 0, -137100.4690950279 1303586.0432593564 0, -136707.06806424246 1303579.3905864523 0, -136701.16278207707 1303988.3108931258 0, -136303.54643248214 1303981.8780328168 0, -136309.4825533003 1303572.6785587189 0)), ((-133887.04354756486 1305164.1306788137 0, -133491.3404844265 1305157.588880618 0, -133497.37769181907 1304746.204896057 0, -133893.09407836397 1304751.9413546915 0, -133887.04354756486 1305164.1306788137 0)), ((-142996.78813341475 1308554.142016431 0, -142989.45688318764 1308969.580860934 0, -142590.4745520935 1308961.656802017 0, -142597.7858748713 1308546.262398 0, -142996.78813341475 1308554.142016431 0)), ((-141407.8490834323 1309749.9982035072 0, -141008.89170567057 1309741.6996568395 0, -141014.65703192184 1309335.7863935425 0, -141413.58809457015 1309344.062073828 0, -141407.8490834323 1309749.9982035072 0)), ((-140198.3716098655 1310122.6823183054 0, -139804.97549499408 1310118.8369902407 0, -139810.703236529 1309719.6009644438 0, -140205.85312624054 1309724.9515690322 0, -140198.3716098655 1310122.6823183054 0)), ((-137107.8599163462 1312919.7884243997 0, -137100.7977474412 1313321.6666433956 0, -136699.65104940033 1313314.4361723603 0, -136705.83734350637 1312912.8573782397 0, -137107.8599163462 1312919.7884243997 0)), ((-129896.42411079406 1314027.0710105351 0, -129902.72970966011 1313620.6465247157 0, -129909.0895354794 1313209.4246535252 0, -130308.81360761348 1313213.3286096363 0, -130302.47462487727 1313626.7100577322 0, -130296.21464684955 1314033.0681423673 0, -129896.42411079406 1314027.0710105351 0)), ((-130680.5686062979 1314857.4775282682 0, -130283.63422203531 1314849.7821925324 0, -130289.9550967352 1314439.3942504218 0, -130296.21464684955 1314033.0681423673 0, -130692.97746949394 1314039.015654003 0, -130686.81810582144 1314445.2760366432 0, -130680.5686062979 1314857.4775282682 0)), ((-136669.4026778369 1315348.4211931974 0, -136270.02841539227 1315341.1478201828 0, -135870.6461883922 1315333.8932045393 0, -135877.1049963062 1314932.2328676383 0, -135883.3656347428 1314522.437010701 0, -136282.55101588773 1314529.6101039622 0, -136276.42789069767 1314938.11031696 0, -136675.76083340234 1314944.0180789041 0, -136669.4026778369 1315348.4211931974 0)), ((-133783.33468803097 1320577.908223658 0, -133390.1033258306 1320574.4307267813 0, -133396.78129673997 1320168.3569447359 0, -133788.26915563343 1320172.1094459286 0, -133783.33468803097 1320577.908223658 0)), ((-133783.33468803097 1320577.908223658 0, -134189.0857350929 1320584.4517344353 0, -134182.1216138577 1320990.1868695873 0, -133778.41021299968 1320983.6414908948 0, -133783.33468803097 1320577.908223658 0)), ((-125741.49574036461 1324537.50966221 0, -125736.60339542222 1324941.9482963434 0, -125342.52962897124 1324936.5295129518 0, -125348.1529863927 1324535.9729836495 0, -125741.49574036461 1324537.50966221 0)), ((-125726.7717892287 1325754.6336819697 0, -125331.17806382211 1325749.2039699377 0, -125336.84927004448 1325342.8715650416 0, -125731.69240681597 1325348.2790993622 0, -125726.7717892287 1325754.6336819697 0)), ((-128914.12430106499 1326209.8697929264 0, -128910.81865287777 1326611.9775393459 0, -128512.64715223933 1326606.4182682214 0, -128517.99072722287 1326201.8122814873 0, -128914.124</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -945,7 +945,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, Normal Schools, University Preparatory, Oklahoma State University, Other Agency, Wildlife Conservation, Aeronautics Commission</t>
+          <t>Oklahoma State University, Common Schools, State Educational Institutions, Normal Schools, University Preparatory</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -954,7 +954,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>764</v>
+        <v>704</v>
       </c>
       <c r="G11" t="n">
         <v>2182.96</v>
@@ -963,13 +963,13 @@
         <v>41</v>
       </c>
       <c r="I11" t="n">
-        <v>28842.21</v>
+        <v>26471.47</v>
       </c>
       <c r="J11" t="n">
-        <v>723</v>
+        <v>663</v>
       </c>
       <c r="K11" t="n">
-        <v>31025.17</v>
+        <v>28654.43</v>
       </c>
       <c r="L11" t="n">
         <v>4773452.85</v>
@@ -978,7 +978,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">MULTIPOLYGON Z (((-39053.08557852209 1204670.5586080533 0, -39049.82885810009 1205081.4590514496 0, -38654.81918022316 1205078.0207224526 0, -38255.14583045471 1205074.557488872 0, -38257.395571118606 1204667.0271474042 0, -38656.98490433854 1204668.7915173538 0, -38659.11872485368 1204264.715484313 0, -38661.25259090927 1203860.641254526 0, -38261.8649592461 1203858.8777620334 0, -38264.079353846566 1203457.364704566 0, -37988.015536997 1203455.262403598 0, -37989.42618239179 1203051.9598257456 0, -37990.83826212459 1202648.3016175616 0, -38381.45034291026 1202651.5223208368 0, -38378.808006334584 1203055.1752285287 0, -38376.15933253325 1203458.2153398572 0, -38663.369522496025 1203460.4128535464 0, -38758.47271829778 1203461.1371679371 0, -39062.65029212109 1203463.4792286989 0, -39059.49257158824 1203862.4180132134 0, -39056.28438535688 1204266.4872719944 0, -39053.08557852209 1204670.5586080533 0)), ((-37049.96036539697 1205470.754209082 0, -37047.535467700385 1205876.5891939884 0, -36644.15966495941 1205873.87667663 0, -36646.56565564063 1205468.0527264397 0, -37049.96036539697 1205470.754209082 0)), ((-37426.553140069016 1209122.3482503386 0, -37832.10437362921 1209124.1012119222 0, -37829.765599720995 1209529.0708293798 0, -37423.077082803706 1209527.3129077065 0, -37426.553140069016 1209122.3482503386 0)), ((-37011.282239101616 1211961.3586499302 0, -37008.88322310077 1212363.4913997846 0, -37006.484224571956 1212765.637293494 0, -36603.43624182882 1212762.9268507806 0, -36200.37894697794 1212760.2462038435 0, -35798.412933311396 1212757.5774502011 0, -35801.8035139302 1212355.0220526385 0, -35805.19427367527 1211952.4573322588 0, -35808.485714006325 1211560.7563950566 0, -35405.20622953264 1211553.9211003282 0, -35407.73541810169 1211139.8348425294 0, -35410.217639825154 1210732.8578447131 0, -35816.83571395736 1210735.7509073673 0, -36212.23388963351 1210738.5827947166 0, -36615.383772592366 1210741.4875416455 0, -37018.53350182051 1210744.4109824528 0, -37016.102793380094 1211151.8126882263 0, -37013.66062387411 1211561.9542941875 0, -37011.282239101616 1211961.3586499302 0)), ((-39423.5475299953 1210756.1783757396 0, -39821.013840244304 1210757.987609001 0, -40218.48008261885 1210759.8148999927 0, -40215.67898047361 1211167.3375768838 0, -40212.877989246976 1211574.8732455708 0, -39815.88156161022 1211574.7468796715 0, -39418.88517621757 1211574.6385608136 0, -39421.23324983813 1211163.7033866218 0, -39423.5475299953 1210756.1783757396 0)), ((-37418.56333377661 1211154.8635682522 0, -37820.387326930104 1211156.6003136563 0, -37818.032254205405 1211565.4011824408 0, -37815.72147302709 1211966.1019528715 0, -37813.39599405851 1212368.1009685765 0, -37412.67358281812 1212366.3690422745 0, -37415.448419359804 1211964.3719975285 0, -37418.22328423072 1211562.3878936332 0, -37418.56333377661 1211154.8635682522 0)), ((-38996.22883033435 1215214.0691893545 0, -38601.53270097137 1215210.3533343931 0, -38603.64652475055 1214802.4059629068 0, -38996.62764884425 1214804.1583036233 0, -38996.22883033435 1215214.0691893545 0)), ((-38199.91357134666 1215206.6026025573 0, -38601.53270097137 1215210.3533343931 0, -38599.45161858576 1215612.8161476273 0, -38197.84249443864 1215608.9089237233 0, -38199.91357134666 1215206.6026025573 0)), ((-35385.56220020281 1215991.8316237738 0, -35790.333050695306 1215994.080118571 0, -35788.64837836472 1216405.264836136 0, -35787.36003022981 1216802.52798794 0, -35786.04347378875 1217208.8899569253 0, -35381.328907500465 1217206.6972067754 0, -35382.74577693953 1216800.313378971 0, -35384.118190969086 1216404.9171401206 0, -35385.56220020281 1215991.8316237738 0)), ((-40185.439272161915 1218035.1850792302 0, -39786.46898281203 1218035.9097123097 0, -39387.498843658395 1218036.652577136 0, -39389.301672344474 1217643.0622578696 0, -39391.15883940555 1217237.4375056766 0, -39789.63061354594 1217241.4196078076 0, -39791.24893552033 1216835.9295339186 0, -40189.48176470423 1216840.0516066188 0, -40188.111361413576 1217245.4088434104 0, -40186.740899538425 1217650.7678499112 0, -40185.439272161915 1218035.1850792302 0)), ((-32989.551579306884 1217194.0965587727 0, -33388.61078105672 1217196.1564222756 0, -33787.67896642341 1217198.234697229 0, -34187.95718965898 1217200.324674953 0, -34184.95476365744 1217606.7597492896 0, -34181.927705521426 1218017.1863702966 0, -33785.39731099478 1218015.6361096168 0, -33386.08036405704 1218014.0931650149 0, -32986.75414634166 1218012.5684828518 0, -32988.16322527649 1217600.5824063087 0, -32989.551579306884 1217194.0965587727 0)), ((-38580.60440538045 1219257.773358617 0, -38179.01572855806 1219254.04427475 0, -38181.1094364495 1218848.569808809 0, -37779.52932281858 1218844.8705308614 0, -37781.61353798687 1218439.409137733 0, -38183.20330911522 1218443.0860266278 0, -38185.31357699938 1218033.8489857034 0, -38586.921292946456 1218035.622155285 0, -38584.792812245025 1218446.781369126 0, -38582.69854052252 1218852.2764295768 0, -38981.30872871029 1218855.9770545384 0, -38978.09606947956 1219261.4801922683 0, -38974.963300245756 1219657.3404164207 0, -38578.54225265939 1219656.01880591 0, -38580.60440538045 1219257.773358617 0)), ((-37379.35689019034 1219246.668006987 0, -37777.43591033376 1219250.3338145844 0, -38179.01572855806 1219254.04427475 0, -38176.95217940392 1219654.6926070165 0, -37775.353024036594 1219653.3847818482 0, -37773.256982194725 1220061.5898875033 0, -37373.42781787858 1220057.9611184753 0, -37375.165124759216 1219652.1015956379 0, -37379.35689019034 1219246.668006987 0)), ((-38164.345340990054 1222095.759078449 0, -38162.246638518875 1222502.4218996372 0, -37760.686653867204 1222499.068423315 0, -37359.83203678782 1222495.7365421858 0, -37362.62650535337 1222089.0098829619 0, -37762.78518094255 1222092.3722468512 0, -37764.88367082823 1221685.6666457814 0, -38166.44410409563 1221689.0869359905 0, -38164.345340990054 1222095.759078449 0)), ((-33625.366070024764 1251261.5120762493 0, -33223.90635115712 1251259.109905045 0, -33220.43750523598 1251666.4106689165 0, -32818.73332823896 1251663.5903087535 0, -32822.44640999504 1251256.7151595827 0, -32420.986387322555 1251254.3501207633 0, -32424.93490708232 1250847.9022713513 0, -32826.15971731097 1250849.8417724068 0, -32829.864024043265 1250442.970071625 0, -33230.84444307737 1250444.5025817466 0, -33631.8156839457 1250446.053634476 0, -33628.59083178507 1250853.7763768116 0, -33625.366070024764 1251261.5120762493 0)), ((-33622.141560113945 1251669.2383585502 0, -33625.366070024764 1251261.5120762493 0, -34026.82573503782 1251263.932766511 0, -34023.836196815675 1251672.0958780192 0, -33622.141560113945 1251669.2383585502 0)), ((-36381.15780876291 1253714.7887358589 0, -36762.279064425784 1253715.9867649062 0, -36760.08892565688 1254122.54117075 0, -36757.889688873154 1254529.0973536097 0, -36755.69061782406 1254935.6439995123 0, -36375.67281804907 1254932.2708512442 0, -36377.50420282563 1254526.4380296916 0, -35988.31011792833 1254523.7475767857 0, -35989.70020467615 1254118.6637006465 0, -36379.32646046567 1254120.6180677733 0, -36381.15780876291 1253714.7887358589 0)), ((-33999.29175028118 1256531.6709076953 0, -34000.88061863621 1256124.3536109678 0, -34002.46940526148 1255717.0379629584 0, -34400.30970047098 1255721.4960064958 0, -34798.15877575504 1255725.961119712 0, -34795.669561081755 1256132.210752456 0, -34398.27523149563 1256128.272990709 0, -34396.23162304663 1256535.062935967 0, -34394.197293572164 1256941.8435149423 0, -33997.70289345602 1256938.9900561573 0, -33999.29175028118 1256531.6709076953 0)), ((-33578.85576657942 1260593.1518265523 0, -33178.43917051708 1260591.182152788 0, -32778.03164504245 1260589.2310276786 0, -32782.42747987758 1260184.4671535078 0, -33183.29327445941 1260185.9954412475 0, -33584.1590186798 1260187.5422046084 0, -33985.02480401805 1260189.1076482 0, -33979.263176170214 1260595.1400006376 0, -33578.85576657942 1260593.1518265523 0)), ((-40697.03616256546 1265913.1827255948 0, -40695.56958162255 1266317.967961245 0, -40295.49310561891 1266315.4034173598 0, -40295.98379020329 1265910.6135551636 0, -40296.465192510856 1265505.825315982 0, -40698.49363198944 1265508.4104049082 0, -41100.54017156118 1265511.0030173897 0, -41098.08840857022 1265915.7817467959 0, -40697.03616256546 1265913.1827255948 0)), ((-35877.38798955494 1276022.498720461 0, -36284.48817791459 1276023.3222271916 0, -36654.33844211225 1276024.0854297963 0, -36651.209203583974 1276428.9039084674 0, -36648.069011168314 1276834.1936597389 0, -36277.6889668693 1276833.4173672195 0, -36281.08658518644 1276427.7370852611 0, -35874.526194684906 1276426.479894224 0, -35877.38798955494 1276022.498720461 0)), ((-40626.90552197229 1279696.110745793 0, -40629.21435894452 1279288.592788259 0, -40631.53227023822 1278881.0764711455 0, -41025.14034672342 1278886.9691573726 0, -41022.76703734461 1279294.585803377 0, -41020.38451671838 1279702.215230265 0, -40626.90552197229 1279696.110745793 0)), ((-37024.68760338922 1280492.2866984792 0, -37025.75046428243 1280083.1709625716 0, -37429.1650895504 1280086.0790067723 0, -37832.57950515319 1280089.0169529025 0, -37830.096140294634 1280497.9251423045 0, -38232.80923061401 1280500.7669020125 0, -38229.62475849309 1280909.56176214 0, -37827.62186487784 1280906.8238864983 0, -37425.627915688056 1280904.1046871145 0, -37427.391928496494 1280495.0909703807 0, -37024.68760338922 1280492.2866984792 0)), ((-40620.894691572496 1280513.2925774585 0, -40617.889395252634 1280921.8859474857 0, -40222.550053379346 1280914.8405654696 0, -40226.172252129174 1280506.5631025138 0, -40229.79446971065 1280098.2983932314 0, -40623.90003312093 1280104.7008756495 0, -40620.894691572496 1280513.2925774585 0)), ((-37412.068847721705 1282539.5330418511 0, -37012.14424967961 1282536.6296240902 0, -37015.616563673044 1282127.929617001 0, -37019.089012065415 1281719.231274031 0, -37022.561597807326 1281310.534495896 0, -37423.854665926934 1281313.1312926842 0, -37825.147589165565 1281315.7353927868 0, -37820.76257071421 1281724.640245084 0, -37816.36866615953 1282133.5467878398 0, -37811.98416459544 1282542.4437787158 0, -37807.59986812152 1282951.3537244438 0, -37408.1315993938 1282948.3332831631 0, -37412.068847721705 1282539.5330418511 0)), ((-40211.668817093945 1282143.0716713793 0, -40215.298355146515 1281733.089300053 0, -40611.24023712344 1281739.4996929877 0, -40607.59634395169 1282148.5312570222 0, -40603.95262849515 1282557.553395801 0, -40208.03931783286 1282553.055812735 0, -40211.668817093945 1282143.0716713793 0)), ((-36188.033404565336 1288640.4815133153 0, -36190.92405446108 1288233.2640038 0, -36566.9843879048 1288237.4377453383 0, -36564.24476712274 1288645.6065506258 0, -36188.033404565336 1288640.4815133153 0)), ((-36976.04886295998 1288241.9924251058 0, -37373.45774160354 1288241.9975694215 0, -37369.17551494328 1288651.1660660005 0, -36971.194436159705 1288651.1586395348 0, -36976.04886295998 1288241.9924251058 0)), ((-36185.14285310008 1289047.7119488423 0, -35804.43454370193 1289041.589383056 0, -35806.894045489775 1288635.3189474833 0, -36188.033404565336 1288640.4815133153 0, -36185.14285310008 1289047.7119488423 0)), ((-37364.90255513973 1289060.336178394 0, -37763.47404360957 1289060.353092556 0, -37759.78234728111 1289469.5272021594 0, -37360.62973496719 1289469.5079295877 0, -37364.90255513973 1289060.336178394 0)), ((-44565.05637021679 1289484.3083048656 0, -44566.97313845113 1289078.1367916511 0, -44965.96586573926 1289079.76316499 0, -45365.35416999236 1289082.2712748593 0, -45362.64975746917 1289487.5884204593 0, -44964.20753505081 1289485.0853244157 0, -44565.05637021679 1289484.3083048656 0)), ((-36556.048106990835 1289869.2726884554 0, -36179.34821007821 1289863.2847890183 0, -36182.252340784384 1289454.9439126567 0, -36558.77468388857 1289461.9713313826 0, -36556.048106990835 1289869.2726884554 0)), ((-38138.72621324051 1290698.5773109815 0, -37740.400156136166 1290695.0098780943 0, -37746.86046524854 1290286.5139576471 0, -37753.321227669716 1289878.019766435 0, -38152.19520940889 1289879.2414843803 0, -38145.465047825965 1290288.908567888 0, -38138.72621324051 1290698.5773109815 0)), ((-35016.71201087956 1290666.47285753 0, -35019.58869778297 1290255.8129683184 0, -35416.27120503046 1290261.6865782521 0, -35413.54917158444 1290672.1344881258 0, -35016.71201087956 1290666.47285753 0)), ((-33426.05783200189 1291865.7752806556 0, -33027.52970312763 1291862.5361765826 0, -32629.001459521824 1291859.3267108377 0, -32230.472873064027 1291856.124490404 0, -32229.902247579503 1291452.0673566896 0, -32628.358520632333 1291455.2692849194 0, -33026.814648741 1291458.4784659 0, -33026.10843750235 1291054.4224386488 0, -33424.492041493446 1291057.6608663723 0, -33822.8754008283 1291060.906444728 0, -33823.72613631045 1291464.9631466165 0, -33824.58562069848 1291869.0214287764 0, -33426.05783200189 1291865.7752806556 0)), ((-25844.686859396563 1205811.0910221117 0, -25846.21223363861 1205405.8329261532 0, -25847.75490564464 1204997.8056531637 0, -26253.93347701667 1204997.7141178036 0, -26253.055428114832 1205407.374906162 0, -26252.18089442567 1205812.7466014219 0, -25844.686859396563 1205811.0910221117 0)), ((-33029.507902799305 1207875.323926976 0, -33027.43491106538 1208293.3637847744 0, -33025.48664016324 1208685.670451726 0, -33023.477739858376 1209091.6119717162 0, -32638.9600927982 1209089.0328855456 0, -32641.869025770407 1208683.0164127469 0, -32225.53832005472 1208680.1463517165 0, -32227.22036461947 1208288.050946027 0, -31827.99279863974 1208283.1959124412 0, -31829.771855740608 1207867.0658312591 0, -31831.49811452821 1207462.9278894102 0, -32230.743956879156 1207465.5592954645 0, -32645.618765226423 1207468.3233435927 0, -33031.52027245656 1207470.918912302 0, -33029.507902799305 1207875.323926976 0)), ((-26239.312623783546 1209879.4291504375 0, -26237.122826275157 1210270.5473312414 0, -25827.86470548573 1210268.830730507 0, -25426.735245498054 1210267.1683112234 0, -25025.61481239904 1210265.5244386096 0, -24635.595447412736 1210263.9415589485 0, -24637.74552079978 1209867.92844455 0, -24638.564143343214 1209452.714863396 0, -24639.355428688596 1209047.1806424966 0, -25030.35689463183 1209048.4646259753 0, -25431.405772249145 1209049.806759053 0, -25832.463684958482 1209051.167240464 0, -26236.072547748772 1209052.5539147428 0, -26237.66349223496 1209458.888778186 0, -26629.74684987126 1209460.4378174713 0, -26628.047373686954 1209877.671455092 0, -26239.312623783546 1209879.4291504375 0)), ((-27027.500585297712 1209462.0332108992 0, -27425.244943804155 1209463.6579722501 0, -27423.262352859045 1209874.1520255823 0, -27025.65480978638 1209875.9026675073 0, -27027.500585297712 1209462.0332108992 0)), ((-28221.151520456544 1209875.3627591287 0, -27824.14578598025 1209872.39655791 0, -27825.439029318353 1209465.2974532933 0, -28223.13506755825 1209467.662388609 0, -28221.151520456544 1209875.3627591287 0)), ((-32633.02769602535 1209914.693284686 0, -33019.400118809535 1209914.5191278905 0, -33419.32432707795 1209914.3470514684 0, -33417.08819698568 1210312.4820908485 0, -33414.8020387901 1210718.9441673283 0, -33015.42116450244 1210716.2128981985 0, -32627.278151516337 1210713.5755339987 0, -32630.205729037534 1210307.3281418043 0, -32633.02769602535 1209914.693284686 0)), ((-30215.63560855812 1211517.355217665 0, -29815.60453462098 1211514.2764244631 0, -29817.270648025504 1211100.5218119202 0, -29818.899629662705 1210695.016274608 0, -30218.98830756709 1210697.603588389 0, -30619.086086059542 1210700.2092490818 0, -30617.391690419572 1211105.9269072858 0, -30615.657345198488 1211520.4411245126 0, -30215.63560855812 1211517.355217665 0)), ((-31817.607603671317 1210708.1300170235 0, -32216.82394415791 1210710.8058739663 0, -32215.08100530224 1211116.947897598 0, -32213.311209864103 1211527.930621965 0, -32211.603827372484 1211926.9356265012 0, -31812.39762110363 1211924.1927962708 0, -31814.10045824139 1211526.4617703168 0, -31815.865395262328 1211114.1715802122 0, -31817.607603671317 1210708.1300170235 0)), ((-30212.34914557332 1212317.9491533556 0, -29812.389549782958 1212315.4294516223 0, -29814.0156911922 1211910.733999793 0, -30214.011652011643 1211913.3879619755 0, -30212.34914557332 1212317.9491533556 0)), ((-29803.00102625223 1214754.169928916 0, -29804.53129123432 1214347.9541966005 0, -30204.63748633975 1214350.0385423226 0, -30203.17353423855 1214755.5503547585 0, -29803.00102625223 1214754.169928916 0)), ((-31388.855837068055 1218804.1956584565 0, -31787.381838554324 1218806.5273922638 0, -31785.97134228955 1219209.231539241 0, -31784.52329843994 1219624.78998413 0, -31386.09863884517 1219619.943744177 0, -30976.034849944335 1219614.9737531838 0, -30977.491895961553 1219204.1207466982 0, -30978.918634681268 1218801.8080221051 0, -31388.855837068055 1218804.1956584565 0)), ((-30104.030370958888 1233006.7389687197 0, -30502.146742476267 1233008.557643333 0, -30900.253812530875 1233010.405800537 0, -30897.0739230963 1233417.1798910007 0, -30499.151626448198 1233414.91892894 0, -30101.238418435954 1233412.676109908 0, -30104.030370958888 1233006.7389687197 0)), ((-27657.28602220359 1249206.4153311315 0, -28055.649108902384 1249207.2644954273 0, -28452.048396953098 1249208.1367323168 0, -28449.680449848176 1249612.8746861494 0, -28447.312644722475 1250017.6032078401 0, -28444.944948161316 1250422.3335840723 0, -28042.56066422429 1250422.7505482165 0, -28047.705644083744 1250017.5818572554 0, -27654.719852749357 1250017.5889427366 0, -27656.003003531583 1249611.9956626869 0, -27657.28602220359 1249206.4153311315 0)), ((-26449.334599702743 1250835.455293353 0, -26454.987456819097 1250835.4054670823 0, -26847.953241794996 1250832.6270157609 0, -26851.454261333267 1250430.033135776 0, -27252.440776480165 1250426.5937307181 0, -27245.156691625853 1250829.8350030147 0, -27237.87328054609 1251233.0669193247 0, -26867.03512962197 1251235.1027956994 0, -26844.461572669898 1251235.2227019714 0, -26459.506174065154 1251237.3439115102 0, -26448.210315826836 1251237.409964976 0, -26449.334599702743 1250835.455293353 0)), ((-28032.31611441856 1251230.6895965827 0, -28027.19432553487 1251634.667219209 0, -27628.711882607004 1251634.7698192894 0, -27636.95592200571 1251230.9024412748 0, -28032.31611441856 1251230.6895965827 0)), ((-25654.950735460643 1252041.9456699928 0, -26054.462620719558 1252042.2698041394 0, -26445.961552698896 1252041.3355838617 0, -26468.54188428978 1252041.2817702666 0, -26837.46988429417 1252040.4189942782 0, -26836.397554755888 1252446.2473142107 0, -26444.297568045124 1252446.6255275635 0, -26442.633680417468 1252851.9172244628 0, -26049.951110947528 1252851.7859718374 0, -25651.52349859387 1252852.5276636037 0, -25653.232506499753 1252447.23575342 0, -25654.950735460643 1252041.9456699928 0)), ((-33216.96888544153 1252073.7130970238 0, -33216.124736672624 1252477.606118376 0, -33215.28040882868 1252881.5009776305 0, -32814.06620578139 1252879.9686990273 0, -32814.547929317676 1252475.2227156174 0, -32815.02044094082 1252070.47840647 0, -33216.96888544153 1252073.7130970238 0)), ((-29617.759872780338 1255298.706237369 0, -29620.110868983422 1254890.959117288 0, -30018.012576664813 1254891.4820672786 0, -30015.39029746182 1255298.3672127456 0, -29617.759872780338 1255298.706237369 0)), ((-32809.09389956164 1255315.3380458676 0, -33207.41516914681 1255313.4484474289 0, -33206.39051509524 1255719.0652296464 0, -33205.375031736075 1256124.6727424555 0, -32807.61788739436 1256124.8652274942 0, -32409.86995511731 1256125.0648703126 0, -32009.345790024458 1256120.8111510423 0, -31608.830515518468 1256116.5649161278 0, -31208.30572163145 1256112.3482897878 0, -30807.789728429463 1256108.1389431295 0, -30809.22051932046 1255702.9459865447 0, -30810.651220428575 1255297.754866681 0, -31210.682238153306 1255302.5999839834 0, -31610.71279291565 1255307.4634962901 0, -32010.743078325046 1255312.3455104115 0, -32410.772894385515 1255317.2460204945 0, -32809.09389956164 1255315.3380458676 0)), ((-27602.078524428674 1256098.985555087 0, -28004.522040850334 1256100.0676935539 0, -28406.974628574422 1256101.179791615 0, -28402.87798683086 1256504.8682713753 0, -28398.78167594794 1256908.558371547 0, -27996.3618885992 1256908.9564325279 0, -27593.951445972474 1256909.3619713734 0, -27598.014826377534 1256504.172897033 0, -27602.078524428674 1256098.985555087 0)), ((-33603.123172681866 1256124.5095457903 0, -33601.8210722637 1256530.9672788342 0, -33204.350409093044 1256530.2930111222 0, -33205.375031736075 1256124.6727424555 0, -33603.123172681866 1256124.5095457903 0)), ((-29201.908558528776 1257313.4520964928 0, -29200.213941205122 1257719.0652804456 0, -28798.698642331354 1257719.4292639692 0, -28799.945529051416 1257313.8032766075 0, -28801.192386855244 1256908.1902150707 0, -29203.61234000713 1256907.8295338394 0, -29201.908558528776 1257313.4520964928 0)), ((-33203.33476192345 1256935.9039008094 0, -33600.51885929753 1256937.4378426936 0, -33599.47254756705 1257343.7993425073 0, -33201.78424695375 1257343.0127479616 0, -33203.33476192345 1256935.9039008094 0)), ((-32398.69474020587 1258567.3151895045 0, -31999.164011354886 1258559.4321843062 0, -31599.641751566018 1258551.5564534576 0, -31601.47053754444 1258145.0801929454 0, -31603.29017495515 1257738.6168852937 0, -32003.560496788243 1257744.3489475027 0, -32403.830446180396 1257750.0994032668 0, -32401.262537161074 1258158.7064701247 0, -32398.69474020587 1258567.3151895045 0)), ((-28395.603383160807 1258531.0498087632 0, -28396.393454259793 1258125.4299520925 0, -28797.451791882082 1258125.0456985545 0, -28796.20490960127 1258530.675156958 0, -28395.603383160807 1258531.0498087632 0)), ((-32398.69474020587 1258567.3151895045 0, -32797.91344749807 1258565.8344264452 0, -33197.13235524284 1258564.3607399631 0, -33193.67227591272 1258969.7696778006 0, -33190.21243239222 1259375.1802402236 0, -32790.170054529255 1259375.141714004 0, -32390.127603077854 1259375.132844545 0, -32394.41104861425 1258971.2232122319 0, -32398.69474020587 1258567.3151895045 0)), ((-27106.17763108524 1272359.498694486 0, -27104.12381683912 1272764.3433019859 0, -26708.639604669213 1272766.9170713737 0, -26710.166154461782 1272361.6457598323 0, -27106.17763108524 1272359.498694486 0)), ((-25912.236246473076 1273178.2638813518 0, -25910.321295017486 1272772.1528651726 0, -26307.78148962226 1272769.5373855114 0, -26309.66992544267 1273175.2234833934 0, -25912.236246473076 1273178.2638813518 0)), ((-28286.9500782183 1273981.300874363 0, -28683.356792991246 1273980.6808716017 0, -28679.932010573513 1274386.6788753725 0, -28676.507443832874 1274792.678555005 0, -28278.74887268936 1274794.7819293246 0, -27880.981449696745 1274796.903622434 0, -27885.766794375722 1274389.4205402234 0, -27890.54339254185 1273981.9503592562 0, -28286.9500782183 1273981.300874363 0)), ((-26298.202089272643 1276013.0962866722 0, -26696.39741263017 1276013.2403766958 0, -26694.864594483108 1276417.6655800175 0, -26297.362330166136 1276417.3000236591 0, -26298.202089272643 1276013.0962866722 0)), ((-32643.350840233394 1287383.5581962639 0, -33045.133109964976 1287384.130205911 0, -33045.4915111583 1287791.3692153748 0, -32643.46160815518 1287791.556899698 0, -32643.350840233394 1287383.5581962639 0)), ((-32228.37600316234 1293068.2912546142 0, -32231.604450488845 1292664.2435046732 0, -32231.03429065531 1292260.1831590321 0, -32629.63499320538 1292263.3856659126 0, -33028.23555141645 1292266.5954227312 0, -33028.95024293771 1292670.6563495381 0, -33027.76538790832 1293074.7116192405 0, -33026.571438603976 1293478.7684139628 0, -32625.8641987376 1293475.5508177455 0, -32225.147694911782 1293472.3405991988 0, -32228.37600316234 1293068.2912546142 0)), ((-26431.48245834174 1311376.6778858216 0, -26837.396757206014 1311378.1358589823 0, -26835.540997670396 1311783.429312913 0, -26430.244570630417 1311781.872599136 0, -26031.40419935339 1311780.3544205194 0, -26032.623113672194 1311375.2602005384 0, -26431.48245834174 1311376.6778858216 0)), ((-27628.561571957453 1311786.230646267 0, -27627.87423260076 1312191.6410616497 0, -27226.649090473195 1312190.3730610986 0, -27227.92505814413 1311784.9645292321 0, -27628.561571957453 1311786.230646267 0)), ((-19056.057488413986 1203344.7100453696 0, -18656.764852811404 1203343.4334001194 0, -18658.21139549234 1202938.7666239466 0, -18659.65898875902 1202533.6772724278 0, -19059.91585576868 1202535.1126476517 0, -19461.1644437575 1202536.568666244 0, -19856.480823020305 1202538.029559395 0, -19855.56426289198 1202943.5445752956 0, -19854.65172926943 1203347.3294585836 0, -19455.350043856637 1203346.0050803695 0, -19056.057488413986 1203344.7100453696 0)), ((-24242.87223975157 1206209.6216509952 0, -24244.542225218484 1205804.7866944561 0, -24649.154414485634 1205806.3482072023 0, -24649.604293760087 1205401.3998944107 0, -24650.058577025862 1204998.163227867 0, -25046.14797586491 1204998.020454325 0, -25446.955965333724 1204997.8982520013 0, -25445.390753607247 1205404.3276227382 0, -25443.838527745593 1205809.4850229356 0, -25042.989996510645 1205807.8974118722 0, -25041.410830530327 1206212.944940769 0, -25039.7949737611 1206627.626721135 0, -24648.229991355445 1206628.173605118 0, -24648.695255743773 1206211.3095433882 0, -24242.87223975157 1206209.6216509952 0)), ((-17457.389013907337 1206184.2966551734 0, -17457.693986252303 1205781.0445270336 0, -17854.175886281853 1205782.4058118497 0, -17853.457817634662 1206185.6682658156 0, -17852.734363506894 1206591.5922395317 0, -17457.082524184723 1206592.9256973832 0, -17061.430819396013 1206594.277202557 0, -16670.90093218625 1206595.6340551286 0, -16670.61156365436 1206181.640091158 0, -17061.320127386796 1206182.943103546 0, -17457.389013907337 1206184.2966551734 0)), ((-17851.292688616802 1207405.4236537353 0, -17850.564435953445 1207813.666396496 0, -17456.148957969584 1207811.9407761435 0, -17456.463781118993 1207403.8087986847 0, -17851.292688616802 1207405.4236537353 0)), ((-23041.15237959757 1207420.941628168 0, -23442.09264834279 1207422.2252771715 0, -23839.967432687466 1207423.507833533 0, -23838.23193165472 1207828.8978025918 0, -23836.465455026064 1208238.971767525 0, -23438.443762398274 1208237.8901429642 0, -23440.283268745763 1207827.8273871986 0, -23040.7929009751 1207826.7599461353 0, -23041.15237959757 1207420.941628168 0)), ((-14123.415488661018 1237407.6614471732 0, -14526.39386971153 1237404.0456001377 0, -14524.147202646402 1237810.0977394388 0, -14521.90066359875 1238216.16277391 0, -14120.709235066883 1238218.2952601688 0, -13719.52712193945 1238220.4350796996 0, -13719.977760308258 1237815.8647293432 0, -13720.43754896617 1237411.3072405176 0, -14123.415488661018 1237407.6614471732 0)), ((-23291.084764272702 1242310.208335649 0, -23689.993946685943 1242310.8709504064 0, -23688.194242663412 1242717.48893643 0, -23686.387875397206 1243124.1153696978 0, -23288.22051427913 1243123.2310816546 0, -22890.043982886025 1243122.3763336504 0, -22891.108567585357 1242715.9602884029 0, -22892.175705173042 1242309.5528692976 0, -23291.084764272702 1242310.208335649 0)), ((-22869.634911173336 1248807.2642380178 0, -22870.694271536424 1248401.2600930731 0, -22871.753605903188 1247995.2578218048 0, -23270.047323248797 1247998.2352853068 0, -23668.34991573755 1248001.2422200257 0, -24066.643185229346 1248004.2562062435 0, -24067.613312003 1248412.4998214222 0, -23668.637485077466 1248408.734870329 0, -23668.934113441595 1248816.2405721662 0, -23269.28462670798 1248811.743244056 0, -22869.634911173336 1248807.2642380178 0)), ((-15684.404055346533 1249185.7872233351 0, -15282.411986428744 1249187.9533997616 0, -15284.946998216126 1248780.5550693562 0, -15687.744359005264 1248777.8535790194 0, -16090.532844773888 1248775.1708292372 0, -16086.396402357675 1249183.6284700518 0, -15684.404055346533 1249185.7872233351 0)), ((-22461.47199780036 1251240.8651334343 0, -22463.467003491274 1250836.6531039013 0, -22858.76384009545 1250838.6377487432 0, -22857.710238787156 1251242.5280395895 0, -22856.656622305916 1251646.4201783042 0, -22459.477212081056 1251645.0677266037 0, -22062.306883547757 1251643.7447244506 0, -22065.242891705013 1251239.2093014827 0, -22461.47199780036 1251240.8651334343 0)), ((-25648.096544247364 1253663.116559938 0, -26045.440107763865 1253661.3092228072 0, -26045.28051220451 1254067.3374812442 0, -26045.12079676901 1254473.3675950402 0, -25647.288337224083 1254474.1115200527 0, -25249.465121183355 1254474.8626056006 0, -25250.10460600573 1254069.8958332746 0, -25250.753202334465 1253664.9309827753 0, -25648.096544247364 1253663.116559938 0)), ((-17266.33174719659 1255682.2676844203 0, -17266.60330059322 1255279.856778298 0, -17664.912959629146 1255281.0758611856 0, -17664.884387261875 1255685.0862054261 0, -17664.85587655184 1256089.0982910062 0, -17266.069266464758 1256084.6913752232 0, -17266.33174719659 1255682.2676844203 0)), ((-22450.226476518405 1256909.8296239174 0, -22451.27000525706 1256506.340136301 0, -22849.516303928714 1256506.9481762447 0, -22849.863007667525 1256909.155672094 0, -22450.226476518405 1256909.8296239174 0)), ((-21247.223088593233 1257317.1346786767 0, -21251.335894664062 1256911.9405974005 0, -21256.156923156203 1256504.625540581 0, -21654.494521543984 1256505.1786995858 0, -21650.962963511167 1256911.222239316 0, -22050.599296190492 1256910.5111395903 0, -22047.149656183603 1257316.5566082553 0, -22043.691149690734 1257722.6149299252 0, -21643.40994038586 1257722.4634947474 0, -21243.11960802591 1257722.330459498 0, -21247.223088593233 1257317.1346786767 0)), ((-25241.83017067106 1257726.6481693746 0, -25642.476629341934 1257723.3328258726 0, -25639.355735628786 1258130.968676206 0, -25238.91099240138 1258134.1730563932 0, -25241.83017067106 1257726.6481693746 0)), ((-23638.985762845183 1260153.8026541856 0, -23236.520950363785 1260146.2596681956 0, -23237.614888265947 1259744.6016127802 0, -23638.51433339778 1259750.9328755646 0, -23638.985762845183 1260153.8026541856 0)), ((-24037.773129872494 1260566.5164314904 0, -23637.714111670324 1260560.2922271183 0, -23638.985762845183 1260153.8026541856 0, -24038.43978397795 1260161.3111884452 0, -24037.773129872494 1260566.5164314904 0)), ((-16830.17499471343 1265436.1611501463 0, -16830.08844093636 1265030.0860015526 0, -17230.734211593102 1265030.4440171798 0, -17230.27327973553 1265436.5182244952 0, -16830.17499471343 1265436.1611501463 0)), ((-22814.70327035399 1265037.3015321563 0, -23213.979588833976 1265037.0776410813 0, -23212.564971298183 1265442.9389861363 0, -22814.008860104324 1265443.37735996 0, -22814.70327035399 1265037.3015321563 0)), ((-23211.15040855101 1265848.8131326823 0, -23212.564971298183 1265442.9389861363 0, -23611.121245634753 1265442.53003826 0, -23608.986511982454 1265848.1785024905 0, -23211.15040855101 1265848.8131326823 0)), ((-14839.070106083762 1267862.6735043144 0, -14839.428478117532 1268270.4934498498 0, -14438.932098828653 1268270.2449785194 0, -14438.819906840894 1267862.0007193112 0, -14438.698586582204 1267453.7694060015 0, -14838.711564361243 1267454.855382654 0, -14839.070106083762 1267862.6735043144 0)), ((-16034.60068649019 1267459.535984406 0, -16035.164099785534 1267864.145793679 0, -15636.463055404118 1267863.6328835927 0, -15635.965041582753 1267457.9611363334 0, -16034.60068649019 1267459.535984406 0)), ((-16434.49397377822 1268268.2152004787 0, -16831.16356344807 1268268.112492075 0, -17227.833294268232 1268268.016709743 0, -17226.507991728988 1268673.275228132 0, -17225.191748762365 1269078.546705106 0, -16826.983415810628 1269078.1920163485 0, -16428.784189845923 1269077.8668079781 0, -16431.63892843344 1268673.045802013 0, -16434.49397377822 1268268.2152004787 0)), ((-21994.4228764276 1270715.1924628012 0, -21990.854831956793 1271140.4717801013 0, -21591.864186464423 1271140.6779613192 0, -21192.882732353428 1271140.9137206317 0, -21196.42450380944 1270714.0686028388 0, -21595.423727186408 1270714.6269703512 0, -21994.4228764276 1270715.1924628012 0)), ((-21523.74346032127 1271565.1150176378 0, -21588.31538647954 1271565.487795777 0, -21924.776086237973 1271567.4716807983 0, -21921.653757771925 1271971.9765068397 0, -21520.627944882097 1271970.7605865742 0, -21523.74346032127 1271565.1150176378 0)), ((-15152.885688487551 1272371.1003895309 0, -15551.806286934872 1272372.4425564208 0, -15554.907905282955 1272779.2002847272 0, -15558.000154380628 1273185.948459032 0, -15159.11591448034 1273185.2434208612 0, -14760.240815641879 1273184.5567629442 0, -14757.10311585997 1272777.1601974997 0, -14753.965034649884 1272369.7653434102 0, -15152.885688487551 1272371.1003895309 0)), ((-13960.393214814774 1273178.9858240287 0, </t>
+          <t>MULTIPOLYGON Z (((-39053.08557852209 1204670.5586080533 0, -39049.82885810009 1205081.4590514496 0, -38654.81918022316 1205078.0207224526 0, -38255.14583045471 1205074.557488872 0, -38257.395571118606 1204667.0271474042 0, -38656.98490433854 1204668.7915173538 0, -38659.11872485368 1204264.715484313 0, -38661.25259090927 1203860.641254526 0, -38261.8649592461 1203858.8777620334 0, -38264.079353846566 1203457.364704566 0, -37988.015536997 1203455.262403598 0, -37989.42618239179 1203051.9598257456 0, -37990.83826212459 1202648.3016175616 0, -38381.45034291026 1202651.5223208368 0, -38378.808006334584 1203055.1752285287 0, -38376.15933253325 1203458.2153398572 0, -38663.369522496025 1203460.4128535464 0, -38758.47271829778 1203461.1371679371 0, -39062.65029212109 1203463.4792286989 0, -39059.49257158824 1203862.4180132134 0, -39056.28438535688 1204266.4872719944 0, -39053.08557852209 1204670.5586080533 0)), ((-36646.56565564063 1205468.0527264397 0, -37049.96036539697 1205470.754209082 0, -37047.535467700385 1205876.5891939884 0, -36644.15966495941 1205873.87667663 0, -36646.56565564063 1205468.0527264397 0)), ((-37426.553140069016 1209122.3482503386 0, -37832.10437362921 1209124.1012119222 0, -37829.765599720995 1209529.0708293798 0, -37423.077082803706 1209527.3129077065 0, -37426.553140069016 1209122.3482503386 0)), ((-37016.102793380094 1211151.8126882263 0, -37013.66062387411 1211561.9542941875 0, -37011.282239101616 1211961.3586499302 0, -37008.88322310077 1212363.4913997846 0, -37006.484224571956 1212765.637293494 0, -36603.43624182882 1212762.9268507806 0, -36200.37894697794 1212760.2462038435 0, -35798.412933311396 1212757.5774502011 0, -35801.8035139302 1212355.0220526385 0, -35805.19427367527 1211952.4573322588 0, -35808.485714006325 1211560.7563950566 0, -35405.20622953264 1211553.9211003282 0, -35407.73541810169 1211139.8348425294 0, -35410.217639825154 1210732.8578447131 0, -35816.83571395736 1210735.7509073673 0, -36212.23388963351 1210738.5827947166 0, -36615.383772592366 1210741.4875416455 0, -37018.53350182051 1210744.4109824528 0, -37016.102793380094 1211151.8126882263 0)), ((-39423.5475299953 1210756.1783757396 0, -39821.013840244304 1210757.987609001 0, -40218.48008261885 1210759.8148999927 0, -40215.67898047361 1211167.3375768838 0, -40212.877989246976 1211574.8732455708 0, -39815.88156161022 1211574.7468796715 0, -39418.88517621757 1211574.6385608136 0, -39421.23324983813 1211163.7033866218 0, -39423.5475299953 1210756.1783757396 0)), ((-37418.56333377661 1211154.8635682522 0, -37820.387326930104 1211156.6003136563 0, -37818.032254205405 1211565.4011824408 0, -37815.72147302709 1211966.1019528715 0, -37813.39599405851 1212368.1009685765 0, -37412.67358281812 1212366.3690422745 0, -37415.448419359804 1211964.3719975285 0, -37418.22328423072 1211562.3878936332 0, -37418.56333377661 1211154.8635682522 0)), ((-38996.62764884425 1214804.1583036233 0, -38996.22883033435 1215214.0691893545 0, -38601.53270097137 1215210.3533343931 0, -38603.64652475055 1214802.4059629068 0, -38996.62764884425 1214804.1583036233 0)), ((-38199.91357134666 1215206.6026025573 0, -38601.53270097137 1215210.3533343931 0, -38599.45161858576 1215612.8161476273 0, -38197.84249443864 1215608.9089237233 0, -38199.91357134666 1215206.6026025573 0)), ((-35385.56220020281 1215991.8316237738 0, -35790.333050695306 1215994.080118571 0, -35788.64837836472 1216405.264836136 0, -35787.36003022981 1216802.52798794 0, -35786.04347378875 1217208.8899569253 0, -35381.328907500465 1217206.6972067754 0, -35382.74577693953 1216800.313378971 0, -35384.118190969086 1216404.9171401206 0, -35385.56220020281 1215991.8316237738 0)), ((-39791.24893552033 1216835.9295339186 0, -40189.48176470423 1216840.0516066188 0, -40188.111361413576 1217245.4088434104 0, -40186.740899538425 1217650.7678499112 0, -40185.439272161915 1218035.1850792302 0, -39786.46898281203 1218035.9097123097 0, -39387.498843658395 1218036.652577136 0, -39389.301672344474 1217643.0622578696 0, -39391.15883940555 1217237.4375056766 0, -39789.63061354594 1217241.4196078076 0, -39791.24893552033 1216835.9295339186 0)), ((-38580.60440538045 1219257.773358617 0, -38179.01572855806 1219254.04427475 0, -38181.1094364495 1218848.569808809 0, -37779.52932281858 1218844.8705308614 0, -37781.61353798687 1218439.409137733 0, -38183.20330911522 1218443.0860266278 0, -38185.31357699938 1218033.8489857034 0, -38586.921292946456 1218035.622155285 0, -38584.792812245025 1218446.781369126 0, -38582.69854052252 1218852.2764295768 0, -38981.30872871029 1218855.9770545384 0, -38978.09606947956 1219261.4801922683 0, -38974.963300245756 1219657.3404164207 0, -38578.54225265939 1219656.01880591 0, -38580.60440538045 1219257.773358617 0)), ((-37375.165124759216 1219652.1015956379 0, -37379.35689019034 1219246.668006987 0, -37777.43591033376 1219250.3338145844 0, -38179.01572855806 1219254.04427475 0, -38176.95217940392 1219654.6926070165 0, -37775.353024036594 1219653.3847818482 0, -37773.256982194725 1220061.5898875033 0, -37373.42781787858 1220057.9611184753 0, -37375.165124759216 1219652.1015956379 0)), ((-38164.345340990054 1222095.759078449 0, -38162.246638518875 1222502.4218996372 0, -37760.686653867204 1222499.068423315 0, -37359.83203678782 1222495.7365421858 0, -37362.62650535337 1222089.0098829619 0, -37762.78518094255 1222092.3722468512 0, -37764.88367082823 1221685.6666457814 0, -38166.44410409563 1221689.0869359905 0, -38164.345340990054 1222095.759078449 0)), ((-36381.15780876291 1253714.7887358589 0, -36762.279064425784 1253715.9867649062 0, -36760.08892565688 1254122.54117075 0, -36757.889688873154 1254529.0973536097 0, -36755.69061782406 1254935.6439995123 0, -36375.67281804907 1254932.2708512442 0, -36377.50420282563 1254526.4380296916 0, -35988.31011792833 1254523.7475767857 0, -35989.70020467615 1254118.6637006465 0, -36379.32646046567 1254120.6180677733 0, -36381.15780876291 1253714.7887358589 0)), ((-33999.29175028118 1256531.6709076953 0, -34000.88061863621 1256124.3536109678 0, -34002.46940526148 1255717.0379629584 0, -34400.30970047098 1255721.4960064958 0, -34798.15877575504 1255725.961119712 0, -34795.669561081755 1256132.210752456 0, -34398.27523149563 1256128.272990709 0, -34396.23162304663 1256535.062935967 0, -34394.197293572164 1256941.8435149423 0, -33997.70289345602 1256938.9900561573 0, -33999.29175028118 1256531.6709076953 0)), ((-40697.03616256546 1265913.1827255948 0, -40695.56958162255 1266317.967961245 0, -40295.49310561891 1266315.4034173598 0, -40295.98379020329 1265910.6135551636 0, -40296.465192510856 1265505.825315982 0, -40698.49363198944 1265508.4104049082 0, -41100.54017156118 1265511.0030173897 0, -41098.08840857022 1265915.7817467959 0, -40697.03616256546 1265913.1827255948 0)), ((-35877.38798955494 1276022.498720461 0, -36284.48817791459 1276023.3222271916 0, -36654.33844211225 1276024.0854297963 0, -36651.209203583974 1276428.9039084674 0, -36648.069011168314 1276834.1936597389 0, -36277.6889668693 1276833.4173672195 0, -36281.08658518644 1276427.7370852611 0, -35874.526194684906 1276426.479894224 0, -35877.38798955494 1276022.498720461 0)), ((-40626.90552197229 1279696.110745793 0, -40629.21435894452 1279288.592788259 0, -40631.53227023822 1278881.0764711455 0, -41025.14034672342 1278886.9691573726 0, -41022.76703734461 1279294.585803377 0, -41020.38451671838 1279702.215230265 0, -40626.90552197229 1279696.110745793 0)), ((-37425.627915688056 1280904.1046871145 0, -37427.391928496494 1280495.0909703807 0, -37024.68760338922 1280492.2866984792 0, -37025.75046428243 1280083.1709625716 0, -37429.1650895504 1280086.0790067723 0, -37832.57950515319 1280089.0169529025 0, -37830.096140294634 1280497.9251423045 0, -38232.80923061401 1280500.7669020125 0, -38229.62475849309 1280909.56176214 0, -37827.62186487784 1280906.8238864983 0, -37425.627915688056 1280904.1046871145 0)), ((-40623.90003312093 1280104.7008756495 0, -40620.894691572496 1280513.2925774585 0, -40617.889395252634 1280921.8859474857 0, -40222.550053379346 1280914.8405654696 0, -40226.172252129174 1280506.5631025138 0, -40229.79446971065 1280098.2983932314 0, -40623.90003312093 1280104.7008756495 0)), ((-37412.068847721705 1282539.5330418511 0, -37012.14424967961 1282536.6296240902 0, -37015.616563673044 1282127.929617001 0, -37019.089012065415 1281719.231274031 0, -37022.561597807326 1281310.534495896 0, -37423.854665926934 1281313.1312926842 0, -37825.147589165565 1281315.7353927868 0, -37820.76257071421 1281724.640245084 0, -37816.36866615953 1282133.5467878398 0, -37811.98416459544 1282542.4437787158 0, -37807.59986812152 1282951.3537244438 0, -37408.1315993938 1282948.3332831631 0, -37412.068847721705 1282539.5330418511 0)), ((-40607.59634395169 1282148.5312570222 0, -40603.95262849515 1282557.553395801 0, -40208.03931783286 1282553.055812735 0, -40211.668817093945 1282143.0716713793 0, -40215.298355146515 1281733.089300053 0, -40611.24023712344 1281739.4996929877 0, -40607.59634395169 1282148.5312570222 0)), ((-36188.033404565336 1288640.4815133153 0, -36190.92405446108 1288233.2640038 0, -36566.9843879048 1288237.4377453383 0, -36564.24476712274 1288645.6065506258 0, -36188.033404565336 1288640.4815133153 0)), ((-36976.04886295998 1288241.9924251058 0, -37373.45774160354 1288241.9975694215 0, -37369.17551494328 1288651.1660660005 0, -36971.194436159705 1288651.1586395348 0, -36976.04886295998 1288241.9924251058 0)), ((-36185.14285310008 1289047.7119488423 0, -35804.43454370193 1289041.589383056 0, -35806.894045489775 1288635.3189474833 0, -36188.033404565336 1288640.4815133153 0, -36185.14285310008 1289047.7119488423 0)), ((-37360.62973496719 1289469.5079295877 0, -37364.90255513973 1289060.336178394 0, -37763.47404360957 1289060.353092556 0, -37759.78234728111 1289469.5272021594 0, -37360.62973496719 1289469.5079295877 0)), ((-44965.96586573926 1289079.76316499 0, -45365.35416999236 1289082.2712748593 0, -45362.64975746917 1289487.5884204593 0, -44964.20753505081 1289485.0853244157 0, -44565.05637021679 1289484.3083048656 0, -44566.97313845113 1289078.1367916511 0, -44965.96586573926 1289079.76316499 0)), ((-36556.048106990835 1289869.2726884554 0, -36179.34821007821 1289863.2847890183 0, -36182.252340784384 1289454.9439126567 0, -36558.77468388857 1289461.9713313826 0, -36556.048106990835 1289869.2726884554 0)), ((-38145.465047825965 1290288.908567888 0, -38138.72621324051 1290698.5773109815 0, -37740.400156136166 1290695.0098780943 0, -37746.86046524854 1290286.5139576471 0, -37753.321227669716 1289878.019766435 0, -38152.19520940889 1289879.2414843803 0, -38145.465047825965 1290288.908567888 0)), ((-35413.54917158444 1290672.1344881258 0, -35016.71201087956 1290666.47285753 0, -35019.58869778297 1290255.8129683184 0, -35416.27120503046 1290261.6865782521 0, -35413.54917158444 1290672.1344881258 0)), ((-33027.43491106538 1208293.3637847744 0, -33025.48664016324 1208685.670451726 0, -33023.477739858376 1209091.6119717162 0, -32638.9600927982 1209089.0328855456 0, -32641.869025770407 1208683.0164127469 0, -32225.53832005472 1208680.1463517165 0, -32227.22036461947 1208288.050946027 0, -31827.99279863974 1208283.1959124412 0, -31829.771855740608 1207867.0658312591 0, -31831.49811452821 1207462.9278894102 0, -32230.743956879156 1207465.5592954645 0, -32645.618765226423 1207468.3233435927 0, -33031.52027245656 1207470.918912302 0, -33029.507902799305 1207875.323926976 0, -33027.43491106538 1208293.3637847744 0)), ((-28221.151520456544 1209875.3627591287 0, -27824.14578598025 1209872.39655791 0, -27825.439029318353 1209465.2974532933 0, -28223.13506755825 1209467.662388609 0, -28221.151520456544 1209875.3627591287 0)), ((-32633.02769602535 1209914.693284686 0, -33019.400118809535 1209914.5191278905 0, -33419.32432707795 1209914.3470514684 0, -33417.08819698568 1210312.4820908485 0, -33414.8020387901 1210718.9441673283 0, -33015.42116450244 1210716.2128981985 0, -32627.278151516337 1210713.5755339987 0, -32630.205729037534 1210307.3281418043 0, -32633.02769602535 1209914.693284686 0)), ((-29818.899629662705 1210695.016274608 0, -30218.98830756709 1210697.603588389 0, -30619.086086059542 1210700.2092490818 0, -30617.391690419572 1211105.9269072858 0, -30615.657345198488 1211520.4411245126 0, -30215.63560855812 1211517.355217665 0, -29815.60453462098 1211514.2764244631 0, -29817.270648025504 1211100.5218119202 0, -29818.899629662705 1210695.016274608 0)), ((-31812.39762110363 1211924.1927962708 0, -31814.10045824139 1211526.4617703168 0, -31815.865395262328 1211114.1715802122 0, -31817.607603671317 1210708.1300170235 0, -32216.82394415791 1210710.8058739663 0, -32215.08100530224 1211116.947897598 0, -32213.311209864103 1211527.930621965 0, -32211.603827372484 1211926.9356265012 0, -31812.39762110363 1211924.1927962708 0)), ((-30212.34914557332 1212317.9491533556 0, -29812.389549782958 1212315.4294516223 0, -29814.0156911922 1211910.733999793 0, -30214.011652011643 1211913.3879619755 0, -30212.34914557332 1212317.9491533556 0)), ((-29803.00102625223 1214754.169928916 0, -29804.53129123432 1214347.9541966005 0, -30204.63748633975 1214350.0385423226 0, -30203.17353423855 1214755.5503547585 0, -29803.00102625223 1214754.169928916 0)), ((-32988.16322527649 1217600.5824063087 0, -32989.551579306884 1217194.0965587727 0, -33388.61078105672 1217196.1564222756 0, -33787.67896642341 1217198.234697229 0, -34187.95718965898 1217200.324674953 0, -34184.95476365744 1217606.7597492896 0, -34181.927705521426 1218017.1863702966 0, -33785.39731099478 1218015.6361096168 0, -33386.08036405704 1218014.0931650149 0, -32986.75414634166 1218012.5684828518 0, -32988.16322527649 1217600.5824063087 0)), ((-31388.855837068055 1218804.1956584565 0, -31787.381838554324 1218806.5273922638 0, -31785.97134228955 1219209.231539241 0, -31784.52329843994 1219624.78998413 0, -31386.09863884517 1219619.943744177 0, -30976.034849944335 1219614.9737531838 0, -30977.491895961553 1219204.1207466982 0, -30978.918634681268 1218801.8080221051 0, -31388.855837068055 1218804.1956584565 0)), ((-30900.253812530875 1233010.405800537 0, -30897.0739230963 1233417.1798910007 0, -30499.151626448198 1233414.91892894 0, -30101.238418435954 1233412.676109908 0, -30104.030370958888 1233006.7389687197 0, -30502.146742476267 1233008.557643333 0, -30900.253812530875 1233010.405800537 0)), ((-28452.048396953098 1249208.1367323168 0, -28449.680449848176 1249612.8746861494 0, -28447.312644722475 1250017.6032078401 0, -28444.944948161316 1250422.3335840723 0, -28042.56066422429 1250422.7505482165 0, -28047.705644083744 1250017.5818572554 0, -27654.719852749357 1250017.5889427366 0, -27656.003003531583 1249611.9956626869 0, -27657.28602220359 1249206.4153311315 0, -28055.649108902384 1249207.2644954273 0, -28452.048396953098 1249208.1367323168 0)), ((-33628.59083178507 1250853.7763768116 0, -33625.366070024764 1251261.5120762493 0, -33223.90635115712 1251259.109905045 0, -33220.43750523598 1251666.4106689165 0, -32818.73332823896 1251663.5903087535 0, -32822.44640999504 1251256.7151595827 0, -32420.986387322555 1251254.3501207633 0, -32424.93490708232 1250847.9022713513 0, -32826.15971731097 1250849.8417724068 0, -32829.864024043265 1250442.970071625 0, -33230.84444307737 1250444.5025817466 0, -33631.8156839457 1250446.053634476 0, -33628.59083178507 1250853.7763768116 0)), ((-27636.95592200571 1251230.9024412748 0, -28032.31611441856 1251230.6895965827 0, -28027.19432553487 1251634.667219209 0, -27628.711882607004 1251634.7698192894 0, -27636.95592200571 1251230.9024412748 0)), ((-34023.836196815675 1251672.0958780192 0, -33622.141560113945 1251669.2383585502 0, -33625.366070024764 1251261.5120762493 0, -34026.82573503782 1251263.932766511 0, -34023.836196815675 1251672.0958780192 0)), ((-32814.06620578139 1252879.9686990273 0, -32814.547929317676 1252475.2227156174 0, -32815.02044094082 1252070.47840647 0, -33216.96888544153 1252073.7130970238 0, -33216.124736672624 1252477.606118376 0, -33215.28040882868 1252881.5009776305 0, -32814.06620578139 1252879.9686990273 0)), ((-29617.759872780338 1255298.706237369 0, -29620.110868983422 1254890.959117288 0, -30018.012576664813 1254891.4820672786 0, -30015.39029746182 1255298.3672127456 0, -29617.759872780338 1255298.706237369 0)), ((-33207.41516914681 1255313.4484474289 0, -33206.39051509524 1255719.0652296464 0, -33205.375031736075 1256124.6727424555 0, -32807.61788739436 1256124.8652274942 0, -32409.86995511731 1256125.0648703126 0, -32009.345790024458 1256120.8111510423 0, -31608.830515518468 1256116.5649161278 0, -31208.30572163145 1256112.3482897878 0, -30807.789728429463 1256108.1389431295 0, -30809.22051932046 1255702.9459865447 0, -30810.651220428575 1255297.754866681 0, -31210.682238153306 1255302.5999839834 0, -31610.71279291565 1255307.4634962901 0, -32010.743078325046 1255312.3455104115 0, -32410.772894385515 1255317.2460204945 0, -32809.09389956164 1255315.3380458676 0, -33207.41516914681 1255313.4484474289 0)), ((-27602.078524428674 1256098.985555087 0, -28004.522040850334 1256100.0676935539 0, -28406.974628574422 1256101.179791615 0, -28402.87798683086 1256504.8682713753 0, -28398.78167594794 1256908.558371547 0, -27996.3618885992 1256908.9564325279 0, -27593.951445972474 1256909.3619713734 0, -27598.014826377534 1256504.172897033 0, -27602.078524428674 1256098.985555087 0)), ((-33205.375031736075 1256124.6727424555 0, -33603.123172681866 1256124.5095457903 0, -33601.8210722637 1256530.9672788342 0, -33204.350409093044 1256530.2930111222 0, -33205.375031736075 1256124.6727424555 0)), ((-28798.698642331354 1257719.4292639692 0, -28799.945529051416 1257313.8032766075 0, -28801.192386855244 1256908.1902150707 0, -29203.61234000713 1256907.8295338394 0, -29201.908558528776 1257313.4520964928 0, -29200.213941205122 1257719.0652804456 0, -28798.698642331354 1257719.4292639692 0)), ((-33600.51885929753 1256937.4378426936 0, -33599.47254756705 1257343.7993425073 0, -33201.78424695375 1257343.0127479616 0, -33203.33476192345 1256935.9039008094 0, -33600.51885929753 1256937.4378426936 0)), ((-31601.47053754444 1258145.0801929454 0, -31603.29017495515 1257738.6168852937 0, -32003.560496788243 1257744.3489475027 0, -32403.830446180396 1257750.0994032668 0, -32401.262537161074 1258158.7064701247 0, -32398.69474020587 1258567.3151895045 0, -31999.164011354886 1258559.4321843062 0, -31599.641751566018 1258551.5564534576 0, -31601.47053754444 1258145.0801929454 0)), ((-28395.603383160807 1258531.0498087632 0, -28396.393454259793 1258125.4299520925 0, -28797.451791882082 1258125.0456985545 0, -28796.20490960127 1258530.675156958 0, -28395.603383160807 1258531.0498087632 0)), ((-32390.127603077854 1259375.132844545 0, -32394.41104861425 1258971.2232122319 0, -32398.69474020587 1258567.3151895045 0, -32797.91344749807 1258565.8344264452 0, -33197.13235524284 1258564.3607399631 0, -33193.67227591272 1258969.7696778006 0, -33190.21243239222 1259375.1802402236 0, -32790.170054529255 1259375.141714004 0, -32390.127603077854 1259375.132844545 0)), ((-33578.85576657942 1260593.1518265523 0, -33178.43917051708 1260591.182152788 0, -32778.03164504245 1260589.2310276786 0, -32782.42747987758 1260184.4671535078 0, -33183.29327445941 1260185.9954412475 0, -33584.1590186798 1260187.5422046084 0, -33985.02480401805 1260189.1076482 0, -33979.263176170214 1260595.1400006376 0, -33578.85576657942 1260593.1518265523 0)), ((-28683.356792991246 1273980.6808716017 0, -28679.932010573513 1274386.6788753725 0, -28676.507443832874 1274792.678555005 0, -28278.74887268936 1274794.7819293246 0, -27880.981449696745 1274796.903622434 0, -27885.766794375722 1274389.4205402234 0, -27890.54339254185 1273981.9503592562 0, -28286.9500782183 1273981.300874363 0, -28683.356792991246 1273980.6808716017 0)), ((-32643.46160815518 1287791.556899698 0, -32643.350840233394 1287383.5581962639 0, -33045.133109964976 1287384.130205911 0, -33045.4915111583 1287791.3692153748 0, -32643.46160815518 1287791.556899698 0)), ((-32629.001459521824 1291859.3267108377 0, -32230.472873064027 1291856.124490404 0, -32229.902247579503 1291452.0673566896 0, -32628.358520632333 1291455.2692849194 0, -33026.814648741 1291458.4784659 0, -33026.10843750235 1291054.4224386488 0, -33424.492041493446 1291057.6608663723 0, -33822.8754008283 1291060.906444728 0, -33823.72613631045 1291464.9631466165 0, -33824.58562069848 1291869.0214287764 0, -33426.05783200189 1291865.7752806556 0, -33027.52970312763 1291862.5361765826 0, -32629.001459521824 1291859.3267108377 0)), ((-32225.147694911782 1293472.3405991988 0, -32228.37600316234 1293068.2912546142 0, -32231.604450488845 1292664.2435046732 0, -32231.03429065531 1292260.1831590321 0, -32629.63499320538 1292263.3856659126 0, -33028.23555141645 1292266.5954227312 0, -33028.95024293771 1292670.6563495381 0, -33027.76538790832 1293074.7116192405 0, -33026.571438603976 1293478.7684139628 0, -32625.8641987376 1293475.5508177455 0, -32225.147694911782 1293472.3405991988 0)), ((-19059.91585576868 1202535.1126476517 0, -19461.1644437575 1202536.568666244 0, -19856.480823020305 1202538.029559395 0, -19855.56426289198 1202943.5445752956 0, -19854.65172926943 1203347.3294585836 0, -19455.350043856637 1203346.0050803695 0, -19056.057488413986 1203344.7100453696 0, -18656.764852811404 1203343.4334001194 0, -18658.21139549234 1202938.7666239466 0, -18659.65898875902 1202533.6772724278 0, -19059.91585576868 1202535.1126476517 0)), ((-24242.87223975157 1206209.6216509952 0, -24244.542225218484 1205804.7866944561 0, -24649.154414485634 1205806.3482072023 0, -24649.604293760087 1205401.3998944107 0, -24650.058577025862 1204998.163227867 0, -25046.14797586491 1204998.020454325 0, -25446.955965333724 1204997.8982520013 0, -25445.390753607247 1205404.3276227382 0, -25443.838527745593 1205809.4850229356 0, -25042.989996510645 1205807.8974118722 0, -25041.410830530327 1206212.944940769 0, -25039.7949737611 1206627.626721135 0, -24648.229991355445 1206628.173605118 0, -24648.695255743773 1206211.3095433882 0, -24242.87223975157 1206209.6216509952 0)), ((-25844.686859396563 1205811.0910221117 0, -25846.21223363861 1205405.8329261532 0, -25847.75490564464 1204997.8056531637 0, -26253.93347701667 1204997.7141178036 0, -26253.055428114832 1205407.374906162 0, -26252.18089442567 1205812.7466014219 0, -25844.686859396563 1205811.0910221117 0)), ((-17852.734363506894 1206591.5922395317 0, -17457.082524184723 1206592.9256973832 0, -17061.430819396013 1206594.277202557 0, -16670.90093218625 1206595.6340551286 0, -16670.61156365436 1206181.640091158 0, -17061.320127386796 1206182.943103546 0, -17457.389013907337 1206184.2966551734 0, -17457.693986252303 1205781.0445270336 0, -17854.175886281853 1205782.4058118497 0, -17853.457817634662 1206185.6682658156 0, -17852.734363506894 1206591.5922395317 0)), ((-17851.292688616802 1207405.4236537353 0, -17850.564435953445 1207813.666396496 0, -17456.148957969584 1207811.9407761435 0, -17456.463781118993 1207403.8087986847 0, -17851.292688616802 1207405.4236537353 0)), ((-23041.15237959757 1207420.941628168 0, -23442.09264834279 1207422.2252771715 0, -23839.967432687466 1207423.507833533 0, -23838.23193165472 1207828.8978025918 0, -23836.465455026064 1208238.971767525 0, -23438.443762398274 1208237.8901429642 0, -23440.283268745763 1207827.8273871986 0, -23040.7929009751 1207826.7599461353 0, -23041.15237959757 1207420.941628168 0)), ((-26239.312623783546 1209879.4291504375 0, -26237.122826275157 1210270.5473312414 0, -25827.86470548573 1210268.830730507 0, -25426.735245498054 1210267.1683112234 0, -25025.61481239904 1210265.5244386096 0, -24635.595447412736 1210263.9415589485 0, -24637.74552079978 1209867.92844455 0, -24638.564143343214 1209452.714863396 0, -24639.355428688596 1209047.1806424966 0, -25030.35689463183 1209048.4646259753 0, -25431.405772249145 1209049.806759053 0, -25832.463684958482 1209051.167240464 0, -26236.072547748772 1209052.5539147428 0, -26237.66349223496 1209458.888778186 0, -26629.74684987126 1209460.4378174713 0, -26628.047373686954 1209877.671455092 0, -26239.312623783546 1209879.4291504375 0)), ((-27027.500585297712 1209462.0332108992 0, -27425.244943804155 1209463.6579722501 0, -27423.262352859045 1209874.1520255823 0, -27025.65480978638 1209875.9026675073 0, -27027.500585297712 1209462.0332108992 0)), ((-23689.993946685943 1242310.8709504064 0, -23688.194242663412 1242717.48893643 0, -23686.387875397206 1243124.1153696978 0, -23288.22051427913 1243123.2310816546 0, -22890.043982886025 1243122.3763336504 0, -22891.108567585357 1242715.9602884029 0, -22892.175705173042 1242309.5528692976 0, -23291.084764272702 1242310.208335649 0, -23689.993946685943 1242310.8709504064 0)), ((-23269.28462670798 1248811.743244056 0, -22869.634911173336 1248807.2642380178 0, -22870.694271536424 1248401.2600930731 0, -22871.753605903188 1247995.2578218048 0, -23270.047323248797 1247998.2352853068 0, -23668.34991573755 1248001.2422200257 0, -24066.643185229346 1248004.2562062435 0, -24067.613312003 1248412.4998214222 0, -23668.637485077466 1248408.734870329 0, -23668.934113441595 1248816.2405721662 0, -23269.28462670798 1248811.743244056 0)), ((-26851.454261333267 1250430.033135776 0, -27252.440776480165 1250426.5937307181 0, -27245.156691625853 1250829.8350030147 0, -27237.87328054609 1251233.0669193247 0, -26867.03512962197 1251235.1027956994 0, -26844.461572669898 1251235.2227019714 0, -26459.506174065154 1251237.3439115102 0, -26448.210315826836 1251237.409964976 0, -26449.334599702743 1250835.455293353 0, -26454.987456819097 1250835.4054670823 0, -26847.953241794996 1250832.6270157609 0, -26851.454261333267 1250430.033135776 0)), ((-22857.710238787156 1251242.5280395895 0, -22856.656622305916 1251646.4201783042 0, -22459.477212081056 1251645.0677266037 0, -22062.306883547757 1251643.7447244506 0, -22065.242891705013 1251239.2093014827 0, -22461.47199780036 1251240.8651334343 0, -22463.467003491274 1250836.6531039013 0, -22858.76384009545 1250838.6377487432 0, -22857.710238787156 1251242.5280395895 0)), ((-26054.462620719558 1252042.2698041394 0, -26445.961552698896 1252041.3355838617 0, -26468.54188428978 1252041.2817702666 0, -26837.46988429417 1252040.4189942782 0, -26836.397554755888 1252446.2473142107 0, -26444.297568045124 1252446.6255275635 0, -26442.633680417468 1252851.9172244628 0, -26049.951110947528 1252851.7859718374 0, -25651.52349859387 1252852.5276636037 0, -25653.232506499753 1252447.23575342 0, -25654.950735460643 1252041.9456699928 0, -26054.462620719558 1252042.2698041394 0)), ((-25250.753202334465 1253664.9309827753 0, -25648.096544247364 1253663.116559938 0, -26045.440107763865 1253661.3092228072 0, -26045.28051220451 1254067.3374812442 0, -26045.12079676901 1254473.3675950402 0, -25647.288337224083 1254474.1115200527 0, -25249.465121183355 1254474.8626056006 0, -25250.10460600573 1254069.8958332746 0, -25250.753202334465 1253664.9309827753 0)), ((-17266.069266464758 1256084.6913752232 0, -17266.33174719659 1255682.2676844203 0, -17266.60330059322 1255279.856778298 0, -17664.912959629146 1255281.0758611856 0, -17664.884387261875 1255685.0862054261 0, -17664.85587655184 1256089.0982910062 0, -17266.069266464758 1256084.6913752232 0)), ((-22450.226476518405 1256909.8296239174 0, -22451.27000525706 1256506.340136301 0, -22849.516303928714 1256506.9481762447 0, -22849.863007667525 1256909.155672094 0, -22450.226476518405 1256909.8296239174 0)), ((-21247.223088593233 1257317.1346786767 0, -21251.335894664062 1256911.9405974005 0, -21256.156923156203 1256504.625540581 0, -21654.494521543984 1256505.1786995858 0, -21650.962963511167 1256911.222239316 0, -22050.599296190492 1256910.5111395903 0, -22047.149656183603 1257316.5566082553 0, -22043.691149690734 1257722.6149299252 0, -21643.40994038586 1257722.4634947474 0, -21243.11960802591 1257722.330459498 0, -21247.223088593233 1257317.1346786767 0)), ((-25241.83017067106 1257726.6481693746 0, -25642.476629341934 1257723.3328258726 0, -25639.355735628786 1258130.968676206 0, -25238.91099240138 1258134.1730563932 0, -25241.83017067106 1257726.6481693746 0)), ((-23638.985762845183 1260153.8026541856 0, -23236.520950363785 1260146.2596681956 0, -23237.614888265947 1259744.6016127802 0, -23638.51433339778 1259750.9328755646 0, -23638.985762845183 1260153.8026541856 0)), ((-23637.714111670324 1260560.2922271183 0, -23638.985762845183 1260153.8026541856 0, -24038.43978397795 1260161.3111884452 0, -24037.773129872494 1260566.5164314904 0, -23637.714111670324 1260560.2922271183 0)), ((-23213.979588833976 1265037.0776410813 0, -23212.564971298183 1265442.9389861363 0, -22814.008860104324 1265443.37735996 0, -22814.70327035399 1265037.3015321563 0, -23213.979588833976 1265037.0776410813 0)), ((-23211.15040855101 1265848.8131326823 0, -23212.564971298183 1265442.9389861363 0, -23611.121245634753 1265442.53003826 0, -23608.986511982454 1265848.1785024905 0, -23211.15040855101 1265848.8131326823 0)), ((-21994.4228764276 1270715.1924628012 0, -21990.854831956793 1271140.4717801013 0, -21591.864186464423 1271140.6779613192 0, -21192.882732353428 1271140.9137206317 0, -21196.42450380944 1270714.0686028388 0, -21595.423727186408 1270714.6269703512 0, -21994.4228764276 1270715.1924628012 0)), ((-21523.74346032127 1271565.1150176378 0, -21588.31538647954 1271565.487795777 0, -21924.776086237973 1271567.4716807983 0, -21921.653757771925 1271971.9765068397 0, -21520.627944882097 1271970.7605865742 0, -21523.74346032127 1271565.1150176378 0)), ((-27106.17763108524 1272359.498694486 0, -27104.12381683912 1272764.3433019859 0, -26708.639604669213 1272766.9170713737 0, -26710.166154461782 1272361.6457598323 0, -27106.17763108524 1272359.498694486 0)), ((-25912.236246473076 1273178.2638813518 0, -25910.321295017486 1272772.1528651726 0, -26307.78148962226 1272769.5373855114 0, -26309.66992544267 1273175.2234833934 0, -25912.236246473076 1273178.2638813518 0)), ((-17539.09060540013 1273984.9064243785 0, -17129.29459012712 1273989.4115756422 0, -17130.817832408648 1273584.558531489 0, -17132.341245332096 1273179.7070671655 0, -17541.874075282743 1273175.6599500894 0, -17540.486802245312 1273580.287979278 0, -17539.09060540013 1273984.9064243785 0)), ((-17922.001652282648 1275602.512597269 0, -18319.992660183634 1275602.6945652692 0, -18317.95500354197 1276009.131581785 0, -17920.119099061427 1276009.05063075 0, -17922.001652282648 1275602.512597269 0)), ((-26297.362330166136 1276417.3000236591 0, -26298.202089272643 1276013.0962866722 0, -26696.39741263017 1276013.2403766958 0, -26694.864594483108 1276417.6655800175 0, -26297.362330166136 1276417.3000236591 0)), ((-23498.85528631343 1278048.3014724706 0, -23898.207453802213 1278050.265637839 0, -23896.753411872116 1278453.7270805412 0, -23497.41665482628 1278452.9485777528 0, -23498.85528631343 1278048.3014724706 0)), ((-19908.9541900475 1278853.7673967304 0, -19909.792345784062 1278447.2044387748 0, -20310.25647971012 1278447.2825225033 0, -20308.79057420953 1278853.4301903208 0, -19908.9541900475 1278853.7673967304 0)), ((-19508.705881499973 1279668.1290340025 0, -19508.907272179877 1279261.1363744896 0, -19908.1250991134 1279260.3430896194 0, -19907.28687661002 1279666.9093893147 0, -19508.705881499973 1279668.1290340025 0)), ((-18712.221342206165 1279668.9472175038 0, -18709.96096071949 1280073.1635806083 0, -18311.738579281213 1280073.0635298286 0, -18313.97927430324 1279669.3838747465 0, -18314.660860177533 1279262.705372547 0, -18712.73990493739 1279262.156647192 0, -18712.221342206165 1279668.9472175038 0)), ((-19493.524249335092 1282099.8886178604 0, -19895.985147241616 1282099.728520884 0, -19893.57672843884 1282504.7146214324 0, -19490.524315561164 1282505.1864966953 0, -19493.524249335092 1282099.8886178604 0)), ((-21100.131166485742 1283719.7320287214 0, -21101.115910475317 1283313.585950691 0, -21500.40369083309 1283312.0055039828 0, -21498.880609901324 1283718.5752707557 0, -21100.131166485742 1283719.7320287214 0)), ((-18672.836599192116 1296699.2740449281 0, -18674.042171079684 1296294.3406992757 0, -19075.156214530612 1296292.0264400854 0, -19074.449238902234 1296697.1621560398 0, -18672.836599192116 1296699.2740449281 0)), ((-19073.742202963575 1297102.3106629248 0, -19074.449238902234 1296697.1621560398 0, -19476.07108412578 1296695.0801473933 0, -19475.86240863063 1297100.4423158364 0, -19073.742202963575 1297102.3106629248 0)), ((-17869.603202466336 1296703.5315218214 0, -18271.215182373588 1296701.393385804 0, -18269.502231056704 1297106.1036048501 0, -17867.382669415398 1297108.028104559 0, -17869.603202466336 1296703.5315218214 0)), ((-25397.169783828027 1309274.4719356818 0, -25399.05369900507 1308864.332681705 0, -25797.6705556573 1308864.221359346 0, -25795.77134142531 1309273.1522238636 0, -25397.169783828027 1309274.4719356</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -993,7 +993,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, University of Oklahoma, Langston University, Oklahoma State University, Normal Schools, University Preparatory, Wildlife Conservation, Other Agency</t>
+          <t>Common Schools, State Educational Institutions, University of Oklahoma, Normal Schools, University Preparatory, Langston University, Oklahoma State University</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1188</v>
+        <v>1080</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -1011,13 +1011,13 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>47069.62</v>
+        <v>42748.64</v>
       </c>
       <c r="J12" t="n">
-        <v>1188</v>
+        <v>1080</v>
       </c>
       <c r="K12" t="n">
-        <v>47069.62</v>
+        <v>42748.64</v>
       </c>
       <c r="L12" t="n">
         <v>6995550.73</v>
@@ -1026,7 +1026,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-118559.78860199626 1324416.086118968 0, -118160.87134183437 1324408.490762127 0, -118166.56910121029 1323984.0706868803 0, -118171.88945702897 1323580.5591783095 0, -118571.98769600078 1323568.9705862713 0, -118566.17801895243 1323975.7536779107 0, -118559.78860199626 1324416.086118968 0)), ((-118129.64936550814 1326421.6286623029 0, -118123.17756806467 1326827.9097110208 0, -117723.13475646079 1326822.0967949047 0, -117725.91953178747 1326416.5709332328 0, -118129.64936550814 1326421.6286623029 0)), ((-116813.9391853527 1334120.0661837044 0, -116819.50557757256 1333714.8849958992 0, -116825.06969841395 1333309.8729937323 0, -117224.67568480992 1333314.982153998 0, -117625.32173768191 1333320.1129362336 0, -117621.50040622786 1333725.2494314522 0, -117617.67036619947 1334131.0138816452 0, -117214.35335177822 1334125.5108148553 0, -116813.9391853527 1334120.0661837044 0)), ((-114346.85754153511 1340631.7976945944 0, -114340.17261258581 1341032.3222610098 0, -114333.39196609255 1341438.0170531531 0, -113935.8076705649 1341428.285684852 0, -113533.73249523416 1341418.4462021037 0, -113513.00559300676 1341417.9487421208 0, -113509.74896754985 1341633.6958187832 0, -113506.86405202247 1341824.7166014917 0, -113500.59997023792 1342233.9351261824 0, -113120.16236855932 1342224.0308512778 0, -112726.20973475832 1342213.7982873933 0, -112730.42087158357 1341814.2887418289 0, -112730.44554445274 1341811.715162787 0, -112734.69771598041 1341408.3804266797 0, -112738.91680032454 1341007.5532839692 0, -112738.96903645646 1341002.8875265375 0, -112743.15224945682 1340605.4744317592 0, -113140.78893471866 1340611.9727966043 0, -113526.17196414941 1340618.2941430346 0, -113540.5318331427 1340618.5284885874 0, -113939.49722290419 1340625.0811591027 0, -114346.85754153511 1340631.7976945944 0)), ((-109522.29259002196 1345392.8853512062 0, -109515.76144907808 1345796.663347934 0, -109509.23951791451 1346200.4316081065 0, -109502.70866112935 1346604.2123752579 0, -109496.18701110258 1347007.9835038052 0, -109099.37315729806 1346999.9477500606 0, -108702.5588278943 1346991.9190399034 0, -108708.35957087454 1346587.9261491862 0, -108714.16034921788 1346183.934642002 0, -109111.70475573237 1346192.1739902063 0, -109117.86615104994 1345788.2891467095 0, -109124.02768456614 1345384.405690915 0, -109522.29259002196 1345392.8853512062 0)), ((-117844.31375286872 1345552.8724710583 0, -117838.8780229834 1345951.0468519721 0, -117439.54188566864 1345947.9080329547 0, -117444.9765387301 1345550.438690692 0, -117844.31375286872 1345552.8724710583 0)), ((-118235.0715050977 1345954.1387512595 0, -118229.5931961534 1346361.2893122216 0, -117833.35962171144 1346358.54382587 0, -117838.8780229834 1345951.0468519721 0, -118235.0715050977 1345954.1387512595 0)), ((-119012.56334631782 1346773.1815694037 0, -119008.99000898006 1347182.263837768 0, -118614.94795527779 1347178.5161622774 0, -118218.6481601709 1347174.7554020977 0, -118224.12425542329 1346768.418959465 0, -118229.5931961534 1346361.2893122216 0, -118625.83600343669 1346364.0420288965 0, -119016.10885670314 1346366.7414651362 0, -119012.56334631782 1346773.1815694037 0)), ((-118094.30938391492 1356490.4121007835 0, -118091.74861136051 1356893.3845473279 0, -117697.16093914752 1356886.2741512647 0, -117301.08470967412 1356879.1503783327 0, -117310.7717087816 1356473.5671227986 0, -117320.3959042449 1356070.6369453582 0, -117330.05388795171 1355666.5781150686 0, -117339.704855358 1355262.418665986 0, -117712.76976504254 1355269.1380548119 0, -117708.38438331963 1355674.2761722747 0, -117703.99368942676 1356078.4965027748 0, -117700.5790498014 1356481.9369705818 0, -117897.4805939922 1356486.1616319162 0, -118094.30938391492 1356490.4121007835 0)), ((-113661.71304653907 1360439.7464031598 0, -113252.63758575395 1360431.8293268944 0, -113259.49608135803 1360028.612266803 0, -113281.22580856434 1360028.9886170898 0, -113668.18565127651 1360035.796804282 0, -113661.71304653907 1360439.7464031598 0)), ((-112863.70968331992 1361239.0867491101 0, -112869.75248839286 1360833.4497317923 0, -113246.44825755537 1360838.3247476257 0, -113242.72257031559 1361088.3380283497 0, -113240.37317265633 1361243.6925950516 0, -112863.70968331992 1361239.0867491101 0)), ((-113530.40020495799 1369780.3736350846 0, -113539.96414796117 1369780.589944662 0, -113936.93857857028 1369789.731821339 0, -113929.53299215686 1370190.723731397 0, -113922.04690786572 1370596.428320509 0, -113914.55181697455 1371002.1453353716 0, -113907.30260652727 1371394.8041175741 0, -113510.19296043238 1371386.5226992478 0, -113110.6876765547 1371378.2167677616 0, -113104.90696060937 1371378.095723977 0, -113109.6111976801 1370999.3948446675 0, -113112.06834764156 1370826.9819067824 0, -113115.27790131785 1370593.5079743771 0, -112731.9635684356 1370588.2100647641 0, -112351.20759482418 1370582.9738857518 0, -112351.5810685068 1370557.9392696826 0, -112357.21124630433 1370177.4845635628 0, -112357.53206439978 1370155.7737209897 0, -112363.48297540058 1369753.6206613558 0, -112745.04958382217 1369762.3486859244 0, -113125.6711244621 1369771.0810456818 0, -113144.80813151246 1369771.5128189307 0, -113530.40020495799 1369780.3736350846 0)), ((-112601.60897410054 1380303.3566903046 0, -112205.30836661912 1380298.6559525274 0, -112212.99237908436 1379895.2617520043 0, -112213.06162542276 1379891.3558927109 0, -112220.79219565334 1379485.803162598 0, -112609.9774005436 1379490.4777110198 0, -112984.98523679533 1379494.9943494613 0, -112979.34421856757 1379908.5447852528 0, -112973.97246560524 1380307.8385735457 0, -112601.60897410054 1380303.3566903046 0)), ((-113111.83349464808 1389676.960075897 0, -113101.15937811643 1389682.1924448288 0, -113089.24748180441 1389692.6702343072 0, -113079.64368855588 1389705.30571605 0, -113077.52000328319 1389708.7112633495 0, -113055.81971625051 1389725.534012182 0, -112948.2141739142 1389724.1902562384 0, -112903.67756781167 1389695.6227126569 0, -112901.23152089251 1389693.0931024007 0, -112898.11914017197 1389690.5889833216 0, -112886.89391179131 1389684.8570107596 0, -112866.24319305625 1389671.6108216338 0, -112867.00082935549 1389633.9832180613 0, -112875.13136002039 1389226.6271241426 0, -112887.78320501046 1389226.8613254253 0, -113269.74409676601 1389234.0173980554 0, -113288.7217694023 1389234.3695200658 0, -113646.65481177715 1389241.089758895 0, -113643.33149232288 1389576.144883839 0, -113642.86860797573 1389623.112974984 0, -113642.65261038295 1389644.08948513 0, -113638.56487203838 1390056.2133263082 0, -113257.79085354638 1390049.0573441545 0, -113255.60916345123 1390045.8369991586 0, -113262.69445577585 1389639.0925695903 0, -113263.67508583379 1389582.7387953566 0, -113135.14721657618 1389664.0368250036 0, -113124.28179675284 1389672.460042096 0, -113122.94207407821 1389672.853007615 0, -113111.83349464808 1389676.960075897 0)), ((-108961.60580476526 1326324.8954503047 0, -108965.83956777902 1325922.4463640077 0, -109367.46586635518 1325927.5351789834 0, -109362.26279785884 1326329.971983933 0, -108961.60580476526 1326324.8954503047 0)), ((-102573.77443063777 1327437.0790865377 0, -102165.12112157764 1327427.009226146 0, -102170.40185537828 1327020.9767840875 0, -102175.68258514833 1326614.945909763 0, -102586.620427456 1326627.2472273542 0, -102984.22672161988 1326639.151478595 0, -102978.2455285201 1327043.0257256723 0, -102972.27347042694 1327446.901605464 0, -102573.77443063777 1327437.0790865377 0)), ((-103317.85927134845 1331916.525398105 0, -103322.053671023 1331509.3547327637 0, -103721.70084824732 1331514.1595532878 0, -104121.34764388262 1331518.983083842 0, -104117.45918715191 1331926.1575769382 0, -104113.57086320131 1332333.3224353741 0, -103713.61792538497 1332328.4950716635 0, -103313.67393238138 1332323.6864016554 0, -103317.85927134845 1331916.525398105 0)), ((-108084.29532726013 1334831.5396286224 0, -107683.31802101682 1334822.249658897 0, -107688.9952375145 1334416.5747179661 0, -107288.26873253818 1334406.6688456307 0, -107282.33999503322 1334812.978496309 0, -106881.3615939498 1334803.7148493777 0, -106480.38243699979 1334794.481108516 0, -106486.80444149967 1334386.9131479885 0, -106493.2355874098 1333979.34671472 0, -106893.71231417876 1333989.8499790102 0, -107294.19724761439 1334000.3719296842 0, -107694.6724349081 1334010.9124140565 0, -108095.1560176016 1334021.4717926641 0, -108089.7210777327 1334426.5105026036 0, -108084.29532726013 1334831.5396286224 0)), ((-104398.06590818788 1342065.4996272956 0, -103995.86442064783 1342056.7647781668 0, -104001.61333695416 1341652.7881969006 0, -104007.36227092014 1341248.8130165916 0, -104013.11136422343 1340844.828041519 0, -104018.86042941852 1340440.8557713237 0, -104421.53526639382 1340446.6084159294 0, -104824.2188797988 1340452.3689289498 0, -104818.2330655357 1340857.837888466 0, -104812.24726800816 1341263.3082598455 0, -104806.26148726072 1341668.7800416395 0, -104800.2759184653 1342074.2533393656 0, -104398.06590818788 1342065.4996272956 0)), ((-107929.24767328279 1345359.0781114774 0, -108327.50522301492 1345367.5021215314 0, -108725.7712746039 1345375.9447684663 0, -108719.9703296113 1345779.9334003902 0, -108322.06481974282 1345771.607228296 0, -107924.16795344326 1345763.2884924468 0, -107929.24767328279 1345359.0781114774 0)), ((-108154.89678118152 1356297.720158007 0, -108152.95480976794 1356697.9661848047 0, -107753.80413908714 1356692.5196739826 0, -107756.41547691992 1356292.080664773 0, -107759.03581087208 1355891.6318686488 0, -108156.8382428046 1355897.4865566047 0, -108554.64924378692 1355903.371034482 0, -108553.37753496063 1356303.3893586586 0, -108154.89678118152 1356297.720158007 0)), ((-108951.2555620091 1356708.9039511657 0, -108552.10541081056 1356703.4202130258 0, -108553.37753496063 1356303.3893586586 0, -108951.85807751214 1356309.0770744418 0, -108951.2555620091 1356708.9039511657 0)), ((-109273.28425350602 1366434.420824356 0, -108875.25755466968 1366429.3563738924 0, -108477.23054482524 1366424.3103915248 0, -108079.20332163286 1366419.2829810695 0, -107681.17598890651 1366414.2740446865 0, -107684.87722985457 1366009.9773468818 0, -107688.58751344724 1365605.682151466 0, -108086.12165878483 1365611.3339859117 0, -108483.66475698304 1365616.9931753941 0, -108881.1983745591 1365622.6819573413 0, -109278.74084270338 1365628.3780914135 0, -109276.00817302614 1366031.3987132914 0, -109273.28425350602 1366434.420824356 0)), ((-104447.36326426534 1370445.1188663272 0, -104047.19228134869 1370434.9115411886 0, -103647.011806099 1370424.7115017676 0, -103642.15577842157 1370827.5309039277 0, -103637.29089125487 1371230.3403210002 0, -103236.4600106018 1371220.3863003133 0, -102835.63768349009 1371210.4399225463 0, -102841.15191703259 1370807.4144446405 0, -102846.6664095676 1370404.3791638564 0, -102852.18078206544 1370001.356275659 0, -102857.69531435877 1369598.323584405 0, -103257.2187544394 1369608.702077609 0, -103656.74162271575 1369619.0880361076 0, -104056.26362838647 1369629.5039594988 0, -104455.78496295503 1369639.9272442826 0, -104451.5696211929 1370042.5279194922 0, -104447.36326426534 1370445.1188663272 0)), ((-107928.2746291788 1376178.824992988 0, -107528.28197644571 1376175.0805355113 0, -107536.46064962691 1375771.2336784373 0, -107544.6398091161 1375367.3770024648 0, -107552.81907170058 1374963.5328050556 0, -107560.9988205348 1374559.6787916836 0, -107962.42259670311 1374563.0278035828 0, -108363.85543327962 1374566.384641587 0, -108354.96013123803 1374970.4308767472 0, -108346.06504034332 1375374.4894930571 0, -108337.17044171046 1375778.5382907696 0, -108328.27619479694 1376182.588367581 0, -107928.2746291788 1376178.824992988 0)), ((-104274.55049671762 1379773.4548623795 0, -103877.25748240731 1379767.438262733 0, -103479.9641675923 1379761.4400782376 0, -103483.32961744542 1379355.1822972533 0, -103881.41934760772 1379360.8765586729 0, -104279.50891886503 1379366.5782389475 0, -104274.55049671762 1379773.4548623795 0)), ((-103473.2416502126 1380573.9709581828 0, -103868.94245419104 1380580.5766924797 0, -104264.63372897323 1380587.2007520343 0, -104259.6754825904 1380994.0700183294 0, -103864.7803105215 1380987.1422333217 0, -103469.8847293741 1380980.2327532428 0, -103473.2416502126 1380573.9709581828 0)), ((-98991.5661045002 1325759.4310509183 0, -99390.12364883219 1325762.3068798182 0, -99386.81964058286 1326167.7425183088 0, -98988.28516351998 1326165.2809846643 0, -98589.74147803921 1326162.8488951274 0, -98593.01757595724 1325756.5626311009 0, -98991.5661045002 1325759.4310509183 0)), ((-100177.24310694287 1326981.873440304 0, -100173.92021743058 1327386.451818234 0, -99775.4179608111 1327385.2403088382 0, -99376.92498514801 1327384.0473035218 0, -98978.42294119613 1327382.8727389507 0, -98579.93017844533 1327381.7167789293 0, -98583.19773121837 1326975.4259185295 0, -98586.47418026078 1326569.1367086126 0, -98984.99493666277 1326571.143408437 0, -98981.71351301535 1326977.0073775554 0, -99380.22032794954 1326978.6071825796 0, -99383.5245376473 1326573.179703947 0, -99782.04530522341 1326575.223253798 0, -100180.5750486242 1326577.2854055134 0, -100177.24310694287 1326981.873440304 0)), ((-100891.15515543938 1332697.458156693 0, -100887.60633158246 1333102.503157431 0, -100493.05395471178 1333097.0268983683 0, -100495.96559821334 1332693.0599392357 0, -100891.15515543938 1332697.458156693 0)), ((-100068.65664579772 1336750.691630401 0, -100062.91137551065 1337154.8638156527 0, -99666.97939251801 1337150.2685202803 0, -99271.05626663935 1337145.6915811314 0, -98875.12385117913 1337141.1328395032 0, -98479.20029912573 1337136.5923530518 0, -98484.16613474589 1336732.411078889 0, -98489.14098401606 1336328.231405308 0, -98494.10680073017 1335924.053077485 0, -98499.0816341248 1335519.8762522473 0, -98895.7848362916 1335524.4256152022 0, -99292.48777789096 1335528.9932619545 0, -99689.19055332465 1335533.5792964867 0, -100085.89306490228 1335538.1836150372 0, -100080.14749052795 1335942.3515286644 0, -100074.40201748101 1336346.5208675978 0, -100068.65664579772 1336750.691630401 0)), ((-100000.36157028419 1345251.1909587882 0, -99998.40892166083 1345655.4372363847 0, -99996.45605946124 1346059.6848078172 0, -99994.50287853723 1346463.9338702364 0, -99594.96544573244 1346458.9808477743 0, -99592.59838367256 1346863.1256108624 0, -99192.65628230856 1346858.0744326126 0, -98792.70474837693 1346853.053025073 0, -98795.88968063382 1346449.130553352 0, -98396.35144772787 1346444.233385091 0, -98399.94081001657 1346040.4178101674 0, -98403.52992152468 1345636.6147200926 0, -98802.2500783041 1345641.2897977824 0, -98799.06537319074 1346045.209490217 0, -99198.19879570323 1346050.0198024155 0, -99200.96997364855 1345645.983325844 0, -99203.74069380149 1345241.9595350488 0, -99602.04675429677 1345246.5659320583 0, -100000.36157028419 1345251.1909587882 0)), ((-99022.82640782211 1356552.3041480414 0, -98623.98256400043 1356548.9987095296 0, -98225.1476843331 1356545.711858135 0, -98230.80786065722 1356141.89633271 0, -98236.46828051217 1355738.070860022 0, -98242.12865376448 1355334.2580393278 0, -98247.79213183348 1354930.4357668527 0, -98644.59260406076 1354936.6987964418 0, -99041.40176313117 1354942.9692146222 0, -99438.20148389338 1354949.268964337 0, -99835.00999046354 1354955.5760050435 0, -99831.3819227015 1355356.422631429 0, -99827.75623721641 1355757.2706731658 0, -99824.13065494676 1356158.1200580532 0, -99820.50487867782 1356558.9707754594 0, -99421.66116435213 1356555.628117643 0, -99022.82640782211 1356552.3041480414 0)), ((-102541.83008083396 1363076.035208118 0, -102150.47463689576 1363071.7789349912 0, -102154.20589948162 1362667.0575214315 0, -102157.92780208499 1362262.3484575767 0, -102548.43577865354 1362267.4339891768 0, -102545.13293058147 1362671.733880326 0, -102541.83008083396 1363076.035208118 0)), ((-99734.74990628962 1365880.0938871626 0, -99729.35671180837 1366283.9446858987 0, -99334.7799147917 1366278.0767585489 0, -98940.21175782262 1366272.227168054 0, -98545.63430215785 1366266.395557993 0, -98151.06548972623 1366260.582284593 0, -98155.37233886408 1365854.5921900016 0, -98159.68823682536 1365448.5924035117 0, -98163.99505739895 1365042.6049710717 0, -98168.31082761876 1364636.6078466019 0, -98563.9664243743 1364644.5602801568 0, -98959.63056103289 1364652.5309624616 0, -99355.2850850141 1364660.5199345532 0, -99750.94814261008 1364668.5272563621 0, -99745.54567280188 1365072.3851220692 0, -99740.1523699373 1365476.2332864106 0, -99734.74990628962 1365880.0938871626 0)), ((-98955.79432428216 1377688.1803242203 0, -98917.99118276802 1377641.1101445598 0, -99195.48779499388 1377646.368648644 0, -99601.19158012232 1377654.0666464702 0, -99995.26492624295 1377657.3720291217 0, -99981.16310940539 1378079.5059332703 0, -99586.05931410841 1378075.1704327862 0, -99530.032008975 1378074.2503250954 0, -99521.73976613203 1378058.3481883977 0, -99487.67313503713 1378007.6472632685 0, -99415.51457544012 1378003.2159107933 0, -99357.75618625492 1378002.545513377 0, -99302.88611474879 1378001.9090236642 0, -99251.19584819191 1377976.168349558 0, -99214.21553038967 1377950.74404423 0, -99186.77538276323 1377926.7847574505 0, -99131.10156645518 1377878.1744807821 0, -99014.89681624496 1377763.447856979 0, -98955.79432428216 1377688.1803242203 0)), ((-96286.92104942148 1319660.9570627061 0, -96290.01249661167 1319262.6813293293 0, -96692.63303787177 1319268.4729105101 0, -97095.2622540194 1319274.283441073 0, -97089.73853521986 1319672.8228017907 0, -97084.21492021649 1320071.363711811 0, -96684.0359216843 1320065.2898139246 0, -96688.33447855698 1319666.880688248 0, -96286.92104942148 1319660.9570627061 0)), ((-95060.57305286372 1322483.7821040847 0, -94666.73290640632 1322479.862286979 0, -94272.88345413977 1322475.9716132854 0, -93879.04302851914 1322472.0878466617 0, -93880.68048458015 1322068.3486240564 0, -93882.31783722047 1321664.5996829926 0, -94278.7924578784 1321668.7133791784 0, -94675.25777321019 1321672.8565329968 0, -95071.73201943234 1321677.0067037197 0, -95468.20612250286 1321681.1752141952 0, -95461.30956378837 1322084.4412489352 0, -95454.4222228463 1322487.7088284758 0, -95060.57305286372 1322483.7821040847 0)), ((-95327.72497813536 1331803.4348303531 0, -95323.26354247855 1332205.8920683125 0, -94927.37715498416 1332207.9301497634 0, -94531.49129314635 1332209.9753252422 0, -94534.5646024337 1331804.5041405042 0, -94137.98928127349 1331805.0717746578 0, -94140.37273027873 1331398.0952267894 0, -93743.1076631912 1331397.1744426144 0, -93744.8006867957 1330988.7037487181 0, -93746.49358877413 1330580.2234337323 0, -94145.14776910836 1330584.1577880816 0, -94543.80195197617 1330588.099457582 0, -94942.45585484299 1330592.0708340271 0, -95341.10966091443 1330596.049421947 0, -95336.64803589275 1330998.513556141 0, -95332.18663370085 1331400.967931103 0, -95327.72497813536 1331803.4348303531 0)), ((-95247.10263417117 1341937.5012440565 0, -94848.94014662055 1341936.513516581 0, -94852.87626839062 1341532.6172776767 0, -94856.81226307341 1341128.7225433027 0, -94458.95821681932 1341127.5552931167 0, -94061.11330689638 1341126.3953836253 0, -94056.86903967829 1341530.4882026734 0, -94052.61558376566 1341934.5934467856 0, -93654.45341267584 1341933.6611010921 0, -93658.86100411288 1341529.456816953 0, -93663.26856798945 1341125.2539397923 0, -93667.67620030264 1340721.0525749398 0, -93672.08370891758 1340316.8525160432 0, -94069.6110191352 1340318.2030577424 0, -94467.14756420227 1340319.5609462627 0, -94864.67491621211 1340320.9483156828 0, -95262.21160202003 1340322.3429344578 0, -95258.42988950148 1340726.1359102987 0, -95254.65731497548 1341129.9192775793 0, -95250.8754550776 1341533.7150680784 0, -95247.10263417117 1341937.5012440565 0)), ((-95095.94296745861 1350846.875847642 0, -95091.46267131959 1351251.1117001404 0, -95086.98245370362 1351655.348928037 0, -94689.32565794382 1351649.2542129965 0, -94291.66874296012 1351643.1668289197 0, -93894.01133445097 1351637.1089661221 0, -93496.35361177518 1351631.0584279988 0, -93497.64447429673 1351228.4989271294 0, -93498.94416649269 1350825.9296715676 0, -93898.19207262916 1350831.1354480395 0, -94297.43948811143 1350836.371052303 0, -94300.32929549739 1350432.969813506 0, -94303.21887835217 1350029.56984366 0, -94342.1534672428 1350029.9981782548 0, -94381.04467838981 1350030.424566107 0, -94542.16760933714 1350032.1984557344 0, -94704.05665073595 1350033.9796414732 0, -94743.17657445904 1350034.411754494 0, -94782.25261882809 1350034.8421070394 0, -95104.90339875617 1350038.4082622556 0, -95100.42314389057 1350442.6413658157 0, -95095.94296745861 1350846.875847642 0)), ((-94213.24021151215 1361351.6465783715 0, -93817.05525522931 1361346.8905808476 0, -93420.87019046245 1361342.141664712 0, -93424.25547880038 1360936.157636792 0, -93427.6408718444 1360530.1637619233 0, -93431.0259867389 1360124.1824349186 0, -93434.4111040335 1359718.191361686 0, -93834.10177058064 1359724.2655063493 0, -94233.80134171344 1359730.3473342166 0, -94633.49129712266 1359736.4587761112 0, -95033.19005783956 1359742.5777974697 0, -95026.28998127709 1360147.2430510272 0, -95019.39925707335 1360551.8986264733 0, -94621.46234923009 1360546.437220298 0, -94615.44353939676 1360951.4284170317 0, -94218.37819917835 1360946.3196813434 0, -94213.24021151215 1361351.6465783715 0)), ((-89873.91094203436 1326093.7915373493 0, -89878.28548757899 1325691.1426088498 0, -90277.8545536678 1325694.0326945854 0, -90677.42331819741 1325696.9410009175 0, -90671.48337651572 1326097.6601207866 0, -90665.54361428751 1326498.3806817373 0, -90267.5400353105 1326497.402193925 0, -89869.53631778796 1326496.453116449 0, -89873.91094203436 1326093.7915373493 0)), ((-85462.64316839623 1332148.4822658612 0, -85063.38779143717 1332144.5292199447 0, -84664.13231411656 1332140.594678898 0, -84264.87663900862 1332136.6786395416 0, -84268.86273189657 1331729.9315276747 0, -84272.84885239214 1331323.1857768183 0, -84276.83499740715 1330916.4414892388 0, -84280.82106474692 1330509.6987641272 0, -84677.72754587787 1330513.5915418614 0, -85074.64294732873 1330517.502800433 0, -85471.54902339615 1330521.4322789428 0, -85868.46401956545 1330525.3801377406 0, -85866.81843513895 1330932.1463462012 0, -85865.18169611928 1331338.91399824 0, -85863.53554938945 1331745.6831336871 0, -85861.89834421746 1332152.4538137084 0, -85462.64316839623 1332148.4822658612 0)), ((-89392.04256851034 1337041.255896904 0, -88994.71915574066 1337038.4245959423 0, -88998.88323074621 1336636.3612499253 0, -89003.04726733199 1336234.2993163497 0, -89007.21126545618 1335832.2387966 0, -89403.58637308462 1335832.497739669 0, -89399.73838774537 1336235.423136261 0, -89796.42061506204 1336236.5540568526 0, -89792.89775457456 1336640.3347410667 0, -89789.3658654702 1337044.1055735438 0, -89392.04256851034 1337041.255896904 0)), ((-86582.06438243955 1339849.0998243566 0, -86587.31623213795 1339447.3061401767 0, -86982.95312488644 1339451.0956699217 0, -86976.41171070383 1339852.5406159344 0, -86582.06438243955 1339849.0998243566 0)), ((-85370.48598387977 1341838.487575738 0, -84972.99001703064 1341839.25121998 0, -84575.49436805543 1341840.0332193377 0, -84177.9989364577 1341840.833671377 0, -84184.38592606629 1341435.3621953204 0, -84190.78218215148 1341029.8922133974 0, -84197.16955816152 1340624.423569045 0, -84203.56629671264 1340218.9565255474 0, -84600.3897266625 1340222.4357439124 0, -84997.2221212728 1340225.9221027067 0, -85394.04524398706 1340229.4380441941 0, -85790.87742726553 1340232.961129405 0, -85785.15334985219 1340634.159928373 0, -85779.42947184666 1341035.349022609 0, -85773.70571705312 1341436.5506077677 0, -85767.98216481121 1341837.7423845246 0, -85370.48598387977 1341838.487575738 0)), ((-90104.74292082452 1345151.5885920723 0, -90497.23884943283 1345152.7125127965 0, -90494.32349436708 1345559.5189055162 0, -90491.41700768624 1345966.326786169 0, -90488.50134206322 1346373.1359976172 0, -90485.59454489786 1346779.946694111 0, -90092.12996023234 1346779.2264435198 0, -89698.66674860203 1346778.524256114 0, -89305.203623395 1346777.840091793 0, -88911.74058314516 1346777.1740512426 0, -88915.61563734534 1346369.9595812662 0, -88919.4997981523 1345962.7354014635 0, -88923.3747367545 1345555.5237513713 0, -88927.25878187078 1345148.3023944127 0, -89319.75332988861 1345149.383597231 0, -89712.24810421921 1345150.4715308438 0, -90104.74292082452 1345151.5885920723 0)), ((-84762.6191761541 1351547.25739327 0, -84364.23862243853 1351543.3356580238 0, -83965.86698198892 1351539.432625941 0, -83966.42271369991 1351132.1693339376 0, -83966.97819516354 1350724.8962403657 0, -83967.53324410347 1350317.6357437402 0, -83968.08804257614 1349910.3654485485 0, -84092.05229056724 1349909.899177103 0, -84366.13522299187 1349916.4132900054 0, -84491.10405504167 1349919.375924036 0, -84764.17548609943 1349925.8817304224 0, -84890.15494891004 1349928.8824030315 0, -85129.17117589164 1349934.5809111614 0, -85162.22414292095 1349935.368582674 0, -85161.90987928574 1350339.9671617982 0, -84763.78783232978 1350332.5048846877 0, -84763.39867314625 1350737.417304489 0, -85161.60387483948 1350743.7054901912 0, -85559.81757981764 1350750.0122777126 0, -85559.59432593666 1351152.5890798052 0, -85559.3707415262 1351555.15615189 0, -85160.99060141247 1351551.1974743458 0, -84762.6191761541 1351547.25739327 0)), ((-90301.31945031024 1355641.5230293234 0, -90299.83538632035 1356044.1067645405 0, -89902.5326184986 1356040.4627761145 0, -89903.15321540358 1355636.7061414868 0, -89504.97845649054 1355631.8966055287 0, -89505.23919539449 1356036.8485857365 0, -89107.93676381417 1356033.241522165 0, -89106.81234722146 1355627.1168537703 0, -88708.64614877533 1355622.3444126442 0, -88706.6487796565 1355215.0372772177 0, -88704.66341789975 1354807.7218243282 0, -89104.56634809003 1354814.8619871135 0, -89504.47780625382 1354822.0096432746 0, -89904.37975625691 1354829.1871417207 0, -90304.2908254913 1354836.3721521231 0, -90302.80322658127 1355238.9518465446 0, -90301.31945031024 1355641.5230293234 0)), ((-89785.02194300582 1364546.0266494376 0, -90184.16598227297 1364548.9272798607 0, -90179.53939209731 1364956.208592455 0, -89780.93927168063 1364953.089866062 0, -89785.02194300582 1364546.0266494376 0)), ((-80799.97995746662 1325580.302377365 0, -81195.76949184874 1325583.5966645654 0, -81189.49393958123 1325992.0131164284 0, -81183.2276701944 1326400.4199374425 0, -80785.9340656138 1326396.462904543 0, -80792.95687212882 1325988.3762474179 0, -80799.97995746662 1325580.302377365 0)), ((-80388.6401786564 1326392.52418571 0, -79991.35513155154 1326388.6039613967 0, -79594.06087995468 1326384.7019772595 0, -79603.34464951337 1325977.6091314107 0, -79612.62899227107 1325570.5065677096 0, -80008.40970609387 1325573.757329047 0, -79999.88220545046 1325981.1798539602 0, -80396.41967960673 1325984.7688946237 0, -80388.6401786564 1326392.52418571 0)), ((-80380.87012757928 1326800.2810386992 0, -80373.09108397418 1327208.0391856362 0, -79974.29291437658 1327203.4676268392 0, -79982.81946598238 1326796.029371597 0, -80380.87012757928 1326800.2810386992 0)), ((-80305.82441855293 1336107.7487284455 0, -80302.3704246819 1336513.229768665 0, -79904.03005415354 1336507.8219766782 0, -79908.1434077422 1336102.3470875816 0, -80305.82441855293 1336107.7487284455 0)), ((-81013.45465693536 1345051.287165079 0, -81008.27871908368 1345453.3704451846 0, -81003.11184112068 1345855.4552845168 0, -80997.93618074385 1346257.5413310383 0, -80992.76958026022 1346659.6289340076 0, -80595.57362802714 1346654.6088876997 0, -80198.38650409965 1346649.607259088 0, -79801.18996247614 1346644.6239875553 0, -79404.00225242287 1346639.6591334753 0, -79409.48876685307 1346232.0349942157 0, -79414.97539499144 1345824.4122671352 0, -79420.462136807 1345416.7909536967 0, -79425.94909136562 1345009.171058438 0, -79822.82668711226 1345019.6725616166 0, -80219.70346454124 1345030.1924132481 0, -80616.57952108866 1345040.7306164335 0, -81013.45465693536 1345051.287165079 0)), ((-81773.87981359164 1348280.6762791753 0, -81373.62349010532 1348277.7500827918 0, -81377.80132169773 1347874.2599434445 0, -81381.97908148414 1347470.7712859777 0, -81780.88517624978 1347474.3336095726 0, -82179.79117583914 1347477.914574522 0, -82578.69708163125 1347481.514080128 0, -82576.53997498205 1347884.0597994502 0, -82176.96365023943 1347880.7671029705 0, -81777.37796721784 1347877.5042635498 0, -81773.87981359164 1348280.6762791753 0)), ((-85123.07061109714 1354783.028855541 0, -84730.06537272964 1354773.568375163 0, -84731.62660155598 1354370.791390712 0, -84733.1965876097 1353968.015841628 0, -85127.98090947427 1353974.6956221673 0, -85125.52133159868 1354378.8615173313 0, -85123.07061109714 1354783.028855541 0)), ((-79965.96531516378 1354727.0426253416 0, -80361.4188503601 1354730.7341813524 0, -80756.87239218365 1354734.4439412414 0, -80752.06036551941 1355135.2768350842 0, -80747.24991202644 1355536.112933869 0, -80742.4395973606 1355936.9504761812 0, -80737.62942155407 1356337.78946063 0, -80343.95150792136 1356335.383512764 0, -79950.2736040019 1356332.9956526326 0, -79556.59571138678 1356330.6258801208 0, -79162.91772955026 1356328.2742928325 0, -79165.95250255754 1355926.131605321 0, -79168.98719606429 1355523.9903677825 0, -79172.0218069742 1355121.8506824472 0, -79175.05747236262 1354719.7143015212 0, -79570.51148791319 1354723.3693646872 0, -79567.02720568898 1355125.1770650526 0, -79563.552964215 1355526.9993444092 0, -79958.118684613 1355530.0153137099 0, -79962.04129822708 1355128.532916322 0, -79965.96531516378 1354727.0426253416 0)), ((-83537.41339989145 1356370.2489600123 0, -83534.47965100185 1356777.1730823973 0, -83125.52260219482 1356767.0816785018 0, -83128.81161201345 1356357.821980564 0, -83537.41339989145 1356370.2489600123 0)), ((-71689.88500786625 1316834.233047365 0, -71722.57181780977 1316884.8044200398 0, -71385.36798467554 1316883.5519623482 0, -71379.2885019345 1317377.4381812878 0, -71011.80406304277 1317377.8179993534 0, -71017.99455141697 1316882.1984627896 0, -70650.62104509865 1316880.8608018125 0, -70655.67638920652 1316481.4698978402 0, -70348.56185943252 1316479.564780346 0, -70353.37036365265 1316102.0561474739 0, -70354.48852525945 1316014.9140816922 0, -70379.70557065666 1315986.9606902658 0, -70469.13213096831 1315944.4841234542 0, -70577.5596898122 1315913.9555263636 0, -70662.85489386959 1315914.653556432 0, -70708.00848870954 1315915.023398199 0, -70784.2938111428 1315923.5024817628 0, -70885.6185431991 1315983.236838613 0, -70964.44741229198 1316070.2862892987 0, -71002.47477607004 1316106.0749615987 0, -71027.38848168145 1316129.516596329 0, -71078.10561444984 1316177.2577239783 0, -71279.64078626699 1316430.260834653 0, -71336.44510164211 1316485.7062702347 0, -71389.77702072014 1316524.778194359 0, -71412.34379352114 1316541.3212585317 0, -71459.61270996093 1316596.6885617347 0, -71611.1031155498 1316743.2496231515 0, -71689.88500786625 1316834.233047365 0)), ((-74862.65591483464 1322268.8725466987 0, -74866.12436761855 1321869.4271267727 0, -74869.59273938599 1321469.983056679 0, -74873.0611231356 1321070.5405424424 0, -75272.30804900322 1321074.8773840207 0, -75268.29364912861 1321475.5906897394 0, -75666.99415576836 1321481.2278606973 0, -75662.4427750188 1321883.213300992 0, -75657.88234777554 1322285.21122658 0, -75260.26495940798 1322277.0326809161 0, -74862.65591483464 1322268.8725466987 0)), ((-76464.40325504442 1321492.535515109 0, -76458.75011251168 1321897.084253459 0, -76060.59668183164 1321890.1396074262 0, -76065.7033517578 1321486.8725540864 0, -76464.40325504442 1321492.535515109 0)), ((-71661.00260202405 1326695.8473209508 0, -71280.32630450437 1326691.0575681366 0, -70901.23378088101 1326686.3088877283 0, -70896.68137886068 1327080.1689653576 0, -70494.73438150414 1327069.5103269066 0, -70218.82913195908 1327062.2012081034 0, -70223.41773430821 1326677.8516245328 0, -70228.25263518761 1326273.2765060044 0, -70233.08762554216 1325868.7027543713 0, -70237.728557169 1325480.1957385873 0, -70521.47375204678 1325480.531652975 0, -70915.15900441035 1325481.0085009348 0, -71292.09485151629 1325481.4767850852 0, -71662.81090477215 1325481.9545113277 0, -71662.20833459932 1325886.5840039244 0, -71661.6056320485 1326291.214976572 0, -71661.00260202405 1326695.8473209508 0)), ((-74785.08421722271 1331987.6057500925 0, -74788.61736198388 1331581.3025834763 0, -74792.15059244892 1331175.0009821618 0, -75187.13105894427 1331181.0127680057 0, -75582.11115001106 1331187.0426446302 0, -75579.05988072374 1331592.9346950299 0, -75576.01766951576 1331998.8169841347 0, -75180.5465475414 1331993.2078825617 0, -74785.0842172</t>
+          <t>MULTIPOLYGON Z (((-118559.78860199626 1324416.086118968 0, -118160.87134183437 1324408.490762127 0, -118166.56910121029 1323984.0706868803 0, -118171.88945702897 1323580.5591783095 0, -118571.98769600078 1323568.9705862713 0, -118566.17801895243 1323975.7536779107 0, -118559.78860199626 1324416.086118968 0)), ((-118129.64936550814 1326421.6286623029 0, -118123.17756806467 1326827.9097110208 0, -117723.13475646079 1326822.0967949047 0, -117725.91953178747 1326416.5709332328 0, -118129.64936550814 1326421.6286623029 0)), ((-116813.9391853527 1334120.0661837044 0, -116819.50557757256 1333714.8849958992 0, -116825.06969841395 1333309.8729937323 0, -117224.67568480992 1333314.982153998 0, -117625.32173768191 1333320.1129362336 0, -117621.50040622786 1333725.2494314522 0, -117617.67036619947 1334131.0138816452 0, -117214.35335177822 1334125.5108148553 0, -116813.9391853527 1334120.0661837044 0)), ((-114346.85754153511 1340631.7976945944 0, -114340.17261258581 1341032.3222610098 0, -114333.39196609255 1341438.0170531531 0, -113935.8076705649 1341428.285684852 0, -113533.73249523416 1341418.4462021037 0, -113513.00559300676 1341417.9487421208 0, -113509.74896754985 1341633.6958187832 0, -113506.86405202247 1341824.7166014917 0, -113500.59997023792 1342233.9351261824 0, -113120.16236855932 1342224.0308512778 0, -112726.20973475832 1342213.7982873933 0, -112730.42087158357 1341814.2887418289 0, -112730.44554445274 1341811.715162787 0, -112734.69771598041 1341408.3804266797 0, -112738.91680032454 1341007.5532839692 0, -112738.96903645646 1341002.8875265375 0, -112743.15224945682 1340605.4744317592 0, -113140.78893471866 1340611.9727966043 0, -113526.17196414941 1340618.2941430346 0, -113540.5318331427 1340618.5284885874 0, -113939.49722290419 1340625.0811591027 0, -114346.85754153511 1340631.7976945944 0)), ((-109522.29259002196 1345392.8853512062 0, -109515.76144907808 1345796.663347934 0, -109509.23951791451 1346200.4316081065 0, -109502.70866112935 1346604.2123752579 0, -109496.18701110258 1347007.9835038052 0, -109099.37315729806 1346999.9477500606 0, -108702.5588278943 1346991.9190399034 0, -108708.35957087454 1346587.9261491862 0, -108714.16034921788 1346183.934642002 0, -109111.70475573237 1346192.1739902063 0, -109117.86615104994 1345788.2891467095 0, -109124.02768456614 1345384.405690915 0, -109522.29259002196 1345392.8853512062 0)), ((-117844.31375286872 1345552.8724710583 0, -117838.8780229834 1345951.0468519721 0, -117439.54188566864 1345947.9080329547 0, -117444.9765387301 1345550.438690692 0, -117844.31375286872 1345552.8724710583 0)), ((-118235.0715050977 1345954.1387512595 0, -118229.5931961534 1346361.2893122216 0, -117833.35962171144 1346358.54382587 0, -117838.8780229834 1345951.0468519721 0, -118235.0715050977 1345954.1387512595 0)), ((-119012.56334631782 1346773.1815694037 0, -119008.99000898006 1347182.263837768 0, -118614.94795527779 1347178.5161622774 0, -118218.6481601709 1347174.7554020977 0, -118224.12425542329 1346768.418959465 0, -118229.5931961534 1346361.2893122216 0, -118625.83600343669 1346364.0420288965 0, -119016.10885670314 1346366.7414651362 0, -119012.56334631782 1346773.1815694037 0)), ((-117301.08470967412 1356879.1503783327 0, -117310.7717087816 1356473.5671227986 0, -117320.3959042449 1356070.6369453582 0, -117330.05388795171 1355666.5781150686 0, -117339.704855358 1355262.418665986 0, -117712.76976504254 1355269.1380548119 0, -117708.38438331963 1355674.2761722747 0, -117703.99368942676 1356078.4965027748 0, -117700.5790498014 1356481.9369705818 0, -117897.4805939922 1356486.1616319162 0, -118094.30938391492 1356490.4121007835 0, -118091.74861136051 1356893.3845473279 0, -117697.16093914752 1356886.2741512647 0, -117301.08470967412 1356879.1503783327 0)), ((-113661.71304653907 1360439.7464031598 0, -113252.63758575395 1360431.8293268944 0, -113259.49608135803 1360028.612266803 0, -113281.22580856434 1360028.9886170898 0, -113668.18565127651 1360035.796804282 0, -113661.71304653907 1360439.7464031598 0)), ((-112863.70968331992 1361239.0867491101 0, -112869.75248839286 1360833.4497317923 0, -113246.44825755537 1360838.3247476257 0, -113242.72257031559 1361088.3380283497 0, -113240.37317265633 1361243.6925950516 0, -112863.70968331992 1361239.0867491101 0)), ((-113922.04690786572 1370596.428320509 0, -113914.55181697455 1371002.1453353716 0, -113907.30260652727 1371394.8041175741 0, -113510.19296043238 1371386.5226992478 0, -113110.6876765547 1371378.2167677616 0, -113104.90696060937 1371378.095723977 0, -113109.6111976801 1370999.3948446675 0, -113112.06834764156 1370826.9819067824 0, -113115.27790131785 1370593.5079743771 0, -112731.9635684356 1370588.2100647641 0, -112351.20759482418 1370582.9738857518 0, -112351.5810685068 1370557.9392696826 0, -112357.21124630433 1370177.4845635628 0, -112357.53206439978 1370155.7737209897 0, -112363.48297540058 1369753.6206613558 0, -112745.04958382217 1369762.3486859244 0, -113125.6711244621 1369771.0810456818 0, -113144.80813151246 1369771.5128189307 0, -113530.40020495799 1369780.3736350846 0, -113539.96414796117 1369780.589944662 0, -113936.93857857028 1369789.731821339 0, -113929.53299215686 1370190.723731397 0, -113922.04690786572 1370596.428320509 0)), ((-112213.06162542276 1379891.3558927109 0, -112220.79219565334 1379485.803162598 0, -112609.9774005436 1379490.4777110198 0, -112984.98523679533 1379494.9943494613 0, -112979.34421856757 1379908.5447852528 0, -112973.97246560524 1380307.8385735457 0, -112601.60897410054 1380303.3566903046 0, -112205.30836661912 1380298.6559525274 0, -112212.99237908436 1379895.2617520043 0, -112213.06162542276 1379891.3558927109 0)), ((-113122.94207407821 1389672.853007615 0, -113111.83349464808 1389676.960075897 0, -113101.15937811643 1389682.1924448288 0, -113089.24748180441 1389692.6702343072 0, -113079.64368855588 1389705.30571605 0, -113077.52000328319 1389708.7112633495 0, -113055.81971625051 1389725.534012182 0, -112948.2141739142 1389724.1902562384 0, -112903.67756781167 1389695.6227126569 0, -112901.23152089251 1389693.0931024007 0, -112898.11914017197 1389690.5889833216 0, -112886.89391179131 1389684.8570107596 0, -112866.24319305625 1389671.6108216338 0, -112867.00082935549 1389633.9832180613 0, -112875.13136002039 1389226.6271241426 0, -112887.78320501046 1389226.8613254253 0, -113269.74409676601 1389234.0173980554 0, -113288.7217694023 1389234.3695200658 0, -113646.65481177715 1389241.089758895 0, -113643.33149232288 1389576.144883839 0, -113642.86860797573 1389623.112974984 0, -113642.65261038295 1389644.08948513 0, -113638.56487203838 1390056.2133263082 0, -113257.79085354638 1390049.0573441545 0, -113255.60916345123 1390045.8369991586 0, -113262.69445577585 1389639.0925695903 0, -113263.67508583379 1389582.7387953566 0, -113135.14721657618 1389664.0368250036 0, -113124.28179675284 1389672.460042096 0, -113122.94207407821 1389672.853007615 0)), ((-108961.60580476526 1326324.8954503047 0, -108965.83956777902 1325922.4463640077 0, -109367.46586635518 1325927.5351789834 0, -109362.26279785884 1326329.971983933 0, -108961.60580476526 1326324.8954503047 0)), ((-102165.12112157764 1327427.009226146 0, -102170.40185537828 1327020.9767840875 0, -102175.68258514833 1326614.945909763 0, -102586.620427456 1326627.2472273542 0, -102984.22672161988 1326639.151478595 0, -102978.2455285201 1327043.0257256723 0, -102972.27347042694 1327446.901605464 0, -102573.77443063777 1327437.0790865377 0, -102165.12112157764 1327427.009226146 0)), ((-103317.85927134845 1331916.525398105 0, -103322.053671023 1331509.3547327637 0, -103721.70084824732 1331514.1595532878 0, -104121.34764388262 1331518.983083842 0, -104117.45918715191 1331926.1575769382 0, -104113.57086320131 1332333.3224353741 0, -103713.61792538497 1332328.4950716635 0, -103313.67393238138 1332323.6864016554 0, -103317.85927134845 1331916.525398105 0)), ((-100891.15515543938 1332697.458156693 0, -100887.60633158246 1333102.503157431 0, -100493.05395471178 1333097.0268983683 0, -100495.96559821334 1332693.0599392357 0, -100891.15515543938 1332697.458156693 0)), ((-104398.06590818788 1342065.4996272956 0, -103995.86442064783 1342056.7647781668 0, -104001.61333695416 1341652.7881969006 0, -104007.36227092014 1341248.8130165916 0, -104013.11136422343 1340844.828041519 0, -104018.86042941852 1340440.8557713237 0, -104421.53526639382 1340446.6084159294 0, -104824.2188797988 1340452.3689289498 0, -104818.2330655357 1340857.837888466 0, -104812.24726800816 1341263.3082598455 0, -104806.26148726072 1341668.7800416395 0, -104800.2759184653 1342074.2533393656 0, -104398.06590818788 1342065.4996272956 0)), ((-107929.24767328279 1345359.0781114774 0, -108327.50522301492 1345367.5021215314 0, -108725.7712746039 1345375.9447684663 0, -108719.9703296113 1345779.9334003902 0, -108322.06481974282 1345771.607228296 0, -107924.16795344326 1345763.2884924468 0, -107929.24767328279 1345359.0781114774 0)), ((-108156.8382428046 1355897.4865566047 0, -108554.64924378692 1355903.371034482 0, -108553.37753496063 1356303.3893586586 0, -108154.89678118152 1356297.720158007 0, -108152.95480976794 1356697.9661848047 0, -107753.80413908714 1356692.5196739826 0, -107756.41547691992 1356292.080664773 0, -107759.03581087208 1355891.6318686488 0, -108156.8382428046 1355897.4865566047 0)), ((-108951.2555620091 1356708.9039511657 0, -108552.10541081056 1356703.4202130258 0, -108553.37753496063 1356303.3893586586 0, -108951.85807751214 1356309.0770744418 0, -108951.2555620091 1356708.9039511657 0)), ((-102541.83008083396 1363076.035208118 0, -102150.47463689576 1363071.7789349912 0, -102154.20589948162 1362667.0575214315 0, -102157.92780208499 1362262.3484575767 0, -102548.43577865354 1362267.4339891768 0, -102545.13293058147 1362671.733880326 0, -102541.83008083396 1363076.035208118 0)), ((-109273.28425350602 1366434.420824356 0, -108875.25755466968 1366429.3563738924 0, -108477.23054482524 1366424.3103915248 0, -108079.20332163286 1366419.2829810695 0, -107681.17598890651 1366414.2740446865 0, -107684.87722985457 1366009.9773468818 0, -107688.58751344724 1365605.682151466 0, -108086.12165878483 1365611.3339859117 0, -108483.66475698304 1365616.9931753941 0, -108881.1983745591 1365622.6819573413 0, -109278.74084270338 1365628.3780914135 0, -109276.00817302614 1366031.3987132914 0, -109273.28425350602 1366434.420824356 0)), ((-104447.36326426534 1370445.1188663272 0, -104047.19228134869 1370434.9115411886 0, -103647.011806099 1370424.7115017676 0, -103642.15577842157 1370827.5309039277 0, -103637.29089125487 1371230.3403210002 0, -103236.4600106018 1371220.3863003133 0, -102835.63768349009 1371210.4399225463 0, -102841.15191703259 1370807.4144446405 0, -102846.6664095676 1370404.3791638564 0, -102852.18078206544 1370001.356275659 0, -102857.69531435877 1369598.323584405 0, -103257.2187544394 1369608.702077609 0, -103656.74162271575 1369619.0880361076 0, -104056.26362838647 1369629.5039594988 0, -104455.78496295503 1369639.9272442826 0, -104451.5696211929 1370042.5279194922 0, -104447.36326426534 1370445.1188663272 0)), ((-107928.2746291788 1376178.824992988 0, -107528.28197644571 1376175.0805355113 0, -107536.46064962691 1375771.2336784373 0, -107544.6398091161 1375367.3770024648 0, -107552.81907170058 1374963.5328050556 0, -107560.9988205348 1374559.6787916836 0, -107962.42259670311 1374563.0278035828 0, -108363.85543327962 1374566.384641587 0, -108354.96013123803 1374970.4308767472 0, -108346.06504034332 1375374.4894930571 0, -108337.17044171046 1375778.5382907696 0, -108328.27619479694 1376182.588367581 0, -107928.2746291788 1376178.824992988 0)), ((-104274.55049671762 1379773.4548623795 0, -103877.25748240731 1379767.438262733 0, -103479.9641675923 1379761.4400782376 0, -103483.32961744542 1379355.1822972533 0, -103881.41934760772 1379360.8765586729 0, -104279.50891886503 1379366.5782389475 0, -104274.55049671762 1379773.4548623795 0)), ((-103473.2416502126 1380573.9709581828 0, -103868.94245419104 1380580.5766924797 0, -104264.63372897323 1380587.2007520343 0, -104259.6754825904 1380994.0700183294 0, -103864.7803105215 1380987.1422333217 0, -103469.8847293741 1380980.2327532428 0, -103473.2416502126 1380573.9709581828 0)), ((-98991.5661045002 1325759.4310509183 0, -99390.12364883219 1325762.3068798182 0, -99386.81964058286 1326167.7425183088 0, -98988.28516351998 1326165.2809846643 0, -98589.74147803921 1326162.8488951274 0, -98593.01757595724 1325756.5626311009 0, -98991.5661045002 1325759.4310509183 0)), ((-100177.24310694287 1326981.873440304 0, -100173.92021743058 1327386.451818234 0, -99775.4179608111 1327385.2403088382 0, -99376.92498514801 1327384.0473035218 0, -98978.42294119613 1327382.8727389507 0, -98579.93017844533 1327381.7167789293 0, -98583.19773121837 1326975.4259185295 0, -98586.47418026078 1326569.1367086126 0, -98984.99493666277 1326571.143408437 0, -98981.71351301535 1326977.0073775554 0, -99380.22032794954 1326978.6071825796 0, -99383.5245376473 1326573.179703947 0, -99782.04530522341 1326575.223253798 0, -100180.5750486242 1326577.2854055134 0, -100177.24310694287 1326981.873440304 0)), ((-100068.65664579772 1336750.691630401 0, -100062.91137551065 1337154.8638156527 0, -99666.97939251801 1337150.2685202803 0, -99271.05626663935 1337145.6915811314 0, -98875.12385117913 1337141.1328395032 0, -98479.20029912573 1337136.5923530518 0, -98484.16613474589 1336732.411078889 0, -98489.14098401606 1336328.231405308 0, -98494.10680073017 1335924.053077485 0, -98499.0816341248 1335519.8762522473 0, -98895.7848362916 1335524.4256152022 0, -99292.48777789096 1335528.9932619545 0, -99689.19055332465 1335533.5792964867 0, -100085.89306490228 1335538.1836150372 0, -100080.14749052795 1335942.3515286644 0, -100074.40201748101 1336346.5208675978 0, -100068.65664579772 1336750.691630401 0)), ((-100000.36157028419 1345251.1909587882 0, -99998.40892166083 1345655.4372363847 0, -99996.45605946124 1346059.6848078172 0, -99994.50287853723 1346463.9338702364 0, -99594.96544573244 1346458.9808477743 0, -99592.59838367256 1346863.1256108624 0, -99192.65628230856 1346858.0744326126 0, -98792.70474837693 1346853.053025073 0, -98795.88968063382 1346449.130553352 0, -98396.35144772787 1346444.233385091 0, -98399.94081001657 1346040.4178101674 0, -98403.52992152468 1345636.6147200926 0, -98802.2500783041 1345641.2897977824 0, -98799.06537319074 1346045.209490217 0, -99198.19879570323 1346050.0198024155 0, -99200.96997364855 1345645.983325844 0, -99203.74069380149 1345241.9595350488 0, -99602.04675429677 1345246.5659320583 0, -100000.36157028419 1345251.1909587882 0)), ((-99824.13065494676 1356158.1200580532 0, -99820.50487867782 1356558.9707754594 0, -99421.66116435213 1356555.628117643 0, -99022.82640782211 1356552.3041480414 0, -98623.98256400043 1356548.9987095296 0, -98225.1476843331 1356545.711858135 0, -98230.80786065722 1356141.89633271 0, -98236.46828051217 1355738.070860022 0, -98242.12865376448 1355334.2580393278 0, -98247.79213183348 1354930.4357668527 0, -98644.59260406076 1354936.6987964418 0, -99041.40176313117 1354942.9692146222 0, -99438.20148389338 1354949.268964337 0, -99835.00999046354 1354955.5760050435 0, -99831.3819227015 1355356.422631429 0, -99827.75623721641 1355757.2706731658 0, -99824.13065494676 1356158.1200580532 0)), ((-99734.74990628962 1365880.0938871626 0, -99729.35671180837 1366283.9446858987 0, -99334.7799147917 1366278.0767585489 0, -98940.21175782262 1366272.227168054 0, -98545.63430215785 1366266.395557993 0, -98151.06548972623 1366260.582284593 0, -98155.37233886408 1365854.5921900016 0, -98159.68823682536 1365448.5924035117 0, -98163.99505739895 1365042.6049710717 0, -98168.31082761876 1364636.6078466019 0, -98563.9664243743 1364644.5602801568 0, -98959.63056103289 1364652.5309624616 0, -99355.2850850141 1364660.5199345532 0, -99750.94814261008 1364668.5272563621 0, -99745.54567280188 1365072.3851220692 0, -99740.1523699373 1365476.2332864106 0, -99734.74990628962 1365880.0938871626 0)), ((-99995.26492624295 1377657.3720291217 0, -99981.16310940539 1378079.5059332703 0, -99586.05931410841 1378075.1704327862 0, -99530.032008975 1378074.2503250954 0, -99521.73976613203 1378058.3481883977 0, -99487.67313503713 1378007.6472632685 0, -99415.51457544012 1378003.2159107933 0, -99357.75618625492 1378002.545513377 0, -99302.88611474879 1378001.9090236642 0, -99251.19584819191 1377976.168349558 0, -99214.21553038967 1377950.74404423 0, -99186.77538276323 1377926.7847574505 0, -99131.10156645518 1377878.1744807821 0, -99014.89681624496 1377763.447856979 0, -98955.79432428216 1377688.1803242203 0, -98917.99118276802 1377641.1101445598 0, -99195.48779499388 1377646.368648644 0, -99601.19158012232 1377654.0666464702 0, -99995.26492624295 1377657.3720291217 0)), ((-96286.92104942148 1319660.9570627061 0, -96290.01249661167 1319262.6813293293 0, -96692.63303787177 1319268.4729105101 0, -97095.2622540194 1319274.283441073 0, -97089.73853521986 1319672.8228017907 0, -97084.21492021649 1320071.363711811 0, -96684.0359216843 1320065.2898139246 0, -96688.33447855698 1319666.880688248 0, -96286.92104942148 1319660.9570627061 0)), ((-95060.57305286372 1322483.7821040847 0, -94666.73290640632 1322479.862286979 0, -94272.88345413977 1322475.9716132854 0, -93879.04302851914 1322472.0878466617 0, -93880.68048458015 1322068.3486240564 0, -93882.31783722047 1321664.5996829926 0, -94278.7924578784 1321668.7133791784 0, -94675.25777321019 1321672.8565329968 0, -95071.73201943234 1321677.0067037197 0, -95468.20612250286 1321681.1752141952 0, -95461.30956378837 1322084.4412489352 0, -95454.4222228463 1322487.7088284758 0, -95060.57305286372 1322483.7821040847 0)), ((-95327.72497813536 1331803.4348303531 0, -95323.26354247855 1332205.8920683125 0, -94927.37715498416 1332207.9301497634 0, -94531.49129314635 1332209.9753252422 0, -94534.5646024337 1331804.5041405042 0, -94137.98928127349 1331805.0717746578 0, -94140.37273027873 1331398.0952267894 0, -93743.1076631912 1331397.1744426144 0, -93744.8006867957 1330988.7037487181 0, -93746.49358877413 1330580.2234337323 0, -94145.14776910836 1330584.1577880816 0, -94543.80195197617 1330588.099457582 0, -94942.45585484299 1330592.0708340271 0, -95341.10966091443 1330596.049421947 0, -95336.64803589275 1330998.513556141 0, -95332.18663370085 1331400.967931103 0, -95327.72497813536 1331803.4348303531 0)), ((-95250.8754550776 1341533.7150680784 0, -95247.10263417117 1341937.5012440565 0, -94848.94014662055 1341936.513516581 0, -94852.87626839062 1341532.6172776767 0, -94856.81226307341 1341128.7225433027 0, -94458.95821681932 1341127.5552931167 0, -94061.11330689638 1341126.3953836253 0, -94056.86903967829 1341530.4882026734 0, -94052.61558376566 1341934.5934467856 0, -93654.45341267584 1341933.6611010921 0, -93658.86100411288 1341529.456816953 0, -93663.26856798945 1341125.2539397923 0, -93667.67620030264 1340721.0525749398 0, -93672.08370891758 1340316.8525160432 0, -94069.6110191352 1340318.2030577424 0, -94467.14756420227 1340319.5609462627 0, -94864.67491621211 1340320.9483156828 0, -95262.21160202003 1340322.3429344578 0, -95258.42988950148 1340726.1359102987 0, -95254.65731497548 1341129.9192775793 0, -95250.8754550776 1341533.7150680784 0)), ((-95095.94296745861 1350846.875847642 0, -95091.46267131959 1351251.1117001404 0, -95086.98245370362 1351655.348928037 0, -94689.32565794382 1351649.2542129965 0, -94291.66874296012 1351643.1668289197 0, -93894.01133445097 1351637.1089661221 0, -93496.35361177518 1351631.0584279988 0, -93497.64447429673 1351228.4989271294 0, -93498.94416649269 1350825.9296715676 0, -93898.19207262916 1350831.1354480395 0, -94297.43948811143 1350836.371052303 0, -94300.32929549739 1350432.969813506 0, -94303.21887835217 1350029.56984366 0, -94342.1534672428 1350029.9981782548 0, -94381.04467838981 1350030.424566107 0, -94542.16760933714 1350032.1984557344 0, -94704.05665073595 1350033.9796414732 0, -94743.17657445904 1350034.411754494 0, -94782.25261882809 1350034.8421070394 0, -95104.90339875617 1350038.4082622556 0, -95100.42314389057 1350442.6413658157 0, -95095.94296745861 1350846.875847642 0)), ((-94213.24021151215 1361351.6465783715 0, -93817.05525522931 1361346.8905808476 0, -93420.87019046245 1361342.141664712 0, -93424.25547880038 1360936.157636792 0, -93427.6408718444 1360530.1637619233 0, -93431.0259867389 1360124.1824349186 0, -93434.4111040335 1359718.191361686 0, -93834.10177058064 1359724.2655063493 0, -94233.80134171344 1359730.3473342166 0, -94633.49129712266 1359736.4587761112 0, -95033.19005783956 1359742.5777974697 0, -95026.28998127709 1360147.2430510272 0, -95019.39925707335 1360551.8986264733 0, -94621.46234923009 1360546.437220298 0, -94615.44353939676 1360951.4284170317 0, -94218.37819917835 1360946.3196813434 0, -94213.24021151215 1361351.6465783715 0)), ((-89873.91094203436 1326093.7915373493 0, -89878.28548757899 1325691.1426088498 0, -90277.8545536678 1325694.0326945854 0, -90677.42331819741 1325696.9410009175 0, -90671.48337651572 1326097.6601207866 0, -90665.54361428751 1326498.3806817373 0, -90267.5400353105 1326497.402193925 0, -89869.53631778796 1326496.453116449 0, -89873.91094203436 1326093.7915373493 0)), ((-85462.64316839623 1332148.4822658612 0, -85063.38779143717 1332144.5292199447 0, -84664.13231411656 1332140.594678898 0, -84264.87663900862 1332136.6786395416 0, -84268.86273189657 1331729.9315276747 0, -84272.84885239214 1331323.1857768183 0, -84276.83499740715 1330916.4414892388 0, -84280.82106474692 1330509.6987641272 0, -84677.72754587787 1330513.5915418614 0, -85074.64294732873 1330517.502800433 0, -85471.54902339615 1330521.4322789428 0, -85868.46401956545 1330525.3801377406 0, -85866.81843513895 1330932.1463462012 0, -85865.18169611928 1331338.91399824 0, -85863.53554938945 1331745.6831336871 0, -85861.89834421746 1332152.4538137084 0, -85462.64316839623 1332148.4822658612 0)), ((-89792.89775457456 1336640.3347410667 0, -89789.3658654702 1337044.1055735438 0, -89392.04256851034 1337041.255896904 0, -88994.71915574066 1337038.4245959423 0, -88998.88323074621 1336636.3612499253 0, -89003.04726733199 1336234.2993163497 0, -89007.21126545618 1335832.2387966 0, -89403.58637308462 1335832.497739669 0, -89399.73838774537 1336235.423136261 0, -89796.42061506204 1336236.5540568526 0, -89792.89775457456 1336640.3347410667 0)), ((-86582.06438243955 1339849.0998243566 0, -86587.31623213795 1339447.3061401767 0, -86982.95312488644 1339451.0956699217 0, -86976.41171070383 1339852.5406159344 0, -86582.06438243955 1339849.0998243566 0)), ((-85370.48598387977 1341838.487575738 0, -84972.99001703064 1341839.25121998 0, -84575.49436805543 1341840.0332193377 0, -84177.9989364577 1341840.833671377 0, -84184.38592606629 1341435.3621953204 0, -84190.78218215148 1341029.8922133974 0, -84197.16955816152 1340624.423569045 0, -84203.56629671264 1340218.9565255474 0, -84600.3897266625 1340222.4357439124 0, -84997.2221212728 1340225.9221027067 0, -85394.04524398706 1340229.4380441941 0, -85790.87742726553 1340232.961129405 0, -85785.15334985219 1340634.159928373 0, -85779.42947184666 1341035.349022609 0, -85773.70571705312 1341436.5506077677 0, -85767.98216481121 1341837.7423845246 0, -85370.48598387977 1341838.487575738 0)), ((-90104.74292082452 1345151.5885920723 0, -90497.23884943283 1345152.7125127965 0, -90494.32349436708 1345559.5189055162 0, -90491.41700768624 1345966.326786169 0, -90488.50134206322 1346373.1359976172 0, -90485.59454489786 1346779.946694111 0, -90092.12996023234 1346779.2264435198 0, -89698.66674860203 1346778.524256114 0, -89305.203623395 1346777.840091793 0, -88911.74058314516 1346777.1740512426 0, -88915.61563734534 1346369.9595812662 0, -88919.4997981523 1345962.7354014635 0, -88923.3747367545 1345555.5237513713 0, -88927.25878187078 1345148.3023944127 0, -89319.75332988861 1345149.383597231 0, -89712.24810421921 1345150.4715308438 0, -90104.74292082452 1345151.5885920723 0)), ((-84762.6191761541 1351547.25739327 0, -84364.23862243853 1351543.3356580238 0, -83965.86698198892 1351539.432625941 0, -83966.42271369991 1351132.1693339376 0, -83966.97819516354 1350724.8962403657 0, -83967.53324410347 1350317.6357437402 0, -83968.08804257614 1349910.3654485485 0, -84092.05229056724 1349909.899177103 0, -84366.13522299187 1349916.4132900054 0, -84491.10405504167 1349919.375924036 0, -84764.17548609943 1349925.8817304224 0, -84890.15494891004 1349928.8824030315 0, -85129.17117589164 1349934.5809111614 0, -85162.22414292095 1349935.368582674 0, -85161.90987928574 1350339.9671617982 0, -84763.78783232978 1350332.5048846877 0, -84763.39867314625 1350737.417304489 0, -85161.60387483948 1350743.7054901912 0, -85559.81757981764 1350750.0122777126 0, -85559.59432593666 1351152.5890798052 0, -85559.3707415262 1351555.15615189 0, -85160.99060141247 1351551.1974743458 0, -84762.6191761541 1351547.25739327 0)), ((-90301.31945031024 1355641.5230293234 0, -90299.83538632035 1356044.1067645405 0, -89902.5326184986 1356040.4627761145 0, -89903.15321540358 1355636.7061414868 0, -89504.97845649054 1355631.8966055287 0, -89505.23919539449 1356036.8485857365 0, -89107.93676381417 1356033.241522165 0, -89106.81234722146 1355627.1168537703 0, -88708.64614877533 1355622.3444126442 0, -88706.6487796565 1355215.0372772177 0, -88704.66341789975 1354807.7218243282 0, -89104.56634809003 1354814.8619871135 0, -89504.47780625382 1354822.0096432746 0, -89904.37975625691 1354829.1871417207 0, -90304.2908254913 1354836.3721521231 0, -90302.80322658127 1355238.9518465446 0, -90301.31945031024 1355641.5230293234 0)), ((-89785.02194300582 1364546.0266494376 0, -90184.16598227297 1364548.9272798607 0, -90179.53939209731 1364956.208592455 0, -89780.93927168063 1364953.089866062 0, -89785.02194300582 1364546.0266494376 0)), ((-80396.41967960673 1325984.7688946237 0, -80388.6401786564 1326392.52418571 0, -79991.35513155154 1326388.6039613967 0, -79594.06087995468 1326384.7019772595 0, -79603.34464951337 1325977.6091314107 0, -79612.62899227107 1325570.5065677096 0, -80008.40970609387 1325573.757329047 0, -79999.88220545046 1325981.1798539602 0, -80396.41967960673 1325984.7688946237 0)), ((-80799.97995746662 1325580.302377365 0, -81195.76949184874 1325583.5966645654 0, -81189.49393958123 1325992.0131164284 0, -81183.2276701944 1326400.4199374425 0, -80785.9340656138 1326396.462904543 0, -80792.95687212882 1325988.3762474179 0, -80799.97995746662 1325580.302377365 0)), ((-80380.87012757928 1326800.2810386992 0, -80373.09108397418 1327208.0391856362 0, -79974.29291437658 1327203.4676268392 0, -79982.81946598238 1326796.029371597 0, -80380.87012757928 1326800.2810386992 0)), ((-80305.82441855293 1336107.7487284455 0, -80302.3704246819 1336513.229768665 0, -79904.03005415354 1336507.8219766782 0, -79908.1434077422 1336102.3470875816 0, -80305.82441855293 1336107.7487284455 0)), ((-81013.45465693536 1345051.287165079 0, -81008.27871908368 1345453.3704451846 0, -81003.11184112068 1345855.4552845168 0, -80997.93618074385 1346257.5413310383 0, -80992.76958026022 1346659.6289340076 0, -80595.57362802714 1346654.6088876997 0, -80198.38650409965 1346649.607259088 0, -79801.18996247614 1346644.6239875553 0, -79404.00225242287 1346639.6591334753 0, -79409.48876685307 1346232.0349942157 0, -79414.97539499144 1345824.4122671352 0, -79420.462136807 1345416.7909536967 0, -79425.94909136562 1345009.171058438 0, -79822.82668711226 1345019.6725616166 0, -80219.70346454124 1345030.1924132481 0, -80616.57952108866 1345040.7306164335 0, -81013.45465693536 1345051.287165079 0)), ((-81773.87981359164 1348280.6762791753 0, -81373.62349010532 1348277.7500827918 0, -81377.80132169773 1347874.2599434445 0, -81381.97908148414 1347470.7712859777 0, -81780.88517624978 1347474.3336095726 0, -82179.79117583914 1347477.914574522 0, -82578.69708163125 1347481.514080128 0, -82576.53997498205 1347884.0597994502 0, -82176.96365023943 1347880.7671029705 0, -81777.37796721784 1347877.5042635498 0, -81773.87981359164 1348280.6762791753 0)), ((-79965.96531516378 1354727.0426253416 0, -80361.4188503601 1354730.7341813524 0, -80756.87239218365 1354734.4439412414 0, -80752.06036551941 1355135.2768350842 0, -80747.24991202644 1355536.112933869 0, -80742.4395973606 1355936.9504761812 0, -80737.62942155407 1356337.78946063 0, -80343.95150792136 1356335.383512764 0, -79950.2736040019 1356332.9956526326 0, -79556.59571138678 1356330.6258801208 0, -79162.91772955026 1356328.2742928325 0, -79165.95250255754 1355926.131605321 0, -79168.98719606429 1355523.9903677825 0, -79172.0218069742 1355121.8506824472 0, -79175.05747236262 1354719.7143015212 0, -79570.51148791319 1354723.3693646872 0, -79567.02720568898 1355125.1770650526 0, -79563.552964215 1355526.9993444092 0, -79958.118684613 1355530.0153137099 0, -79962.04129822708 1355128.532916322 0, -79965.96531516378 1354727.0426253416 0)), ((-83537.41339989145 1356370.2489600123 0, -83534.47965100185 1356777.1730823973 0, -83125.52260219482 1356767.0816785018 0, -83128.81161201345 1356357.821980564 0, -83537.41339989145 1356370.2489600123 0)), ((-71689.88500786625 1316834.233047365 0, -71722.57181780977 1316884.8044200398 0, -71385.36798467554 1316883.5519623482 0, -71379.2885019345 1317377.4381812878 0, -71011.80406304277 1317377.8179993534 0, -71017.99455141697 1316882.1984627896 0, -70650.62104509865 1316880.8608018125 0, -70655.67638920652 1316481.4698978402 0, -70348.56185943252 1316479.564780346 0, -70353.37036365265 1316102.0561474739 0, -70354.48852525945 1316014.9140816922 0, -70379.70557065666 1315986.9606902658 0, -70469.13213096831 1315944.4841234542 0, -70577.5596898122 1315913.9555263636 0, -70662.85489386959 1315914.653556432 0, -70708.00848870954 1315915.023398199 0, -70784.2938111428 1315923.5024817628 0, -70885.6185431991 1315983.236838613 0, -70964.44741229198 1316070.2862892987 0, -71002.47477607004 1316106.0749615987 0, -71027.38848168145 1316129.516596329 0, -71078.10561444984 1316177.2577239783 0, -71279.64078626699 1316430.260834653 0, -71336.44510164211 1316485.7062702347 0, -71389.77702072014 1316524.778194359 0, -71412.34379352114 1316541.3212585317 0, -71459.61270996093 1316596.6885617347 0, -71611.1031155498 1316743.2496231515 0, -71689.88500786625 1316834.233047365 0)), ((-74862.65591483464 1322268.8725466987 0, -74866.12436761855 1321869.4271267727 0, -74869.59273938599 1321469.983056679 0, -74873.0611231356 1321070.5405424424 0, -75272.30804900322 1321074.8773840207 0, -75268.29364912861 1321475.5906897394 0, -75666.99415576836 1321481.2278606973 0, -75662.4427750188 1321883.213300992 0, -75657.88234777554 1322285.21122658 0, -75260.26495940798 1322277.0326809161 0, -74862.65591483464 1322268.8725466987 0)), ((-76464.40325504442 1321492.535515109 0, -76458.75011251168 1321897.084253459 0, -76060.59668183164 1321890.1396074262 0, -76065.7033517578 1321486.8725540864 0, -76464.40325504442 1321492.535515109 0)), ((-71661.00260202405 1326695.8473209508 0, -71280.32630450437 1326691.0575681366 0, -70901.23378088101 1326686.3088877283 0, -70896.68137886068 1327080.1689653576 0, -70494.73438150414 1327069.5103269066 0, -70218.82913195908 1327062.2012081034 0, -70223.41773430821 1326677.8516245328 0, -70228.25263518761 1326273.2765060044 0, -70233.08762554216 1325868.7027543713 0, -70237.728557169 1325480.1957385873 0, -70521.47375204678 1325480.531652975 0, -70915.15900441035 1325481.0085009348 0, -71292.09485151629 1325481.4767850852 0, -71662.81090477215 1325481.9545113277 0, -71662.20833459932 1325886.5840039244 0, -71661.6056320485 1326291.214976572 0, -71661.00260202405 1326695.8473209508 0)), ((-74788.61736198388 1331581.3025834763 0, -74792.15059244892 1331175.0009821618 0, -75187.13105894427 1331181.0127680057 0, -75582.11115001106 1331187.0426446302 0, -75579.05988072374 1331592.9346950299 0, -75576.01766951576 1331998.8169841347 0, -75180.5465475414 1331993.2078825617 0, -74785.08421722271 1331987.6057500925 0, -74788.61736198388 1331581.3025834763 0)), ((-71584.02079882506 1335612.0964789405 0, -71582.03862891332 1336016.300934322 0, -71186.07845687961 1336006.975839906 0, -70790.14464259507 1335997.6802519485 0, -70785.26627548075 1336399.0312841816 0, -71182.63452621787 1336409.7597294669 0, -71580.04721257182 1336420.5068466056 0, -71578.06479805868 1336824.7142734278 0, -71179.12517518728 1336820.4554911887 0, -70780.18516264533 1336816.2264827078 0, -70369.43734184405 1336811.8859057298 0, -70133.85227089559 1336809.4040640718 0, -70136.89087416 1336381.5731850546 0, -70139.72249162063 1335982.4321935193 0, -70142.55400842211 1335583.292604567 0, -70145.38538491463 1335184.1656176054 0, -70387.08018703602 1335188.1295633488 0, -70799.91143608406 1335194.9155353433 0, -71192.95730752946 1335201.4010618003 0, -71586.01197353196 1335207.893440114 0, -71584.02079882506 1335612.0964789405 0)), ((-70701.43724967567</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Oklahoma State University, Common Schools, Normal Schools, Wildlife Conservation, Other Agency, State Educational Institutions</t>
+          <t>Oklahoma State University, Common Schools, Normal Schools, State Educational Institutions</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="G13" t="n">
         <v>3761.53</v>
@@ -1059,13 +1059,13 @@
         <v>106</v>
       </c>
       <c r="I13" t="n">
-        <v>16524.48</v>
+        <v>16164.18</v>
       </c>
       <c r="J13" t="n">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="K13" t="n">
-        <v>20286.01</v>
+        <v>19925.71</v>
       </c>
       <c r="L13" t="n">
         <v>725652.6800000001</v>
@@ -1218,7 +1218,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-26399.35398685237 1326000.0133666394 0, -25995.96996745387 1325996.625874207 0, -25592.576635622554 1325993.2685226349 0, -25594.099043366954 1325592.5081242207 0, -25595.630598020878 1325191.749269161 0, -25998.46523582459 1325191.6367746638 0, -26401.300038869995 1325191.5430964984 0, -26400.327075755373 1325595.7718909876 0, -26399.35398685237 1326000.0133666394 0)), ((-39529.226980711166 1330104.1367276963 0, -39525.72608157453 1330509.6920674623 0, -39127.838572195666 1330510.1228858428 0, -38729.95122741543 1330510.5832821408 0, -38731.851478464676 1330106.5196841168 0, -39130.539144705785 1330105.3133663572 0, -39529.226980711166 1330104.1367276963 0)), ((-35139.07853734465 1339021.298573852 0, -34738.74706374294 1339019.7538136207 0, -34740.914447515635 1338613.2309835711 0, -35141.44709580831 1338614.3962972057 0, -35139.07853734465 1339021.298573852 0)), ((-34336.43254267719 1339428.6021044143 0, -34338.424624424544 1339018.227687109 0, -34738.74706374294 1339019.7538136207 0, -34736.563128944676 1339430.3846033008 0, -34336.43254267719 1339428.6021044143 0)), ((-42876.993197154545 1380494.2518637916 0, -42875.29389178049 1380899.0362035015 0, -42477.58689898039 1380900.599397924 0, -42475.90591510374 1381305.485977029 0, -42078.21739486426 1381307.1798982997 0, -42079.871254166654 1380902.1810974954 0, -42081.533970845296 1380497.1947600073 0, -42479.25893878103 1380495.7140319387 0, -42876.993197154545 1380494.2518637916 0)), ((-48775.67752818942 1398863.7494075801 0, -48775.54639672105 1399274.058581474 0, -48377.66594092118 1399273.3008493872 0, -48378.28657226119 1398863.5317733763 0, -48775.67752818942 1398863.7494075801 0)), ((-44792.53216144727 1400068.2313686332 0, -44795.620693234436 1399660.1855093662 0, -44798.70014203372 1399252.152102546 0, -45192.98415764783 1399252.0569390927 0, -45587.27818838959 1399251.9976460421 0, -45585.02498748347 1399659.6210403387 0, -45582.76284806343 1400067.245589532 0, -45187.651348236825 1400067.726069988 0, -44792.53216144727 1400068.2313686332 0)), ((-49965.769996296774 1400906.5698350277 0, -49568.99494745188 1400907.6772872256 0, -49172.22002896872 1400908.8032385914 0, -49173.190595656364 1400502.6697555785 0, -49174.16991754589 1400096.5264679706 0, -49572.689141044815 1400096.6981562348 0, -49572.849242732176 1399686.487361107 0, -49971.9044398194 1399687.318903464 0, -50370.95064323191 1399688.1690807317 0, -50369.73679496258 1400097.097439747 0, -49971.21741352084 1400096.8885319943 0, -49968.493678153754 1400501.734178372 0, -49965.769996296774 1400906.5698350277 0)), ((-41979.47744220164 1402900.610054686 0, -42380.53691005413 1402899.774514179 0, -42384.01596812083 1402494.72263993 0, -42785.689952522145 1402493.2820256446 0, -42781.587481921495 1402898.968994993 0, -42777.48523638775 1403304.6460713127 0, -42377.04897408744 1403304.8388188186 0, -41976.62173153774 1403305.0393376478 0, -41979.47744220164 1402900.610054686 0)), ((-29178.459274632463 1403223.597371753 0, -29175.009383286055 1403630.1637615603 0, -28775.827514534387 1403623.7223585634 0, -28376.645096421125 1403617.3107573318 0, -28381.773513563672 1403209.8878311224 0, -28780.112240131755 1403216.7333134527 0, -29178.459274632463 1403223.597371753 0)), ((-32368.82905471825 1403675.5850326004 0, -32768.86913830482 1403681.7837495208 0, -33168.89981898825 1403687.9899923035 0, -33162.18951377006 1404092.8544557206 0, -32762.848985767087 1404087.0763598508 0, -32363.516948731987 1404081.3171416975 0, -32368.82905471825 1403675.5850326004 0)), ((-41969.93734505687 1404942.4397514556 0, -41568.21255516822 1404943.077918623 0, -41570.203575110885 1404533.623999832 0, -41971.60628718011 1404533.084939842 0, -41969.93734505687 1404942.4397514556 0)), ((-52714.72932805476 1407423.0993317056 0, -52316.036235955566 1407421.7269295193 0, -52321.95167778334 1407013.4437566688 0, -52327.86753668571 1406605.1617870482 0, -52727.43339117751 1406609.3278637026 0, -53126.999087072414 1406613.5015343628 0, -53120.210658749726 1407018.9898359776 0, -53113.42252787566 1407424.4904223008 0, -52714.72932805476 1407423.0993317056 0)), ((-37149.28517456842 1407380.9379172502 0, -36750.25490070068 1407380.7278270281 0, -36754.138667878295 1406973.8392254834 0, -37152.93448147918 1406974.5745271365 0, -37149.28517456842 1407380.9379172502 0)), ((-49098.771098366145 1409014.5651108618 0, -48700.97948075122 1409016.1323291631 0, -48303.179118496366 1409017.7069356043 0, -48306.18649131874 1408609.4000531365 0, -48309.18503675674 1408201.0942950188 0, -48707.37613487595 1408197.394929061 0, -48704.17330348932 1408606.7629881366 0, -49102.16941304026 1408604.1334681888 0, -49098.771098366145 1409014.5651108618 0)), ((-34308.21071284382 1408980.8766159413 0, -33911.65594498215 1408976.9684255489 0, -33913.462953848604 1408566.7526814279 0, -34310.62981318454 1408570.3385677047 0, -34308.21071284382 1408980.8766159413 0)), ((-45121.80013026185 1409419.5188985867 0, -45124.123486985474 1409011.8668331797 0, -45525.13324641677 1409013.3517159699 0, -45522.70408248892 1409420.4657696087 0, -45121.80013026185 1409419.5188985867 0)), ((-41062.49759960651 1417147.2511186171 0, -41465.691388980056 1417148.1124635085 0, -41464.55554254951 1417557.1782710648 0, -41061.897261498525 1417555.1437058153 0, -41062.49759960651 1417147.2511186171 0)), ((-27492.229832118806 1421135.881236054 0, -27095.041551361763 1421134.2210739213 0, -27095.653747211007 1420726.6362619468 0, -27493.54178899811 1420728.1977070721 0, -27891.42983173623 1420729.777774886 0, -27893.441604960874 1420321.985690067 0, -28292.038334326593 1420323.4858422014 0, -28289.317672711513 1420731.376560197 0, -28286.606152507487 1421139.268316226 0, -27889.41807114016 1421137.5711199862 0, -27492.229832118806 1421135.881236054 0)), ((-47430.46086562605 1422460.9894159003 0, -47433.74788623179 1422051.8084673008 0, -47835.68021531909 1422054.0479070193 0, -48237.60335211903 1422056.3062949115 0, -48639.53542901838 1422058.5837951445 0, -48637.72102840831 1422467.7728703206 0, -48235.307059552346 1422465.4927755257 0, -47832.883997863995 1422463.2316308944 0, -47430.46086562605 1422460.9894159003 0)), ((-53822.994419295734 1422088.8161936356 0, -53821.77445909299 1422497.5949104598 0, -53820.563469702094 1422906.363556534 0, -53416.62164358641 1422903.8285592874 0, -53012.688738576195 1422901.3128766587 0, -53014.031033634565 1422492.5450216045 0, -53015.37317404327 1422083.7672134412 0, -53419.18389470685 1422086.2820864092 0, -53822.994419295734 1422088.8161936356 0)), ((-42611.47598931688 1439188.1485232387 0, -42210.34669705169 1439186.595240791 0, -42201.626493783304 1438778.3713566647 0, -42601.914100250455 1438780.569365161 0, -42611.47598931688 1439188.1485232387 0)), ((-35788.69532467838 1448131.3822505649 0, -35784.95560054726 1448537.9470481137 0, -35781.216036558966 1448944.512891209 0, -35398.17613390845 1448944.1717408116 0, -35402.05211507699 1448536.8784310052 0, -35405.92820503735 1448129.5974737445 0, -35788.69532467838 1448131.3822505649 0)), ((-54128.12622772996 1448198.645029484 0, -54124.33551225782 1448606.939795728 0, -53721.13041468253 1448602.1397421001 0, -53725.077380183204 1448192.893913813 0, -54128.12622772996 1448198.645029484 0)), ((-52126.32439893466 1450631.783255937 0, -52124.167849469064 1451038.0568473537 0, -51723.10555888988 1451035.9294243853 0, -51724.724748766275 1450629.7645035202 0, -52126.32439893466 1450631.783255937 0)), ((-35729.02766132224 1454618.8491860363 0, -35344.205699662365 1454619.5656348164 0, -35348.046939431704 1454215.6400177216 0, -35732.73423408619 1454215.247812748 0, -35729.02766132224 1454618.8491860363 0)), ((-16813.79001415544 1330038.4636402174 0, -17215.857182495096 1330037.1132214172 0, -17215.37495653053 1330440.899287381 0, -16812.97296936808 1330442.6743913456 0, -16813.79001415544 1330038.4636402174 0)), ((-25591.53468963998 1331686.0846157465 0, -25988.001756558864 1331686.8353816795 0, -25986.240551780407 1332093.070546633 0, -25589.28653234187 1332091.9940499857 0, -25591.53468963998 1331686.0846157465 0)), ((-18657.710171378043 1356841.8069995563 0, -19057.212188955655 1356842.2396951579 0, -19055.600761370322 1357249.1073492498 0, -19053.99853492281 1357655.9762739257 0, -18655.92631586334 1357654.260003071 0, -18257.853893923802 1357652.551101258 0, -18258.03565067079 1357246.9657366814 0, -18656.82273612158 1357248.0271945216 0, -18657.710171378043 1356841.8069995563 0)), ((-17681.45288699688 1399983.9545496418 0, -17681.383920416778 1400387.0933994888 0, -17681.305883326095 1400790.2446931095 0, -17284.370019549686 1400790.311653504 0, -17285.191209432265 1400387.5985608376 0, -17286.012534699414 1399984.8753871066 0, -17681.45288699688 1399983.9545496418 0)), ((-20471.082270641247 1402822.253860498 0, -20469.069541656016 1403228.812082379 0, -20069.6657935113 1403231.306708366 0, -19670.271124686282 1403233.8199862884 0, -19671.89985932931 1402825.559266863 0, -19673.52861299805 1402417.2885777934 0, -19273.75009190126 1402418.1181590357 0, -18873.971766966377 1402418.9552289136 0, -18875.216170567768 1402008.983310272 0, -18876.469658762377 1401599.0126167128 0, -19276.632523114244 1401599.8779022356 0, -19275.19127038341 1402008.9974602174 0, -19675.16642444242 1402009.0303018533 0, -20075.132651135576 1402009.070657193 0, -20475.10780360808 1402009.1410813185 0, -20473.094991630474 1402415.6968586221 0, -20471.082270641247 1402822.253860498 0)), ((-9335.554293245637 1402424.4290325504 0, -8936.120499337989 1402424.4561156821 0, -8536.695754503038 1402424.4907618808 0, -8137.262044787554 1402424.555315426 0, -8139.379748312747 1402017.126761258 0, -8538.141592994476 1402017.072794737 0, -8936.9034685794 1402017.0263130628 0, -9335.665297644362 1402017.0096139356 0, -9335.554293245637 1402424.4290325504 0)), ((-10526.003541098957 1404853.1758405592 0, -10126.692731023895 1404852.721349654 0, -10127.86026501288 1404448.7215429984 0, -10129.02786441581 1404044.7228453762 0, -10130.204483135805 1403640.7142355978 0, -10131.37220717983 1403236.7179620445 0, -10529.397050592761 1403235.4691104281 0, -10528.550822250867 1403639.8911888264 0, -10527.704753050168 1404044.314486788 0, -10926.372665945557 1404043.9360268607 0, -10925.848009200025 1404448.79754946 0, -10925.323351159866 1404853.6490867946 0, -10526.003541098957 1404853.1758405592 0)), ((-10915.36546449211 1415017.5340739773 0, -10513.868736640456 1415017.2580513377 0, -10513.59741987875 1414609.5916331853 0, -10915.55211069821 1414610.0695756353 0, -10915.36546449211 1415017.5340739773 0)), ((-9304.061652257771 1418676.0223332094 0, -8904.706838474583 1418676.2717458885 0, -8905.989438393268 1418268.2719635128 0, -8506.444262784087 1418269.7044243019 0, -8507.527504052996 1417862.881166446 0, -8907.263158389378 1417860.2733829804 0, -9307.007970173914 1417857.6730894672 0, -9305.534743711994 1418266.847118715 0, -9304.061652257771 1418676.0223332094 0)), ((-14866.391066457734 1423146.963400424 0, -14468.094564317249 1423147.5908709764 0, -14467.923093257088 1422740.550027355 0, -14866.069362340162 1422739.496769748 0, -14866.391066457734 1423146.963400424 0)), ((-22789.443742307823 1423566.7692361907 0, -22787.51202399189 1423972.3195133617 0, -22387.992789169282 1423968.1960098222 0, -21988.46488345091 1423964.0900493446 0, -21990.875879724364 1423559.179142646 0, -22390.15515739111 1423562.9709903942 0, -22789.443742307823 1423566.7692361907 0)), ((-22385.71866048286 1425188.1883419468 0, -21987.366844277287 1425183.9730755894 0, -21588.313688825467 1425184.4775449648 0, -21189.260663703197 1425185.000813099 0, -21189.255988402725 1424779.0056759224 0, -21587.980930794965 1424777.7314231538 0, -21986.714889463517 1424776.4869431814 0, -21986.062858859892 1424368.9908637865 0, -22385.821509603033 1424373.4221883689 0, -22785.58050831966 1424377.8710356434 0, -22784.825696333606 1424785.151058108 0, -22784.079696781024 1425192.432303488 0, -22385.71866048286 1425188.1883419468 0)), ((-23978.828136152653 1425199.4751542774 0, -23580.79196708526 1425200.9537681327 0, -23582.944604269494 1424793.8888952406 0, -23981.001007539067 1424791.9847933468 0, -23978.828136152653 1425199.4751542774 0)), ((-21189.287775086705 1425996.9831696847 0, -21185.214854753423 1426416.329983808 0, -20785.54565489438 1426414.3958039356 0, -20789.596470993583 1425996.0230049703 0, -21189.287775086705 1425996.9831696847 0)), ((-23171.207783262966 1426850.3651475555 0, -22774.28095923866 1426847.3939030806 0, -22778.43424381945 1426427.1841696575 0, -23175.370304686894 1426430.6930010836 0, -23171.207783262966 1426850.3651475555 0)), ((-16789.083962667504 1427236.6167654917 0, -16410.562104026943 1427237.0671452514 0, -16412.05089674044 1426810.8367828603 0, -16790.44196712572 1426809.2328464147 0, -16789.083962667504 1427236.6167654917 0)), ((-13267.232270095765 1427673.8767490105 0, -13358.982454266945 1427674.1298883737 0, -13431.370974292846 1427674.3253353133 0, -13430.38844995718 1428083.8636999105 0, -13032.160889656467 1428085.2070814408 0, -13033.127861560351 1427673.250076099 0, -13267.232270095765 1427673.8767490105 0)), ((-9035.14082254688 1430105.789552606 0, -8636.490342269948 1430107.1142109348 0, -8237.83988644801 1430108.446432914 0, -8239.08548537257 1429695.823676703 0, -8240.331098908558 1429283.2020766777 0, -8638.499665996944 1429283.5714577914 0, -9036.677129157448 1429283.959491114 0, -9035.904484906856 1429694.87950811 0, -9035.14082254688 1430105.789552606 0)), ((-10628.327496412647 1430125.4447252818 0, -11027.307870485187 1430124.6505926007 0, -11426.297293488356 1430123.8864121072 0, -11423.87629517472 1430530.9436893223 0, -11421.45551027663 1430938.013396714 0, -11024.383214862646 1430937.9402138188 0, -10627.31984301746 1430937.8744735995 0, -10627.823622210308 1430531.6646358366 0, -10628.327496412647 1430125.4447252818 0)), ((-10228.891362849288 1430935.283870418 0, -9830.462647546681 1430932.7119418927 0, -9831.101057816106 1430524.1509334827 0, -10229.458051555841 1430527.8984062965 0, -10228.891362849288 1430935.283870418 0)), ((-9034.87361266772 1431335.9753902326 0, -8635.420667953747 1431338.8891262284 0, -8634.472222275765 1430930.6502939675 0, -9033.604617063873 1430927.6241112824 0, -9034.87361266772 1431335.9753902326 0)), ((-19009.012775334453 1433386.9683659235 0, -18608.470759935877 1433385.894544539 0, -18610.03758042259 1432982.6691262762 0, -19009.99932296014 1432983.842415 0, -19409.961000773546 1432985.0345736654 0, -19409.545809704283 1433388.0610785992 0, -19409.13948397715 1433791.0774558517 0, -19008.017353386418 1433790.0842361224 0, -19009.012775334453 1433386.9683659235 0)), ((-22606.23040344618 1436666.1152199202 0, -22202.602143661108 1436667.0132464555 0, -22205.382885786 1436254.2636753346 0, -22609.371746348683 1436252.8403621526 0, -22606.23040344618 1436666.1152199202 0)), ((-11423.07139881989 1445586.6038086324 0, -11420.832536331181 1445994.5797821297 0, -11418.593789528952 1446402.56792934 0, -11019.858202751246 1446402.9151716887 0, -10621.1225762552 1446403.2813196506 0, -10623.321479082679 1445996.5809311701 0, -11022.076947054102 1445995.565350942 0, -11024.295907715403 1445588.2277044833 0, -11423.07139881989 1445586.6038086324 0)), ((3667.9825984933127 1361261.7398869595 0, 3271.78654365735 1361261.1539787692 0, 3273.0036903186738 1361670.1743525688 0, 3274.229878352892 1362079.1962443583 0, 3670.38771573775 1362080.6325772642 0, 4066.545433218391 1362082.098434959 0, 4067.7241128938367 1362491.9721308534 0, 4463.8624672441565 1362493.8815290402 0, 4462.702957869996 1362083.5714265972 0, 4858.860458343389 1362085.0739394808 0, 5253.98368202005 1362082.3186949585 0, 5649.116185252295 1362079.5817119617 0, 6044.239921942827 1362076.8628403149 0, 6439.372937904981 1362074.1623306684 0, 6439.068473020606 1362483.1838317905 0, 6840.032169585244 1362481.7931835607 0, 7240.996056238836 1362480.4099830554 0, 7641.960109142892 1362479.0568248993 0, 7643.3486903328685 1362071.3125821124 0, 8044.683089297442 1362070.4039864596 0, 8046.433109344914 1361663.0869280046 0, 7644.746329533392 1361663.5696624122 0, 7243.059606475476 1361664.0824420338 0, 7244.086963629996 1361255.91521118 0, 7245.114354230808 1360847.7491811982 0, 6842.704903434866 1360847.4181448165 0, 6440.286348916336 1360847.1059374984 0, 6444.716915792633 1360442.7937164959 0, 6048.391730703132 1360443.7803158313 0, 5652.075646549183 1360444.7964780284 0, 5255.7506515987925 1360445.8197606804 0, 4859.43485699078 1360446.8725027794 0, 4855.42075257052 1360852.8875004998 0, 4459.205643526083 1360852.6718899938 0, 4460.374546033734 1361262.9666056344 0, 4064.1785978289695 1361262.3440288014 0, 3667.9825984933127 1361261.7398869595 0)), ((5823.608368952152 1394651.6824361044 0, 5824.362499928453 1395056.9411885086 0, 6223.10474819421 1395061.9203327792 0, 6222.030249948082 1394653.8848904457 0, 5823.608368952152 1394651.6824361044 0)), ((-5361.365436736465 1396706.389520424 0, -5364.350844424533 1397117.2193848565 0, -5367.345002458819 1397528.0393127569 0, -4969.57010572615 1397524.414390651 0, -4571.803921819303 1397520.807954872 0, -4574.314550043019 1397932.92711166 0, -4176.04604837338 1397930.3911647056 0, -3777.7772477648164 1397927.8738202546 0, -3775.2280531525967 1397516.202901101 0, -3772.6785780104005 1397104.5221693125 0, -3770.128789514529 1396692.84262332 0, -4168.455411153753 1396694.7100118548 0, -4566.781875192641 1396696.5848091142 0, -4964.073910931336 1396701.4779592021 0, -5361.365436736465 1396706.389520424 0)), ((-5765.110472497799 1397531.682762787 0, -5768.345949020082 1397941.866243841 0, -5370.32979734723 1397938.8716434934 0, -5367.345002458819 1397528.0393127569 0, -5765.110472497799 1397531.682762787 0)), ((-6169.820763855996 1398354.4263220024 0, -6171.227780572272 1398758.4316575201 0, -5772.567240366206 1398755.9438749435 0, -5771.572105101918 1398352.0509255244 0, -6169.820763855996 1398354.4263220024 0)), ((-8934.563732245302 1403239.3083074307 0, -8533.80435657979 1403239.3415977538 0, -8535.250015733654 1402831.9211638675 0, -8935.346624428304 1402831.8760341003 0, -8934.563732245302 1403239.3083074307 0)), ((-7334.198764802522 1404450.2857351075 0, -7333.162567600376 1404855.1474478755 0, -6942.455389159213 1404853.1472148248 0, -6943.177369489856 1404447.8598481591 0, -6943.90840819948 1404042.5737791944 0, -7335.235009246853 1404045.4252372885 0, -7334.198764802522 1404450.2857351075 0)), ((-4557.163246030039 1411756.4275401917 0, -4954.868797630099 1411758.3234733166 0, -5352.565081841449 1411760.249273872 0, -5351.8027466804315 1412166.4056463034 0, -4954.37622726193 1412164.491197959 0, -4556.949639424531 1412162.584096889 0, -4557.163246030039 1411756.4275401917 0)), ((-4556.5223704270975 1412974.9119984435 0, -4158.255820068959 1412971.746704302 0, -3759.997924781146 1412968.5887309117 0, -3361.7308632521444 1412965.4606299805 0, -3362.666935595453 1412560.2537727468 0, -3760.684257698535 1412563.0682345585 0, -4158.710190737591 1412565.9014178016 0, -4556.736020626283 1412568.7530508554 0, -4556.5223704270975 1412974.9119984435 0)), ((-2164.148707155827 1413361.7316667805 0, -1762.6735150481454 1413358.5768788927 0, -1361.1890706803822 1413355.4523649502 0, -1360.918643760784 1412951.8564340037 0, -1761.5529792107493 1412954.4546278045 0, -2162.1959817704023 1412957.0605449257 0, -2164.148707155827 1413361.7316667805 0)), ((-4951.617552818249 1415010.855641058 0, -5350.541080552994 1415014.2826657707 0, -5351.8207268759315 1415421.737163806 0, -4952.835513228912 1415418.5338483811 0, -4951.617552818249 1415010.855641058 0)), ((-7710.143076527786 1416649.6378918309 0, -7710.847453084787 1416243.4572238165 0, -8111.686877348239 1416242.940041786 0, -8110.713061252357 1416648.583087173 0, -7710.143076527786 1416649.6378918309 0)), ((2955.9121317924337 1433763.453534519 0, 2957.933130431322 1433358.3113172445 0, 2557.736064451555 1433356.2460894657 0, 2555.3142098843346 1433760.64916279 0, 2955.9121317924337 1433763.453534519 0)), ((-8633.715191359259 1433788.7303183426 0, -8632.195720477703 1434197.0978310718 0, -8232.888047910925 1434198.0147026908 0, -8234.12870768069 1433790.0724934114 0, -8633.715191359259 1433788.7303183426 0)), ((-7833.580459802765 1434198.9503277177 0, -7434.272954745794 1434199.9048067678 0, -7434.9561009814215 1433792.813206365 0, -7834.542311690426 1433791.4334215142 0, -7833.580459802765 1434198.9503277177 0)), ((-8632.195720477703 1434197.0978310718 0, -9031.503577910615 1434196.1996153423 0, -9032.434824085603 1434602.0062985152 0, -9033.374931554772 1435007.8141755809 0, -8632.737370810704 1435008.9235803874 0, -8632.466642936506 1434603.004550072 0, -8632.195720477703 1434197.0978310718 0)), ((8444.880493471079 1362070.9009648135 0, 8044.683089297442 1362070.4039864596 0, 8042.924351811976 1362477.711214934 0, 8443.1933103591 1362477.6820288904 0, 8444.880493471079 1362070.9009648135 0)), ((23940.560208683208 1373469.3187106117 0, 24338.944682764537 1373470.8625426325 0, 24339.07837204787 1373062.234071008 0, 23940.324977742097 1373060.26375857 0, 23940.560208683208 1373469.3187106117 0)), ((31457.32905047353 1382027.5795071495 0, 31072.418972391926 1382026.1780485814 0, 31070.166782830627 1382436.1037282096 0, 31067.914756997994 1382846.0415448265 0, 31454.589767365553 1382846.5986615878 0, 31455.959376295417 1382437.08291745 0, 31457.32905047353 1382027.5795071495 0)), ((16183.134649492826 1397485.5940972685 0, 16180.29221551345 1397899.4112098631 0, 16578.479224376555 1397897.4965675476 0, 16581.247317668774 1397485.7167950193 0, 16183.134649492826 1397485.5940972685 0)), ((33683.60136555491 1402005.813072489 0, 33287.30336291887 1402005.962124299 0, 32891.00544631004 1402006.140735376 0, 32886.187307161636 1402412.2612932723 0, 33282.044543635624 1402412.0919879964 0, 33677.89297967957 1402411.9299202596 0, 33683.60136555491 1402005.813072489 0)), ((38406.40211271971 1421955.8312380896 0, 38404.56646098126 1422362.8962009393 0, 38402.73075164401 1422769.9622514741 0, 38402.597674843244 1423176.5893333852 0, 38803.548275132714 1423175.2046724006 0, 38803.48642233556 1423581.620480224 0, 39204.508542976175 1423580.042460372 0, 39204.49982317129 1423986.2581472802 0, 39204.499916927765 1424392.4638287493 0, 39605.65606749139 1424390.4911672135 0, 40006.80349028758 1424388.5262709367 0, 40006.67860253812 1423982.7340392247 0, 40006.54463791348 1423576.9430517226 0, 39605.52197153495 1423578.4833025062 0, 39605.45923229114 1423172.481033212 0, 39204.50811909615 1423173.8390200117 0, 39204.507493604215 1422767.6255561172 0, 39605.396169626394 1422766.4911386305 0, 40006.28502603324 1422765.364310312 0, 40006.83871934901 1422357.878006152 0, 39606.270363169286 1422359.0958218528 0, 39607.13552717114 1421951.7128645603 0, 39206.89683396617 1421953.0743786842 0, 38806.64930915564 1421954.4433643622 0, 38406.40211271971 1421955.8312380896 0)), ((26866.55161481218 1424351.0112435762 0, 26465.7501644804 1424350.1706930618 0, 26463.81185736509 1424755.1035903455 0, 26461.873634159176 1425160.0375492498 0, 26863.31844409047 1425160.4321838315 0, 27264.763261928903 1425160.8569972059 0, 27266.058184565798 1424756.3576554847 0, 27267.353191917606 1424351.8594704461 0, 27265.927961733414 1423944.3639850963 0, 26865.707194103503 1423943.4057701565 0, 26866.55161481218 1424351.0112435762 0)), ((26060.41993769151 1425159.6506708313 0, 25658.975127555535 1425159.2826969242 0, 25656.393794269112 1425564.6526376398 0, 25653.803692757112 1425970.0125184932 0, 26055.900517841197 1425969.945695891 0, 26457.988492210385 1425969.8977265272 0, 26459.92654172446 1425564.961447212 0, 26461.873634159176 1425160.0375492498 0, 26060.41993769151 1425159.6506708313 0)), ((31247.72355206856 1425997.214155054 0, 30859.035554903632 1425995.7965056936 0, 30857.92172808006 1426394.4660426967 0, 30856.7990119094 1426793.1255830203 0, 30855.6277738817 1427210.082708338 0, 31244.60172732294 1427211.0760542026 0, 31245.6712115144 1426795.3501840306 0, 31246.69736943687 1426396.2872560483 0, 31247.72355206856 1425997.214155054 0)), ((8952.787569943277 1429299.5734824378 0, 9353.012976431766 1429301.2995553396 0, 9350.741017799015 1428895.938977767 0, 9348.459750747645 1428490.5794107786 0, 8948.195416330112 1428489.7049244102 0, 8547.913189324241 1428488.849261566 0, 8550.233287715257 1428893.3572431286 0, 8552.553083955652 1429297.8661509356 0, 8952.787569943277 1429299.5734824378 0)), ((31295.758602089732 1430966.8926517228 0, 31696.58739736454 1430965.8009903564 0, 31696.052619579787 1430559.576755768 0, 31295.376075100503 1430560.2322901199 0, 31295.758602089732 1430966.8926517228 0)), ((29686.062504212765 1431772.9774655506 0, 30087.34661815999 1431776.3131798077 0, 30088.61242679468 1431370.2950810643 0, 29686.707393049925 1431367.707428021 0, 29284.81106820321 1431365.1500453851 0, 29284.778081444532 1431769.6718939259 0, 29686.062504212765 1431772.9774655506 0)), ((33683.80416495708 1434219.528943654 0, 34080.38324314484 1434221.5233833797 0, 34081.32607723757 1433814.422182862 0, 34082.26001869907 1433407.3220958428 0, 33686.66509483637 1433406.8209388969 0, 33291.07017076232 1433406.3493162342 0, 32895.47527458937 1433405.8850309239 0, 32499.88054007314 1433405.4390762865 0, 32496.97783733379 1433809.541680142 0, 32494.06628576845 1434213.634195175 0, 32890.64573416791 1434215.5843478052 0, 33287.224999517806 1434217.5417315776 0, 33683.80416495708 1434219.528943654 0)), ((23281.322702587666 1438277.2391299286 0, 22882.533827512445 1438277.2315967374 0, 22881.780440430874 1438683.4822760036 0, 22881.01722435602 1439089.71772625 0, 23279.09729235261 1439089.9361779206 0, 23677.16840119339 1439090.16202897 0, 23678.640419087376 1438683.7156600135 0, 23280.210382243655 1438683.5896576294 0, 23281.322702587666 1438277.2391299286 0)), ((27663.841729979835 1438277.7829419072 0, 27664.91447690076 1438684.0399115272 0, 28064.273757122275 1438684.4755179365 0, 28063.81872562032 1438278.2316913216 0, 27663.841729979835 1438277.7829419072 0)), ((47020.47849513442 1368736.2481735882 0, 46620.89317356774 1368731.7593223478 0, 46617.469121503826 1369137.7034668713 0, 47017.08623459795 1369141.1738510272 0, 47020.47849513442 1368736.2481735882 0)), ((40888.28612163332 1398810.3029173778 0, 40888.972769718814 1398405.876715197 0, 40495.0978197868 1398402.300439157 0, 40493.53424201792 1398808.2113143476 0, 40491.97051295857 1399214.1234603913 0, 40887.59937367966 1399214.7191793837 0, 40888.28612163332 1398810.3029173778 0)), ((42874.2029053432 1398413.9005779398 0, 42477.30466783581 1398413.6209137712 0, 42475.298920180656 1398817.1902526526 0, 42473.29321129 1399220.7607468076 0, 42871.50745512726 1399223.1742548398 0, 43269.721530897696 1399225.6175239717 0, 43270.41149543613 1398819.9018874515 0, 43271.092297385214 1398414.187492674 0, 42874.2029053432 1398413.9005779398 0)), ((43666.53488203963 1400037.7903975674 0, 44064.719689143145 1400038.5469528188 0, 44462.90449046147 1400039.321974186 0, 44861.08938933239 1400040.115659923 0, 44865.975414254666 1399631.004485344 0, 44870.86163563032 1399221.8946078059 0, 44470.57390683882 1399222.8027402053 0, 44070.295649211956 1399223.7184704212 0, 44067.5030938263 1399631.1377106193 0, 43668.27171446209 1399631.2266916141 0, 43666.53488203963 1400037.7903975674 0)), ((46841.191059362725 1402487.626957288 0, 47241.14319177912 1402489.8305816215 0, 47641.09519900555 1402492.0529595895 0, 48041.04707938586 1402494.2940909364 0, 48041.9679617501 1402088.1545416329 0, 48042.87966707962 1401682.0050320977 0, 47643.41018167249 1401679.766755122 0, 47243.93155347336 1401677.5471107825 0, 46844.46181867459 1401675.346245597 0, 46444.98294733287 1401673.164114298 0, 46443.11536730105 1402079.308131211 0, 46441.238806422916 1402485.4421875922 0, 46841.191059362725 1402487.626957288 0)), ((42785.09444482231 1417090.9633374624 0, 42782.7786846216 1416683.36623433 0, 42387.01112364234 1416681.074765728 0, 41991.23446168209 1416678.801665917 0, 41595.45771569893 1416676.546956754 0, 41594.496786162796 1417084.4410256709 0, 41991.36571175268 1417086.6003795962 0, 42388.22563370831 1417088.778200191 0, 42389.448776286794 1417496.4716614427 0, 42787.400741392106 1417498.5616158939 0, 42785.09444482231 1417090.9633374624 0)), ((39617.44812457834 1419510.9341122413 0, 39615.30688680268 1419917.4308357595 0, 40015.22313970617 1419915.5716193852 0, 40017.46458048802 1419508.9633105693 0, 39617.44812457834 1419510.9341122413 0)), ((39615.30688680268 1419917.4308357595 0, 39215.390962748206 1419919.3089511516 0, 39213.35886891121 1420325.7178009108 0, 39613.16573389828 1420323.939949648 0, 39615.30688680268 1419917.4308357595 0)), ((43173.69029112402 1421144.0310060869 0, 43176.43916487922 1420739.5494228874 0, 43179.17907083359 1420335.0689035067 0, 43181.92803934463 1419930.5894921254 0, 42782.706631937515 1419929.32501479 0, 42780.06233488799 1420334.5551007758 0, 42777.427205059925 1420739.7863952087 0, 42774.783014100234 1421145.0188600898 0, 43173.69029112402 1421144.0310060869 0)), ((43138.04640519117 1426021.8478903729 0, 43538.76135342203 1426025.1537048742 0, 43541.603397614286 1425619.99836545 0, 43544.454352355264 1425214.855421625 0, 43144.20916999163 1425211.9661225507 0, 43141.12776070853 1425616.9064202525 0, 43138.04640519117 1426021.8478903729 0)), ((44739.685339029646 1426457.9074079415 0, 44740.90538453007 1426035.162281295 0, 44340.19060033626 1426031.8110090827 0, 43939.47615927323 1426028.4672771217 0, 43938.301364346866 1426451.8955513118 0, 43937.11741817147 1426875.324955872 0, 44337.795621394325 1426877.9855594186 0, 44738.474110031995 1426880.664903494 0, 44739.685339029646 1426457.9074079415 0)), ((46869.96596747712 1432650.623596509 0, 47268.66723910053 1432652.3826046637 0, 47667.35949100986 1432654.1603220715 0, 47673.89109074998 1432251.381770946 0, 47277.63404356351 1432250.468467218 0, 46881.38601479509 1432249.5736171429 0, 46869.96596747712 1432650.623596509 0)), ((42868.01310278643 1433041.7058540962 0, 42867.49884318979 1433448.8081239166 0, 43265.968432692425 1433452.1142425379 0, 43664.44684166865 1433455.4390048862 0, 43666.208349569075 1433047.9286215845 0, 43667.9610672845 1432640.4081629838 0, 43268.25317585796 1432637.5026522633 0, 42868.53623069662 1432634.6046485733 0, 42868.01310278643 1433041.7058540962 0)), ((43653.91339690792 1436707.8980509616 0, 44053.96147105286 1436708.2602473078 0, 44054.96289458775 1436301.1626489803 0, 44055.97329119365 1435894.0661028347 0, 43655.35974547469 1435895.4145927127 0, 43654.641072934384 1436301.6614188931 0, 43653.91339690792 1436707.8980509616 0)), ((46404.75248527372 1443218.9348788622 0, 46405.68200738294 1443625.092973874 0, 46406.62014062616 1444031.2632870579 0, 46803.07579062691 1444033.852884718 0, 46802.5948313296 1443627.595366188 0, 46802.11359220333 1443221.3276486797 0, 46404.75248527372 1443218.9348788622 0)), ((47584.42243595406 1445256.1253108757 0, 47588.75214598574 1444849.0402966023 0, 47190.943998306866 1444847.6718798936 0, 46793.14477073483 1444846.3221683097 0, 46788.17959641289 1445252.5640334038 0, 46783.21475897675 1445658.795810624 0, 47181.65840850225 1445660.9997947437 0, 47186.29668652955 1445254.3297183749 0, 47584.42243595406 1445256.1253108757 0)), ((39615.30598304039 1447270.4530876006 0, 39613.232407284864 1447676.0676543007 0, 40014.37128167269 1447677.613971607 0, 40012.02808899113 1448083.3403358555 0, 40412.88821855661 1448085.0163195592 0, 40415.518895215544 1447679.1792925685 0, 40418.14070110221 1447273.3433349424 0, 40016.72333185001 1447271.8887225995 0, 39615.30598304039 1447270.4530876006 0)), ((48513.71539533341 1390310.7813282115 0, 48514.99058104809 1389903.8075344223 0, 48516.25682956984 1389496.8349181768 0, 48118.98701178249 1389494.1652600924 0, 48115.66162806901 1389901.5515562808 0, 47718.545019807425 1389900.6027192597 0, 47715.4070200948 1390308.4056199603 0, 48112.336497515316 1390308.9278693572 0, 48513.71539533341 1390310.7813282115 0)), ((47238.354420708085 1403302.1189828473 0, 47235.93957838741 1403707.8394884814 0, 47233.53362725059 1404113.561275337 0, 47632.718781534306 1404115.7794895691 0, 48031.91282992488 1404118.0164722488 0, 48035.56782706858 1403712.3017046698 0, 48039.21398645571 1403306.5880712736 0, 47638.78872526139 1403304.344114229 0, 47238.354420708085 1403302.1189828473 0)), ((50633.34644255004 1425273.2099711886 0, 50222.1039051346 1425269.3624932896 0, 50219.46031970321 1425676.4437477218 0, 50216.825638972914 1426083.526109069 0, 50214.10805921313 1426503.1503888394 0, 50211.38151345291 1426922.7982818997 0, 50612.09544493938 1426927.8820066527 0, 50618.97932716806 1426507.609393369 0, 51028.0016209734</t>
+          <t>MULTIPOLYGON Z (((-25595.630598020878 1325191.749269161 0, -25998.46523582459 1325191.6367746638 0, -26401.300038869995 1325191.5430964984 0, -26400.327075755373 1325595.7718909876 0, -26399.35398685237 1326000.0133666394 0, -25995.96996745387 1325996.625874207 0, -25592.576635622554 1325993.2685226349 0, -25594.099043366954 1325592.5081242207 0, -25595.630598020878 1325191.749269161 0)), ((-38729.95122741543 1330510.5832821408 0, -38731.851478464676 1330106.5196841168 0, -39130.539144705785 1330105.3133663572 0, -39529.226980711166 1330104.1367276963 0, -39525.72608157453 1330509.6920674623 0, -39127.838572195666 1330510.1228858428 0, -38729.95122741543 1330510.5832821408 0)), ((-25589.28653234187 1332091.9940499857 0, -25591.53468963998 1331686.0846157465 0, -25988.001756558864 1331686.8353816795 0, -25986.240551780407 1332093.070546633 0, -25589.28653234187 1332091.9940499857 0)), ((-35139.07853734465 1339021.298573852 0, -34738.74706374294 1339019.7538136207 0, -34740.914447515635 1338613.2309835711 0, -35141.44709580831 1338614.3962972057 0, -35139.07853734465 1339021.298573852 0)), ((-34336.43254267719 1339428.6021044143 0, -34338.424624424544 1339018.227687109 0, -34738.74706374294 1339019.7538136207 0, -34736.563128944676 1339430.3846033008 0, -34336.43254267719 1339428.6021044143 0)), ((-28376.645096421125 1403617.3107573318 0, -28381.773513563672 1403209.8878311224 0, -28780.112240131755 1403216.7333134527 0, -29178.459274632463 1403223.597371753 0, -29175.009383286055 1403630.1637615603 0, -28775.827514534387 1403623.7223585634 0, -28376.645096421125 1403617.3107573318 0)), ((-10126.692731023895 1404852.721349654 0, -10127.86026501288 1404448.7215429984 0, -10129.02786441581 1404044.7228453762 0, -10130.204483135805 1403640.7142355978 0, -10131.37220717983 1403236.7179620445 0, -10529.397050592761 1403235.4691104281 0, -10528.550822250867 1403639.8911888264 0, -10527.704753050168 1404044.314486788 0, -10926.372665945557 1404043.9360268607 0, -10925.848009200025 1404448.79754946 0, -10925.323351159866 1404853.6490867946 0, -10526.003541098957 1404853.1758405592 0, -10126.692731023895 1404852.721349654 0)), ((-10915.36546449211 1415017.5340739773 0, -10513.868736640456 1415017.2580513377 0, -10513.59741987875 1414609.5916331853 0, -10915.55211069821 1414610.0695756353 0, -10915.36546449211 1415017.5340739773 0)), ((-8110.713061252357 1416648.583087173 0, -7710.143076527786 1416649.6378918309 0, -7710.847453084787 1416243.4572238165 0, -8111.686877348239 1416242.940041786 0, -8110.713061252357 1416648.583087173 0)), ((-8507.527504052996 1417862.881166446 0, -8907.263158389378 1417860.2733829804 0, -9307.007970173914 1417857.6730894672 0, -9305.534743711994 1418266.847118715 0, -9304.061652257771 1418676.0223332094 0, -8904.706838474583 1418676.2717458885 0, -8905.989438393268 1418268.2719635128 0, -8506.444262784087 1418269.7044243019 0, -8507.527504052996 1417862.881166446 0)), ((-27492.229832118806 1421135.881236054 0, -27095.041551361763 1421134.2210739213 0, -27095.653747211007 1420726.6362619468 0, -27493.54178899811 1420728.1977070721 0, -27891.42983173623 1420729.777774886 0, -27893.441604960874 1420321.985690067 0, -28292.038334326593 1420323.4858422014 0, -28289.317672711513 1420731.376560197 0, -28286.606152507487 1421139.268316226 0, -27889.41807114016 1421137.5711199862 0, -27492.229832118806 1421135.881236054 0)), ((-53014.031033634565 1422492.5450216045 0, -53015.37317404327 1422083.7672134412 0, -53419.18389470685 1422086.2820864092 0, -53822.994419295734 1422088.8161936356 0, -53821.77445909299 1422497.5949104598 0, -53820.563469702094 1422906.363556534 0, -53416.62164358641 1422903.8285592874 0, -53012.688738576195 1422901.3128766587 0, -53014.031033634565 1422492.5450216045 0)), ((-22789.443742307823 1423566.7692361907 0, -22787.51202399189 1423972.3195133617 0, -22387.992789169282 1423968.1960098222 0, -21988.46488345091 1423964.0900493446 0, -21990.875879724364 1423559.179142646 0, -22390.15515739111 1423562.9709903942 0, -22789.443742307823 1423566.7692361907 0)), ((-22385.71866048286 1425188.1883419468 0, -21987.366844277287 1425183.9730755894 0, -21588.313688825467 1425184.4775449648 0, -21189.260663703197 1425185.000813099 0, -21189.255988402725 1424779.0056759224 0, -21587.980930794965 1424777.7314231538 0, -21986.714889463517 1424776.4869431814 0, -21986.062858859892 1424368.9908637865 0, -22385.821509603033 1424373.4221883689 0, -22785.58050831966 1424377.8710356434 0, -22784.825696333606 1424785.151058108 0, -22784.079696781024 1425192.432303488 0, -22385.71866048286 1425188.1883419468 0)), ((-9033.604617063873 1430927.6241112824 0, -9034.87361266772 1431335.9753902326 0, -8635.420667953747 1431338.8891262284 0, -8634.472222275765 1430930.6502939675 0, -9033.604617063873 1430927.6241112824 0)), ((-19009.99932296014 1432983.842415 0, -19409.961000773546 1432985.0345736654 0, -19409.545809704283 1433388.0610785992 0, -19009.012775334453 1433386.9683659235 0, -19009.99932296014 1432983.842415 0)), ((-8633.715191359259 1433788.7303183426 0, -8632.195720477703 1434197.0978310718 0, -8232.888047910925 1434198.0147026908 0, -8234.12870768069 1433790.0724934114 0, -8633.715191359259 1433788.7303183426 0)), ((-7834.542311690426 1433791.4334215142 0, -7833.580459802765 1434198.9503277177 0, -7434.272954745794 1434199.9048067678 0, -7434.9561009814215 1433792.813206365 0, -7834.542311690426 1433791.4334215142 0)), ((-9033.374931554772 1435007.8141755809 0, -8632.737370810704 1435008.9235803874 0, -8632.466642936506 1434603.004550072 0, -8632.195720477703 1434197.0978310718 0, -9031.503577910615 1434196.1996153423 0, -9032.434824085603 1434602.0062985152 0, -9033.374931554772 1435007.8141755809 0)), ((-11423.07139881989 1445586.6038086324 0, -11420.832536331181 1445994.5797821297 0, -11418.593789528952 1446402.56792934 0, -11019.858202751246 1446402.9151716887 0, -10621.1225762552 1446403.2813196506 0, -10623.321479082679 1445996.5809311701 0, -11022.076947054102 1445995.565350942 0, -11024.295907715403 1445588.2277044833 0, -11423.07139881989 1445586.6038086324 0)), ((-35788.69532467838 1448131.3822505649 0, -35784.95560054726 1448537.9470481137 0, -35781.216036558966 1448944.512891209 0, -35398.17613390845 1448944.1717408116 0, -35402.05211507699 1448536.8784310052 0, -35405.92820503735 1448129.5974737445 0, -35788.69532467838 1448131.3822505649 0)), ((-53725.077380183204 1448192.893913813 0, -54128.12622772996 1448198.645029484 0, -54124.33551225782 1448606.939795728 0, -53721.13041468253 1448602.1397421001 0, -53725.077380183204 1448192.893913813 0)), ((-52124.167849469064 1451038.0568473537 0, -51723.10555888988 1451035.9294243853 0, -51724.724748766275 1450629.7645035202 0, -52126.32439893466 1450631.783255937 0, -52124.167849469064 1451038.0568473537 0)), ((-35729.02766132224 1454618.8491860363 0, -35344.205699662365 1454619.5656348164 0, -35348.046939431704 1454215.6400177216 0, -35732.73423408619 1454215.247812748 0, -35729.02766132224 1454618.8491860363 0)), ((4459.205643526083 1360852.6718899938 0, 4460.374546033734 1361262.9666056344 0, 4064.1785978289695 1361262.3440288014 0, 3667.9825984933127 1361261.7398869595 0, 3271.78654365735 1361261.1539787692 0, 3273.0036903186738 1361670.1743525688 0, 3274.229878352892 1362079.1962443583 0, 3670.38771573775 1362080.6325772642 0, 4066.545433218391 1362082.098434959 0, 4067.7241128938367 1362491.9721308534 0, 4463.8624672441565 1362493.8815290402 0, 4462.702957869996 1362083.5714265972 0, 4858.860458343389 1362085.0739394808 0, 5253.98368202005 1362082.3186949585 0, 5649.116185252295 1362079.5817119617 0, 6044.239921942827 1362076.8628403149 0, 6439.372937904981 1362074.1623306684 0, 6439.068473020606 1362483.1838317905 0, 6840.032169585244 1362481.7931835607 0, 7240.996056238836 1362480.4099830554 0, 7641.960109142892 1362479.0568248993 0, 7643.3486903328685 1362071.3125821124 0, 8044.683089297442 1362070.4039864596 0, 8046.433109344914 1361663.0869280046 0, 7644.746329533392 1361663.5696624122 0, 7243.059606475476 1361664.0824420338 0, 7244.086963629996 1361255.91521118 0, 7245.114354230808 1360847.7491811982 0, 6842.704903434866 1360847.4181448165 0, 6440.286348916336 1360847.1059374984 0, 6444.716915792633 1360442.7937164959 0, 6048.391730703132 1360443.7803158313 0, 5652.075646549183 1360444.7964780284 0, 5255.7506515987925 1360445.8197606804 0, 4859.43485699078 1360446.8725027794 0, 4855.42075257052 1360852.8875004998 0, 4459.205643526083 1360852.6718899938 0)), ((8044.683089297442 1362070.4039864596 0, 8042.924351811976 1362477.711214934 0, 8443.1933103591 1362477.6820288904 0, 8444.880493471079 1362070.9009648135 0, 8044.683089297442 1362070.4039864596 0)), ((5824.362499928453 1395056.9411885086 0, 6223.10474819421 1395061.9203327792 0, 6222.030249948082 1394653.8848904457 0, 5823.608368952152 1394651.6824361044 0, 5824.362499928453 1395056.9411885086 0)), ((-7334.198764802522 1404450.2857351075 0, -7333.162567600376 1404855.1474478755 0, -6942.455389159213 1404853.1472148248 0, -6943.177369489856 1404447.8598481591 0, -6943.90840819948 1404042.5737791944 0, -7335.235009246853 1404045.4252372885 0, -7334.198764802522 1404450.2857351075 0)), ((-4557.163246030039 1411756.4275401917 0, -4954.868797630099 1411758.3234733166 0, -5352.565081841449 1411760.249273872 0, -5351.8027466804315 1412166.4056463034 0, -4954.37622726193 1412164.491197959 0, -4556.949639424531 1412162.584096889 0, -4557.163246030039 1411756.4275401917 0)), ((-4158.710190737591 1412565.9014178016 0, -4556.736020626283 1412568.7530508554 0, -4556.5223704270975 1412974.9119984435 0, -4158.255820068959 1412971.746704302 0, -3759.997924781146 1412968.5887309117 0, -3361.7308632521444 1412965.4606299805 0, -3362.666935595453 1412560.2537727468 0, -3760.684257698535 1412563.0682345585 0, -4158.710190737591 1412565.9014178016 0)), ((-2162.1959817704023 1412957.0605449257 0, -2164.148707155827 1413361.7316667805 0, -1762.6735150481454 1413358.5768788927 0, -1361.1890706803822 1413355.4523649502 0, -1360.918643760784 1412951.8564340037 0, -1761.5529792107493 1412954.4546278045 0, -2162.1959817704023 1412957.0605449257 0)), ((-5350.541080552994 1415014.2826657707 0, -5351.8207268759315 1415421.737163806 0, -4952.835513228912 1415418.5338483811 0, -4951.617552818249 1415010.855641058 0, -5350.541080552994 1415014.2826657707 0)), ((8952.787569943277 1429299.5734824378 0, 9353.012976431766 1429301.2995553396 0, 9350.741017799015 1428895.938977767 0, 9348.459750747645 1428490.5794107786 0, 8948.195416330112 1428489.7049244102 0, 8547.913189324241 1428488.849261566 0, 8550.233287715257 1428893.3572431286 0, 8552.553083955652 1429297.8661509356 0, 8952.787569943277 1429299.5734824378 0)), ((2955.9121317924337 1433763.453534519 0, 2957.933130431322 1433358.3113172445 0, 2557.736064451555 1433356.2460894657 0, 2555.3142098843346 1433760.64916279 0, 2955.9121317924337 1433763.453534519 0)), ((31455.959376295417 1382437.08291745 0, 31457.32905047353 1382027.5795071495 0, 31072.418972391926 1382026.1780485814 0, 31070.166782830627 1382436.1037282096 0, 31067.914756997994 1382846.0415448265 0, 31454.589767365553 1382846.5986615878 0, 31455.959376295417 1382437.08291745 0)), ((16581.247317668774 1397485.7167950193 0, 16183.134649492826 1397485.5940972685 0, 16180.29221551345 1397899.4112098631 0, 16578.479224376555 1397897.4965675476 0, 16581.247317668774 1397485.7167950193 0)), ((33683.60136555491 1402005.813072489 0, 33287.30336291887 1402005.962124299 0, 32891.00544631004 1402006.140735376 0, 32886.187307161636 1402412.2612932723 0, 33282.044543635624 1402412.0919879964 0, 33677.89297967957 1402411.9299202596 0, 33683.60136555491 1402005.813072489 0)), ((39617.44812457834 1419510.9341122413 0, 39615.30688680268 1419917.4308357595 0, 40015.22313970617 1419915.5716193852 0, 40017.46458048802 1419508.9633105693 0, 39617.44812457834 1419510.9341122413 0)), ((39615.30688680268 1419917.4308357595 0, 39215.390962748206 1419919.3089511516 0, 39213.35886891121 1420325.7178009108 0, 39613.16573389828 1420323.939949648 0, 39615.30688680268 1419917.4308357595 0)), ((38402.73075164401 1422769.9622514741 0, 38402.597674843244 1423176.5893333852 0, 38803.548275132714 1423175.2046724006 0, 38803.48642233556 1423581.620480224 0, 39204.508542976175 1423580.042460372 0, 39204.49982317129 1423986.2581472802 0, 39204.499916927765 1424392.4638287493 0, 39605.65606749139 1424390.4911672135 0, 40006.80349028758 1424388.5262709367 0, 40006.67860253812 1423982.7340392247 0, 40006.54463791348 1423576.9430517226 0, 39605.52197153495 1423578.4833025062 0, 39605.45923229114 1423172.481033212 0, 39204.50811909615 1423173.8390200117 0, 39204.507493604215 1422767.6255561172 0, 39605.396169626394 1422766.4911386305 0, 40006.28502603324 1422765.364310312 0, 40006.83871934901 1422357.878006152 0, 39606.270363169286 1422359.0958218528 0, 39607.13552717114 1421951.7128645603 0, 39206.89683396617 1421953.0743786842 0, 38806.64930915564 1421954.4433643622 0, 38406.40211271971 1421955.8312380896 0, 38404.56646098126 1422362.8962009393 0, 38402.73075164401 1422769.9622514741 0)), ((26863.31844409047 1425160.4321838315 0, 27264.763261928903 1425160.8569972059 0, 27266.058184565798 1424756.3576554847 0, 27267.353191917606 1424351.8594704461 0, 27265.927961733414 1423944.3639850963 0, 26865.707194103503 1423943.4057701565 0, 26866.55161481218 1424351.0112435762 0, 26465.7501644804 1424350.1706930618 0, 26463.81185736509 1424755.1035903455 0, 26461.873634159176 1425160.0375492498 0, 26863.31844409047 1425160.4321838315 0)), ((25656.393794269112 1425564.6526376398 0, 25653.803692757112 1425970.0125184932 0, 26055.900517841197 1425969.945695891 0, 26457.988492210385 1425969.8977265272 0, 26459.92654172446 1425564.961447212 0, 26461.873634159176 1425160.0375492498 0, 26060.41993769151 1425159.6506708313 0, 25658.975127555535 1425159.2826969242 0, 25656.393794269112 1425564.6526376398 0)), ((31246.69736943687 1426396.2872560483 0, 31247.72355206856 1425997.214155054 0, 30859.035554903632 1425995.7965056936 0, 30857.92172808006 1426394.4660426967 0, 30856.7990119094 1426793.1255830203 0, 30855.6277738817 1427210.082708338 0, 31244.60172732294 1427211.0760542026 0, 31245.6712115144 1426795.3501840306 0, 31246.69736943687 1426396.2872560483 0)), ((31295.376075100503 1430560.2322901199 0, 31295.758602089732 1430966.8926517228 0, 31696.58739736454 1430965.8009903564 0, 31696.052619579787 1430559.576755768 0, 31295.376075100503 1430560.2322901199 0)), ((29686.062504212765 1431772.9774655506 0, 30087.34661815999 1431776.3131798077 0, 30088.61242679468 1431370.2950810643 0, 29686.707393049925 1431367.707428021 0, 29284.81106820321 1431365.1500453851 0, 29284.778081444532 1431769.6718939259 0, 29686.062504212765 1431772.9774655506 0)), ((32890.64573416791 1434215.5843478052 0, 33287.224999517806 1434217.5417315776 0, 33683.80416495708 1434219.528943654 0, 34080.38324314484 1434221.5233833797 0, 34081.32607723757 1433814.422182862 0, 34082.26001869907 1433407.3220958428 0, 33686.66509483637 1433406.8209388969 0, 33291.07017076232 1433406.3493162342 0, 32895.47527458937 1433405.8850309239 0, 32499.88054007314 1433405.4390762865 0, 32496.97783733379 1433809.541680142 0, 32494.06628576845 1434213.634195175 0, 32890.64573416791 1434215.5843478052 0)), ((23281.322702587666 1438277.2391299286 0, 22882.533827512445 1438277.2315967374 0, 22881.780440430874 1438683.4822760036 0, 22881.01722435602 1439089.71772625 0, 23279.09729235261 1439089.9361779206 0, 23677.16840119339 1439090.16202897 0, 23678.640419087376 1438683.7156600135 0, 23280.210382243655 1438683.5896576294 0, 23281.322702587666 1438277.2391299286 0)), ((28063.81872562032 1438278.2316913216 0, 27663.841729979835 1438277.7829419072 0, 27664.91447690076 1438684.0399115272 0, 28064.273757122275 1438684.4755179365 0, 28063.81872562032 1438278.2316913216 0)), ((40016.72333185001 1447271.8887225995 0, 39615.30598304039 1447270.4530876006 0, 39613.232407284864 1447676.0676543007 0, 40014.37128167269 1447677.613971607 0, 40012.02808899113 1448083.3403358555 0, 40412.88821855661 1448085.0163195592 0, 40415.518895215544 1447679.1792925685 0, 40418.14070110221 1447273.3433349424 0, 40016.72333185001 1447271.8887225995 0)), ((47017.08623459795 1369141.1738510272 0, 47020.47849513442 1368736.2481735882 0, 46620.89317356774 1368731.7593223478 0, 46617.469121503826 1369137.7034668713 0, 47017.08623459795 1369141.1738510272 0)), ((40495.0978197868 1398402.300439157 0, 40493.53424201792 1398808.2113143476 0, 40491.97051295857 1399214.1234603913 0, 40887.59937367966 1399214.7191793837 0, 40888.28612163332 1398810.3029173778 0, 40888.972769718814 1398405.876715197 0, 40495.0978197868 1398402.300439157 0)), ((42874.2029053432 1398413.9005779398 0, 42477.30466783581 1398413.6209137712 0, 42475.298920180656 1398817.1902526526 0, 42473.29321129 1399220.7607468076 0, 42871.50745512726 1399223.1742548398 0, 43269.721530897696 1399225.6175239717 0, 43270.41149543613 1398819.9018874515 0, 43271.092297385214 1398414.187492674 0, 42874.2029053432 1398413.9005779398 0)), ((43666.53488203963 1400037.7903975674 0, 44064.719689143145 1400038.5469528188 0, 44462.90449046147 1400039.321974186 0, 44861.08938933239 1400040.115659923 0, 44865.975414254666 1399631.004485344 0, 44870.86163563032 1399221.8946078059 0, 44470.57390683882 1399222.8027402053 0, 44070.295649211956 1399223.7184704212 0, 44067.5030938263 1399631.1377106193 0, 43668.27171446209 1399631.2266916141 0, 43666.53488203963 1400037.7903975674 0)), ((46844.46181867459 1401675.346245597 0, 46444.98294733287 1401673.164114298 0, 46443.11536730105 1402079.308131211 0, 46441.238806422916 1402485.4421875922 0, 46841.191059362725 1402487.626957288 0, 47241.14319177912 1402489.8305816215 0, 47641.09519900555 1402492.0529595895 0, 48041.04707938586 1402494.2940909364 0, 48041.9679617501 1402088.1545416329 0, 48042.87966707962 1401682.0050320977 0, 47643.41018167249 1401679.766755122 0, 47243.93155347336 1401677.5471107825 0, 46844.46181867459 1401675.346245597 0)), ((48035.56782706858 1403712.3017046698 0, 48039.21398645571 1403306.5880712736 0, 47638.78872526139 1403304.344114229 0, 47238.354420708085 1403302.1189828473 0, 47235.93957838741 1403707.8394884814 0, 47233.53362725059 1404113.561275337 0, 47632.718781534306 1404115.7794895691 0, 48031.91282992488 1404118.0164722488 0, 48035.56782706858 1403712.3017046698 0)), ((42388.22563370831 1417088.778200191 0, 42389.448776286794 1417496.4716614427 0, 42787.400741392106 1417498.5616158939 0, 42785.09444482231 1417090.9633374624 0, 42782.7786846216 1416683.36623433 0, 42387.01112364234 1416681.074765728 0, 41991.23446168209 1416678.801665917 0, 41595.45771569893 1416676.546956754 0, 41594.496786162796 1417084.4410256709 0, 41991.36571175268 1417086.6003795962 0, 42388.22563370831 1417088.778200191 0)), ((42782.706631937515 1419929.32501479 0, 42780.06233488799 1420334.5551007758 0, 42777.427205059925 1420739.7863952087 0, 42774.783014100234 1421145.0188600898 0, 43173.69029112402 1421144.0310060869 0, 43176.43916487922 1420739.5494228874 0, 43179.17907083359 1420335.0689035067 0, 43181.92803934463 1419930.5894921254 0, 42782.706631937515 1419929.32501479 0)), ((43138.04640519117 1426021.8478903729 0, 43538.76135342203 1426025.1537048742 0, 43541.603397614286 1425619.99836545 0, 43544.454352355264 1425214.855421625 0, 43144.20916999163 1425211.9661225507 0, 43141.12776070853 1425616.9064202525 0, 43138.04640519117 1426021.8478903729 0)), ((43939.47615927323 1426028.4672771217 0, 43938.301364346866 1426451.8955513118 0, 43937.11741817147 1426875.324955872 0, 44337.795621394325 1426877.9855594186 0, 44738.474110031995 1426880.664903494 0, 44739.685339029646 1426457.9074079415 0, 44740.90538453007 1426035.162281295 0, 44340.19060033626 1426031.8110090827 0, 43939.47615927323 1426028.4672771217 0)), ((48469.65658740975 1431444.2169722288 0, 48471.29111545537 1431039.7008577932 0, 48082.38522873011 1431041.3565604272 0, 47693.470662592554 1431043.0300777848 0, 47686.94672439713 1431445.8165954074 0, 48078.29708788495 1431445.0078050692 0, 48469.65658740975 1431444.2169722288 0)), ((46869.96596747712 1432650.623596509 0, 47268.66723910053 1432652.3826046637 0, 47667.35949100986 1432654.1603220715 0, 47673.89109074998 1432251.381770946 0, 47277.63404356351 1432250.468467218 0, 46881.38601479509 1432249.5736171429 0, 46869.96596747712 1432650.623596509 0)), ((43664.44684166865 1433455.4390048862 0, 43666.208349569075 1433047.9286215845 0, 43667.9610672845 1432640.4081629838 0, 43268.25317585796 1432637.5026522633 0, 42868.53623069662 1432634.6046485733 0, 42868.01310278643 1433041.7058540962 0, 42867.49884318979 1433448.8081239166 0, 43265.968432692425 1433452.1142425379 0, 43664.44684166865 1433455.4390048862 0)), ((44054.96289458775 1436301.1626489803 0, 44055.97329119365 1435894.0661028347 0, 43655.35974547469 1435895.4145927127 0, 43654.641072934384 1436301.6614188931 0, 43653.91339690792 1436707.8980509616 0, 44053.96147105286 1436708.2602473078 0, 44054.96289458775 1436301.1626489803 0)), ((47616.72297200835 1439559.2484255596 0, 47613.40557171988 1439967.209774282 0, 48014.84996374706 1439968.1925056134 0, 48416.285327135825 1439969.1941243426 0, 48417.951453456655 1439559.958165253 0, 48017.341592828525 1439559.5994017401 0, 48019.83331204706 1439151.0074321728 0, 47620.040397181525 1439151.2993129434 0, 47616.72297200835 1439559.2484255596 0)), ((46405.68200738294 1443625.092973874 0, 46406.62014062616 1444031.2632870579 0, 46803.07579062691 1444033.852884718 0, 46802.5948313296 1443627.595366188 0, 46802.11359220333 1443221.3276486797 0, 46404.75248527372 1443218.9348788622 0, 46405.68200738294 1443625.092973874 0)), ((47190.943998306866 1444847.6718798936 0, 46793.14477073483 1444846.3221683097 0, 46788.17959641289 1445252.5640334038 0, 46783.21475897675 1445658.795810624 0, 47181.65840850225 1445660.9997947437 0, 47186.29668652955 1445254.3297183749 0, 47584.42243595406 1445256.1253108757 0, 47588.75214598574 1444849.0402966023 0, 47190.943998306866 1444847.6718798936 0)), ((48513.71539533341 1390310.7813282115 0, 48514.99058104809 1389903.8075344223 0, 48516.25682956984 1389496.8349181768 0, 48118.98701178249 1389494.1652600924 0, 48115.66162806901 1389901.5515562808 0, 48112.336497515316 1390308.9278693572 0, 48513.71539533341 1390310.7813282115 0)), ((51028.001620973446 1426512.1349859063 0, 51034.91916882286 1426091.1809812025 0, 51039.75837372786 1425684.122964784 0, 51044.5888652827 1425277.0661160594 0, 50633.34644255004 1425273.2099711886 0, 50222.1039051346 1425269.3624932896 0, 50219.46031970321 1425676.4437477218 0, 50216.825638972914 1426083.526109069 0, 50214.10805921313 1426503.1503888394 0, 50211.38151345291 1426922.7982818997 0, 50612.09544493938 1426927.8820066527 0, 50618.97932716806 1426507.609393369 0, 51028.001620973446 1426512.1349859063 0)), ((50878.36418830612 1428198.077238716 0, 50875.35688616083 1427788.3686053446 0, 50597.96907654439 1427789.8162273697 0, 50473.7283005472 1427790.4780743516 0, 50476.74514544124 1428198.8202952587 0, 50479.746834853955 1428606.614963521 0, 50482.75679689775 1429014.4332084334 0, 50884.34603997299 1429015.2133293266 0, 50881.35102570782 1428606.6335428134 0, 50878.36418830612 1428198.077238716 0)), ((50481.55701435381 1431046.2780705919 0, 50478.11443102988 1431453.0344633386 0, 50474.67203933756 1431859.7920159784 0, 50878.87387813837 1431863.2646308537 0, 50882.333684398785 1431456.8318941027 0, 50885.79364675383 1431050.3892205912 0, 50481.55701435381 1431046.2780705919 0)), ((48066.060651204374 1432655.9567926284 0, 48464.75278847054 1432657.7719719468 0, 48466.38742395622 1432253.252530779 0, 48070.13928568368 1432252.302284332 0, 48066.060651204374 1432655.9567926284 0)), ((52479.735130063455 1432685.9158840133 0, 52879.46303307594 1432687.9781650873 0, 52875.74094322724 1433093.8747921025 0, 52872.02796431994 1433499.7725950468 0, 53273.426436124624 1433501.6513569185 0, 53276.30865162764 1433095.849090521 0, 53279.1819478893 1432690.0479531 0, 53282.75004613058 1432284.677749301 0, 52883.01276771561 1432282.4958319438 0, 52483.26634063314 1432280.3326247504 0, 52479.735130063455 1432685.9158840133 0)), ((49258.66237988386 1433884.7628581703 0, 49256.814737454006 1434291.6482744317 0, 49656.829631218825 1434292.6876763592 0, 50056.83559002344 1434293.7457824624 0, 50058.53635404517 1433887.9344225524 0, 50060.22817901276 1433482.124079714 0, 49660.36910248364 1433479.9919218905 0, 49260.50098850963 1433477.8784676606 0, 49258.66237988386 1433884.7628581703 0)), ((52063.84737018516 1433902.1848754259 0, 52466.08575120417 1433903.9186597008 0, 52868.31492270268 1433905.682754219 0, 52872.02796431994 1433499.7725950468 0, 52470.638211951795 1433497.9240869957 0, 52069.23967023565 1433496.083381142 0, 52063.84737018516 1433902.1848754259 0)), ((52461.53322712701 1434309.9254923034 0, 52058.4643806963 1434308.287447351 0, 52055.63776384267 1434715.9074381827 0, 52457.66770668609 1434717.6398090322 0, 52461.53322712701 1434309.9254923034 0)), ((48453.93505964872 1435509.5987152308 0, 48452.97574645545 1435916.2584260146 0, 48851.54417273739 1435917.6776792777 0, 48852.86275685598 1435510.9079606803 0, 48854.17224534647 1435104.1505583904 0, 48454.88513610351 1435102.940124394 0, 48453.93505964872 1435509.5987152308 0)), ((51249.947294463615 1435525.6394253515 0, 51251.88504554989 1435118.224678227 0, 50851.94072154265 1435114.7587525318 0, 50849.84412318178 1435522.0604653999 0, 50847.75639695947 1435929.3522507043 0, 51248.00959506684 1435933.0440163813 0, 51648.262566833204 1435936.7547942032 0, 51650.050333583975 1435529.237195103 0, 51249.947294463615 1435525.6394253515 0)), ((49210.946431910255 1440794.8302169966 0, 48811.94979876997 1440791.2403842988 0, 48412.952955791625 1440787.6694441242 0, 48409.27625687309 1441193.9071871832 0, 48405.59078425571 1441600.1348329706 0, 48804.54791892855 1441603.9181682616 0, 49203.504837451226 1441607.7201898205 0, 49207.23007917282 1441201.2690513341 0, 49210.946431910255 1440794.8302169966 0)), ((48781.43134226861 1446891.9686025647 0, 49181.688019480294 1446894.8034083438 0, 49182.01445844508 1446487.882113719 0, 48780.90009740864 1446484.9303741963 0, 48379.77654317822 1446482.0086863146 0, 48381.18346557238 1446889.1526890227 0, 48781.43134226861 1446891.9686025647 0)), ((51536.81465690338 1450162.9971635407 0, 51534.677629603575 1450568.39408978 0, 51936.26374665766 1450573.4169269 0, 52337.840516728036 1450578.4587920976 0, 52739.425862577526 1450583.5196258912 0, 53141.001957129396 1450588.5994840674 0, 53142.55794371806 1450181.4632644136 0, 53144.10491076716 1449774.3280110767 0, 52742.81474311268 1449770.1234781446 0, 52341.524395316475 1449765.926596018 0, 51940.23366049321 1449761.7600708504 0, 51538.94264985227 1449757.6012000623 0, 51536.81465690338 1450162.9971635407 0)), ((52306.25858049324 1454646.2518213629 0, 52309.27149413075 1454239.562204722 0, 52312.284400320816 1453832.8735662366 0, 51913.60633274859 1453824.0199660552 0, 51514.91868098536 1453815.173963522 0, 51512.42538492756 1454224.8672754406 0, 51509.93215727512 1454634.550474458 0, 51908.091072988194 1454640.3917754882 0, 52306.25858049324 1454646.2518213629 0)), ((49928.2361357252 1455876.4429383543 0, 49531.28745492539 1455873.3334849584 0, 49534.17198308989 1455441.3396520985 0, 49137.56966342652 1455436.4811138583 0, 49134.329657279 1455870.2425408706 0, 49131.089666279106 1456303.9938590815 0, 49528.3939577778 1456305.328377982 0, 49925.698254634335 1456306.681632933 0, 49928.2361357252 1455876.4429383543 0)), ((53968.08643304752 1406192.099877982 0, 53965.80075506385 1406594.7286503164 0, 54366.40154819277 1406598.973738312 0, 54369.29940057987 1406197.535676694 0, 53968.08643304752 1406192.099877982 0)), ((57807.086478795376 1426151.9584999797 0, 58204.72445130463 1426156.7967001016 0, 58208.182737823794 1425750.6042395318 0, 58211.65012254668 1425344.4018888408 0, 57814.31417689341 1425339.5656820738 0, 57416.97797821976 1425334.7481164008 0, 57413.208470706864 1425740.9485751418 0, 57409.439138756374 1426147.138919864 0, 57807.086478795376 1426151.9584999797 0)), ((58594.6246465146 1427434.6430144673 0, 58992.20019538917 1427439.8428001578 0, 58994.65975986571 1427038.6453843745 0, 58597.06703195973 1427033.210384146 0, 58199.464990375534 1427027.7826971004 0, 58197.03972353922 1427429.461740239 0, 58594.6246465146 1427434.6430144673 0)), ((58088.79934147983 1427834.7636186986 0, 58087.39750674176 1428240.5614981682 0, 58085.98656432424 1428646.3604205174 0, 58485.65747505782 1428648.225560024 0, 58487.740443353956 1428242.4311052302 0, 58489.813535019326 1427836.7609836282 0, 58422.89849916002 1427836.4277216145 0, 58194.59492953678 1427835.2850340318 0, 58088.79934147983 1427834.7636186986 0)), ((53293.10620139186 1430253.5077602807 0, 53693.9892159369 1430253.688729525 0, 54094.86332038596 1430253.899821637 0, 54095.06546596552 1429846.5889147026 0, 54095.25859229619 1429439.2790399161 0, 54098.53309986563 1429032.6393169558 0, 54101.81666820125 1428626.0120854524 0, 53700.53246871296 1428624.757195098 0, 53697.26547085053 1429031.8101402526 0, 53296.006817598594 1429030.999936441 0, 53292.75645850395 1429438.4684741865 0, 53694.007494116486 1429438.864282053 0, 53693.99399842676 1429846.2759143377 0, 53292.931449064316 1429845.9930856493 0, 53293.10620139186 1430253.5077602807 0)), ((56094.49023233689 1429853.1463556248 0, 56092.59655578215 1430258.2967066532 0, 56491.255179838816 1430259.6476278245 0, 56493.58388545141 1429855.138368571 0, 56495.91258562352 1429450.6301642016 0, 56096.37485279134 1429447.9858430107 0, 56094.49023233689 1429853.1463556248 0)), ((57671.527840594295 1431483.4580849002 0, 57675.71723141975 1431077.99503547 0, 57279.34414644583 1431074.8679694794 0, 56882.970924191686 1431071.7595290341 0, 56486.59745826557 1431068.6694151452 0, 56484.23366971597 1431475.7572956616 0, 56879.99255229204 1431478.305751311 0, 57275.76021705949 1431480.8727572768 0, 57671.527840594295 1431483.4580849002 0)), ((54478.45147747839 1432691.2646908422 0, 54878.2081539972 1432691.7078712105 0, 54882.52584599025 1432285.9172059959 0, 54886.843641237036 1431880.127602297 0, 54486.716674589385 1431879.894653781 0, 54086.580756030206 1431879.6804232916 0, 54082.64227154176 1432285.2599158732 0, 54078.69486769894 1432690.8403449897 0, 54478.45147747839 1432691.2646908422 0)), ((58052.760241377866 1433519.2827974944 0, 57657.155158409296 1433517.2399327778 0, 57656.25215112807 1433925.9345872109 0, 58052.69271993475 1433928.5206852555 0, 58052.760241377866 1433519.2827974944 0)), ((58047.75326906359 1435149.3780382473 0, 58045.32186115472 1435555.188770266 0, 58042.88144816895 1435961.0005226957 0, 58439.274278620884 1435964.545873385 0, 58835.65788367383 1435968.120702861 0, 58838.41611938614 1435561.8966839844 0, 58841.17433525553 1435155.6626150915 0, 58843.93250541117 1434749.4407913801 0, 58846.690693824996 1434343.2201163068 0, 58449.65342578659 1434340.480653858 0, 58052.62492857351 1434337.7598298534 0, 58050.19359982092 1434743.5683719993 0, 58047.75326906359 1435149.3780382473 0)), ((54434.53207798426 1437167.0071910585 0, 54834.63372431591 1437169.9828379836 0, 54837.570502486444 1436766.0524952633 0, 54437.53042558216 1436763.043622438 0, 54037.49918523009 1436760.0424819302 0, 54034.42111671809 1437164.061532398 0, 54434.53207798426 1437167.0071910585 0)), ((54814.337626293665 1439210.0690365506 0, 55211.703833065374 1439212.22791471 0, 55609.06115803343 1439214.3942679656 0, 55614.44513713918 1438808.8111020096 0, 55619.82481211739 1438403.2238725615 0, 55221.39510243747 1438402.1142761717 0, 54822.95638394955 1438401.0344633712 0, 54818.64906362254 1438805.5537404018 0, 54814.337626293665 1439210.0690365506 0)), ((53200.68272133371 1441634.803933089 0, 53199.162526622895 1442040.6303924324 0, 53197.64221925213 1442446.4578649248 0, 53597.577184990005 1442448.972181875 0, 53997.50309896658 1442451.5051625392 0, 53999.40203926735 1442046.9567318314 0, 54001.30096227003 1441642.4093083302 0, 53600.98750336561 1441638.5971659464 0, 53200.68272133371 1441634.803933089 0)), ((55942.5694714764 1448159.7149057686 0, 55544.24919932989 1448159.0259783033 0, 55541.23216538009 1448565.9010514794 0, 55538.215075336615 1448972.7882244154 0, 55935.82013904711 1448973.2706563314 0, 56333.42517635881 1448973.7716562557 0, 56337.1574102906 1448567.102177729 0, 56340.889750924995 1448160.433600028 0, 55942.5694714764 1448159.7149057686 0)))</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Common Schools, Other Agency, Wildlife Conservation, State Educational Institutions, Normal Schools, University of Oklahoma</t>
+          <t>Common Schools, Normal Schools, State Educational Institutions, University of Oklahoma</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>399</v>
+        <v>313</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -1251,13 +1251,13 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>15982.61</v>
+        <v>12523.26</v>
       </c>
       <c r="J17" t="n">
-        <v>399</v>
+        <v>313</v>
       </c>
       <c r="K17" t="n">
-        <v>15982.61</v>
+        <v>12523.26</v>
       </c>
       <c r="L17" t="n">
         <v>3063071.94</v>
@@ -1362,7 +1362,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1406379.8180101914 2835502.9676008387 0, -1406473.9785516895 2835521.734531294 0, -1406778.7770429626 2835582.4882667917 0, -1406872.8312997553 2835601.148932945 0, -1406791.7645722493 2835992.9266004586 0, -1406710.698745883 2836384.702508994 0, -1406629.6366764735 2836776.4711096287 0, -1406548.5739271764 2837168.2345223785 0, -1406152.1431418383 2837088.956904065 0, -1406087.6405494164 2837076.280484532 0, -1405796.91670816 2837018.1569047323 0, -1405755.7083628573 2837009.698301688 0, -1405535.803621465 2836965.9663151815 0, -1405487.176097592 2836956.2471401114 0, -1405359.2691901615 2836930.461773824 0, -1405080.115136758 2836874.9046132243 0, -1404962.8255844747 2836851.2476163614 0, -1405025.8156075906 2836537.4335374683 0, -1405029.769174486 2836517.7370062955 0, -1405041.4965421397 2836459.306839623 0, -1405041.4965422011 2836459.306839316 0, -1405081.6600892353 2836258.4058300443 0, -1405108.2831449925 2836126.578187748 0, -1405120.0309416638 2836067.337313631 0, -1405133.2551556446 2836000.645850542 0, -1405186.659309687 2835735.386966785 0, -1405188.114813715 2835727.329112005 0, -1405192.8804176834 2835703.5856685042 0, -1405198.701406638 2835675.389715876 0, -1405261.8129454285 2835360.1547357994 0, -1405265.1738896933 2835344.2151984107 0, -1405277.2234497615 2835283.407895384 0, -1405277.2234497755 2835283.4078953867 0, -1405277.2234497757 2835283.4078953853 0, -1405581.9305416776 2835344.089946119 0, -1405676.1759969064 2835362.862839606 0, -1405980.8366573509 2835423.550296702 0, -1406075.138144352 2835442.2583379205 0, -1406202.3274685177 2835467.601562032 0, -1406379.8180101914 2835502.9676008387 0)), ((-1399356.4079068387 2840020.2810208434 0, -1399368.1809894112 2839960.4057747424 0, -1399384.6546780465 2839877.227700831 0, -1399462.396458146 2839484.6995438226 0, -1399540.139008013 2839092.1665506647 0, -1399542.905688448 2839092.835199241 0, -1399556.3294038298 2839095.3861888293 0, -1399556.3294040805 2839095.3861888773 0, -1399561.6720821362 2839096.376602012 0, -1399582.007635379 2839100.423022579 0, -1399599.5649045492 2839103.916675662 0, -1399623.3376730068 2839108.6470440533 0, -1399644.5027693652 2839112.8586522965 0, -1399667.8546858106 2839117.505222619 0, -1399689.9714188937 2839121.9060038663 0, -1399712.3326666437 2839126.3553711157 0, -1399735.4324632378 2839130.9517879887 0, -1399753.6615634388 2839134.578885354 0, -1399780.8692110055 2839139.992492276 0, -1399798.1407629494 2839143.429084783 0, -1399826.33910559 2839149.039729029 0, -1399842.651850635 2839152.2853515954 0, -1399871.8019453995 2839158.085069711 0, -1399883.9572934853 2839160.5036009005 0, -1399916.771608468 2839167.0324040405 0, -1399928.497425498 2839169.3652046104 0, -1399934.4273121587 2839170.492037641 0, -1399937.3344581702 2839171.1505293464 0, -1399937.334458662 2839171.150529451 0, -1399937.3344698094 2839171.1505316654 0, -1399961.7740465652 2839175.991441545 0, -1399972.9727293379 2839178.2173738675 0, -1400007.6713144428 2839185.123969481 0, -1400014.3015124146 2839186.44347234 0, -1400053.0843019113 2839194.164184724 0, -1400059.1674090049 2839195.3749906607 0, -1400062.5253671096 2839196.043416641 0, -1400098.5195565978 2839203.2079879213 0, -1400103.2938011107 2839204.1582646235 0, -1400135.8492566794 2839210.638179495 0, -1400143.9549004098 2839212.251141099 0, -1400147.7740981488 2839213.0111707496 0, -1400189.1188868866 2839221.238374427 0, -1400322.934807602 2839247.8660599813 0, -1400331.4578416802 2839249.561483696 0, -1400334.5232879098 2839250.1564733693 0, -1400337.289539137 2839250.8269082224 0, -1400438.6676987924 2839270.9013746134 0, -1400616.4727830754 2839306.2846389473 0, -1400666.7624768384 2839316.2673303704 0, -1400731.7096861927 2839329.18493668 0, -1400734.4720727175 2839329.8709867066 0, -1400774.2737872985 2839337.662505503 0, -1400819.7837660834 2839346.7515740218 0, -1401125.8721471464 2839407.6680866037 0, -1401128.8917457967 2839408.235767459 0, -1401123.9478869513 2839432.9798185662 0, -1401114.9923184975 2839478.068050874 0, -1401105.4885421125 2839525.9158027335 0, -1401103.154785328 2839537.809666259 0, -1401103.15478518 2839537.809667019 0, -1401067.6565216575 2839720.071360423 0, -1401063.830226231 2839739.28926802 0, -1401063.2021711767 2839742.434400068 0, -1401053.3518599859 2839788.545631688 0, -1401050.9229196983 2839800.7740466096 0, -1401050.9229196971 2839800.7740466157 0, -1401053.6475980359 2839801.596686764 0, -1400999.4443926136 2840062.6907491884 0, -1400998.724069705 2840066.308780294 0, -1400989.0886561542 2840114.569291522 0, -1400975.3905077311 2840183.1795261377 0, -1400973.5361308325 2840190.3820250407 0, -1400973.536130806 2840190.382025154 0, -1400972.9550610757 2840193.3075143024 0, -1400954.6895441287 2840190.4323968505 0, -1400920.226759528 2840183.5676653488 0, -1400578.8062332084 2840115.124226884 0, -1400575.8805057171 2840114.2936359607 0, -1400575.7633936796 2840117.3285491103 0, -1400574.844702643 2840122.2522871094 0, -1400574.022585394 2840126.3318334757 0, -1400566.8949736727 2840162.4611979346 0, -1400542.6533913193 2840284.271411241 0, -1400539.2966141847 2840301.1361504267 0, -1400517.715227514 2840409.5622253655 0, -1400512.0344126902 2840438.1135863895 0, -1400502.104311991 2840485.9874962857 0, -1400497.9721403266 2840506.8058186676 0, -1400497.390664912 2840509.80477352 0, -1400452.1259811474 2840738.4564959686 0, -1400451.4587958015 2840741.808285925 0, -1400428.6235849268 2840856.2023643884 0, -1400420.8018900126 2840895.468983268 0, -1400420.069223923 2840899.301431375 0, -1400274.7199397993 2840870.543052567 0, -1400213.4646311947 2840858.3298914144 0, -1400023.1088309977 2840820.26744506 0, -1400022.4191629284 2840823.311960139 0, -1399739.523394895 2840764.6045222455 0, -1399736.5386692584 2840764.0057220142 0, -1399709.2365354546 2840758.5145079345 0, -1399626.1434866686 2840741.2589619365 0, -1399229.1764102448 2840662.2699850057 0, -1399306.9140804114 2840269.750971841 0, -1399306.9140826785 2840269.7509606453 0, -1399308.926485363 2840259.6770075844 0, -1399310.6939220119 2840250.9220541627 0, -1399335.4899758273 2840125.914068922 0, -1399347.1961440216 2840066.79943821 0, -1399356.4079068387 2840020.2810208434 0)), ((-1399229.1764102448 2840662.2699850057 0, -1399151.2946448606 2841054.7992079007 0, -1398754.3652302015 2840975.7562494082 0, -1398357.4368467703 2840896.7085765144 0, -1398434.9954991627 2840504.121791033 0, -1398832.0885730598 2840583.1832069866 0, -1399229.1764102448 2840662.2699850057 0)), ((-1410207.0886851817 2841171.569820003 0, -1410292.106862424 2841187.9271961376 0, -1410693.8600138929 2841265.8675316847 0, -1410641.7045664315 2841528.5669757756 0, -1410634.2942596902 2841565.9644431355 0, -1410616.0088154103 2841658.7990578404 0, -1410598.9623274822 2841744.276462479 0, -1410583.5237163594 2841822.194011335 0, -1410567.3071516913 2841904.0386808235 0, -1410550.4485024924 2841989.125877908 0, -1410546.7760295542 2842007.661339168 0, -1410538.1586854516 2842051.725978964 0, -1410475.0699257555 2842369.6151062693 0, -1410460.3759917119 2842444.344847481 0, -1410410.353163191 2842696.3028291394 0, -1410373.9500720813 2842880.5766738653 0, -1410314.8445090398 2842868.6933648163 0, -1410314.8445067066 2842868.6933643688 0, -1410074.8976017982 2842822.7379557453 0, -1409974.2514204897 2842803.210860995 0, -1409926.9607263294 2842794.120359546 0, -1409574.4517075391 2842726.364992527 0, -1409539.7596685698 2842719.476227892 0, -1409539.1167997618 2842719.3485740544 0, -1409539.1167996211 2842719.3485740265 0, -1409407.3427740564 2842693.406117487 0, -1409174.87310327 2842647.185105116 0, -1409135.3708942847 2842639.3610066515 0, -1408775.2871312238 2842568.0429873103 0, -1408775.2871312243 2842568.042987308 0, -1408775.2871312224 2842568.0429873075 0, -1408791.982561276 2842482.1825481723 0, -1408859.431612287 2842135.3088754904 0, -1408936.0102514483 2841742.172147534 0, -1409010.5622617726 2841352.679039439 0, -1409011.4184577104 2841348.2058882047 0, -1409086.8267116826 2840954.237889088 0, -1409107.1392109245 2840958.307386213 0, -1409374.2239804657 2841010.0749029545 0, -1409488.590801991 2841032.1093411823 0, -1409488.590810442 2841032.1093428046 0, -1409488.5908287365 2841032.1093463674 0, -1409735.5629954843 2841080.1273449566 0, -1409890.3520447423 2841110.0070721535 0, -1410027.3861210642 2841136.7169916257 0, -1410207.0886851817 2841171.569820003 0)), ((-1404413.0040087868 2845598.7170888362 0, -1404411.9634668445 2845599.4135239385 0, -1404403.6665685656 2845604.966773168 0, -1404367.6175215868 2845629.094281301 0, -1404365.3857084531 2845630.5880346466 0, -1404365.3856752666 2845630.588048675 0, -1404359.7842581766 2845634.337058641 0, -1404209.994285118 2845697.6924938657 0, -1403967.0449391939 2845739.4757514074 0, -1403962.6991410798 2845740.222877639 0, -1403925.888990231 2845756.5350805065 0, -1403811.697381762 2845808.3746001213 0, -1403763.0290770517 2845813.871618658 0, -1403678.995867877 2845799.875162555 0, -1403644.1093635445 2845787.7281875107 0, -1403561.9104531568 2845792.578875461 0, -1403546.0403714462 2845795.453029865 0, -1403471.1140033456 2845809.0260385834 0, -1403350.954397719 2845815.8751161206 0, -1403137.9662648952 2845786.6090687537 0, -1403161.1101112196 2845669.769369071 0, -1403161.3519901694 2845669.741687514 0, -1403161.3953671006 2845669.522701863 0, -1403166.1869040276 2845668.9743470913 0, -1403166.6076956226 2845666.871903373 0, -1403587.2478790737 2845618.1462674816 0, -1403645.7782884282 2845611.3678443404 0, -1403671.7299334654 2845608.36233764 0, -1403654.8238005526 2845469.124905376 0, -1403609.740873767 2845474.285456348 0, -1403190.3208668637 2845522.3126093117 0, -1403267.3277244826 2845133.712013439 0, -1403345.307317196 2844741.3896947694 0, -1403345.3073174688 2844741.3896933924 0, -1403351.278613076 2844742.575062426 0, -1403351.9856773617 2844739.030921994 0, -1403739.775040757 2844819.6959529603 0, -1403739.7750432093 2844819.695953447 0, -1403739.775176096 2844819.695979834 0, -1404142.2220031724 2844899.538941732 0, -1404538.6548402628 2844972.33059754 0, -1404934.1430632109 2845049.787531759 0, -1404468.8456640067 2845562.344196431 0, -1404413.0040087868 2845598.7170888362 0)), ((-1404384.173923037 2845913.506921877 0, -1404460.723088921 2845877.299411543 0, -1404498.694650209 2845842.6323788343 0, -1404543.1465726472 2845794.266376779 0, -1404553.1898897956 2845768.42480921 0, -1404560.4058094958 2845767.591449572 0, -1404562.263610549 2845762.872978879 0, -1404602.726522319 2845758.1884405124 0, -1404617.3759774447 2845736.0786963697 0, -1404641.038383801 2845700.366122346 0, -1404770.6570928784 2845608.785523316 0, -1404825.8077152742 2845544.414600234 0, -1404824.4991240369 2845551.0100588636 0, -1404835.93094067 2845538.743090079 0, -1404776.9849010152 2845832.7790643815 0, -1404698.3157223004 2846224.9341655592 0, -1404619.6501308896 2846617.0814418728 0, -1404613.1333087308 2846615.800988013 0, -1404611.440918708 2846624.325265719 0, -1404217.1673162603 2846545.7387325265 0, -1403822.8913253082 2846467.1743903724 0, -1403428.6090668149 2846388.631626333 0, -1403034.3220979962 2846310.11094714 0, -1403053.4782844791 2846213.634980691 0, -1403098.5972614503 2845986.403067261 0, -1403102.6692528867 2845986.22169955 0, -1403103.248347781 2845983.290500964 0, -1403194.7240722105 2845979.1141459174 0, -1403449.0559606147 2846028.010740485 0, -1403504.9632931324 2846028.6813831767 0, -1403799.7788403556 2846032.221859208 0, -1403917.369560205 2846021.144461339 0, -1404023.201279463 2846011.177178477 0, -1404120.1833968922 2845982.644777186 0, -1404347.9635557476 2845922.9921767535 0, -1404384.173923037 2845913.506921877 0)), ((-1397408.2962231054 2850092.3249010867 0, -1397368.4896856248 2850084.068534674 0, -1397446.3713279825 2849691.2643500497 0, -1397505.381414212 2849392.6996998107 0, -1397510.6108350344 2849365.822199518 0, -1397524.2513040218 2849298.457697818 0, -1397541.4491653107 2849211.7165610585 0, -1397541.458220491 2849211.6708892966 0, -1397542.5345600036 2849206.2421379318 0, -1397543.8495907197 2849199.6533351694 0, -1397552.4185829689 2849156.451312542 0, -1397575.9850958055 2849037.5695722825 0, -1397592.0332196734 2848956.627131109 0, -1397592.679842527 2848953.3228822346 0, -1397592.6798425396 2848953.3228821703 0, -1397602.13302944 2848905.6434157547 0, -1397665.8361152133 2848583.3899085936 0, -1397680.0171525239 2848512.827412834 0, -1397680.0171525334 2848512.8274127864 0, -1397929.700960232 2848562.7028559577 0, -1397929.7009632865 2848562.702856566 0, -1397948.4323890347 2848566.4242267665 0, -1397957.4309592475 2848568.2419514772 0, -1397957.4309620752 2848568.241952046 0, -1398077.2551434217 2848592.176531594 0, -1398141.5814011388 2848605.029787731 0, -1398239.0745437716 2848624.510235964 0, -1398247.1236719787 2848626.1050571734 0, -1398282.7133075856 2848633.219462183 0, -1398287.580911698 2848634.192208714 0, -1398327.5059190358 2848642.169873064 0, -1398332.0947335428 2848643.086969197 0, -1398372.692625795 2848651.1939333444 0, -1398377.8822906353 2848652.2453921833 0, -1398377.8822907384 2848652.2453922043 0, -1398377.8822960923 2848652.2453932827 0, -1398474.4887164899 2848671.5479072505 0, -1398871.7176727587 2848750.941513455 0, -1398936.6503813192 2848763.925655422 0, -1398962.2122963727 2848769.0345055317 0, -1399102.7436877913 2848797.11353484 0, -1399111.7925354156 2848798.9398238114 0, -1399113.3217560383 2848799.2471367856 0, -1399268.9442821615 2848830.357851166 0, -1399266.4973957373 2848842.226063975 0, -1399231.7310575226 2849019.0364407757 0, -1399231.7310429218 2849019.036515031 0, -1399221.9107939033 2849069.0883870637 0, -1399215.8337490482 2849099.6392980004 0, -1399215.8337490472 2849099.639298005 0, -1399215.833740717 2849099.639340032 0, -1399191.420180221 2849223.420864117 0, -1399191.322303488 2849223.9171182876 0, -1399113.7035125983 2849617.4718418084 0, -1399036.0835453114 2850011.0212396816 0, -1398958.4665678807 2850404.5660594977 0, -1398945.88544305 2850402.2433631923 0, -1398647.0857153283 2850341.77419907 0, -1398647.0857049285 2850341.774196965 0, -1398647.085704724 2850341.7741969237 0, -1398622.6991095608 2850336.8458357486 0, -1398618.7863314683 2850336.06729265 0, -1398618.7863266538 2850336.0672917007 0, -1398560.9794564047 2850324.409822854 0, -1398193.5005080379 2850250.547556947 0, -1398163.4883337207 2850244.272879605 0, -1397765.99050446 2850164.157983164 0, -1397408.2962231054 2850092.3249010867 0)), ((-1408499.7917902402 2851897.0108265877 0, -1408421.0447701633 2852289.2328041033 0, -1408208.4406804384 2852246.8743553446 0, -1408024.111393916 2852209.763787432 0, -1407803.8467946316 2852165.883525409 0, -1407627.1719187878 2852130.313602257 0, -1407230.2294260436 2852050.8889755737 0, -1407230.2294255465 2852050.888975477 0, -1407206.2683501462 2852046.303831964 0, -1406833.2804088348 2851971.486434671 0, -1406833.280408835 2851971.4864346697 0, -1406911.933817793 2851579.414764962 0, -1406921.6758014641 2851530.0046396935 0, -1406934.686355972 2851465.14776617 0, -1406956.335386052 2851357.2290452607 0, -1406990.586042128 2851187.337697579 0, -1406990.5860421804 2851187.3376973188 0, -1406990.5860422545 2851187.3376969495 0, -1407041.0215364834 2850935.08214724 0, -1407069.2414205894 2850795.256210503 0, -1407069.2414206765 2850795.2562100706 0, -1407069.2414206867 2850795.2562100184 0, -1407073.5684860025 2850772.8424741207 0, -1407147.89795659 2850403.1700436547 0, -1407147.8979565974 2850403.170043656 0, -1407147.897956598 2850403.1700436533 0, -1407506.3690000873 2850474.723267223 0, -1407544.9384991385 2850482.421997814 0, -1407941.9745221676 2850561.6962001207 0, -1408339.0062130108 2850640.9927756977 0, -1408736.0331859435 2850720.3115733187 0, -1408657.41158823 2851111.919579926 0, -1408657.2847018465 2851112.5515910415 0, -1408578.5377025602 2851504.7836576267 0, -1408499.7917902402 2851897.0108265877 0)), ((-1402322.4997742055 2855962.8549554977 0, -1401926.2423490663 2855884.0684591965 0, -1401529.9818892553 2855805.3075370626 0, -1401133.7178690603 2855726.5661011315 0, -1401213.211228292 2855335.412905123 0, -1401292.708138397 2854944.2551045995 0, -1401372.2039204885 2854553.0919847465 0, -1401451.7031004892 2854161.9246495627 0, -1401847.939906079 2854240.6579817794 0, -1402244.174336076 2854319.414166907 0, -1402640.4039476456 2854398.195590499 0, -1403036.6295266182 2854476.9962373967 0, -1402957.1582407928 2854868.1687561497 0, -1402877.6877139623 2855259.339419323 0, -1402798.2189316931 2855650.5022341553 0, -1402718.750697533 2856041.6632575803 0, -1402322.4997742055 2855962.8549554977 0)), ((-1411751.5853603992 2856418.185144432 0, -1411754.7571084467 2856429.033555226 0, -1411767.7582414288 2856473.501728358 0, -1411817.3561956498 2856643.1425894992 0, -1411842.2963358818 2856728.4480426703 0, -1411857.2971659566 2856779.7566173365 0, -1411866.2335776836 2856810.323187832 0, -1411899.5147161097 2856924.1581729716 0, -1411899.2923966853 2856930.5015921816 0, -1411897.9417615307 2856969.061157462 0, -1411894.9402896597 2857054.74085981 0, -1411894.5358408932 2857066.285733073 0, -1411894.0926921885 2857078.934847568 0, -1411893.5171049975 2857095.3595575998 0, -1411891.713688685 2857146.8214332475 0, -1411889.994330014 2857195.9125946364 0, -1411889.699684305 2857204.325522127 0, -1411880.874398725 2857470.4536910965 0, -1411878.0360349421 2857552.343632654 0, -1411875.6033314364 2857624.912060565 0, -1411877.2522324275 2857628.9538111114 0, -1411915.182499596 2857721.932867112 0, -1411933.3960081232 2857766.5799572086 0, -1411978.6628281383 2857877.543262183 0, -1411987.1789034253 2857898.418955808 0, -1411967.8125782465 2857894.7388543542 0, -1411940.9460620254 2857889.3657909026 0, -1411827.0057558136 2857866.5978943333 0, -1411816.2609931997 2857864.4504358424 0, -1411785.6653254726 2857858.335715912 0, -1411778.7458917818 2857856.7582134116 0, -1411778.7458915478 2857856.758213361 0, -1411594.861806844 2857819.9848252423 0, -1411383.7384575654 2857777.7640921324 0, -1411367.0593044949 2857774.617511555 0, -1410990.311091655 2857698.9297966924 0, -1410858.0004306268 2857672.622335774 0, -1410596.879148821 2857620.1174235255 0, -1410621.9852533883 2857491.62132465 0, -1410633.7672996472 2857431.7274165326 0, -1410674.0526222952 2857227.8057096056 0, -1410674.0526223222 2857227.805709468 0, -1410751.224144693 2856835.4917604737 0, -1410757.8768594344 2856800.8060144023 0, -1410820.825048066 2856480.8087421665 0, -1410828.3986047867 2856443.173116284 0, -1410828.3986047988 2856443.1731162234 0, -1410828.3986048105 2856443.173116164 0, -1410842.1263099334 2856372.5611441107 0, -1410905.5745906155 2856050.8465852523 0, -1411295.5805096321 2856130.8219032804 0, -1411432.25054098 2856158.360234526 0, -1411432.2505409804 2856158.360234527 0, -1411432.3744690558 2856158.659060573 0, -1411528.0464481325 2856236.440972607 0, -1411560.3916010382 2856262.7377897943 0, -1411667.3655141646 2856349.7080069594 0, -1411702.6279902614 2856378.379090404 0, -1411740.73912433 2856409.366361044 0, -1411751.5853603992 2856418.185144432 0)), ((-1405261.3863524538 2859814.963898068 0, -1405651.2703595373 2859892.5344997076 0, -1406048.3939748404 2859971.7027081377 0, -1406445.5149132037 2860050.8938099025 0, -1406842.6286486182 2860130.1098150183 0, -1406842.628648618 2860130.1098150196 0, -1406764.8265913033 2860522.0183203532 0, -1406688.7504382622 2860905.23269522 0, -1406687.0248609448 2860913.924854412 0, -1406687.0248609437 2860913.924854418 0, -1406415.590490284 2860859.6128464383 0, -1406290.115452382 2860834.5054980735 0, -1405897.4905057237 2860756.1532146623 0, -1405893.2084571854 2860755.084839173 0, -1405815.6258750965 2861146.7138585607 0, -1406212.4251978938 2861226.269456487 0, -1406609.224541734 2861305.8234384237 0, -1406531.4236872834 2861697.717321509 0, -1406531.4236872534 2861697.717321503 0, -1406531.4236872522 2861697.717321509 0, -1406134.7369737187 2861618.013712855 0, -1405738.045266009 2861538.3353076545 0, -1405341.3495085759 2861458.6764138103 0, -1404944.6466850971 2861379.042249062 0, -1405022.0205961196 2860987.6359433997 0, -1405099.3936611253 2860596.2250118344 0, -1405176.7677404573 2860204.8092027605 0, -1404780.8769870354 2860124.730539985 0, -1404858.3628771487 2859733.3601081683 0, -1404935.3719751574 2859342.672009466 0, -1405331.1001697828 2859423.1280607716 0, -1405254.1434443628 2859813.3853914333 0, -1405261.3863524538 2859814.963898068 0)), ((-1402682.2020684432 2864118.7237778557 0, -1402695.4529211784 2864121.2283095215 0, -1402695.4529211782 2864121.228309523 0, -1402616.8936437613 2864513.0297153555 0, -1402538.3358605783 2864904.823133617 0, -1402499.8153482743 2865096.9325434817 0, -1402459.7765047003 2865296.6141715446 0, -1402419.7474271564 2865496.252592065 0, -1402381.2202299368 2865688.4006322375 0, -1402381.2202299358 2865688.4006322417 0, -1401983.5451695155 2865608.8553613233 0, -1401712.7970666003 2865554.720197429 0, -1401585.8632989998 2865529.3320246567 0, -1401188.179284525 2865449.831439479 0, -1401188.1792117932 2865449.831424936 0, -1401097.3997936426 2865431.6841614405 0, -1401084.8622124526 2865429.1840025107 0, -1400799.226584094 2865372.3078978863 0, -1400790.4886198821 2865370.35311039 0, -1400868.6112097064 2864978.9369326024 0, -1400945.8802026587 2864590.1986702695 0, -1400946.7321918367 2864587.5186793273 0, -1401024.8546978398 2864196.092250667 0, -1401100.9681356936 2863813.8579939683 0, -1401102.9804730942 2863804.661391134 0, -1401161.397036985 2863816.255982978 0, -1401501.1095115985 2863883.7670430006 0, -1401558.569074346 2863895.1879364145 0, -1401899.2323785443 2863962.904431385 0, -1401955.7386749384 2863974.1206539576 0, -1402297.3480475233 2864042.044840975 0, -1402352.9085788366 2864053.0954119097 0, -1402682.2020684432 2864118.7237778557 0)), ((-1411465.037336772 2865648.779537992 0, -1411463.8557415532 2865655.0362547883 0, -1411467.7572204815 2865655.390586278 0, -1411528.471929807 2865656.642773342 0, -1411528.4719302277 2865656.6427733493 0, -1411528.471930238 2865656.6427733507 0, -1411528.4719302412 2865656.6427733507 0, -1411569.6250164183 2865661.9779159166 0, -1411578.782938681 2865663.366841497 0, -1411605.6501287578 2865674.490354063 0, -1411625.477942975 2865682.6947615296 0, -1411631.7469223023 2865685.3064114386 0, -1411632.7949084023 2865685.7423111056 0, -1411635.878725861 2865685.393298609 0, -1411647.15672865 2865684.1156663178 0, -1411652.734374543 2865683.483661498 0, -1411663.069627925 2865682.308265712 0, -1411676.9610435506 2865680.725924123 0, -1411731.4632386134 2865723.2860093727 0, -1411740.6671240507 2865730.519389325 0, -1411822.090020838 2865718.2191672903 0, -1411838.3978266304 2865715.9588456973 0, -1411841.073689812 2865717.1605165387 0, -1411983.169821221 2865779.4717531553 0, -1411983.1698278135 2865779.4717560387 0, -1411999.7797165555 2865786.7246760647 0, -1412158.2912243297 2865835.9466782827 0, -1412170.146075653 2865836.9489773572 0, -1412170.146076222 2865836.9489774047 0, -1412229.6105864234 2865841.7906655665 0, -1412229.6105864223 2865841.790665572 0, -1412229.6105864225 2865841.790665572 0, -1412229.6105863927 2865841.7906657173 0, -1412219.1846687484 2865892.884224412 0, -1412162.0192036116 2866176.968186281 0, -1412082.825008011 2866569.0058447286 0, -1412002.6728112134 2866961.1972452626 0, -1411922.5221962316 2867353.380643108 0, -1411922.5221962258 2867353.3806431065 0, -1411922.522196224 2867353.3806431163 0, -1411583.5471875449 2867284.2856640294 0, -1411524.470183467 2867272.0276043857 0, -1411445.3103906135 2867256.03696549 0, -1411360.55465754 2867238.708295354 0, -1411126.4154879246 2867190.697131833 0, -1411025.867544467 2867170.3460400575 0, -1410917.9101386506 2867148.296874894 0, -1410817.3561835214 2867127.759786799 0, -1410728.3555018317 2867109.3920901567 0, -1410728.3549554553 2867109.3919785875 0, -1410610.287801935 2867085.2829328044 0, -1410330.3074244468 2867028.109796696 0, -1410330.291306805 2867028.1065054135 0, -1410361.2985384562 2866873.7711350676 0, -1410409.33354803 2866634.6905706557 0, -1410420.9139694646 2866577.055654584 0, -1410440.2146718572 2866480.997461124 0, -1410440.2146719096 2866480.9974608603 0, -1410456.6149111663 2866398.174093309 0, -1410463.2236422338 2866365.1634405 0, -1410488.222008319 2866241.2386903674 0, -1410504.0888303516 2866161.32310462 0, -1410519.0021884008 2866088.0397656164 0, -1410519.002188406 2866088.0397655913 0, -1410566.296370515 2865852.6473873486 0, -1410597.9484032183 2865695.10541922 0, -1410644.2002541109 2865464.0360314716 0, -1410644.2099788839 2865464.0379698332 0, -1410644.2113585516 2865464.0310786646 0, -1410684.423421186 2865472.053394944 0, -1411044.5673082075 2865544.3390496573 0, -1411064.664278303 2865548.3758619865 0, -1411303.885356992 2865596.5309854182 0, -1411444.901632407 2865624.715773975 0, -1411454.7045603914 2865626.808822695 0, -1411468.8876433342 2865629.512212369 0, -1411468.8876433324 2865629.512212379 0, -1411465.037336772 2865648.779537992 0)), ((-1405352.3578766033 2869543.935077524 0, -1405359.1363504976 2869545.2042935197 0, -1405436.3132154464 2869560.2322490425 0, -1405502.746418892 2869573.2515146 0, -1405502.7464338238 2869573.2515175208 0, -1405720.6097105232 2869615.720096893 0, -1406118.040747909 2869693.2168943826 0, -1406295.4979188778 2869727.8309028526 0, -1406335.326025477 2869735.548965003 0, -1406368.3830205046 2869742.047260953 0, -1406368.3830230972 2869742.047261461 0, -1406515.4696160685 2869770.7362509747 0, -1406515.4696160683 2869770.736250976 0, -1406515.3518045028 2869771.324431194 0, -1406436.8880400027 2870163.058756294 0, -1406358.3075719213 2870555.3763669888 0, -1406349.6235684261 2870598.7326819636 0, -1406349.6235644566 2870598.7327020443 0, -1406348.2495920586 2870605.7389051924 0, -1406343.9503185805 2870627.2036582665 0, -1406334.9120333896 2870672.1828832966 0, -1406279.7301098744 2870947.689329546 0, -1406259.8342604002 2871047.0207821187 0, -1406256.6776818188 2871062.9237264954 0, -1406248.9494264596 2871101.3638142054 0, -1406201.1516861857 2871339.9969154075 0, -1405935.8783990357 2871288.0464658416 0, -1405919.2268095443 2871284.7765399343 0, -1405859.9066085038 2871273.1582050133 0, -1405856.2419319113 2871272.450294864 0, -1405856.241927392 2871272.4502939982 0, -1405803.751681128 2871262.170407299 0, -1405658.300430607 2871233.6943604634 0, -1405644.932170153 2871231.0641286485 0, -1405623.858496985 2871226.937981929 0, -1405605.0992181995 2871223.278679066 0, -1405605.0992040872 2871223.278676319 0, -1405406.3471053601 2871184.366241646 0, -1405435.624495818 2871038.2277601827 0, -1405437.0592010934 2871031.0664098286 0, -1405441.9988417523 2871006.4998400114 0, -1405484.3701475295 2870794.999082076 0, -1405484.9057895474 2870792.2393457848 0, -1405479.7815442246 2870791.226744264 0, -1405424.8324013767 2870780.4771098006 0, -1405420.8968640964 2870779.7077110303 0, -1405370.7645056879 2870769.9052323746 0, -1405367.6517246566 2870769.2986274436 0, -1405283.9653302229 2870752.933274581 0, -1405255.9106829148 2870747.465511902 0, -1405255.9106593088 2870747.46550731 0, -1405205.8767456764 2870737.7331411466 0, -1405087.490981406 2870714.534637766 0, -1405066.3558166963 2870710.5732503003 0, -1404937.6800193107 2870685.241462984 0, -1404912.420841931 2870680.2812086833 0, -1404873.690080004 2870672.728276086 0, -1404690.0778117212 2870636.8252614536 0, -1404690.077166699 2870636.8251353293 0, -1404690.0771666993 2870636.825135328 0, -1404708.0471434693 2870547.146432178 0, -1404710.958022651 2870532.710837276 0, -1404753.5632293806 2870320.0914300634 0, -1404767.9136741732 2870248.445385562 0, -1404768.6279536458 2870244.8196088024 0, -1404768.6279536616 2870244.819608721 0, -1404775.7641339956 2870209.20661129 0, -1404775.7641365211 2870209.206598999 0, -1404776.9359453998 2870203.4499911657 0, -1404809.6746020482 2870040.0693464084 0, -1404828.469240713 2869946.2757398025 0, -1404829.4227403163 2869941.5171959335 0, -1404831.863324543 2869929.2458460294 0, -1404847.1798434148 2869852.8091909704 0, -1404851.4089969185 2869831.7039236957 0, -1404851.4422845743 2869831.5378041933 0, -1404852.1575244702 2869828.0605850974 0, -1404853.231110614 2869822.7023808896 0, -1404856.9175901003 2869804.3054733314 0, -1404883.9239550708 2869669.5310635734 0, -1404889.6944281512 2869640.6415555426 0, -1404889.6944321946 2869640.6415352616 0, -1404925.732661221 2869460.793662609 0, -1405323.1722710785 2869538.245600288 0, -1405352.3578766033 2869543.935077524 0)), ((-1403270.9110435373 2873607.989720598 0, -1403195.57265247 2873987.095011088 0, -1402798.6169425067 2873907.8261163756 0, -1402874.1480264233 2873528.383814522 0, -1402952.0604383987 2873136.965264704 0, -1403348.7412445976 2873216.3452473097 0, -1403270.9110435373 2873607.989720598 0)), ((-1400722.020211627 2873987.416916897 0, -1400659.8349719865 2874300.9579526847 0, -1400582.1008802357 2874692.897713141 0, -1400504.368199048 2875084.8295678613 0, -1400504.3681990472 2875084.8295678655 0, -1400306.06796822 2875046.0779310446 0, -1400108.2805656404 2875006.994913384 0, -1399712.1886875827 2874929.1824742686 0, -1399316.0923516774 2874851.392322538 0, -1398919.9918312414 2874773.6246947986 0, -1398997.4825770769 2874381.3695183387 0, -1399074.9721307347 2873989.109292349 0, -1399152.464837142 2873596.8441945347 0, -1399229.9583728071 2873204.574122286 0, -1399626.3009079173 2873282.6651033484 0, -1400022.6398035127 2873360.7752654627 0, -1400418.9757098868 2873438.911310901 0, -1400341.2951306698 2873830.9661018522 0, -1400408.590619487 2873844.220564607 0, -1400737.569628418 2873909.015992905 0, -1400737.5696284168 2873909.0159929106 0, -1400737.5696284187 2873909.015992911 0, -1400722.020211627 2873987.416916897 0)), ((-1409103.6964492481 2875025.2421185113 0, -1409141.8900567754 2875032.891256656 0, -1409213.6801065572 2875047.2731291484 0, -1409213.6801090706 2875047.273129647 0, -1409229.77988655 2875050.449152512 0, -1409285.8021089113 2875061.721309533 0, -1409285.8021396676 2875061.7213157113 0, -1409535.654514666 2875111.773087116 0, -1409929.4117891053 2875190.679700427 0, -1409971.24784557 2875199.065926775 0, -1409971.2478463105 2875199.065926921 0, -1409978.7519803427 2875200.531137577 0, -1410108.979261336 2875226.637376353 0, -1410140.157719893 2875232.924347864 0, -1410323.172103583 2875269.6090371227 0, -1410323.1721035815 2875269.609037131 0, -1410323.1721035817 2875269.609037131 0, -1410280.0390395173 2875485.7118710545 0, -1410275.657886319 2875507.7470515314 0, -1410272.7716184133 2875522.122472482 0, -1410244.8465344294 2875662.031449576 0, -1410244.846486525 2875662.031689817 0, -1410238.80266182 2875692.360027673 0, -1410188.7019879804 2875943.3155002077 0, -1410185.8364133637 2875957.6702931076 0, -1410166.5198291473 2876054.448420859 0, -1410154.9493124203 2876112.3908099523 0, -1410129.6492050847 2876239.1153764776 0, -1410097.0531707695 2876404.0092286854 0, -1410096.267817752 2876406.490527884 0, -1410095.9545911942 2876406.9131187014 0, -1410092.6124654415 2876411.4155137967 0, -1410071.9405331241 2876439.594348282 0, -1410067.334844834 2876445.872557595 0, -1410044.8896179674 2876476.467052874 0, -1410017.2528691767 2876514.1379344515 0, -1410017.2528691764 2876514.1379344515 0, -1410017.2513635792 2876514.139986689 0, -1409975.5495828802 2876541.3013308863 0, -1409950.1803787204 2876557.8212493835 0, -1409908.6595203627 2876584.8949637697 0, -1409866.487935356 2876612.392758426 0, -1409766.4990217146 2876677.5969618005 0, -1409766.4997185215 2876677.6499651307 0, -1409766.2500051307 2876677.812799691 0, -1409766.6451122717 2876704.2036529 0, -1409767.1408562034 2876737.3104113834 0, -1409767.507660834 2876761.8052125834 0, -1409769.9336998635 2876795.1547505893 0, -1409764.5592822868 2876794.095048755 0, -1409627.5944055112 2876766.6532114935 0, -1409510.6739233304 2876743.2241767757 0, -1409446.8540509548 2876730.4106893907 0, -1409310.6548475022 2876703.0646280306 0, -1409263.1621494931 2876693.52887364 0, -1409260.287299188 2876692.9515570784 0, -1409230.218035185 2876686.8663708684 0, -1408832.1384908531 2876608.0227922006 0, -1408774.6639410295 2876596.8008374856 0, -1408728.6500602255 2876587.657983948 0, -1408514.9915482828 2876545.2276930353 0, -1408514.9915142735 2876545.2276862813 0, -1408455.7443594562 2876533.474764181 0, -1408452.775912659 2876532.908685063 0, -1408434.0567597842 2876529.2021547086 0, -1408446.2223965924 2876468.189760085 0, -1408486.3784147138 2876266.7236018917 0, -1408489.3887333323 2876251.6218461953 0, -1408512.5581591323 2876135.3886321625 0, -1408529.94382</t>
+          <t>MULTIPOLYGON Z (((-1406379.8180101914 2835502.9676008387 0, -1406473.9785516895 2835521.734531294 0, -1406778.7770429626 2835582.4882667917 0, -1406872.8312997553 2835601.148932945 0, -1406791.7645722493 2835992.9266004586 0, -1406710.698745883 2836384.702508994 0, -1406629.6366764735 2836776.4711096287 0, -1406548.5739271764 2837168.2345223785 0, -1406152.1431418383 2837088.956904065 0, -1406087.6405494164 2837076.280484532 0, -1405796.91670816 2837018.1569047323 0, -1405755.7083628573 2837009.698301688 0, -1405535.803621465 2836965.9663151815 0, -1405487.176097592 2836956.2471401114 0, -1405359.2691901615 2836930.461773824 0, -1405080.115136758 2836874.9046132243 0, -1404962.8255844747 2836851.2476163614 0, -1405025.8156075906 2836537.4335374683 0, -1405029.769174486 2836517.7370062955 0, -1405041.4965421397 2836459.306839623 0, -1405041.4965422011 2836459.306839316 0, -1405081.6600892353 2836258.4058300443 0, -1405108.2831449925 2836126.578187748 0, -1405120.0309416638 2836067.337313631 0, -1405133.2551556446 2836000.645850542 0, -1405186.659309687 2835735.386966785 0, -1405188.114813715 2835727.329112005 0, -1405192.8804176834 2835703.5856685042 0, -1405198.701406638 2835675.389715876 0, -1405261.8129454285 2835360.1547357994 0, -1405265.1738896933 2835344.2151984107 0, -1405277.2234497615 2835283.407895384 0, -1405277.2234497755 2835283.4078953867 0, -1405277.2234497757 2835283.4078953853 0, -1405581.9305416776 2835344.089946119 0, -1405676.1759969064 2835362.862839606 0, -1405980.8366573509 2835423.550296702 0, -1406075.138144352 2835442.2583379205 0, -1406202.3274685177 2835467.601562032 0, -1406379.8180101914 2835502.9676008387 0)), ((-1399310.6939220119 2840250.9220541627 0, -1399335.4899758273 2840125.914068922 0, -1399347.1961440216 2840066.79943821 0, -1399356.4079068387 2840020.2810208434 0, -1399368.1809894112 2839960.4057747424 0, -1399384.6546780465 2839877.227700831 0, -1399462.396458146 2839484.6995438226 0, -1399540.139008013 2839092.1665506647 0, -1399542.905688448 2839092.835199241 0, -1399556.3294038298 2839095.3861888293 0, -1399556.329404045 2839095.3861888703 0, -1399561.6720821362 2839096.376602012 0, -1399582.007635379 2839100.423022579 0, -1399599.5649045492 2839103.916675662 0, -1399623.3376730068 2839108.6470440533 0, -1399644.5027693652 2839112.8586522965 0, -1399667.8546858106 2839117.505222619 0, -1399689.9714188937 2839121.9060038663 0, -1399712.3326666437 2839126.3553711157 0, -1399735.4324632378 2839130.9517879887 0, -1399753.6615634388 2839134.578885354 0, -1399780.8692110055 2839139.992492276 0, -1399798.1407629494 2839143.429084783 0, -1399826.33910559 2839149.039729029 0, -1399842.651850635 2839152.2853515954 0, -1399871.8019453995 2839158.085069711 0, -1399883.9572934853 2839160.5036009005 0, -1399916.771608468 2839167.0324040405 0, -1399928.497425498 2839169.3652046104 0, -1399934.4273121587 2839170.492037641 0, -1399937.3344581702 2839171.1505293464 0, -1399937.334458662 2839171.150529451 0, -1399937.3344694409 2839171.1505315923 0, -1399961.7740465652 2839175.991441545 0, -1399972.9727293379 2839178.2173738675 0, -1400007.6713144428 2839185.123969481 0, -1400014.3015124146 2839186.44347234 0, -1400053.0843019113 2839194.164184724 0, -1400059.1674090049 2839195.3749906607 0, -1400062.5253671096 2839196.043416641 0, -1400098.5195565978 2839203.2079879213 0, -1400103.2938011107 2839204.1582646235 0, -1400135.8492566794 2839210.638179495 0, -1400135.84925794 2839210.638179746 0, -1400143.9549004098 2839212.251141099 0, -1400147.7740981488 2839213.0111707496 0, -1400189.1188868866 2839221.238374427 0, -1400322.934807602 2839247.8660599813 0, -1400331.4578416802 2839249.561483696 0, -1400334.5232879098 2839250.1564733693 0, -1400337.289539137 2839250.8269082224 0, -1400438.6676987924 2839270.9013746134 0, -1400616.4727830754 2839306.2846389473 0, -1400666.7624768384 2839316.2673303704 0, -1400731.7096861927 2839329.18493668 0, -1400734.4720727175 2839329.8709867066 0, -1400774.2737872985 2839337.662505503 0, -1400819.7837660834 2839346.7515740218 0, -1401125.8721471464 2839407.6680866037 0, -1401128.8917457967 2839408.235767459 0, -1401123.9478869513 2839432.9798185662 0, -1401114.9923184975 2839478.068050874 0, -1401105.4885421125 2839525.9158027335 0, -1401103.154785328 2839537.809666259 0, -1401103.15478518 2839537.809667019 0, -1401067.6565216575 2839720.071360423 0, -1401063.830226231 2839739.28926802 0, -1401063.2021711767 2839742.434400068 0, -1401053.3518599859 2839788.545631688 0, -1401050.9229196983 2839800.7740466096 0, -1401050.9229196971 2839800.7740466157 0, -1401053.6475980359 2839801.596686764 0, -1400999.4443926136 2840062.6907491884 0, -1400998.724069705 2840066.308780294 0, -1400989.0886561542 2840114.569291522 0, -1400975.3905077311 2840183.1795261377 0, -1400973.5361308318 2840190.382025044 0, -1400973.536130806 2840190.382025154 0, -1400972.9550610757 2840193.3075143024 0, -1400954.6895441287 2840190.4323968505 0, -1400920.226759528 2840183.5676653488 0, -1400578.8062332084 2840115.124226884 0, -1400575.8805057171 2840114.2936359607 0, -1400575.7633936796 2840117.3285491103 0, -1400574.844702643 2840122.2522871094 0, -1400574.022585394 2840126.3318334757 0, -1400566.8949736727 2840162.4611979346 0, -1400542.6533913193 2840284.271411241 0, -1400539.2966141847 2840301.1361504267 0, -1400517.715227514 2840409.5622253655 0, -1400512.0344126902 2840438.1135863895 0, -1400502.104311991 2840485.9874962857 0, -1400497.9721403266 2840506.8058186676 0, -1400497.390664912 2840509.80477352 0, -1400452.1259811474 2840738.4564959686 0, -1400451.4587958015 2840741.808285925 0, -1400428.6235849268 2840856.2023643884 0, -1400420.8018900126 2840895.468983268 0, -1400420.069223923 2840899.301431375 0, -1400274.7199397993 2840870.543052567 0, -1400213.4646311947 2840858.3298914144 0, -1400023.1088309977 2840820.26744506 0, -1400022.4191629284 2840823.311960139 0, -1399739.523394895 2840764.6045222455 0, -1399736.5386692584 2840764.0057220142 0, -1399709.2365354546 2840758.5145079345 0, -1399626.1434866686 2840741.2589619365 0, -1399229.1764102448 2840662.2699850057 0, -1399306.9140804114 2840269.750971841 0, -1399306.9140826785 2840269.7509606453 0, -1399308.926485363 2840259.6770075844 0, -1399310.6939220119 2840250.9220541627 0)), ((-1399229.1764102448 2840662.2699850057 0, -1399151.2946448606 2841054.7992079007 0, -1398754.3652302015 2840975.7562494082 0, -1398357.4368467703 2840896.7085765144 0, -1398434.9954991627 2840504.121791033 0, -1398832.0885730598 2840583.1832069866 0, -1399229.1764102448 2840662.2699850057 0)), ((-1410207.0886851817 2841171.569820003 0, -1410292.106862424 2841187.9271961376 0, -1410693.8600138929 2841265.8675316847 0, -1410641.7045664315 2841528.5669757756 0, -1410634.2942596902 2841565.9644431355 0, -1410616.0088154103 2841658.7990578404 0, -1410598.9623274822 2841744.276462479 0, -1410583.5237163594 2841822.194011335 0, -1410567.3071516913 2841904.0386808235 0, -1410550.4485024924 2841989.125877908 0, -1410546.7760295542 2842007.661339168 0, -1410538.1586854516 2842051.725978964 0, -1410475.0699257555 2842369.6151062693 0, -1410460.3759917119 2842444.344847481 0, -1410410.353163191 2842696.3028291394 0, -1410373.9500720813 2842880.5766738653 0, -1410314.8445090398 2842868.6933648163 0, -1410314.8445067066 2842868.6933643688 0, -1410074.8976017982 2842822.7379557453 0, -1409974.2514204897 2842803.210860995 0, -1409926.9607263294 2842794.120359546 0, -1409574.4517075391 2842726.364992527 0, -1409539.7596685698 2842719.476227892 0, -1409539.1167997618 2842719.3485740544 0, -1409539.1167996211 2842719.3485740265 0, -1409407.3427740564 2842693.406117487 0, -1409174.87310327 2842647.185105116 0, -1409135.3708942847 2842639.3610066515 0, -1408775.2871312238 2842568.0429873103 0, -1408775.2871312243 2842568.042987308 0, -1408775.2871312224 2842568.0429873075 0, -1408791.982561276 2842482.1825481723 0, -1408859.431612287 2842135.3088754904 0, -1408936.0102514483 2841742.172147534 0, -1409010.5622617726 2841352.679039439 0, -1409011.4184577104 2841348.2058882047 0, -1409086.8267116826 2840954.237889088 0, -1409107.1392109245 2840958.307386213 0, -1409374.2239804657 2841010.0749029545 0, -1409488.590801991 2841032.1093411823 0, -1409488.590810442 2841032.1093428046 0, -1409488.5908287365 2841032.1093463674 0, -1409735.5629954843 2841080.1273449566 0, -1409890.3520447423 2841110.0070721535 0, -1410027.3861210642 2841136.7169916257 0, -1410207.0886851817 2841171.569820003 0)), ((-1404413.0040087868 2845598.7170888362 0, -1404411.9634668445 2845599.4135239385 0, -1404403.6665685656 2845604.966773168 0, -1404367.6175215868 2845629.094281301 0, -1404365.3857084531 2845630.5880346466 0, -1404365.3856752666 2845630.588048675 0, -1404359.7842581766 2845634.337058641 0, -1404209.994285118 2845697.6924938657 0, -1403967.0449391939 2845739.4757514074 0, -1403962.6991410798 2845740.222877639 0, -1403925.888990231 2845756.5350805065 0, -1403811.697381762 2845808.3746001213 0, -1403763.0290770517 2845813.871618658 0, -1403678.995867877 2845799.875162555 0, -1403644.1093635445 2845787.7281875107 0, -1403561.9104531568 2845792.578875461 0, -1403546.0403714462 2845795.453029865 0, -1403471.1140033456 2845809.0260385834 0, -1403350.954397719 2845815.8751161206 0, -1403137.9662648952 2845786.6090687537 0, -1403161.1101112196 2845669.769369071 0, -1403161.3519901694 2845669.741687514 0, -1403161.3953671006 2845669.522701863 0, -1403166.1869040276 2845668.9743470913 0, -1403166.6076956226 2845666.871903373 0, -1403587.2478790737 2845618.1462674816 0, -1403645.7782884282 2845611.3678443404 0, -1403671.7299334654 2845608.36233764 0, -1403654.8238005526 2845469.124905376 0, -1403609.740873767 2845474.285456348 0, -1403190.3208668637 2845522.3126093117 0, -1403267.3277244826 2845133.712013439 0, -1403345.307317196 2844741.3896947694 0, -1403345.3073174688 2844741.3896933924 0, -1403351.278613076 2844742.575062426 0, -1403351.9856773617 2844739.030921994 0, -1403739.775040757 2844819.6959529603 0, -1403739.7750432093 2844819.695953447 0, -1403739.775176096 2844819.695979834 0, -1404142.2220031724 2844899.538941732 0, -1404538.6548402628 2844972.33059754 0, -1404934.1430632109 2845049.787531759 0, -1404468.8456640067 2845562.344196431 0, -1404413.0040087868 2845598.7170888362 0)), ((-1404384.173923037 2845913.506921877 0, -1404460.723088921 2845877.299411543 0, -1404498.694650209 2845842.6323788343 0, -1404543.1465726472 2845794.266376779 0, -1404553.1898897956 2845768.42480921 0, -1404560.4058094958 2845767.591449572 0, -1404562.263610549 2845762.872978879 0, -1404602.726522319 2845758.1884405124 0, -1404617.3759774447 2845736.0786963697 0, -1404641.038383801 2845700.366122346 0, -1404770.6570928784 2845608.785523316 0, -1404825.8077152742 2845544.414600234 0, -1404824.4991240369 2845551.0100588636 0, -1404835.93094067 2845538.743090079 0, -1404776.9849010152 2845832.7790643815 0, -1404698.3157223004 2846224.9341655592 0, -1404619.6501308896 2846617.0814418728 0, -1404613.1333087308 2846615.800988013 0, -1404611.440918708 2846624.325265719 0, -1404217.1673162603 2846545.7387325265 0, -1403822.8913253082 2846467.1743903724 0, -1403428.6090668149 2846388.631626333 0, -1403034.3220979962 2846310.11094714 0, -1403053.4782844791 2846213.634980691 0, -1403098.5972614503 2845986.403067261 0, -1403102.6692528867 2845986.22169955 0, -1403103.248347781 2845983.290500964 0, -1403194.7240722105 2845979.1141459174 0, -1403449.0559606147 2846028.010740485 0, -1403504.9632931324 2846028.6813831767 0, -1403799.7788403556 2846032.221859208 0, -1403917.369560205 2846021.144461339 0, -1404023.201279463 2846011.177178477 0, -1404120.1833968922 2845982.644777186 0, -1404347.9635557476 2845922.9921767535 0, -1404384.173923037 2845913.506921877 0)), ((-1397408.2962231054 2850092.3249010867 0, -1397368.4896856248 2850084.068534674 0, -1397446.3713279825 2849691.2643500497 0, -1397505.381414212 2849392.6996998107 0, -1397510.6108350344 2849365.822199518 0, -1397524.2513040218 2849298.457697818 0, -1397541.4491653107 2849211.7165610585 0, -1397541.458220491 2849211.6708892966 0, -1397542.5345600036 2849206.2421379318 0, -1397543.8495907197 2849199.6533351694 0, -1397552.4185829689 2849156.451312542 0, -1397575.9850958055 2849037.5695722825 0, -1397592.0332196734 2848956.627131109 0, -1397592.679842527 2848953.3228822346 0, -1397592.6798425396 2848953.3228821703 0, -1397602.13302944 2848905.6434157547 0, -1397665.8361152133 2848583.3899085936 0, -1397680.0171525239 2848512.827412834 0, -1397680.0171525334 2848512.8274127864 0, -1397929.700960232 2848562.7028559577 0, -1397929.7009632865 2848562.702856566 0, -1397948.4323890347 2848566.4242267665 0, -1397957.4309592475 2848568.2419514772 0, -1397957.4309620752 2848568.241952046 0, -1398077.2551434217 2848592.176531594 0, -1398141.5814011388 2848605.029787731 0, -1398239.0745437716 2848624.510235964 0, -1398247.1236719787 2848626.1050571734 0, -1398282.7133075856 2848633.219462183 0, -1398287.580911698 2848634.192208714 0, -1398327.5059190358 2848642.169873064 0, -1398332.0947335428 2848643.086969197 0, -1398372.692625795 2848651.1939333444 0, -1398377.8822906353 2848652.2453921833 0, -1398377.8822907384 2848652.2453922043 0, -1398377.8822960923 2848652.2453932827 0, -1398474.4887164899 2848671.5479072505 0, -1398871.7176727587 2848750.941513455 0, -1398936.6503813192 2848763.925655422 0, -1398962.2122963727 2848769.0345055317 0, -1399102.7436877913 2848797.11353484 0, -1399111.7925354156 2848798.9398238114 0, -1399113.3217560383 2848799.2471367856 0, -1399268.9442821615 2848830.357851166 0, -1399266.4973957373 2848842.226063975 0, -1399231.7310575226 2849019.0364407757 0, -1399231.7310429218 2849019.036515031 0, -1399221.9107939033 2849069.0883870637 0, -1399215.8337490482 2849099.6392980004 0, -1399215.8337490472 2849099.639298005 0, -1399215.833740717 2849099.639340032 0, -1399191.420180221 2849223.420864117 0, -1399191.322303488 2849223.9171182876 0, -1399113.7035125983 2849617.4718418084 0, -1399036.0835453114 2850011.0212396816 0, -1398958.4665678807 2850404.5660594977 0, -1398945.88544305 2850402.2433631923 0, -1398647.0857153283 2850341.77419907 0, -1398647.0857049285 2850341.774196965 0, -1398647.085704724 2850341.7741969237 0, -1398622.6991095608 2850336.8458357486 0, -1398618.7863314683 2850336.06729265 0, -1398618.7863266538 2850336.0672917007 0, -1398560.9794564047 2850324.409822854 0, -1398193.5005080379 2850250.547556947 0, -1398163.4883337207 2850244.272879605 0, -1397765.99050446 2850164.157983164 0, -1397408.2962231054 2850092.3249010867 0)), ((-1408499.7917902402 2851897.0108265877 0, -1408421.0447701633 2852289.2328041033 0, -1408208.4406804384 2852246.8743553446 0, -1408024.111393916 2852209.763787432 0, -1407803.8467946316 2852165.883525409 0, -1407627.1719187878 2852130.313602257 0, -1407230.2294260436 2852050.8889755737 0, -1407230.2294255465 2852050.888975477 0, -1407206.2683501462 2852046.303831964 0, -1406833.2804088348 2851971.486434671 0, -1406833.280408835 2851971.4864346697 0, -1406911.933817793 2851579.414764962 0, -1406921.6758014641 2851530.0046396935 0, -1406934.686355972 2851465.14776617 0, -1406956.335386052 2851357.2290452607 0, -1406990.586042128 2851187.337697579 0, -1406990.5860421804 2851187.3376973188 0, -1406990.5860422545 2851187.3376969495 0, -1407041.0215364834 2850935.08214724 0, -1407069.2414205894 2850795.256210503 0, -1407069.2414206765 2850795.2562100706 0, -1407069.2414206867 2850795.2562100184 0, -1407073.5684860025 2850772.8424741207 0, -1407147.89795659 2850403.1700436547 0, -1407147.8979565974 2850403.170043656 0, -1407147.897956598 2850403.1700436533 0, -1407506.3690000873 2850474.723267223 0, -1407544.9384991385 2850482.421997814 0, -1407941.9745221676 2850561.6962001207 0, -1408339.0062130108 2850640.9927756977 0, -1408736.0331859435 2850720.3115733187 0, -1408657.41158823 2851111.919579926 0, -1408657.2847018465 2851112.5515910415 0, -1408578.5377025602 2851504.7836576267 0, -1408499.7917902402 2851897.0108265877 0)), ((-1402322.4997742055 2855962.8549554977 0, -1401926.2423490663 2855884.0684591965 0, -1401529.9818892553 2855805.3075370626 0, -1401133.7178690603 2855726.5661011315 0, -1401213.211228292 2855335.412905123 0, -1401292.708138397 2854944.2551045995 0, -1401372.2039204885 2854553.0919847465 0, -1401451.7031004892 2854161.9246495627 0, -1401847.939906079 2854240.6579817794 0, -1402244.174336076 2854319.414166907 0, -1402640.4039476456 2854398.195590499 0, -1403036.6295266182 2854476.9962373967 0, -1402957.1582407928 2854868.1687561497 0, -1402877.6877139623 2855259.339419323 0, -1402798.2189316931 2855650.5022341553 0, -1402718.750697533 2856041.6632575803 0, -1402322.4997742055 2855962.8549554977 0)), ((-1411751.5853603992 2856418.185144432 0, -1411754.7571084467 2856429.033555226 0, -1411767.7582414288 2856473.501728358 0, -1411817.3561956498 2856643.1425894992 0, -1411842.2963358818 2856728.4480426703 0, -1411857.2971659566 2856779.7566173365 0, -1411866.2335776836 2856810.323187832 0, -1411899.5147161097 2856924.1581729716 0, -1411899.2923966853 2856930.5015921816 0, -1411897.9417615307 2856969.061157462 0, -1411894.9402896597 2857054.74085981 0, -1411894.5358408932 2857066.285733073 0, -1411894.0926921885 2857078.934847568 0, -1411893.5171049975 2857095.3595575998 0, -1411891.713688685 2857146.8214332475 0, -1411889.994330014 2857195.9125946364 0, -1411889.699684305 2857204.325522127 0, -1411880.874398725 2857470.4536910965 0, -1411878.0360349421 2857552.343632654 0, -1411875.6033314364 2857624.912060565 0, -1411877.2522324275 2857628.9538111114 0, -1411915.182499596 2857721.932867112 0, -1411933.3960081232 2857766.5799572086 0, -1411978.6628281383 2857877.543262183 0, -1411987.1789034253 2857898.418955808 0, -1411967.8125782465 2857894.7388543542 0, -1411940.9460620254 2857889.3657909026 0, -1411827.0057558136 2857866.5978943333 0, -1411816.2609931997 2857864.4504358424 0, -1411785.6653254726 2857858.335715912 0, -1411778.7458917818 2857856.7582134116 0, -1411778.7458915478 2857856.758213361 0, -1411594.861806844 2857819.9848252423 0, -1411383.7384575654 2857777.7640921324 0, -1411367.0593044949 2857774.617511555 0, -1410990.311091655 2857698.9297966924 0, -1410858.0004306268 2857672.622335774 0, -1410596.879148821 2857620.1174235255 0, -1410621.9852533883 2857491.62132465 0, -1410633.7672996472 2857431.7274165326 0, -1410674.0526222952 2857227.8057096056 0, -1410674.0526223222 2857227.805709468 0, -1410751.224144693 2856835.4917604737 0, -1410757.8768594344 2856800.8060144023 0, -1410820.825048066 2856480.8087421665 0, -1410828.3986047867 2856443.173116284 0, -1410828.3986047988 2856443.1731162234 0, -1410828.3986048105 2856443.173116164 0, -1410842.1263099334 2856372.5611441107 0, -1410905.5745906155 2856050.8465852523 0, -1411295.5805096321 2856130.8219032804 0, -1411432.25054098 2856158.360234526 0, -1411432.2505409804 2856158.360234527 0, -1411432.3744690558 2856158.659060573 0, -1411528.0464481325 2856236.440972607 0, -1411560.3916010382 2856262.7377897943 0, -1411667.3655141646 2856349.7080069594 0, -1411702.6279902614 2856378.379090404 0, -1411740.73912433 2856409.366361044 0, -1411751.5853603992 2856418.185144432 0)), ((-1405261.3863524538 2859814.963898068 0, -1405651.2703595373 2859892.5344997076 0, -1406048.3939748404 2859971.7027081377 0, -1406445.5149132037 2860050.8938099025 0, -1406842.6286486182 2860130.1098150183 0, -1406842.628648618 2860130.1098150196 0, -1406764.8265913033 2860522.0183203532 0, -1406688.7504382622 2860905.23269522 0, -1406687.0248609448 2860913.924854412 0, -1406687.0248609437 2860913.924854418 0, -1406415.590490284 2860859.6128464383 0, -1406290.115452382 2860834.5054980735 0, -1405897.4905057237 2860756.1532146623 0, -1405893.2084571854 2860755.084839173 0, -1405815.6258750965 2861146.7138585607 0, -1406212.4251978938 2861226.269456487 0, -1406609.224541734 2861305.8234384237 0, -1406531.4236872834 2861697.717321509 0, -1406531.4236872534 2861697.717321503 0, -1406531.4236872522 2861697.717321509 0, -1406134.7369737187 2861618.013712855 0, -1405738.045266009 2861538.3353076545 0, -1405341.3495085759 2861458.6764138103 0, -1404944.6466850971 2861379.042249062 0, -1405022.0205961196 2860987.6359433997 0, -1405099.3936611253 2860596.2250118344 0, -1405176.7677404573 2860204.8092027605 0, -1404780.8769870354 2860124.730539985 0, -1404858.3628771487 2859733.3601081683 0, -1404935.3719751574 2859342.672009466 0, -1405331.1001697828 2859423.1280607716 0, -1405254.1434443628 2859813.3853914333 0, -1405261.3863524538 2859814.963898068 0)), ((-1402682.2020684432 2864118.7237778557 0, -1402695.4529211784 2864121.2283095215 0, -1402695.4529211782 2864121.228309523 0, -1402616.8936437613 2864513.0297153555 0, -1402538.3358605783 2864904.823133617 0, -1402499.8153482743 2865096.9325434817 0, -1402459.7765047003 2865296.6141715446 0, -1402419.7474271564 2865496.252592065 0, -1402381.2202299368 2865688.4006322375 0, -1402381.2202299358 2865688.4006322417 0, -1401983.5451695155 2865608.8553613233 0, -1401712.7970666003 2865554.720197429 0, -1401585.8632989998 2865529.3320246567 0, -1401188.179284525 2865449.831439479 0, -1401188.1792117932 2865449.831424936 0, -1401097.3997936426 2865431.6841614405 0, -1401084.8622124526 2865429.1840025107 0, -1400799.226584094 2865372.3078978863 0, -1400790.4886198821 2865370.35311039 0, -1400868.6112097064 2864978.9369326024 0, -1400945.8802026587 2864590.1986702695 0, -1400946.7321918367 2864587.5186793273 0, -1401024.8546978398 2864196.092250667 0, -1401100.9681356936 2863813.8579939683 0, -1401102.9804730942 2863804.661391134 0, -1401161.397036985 2863816.255982978 0, -1401501.1095115985 2863883.7670430006 0, -1401558.569074346 2863895.1879364145 0, -1401899.2323785443 2863962.904431385 0, -1401955.7386749384 2863974.1206539576 0, -1402297.3480475233 2864042.044840975 0, -1402352.9085788366 2864053.0954119097 0, -1402682.2020684432 2864118.7237778557 0)), ((-1411465.037336772 2865648.779537992 0, -1411463.8557415532 2865655.0362547883 0, -1411467.7572204815 2865655.390586278 0, -1411528.471929807 2865656.642773342 0, -1411528.4719302277 2865656.6427733493 0, -1411528.471930238 2865656.6427733507 0, -1411528.4719302412 2865656.6427733507 0, -1411569.6250164183 2865661.9779159166 0, -1411578.782938681 2865663.366841497 0, -1411605.6501287578 2865674.490354063 0, -1411625.477942975 2865682.6947615296 0, -1411631.7469223023 2865685.3064114386 0, -1411632.7949084023 2865685.7423111056 0, -1411635.878725861 2865685.393298609 0, -1411647.15672865 2865684.1156663178 0, -1411652.734374543 2865683.483661498 0, -1411663.069627925 2865682.308265712 0, -1411676.9610435506 2865680.725924123 0, -1411731.4632386134 2865723.2860093727 0, -1411740.6671240507 2865730.519389325 0, -1411822.090020838 2865718.2191672903 0, -1411838.3978266304 2865715.9588456973 0, -1411841.073689812 2865717.1605165387 0, -1411983.169821221 2865779.4717531553 0, -1411983.1698278135 2865779.4717560387 0, -1411999.7797165555 2865786.7246760647 0, -1412158.2912243297 2865835.9466782827 0, -1412170.146075653 2865836.9489773572 0, -1412170.146076222 2865836.9489774047 0, -1412229.6105864234 2865841.7906655665 0, -1412229.6105864223 2865841.790665572 0, -1412229.6105864225 2865841.790665572 0, -1412229.6105863927 2865841.7906657173 0, -1412219.1846687484 2865892.884224412 0, -1412162.0192036116 2866176.968186281 0, -1412082.825008011 2866569.0058447286 0, -1412002.6728112134 2866961.1972452626 0, -1411922.5221962316 2867353.380643108 0, -1411922.5221962258 2867353.3806431065 0, -1411922.522196224 2867353.3806431163 0, -1411583.5471875449 2867284.2856640294 0, -1411524.470183467 2867272.0276043857 0, -1411445.3103906135 2867256.03696549 0, -1411360.55465754 2867238.708295354 0, -1411126.4154879246 2867190.697131833 0, -1411025.867544467 2867170.3460400575 0, -1410917.9101386506 2867148.296874894 0, -1410817.3561835214 2867127.759786799 0, -1410728.3555018317 2867109.3920901567 0, -1410728.3549554553 2867109.3919785875 0, -1410610.287801935 2867085.2829328044 0, -1410330.3074244468 2867028.109796696 0, -1410330.291306805 2867028.1065054135 0, -1410361.2985384562 2866873.7711350676 0, -1410409.33354803 2866634.6905706557 0, -1410420.9139694646 2866577.055654584 0, -1410440.2146718572 2866480.997461124 0, -1410440.2146719096 2866480.9974608603 0, -1410456.6149111663 2866398.174093309 0, -1410463.2236422338 2866365.1634405 0, -1410488.222008319 2866241.2386903674 0, -1410504.0888303516 2866161.32310462 0, -1410519.0021884008 2866088.0397656164 0, -1410519.002188406 2866088.0397655913 0, -1410566.296370515 2865852.6473873486 0, -1410597.9484032183 2865695.10541922 0, -1410644.2002541109 2865464.0360314716 0, -1410644.2099788839 2865464.0379698332 0, -1410644.2113585516 2865464.0310786646 0, -1410684.423421186 2865472.053394944 0, -1411044.5673082075 2865544.3390496573 0, -1411064.664278303 2865548.3758619865 0, -1411303.885356992 2865596.5309854182 0, -1411444.901632407 2865624.715773975 0, -1411454.7045603914 2865626.808822695 0, -1411468.8876433342 2865629.512212369 0, -1411468.8876433324 2865629.512212379 0, -1411465.037336772 2865648.779537992 0)), ((-1405352.3578766033 2869543.935077524 0, -1405359.1363504976 2869545.2042935197 0, -1405436.3132154464 2869560.2322490425 0, -1405502.746418892 2869573.2515146 0, -1405502.7464338238 2869573.2515175208 0, -1405720.6097105232 2869615.720096893 0, -1406118.040747909 2869693.2168943826 0, -1406295.4979188778 2869727.8309028526 0, -1406335.326025477 2869735.548965003 0, -1406368.3830205046 2869742.047260953 0, -1406368.3830230972 2869742.047261461 0, -1406515.4696160685 2869770.7362509747 0, -1406515.4696160683 2869770.736250976 0, -1406515.3518045028 2869771.324431194 0, -1406436.8880400027 2870163.058756294 0, -1406358.3075719213 2870555.3763669888 0, -1406349.6235684261 2870598.7326819636 0, -1406349.6235644566 2870598.7327020443 0, -1406348.2495920586 2870605.7389051924 0, -1406343.9503185805 2870627.2036582665 0, -1406334.9120333896 2870672.1828832966 0, -1406279.7301098744 2870947.689329546 0, -1406259.8342604002 2871047.0207821187 0, -1406256.6776818188 2871062.9237264954 0, -1406248.9494264596 2871101.3638142054 0, -1406201.1516861857 2871339.9969154075 0, -1405935.8783990357 2871288.0464658416 0, -1405919.2268095443 2871284.7765399343 0, -1405859.9066085038 2871273.1582050133 0, -1405856.2419319113 2871272.450294864 0, -1405856.241927392 2871272.4502939982 0, -1405803.751681128 2871262.170407299 0, -1405658.300430607 2871233.6943604634 0, -1405644.932170153 2871231.0641286485 0, -1405623.858496985 2871226.937981929 0, -1405605.0992181995 2871223.278679066 0, -1405605.0992040872 2871223.278676319 0, -1405406.3471053601 2871184.366241646 0, -1405435.624495818 2871038.2277601827 0, -1405437.0592010934 2871031.0664098286 0, -1405441.9988417523 2871006.4998400114 0, -1405484.3701475295 2870794.999082076 0, -1405484.9057895474 2870792.2393457848 0, -1405479.7815442246 2870791.226744264 0, -1405424.8324013767 2870780.4771098006 0, -1405420.8968640964 2870779.7077110303 0, -1405370.7645056879 2870769.9052323746 0, -1405367.6517246566 2870769.2986274436 0, -1405283.9653302229 2870752.933274581 0, -1405255.9106829148 2870747.465511902 0, -1405255.9106593088 2870747.46550731 0, -1405205.8767456764 2870737.7331411466 0, -1405087.490981406 2870714.534637766 0, -1405066.3558166963 2870710.5732503003 0, -1404937.6800193107 2870685.241462984 0, -1404912.420841931 2870680.2812086833 0, -1404873.690080004 2870672.728276086 0, -1404690.0778117212 2870636.8252614536 0, -1404690.077166699 2870636.8251353293 0, -1404690.0771666993 2870636.825135328 0, -1404708.0471434693 2870547.146432178 0, -1404710.958022651 2870532.710837276 0, -1404753.5632293806 2870320.0914300634 0, -1404767.9136741732 2870248.445385562 0, -1404768.6279536458 2870244.8196088024 0, -1404768.6279536616 2870244.819608721 0, -1404775.7641339956 2870209.20661129 0, -1404775.7641365211 2870209.206598999 0, -1404776.9359453998 2870203.4499911657 0, -1404809.6746020482 2870040.0693464084 0, -1404828.469240713 2869946.2757398025 0, -1404829.4227403163 2869941.5171959335 0, -1404831.863324543 2869929.2458460294 0, -1404847.1798434148 2869852.8091909704 0, -1404851.4089969185 2869831.7039236957 0, -1404851.4422845743 2869831.5378041933 0, -1404852.1575244702 2869828.0605850974 0, -1404853.231110614 2869822.7023808896 0, -1404856.9175901003 2869804.3054733314 0, -1404883.9239550708 2869669.5310635734 0, -1404889.6944281512 2869640.6415555426 0, -1404889.6944321946 2869640.6415352616 0, -1404925.732661221 2869460.793662609 0, -1405323.1722710785 2869538.245600288 0, -1405352.3578766033 2869543.935077524 0)), ((-1403270.9110435373 2873607.989720598 0, -1403195.57265247 2873987.095011088 0, -1402798.6169425067 2873907.8261163756 0, -1402874.1480264233 2873528.383814522 0, -1402952.0604383987 2873136.965264704 0, -1403348.7412445976 2873216.3452473097 0, -1403270.9110435373 2873607.989720598 0)), ((-1400722.020211627 2873987.416916897 0, -1400659.8349719865 2874300.9579526847 0, -1400582.1008802357 2874692.897713141 0, -1400504.368199048 2875084.8295678613 0, -1400504.3681990472 2875084.8295678655 0, -1400306.06796822 2875046.0779310446 0, -1400108.2805656404 2875006.994913384 0, -1399712.1886875827 2874929.1824742686 0, -1399316.0923516774 2874851.392322538 0, -1398919.9918312414 2874773.6246947986 0, -1398997.4825770769 2874381.3695183387 0, -1399074.9721307347 2873989.109292349 0, -1399152.464837142 2873596.8441945347 0, -1399229.9583728071 2873204.574122286 0, -1399626.3009079173 2873282.6651033484 0, -1400022.6398035127 2873360.7752654627 0, -1400418.9757098868 2873438.911310901 0, -1400341.2951306698 2873830.9661018522 0, -1400408.590619487 2873844.220564607 0, -1400737.569628418 2873909.015992905 0, -1400737.5696284168 2873909.0159929106 0, -1400737.5696284187 2873909.015992911 0, -1400722.020211627 2873987.416916897 0)), ((-1409103.6964492481 2875025.2421185113 0, -1409141.8900567754 2875032.891256656 0, -1409213.6801065572 2875047.2731291484 0, -1409213.6801090706 2875047.273129647 0, -1409229.77988655 2875050.449152512 0, -1409285.8021089113 2875061.721309533 0, -1409285.8021396676 2875061.7213157113 0, -1409535.654514666 2875111.773087116 0, -1409929.4117891053 2875190.679700427 0, -1409971.24784557 2875199.065926775 0, -1409971.2478463105 2875199.065926921 0, -1409978.7519803427 2875200.531137577 0, -1410108.979261336 2875226.637376353 0, -1410140.157719893 2875232.924347864 0, -1410323.172103583 2875269.6090371227 0, -1410323.1721035815 2875269.609037131 0, -1410323.1721035817 2875269.609037131 0, -1410280.0390395173 2875485.7118710545 0, -1410275.657886319 2875507.7470515314 0, -1410272.7716184133 2875522.122472482 0, -1410244.8465344294 2875662.031449576 0, -1410244.846486525 2875662.031689817 0, -1410238.80266182 2875692.360027673 0, -1410188.7019879804 2875943.3155002077 0, -1410185.8364133637 2875957.6702931076 0, -1410166.5198291473 2876054.448420859 0, -1410154.9493124203 2876112.3908099523 0, -1410129.6492050847 2876239.1153764776 0, -1410097.0531707695 2876404.0092286854 0, -1410096.267817752 2876406.490527884 0, -1410095.9545911942 2876406.9131187014 0, -1410092.6124654415 2876411.4155137967 0, -1410071.9405331241 2876439.594348282 0, -1410067.334844834 2876445.872557595 0, -1410044.8896179674 2876476.467052874 0, -1410017.2528691767 2876514.1379344515 0, -1410017.2528691764 2876514.1379344515 0, -1410017.2513635792 2876514.139986689 0, -1409975.5495828802 2876541.3013308863 0, -1409950.1803787204 2876557.8212493835 0, -1409908.6595203627 2876584.8949637697 0, -1409866.487935356 2876612.392758426 0, -1409766.4990217146 2876677.5969618005 0, -1409766.4997185215 2876677.6499651307 0, -1409766.2500051307 2876677.812799691 0, -1409766.6451122717 2876704.2036529 0, -1409767.1408562034 2876737.3104113834 0, -1409767.507660834 2876761.8052125834 0, -1409769.9336998635 2876795.1547505893 0, -1409764.5592822868 2876794.095048755 0, -1409627.5944055112 2876766.6532114935 0, -1409510.6739233304 2876743.2241767757 0, -1409446.8540509548 2876730.4106893907 0, -1409310.6548475022 2876703.0646280306 0, -1409263.1621494931 2876693.52887364 0, -1409260.287299188 2876692.9515570784 0, -1409230.218035185 2876686.8663708684 0, -1408832.1384908531 2876608.0227922006 0, -1408774.6639410295 2876596.8008374856 0, -1408728.6500602255 2876587.657983948 0, -1408514.9915482828 2876545.2276930353 0, -1408514.9915142735 2876545.2276862813 0, -1408455.7443594562 2876533.474764181 0, -1408452.775912659 2876532.908685063 0, -1408434.0567597842 2876529.2021547086 0, -1408446.2223965924 2876468.189760085 0, -1408486.3784147138 2876266.7236018917 0, -1408489.3887333323 2876251.6218461953 0, -1408512.5581591323</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>subsurface, Surface</t>
+          <t>Surface, subsurface</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Strategic Investment and Improvement Fund, Sovereign Lands, ND State University, Common Schools, ND Industrial School, School of Mines, Ellendale, School for the Blind, ND School of Science, University of ND, ND State Treasurer, Mayville, Valley City</t>
+          <t>Sovereign Lands, Strategic Investment and Improvement Fund, ND State University, ND Industrial School, Common Schools, School of Mines, Ellendale, School for the Blind, ND School of Science, University of ND, ND State Treasurer, Mayville, Valley City</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1857,12 +1857,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Perm Common Schls, Agriculture &amp; Mechanical Cllge</t>
+          <t>Agriculture &amp; Mechanical Cllge, Perm Common Schls</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Subsurface, Surface</t>
+          <t>Surface, Subsurface</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1890,7 +1890,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-108341.97191857763 1404561.9027005068 0, -107945.60258208308 1404553.8840211239 0, -107549.22354405018 1404545.8949796 0, -107152.85314104144 1404537.9132319037 0, -107157.93271856382 1404133.5156715682 0, -107163.01242622903 1403729.1193964 0, -107555.81572348381 1403738.3439330538 0, -107948.62764797636 1403747.5754633446 0, -108341.42977029631 1403756.8361264358 0, -108734.24041462474 1403766.103880993 0, -108736.29553945966 1404168.0156940103 0, -108738.3499890904 1404569.9285760538 0, -108341.97191857763 1404561.9027005068 0)), ((-107810.32276756843 1413484.0564166575 0, -107807.276609632 1413887.645320616 0, -107804.23052666767 1414291.2242681908 0, -108200.34303888392 1414297.949900839 0, -108203.235986383 1413895.2087524624 0, -108599.18576566063 1413902.8015844526 0, -108596.46418754176 1414304.6827835625 0, -108593.73352558199 1414706.5651397514 0, -108591.01152681139 1415108.448703035 0, -108194.57458505986 1415103.413553814 0, -107798.13741943479 1415098.3967775719 0, -107401.69992630578 1415093.3985728486 0, -107005.26231159158 1415088.4187440102 0, -107008.62435393337 1414683.1284872352 0, -107011.99514438768 1414277.8394543822 0, -107015.35684008521 1413872.5514915457 0, -107018.72738286007 1413467.2647586477 0, -107414.5252946043 1413475.6513456143 0, -107810.32276756843 1413484.0564166575 0)), ((-108096.22211288824 1423140.2380230955 0, -108495.34425831848 1423146.1690621856 0, -108493.28644287433 1423549.7980220078 0, -108491.22850801035 1423953.416885929 0, -108489.17006305745 1424357.04805589 0, -108487.11149888618 1424760.6691269618 0, -108086.35764156858 1424753.877134496 0, -107685.60349830733 1424747.0927805582 0, -107284.84877595655 1424740.338572541 0, -106884.09387000152 1424733.5920060303 0, -106887.78414715634 1424330.831602444 0, -106891.4833258544 1423928.0612732428 0, -106895.17327572586 1423525.3031693732 0, -106898.87222916893 1423122.5350450552 0, -107297.98619730644 1423128.42096728 0, -107697.10880217039 1423134.3146083243 0, -108096.22211288824 1423140.2380230955 0)), ((-108329.76500969507 1432921.0976291755 0, -108325.27088097774 1433327.7458955857 0, -108320.7857506205 1433734.3842206327 0, -108317.31958403609 1434048.436084898 0, -108271.24235125513 1434008.946531518 0, -108140.33972360729 1433896.7879785388 0, -108092.76983325138 1433844.2438453573 0, -108065.48119479089 1433730.462561917 0, -108055.69148151703 1433689.643884121 0, -108003.92051171514 1433584.5010516958 0, -107998.86664325111 1433574.1339411687 0, -107993.92607475584 1433568.9197046687 0, -107988.89468311374 1433563.8163044022 0, -107969.21460241945 1433543.520384907 0, -107949.53442703391 1433523.2245136697 0, -107944.32988366806 1433517.6709915493 0, -107939.12391081538 1433512.2294422896 0, -107925.77420400832 1433498.5532462653 0, -107927.89220709668 1433322.8139756143 0, -107728.37878322226 1433320.346411263 0, -107603.48193967047 1433237.0740361225 0, -107553.31424403274 1433216.505042089 0, -107531.93540055724 1433208.5855277285 0, -107424.983576923 1433168.9666164385 0, -107248.79651131877 1433091.6518696344 0, -107137.22211275306 1433022.0320571044 0, -107129.92053730217 1433017.4832659357 0, -106995.79370207501 1432975.0801109788 0, -106829.34117979447 1432917.749422436 0, -106802.76133231136 1432906.766451299 0, -107138.79650581299 1432909.89964916 0, -107535.78910702739 1432913.6137655776 0, -107932.7726607902 1432917.346406936 0, -108329.76500969507 1432921.0976291755 0)), ((-103888.75891972643 1408513.2603350764 0, -103883.44151454806 1408920.2437055437 0, -103878.12412180073 1409327.2283520366 0, -103872.80674461676 1409734.2141721996 0, -103867.48938303896 1410141.2011645401 0, -103470.87841548683 1410131.6835878415 0, -103074.26682727227 1410122.1844059231 0, -102677.65451786568 1410112.703716494 0, -102281.04148889238 1410103.2415195168 0, -102287.94548795457 1409699.688189708 0, -102294.84951560387 1409296.1360108957 0, -102301.75386898944 1408892.5849938514 0, -102308.65834997402 1408489.035133807 0, -102703.68400398006 1408495.0639910852 0, -103098.70925197075 1408501.1111416013 0, -103493.73429045972 1408507.1765916406 0, -103888.75891972643 1408513.2603350764 0)), ((-99053.57924581278 1413307.8649394184 0, -99046.47555863338 1413712.2677027765 0, -98649.22720056682 1413713.3225742935 0, -98655.62813787466 1413308.385398984 0, -99053.57924581278 1413307.8649394184 0)), ((-99032.27774895268 1414521.0766419354 0, -99025.18371932303 1414925.4830196623 0, -98630.01601487662 1414928.1636144198 0, -98636.42559804795 1414523.211772694 0, -99032.27774895268 1414521.0766419354 0)), ((-102573.73008625153 1418201.6494684827 0, -102573.84227282721 1418604.2255107036 0, -102177.37979169976 1418600.9690474125 0, -102177.0852478158 1418198.5925258938 0, -102573.73008625153 1418201.6494684827 0)), ((-102574.06497598997 1419409.4034681309 0, -102573.95381921457 1419006.8139781673 0, -102573.84227282721 1418604.2255107036 0, -102970.3045065936 1418607.5117338966 0, -103366.76678810467 1418610.80511 0, -103763.21994417445 1418614.1169626303 0, -103762.7662842679 1419017.326135117 0, -103762.3031171501 1419420.5363477732 0, -103366.22388905576 1419416.803232996 0, -103365.95161240076 1419819.8151281285 0, -102970.06370104977 1419815.8898234847 0, -102574.16661798784 1419811.9940968393 0, -102574.06497598997 1419409.4034681309 0), (-103366.49553182158 1419013.8036599872 0, -102970.22477769863 1419010.2995425325 0, -102970.14441021612 1419413.0997752808 0, -103366.22388905576 1419416.803232996 0, -103366.49553182158 1419013.8036599872 0)), ((-98979.3313871927 1423862.5104601963 0, -98974.89317401552 1424272.516703981 0, -98970.46376188945 1424682.5243592479 0, -98569.27515605523 1424683.8686252483 0, -98168.09580278337 1424685.231905905 0, -97766.90786257098 1424686.6140450826 0, -97365.72927417218 1424688.0153025105 0, -97370.03781566468 1424281.8133445985 0, -97374.35516795557 1423875.6126806713 0, -97378.66359198703 1423469.4130585787 0, -97382.98092889391 1423063.2146356527 0, -97784.27985432954 1423058.0077998515 0, -98185.58844868181 1423052.8199848952 0, -98586.8887699464 1423047.6510321011 0, -98988.19885279374 1423042.501204599 0, -98983.7606684282 1423452.505174026 0, -98979.3313871927 1423862.5104601963 0)), ((-102423.47317896172 1427981.4294510542 0, -102481.7601933639 1427982.3952424342 0, -102490.00610556726 1427982.5314548574 0, -102821.3466392487 1427988.0221814779 0, -102897.12866658544 1427989.2726389929 0, -103215.09609969346 1427994.561316661 0, -103286.45030234217 1427995.7391205232 0, -103612.9688756502 1428001.1798864868 0, -103607.68049878148 1428407.3574287463 0, -103602.40120548545 1428813.5250465341 0, -103597.1127701952 1429219.7047838513 0, -103199.30242564008 1429212.6391023616 0, -102802.52907081215 1429205.6157317858 0, -102404.71774511709 1429198.5984923455 0, -102398.46926949982 1429603.8161399195 0, -102000.6803171128 1429596.4931193087 0, -102006.89713429322 1429191.5884869024 0, -102013.12298757605 1428786.6852258453 0, -102410.95746916845 1428793.3706528917 0, -102808.79138893947 1428800.0860042188 0, -103204.56787206174 1428806.7837567737 0, -103209.824464444 1428400.9182236337 0, -102815.06285254596 1428394.5573525112 0, -102417.20618624233 1428388.1552930959 0, -102423.47317896172 1427981.4294510542 0)), ((-93521.54118873226 1409207.0966037768 0, -93919.80153974675 1409210.8280514209 0, -94318.05285296372 1409214.5668109718 0, -94313.57850111574 1409619.022735214 0, -94309.1042760259 1410023.4687219525 0, -93910.7370159215 1410018.2172915097 0, -93512.36962967928 1410012.9733532104 0, -93516.95980339825 1409610.040040049 0, -93521.54118873226 1409207.0966037768 0)), ((-97844.70466653934 1414527.5369802641 0, -97448.84480714846 1414529.7272351652 0, -97453.16437133847 1414123.1623551168 0, -97849.71790442427 1414121.5175330746 0, -97844.70466653934 1414527.5369802641 0)), ((-93847.6463245715 1418129.8560985199 0, -93844.27361685838 1418537.4173234731 0, -93444.30928149664 1418534.417183636 0, -93448.604266527 1418126.7652493648 0, -93847.6463245715 1418129.8560985199 0)), ((-94239.3367776905 1419355.3697970596 0, -94236.88589608682 1419762.8327458396 0, -93834.15491137239 1419760.1079739258 0, -93837.52790865419 1419352.5433131184 0, -94239.3367776905 1419355.3697970596 0)), ((-94059.83675285004 1428297.134849285 0, -94047.78830087288 1428707.0701078374 0, -93660.84167730855 1428702.597829106 0, -93273.88581301915 1428698.1541748669 0, -93285.8947014553 1428288.43052082 0, -93297.86818946092 1427879.5587093967 0, -93308.20619673278 1427879.6605550156 0, -93356.52519114394 1427880.1335441836 0, -93684.87710900807 1427883.3765095805 0, -93749.60825373865 1427884.009547773 0, -94071.88599501901 1427887.200809396 0, -94059.83675285004 1428297.134849285 0)), ((-98755.17724356256 1434045.3479738326 0, -98743.7399073762 1434443.3751392881 0, -98345.39509216356 1434443.4710080456 0, -97947.05941962759 1434443.585649036 0, -97548.71495209764 1434443.71890229 0, -97150.37972951063 1434443.870930553 0, -97160.45694265144 1434039.4213868643 0, -97170.53481982657 1433634.9617107953 0, -97180.61306974819 1433230.5143105339 0, -97190.69188155713 1432826.0568786473 0, -97590.39717530237 1432832.3383533764 0, -97990.10211981475 1432838.6275274365 0, -98389.80662644192 1432844.9466120554 0, -98789.51088271826 1432851.2732983914 0, -98778.06278070486 1433249.2970535443 0, -98766.62414708053 1433647.322030613 0, -98755.17724356256 1434045.3479738326 0)), ((-88836.91899951367 1403669.0709653178 0, -88831.6854981431 1403690.8822506166 0, -88824.02498805917 1403705.379662453 0, -88814.77179651076 1403712.5609192643 0, -88799.64410296819 1403723.8570922113 0, -88792.93709899105 1403726.9110280115 0, -88778.6780343103 1403734.0514531864 0, -88759.42225685729 1403741.1400268704 0, -88724.21905985722 1403756.3927755377 0, -88713.27392618128 1403766.6800876986 0, -88696.47960766022 1403776.917967307 0, -88690.498842239 1403790.391860605 0, -88682.8044439963 1403809.0427500082 0, -88682.67456277554 1403821.5361271796 0, -88682.50142181 1403838.1938986422 0, -88678.95863057926 1403857.9404021914 0, -88672.10046281546 1403875.5587691814 0, -88668.25123725247 1403883.3560058752 0, -88664.4294907722 1403891.0975692882 0, -88655.91346871144 1403907.66872193 0, -88639.04209755229 1403926.2245789361 0, -88612.96296971402 1403946.7785633283 0, -88593.5997072146 1403964.2673830134 0, -88561.72403452882 1403980.5965202968 0, -88521.41752418655 1404006.2094880154 0, -88502.18415427324 1404011.2051240979 0, -88482.16155511585 1404010.997796026 0, -88470.5444329498 1404005.6825950437 0, -88466.17146120236 1403996.5349670348 0, -88466.85415051879 1403881.380469961 0, -88469.30016250984 1403472.46306391 0, -88865.58899476523 1403476.575173842 0, -88865.25748956957 1403534.2419241183 0, -88863.3053891457 1403538.1850077892 0, -88844.77494207515 1403555.693108859 0, -88839.54139602723 1403577.493074574 0, -88836.77827381823 1403602.453731996 0, -88838.24106564456 1403622.24094297 0, -88840.47291102435 1403648.2947113698 0, -88836.91899951367 1403669.0709653178 0)), ((-88713.1954354032 1403883.8001671943 0, -88714.03828920037 1403869.1869952437 0, -88714.4245299299 1403832.042810073 0, -88724.1084906146 1403811.8786831452 0, -88759.54698553265 1403786.9214987422 0, -88820.70516902128 1403760.5412220194 0, -88852.12450506247 1403732.1614000539 0, -88864.2201025576 1403713.0862248677 0, -88863.21610825672 1403885.2693890778 0, -88860.84281636066 1404293.976112206 0, -88858.46951175705 1404702.6727409104 0, -88856.09594561267 1405111.370673376 0, -88459.51528958166 1405108.128740152 0, -88062.9435608325 1405104.8940869458 0, -88065.46294442056 1404695.7610628824 0, -88067.98216166053 1404286.6293473286 0, -88070.28832533426 1403912.024937353 0, -88073.74349464526 1403898.0207511957 0, -88090.17249826937 1403879.6160516897 0, -88091.95069010492 1403877.708661751 0, -88112.0634291369 1403856.1959834045 0, -88124.42874220115 1403837.7494265507 0, -88144.82544856593 1403827.8386157192 0, -88169.09432181073 1403836.530750426 0, -88195.941216318 1403857.0612416037 0, -88229.69155183861 1403864.1720564931 0, -88255.40202713582 1403864.4375805848 0, -88281.17357334016 1403857.941405816 0, -88312.46837830478 1403841.3813041546 0, -88345.0914336815 1403826.5256958173 0, -88361.24133475311 1403835.134392439 0, -88377.14638989799 1403867.3753194625 0, -88380.99358967648 1403880.5367588485 0, -88391.52182953307 1403916.4950833682 0, -88407.31269455753 1403958.8671415611 0, -88432.28792920607 1404030.0408320809 0, -88449.66039120684 1404050.48533603 0, -88465.8220318481 1404055.3213871433 0, -88498.33617965213 1404054.370519267 0, -88537.68758383242 1404042.9552367812 0, -88574.44410220372 1404021.3920682364 0, -88615.32580272321 1403993.109561932 0, -88653.61276931937 1403954.6678664968 0, -88687.81016374502 1403919.5651586987 0, -88712.3852857559 1403897.8649869259 0, -88713.1954354032 1403883.8001671943 0)), ((-93521.54118873226 1409207.0966037768 0, -93123.2895503766 1409203.3951329854 0, -92725.03789765219 1409199.701054333 0, -92729.7353918301 1408798.2826408655 0, -92734.44204175068 1408396.854257546 0, -93132.57732298844 1408399.0357749355 0, -93530.72171557856 1408401.2247658973 0, -93526.13143536559 1408804.165707803 0, -93521.54118873226 1409207.0966037768 0)), ((-92360.08833965978 1413653.2308525657 0, -91956.70286996344 1413652.113093171 0, -91958.10720580119 1413247.2095826631 0, -92361.26571403957 1413247.8767948232 0, -92693.94829534723 1413248.4361525474 0, -92689.5338731609 1413654.158183343 0, -92685.1193274322 1414059.8813657921 0, -92358.91053331329 1414058.5859613924 0, -92360.08833965978 1413653.2308525657 0)), ((-89618.15005361554 1413637.1595225923 0, -89613.52784421502 1414045.0083209148 0, -89215.86687084337 1414038.279547381 0, -88818.2052965973 1414031.5805498827 0, -88821.2704054541 1413623.2787557838 0, -89219.71050648029 1413630.2098519409 0, -89618.15005361554 1413637.1595225923 0)), ((-88791.4343888765 1418513.9579196223 0, -89187.81338683216 1418517.0269236846 0, -89584.18331541786 1418520.1144013363 0, -89584.67786338253 1418928.4787904194 0, -89187.21429888748 1418924.7415439982 0, -88789.75073105896 1418921.011648495 0, -88791.4343888765 1418513.9579196223 0)), ((-89161.24456082463 1423385.2661774433 0, -89560.97516376973 1423388.4899375397 0, -89559.41628051212 1423795.9730736206 0, -89159.80662224842 1423792.437049666 0, -89161.24456082463 1423385.2661774433 0)), ((-87965.01365035953 1423781.9610804282 0, -87964.08395915708 1423375.740048612 0, -88362.80353756399 1423378.8857737677 0, -88362.60089704483 1423785.4310671838 0, -88362.40686239593 1424191.9664608913 0, -88362.20345482265 1424598.5027982828 0, -87966.86249210453 1424594.417442006 0, -87965.933821876 1424188.1941615948 0, -87965.01365035953 1423781.9610804282 0)), ((-89557.85700147413 1424203.4685414871 0, -89556.29751406678 1424610.9540325832 0, -89156.92091686802 1424606.7708883083 0, -89158.35945816005 1424199.5977638592 0, -89557.85700147413 1424203.4685414871 0)), ((-93273.88581301915 1428698.1541748669 0, -93261.88663257027 1429107.879123261 0, -93249.87912469619 1429517.6051012098 0, -92862.97165813525 1429512.9676199823 0, -92476.06396225932 1429508.336527517 0, -92478.14842891505 1429098.7149461762 0, -92480.23269712989 1428689.0832759927 0, -92867.17994476062 1428693.50184052 0, -93273.88581301915 1428698.1541748669 0)), ((-89279.39345416121 1433127.8646544064 0, -89266.6252196684 1433533.1072736336 0, -89253.84886037794 1433938.3508895955 0, -89241.08221584412 1434343.5956572872 0, -88846.52636626638 1434341.1880825984 0, -88451.97943371661 1434338.7876654088 0, -88057.42348487477 1434336.416762109 0, -87662.8765551925 1434334.0530191802 0, -87668.46902625533 1433923.6148717504 0, -87674.07080429922 1433513.1668060871 0, -87679.6635646027 1433102.730965972 0, -87685.26553587045 1432692.2851067442 0, -88086.98823304276 1432699.8410496197 0, -88488.71948750077 1432707.416183666 0, -88890.44126604153 1432715.01014463 0, -89292.17140046127 1432722.6232907092 0, -89279.39345416121 1433127.8646544064 0), (-88079.60118010656 1433108.9805231334 0, -88072.20536416599 1433518.1211127618 0, -88470.34844821837 1433523.1052969876 0, -88479.52927416314 1433115.2601053773 0, -88079.60118010656 1433108.9805231334 0)), ((-84065.84498233233 1408324.2226089637 0, -84463.97843334367 1408326.4479603695 0, -84862.1210284208 1408328.6807842955 0, -84859.44172793816 1408734.8334773607 0, -84461.74653644364 1408732.8066040988 0, -84064.05118110597 1408730.8095224833 0, -84065.84498233233 1408324.2226089637 0)), ((-84811.54834895539 1418080.132914788 0, -84807.50753888277 1418485.8740994087 0, -84803.46677356583 1418891.6164255978 0, -84799.42595400776 1419297.3598887625 0, -84795.38508025554 1419703.1044874315 0, -84399.81260786249 1419701.3113486073 0, -84004.24020863081 1419699.5366552393 0, -83608.66778511007 1419697.7804040853 0, -83213.09534199277 1419696.0424941326 0, -83215.3465778014 1419291.5676956056 0, -83217.59764840879 1418887.0941311917 0, -83219.84845779113 1418482.621698406 0, -83222.09910492194 1418078.150401817 0, -83619.46118999693 1418078.618202269 0, -84016.8234597905 1418079.1045555063 0, -84414.18591268072 1418079.6094616929 0, -84811.54834895539 1418080.132914788 0), (-83614.06473544164 1418888.2026350643 0, -83611.36190419116 1419292.9852613672 0, -84007.38608612366 1419294.4325526417 0, -84010.53205221213 1418889.3182832596 0, -83614.06473544164 1418888.2026350643 0)), ((-82426.75742351369 1419690.9886109696 0, -82033.58386966141 1419688.488938 0, -81640.41911741834 1419686.0074791266 0, -81642.63205846843 1419277.7028963615 0, -81644.8449579429 1418869.3883637388 0, -81647.0575308344 1418461.086185313 0, -82040.25133292488 1418466.4343270094 0, -82433.45367863952 1418471.811997542 0, -82431.22163584364 1418878.210559317 0, -82428.989666873 1419284.598965215 0, -82426.75742351369 1419690.9886109696 0)), ((-83737.44065891691 1427785.297279914 0, -83733.77440182888 1428192.2788242535 0, -83335.18560179621 1428189.1150599332 0, -83338.84481935522 1427780.9015110661 0, -83582.80791439058 1427783.590553651 0, -83618.43907365491 1427783.9848509997 0, -83737.44065891691 1427785.297279914 0)), ((-84542.76302844692 1427794.2477651588 0, -84537.04341170983 1428198.7118047865 0, -84136.42428546058 1428195.4902023987 0, -84142.14602517396 1427789.7831282464 0, -84328.54614853674 1427791.8604490892 0, -84354.62052558582 1427792.1501634372 0, -84542.76302844692 1427794.2477651588 0)), ((-83331.55346692208 1428594.5639834472 0, -83730.11738763128 1428597.402833054 0, -83726.4692938403 1429002.539127675 0, -83327.91235049146 1429000.0140313976 0, -83331.55346692208 1428594.5639834472 0)), ((-84531.32395423243 1428603.1768408744 0, -84525.60464986345 1429007.6430736787 0, -84126.03693441047 1429005.0817423589 0, -84130.72068482457 1428600.2803774886 0, -84531.32395423243 1428603.1768408744 0)), ((-84126.03693441047 1429005.0817423589 0, -84121.34431743283 1429409.8840248408 0, -83722.81216782187 1429407.6653351416 0, -83726.4692938403 1429002.539127675 0, -84126.03693441047 1429005.0817423589 0)))</t>
+          <t>MULTIPOLYGON Z (((-108341.97191857763 1404561.9027005068 0, -107945.60258208308 1404553.8840211239 0, -107549.22354405018 1404545.8949796 0, -107152.85314104144 1404537.9132319037 0, -107157.93271856382 1404133.5156715682 0, -107163.01242622903 1403729.1193964 0, -107555.81572348381 1403738.3439330538 0, -107948.62764797636 1403747.5754633446 0, -108341.42977029631 1403756.8361264358 0, -108734.24041462474 1403766.103880993 0, -108736.29553945966 1404168.0156940103 0, -108738.3499890904 1404569.9285760538 0, -108341.97191857763 1404561.9027005068 0)), ((-107810.32276756843 1413484.0564166575 0, -107807.276609632 1413887.645320616 0, -107804.23052666767 1414291.2242681908 0, -108200.34303888392 1414297.949900839 0, -108203.235986383 1413895.2087524624 0, -108599.18576566063 1413902.8015844526 0, -108596.46418754176 1414304.6827835625 0, -108593.73352558199 1414706.5651397514 0, -108591.01152681139 1415108.448703035 0, -108194.57458505986 1415103.413553814 0, -107798.13741943479 1415098.3967775719 0, -107401.69992630578 1415093.3985728486 0, -107005.26231159158 1415088.4187440102 0, -107008.62435393337 1414683.1284872352 0, -107011.99514438768 1414277.8394543822 0, -107015.35684008521 1413872.5514915457 0, -107018.72738286007 1413467.2647586477 0, -107414.5252946043 1413475.6513456143 0, -107810.32276756843 1413484.0564166575 0)), ((-108096.22211288824 1423140.2380230955 0, -108495.34425831848 1423146.1690621856 0, -108493.28644287433 1423549.7980220078 0, -108491.22850801035 1423953.416885929 0, -108489.17006305745 1424357.04805589 0, -108487.11149888618 1424760.6691269618 0, -108086.35764156858 1424753.877134496 0, -107685.60349830733 1424747.0927805582 0, -107284.84877595655 1424740.338572541 0, -106884.09387000152 1424733.5920060303 0, -106887.78414715634 1424330.831602444 0, -106891.4833258544 1423928.0612732428 0, -106895.17327572586 1423525.3031693732 0, -106898.87222916893 1423122.5350450552 0, -107297.98619730644 1423128.42096728 0, -107697.10880217039 1423134.3146083243 0, -108096.22211288824 1423140.2380230955 0)), ((-107531.93540055724 1433208.5855277285 0, -107424.983576923 1433168.9666164385 0, -107248.79651131877 1433091.6518696344 0, -107137.22211275306 1433022.0320571044 0, -107129.92053730217 1433017.4832659357 0, -106995.79370207501 1432975.0801109788 0, -106829.34117979447 1432917.749422436 0, -106802.76133231136 1432906.766451299 0, -107138.79650581299 1432909.89964916 0, -107535.78910702739 1432913.6137655776 0, -107932.7726607902 1432917.346406936 0, -108329.76500969507 1432921.0976291755 0, -108325.27088097774 1433327.7458955857 0, -108320.7857506205 1433734.3842206327 0, -108317.31958403609 1434048.436084898 0, -108271.24235125513 1434008.946531518 0, -108140.33972360729 1433896.7879785388 0, -108092.76983325138 1433844.2438453573 0, -108065.48119479089 1433730.462561917 0, -108055.69148151703 1433689.643884121 0, -108003.92051171514 1433584.5010516958 0, -107998.86664325111 1433574.1339411687 0, -107993.92607475584 1433568.9197046687 0, -107988.89468311374 1433563.8163044022 0, -107969.21460241945 1433543.520384907 0, -107949.53442703391 1433523.2245136697 0, -107944.32988366806 1433517.6709915493 0, -107939.12391081538 1433512.2294422896 0, -107925.77420400832 1433498.5532462653 0, -107927.89220709668 1433322.8139756143 0, -107728.37878322226 1433320.346411263 0, -107603.48193967047 1433237.0740361225 0, -107553.31424403274 1433216.505042089 0, -107531.93540055724 1433208.5855277285 0)), ((-103872.80674461676 1409734.2141721996 0, -103867.48938303896 1410141.2011645401 0, -103470.87841548683 1410131.6835878415 0, -103074.26682727227 1410122.1844059231 0, -102677.65451786568 1410112.703716494 0, -102281.04148889238 1410103.2415195168 0, -102287.94548795457 1409699.688189708 0, -102294.84951560387 1409296.1360108957 0, -102301.75386898944 1408892.5849938514 0, -102308.65834997402 1408489.035133807 0, -102703.68400398006 1408495.0639910852 0, -103098.70925197075 1408501.1111416013 0, -103493.73429045972 1408507.1765916406 0, -103888.75891972643 1408513.2603350764 0, -103883.44151454806 1408920.2437055437 0, -103878.12412180073 1409327.2283520366 0, -103872.80674461676 1409734.2141721996 0)), ((-99053.57924581278 1413307.8649394184 0, -99046.47555863338 1413712.2677027765 0, -98649.22720056682 1413713.3225742935 0, -98655.62813787466 1413308.385398984 0, -99053.57924581278 1413307.8649394184 0)), ((-102573.84227282721 1418604.2255107036 0, -102177.37979169976 1418600.9690474125 0, -102177.0852478158 1418198.5925258938 0, -102573.73008625153 1418201.6494684827 0, -102573.84227282721 1418604.2255107036 0)), ((-103762.3031171501 1419420.5363477732 0, -103366.22388905576 1419416.803232996 0, -103365.95161240076 1419819.8151281285 0, -102970.06370104977 1419815.8898234847 0, -102574.16661798784 1419811.9940968393 0, -102574.06497598997 1419409.4034681309 0, -102573.95381921457 1419006.8139781673 0, -102573.84227282721 1418604.2255107036 0, -102970.3045065936 1418607.5117338966 0, -103366.76678810467 1418610.80511 0, -103763.21994417445 1418614.1169626303 0, -103762.7662842679 1419017.326135117 0, -103762.3031171501 1419420.5363477732 0), (-103366.49553182158 1419013.8036599872 0, -102970.22477769863 1419010.2995425325 0, -102970.14441021612 1419413.0997752808 0, -103366.22388905576 1419416.803232996 0, -103366.49553182158 1419013.8036599872 0)), ((-103607.68049878148 1428407.3574287463 0, -103602.40120548545 1428813.5250465341 0, -103597.1127701952 1429219.7047838513 0, -103199.30242564008 1429212.6391023616 0, -102802.52907081215 1429205.6157317858 0, -102404.71774511709 1429198.5984923455 0, -102398.46926949982 1429603.8161399195 0, -102000.6803171128 1429596.4931193087 0, -102006.89713429322 1429191.5884869024 0, -102013.12298757605 1428786.6852258453 0, -102410.95746916845 1428793.3706528917 0, -102808.79138893947 1428800.0860042188 0, -103204.56787206174 1428806.7837567737 0, -103209.824464444 1428400.9182236337 0, -102815.06285254596 1428394.5573525112 0, -102417.20618624233 1428388.1552930959 0, -102423.47317896172 1427981.4294510542 0, -102481.7601933639 1427982.3952424342 0, -102490.00610556726 1427982.5314548574 0, -102821.3466392487 1427988.0221814779 0, -102897.12866658544 1427989.2726389929 0, -103215.09609969346 1427994.561316661 0, -103286.45030234217 1427995.7391205232 0, -103612.9688756502 1428001.1798864868 0, -103607.68049878148 1428407.3574287463 0)), ((-94318.05285296372 1409214.5668109718 0, -94313.57850111574 1409619.022735214 0, -94309.1042760259 1410023.4687219525 0, -93910.7370159215 1410018.2172915097 0, -93512.36962967928 1410012.9733532104 0, -93516.95980339825 1409610.040040049 0, -93521.54118873226 1409207.0966037768 0, -93919.80153974675 1409210.8280514209 0, -94318.05285296372 1409214.5668109718 0)), ((-97844.70466653934 1414527.5369802641 0, -97448.84480714846 1414529.7272351652 0, -97453.16437133847 1414123.1623551168 0, -97849.71790442427 1414121.5175330746 0, -97844.70466653934 1414527.5369802641 0)), ((-98636.42559804795 1414523.211772694 0, -99032.27774895268 1414521.0766419354 0, -99025.18371932303 1414925.4830196623 0, -98630.01601487662 1414928.1636144198 0, -98636.42559804795 1414523.211772694 0)), ((-94239.3367776905 1419355.3697970596 0, -94236.88589608682 1419762.8327458396 0, -93834.15491137239 1419760.1079739258 0, -93837.52790865419 1419352.5433131184 0, -94239.3367776905 1419355.3697970596 0)), ((-98970.46376188945 1424682.5243592479 0, -98569.27515605523 1424683.8686252483 0, -98168.09580278337 1424685.231905905 0, -97766.90786257098 1424686.6140450826 0, -97365.72927417218 1424688.0153025105 0, -97370.03781566468 1424281.8133445985 0, -97374.35516795557 1423875.6126806713 0, -97378.66359198703 1423469.4130585787 0, -97382.98092889391 1423063.2146356527 0, -97784.27985432954 1423058.0077998515 0, -98185.58844868181 1423052.8199848952 0, -98586.8887699464 1423047.6510321011 0, -98988.19885279374 1423042.501204599 0, -98983.7606684282 1423452.505174026 0, -98979.3313871927 1423862.5104601963 0, -98974.89317401552 1424272.516703981 0, -98970.46376188945 1424682.5243592479 0)), ((-94059.83675285004 1428297.134849285 0, -94047.78830087288 1428707.0701078374 0, -93660.84167730855 1428702.597829106 0, -93273.88581301915 1428698.1541748669 0, -93285.8947014553 1428288.43052082 0, -93297.86818946092 1427879.5587093967 0, -93308.20619673278 1427879.6605550156 0, -93356.52519114394 1427880.1335441836 0, -93684.87710900807 1427883.3765095805 0, -93749.60825373865 1427884.009547773 0, -94071.88599501901 1427887.200809396 0, -94059.83675285004 1428297.134849285 0)), ((-98789.51088271826 1432851.2732983914 0, -98778.06278070486 1433249.2970535443 0, -98766.62414708053 1433647.322030613 0, -98755.17724356256 1434045.3479738326 0, -98743.7399073762 1434443.3751392881 0, -98345.39509216356 1434443.4710080456 0, -97947.05941962759 1434443.585649036 0, -97548.71495209764 1434443.71890229 0, -97150.37972951063 1434443.870930553 0, -97160.45694265144 1434039.4213868643 0, -97170.53481982657 1433634.9617107953 0, -97180.61306974819 1433230.5143105339 0, -97190.69188155713 1432826.0568786473 0, -97590.39717530237 1432832.3383533764 0, -97990.10211981475 1432838.6275274365 0, -98389.80662644192 1432844.9466120554 0, -98789.51088271826 1432851.2732983914 0)), ((-88836.91899951367 1403669.0709653178 0, -88831.6854981431 1403690.8822506166 0, -88824.02498805917 1403705.379662453 0, -88814.77179651076 1403712.5609192643 0, -88799.64410296819 1403723.8570922113 0, -88792.93709899105 1403726.9110280115 0, -88778.6780343103 1403734.0514531864 0, -88759.42225685729 1403741.1400268704 0, -88724.21905985722 1403756.3927755377 0, -88713.27392618128 1403766.6800876986 0, -88696.47960766022 1403776.917967307 0, -88690.498842239 1403790.391860605 0, -88682.8044439963 1403809.0427500082 0, -88682.67456277554 1403821.5361271796 0, -88682.50142181 1403838.1938986422 0, -88678.95863057926 1403857.9404021914 0, -88672.10046281546 1403875.5587691814 0, -88668.25123725247 1403883.3560058752 0, -88664.4294907722 1403891.0975692882 0, -88655.91346871144 1403907.66872193 0, -88639.04209755229 1403926.2245789361 0, -88612.96296971402 1403946.7785633283 0, -88593.5997072146 1403964.2673830134 0, -88561.72403452882 1403980.5965202968 0, -88521.41752418655 1404006.2094880154 0, -88502.18415427324 1404011.2051240979 0, -88482.16155511585 1404010.997796026 0, -88470.5444329498 1404005.6825950437 0, -88466.17146120236 1403996.5349670348 0, -88466.85415051879 1403881.380469961 0, -88469.30016250984 1403472.46306391 0, -88865.58899476523 1403476.575173842 0, -88865.25748956957 1403534.2419241183 0, -88863.3053891457 1403538.1850077892 0, -88844.77494207515 1403555.693108859 0, -88839.54139602723 1403577.493074574 0, -88836.77827381823 1403602.453731996 0, -88838.24106564456 1403622.24094297 0, -88840.47291102435 1403648.2947113698 0, -88836.91899951367 1403669.0709653178 0)), ((-88712.3852857559 1403897.8649869259 0, -88713.1954354032 1403883.8001671943 0, -88714.03828920037 1403869.1869952437 0, -88714.4245299299 1403832.042810073 0, -88724.1084906146 1403811.8786831452 0, -88759.54698553265 1403786.9214987422 0, -88820.70516902128 1403760.5412220194 0, -88852.12450506247 1403732.1614000539 0, -88864.2201025576 1403713.0862248677 0, -88863.21610825672 1403885.2693890778 0, -88860.84281636066 1404293.976112206 0, -88858.46951175705 1404702.6727409104 0, -88856.09594561267 1405111.370673376 0, -88459.51528958166 1405108.128740152 0, -88062.9435608325 1405104.8940869458 0, -88065.46294442056 1404695.7610628824 0, -88067.98216166053 1404286.6293473286 0, -88070.28832533426 1403912.024937353 0, -88073.74349464526 1403898.0207511957 0, -88090.17249826937 1403879.6160516897 0, -88091.95069010492 1403877.708661751 0, -88112.0634291369 1403856.1959834045 0, -88124.42874220115 1403837.7494265507 0, -88144.82544856593 1403827.8386157192 0, -88169.09432181073 1403836.530750426 0, -88195.941216318 1403857.0612416037 0, -88229.69155183861 1403864.1720564931 0, -88255.40202713582 1403864.4375805848 0, -88281.17357334016 1403857.941405816 0, -88312.46837830478 1403841.3813041546 0, -88345.0914336815 1403826.5256958173 0, -88361.24133475311 1403835.134392439 0, -88377.14638989799 1403867.3753194625 0, -88380.99358967648 1403880.5367588485 0, -88391.52182953307 1403916.4950833682 0, -88407.31269455753 1403958.8671415611 0, -88432.28792920607 1404030.0408320809 0, -88449.66039120684 1404050.48533603 0, -88465.8220318481 1404055.3213871433 0, -88498.33617965213 1404054.370519267 0, -88537.68758383242 1404042.9552367812 0, -88574.44410220372 1404021.3920682364 0, -88615.32580272321 1403993.109561932 0, -88653.61276931937 1403954.6678664968 0, -88687.81016374502 1403919.5651586987 0, -88712.3852857559 1403897.8649869259 0)), ((-92725.03789765219 1409199.701054333 0, -92729.7353918301 1408798.2826408655 0, -92734.44204175068 1408396.854257546 0, -93132.57732298844 1408399.0357749355 0, -93530.72171557856 1408401.2247658973 0, -93526.13143536559 1408804.165707803 0, -93521.54118873226 1409207.0966037768 0, -93123.2895503766 1409203.3951329854 0, -92725.03789765219 1409199.701054333 0)), ((-92360.08833965978 1413653.2308525657 0, -91956.70286996344 1413652.113093171 0, -91958.10720580119 1413247.2095826631 0, -92361.26571403957 1413247.8767948232 0, -92693.94829534723 1413248.4361525474 0, -92689.5338731609 1413654.158183343 0, -92685.1193274322 1414059.8813657921 0, -92358.91053331329 1414058.5859613924 0, -92360.08833965978 1413653.2308525657 0)), ((-89618.15005361554 1413637.1595225923 0, -89613.52784421502 1414045.0083209148 0, -89215.86687084337 1414038.279547381 0, -88818.2052965973 1414031.5805498827 0, -88821.2704054541 1413623.2787557838 0, -89219.71050648029 1413630.2098519409 0, -89618.15005361554 1413637.1595225923 0)), ((-93844.27361685838 1418537.4173234731 0, -93444.30928149664 1418534.417183636 0, -93448.604266527 1418126.7652493648 0, -93847.6463245715 1418129.8560985199 0, -93844.27361685838 1418537.4173234731 0)), ((-89560.97516376973 1423388.4899375397 0, -89559.41628051212 1423795.9730736206 0, -89159.80662224842 1423792.437049666 0, -89161.24456082463 1423385.2661774433 0, -89560.97516376973 1423388.4899375397 0)), ((-89158.35945816005 1424199.5977638592 0, -89557.85700147413 1424203.4685414871 0, -89556.29751406678 1424610.9540325832 0, -89156.92091686802 1424606.7708883083 0, -89158.35945816005 1424199.5977638592 0)), ((-92478.14842891505 1429098.7149461762 0, -92480.23269712989 1428689.0832759927 0, -92867.17994476062 1428693.50184052 0, -93273.88581301915 1428698.1541748669 0, -93261.88663257027 1429107.879123261 0, -93249.87912469619 1429517.6051012098 0, -92862.97165813525 1429512.9676199823 0, -92476.06396225932 1429508.336527517 0, -92478.14842891505 1429098.7149461762 0)), ((-89279.39345416121 1433127.8646544064 0, -89266.6252196684 1433533.1072736336 0, -89253.84886037794 1433938.3508895955 0, -89241.08221584412 1434343.5956572872 0, -88846.52636626638 1434341.1880825984 0, -88451.97943371661 1434338.7876654088 0, -88057.42348487477 1434336.416762109 0, -87662.8765551925 1434334.0530191802 0, -87668.46902625533 1433923.6148717504 0, -87674.07080429922 1433513.1668060871 0, -87679.6635646027 1433102.730965972 0, -87685.26553587045 1432692.2851067442 0, -88086.98823304276 1432699.8410496197 0, -88488.71948750077 1432707.416183666 0, -88890.44126604153 1432715.01014463 0, -89292.17140046127 1432722.6232907092 0, -89279.39345416121 1433127.8646544064 0), (-88079.60118010656 1433108.9805231334 0, -88072.20536416599 1433518.1211127618 0, -88470.34844821837 1433523.1052969876 0, -88479.52927416314 1433115.2601053773 0, -88079.60118010656 1433108.9805231334 0)), ((-84862.1210284208 1408328.6807842955 0, -84859.44172793816 1408734.8334773607 0, -84461.74653644364 1408732.8066040988 0, -84064.05118110597 1408730.8095224833 0, -84065.84498233233 1408324.2226089637 0, -84463.97843334367 1408326.4479603695 0, -84862.1210284208 1408328.6807842955 0)), ((-84807.50753888277 1418485.8740994087 0, -84803.46677356583 1418891.6164255978 0, -84799.42595400776 1419297.3598887625 0, -84795.38508025554 1419703.1044874315 0, -84399.81260786249 1419701.3113486073 0, -84004.24020863081 1419699.5366552393 0, -83608.66778511007 1419697.7804040853 0, -83213.09534199277 1419696.0424941326 0, -83215.3465778014 1419291.5676956056 0, -83217.59764840879 1418887.0941311917 0, -83219.84845779113 1418482.621698406 0, -83222.09910492194 1418078.150401817 0, -83619.46118999693 1418078.618202269 0, -84016.8234597905 1418079.1045555063 0, -84414.18591268072 1418079.6094616929 0, -84811.54834895539 1418080.132914788 0, -84807.50753888277 1418485.8740994087 0), (-84007.38608612366 1419294.4325526417 0, -84010.53205221213 1418889.3182832596 0, -83614.06473544164 1418888.2026350643 0, -83611.36190419116 1419292.9852613672 0, -84007.38608612366 1419294.4325526417 0)), ((-82433.45367863952 1418471.811997542 0, -82431.22163584364 1418878.210559317 0, -82428.989666873 1419284.598965215 0, -82426.75742351369 1419690.9886109696 0, -82033.58386966141 1419688.488938 0, -81640.41911741834 1419686.0074791266 0, -81642.63205846843 1419277.7028963615 0, -81644.8449579429 1418869.3883637388 0, -81647.0575308344 1418461.086185313 0, -82040.25133292488 1418466.4343270094 0, -82433.45367863952 1418471.811997542 0)), ((-87964.08395915708 1423375.740048612 0, -88362.80353756399 1423378.8857737677 0, -88362.60089704483 1423785.4310671838 0, -88362.40686239593 1424191.9664608913 0, -88362.20345482265 1424598.5027982828 0, -87966.86249210453 1424594.417442006 0, -87965.933821876 1424188.1941615948 0, -87965.01365035953 1423781.9610804282 0, -87964.08395915708 1423375.740048612 0)), ((-83618.43907365491 1427783.9848509997 0, -83737.44065891691 1427785.297279914 0, -83733.77440182888 1428192.2788242535 0, -83335.18560179621 1428189.1150599332 0, -83338.84481935522 1427780.9015110661 0, -83582.80791439058 1427783.590553651 0, -83618.43907365491 1427783.9848509997 0)), ((-84542.76302844692 1427794.2477651588 0, -84537.04341170983 1428198.7118047865 0, -84136.42428546058 1428195.4902023987 0, -84142.14602517396 1427789.7831282464 0, -84328.54614853674 1427791.8604490892 0, -84354.62052558582 1427792.1501634372 0, -84542.76302844692 1427794.2477651588 0)), ((-83730.11738763128 1428597.402833054 0, -83726.4692938403 1429002.539127675 0, -83327.91235049146 1429000.0140313976 0, -83331.55346692208 1428594.5639834472 0, -83730.11738763128 1428597.402833054 0)), ((-84130.72068482457 1428600.2803774886 0, -84531.32395423243 1428603.1768408744 0, -84525.60464986345 1429007.6430736787 0, -84126.03693441047 1429005.0817423589 0, -84130.72068482457 1428600.2803774886 0)), ((-84126.03693441047 1429005.0817423589 0, -84121.34431743283 1429409.8840248408 0, -83722.81216782187 1429407.6653351416 0, -83726.4692938403 1429002.539127675 0, -84126.03693441047 1429005.0817423589 0)))</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1905,16 +1905,16 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Oklahoma State University, Common Schools, Other Agency</t>
+          <t>Common Schools, Oklahoma State University</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>surface, subsurface</t>
+          <t>subsurface, surface</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G31" t="n">
         <v>529.04</v>
@@ -1923,13 +1923,13 @@
         <v>15</v>
       </c>
       <c r="I31" t="n">
-        <v>7203.18</v>
+        <v>7123.2</v>
       </c>
       <c r="J31" t="n">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K31" t="n">
-        <v>7732.22</v>
+        <v>7652.24</v>
       </c>
       <c r="L31" t="n">
         <v>242350.66</v>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Common Schools, Public Building, State Educational Institutions, Oklahoma State University</t>
+          <t>Common Schools, State Educational Institutions, Public Building, Oklahoma State University</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Greer 33, State Educational Institutions, Common Schools, Oklahoma State University, University Preparatory, Public Building, Normal Schools</t>
+          <t>Greer 33, State Educational Institutions, Common Schools, Oklahoma State University, University Preparatory, Normal Schools, Public Building</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Common Schools, State Educational Institutions, Public Building, Oklahoma State University</t>
+          <t>Common Schools, Public Building, State Educational Institutions, Oklahoma State University</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2524,12 +2524,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>NM</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Common Schools, Perm Common Schls, Perm Cmn Schls (Indmty Selec), New Mexico Institute of Mining and Technology, County Bond, Public Schools</t>
+          <t>Perm Common Schls, Perm Cmn Schls (Indmty Selec), New Mexico Institute of Mining and Technology, County Bond, Common Schools, Public Schools</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2610,7 +2610,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-1128240.0266006347 1378385.842705121 0, -1128291.4118384456 1377979.326853167 0, -1128342.7987068966 1377572.8160258273 0, -1128394.1825966947 1377166.3064404274 0, -1128445.5661708254 1376759.7983549957 0, -1128749.6406870573 1376822.4775944548 0, -1128821.7536744415 1376837.34235038 0, -1128821.7536768704 1376837.3423508808 0, -1128989.9337826155 1376872.0186683617 0, -1129197.9385976936 1376914.906293252 0, -1129583.9323733568 1376989.0503674888 0, -1129864.5582041873 1377042.970132364 0, -1129969.923935293 1377063.21524373 0, -1129969.923937703 1377063.2152440413 0, -1129923.1689375208 1377456.5381096725 0, -1129876.3925645563 1377849.8671347466 0, -1129829.631616595 1378243.1996696473 0, -1129782.8699666883 1378636.5336530393 0, -1129397.162708549 1378573.8433946485 0, -1129011.4546921998 1378511.150635521 0, -1128625.7407553326 1378448.495060322 0, -1128240.0266006347 1378385.842705121 0)), ((-1135595.559496878 1377811.9031924587 0, -1135887.6696735772 1377852.1807593098 0, -1135887.6696980635 1377852.180762686 0, -1136279.8713540055 1377906.2775453748 0, -1136241.722985257 1378299.5766089533 0, -1136203.5903955773 1378692.859858292 0, -1136165.437431932 1379086.1621313123 0, -1136127.3019961263 1379479.448013669 0, -1135730.8287856497 1379431.1010282724 0, -1135334.3670495097 1379382.7946452815 0, -1134937.9059860434 1379334.4865309978 0, -1134541.4267154012 1379286.1947030055 0, -1134583.8463221386 1378887.1427064238 0, -1134626.2484252655 1378488.0900345193 0, -1134668.6494565508 1378089.0386769765 0, -1134711.052073863 1377689.9950650113 0, -1134711.988625318 1377690.1241135423 0, -1134711.9886247334 1377690.1241176976 0, -1135103.26140334 1377744.038139601 0, -1135103.2615086911 1377744.0381541231 0, -1135390.6623790655 1377783.655098396 0, -1135495.4654497516 1377798.101772217 0, -1135595.559496878 1377811.9031924587 0)), ((-1134091.870668225 1379633.0829632925 0, -1134142.6328566815 1379228.2713369778 0, -1134541.4267154012 1379286.1947030055 0, -1134490.9373794342 1379691.1645645178 0, -1134440.431316512 1380096.1338175663 0, -1134041.107967413 1380037.896151915 0, -1134091.870668225 1379633.0829632925 0)), ((-1133641.7843699907 1379979.6572193601 0, -1134041.107967413 1380037.896151915 0, -1133990.350244433 1380442.6709463447 0, -1133590.7537812414 1380384.2738787679 0, -1133641.7843699907 1379979.6572193601 0)), ((-1133914.8617393444 1384123.1434420596 0, -1133518.0546113998 1384067.3718153553 0, -1133121.2474062436 1384011.598521716 0, -1132724.43745024 1383955.843850081 0, -1132327.6384421403 1383900.1296666614 0, -1132380.1294119284 1383497.7645706153 0, -1132432.6175352833 1383095.4208360729 0, -1132485.124200542 1382693.060849111 0, -1132537.614331775 1382290.7002605456 0, -1132937.4076582661 1382345.7752826675 0, -1133337.2009549243 1382400.8490701108 0, -1133736.9888489267 1382455.9613874163 0, -1134136.7902785065 1382511.0946259433 0, -1134081.3054377616 1382914.094062059 0, -1134025.8178849416 1383317.114801045 0, -1133970.349285169 1383720.1194558472 0, -1133914.8617393444 1384123.1434420596 0)), ((-1129911.9617069426 1386914.4819080972 0, -1129531.3123497304 1386858.238160551 0, -1129150.6577348115 1386802.011203176 0, -1128770.0029034042 1386745.8014204486 0, -1128810.18117793 1386343.5014383916 0, -1128851.8116658041 1385926.8742460005 0, -1128893.5163361796 1385510.2992053425 0, -1128935.235608927 1385093.7277662717 0, -1129330.3991150372 1385149.765814424 0, -1129725.5760493914 1385205.8242323347 0, -1130118.2504813895 1385276.1945416632 0, -1130510.919103605 1385346.603010369 0, -1130455.6097842276 1385758.0277571783 0, -1130400.3003183224 1386169.4539493052 0, -1130345.0253977205 1386580.7442335933 0, -1130292.6112126154 1386970.7462049725 0, -1129911.9617069426 1386914.4819080972 0)), ((-1131694.5584177857 1403154.8460936155 0, -1131674.7643498778 1403327.0536281727 0, -1131674.7633971802 1403327.0619166011 0, -1131629.6108235891 1403719.8596693594 0, -1131233.8760388307 1403659.806582935 0, -1130838.132058296 1403599.7711531953 0, -1130442.38485147 1403539.7539864825 0, -1130046.6507314045 1403479.7572590564 0, -1130091.02808195 1403079.3536275472 0, -1130135.4042871143 1402678.9512385186 0, -1130190.2168448102 1402276.9270303233 0, -1130245.0428887089 1401874.9263128457 0, -1130636.3358691412 1401943.3328004412 0, -1131027.6410377992 1402011.759481511 0, -1131418.9261743415 1402080.2019411225 0, -1131810.2073915359 1402148.6623356345 0, -1131765.056338869 1402541.4644241468 0, -1131719.9044020802 1402934.2678488703 0, -1131694.5584177857 1403154.8460936155 0)), ((-1131629.6108235905 1403719.8596693596 0, -1131674.7634721666 1403327.0620394223 0, -1131674.7644374084 1403327.0536418608 0, -1131694.2720732396 1403157.3380614424 0, -1131674.7704569306 1403327.0545832047 0, -1131629.6168607788 1403719.860585508 0, -1131629.6108235905 1403719.8596693596 0)), ((-1130470.0476174715 1411622.0767788892 0, -1130471.3870147462 1411612.0801684652 0, -1130471.3875700883 1411612.0760384062 0, -1130471.3881286476 1411612.0761204213 0, -1130422.6596337657 1411975.7695378698 0, -1130417.698511745 1412012.7793159194 0, -1130379.3193196955 1412299.1391630087 0, -1130417.692801543 1412012.7784684966 0, -1130379.3185861527 1412299.1446362145 0, -1130368.8478305305 1412377.2704074662 0, -1130367.705419441 1412385.6771458772 0, -1130363.9256571524 1412413.452444389 0, -1130363.92492276 1412413.4578410152 0, -1130316.2237182234 1412778.9640306754 0, -1130363.9250123813 1412413.45785291 0, -1130363.9257465557 1412413.4524577858 0, -1130367.6899678416 1412385.7908506168 0, -1130363.9308639802 1412413.4532246208 0, -1130316.2242222133 1412778.9710565119 0, -1130311.715413668 1412813.5625438425 0, -1130271.0147584558 1413125.3791732949 0, -1130311.7080710516 1412813.5614359821 0, -1130311.708304903 1412813.5596440658 0, -1130311.7080710505 1412813.561435982 0, -1130298.939608259 1412911.4009462243 0, -1130270.5494316898 1413128.9441435148 0, -1130263.7966130837 1413180.6789651318 0, -1130263.1874864711 1413185.2859392043 0, -1130259.4305079263 1413213.6435761505 0, -1129843.5671898066 1413150.4769921284 0, -1129427.6928954879 1413087.329438535 0, -1129011.8339981886 1413024.1843259658 0, -1128595.9555229982 1412961.0574279884 0, -1128666.7902152468 1412565.3853512001 0, -1128737.6424725812 1412169.71695834 0, -1128808.480147453 1411774.0481500102 0, -1128879.319372785 1411378.380882504 0, -1129277.335666687 1411436.7863361777 0, -1129675.367770541 1411495.1924299735 0, -1130073.3781521877 1411553.6350381465 0, -1130471.387480631 1411612.0760252709 0, -1130471.3869251222 1411612.0801565703 0, -1130422.6513729764 1411975.778441062 0, -1130417.6934915904 1412012.7733190442 0, -1130422.651447872 1411975.7785638876 0, -1130470.0476174715 1411622.0767788892 0)), ((-1130263.1423691805 1413185.627172347 0, -1130259.4379366827 1413213.644704524 0, -1130259.4305973367 1413213.6435897313 0, -1130263.1423691805 1413185.627172347 0)), ((-1128199.4941676722 1388258.092569399 0, -1127813.8064076349 1388197.2454368593 0, -1127428.1181161546 1388136.3956955457 0, -1127042.4150374373 1388075.5793239689 0, -1127092.549571546 1387674.5276768932 0, -1127142.683761955 1387273.4774474546 0, -1127192.8150246062 1386872.4285907475 0, -1127242.9482214623 1386471.3812725784 0, -1127612.3575455945 1386550.9617211486 0, -1127981.7620197614 1386630.5581261318 0, -1128375.8853373388 1386688.1692564106 0, -1128770.0029034042 1386745.8014204486 0, -1128723.7931344162 1387139.0964353874 0, -1128677.5899458732 1387532.3753459016 0, -1128631.3833221574 1387925.67554847 0, -1128585.1787404602 1388318.9571824968 0, -1128199.4941676722 1388258.092569399 0)), ((-1128902.256667591 1394855.7506675306 0, -1129301.3881760822 1394893.8064189097 0, -1129240.6210568582 1395348.951187639 0, -1129179.8674093112 1395804.119944101 0, -1129145.4072263225 1396173.6745128701 0, -1129110.945593145 1396543.2301865914 0, -1128716.8824294384 1396492.5587382494 0, -1128324.7787728661 1396442.1240041174 0, -1127932.6122955997 1396389.180351191 0, -1127541.496440933 1396336.3737075853 0, -1127586.3635830584 1395936.8323112822 0, -1127631.2459652512 1395537.294464622 0, -1127668.0067557807 1395140.2193864277 0, -1127704.7658234667 1394743.1455489877 0, -1128103.9459806434 1394780.420277149 0, -1128503.1385945815 1394817.735617346 0, -1128902.256667591 1394855.7506675306 0)), ((-1127493.076462513 1397209.5182006557 0, -1127423.921724395 1397604.818929388 0, -1127354.7683083252 1398000.1213105617 0, -1126989.1006696948 1397948.6614400165 0, -1126623.4495540212 1397897.199336939 0, -1126257.793353734 1397845.7729081265 0, -1125892.132160036 1397794.352604225 0, -1125933.612666578 1397396.8683351292 0, -1125975.092380122 1396999.382184817 0, -1126016.570586621 1396601.9004633154 0, -1126058.0474899095 1396204.4200535296 0, -1126366.48689195 1396246.6194582006 0, -1126451.3593452626 1396258.2303121325 0, -1126738.3557137987 1396297.5093653526 0, -1126844.7242997878 1396311.6365292708 0, -1127135.451325891 1396351.6820569288 0, -1127238.0332831962 1396365.505238777 0, -1127532.5461209563 1396405.8579272463 0, -1127631.4018461602 1396418.9207291915 0, -1127562.2326115884 1396814.2192355755 0, -1127493.076462513 1397209.5182006557 0)), ((-1127208.5940730576 1406269.8185887574 0, -1126810.7331826407 1406208.0119500705 0, -1126412.8668680415 1406146.2205139736 0, -1126471.18721819 1405743.5383591235 0, -1126529.5671999634 1405340.4486460553 0, -1126592.1225184647 1404936.3481409336 0, -1126654.6785942863 1404532.2490064232 0, -1127054.162652761 1404619.2846886918 0, -1127453.6544733664 1404706.3609974007 0, -1127853.127288661 1404793.4338540144 0, -1128252.5926652716 1404880.5449631338 0, -1128186.447389112 1405249.7336289717 0, -1128120.3060441387 1405618.903758814 0, -1128062.533436392 1406004.9067246353 0, -1128004.306815114 1406393.4900116608 0, -1127606.4515062582 1406331.6467938172 0, -1127208.5940730576 1406269.8185887574 0)), ((-1125845.4282341187 1371936.845910621 0, -1125793.15533219 1372343.1998504114 0, -1125740.9008406678 1372749.536772335 0, -1125688.6270627417 1373155.892008587 0, -1125290.0192406122 1373103.928756387 0, -1124891.4089248725 1373051.984023202 0, -1124492.8097970292 1373000.079876511 0, -1124094.194676932 1372948.1724022934 0, -1124150.9520465452 1372541.6143547052 0, -1124207.7067449703 1372135.077067238 0, -1124264.4641428345 1371728.520775997 0, -1124321.2027708457 1371321.9838986052 0, -1124715.3335886346 1371374.094588449 0, -1124969.197274951 1371407.6584505804 0, -1125109.4613311233 1371426.2084159509 0, -1125109.4640081115 1371426.2087701303 0, -1125503.583424903 1371478.3528167694 0, -1125503.5902477072 1371478.353719727 0, -1125739.166247116 1371509.5308019777 0, -1125897.698146327 1371530.5136803943 0, -1125845.4282341187 1371936.845910621 0)), ((-1126220.619844299 1378132.9269923076 0, -1125821.5358651546 1378081.5561233014 0, -1125423.0038183618 1378030.5003883932 0, -1125024.4667478797 1377979.4830556442 0, -1125077.1341659254 1377574.7647088985 0, -1125129.7851389097 1377170.04569603 0, -1125182.435765012 1376765.328378942 0, -1125583.377213075 1376815.6668737624 0, -1125636.8485578434 1376410.6540712777 0, -1126038.603509141 1376460.7117040104 0, -1126440.3532680192 1376510.790946046 0, -1126842.1032454043 1376560.8893832208 0, -1126786.5091987266 1376966.7358099273 0, -1126730.9103575198 1377372.6084336329 0, -1126675.2978345868 1377778.4605466411 0, -1126619.6988799425 1378184.3363719773 0, -1126220.619844299 1378132.9269923076 0)), ((-1125545.3371591107 1387083.0203807312 0, -1125544.729486463 1387087.6319533226 0, -1125492.6124915709 1387483.9288486124 0, -1125439.8876767652 1387884.8388722134 0, -1125063.804140553 1387838.0170659635 0, -1124687.737427861 1387791.1938643027 0, -1124311.666115539 1387744.4072896393 0, -1123935.5767421848 1387697.6350934738 0, -1123970.1022329344 1387296.5240704399 0, -1124004.606926887 1386895.4321212138 0, -1124039.1123274586 1386494.3214349453 0, -1124073.6319960393 1386093.2142716632 0, -1124467.9235235755 1386140.185400604 0, -1124862.2128556487 1386187.174632246 0, -1125256.5003753917 1386234.182104476 0, -1125650.7858936845 1386281.2076976425 0, -1125598.0616001636 1386682.1132599206 0, -1125545.3371591107 1387083.0203807312 0)), ((-1126361.9101554158 1406535.9827642022 0, -1126310.9572366572 1406925.7566291431 0, -1126260.0041376273 1407315.5318047248 0, -1126209.0533922075 1407705.2883876492 0, -1125807.5534071801 1407655.5281003006 0, -1125406.0351721765 1407605.784495414 0, -1125004.5335496573 1407556.041992541 0, -1124603.0129532327 1407506.3379697264 0, -1124655.2105047817 1407104.6738516432 0, -1124707.4050813988 1406703.0107462956 0, -1124764.304567047 1406301.1705137906 0, -1124821.204543008 1405899.3287299788 0, -1125219.12483808 1405961.0261111686 0, -1125617.0420723448 1406022.7390251865 0, -1126014.9561486228 1406084.4704992943 0, -1126412.8668680415 1406146.2205139736 0, -1126361.9101554158 1406535.9827642022 0)), ((-1126103.52059037 1414251.3650786027 0, -1126495.1129209618 1414309.6826994368 0, -1126886.689042538 1414367.9960305768 0, -1126836.1631484919 1414763.176372017 0, -1126785.6206852472 1415158.3559435843 0, -1126392.2930198866 1415104.2599242062 0, -1125998.9816615938 1415050.1641830564 0, -1126051.243126521 1414650.7629280959 0, -1126103.52059037 1414251.3650786027 0)), ((-1125240.9989922796 1414945.9322766422 0, -1125240.9989986802 1414945.9322930144 0, -1125368.1904321758 1414963.4195661335 0, -1125368.190386117 1414963.4194649837 0, -1125605.0092473277 1414995.9792691455 0, -1125552.1970623517 1415397.9503565687 0, -1125499.2574982783 1415800.8047305925 0, -1125486.16671321 1415799.043438584 0, -1125486.1667134678 1415799.0434365747 0, -1125104.735172474 1415747.7238937775 0, -1125122.286096165 1415614.6927755333 0, -1125122.2859603993 1415614.6927563478 0, -1125157.8990082943 1415344.756810457 0, -1125211.0502907436 1414941.8147104 0, -1125240.9989922796 1414945.9322766422 0)), ((-1124488.4534969144 1375863.9466505046 0, -1124545.9164180295 1375465.2077496115 0, -1124945.8408690132 1375515.3136150604 0, -1125345.7819611502 1375565.4205175303 0, -1125290.4420950527 1375963.0168664292 0, -1125235.0942204224 1376360.6126358563 0, -1124833.184652902 1376310.6326070586 0, -1124431.2708092097 1376260.6679009446 0, -1124488.4534969144 1375863.9466505046 0)), ((-1123244.3993556977 1382689.5563968648 0, -1122851.6047364774 1382637.9446412507 0, -1122894.7821541948 1382232.3261767775 0, -1122937.958270201 1381826.7093334198 0, -1122981.1170945005 1381421.0916619352 0, -1123024.29095105 1381015.4775920846 0, -1123417.2579000075 1381065.0995536167 0, -1123810.2225495384 1381114.7396071162 0, -1124205.8333911672 1381165.8018399097 0, -1124601.4255426365 1381216.8804861498 0, -1124556.7575178389 1381623.7622372766 0, -1124512.1020188408 1382030.6674087287 0, -1124467.4292292793 1382437.5719731501 0, -1124422.7716010276 1382844.4800661337 0, -1124029.9841118657 1382792.8141149967 0, -1123637.1915669353 1382741.1862149024 0, -1123244.3993556977 1382689.5563968648 0)), ((-1123506.280545221 1397523.807386724 0, -1123113.546769394 1397477.8898072825 0, -1122720.8137690278 1397431.9702237793 0, -1122763.109827633 1397024.0858502928 0, -1122805.4073543407 1396616.1829707017 0, -1122847.7008853767 1396208.3013505863 0, -1122889.9958938463 1395800.401127108 0, -1123189.3111801764 1395840.1973796408 0, -1123290.6333705958 1395853.6759272644 0, -1123592.4170097834 1395893.8317720902 0, -1123691.2390760726 1395907.0673611416 0, -1123995.590683897 1395947.575784164 0, -1124091.8688309146 1395960.3997998708 0, -1124398.7883693685 1396001.2610068868 0, -1124492.488340714 1396013.8107537832 0, -1124442.2964177344 1396414.2945269318 0, -1124392.106770431 1396814.7598914225 0, -1124341.9167850271 1397215.22653639 0, -1124291.7262449125 1397615.6946420253 0, -1123898.9962280719 1397569.7408873076 0, -1123506.280545221 1397523.807386724 0)), ((-1125050.7333485072 1416089.8860668119 0, -1125041.8281434458 1416146.347519247 0, -1124978.9282343488 1416544.9784228264 0, -1124916.0316808743 1416943.5908303708 0, -1124853.1493242446 1417342.2267834733 0, -1124457.9174930924 1417298.9261537998 0, -1124062.6679361095 1417255.6417318368 0, -1123667.4356306635 1417212.357741493 0, -1123272.2015044442 1417169.1221639696 0, -1123272.2015071386 1417169.1221471285 0, -1123337.6065180777 1416760.321508964 0, -1123337.6065258821 1416760.321460184 0, -1123403.0153526028 1416351.5196232654 0, -1123403.0153590597 1416351.5195829112 0, -1123468.4250636017 1415942.7194489401 0, -1123468.4250693142 1415942.7194132379 0, -1123473.747317706 1415909.4555252187 0, -1123533.8327863354 1415533.9235664124 0, -1123926.56349187 1415587.3460286171 0, -1124319.2892320438 1415640.786062571 0, -1124712.0120305463 1415694.2474056818 0, -1125104.735172474 1415747.7238937775 0, -1125089.1809641218 1415846.2507992552 0, -1125069.5971794683 1415970.357194465 0, -1125050.7333485072 1416089.8860668119 0)), ((-1122019.1521206042 1375956.1699800775 0, -1121618.804655642 1375905.4827582964 0, -1121218.457656987 1375854.811407748 0, -1120841.116851507 1375802.8648016313 0, -1120463.7737590438 1375750.9349210237 0, -1120516.200899676 1375355.6310267446 0, -1120569.7512673917 1374952.2348903345 0, -1120625.6667781945 1374547.7692953877 0, -1120681.5959395962 1374143.3273205212 0, -1121074.12740433 1374194.9156548358 0, -1121466.6566759371 1374246.5220041089 0, -1121859.183348471 1374298.146430173 0, -1122251.7077260332 1374349.788860836 0, -1122191.2815362918 1374752.3813441172 0, -1122130.839695816 1375154.9734927684 0, -1122074.7236576332 1375557.3833075035 0, -1122019.1521206042 1375956.1699800775 0)), ((-1123376.9303048812 1391741.2576516299 0, -1123314.5698582318 1392137.5653234327 0, -1123252.1940557153 1392533.8726081797 0, -1122851.979595349 1392490.8314365125 0, -1122451.7663102946 1392447.7890737671 0, -1122051.548718278 1392404.7854837133 0, -1121651.3323146391 1392361.7806028118 0, -1121722.701105602 1391969.9432715562 0, -1121794.0714790968 1391578.1077279423 0, -1121865.4435533658 1391186.2737822745 0, -1121936.8172005732 1390794.44172734 0, -1122328.038850107 1390832.9778433996 0, -1122719.2619607688 1390871.511682969 0, -1123110.4650883302 1390910.0814708392 0, -1123501.685879371 1390948.6512496257 0, -1123439.307756312 1391344.953618665 0, -1123376.9303048812 1391741.2576516299 0)), ((-1121290.518223922 1402189.6028911723 0, -1120898.946553349 1402139.7069227165 0, -1120507.3727919913 1402089.8290760154 0, -1120560.475735779 1401673.8246992396 0, -1120613.578409893 1401257.821800938 0, -1120666.6832297882 1400841.8006717367 0, -1120719.7852362166 1400425.8010265727 0, -1121110.7986750705 1400489.7828177535 0, -1121501.8087625043 1400553.782531097 0, -1121892.8339492006 1400617.7824019396 0, -1122283.8369248898 1400681.8180203056 0, -1122231.280922139 1401083.7118800778 0, -1122178.7382479333 1401485.6293996815 0, -1122126.1978938389 1401887.5282161443 0, -1122073.6572772407 1402289.4287313183 0, -1121682.0875257791 1402239.5167519285 0, -1121290.518223922 1402189.6028911723 0)), ((-1123193.293392606 1406083.5382776444 0, -1123144.6723689795 1406491.0077775405 0, -1123096.0344954468 1406898.476659974 0, -1123047.4120210616 1407305.9490347523 0, -1122641.1381050788 1407241.9584489563 0, -1122234.8580531853 1407178.007303228 0, -1121838.8895895265 1407124.5338010213 0, -1121442.932036701 1407071.1008011792 0, -1121497.408968595 1406668.462640541 0, -1121551.9021824973 1406265.8281743904 0, -1121606.3951982583 1405863.194909579 0, -1121660.8756521624 1405460.5743139726 0, -1122056.1404709648 1405514.4236066951 0, -1122451.402855788 1405568.2909629247 0, -1122846.662549228 1405622.1769650364 0, -1123241.9222513768 1405676.081467265 0, -1123193.293392606 1406083.5382776444 0)), ((-1120370.8519903524 1376558.8173142108 0, -1120318.5523466591 1376963.4801781676 0, -1120266.2522479899 1377368.1446207205 0, -1119880.8900891547 1377319.3201747807 0, -1119495.5121968861 1377270.4908559385 0, -1119110.1457082026 1377221.7010819372 0, -1118724.7796867318 1377172.9088053552 0, -1118778.2443194068 1376768.5999457866 0, -1118831.725020293 1376364.2947682526 0, -1118884.8882999346 1375959.6451455804 0, -1118938.0538767064 1375554.9872533744 0, -1119319.4882878212 1375603.949662015 0, -1119700.917847579 1375652.9285817863 0, -1120082.3483423563 1375701.9218368852 0, -1120463.7737590438 1375750.9349210237 0, -1120417.3068957361 1376154.8728294435 0, -1120370.8519903524 1376558.8173142108 0)), ((-1120491.9494602073 1385624.6256410768 0, -1120093.763575009 1385573.8576330252 0, -1119695.5940897868 1385523.0902777323 0, -1119297.4198083158 1385472.3613170802 0, -1119340.9472703985 1385061.9468487294 0, -1119384.0188619152 1384655.7591478426 0, -1119427.0704806547 1384249.5909008489 0, -1119470.1371432533 1383843.4260441957 0, -1119868.8971800464 1383892.909579033 0, -1120267.6523941972 1383942.4318258371 0, -1120666.4080914243 1383991.9526028684 0, -1121065.1589723115 1384041.511990617 0, -1121021.4782800283 1384449.263482045 0, -1120977.7938667354 1384857.036411433 0, -1120934.1213892677 1385264.7109163136 0, -1120890.1143988897 1385675.4301850495 0, -1120491.9494602073 1385624.6256410768 0)), ((-1119210.4431516875 1395311.3163535972 0, -1118934.7090922128 1395276.3787889068 0, -1118813.6356889023 1395261.0540254316 0, -1118539.2900616706 1395226.3112991361 0, -1118416.728878138 1395210.7972705083 0, -1118143.8849135807 1395176.264417947 0, -1118098.301202479 1395578.1417531045 0, -1118052.7300718888 1395980.0426425133 0, -1118014.0373714229 1396382.7649197942 0, -1117975.3431394938 1396785.4885941045 0, -1117571.6254414623 1396735.1006511487 0, -1117167.8919210657 1396684.7097284375 0, -1116764.1535303488 1396634.3577780328 0, -1116360.421244751 1396584.0230776295 0, -1116412.5612726118 1396182.507904486 0, -1116464.7032912923 1395780.9975934473 0, -1116516.842493938 1395379.4883429958 0, -1116568.9815043674 1394977.9808117792 0, -1116834.5780802164 1395011.4059938502 0, -1116962.7155866746 1395027.5252937344 0, -1117229.599019029 1395061.1176071411 0, -1117356.4427145289 1395077.0734968886 0, -1117624.6985429188 1395110.858177675 0, -1117750.1649038973 1395126.6599330301 0, -1118019.812084375 1395160.6190671015 0, -1118103.80581375 1394719.2757708228 0, -1118179.194871264 1394323.174766747 0, -1118254.6177017856 1393926.957919362 0, -1118330.045173897 1393530.7230543261 0, -1118723.858239953 1393579.8287040037 0, -1119117.6529882865 1393628.9504550146 0, -1119511.4457410742 1393678.0903830659 0, -1119905.2362008188 1393727.2484592765 0, -1119832.7602143239 1394124.2319429151 0, -1119760.2884778217 1394521.1972540407 0, -1119688.0464158494 1394917.9302005172 0, -1119607.2322423405 1395361.5950784427 0, -1119330.109592792 1395326.462352874 0, -1119210.4431516875 1395311.3163535972 0)), ((-1120017.2218312682 1411823.245533616 0, -1119624.4961145993 1411764.1988645403 0, -1119231.7673409404 1411705.1704383884 0, -1119272.5596525783 1411301.4272396904 0, -1119313.366888842 1410897.6874931958 0, -1119354.1727376643 1410493.9490263194 0, -1119394.9610742857 1410090.209785507 0, -1119798.6280583078 1410143.523002227 0, -1120202.3085699002 1410196.8576489014 0, -1120592.3456760987 1410247.2185010735 0, -1120982.3778819165 1410297.6172102676 0, -1120937.463806247 1410708.5557827086 0, -1120892.5298556273 1411119.5134683042 0, -1120847.597506007 1411530.4526423176 0, -1120802.664136076 1411941.3930969462 0, -1120409.9445088701 1411882.3102444937 0, -1120017.2218312682 1411823.245533616 0)), ((-1118611.105025861 1366097.0532489782 0, -1118558.8563670083 1366495.3897124978 0, -1118506.5913973786 1366893.7255140257 0, -1118454.342544761 1367292.0650934004 0, -1118055.342904511 1367241.9869817195 0, -1117656.3274022678 1367191.9055899843 0, -1117257.3233436814 1367141.8646434117 0, -1116858.317118064 1367091.842385068 0, -1116909.8833289621 1366688.2974139208 0, -1116961.4466174536 1366284.7739470403 0, -1117013.028493065 1365881.2341799582 0, -1117064.5933234126 1365477.7085871068 0, -1117075.2175828249 1365479.176522235 0, -1117135.5558840279 1365487.5133749652 0, -1117464.2869575792 1365532.9336654537 0, -1117464.287008481 1365532.9336724868 0, -1117863.9807288654 1365588.1746178728 0, -1117863.9807545831 1365588.1746214286 0, -1118263.6688977159 1365643.436894331 0, -1118263.668992807 1365643.4369074786 0, -1118663.35432386 1365698.7180505735 0, -1118663.3544092162 1365698.7180587589 0, -1118611.105025861 1366097.0532489782 0)), ((-1117189.2932919015 1376550.2051515838 0, -1117110.5151065283 1376963.1067198256 0, -1116711.3172738892 1376914.2650301782 0, -1116312.1172849792 1376865.4419970491 0, -1115913.7940967216 1376819.3715731637 0, -1115515.4527668075 1376773.3175712095 0, -1115594.3383009331 1376364.5472763253 0, -1115673.22600663 1375955.7790357363 0, -1115752.1158840456 1375547.0128510601 0, -1115830.9958592872 1375138.2581894842 0, -1116230.3826382225 1375167.540709523 0, -1116629.771235196 1375196.845431583 0, -1117027.7077151476 1375254.1685232958 0, -1117425.6443661659 1375311.5073099232 0, -1117346.8560745905 1375724.4080506726 0, -1117268.0734960402 1376137.3054482758 0, -1117189.2932919015 1376550.2051515838 0)), ((-1119185.7792514544 1379685.700942679 0, -1118795.3851939102 1379641.9387300296 0, -1118404.9948042564 1379598.1545219317 0, -1118457.930092059 1379194.11211182 0, -1118847.614990889 1379237.0121130517 0, -1119237.2981003602 1379279.9298840172 0, -1119185.7792514544 1379685.700942679 0)), ((-1117018.5340397567 1381042.8103848211 0, -1117424.2646438633 1381103.0848327184 0, -1117359.230112336 1381497.4307794517 0, -1116947.939467744 1381431.840926394 0, -1117018.5340397567 1381042.8103848211 0)), ((-1119114.1912407677 1387078.1539595884 0, -1118710.407157063 1387028.6169571707 0, -1118306.604704382 1386979.0970227346 0, -1117909.6519800108 1386930.4317708092 0, -1117512.6855504394 1386881.7739938835 0, -1117560.7465247782 1386476.8190029685 0, -1117608.8088853294 1386071.8688412127 0, -1117661.7650544855 1385668.1432982194 0, -1117714.7240180697 1385264.416576316 0, -1118110.004116254 1385315.5522046068 0, -1118505.2923531365 1385366.6999264034 0, -1118901.3505172192 1385419.5103644102 0, -1119297.4198083158 1385472.3613170802 0, -1119251.6098520532 1385873.806871388 0, -1119205.7991053527 1386275.2537726094 0, -1119160.0036859268 1386676.704177705 0, -1119114.1912407677 1387078.1539595884 0)), ((-1118662.111614961 1403452.7498157609 0, -1118622.5437863856 1403851.4642660618 0, -1118582.988124498 1404250.2019398885 0, -1118543.3936028015 1404648.9767631488 0, -1118504.1986571378 1405043.711665212 0, -1118107.2315810733 1404991.00743132 0, -1117710.2595882423 1404938.3213404317 0, -1117314.118173709 1404884.6910027026 0, -1116917.974310593 1404831.079037254 0, -1116968.1458393948 1404429.49774891 0, -1117018.3326361047 1404027.9085850802 0, -1117409.4293773554 1404083.4659481624 0, -1117457.4441982775 1403681.7967623856 0, -1117069.1176739975 1403625.262035704 0, -1117119.9049988 1403222.596860389 0, -1117505.460982016 1403280.108995511 0, -1117891.0140504884 1403337.638496846 0, -1118276.5643013476 1403395.1853733838 0, -1118662.111614961 1403452.7498157609 0)), ((-1117317.8398769652 1413916.8720055358 0, -1116923.3634524494 1413865.2644651786 0, -1116528.8872638717 1413813.655073302 0, -1116134.1073801508 1413761.9838715512 0, -1115739.3252709561 1413710.3310343996 0, -1115793.013311971 1413309.2076450454 0, -1115846.698637258 1412908.105927389 0, -1116240.9136658087 1412960.6188934338 0, -1116635.1423940116 1413013.152255771 0, -1117029.3523837791 1413065.701785874 0, -1117423.576168497 1413118.2717208778 0, -1117370.708093865 1413517.5712385045 0, -1117317.8398769652 1413916.8720055358 0)), ((-1115833.3656671576 1371877.5591570935 0, -1115438.1144834477 1371822.8658539534 0, -1115042.8580346717 1371768.2107182206 0, -1114647.6151953572 1371713.5758303313 0, -1114697.086335208 1371310.857357119 0, -1114746.571046667 1370908.1615354095 0, -1114796.0390933577 1370505.4645013174 0, -1114845.5092699367 1370102.7491386028 0, -1115238.3381507492 1370154.3479434708 0, -1115631.150968839 1370205.9427950433 0, -1116023.9587798512 1370257.5755494772 0, -1116416.7830804472 1370309.208498443 0, -1116369.7268699668 1370714.9603258774 0, -1116322.6863069464 1371120.7155747996 0, -1116275.6424492747 1371526.4918530076 0, -1116228.60063545 1371932.2486794905 0, -1115833.3656671576 1371877.5591570935 0)), ((-1116022.7089924891 1385406.5962572389 0, -1115959.67820087 1385778.5180585426 0, -1115896.664561576 1386150.443591691 0, -1115833.635848409 1386522.3684386956 0, -1115430.3606568763 1386471.797216954 0, -1115027.066937816 1386421.2427379764 0, -1114623.784562455 1386370.729539384 0, -1114220.4862765665 1386320.2133935723 0, -1114289.7072830496 1385949.722949249 0, -1114358.9325702668 1385579.2142781625 0, -1114428.1756430103 1385208.709230789 0, -1114497.3952443714 1384838.2174034084 0, -1114894.47970747 1384887.3075657897 0, -1115291.5624348433 1384936.413244068 0, -1115688.6428555646 1384985.5372174808 0, -1116085.7232992365 1385034.683151742 0, -1116022.7089924891 1385406.5962572389 0)), ((-1116860.3005500005 1405229.2839743113 0, -1116802.6426363084 1405627.4815285993 0, -1116744.9689811217 1406025.6781803533 0, -1116687.2955526991 1406423.876576 0, -1116294.1719715425 1406377.3754102292 0, -1115901.0489499893 1406330.8725825709 0, -1115507.9052103704 1406284.4057358704 0, -1115114.782160014 1406237.9370352374 0, -1115168.7230674485 1405835.956606664 0, -1115222.6637482992 1405433.977365807 0, -1115276.6022960509 1405031.996397434 0, -1115330.5430566077 1404630.020194993 0, -1115727.0331075906 1404679.6123850017 0, -1116123.523107197 1404729.2262405918 0, -1116520.7499910598 1404780.143296488 0, -1116917.974310593 1404831.079037254 0, -1116860.3005500005 1405229.2839743113 0)), ((-1115633.1418777418 1414505.1746285215 0, -1115685.6684730274 1414111.967563779 0, -1116080.7040769043 1414163.0441810472 0, -1116475.7400876503 1414214.119270351 0, -1116423.3384940496 1414608.9762151756 0, -1116028.2414423139 1414557.0663104777 0, -1115741.168306802 1414519.3626365417 0, -1115633.141902626 1414505.1746318107 0, -1115633.1418777418 1414505.1746285215 0)), ((-1114994.5155381316 1380791.8029875185 0, -1114912.8396462698 1381180.7940371966 0, -1114831.1664392145 1381569.7870667868 0, -1114425.432657003 1381512.7190591858 0, -1114019.6797628058 1381455.6681342002 0, -1113612.9360044668 1381397.8783298861 0, -1113206.1892360575 1381340.1078665403 0, -1113294.535637208 1380948.2215568393 0, -1113382.8851522834 1380556.33743563 0, -1113471.221573711 1380164.4532357715 0, -1113559.5774453334 1379772.57320461 0, -1113959.1579454546 1379832.848510015 0, -1114358.73257916 1379893.1624846621 0, -1114758.3066317681 1379953.4751462238 0, -1115157.8775567808 1380013.8064945654 0, -1115076.1964821767 1380402.793699327 0, -1114994.5155381316 1380791.8029875185 0)), ((-1113724.2650150552 1390913.7943994924 0, -1113681.2784560448 1391315.728650421 0, -1113283.1984357322 1391260.3218896058 0, -1112885.1130982367 1391204.9537267606 0, -1112487.0275419522 1391149.5840573346 0, -1112088.9392055061 1391094.233084737 0, -1112131.393906547 1390689.6118045177 0, -1112173.8609604845 1390285.0140644608 0, -1112216.3296320504 1389880.3977322194 0, -1112258.7808553192 1389475.7807164525 0, -1112657.404122839 1389533.7986590758 0, -1113056.0243928742 1389591.8352707692 0, -1113454.6254375621 1389649.8884842056 0, -1113853.2398258522 1389707.962241377 0, -1113810.2564457653 1390109.8923346056 0, -1113767.269297699 1390511.8438013617 0, -1113724.2650150552 1390913.7943994924 0)), ((-1114854.4823440555 1394754.0659244068 0, -1114988.1133118349 1394771.7419968795 0, -1114935.9763585539 1395176.9893065458 0, -1114883.8420186962 1395582.213722154 0, -1114490.2072317007 1395529.8639128143 0, -1114096.5563731056 1395477.5101458756 0, -1114041.8714879374 1395882.0374893171 0, -1113647.0157602965 1395829.3622528506 0, -1113252.1761896233 1395776.6873727671 0, -1113309.4276504589 1395372.8603975344 0, -1113366.7005648857 1394968.99718064 0, -1113423.9624049892 1394565.1516942214 0, -1113679.838309738 1394598.9463572563 0, -1113814.9614845193 1394616.7950241456 0, -1114071.3347776176 1394650.6663991376 0, -1114205.9527542805 1394668.4776072593 0, -1114462.9051152733 1394702.383234385 0, -1114597.0377418634 1394720.0839761526 0, -1114854.4823440555 1394754.0659244068 0)), ((-1112361.6383310102 1405880.9739550042 0, -1111968.8366323074 1405830.8988658648 0, -1112021.4546696176 1405427.5697413757 0, -1112074.088564408 1405024.2441567262 0, -1112126.7222990901 1404620.9199674067 0, -11121</t>
+          <t>MULTIPOLYGON Z (((-1128240.0266006347 1378385.842705121 0, -1128291.4118384456 1377979.326853167 0, -1128342.7987068966 1377572.8160258273 0, -1128394.1825966947 1377166.3064404274 0, -1128445.5661708254 1376759.7983549957 0, -1128749.6406870573 1376822.4775944548 0, -1128821.7536744415 1376837.34235038 0, -1128821.7536768704 1376837.3423508808 0, -1128989.9337826155 1376872.0186683617 0, -1129197.9385976936 1376914.906293252 0, -1129583.9323733568 1376989.0503674888 0, -1129864.5582041873 1377042.970132364 0, -1129969.923935293 1377063.21524373 0, -1129969.923937703 1377063.2152440413 0, -1129923.1689375208 1377456.5381096725 0, -1129876.3925645563 1377849.8671347466 0, -1129829.631616595 1378243.1996696473 0, -1129782.8699666883 1378636.5336530393 0, -1129397.162708549 1378573.8433946485 0, -1129011.4546921998 1378511.150635521 0, -1128625.7407553326 1378448.495060322 0, -1128240.0266006347 1378385.842705121 0)), ((-1135595.559496878 1377811.9031924587 0, -1135887.6696735772 1377852.1807593098 0, -1135887.6696980635 1377852.180762686 0, -1136279.8713540055 1377906.2775453748 0, -1136241.722985257 1378299.5766089533 0, -1136203.5903955773 1378692.859858292 0, -1136165.437431932 1379086.1621313123 0, -1136127.3019961263 1379479.448013669 0, -1135730.8287856497 1379431.1010282724 0, -1135334.3670495097 1379382.7946452815 0, -1134937.9059860434 1379334.4865309978 0, -1134541.4267154012 1379286.1947030055 0, -1134583.8463221386 1378887.1427064238 0, -1134626.2484252655 1378488.0900345193 0, -1134668.6494565508 1378089.0386769765 0, -1134711.052073863 1377689.9950650113 0, -1134711.988625318 1377690.1241135423 0, -1134711.9886247334 1377690.1241176976 0, -1135103.26140334 1377744.038139601 0, -1135103.2615086911 1377744.0381541231 0, -1135390.6623790655 1377783.655098396 0, -1135495.4654497516 1377798.101772217 0, -1135595.559496878 1377811.9031924587 0)), ((-1134091.870668225 1379633.0829632925 0, -1134142.6328566815 1379228.2713369778 0, -1134541.4267154012 1379286.1947030055 0, -1134490.9373794342 1379691.1645645178 0, -1134440.431316512 1380096.1338175663 0, -1134041.107967413 1380037.896151915 0, -1134091.870668225 1379633.0829632925 0)), ((-1133641.7843699907 1379979.6572193601 0, -1134041.107967413 1380037.896151915 0, -1133990.350244433 1380442.6709463447 0, -1133590.7537812414 1380384.2738787679 0, -1133641.7843699907 1379979.6572193601 0)), ((-1133914.8617393444 1384123.1434420596 0, -1133518.0546113998 1384067.3718153553 0, -1133121.2474062436 1384011.598521716 0, -1132724.43745024 1383955.843850081 0, -1132327.6384421403 1383900.1296666614 0, -1132380.1294119284 1383497.7645706153 0, -1132432.6175352833 1383095.4208360729 0, -1132485.124200542 1382693.060849111 0, -1132537.614331775 1382290.7002605456 0, -1132937.4076582661 1382345.7752826675 0, -1133337.2009549243 1382400.8490701108 0, -1133736.9888489267 1382455.9613874163 0, -1134136.7902785065 1382511.0946259433 0, -1134081.3054377616 1382914.094062059 0, -1134025.8178849416 1383317.114801045 0, -1133970.349285169 1383720.1194558472 0, -1133914.8617393444 1384123.1434420596 0)), ((-1129911.9617069426 1386914.4819080972 0, -1129531.3123497304 1386858.238160551 0, -1129150.6577348115 1386802.011203176 0, -1128770.0029034042 1386745.8014204486 0, -1128810.18117793 1386343.5014383916 0, -1128851.8116658041 1385926.8742460005 0, -1128893.5163361796 1385510.2992053425 0, -1128935.235608927 1385093.7277662717 0, -1129330.3991150372 1385149.765814424 0, -1129725.5760493914 1385205.8242323347 0, -1130118.2504813895 1385276.1945416632 0, -1130510.919103605 1385346.603010369 0, -1130455.6097842276 1385758.0277571783 0, -1130400.3003183224 1386169.4539493052 0, -1130345.0253977205 1386580.7442335933 0, -1130292.6112126154 1386970.7462049725 0, -1129911.9617069426 1386914.4819080972 0)), ((-1131694.5584177857 1403154.8460936155 0, -1131674.7643498778 1403327.0536281727 0, -1131674.7633971802 1403327.0619166011 0, -1131629.6108235891 1403719.8596693594 0, -1131233.8760388307 1403659.806582935 0, -1130838.132058296 1403599.7711531953 0, -1130442.38485147 1403539.7539864825 0, -1130046.6507314045 1403479.7572590564 0, -1130091.02808195 1403079.3536275472 0, -1130135.4042871143 1402678.9512385186 0, -1130190.2168448102 1402276.9270303233 0, -1130245.0428887089 1401874.9263128457 0, -1130636.3358691412 1401943.3328004412 0, -1131027.6410377992 1402011.759481511 0, -1131418.9261743415 1402080.2019411225 0, -1131810.2073915359 1402148.6623356345 0, -1131765.056338869 1402541.4644241468 0, -1131719.9044020802 1402934.2678488703 0, -1131694.5584177857 1403154.8460936155 0)), ((-1131629.6108235905 1403719.8596693596 0, -1131674.7634721666 1403327.0620394223 0, -1131674.7644374084 1403327.0536418608 0, -1131694.2720732396 1403157.3380614424 0, -1131674.7704569306 1403327.0545832047 0, -1131629.6168607788 1403719.860585508 0, -1131629.6108235905 1403719.8596693596 0)), ((-1130470.0476174715 1411622.0767788892 0, -1130471.3870147462 1411612.0801684652 0, -1130471.3875700883 1411612.0760384062 0, -1130471.3881286476 1411612.0761204213 0, -1130422.6596337657 1411975.7695378698 0, -1130417.698511745 1412012.7793159194 0, -1130379.3193196955 1412299.1391630087 0, -1130417.692801543 1412012.7784684966 0, -1130379.3185861527 1412299.1446362145 0, -1130368.8478305305 1412377.2704074662 0, -1130367.705419441 1412385.6771458772 0, -1130363.9256571524 1412413.452444389 0, -1130363.92492276 1412413.4578410152 0, -1130316.2237182234 1412778.9640306754 0, -1130363.9250123813 1412413.45785291 0, -1130363.9257465557 1412413.4524577858 0, -1130367.6899678416 1412385.7908506168 0, -1130363.9308639802 1412413.4532246208 0, -1130316.2242222133 1412778.9710565119 0, -1130311.715413668 1412813.5625438425 0, -1130271.0147584558 1413125.3791732949 0, -1130311.7080710516 1412813.5614359821 0, -1130311.708304903 1412813.5596440658 0, -1130311.7080710505 1412813.561435982 0, -1130298.939608259 1412911.4009462243 0, -1130270.5494316898 1413128.9441435148 0, -1130263.7966130837 1413180.6789651318 0, -1130263.1874864711 1413185.2859392043 0, -1130259.4305079263 1413213.6435761505 0, -1129843.5671898066 1413150.4769921284 0, -1129427.6928954879 1413087.329438535 0, -1129011.8339981886 1413024.1843259658 0, -1128595.9555229982 1412961.0574279884 0, -1128666.7902152468 1412565.3853512001 0, -1128737.6424725812 1412169.71695834 0, -1128808.480147453 1411774.0481500102 0, -1128879.319372785 1411378.380882504 0, -1129277.335666687 1411436.7863361777 0, -1129675.367770541 1411495.1924299735 0, -1130073.3781521877 1411553.6350381465 0, -1130471.387480631 1411612.0760252709 0, -1130471.3869251222 1411612.0801565703 0, -1130422.6513729764 1411975.778441062 0, -1130417.6934915904 1412012.7733190442 0, -1130422.651447872 1411975.7785638876 0, -1130470.0476174715 1411622.0767788892 0)), ((-1130263.1423691805 1413185.627172347 0, -1130259.4379366827 1413213.644704524 0, -1130259.4305973367 1413213.6435897313 0, -1130263.1423691805 1413185.627172347 0)), ((-1128199.4941676722 1388258.092569399 0, -1127813.8064076349 1388197.2454368593 0, -1127428.1181161546 1388136.3956955457 0, -1127042.4150374373 1388075.5793239689 0, -1127092.549571546 1387674.5276768932 0, -1127142.683761955 1387273.4774474546 0, -1127192.8150246062 1386872.4285907475 0, -1127242.9482214623 1386471.3812725784 0, -1127612.3575455945 1386550.9617211486 0, -1127981.7620197614 1386630.5581261318 0, -1128375.8853373388 1386688.1692564106 0, -1128770.0029034042 1386745.8014204486 0, -1128723.7931344162 1387139.0964353874 0, -1128677.5899458732 1387532.3753459016 0, -1128631.3833221574 1387925.67554847 0, -1128585.1787404602 1388318.9571824968 0, -1128199.4941676722 1388258.092569399 0)), ((-1128902.256667591 1394855.7506675306 0, -1129301.3881760822 1394893.8064189097 0, -1129240.6210568582 1395348.951187639 0, -1129179.8674093112 1395804.119944101 0, -1129145.4072263225 1396173.6745128701 0, -1129110.945593145 1396543.2301865914 0, -1128716.8824294384 1396492.5587382494 0, -1128324.7787728661 1396442.1240041174 0, -1127932.6122955997 1396389.180351191 0, -1127541.496440933 1396336.3737075853 0, -1127586.3635830584 1395936.8323112822 0, -1127631.2459652512 1395537.294464622 0, -1127668.0067557807 1395140.2193864277 0, -1127704.7658234667 1394743.1455489877 0, -1128103.9459806434 1394780.420277149 0, -1128503.1385945815 1394817.735617346 0, -1128902.256667591 1394855.7506675306 0)), ((-1127493.076462513 1397209.5182006557 0, -1127423.921724395 1397604.818929388 0, -1127354.7683083252 1398000.1213105617 0, -1126989.1006696948 1397948.6614400165 0, -1126623.4495540212 1397897.199336939 0, -1126257.793353734 1397845.7729081265 0, -1125892.132160036 1397794.352604225 0, -1125933.612666578 1397396.8683351292 0, -1125975.092380122 1396999.382184817 0, -1126016.570586621 1396601.9004633154 0, -1126058.0474899095 1396204.4200535296 0, -1126366.48689195 1396246.6194582006 0, -1126451.3593452626 1396258.2303121325 0, -1126738.3557137987 1396297.5093653526 0, -1126844.7242997878 1396311.6365292708 0, -1127135.451325891 1396351.6820569288 0, -1127238.0332831962 1396365.505238777 0, -1127532.5461209563 1396405.8579272463 0, -1127631.4018461602 1396418.9207291915 0, -1127562.2326115884 1396814.2192355755 0, -1127493.076462513 1397209.5182006557 0)), ((-1127208.5940730576 1406269.8185887574 0, -1126810.7331826407 1406208.0119500705 0, -1126412.8668680415 1406146.2205139736 0, -1126471.18721819 1405743.5383591235 0, -1126529.5671999634 1405340.4486460553 0, -1126592.1225184647 1404936.3481409336 0, -1126654.6785942863 1404532.2490064232 0, -1127054.162652761 1404619.2846886918 0, -1127453.6544733664 1404706.3609974007 0, -1127853.127288661 1404793.4338540144 0, -1128252.5926652716 1404880.5449631338 0, -1128186.447389112 1405249.7336289717 0, -1128120.3060441387 1405618.903758814 0, -1128062.533436392 1406004.9067246353 0, -1128004.306815114 1406393.4900116608 0, -1127606.4515062582 1406331.6467938172 0, -1127208.5940730576 1406269.8185887574 0)), ((-1125845.4282341187 1371936.845910621 0, -1125793.15533219 1372343.1998504114 0, -1125740.9008406678 1372749.536772335 0, -1125688.6270627417 1373155.892008587 0, -1125290.0192406122 1373103.928756387 0, -1124891.4089248725 1373051.984023202 0, -1124492.8097970292 1373000.079876511 0, -1124094.194676932 1372948.1724022934 0, -1124150.9520465452 1372541.6143547052 0, -1124207.7067449703 1372135.077067238 0, -1124264.4641428345 1371728.520775997 0, -1124321.2027708457 1371321.9838986052 0, -1124715.3335886346 1371374.094588449 0, -1124969.197274951 1371407.6584505804 0, -1125109.4613311233 1371426.2084159509 0, -1125109.4640081115 1371426.2087701303 0, -1125503.583424903 1371478.3528167694 0, -1125503.5902477072 1371478.353719727 0, -1125739.166247116 1371509.5308019777 0, -1125897.698146327 1371530.5136803943 0, -1125845.4282341187 1371936.845910621 0)), ((-1126220.619844299 1378132.9269923076 0, -1125821.5358651546 1378081.5561233014 0, -1125423.0038183618 1378030.5003883932 0, -1125024.4667478797 1377979.4830556442 0, -1125077.1341659254 1377574.7647088985 0, -1125129.7851389097 1377170.04569603 0, -1125182.435765012 1376765.328378942 0, -1125583.377213075 1376815.6668737624 0, -1125636.8485578434 1376410.6540712777 0, -1126038.603509141 1376460.7117040104 0, -1126440.3532680192 1376510.790946046 0, -1126842.1032454043 1376560.8893832208 0, -1126786.5091987266 1376966.7358099273 0, -1126730.9103575198 1377372.6084336329 0, -1126675.2978345868 1377778.4605466411 0, -1126619.6988799425 1378184.3363719773 0, -1126220.619844299 1378132.9269923076 0)), ((-1125545.3371591107 1387083.0203807312 0, -1125544.729486463 1387087.6319533226 0, -1125492.6124915709 1387483.9288486124 0, -1125439.8876767652 1387884.8388722134 0, -1125063.804140553 1387838.0170659635 0, -1124687.737427861 1387791.1938643027 0, -1124311.666115539 1387744.4072896393 0, -1123935.5767421848 1387697.6350934738 0, -1123970.1022329344 1387296.5240704399 0, -1124004.606926887 1386895.4321212138 0, -1124039.1123274586 1386494.3214349453 0, -1124073.6319960393 1386093.2142716632 0, -1124467.9235235755 1386140.185400604 0, -1124862.2128556487 1386187.174632246 0, -1125256.5003753917 1386234.182104476 0, -1125650.7858936845 1386281.2076976425 0, -1125598.0616001636 1386682.1132599206 0, -1125545.3371591107 1387083.0203807312 0)), ((-1126361.9101554158 1406535.9827642022 0, -1126310.9572366572 1406925.7566291431 0, -1126260.0041376273 1407315.5318047248 0, -1126209.0533922075 1407705.2883876492 0, -1125807.5534071801 1407655.5281003006 0, -1125406.0351721765 1407605.784495414 0, -1125004.5335496573 1407556.041992541 0, -1124603.0129532327 1407506.3379697264 0, -1124655.2105047817 1407104.6738516432 0, -1124707.4050813988 1406703.0107462956 0, -1124764.304567047 1406301.1705137906 0, -1124821.204543008 1405899.3287299788 0, -1125219.12483808 1405961.0261111686 0, -1125617.0420723448 1406022.7390251865 0, -1126014.9561486228 1406084.4704992943 0, -1126412.8668680415 1406146.2205139736 0, -1126361.9101554158 1406535.9827642022 0)), ((-1126103.52059037 1414251.3650786027 0, -1126495.1129209618 1414309.6826994368 0, -1126886.689042538 1414367.9960305768 0, -1126836.1631484919 1414763.176372017 0, -1126785.6206852472 1415158.3559435843 0, -1126392.2930198866 1415104.2599242062 0, -1125998.9816615938 1415050.1641830564 0, -1126051.243126521 1414650.7629280959 0, -1126103.52059037 1414251.3650786027 0)), ((-1125368.1904321758 1414963.4195661335 0, -1125368.190386117 1414963.4194649837 0, -1125605.0092473277 1414995.9792691455 0, -1125552.1970623517 1415397.9503565687 0, -1125499.2574982783 1415800.8047305925 0, -1125486.16671321 1415799.043438584 0, -1125486.1667134678 1415799.0434365747 0, -1125104.735172474 1415747.7238937775 0, -1125122.286096165 1415614.6927755333 0, -1125122.2859603993 1415614.6927563478 0, -1125157.8990082943 1415344.756810457 0, -1125211.0502907436 1414941.8147104 0, -1125240.9989922796 1414945.9322766422 0, -1125240.9989986802 1414945.9322930144 0, -1125368.1904321758 1414963.4195661335 0)), ((-1124488.4534969144 1375863.9466505046 0, -1124545.9164180295 1375465.2077496115 0, -1124945.8408690132 1375515.3136150604 0, -1125345.7819611502 1375565.4205175303 0, -1125290.4420950527 1375963.0168664292 0, -1125235.0942204224 1376360.6126358563 0, -1124833.184652902 1376310.6326070586 0, -1124431.2708092097 1376260.6679009446 0, -1124488.4534969144 1375863.9466505046 0)), ((-1123244.3993556977 1382689.5563968648 0, -1122851.6047364774 1382637.9446412507 0, -1122894.7821541948 1382232.3261767775 0, -1122937.958270201 1381826.7093334198 0, -1122981.1170945005 1381421.0916619352 0, -1123024.29095105 1381015.4775920846 0, -1123417.2579000075 1381065.0995536167 0, -1123810.2225495384 1381114.7396071162 0, -1124205.8333911672 1381165.8018399097 0, -1124601.4255426365 1381216.8804861498 0, -1124556.7575178389 1381623.7622372766 0, -1124512.1020188408 1382030.6674087287 0, -1124467.4292292793 1382437.5719731501 0, -1124422.7716010276 1382844.4800661337 0, -1124029.9841118657 1382792.8141149967 0, -1123637.1915669353 1382741.1862149024 0, -1123244.3993556977 1382689.5563968648 0)), ((-1123506.280545221 1397523.807386724 0, -1123113.546769394 1397477.8898072825 0, -1122720.8137690278 1397431.9702237793 0, -1122763.109827633 1397024.0858502928 0, -1122805.4073543407 1396616.1829707017 0, -1122847.7008853767 1396208.3013505863 0, -1122889.9958938463 1395800.401127108 0, -1123189.3111801764 1395840.1973796408 0, -1123290.6333705958 1395853.6759272644 0, -1123592.4170097834 1395893.8317720902 0, -1123691.2390760726 1395907.0673611416 0, -1123995.590683897 1395947.575784164 0, -1124091.8688309146 1395960.3997998708 0, -1124398.7883693685 1396001.2610068868 0, -1124492.488340714 1396013.8107537832 0, -1124442.2964177344 1396414.2945269318 0, -1124392.106770431 1396814.7598914225 0, -1124341.9167850271 1397215.22653639 0, -1124291.7262449125 1397615.6946420253 0, -1123898.9962280719 1397569.7408873076 0, -1123506.280545221 1397523.807386724 0)), ((-1125050.7333485072 1416089.8860668119 0, -1125041.8281434458 1416146.347519247 0, -1124978.9282343488 1416544.9784228264 0, -1124916.0316808743 1416943.5908303708 0, -1124853.1493242446 1417342.2267834733 0, -1124457.9174930924 1417298.9261537998 0, -1124062.6679361095 1417255.6417318368 0, -1123667.4356306635 1417212.357741493 0, -1123272.2015044442 1417169.1221639696 0, -1123272.2015071386 1417169.1221471285 0, -1123337.6065180777 1416760.321508964 0, -1123337.6065258821 1416760.321460184 0, -1123403.0153526028 1416351.5196232654 0, -1123403.0153590597 1416351.5195829112 0, -1123468.4250636017 1415942.7194489401 0, -1123468.4250693142 1415942.7194132379 0, -1123473.747317706 1415909.4555252187 0, -1123533.8327863354 1415533.9235664124 0, -1123926.56349187 1415587.3460286171 0, -1124319.2892320438 1415640.786062571 0, -1124712.0120305463 1415694.2474056818 0, -1125104.735172474 1415747.7238937775 0, -1125089.1809641218 1415846.2507992552 0, -1125069.5971794683 1415970.357194465 0, -1125050.7333485072 1416089.8860668119 0)), ((-1122019.1521206042 1375956.1699800775 0, -1121618.804655642 1375905.4827582964 0, -1121218.457656987 1375854.811407748 0, -1120841.116851507 1375802.8648016313 0, -1120463.7737590438 1375750.9349210237 0, -1120516.200899676 1375355.6310267446 0, -1120569.7512673917 1374952.2348903345 0, -1120625.6667781945 1374547.7692953877 0, -1120681.5959395962 1374143.3273205212 0, -1121074.12740433 1374194.9156548358 0, -1121466.6566759371 1374246.5220041089 0, -1121859.183348471 1374298.146430173 0, -1122251.7077260332 1374349.788860836 0, -1122191.2815362918 1374752.3813441172 0, -1122130.839695816 1375154.9734927684 0, -1122074.7236576332 1375557.3833075035 0, -1122019.1521206042 1375956.1699800775 0)), ((-1123376.9303048812 1391741.2576516299 0, -1123314.5698582318 1392137.5653234327 0, -1123252.1940557153 1392533.8726081797 0, -1122851.979595349 1392490.8314365125 0, -1122451.7663102946 1392447.7890737671 0, -1122051.548718278 1392404.7854837133 0, -1121651.3323146391 1392361.7806028118 0, -1121722.701105602 1391969.9432715562 0, -1121794.0714790968 1391578.1077279423 0, -1121865.4435533658 1391186.2737822745 0, -1121936.8172005732 1390794.44172734 0, -1122328.038850107 1390832.9778433996 0, -1122719.2619607688 1390871.511682969 0, -1123110.4650883302 1390910.0814708392 0, -1123501.685879371 1390948.6512496257 0, -1123439.307756312 1391344.953618665 0, -1123376.9303048812 1391741.2576516299 0)), ((-1121290.518223922 1402189.6028911723 0, -1120898.946553349 1402139.7069227165 0, -1120507.3727919913 1402089.8290760154 0, -1120560.475735779 1401673.8246992396 0, -1120613.578409893 1401257.821800938 0, -1120666.6832297882 1400841.8006717367 0, -1120719.7852362166 1400425.8010265727 0, -1121110.7986750705 1400489.7828177535 0, -1121501.8087625043 1400553.782531097 0, -1121892.8339492006 1400617.7824019396 0, -1122283.8369248898 1400681.8180203056 0, -1122231.280922139 1401083.7118800778 0, -1122178.7382479333 1401485.6293996815 0, -1122126.1978938389 1401887.5282161443 0, -1122073.6572772407 1402289.4287313183 0, -1121682.0875257791 1402239.5167519285 0, -1121290.518223922 1402189.6028911723 0)), ((-1123193.293392606 1406083.5382776444 0, -1123144.6723689795 1406491.0077775405 0, -1123096.0344954468 1406898.476659974 0, -1123047.4120210616 1407305.9490347523 0, -1122641.1381050788 1407241.9584489563 0, -1122234.8580531853 1407178.007303228 0, -1121838.8895895265 1407124.5338010213 0, -1121442.932036701 1407071.1008011792 0, -1121497.408968595 1406668.462640541 0, -1121551.9021824973 1406265.8281743904 0, -1121606.3951982583 1405863.194909579 0, -1121660.8756521624 1405460.5743139726 0, -1122056.1404709648 1405514.4236066951 0, -1122451.402855788 1405568.2909629247 0, -1122846.662549228 1405622.1769650364 0, -1123241.9222513768 1405676.081467265 0, -1123193.293392606 1406083.5382776444 0)), ((-1120370.8519903524 1376558.8173142108 0, -1120318.5523466591 1376963.4801781676 0, -1120266.2522479899 1377368.1446207205 0, -1119880.8900891547 1377319.3201747807 0, -1119495.5121968861 1377270.4908559385 0, -1119110.1457082026 1377221.7010819372 0, -1118724.7796867318 1377172.9088053552 0, -1118778.2443194068 1376768.5999457866 0, -1118831.725020293 1376364.2947682526 0, -1118884.8882999346 1375959.6451455804 0, -1118938.0538767064 1375554.9872533744 0, -1119319.4882878212 1375603.949662015 0, -1119700.917847579 1375652.9285817863 0, -1120082.3483423563 1375701.9218368852 0, -1120463.7737590438 1375750.9349210237 0, -1120417.3068957361 1376154.8728294435 0, -1120370.8519903524 1376558.8173142108 0)), ((-1120491.9494602073 1385624.6256410768 0, -1120093.763575009 1385573.8576330252 0, -1119695.5940897868 1385523.0902777323 0, -1119297.4198083158 1385472.3613170802 0, -1119340.9472703985 1385061.9468487294 0, -1119384.0188619152 1384655.7591478426 0, -1119427.0704806547 1384249.5909008489 0, -1119470.1371432533 1383843.4260441957 0, -1119868.8971800464 1383892.909579033 0, -1120267.6523941972 1383942.4318258371 0, -1120666.4080914243 1383991.9526028684 0, -1121065.1589723115 1384041.511990617 0, -1121021.4782800283 1384449.263482045 0, -1120977.7938667354 1384857.036411433 0, -1120934.1213892677 1385264.7109163136 0, -1120890.1143988897 1385675.4301850495 0, -1120491.9494602073 1385624.6256410768 0)), ((-1119210.4431516875 1395311.3163535972 0, -1118934.7090922128 1395276.3787889068 0, -1118813.6356889023 1395261.0540254316 0, -1118539.2900616706 1395226.3112991361 0, -1118416.728878138 1395210.7972705083 0, -1118143.8849135807 1395176.264417947 0, -1118098.301202479 1395578.1417531045 0, -1118052.7300718888 1395980.0426425133 0, -1118014.0373714229 1396382.7649197942 0, -1117975.3431394938 1396785.4885941045 0, -1117571.6254414623 1396735.1006511487 0, -1117167.8919210657 1396684.7097284375 0, -1116764.1535303488 1396634.3577780328 0, -1116360.421244751 1396584.0230776295 0, -1116412.5612726118 1396182.507904486 0, -1116464.7032912923 1395780.9975934473 0, -1116516.842493938 1395379.4883429958 0, -1116568.9815043674 1394977.9808117792 0, -1116834.5780802164 1395011.4059938502 0, -1116962.7155866746 1395027.5252937344 0, -1117229.599019029 1395061.1176071411 0, -1117356.4427145289 1395077.0734968886 0, -1117624.6985429188 1395110.858177675 0, -1117750.1649038973 1395126.6599330301 0, -1118019.812084375 1395160.6190671015 0, -1118103.80581375 1394719.2757708228 0, -1118179.194871264 1394323.174766747 0, -1118254.6177017856 1393926.957919362 0, -1118330.045173897 1393530.7230543261 0, -1118723.858239953 1393579.8287040037 0, -1119117.6529882865 1393628.9504550146 0, -1119511.4457410742 1393678.0903830659 0, -1119905.2362008188 1393727.2484592765 0, -1119832.7602143239 1394124.2319429151 0, -1119760.2884778217 1394521.1972540407 0, -1119688.0464158494 1394917.9302005172 0, -1119607.2322423405 1395361.5950784427 0, -1119330.109592792 1395326.462352874 0, -1119210.4431516875 1395311.3163535972 0)), ((-1120017.2218312682 1411823.245533616 0, -1119624.4961145993 1411764.1988645403 0, -1119231.7673409404 1411705.1704383884 0, -1119272.5596525783 1411301.4272396904 0, -1119313.366888842 1410897.6874931958 0, -1119354.1727376643 1410493.9490263194 0, -1119394.9610742857 1410090.209785507 0, -1119798.6280583078 1410143.523002227 0, -1120202.3085699002 1410196.8576489014 0, -1120592.3456760987 1410247.2185010735 0, -1120982.3778819165 1410297.6172102676 0, -1120937.463806247 1410708.5557827086 0, -1120892.5298556273 1411119.5134683042 0, -1120847.597506007 1411530.4526423176 0, -1120802.664136076 1411941.3930969462 0, -1120409.9445088701 1411882.3102444937 0, -1120017.2218312682 1411823.245533616 0)), ((-1118611.105025861 1366097.0532489782 0, -1118558.8563670083 1366495.3897124978 0, -1118506.5913973786 1366893.7255140257 0, -1118454.342544761 1367292.0650934004 0, -1118055.342904511 1367241.9869817195 0, -1117656.3274022678 1367191.9055899843 0, -1117257.3233436814 1367141.8646434117 0, -1116858.317118064 1367091.842385068 0, -1116909.8833289621 1366688.2974139208 0, -1116961.4466174536 1366284.7739470403 0, -1117013.028493065 1365881.2341799582 0, -1117064.5933234126 1365477.7085871068 0, -1117075.2175828249 1365479.176522235 0, -1117135.5558840279 1365487.5133749652 0, -1117464.2869575792 1365532.9336654537 0, -1117464.287008481 1365532.9336724868 0, -1117863.9807288654 1365588.1746178728 0, -1117863.9807545831 1365588.1746214286 0, -1118263.6688977159 1365643.436894331 0, -1118263.668992807 1365643.4369074786 0, -1118663.35432386 1365698.7180505735 0, -1118663.3544092162 1365698.7180587589 0, -1118611.105025861 1366097.0532489782 0)), ((-1117189.2932919015 1376550.2051515838 0, -1117110.5151065283 1376963.1067198256 0, -1116711.3172738892 1376914.2650301782 0, -1116312.1172849792 1376865.4419970491 0, -1115913.7940967216 1376819.3715731637 0, -1115515.4527668075 1376773.3175712095 0, -1115594.3383009331 1376364.5472763253 0, -1115673.22600663 1375955.7790357363 0, -1115752.1158840456 1375547.0128510601 0, -1115830.9958592872 1375138.2581894842 0, -1116230.3826382225 1375167.540709523 0, -1116629.771235196 1375196.845431583 0, -1117027.7077151476 1375254.1685232958 0, -1117425.6443661659 1375311.5073099232 0, -1117346.8560745905 1375724.4080506726 0, -1117268.0734960402 1376137.3054482758 0, -1117189.2932919015 1376550.2051515838 0)), ((-1119185.7792514544 1379685.700942679 0, -1118795.3851939102 1379641.9387300296 0, -1118404.9948042564 1379598.1545219317 0, -1118457.930092059 1379194.11211182 0, -1118847.614990889 1379237.0121130517 0, -1119237.2981003602 1379279.9298840172 0, -1119185.7792514544 1379685.700942679 0)), ((-1117018.5340397567 1381042.8103848211 0, -1117424.2646438633 1381103.0848327184 0, -1117359.230112336 1381497.4307794517 0, -1116947.939467744 1381431.840926394 0, -1117018.5340397567 1381042.8103848211 0)), ((-1119114.1912407677 1387078.1539595884 0, -1118710.407157063 1387028.6169571707 0, -1118306.604704382 1386979.0970227346 0, -1117909.6519800108 1386930.4317708092 0, -1117512.6855504394 1386881.7739938835 0, -1117560.7465247782 1386476.8190029685 0, -1117608.8088853294 1386071.8688412127 0, -1117661.7650544855 1385668.1432982194 0, -1117714.7240180697 1385264.416576316 0, -1118110.004116254 1385315.5522046068 0, -1118505.2923531365 1385366.6999264034 0, -1118901.3505172192 1385419.5103644102 0, -1119297.4198083158 1385472.3613170802 0, -1119251.6098520532 1385873.806871388 0, -1119205.7991053527 1386275.2537726094 0, -1119160.0036859268 1386676.704177705 0, -1119114.1912407677 1387078.1539595884 0)), ((-1118662.111614961 1403452.7498157609 0, -1118622.5437863856 1403851.4642660618 0, -1118582.988124498 1404250.2019398885 0, -1118543.3936028015 1404648.9767631488 0, -1118504.1986571378 1405043.711665212 0, -1118107.2315810733 1404991.00743132 0, -1117710.2595882423 1404938.3213404317 0, -1117314.118173709 1404884.6910027026 0, -1116917.974310593 1404831.079037254 0, -1116968.1458393948 1404429.49774891 0, -1117018.3326361047 1404027.9085850802 0, -1117409.4293773554 1404083.4659481624 0, -1117457.4441982775 1403681.7967623856 0, -1117069.1176739975 1403625.262035704 0, -1117119.9049988 1403222.596860389 0, -1117505.460982016 1403280.108995511 0, -1117891.0140504884 1403337.638496846 0, -1118276.5643013476 1403395.1853733838 0, -1118662.111614961 1403452.7498157609 0)), ((-1117317.8398769652 1413916.8720055358 0, -1116923.3634524494 1413865.2644651786 0, -1116528.8872638717 1413813.655073302 0, -1116134.1073801508 1413761.9838715512 0, -1115739.3252709561 1413710.3310343996 0, -1115793.013311971 1413309.2076450454 0, -1115846.698637258 1412908.105927389 0, -1116240.9136658087 1412960.6188934338 0, -1116635.1423940116 1413013.152255771 0, -1117029.3523837791 1413065.701785874 0, -1117423.576168497 1413118.2717208778 0, -1117370.708093865 1413517.5712385045 0, -1117317.8398769652 1413916.8720055358 0)), ((-1115833.3656671576 1371877.5591570935 0, -1115438.1144834477 1371822.8658539534 0, -1115042.8580346717 1371768.2107182206 0, -1114647.6151953572 1371713.5758303313 0, -1114697.086335208 1371310.857357119 0, -1114746.571046667 1370908.1615354095 0, -1114796.0390933577 1370505.4645013174 0, -1114845.5092699367 1370102.7491386028 0, -1115238.3381507492 1370154.3479434708 0, -1115631.150968839 1370205.9427950433 0, -1116023.9587798512 1370257.5755494772 0, -1116416.7830804472 1370309.208498443 0, -1116369.7268699668 1370714.9603258774 0, -1116322.6863069464 1371120.7155747996 0, -1116275.6424492747 1371526.4918530076 0, -1116228.60063545 1371932.2486794905 0, -1115833.3656671576 1371877.5591570935 0)), ((-1116022.7089924891 1385406.5962572389 0, -1115959.67820087 1385778.5180585426 0, -1115896.664561576 1386150.443591691 0, -1115833.635848409 1386522.3684386956 0, -1115430.3606568763 1386471.797216954 0, -1115027.066937816 1386421.2427379764 0, -1114623.784562455 1386370.729539384 0, -1114220.4862765665 1386320.2133935723 0, -1114289.7072830496 1385949.722949249 0, -1114358.9325702668 1385579.2142781625 0, -1114428.1756430103 1385208.709230789 0, -1114497.3952443714 1384838.2174034084 0, -1114894.47970747 1384887.3075657897 0, -1115291.5624348433 1384936.413244068 0, -1115688.6428555646 1384985.5372174808 0, -1116085.7232992365 1385034.683151742 0, -1116022.7089924891 1385406.5962572389 0)), ((-1116860.3005500005 1405229.2839743113 0, -1116802.6426363084 1405627.4815285993 0, -1116744.9689811217 1406025.6781803533 0, -1116687.2955526991 1406423.876576 0, -1116294.1719715425 1406377.3754102292 0, -1115901.0489499893 1406330.8725825709 0, -1115507.9052103704 1406284.4057358704 0, -1115114.782160014 1406237.9370352374 0, -1115168.7230674485 1405835.956606664 0, -1115222.6637482992 1405433.977365807 0, -1115276.6022960509 1405031.996397434 0, -1115330.5430566077 1404630.020194993 0, -1115727.0331075906 1404679.6123850017 0, -1116123.523107197 1404729.2262405918 0, -1116520.7499910598 1404780.143296488 0, -1116917.974310593 1404831.079037254 0, -1116860.3005500005 1405229.2839743113 0)), ((-1115633.1418777418 1414505.1746285215 0, -1115685.6684730274 1414111.967563779 0, -1116080.7040769043 1414163.0441810472 0, -1116475.7400876503 1414214.119270351 0, -1116423.3384940496 1414608.9762151756 0, -1116028.2414423139 1414557.0663104777 0, -1115741.168306802 1414519.3626365417 0, -1115633.141902626 1414505.1746318107 0, -1115633.1418777418 1414505.1746285215 0)), ((-1114994.5155381316 1380791.8029875185 0, -1114912.8396462698 1381180.7940371966 0, -1114831.1664392145 1381569.7870667868 0, -1114425.432657003 1381512.7190591858 0, -1114019.6797628058 1381455.6681342002 0, -1113612.9360044668 1381397.8783298861 0, -1113206.1892360575 1381340.1078665403 0, -1113294.535637208 1380948.2215568393 0, -1113382.8851522834 1380556.33743563 0, -1113471.221573711 1380164.4532357715 0, -1113559.5774453334 1379772.57320461 0, -1113959.1579454546 1379832.848510015 0, -1114358.73257916 1379893.1624846621 0, -1114758.3066317681 1379953.4751462238 0, -1115157.8775567808 1380013.8064945654 0, -1115076.1964821767 1380402.793699327 0, -1114994.5155381316 1380791.8029875185 0)), ((-1113724.2650150552 1390913.7943994924 0, -1113681.2784560448 1391315.728650421 0, -1113283.1984357322 1391260.3218896058 0, -1112885.1130982367 1391204.9537267606 0, -1112487.0275419522 1391149.5840573346 0, -1112088.9392055061 1391094.233084737 0, -1112131.393906547 1390689.6118045177 0, -1112173.8609604845 1390285.0140644608 0, -1112216.3296320504 1389880.3977322194 0, -1112258.7808553192 1389475.7807164525 0, -1112657.404122839 1389533.7986590758 0, -1113056.0243928742 1389591.8352707692 0, -1113454.6254375621 1389649.8884842056 0, -1113853.2398258522 1389707.962241377 0, -1113810.2564457653 1390109.8923346056 0, -1113767.269297699 1390511.8438013617 0, -1113724.2650150552 1390913.7943994924 0)), ((-1114854.4823440555 1394754.0659244068 0, -1114988.1133118349 1394771.7419968795 0, -1114935.9763585539 1395176.9893065458 0, -1114883.8420186962 1395582.213722154 0, -1114490.2072317007 1395529.8639128143 0, -1114096.5563731056 1395477.5101458756 0, -1114041.8714879374 1395882.0374893171 0, -1113647.0157602965 1395829.3622528506 0, -1113252.1761896233 1395776.6873727671 0, -1113309.4276504589 1395372.8603975344 0, -1113366.7005648857 1394968.99718064 0, -1113423.9624049892 1394565.1516942214 0, -1113679.838309738 1394598.9463572563 0, -1113814.9614845193 1394616.7950241456 0, -1114071.3347776176 1394650.6663991376 0, -1114205.9527542805 1394668.4776072593 0, -1114462.9051152733 1394702.383234385 0, -1114597.0377418634 1394720.0839761526 0, -1114854.4823440555 1394754.0659244068 0)), ((-1112361.6383310102 1405880.9739550042 0, -1111968.8366323074 1405830.8988658648 0, -1112021.4546696176 1405427.5697413757 0, -1112074.088564408 1405024.2441567262 0, -1112126.7222990901 1404620.9199674067 0, -11121</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Surface, Subsurface</t>
+          <t>Subsurface, Surface</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -2706,7 +2706,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-74418.87006271395 1467480.1590942924 0, -74416.04098262447 1467880.0422387214 0, -74413.22075045682 1468279.9265030606 0, -74014.15315680247 1468277.319849597 0, -73615.09452486291 1468274.7209222964 0, -73216.0267285189 1468272.151969932 0, -73220.86382510237 1467870.3480019812 0, -73225.6920834597 1467468.5561065474 0, -72826.60637350507 1467464.7068374576 0, -72831.42133672876 1467062.266267154 0, -72836.23838146002 1466659.8209532525 0, -72932.69091798979 1466658.9665849993 0, -73235.36528261697 1466663.2898427595 0, -73300.25282739366 1466664.221042388 0, -73339.10900620786 1466664.7765644249 0, -73634.46368984588 1466669.0175043961 0, -73745.53561201082 1466670.6061897657 0, -74033.57075592288 1466674.7528005103 0, -74151.96181903427 1466676.4552807175 0, -74259.50465004738 1466678.0081120091 0, -74286.51108513729 1466678.7696970543 0, -74297.55805295368 1466678.5575722964 0, -74424.51221705906 1466680.3906875006 0, -74421.69025725653 1467080.2768143052 0, -74418.87006271395 1467480.1590942924 0)), ((-78392.1734950474 1467516.7065576164 0, -78787.18265120554 1467520.332725089 0, -79182.19153687877 1467523.9884510755 0, -79180.47917577751 1467926.0460390388 0, -79178.76670476815 1468328.0932666343 0, -78783.80244007387 1468322.7237629287 0, -78388.83799037462 1468317.361506945 0, -78390.50584486716 1467917.0279575954 0, -77995.51437802658 1467912.5465573752 0, -77602.2230717691 1467908.1103326255 0, -77598.90786077552 1468306.703451055 0, -77200.18359123629 1468303.5016689505 0, -76801.45925100632 1468300.3075329098 0, -76802.03431127718 1467901.2531946185 0, -76802.60901184396 1467502.199791674 0, -77206.78939066017 1467505.8796845758 0, -77605.54725098587 1467509.5182296687 0, -77608.86236453296 1467110.92697817 0, -77612.17940369465 1466712.3336952042 0, -77707.29768090852 1466711.409553167 0, -78000.44862841813 1466713.0722712893 0, -78077.94959848991 1466713.5141808693 0, -78097.1652613044 1466713.6233066784 0, -78395.50783970584 1466715.3248715913 0, -78393.84103240023 1467116.3749945476 0, -78392.1734950474 1467516.7065576164 0)), ((-76782.72420252988 1470740.2808473867 0, -76781.08203179369 1471145.9517177728 0, -76380.50208992962 1471138.378970792 0, -76381.78392098352 1470733.0298483379 0, -76782.72420252988 1470740.2808473867 0)), ((-77179.65864762946 1471559.5372781712 0, -76779.43967544501 1471551.6236386464 0, -76781.08203179369 1471145.9517177728 0, -77181.66134467519 1471153.5436100482 0, -77179.65864762946 1471559.5372781712 0)), ((-79146.81281348842 1472396.2512589945 0, -79140.61974757117 1472803.3747966662 0, -79134.43577765398 1473210.4882480218 0, -78739.35727956427 1473205.5637737243 0, -78344.28751587989 1473200.6466055228 0, -77949.2084553448 1473195.7590968036 0, -77554.13813230445 1473190.8788940117 0, -77560.57246205317 1472785.022397899 0, -77567.00712318752 1472379.166843352 0, -77573.44201667445 1471973.3122287374 0, -77579.87724151628 1471567.4585586996 0, -77974.70586533543 1471571.07077523 0, -78369.53426474784 1471574.7014273494 0, -78764.3626362148 1471578.3505214434 0, -79159.19068110157 1471582.0180482545 0, -79152.99714981088 1471989.139693693 0, -79146.81281348842 1472396.2512589945 0)), ((-75155.10049342593 1473970.4365271246 0, -74758.52890858566 1473965.4377548 0, -74361.9569061379 1473960.4577092486 0, -74370.26947124716 1473556.329627542 0, -74765.9290483378 1473560.9770007825 0, -75161.58816727453 1473565.6540061552 0, -75155.10049342593 1473970.4365271246 0)), ((-75896.04569409085 1477223.8999372446 0, -75907.53815585666 1476812.5349223502 0, -75919.04025620785 1476401.1708250658 0, -76316.6850277755 1476404.7347425506 0, -76714.3385027527 1476408.3173569816 0, -76704.83045532278 1476820.1357947802 0, -76695.32292237412 1477231.9551742098 0, -76295.68441689387 1477227.9180969333 0, -75896.04569409085 1477223.8999372446 0)), ((-77502.12188235376 1476827.8118377703 0, -77509.63597611152 1476415.5386631575 0, -77905.59010033954 1476419.1618015105 0, -78301.55301737858 1476422.80353985 0, -78295.7128441506 1476833.5912921042 0, -77898.91747393653 1476830.6922583473 0, -77502.12188235376 1476827.8118377703 0)), ((-79044.65767861178 1481725.5478045952 0, -79038.78535595296 1482134.846635242 0, -79032.9132606372 1482544.1462823348 0, -79027.04128746063 1482953.4469429601 0, -78630.01767268042 1482951.4698751802 0, -78232.99418151262 1482949.5001937947 0, -77835.97061717378 1482947.5604127108 0, -77842.02191911906 1482539.5384921462 0, -77848.07334406668 1482131.5175800927 0, -77451.17248735616 1482130.4489151596 0, -77457.28099824005 1481722.8662424556 0, -77463.39869682437 1481315.273454886 0, -77860.17692336692 1481315.4896046645 0, -78256.96415067052 1481315.7244291909 0, -78653.74264131994 1481315.9777714645 0, -79050.53022548153 1481316.2498928355 0, -79044.65767861178 1481725.5478045952 0)), ((-81737.67655415121 1489839.4998658367 0, -81734.41467692757 1490246.1763924775 0, -81337.73142633653 1490244.2821665567 0, -81340.26886977302 1489839.839216485 0, -81342.81482949035 1489435.4084213425 0, -81740.9293065554 1489432.835344033 0, -81737.67655415121 1489839.4998658367 0)), ((-78105.9029157806 1491651.3180214781 0, -77943.4635285838 1491697.9103538394 0, -77800.2354278012 1491728.6524002533 0, -77758.57586558502 1491755.523819623 0, -77726.74181623857 1491776.0669087328 0, -77685.11704560723 1491811.7549599071 0, -77641.55962309029 1491843.3032152257 0, -77361.53984036179 1491838.924181439 0, -77372.70585425894 1491434.357054196 0, -77383.8726132515 1491029.7908901575 0, -77776.0745694919 1491033.811189111 0, -78168.28525969242 1491037.8385189262 0, -78159.77794303854 1491444.5684911206 0, -78155.76251619754 1491636.5996594129 0, -78105.9029157806 1491651.3180214781 0)), ((-72783.8423901512 1471704.0374508759 0, -72785.0804528673 1471501.0939703688 0, -73186.01866375015 1471505.4085435928 0, -73586.96563943435 1471509.7309307079 0, -73584.44881395398 1471916.8951096733 0, -73581.93179138654 1472324.0602375388 0, -73181.03458503803 1472318.4496924768 0, -72780.14584311745 1472312.8694722622 0, -72782.61324409813 1471906.9812994741 0, -72783.8423901512 1471704.0374508759 0)), ((-73142.83948542511 1475572.7132053568 0, -73541.0651393629 1475576.2291789672 0, -73535.96646405043 1475985.6766884283 0, -73137.16251427079 1475982.346013629 0, -72738.34959107195 1475979.022873201 0, -72744.61348273417 1475569.2271564167 0, -73142.83948542511 1475572.7132053568 0)), ((-73513.72244872533 1477613.3569525203 0, -73507.95495026246 1478024.1475031818 0, -73106.98046267036 1478020.6858961042 0, -72706.00587628513 1478017.2432034067 0, -72712.5810310503 1477606.2580667168 0, -72719.1654451168 1477195.2627430637 0, -72725.7411886632 1476784.279489158 0, -72732.32628738073 1476373.286155441 0, -73131.68527515934 1476377.1404321832 0, -73531.0441051904 1476381.0024212839 0, -73525.2671029627 1476791.7899665176 0, -73519.49911247358 1477202.578632568 0, -73513.72244872533 1477613.3569525203 0)), ((-73061.99030506378 1482867.0610211508 0, -72661.63868421168 1482857.2037324922 0, -72666.7907703602 1482456.4443878005 0, -72671.95195291903 1482055.6748024123 0, -72677.10430189109 1481654.9172329714 0, -72682.26584621612 1481254.1494288705 0, -73080.68958295415 1481259.2852823783 0, -73479.12197519674 1481264.4288094074 0, -73474.92443418386 1481667.5573181163 0, -73470.73597732947 1482070.675701458 0, -73466.53847965538 1482473.8061060975 0, -73462.35017146051 1482876.926183777 0, -73061.99030506378 1482867.0610211508 0)), ((-74215.31987961197 1486939.408571468 0, -74213.10021863587 1487345.75974349 0, -74210.88933316348 1487752.100677042 0, -73811.07199247112 1487747.3197786026 0, -73411.26325581915 1487742.5579352174 0, -73011.44529394088 1487737.8148849728 0, -72611.63593622523 1487733.090990431 0, -72615.44642045179 1487328.0527376777 0, -72619.26597795894 1486923.0043464545 0, -72623.07648364383 1486517.967966331 0, -72626.89606561416 1486112.9213498733 0, -73025.10532035124 1486116.3427618532 0, -73423.32328251275 1486119.7831331035 0, -73821.53222162319 1486123.2421043727 0, -74219.7499639757 1486126.7200383083 0, -74217.53048460835 1486533.06942103 0, -74215.31987961197 1486939.408571468 0)), ((-73003.04512184244 1488552.4129915608 0, -73402.83016393267 1488556.506249862 0, -73398.61813673293 1488963.4818785738 0, -73394.406220938 1489370.4582932952 0, -72994.63650286454 1489367.0033677176 0, -72594.86667667152 1489363.5674111494 0, -72599.05435651711 1488955.9524841164 0, -72603.25120009242 1488548.3274226103 0, -73003.04512184244 1488552.4129915608 0)), ((-74153.14957895926 1492626.3752554955 0, -73755.23860029077 1492622.898048667 0, -73357.33642570979 1492619.439677622 0, -72959.42522314904 1492615.9999809267 0, -72561.52272884907 1492612.5791166173 0, -72566.03623421623 1492206.2480470145 0, -72570.5499928527 1491799.9067446238 0, -72575.06371311886 1491393.5775203118 0, -72579.57768964935 1490987.2379654038 0, -72977.89432331357 1490990.661885849 0, -73376.21074710423 1490994.1046653092 0, -73774.52705842246 1490997.566307073 0, -74172.84325876497 1491001.0467103643 0, -74167.91513231414 1491407.3831011858 0, -74162.9961863709 1491813.7092402768 0, -74158.06829237098 1492220.0473752772 0, -74153.14957895926 1492626.3752554955 0)), ((-73315.39576219047 1496667.5184320232 0, -73311.87112640621 1497072.5860726952 0, -73308.3465547544 1497477.6433546988 0, -72910.65339447763 1497475.492414335 0, -72512.96894450676 1497473.3602820307 0, -72515.09779713205 1497068.2913186175 0, -72517.23542850235 1496663.2119757372 0, -72519.36400391452 1496258.1446141803 0, -72521.50145070507 1495853.0670811085 0, -72921.96873490834 1495855.2224859106 0, -73322.44493234492 1495857.3969116756 0, -73318.9202657671 1496262.462848082 0, -73718.69392889713 1496264.6502827364 0, -74118.46758251335 1496266.8566566226 0, -74113.55596362872 1496671.9003338972 0, -73714.47591854482 1496669.699915538 0, -73315.39576219047 1496667.5184320232 0)), ((-68716.28715733084 1457662.6673331738 0, -68319.78673984166 1457660.2634012292 0, -68323.3085050544 1457296.5798658333 0, -68327.55830284423 1456858.134074846 0, -68404.78808497394 1456856.9607504753 0, -68542.26614334645 1456856.7278929604 0, -68718.23827123755 1456859.0493941552 0, -68726.15282215334 1456859.0229096212 0, -69124.77482946745 1456857.6889971583 0, -69118.08395414182 1457307.7263641078 0, -69112.76960980173 1457665.101003152 0, -68716.28715733084 1457662.6673331738 0)), ((-69112.76960980173 1457665.101003152 0, -69509.2252300812 1457667.5529240628 0, -69905.66293127806 1457670.0232760746 0, -69897.71093876303 1458065.4895449802 0, -69889.76831001487 1458460.9568472856 0, -69495.29309643655 1458465.0102036747 0, -69100.81851394827 1458469.081940904 0, -69106.79836496325 1458067.0910200493 0, -69112.76960980173 1457665.101003152 0)), ((-68265.55376762456 1462120.842958668 0, -68270.86257824222 1461715.4101024538 0, -68672.35854252106 1461707.9745270105 0, -68667.87901178085 1462114.2538504149 0, -68265.55376762456 1462120.842958668 0)), ((-69469.7016877606 1462509.117615047 0, -69472.53194670076 1462101.132937958 0, -69874.85953203446 1462094.601232029 0, -69872.85819620869 1462503.4438875634 0, -69469.7016877606 1462509.117615047 0)), ((-68658.91150164811 1462926.815374739 0, -68663.39967038295 1462520.534160996 0, -69066.54587462494 1462514.82181863 0, -69062.89568996085 1462921.9497890717 0, -68658.91150164811 1462926.815374739 0)), ((-69464.04116429258 1463325.101255726 0, -69059.23643160626 1463329.0897672 0, -69062.89568996085 1462921.9497890717 0, -69466.87136078413 1462917.1145921382 0, -69464.04116429258 1463325.101255726 0)), ((-68070.97382668841 1467017.7268901884 0, -68469.7292301333 1467021.8865791103 0, -68857.30066220576 1467025.9521993226 0, -68854.04034194387 1467426.9148184566 0, -68462.74164021191 1467423.5583364775 0, -68063.99915069967 1467420.1491944445 0, -68070.97382668841 1467017.7268901884 0)), ((-68823.85284031251 1471473.2720650278 0, -69219.00827020477 1471477.3181145815 0, -69214.52457870312 1471880.8238985334 0, -69609.49699118786 1471884.259872912 0, -69604.83073161803 1472287.1267754582 0, -70003.68883720908 1472290.8372440063 0, -70402.5556694541 1472294.566627038 0, -70399.19699834677 1472698.2967443974 0, -70395.83818638064 1473102.0390026513 0, -69995.66397521242 1473097.4473370858 0, -69595.489572429 1473092.8746070163 0, -69201.04718028326 1473091.3692442202 0, -68806.61386720366 1473089.8710823462 0, -68412.17160365012 1473088.402473695 0, -68017.73832011299 1473086.941163461 0, -68021.68231955219 1472681.5131904404 0, -68025.63522818575 1472276.0862378 0, -68029.579307281 1471870.6602514712 0, -68033.53229862524 1471465.2351876101 0, -68428.68820467472 1471469.2443685364 0, -68823.85284031251 1471473.2720650278 0), (-69210.03192517218 1472284.3418452954 0, -68815.23313162997 1472281.5752484035 0, -68420.43429445382 1472278.8159761755 0, -68416.30743302511 1472683.6031924854 0, -68810.92349732069 1472685.722748532 0, -69205.53962453955 1472687.8494265021 0, -69210.03192517218 1472284.3418452954 0)), ((-69538.31417771222 1481611.980797098 0, -69532.92745992675 1482018.280421368 0, -69527.54079047615 1482424.5922603 0, -69522.15446900025 1482830.893701603 0, -69123.47348779865 1482825.059908694 0, -68724.79211528102 1482819.2448085628 0, -68326.11034684895 1482813.448602851 0, -67927.4281872374 1482807.671190586 0, -67933.70917368594 1482404.3678271857 0, -67939.99938292651 1482001.0654413034 0, -67946.2809779465 1481597.763974841 0, -67952.57179886349 1481194.4633879473 0, -68350.34985628433 1481197.2427551718 0, -68748.13669430156 1481200.0296888822 0, -69145.91448110873 1481202.8464470827 0, -69543.7011412685 1481205.670876026 0, -69538.31417771222 1481611.980797098 0)), ((-68686.50926408112 1487696.949071745 0, -68289.37338325944 1487695.4535024615 0, -67892.24638253797 1487693.9654716563 0, -67893.12802024258 1487288.0317217195 0, -67894.01836183699 1486882.0988450435 0, -68291.85192239353 1486885.518761311 0, -68689.6764785695 1486888.9572735499 0, -68688.09730991194 1487292.958320995 0, -68686.50926408112 1487696.949071745 0)), ((-69445.73650491417 1492164.6712367663 0, -69440.73563277465 1492567.5808507903 0, -69041.46205833417 1492565.6029826896 0, -68642.1883931633 1492563.6440642118 0, -68242.91474100157 1492561.7039974695 0, -67843.641100357 1492559.7828831812 0, -67848.24540976863 1492154.742009156 0, -67852.85878052186 1491749.690874933 0, -67857.46338207013 1491344.651739831 0, -67862.07704177184 1490939.6024484432 0, -68261.73875772397 1490943.6546189454 0, -68661.40909716283 1490947.7259288074 0, -69061.07042935371 1490951.8160214415 0, -69460.74028591247 1490955.9251496722 0, -69455.73883153363 1491358.843384699 0, -69450.73763632438 1491761.7512765592 0, -69445.73650491417 1492164.6712367663 0)), ((-68116.37177006259 1501897.3383576204 0, -68126.84491657955 1501490.7161943768 0, -68529.21037161048 1501496.7372952104 0, -68932.82558906545 1501502.7990234075 0, -69333.93974638608 1501508.8483561627 0, -69331.77042311574 1501622.5889506491 0, -69286.69055662438 1501638.9104242355 0, -69111.00870344945 1501760.628430932 0, -68988.62228568728 1501823.7718888212 0, -68925.74729243135 1501860.449990843 0, -68919.23347249403 1501864.25042706 0, -68878.58974007465 1501866.4842912147 0, -68833.85157873812 1501873.815571348 0, -68519.65665870799 1501902.4034048666 0, -68158.85789087966 1501955.57406742 0, -68114.76744510683 1501959.7104836234 0, -68116.37177006259 1501897.3383576204 0)), ((-62765.870463157684 1457631.1113722716 0, -63173.204197965686 1457631.9602979622 0, -63169.192205450105 1458050.5886319955 0, -62762.670236827405 1458049.992290071 0, -62765.870463157684 1457631.1113722716 0)), ((-64357.87710152739 1458472.9253500819 0, -64362.94966577158 1458055.065998283 0, -64756.8480301289 1458057.020718102 0, -64750.27846745622 1458474.6108937962 0, -64357.87710152739 1458472.9253500819 0)), ((-64689.91265037442 1462518.0587928589 0, -64692.678469094346 1462110.4870911818 0, -65083.91148158896 1462110.0514362354 0, -65082.481088544344 1462517.633267065 0, -64689.91265037442 1462518.0587928589 0)), ((-61968.10040083134 1464156.395643531 0, -61968.65236750214 1463753.507234142 0, -61969.21316840847 1463350.6085721855 0, -62345.70425986705 1463346.6241027862 0, -62722.18682288851 1463342.667499843 0, -62719.0939929303 1463747.0146269056 0, -62343.87296629526 1463750.2525600914 0, -62342.05060267976 1464153.8709672058 0, -61968.10040083134 1464156.395643531 0)), ((-64639.10250741785 1466586.2624055236 0, -64871.18963472081 1466591.947183293 0, -64871.49262868909 1466997.4360953786 0, -64871.79721500024 1467402.9052374384 0, -64872.0926068738 1467808.3863771397 0, -64872.39652821976 1468213.8574542922 0, -64473.66708744734 1468210.4148012123 0, -64074.9376274702 1468206.979692928 0, -63676.20775951663 1468203.5745332444 0, -63277.477872478405 1468200.1770189996 0, -63283.2422025026 1467792.1980356672 0, -63289.00679604657 1467384.220123276 0, -63294.77146125358 1466976.2430753692 0, -63300.52947156712 1466568.256785785 0, -63458.23743561229 1466557.445906576 0, -63699.45233110076 1466563.3232785854 0, -63851.85992591725 1466567.029380438 0, -64073.565981780346 1466572.446444327 0, -64245.4815870214 1466576.6423174897 0, -64451.32960565389 1466581.6733178198 0, -64472.37824943185 1466582.1873840007 0, -64481.98856551679 1466582.422583497 0, -64639.10250741785 1466586.2624055236 0)), ((-64857.43545704778 1469806.5296919842 0, -64852.95751281315 1470213.2683675576 0, -64848.48880907546 1470619.9967769198 0, -64844.011216611136 1471026.7372673748 0, -64447.18490131639 1471026.9157780155 0, -64050.349761172336 1471027.1240467762 0, -64054.28248218588 1470619.1136933358 0, -64058.21541743825 1470211.0929962094 0, -64062.14826908621 1469803.0845659624 0, -64459.79179643762 1469804.7977567685 0, -64857.43545704778 1469806.5296919842 0)), ((-63154.27943166256 1481963.3078288932 0, -63155.295641045705 1481553.5588365025 0, -63156.31164463289 1481143.799665942 0, -63558.49961570791 1481146.3819734827 0, -63960.69658685198 1481148.9723554885 0, -63958.63545885184 1481556.5733181941 0, -63956.57424655755 1481964.1864108923 0, -63954.51294586771 1482371.7892143116 0, -63553.88793631426 1482372.4139900033 0, -63153.263026998946 1482373.0688574577 0, -63154.27943166256 1481963.3078288932 0)), ((-64761.97528442547 1481559.6753837664 0, -64360.30535164532 1481558.114853869 0, -64362.884331031826 1481151.593056879 0, -64765.08107513099 1481154.2217321144 0, -64761.97528442547 1481559.6753837664 0)), ((-61122.543482454974 1483582.4299722 0, -61117.23893683938 1483987.8845531826 0, -61518.62222184279 1483989.5025764795 0, -61512.96417637525 1484394.5185458958 0, -61111.93475603687 1484393.3401405702 0, -60710.91425145823 1484392.1695856592 0, -60715.864616257815 1483986.2856948737 0, -60720.80617953477 1483580.413934021 0, -60725.756872276506 1483174.531949947 0, -61127.84805467721 1483176.987395192 0, -61133.152940064036 1482771.5346172468 0, -61535.59799695511 1482774.4375526197 0, -61529.93918322497 1483179.4620294496 0, -61524.2805911519 1483584.4761984076 0, -61122.543482454974 1483582.4299722 0)), ((-67108.53758810216 1485249.161130611 0, -66711.63964930753 1485245.8168478608 0, -66718.91239671793 1484838.9874636875 0, -66726.19430410383 1484432.17026336 0, -67120.42201569056 1484435.2806208015 0, -67114.47965807382 1484842.2204248803 0, -67108.53758810216 1485249.161130611 0)), ((-64707.24631959418 1486848.693344332 0, -64310.89982134748 1486848.461877233 0, -63914.562519170686 1486848.2378552218 0, -63518.216284888484 1486848.0436269615 0, -63121.87915077506 1486847.8568403702 0, -63122.211479229285 1486440.6344615344 0, -63122.54346765946 1486033.4129834045 0, -63520.77990167543 1486034.2522291723 0, -63919.02519303734 1486035.1102237697 0, -64317.261599684854 1486035.9870114299 0, -64715.50705539568 1486036.8826554 0, -64711.376596860944 1486442.7876021147 0, -64707.24631959418 1486848.693344332 0)), ((-63862.80037408337 1491719.1394664752 0, -63857.864542699404 1492125.2525310528 0, -63852.92893964328 1492531.3776790355 0, -63453.975790968056 1492529.6750046334 0, -63119.644567315525 1492528.2584630174 0, -63152.39721863247 1492279.992425256 0, -63162.926657931355 1492120.9957428244 0, -63166.029102282315 1492074.1845585853 0, -63255.193911809416 1491714.266784929 0, -63288.61311190588 1491579.3903222217 0, -63352.9430670904 1491330.7455435104 0, -63366.92969748732 1491308.0546361422 0, -63405.986436760286 1491244.709654339 0, -63455.04808429261 1491151.0272579635 0, -63470.196742531036 1491115.5641529025 0, -63472.64394193631 1490902.1917070018 0, -63872.672661517754 1490906.893646237 0, -63867.73643073226 1491313.0160681396 0, -63862.80037408337 1491719.1394664752 0)), ((-59211.873119999356 1456830.77603724 0, -59224.456019261 1456831.0429567136 0, -59434.29515542788 1456834.9764043195 0, -59610.826408002096 1456832.3784809886 0, -59635.17836743209 1456832.0201052187 0, -59824.285306299025 1456830.217385985 0, -60001.68925675221 1456831.8079452873 0, -60009.78134123556 1456831.7819637796 0, -60066.95101347023 1456831.5984073314 0, -60068.73478554488 1456831.4990560154 0, -60205.943693296336 1456831.2410202716 0, -60406.36478885451 1456830.6516865261 0, -60408.74791975078 1456830.6444257058 0, -60406.55116278666 1457231.3319150514 0, -60404.39372121041 1457626.5660628132 0, -60005.654377707615 1457625.8660749742 0, -59606.91500056899 1457625.1847687091 0, -59208.175829105116 1457624.5111460083 0, -58809.44549885816 1457623.8674895084 0, -58811.1596926088 1457231.6650203892 0, -58812.92706610567 1456829.252493636 0, -58867.93547895349 1456830.5741624483 0, -58929.096305208244 1456830.3273659032 0, -58940.15622452364 1456829.6203141364 0, -58942.49075221615 1456828.6903588783 0, -58984.34670962438 1456828.5747660052 0, -58984.73614294449 1456829.1465843164 0, -58989.43140436629 1456833.435210305 0, -58995.11587666236 1456836.498746018 0, -58998.68339046342 1456836.299592404 0, -59004.656363540285 1456836.3411895714 0, -59013.13945699367 1456834.3843056366 0, -59014.74578607603 1456834.1714982127 0, -59022.32890190666 1456833.4403357664 0, -59200.833906289445 1456830.5418637756 0, -59211.873119999356 1456830.77603724 0)), ((-56396.486349868755 1461704.5882537488 0, -56000.50767029506 1461699.8501837708 0, -55604.53757540827 1461695.13056186 0, -55607.88948005015 1461287.5621334126 0, -55611.25037662114 1460879.9836761837 0, -56008.45217788736 1460883.4347875428 0, -56405.6537992782 1460886.915780435 0, -56401.06995850919 1461295.7515157794 0, -56396.486349868755 1461704.5882537488 0)), ((-60388.29282570612 1463344.4094275492 0, -59987.619695360954 1463344.1330602881 0, -59586.946774718184 1463343.864452334 0, -59586.90384327079 1462937.1210004834 0, -59586.860755434 1462530.378443201 0, -59586.81735612491 1462123.625670543 0, -59184.79447096355 1462125.953944134 0, -58782.780833740486 1462128.3125697288 0, -58781.84013370392 1461723.2794581729 0, -59184.306604525525 1461720.072692798 0, -59586.77355300804 1461716.8850962117 0, -59989.24097749075 1461713.7166686326 0, -60391.708879395715 1461710.5673094199 0, -60390.85513152627 1462119.0263394606 0, -60390.0012230727 1462527.4863707004 0, -60389.14715411335 1462935.9474016263 0, -60388.29282570612 1463344.4094275492 0)), ((-59186.27387403317 1463343.6260126813 0, -58785.60108729455 1463343.3953288926 0, -58784.66140788706 1462938.3705601618 0, -59185.7781056678 1462937.730605538 0, -59186.27387403317 1463343.6260126813 0)), ((-58428.113420171954 1471813.8813861432 0, -58432.279211508205 1471407.5836558864 0, -58827.14676193457 1471406.8855596685 0, -59222.01447282238 1471406.20588804 0, -59616.88234259795 1471405.5446411776 0, -60011.75046559958 1471404.9019232679 0, -60006.48534666255 1471811.1915328652 0, -60001.22934914714 1472217.4710642956 0, -59995.964647882356 1472623.7626719454 0, -59990.7090711926 1473030.0440975253 0, -59596.94026538472 1473030.6950534307 0, -59203.17161203407 1473031.3644279628 0, -58809.403118890616 1473032.0520191959 0, -58415.634883428844 1473032.7579309447 0, -58419.79125454428 1472626.4685756273 0, -58423.95674350775 1472220.1689420724 0, -58428.113420171954 1471813.8813861432 0)), ((-59157.76911337094 1477096.5006008502 0, -58754.681169332514 1477098.6144312948 0, -58756.60498100959 1477505.4938260838 0, -58758.52847541702 1477912.3629571062 0, -58356.15109488709 1477915.1388394057 0, -58353.863665549 1477507.9538110218 0, -58351.58463358268 1477100.7585953618 0, -58349.29607167435 1476693.5754474406 0, -58347.01610491499 1476286.3821215695 0, -58750.82314530572 1476284.8808011408 0, -59154.63050365464 1476283.3875843715 0, -59558.438084494635 1476281.9248849947 0, -59962.246078974735 1476280.4702927878 0, -59963.10518517892 1476686.38882966 0, -59963.96403483528 1477092.3084086585 0, -59560.86639134121 1477094.394850683 0, -59157.76911337094 1477096.5006008502 0)), ((-59928.21754873335 1481947.6895804033 0, -59927.01725610088 1482355.320456829 0, -59925.81705803572 1482762.9409519762 0, -59521.43327767718 1482763.9767366445 0, -59125.627041188716 1482765.0130992145 0, -58725.52798958133 1482766.0832141032 0, -58325.43806745689 1482767.1610821565 0, -58326.88108155291 1482360.830585806 0, -58328.3328035355 1481954.4899755341 0, -58329.77551014224 1481548.1613108742 0, -58331.227023492705 1481141.8225384678 0, -58731.074028531446 1481139.4545733768 0, -59130.921444746746 1481137.0943898559 0, -59530.769179281066 1481134.7643012118 0, -59930.617321770456 1481132.4419944976 0, -59929.4174391128 1481540.0709276577 0, -59928.21754873335 1481947.6895804033 0)), ((-55634.47571773122 1457619.3902288661 0, -55233.18763976876 1457618.909409966 0, -55233.63037835485 1458031.2197791704 0, -55634.8939439233 1458033.8283480564 0, -55635.311805134625 1458448.2564021756 0, -55234.06788554167 1458445.6478521451 0, -54832.82394546621 1458443.0582901954 0, -54834.00679921864 1458028.640697642 0, -54835.18010645418 1457618.457472443 0, -54433.89219920776 1457618.0145234528 0, -54432.74299621733 1458026.070000953 0, -54431.579785453105 1458440.4878108113 0, -54030.33550926287 1458437.9363160762 0, -54026.801712754015 1458362.7633765682 0, -54027.73524043028 1458023.4945903153 0, -54028.86004789654 1457617.5893669114 0, -54029.961793319126 1457219.5135328933 0, -54398.89015186742 1457223.8635567462 0, -54435.00294333219 1457224.2955838796 0, -54602.8733692096 1457226.2846808631 0, -54796.34469878411 1457228.580805024 0, -54836.29961639585 1457229.0505198918 0, -55232.7821470563 1457233.77078032 0, -55284.147643807395 1457234.3837291652 0, -55405.222825814955 1457233.3776000831 0, -55405.980958980166 1457156.6757374194 0, -55409.17514890151 1456831.8942117542 0, -55633.673235305636 1456831.5640444045 0, -55634.0774492578 1457233.2212568552 0, -55634.47571773122 1457619.3902288661 0)), ((-55602.56072466702 1462102.272144537 0, -55205.75826270731 1462098.2937470493 0, -54808.95546817549 1462094.334016074 0, -54806.720387551344 1462493.5677850095 0, -54806.63057639425 1462510.2553047605 0, -55203.61165645563 1462509.8144673905 0, -55600.59277002397 1462509.40349477 0, -55598.615779268766 1462916.5470658548 0, -55596.64768165351 1463323.6805023204 0, -55199.35733823885 1463324.100877033 0, -54802.0671244379 1463324.5286006304 0, -54404.77714178713 1463324.986292651 0, -54007.4872919243 1463325.4513332203 0, -54007.899913989975 1463260.493309037 0, -54010.073801764265 1462918.310309561 0, -54010.38603975884 1462869.155090864 0, -54012.66023790727 1462511.170275272 0, -54012.872203118364 1462477.8065984 0, -54015.35821327567 1462086.4702414405 0, -54015.65897780112 1462039.129614401 0, -54017.84435989956 1461695.1236160547 0, -54414.512936381434 1461695.1030421993 0, -54811.19075683259 1461695.0899109629 0, -55207.85959365853 1461695.1065669444 0, -55604.53757540827 1461695.13056186 0, -55602.56072466702 1462102.272144537 0)), ((-55334.037804795356 1467320.2820014 0, -55325.319653137354 1467717.132925389 0, -55316.61115344242 1468113.9736530425 0, -54919.92161127385 1468111.408879433 0, -54523.232038017624 1468108.8627514371 0, -54126.54224034806 1468106.3351617833 0, -53729.85241788153 1468103.8261165686 0, -53736.79328923291 1467704.397088806 0, -53743.734573035275 1467304.957893284 0, -53750.67609346391 1466905.5304359812 0, -53757.61087573576 1466506.0803710104 0, -53984.61150689138 1466505.834221939 0, -54154.376942137504 1466508.4003595642 0, -54383.767297157516 1466511.8650833538 0, -54558.08271729824 1466514.5130482686 0, -54673.455910126984 1466516.2636795097 0, -54782.91369506975 1466517.9258263514 0, -54954.771379526945 1466520.532554123 0, -55085.22242571772 1466522.5219543953 0, -55182.06852604135 1466523.994194958 0, -55351.459457735815 1466526.5819171064 0, -55342.74748418175 1466923.4431292922 0, -55334.037804795356 1467320.2820014 0)), ((-55239.869331834845 1473011.5706242684 0, -54838.66304542229 1473006.8507078427 0, -54437.45633102092 1473002.149816702 0, -54036.249385205825 1472997.4680578422 0, -53635.042017812564 1472992.8052231288 0, -53640.33547453616 1472585.6486189482 0, -53645.62916690169 1472178.4928648104 0, -53650.923187708395 1471771.338167099 0, -53656.21734202122 1471364.1844202094 0, -54053.777630043645 1471366.6965263225 0, -54451.33779454803 1471369.2272613645 0, -54848.897929839084 1471371.7767294815 0, -55246.45783938789 1471374.3448236906 0, -55244.81088354941 1471783.649774568 0, -55243.16384457587 1472192.9557942764 0, -55241.51662971217 1472602.2626764013 0, -55239.869331834845 1473011.5706242684 0)), ((-55161.845458281394 1477479.4481800615 0, -55161.922900922014 1477883.6487785915 0, -54763.31704102112 1477879.787651511 0, -54364.71976297105 1477875.9455088866 0, -53966.113436532076 1477872.12209582 0, -53567.51570134676 1477868.3174651999 0, -53572.77871317961 1477465.4391570096 0, -53578.04212444378 1477062.5504625118 0, -53583.3056375242 1476659.6739916531 0, -53588.56954686063 1476256.7872383534 0, -53981.82571534432 1476259.2703887362 0, -54375.0906704107 1476261.771825559 0, -54768.34667027248 1476264.291593851 0, -55161.61145363829 1476266.8296488635 0, -55161.68973319344 1476671.0386641163 0, -55161.76770194499 1477075.2373012968 0, -55161.845458281394 1477479.4481800615 0)), ((-55536.725664160724 1481950.9764349603 0, -55140.18882863359 1481946.8969264938 0, -55139.8058213658 1481537.9808017237 0, -55139.43139998577 1481129.0543784054 0, -55535.49287120528 1481134.2058046963 0, -55536.109432048936 1481542.5850004298 0, -55536.725664160724 1481950.9764349603 0)), ((-53984.40696238312 1482787.3021100988 0, -53964.32770064578 1482738.6518689082 0, -53954.282528593365 1482708.2111093053 0, -53952.327663839846 1482370.9475391738 0, -53817.48392704566 1482372.6813293078 0, -53801.1286038638 1482337.7652295681 0, -53756.56172820017 1482271.8458778798 0, -53728.543505835885 1482208.999409983 0, -53693.42278967698 1482146.119509787 0, -53677.54624363191 1482035.6113478327 0, -53630.48998021395 1481987.576223098 0, -53612.10264307511 1481956.0641150791 0, -53949.90300319273 1481954.0091899482 0, -54346.667441162 1481951.6273160973 0, -54348.405468717596 1482365.8845208483 0, -54350.14284359606 1482780.153775593 0, -53984.40696238312 1482787.3021100988 0)), ((-54744.7872843303 1483990.2142077207 0, -54345.38248094375 1483997.9028974713 0, -54346.96940176124 1483591.9856132441 0, -54745.04259450156 1483584.2883362921 0, -55143.11657692817 1483576.6098261075 0, -55144.20179620003 1483982.5444637067 0, -55145.286645822125 1484388.4800136928 0, -54744.54062250704 1484396.1410693242 0, -54744.7872843303 1483990.2142077207 0)), ((-45679.57774402716 1458344.7745282666 0, -45283.80216922092 1458340.953023227 0, -45286.2128981814 1457932.8013932784 0, -44890.52537205971 1457928.9091915225 0, -44893.033490231304 1457520.658180095 0, -45288.614694046126 1457524.650801352 0, -45290.41695972511 1457185.6785385848 0, -45672.17033124869 1457187.7117994644 0, -45686.02371036831 1457187.8418430975 0, -45903.64319281727 1457189.9046413011 0, -46021.46564800319 1457191.0207629127 0, -46081.62189090691 1457191.5916571051 0, -46079.776422967625 1457532.6913938012 0, -46077.569187922614 1457940.6524837103 0, -46075.361987954195 1458348.6033849001 0, -45679.57774402716 1458344.7745282666 0)), ((-49279.886499582135 1457967.0842251172 0, -49682.49577839283 1457968.4667465738 0, -49678.31743328168 1458366.6614022406 0, -49275.7104058897 1458368.1574746585 0, -49279.886499582135 1457967.0842251172 0)), ((-45287.8635580826 1463198.7280879538 0, -44899.79643893018 1463190.2725606281 0, -44511.72832889258 1463181.8243846882 0, -44512.14211326173 1462778.9367030575 0, -44512.5556498546 1462376.0386931805 0, -44512.96903963658 1461973.152974902 0,</t>
+          <t>MULTIPOLYGON Z (((-74418.87006271395 1467480.1590942924 0, -74416.04098262447 1467880.0422387214 0, -74413.22075045682 1468279.9265030606 0, -74014.15315680247 1468277.319849597 0, -73615.09452486291 1468274.7209222964 0, -73216.0267285189 1468272.151969932 0, -73220.86382510237 1467870.3480019812 0, -73225.6920834597 1467468.5561065474 0, -72826.60637350507 1467464.7068374576 0, -72831.42133672876 1467062.266267154 0, -72836.23838146002 1466659.8209532525 0, -72932.69091798979 1466658.9665849993 0, -73235.36528261697 1466663.2898427595 0, -73300.25282739366 1466664.221042388 0, -73339.10900620786 1466664.7765644249 0, -73634.46368984588 1466669.0175043961 0, -73745.53561201082 1466670.6061897657 0, -74033.57075592288 1466674.7528005103 0, -74151.96181903427 1466676.4552807175 0, -74259.50465004738 1466678.0081120091 0, -74286.51108513729 1466678.7696970543 0, -74297.55805295368 1466678.5575722964 0, -74424.51221705906 1466680.3906875006 0, -74421.69025725653 1467080.2768143052 0, -74418.87006271395 1467480.1590942924 0)), ((-78392.1734950474 1467516.7065576164 0, -78787.18265120554 1467520.332725089 0, -79182.19153687877 1467523.9884510755 0, -79180.47917577751 1467926.0460390388 0, -79178.76670476815 1468328.0932666343 0, -78783.80244007387 1468322.7237629287 0, -78388.83799037462 1468317.361506945 0, -78390.50584486716 1467917.0279575954 0, -77995.51437802658 1467912.5465573752 0, -77602.2230717691 1467908.1103326255 0, -77598.90786077552 1468306.703451055 0, -77200.18359123629 1468303.5016689505 0, -76801.45925100632 1468300.3075329098 0, -76802.03431127718 1467901.2531946185 0, -76802.60901184396 1467502.199791674 0, -77206.78939066017 1467505.8796845758 0, -77605.54725098587 1467509.5182296687 0, -77608.86236453296 1467110.92697817 0, -77612.17940369465 1466712.3336952042 0, -77707.29768090852 1466711.409553167 0, -78000.44862841813 1466713.0722712893 0, -78077.94959848991 1466713.5141808693 0, -78097.1652613044 1466713.6233066784 0, -78395.50783970584 1466715.3248715913 0, -78393.84103240023 1467116.3749945476 0, -78392.1734950474 1467516.7065576164 0)), ((-76782.72420252988 1470740.2808473867 0, -76781.08203179369 1471145.9517177728 0, -76380.50208992962 1471138.378970792 0, -76381.78392098352 1470733.0298483379 0, -76782.72420252988 1470740.2808473867 0)), ((-77179.65864762946 1471559.5372781712 0, -76779.43967544501 1471551.6236386464 0, -76781.08203179369 1471145.9517177728 0, -77181.66134467519 1471153.5436100482 0, -77179.65864762946 1471559.5372781712 0)), ((-79146.81281348842 1472396.2512589945 0, -79140.61974757117 1472803.3747966662 0, -79134.43577765398 1473210.4882480218 0, -78739.35727956427 1473205.5637737243 0, -78344.28751587989 1473200.6466055228 0, -77949.2084553448 1473195.7590968036 0, -77554.13813230445 1473190.8788940117 0, -77560.57246205317 1472785.022397899 0, -77567.00712318752 1472379.166843352 0, -77573.44201667445 1471973.3122287374 0, -77579.87724151628 1471567.4585586996 0, -77974.70586533543 1471571.07077523 0, -78369.53426474784 1471574.7014273494 0, -78764.3626362148 1471578.3505214434 0, -79159.19068110157 1471582.0180482545 0, -79152.99714981088 1471989.139693693 0, -79146.81281348842 1472396.2512589945 0)), ((-75155.10049342593 1473970.4365271246 0, -74758.52890858566 1473965.4377548 0, -74361.9569061379 1473960.4577092486 0, -74370.26947124716 1473556.329627542 0, -74765.9290483378 1473560.9770007825 0, -75161.58816727453 1473565.6540061552 0, -75155.10049342593 1473970.4365271246 0)), ((-75896.04569409085 1477223.8999372446 0, -75907.53815585666 1476812.5349223502 0, -75919.04025620785 1476401.1708250658 0, -76316.6850277755 1476404.7347425506 0, -76714.3385027527 1476408.3173569816 0, -76704.83045532278 1476820.1357947802 0, -76695.32292237412 1477231.9551742098 0, -76295.68441689387 1477227.9180969333 0, -75896.04569409085 1477223.8999372446 0)), ((-77502.12188235376 1476827.8118377703 0, -77509.63597611152 1476415.5386631575 0, -77905.59010033954 1476419.1618015105 0, -78301.55301737858 1476422.80353985 0, -78295.7128441506 1476833.5912921042 0, -77898.91747393653 1476830.6922583473 0, -77502.12188235376 1476827.8118377703 0)), ((-79044.65767861178 1481725.5478045952 0, -79038.78535595296 1482134.846635242 0, -79032.9132606372 1482544.1462823348 0, -79027.04128746063 1482953.4469429601 0, -78630.01767268042 1482951.4698751802 0, -78232.99418151262 1482949.5001937947 0, -77835.97061717378 1482947.5604127108 0, -77842.02191911906 1482539.5384921462 0, -77848.07334406668 1482131.5175800927 0, -77451.17248735616 1482130.4489151596 0, -77457.28099824005 1481722.8662424556 0, -77463.39869682437 1481315.273454886 0, -77860.17692336692 1481315.4896046645 0, -78256.96415067052 1481315.7244291909 0, -78653.74264131994 1481315.9777714645 0, -79050.53022548153 1481316.2498928355 0, -79044.65767861178 1481725.5478045952 0)), ((-81737.67655415121 1489839.4998658367 0, -81734.41467692757 1490246.1763924775 0, -81337.73142633653 1490244.2821665567 0, -81340.26886977302 1489839.839216485 0, -81342.81482949035 1489435.4084213425 0, -81740.9293065554 1489432.835344033 0, -81737.67655415121 1489839.4998658367 0)), ((-78105.9029157806 1491651.3180214781 0, -77943.4635285838 1491697.9103538394 0, -77800.2354278012 1491728.6524002533 0, -77758.57586558502 1491755.523819623 0, -77726.74181623857 1491776.0669087328 0, -77685.11704560723 1491811.7549599071 0, -77641.55962309029 1491843.3032152257 0, -77361.53984036179 1491838.924181439 0, -77372.70585425894 1491434.357054196 0, -77383.8726132515 1491029.7908901575 0, -77776.0745694919 1491033.811189111 0, -78168.28525969242 1491037.8385189262 0, -78159.77794303854 1491444.5684911206 0, -78155.76251619754 1491636.5996594129 0, -78105.9029157806 1491651.3180214781 0)), ((-72783.8423901512 1471704.0374508759 0, -72785.0804528673 1471501.0939703688 0, -73186.01866375015 1471505.4085435928 0, -73586.96563943435 1471509.7309307079 0, -73584.44881395398 1471916.8951096733 0, -73581.93179138654 1472324.0602375388 0, -73181.03458503803 1472318.4496924768 0, -72780.14584311745 1472312.8694722622 0, -72782.61324409813 1471906.9812994741 0, -72783.8423901512 1471704.0374508759 0)), ((-73106.98046267036 1478020.6858961042 0, -72706.00587628513 1478017.2432034067 0, -72712.5810310503 1477606.2580667168 0, -72719.1654451168 1477195.2627430637 0, -72725.7411886632 1476784.279489158 0, -72732.32628738073 1476373.286155441 0, -73131.68527515934 1476377.1404321832 0, -73531.0441051904 1476381.0024212839 0, -73525.2671029627 1476791.7899665176 0, -73519.49911247358 1477202.578632568 0, -73513.72244872533 1477613.3569525203 0, -73507.95495026246 1478024.1475031818 0, -73106.98046267036 1478020.6858961042 0)), ((-73462.35017146051 1482876.926183777 0, -73061.99030506378 1482867.0610211508 0, -72661.63868421168 1482857.2037324922 0, -72666.7907703602 1482456.4443878005 0, -72671.95195291903 1482055.6748024123 0, -72677.10430189109 1481654.9172329714 0, -72682.26584621612 1481254.1494288705 0, -73080.68958295415 1481259.2852823783 0, -73479.12197519674 1481264.4288094074 0, -73474.92443418386 1481667.5573181163 0, -73470.73597732947 1482070.675701458 0, -73466.53847965538 1482473.8061060975 0, -73462.35017146051 1482876.926183777 0)), ((-73811.07199247112 1487747.3197786026 0, -73411.26325581915 1487742.5579352174 0, -73011.44529394088 1487737.8148849728 0, -72611.63593622523 1487733.090990431 0, -72615.44642045179 1487328.0527376777 0, -72619.26597795894 1486923.0043464545 0, -72623.07648364383 1486517.967966331 0, -72626.89606561416 1486112.9213498733 0, -73025.10532035124 1486116.3427618532 0, -73423.32328251275 1486119.7831331035 0, -73821.53222162319 1486123.2421043727 0, -74219.7499639757 1486126.7200383083 0, -74217.53048460835 1486533.06942103 0, -74215.31987961197 1486939.408571468 0, -74213.10021863587 1487345.75974349 0, -74210.88933316348 1487752.100677042 0, -73811.07199247112 1487747.3197786026 0)), ((-73394.406220938 1489370.4582932952 0, -72994.63650286454 1489367.0033677176 0, -72594.86667667152 1489363.5674111494 0, -72599.05435651711 1488955.9524841164 0, -72603.25120009242 1488548.3274226103 0, -73003.04512184244 1488552.4129915608 0, -73402.83016393267 1488556.506249862 0, -73398.61813673293 1488963.4818785738 0, -73394.406220938 1489370.4582932952 0)), ((-74158.06829237098 1492220.0473752772 0, -74153.14957895926 1492626.3752554955 0, -73755.23860029077 1492622.898048667 0, -73357.33642570979 1492619.439677622 0, -72959.42522314904 1492615.9999809267 0, -72561.52272884907 1492612.5791166173 0, -72566.03623421623 1492206.2480470145 0, -72570.5499928527 1491799.9067446238 0, -72575.06371311886 1491393.5775203118 0, -72579.57768964935 1490987.2379654038 0, -72977.89432331357 1490990.661885849 0, -73376.21074710423 1490994.1046653092 0, -73774.52705842246 1490997.566307073 0, -74172.84325876497 1491001.0467103643 0, -74167.91513231414 1491407.3831011858 0, -74162.9961863709 1491813.7092402768 0, -74158.06829237098 1492220.0473752772 0)), ((-73315.39576219047 1496667.5184320232 0, -73311.87112640621 1497072.5860726952 0, -73308.3465547544 1497477.6433546988 0, -72910.65339447763 1497475.492414335 0, -72512.96894450676 1497473.3602820307 0, -72515.09779713205 1497068.2913186175 0, -72517.23542850235 1496663.2119757372 0, -72519.36400391452 1496258.1446141803 0, -72521.50145070507 1495853.0670811085 0, -72921.96873490834 1495855.2224859106 0, -73322.44493234492 1495857.3969116756 0, -73318.9202657671 1496262.462848082 0, -73718.69392889713 1496264.6502827364 0, -74118.46758251335 1496266.8566566226 0, -74113.55596362872 1496671.9003338972 0, -73714.47591854482 1496669.699915538 0, -73315.39576219047 1496667.5184320232 0)), ((-68716.28715733084 1457662.6673331738 0, -68319.78673984166 1457660.2634012292 0, -68323.3085050544 1457296.5798658333 0, -68327.55830284423 1456858.134074846 0, -68404.78808497394 1456856.9607504753 0, -68542.26614334645 1456856.7278929604 0, -68718.23827123755 1456859.0493941552 0, -68726.15282215334 1456859.0229096212 0, -69124.77482946745 1456857.6889971583 0, -69118.08395414182 1457307.7263641078 0, -69112.76960980173 1457665.101003152 0, -68716.28715733084 1457662.6673331738 0)), ((-69112.76960980173 1457665.101003152 0, -69509.2252300812 1457667.5529240628 0, -69905.66293127806 1457670.0232760746 0, -69897.71093876303 1458065.4895449802 0, -69889.76831001487 1458460.9568472856 0, -69495.29309643655 1458465.0102036747 0, -69100.81851394827 1458469.081940904 0, -69106.79836496325 1458067.0910200493 0, -69112.76960980173 1457665.101003152 0)), ((-68265.55376762456 1462120.842958668 0, -68270.86257824222 1461715.4101024538 0, -68672.35854252106 1461707.9745270105 0, -68667.87901178085 1462114.2538504149 0, -68265.55376762456 1462120.842958668 0)), ((-69469.7016877606 1462509.117615047 0, -69472.53194670076 1462101.132937958 0, -69874.85953203446 1462094.601232029 0, -69872.85819620869 1462503.4438875634 0, -69469.7016877606 1462509.117615047 0)), ((-68658.91150164811 1462926.815374739 0, -68663.39967038295 1462520.534160996 0, -69066.54587462494 1462514.82181863 0, -69062.89568996085 1462921.9497890717 0, -68658.91150164811 1462926.815374739 0)), ((-69464.04116429258 1463325.101255726 0, -69059.23643160626 1463329.0897672 0, -69062.89568996085 1462921.9497890717 0, -69466.87136078413 1462917.1145921382 0, -69464.04116429258 1463325.101255726 0)), ((-68070.97382668841 1467017.7268901884 0, -68469.7292301333 1467021.8865791103 0, -68857.30066220576 1467025.9521993226 0, -68854.04034194387 1467426.9148184566 0, -68462.74164021191 1467423.5583364775 0, -68063.99915069967 1467420.1491944445 0, -68070.97382668841 1467017.7268901884 0)), ((-68823.85284031251 1471473.2720650278 0, -69219.00827020477 1471477.3181145815 0, -69214.52457870312 1471880.8238985334 0, -69609.49699118786 1471884.259872912 0, -69604.83073161803 1472287.1267754582 0, -70003.68883720908 1472290.8372440063 0, -70402.5556694541 1472294.566627038 0, -70399.19699834677 1472698.2967443974 0, -70395.83818638064 1473102.0390026513 0, -69995.66397521242 1473097.4473370858 0, -69595.489572429 1473092.8746070163 0, -69201.04718028326 1473091.3692442202 0, -68806.61386720366 1473089.8710823462 0, -68412.17160365012 1473088.402473695 0, -68017.73832011299 1473086.941163461 0, -68021.68231955219 1472681.5131904404 0, -68025.63522818575 1472276.0862378 0, -68029.579307281 1471870.6602514712 0, -68033.53229862524 1471465.2351876101 0, -68428.68820467472 1471469.2443685364 0, -68823.85284031251 1471473.2720650278 0), (-68815.23313162997 1472281.5752484035 0, -68420.43429445382 1472278.8159761755 0, -68416.30743302511 1472683.6031924854 0, -68810.92349732069 1472685.722748532 0, -69205.53962453955 1472687.8494265021 0, -69210.03192517218 1472284.3418452954 0, -68815.23313162997 1472281.5752484035 0)), ((-69522.15446900025 1482830.893701603 0, -69123.47348779865 1482825.059908694 0, -68724.79211528102 1482819.2448085628 0, -68326.11034684895 1482813.448602851 0, -67927.4281872374 1482807.671190586 0, -67933.70917368594 1482404.3678271857 0, -67939.99938292651 1482001.0654413034 0, -67946.2809779465 1481597.763974841 0, -67952.57179886349 1481194.4633879473 0, -68350.34985628433 1481197.2427551718 0, -68748.13669430156 1481200.0296888822 0, -69145.91448110873 1481202.8464470827 0, -69543.7011412685 1481205.670876026 0, -69538.31417771222 1481611.980797098 0, -69532.92745992675 1482018.280421368 0, -69527.54079047615 1482424.5922603 0, -69522.15446900025 1482830.893701603 0)), ((-67892.24638253797 1487693.9654716563 0, -67893.12802024258 1487288.0317217195 0, -67894.01836183699 1486882.0988450435 0, -68291.85192239353 1486885.518761311 0, -68689.6764785695 1486888.9572735499 0, -68688.09730991194 1487292.958320995 0, -68686.50926408112 1487696.949071745 0, -68289.37338325944 1487695.4535024615 0, -67892.24638253797 1487693.9654716563 0)), ((-69460.74028591247 1490955.9251496722 0, -69455.73883153363 1491358.843384699 0, -69450.73763632438 1491761.7512765592 0, -69445.73650491417 1492164.6712367663 0, -69440.73563277465 1492567.5808507903 0, -69041.46205833417 1492565.6029826896 0, -68642.1883931633 1492563.6440642118 0, -68242.91474100157 1492561.7039974695 0, -67843.641100357 1492559.7828831812 0, -67848.24540976863 1492154.742009156 0, -67852.85878052186 1491749.690874933 0, -67857.46338207013 1491344.651739831 0, -67862.07704177184 1490939.6024484432 0, -68261.73875772397 1490943.6546189454 0, -68661.40909716283 1490947.7259288074 0, -69061.07042935371 1490951.8160214415 0, -69460.74028591247 1490955.9251496722 0)), ((-68116.37177006259 1501897.3383576204 0, -68126.84491657955 1501490.7161943768 0, -68529.21037161048 1501496.7372952104 0, -68932.82558906545 1501502.7990234075 0, -69333.93974638608 1501508.8483561627 0, -69331.77042311574 1501622.5889506491 0, -69286.69055662438 1501638.9104242355 0, -69111.00870344945 1501760.628430932 0, -68988.62228568728 1501823.7718888212 0, -68925.74729243135 1501860.449990843 0, -68919.23347249403 1501864.25042706 0, -68878.58974007465 1501866.4842912147 0, -68833.85157873812 1501873.815571348 0, -68519.65665870799 1501902.4034048666 0, -68158.85789087966 1501955.57406742 0, -68114.76744510683 1501959.7104836234 0, -68116.37177006259 1501897.3383576204 0)), ((-62765.870463157684 1457631.1113722716 0, -63173.204197965686 1457631.9602979622 0, -63169.192205450105 1458050.5886319955 0, -62762.670236827405 1458049.992290071 0, -62765.870463157684 1457631.1113722716 0)), ((-64357.87710152739 1458472.9253500819 0, -64362.94966577158 1458055.065998283 0, -64756.8480301289 1458057.020718102 0, -64750.27846745622 1458474.6108937962 0, -64357.87710152739 1458472.9253500819 0)), ((-64689.91265037442 1462518.0587928589 0, -64692.678469094346 1462110.4870911818 0, -65083.91148158896 1462110.0514362354 0, -65082.481088544344 1462517.633267065 0, -64689.91265037442 1462518.0587928589 0)), ((-61968.10040083134 1464156.395643531 0, -61968.65236750214 1463753.507234142 0, -61969.21316840847 1463350.6085721855 0, -62345.70425986705 1463346.6241027862 0, -62722.18682288851 1463342.667499843 0, -62719.0939929303 1463747.0146269056 0, -62343.87296629526 1463750.2525600914 0, -62342.05060267976 1464153.8709672058 0, -61968.10040083134 1464156.395643531 0)), ((-64639.10250741785 1466586.2624055236 0, -64871.18963472081 1466591.947183293 0, -64871.49262868909 1466997.4360953786 0, -64871.79721500024 1467402.9052374384 0, -64872.0926068738 1467808.3863771397 0, -64872.39652821976 1468213.8574542922 0, -64473.66708744734 1468210.4148012123 0, -64074.9376274702 1468206.979692928 0, -63676.20775951663 1468203.5745332444 0, -63277.477872478405 1468200.1770189996 0, -63283.2422025026 1467792.1980356672 0, -63289.00679604657 1467384.220123276 0, -63294.77146125358 1466976.2430753692 0, -63300.52947156712 1466568.256785785 0, -63458.23743561229 1466557.445906576 0, -63699.45233110076 1466563.3232785854 0, -63851.85992591725 1466567.029380438 0, -64073.565981780346 1466572.446444327 0, -64245.4815870214 1466576.6423174897 0, -64451.32960565389 1466581.6733178198 0, -64472.37824943185 1466582.1873840007 0, -64481.98856551679 1466582.422583497 0, -64639.10250741785 1466586.2624055236 0)), ((-64857.43545704778 1469806.5296919842 0, -64852.95751281315 1470213.2683675576 0, -64848.48880907546 1470619.9967769198 0, -64844.011216611136 1471026.7372673748 0, -64447.18490131639 1471026.9157780155 0, -64050.349761172336 1471027.1240467762 0, -64054.28248218588 1470619.1136933358 0, -64058.21541743825 1470211.0929962094 0, -64062.14826908621 1469803.0845659624 0, -64459.79179643762 1469804.7977567685 0, -64857.43545704778 1469806.5296919842 0)), ((-63153.263026998946 1482373.0688574577 0, -63154.27943166256 1481963.3078288932 0, -63155.295641045705 1481553.5588365025 0, -63156.31164463289 1481143.799665942 0, -63558.49961570791 1481146.3819734827 0, -63960.69658685198 1481148.9723554885 0, -63958.63545885184 1481556.5733181941 0, -63956.57424655755 1481964.1864108923 0, -63954.51294586771 1482371.7892143116 0, -63553.88793631426 1482372.4139900033 0, -63153.263026998946 1482373.0688574577 0)), ((-64360.30535164532 1481558.114853869 0, -64362.884331031826 1481151.593056879 0, -64765.08107513099 1481154.2217321144 0, -64761.97528442547 1481559.6753837664 0, -64360.30535164532 1481558.114853869 0)), ((-61529.93918322497 1483179.4620294496 0, -61524.2805911519 1483584.4761984076 0, -61122.543482454974 1483582.4299722 0, -61117.23893683938 1483987.8845531826 0, -61518.62222184279 1483989.5025764795 0, -61512.96417637525 1484394.5185458958 0, -61111.93475603687 1484393.3401405702 0, -60710.91425145823 1484392.1695856592 0, -60715.864616257815 1483986.2856948737 0, -60720.80617953477 1483580.413934021 0, -60725.756872276506 1483174.531949947 0, -61127.84805467721 1483176.987395192 0, -61133.152940064036 1482771.5346172468 0, -61535.59799695511 1482774.4375526197 0, -61529.93918322497 1483179.4620294496 0)), ((-67108.53758810216 1485249.161130611 0, -66711.63964930753 1485245.8168478608 0, -66718.91239671793 1484838.9874636875 0, -66726.19430410383 1484432.17026336 0, -67120.42201569056 1484435.2806208015 0, -67114.47965807382 1484842.2204248803 0, -67108.53758810216 1485249.161130611 0)), ((-64707.24631959418 1486848.693344332 0, -64310.89982134748 1486848.461877233 0, -63914.562519170686 1486848.2378552218 0, -63518.216284888484 1486848.0436269615 0, -63121.87915077506 1486847.8568403702 0, -63122.211479229285 1486440.6344615344 0, -63122.54346765946 1486033.4129834045 0, -63520.77990167543 1486034.2522291723 0, -63919.02519303734 1486035.1102237697 0, -64317.261599684854 1486035.9870114299 0, -64715.50705539568 1486036.8826554 0, -64711.376596860944 1486442.7876021147 0, -64707.24631959418 1486848.693344332 0)), ((-63862.80037408337 1491719.1394664752 0, -63857.864542699404 1492125.2525310528 0, -63852.92893964328 1492531.3776790355 0, -63453.975790968056 1492529.6750046334 0, -63119.644567315525 1492528.2584630174 0, -63152.39721863247 1492279.992425256 0, -63162.926657931355 1492120.9957428244 0, -63166.029102282315 1492074.1845585853 0, -63255.193911809416 1491714.266784929 0, -63288.61311190588 1491579.3903222217 0, -63352.9430670904 1491330.7455435104 0, -63366.92969748732 1491308.0546361422 0, -63405.986436760286 1491244.709654339 0, -63455.04808429261 1491151.0272579635 0, -63470.196742531036 1491115.5641529025 0, -63472.64394193631 1490902.1917070018 0, -63872.672661517754 1490906.893646237 0, -63867.73643073226 1491313.0160681396 0, -63862.80037408337 1491719.1394664752 0)), ((-59211.873119999356 1456830.77603724 0, -59224.456019261 1456831.0429567136 0, -59434.29515542788 1456834.9764043195 0, -59610.826408002096 1456832.3784809886 0, -59635.17836743209 1456832.0201052187 0, -59824.285306299025 1456830.217385985 0, -60001.68925675221 1456831.8079452873 0, -60009.78134123556 1456831.7819637796 0, -60066.95101347023 1456831.5984073314 0, -60068.73478554488 1456831.4990560154 0, -60205.943693296336 1456831.2410202716 0, -60406.36478885451 1456830.6516865261 0, -60408.74791975078 1456830.6444257058 0, -60406.55116278666 1457231.3319150514 0, -60404.39372121041 1457626.5660628132 0, -60005.654377707615 1457625.8660749742 0, -59606.91500056899 1457625.1847687091 0, -59208.175829105116 1457624.5111460083 0, -58809.44549885816 1457623.8674895084 0, -58811.1596926088 1457231.6650203892 0, -58812.92706610567 1456829.252493636 0, -58867.93547895349 1456830.5741624483 0, -58929.096305208244 1456830.3273659032 0, -58940.15622452364 1456829.6203141364 0, -58942.49075221615 1456828.6903588783 0, -58984.34670962438 1456828.5747660052 0, -58984.73614294449 1456829.1465843164 0, -58989.43140436629 1456833.435210305 0, -58995.11587666236 1456836.498746018 0, -58998.68339046342 1456836.299592404 0, -59004.656363540285 1456836.3411895714 0, -59013.13945699367 1456834.3843056366 0, -59014.74578607603 1456834.1714982127 0, -59022.32890190666 1456833.4403357664 0, -59200.833906289445 1456830.5418637756 0, -59211.873119999356 1456830.77603724 0)), ((-55611.25037662114 1460879.9836761837 0, -56008.45217788736 1460883.4347875428 0, -56405.6537992782 1460886.915780435 0, -56401.06995850919 1461295.7515157794 0, -56396.486349868755 1461704.5882537488 0, -56000.50767029506 1461699.8501837708 0, -55604.53757540827 1461695.13056186 0, -55607.88948005015 1461287.5621334126 0, -55611.25037662114 1460879.9836761837 0)), ((-59586.90384327079 1462937.1210004834 0, -59586.860755434 1462530.378443201 0, -59586.81735612491 1462123.625670543 0, -59184.79447096355 1462125.953944134 0, -58782.780833740486 1462128.3125697288 0, -58781.84013370392 1461723.2794581729 0, -59184.306604525525 1461720.072692798 0, -59586.77355300804 1461716.8850962117 0, -59989.24097749075 1461713.7166686326 0, -60391.708879395715 1461710.5673094199 0, -60390.85513152627 1462119.0263394606 0, -60390.0012230727 1462527.4863707004 0, -60389.14715411335 1462935.9474016263 0, -60388.29282570612 1463344.4094275492 0, -59987.619695360954 1463344.1330602881 0, -59586.946774718184 1463343.864452334 0, -59586.90384327079 1462937.1210004834 0)), ((-58785.60108729455 1463343.3953288926 0, -58784.66140788706 1462938.3705601618 0, -59185.7781056678 1462937.730605538 0, -59186.27387403317 1463343.6260126813 0, -58785.60108729455 1463343.3953288926 0)), ((-60011.75046559958 1471404.9019232679 0, -60006.48534666255 1471811.1915328652 0, -60001.22934914714 1472217.4710642956 0, -59995.964647882356 1472623.7626719454 0, -59990.7090711926 1473030.0440975253 0, -59596.94026538472 1473030.6950534307 0, -59203.17161203407 1473031.3644279628 0, -58809.403118890616 1473032.0520191959 0, -58415.634883428844 1473032.7579309447 0, -58419.79125454428 1472626.4685756273 0, -58423.95674350775 1472220.1689420724 0, -58428.113420171954 1471813.8813861432 0, -58432.279211508205 1471407.5836558864 0, -58827.14676193457 1471406.8855596685 0, -59222.01447282238 1471406.20588804 0, -59616.88234259795 1471405.5446411776 0, -60011.75046559958 1471404.9019232679 0)), ((-59963.96403483528 1477092.3084086585 0, -59560.86639134121 1477094.394850683 0, -59157.76911337094 1477096.5006008502 0, -58754.681169332514 1477098.6144312948 0, -58756.60498100959 1477505.4938260838 0, -58758.52847541702 1477912.3629571062 0, -58356.15109488709 1477915.1388394057 0, -58353.863665549 1477507.9538110218 0, -58351.58463358268 1477100.7585953618 0, -58349.29607167435 1476693.5754474406 0, -58347.01610491499 1476286.3821215695 0, -58750.82314530572 1476284.8808011408 0, -59154.63050365464 1476283.3875843715 0, -59558.438084494635 1476281.9248849947 0, -59962.246078974735 1476280.4702927878 0, -59963.10518517892 1476686.38882966 0, -59963.96403483528 1477092.3084086585 0)), ((-59521.43327767718 1482763.9767366445 0, -59125.627041188716 1482765.0130992145 0, -58725.52798958133 1482766.0832141032 0, -58325.43806745689 1482767.1610821565 0, -58326.88108155291 1482360.830585806 0, -58328.3328035355 1481954.4899755341 0, -58329.77551014224 1481548.1613108742 0, -58331.227023492705 1481141.8225384678 0, -58731.074028531446 1481139.4545733768 0, -59130.921444746746 1481137.0943898559 0, -59530.769179281066 1481134.7643012118 0, -59930.617321770456 1481132.4419944976 0, -59929.4174391128 1481540.0709276577 0, -59928.21754873335 1481947.6895804033 0, -59927.01725610088 1482355.320456829 0, -59925.81705803572 1482762.9409519762 0, -59521.43327767718 1482763.9767366445 0)), ((-55635.311805134625 1458448.2564021756 0, -55234.06788554167 1458445.6478521451 0, -54832.82394546621 1458443.0582901954 0, -54834.00679921864 1458028.640697642 0, -54835.18010645418 1457618.457472443 0, -54433.89219920776 1457618.0145234528 0, -54432.74299621733 1458026.070000953 0, -54431.579785453105 1458440.4878108113 0, -54030.33550926287 1458437.9363160762 0, -54026.801712754015 1458362.7633765682 0, -54027.73524043028 1458023.4945903153 0, -54028.86004789654 1457617.5893669114 0, -54029.961793319126 1457219.5135328933 0, -54398.89015186742 1457223.8635567462 0, -54435.00294333219 1457224.2955838796 0, -54602.8733692096 1457226.2846808631 0, -54796.34469878411 1457228.580805024 0, -54836.29961639585 1457229.0505198918 0, -55232.7821470563 1457233.77078032 0, -55284.147643807395 1457234.3837291652 0, -55405.222825814955 1457233.3776000831 0, -55405.980958980166 1457156.6757374194 0, -55409.17514890151 1456831.8942117542 0, -55633.673235305636 1456831.5640444045 0, -55634.0774492578 1457233.2212568552 0, -55634.47571773122 1457619.3902288661 0, -55233.18763976876 1457618.909409966 0, -55233.63037835485 1458031.2197791704 0, -55634.8939439233 1458033.8283480564 0, -55635.311805134625 1458448.2564021756 0)), ((-55602.56072466702 1462102.272144537 0, -55205.75826270731 1462098.2937470493 0, -54808.95546817549 1462094.334016074 0, -54806.720387551344 1462493.5677850095 0, -54806.63057639425 1462510.2553047605 0, -55203.61165645563 1462509.8144673905 0, -55600.59277002397 1462509.40349477 0, -55598.615779268766 1462916.5470658548 0, -55596.64768165351 1463323.6805023204 0, -55199.35733823885 1463324.100877033 0, -54802.0671244379 1463324.5286006304 0, -54404.77714178713 1463324.986292651 0, -54007.4872919243 1463325.4513332203 0, -54007.899913989975 1463260.493309037 0, -54010.073801764265 1462918.310309561 0, -54010.38603975884 1462869.155090864 0, -54012.66023790727 1462511.170275272 0, -54012.872203118364 1462477.8065984 0, -54015.35821327567 1462086.4702414405 0, -54015.65897780112 1462039.129614401 0, -54017.84435989956 1461695.1236160547 0, -54414.512936381434 1461695.1030421993 0, -54811.19075683259 1461695.0899109629 0, -55207.85959365853 1461695.1065669444 0, -55604.53757540827 1461695.13056186 0, -55602.56072466702 1462102.272144537 0)), ((-55342.74748418175 1466923.4431292922 0, -55334.037804795356 1467320.2820014 0, -55325.319653137354 1467717.132925389 0, -55316.61115344242 1468113.9736530425 0, -54919.92161127385 1468111.408879433 0, -54523.232038017624 1468108.8627514371 0, -54126.54224034806 1468106.3351617833 0, -53729.85241788153 1468103.8261165686 0, -53736.79328923291 1467704.397088806 0, -53743.734573035275 1467304.957893284 0, -53750.67609346391 1466905.5304359812 0, -53757.61087573576 1466506.0803710104 0, -53984.61150689138 1466505.834221939 0, -54154.376942137504 1466508.4003595642 0, -54383.767297157516 1466511.8650833538 0, -54558.08271729824 1466514.5130482686 0, -54673.455910126984 1466516.2636795097 0, -54782.91369506975 1466517.9258263514 0, -54954.771379526945 1466520.532554123 0, -55085.22242571772 1466522.5219543953 0, -55182.06852604135 1466523.994194958 0, -55351.459457735815 1466526.5819171064 0, -55342.74748418175 1466923.4431292922 0)), ((-54437.45633102092 1473002.149816702 0, -54036.249385205825 1472997.4680578422 0, -53635.042017812564 1472992.8052231288 0, -53640.33547453616 1472585.6486189482 0, -53645.62916690169 1472178.4928648104 0, -53650.923187708395 1471771.338167099 0, -53656.21734202122 1471364.1844202094 0, -54053.777630043645 1471366.6965263225 0, -54451.33779454803 1471369.2272613645 0, -54848.897929839084 1471371.7767294815 0, -55246.45783938789 1471374.3448236906 0, -55244.81088354941 1471783.649774568 0, -55243.16384457587 1472192.9557942764 0, -55241.51662971217 1472602.2626764013 0, -55239.869331834845 1473011.5706242684 0, -54838.66304542229 1473006.8507078427 0, -54437.45633102092 1473002.149816702 0)), ((-54364.71976297105 1477875.9455088866 0, -53966.113436532076 1477872.12209582 0, -53567.51570134676 1477868.3174651999 0, -53572.77871317961 1477465.4391570096 0, -53578.04212444378 1477062.5504625118 0, -53583.3056375242 1476659.6739916531 0, -53588.56954686063 1476256.7872383534 0, -53981.82571534432 1476259.2703887362 0, -54375.0906704107 1476261.771825559 0, -54768.34667027248 1476264.291593851 0, -55161.61145363829 1476266.8296488635 0, -55161.68973319344 1476671.0386641163 0, -55161.76770194499 1477075.2373012968 0, -55161.845458281394 1477479.4481800615 0, -55161.922900922014 1477883.6487785915 0, -54763.31704102112 1477879.787651511 0, -54364.71976297105 1477875.9455088866 0)), ((-55139.43139998577 1481129.0543784054 0, -55535.49287120528 1481134.2058046963 0, -55536.109432048936 1481542.5850004298 0, -55536.725664160724 1481950.9764349603 0, -55140.18882863359 1481946.8969264938 0, -55139.8058213658 1481537.9808017237 0, -55139.43139998577 1481129.0543784054 0)), ((-53952.327663839846 1482370.9475391738 0, -53817.48392704566 1482372.6813293078 0, -53801.1286038638 1482337.7652295681 0, -53756.56172820017 1482271.8458778798 0, -53728.543505835885 1482208.999409983 0, -53693.42278967698 1482146.119509787 0, -53677.54624363191 1482035.6113478327 0, -53630.48998021395 1481987.576223098 0, -53612.10264307511 1481956.0641150791 0, -53949.90300319273 1481954.0091899482 0, -54346.667441162 1481951.6273160973 0, -54348.405468717596 1482365.8845208483 0, -54350.14284359606 1482780.153775593 0, -53984.40696238312 1482787.3021100988 0, -53964.32770064578 1482738.6518689082 0, -53954.282528593365 1482708.2111093053 0, -53952.327663839846 1482370.9475391738 0)), ((-54346.96940176124 1483591.9856132441 0, -54745.04259450156 1483584.2883362921 0, -55143.11657692817 1483576.6098261075 0, -55144.20179620003 1483982.5444637067 0, -55145.286645822125 1484388.4800136928 0, -54744.54062250704 1484396.1410693242 0, -54744.7872843303 1483990.2142077207 0, -54345.38248094375 1483997.9028974713 0, -54346.96940176124 1483591.9856132441 0)), ((-45679.57774402716 1458344.7745282666 0, -45283.80216922092 1458340.953023227 0, -45286.2128981814 1457932.8013932784 0, -44890.52537205971 1457928.9091915225 0, -44893.033490231304 1457520.658180095 0, -45288.614694046126 1457524.650801352 0, -45290.41695972511 1457185.6785385848 0, -45672.17033124869 1457187.7117994644 0, -45686.02371036831 1457187.8418430975 0, -45903.64319281727 1457189.9046413011 0, -46021.46564800319 1457191.0207629127 0, -46081.62189090691 1457191.5916571051 0, -46079.776422967625 1457532.6913938012 0, -46077.569187922614 1457940.6524837103 0, -46075.361987954195 1458348.6033849001 0, -45679.57774402716 1458344.7745282666 0)), ((-49275.7104058897 1458368.1574746585 0, -49279.886499582135 1457967.0842251172 0, -49682.49577839283 1457968.4667465738 0, -49678.31743328168 1458366.6614022406 0, -49275.7104058897 1458368.1574746585 0)), ((-46066.496649131455 1462814.529511264 0, -46063.99570306126 1463215.7035277206 0, -45675.93001461384 1463207.2125828606 0, -45287.8635580826 1463198.7280879538 0, -44899.79643893018 1463190.2725606281 0, -44511.72832889258 1463181.8243846882 0, -44512.14211326173 1462778.9367030575 0, -44512.5556498546 1462376.0386931805 0, -44512.96903963658 1461973.152974902 0, -44513.3823794641 1461570.2569376165 0, -44903.538085769665 1461580.4183427014 0, -45293.70166619253 1461590.5987003916 0, -45683.855412694014 1461600.79694751 0, -46</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Oklahoma State University, Common Schools, Public Building, State Educational Institutions, Other Agency</t>
+          <t>Oklahoma State University, Public Building, State Educational Institutions, Common Schools</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2730,7 +2730,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="G48" t="n">
         <v>3626.53</v>
@@ -2739,13 +2739,13 @@
         <v>97</v>
       </c>
       <c r="I48" t="n">
-        <v>21551.98</v>
+        <v>21471.29</v>
       </c>
       <c r="J48" t="n">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="K48" t="n">
-        <v>25178.51</v>
+        <v>25097.82</v>
       </c>
       <c r="L48" t="n">
         <v>343426.64</v>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Rural Credit, Indemnity, School and Public Lands, Common School</t>
+          <t>Rural Credit, School and Public Lands, Indemnity, Common School</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -3090,7 +3090,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON Z (((-80095.75316409435 1375386.379813748 0, -79699.10540708507 1375380.7669570895 0, -79302.45744365401 1375375.1725275088 0, -79294.48890637417 1375780.5345047028 0, -78898.29312064026 1375774.750143596 0, -78905.80898128415 1375369.5964148229 0, -78913.32531422056 1374964.4328799224 0, -78920.84184250125 1374559.2817358444 0, -78928.3588430248 1374154.1207886033 0, -79326.3474721523 1374159.0830010828 0, -79724.34472815561 1374164.0637182842 0, -80122.3327583849 1374169.0629906587 0, -80520.32951129682 1374174.080771068 0, -80511.0192425397 1374580.0636461677 0, -80501.70965628329 1374986.036721874 0, -80492.40037325167 1375392.0222900882 0, -80483.09177579182 1375797.9979551008 0, -80086.88818449556 1375792.158459221 0, -80095.75316409435 1375386.379813748 0)), ((-79663.3673255158 1381079.2003433711 0, -79669.22128833455 1380671.8766682937 0, -80064.19233757578 1380673.8590554853 0, -80459.1725541262 1380675.8486173295 0, -80455.34098896883 1381083.1911108359 0, -80451.5094824221 1381490.5236892316 0, -80054.51608741215 1381488.5153901821 0, -79657.51372285634 1381486.51420574 0, -79663.3673255158 1381079.2003433711 0)), ((-80417.18111603762 1384337.1680812407 0, -80411.26241137735 1384746.620682147 0, -80405.343778195 1385156.0858661942 0, -80399.42540788466 1385565.5410283895 0, -79996.09610218088 1385565.1761681933 0, -79592.76691785129 1385564.8302999968 0, -79189.43785660833 1385564.503423622 0, -78786.10891709107 1385564.1956397383 0, -78794.32068920239 1385156.0481444192 0, -78802.53282765877 1384747.8908165589 0, -78810.74534864214 1384339.7459646205 0, -78818.95843712795 1383931.5911885067 0, -79219.99346088669 1383930.591518075 0, -79621.02871231778 1383929.610638675 0, -80022.06428574152 1383928.648654411 0, -80423.10018254477 1383927.705464625 0, -80417.18111603762 1384337.1680812407 0)), ((-80168.65038328448 1394882.830597532 0, -80166.89567565001 1395289.8140611292 0, -79763.69404477252 1395286.4695903969 0, -79360.49236172777 1395283.1329738207 0, -78957.29044200816 1395279.8266144472 0, -78554.08857253747 1395276.5281120907 0, -78559.58517660324 1394864.4630645702 0, -78565.08202310812 1394452.3880741769 0, -78570.57892601035 1394040.325545436 0, -78576.07616723729 1393628.2531809034 0, -78975.53638895618 1393636.6338305725 0, -79374.99599673512 1393645.0331389538 0, -79774.45498583768 1393653.4512069547 0, -80173.91335767227 1393661.8879337937 0, -80172.15922283428 1394068.8675828013 0, -80170.40489801507 1394475.8484712108 0, -80168.65038328448 1394882.830597532 0)), ((-79331.23815216623 1404597.1470643461 0, -78938.50871315486 1404592.5366995477 0, -78939.45673192157 1404185.6522471572 0, -78546.12385046994 1404179.2519333921 0, -78546.47749473421 1403770.5495255494 0, -78546.83073371365 1403361.8483291662 0, -78941.35207170811 1403371.8645452405 0, -79335.88170223177 1403381.8990532432 0, -79730.40168293759 1403391.95169635 0, -80124.9297548984 1403402.0226252924 0, -80122.19133715013 1403803.4806207854 0, -80119.45285887225 1404204.9396919622 0, -80116.7143170485 1404606.3999382537 0, -80113.97560961115 1405007.8614559695 0, -79721.83132028599 1405005.0340105535 0, -79329.6958423238 1405002.2247352568 0, -79331.23815216623 1404597.1470643461 0)), ((-80069.72565184273 1413538.4249001627 0, -80068.9550786488 1413947.599890792 0, -80068.17518784608 1414356.7759782397 0, -80067.40391925538 1414765.9533187926 0, -79668.29755106315 1414753.6888200454 0, -79269.19028742381 1414741.431896158 0, -78870.08194480596 1414729.204852005 0, -78470.97280904154 1414716.9853858205 0, -78476.4111616019 1414311.2662390275 0, -78481.84973640332 1413905.5483507852 0, -78487.16972251602 1413508.8325250563 0, -78492.72726779335 1413094.1159431427 0, -78887.16816929696 1413102.8779558737 0, -79281.61740929245 1413111.647113821 0, -79676.05696051444 1413120.4455670826 0, -80070.50494308618 1413129.2512695955 0, -80069.72565184273 1413538.4249001627 0)), ((-80032.0064657411 1424495.8148202808 0, -79636.03941873503 1424488.695630517 0, -79240.07174824749 1424481.5948644897 0, -78844.1036539705 1424474.5125283413 0, -78448.13513751305 1424467.4486219725 0, -78448.11573366894 1424061.6517925377 0, -78448.09603747445 1423655.8560905743 0, -78448.0760488453 1423250.0615175648 0, -78448.05556960235 1422844.2680687795 0, -78846.86960073255 1422847.0804530159 0, -79245.68367363935 1422849.9002694085 0, -79644.49749550546 1422852.7500225715 0, -80043.31135283226 1422855.6073089882 0, -80040.48524821257 1423265.6630482927 0, -80037.65909602337 1423675.7087274988 0, -80034.83280612587 1424085.7667550715 0, -80032.0064657411 1424495.8148202808 0)), ((-79710.36863067093 1433784.0035331955 0, -79308.10237544689 1433796.1775997076 0, -79318.31912815449 1433387.1355027698 0, -79328.53646977848 1432978.1057076203 0, -79732.41442013884 1432963.1592898376 0, -79721.395618494 1433373.5808994535 0, -79710.36863067093 1433784.0035331955 0)), ((-76563.9261230747 1368439.1828783904 0, -76161.27347439683 1368434.6234563526 0, -76160.13206153525 1368026.0575461774 0, -76158.90794607016 1367588.2233920358 0, -76556.87555699312 1367592.180915083 0, -76560.48064201119 1368025.4363120983 0, -76563.9261230747 1368439.1828783904 0)), ((-76894.69093255623 1378618.792492289 0, -76500.7049210963 1378615.0408743955 0, -76495.38712744905 1378207.4898598115 0, -76489.96052108797 1377791.891191295 0, -76879.45546421342 1377795.9039369412 0, -77268.94104768967 1377799.945595253 0, -77278.91708364207 1378215.787688862 0, -77288.67689167186 1378622.5512123925 0, -76894.69093255623 1378618.792492289 0)), ((-75692.46671650895 1380603.39656104 0, -75294.73688792682 1380602.0172417199 0, -74897.01620656354 1380600.6566033792 0, -74499.28644014617 1380599.3142801898 0, -74101.56582418969 1380597.990637644 0, -74106.44831242497 1380192.3708799365 0, -74111.3399221295 1379786.752582277 0, -74116.22271350438 1379381.1354906242 0, -74121.11453032687 1378975.519757998 0, -74519.22613061391 1378979.8469770423 0, -74917.33749029542 1378984.1817034585 0, -75315.44863122451 1378988.5460413783 0, -75713.55953136727 1378992.9177860296 0, -75708.28599979458 1379395.5411287076 0, -75703.01282862006 1379798.1546426737 0, -75697.73964185052 1380200.780519211 0, -75692.46671650895 1380603.39656104 0)), ((-75468.69983276029 1389932.3750534386 0, -75467.8616567652 1390337.6382175677 0, -75065.09557420744 1390337.0957179184 0, -74662.33869195679 1390336.5610658142 0, -74665.88319160925 1389930.8737643668 0, -74669.42768923368 1389525.1878112464 0, -74266.6274258654 1389524.246253652 0, -73863.836080397 1389523.334947111 0, -73867.34597268527 1389117.2244490741 0, -73870.85596326522 1388711.1151060327 0, -74025.81779963558 1388709.095695478 0, -74273.70009856824 1388710.358984369 0, -74302.56273684991 1388710.5075744877 0, -74417.68247886407 1388711.0947694157 0, -74579.61531733074 1388711.9329209244 0, -74676.52891652026 1388712.4315768434 0, -74809.54693538503 1388713.123094548 0, -75068.37541876784 1388714.460442364 0, -75201.40243409414 1388715.1580922266 0, -75471.21321513873 1388716.5705587373 0, -75470.37561358031 1389121.8411721063 0, -75469.53794816439 1389527.1018386343 0, -75468.69983276029 1389932.3750534386 0)), ((-74987.86592843986 1400061.7927727944 0, -74592.41763212152 1400060.0357204955 0, -74592.36152113555 1399655.6084789867 0, -74196.47479661202 1399652.5897364027 0, -74195.98884143989 1399246.8837830767 0, -74592.30496083344 1399251.1936481358 0, -74592.24803808007 1398846.7688231007 0, -74988.99345559473 1398852.3658292615 0, -74988.62093572311 1399255.510735821 0, -75384.9366250677 1399259.8461454243 0, -75384.12560156127 1399661.7009448302 0, -75383.31418607703 1400063.5570365877 0, -74987.86592843986 1400061.7927727944 0)), ((-75344.20586881806 1408598.620260533 0, -74946.18055319267 1408595.344047859 0, -74957.519911011 1408190.7563225403 0, -75358.03838176696 1408195.1185620888 0, -75344.20586881806 1408598.620260533 0)), ((-75316.543700469 1409405.6272299301 0, -74923.50404959724 1409404.5230958904 0, -74934.84193376111 1408999.932939182 0, -75330.37430943504 1409002.1231166807 0, -75316.543700469 1409405.6272299301 0)), ((-75296.00998059571 1418348.0203656272 0, -75288.67061476 1418752.8621855217 0, -74889.48168387203 1418750.6285595133 0, -74490.29267095053 1418748.413581452 0, -74496.05214501353 1418342.6952593785 0, -74096.07768125173 1418340.0553760168 0, -74101.05160792406 1417933.9169459932 0, -74501.82085069464 1417936.978159443 0, -74902.58084391568 1417940.069452228 0, -75303.34981803682 1417943.168378233 0, -75296.00998059571 1418348.0203656272 0)), ((-76964.0919416985 1428529.823462683 0, -76963.94023052086 1428130.2179929267 0, -76963.78189812734 1427728.340506833 0, -77098.68640378973 1427730.2554828764 0, -77229.65404165904 1427732.1085600962 0, -77359.22659842776 1427733.9540327059 0, -77627.50494730953 1427737.7563790106 0, -77754.671030202 1427739.5747671456 0, -77754.78750870474 1428142.907853539 0, -77754.91058298995 1428545.4918189293 0, -77359.50605481253 1428537.6428724232 0, -76964.0919416985 1428529.823462683 0)), ((-78512.17053456653 1433414.3133732057 0, -78109.09838425247 1433427.9253300969 0, -78116.90344344855 1433023.0491050887 0, -78520.78555970703 1433008.0451054575 0, -78512.17053456653 1433414.3133732057 0)), ((-78896.41338054092 1434216.0219300934 0, -78494.9417955644 1434226.8531595692 0, -78503.55594652056 1433820.5827250672 0, -78905.82843998683 1433808.370669267 0, -78896.41338054092 1434216.0219300934 0)), ((-70953.49515491728 1372952.122442159 0, -71019.6918590828 1372979.2989408094 0, -71026.0715822088 1372979.7883610334 0, -71022.39640334132 1373268.5283425841 0, -70628.21306633759 1373263.5700373654 0, -70232.93996763245 1373258.620924124 0, -69826.7643949763 1373253.556523012 0, -69431.82376677058 1373248.6471515947 0, -69436.69929343488 1372861.9997845404 0, -69514.49779815912 1372862.6638439326 0, -69661.46054982157 1372863.924045245 0, -69666.55527973705 1372869.6515032987 0, -69721.79477338563 1372926.0323077522 0, -69766.48072406842 1372963.679957456 0, -69787.88297937764 1373001.2166222513 0, -69793.93695922014 1373011.8433724463 0, -69828.74879082786 1373039.079772869 0, -69838.64382748687 1373046.827603465 0, -69874.97496816084 1373057.779474422 0, -69892.444643586 1373054.2058328225 0, -69927.29370637753 1373047.0801674505 0, -69950.09360929824 1373042.4196189458 0, -70068.22462814557 1373006.0890960423 0, -70188.4993756712 1372969.7889536286 0, -70239.02522076802 1372954.9578025867 0, -70267.9615043276 1372946.4755888665 0, -70315.1945945062 1372933.543094523 0, -70336.86341989083 1372904.417439715 0, -70354.21590025211 1372877.9314952835 0, -70355.49736095646 1372869.9054383358 0, -70634.89106451537 1372872.326201862 0, -70815.985509982 1372873.9099045643 0, -70872.41769111576 1372911.4924396174 0, -70953.49515491728 1372952.122442159 0)), ((-72249.01456878973 1373032.1843635074 0, -72318.0605622825 1372974.170725103 0, -72363.23029181412 1372953.251534871 0, -72457.46383751903 1372956.7115436483 0, -72594.57582510167 1372957.8716177002 0, -72625.65029567882 1372956.612568816 0, -72621.40851611855 1373288.8103433535 0, -72221.65374472973 1373283.708969868 0, -72224.67773189604 1373047.0338986514 0, -72249.01456878973 1373032.1843635074 0)), ((-74094.52092507965 1381410.936449048 0, -73709.12152542871 1381404.8568224949 0, -73713.16984611681 1380998.9139183913 0, -74098.04332640096 1381004.4629501747 0, -74094.52092507965 1381410.936449048 0)), ((-74090.99841602649 1381817.4113282792 0, -74094.52092507965 1381410.936449048 0, -74489.63891101928 1381411.3867809647 0, -74484.81525016282 1381817.4249984948 0, -74090.99841602649 1381817.4113282792 0)), ((-71855.00909606219 1392346.686886785 0, -71853.16376852014 1392750.8850023635 0, -71453.61159825143 1392748.4011053084 0, -71455.95719305826 1392344.4310718684 0, -71458.3028245626 1391940.4509699827 0, -71856.8631947468 1391942.501183999 0, -71855.00909606219 1392346.686886785 0)), ((-74195.98884143989 1399246.8837830767 0, -73799.67229108275 1399242.603641443 0, -73798.74724935081 1398835.6190159754 0, -74195.49334978589 1398841.1790648103 0, -74195.98884143989 1399246.8837830767 0)), ((-74156.48231175961 1408182.0882360137 0, -74150.1295650668 1408588.8473926329 0, -74143.76820598434 1408995.6076551725 0, -73748.23568147984 1408993.4725214965 0, -73752.09487644274 1408585.6268696892 0, -73755.96308755224 1408177.782385693 0, -74156.48231175961 1408182.0882360137 0)), ((-74131.0550350306 1409809.131790904 0, -74137.41597619068 1409402.3691731342 0, -74530.45549644524 1409403.4369573516 0, -74521.61086146162 1409809.1141186522 0, -74131.0550350306 1409809.131790904 0)), ((-74081.14738505127 1419558.5112552473 0, -73683.53822816371 1419557.1986664261 0, -73687.72648080549 1419150.6131504758 0, -74086.12995795623 1419152.358171505 0, -74081.14738505127 1419558.5112552473 0)), ((-74876.37467927313 1419561.1921358241 0, -74478.76548252022 1419559.8424633353 0, -74484.52453116345 1419154.1218625633 0, -74882.92804466201 1419155.9041770976 0, -74876.37467927313 1419561.1921358241 0)), ((-74318.43308818841 1427705.9048424552 0, -74449.75485614315 1427707.0472413164 0, -74517.26780436006 1427707.6376727556 0, -74585.2738858972 1427708.2303512788 0, -74720.30329174365 1427709.4135659162 0, -74851.7137283641 1427710.562932989 0, -74983.6006213278 1427711.7205979612 0, -74984.16989560438 1428111.1264783475 0, -74984.74784969432 1428510.5224194666 0, -74985.31636275315 1428909.930466216 0, -74985.8934567793 1429309.3285677375 0, -74585.945100471 1429312.6544497365 0, -74185.9972781474 1429315.9990354313 0, -73786.04988625571 1429319.3625232258 0, -73386.10292643913 1429322.7449128935 0, -73385.87080160918 1428916.0939764348 0, -73385.64717994576 1428509.4443303 0, -73385.41432782568 1428102.7956215697 0, -73385.18997872937 1427696.1482061304 0, -73645.85459001745 1427700.0729754742 0, -73785.22033651509 1427701.2765981138 0, -73917.42501024819 1427702.4226001978 0, -74047.8048176935 1427703.5505486066 0, -74116.27538136691 1427704.146157783 0, -74185.2472052346 1427704.7440669923 0, -74318.43308818841 1427705.9048424552 0)), ((-74876.20642381509 1438273.0679456573 0, -74874.34310515421 1438679.3341558017 0, -74872.48870917276 1439085.6014214135 0, -74467.62325541282 1439080.7690335612 0, -74062.75760881112 1439075.9559269308 0, -73657.89156993396 1439071.1621960572 0, -73253.02524569955 1439066.3876421822 0, -73260.93763766639 1438661.4602670039 0, -73268.85055207222 1438256.533855518 0, -73276.76378777856 1437851.6085038518 0, -73284.67744072834 1437446.6843174647 0, -73683.48474600783 1437450.1198034221 0, -74082.3008800325 1437453.5740444446 0, -74481.10790105989 1437457.0469818453 0, -74879.92364547713 1437460.5387723357 0, -74878.06062595797 1437866.802730469 0, -74876.20642381509 1438273.0679456573 0)), ((-70213.60124323776 1374454.2487342053 0, -70210.10651071917 1374859.2131047058 0, -69811.97613065888 1374854.8975020647 0, -69815.70529598196 1374450.8975964328 0, -70213.60124323776 1374454.2487342053 0)), ((-71009.39271226941 1374460.9952794784 0, -71006.37551234754 1374867.899958987 0, -70608.24565254695 1374863.5473093514 0, -70611.4971781951 1374457.6070969377 0, -71009.39271226941 1374460.9952794784 0)), ((-69409.8728652747 1375253.636973216 0, -69413.84549293386 1374850.6004227311 0, -69811.97613065888 1374854.8975020647 0, -69808.24705624035 1375258.898602443 0, -69409.8728652747 1375253.636973216 0)), ((-70604.985186337 1375269.4887509488 0, -70601.7337257383 1375675.431473517 0, -70482.24152603654 1375673.5412024194 0, -70203.12598033666 1375669.1570197172 0, -70206.62074254548 1375264.1900535333 0, -70604.985186337 1375269.4887509488 0)), ((-69740.44777462445 1383767.8050050468 0, -69735.59705701222 1384174.0902394976 0, -69339.28257034115 1384167.6476691056 0, -69344.29053304801 1383760.7255553638 0, -69740.44777462445 1383767.8050050468 0)), ((-70911.36652364708 1385406.5695318102 0, -70514.59020788902 1385402.0049691063 0, -70117.81372568327 1385397.4587880285 0, -70122.50668783911 1384991.8178367654 0, -69725.88709814323 1384986.6532405412 0, -69730.73754574491 1384580.3654656312 0, -70127.20885830084 1384586.1782313664 0, -70131.90219298856 1384180.5399160986 0, -70136.60454090746 1383774.902842589 0, -70532.76083332341 1383782.018967234 0, -70928.91654507452 1383789.153577652 0, -70924.52894652775 1384193.505677314 0, -70920.14134404415 1384597.8590351369 0, -70915.75393577742 1385002.2136558397 0, -70911.36652364708 1385406.5695318102 0)), ((-69062.78291947489 1392320.5273774997 0, -69064.34148999891 1391916.5409425197 0, -69463.55199448287 1391921.4848942056 0, -69862.76237706737 1391926.436306634 0, -69860.3142784658 1392330.2027878764 0, -69857.8662621767 1392733.970606617 0, -69459.54534865153 1392729.2279475818 0, -69061.22427092413 1392724.503845289 0, -69062.78291947489 1392320.5273774997 0)), ((-69455.53813403368 1393536.9760241495 0, -69452.65938258557 1393942.971819392 0, -69055.15567404097 1393938.5789539025 0, -69058.10626890894 1393532.471774508 0, -69455.53813403368 1393536.9760241495 0)), ((-69844.55749505378 1394759.1780290762 0, -69847.36464079762 1394353.29115373 0, -70244.9395250728 1394357.6208219528 0, -70247.79165474746 1393951.8251824423 0, -69850.16278623152 1393947.394332721 0, -69852.96983540723 1393541.4987241838 0, -70250.63470643398 1393546.0418014273 0, -70647.83223896606 1393550.599662106 0, -70645.16873844223 1393956.2836919893 0, -70642.51424380059 1394361.9689368922 0, -70639.85060989897 1394767.6554350534 0, -70243.56919730378 1394763.4186952491 0, -70242.18958338154 1395169.2289247052 0, -69841.75920716678 1395165.0774173578 0, -69844.55749505378 1394759.1780290762 0)), ((-69046.32167429027 1395156.8857596773 0, -69049.26337514754 1394750.7859983926 0, -69446.91063636221 1394754.9671932866 0, -69444.04049968858 1395160.9779685102 0, -69046.32167429027 1395156.8857596773 0)), ((-70603.83059042333 1400446.8798159915 0, -70603.7545996068 1400041.5677893285 0, -71004.32930492684 1400044.0445263677 0, -71005.75502999102 1400449.8941315806 0, -70603.83059042333 1400446.8798159915 0)), ((-69403.41059370458 1403275.3964976284 0, -69801.42058359813 1403279.9238526311 0, -70199.4304030552 1403284.4698212517 0, -70198.7778880352 1403686.5722776775 0, -69800.68844473343 1403683.089244046 0, -69402.60781524987 1403679.6360004465 0, -69403.41059370458 1403275.3964976284 0)), ((-70198.11618676876 1404088.664636489 0, -70596.27631636243 1404091.0921564563 0, -70595.6941405752 1404492.1228527282 0, -70595.11166102947 1404893.1547236193 0, -70196.80098751538 1404892.8753879382 0, -70197.46315236835 1404490.7694593165 0, -70198.11618676876 1404088.664636489 0)), ((-69400.18893704774 1404892.3615886432 0, -69001.88766540117 1404892.1270269607 0, -69002.76161471274 1404486.8210224414 0, -69401.00139749574 1404488.1185842736 0, -69400.18893704774 1404892.3615886432 0)), ((-70545.15914766671 1413410.9366349091 0, -70541.78141307188 1413819.215332436 0, -70538.40361314353 1414227.5064070616 0, -70535.02593501545 1414635.7874525802 0, -70136.21082806465 1414626.9618901764 0, -69737.40395675269 1414618.1549751363 0, -69338.58747681546 1414609.3667545991 0, -68939.77923270661 1414600.5972821424 0, -68943.04578828329 1414196.569780583 0, -68946.31247616025 1413792.5322308638 0, -68949.5790103671 1413388.5070358743 0, -68952.84567366229 1412984.471896546 0, -69351.76440114896 1412988.987850601 0, -69750.69178006143 1412993.5225547545 0, -70149.60996886369 1412998.0758547804 0, -70548.53690180369 1413002.6480090981 0, -70545.15914766671 1413410.9366349091 0)), ((-69708.50492957396 1423576.1603419692 0, -69705.8504734138 1423984.7092345366 0, -70104.94408499658 1423988.928120578 0, -70102.60242439799 1424397.3575527621 0, -69703.18701638676 1424393.2479814028 0, -69303.7625140672 1424389.1571624617 0, -68904.3466650034 1424385.0850463337 0, -68907.6536168998 1423976.3274707596 0, -68910.96058835229 1423567.5597278709 0, -68914.26748423825 1423158.804429739 0, -68917.5744954963 1422750.0390713415 0, -69315.70316340054 1422754.5488396653 0, -69312.7180456523 1423163.2047869696 0, -69711.16823677675 1423167.62377168 0, -69713.83155835344 1422759.0772403746 0, -70111.95967564765 1422763.6243744425 0, -70510.0875197999 1422768.19004028 0, -70508.06789161041 1423176.5178381486 0, -70506.0572974234 1423584.835757219 0, -70107.28566165765 1423580.4887219206 0, -69708.50492957396 1423576.1603419692 0)), ((-69771.85063772494 1432551.3163925102 0, -70164.40496803727 1432555.8222495795 0, -70162.41388179794 1432962.0498513037 0, -70160.43164648437 1433368.267320758 0, -69769.44565835792 1433364.6253224395 0, -69770.65264634372 1432957.9759487123 0, -69378.88230679517 1432953.9200517014 0, -69379.30494373004 1432546.8286978265 0, -69771.85063772494 1432551.3163925102 0)), ((-69378.02737593632 1433768.094779332 0, -69768.23840378977 1433771.2869971872 0, -70158.4403278608 1433774.4971121536 0, -70156.4578602995 1434180.7167682713 0, -69767.03082560771 1434177.9498641943 0, -69377.6038540263 1434175.1895309247 0, -69378.02737593632 1433768.094779332 0)), ((-70130.49985360415 1442281.6832412176 0, -70122.73211840098 1442687.8858087463 0, -70114.96492823254 1443094.078326822 0, -70107.19800006023 1443500.282997227 0, -69708.48092107165 1443498.9075806611 0, -69714.0371446723 1443092.068512529 0, -69313.11830475403 1443090.077831705 0, -69320.51834354026 1442682.5939849466 0, -68917.8528773215 1442679.9694564538 0, -68923.51551297866 1442271.8452614627 0, -69327.92755040913 1442275.1224779438 0, -69723.15001884844 1442278.3437871775 0, -70130.49985360415 1442281.6832412176 0)), ((-66175.28684677364 1380084.7482948548 0, -66169.74941031153 1380492.0659141543 0, -65774.8175668997 1380483.4592752825 0, -65379.89412173236 1380474.8597105802 0, -64984.96094867513 1380466.2895660144 0, -64590.036176994814 1380457.7264955349 0, -64592.74806583639 1380051.2491116796 0, -64595.46000924576 1379644.7730219816 0, -64598.171905066934 1379238.298325654 0, -64600.883660296364 1378831.8248194347 0, -64998.63423017764 1378839.536133617 0, -65396.393268404936 1378847.2659360964 0, -65794.14272907938 1378855.0141704897 0, -66191.90054967553 1378862.7810919194 0, -66186.36236543983 1379270.1059311088 0, -66180.82459139584 1379677.4208681337 0, -66175.28684677364 1380084.7482948548 0)), ((-65514.4720704723 1388652.6398153561 0, -65604.00066048065 1388653.8696493935 0, -65703.42297601527 1388655.2305463082 0, -65911.81160324326 1388658.0982929314 0, -65912.4738433709 1389061.6665306892 0, -65913.1357466665 1389465.2359154678 0, -65913.79730710333 1389868.8066474802 0, -65914.45852782854 1390272.37862445 0, -65517.19322739473 1390269.3271651533 0, -65119.9368022681 1390266.2943426184 0, -64722.67121719025 1390263.2798975292 0, -64325.41461276027 1390260.2839911531 0, -64329.12665142282 1389856.7452634894 0, -64332.838660103254 1389453.2078730566 0, -64336.55084298443 1389049.6716257955 0, -64340.26309791693 1388646.1366208973 0, -64506.31640641752 1388638.879027665 0, -64737.66622302548 1388642.0256413866 0, -64905.35526924965 1388644.3146564267 0, -65134.97950889761 1388647.447671809 0, -65304.38476451703 1388649.7688774562 0, -65514.4720704723 1388652.6398153561 0)), ((-65846.22910086627 1400001.9358505697 0, -65449.71579343671 1400004.019515677 0, -65053.20290154075 1400006.110389473 0, -64656.69024194073 1400008.2308740187 0, -64260.17799798589 1400010.3586677383 0, -64262.91738809907 1399601.2413231283 0, -64265.66574135033 1399192.1253916223 0, -64268.40502494338 1398783.0105138829 0, -64271.15327161535 1398373.8970522282 0, -64666.66343185949 1398377.751502045 0, -65062.173484246916 1398381.613174043 0, -65457.683245613436 1398385.5043694987 0, -65853.19279997265 1398389.4026834026 0, -65851.44762681382 1398792.5342293603 0, -65849.71125345805 1399195.666857219 0, -65847.96573075716 1399598.8007119857 0, -65846.22910086627 1400001.9358505697 0)), ((-65786.46958184676 1409302.1884285444 0, -65785.09243110886 1409704.9294377803 0, -65389.37910808575 1409704.4458165206 0, -65390.58128043699 1409301.0541317419 0, -64994.692992200136 1409299.9494150167 0, -64993.67500206093 1409703.9695483516 0, -64597.96199598496 1409703.5226779059 0, -64202.258110991854 1409703.0831571503 0, -64202.90761649966 1409297.783827929 0, -64203.565993228156 1408892.4858636104 0, -64204.215107253905 1408487.1890016843 0, -64204.87289737453 1408081.8934005369 0, -64601.30501046832 1408084.879903502 0, -64997.7457971499 1408087.8849645872 0, -65394.177617009336 1408090.908335503 0, -65790.6182062984 1408093.950267919 0, -65789.23246797592 1408496.6988925857 0, -65392.984996478604 1408494.285377825 0, -65391.783180270635 1408897.6748198008 0, -65787.85566676607 1408899.4375657488 0, -65786.46958184676 1409302.1884285444 0)), ((-65354.38810012556 1418657.1851876287 0, -65752.91688147366 1418657.8927709209 0, -65751.14489716385 1419064.0835945304 0, -65749.38184264915 1419470.2643415802 0, -65350.71928510125 1419469.7796384334 0, -64952.06580249973 1419469.3137552561 0, -64553.40346166067 1419468.8664330922 0, -64154.75020208084 1419468.4378296926 0, -64156.78071240717 1419061.8112300108 0, -64158.811223340694 1418655.1745783584 0, -64160.841445873215 1418248.5503785932 0, -64162.871770954276 1417841.916032148 0, -64561.266508017914 1417842.79055173 0, -64959.66140734351 1417843.6836199658 0, -65358.05626615242 1417844.5953316747 0, -65756.45128088201 1417845.52569322 0, -65754.67956836389 1418251.7142168777 0, -65356.22222841105 1418250.8953365244 0, -64957.76485002984 1418250.094996921 0, -64955.85937393276 1418656.4963478495 0, -65354.38810012556 1418657.1851876287 0)), ((-67326.66458140808 1421928.3466211436 0, -66930.53828043274 1421925.4564285874 0, -66534.40797293658 1421922.5840391258 0, -66537.91601416412 1421515.7603839226 0, -66541.4329463198 1421108.9379438155 0, -66936.23968048696 1421110.7362918213 0, -67331.05162705018 1421112.552426695 0, -67328.85817000733 1421520.449002016 0, -67326.66458140808 1421928.3466211436 0)), ((-67320.43453546241 1423149.5074987488 0, -67322.27719555334 1422744.1453943504 0, -67721.10143391095 1422745.5963699 0, -68119.92585867815